<commit_message>
Harmonized ReadMe directions and model guide and main readme.
Starting to update the guide and links from the spreadsheet to it.
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4F2B39-81C2-448D-A346-621FC1D6CB48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AED6EB-FB37-4854-8CE8-3C7921535987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-1200" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="62" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="360">
   <si>
     <t>Year 1</t>
   </si>
@@ -711,29 +711,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Number of People:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 2 or more (facilitator may also participate).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>Time:</t>
     </r>
     <r>
@@ -745,29 +722,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> 1 to 3 hours.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Software:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Facilitator has a Google Account.</t>
     </r>
   </si>
   <si>
@@ -997,21 +951,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> worksheet.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Facilitator: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 person to setup in Google Sheets (see Setup below), invite participants, and organize play.</t>
     </r>
   </si>
   <si>
@@ -1291,74 +1230,6 @@
     <t>A transformation uses percentage splits of shortages to specify percentage splits of Lake Mead Inflow.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">a. For example, in Rows 4-10, particants select a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>User</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and enter a the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>User's vulneravility</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>strategy to manage vulnerability</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>. If fewer than 6 participants, participants select multiple parties.</t>
-    </r>
-  </si>
-  <si>
     <t>Make a copy before use. Use to play. This worksheet allows comparison to current (Law of River) operations. See Today-Plots. [[Feature not yet enabled]]</t>
   </si>
   <si>
@@ -1581,9 +1452,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">    2) Provoke discussion about new alternatives for Colorado River management post 2026.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">View the </t>
     </r>
@@ -1637,6 +1505,106 @@
   </si>
   <si>
     <t xml:space="preserve">     Remaining Storage above Protect and ICS Balances (maf)</t>
+  </si>
+  <si>
+    <t>Tribal Nations of the Lower Basin</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enter the Lake Mead starting storage in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Cell B19</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Find the current storage at https://www.usbr.gov/lc/region/g4000/hourly/mead-elv.html</t>
+    </r>
+  </si>
+  <si>
+    <t>DIRECTIONS to GUIDE a MODEL SESSION</t>
+  </si>
+  <si>
+    <r>
+      <t>The purpose of this tool is to give users the opportunity to immerse in water user roles and experiment with a Lake Mead Water Bank. The Bank works on the principles of</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> A) Divide reservoir inflow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>B) Subtract evaporation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, and</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> C) Users withdraw and conserve within their available water</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, others choices, and real-time discussion of choices. We see uses of the tool for two purposes:</t>
+    </r>
   </si>
   <si>
     <r>
@@ -1724,7 +1692,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> basin partners manage their risk of uncertain future water supply; </t>
+      <t xml:space="preserve"> basin partners articulate their risk of uncertain future water supply and manage their vulnerability; and </t>
     </r>
     <r>
       <rPr>
@@ -1749,22 +1717,8 @@
     </r>
   </si>
   <si>
-    <t>Tribal Nations of the Lower Basin</t>
-  </si>
-  <si>
     <r>
-      <t xml:space="preserve">Enter the Lake Mead starting storage in </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Cell B19</t>
+      <t xml:space="preserve">Session Guide: </t>
     </r>
     <r>
       <rPr>
@@ -1774,13 +1728,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>. Find the current storage at https://www.usbr.gov/lc/region/g4000/hourly/mead-elv.html</t>
+      <t>1 person to setup in Google Sheets (see Setup below), invite participants, and organize play.</t>
     </r>
   </si>
   <si>
-    <r>
-      <t>The purpose of this tool is to give users the opportunity to experiment with a Lake Mead Water Bank. The Bank works on the principles of</t>
-    </r>
+    <t xml:space="preserve">    2) Provoke discussion about new alternatives for Colorado River management post 2026 and their possible benefits to:</t>
+  </si>
+  <si>
+    <t>a) 	Stabilize and recover reservoir storage under conditions of low storage and low inflow, and</t>
+  </si>
+  <si>
+    <t>b) Give users more autonomy to manage their vulnerability to water shortages more independently of other users.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -1790,7 +1750,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> A) Divide reservoir inflow</t>
+      <t>Number of People:</t>
     </r>
     <r>
       <rPr>
@@ -1800,8 +1760,10 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">, </t>
+      <t xml:space="preserve"> 2 or more (Session guide may also participate).</t>
     </r>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -1811,7 +1773,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>B) Subtract evaporation</t>
+      <t>Software:</t>
     </r>
     <r>
       <rPr>
@@ -1821,32 +1783,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, and</t>
+      <t xml:space="preserve"> Session Guide has a Google Account.</t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> C) Users withdraw and conserve within their available water</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, others choices, and real-time discussion of choices. We see uses of the tool for two purposes:</t>
-    </r>
-  </si>
-  <si>
-    <t>DIRECTIONS to GUIDE a MODEL SESSION</t>
   </si>
   <si>
     <r>
@@ -1871,11 +1809,102 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> Worksheet toto work on in this session and save a blank version for later use.</t>
+      <t xml:space="preserve"> Worksheet to work on in this session and save a blank version for later use.</t>
     </r>
   </si>
   <si>
-    <t>Test</t>
+    <r>
+      <t xml:space="preserve">a. For example, in Rows 4-10, particants select a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> articulate the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>User's vulneravility to water shortages,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and define a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>strategy to manage vulnerability</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. If fewer than 6 participants, participants select multiple users.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">In  Cell </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>B21</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, enter the total Water Conservation Account (Intentionally Created Surplus) Balance. This value includes California, Arizona, Nevada, and Mexico.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2519,7 +2548,7 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="320">
+  <cellXfs count="321">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3147,6 +3176,57 @@
     <xf numFmtId="171" fontId="0" fillId="28" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3174,13 +3254,7 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3210,12 +3284,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3233,45 +3301,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3333,12 +3362,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3381,6 +3404,12 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3401,6 +3430,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -14797,10 +14829,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EA02F4-5F19-409C-8BC6-A0D8FEB3A90D}">
-  <dimension ref="A1:R67"/>
+  <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48:XFD48"/>
+    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14819,20 +14851,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="238" t="s">
-        <v>324</v>
-      </c>
-      <c r="B1" s="238"/>
-      <c r="C1" s="238"/>
-      <c r="D1" s="238"/>
-      <c r="E1" s="238"/>
-      <c r="F1" s="238"/>
-      <c r="G1" s="238"/>
-      <c r="H1" s="238"/>
-      <c r="I1" s="238"/>
-      <c r="J1" s="238"/>
-      <c r="K1" s="238"/>
-      <c r="L1" s="238"/>
+      <c r="A1" s="255" t="s">
+        <v>321</v>
+      </c>
+      <c r="B1" s="255"/>
+      <c r="C1" s="255"/>
+      <c r="D1" s="255"/>
+      <c r="E1" s="255"/>
+      <c r="F1" s="255"/>
+      <c r="G1" s="255"/>
+      <c r="H1" s="255"/>
+      <c r="I1" s="255"/>
+      <c r="J1" s="255"/>
+      <c r="K1" s="255"/>
+      <c r="L1" s="255"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -14858,41 +14890,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="239" t="s">
-        <v>354</v>
-      </c>
-      <c r="B4" s="240"/>
-      <c r="C4" s="240"/>
-      <c r="D4" s="240"/>
-      <c r="E4" s="240"/>
-      <c r="F4" s="240"/>
-      <c r="G4" s="240"/>
-      <c r="H4" s="240"/>
-      <c r="I4" s="240"/>
-      <c r="J4" s="240"/>
-      <c r="K4" s="240"/>
-      <c r="L4" s="241"/>
-      <c r="N4" s="242"/>
-      <c r="O4" s="242"/>
-      <c r="P4" s="242"/>
-      <c r="Q4" s="242"/>
-      <c r="R4" s="242"/>
+      <c r="A4" s="256" t="s">
+        <v>349</v>
+      </c>
+      <c r="B4" s="257"/>
+      <c r="C4" s="257"/>
+      <c r="D4" s="257"/>
+      <c r="E4" s="257"/>
+      <c r="F4" s="257"/>
+      <c r="G4" s="257"/>
+      <c r="H4" s="257"/>
+      <c r="I4" s="257"/>
+      <c r="J4" s="257"/>
+      <c r="K4" s="257"/>
+      <c r="L4" s="258"/>
+      <c r="N4" s="259"/>
+      <c r="O4" s="259"/>
+      <c r="P4" s="259"/>
+      <c r="Q4" s="259"/>
+      <c r="R4" s="259"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="243" t="s">
-        <v>351</v>
-      </c>
-      <c r="B5" s="244"/>
-      <c r="C5" s="244"/>
-      <c r="D5" s="244"/>
-      <c r="E5" s="244"/>
-      <c r="F5" s="244"/>
-      <c r="G5" s="244"/>
-      <c r="H5" s="244"/>
-      <c r="I5" s="244"/>
-      <c r="J5" s="244"/>
-      <c r="K5" s="244"/>
-      <c r="L5" s="245"/>
+      <c r="A5" s="260" t="s">
+        <v>350</v>
+      </c>
+      <c r="B5" s="320"/>
+      <c r="C5" s="320"/>
+      <c r="D5" s="320"/>
+      <c r="E5" s="320"/>
+      <c r="F5" s="320"/>
+      <c r="G5" s="320"/>
+      <c r="H5" s="320"/>
+      <c r="I5" s="320"/>
+      <c r="J5" s="320"/>
+      <c r="K5" s="320"/>
+      <c r="L5" s="261"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -14900,871 +14932,935 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="246" t="s">
-        <v>347</v>
-      </c>
-      <c r="B6" s="247"/>
-      <c r="C6" s="247"/>
-      <c r="D6" s="247"/>
-      <c r="E6" s="247"/>
-      <c r="F6" s="247"/>
-      <c r="G6" s="247"/>
-      <c r="H6" s="247"/>
-      <c r="I6" s="247"/>
-      <c r="J6" s="247"/>
-      <c r="K6" s="247"/>
-      <c r="L6" s="248"/>
+      <c r="A6" s="260" t="s">
+        <v>352</v>
+      </c>
+      <c r="B6" s="320"/>
+      <c r="C6" s="320"/>
+      <c r="D6" s="320"/>
+      <c r="E6" s="320"/>
+      <c r="F6" s="320"/>
+      <c r="G6" s="320"/>
+      <c r="H6" s="320"/>
+      <c r="I6" s="320"/>
+      <c r="J6" s="320"/>
+      <c r="K6" s="320"/>
+      <c r="L6" s="261"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
       <c r="Q6" s="113"/>
       <c r="R6" s="113"/>
     </row>
-    <row r="7" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="113"/>
-      <c r="B7" s="113"/>
-      <c r="C7" s="113"/>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="113"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="113"/>
-      <c r="J7" s="113"/>
-      <c r="K7" s="113"/>
-      <c r="L7" s="113"/>
-    </row>
-    <row r="8" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="249" t="s">
+    <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="235"/>
+      <c r="B7" s="320" t="s">
+        <v>353</v>
+      </c>
+      <c r="C7" s="320"/>
+      <c r="D7" s="320"/>
+      <c r="E7" s="320"/>
+      <c r="F7" s="320"/>
+      <c r="G7" s="320"/>
+      <c r="H7" s="320"/>
+      <c r="I7" s="320"/>
+      <c r="J7" s="320"/>
+      <c r="K7" s="320"/>
+      <c r="L7" s="261"/>
+      <c r="N7" s="113"/>
+      <c r="O7" s="113"/>
+      <c r="P7" s="113"/>
+      <c r="Q7" s="113"/>
+      <c r="R7" s="113"/>
+    </row>
+    <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="236"/>
+      <c r="B8" s="262" t="s">
+        <v>354</v>
+      </c>
+      <c r="C8" s="262"/>
+      <c r="D8" s="262"/>
+      <c r="E8" s="262"/>
+      <c r="F8" s="262"/>
+      <c r="G8" s="262"/>
+      <c r="H8" s="262"/>
+      <c r="I8" s="262"/>
+      <c r="J8" s="262"/>
+      <c r="K8" s="262"/>
+      <c r="L8" s="263"/>
+      <c r="N8" s="113"/>
+      <c r="O8" s="113"/>
+      <c r="P8" s="113"/>
+      <c r="Q8" s="113"/>
+      <c r="R8" s="113"/>
+    </row>
+    <row r="9" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="113"/>
+      <c r="B9" s="113"/>
+      <c r="C9" s="113"/>
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
+      <c r="G9" s="113"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="113"/>
+      <c r="J9" s="113"/>
+      <c r="K9" s="113"/>
+      <c r="L9" s="113"/>
+    </row>
+    <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="264" t="s">
         <v>217</v>
       </c>
-      <c r="B8" s="250"/>
-      <c r="C8" s="250"/>
-      <c r="D8" s="250"/>
-      <c r="E8" s="250"/>
-      <c r="F8" s="250"/>
-      <c r="G8" s="250"/>
-      <c r="H8" s="250"/>
-      <c r="I8" s="250"/>
-      <c r="J8" s="250"/>
-      <c r="K8" s="250"/>
-      <c r="L8" s="251"/>
-    </row>
-    <row r="9" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="252" t="s">
-        <v>236</v>
-      </c>
-      <c r="B9" s="253"/>
-      <c r="C9" s="253"/>
-      <c r="D9" s="253"/>
-      <c r="E9" s="253"/>
-      <c r="F9" s="253"/>
-      <c r="G9" s="253"/>
-      <c r="H9" s="253"/>
-      <c r="I9" s="253"/>
-      <c r="J9" s="253"/>
-      <c r="K9" s="253"/>
-      <c r="L9" s="254"/>
-    </row>
-    <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="255" t="s">
+      <c r="B10" s="265"/>
+      <c r="C10" s="265"/>
+      <c r="D10" s="265"/>
+      <c r="E10" s="265"/>
+      <c r="F10" s="265"/>
+      <c r="G10" s="265"/>
+      <c r="H10" s="265"/>
+      <c r="I10" s="265"/>
+      <c r="J10" s="265"/>
+      <c r="K10" s="265"/>
+      <c r="L10" s="266"/>
+    </row>
+    <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="267" t="s">
+        <v>351</v>
+      </c>
+      <c r="B11" s="268"/>
+      <c r="C11" s="268"/>
+      <c r="D11" s="268"/>
+      <c r="E11" s="268"/>
+      <c r="F11" s="268"/>
+      <c r="G11" s="268"/>
+      <c r="H11" s="268"/>
+      <c r="I11" s="268"/>
+      <c r="J11" s="268"/>
+      <c r="K11" s="268"/>
+      <c r="L11" s="269"/>
+    </row>
+    <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="270" t="s">
+        <v>355</v>
+      </c>
+      <c r="B12" s="247"/>
+      <c r="C12" s="247"/>
+      <c r="D12" s="247"/>
+      <c r="E12" s="247"/>
+      <c r="F12" s="247"/>
+      <c r="G12" s="247"/>
+      <c r="H12" s="247"/>
+      <c r="I12" s="247"/>
+      <c r="J12" s="247"/>
+      <c r="K12" s="247"/>
+      <c r="L12" s="248"/>
+    </row>
+    <row r="13" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="270" t="s">
         <v>218</v>
       </c>
-      <c r="B10" s="256"/>
-      <c r="C10" s="256"/>
-      <c r="D10" s="256"/>
-      <c r="E10" s="256"/>
-      <c r="F10" s="256"/>
-      <c r="G10" s="256"/>
-      <c r="H10" s="256"/>
-      <c r="I10" s="256"/>
-      <c r="J10" s="256"/>
-      <c r="K10" s="256"/>
-      <c r="L10" s="257"/>
-    </row>
-    <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="255" t="s">
-        <v>219</v>
-      </c>
-      <c r="B11" s="256"/>
-      <c r="C11" s="256"/>
-      <c r="D11" s="256"/>
-      <c r="E11" s="256"/>
-      <c r="F11" s="256"/>
-      <c r="G11" s="256"/>
-      <c r="H11" s="256"/>
-      <c r="I11" s="256"/>
-      <c r="J11" s="256"/>
-      <c r="K11" s="256"/>
-      <c r="L11" s="257"/>
-    </row>
-    <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="258" t="s">
-        <v>220</v>
-      </c>
-      <c r="B12" s="259"/>
-      <c r="C12" s="259"/>
-      <c r="D12" s="259"/>
-      <c r="E12" s="259"/>
-      <c r="F12" s="259"/>
-      <c r="G12" s="259"/>
-      <c r="H12" s="259"/>
-      <c r="I12" s="259"/>
-      <c r="J12" s="259"/>
-      <c r="K12" s="259"/>
-      <c r="L12" s="260"/>
-    </row>
-    <row r="13" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="113"/>
-      <c r="B13" s="113"/>
-      <c r="C13" s="113"/>
-      <c r="D13" s="113"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="113"/>
-      <c r="G13" s="113"/>
-      <c r="H13" s="113"/>
-      <c r="I13" s="113"/>
-      <c r="J13" s="113"/>
-      <c r="K13" s="113"/>
-      <c r="L13" s="113"/>
-    </row>
-    <row r="14" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="261" t="s">
-        <v>355</v>
-      </c>
-      <c r="B14" s="262"/>
-      <c r="C14" s="262"/>
-      <c r="D14" s="262"/>
-      <c r="E14" s="262"/>
-      <c r="F14" s="262"/>
-      <c r="G14" s="262"/>
-      <c r="H14" s="262"/>
-      <c r="I14" s="262"/>
-      <c r="J14" s="262"/>
-      <c r="K14" s="262"/>
-      <c r="L14" s="263"/>
-      <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="235" t="s">
-        <v>229</v>
-      </c>
-      <c r="B15" s="236"/>
-      <c r="C15" s="236"/>
-      <c r="D15" s="236"/>
-      <c r="E15" s="236"/>
-      <c r="F15" s="236"/>
-      <c r="G15" s="236"/>
-      <c r="H15" s="236"/>
-      <c r="I15" s="236"/>
-      <c r="J15" s="236"/>
-      <c r="K15" s="236"/>
-      <c r="L15" s="237"/>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:18" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="230">
-        <v>1</v>
-      </c>
-      <c r="B16" s="266" t="s">
-        <v>228</v>
-      </c>
-      <c r="C16" s="266"/>
-      <c r="D16" s="266"/>
-      <c r="E16" s="266"/>
-      <c r="F16" s="266"/>
-      <c r="G16" s="266"/>
-      <c r="H16" s="266"/>
-      <c r="I16" s="266"/>
-      <c r="J16" s="266"/>
-      <c r="K16" s="266"/>
-      <c r="L16" s="267"/>
-    </row>
-    <row r="17" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="230">
-        <v>2</v>
-      </c>
-      <c r="B17" s="266" t="s">
-        <v>349</v>
-      </c>
-      <c r="C17" s="266"/>
-      <c r="D17" s="266"/>
-      <c r="E17" s="266"/>
-      <c r="F17" s="266"/>
-      <c r="G17" s="266"/>
-      <c r="H17" s="266"/>
-      <c r="I17" s="266"/>
-      <c r="J17" s="266"/>
-      <c r="K17" s="266"/>
-      <c r="L17" s="267"/>
-      <c r="N17" s="106"/>
+      <c r="B13" s="247"/>
+      <c r="C13" s="247"/>
+      <c r="D13" s="247"/>
+      <c r="E13" s="247"/>
+      <c r="F13" s="247"/>
+      <c r="G13" s="247"/>
+      <c r="H13" s="247"/>
+      <c r="I13" s="247"/>
+      <c r="J13" s="247"/>
+      <c r="K13" s="247"/>
+      <c r="L13" s="248"/>
+    </row>
+    <row r="14" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="271" t="s">
+        <v>356</v>
+      </c>
+      <c r="B14" s="272"/>
+      <c r="C14" s="272"/>
+      <c r="D14" s="272"/>
+      <c r="E14" s="272"/>
+      <c r="F14" s="272"/>
+      <c r="G14" s="272"/>
+      <c r="H14" s="272"/>
+      <c r="I14" s="272"/>
+      <c r="J14" s="272"/>
+      <c r="K14" s="272"/>
+      <c r="L14" s="273"/>
+    </row>
+    <row r="15" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="113"/>
+      <c r="B15" s="113"/>
+      <c r="C15" s="113"/>
+      <c r="D15" s="113"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="113"/>
+      <c r="G15" s="113"/>
+      <c r="H15" s="113"/>
+      <c r="I15" s="113"/>
+      <c r="J15" s="113"/>
+      <c r="K15" s="113"/>
+      <c r="L15" s="113"/>
+    </row>
+    <row r="16" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="274" t="s">
+        <v>348</v>
+      </c>
+      <c r="B16" s="275"/>
+      <c r="C16" s="275"/>
+      <c r="D16" s="275"/>
+      <c r="E16" s="275"/>
+      <c r="F16" s="275"/>
+      <c r="G16" s="275"/>
+      <c r="H16" s="275"/>
+      <c r="I16" s="275"/>
+      <c r="J16" s="275"/>
+      <c r="K16" s="275"/>
+      <c r="L16" s="276"/>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="252" t="s">
+        <v>227</v>
+      </c>
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="253"/>
+      <c r="J17" s="253"/>
+      <c r="K17" s="253"/>
+      <c r="L17" s="254"/>
+      <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="230">
-        <v>3</v>
-      </c>
-      <c r="B18" s="266" t="s">
-        <v>221</v>
-      </c>
-      <c r="C18" s="266"/>
-      <c r="D18" s="266"/>
-      <c r="E18" s="266"/>
-      <c r="F18" s="266"/>
-      <c r="G18" s="266"/>
-      <c r="H18" s="266"/>
-      <c r="I18" s="266"/>
-      <c r="J18" s="266"/>
-      <c r="K18" s="266"/>
-      <c r="L18" s="267"/>
-      <c r="N18" s="106"/>
-    </row>
-    <row r="19" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="B18" s="240" t="s">
+        <v>226</v>
+      </c>
+      <c r="C18" s="240"/>
+      <c r="D18" s="240"/>
+      <c r="E18" s="240"/>
+      <c r="F18" s="240"/>
+      <c r="G18" s="240"/>
+      <c r="H18" s="240"/>
+      <c r="I18" s="240"/>
+      <c r="J18" s="240"/>
+      <c r="K18" s="240"/>
+      <c r="L18" s="241"/>
+    </row>
+    <row r="19" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="230">
-        <v>4</v>
-      </c>
-      <c r="B19" s="266" t="s">
-        <v>356</v>
-      </c>
-      <c r="C19" s="266"/>
-      <c r="D19" s="266"/>
-      <c r="E19" s="266"/>
-      <c r="F19" s="266"/>
-      <c r="G19" s="266"/>
-      <c r="H19" s="266"/>
-      <c r="I19" s="266"/>
-      <c r="J19" s="266"/>
-      <c r="K19" s="266"/>
-      <c r="L19" s="267"/>
+        <v>2</v>
+      </c>
+      <c r="B19" s="240" t="s">
+        <v>344</v>
+      </c>
+      <c r="C19" s="240"/>
+      <c r="D19" s="240"/>
+      <c r="E19" s="240"/>
+      <c r="F19" s="240"/>
+      <c r="G19" s="240"/>
+      <c r="H19" s="240"/>
+      <c r="I19" s="240"/>
+      <c r="J19" s="240"/>
+      <c r="K19" s="240"/>
+      <c r="L19" s="241"/>
       <c r="N19" s="106"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="230">
+        <v>3</v>
+      </c>
+      <c r="B20" s="240" t="s">
+        <v>219</v>
+      </c>
+      <c r="C20" s="240"/>
+      <c r="D20" s="240"/>
+      <c r="E20" s="240"/>
+      <c r="F20" s="240"/>
+      <c r="G20" s="240"/>
+      <c r="H20" s="240"/>
+      <c r="I20" s="240"/>
+      <c r="J20" s="240"/>
+      <c r="K20" s="240"/>
+      <c r="L20" s="241"/>
+      <c r="N20" s="106"/>
+    </row>
+    <row r="21" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="230">
+        <v>4</v>
+      </c>
+      <c r="B21" s="240" t="s">
+        <v>357</v>
+      </c>
+      <c r="C21" s="240"/>
+      <c r="D21" s="240"/>
+      <c r="E21" s="240"/>
+      <c r="F21" s="240"/>
+      <c r="G21" s="240"/>
+      <c r="H21" s="240"/>
+      <c r="I21" s="240"/>
+      <c r="J21" s="240"/>
+      <c r="K21" s="240"/>
+      <c r="L21" s="241"/>
+      <c r="N21" s="106"/>
+    </row>
+    <row r="22" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="230">
         <v>5</v>
       </c>
-      <c r="B20" s="266" t="s">
+      <c r="B22" s="240" t="s">
+        <v>220</v>
+      </c>
+      <c r="C22" s="240"/>
+      <c r="D22" s="240"/>
+      <c r="E22" s="240"/>
+      <c r="F22" s="240"/>
+      <c r="G22" s="240"/>
+      <c r="H22" s="240"/>
+      <c r="I22" s="240"/>
+      <c r="J22" s="240"/>
+      <c r="K22" s="240"/>
+      <c r="L22" s="241"/>
+      <c r="N22" s="106"/>
+    </row>
+    <row r="23" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="230"/>
+      <c r="B23" s="240" t="s">
+        <v>221</v>
+      </c>
+      <c r="C23" s="240"/>
+      <c r="D23" s="240"/>
+      <c r="E23" s="240"/>
+      <c r="F23" s="240"/>
+      <c r="G23" s="240"/>
+      <c r="H23" s="240"/>
+      <c r="I23" s="240"/>
+      <c r="J23" s="240"/>
+      <c r="K23" s="240"/>
+      <c r="L23" s="241"/>
+      <c r="N23" s="106"/>
+    </row>
+    <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="230"/>
+      <c r="B24" s="240" t="s">
         <v>222</v>
       </c>
-      <c r="C20" s="266"/>
-      <c r="D20" s="266"/>
-      <c r="E20" s="266"/>
-      <c r="F20" s="266"/>
-      <c r="G20" s="266"/>
-      <c r="H20" s="266"/>
-      <c r="I20" s="266"/>
-      <c r="J20" s="266"/>
-      <c r="K20" s="266"/>
-      <c r="L20" s="267"/>
-      <c r="N20" s="106"/>
-    </row>
-    <row r="21" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="230"/>
-      <c r="B21" s="266" t="s">
+      <c r="C24" s="240"/>
+      <c r="D24" s="240"/>
+      <c r="E24" s="240"/>
+      <c r="F24" s="240"/>
+      <c r="G24" s="240"/>
+      <c r="H24" s="240"/>
+      <c r="I24" s="240"/>
+      <c r="J24" s="240"/>
+      <c r="K24" s="240"/>
+      <c r="L24" s="241"/>
+      <c r="N24" s="106"/>
+    </row>
+    <row r="25" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="249" t="s">
+        <v>228</v>
+      </c>
+      <c r="B25" s="250"/>
+      <c r="C25" s="250"/>
+      <c r="D25" s="250"/>
+      <c r="E25" s="250"/>
+      <c r="F25" s="250"/>
+      <c r="G25" s="250"/>
+      <c r="H25" s="250"/>
+      <c r="I25" s="250"/>
+      <c r="J25" s="250"/>
+      <c r="K25" s="250"/>
+      <c r="L25" s="251"/>
+      <c r="N25" s="106"/>
+    </row>
+    <row r="26" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="230">
+        <v>1</v>
+      </c>
+      <c r="B26" s="240" t="s">
         <v>223</v>
       </c>
-      <c r="C21" s="266"/>
-      <c r="D21" s="266"/>
-      <c r="E21" s="266"/>
-      <c r="F21" s="266"/>
-      <c r="G21" s="266"/>
-      <c r="H21" s="266"/>
-      <c r="I21" s="266"/>
-      <c r="J21" s="266"/>
-      <c r="K21" s="266"/>
-      <c r="L21" s="267"/>
-      <c r="N21" s="106"/>
-    </row>
-    <row r="22" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="230"/>
-      <c r="B22" s="266" t="s">
+      <c r="C26" s="240"/>
+      <c r="D26" s="240"/>
+      <c r="E26" s="240"/>
+      <c r="F26" s="240"/>
+      <c r="G26" s="240"/>
+      <c r="H26" s="240"/>
+      <c r="I26" s="240"/>
+      <c r="J26" s="240"/>
+      <c r="K26" s="240"/>
+      <c r="L26" s="241"/>
+      <c r="N26" s="106"/>
+    </row>
+    <row r="27" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="230"/>
+      <c r="B27" s="238" t="s">
+        <v>358</v>
+      </c>
+      <c r="C27" s="238"/>
+      <c r="D27" s="238"/>
+      <c r="E27" s="238"/>
+      <c r="F27" s="238"/>
+      <c r="G27" s="238"/>
+      <c r="H27" s="238"/>
+      <c r="I27" s="238"/>
+      <c r="J27" s="238"/>
+      <c r="K27" s="238"/>
+      <c r="L27" s="239"/>
+      <c r="N27" s="106"/>
+    </row>
+    <row r="28" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="230">
+        <v>2</v>
+      </c>
+      <c r="B28" s="240" t="s">
+        <v>347</v>
+      </c>
+      <c r="C28" s="240"/>
+      <c r="D28" s="240"/>
+      <c r="E28" s="240"/>
+      <c r="F28" s="240"/>
+      <c r="G28" s="240"/>
+      <c r="H28" s="240"/>
+      <c r="I28" s="240"/>
+      <c r="J28" s="240"/>
+      <c r="K28" s="240"/>
+      <c r="L28" s="241"/>
+      <c r="N28" s="106"/>
+    </row>
+    <row r="29" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="230">
+        <v>3</v>
+      </c>
+      <c r="B29" s="240" t="s">
+        <v>336</v>
+      </c>
+      <c r="C29" s="240"/>
+      <c r="D29" s="240"/>
+      <c r="E29" s="240"/>
+      <c r="F29" s="240"/>
+      <c r="G29" s="240"/>
+      <c r="H29" s="240"/>
+      <c r="I29" s="240"/>
+      <c r="J29" s="240"/>
+      <c r="K29" s="240"/>
+      <c r="L29" s="241"/>
+      <c r="N29" s="106"/>
+    </row>
+    <row r="30" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="230">
+        <v>4</v>
+      </c>
+      <c r="B30" s="240" t="s">
+        <v>359</v>
+      </c>
+      <c r="C30" s="240"/>
+      <c r="D30" s="240"/>
+      <c r="E30" s="240"/>
+      <c r="F30" s="240"/>
+      <c r="G30" s="240"/>
+      <c r="H30" s="240"/>
+      <c r="I30" s="240"/>
+      <c r="J30" s="240"/>
+      <c r="K30" s="240"/>
+      <c r="L30" s="241"/>
+      <c r="N30" s="106"/>
+    </row>
+    <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="230">
+        <v>5</v>
+      </c>
+      <c r="B31" s="238" t="s">
+        <v>337</v>
+      </c>
+      <c r="C31" s="238"/>
+      <c r="D31" s="238"/>
+      <c r="E31" s="238"/>
+      <c r="F31" s="238"/>
+      <c r="G31" s="238"/>
+      <c r="H31" s="238"/>
+      <c r="I31" s="238"/>
+      <c r="J31" s="238"/>
+      <c r="K31" s="238"/>
+      <c r="L31" s="239"/>
+      <c r="N31" s="106"/>
+    </row>
+    <row r="32" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="230">
+        <v>6</v>
+      </c>
+      <c r="B32" s="238" t="s">
+        <v>342</v>
+      </c>
+      <c r="C32" s="238"/>
+      <c r="D32" s="238"/>
+      <c r="E32" s="238"/>
+      <c r="F32" s="238"/>
+      <c r="G32" s="238"/>
+      <c r="H32" s="238"/>
+      <c r="I32" s="238"/>
+      <c r="J32" s="238"/>
+      <c r="K32" s="238"/>
+      <c r="L32" s="239"/>
+      <c r="N32" s="106"/>
+    </row>
+    <row r="33" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="230">
+        <v>7</v>
+      </c>
+      <c r="B33" s="240" t="s">
+        <v>338</v>
+      </c>
+      <c r="C33" s="240"/>
+      <c r="D33" s="240"/>
+      <c r="E33" s="240"/>
+      <c r="F33" s="240"/>
+      <c r="G33" s="240"/>
+      <c r="H33" s="240"/>
+      <c r="I33" s="240"/>
+      <c r="J33" s="240"/>
+      <c r="K33" s="240"/>
+      <c r="L33" s="241"/>
+    </row>
+    <row r="34" spans="1:12" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="230"/>
+      <c r="B34" s="231"/>
+      <c r="C34" s="231"/>
+      <c r="D34" s="231"/>
+      <c r="E34" s="231"/>
+      <c r="F34" s="231"/>
+      <c r="G34" s="231"/>
+      <c r="H34" s="231"/>
+      <c r="I34" s="231"/>
+      <c r="J34" s="231"/>
+      <c r="K34" s="231"/>
+      <c r="L34" s="232"/>
+    </row>
+    <row r="35" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="249" t="s">
+        <v>341</v>
+      </c>
+      <c r="B35" s="250"/>
+      <c r="C35" s="250"/>
+      <c r="D35" s="250"/>
+      <c r="E35" s="250"/>
+      <c r="F35" s="250"/>
+      <c r="G35" s="250"/>
+      <c r="H35" s="250"/>
+      <c r="I35" s="250"/>
+      <c r="J35" s="250"/>
+      <c r="K35" s="250"/>
+      <c r="L35" s="251"/>
+    </row>
+    <row r="36" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="233" t="s">
+        <v>339</v>
+      </c>
+      <c r="B36" s="240" t="s">
         <v>224</v>
       </c>
-      <c r="C22" s="266"/>
-      <c r="D22" s="266"/>
-      <c r="E22" s="266"/>
-      <c r="F22" s="266"/>
-      <c r="G22" s="266"/>
-      <c r="H22" s="266"/>
-      <c r="I22" s="266"/>
-      <c r="J22" s="266"/>
-      <c r="K22" s="266"/>
-      <c r="L22" s="267"/>
-      <c r="N22" s="106"/>
-    </row>
-    <row r="23" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="268" t="s">
-        <v>230</v>
-      </c>
-      <c r="B23" s="269"/>
-      <c r="C23" s="269"/>
-      <c r="D23" s="269"/>
-      <c r="E23" s="269"/>
-      <c r="F23" s="269"/>
-      <c r="G23" s="269"/>
-      <c r="H23" s="269"/>
-      <c r="I23" s="269"/>
-      <c r="J23" s="269"/>
-      <c r="K23" s="269"/>
-      <c r="L23" s="270"/>
-      <c r="N23" s="106"/>
-    </row>
-    <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="230">
-        <v>1</v>
-      </c>
-      <c r="B24" s="266" t="s">
+      <c r="C36" s="240"/>
+      <c r="D36" s="240"/>
+      <c r="E36" s="240"/>
+      <c r="F36" s="240"/>
+      <c r="G36" s="240"/>
+      <c r="H36" s="240"/>
+      <c r="I36" s="240"/>
+      <c r="J36" s="240"/>
+      <c r="K36" s="240"/>
+      <c r="L36" s="241"/>
+    </row>
+    <row r="37" spans="1:12" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="234" t="s">
+        <v>340</v>
+      </c>
+      <c r="B37" s="242" t="s">
+        <v>343</v>
+      </c>
+      <c r="C37" s="242"/>
+      <c r="D37" s="242"/>
+      <c r="E37" s="242"/>
+      <c r="F37" s="242"/>
+      <c r="G37" s="242"/>
+      <c r="H37" s="242"/>
+      <c r="I37" s="242"/>
+      <c r="J37" s="242"/>
+      <c r="K37" s="242"/>
+      <c r="L37" s="243"/>
+    </row>
+    <row r="38" spans="1:12" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="161"/>
+      <c r="B38" s="113"/>
+      <c r="C38" s="113"/>
+      <c r="D38" s="113"/>
+      <c r="E38" s="113"/>
+      <c r="F38" s="113"/>
+      <c r="G38" s="113"/>
+      <c r="H38" s="113"/>
+      <c r="I38" s="113"/>
+      <c r="J38" s="113"/>
+      <c r="K38" s="113"/>
+      <c r="L38" s="113"/>
+    </row>
+    <row r="39" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="244" t="s">
+        <v>252</v>
+      </c>
+      <c r="B39" s="245"/>
+      <c r="C39" s="245"/>
+      <c r="D39" s="245"/>
+      <c r="E39" s="245"/>
+      <c r="F39" s="245"/>
+      <c r="G39" s="245"/>
+      <c r="H39" s="245"/>
+      <c r="I39" s="245"/>
+      <c r="J39" s="245"/>
+      <c r="K39" s="245"/>
+      <c r="L39" s="246"/>
+    </row>
+    <row r="40" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="162" t="s">
         <v>225</v>
       </c>
-      <c r="C24" s="266"/>
-      <c r="D24" s="266"/>
-      <c r="E24" s="266"/>
-      <c r="F24" s="266"/>
-      <c r="G24" s="266"/>
-      <c r="H24" s="266"/>
-      <c r="I24" s="266"/>
-      <c r="J24" s="266"/>
-      <c r="K24" s="266"/>
-      <c r="L24" s="267"/>
-      <c r="N24" s="106"/>
-    </row>
-    <row r="25" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="230"/>
-      <c r="B25" s="264" t="s">
-        <v>329</v>
-      </c>
-      <c r="C25" s="264"/>
-      <c r="D25" s="264"/>
-      <c r="E25" s="264"/>
-      <c r="F25" s="264"/>
-      <c r="G25" s="264"/>
-      <c r="H25" s="264"/>
-      <c r="I25" s="264"/>
-      <c r="J25" s="264"/>
-      <c r="K25" s="264"/>
-      <c r="L25" s="265"/>
-      <c r="N25" s="106"/>
-    </row>
-    <row r="26" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="230">
-        <v>2</v>
-      </c>
-      <c r="B26" s="266" t="s">
-        <v>353</v>
-      </c>
-      <c r="C26" s="266"/>
-      <c r="D26" s="266"/>
-      <c r="E26" s="266"/>
-      <c r="F26" s="266"/>
-      <c r="G26" s="266"/>
-      <c r="H26" s="266"/>
-      <c r="I26" s="266"/>
-      <c r="J26" s="266"/>
-      <c r="K26" s="266"/>
-      <c r="L26" s="267"/>
-      <c r="N26" s="106"/>
-    </row>
-    <row r="27" spans="1:14" s="59" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="230">
-        <v>3</v>
-      </c>
-      <c r="B27" s="266" t="s">
-        <v>340</v>
-      </c>
-      <c r="C27" s="266"/>
-      <c r="D27" s="266"/>
-      <c r="E27" s="266"/>
-      <c r="F27" s="266"/>
-      <c r="G27" s="266"/>
-      <c r="H27" s="266"/>
-      <c r="I27" s="266"/>
-      <c r="J27" s="266"/>
-      <c r="K27" s="266"/>
-      <c r="L27" s="267"/>
-      <c r="N27" s="106"/>
-    </row>
-    <row r="28" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="230">
-        <v>4</v>
-      </c>
-      <c r="B28" s="264" t="s">
-        <v>341</v>
-      </c>
-      <c r="C28" s="264"/>
-      <c r="D28" s="264"/>
-      <c r="E28" s="264"/>
-      <c r="F28" s="264"/>
-      <c r="G28" s="264"/>
-      <c r="H28" s="264"/>
-      <c r="I28" s="264"/>
-      <c r="J28" s="264"/>
-      <c r="K28" s="264"/>
-      <c r="L28" s="265"/>
-      <c r="N28" s="106"/>
-    </row>
-    <row r="29" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="230">
-        <v>5</v>
-      </c>
-      <c r="B29" s="264" t="s">
-        <v>346</v>
-      </c>
-      <c r="C29" s="264"/>
-      <c r="D29" s="264"/>
-      <c r="E29" s="264"/>
-      <c r="F29" s="264"/>
-      <c r="G29" s="264"/>
-      <c r="H29" s="264"/>
-      <c r="I29" s="264"/>
-      <c r="J29" s="264"/>
-      <c r="K29" s="264"/>
-      <c r="L29" s="265"/>
-      <c r="N29" s="106"/>
-    </row>
-    <row r="30" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="230">
-        <v>6</v>
-      </c>
-      <c r="B30" s="266" t="s">
-        <v>342</v>
-      </c>
-      <c r="C30" s="266"/>
-      <c r="D30" s="266"/>
-      <c r="E30" s="266"/>
-      <c r="F30" s="266"/>
-      <c r="G30" s="266"/>
-      <c r="H30" s="266"/>
-      <c r="I30" s="266"/>
-      <c r="J30" s="266"/>
-      <c r="K30" s="266"/>
-      <c r="L30" s="267"/>
-    </row>
-    <row r="31" spans="1:14" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="230"/>
-      <c r="B31" s="231"/>
-      <c r="C31" s="231"/>
-      <c r="D31" s="231"/>
-      <c r="E31" s="231"/>
-      <c r="F31" s="231"/>
-      <c r="G31" s="231"/>
-      <c r="H31" s="231"/>
-      <c r="I31" s="231"/>
-      <c r="J31" s="231"/>
-      <c r="K31" s="231"/>
-      <c r="L31" s="232"/>
-    </row>
-    <row r="32" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="268" t="s">
-        <v>345</v>
-      </c>
-      <c r="B32" s="269"/>
-      <c r="C32" s="269"/>
-      <c r="D32" s="269"/>
-      <c r="E32" s="269"/>
-      <c r="F32" s="269"/>
-      <c r="G32" s="269"/>
-      <c r="H32" s="269"/>
-      <c r="I32" s="269"/>
-      <c r="J32" s="269"/>
-      <c r="K32" s="269"/>
-      <c r="L32" s="270"/>
-    </row>
-    <row r="33" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="233" t="s">
-        <v>343</v>
-      </c>
-      <c r="B33" s="266" t="s">
-        <v>226</v>
-      </c>
-      <c r="C33" s="266"/>
-      <c r="D33" s="266"/>
-      <c r="E33" s="266"/>
-      <c r="F33" s="266"/>
-      <c r="G33" s="266"/>
-      <c r="H33" s="266"/>
-      <c r="I33" s="266"/>
-      <c r="J33" s="266"/>
-      <c r="K33" s="266"/>
-      <c r="L33" s="267"/>
-    </row>
-    <row r="34" spans="1:12" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="234" t="s">
-        <v>344</v>
-      </c>
-      <c r="B34" s="272" t="s">
-        <v>348</v>
-      </c>
-      <c r="C34" s="272"/>
-      <c r="D34" s="272"/>
-      <c r="E34" s="272"/>
-      <c r="F34" s="272"/>
-      <c r="G34" s="272"/>
-      <c r="H34" s="272"/>
-      <c r="I34" s="272"/>
-      <c r="J34" s="272"/>
-      <c r="K34" s="272"/>
-      <c r="L34" s="273"/>
-    </row>
-    <row r="35" spans="1:12" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="161"/>
-      <c r="B35" s="113"/>
-      <c r="C35" s="113"/>
-      <c r="D35" s="113"/>
-      <c r="E35" s="113"/>
-      <c r="F35" s="113"/>
-      <c r="G35" s="113"/>
-      <c r="H35" s="113"/>
-      <c r="I35" s="113"/>
-      <c r="J35" s="113"/>
-      <c r="K35" s="113"/>
-      <c r="L35" s="113"/>
-    </row>
-    <row r="36" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="274" t="s">
-        <v>255</v>
-      </c>
-      <c r="B36" s="275"/>
-      <c r="C36" s="275"/>
-      <c r="D36" s="275"/>
-      <c r="E36" s="275"/>
-      <c r="F36" s="275"/>
-      <c r="G36" s="275"/>
-      <c r="H36" s="275"/>
-      <c r="I36" s="275"/>
-      <c r="J36" s="275"/>
-      <c r="K36" s="275"/>
-      <c r="L36" s="276"/>
-    </row>
-    <row r="37" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="162" t="s">
-        <v>227</v>
-      </c>
-      <c r="B37" s="163"/>
-      <c r="C37" s="163"/>
-      <c r="D37" s="163"/>
-      <c r="E37" s="163"/>
-      <c r="F37" s="163"/>
-      <c r="G37" s="163"/>
-      <c r="H37" s="163"/>
-      <c r="I37" s="163"/>
-      <c r="J37" s="163"/>
-      <c r="K37" s="163"/>
-      <c r="L37" s="164"/>
-    </row>
-    <row r="38" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="84"/>
-      <c r="C38" s="84"/>
-      <c r="D38" s="84"/>
-      <c r="E38" s="84"/>
-      <c r="F38" s="84"/>
-      <c r="G38" s="84"/>
-      <c r="H38" s="84"/>
-      <c r="I38" s="84"/>
-      <c r="J38" s="84"/>
-      <c r="K38" s="84"/>
-      <c r="L38" s="84"/>
-    </row>
-    <row r="39" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="165" t="s">
+      <c r="B40" s="163"/>
+      <c r="C40" s="163"/>
+      <c r="D40" s="163"/>
+      <c r="E40" s="163"/>
+      <c r="F40" s="163"/>
+      <c r="G40" s="163"/>
+      <c r="H40" s="163"/>
+      <c r="I40" s="163"/>
+      <c r="J40" s="163"/>
+      <c r="K40" s="163"/>
+      <c r="L40" s="164"/>
+    </row>
+    <row r="41" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="84"/>
+      <c r="C41" s="84"/>
+      <c r="D41" s="84"/>
+      <c r="E41" s="84"/>
+      <c r="F41" s="84"/>
+      <c r="G41" s="84"/>
+      <c r="H41" s="84"/>
+      <c r="I41" s="84"/>
+      <c r="J41" s="84"/>
+      <c r="K41" s="84"/>
+      <c r="L41" s="84"/>
+    </row>
+    <row r="42" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="165" t="s">
         <v>174</v>
       </c>
-      <c r="B39" s="166"/>
-      <c r="C39" s="166"/>
-      <c r="D39" s="167"/>
-      <c r="E39" s="166"/>
-      <c r="F39" s="166"/>
-      <c r="G39" s="166"/>
-      <c r="H39" s="166"/>
-      <c r="I39" s="166"/>
-      <c r="J39" s="166"/>
-      <c r="K39" s="166"/>
-      <c r="L39" s="168"/>
-    </row>
-    <row r="40" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="169"/>
-      <c r="B40" s="170" t="s">
-        <v>62</v>
-      </c>
-      <c r="C40" s="171" t="s">
-        <v>80</v>
-      </c>
-      <c r="D40" s="171"/>
-      <c r="E40" s="171"/>
-      <c r="F40" s="171"/>
-      <c r="G40" s="171"/>
-      <c r="H40" s="171"/>
-      <c r="I40" s="171"/>
-      <c r="J40" s="171"/>
-      <c r="K40" s="171"/>
-      <c r="L40" s="172"/>
-    </row>
-    <row r="41" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="169"/>
-      <c r="B41" s="170" t="s">
-        <v>82</v>
-      </c>
-      <c r="C41" s="171" t="s">
-        <v>92</v>
-      </c>
-      <c r="D41" s="171"/>
-      <c r="E41" s="171"/>
-      <c r="F41" s="171"/>
-      <c r="G41" s="171"/>
-      <c r="H41" s="171"/>
-      <c r="I41" s="171"/>
-      <c r="J41" s="171"/>
-      <c r="K41" s="171"/>
-      <c r="L41" s="172"/>
-    </row>
-    <row r="42" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="169"/>
-      <c r="B42" s="170" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="256" t="s">
-        <v>330</v>
-      </c>
-      <c r="D42" s="256"/>
-      <c r="E42" s="256"/>
-      <c r="F42" s="256"/>
-      <c r="G42" s="256"/>
-      <c r="H42" s="256"/>
-      <c r="I42" s="256"/>
-      <c r="J42" s="256"/>
-      <c r="K42" s="256"/>
-      <c r="L42" s="257"/>
-    </row>
-    <row r="43" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B42" s="166"/>
+      <c r="C42" s="166"/>
+      <c r="D42" s="167"/>
+      <c r="E42" s="166"/>
+      <c r="F42" s="166"/>
+      <c r="G42" s="166"/>
+      <c r="H42" s="166"/>
+      <c r="I42" s="166"/>
+      <c r="J42" s="166"/>
+      <c r="K42" s="166"/>
+      <c r="L42" s="168"/>
+    </row>
+    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="169"/>
       <c r="B43" s="170" t="s">
-        <v>146</v>
-      </c>
-      <c r="C43" s="256" t="s">
-        <v>147</v>
-      </c>
-      <c r="D43" s="256"/>
-      <c r="E43" s="256"/>
-      <c r="F43" s="256"/>
-      <c r="G43" s="256"/>
-      <c r="H43" s="256"/>
-      <c r="I43" s="256"/>
-      <c r="J43" s="256"/>
-      <c r="K43" s="256"/>
-      <c r="L43" s="257"/>
-    </row>
-    <row r="44" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="C43" s="171" t="s">
+        <v>80</v>
+      </c>
+      <c r="D43" s="171"/>
+      <c r="E43" s="171"/>
+      <c r="F43" s="171"/>
+      <c r="G43" s="171"/>
+      <c r="H43" s="171"/>
+      <c r="I43" s="171"/>
+      <c r="J43" s="171"/>
+      <c r="K43" s="171"/>
+      <c r="L43" s="172"/>
+    </row>
+    <row r="44" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="169"/>
       <c r="B44" s="170" t="s">
-        <v>253</v>
-      </c>
-      <c r="C44" s="256" t="s">
-        <v>254</v>
-      </c>
-      <c r="D44" s="256"/>
-      <c r="E44" s="256"/>
-      <c r="F44" s="256"/>
-      <c r="G44" s="256"/>
-      <c r="H44" s="256"/>
-      <c r="I44" s="256"/>
-      <c r="J44" s="256"/>
-      <c r="K44" s="256"/>
-      <c r="L44" s="257"/>
-    </row>
-    <row r="45" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+      <c r="C44" s="171" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="171"/>
+      <c r="E44" s="171"/>
+      <c r="F44" s="171"/>
+      <c r="G44" s="171"/>
+      <c r="H44" s="171"/>
+      <c r="I44" s="171"/>
+      <c r="J44" s="171"/>
+      <c r="K44" s="171"/>
+      <c r="L44" s="172"/>
+    </row>
+    <row r="45" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="169"/>
       <c r="B45" s="170" t="s">
-        <v>331</v>
-      </c>
-      <c r="C45" s="256" t="s">
-        <v>332</v>
-      </c>
-      <c r="D45" s="256"/>
-      <c r="E45" s="256"/>
-      <c r="F45" s="256"/>
-      <c r="G45" s="256"/>
-      <c r="H45" s="256"/>
-      <c r="I45" s="256"/>
-      <c r="J45" s="256"/>
-      <c r="K45" s="256"/>
-      <c r="L45" s="257"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="C45" s="247" t="s">
+        <v>326</v>
+      </c>
+      <c r="D45" s="247"/>
+      <c r="E45" s="247"/>
+      <c r="F45" s="247"/>
+      <c r="G45" s="247"/>
+      <c r="H45" s="247"/>
+      <c r="I45" s="247"/>
+      <c r="J45" s="247"/>
+      <c r="K45" s="247"/>
+      <c r="L45" s="248"/>
+    </row>
+    <row r="46" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="169"/>
       <c r="B46" s="170" t="s">
-        <v>215</v>
-      </c>
-      <c r="C46" s="171" t="s">
-        <v>333</v>
-      </c>
-      <c r="D46" s="171"/>
-      <c r="E46" s="171"/>
-      <c r="F46" s="171"/>
-      <c r="G46" s="171"/>
-      <c r="H46" s="171"/>
-      <c r="I46" s="171"/>
-      <c r="J46" s="171"/>
-      <c r="K46" s="171"/>
-      <c r="L46" s="172"/>
-    </row>
-    <row r="47" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>146</v>
+      </c>
+      <c r="C46" s="247" t="s">
+        <v>147</v>
+      </c>
+      <c r="D46" s="247"/>
+      <c r="E46" s="247"/>
+      <c r="F46" s="247"/>
+      <c r="G46" s="247"/>
+      <c r="H46" s="247"/>
+      <c r="I46" s="247"/>
+      <c r="J46" s="247"/>
+      <c r="K46" s="247"/>
+      <c r="L46" s="248"/>
+    </row>
+    <row r="47" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="169"/>
       <c r="B47" s="170" t="s">
-        <v>63</v>
-      </c>
-      <c r="C47" s="256" t="s">
-        <v>334</v>
-      </c>
-      <c r="D47" s="256"/>
-      <c r="E47" s="256"/>
-      <c r="F47" s="256"/>
-      <c r="G47" s="256"/>
-      <c r="H47" s="256"/>
-      <c r="I47" s="256"/>
-      <c r="J47" s="256"/>
-      <c r="K47" s="256"/>
-      <c r="L47" s="257"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+        <v>250</v>
+      </c>
+      <c r="C47" s="247" t="s">
+        <v>251</v>
+      </c>
+      <c r="D47" s="247"/>
+      <c r="E47" s="247"/>
+      <c r="F47" s="247"/>
+      <c r="G47" s="247"/>
+      <c r="H47" s="247"/>
+      <c r="I47" s="247"/>
+      <c r="J47" s="247"/>
+      <c r="K47" s="247"/>
+      <c r="L47" s="248"/>
+    </row>
+    <row r="48" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="169"/>
       <c r="B48" s="170" t="s">
+        <v>327</v>
+      </c>
+      <c r="C48" s="247" t="s">
+        <v>328</v>
+      </c>
+      <c r="D48" s="247"/>
+      <c r="E48" s="247"/>
+      <c r="F48" s="247"/>
+      <c r="G48" s="247"/>
+      <c r="H48" s="247"/>
+      <c r="I48" s="247"/>
+      <c r="J48" s="247"/>
+      <c r="K48" s="247"/>
+      <c r="L48" s="248"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A49" s="169"/>
+      <c r="B49" s="170" t="s">
+        <v>215</v>
+      </c>
+      <c r="C49" s="171" t="s">
+        <v>329</v>
+      </c>
+      <c r="D49" s="171"/>
+      <c r="E49" s="171"/>
+      <c r="F49" s="171"/>
+      <c r="G49" s="171"/>
+      <c r="H49" s="171"/>
+      <c r="I49" s="171"/>
+      <c r="J49" s="171"/>
+      <c r="K49" s="171"/>
+      <c r="L49" s="172"/>
+    </row>
+    <row r="50" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="169"/>
+      <c r="B50" s="170" t="s">
+        <v>63</v>
+      </c>
+      <c r="C50" s="247" t="s">
+        <v>330</v>
+      </c>
+      <c r="D50" s="247"/>
+      <c r="E50" s="247"/>
+      <c r="F50" s="247"/>
+      <c r="G50" s="247"/>
+      <c r="H50" s="247"/>
+      <c r="I50" s="247"/>
+      <c r="J50" s="247"/>
+      <c r="K50" s="247"/>
+      <c r="L50" s="248"/>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A51" s="169"/>
+      <c r="B51" s="170" t="s">
         <v>75</v>
       </c>
-      <c r="C48" s="171" t="s">
+      <c r="C51" s="171" t="s">
         <v>76</v>
       </c>
-      <c r="D48" s="171"/>
-      <c r="E48" s="171"/>
-      <c r="F48" s="171"/>
-      <c r="G48" s="171"/>
-      <c r="H48" s="171"/>
-      <c r="I48" s="171"/>
-      <c r="J48" s="171"/>
-      <c r="K48" s="171"/>
-      <c r="L48" s="172"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A49" s="173"/>
-      <c r="B49" s="174" t="s">
+      <c r="D51" s="171"/>
+      <c r="E51" s="171"/>
+      <c r="F51" s="171"/>
+      <c r="G51" s="171"/>
+      <c r="H51" s="171"/>
+      <c r="I51" s="171"/>
+      <c r="J51" s="171"/>
+      <c r="K51" s="171"/>
+      <c r="L51" s="172"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52" s="173"/>
+      <c r="B52" s="174" t="s">
         <v>167</v>
       </c>
-      <c r="C49" s="175" t="s">
+      <c r="C52" s="175" t="s">
         <v>168</v>
       </c>
-      <c r="D49" s="175"/>
-      <c r="E49" s="175"/>
-      <c r="F49" s="175"/>
-      <c r="G49" s="175"/>
-      <c r="H49" s="175"/>
-      <c r="I49" s="175"/>
-      <c r="J49" s="175"/>
-      <c r="K49" s="175"/>
-      <c r="L49" s="176"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A51" s="1" t="s">
+      <c r="D52" s="175"/>
+      <c r="E52" s="175"/>
+      <c r="F52" s="175"/>
+      <c r="G52" s="175"/>
+      <c r="H52" s="175"/>
+      <c r="I52" s="175"/>
+      <c r="J52" s="175"/>
+      <c r="K52" s="175"/>
+      <c r="L52" s="176"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A54" s="45" t="s">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A57" s="45" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A55" s="45" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A56" s="45"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A57" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="45" t="s">
-        <v>335</v>
-      </c>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A59" s="45"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A61" s="45" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="271" t="s">
-        <v>336</v>
-      </c>
-      <c r="B61" s="271"/>
-      <c r="C61" s="271"/>
-      <c r="D61" s="271"/>
-      <c r="E61" s="271"/>
-      <c r="F61" s="271"/>
-      <c r="G61" s="271"/>
-      <c r="H61" s="271"/>
-      <c r="I61" s="271"/>
-      <c r="J61" s="271"/>
-      <c r="K61" s="271"/>
-      <c r="L61" s="271"/>
-    </row>
-    <row r="66" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="67" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="64" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="237" t="s">
+        <v>332</v>
+      </c>
+      <c r="B64" s="237"/>
+      <c r="C64" s="237"/>
+      <c r="D64" s="237"/>
+      <c r="E64" s="237"/>
+      <c r="F64" s="237"/>
+      <c r="G64" s="237"/>
+      <c r="H64" s="237"/>
+      <c r="I64" s="237"/>
+      <c r="J64" s="237"/>
+      <c r="K64" s="237"/>
+      <c r="L64" s="237"/>
+    </row>
+    <row r="69" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="70" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="A61:L61"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="B34:L34"/>
-    <mergeCell ref="A36:L36"/>
-    <mergeCell ref="C42:L42"/>
-    <mergeCell ref="C43:L43"/>
-    <mergeCell ref="C44:L44"/>
-    <mergeCell ref="C45:L45"/>
-    <mergeCell ref="C47:L47"/>
-    <mergeCell ref="A32:L32"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B16:L16"/>
-    <mergeCell ref="B17:L17"/>
+  <mergeCells count="40">
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="B31:L31"/>
     <mergeCell ref="B18:L18"/>
     <mergeCell ref="B19:L19"/>
     <mergeCell ref="B20:L20"/>
     <mergeCell ref="B21:L21"/>
     <mergeCell ref="B22:L22"/>
-    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="B23:L23"/>
     <mergeCell ref="B24:L24"/>
-    <mergeCell ref="B25:L25"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="B26:L26"/>
     <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B26:L26"/>
-    <mergeCell ref="A15:L15"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B30:L30"/>
+    <mergeCell ref="A64:L64"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="C45:L45"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="C48:L48"/>
+    <mergeCell ref="C50:L50"/>
+    <mergeCell ref="A35:L35"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A54" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
-    <hyperlink ref="A55" r:id="rId2" xr:uid="{66F54200-A2AB-43DA-A0E0-F2A25A075EE5}"/>
-    <hyperlink ref="A58" r:id="rId3" xr:uid="{A0F8DE06-D9FC-495F-9A01-AA199CB82365}"/>
-    <hyperlink ref="A36:L36" r:id="rId4" display="VISUALS of KEY IDEAS" xr:uid="{0D075873-7EBB-4309-B00A-6A62EA192A0C}"/>
-    <hyperlink ref="A37" r:id="rId5" display="Model Guide (Help)" xr:uid="{25154A32-BA44-496E-9945-086DE0980DBD}"/>
+    <hyperlink ref="A57" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
+    <hyperlink ref="A58" r:id="rId2" xr:uid="{66F54200-A2AB-43DA-A0E0-F2A25A075EE5}"/>
+    <hyperlink ref="A61" r:id="rId3" xr:uid="{A0F8DE06-D9FC-495F-9A01-AA199CB82365}"/>
+    <hyperlink ref="A39:L39" r:id="rId4" display="VISUALS of KEY IDEAS" xr:uid="{0D075873-7EBB-4309-B00A-6A62EA192A0C}"/>
+    <hyperlink ref="A40" r:id="rId5" display="Model Guide (Help)" xr:uid="{25154A32-BA44-496E-9945-086DE0980DBD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15807,27 +15903,27 @@
       <c r="B4" s="315"/>
       <c r="C4" s="315"/>
       <c r="D4" s="177" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="319" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B5" s="316"/>
       <c r="C5" s="316"/>
       <c r="D5" s="178" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="317" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B6" s="317"/>
       <c r="C6" s="317"/>
       <c r="D6" s="179" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
@@ -15837,7 +15933,7 @@
       <c r="B7" s="318"/>
       <c r="C7" s="318"/>
       <c r="D7" s="180" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -15917,7 +16013,7 @@
         <v>84</v>
       </c>
       <c r="D1" s="36" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="E1" s="36" t="s">
         <v>86</v>
@@ -15943,19 +16039,19 @@
         <v>45413</v>
       </c>
       <c r="B2" s="150" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="D2" s="55">
         <v>0.3</v>
       </c>
       <c r="E2" s="55" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F2" s="55" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G2" s="57"/>
       <c r="I2" s="38"/>
@@ -15967,19 +16063,19 @@
         <v>45604</v>
       </c>
       <c r="B3" s="150" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="D3" s="55">
         <v>4</v>
       </c>
       <c r="E3" s="55" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F3" s="55" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G3" s="57"/>
       <c r="I3" s="38"/>
@@ -15991,19 +16087,19 @@
         <v>45611</v>
       </c>
       <c r="B4" s="150" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="D4" s="55">
         <v>0.3</v>
       </c>
       <c r="E4" s="55" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="F4" s="55" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G4" s="57"/>
       <c r="I4" s="38"/>
@@ -16416,7 +16512,7 @@
   <dimension ref="A1:P139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16458,13 +16554,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="285" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B3" s="285"/>
       <c r="C3" s="285"/>
@@ -16482,13 +16578,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="127" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="286" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D4" s="287"/>
       <c r="E4" s="287"/>
@@ -16500,7 +16596,7 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="90" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B5" s="114"/>
       <c r="C5" s="289"/>
@@ -16508,13 +16604,11 @@
       <c r="E5" s="284"/>
       <c r="F5" s="284"/>
       <c r="G5" s="284"/>
-      <c r="N5" s="141" t="s">
-        <v>357</v>
-      </c>
+      <c r="N5" s="141"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="90" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B6" s="114"/>
       <c r="C6" s="289"/>
@@ -16526,7 +16620,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="90" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B7" s="114"/>
       <c r="C7" s="289"/>
@@ -16538,7 +16632,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="114" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B8" s="90"/>
       <c r="C8" s="284"/>
@@ -16562,7 +16656,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="90" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="B10" s="90"/>
       <c r="C10" s="284"/>
@@ -16593,18 +16687,21 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B13" s="294" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C13" s="295"/>
       <c r="D13" s="296"/>
-      <c r="N13" s="142"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B14" s="278" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C14" s="279"/>
       <c r="D14" s="280"/>
+      <c r="F14">
+        <f>0.95/2</f>
+        <v>0.47499999999999998</v>
+      </c>
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -16620,13 +16717,13 @@
     </row>
     <row r="17" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B17" s="229" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C17" s="229" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="N17" s="141" t="s">
         <v>178</v>
@@ -16634,7 +16731,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B18" s="228">
         <v>6</v>
@@ -16646,7 +16743,7 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B19" s="220">
         <v>1061.22</v>
@@ -16656,10 +16753,10 @@
         <v>8.4990979999700009</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F19" s="187" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="N19" s="141" t="s">
         <v>179</v>
@@ -16684,7 +16781,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C21" s="12">
         <f>C19-C20</f>
@@ -16699,13 +16796,13 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C22" s="188">
         <v>3.5339999999999998</v>
       </c>
       <c r="D22" s="111" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
@@ -16715,7 +16812,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="C23" s="12">
         <f>C21-C22</f>
@@ -16810,7 +16907,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="125" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="97">
@@ -16978,7 +17075,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B32" s="1"/>
       <c r="H32" s="96"/>
@@ -16990,7 +17087,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="12">
@@ -17022,7 +17119,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="221">
@@ -17054,7 +17151,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="125" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C35"/>
       <c r="H35" s="12" t="str">
@@ -17466,7 +17563,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B45" s="189"/>
       <c r="C45" s="12">
@@ -17802,7 +17899,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" s="125" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B52" s="217"/>
       <c r="C52" s="218">
@@ -17856,7 +17953,7 @@
         <v xml:space="preserve">    To Reclamation - Protect Zone</v>
       </c>
       <c r="B53" s="190" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C53" s="82">
         <f>IF(OR(C$28="",$A55=""),"",C46)</f>
@@ -17911,7 +18008,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C54" s="82">
         <f>IF(OR(C$28="",$A56=""),"",C52-C53)</f>
@@ -17969,7 +18066,7 @@
         <v xml:space="preserve">       To California</v>
       </c>
       <c r="B55" s="95" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C55" s="82">
         <f>IF(OR(C$28="",$A55=""),"",(VLOOKUP(C$54,DivideInflow!$K$19:$W$25,9)-IF($A$59&lt;&gt;"",$B$59/2))*(C$54))</f>
@@ -18027,7 +18124,7 @@
         <v xml:space="preserve">       To Arizona</v>
       </c>
       <c r="B56" s="95" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C56" s="82">
         <f>IF(OR(C$28="",$A56=""),"",(VLOOKUP(C$54,DivideInflow!$K$19:$W$25,7)-IF($A$59&lt;&gt;"",$B$59/2))*(C$54))</f>
@@ -18303,7 +18400,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" s="101" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B62" s="98"/>
       <c r="C62" s="98"/>
@@ -19770,7 +19867,7 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A111" s="101" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B111" s="101"/>
       <c r="C111" s="101"/>
@@ -20459,7 +20556,7 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A127" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B127" s="1"/>
       <c r="D127" s="2"/>
@@ -20757,7 +20854,7 @@
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A134" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H134" s="12" t="str">
         <f t="shared" ref="H134:L134" si="90">IF(H$28&lt;&gt;"",SUM(H128:H133),"")</f>
@@ -20785,7 +20882,7 @@
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B135" s="1"/>
       <c r="C135" s="12">
@@ -20817,7 +20914,7 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="B136" s="1"/>
       <c r="C136" s="222">
@@ -20849,7 +20946,7 @@
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A137" s="125" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C137" s="18"/>
       <c r="N137" s="141" t="s">
@@ -21132,65 +21229,64 @@
   </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" xr:uid="{DF55C70C-AEA5-4BB4-9BD1-23B882C83781}"/>
-    <hyperlink ref="N12" r:id="rId2" location="1a-explain-cell-types" xr:uid="{01F4C9FA-7DCC-4CB5-876D-65C85595E561}"/>
-    <hyperlink ref="N17" r:id="rId3" location="1b-make-assumptions" xr:uid="{91CC7212-C579-4B1B-A8B8-969D4549837D}"/>
-    <hyperlink ref="N18" r:id="rId4" location="i-evaporation-rates" xr:uid="{23C61350-606E-472B-90E1-88574D6741EE}"/>
-    <hyperlink ref="N19" r:id="rId5" location="ii-start-storage" xr:uid="{692C3AE6-515B-4C08-B6EC-0557E75E9511}"/>
-    <hyperlink ref="N20" r:id="rId6" location="iii-protection-elevations" xr:uid="{16CC5ED4-0369-416C-AC3E-3AD6F831A454}"/>
-    <hyperlink ref="N21" r:id="rId7" location="iv-the-protection-volumes" xr:uid="{D7802E8D-5298-4564-9936-B3226B6E96DA}"/>
-    <hyperlink ref="N22" r:id="rId8" location="v-prior-9-year-lake-powell-release" xr:uid="{9E773CCF-F296-48D2-ADA9-5456ABC7F062}"/>
-    <hyperlink ref="N23" r:id="rId9" location="vi-prior-9-year-paria-river-flow" xr:uid="{8CAE8559-5BD9-4D9F-8655-D1F3AE1FCD4D}"/>
-    <hyperlink ref="N24" r:id="rId10" location="vii-delivery-to-meet-10-year-requirement" xr:uid="{B6DDA7AA-2218-4D2F-9A7A-A0EDBEFDC5B1}"/>
-    <hyperlink ref="N28" r:id="rId11" location="step-2-specify-natural-inflow-to-lake-powell" xr:uid="{78DF76B4-BE79-4AC1-9F08-EC86A0A72F91}"/>
-    <hyperlink ref="N29" r:id="rId12" location="2a-intervening-grand-canyon-flow" xr:uid="{CFD884C0-2149-42F6-AD5A-482CF40D5292}"/>
-    <hyperlink ref="N30" r:id="rId13" location="2b-mead-to-imperial-dam-intervening-flow" xr:uid="{B8EF30C2-739D-4E21-B63A-F17F9947326A}"/>
-    <hyperlink ref="N31" r:id="rId14" location="2c-havasuparker-evaporation-and-evapotranspiration" xr:uid="{70E7AC6A-42AC-4DE1-ADFB-FBA8230C308E}"/>
-    <hyperlink ref="N35" r:id="rId15" location="step-3-split-existing-reservoir-storage-among-accounts-year-1-only" xr:uid="{B36B453C-62F8-4461-8E49-8546C848C695}"/>
-    <hyperlink ref="N42" r:id="rId16" location="3a-begin-of-year-reservoir-storage" display="Help begin year storage" xr:uid="{52EB1038-72CB-4676-AD3B-3DD4322D2D3C}"/>
-    <hyperlink ref="N45" r:id="rId17" location="3b-calculate-powell--mead-evaporation" xr:uid="{9002111C-2D36-45B1-97D8-5FCB363BD9BD}"/>
-    <hyperlink ref="N52" r:id="rId18" location="3c-calculate-mexico-water-allocation" xr:uid="{C14FC6B3-6E3C-48F5-B820-A74ADC9C86D6}"/>
-    <hyperlink ref="N53" r:id="rId19" location="split-combined-natural-inflow-among-accounts" xr:uid="{63C31A0C-C046-4C6B-B63E-AA3031EC5E49}"/>
-    <hyperlink ref="N63" r:id="rId20" location="step-5-participant-dashboards--conserve-consume-and-trade" xr:uid="{E1DA626C-61A5-4CB7-94B9-52C34A1556D5}"/>
-    <hyperlink ref="N65" r:id="rId21" location="ii-compensation" xr:uid="{19918E71-71AD-4C9C-BB3F-A5AF3D55F1D7}"/>
-    <hyperlink ref="N66" r:id="rId22" location="iii-net-trade-volume-all-participants" xr:uid="{3E7AF6CA-1278-4129-B9E4-725FD18D820D}"/>
-    <hyperlink ref="N67" r:id="rId23" location="iv-available-water" xr:uid="{4566CC8F-1D0F-43BA-BAD8-C66179151606}"/>
-    <hyperlink ref="N68" r:id="rId24" location="v-enter-withdraw-within-available-water" display="Help withdraw" xr:uid="{FA435611-F017-4A4C-84C0-3BC240C90BC3}"/>
-    <hyperlink ref="N69" r:id="rId25" location="vi-end-of-year-balance" xr:uid="{43A45EF2-1AE7-497D-9090-A6710371091B}"/>
-    <hyperlink ref="N103" r:id="rId26" location="5a-shared-reserve-dashboard" display="Help shared, reserve" xr:uid="{93564FFE-2F11-4E1B-8E30-F04D091042B0}"/>
-    <hyperlink ref="N111" r:id="rId27" location="step-6-summary-of-participant-actions" xr:uid="{39E9E91B-EE9B-4603-9A19-992E43688C4C}"/>
-    <hyperlink ref="N134" r:id="rId28" location="6a-combined-storage--end-of-year" xr:uid="{18709FDC-6FB8-4FF1-82C7-3E0140C4C207}"/>
-    <hyperlink ref="N137" r:id="rId29" location="step-8-move-to-next-year" xr:uid="{0D1EBCA9-BE7F-441F-A17C-5330CFCE7596}"/>
-    <hyperlink ref="N79" r:id="rId30" location="step-5-player-dashboards--conserve-consume-and-trade" xr:uid="{115088D1-B3CF-4D72-A6D6-92770E18F116}"/>
-    <hyperlink ref="N80" r:id="rId31" location="i-buy-or-sell-water-from-other-players" xr:uid="{D5A878F8-1AB0-4367-BFA6-4F25001F73AD}"/>
-    <hyperlink ref="N81" r:id="rId32" location="ii-compensation" xr:uid="{74477D73-291E-4A7F-86F2-C21A0DF60CEA}"/>
-    <hyperlink ref="N83" r:id="rId33" location="iv-available-water" xr:uid="{096A8B03-D32B-4628-BC3E-B3E64954FA42}"/>
-    <hyperlink ref="N84" r:id="rId34" location="v-enter-withdraw-within-available-water" display="Help withdraw" xr:uid="{4ED17C45-EBF9-4C45-9229-5218A5ECD61F}"/>
-    <hyperlink ref="N85" r:id="rId35" location="vi-end-of-year-balance" xr:uid="{C6E40832-042B-43D8-90B9-CD82703389C7}"/>
-    <hyperlink ref="N25" r:id="rId36" location="upper-basin-pre-1922-water-rights" xr:uid="{25504FB1-E197-4C3D-945D-5BDD83C2C59E}"/>
-    <hyperlink ref="N64" r:id="rId37" location="i-buy-or-sell-water-from-other-participantss" xr:uid="{D2AC05B4-FD61-425B-9046-D87C8AAAAEA0}"/>
-    <hyperlink ref="N71" r:id="rId38" location="step-5-participant-dashboards--conserve-consume-and-trade" xr:uid="{D67E6EF8-391E-4D21-9E33-260AECB2DB20}"/>
-    <hyperlink ref="N73" r:id="rId39" location="ii-compensation" xr:uid="{5D3E22F6-98D1-4F8D-AC9B-79BC60BD9D4C}"/>
-    <hyperlink ref="N74" r:id="rId40" location="iii-net-trade-volume-all-participants" xr:uid="{E4C097D5-D12A-4D05-9CB5-F12180A8841F}"/>
-    <hyperlink ref="N75" r:id="rId41" location="iv-available-water" xr:uid="{92A2BD5E-9234-4CDA-B631-2F26F1EDA2F6}"/>
-    <hyperlink ref="N76" r:id="rId42" location="v-enter-withdraw-within-available-water" display="Help withdraw" xr:uid="{D566555A-5FE4-4D77-A91F-AB8CA37C5882}"/>
-    <hyperlink ref="N77" r:id="rId43" location="vi-end-of-year-balance" xr:uid="{43994CDC-2740-40CF-8975-5A1D654DE92E}"/>
-    <hyperlink ref="N72" r:id="rId44" location="i-buy-or-sell-water-from-other-participantss" xr:uid="{99CA01B4-F83D-4392-BFD6-E3696F3B060F}"/>
-    <hyperlink ref="N82" r:id="rId45" location="iii-net-trade-volume-all-participants" xr:uid="{35106ED0-ED39-4B94-A4D9-B79EFE11A2E6}"/>
-    <hyperlink ref="N87" r:id="rId46" location="step-5-player-dashboards--conserve-consume-and-trade" xr:uid="{AEF1AABF-406E-492C-A9C6-6D4F230E19E9}"/>
-    <hyperlink ref="N88" r:id="rId47" location="i-buy-or-sell-water-from-other-players" xr:uid="{A414CAB3-AC71-40F2-BCEE-3B4BD79CCEC2}"/>
-    <hyperlink ref="N89" r:id="rId48" location="ii-compensation" xr:uid="{8233903D-3600-4882-9905-8BB60669B1D3}"/>
-    <hyperlink ref="N91" r:id="rId49" location="iv-available-water" xr:uid="{BD162207-CEDD-4927-ACFE-B798DB92B590}"/>
-    <hyperlink ref="N92" r:id="rId50" location="v-enter-withdraw-within-available-water" display="Help withdraw" xr:uid="{80D88F54-62DF-498A-A03F-9FC4097F6B84}"/>
-    <hyperlink ref="N93" r:id="rId51" location="vi-end-of-year-balance" xr:uid="{3C22C7BF-428B-4FE8-9C2E-F555E1D2FB9F}"/>
-    <hyperlink ref="N90" r:id="rId52" location="iii-net-trade-volume-all-participants" xr:uid="{4F49F47E-D9E6-4681-A7EF-3B21819F5A2A}"/>
-    <hyperlink ref="N95" r:id="rId53" location="step-5-player-dashboards--conserve-consume-and-trade" xr:uid="{0EF1BC22-639A-4CAC-8C5C-1003B2A67B6B}"/>
-    <hyperlink ref="N96" r:id="rId54" location="i-buy-or-sell-water-from-other-players" xr:uid="{7B556B5C-2F11-4498-8C4A-C03479306858}"/>
-    <hyperlink ref="N97" r:id="rId55" location="ii-compensation" xr:uid="{9ABDDEAE-D66A-426B-9D45-11CC8D3256D9}"/>
-    <hyperlink ref="N99" r:id="rId56" location="iv-available-water" xr:uid="{7C9A8246-47D9-49E9-B1F6-3C1231D8F415}"/>
-    <hyperlink ref="N100" r:id="rId57" location="v-enter-withdraw-within-available-water" display="Help withdraw" xr:uid="{3ACF8917-D3A9-467E-B1B3-4EFD5F90425B}"/>
-    <hyperlink ref="N101" r:id="rId58" location="vi-end-of-year-balance" xr:uid="{64582986-19BE-4DA6-A576-9ED7048A63F6}"/>
-    <hyperlink ref="N98" r:id="rId59" location="iii-net-trade-volume-all-participants" xr:uid="{00DE0E22-6C57-4CFB-AC1B-701E93DC729D}"/>
-    <hyperlink ref="N5" r:id="rId60" xr:uid="{F3F98DA2-630F-4A3D-9677-FDD7F3BB102E}"/>
+    <hyperlink ref="N17" r:id="rId2" location="1b-make-assumptions" xr:uid="{91CC7212-C579-4B1B-A8B8-969D4549837D}"/>
+    <hyperlink ref="N18" r:id="rId3" location="i-evaporation-rates" xr:uid="{23C61350-606E-472B-90E1-88574D6741EE}"/>
+    <hyperlink ref="N19" r:id="rId4" location="ii-start-storage" xr:uid="{692C3AE6-515B-4C08-B6EC-0557E75E9511}"/>
+    <hyperlink ref="N20" r:id="rId5" location="iii-protection-elevations" xr:uid="{16CC5ED4-0369-416C-AC3E-3AD6F831A454}"/>
+    <hyperlink ref="N21" r:id="rId6" location="iv-the-protection-volumes" xr:uid="{D7802E8D-5298-4564-9936-B3226B6E96DA}"/>
+    <hyperlink ref="N22" r:id="rId7" location="v-prior-9-year-lake-powell-release" xr:uid="{9E773CCF-F296-48D2-ADA9-5456ABC7F062}"/>
+    <hyperlink ref="N23" r:id="rId8" location="vi-prior-9-year-paria-river-flow" xr:uid="{8CAE8559-5BD9-4D9F-8655-D1F3AE1FCD4D}"/>
+    <hyperlink ref="N24" r:id="rId9" location="vii-delivery-to-meet-10-year-requirement" xr:uid="{B6DDA7AA-2218-4D2F-9A7A-A0EDBEFDC5B1}"/>
+    <hyperlink ref="N28" r:id="rId10" location="step-2-specify-natural-inflow-to-lake-powell" xr:uid="{78DF76B4-BE79-4AC1-9F08-EC86A0A72F91}"/>
+    <hyperlink ref="N29" r:id="rId11" location="2a-intervening-grand-canyon-flow" xr:uid="{CFD884C0-2149-42F6-AD5A-482CF40D5292}"/>
+    <hyperlink ref="N30" r:id="rId12" location="2b-mead-to-imperial-dam-intervening-flow" xr:uid="{B8EF30C2-739D-4E21-B63A-F17F9947326A}"/>
+    <hyperlink ref="N31" r:id="rId13" location="2c-havasuparker-evaporation-and-evapotranspiration" xr:uid="{70E7AC6A-42AC-4DE1-ADFB-FBA8230C308E}"/>
+    <hyperlink ref="N35" r:id="rId14" location="step-3-split-existing-reservoir-storage-among-accounts-year-1-only" xr:uid="{B36B453C-62F8-4461-8E49-8546C848C695}"/>
+    <hyperlink ref="N42" r:id="rId15" location="3a-begin-of-year-reservoir-storage" display="Help begin year storage" xr:uid="{52EB1038-72CB-4676-AD3B-3DD4322D2D3C}"/>
+    <hyperlink ref="N45" r:id="rId16" location="3b-calculate-powell--mead-evaporation" xr:uid="{9002111C-2D36-45B1-97D8-5FCB363BD9BD}"/>
+    <hyperlink ref="N52" r:id="rId17" location="3c-calculate-mexico-water-allocation" xr:uid="{C14FC6B3-6E3C-48F5-B820-A74ADC9C86D6}"/>
+    <hyperlink ref="N53" r:id="rId18" location="split-combined-natural-inflow-among-accounts" xr:uid="{63C31A0C-C046-4C6B-B63E-AA3031EC5E49}"/>
+    <hyperlink ref="N63" r:id="rId19" location="step-5-participant-dashboards--conserve-consume-and-trade" xr:uid="{E1DA626C-61A5-4CB7-94B9-52C34A1556D5}"/>
+    <hyperlink ref="N65" r:id="rId20" location="ii-compensation" xr:uid="{19918E71-71AD-4C9C-BB3F-A5AF3D55F1D7}"/>
+    <hyperlink ref="N66" r:id="rId21" location="iii-net-trade-volume-all-participants" xr:uid="{3E7AF6CA-1278-4129-B9E4-725FD18D820D}"/>
+    <hyperlink ref="N67" r:id="rId22" location="iv-available-water" xr:uid="{4566CC8F-1D0F-43BA-BAD8-C66179151606}"/>
+    <hyperlink ref="N68" r:id="rId23" location="v-enter-withdraw-within-available-water" display="Help withdraw" xr:uid="{FA435611-F017-4A4C-84C0-3BC240C90BC3}"/>
+    <hyperlink ref="N69" r:id="rId24" location="vi-end-of-year-balance" xr:uid="{43A45EF2-1AE7-497D-9090-A6710371091B}"/>
+    <hyperlink ref="N103" r:id="rId25" location="5a-shared-reserve-dashboard" display="Help shared, reserve" xr:uid="{93564FFE-2F11-4E1B-8E30-F04D091042B0}"/>
+    <hyperlink ref="N111" r:id="rId26" location="step-6-summary-of-participant-actions" xr:uid="{39E9E91B-EE9B-4603-9A19-992E43688C4C}"/>
+    <hyperlink ref="N134" r:id="rId27" location="6a-combined-storage--end-of-year" xr:uid="{18709FDC-6FB8-4FF1-82C7-3E0140C4C207}"/>
+    <hyperlink ref="N137" r:id="rId28" location="step-8-move-to-next-year" xr:uid="{0D1EBCA9-BE7F-441F-A17C-5330CFCE7596}"/>
+    <hyperlink ref="N79" r:id="rId29" location="step-5-player-dashboards--conserve-consume-and-trade" xr:uid="{115088D1-B3CF-4D72-A6D6-92770E18F116}"/>
+    <hyperlink ref="N80" r:id="rId30" location="i-buy-or-sell-water-from-other-players" xr:uid="{D5A878F8-1AB0-4367-BFA6-4F25001F73AD}"/>
+    <hyperlink ref="N81" r:id="rId31" location="ii-compensation" xr:uid="{74477D73-291E-4A7F-86F2-C21A0DF60CEA}"/>
+    <hyperlink ref="N83" r:id="rId32" location="iv-available-water" xr:uid="{096A8B03-D32B-4628-BC3E-B3E64954FA42}"/>
+    <hyperlink ref="N84" r:id="rId33" location="v-enter-withdraw-within-available-water" display="Help withdraw" xr:uid="{4ED17C45-EBF9-4C45-9229-5218A5ECD61F}"/>
+    <hyperlink ref="N85" r:id="rId34" location="vi-end-of-year-balance" xr:uid="{C6E40832-042B-43D8-90B9-CD82703389C7}"/>
+    <hyperlink ref="N25" r:id="rId35" location="upper-basin-pre-1922-water-rights" xr:uid="{25504FB1-E197-4C3D-945D-5BDD83C2C59E}"/>
+    <hyperlink ref="N64" r:id="rId36" location="i-buy-or-sell-water-from-other-participantss" xr:uid="{D2AC05B4-FD61-425B-9046-D87C8AAAAEA0}"/>
+    <hyperlink ref="N71" r:id="rId37" location="step-5-participant-dashboards--conserve-consume-and-trade" xr:uid="{D67E6EF8-391E-4D21-9E33-260AECB2DB20}"/>
+    <hyperlink ref="N73" r:id="rId38" location="ii-compensation" xr:uid="{5D3E22F6-98D1-4F8D-AC9B-79BC60BD9D4C}"/>
+    <hyperlink ref="N74" r:id="rId39" location="iii-net-trade-volume-all-participants" xr:uid="{E4C097D5-D12A-4D05-9CB5-F12180A8841F}"/>
+    <hyperlink ref="N75" r:id="rId40" location="iv-available-water" xr:uid="{92A2BD5E-9234-4CDA-B631-2F26F1EDA2F6}"/>
+    <hyperlink ref="N76" r:id="rId41" location="v-enter-withdraw-within-available-water" display="Help withdraw" xr:uid="{D566555A-5FE4-4D77-A91F-AB8CA37C5882}"/>
+    <hyperlink ref="N77" r:id="rId42" location="vi-end-of-year-balance" xr:uid="{43994CDC-2740-40CF-8975-5A1D654DE92E}"/>
+    <hyperlink ref="N72" r:id="rId43" location="i-buy-or-sell-water-from-other-participantss" xr:uid="{99CA01B4-F83D-4392-BFD6-E3696F3B060F}"/>
+    <hyperlink ref="N82" r:id="rId44" location="iii-net-trade-volume-all-participants" xr:uid="{35106ED0-ED39-4B94-A4D9-B79EFE11A2E6}"/>
+    <hyperlink ref="N87" r:id="rId45" location="step-5-player-dashboards--conserve-consume-and-trade" xr:uid="{AEF1AABF-406E-492C-A9C6-6D4F230E19E9}"/>
+    <hyperlink ref="N88" r:id="rId46" location="i-buy-or-sell-water-from-other-players" xr:uid="{A414CAB3-AC71-40F2-BCEE-3B4BD79CCEC2}"/>
+    <hyperlink ref="N89" r:id="rId47" location="ii-compensation" xr:uid="{8233903D-3600-4882-9905-8BB60669B1D3}"/>
+    <hyperlink ref="N91" r:id="rId48" location="iv-available-water" xr:uid="{BD162207-CEDD-4927-ACFE-B798DB92B590}"/>
+    <hyperlink ref="N92" r:id="rId49" location="v-enter-withdraw-within-available-water" display="Help withdraw" xr:uid="{80D88F54-62DF-498A-A03F-9FC4097F6B84}"/>
+    <hyperlink ref="N93" r:id="rId50" location="vi-end-of-year-balance" xr:uid="{3C22C7BF-428B-4FE8-9C2E-F555E1D2FB9F}"/>
+    <hyperlink ref="N90" r:id="rId51" location="iii-net-trade-volume-all-participants" xr:uid="{4F49F47E-D9E6-4681-A7EF-3B21819F5A2A}"/>
+    <hyperlink ref="N95" r:id="rId52" location="step-5-player-dashboards--conserve-consume-and-trade" xr:uid="{0EF1BC22-639A-4CAC-8C5C-1003B2A67B6B}"/>
+    <hyperlink ref="N96" r:id="rId53" location="i-buy-or-sell-water-from-other-players" xr:uid="{7B556B5C-2F11-4498-8C4A-C03479306858}"/>
+    <hyperlink ref="N97" r:id="rId54" location="ii-compensation" xr:uid="{9ABDDEAE-D66A-426B-9D45-11CC8D3256D9}"/>
+    <hyperlink ref="N99" r:id="rId55" location="iv-available-water" xr:uid="{7C9A8246-47D9-49E9-B1F6-3C1231D8F415}"/>
+    <hyperlink ref="N100" r:id="rId56" location="v-enter-withdraw-within-available-water" display="Help withdraw" xr:uid="{3ACF8917-D3A9-467E-B1B3-4EFD5F90425B}"/>
+    <hyperlink ref="N101" r:id="rId57" location="vi-end-of-year-balance" xr:uid="{64582986-19BE-4DA6-A576-9ED7048A63F6}"/>
+    <hyperlink ref="N98" r:id="rId58" location="iii-net-trade-volume-all-participants" xr:uid="{00DE0E22-6C57-4CFB-AC1B-701E93DC729D}"/>
+    <hyperlink ref="N12" r:id="rId59" location="1a-explain-cell-types" xr:uid="{5E0F137C-003B-4215-AD3B-C722FAB0B485}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -21423,57 +21519,57 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="I5" s="311" t="s">
+      <c r="I5" s="309" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="311" t="s">
+      <c r="J5" s="309" t="s">
+        <v>265</v>
+      </c>
+      <c r="K5" s="309" t="s">
+        <v>266</v>
+      </c>
+      <c r="L5" s="306" t="s">
+        <v>267</v>
+      </c>
+      <c r="M5" s="307"/>
+      <c r="N5" s="307"/>
+      <c r="O5" s="307"/>
+      <c r="P5" s="308"/>
+      <c r="Q5" s="298" t="s">
         <v>268</v>
       </c>
-      <c r="K5" s="311" t="s">
-        <v>269</v>
-      </c>
-      <c r="L5" s="308" t="s">
-        <v>270</v>
-      </c>
-      <c r="M5" s="309"/>
-      <c r="N5" s="309"/>
-      <c r="O5" s="309"/>
-      <c r="P5" s="310"/>
-      <c r="Q5" s="300" t="s">
-        <v>271</v>
-      </c>
-      <c r="R5" s="301"/>
-      <c r="S5" s="301"/>
-      <c r="T5" s="301"/>
-      <c r="U5" s="302"/>
+      <c r="R5" s="299"/>
+      <c r="S5" s="299"/>
+      <c r="T5" s="299"/>
+      <c r="U5" s="300"/>
     </row>
     <row r="6" spans="1:21" s="191" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="192" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C6" s="192" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D6" s="192" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E6" s="192" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="F6" s="192" t="s">
         <v>18</v>
@@ -21481,51 +21577,51 @@
       <c r="G6" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="312"/>
-      <c r="J6" s="312"/>
-      <c r="K6" s="312"/>
+      <c r="I6" s="310"/>
+      <c r="J6" s="310"/>
+      <c r="K6" s="310"/>
       <c r="L6" s="193" t="s">
+        <v>270</v>
+      </c>
+      <c r="M6" s="193" t="s">
+        <v>271</v>
+      </c>
+      <c r="N6" s="193" t="s">
+        <v>272</v>
+      </c>
+      <c r="O6" s="193" t="s">
         <v>273</v>
       </c>
-      <c r="M6" s="193" t="s">
+      <c r="P6" s="193" t="s">
         <v>274</v>
       </c>
-      <c r="N6" s="193" t="s">
+      <c r="Q6" s="194" t="s">
         <v>275</v>
       </c>
-      <c r="O6" s="193" t="s">
+      <c r="R6" s="194" t="s">
         <v>276</v>
       </c>
-      <c r="P6" s="193" t="s">
+      <c r="S6" s="194" t="s">
         <v>277</v>
       </c>
-      <c r="Q6" s="194" t="s">
+      <c r="T6" s="194" t="s">
         <v>278</v>
       </c>
-      <c r="R6" s="194" t="s">
+      <c r="U6" s="194" t="s">
         <v>279</v>
       </c>
-      <c r="S6" s="194" t="s">
+    </row>
+    <row r="7" spans="1:21" s="191" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="306" t="s">
         <v>280</v>
       </c>
-      <c r="T6" s="194" t="s">
+      <c r="C7" s="307"/>
+      <c r="D7" s="307"/>
+      <c r="E7" s="307"/>
+      <c r="F7" s="307"/>
+      <c r="G7" s="308"/>
+      <c r="I7" s="195" t="s">
         <v>281</v>
-      </c>
-      <c r="U6" s="194" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" s="191" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="308" t="s">
-        <v>283</v>
-      </c>
-      <c r="C7" s="309"/>
-      <c r="D7" s="309"/>
-      <c r="E7" s="309"/>
-      <c r="F7" s="309"/>
-      <c r="G7" s="310"/>
-      <c r="I7" s="195" t="s">
-        <v>284</v>
       </c>
       <c r="J7" s="195">
         <f>B13</f>
@@ -21592,7 +21688,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="195" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J8" s="195">
         <f>B14</f>
@@ -21645,7 +21741,7 @@
     </row>
     <row r="9" spans="1:21" s="200" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B9" s="201" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C9" s="205">
         <v>0.8</v>
@@ -21664,7 +21760,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="195" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="J9" s="195">
         <f>B15</f>
@@ -21717,7 +21813,7 @@
     </row>
     <row r="10" spans="1:21" s="200" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B10" s="201" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C10" s="205">
         <v>0.43330000000000002</v>
@@ -21736,7 +21832,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="195" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="J10" s="195">
         <f>B16</f>
@@ -21789,17 +21885,17 @@
     </row>
     <row r="11" spans="1:21" s="200" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B11" s="201" t="s">
-        <v>290</v>
-      </c>
-      <c r="C11" s="299" t="s">
-        <v>291</v>
-      </c>
-      <c r="D11" s="299"/>
-      <c r="E11" s="299"/>
-      <c r="F11" s="299"/>
-      <c r="G11" s="299"/>
+        <v>287</v>
+      </c>
+      <c r="C11" s="297" t="s">
+        <v>288</v>
+      </c>
+      <c r="D11" s="297"/>
+      <c r="E11" s="297"/>
+      <c r="F11" s="297"/>
+      <c r="G11" s="297"/>
       <c r="I11" s="195" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J11" s="195">
         <f>B17</f>
@@ -21851,37 +21947,37 @@
       </c>
     </row>
     <row r="12" spans="1:21" s="200" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B12" s="303" t="s">
-        <v>293</v>
-      </c>
-      <c r="C12" s="304"/>
-      <c r="D12" s="304"/>
-      <c r="E12" s="304"/>
-      <c r="F12" s="304"/>
-      <c r="G12" s="304"/>
+      <c r="B12" s="301" t="s">
+        <v>290</v>
+      </c>
+      <c r="C12" s="302"/>
+      <c r="D12" s="302"/>
+      <c r="E12" s="302"/>
+      <c r="F12" s="302"/>
+      <c r="G12" s="302"/>
       <c r="I12" s="195" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J12" s="195" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="K12" s="203" t="s">
-        <v>295</v>
-      </c>
-      <c r="L12" s="305" t="s">
-        <v>291</v>
-      </c>
-      <c r="M12" s="306"/>
-      <c r="N12" s="306"/>
-      <c r="O12" s="306"/>
-      <c r="P12" s="307"/>
-      <c r="Q12" s="305" t="s">
-        <v>291</v>
-      </c>
-      <c r="R12" s="306"/>
-      <c r="S12" s="306"/>
-      <c r="T12" s="306"/>
-      <c r="U12" s="307"/>
+        <v>292</v>
+      </c>
+      <c r="L12" s="303" t="s">
+        <v>288</v>
+      </c>
+      <c r="M12" s="304"/>
+      <c r="N12" s="304"/>
+      <c r="O12" s="304"/>
+      <c r="P12" s="305"/>
+      <c r="Q12" s="303" t="s">
+        <v>288</v>
+      </c>
+      <c r="R12" s="304"/>
+      <c r="S12" s="304"/>
+      <c r="T12" s="304"/>
+      <c r="U12" s="305"/>
     </row>
     <row r="13" spans="1:21" s="200" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B13" s="201">
@@ -21904,7 +22000,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="195" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="J13" s="195">
         <v>2.7</v>
@@ -21979,7 +22075,7 @@
         <v>0.3</v>
       </c>
       <c r="I14" s="195" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="J14" s="195">
         <v>8</v>
@@ -22054,7 +22150,7 @@
         <v>0.4</v>
       </c>
       <c r="I15" s="207" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="J15" s="208"/>
       <c r="K15" s="209"/>
@@ -22094,7 +22190,7 @@
         <v>0.99999999999999989</v>
       </c>
       <c r="I16" s="208" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J16" s="208"/>
       <c r="U16" s="213"/>
@@ -22124,25 +22220,25 @@
         <v>1.5</v>
       </c>
       <c r="I17" s="208" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="U17" s="213"/>
     </row>
     <row r="18" spans="2:21" s="200" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B18" s="201" t="s">
-        <v>290</v>
-      </c>
-      <c r="C18" s="299" t="s">
-        <v>291</v>
-      </c>
-      <c r="D18" s="299"/>
-      <c r="E18" s="299"/>
-      <c r="F18" s="299"/>
-      <c r="G18" s="299"/>
+        <v>287</v>
+      </c>
+      <c r="C18" s="297" t="s">
+        <v>288</v>
+      </c>
+      <c r="D18" s="297"/>
+      <c r="E18" s="297"/>
+      <c r="F18" s="297"/>
+      <c r="G18" s="297"/>
     </row>
     <row r="19" spans="2:21" s="200" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="I19" s="200" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="J19" s="209">
         <f t="shared" ref="J19:U19" si="9">J14</f>
@@ -22590,26 +22686,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="298" t="e">
+      <c r="A1" s="312" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="298"/>
-      <c r="C1" s="298"/>
-      <c r="D1" s="298"/>
-      <c r="E1" s="298"/>
-      <c r="F1" s="298"/>
-      <c r="G1" s="298"/>
+      <c r="B1" s="312"/>
+      <c r="C1" s="312"/>
+      <c r="D1" s="312"/>
+      <c r="E1" s="312"/>
+      <c r="F1" s="312"/>
+      <c r="G1" s="312"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="285" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B3" s="285"/>
       <c r="C3" s="285"/>
@@ -22708,11 +22804,11 @@
         <v>81</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="297"/>
-      <c r="D10" s="297"/>
-      <c r="E10" s="297"/>
-      <c r="F10" s="297"/>
-      <c r="G10" s="297"/>
+      <c r="C10" s="311"/>
+      <c r="D10" s="311"/>
+      <c r="E10" s="311"/>
+      <c r="F10" s="311"/>
+      <c r="G10" s="311"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -23133,7 +23229,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C32"/>
       <c r="N32" s="141" t="s">
@@ -23234,7 +23330,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B35" s="49"/>
       <c r="C35" s="12" t="e">
@@ -23598,7 +23694,7 @@
         <v xml:space="preserve">    To Mexico</v>
       </c>
       <c r="B42" s="95" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C42" s="82" t="e">
         <f>IF(OR(C$28="",$A42=""),"",MIN(C38,C$39-SUM(C43:C46)))</f>
@@ -23875,7 +23971,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C48" s="181" t="e">
         <f>SUM(C40:C46)</f>
@@ -23930,7 +24026,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B53">
         <v>8.1999999999999993</v>
@@ -23938,7 +24034,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B54">
         <v>1.2</v>
@@ -23946,7 +24042,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B55">
         <v>0.95</v>
@@ -23954,7 +24050,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B56">
         <f>1.5/2</f>
@@ -23963,7 +24059,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B57">
         <f>B53-SUM(B54:B56)</f>
@@ -23975,6 +24071,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -23982,12 +24084,6 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>

</xml_diff>

<commit_message>
Reservoir start storage help
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AED6EB-FB37-4854-8CE8-3C7921535987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB80E85A-B129-48F6-92C1-510E2FB320E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -3182,51 +3182,6 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3254,13 +3209,10 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3284,6 +3236,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3301,6 +3259,51 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3404,11 +3407,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3430,9 +3433,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -14851,20 +14851,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="255" t="s">
+      <c r="A1" s="240" t="s">
         <v>321</v>
       </c>
-      <c r="B1" s="255"/>
-      <c r="C1" s="255"/>
-      <c r="D1" s="255"/>
-      <c r="E1" s="255"/>
-      <c r="F1" s="255"/>
-      <c r="G1" s="255"/>
-      <c r="H1" s="255"/>
-      <c r="I1" s="255"/>
-      <c r="J1" s="255"/>
-      <c r="K1" s="255"/>
-      <c r="L1" s="255"/>
+      <c r="B1" s="240"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
+      <c r="F1" s="240"/>
+      <c r="G1" s="240"/>
+      <c r="H1" s="240"/>
+      <c r="I1" s="240"/>
+      <c r="J1" s="240"/>
+      <c r="K1" s="240"/>
+      <c r="L1" s="240"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -14890,41 +14890,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="256" t="s">
+      <c r="A4" s="241" t="s">
         <v>349</v>
       </c>
-      <c r="B4" s="257"/>
-      <c r="C4" s="257"/>
-      <c r="D4" s="257"/>
-      <c r="E4" s="257"/>
-      <c r="F4" s="257"/>
-      <c r="G4" s="257"/>
-      <c r="H4" s="257"/>
-      <c r="I4" s="257"/>
-      <c r="J4" s="257"/>
-      <c r="K4" s="257"/>
-      <c r="L4" s="258"/>
-      <c r="N4" s="259"/>
-      <c r="O4" s="259"/>
-      <c r="P4" s="259"/>
-      <c r="Q4" s="259"/>
-      <c r="R4" s="259"/>
+      <c r="B4" s="242"/>
+      <c r="C4" s="242"/>
+      <c r="D4" s="242"/>
+      <c r="E4" s="242"/>
+      <c r="F4" s="242"/>
+      <c r="G4" s="242"/>
+      <c r="H4" s="242"/>
+      <c r="I4" s="242"/>
+      <c r="J4" s="242"/>
+      <c r="K4" s="242"/>
+      <c r="L4" s="243"/>
+      <c r="N4" s="244"/>
+      <c r="O4" s="244"/>
+      <c r="P4" s="244"/>
+      <c r="Q4" s="244"/>
+      <c r="R4" s="244"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="260" t="s">
+      <c r="A5" s="245" t="s">
         <v>350</v>
       </c>
-      <c r="B5" s="320"/>
-      <c r="C5" s="320"/>
-      <c r="D5" s="320"/>
-      <c r="E5" s="320"/>
-      <c r="F5" s="320"/>
-      <c r="G5" s="320"/>
-      <c r="H5" s="320"/>
-      <c r="I5" s="320"/>
-      <c r="J5" s="320"/>
-      <c r="K5" s="320"/>
-      <c r="L5" s="261"/>
+      <c r="B5" s="246"/>
+      <c r="C5" s="246"/>
+      <c r="D5" s="246"/>
+      <c r="E5" s="246"/>
+      <c r="F5" s="246"/>
+      <c r="G5" s="246"/>
+      <c r="H5" s="246"/>
+      <c r="I5" s="246"/>
+      <c r="J5" s="246"/>
+      <c r="K5" s="246"/>
+      <c r="L5" s="247"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -14932,20 +14932,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="260" t="s">
+      <c r="A6" s="245" t="s">
         <v>352</v>
       </c>
-      <c r="B6" s="320"/>
-      <c r="C6" s="320"/>
-      <c r="D6" s="320"/>
-      <c r="E6" s="320"/>
-      <c r="F6" s="320"/>
-      <c r="G6" s="320"/>
-      <c r="H6" s="320"/>
-      <c r="I6" s="320"/>
-      <c r="J6" s="320"/>
-      <c r="K6" s="320"/>
-      <c r="L6" s="261"/>
+      <c r="B6" s="246"/>
+      <c r="C6" s="246"/>
+      <c r="D6" s="246"/>
+      <c r="E6" s="246"/>
+      <c r="F6" s="246"/>
+      <c r="G6" s="246"/>
+      <c r="H6" s="246"/>
+      <c r="I6" s="246"/>
+      <c r="J6" s="246"/>
+      <c r="K6" s="246"/>
+      <c r="L6" s="247"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -14954,19 +14954,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="235"/>
-      <c r="B7" s="320" t="s">
+      <c r="B7" s="246" t="s">
         <v>353</v>
       </c>
-      <c r="C7" s="320"/>
-      <c r="D7" s="320"/>
-      <c r="E7" s="320"/>
-      <c r="F7" s="320"/>
-      <c r="G7" s="320"/>
-      <c r="H7" s="320"/>
-      <c r="I7" s="320"/>
-      <c r="J7" s="320"/>
-      <c r="K7" s="320"/>
-      <c r="L7" s="261"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246"/>
+      <c r="K7" s="246"/>
+      <c r="L7" s="247"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -14975,19 +14975,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="236"/>
-      <c r="B8" s="262" t="s">
+      <c r="B8" s="263" t="s">
         <v>354</v>
       </c>
-      <c r="C8" s="262"/>
-      <c r="D8" s="262"/>
-      <c r="E8" s="262"/>
-      <c r="F8" s="262"/>
-      <c r="G8" s="262"/>
-      <c r="H8" s="262"/>
-      <c r="I8" s="262"/>
-      <c r="J8" s="262"/>
-      <c r="K8" s="262"/>
-      <c r="L8" s="263"/>
+      <c r="C8" s="263"/>
+      <c r="D8" s="263"/>
+      <c r="E8" s="263"/>
+      <c r="F8" s="263"/>
+      <c r="G8" s="263"/>
+      <c r="H8" s="263"/>
+      <c r="I8" s="263"/>
+      <c r="J8" s="263"/>
+      <c r="K8" s="263"/>
+      <c r="L8" s="264"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15009,84 +15009,84 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="264" t="s">
+      <c r="A10" s="248" t="s">
         <v>217</v>
       </c>
-      <c r="B10" s="265"/>
-      <c r="C10" s="265"/>
-      <c r="D10" s="265"/>
-      <c r="E10" s="265"/>
-      <c r="F10" s="265"/>
-      <c r="G10" s="265"/>
-      <c r="H10" s="265"/>
-      <c r="I10" s="265"/>
-      <c r="J10" s="265"/>
-      <c r="K10" s="265"/>
-      <c r="L10" s="266"/>
+      <c r="B10" s="249"/>
+      <c r="C10" s="249"/>
+      <c r="D10" s="249"/>
+      <c r="E10" s="249"/>
+      <c r="F10" s="249"/>
+      <c r="G10" s="249"/>
+      <c r="H10" s="249"/>
+      <c r="I10" s="249"/>
+      <c r="J10" s="249"/>
+      <c r="K10" s="249"/>
+      <c r="L10" s="250"/>
     </row>
     <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="267" t="s">
+      <c r="A11" s="251" t="s">
         <v>351</v>
       </c>
-      <c r="B11" s="268"/>
-      <c r="C11" s="268"/>
-      <c r="D11" s="268"/>
-      <c r="E11" s="268"/>
-      <c r="F11" s="268"/>
-      <c r="G11" s="268"/>
-      <c r="H11" s="268"/>
-      <c r="I11" s="268"/>
-      <c r="J11" s="268"/>
-      <c r="K11" s="268"/>
-      <c r="L11" s="269"/>
+      <c r="B11" s="252"/>
+      <c r="C11" s="252"/>
+      <c r="D11" s="252"/>
+      <c r="E11" s="252"/>
+      <c r="F11" s="252"/>
+      <c r="G11" s="252"/>
+      <c r="H11" s="252"/>
+      <c r="I11" s="252"/>
+      <c r="J11" s="252"/>
+      <c r="K11" s="252"/>
+      <c r="L11" s="253"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="270" t="s">
+      <c r="A12" s="254" t="s">
         <v>355</v>
       </c>
-      <c r="B12" s="247"/>
-      <c r="C12" s="247"/>
-      <c r="D12" s="247"/>
-      <c r="E12" s="247"/>
-      <c r="F12" s="247"/>
-      <c r="G12" s="247"/>
-      <c r="H12" s="247"/>
-      <c r="I12" s="247"/>
-      <c r="J12" s="247"/>
-      <c r="K12" s="247"/>
-      <c r="L12" s="248"/>
+      <c r="B12" s="255"/>
+      <c r="C12" s="255"/>
+      <c r="D12" s="255"/>
+      <c r="E12" s="255"/>
+      <c r="F12" s="255"/>
+      <c r="G12" s="255"/>
+      <c r="H12" s="255"/>
+      <c r="I12" s="255"/>
+      <c r="J12" s="255"/>
+      <c r="K12" s="255"/>
+      <c r="L12" s="256"/>
     </row>
     <row r="13" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="270" t="s">
+      <c r="A13" s="254" t="s">
         <v>218</v>
       </c>
-      <c r="B13" s="247"/>
-      <c r="C13" s="247"/>
-      <c r="D13" s="247"/>
-      <c r="E13" s="247"/>
-      <c r="F13" s="247"/>
-      <c r="G13" s="247"/>
-      <c r="H13" s="247"/>
-      <c r="I13" s="247"/>
-      <c r="J13" s="247"/>
-      <c r="K13" s="247"/>
-      <c r="L13" s="248"/>
+      <c r="B13" s="255"/>
+      <c r="C13" s="255"/>
+      <c r="D13" s="255"/>
+      <c r="E13" s="255"/>
+      <c r="F13" s="255"/>
+      <c r="G13" s="255"/>
+      <c r="H13" s="255"/>
+      <c r="I13" s="255"/>
+      <c r="J13" s="255"/>
+      <c r="K13" s="255"/>
+      <c r="L13" s="256"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="271" t="s">
+      <c r="A14" s="257" t="s">
         <v>356</v>
       </c>
-      <c r="B14" s="272"/>
-      <c r="C14" s="272"/>
-      <c r="D14" s="272"/>
-      <c r="E14" s="272"/>
-      <c r="F14" s="272"/>
-      <c r="G14" s="272"/>
-      <c r="H14" s="272"/>
-      <c r="I14" s="272"/>
-      <c r="J14" s="272"/>
-      <c r="K14" s="272"/>
-      <c r="L14" s="273"/>
+      <c r="B14" s="258"/>
+      <c r="C14" s="258"/>
+      <c r="D14" s="258"/>
+      <c r="E14" s="258"/>
+      <c r="F14" s="258"/>
+      <c r="G14" s="258"/>
+      <c r="H14" s="258"/>
+      <c r="I14" s="258"/>
+      <c r="J14" s="258"/>
+      <c r="K14" s="258"/>
+      <c r="L14" s="259"/>
     </row>
     <row r="15" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="113"/>
@@ -15103,332 +15103,332 @@
       <c r="L15" s="113"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="274" t="s">
+      <c r="A16" s="260" t="s">
         <v>348</v>
       </c>
-      <c r="B16" s="275"/>
-      <c r="C16" s="275"/>
-      <c r="D16" s="275"/>
-      <c r="E16" s="275"/>
-      <c r="F16" s="275"/>
-      <c r="G16" s="275"/>
-      <c r="H16" s="275"/>
-      <c r="I16" s="275"/>
-      <c r="J16" s="275"/>
-      <c r="K16" s="275"/>
-      <c r="L16" s="276"/>
+      <c r="B16" s="261"/>
+      <c r="C16" s="261"/>
+      <c r="D16" s="261"/>
+      <c r="E16" s="261"/>
+      <c r="F16" s="261"/>
+      <c r="G16" s="261"/>
+      <c r="H16" s="261"/>
+      <c r="I16" s="261"/>
+      <c r="J16" s="261"/>
+      <c r="K16" s="261"/>
+      <c r="L16" s="262"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="252" t="s">
+      <c r="A17" s="237" t="s">
         <v>227</v>
       </c>
-      <c r="B17" s="253"/>
-      <c r="C17" s="253"/>
-      <c r="D17" s="253"/>
-      <c r="E17" s="253"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="253"/>
-      <c r="I17" s="253"/>
-      <c r="J17" s="253"/>
-      <c r="K17" s="253"/>
-      <c r="L17" s="254"/>
+      <c r="B17" s="238"/>
+      <c r="C17" s="238"/>
+      <c r="D17" s="238"/>
+      <c r="E17" s="238"/>
+      <c r="F17" s="238"/>
+      <c r="G17" s="238"/>
+      <c r="H17" s="238"/>
+      <c r="I17" s="238"/>
+      <c r="J17" s="238"/>
+      <c r="K17" s="238"/>
+      <c r="L17" s="239"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="230">
         <v>1</v>
       </c>
-      <c r="B18" s="240" t="s">
+      <c r="B18" s="267" t="s">
         <v>226</v>
       </c>
-      <c r="C18" s="240"/>
-      <c r="D18" s="240"/>
-      <c r="E18" s="240"/>
-      <c r="F18" s="240"/>
-      <c r="G18" s="240"/>
-      <c r="H18" s="240"/>
-      <c r="I18" s="240"/>
-      <c r="J18" s="240"/>
-      <c r="K18" s="240"/>
-      <c r="L18" s="241"/>
+      <c r="C18" s="267"/>
+      <c r="D18" s="267"/>
+      <c r="E18" s="267"/>
+      <c r="F18" s="267"/>
+      <c r="G18" s="267"/>
+      <c r="H18" s="267"/>
+      <c r="I18" s="267"/>
+      <c r="J18" s="267"/>
+      <c r="K18" s="267"/>
+      <c r="L18" s="268"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="230">
         <v>2</v>
       </c>
-      <c r="B19" s="240" t="s">
+      <c r="B19" s="267" t="s">
         <v>344</v>
       </c>
-      <c r="C19" s="240"/>
-      <c r="D19" s="240"/>
-      <c r="E19" s="240"/>
-      <c r="F19" s="240"/>
-      <c r="G19" s="240"/>
-      <c r="H19" s="240"/>
-      <c r="I19" s="240"/>
-      <c r="J19" s="240"/>
-      <c r="K19" s="240"/>
-      <c r="L19" s="241"/>
+      <c r="C19" s="267"/>
+      <c r="D19" s="267"/>
+      <c r="E19" s="267"/>
+      <c r="F19" s="267"/>
+      <c r="G19" s="267"/>
+      <c r="H19" s="267"/>
+      <c r="I19" s="267"/>
+      <c r="J19" s="267"/>
+      <c r="K19" s="267"/>
+      <c r="L19" s="268"/>
       <c r="N19" s="106"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="230">
         <v>3</v>
       </c>
-      <c r="B20" s="240" t="s">
+      <c r="B20" s="267" t="s">
         <v>219</v>
       </c>
-      <c r="C20" s="240"/>
-      <c r="D20" s="240"/>
-      <c r="E20" s="240"/>
-      <c r="F20" s="240"/>
-      <c r="G20" s="240"/>
-      <c r="H20" s="240"/>
-      <c r="I20" s="240"/>
-      <c r="J20" s="240"/>
-      <c r="K20" s="240"/>
-      <c r="L20" s="241"/>
+      <c r="C20" s="267"/>
+      <c r="D20" s="267"/>
+      <c r="E20" s="267"/>
+      <c r="F20" s="267"/>
+      <c r="G20" s="267"/>
+      <c r="H20" s="267"/>
+      <c r="I20" s="267"/>
+      <c r="J20" s="267"/>
+      <c r="K20" s="267"/>
+      <c r="L20" s="268"/>
       <c r="N20" s="106"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="230">
         <v>4</v>
       </c>
-      <c r="B21" s="240" t="s">
+      <c r="B21" s="267" t="s">
         <v>357</v>
       </c>
-      <c r="C21" s="240"/>
-      <c r="D21" s="240"/>
-      <c r="E21" s="240"/>
-      <c r="F21" s="240"/>
-      <c r="G21" s="240"/>
-      <c r="H21" s="240"/>
-      <c r="I21" s="240"/>
-      <c r="J21" s="240"/>
-      <c r="K21" s="240"/>
-      <c r="L21" s="241"/>
+      <c r="C21" s="267"/>
+      <c r="D21" s="267"/>
+      <c r="E21" s="267"/>
+      <c r="F21" s="267"/>
+      <c r="G21" s="267"/>
+      <c r="H21" s="267"/>
+      <c r="I21" s="267"/>
+      <c r="J21" s="267"/>
+      <c r="K21" s="267"/>
+      <c r="L21" s="268"/>
       <c r="N21" s="106"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="230">
         <v>5</v>
       </c>
-      <c r="B22" s="240" t="s">
+      <c r="B22" s="267" t="s">
         <v>220</v>
       </c>
-      <c r="C22" s="240"/>
-      <c r="D22" s="240"/>
-      <c r="E22" s="240"/>
-      <c r="F22" s="240"/>
-      <c r="G22" s="240"/>
-      <c r="H22" s="240"/>
-      <c r="I22" s="240"/>
-      <c r="J22" s="240"/>
-      <c r="K22" s="240"/>
-      <c r="L22" s="241"/>
+      <c r="C22" s="267"/>
+      <c r="D22" s="267"/>
+      <c r="E22" s="267"/>
+      <c r="F22" s="267"/>
+      <c r="G22" s="267"/>
+      <c r="H22" s="267"/>
+      <c r="I22" s="267"/>
+      <c r="J22" s="267"/>
+      <c r="K22" s="267"/>
+      <c r="L22" s="268"/>
       <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="230"/>
-      <c r="B23" s="240" t="s">
+      <c r="B23" s="267" t="s">
         <v>221</v>
       </c>
-      <c r="C23" s="240"/>
-      <c r="D23" s="240"/>
-      <c r="E23" s="240"/>
-      <c r="F23" s="240"/>
-      <c r="G23" s="240"/>
-      <c r="H23" s="240"/>
-      <c r="I23" s="240"/>
-      <c r="J23" s="240"/>
-      <c r="K23" s="240"/>
-      <c r="L23" s="241"/>
+      <c r="C23" s="267"/>
+      <c r="D23" s="267"/>
+      <c r="E23" s="267"/>
+      <c r="F23" s="267"/>
+      <c r="G23" s="267"/>
+      <c r="H23" s="267"/>
+      <c r="I23" s="267"/>
+      <c r="J23" s="267"/>
+      <c r="K23" s="267"/>
+      <c r="L23" s="268"/>
       <c r="N23" s="106"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="230"/>
-      <c r="B24" s="240" t="s">
+      <c r="B24" s="267" t="s">
         <v>222</v>
       </c>
-      <c r="C24" s="240"/>
-      <c r="D24" s="240"/>
-      <c r="E24" s="240"/>
-      <c r="F24" s="240"/>
-      <c r="G24" s="240"/>
-      <c r="H24" s="240"/>
-      <c r="I24" s="240"/>
-      <c r="J24" s="240"/>
-      <c r="K24" s="240"/>
-      <c r="L24" s="241"/>
+      <c r="C24" s="267"/>
+      <c r="D24" s="267"/>
+      <c r="E24" s="267"/>
+      <c r="F24" s="267"/>
+      <c r="G24" s="267"/>
+      <c r="H24" s="267"/>
+      <c r="I24" s="267"/>
+      <c r="J24" s="267"/>
+      <c r="K24" s="267"/>
+      <c r="L24" s="268"/>
       <c r="N24" s="106"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="249" t="s">
+      <c r="A25" s="269" t="s">
         <v>228</v>
       </c>
-      <c r="B25" s="250"/>
-      <c r="C25" s="250"/>
-      <c r="D25" s="250"/>
-      <c r="E25" s="250"/>
-      <c r="F25" s="250"/>
-      <c r="G25" s="250"/>
-      <c r="H25" s="250"/>
-      <c r="I25" s="250"/>
-      <c r="J25" s="250"/>
-      <c r="K25" s="250"/>
-      <c r="L25" s="251"/>
+      <c r="B25" s="270"/>
+      <c r="C25" s="270"/>
+      <c r="D25" s="270"/>
+      <c r="E25" s="270"/>
+      <c r="F25" s="270"/>
+      <c r="G25" s="270"/>
+      <c r="H25" s="270"/>
+      <c r="I25" s="270"/>
+      <c r="J25" s="270"/>
+      <c r="K25" s="270"/>
+      <c r="L25" s="271"/>
       <c r="N25" s="106"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="230">
         <v>1</v>
       </c>
-      <c r="B26" s="240" t="s">
+      <c r="B26" s="267" t="s">
         <v>223</v>
       </c>
-      <c r="C26" s="240"/>
-      <c r="D26" s="240"/>
-      <c r="E26" s="240"/>
-      <c r="F26" s="240"/>
-      <c r="G26" s="240"/>
-      <c r="H26" s="240"/>
-      <c r="I26" s="240"/>
-      <c r="J26" s="240"/>
-      <c r="K26" s="240"/>
-      <c r="L26" s="241"/>
+      <c r="C26" s="267"/>
+      <c r="D26" s="267"/>
+      <c r="E26" s="267"/>
+      <c r="F26" s="267"/>
+      <c r="G26" s="267"/>
+      <c r="H26" s="267"/>
+      <c r="I26" s="267"/>
+      <c r="J26" s="267"/>
+      <c r="K26" s="267"/>
+      <c r="L26" s="268"/>
       <c r="N26" s="106"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="230"/>
-      <c r="B27" s="238" t="s">
+      <c r="B27" s="265" t="s">
         <v>358</v>
       </c>
-      <c r="C27" s="238"/>
-      <c r="D27" s="238"/>
-      <c r="E27" s="238"/>
-      <c r="F27" s="238"/>
-      <c r="G27" s="238"/>
-      <c r="H27" s="238"/>
-      <c r="I27" s="238"/>
-      <c r="J27" s="238"/>
-      <c r="K27" s="238"/>
-      <c r="L27" s="239"/>
+      <c r="C27" s="265"/>
+      <c r="D27" s="265"/>
+      <c r="E27" s="265"/>
+      <c r="F27" s="265"/>
+      <c r="G27" s="265"/>
+      <c r="H27" s="265"/>
+      <c r="I27" s="265"/>
+      <c r="J27" s="265"/>
+      <c r="K27" s="265"/>
+      <c r="L27" s="266"/>
       <c r="N27" s="106"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="230">
         <v>2</v>
       </c>
-      <c r="B28" s="240" t="s">
+      <c r="B28" s="267" t="s">
         <v>347</v>
       </c>
-      <c r="C28" s="240"/>
-      <c r="D28" s="240"/>
-      <c r="E28" s="240"/>
-      <c r="F28" s="240"/>
-      <c r="G28" s="240"/>
-      <c r="H28" s="240"/>
-      <c r="I28" s="240"/>
-      <c r="J28" s="240"/>
-      <c r="K28" s="240"/>
-      <c r="L28" s="241"/>
+      <c r="C28" s="267"/>
+      <c r="D28" s="267"/>
+      <c r="E28" s="267"/>
+      <c r="F28" s="267"/>
+      <c r="G28" s="267"/>
+      <c r="H28" s="267"/>
+      <c r="I28" s="267"/>
+      <c r="J28" s="267"/>
+      <c r="K28" s="267"/>
+      <c r="L28" s="268"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="230">
         <v>3</v>
       </c>
-      <c r="B29" s="240" t="s">
+      <c r="B29" s="267" t="s">
         <v>336</v>
       </c>
-      <c r="C29" s="240"/>
-      <c r="D29" s="240"/>
-      <c r="E29" s="240"/>
-      <c r="F29" s="240"/>
-      <c r="G29" s="240"/>
-      <c r="H29" s="240"/>
-      <c r="I29" s="240"/>
-      <c r="J29" s="240"/>
-      <c r="K29" s="240"/>
-      <c r="L29" s="241"/>
+      <c r="C29" s="267"/>
+      <c r="D29" s="267"/>
+      <c r="E29" s="267"/>
+      <c r="F29" s="267"/>
+      <c r="G29" s="267"/>
+      <c r="H29" s="267"/>
+      <c r="I29" s="267"/>
+      <c r="J29" s="267"/>
+      <c r="K29" s="267"/>
+      <c r="L29" s="268"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="230">
         <v>4</v>
       </c>
-      <c r="B30" s="240" t="s">
+      <c r="B30" s="267" t="s">
         <v>359</v>
       </c>
-      <c r="C30" s="240"/>
-      <c r="D30" s="240"/>
-      <c r="E30" s="240"/>
-      <c r="F30" s="240"/>
-      <c r="G30" s="240"/>
-      <c r="H30" s="240"/>
-      <c r="I30" s="240"/>
-      <c r="J30" s="240"/>
-      <c r="K30" s="240"/>
-      <c r="L30" s="241"/>
+      <c r="C30" s="267"/>
+      <c r="D30" s="267"/>
+      <c r="E30" s="267"/>
+      <c r="F30" s="267"/>
+      <c r="G30" s="267"/>
+      <c r="H30" s="267"/>
+      <c r="I30" s="267"/>
+      <c r="J30" s="267"/>
+      <c r="K30" s="267"/>
+      <c r="L30" s="268"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="230">
         <v>5</v>
       </c>
-      <c r="B31" s="238" t="s">
+      <c r="B31" s="265" t="s">
         <v>337</v>
       </c>
-      <c r="C31" s="238"/>
-      <c r="D31" s="238"/>
-      <c r="E31" s="238"/>
-      <c r="F31" s="238"/>
-      <c r="G31" s="238"/>
-      <c r="H31" s="238"/>
-      <c r="I31" s="238"/>
-      <c r="J31" s="238"/>
-      <c r="K31" s="238"/>
-      <c r="L31" s="239"/>
+      <c r="C31" s="265"/>
+      <c r="D31" s="265"/>
+      <c r="E31" s="265"/>
+      <c r="F31" s="265"/>
+      <c r="G31" s="265"/>
+      <c r="H31" s="265"/>
+      <c r="I31" s="265"/>
+      <c r="J31" s="265"/>
+      <c r="K31" s="265"/>
+      <c r="L31" s="266"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="230">
         <v>6</v>
       </c>
-      <c r="B32" s="238" t="s">
+      <c r="B32" s="265" t="s">
         <v>342</v>
       </c>
-      <c r="C32" s="238"/>
-      <c r="D32" s="238"/>
-      <c r="E32" s="238"/>
-      <c r="F32" s="238"/>
-      <c r="G32" s="238"/>
-      <c r="H32" s="238"/>
-      <c r="I32" s="238"/>
-      <c r="J32" s="238"/>
-      <c r="K32" s="238"/>
-      <c r="L32" s="239"/>
+      <c r="C32" s="265"/>
+      <c r="D32" s="265"/>
+      <c r="E32" s="265"/>
+      <c r="F32" s="265"/>
+      <c r="G32" s="265"/>
+      <c r="H32" s="265"/>
+      <c r="I32" s="265"/>
+      <c r="J32" s="265"/>
+      <c r="K32" s="265"/>
+      <c r="L32" s="266"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="230">
         <v>7</v>
       </c>
-      <c r="B33" s="240" t="s">
+      <c r="B33" s="267" t="s">
         <v>338</v>
       </c>
-      <c r="C33" s="240"/>
-      <c r="D33" s="240"/>
-      <c r="E33" s="240"/>
-      <c r="F33" s="240"/>
-      <c r="G33" s="240"/>
-      <c r="H33" s="240"/>
-      <c r="I33" s="240"/>
-      <c r="J33" s="240"/>
-      <c r="K33" s="240"/>
-      <c r="L33" s="241"/>
+      <c r="C33" s="267"/>
+      <c r="D33" s="267"/>
+      <c r="E33" s="267"/>
+      <c r="F33" s="267"/>
+      <c r="G33" s="267"/>
+      <c r="H33" s="267"/>
+      <c r="I33" s="267"/>
+      <c r="J33" s="267"/>
+      <c r="K33" s="267"/>
+      <c r="L33" s="268"/>
     </row>
     <row r="34" spans="1:12" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="230"/>
@@ -15445,56 +15445,56 @@
       <c r="L34" s="232"/>
     </row>
     <row r="35" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="249" t="s">
+      <c r="A35" s="269" t="s">
         <v>341</v>
       </c>
-      <c r="B35" s="250"/>
-      <c r="C35" s="250"/>
-      <c r="D35" s="250"/>
-      <c r="E35" s="250"/>
-      <c r="F35" s="250"/>
-      <c r="G35" s="250"/>
-      <c r="H35" s="250"/>
-      <c r="I35" s="250"/>
-      <c r="J35" s="250"/>
-      <c r="K35" s="250"/>
-      <c r="L35" s="251"/>
+      <c r="B35" s="270"/>
+      <c r="C35" s="270"/>
+      <c r="D35" s="270"/>
+      <c r="E35" s="270"/>
+      <c r="F35" s="270"/>
+      <c r="G35" s="270"/>
+      <c r="H35" s="270"/>
+      <c r="I35" s="270"/>
+      <c r="J35" s="270"/>
+      <c r="K35" s="270"/>
+      <c r="L35" s="271"/>
     </row>
     <row r="36" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="233" t="s">
         <v>339</v>
       </c>
-      <c r="B36" s="240" t="s">
+      <c r="B36" s="267" t="s">
         <v>224</v>
       </c>
-      <c r="C36" s="240"/>
-      <c r="D36" s="240"/>
-      <c r="E36" s="240"/>
-      <c r="F36" s="240"/>
-      <c r="G36" s="240"/>
-      <c r="H36" s="240"/>
-      <c r="I36" s="240"/>
-      <c r="J36" s="240"/>
-      <c r="K36" s="240"/>
-      <c r="L36" s="241"/>
+      <c r="C36" s="267"/>
+      <c r="D36" s="267"/>
+      <c r="E36" s="267"/>
+      <c r="F36" s="267"/>
+      <c r="G36" s="267"/>
+      <c r="H36" s="267"/>
+      <c r="I36" s="267"/>
+      <c r="J36" s="267"/>
+      <c r="K36" s="267"/>
+      <c r="L36" s="268"/>
     </row>
     <row r="37" spans="1:12" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="234" t="s">
         <v>340</v>
       </c>
-      <c r="B37" s="242" t="s">
+      <c r="B37" s="273" t="s">
         <v>343</v>
       </c>
-      <c r="C37" s="242"/>
-      <c r="D37" s="242"/>
-      <c r="E37" s="242"/>
-      <c r="F37" s="242"/>
-      <c r="G37" s="242"/>
-      <c r="H37" s="242"/>
-      <c r="I37" s="242"/>
-      <c r="J37" s="242"/>
-      <c r="K37" s="242"/>
-      <c r="L37" s="243"/>
+      <c r="C37" s="273"/>
+      <c r="D37" s="273"/>
+      <c r="E37" s="273"/>
+      <c r="F37" s="273"/>
+      <c r="G37" s="273"/>
+      <c r="H37" s="273"/>
+      <c r="I37" s="273"/>
+      <c r="J37" s="273"/>
+      <c r="K37" s="273"/>
+      <c r="L37" s="274"/>
     </row>
     <row r="38" spans="1:12" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="161"/>
@@ -15511,20 +15511,20 @@
       <c r="L38" s="113"/>
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="244" t="s">
+      <c r="A39" s="275" t="s">
         <v>252</v>
       </c>
-      <c r="B39" s="245"/>
-      <c r="C39" s="245"/>
-      <c r="D39" s="245"/>
-      <c r="E39" s="245"/>
-      <c r="F39" s="245"/>
-      <c r="G39" s="245"/>
-      <c r="H39" s="245"/>
-      <c r="I39" s="245"/>
-      <c r="J39" s="245"/>
-      <c r="K39" s="245"/>
-      <c r="L39" s="246"/>
+      <c r="B39" s="276"/>
+      <c r="C39" s="276"/>
+      <c r="D39" s="276"/>
+      <c r="E39" s="276"/>
+      <c r="F39" s="276"/>
+      <c r="G39" s="276"/>
+      <c r="H39" s="276"/>
+      <c r="I39" s="276"/>
+      <c r="J39" s="276"/>
+      <c r="K39" s="276"/>
+      <c r="L39" s="277"/>
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="162" t="s">
@@ -15612,72 +15612,72 @@
       <c r="B45" s="170" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="247" t="s">
+      <c r="C45" s="255" t="s">
         <v>326</v>
       </c>
-      <c r="D45" s="247"/>
-      <c r="E45" s="247"/>
-      <c r="F45" s="247"/>
-      <c r="G45" s="247"/>
-      <c r="H45" s="247"/>
-      <c r="I45" s="247"/>
-      <c r="J45" s="247"/>
-      <c r="K45" s="247"/>
-      <c r="L45" s="248"/>
+      <c r="D45" s="255"/>
+      <c r="E45" s="255"/>
+      <c r="F45" s="255"/>
+      <c r="G45" s="255"/>
+      <c r="H45" s="255"/>
+      <c r="I45" s="255"/>
+      <c r="J45" s="255"/>
+      <c r="K45" s="255"/>
+      <c r="L45" s="256"/>
     </row>
     <row r="46" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="169"/>
       <c r="B46" s="170" t="s">
         <v>146</v>
       </c>
-      <c r="C46" s="247" t="s">
+      <c r="C46" s="255" t="s">
         <v>147</v>
       </c>
-      <c r="D46" s="247"/>
-      <c r="E46" s="247"/>
-      <c r="F46" s="247"/>
-      <c r="G46" s="247"/>
-      <c r="H46" s="247"/>
-      <c r="I46" s="247"/>
-      <c r="J46" s="247"/>
-      <c r="K46" s="247"/>
-      <c r="L46" s="248"/>
+      <c r="D46" s="255"/>
+      <c r="E46" s="255"/>
+      <c r="F46" s="255"/>
+      <c r="G46" s="255"/>
+      <c r="H46" s="255"/>
+      <c r="I46" s="255"/>
+      <c r="J46" s="255"/>
+      <c r="K46" s="255"/>
+      <c r="L46" s="256"/>
     </row>
     <row r="47" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="169"/>
       <c r="B47" s="170" t="s">
         <v>250</v>
       </c>
-      <c r="C47" s="247" t="s">
+      <c r="C47" s="255" t="s">
         <v>251</v>
       </c>
-      <c r="D47" s="247"/>
-      <c r="E47" s="247"/>
-      <c r="F47" s="247"/>
-      <c r="G47" s="247"/>
-      <c r="H47" s="247"/>
-      <c r="I47" s="247"/>
-      <c r="J47" s="247"/>
-      <c r="K47" s="247"/>
-      <c r="L47" s="248"/>
+      <c r="D47" s="255"/>
+      <c r="E47" s="255"/>
+      <c r="F47" s="255"/>
+      <c r="G47" s="255"/>
+      <c r="H47" s="255"/>
+      <c r="I47" s="255"/>
+      <c r="J47" s="255"/>
+      <c r="K47" s="255"/>
+      <c r="L47" s="256"/>
     </row>
     <row r="48" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="169"/>
       <c r="B48" s="170" t="s">
         <v>327</v>
       </c>
-      <c r="C48" s="247" t="s">
+      <c r="C48" s="255" t="s">
         <v>328</v>
       </c>
-      <c r="D48" s="247"/>
-      <c r="E48" s="247"/>
-      <c r="F48" s="247"/>
-      <c r="G48" s="247"/>
-      <c r="H48" s="247"/>
-      <c r="I48" s="247"/>
-      <c r="J48" s="247"/>
-      <c r="K48" s="247"/>
-      <c r="L48" s="248"/>
+      <c r="D48" s="255"/>
+      <c r="E48" s="255"/>
+      <c r="F48" s="255"/>
+      <c r="G48" s="255"/>
+      <c r="H48" s="255"/>
+      <c r="I48" s="255"/>
+      <c r="J48" s="255"/>
+      <c r="K48" s="255"/>
+      <c r="L48" s="256"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="169"/>
@@ -15702,18 +15702,18 @@
       <c r="B50" s="170" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="247" t="s">
+      <c r="C50" s="255" t="s">
         <v>330</v>
       </c>
-      <c r="D50" s="247"/>
-      <c r="E50" s="247"/>
-      <c r="F50" s="247"/>
-      <c r="G50" s="247"/>
-      <c r="H50" s="247"/>
-      <c r="I50" s="247"/>
-      <c r="J50" s="247"/>
-      <c r="K50" s="247"/>
-      <c r="L50" s="248"/>
+      <c r="D50" s="255"/>
+      <c r="E50" s="255"/>
+      <c r="F50" s="255"/>
+      <c r="G50" s="255"/>
+      <c r="H50" s="255"/>
+      <c r="I50" s="255"/>
+      <c r="J50" s="255"/>
+      <c r="K50" s="255"/>
+      <c r="L50" s="256"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="169"/>
@@ -15795,25 +15795,51 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="237" t="s">
+      <c r="A64" s="272" t="s">
         <v>332</v>
       </c>
-      <c r="B64" s="237"/>
-      <c r="C64" s="237"/>
-      <c r="D64" s="237"/>
-      <c r="E64" s="237"/>
-      <c r="F64" s="237"/>
-      <c r="G64" s="237"/>
-      <c r="H64" s="237"/>
-      <c r="I64" s="237"/>
-      <c r="J64" s="237"/>
-      <c r="K64" s="237"/>
-      <c r="L64" s="237"/>
+      <c r="B64" s="272"/>
+      <c r="C64" s="272"/>
+      <c r="D64" s="272"/>
+      <c r="E64" s="272"/>
+      <c r="F64" s="272"/>
+      <c r="G64" s="272"/>
+      <c r="H64" s="272"/>
+      <c r="I64" s="272"/>
+      <c r="J64" s="272"/>
+      <c r="K64" s="272"/>
+      <c r="L64" s="272"/>
     </row>
     <row r="69" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="70" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A64:L64"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="C45:L45"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="C48:L48"/>
+    <mergeCell ref="C50:L50"/>
+    <mergeCell ref="A35:L35"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B18:L18"/>
+    <mergeCell ref="B19:L19"/>
+    <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="B22:L22"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="B26:L26"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B30:L30"/>
     <mergeCell ref="A17:L17"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A4:L4"/>
@@ -15828,32 +15854,6 @@
     <mergeCell ref="A16:L16"/>
     <mergeCell ref="B7:L7"/>
     <mergeCell ref="B8:L8"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B18:L18"/>
-    <mergeCell ref="B19:L19"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="B22:L22"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="B24:L24"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="B26:L26"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="A64:L64"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="C45:L45"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="C47:L47"/>
-    <mergeCell ref="C48:L48"/>
-    <mergeCell ref="C50:L50"/>
-    <mergeCell ref="A35:L35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A57" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -15887,82 +15887,82 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="314" t="s">
+      <c r="A3" s="315" t="s">
         <v>164</v>
       </c>
-      <c r="B3" s="314"/>
-      <c r="C3" s="314"/>
+      <c r="B3" s="315"/>
+      <c r="C3" s="315"/>
       <c r="D3" s="128" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="315" t="s">
+      <c r="A4" s="316" t="s">
         <v>160</v>
       </c>
-      <c r="B4" s="315"/>
-      <c r="C4" s="315"/>
+      <c r="B4" s="316"/>
+      <c r="C4" s="316"/>
       <c r="D4" s="177" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="319" t="s">
+      <c r="A5" s="320" t="s">
         <v>235</v>
       </c>
-      <c r="B5" s="316"/>
-      <c r="C5" s="316"/>
+      <c r="B5" s="317"/>
+      <c r="C5" s="317"/>
       <c r="D5" s="178" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="317" t="s">
+      <c r="A6" s="318" t="s">
         <v>236</v>
       </c>
-      <c r="B6" s="317"/>
-      <c r="C6" s="317"/>
+      <c r="B6" s="318"/>
+      <c r="C6" s="318"/>
       <c r="D6" s="179" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="318" t="s">
+      <c r="A7" s="319" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="318"/>
-      <c r="C7" s="318"/>
+      <c r="B7" s="319"/>
+      <c r="C7" s="319"/>
       <c r="D7" s="180" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="315" t="s">
+      <c r="A11" s="316" t="s">
         <v>160</v>
       </c>
-      <c r="B11" s="315"/>
-      <c r="C11" s="315"/>
+      <c r="B11" s="316"/>
+      <c r="C11" s="316"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="316" t="s">
+      <c r="A12" s="317" t="s">
         <v>161</v>
       </c>
-      <c r="B12" s="316"/>
-      <c r="C12" s="316"/>
+      <c r="B12" s="317"/>
+      <c r="C12" s="317"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="317" t="s">
+      <c r="A13" s="318" t="s">
         <v>162</v>
       </c>
-      <c r="B13" s="317"/>
-      <c r="C13" s="317"/>
+      <c r="B13" s="318"/>
+      <c r="C13" s="318"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="318" t="s">
+      <c r="A14" s="319" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="318"/>
-      <c r="C14" s="318"/>
+      <c r="B14" s="319"/>
+      <c r="C14" s="319"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -16511,8 +16511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BF7D8F-86F3-47E9-AB85-EE9B4CAB70E4}">
   <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N20" sqref="N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16541,16 +16541,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="277" t="str">
+      <c r="A1" s="278" t="str">
         <f>'ReadMe-Directions'!A1</f>
         <v>Lake Mead Water Bank based on the Principle of Divide Reservoir Inflow</v>
       </c>
-      <c r="B1" s="277"/>
-      <c r="C1" s="277"/>
-      <c r="D1" s="277"/>
-      <c r="E1" s="277"/>
-      <c r="F1" s="277"/>
-      <c r="G1" s="277"/>
+      <c r="B1" s="278"/>
+      <c r="C1" s="278"/>
+      <c r="D1" s="278"/>
+      <c r="E1" s="278"/>
+      <c r="F1" s="278"/>
+      <c r="G1" s="278"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -16559,15 +16559,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="285" t="s">
+      <c r="A3" s="286" t="s">
         <v>242</v>
       </c>
-      <c r="B3" s="285"/>
-      <c r="C3" s="285"/>
-      <c r="D3" s="285"/>
-      <c r="E3" s="285"/>
-      <c r="F3" s="285"/>
-      <c r="G3" s="285"/>
+      <c r="B3" s="286"/>
+      <c r="C3" s="286"/>
+      <c r="D3" s="286"/>
+      <c r="E3" s="286"/>
+      <c r="F3" s="286"/>
+      <c r="G3" s="286"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -16583,13 +16583,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="286" t="s">
+      <c r="C4" s="287" t="s">
         <v>323</v>
       </c>
-      <c r="D4" s="287"/>
-      <c r="E4" s="287"/>
-      <c r="F4" s="287"/>
-      <c r="G4" s="288"/>
+      <c r="D4" s="288"/>
+      <c r="E4" s="288"/>
+      <c r="F4" s="288"/>
+      <c r="G4" s="289"/>
       <c r="N4" s="141" t="s">
         <v>176</v>
       </c>
@@ -16599,11 +16599,11 @@
         <v>295</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="289"/>
-      <c r="D5" s="284"/>
-      <c r="E5" s="284"/>
-      <c r="F5" s="284"/>
-      <c r="G5" s="284"/>
+      <c r="C5" s="290"/>
+      <c r="D5" s="285"/>
+      <c r="E5" s="285"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="285"/>
       <c r="N5" s="141"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -16611,11 +16611,11 @@
         <v>254</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="289"/>
-      <c r="D6" s="284"/>
-      <c r="E6" s="284"/>
-      <c r="F6" s="284"/>
-      <c r="G6" s="284"/>
+      <c r="C6" s="290"/>
+      <c r="D6" s="285"/>
+      <c r="E6" s="285"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="285"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -16623,11 +16623,11 @@
         <v>255</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="289"/>
-      <c r="D7" s="284"/>
-      <c r="E7" s="284"/>
-      <c r="F7" s="284"/>
-      <c r="G7" s="284"/>
+      <c r="C7" s="290"/>
+      <c r="D7" s="285"/>
+      <c r="E7" s="285"/>
+      <c r="F7" s="285"/>
+      <c r="G7" s="285"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -16635,11 +16635,11 @@
         <v>256</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="284"/>
-      <c r="D8" s="284"/>
-      <c r="E8" s="284"/>
-      <c r="F8" s="284"/>
-      <c r="G8" s="284"/>
+      <c r="C8" s="285"/>
+      <c r="D8" s="285"/>
+      <c r="E8" s="285"/>
+      <c r="F8" s="285"/>
+      <c r="G8" s="285"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -16647,11 +16647,11 @@
         <v>18</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="290"/>
-      <c r="D9" s="290"/>
-      <c r="E9" s="290"/>
-      <c r="F9" s="290"/>
-      <c r="G9" s="290"/>
+      <c r="C9" s="291"/>
+      <c r="D9" s="291"/>
+      <c r="E9" s="291"/>
+      <c r="F9" s="291"/>
+      <c r="G9" s="291"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -16659,11 +16659,11 @@
         <v>346</v>
       </c>
       <c r="B10" s="90"/>
-      <c r="C10" s="284"/>
-      <c r="D10" s="284"/>
-      <c r="E10" s="284"/>
-      <c r="F10" s="284"/>
-      <c r="G10" s="284"/>
+      <c r="C10" s="285"/>
+      <c r="D10" s="285"/>
+      <c r="E10" s="285"/>
+      <c r="F10" s="285"/>
+      <c r="G10" s="285"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -16676,28 +16676,28 @@
       <c r="A12" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="291" t="s">
+      <c r="B12" s="292" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="292"/>
-      <c r="D12" s="293"/>
+      <c r="C12" s="293"/>
+      <c r="D12" s="294"/>
       <c r="N12" s="141" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="294" t="s">
+      <c r="B13" s="295" t="s">
         <v>241</v>
       </c>
-      <c r="C13" s="295"/>
-      <c r="D13" s="296"/>
+      <c r="C13" s="296"/>
+      <c r="D13" s="297"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="278" t="s">
+      <c r="B14" s="279" t="s">
         <v>236</v>
       </c>
-      <c r="C14" s="279"/>
-      <c r="D14" s="280"/>
+      <c r="C14" s="280"/>
+      <c r="D14" s="281"/>
       <c r="F14">
         <f>0.95/2</f>
         <v>0.47499999999999998</v>
@@ -16705,11 +16705,11 @@
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="281" t="s">
+      <c r="B15" s="282" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="282"/>
-      <c r="D15" s="283"/>
+      <c r="C15" s="283"/>
+      <c r="D15" s="284"/>
       <c r="N15" s="142"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -21228,7 +21228,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="N4" r:id="rId1" xr:uid="{DF55C70C-AEA5-4BB4-9BD1-23B882C83781}"/>
+    <hyperlink ref="N4" r:id="rId1" location="step-1-assign-accounts-articulate-vulnerabilities-and-strategies-to-manage-vulnerability" xr:uid="{DF55C70C-AEA5-4BB4-9BD1-23B882C83781}"/>
     <hyperlink ref="N17" r:id="rId2" location="1b-make-assumptions" xr:uid="{91CC7212-C579-4B1B-A8B8-969D4549837D}"/>
     <hyperlink ref="N18" r:id="rId3" location="i-evaporation-rates" xr:uid="{23C61350-606E-472B-90E1-88574D6741EE}"/>
     <hyperlink ref="N19" r:id="rId4" location="ii-start-storage" xr:uid="{692C3AE6-515B-4C08-B6EC-0557E75E9511}"/>
@@ -21534,29 +21534,29 @@
     </row>
     <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="I5" s="309" t="s">
+      <c r="I5" s="310" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="309" t="s">
+      <c r="J5" s="310" t="s">
         <v>265</v>
       </c>
-      <c r="K5" s="309" t="s">
+      <c r="K5" s="310" t="s">
         <v>266</v>
       </c>
-      <c r="L5" s="306" t="s">
+      <c r="L5" s="307" t="s">
         <v>267</v>
       </c>
-      <c r="M5" s="307"/>
-      <c r="N5" s="307"/>
-      <c r="O5" s="307"/>
-      <c r="P5" s="308"/>
-      <c r="Q5" s="298" t="s">
+      <c r="M5" s="308"/>
+      <c r="N5" s="308"/>
+      <c r="O5" s="308"/>
+      <c r="P5" s="309"/>
+      <c r="Q5" s="299" t="s">
         <v>268</v>
       </c>
-      <c r="R5" s="299"/>
-      <c r="S5" s="299"/>
-      <c r="T5" s="299"/>
-      <c r="U5" s="300"/>
+      <c r="R5" s="300"/>
+      <c r="S5" s="300"/>
+      <c r="T5" s="300"/>
+      <c r="U5" s="301"/>
     </row>
     <row r="6" spans="1:21" s="191" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="192" t="s">
@@ -21577,9 +21577,9 @@
       <c r="G6" s="192" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="310"/>
-      <c r="J6" s="310"/>
-      <c r="K6" s="310"/>
+      <c r="I6" s="311"/>
+      <c r="J6" s="311"/>
+      <c r="K6" s="311"/>
       <c r="L6" s="193" t="s">
         <v>270</v>
       </c>
@@ -21612,14 +21612,14 @@
       </c>
     </row>
     <row r="7" spans="1:21" s="191" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="306" t="s">
+      <c r="B7" s="307" t="s">
         <v>280</v>
       </c>
-      <c r="C7" s="307"/>
-      <c r="D7" s="307"/>
-      <c r="E7" s="307"/>
-      <c r="F7" s="307"/>
-      <c r="G7" s="308"/>
+      <c r="C7" s="308"/>
+      <c r="D7" s="308"/>
+      <c r="E7" s="308"/>
+      <c r="F7" s="308"/>
+      <c r="G7" s="309"/>
       <c r="I7" s="195" t="s">
         <v>281</v>
       </c>
@@ -21887,13 +21887,13 @@
       <c r="B11" s="201" t="s">
         <v>287</v>
       </c>
-      <c r="C11" s="297" t="s">
+      <c r="C11" s="298" t="s">
         <v>288</v>
       </c>
-      <c r="D11" s="297"/>
-      <c r="E11" s="297"/>
-      <c r="F11" s="297"/>
-      <c r="G11" s="297"/>
+      <c r="D11" s="298"/>
+      <c r="E11" s="298"/>
+      <c r="F11" s="298"/>
+      <c r="G11" s="298"/>
       <c r="I11" s="195" t="s">
         <v>289</v>
       </c>
@@ -21947,14 +21947,14 @@
       </c>
     </row>
     <row r="12" spans="1:21" s="200" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B12" s="301" t="s">
+      <c r="B12" s="302" t="s">
         <v>290</v>
       </c>
-      <c r="C12" s="302"/>
-      <c r="D12" s="302"/>
-      <c r="E12" s="302"/>
-      <c r="F12" s="302"/>
-      <c r="G12" s="302"/>
+      <c r="C12" s="303"/>
+      <c r="D12" s="303"/>
+      <c r="E12" s="303"/>
+      <c r="F12" s="303"/>
+      <c r="G12" s="303"/>
       <c r="I12" s="195" t="s">
         <v>291</v>
       </c>
@@ -21964,20 +21964,20 @@
       <c r="K12" s="203" t="s">
         <v>292</v>
       </c>
-      <c r="L12" s="303" t="s">
+      <c r="L12" s="304" t="s">
         <v>288</v>
       </c>
-      <c r="M12" s="304"/>
-      <c r="N12" s="304"/>
-      <c r="O12" s="304"/>
-      <c r="P12" s="305"/>
-      <c r="Q12" s="303" t="s">
+      <c r="M12" s="305"/>
+      <c r="N12" s="305"/>
+      <c r="O12" s="305"/>
+      <c r="P12" s="306"/>
+      <c r="Q12" s="304" t="s">
         <v>288</v>
       </c>
-      <c r="R12" s="304"/>
-      <c r="S12" s="304"/>
-      <c r="T12" s="304"/>
-      <c r="U12" s="305"/>
+      <c r="R12" s="305"/>
+      <c r="S12" s="305"/>
+      <c r="T12" s="305"/>
+      <c r="U12" s="306"/>
     </row>
     <row r="13" spans="1:21" s="200" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B13" s="201">
@@ -22228,13 +22228,13 @@
       <c r="B18" s="201" t="s">
         <v>287</v>
       </c>
-      <c r="C18" s="297" t="s">
+      <c r="C18" s="298" t="s">
         <v>288</v>
       </c>
-      <c r="D18" s="297"/>
-      <c r="E18" s="297"/>
-      <c r="F18" s="297"/>
-      <c r="G18" s="297"/>
+      <c r="D18" s="298"/>
+      <c r="E18" s="298"/>
+      <c r="F18" s="298"/>
+      <c r="G18" s="298"/>
     </row>
     <row r="19" spans="2:21" s="200" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="I19" s="200" t="s">
@@ -22704,15 +22704,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="285" t="s">
+      <c r="A3" s="286" t="s">
         <v>229</v>
       </c>
-      <c r="B3" s="285"/>
-      <c r="C3" s="285"/>
-      <c r="D3" s="285"/>
-      <c r="E3" s="285"/>
-      <c r="F3" s="285"/>
-      <c r="G3" s="285"/>
+      <c r="B3" s="286"/>
+      <c r="C3" s="286"/>
+      <c r="D3" s="286"/>
+      <c r="E3" s="286"/>
+      <c r="F3" s="286"/>
+      <c r="G3" s="286"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -22728,13 +22728,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="286" t="s">
+      <c r="C4" s="287" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="287"/>
-      <c r="E4" s="287"/>
-      <c r="F4" s="287"/>
-      <c r="G4" s="288"/>
+      <c r="D4" s="288"/>
+      <c r="E4" s="288"/>
+      <c r="F4" s="288"/>
+      <c r="G4" s="289"/>
       <c r="N4" s="139" t="s">
         <v>176</v>
       </c>
@@ -22744,11 +22744,11 @@
         <v>16</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="289"/>
-      <c r="D5" s="284"/>
-      <c r="E5" s="284"/>
-      <c r="F5" s="284"/>
-      <c r="G5" s="284"/>
+      <c r="C5" s="290"/>
+      <c r="D5" s="285"/>
+      <c r="E5" s="285"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="285"/>
       <c r="N5" s="142"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -22756,11 +22756,11 @@
         <v>17</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="289"/>
-      <c r="D6" s="284"/>
-      <c r="E6" s="284"/>
-      <c r="F6" s="284"/>
-      <c r="G6" s="284"/>
+      <c r="C6" s="290"/>
+      <c r="D6" s="285"/>
+      <c r="E6" s="285"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="285"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -22768,11 +22768,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="289"/>
-      <c r="D7" s="284"/>
-      <c r="E7" s="284"/>
-      <c r="F7" s="284"/>
-      <c r="G7" s="284"/>
+      <c r="C7" s="290"/>
+      <c r="D7" s="285"/>
+      <c r="E7" s="285"/>
+      <c r="F7" s="285"/>
+      <c r="G7" s="285"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -22780,11 +22780,11 @@
         <v>78</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="284"/>
-      <c r="D8" s="284"/>
-      <c r="E8" s="284"/>
-      <c r="F8" s="284"/>
-      <c r="G8" s="284"/>
+      <c r="C8" s="285"/>
+      <c r="D8" s="285"/>
+      <c r="E8" s="285"/>
+      <c r="F8" s="285"/>
+      <c r="G8" s="285"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -22792,11 +22792,11 @@
         <v>214</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="290"/>
-      <c r="D9" s="290"/>
-      <c r="E9" s="290"/>
-      <c r="F9" s="290"/>
-      <c r="G9" s="290"/>
+      <c r="C9" s="291"/>
+      <c r="D9" s="291"/>
+      <c r="E9" s="291"/>
+      <c r="F9" s="291"/>
+      <c r="G9" s="291"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -22804,11 +22804,11 @@
         <v>81</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="311"/>
-      <c r="D10" s="311"/>
-      <c r="E10" s="311"/>
-      <c r="F10" s="311"/>
-      <c r="G10" s="311"/>
+      <c r="C10" s="313"/>
+      <c r="D10" s="313"/>
+      <c r="E10" s="313"/>
+      <c r="F10" s="313"/>
+      <c r="G10" s="313"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -22821,37 +22821,37 @@
       <c r="A12" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="B12" s="291" t="s">
+      <c r="B12" s="292" t="s">
         <v>160</v>
       </c>
-      <c r="C12" s="292"/>
-      <c r="D12" s="293"/>
+      <c r="C12" s="293"/>
+      <c r="D12" s="294"/>
       <c r="N12" s="141" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="294" t="s">
+      <c r="B13" s="295" t="s">
         <v>161</v>
       </c>
-      <c r="C13" s="295"/>
-      <c r="D13" s="296"/>
+      <c r="C13" s="296"/>
+      <c r="D13" s="297"/>
       <c r="N13" s="142"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="278" t="s">
+      <c r="B14" s="279" t="s">
         <v>162</v>
       </c>
-      <c r="C14" s="279"/>
-      <c r="D14" s="280"/>
+      <c r="C14" s="280"/>
+      <c r="D14" s="281"/>
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="281" t="s">
+      <c r="B15" s="282" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="282"/>
-      <c r="D15" s="283"/>
+      <c r="C15" s="283"/>
+      <c r="D15" s="284"/>
       <c r="N15" s="142"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -24071,12 +24071,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -24084,6 +24078,12 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>
@@ -24141,26 +24141,26 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="313" t="s">
+      <c r="D3" s="314" t="s">
         <v>101</v>
       </c>
-      <c r="E3" s="313"/>
-      <c r="F3" s="313" t="s">
+      <c r="E3" s="314"/>
+      <c r="F3" s="314" t="s">
         <v>102</v>
       </c>
-      <c r="G3" s="313"/>
-      <c r="H3" s="313"/>
-      <c r="I3" s="313" t="s">
+      <c r="G3" s="314"/>
+      <c r="H3" s="314"/>
+      <c r="I3" s="314" t="s">
         <v>103</v>
       </c>
-      <c r="J3" s="313"/>
-      <c r="K3" s="313"/>
+      <c r="J3" s="314"/>
+      <c r="K3" s="314"/>
       <c r="L3" s="134"/>
-      <c r="M3" s="313" t="s">
+      <c r="M3" s="314" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="313"/>
-      <c r="O3" s="313"/>
+      <c r="N3" s="314"/>
+      <c r="O3" s="314"/>
     </row>
     <row r="4" spans="1:16" s="47" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="46" t="s">

</xml_diff>

<commit_message>
Finish input assumptions in model guide
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB80E85A-B129-48F6-92C1-510E2FB320E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C7EB55-DC86-4E02-8B6A-A245AC8AE669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="361">
   <si>
     <t>Year 1</t>
   </si>
@@ -1906,6 +1906,9 @@
       <t>, enter the total Water Conservation Account (Intentionally Created Surplus) Balance. This value includes California, Arizona, Nevada, and Mexico.</t>
     </r>
   </si>
+  <si>
+    <t>Help Water Conservation Program Total Balance</t>
+  </si>
 </sst>
 </file>
 
@@ -3182,6 +3185,51 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3236,12 +3284,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3265,45 +3307,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3407,11 +3410,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14851,20 +14854,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="240" t="s">
+      <c r="A1" s="255" t="s">
         <v>321</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
+      <c r="B1" s="255"/>
+      <c r="C1" s="255"/>
+      <c r="D1" s="255"/>
+      <c r="E1" s="255"/>
+      <c r="F1" s="255"/>
+      <c r="G1" s="255"/>
+      <c r="H1" s="255"/>
+      <c r="I1" s="255"/>
+      <c r="J1" s="255"/>
+      <c r="K1" s="255"/>
+      <c r="L1" s="255"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -14890,41 +14893,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="241" t="s">
+      <c r="A4" s="256" t="s">
         <v>349</v>
       </c>
-      <c r="B4" s="242"/>
-      <c r="C4" s="242"/>
-      <c r="D4" s="242"/>
-      <c r="E4" s="242"/>
-      <c r="F4" s="242"/>
-      <c r="G4" s="242"/>
-      <c r="H4" s="242"/>
-      <c r="I4" s="242"/>
-      <c r="J4" s="242"/>
-      <c r="K4" s="242"/>
-      <c r="L4" s="243"/>
-      <c r="N4" s="244"/>
-      <c r="O4" s="244"/>
-      <c r="P4" s="244"/>
-      <c r="Q4" s="244"/>
-      <c r="R4" s="244"/>
+      <c r="B4" s="257"/>
+      <c r="C4" s="257"/>
+      <c r="D4" s="257"/>
+      <c r="E4" s="257"/>
+      <c r="F4" s="257"/>
+      <c r="G4" s="257"/>
+      <c r="H4" s="257"/>
+      <c r="I4" s="257"/>
+      <c r="J4" s="257"/>
+      <c r="K4" s="257"/>
+      <c r="L4" s="258"/>
+      <c r="N4" s="259"/>
+      <c r="O4" s="259"/>
+      <c r="P4" s="259"/>
+      <c r="Q4" s="259"/>
+      <c r="R4" s="259"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="245" t="s">
+      <c r="A5" s="260" t="s">
         <v>350</v>
       </c>
-      <c r="B5" s="246"/>
-      <c r="C5" s="246"/>
-      <c r="D5" s="246"/>
-      <c r="E5" s="246"/>
-      <c r="F5" s="246"/>
-      <c r="G5" s="246"/>
-      <c r="H5" s="246"/>
-      <c r="I5" s="246"/>
-      <c r="J5" s="246"/>
-      <c r="K5" s="246"/>
-      <c r="L5" s="247"/>
+      <c r="B5" s="261"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
+      <c r="G5" s="261"/>
+      <c r="H5" s="261"/>
+      <c r="I5" s="261"/>
+      <c r="J5" s="261"/>
+      <c r="K5" s="261"/>
+      <c r="L5" s="262"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -14932,20 +14935,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="245" t="s">
+      <c r="A6" s="260" t="s">
         <v>352</v>
       </c>
-      <c r="B6" s="246"/>
-      <c r="C6" s="246"/>
-      <c r="D6" s="246"/>
-      <c r="E6" s="246"/>
-      <c r="F6" s="246"/>
-      <c r="G6" s="246"/>
-      <c r="H6" s="246"/>
-      <c r="I6" s="246"/>
-      <c r="J6" s="246"/>
-      <c r="K6" s="246"/>
-      <c r="L6" s="247"/>
+      <c r="B6" s="261"/>
+      <c r="C6" s="261"/>
+      <c r="D6" s="261"/>
+      <c r="E6" s="261"/>
+      <c r="F6" s="261"/>
+      <c r="G6" s="261"/>
+      <c r="H6" s="261"/>
+      <c r="I6" s="261"/>
+      <c r="J6" s="261"/>
+      <c r="K6" s="261"/>
+      <c r="L6" s="262"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -14954,19 +14957,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="235"/>
-      <c r="B7" s="246" t="s">
+      <c r="B7" s="261" t="s">
         <v>353</v>
       </c>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246"/>
-      <c r="K7" s="246"/>
-      <c r="L7" s="247"/>
+      <c r="C7" s="261"/>
+      <c r="D7" s="261"/>
+      <c r="E7" s="261"/>
+      <c r="F7" s="261"/>
+      <c r="G7" s="261"/>
+      <c r="H7" s="261"/>
+      <c r="I7" s="261"/>
+      <c r="J7" s="261"/>
+      <c r="K7" s="261"/>
+      <c r="L7" s="262"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -14975,19 +14978,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="236"/>
-      <c r="B8" s="263" t="s">
+      <c r="B8" s="276" t="s">
         <v>354</v>
       </c>
-      <c r="C8" s="263"/>
-      <c r="D8" s="263"/>
-      <c r="E8" s="263"/>
-      <c r="F8" s="263"/>
-      <c r="G8" s="263"/>
-      <c r="H8" s="263"/>
-      <c r="I8" s="263"/>
-      <c r="J8" s="263"/>
-      <c r="K8" s="263"/>
-      <c r="L8" s="264"/>
+      <c r="C8" s="276"/>
+      <c r="D8" s="276"/>
+      <c r="E8" s="276"/>
+      <c r="F8" s="276"/>
+      <c r="G8" s="276"/>
+      <c r="H8" s="276"/>
+      <c r="I8" s="276"/>
+      <c r="J8" s="276"/>
+      <c r="K8" s="276"/>
+      <c r="L8" s="277"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15009,84 +15012,84 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="248" t="s">
+      <c r="A10" s="263" t="s">
         <v>217</v>
       </c>
-      <c r="B10" s="249"/>
-      <c r="C10" s="249"/>
-      <c r="D10" s="249"/>
-      <c r="E10" s="249"/>
-      <c r="F10" s="249"/>
-      <c r="G10" s="249"/>
-      <c r="H10" s="249"/>
-      <c r="I10" s="249"/>
-      <c r="J10" s="249"/>
-      <c r="K10" s="249"/>
-      <c r="L10" s="250"/>
+      <c r="B10" s="264"/>
+      <c r="C10" s="264"/>
+      <c r="D10" s="264"/>
+      <c r="E10" s="264"/>
+      <c r="F10" s="264"/>
+      <c r="G10" s="264"/>
+      <c r="H10" s="264"/>
+      <c r="I10" s="264"/>
+      <c r="J10" s="264"/>
+      <c r="K10" s="264"/>
+      <c r="L10" s="265"/>
     </row>
     <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="251" t="s">
+      <c r="A11" s="266" t="s">
         <v>351</v>
       </c>
-      <c r="B11" s="252"/>
-      <c r="C11" s="252"/>
-      <c r="D11" s="252"/>
-      <c r="E11" s="252"/>
-      <c r="F11" s="252"/>
-      <c r="G11" s="252"/>
-      <c r="H11" s="252"/>
-      <c r="I11" s="252"/>
-      <c r="J11" s="252"/>
-      <c r="K11" s="252"/>
-      <c r="L11" s="253"/>
+      <c r="B11" s="267"/>
+      <c r="C11" s="267"/>
+      <c r="D11" s="267"/>
+      <c r="E11" s="267"/>
+      <c r="F11" s="267"/>
+      <c r="G11" s="267"/>
+      <c r="H11" s="267"/>
+      <c r="I11" s="267"/>
+      <c r="J11" s="267"/>
+      <c r="K11" s="267"/>
+      <c r="L11" s="268"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="254" t="s">
+      <c r="A12" s="269" t="s">
         <v>355</v>
       </c>
-      <c r="B12" s="255"/>
-      <c r="C12" s="255"/>
-      <c r="D12" s="255"/>
-      <c r="E12" s="255"/>
-      <c r="F12" s="255"/>
-      <c r="G12" s="255"/>
-      <c r="H12" s="255"/>
-      <c r="I12" s="255"/>
-      <c r="J12" s="255"/>
-      <c r="K12" s="255"/>
-      <c r="L12" s="256"/>
+      <c r="B12" s="247"/>
+      <c r="C12" s="247"/>
+      <c r="D12" s="247"/>
+      <c r="E12" s="247"/>
+      <c r="F12" s="247"/>
+      <c r="G12" s="247"/>
+      <c r="H12" s="247"/>
+      <c r="I12" s="247"/>
+      <c r="J12" s="247"/>
+      <c r="K12" s="247"/>
+      <c r="L12" s="248"/>
     </row>
     <row r="13" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="254" t="s">
+      <c r="A13" s="269" t="s">
         <v>218</v>
       </c>
-      <c r="B13" s="255"/>
-      <c r="C13" s="255"/>
-      <c r="D13" s="255"/>
-      <c r="E13" s="255"/>
-      <c r="F13" s="255"/>
-      <c r="G13" s="255"/>
-      <c r="H13" s="255"/>
-      <c r="I13" s="255"/>
-      <c r="J13" s="255"/>
-      <c r="K13" s="255"/>
-      <c r="L13" s="256"/>
+      <c r="B13" s="247"/>
+      <c r="C13" s="247"/>
+      <c r="D13" s="247"/>
+      <c r="E13" s="247"/>
+      <c r="F13" s="247"/>
+      <c r="G13" s="247"/>
+      <c r="H13" s="247"/>
+      <c r="I13" s="247"/>
+      <c r="J13" s="247"/>
+      <c r="K13" s="247"/>
+      <c r="L13" s="248"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="257" t="s">
+      <c r="A14" s="270" t="s">
         <v>356</v>
       </c>
-      <c r="B14" s="258"/>
-      <c r="C14" s="258"/>
-      <c r="D14" s="258"/>
-      <c r="E14" s="258"/>
-      <c r="F14" s="258"/>
-      <c r="G14" s="258"/>
-      <c r="H14" s="258"/>
-      <c r="I14" s="258"/>
-      <c r="J14" s="258"/>
-      <c r="K14" s="258"/>
-      <c r="L14" s="259"/>
+      <c r="B14" s="271"/>
+      <c r="C14" s="271"/>
+      <c r="D14" s="271"/>
+      <c r="E14" s="271"/>
+      <c r="F14" s="271"/>
+      <c r="G14" s="271"/>
+      <c r="H14" s="271"/>
+      <c r="I14" s="271"/>
+      <c r="J14" s="271"/>
+      <c r="K14" s="271"/>
+      <c r="L14" s="272"/>
     </row>
     <row r="15" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="113"/>
@@ -15103,332 +15106,332 @@
       <c r="L15" s="113"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="260" t="s">
+      <c r="A16" s="273" t="s">
         <v>348</v>
       </c>
-      <c r="B16" s="261"/>
-      <c r="C16" s="261"/>
-      <c r="D16" s="261"/>
-      <c r="E16" s="261"/>
-      <c r="F16" s="261"/>
-      <c r="G16" s="261"/>
-      <c r="H16" s="261"/>
-      <c r="I16" s="261"/>
-      <c r="J16" s="261"/>
-      <c r="K16" s="261"/>
-      <c r="L16" s="262"/>
+      <c r="B16" s="274"/>
+      <c r="C16" s="274"/>
+      <c r="D16" s="274"/>
+      <c r="E16" s="274"/>
+      <c r="F16" s="274"/>
+      <c r="G16" s="274"/>
+      <c r="H16" s="274"/>
+      <c r="I16" s="274"/>
+      <c r="J16" s="274"/>
+      <c r="K16" s="274"/>
+      <c r="L16" s="275"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="237" t="s">
+      <c r="A17" s="252" t="s">
         <v>227</v>
       </c>
-      <c r="B17" s="238"/>
-      <c r="C17" s="238"/>
-      <c r="D17" s="238"/>
-      <c r="E17" s="238"/>
-      <c r="F17" s="238"/>
-      <c r="G17" s="238"/>
-      <c r="H17" s="238"/>
-      <c r="I17" s="238"/>
-      <c r="J17" s="238"/>
-      <c r="K17" s="238"/>
-      <c r="L17" s="239"/>
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="253"/>
+      <c r="J17" s="253"/>
+      <c r="K17" s="253"/>
+      <c r="L17" s="254"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="230">
         <v>1</v>
       </c>
-      <c r="B18" s="267" t="s">
+      <c r="B18" s="240" t="s">
         <v>226</v>
       </c>
-      <c r="C18" s="267"/>
-      <c r="D18" s="267"/>
-      <c r="E18" s="267"/>
-      <c r="F18" s="267"/>
-      <c r="G18" s="267"/>
-      <c r="H18" s="267"/>
-      <c r="I18" s="267"/>
-      <c r="J18" s="267"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="268"/>
+      <c r="C18" s="240"/>
+      <c r="D18" s="240"/>
+      <c r="E18" s="240"/>
+      <c r="F18" s="240"/>
+      <c r="G18" s="240"/>
+      <c r="H18" s="240"/>
+      <c r="I18" s="240"/>
+      <c r="J18" s="240"/>
+      <c r="K18" s="240"/>
+      <c r="L18" s="241"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="230">
         <v>2</v>
       </c>
-      <c r="B19" s="267" t="s">
+      <c r="B19" s="240" t="s">
         <v>344</v>
       </c>
-      <c r="C19" s="267"/>
-      <c r="D19" s="267"/>
-      <c r="E19" s="267"/>
-      <c r="F19" s="267"/>
-      <c r="G19" s="267"/>
-      <c r="H19" s="267"/>
-      <c r="I19" s="267"/>
-      <c r="J19" s="267"/>
-      <c r="K19" s="267"/>
-      <c r="L19" s="268"/>
+      <c r="C19" s="240"/>
+      <c r="D19" s="240"/>
+      <c r="E19" s="240"/>
+      <c r="F19" s="240"/>
+      <c r="G19" s="240"/>
+      <c r="H19" s="240"/>
+      <c r="I19" s="240"/>
+      <c r="J19" s="240"/>
+      <c r="K19" s="240"/>
+      <c r="L19" s="241"/>
       <c r="N19" s="106"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="230">
         <v>3</v>
       </c>
-      <c r="B20" s="267" t="s">
+      <c r="B20" s="240" t="s">
         <v>219</v>
       </c>
-      <c r="C20" s="267"/>
-      <c r="D20" s="267"/>
-      <c r="E20" s="267"/>
-      <c r="F20" s="267"/>
-      <c r="G20" s="267"/>
-      <c r="H20" s="267"/>
-      <c r="I20" s="267"/>
-      <c r="J20" s="267"/>
-      <c r="K20" s="267"/>
-      <c r="L20" s="268"/>
+      <c r="C20" s="240"/>
+      <c r="D20" s="240"/>
+      <c r="E20" s="240"/>
+      <c r="F20" s="240"/>
+      <c r="G20" s="240"/>
+      <c r="H20" s="240"/>
+      <c r="I20" s="240"/>
+      <c r="J20" s="240"/>
+      <c r="K20" s="240"/>
+      <c r="L20" s="241"/>
       <c r="N20" s="106"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="230">
         <v>4</v>
       </c>
-      <c r="B21" s="267" t="s">
+      <c r="B21" s="240" t="s">
         <v>357</v>
       </c>
-      <c r="C21" s="267"/>
-      <c r="D21" s="267"/>
-      <c r="E21" s="267"/>
-      <c r="F21" s="267"/>
-      <c r="G21" s="267"/>
-      <c r="H21" s="267"/>
-      <c r="I21" s="267"/>
-      <c r="J21" s="267"/>
-      <c r="K21" s="267"/>
-      <c r="L21" s="268"/>
+      <c r="C21" s="240"/>
+      <c r="D21" s="240"/>
+      <c r="E21" s="240"/>
+      <c r="F21" s="240"/>
+      <c r="G21" s="240"/>
+      <c r="H21" s="240"/>
+      <c r="I21" s="240"/>
+      <c r="J21" s="240"/>
+      <c r="K21" s="240"/>
+      <c r="L21" s="241"/>
       <c r="N21" s="106"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="230">
         <v>5</v>
       </c>
-      <c r="B22" s="267" t="s">
+      <c r="B22" s="240" t="s">
         <v>220</v>
       </c>
-      <c r="C22" s="267"/>
-      <c r="D22" s="267"/>
-      <c r="E22" s="267"/>
-      <c r="F22" s="267"/>
-      <c r="G22" s="267"/>
-      <c r="H22" s="267"/>
-      <c r="I22" s="267"/>
-      <c r="J22" s="267"/>
-      <c r="K22" s="267"/>
-      <c r="L22" s="268"/>
+      <c r="C22" s="240"/>
+      <c r="D22" s="240"/>
+      <c r="E22" s="240"/>
+      <c r="F22" s="240"/>
+      <c r="G22" s="240"/>
+      <c r="H22" s="240"/>
+      <c r="I22" s="240"/>
+      <c r="J22" s="240"/>
+      <c r="K22" s="240"/>
+      <c r="L22" s="241"/>
       <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="230"/>
-      <c r="B23" s="267" t="s">
+      <c r="B23" s="240" t="s">
         <v>221</v>
       </c>
-      <c r="C23" s="267"/>
-      <c r="D23" s="267"/>
-      <c r="E23" s="267"/>
-      <c r="F23" s="267"/>
-      <c r="G23" s="267"/>
-      <c r="H23" s="267"/>
-      <c r="I23" s="267"/>
-      <c r="J23" s="267"/>
-      <c r="K23" s="267"/>
-      <c r="L23" s="268"/>
+      <c r="C23" s="240"/>
+      <c r="D23" s="240"/>
+      <c r="E23" s="240"/>
+      <c r="F23" s="240"/>
+      <c r="G23" s="240"/>
+      <c r="H23" s="240"/>
+      <c r="I23" s="240"/>
+      <c r="J23" s="240"/>
+      <c r="K23" s="240"/>
+      <c r="L23" s="241"/>
       <c r="N23" s="106"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="230"/>
-      <c r="B24" s="267" t="s">
+      <c r="B24" s="240" t="s">
         <v>222</v>
       </c>
-      <c r="C24" s="267"/>
-      <c r="D24" s="267"/>
-      <c r="E24" s="267"/>
-      <c r="F24" s="267"/>
-      <c r="G24" s="267"/>
-      <c r="H24" s="267"/>
-      <c r="I24" s="267"/>
-      <c r="J24" s="267"/>
-      <c r="K24" s="267"/>
-      <c r="L24" s="268"/>
+      <c r="C24" s="240"/>
+      <c r="D24" s="240"/>
+      <c r="E24" s="240"/>
+      <c r="F24" s="240"/>
+      <c r="G24" s="240"/>
+      <c r="H24" s="240"/>
+      <c r="I24" s="240"/>
+      <c r="J24" s="240"/>
+      <c r="K24" s="240"/>
+      <c r="L24" s="241"/>
       <c r="N24" s="106"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="269" t="s">
+      <c r="A25" s="249" t="s">
         <v>228</v>
       </c>
-      <c r="B25" s="270"/>
-      <c r="C25" s="270"/>
-      <c r="D25" s="270"/>
-      <c r="E25" s="270"/>
-      <c r="F25" s="270"/>
-      <c r="G25" s="270"/>
-      <c r="H25" s="270"/>
-      <c r="I25" s="270"/>
-      <c r="J25" s="270"/>
-      <c r="K25" s="270"/>
-      <c r="L25" s="271"/>
+      <c r="B25" s="250"/>
+      <c r="C25" s="250"/>
+      <c r="D25" s="250"/>
+      <c r="E25" s="250"/>
+      <c r="F25" s="250"/>
+      <c r="G25" s="250"/>
+      <c r="H25" s="250"/>
+      <c r="I25" s="250"/>
+      <c r="J25" s="250"/>
+      <c r="K25" s="250"/>
+      <c r="L25" s="251"/>
       <c r="N25" s="106"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="230">
         <v>1</v>
       </c>
-      <c r="B26" s="267" t="s">
+      <c r="B26" s="240" t="s">
         <v>223</v>
       </c>
-      <c r="C26" s="267"/>
-      <c r="D26" s="267"/>
-      <c r="E26" s="267"/>
-      <c r="F26" s="267"/>
-      <c r="G26" s="267"/>
-      <c r="H26" s="267"/>
-      <c r="I26" s="267"/>
-      <c r="J26" s="267"/>
-      <c r="K26" s="267"/>
-      <c r="L26" s="268"/>
+      <c r="C26" s="240"/>
+      <c r="D26" s="240"/>
+      <c r="E26" s="240"/>
+      <c r="F26" s="240"/>
+      <c r="G26" s="240"/>
+      <c r="H26" s="240"/>
+      <c r="I26" s="240"/>
+      <c r="J26" s="240"/>
+      <c r="K26" s="240"/>
+      <c r="L26" s="241"/>
       <c r="N26" s="106"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="230"/>
-      <c r="B27" s="265" t="s">
+      <c r="B27" s="238" t="s">
         <v>358</v>
       </c>
-      <c r="C27" s="265"/>
-      <c r="D27" s="265"/>
-      <c r="E27" s="265"/>
-      <c r="F27" s="265"/>
-      <c r="G27" s="265"/>
-      <c r="H27" s="265"/>
-      <c r="I27" s="265"/>
-      <c r="J27" s="265"/>
-      <c r="K27" s="265"/>
-      <c r="L27" s="266"/>
+      <c r="C27" s="238"/>
+      <c r="D27" s="238"/>
+      <c r="E27" s="238"/>
+      <c r="F27" s="238"/>
+      <c r="G27" s="238"/>
+      <c r="H27" s="238"/>
+      <c r="I27" s="238"/>
+      <c r="J27" s="238"/>
+      <c r="K27" s="238"/>
+      <c r="L27" s="239"/>
       <c r="N27" s="106"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="230">
         <v>2</v>
       </c>
-      <c r="B28" s="267" t="s">
+      <c r="B28" s="240" t="s">
         <v>347</v>
       </c>
-      <c r="C28" s="267"/>
-      <c r="D28" s="267"/>
-      <c r="E28" s="267"/>
-      <c r="F28" s="267"/>
-      <c r="G28" s="267"/>
-      <c r="H28" s="267"/>
-      <c r="I28" s="267"/>
-      <c r="J28" s="267"/>
-      <c r="K28" s="267"/>
-      <c r="L28" s="268"/>
+      <c r="C28" s="240"/>
+      <c r="D28" s="240"/>
+      <c r="E28" s="240"/>
+      <c r="F28" s="240"/>
+      <c r="G28" s="240"/>
+      <c r="H28" s="240"/>
+      <c r="I28" s="240"/>
+      <c r="J28" s="240"/>
+      <c r="K28" s="240"/>
+      <c r="L28" s="241"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="230">
         <v>3</v>
       </c>
-      <c r="B29" s="267" t="s">
+      <c r="B29" s="240" t="s">
         <v>336</v>
       </c>
-      <c r="C29" s="267"/>
-      <c r="D29" s="267"/>
-      <c r="E29" s="267"/>
-      <c r="F29" s="267"/>
-      <c r="G29" s="267"/>
-      <c r="H29" s="267"/>
-      <c r="I29" s="267"/>
-      <c r="J29" s="267"/>
-      <c r="K29" s="267"/>
-      <c r="L29" s="268"/>
+      <c r="C29" s="240"/>
+      <c r="D29" s="240"/>
+      <c r="E29" s="240"/>
+      <c r="F29" s="240"/>
+      <c r="G29" s="240"/>
+      <c r="H29" s="240"/>
+      <c r="I29" s="240"/>
+      <c r="J29" s="240"/>
+      <c r="K29" s="240"/>
+      <c r="L29" s="241"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="230">
         <v>4</v>
       </c>
-      <c r="B30" s="267" t="s">
+      <c r="B30" s="240" t="s">
         <v>359</v>
       </c>
-      <c r="C30" s="267"/>
-      <c r="D30" s="267"/>
-      <c r="E30" s="267"/>
-      <c r="F30" s="267"/>
-      <c r="G30" s="267"/>
-      <c r="H30" s="267"/>
-      <c r="I30" s="267"/>
-      <c r="J30" s="267"/>
-      <c r="K30" s="267"/>
-      <c r="L30" s="268"/>
+      <c r="C30" s="240"/>
+      <c r="D30" s="240"/>
+      <c r="E30" s="240"/>
+      <c r="F30" s="240"/>
+      <c r="G30" s="240"/>
+      <c r="H30" s="240"/>
+      <c r="I30" s="240"/>
+      <c r="J30" s="240"/>
+      <c r="K30" s="240"/>
+      <c r="L30" s="241"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="230">
         <v>5</v>
       </c>
-      <c r="B31" s="265" t="s">
+      <c r="B31" s="238" t="s">
         <v>337</v>
       </c>
-      <c r="C31" s="265"/>
-      <c r="D31" s="265"/>
-      <c r="E31" s="265"/>
-      <c r="F31" s="265"/>
-      <c r="G31" s="265"/>
-      <c r="H31" s="265"/>
-      <c r="I31" s="265"/>
-      <c r="J31" s="265"/>
-      <c r="K31" s="265"/>
-      <c r="L31" s="266"/>
+      <c r="C31" s="238"/>
+      <c r="D31" s="238"/>
+      <c r="E31" s="238"/>
+      <c r="F31" s="238"/>
+      <c r="G31" s="238"/>
+      <c r="H31" s="238"/>
+      <c r="I31" s="238"/>
+      <c r="J31" s="238"/>
+      <c r="K31" s="238"/>
+      <c r="L31" s="239"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="230">
         <v>6</v>
       </c>
-      <c r="B32" s="265" t="s">
+      <c r="B32" s="238" t="s">
         <v>342</v>
       </c>
-      <c r="C32" s="265"/>
-      <c r="D32" s="265"/>
-      <c r="E32" s="265"/>
-      <c r="F32" s="265"/>
-      <c r="G32" s="265"/>
-      <c r="H32" s="265"/>
-      <c r="I32" s="265"/>
-      <c r="J32" s="265"/>
-      <c r="K32" s="265"/>
-      <c r="L32" s="266"/>
+      <c r="C32" s="238"/>
+      <c r="D32" s="238"/>
+      <c r="E32" s="238"/>
+      <c r="F32" s="238"/>
+      <c r="G32" s="238"/>
+      <c r="H32" s="238"/>
+      <c r="I32" s="238"/>
+      <c r="J32" s="238"/>
+      <c r="K32" s="238"/>
+      <c r="L32" s="239"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="230">
         <v>7</v>
       </c>
-      <c r="B33" s="267" t="s">
+      <c r="B33" s="240" t="s">
         <v>338</v>
       </c>
-      <c r="C33" s="267"/>
-      <c r="D33" s="267"/>
-      <c r="E33" s="267"/>
-      <c r="F33" s="267"/>
-      <c r="G33" s="267"/>
-      <c r="H33" s="267"/>
-      <c r="I33" s="267"/>
-      <c r="J33" s="267"/>
-      <c r="K33" s="267"/>
-      <c r="L33" s="268"/>
+      <c r="C33" s="240"/>
+      <c r="D33" s="240"/>
+      <c r="E33" s="240"/>
+      <c r="F33" s="240"/>
+      <c r="G33" s="240"/>
+      <c r="H33" s="240"/>
+      <c r="I33" s="240"/>
+      <c r="J33" s="240"/>
+      <c r="K33" s="240"/>
+      <c r="L33" s="241"/>
     </row>
     <row r="34" spans="1:12" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="230"/>
@@ -15445,56 +15448,56 @@
       <c r="L34" s="232"/>
     </row>
     <row r="35" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="269" t="s">
+      <c r="A35" s="249" t="s">
         <v>341</v>
       </c>
-      <c r="B35" s="270"/>
-      <c r="C35" s="270"/>
-      <c r="D35" s="270"/>
-      <c r="E35" s="270"/>
-      <c r="F35" s="270"/>
-      <c r="G35" s="270"/>
-      <c r="H35" s="270"/>
-      <c r="I35" s="270"/>
-      <c r="J35" s="270"/>
-      <c r="K35" s="270"/>
-      <c r="L35" s="271"/>
+      <c r="B35" s="250"/>
+      <c r="C35" s="250"/>
+      <c r="D35" s="250"/>
+      <c r="E35" s="250"/>
+      <c r="F35" s="250"/>
+      <c r="G35" s="250"/>
+      <c r="H35" s="250"/>
+      <c r="I35" s="250"/>
+      <c r="J35" s="250"/>
+      <c r="K35" s="250"/>
+      <c r="L35" s="251"/>
     </row>
     <row r="36" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="233" t="s">
         <v>339</v>
       </c>
-      <c r="B36" s="267" t="s">
+      <c r="B36" s="240" t="s">
         <v>224</v>
       </c>
-      <c r="C36" s="267"/>
-      <c r="D36" s="267"/>
-      <c r="E36" s="267"/>
-      <c r="F36" s="267"/>
-      <c r="G36" s="267"/>
-      <c r="H36" s="267"/>
-      <c r="I36" s="267"/>
-      <c r="J36" s="267"/>
-      <c r="K36" s="267"/>
-      <c r="L36" s="268"/>
+      <c r="C36" s="240"/>
+      <c r="D36" s="240"/>
+      <c r="E36" s="240"/>
+      <c r="F36" s="240"/>
+      <c r="G36" s="240"/>
+      <c r="H36" s="240"/>
+      <c r="I36" s="240"/>
+      <c r="J36" s="240"/>
+      <c r="K36" s="240"/>
+      <c r="L36" s="241"/>
     </row>
     <row r="37" spans="1:12" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="234" t="s">
         <v>340</v>
       </c>
-      <c r="B37" s="273" t="s">
+      <c r="B37" s="242" t="s">
         <v>343</v>
       </c>
-      <c r="C37" s="273"/>
-      <c r="D37" s="273"/>
-      <c r="E37" s="273"/>
-      <c r="F37" s="273"/>
-      <c r="G37" s="273"/>
-      <c r="H37" s="273"/>
-      <c r="I37" s="273"/>
-      <c r="J37" s="273"/>
-      <c r="K37" s="273"/>
-      <c r="L37" s="274"/>
+      <c r="C37" s="242"/>
+      <c r="D37" s="242"/>
+      <c r="E37" s="242"/>
+      <c r="F37" s="242"/>
+      <c r="G37" s="242"/>
+      <c r="H37" s="242"/>
+      <c r="I37" s="242"/>
+      <c r="J37" s="242"/>
+      <c r="K37" s="242"/>
+      <c r="L37" s="243"/>
     </row>
     <row r="38" spans="1:12" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="161"/>
@@ -15511,20 +15514,20 @@
       <c r="L38" s="113"/>
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="275" t="s">
+      <c r="A39" s="244" t="s">
         <v>252</v>
       </c>
-      <c r="B39" s="276"/>
-      <c r="C39" s="276"/>
-      <c r="D39" s="276"/>
-      <c r="E39" s="276"/>
-      <c r="F39" s="276"/>
-      <c r="G39" s="276"/>
-      <c r="H39" s="276"/>
-      <c r="I39" s="276"/>
-      <c r="J39" s="276"/>
-      <c r="K39" s="276"/>
-      <c r="L39" s="277"/>
+      <c r="B39" s="245"/>
+      <c r="C39" s="245"/>
+      <c r="D39" s="245"/>
+      <c r="E39" s="245"/>
+      <c r="F39" s="245"/>
+      <c r="G39" s="245"/>
+      <c r="H39" s="245"/>
+      <c r="I39" s="245"/>
+      <c r="J39" s="245"/>
+      <c r="K39" s="245"/>
+      <c r="L39" s="246"/>
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="162" t="s">
@@ -15612,72 +15615,72 @@
       <c r="B45" s="170" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="255" t="s">
+      <c r="C45" s="247" t="s">
         <v>326</v>
       </c>
-      <c r="D45" s="255"/>
-      <c r="E45" s="255"/>
-      <c r="F45" s="255"/>
-      <c r="G45" s="255"/>
-      <c r="H45" s="255"/>
-      <c r="I45" s="255"/>
-      <c r="J45" s="255"/>
-      <c r="K45" s="255"/>
-      <c r="L45" s="256"/>
+      <c r="D45" s="247"/>
+      <c r="E45" s="247"/>
+      <c r="F45" s="247"/>
+      <c r="G45" s="247"/>
+      <c r="H45" s="247"/>
+      <c r="I45" s="247"/>
+      <c r="J45" s="247"/>
+      <c r="K45" s="247"/>
+      <c r="L45" s="248"/>
     </row>
     <row r="46" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="169"/>
       <c r="B46" s="170" t="s">
         <v>146</v>
       </c>
-      <c r="C46" s="255" t="s">
+      <c r="C46" s="247" t="s">
         <v>147</v>
       </c>
-      <c r="D46" s="255"/>
-      <c r="E46" s="255"/>
-      <c r="F46" s="255"/>
-      <c r="G46" s="255"/>
-      <c r="H46" s="255"/>
-      <c r="I46" s="255"/>
-      <c r="J46" s="255"/>
-      <c r="K46" s="255"/>
-      <c r="L46" s="256"/>
+      <c r="D46" s="247"/>
+      <c r="E46" s="247"/>
+      <c r="F46" s="247"/>
+      <c r="G46" s="247"/>
+      <c r="H46" s="247"/>
+      <c r="I46" s="247"/>
+      <c r="J46" s="247"/>
+      <c r="K46" s="247"/>
+      <c r="L46" s="248"/>
     </row>
     <row r="47" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="169"/>
       <c r="B47" s="170" t="s">
         <v>250</v>
       </c>
-      <c r="C47" s="255" t="s">
+      <c r="C47" s="247" t="s">
         <v>251</v>
       </c>
-      <c r="D47" s="255"/>
-      <c r="E47" s="255"/>
-      <c r="F47" s="255"/>
-      <c r="G47" s="255"/>
-      <c r="H47" s="255"/>
-      <c r="I47" s="255"/>
-      <c r="J47" s="255"/>
-      <c r="K47" s="255"/>
-      <c r="L47" s="256"/>
+      <c r="D47" s="247"/>
+      <c r="E47" s="247"/>
+      <c r="F47" s="247"/>
+      <c r="G47" s="247"/>
+      <c r="H47" s="247"/>
+      <c r="I47" s="247"/>
+      <c r="J47" s="247"/>
+      <c r="K47" s="247"/>
+      <c r="L47" s="248"/>
     </row>
     <row r="48" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="169"/>
       <c r="B48" s="170" t="s">
         <v>327</v>
       </c>
-      <c r="C48" s="255" t="s">
+      <c r="C48" s="247" t="s">
         <v>328</v>
       </c>
-      <c r="D48" s="255"/>
-      <c r="E48" s="255"/>
-      <c r="F48" s="255"/>
-      <c r="G48" s="255"/>
-      <c r="H48" s="255"/>
-      <c r="I48" s="255"/>
-      <c r="J48" s="255"/>
-      <c r="K48" s="255"/>
-      <c r="L48" s="256"/>
+      <c r="D48" s="247"/>
+      <c r="E48" s="247"/>
+      <c r="F48" s="247"/>
+      <c r="G48" s="247"/>
+      <c r="H48" s="247"/>
+      <c r="I48" s="247"/>
+      <c r="J48" s="247"/>
+      <c r="K48" s="247"/>
+      <c r="L48" s="248"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="169"/>
@@ -15702,18 +15705,18 @@
       <c r="B50" s="170" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="255" t="s">
+      <c r="C50" s="247" t="s">
         <v>330</v>
       </c>
-      <c r="D50" s="255"/>
-      <c r="E50" s="255"/>
-      <c r="F50" s="255"/>
-      <c r="G50" s="255"/>
-      <c r="H50" s="255"/>
-      <c r="I50" s="255"/>
-      <c r="J50" s="255"/>
-      <c r="K50" s="255"/>
-      <c r="L50" s="256"/>
+      <c r="D50" s="247"/>
+      <c r="E50" s="247"/>
+      <c r="F50" s="247"/>
+      <c r="G50" s="247"/>
+      <c r="H50" s="247"/>
+      <c r="I50" s="247"/>
+      <c r="J50" s="247"/>
+      <c r="K50" s="247"/>
+      <c r="L50" s="248"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="169"/>
@@ -15795,37 +15798,39 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="272" t="s">
+      <c r="A64" s="237" t="s">
         <v>332</v>
       </c>
-      <c r="B64" s="272"/>
-      <c r="C64" s="272"/>
-      <c r="D64" s="272"/>
-      <c r="E64" s="272"/>
-      <c r="F64" s="272"/>
-      <c r="G64" s="272"/>
-      <c r="H64" s="272"/>
-      <c r="I64" s="272"/>
-      <c r="J64" s="272"/>
-      <c r="K64" s="272"/>
-      <c r="L64" s="272"/>
+      <c r="B64" s="237"/>
+      <c r="C64" s="237"/>
+      <c r="D64" s="237"/>
+      <c r="E64" s="237"/>
+      <c r="F64" s="237"/>
+      <c r="G64" s="237"/>
+      <c r="H64" s="237"/>
+      <c r="I64" s="237"/>
+      <c r="J64" s="237"/>
+      <c r="K64" s="237"/>
+      <c r="L64" s="237"/>
     </row>
     <row r="69" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="70" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A64:L64"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="C45:L45"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="C47:L47"/>
-    <mergeCell ref="C48:L48"/>
-    <mergeCell ref="C50:L50"/>
-    <mergeCell ref="A35:L35"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B8:L8"/>
     <mergeCell ref="B31:L31"/>
     <mergeCell ref="B18:L18"/>
     <mergeCell ref="B19:L19"/>
@@ -15840,20 +15845,18 @@
     <mergeCell ref="B29:L29"/>
     <mergeCell ref="B28:L28"/>
     <mergeCell ref="B30:L30"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="A64:L64"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="C45:L45"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="C48:L48"/>
+    <mergeCell ref="C50:L50"/>
+    <mergeCell ref="A35:L35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A57" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -16512,7 +16515,7 @@
   <dimension ref="A1:P139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16528,7 +16531,7 @@
     <col min="9" max="9" width="7.7265625" hidden="1" customWidth="1"/>
     <col min="10" max="12" width="8.7265625" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="10.81640625" customWidth="1"/>
-    <col min="14" max="14" width="37.7265625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="42" style="2" customWidth="1"/>
     <col min="15" max="15" width="13" customWidth="1"/>
     <col min="16" max="16" width="9.81640625" customWidth="1"/>
     <col min="17" max="17" width="10.81640625" customWidth="1"/>
@@ -16807,7 +16810,7 @@
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
       <c r="N22" s="141" t="s">
-        <v>182</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
@@ -21234,7 +21237,7 @@
     <hyperlink ref="N19" r:id="rId4" location="ii-start-storage" xr:uid="{692C3AE6-515B-4C08-B6EC-0557E75E9511}"/>
     <hyperlink ref="N20" r:id="rId5" location="iii-protection-elevations" xr:uid="{16CC5ED4-0369-416C-AC3E-3AD6F831A454}"/>
     <hyperlink ref="N21" r:id="rId6" location="iv-the-protection-volumes" xr:uid="{D7802E8D-5298-4564-9936-B3226B6E96DA}"/>
-    <hyperlink ref="N22" r:id="rId7" location="v-prior-9-year-lake-powell-release" xr:uid="{9E773CCF-F296-48D2-ADA9-5456ABC7F062}"/>
+    <hyperlink ref="N22" r:id="rId7" location="v-prior-9-year-lake-powell-release" display="Help 9-year prior Powell release" xr:uid="{9E773CCF-F296-48D2-ADA9-5456ABC7F062}"/>
     <hyperlink ref="N23" r:id="rId8" location="vi-prior-9-year-paria-river-flow" xr:uid="{8CAE8559-5BD9-4D9F-8655-D1F3AE1FCD4D}"/>
     <hyperlink ref="N24" r:id="rId9" location="vii-delivery-to-meet-10-year-requirement" xr:uid="{B6DDA7AA-2218-4D2F-9A7A-A0EDBEFDC5B1}"/>
     <hyperlink ref="N28" r:id="rId10" location="step-2-specify-natural-inflow-to-lake-powell" xr:uid="{78DF76B4-BE79-4AC1-9F08-EC86A0A72F91}"/>
@@ -22686,16 +22689,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="312" t="e">
+      <c r="A1" s="313" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="312"/>
-      <c r="C1" s="312"/>
-      <c r="D1" s="312"/>
-      <c r="E1" s="312"/>
-      <c r="F1" s="312"/>
-      <c r="G1" s="312"/>
+      <c r="B1" s="313"/>
+      <c r="C1" s="313"/>
+      <c r="D1" s="313"/>
+      <c r="E1" s="313"/>
+      <c r="F1" s="313"/>
+      <c r="G1" s="313"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -22804,11 +22807,11 @@
         <v>81</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="313"/>
-      <c r="D10" s="313"/>
-      <c r="E10" s="313"/>
-      <c r="F10" s="313"/>
-      <c r="G10" s="313"/>
+      <c r="C10" s="312"/>
+      <c r="D10" s="312"/>
+      <c r="E10" s="312"/>
+      <c r="F10" s="312"/>
+      <c r="G10" s="312"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -24071,6 +24074,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -24078,12 +24087,6 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>

</xml_diff>

<commit_message>
Update Lake Mead inflow in model guide and links
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6C7EB55-DC86-4E02-8B6A-A245AC8AE669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD2E151-0182-4BED-A2C0-F9BAD1D5E18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="365">
   <si>
     <t>Year 1</t>
   </si>
@@ -1909,6 +1909,18 @@
   <si>
     <t>Help Water Conservation Program Total Balance</t>
   </si>
+  <si>
+    <t>Help storage above protect zone</t>
+  </si>
+  <si>
+    <t>Help remaining storage above protect and ICS</t>
+  </si>
+  <si>
+    <t>Help calculate Mead evaporation</t>
+  </si>
+  <si>
+    <t>Help specify Lake Mead inflow</t>
+  </si>
 </sst>
 </file>
 
@@ -3185,51 +3197,6 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3284,6 +3251,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3307,6 +3280,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3410,11 +3422,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14854,20 +14866,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="255" t="s">
+      <c r="A1" s="240" t="s">
         <v>321</v>
       </c>
-      <c r="B1" s="255"/>
-      <c r="C1" s="255"/>
-      <c r="D1" s="255"/>
-      <c r="E1" s="255"/>
-      <c r="F1" s="255"/>
-      <c r="G1" s="255"/>
-      <c r="H1" s="255"/>
-      <c r="I1" s="255"/>
-      <c r="J1" s="255"/>
-      <c r="K1" s="255"/>
-      <c r="L1" s="255"/>
+      <c r="B1" s="240"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
+      <c r="F1" s="240"/>
+      <c r="G1" s="240"/>
+      <c r="H1" s="240"/>
+      <c r="I1" s="240"/>
+      <c r="J1" s="240"/>
+      <c r="K1" s="240"/>
+      <c r="L1" s="240"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -14893,41 +14905,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="256" t="s">
+      <c r="A4" s="241" t="s">
         <v>349</v>
       </c>
-      <c r="B4" s="257"/>
-      <c r="C4" s="257"/>
-      <c r="D4" s="257"/>
-      <c r="E4" s="257"/>
-      <c r="F4" s="257"/>
-      <c r="G4" s="257"/>
-      <c r="H4" s="257"/>
-      <c r="I4" s="257"/>
-      <c r="J4" s="257"/>
-      <c r="K4" s="257"/>
-      <c r="L4" s="258"/>
-      <c r="N4" s="259"/>
-      <c r="O4" s="259"/>
-      <c r="P4" s="259"/>
-      <c r="Q4" s="259"/>
-      <c r="R4" s="259"/>
+      <c r="B4" s="242"/>
+      <c r="C4" s="242"/>
+      <c r="D4" s="242"/>
+      <c r="E4" s="242"/>
+      <c r="F4" s="242"/>
+      <c r="G4" s="242"/>
+      <c r="H4" s="242"/>
+      <c r="I4" s="242"/>
+      <c r="J4" s="242"/>
+      <c r="K4" s="242"/>
+      <c r="L4" s="243"/>
+      <c r="N4" s="244"/>
+      <c r="O4" s="244"/>
+      <c r="P4" s="244"/>
+      <c r="Q4" s="244"/>
+      <c r="R4" s="244"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="260" t="s">
+      <c r="A5" s="245" t="s">
         <v>350</v>
       </c>
-      <c r="B5" s="261"/>
-      <c r="C5" s="261"/>
-      <c r="D5" s="261"/>
-      <c r="E5" s="261"/>
-      <c r="F5" s="261"/>
-      <c r="G5" s="261"/>
-      <c r="H5" s="261"/>
-      <c r="I5" s="261"/>
-      <c r="J5" s="261"/>
-      <c r="K5" s="261"/>
-      <c r="L5" s="262"/>
+      <c r="B5" s="246"/>
+      <c r="C5" s="246"/>
+      <c r="D5" s="246"/>
+      <c r="E5" s="246"/>
+      <c r="F5" s="246"/>
+      <c r="G5" s="246"/>
+      <c r="H5" s="246"/>
+      <c r="I5" s="246"/>
+      <c r="J5" s="246"/>
+      <c r="K5" s="246"/>
+      <c r="L5" s="247"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -14935,20 +14947,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="260" t="s">
+      <c r="A6" s="245" t="s">
         <v>352</v>
       </c>
-      <c r="B6" s="261"/>
-      <c r="C6" s="261"/>
-      <c r="D6" s="261"/>
-      <c r="E6" s="261"/>
-      <c r="F6" s="261"/>
-      <c r="G6" s="261"/>
-      <c r="H6" s="261"/>
-      <c r="I6" s="261"/>
-      <c r="J6" s="261"/>
-      <c r="K6" s="261"/>
-      <c r="L6" s="262"/>
+      <c r="B6" s="246"/>
+      <c r="C6" s="246"/>
+      <c r="D6" s="246"/>
+      <c r="E6" s="246"/>
+      <c r="F6" s="246"/>
+      <c r="G6" s="246"/>
+      <c r="H6" s="246"/>
+      <c r="I6" s="246"/>
+      <c r="J6" s="246"/>
+      <c r="K6" s="246"/>
+      <c r="L6" s="247"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -14957,19 +14969,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="235"/>
-      <c r="B7" s="261" t="s">
+      <c r="B7" s="246" t="s">
         <v>353</v>
       </c>
-      <c r="C7" s="261"/>
-      <c r="D7" s="261"/>
-      <c r="E7" s="261"/>
-      <c r="F7" s="261"/>
-      <c r="G7" s="261"/>
-      <c r="H7" s="261"/>
-      <c r="I7" s="261"/>
-      <c r="J7" s="261"/>
-      <c r="K7" s="261"/>
-      <c r="L7" s="262"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246"/>
+      <c r="K7" s="246"/>
+      <c r="L7" s="247"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -14978,19 +14990,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="236"/>
-      <c r="B8" s="276" t="s">
+      <c r="B8" s="263" t="s">
         <v>354</v>
       </c>
-      <c r="C8" s="276"/>
-      <c r="D8" s="276"/>
-      <c r="E8" s="276"/>
-      <c r="F8" s="276"/>
-      <c r="G8" s="276"/>
-      <c r="H8" s="276"/>
-      <c r="I8" s="276"/>
-      <c r="J8" s="276"/>
-      <c r="K8" s="276"/>
-      <c r="L8" s="277"/>
+      <c r="C8" s="263"/>
+      <c r="D8" s="263"/>
+      <c r="E8" s="263"/>
+      <c r="F8" s="263"/>
+      <c r="G8" s="263"/>
+      <c r="H8" s="263"/>
+      <c r="I8" s="263"/>
+      <c r="J8" s="263"/>
+      <c r="K8" s="263"/>
+      <c r="L8" s="264"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15012,84 +15024,84 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="263" t="s">
+      <c r="A10" s="248" t="s">
         <v>217</v>
       </c>
-      <c r="B10" s="264"/>
-      <c r="C10" s="264"/>
-      <c r="D10" s="264"/>
-      <c r="E10" s="264"/>
-      <c r="F10" s="264"/>
-      <c r="G10" s="264"/>
-      <c r="H10" s="264"/>
-      <c r="I10" s="264"/>
-      <c r="J10" s="264"/>
-      <c r="K10" s="264"/>
-      <c r="L10" s="265"/>
+      <c r="B10" s="249"/>
+      <c r="C10" s="249"/>
+      <c r="D10" s="249"/>
+      <c r="E10" s="249"/>
+      <c r="F10" s="249"/>
+      <c r="G10" s="249"/>
+      <c r="H10" s="249"/>
+      <c r="I10" s="249"/>
+      <c r="J10" s="249"/>
+      <c r="K10" s="249"/>
+      <c r="L10" s="250"/>
     </row>
     <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="266" t="s">
+      <c r="A11" s="251" t="s">
         <v>351</v>
       </c>
-      <c r="B11" s="267"/>
-      <c r="C11" s="267"/>
-      <c r="D11" s="267"/>
-      <c r="E11" s="267"/>
-      <c r="F11" s="267"/>
-      <c r="G11" s="267"/>
-      <c r="H11" s="267"/>
-      <c r="I11" s="267"/>
-      <c r="J11" s="267"/>
-      <c r="K11" s="267"/>
-      <c r="L11" s="268"/>
+      <c r="B11" s="252"/>
+      <c r="C11" s="252"/>
+      <c r="D11" s="252"/>
+      <c r="E11" s="252"/>
+      <c r="F11" s="252"/>
+      <c r="G11" s="252"/>
+      <c r="H11" s="252"/>
+      <c r="I11" s="252"/>
+      <c r="J11" s="252"/>
+      <c r="K11" s="252"/>
+      <c r="L11" s="253"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="269" t="s">
+      <c r="A12" s="254" t="s">
         <v>355</v>
       </c>
-      <c r="B12" s="247"/>
-      <c r="C12" s="247"/>
-      <c r="D12" s="247"/>
-      <c r="E12" s="247"/>
-      <c r="F12" s="247"/>
-      <c r="G12" s="247"/>
-      <c r="H12" s="247"/>
-      <c r="I12" s="247"/>
-      <c r="J12" s="247"/>
-      <c r="K12" s="247"/>
-      <c r="L12" s="248"/>
+      <c r="B12" s="255"/>
+      <c r="C12" s="255"/>
+      <c r="D12" s="255"/>
+      <c r="E12" s="255"/>
+      <c r="F12" s="255"/>
+      <c r="G12" s="255"/>
+      <c r="H12" s="255"/>
+      <c r="I12" s="255"/>
+      <c r="J12" s="255"/>
+      <c r="K12" s="255"/>
+      <c r="L12" s="256"/>
     </row>
     <row r="13" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="269" t="s">
+      <c r="A13" s="254" t="s">
         <v>218</v>
       </c>
-      <c r="B13" s="247"/>
-      <c r="C13" s="247"/>
-      <c r="D13" s="247"/>
-      <c r="E13" s="247"/>
-      <c r="F13" s="247"/>
-      <c r="G13" s="247"/>
-      <c r="H13" s="247"/>
-      <c r="I13" s="247"/>
-      <c r="J13" s="247"/>
-      <c r="K13" s="247"/>
-      <c r="L13" s="248"/>
+      <c r="B13" s="255"/>
+      <c r="C13" s="255"/>
+      <c r="D13" s="255"/>
+      <c r="E13" s="255"/>
+      <c r="F13" s="255"/>
+      <c r="G13" s="255"/>
+      <c r="H13" s="255"/>
+      <c r="I13" s="255"/>
+      <c r="J13" s="255"/>
+      <c r="K13" s="255"/>
+      <c r="L13" s="256"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="270" t="s">
+      <c r="A14" s="257" t="s">
         <v>356</v>
       </c>
-      <c r="B14" s="271"/>
-      <c r="C14" s="271"/>
-      <c r="D14" s="271"/>
-      <c r="E14" s="271"/>
-      <c r="F14" s="271"/>
-      <c r="G14" s="271"/>
-      <c r="H14" s="271"/>
-      <c r="I14" s="271"/>
-      <c r="J14" s="271"/>
-      <c r="K14" s="271"/>
-      <c r="L14" s="272"/>
+      <c r="B14" s="258"/>
+      <c r="C14" s="258"/>
+      <c r="D14" s="258"/>
+      <c r="E14" s="258"/>
+      <c r="F14" s="258"/>
+      <c r="G14" s="258"/>
+      <c r="H14" s="258"/>
+      <c r="I14" s="258"/>
+      <c r="J14" s="258"/>
+      <c r="K14" s="258"/>
+      <c r="L14" s="259"/>
     </row>
     <row r="15" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="113"/>
@@ -15106,332 +15118,332 @@
       <c r="L15" s="113"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="273" t="s">
+      <c r="A16" s="260" t="s">
         <v>348</v>
       </c>
-      <c r="B16" s="274"/>
-      <c r="C16" s="274"/>
-      <c r="D16" s="274"/>
-      <c r="E16" s="274"/>
-      <c r="F16" s="274"/>
-      <c r="G16" s="274"/>
-      <c r="H16" s="274"/>
-      <c r="I16" s="274"/>
-      <c r="J16" s="274"/>
-      <c r="K16" s="274"/>
-      <c r="L16" s="275"/>
+      <c r="B16" s="261"/>
+      <c r="C16" s="261"/>
+      <c r="D16" s="261"/>
+      <c r="E16" s="261"/>
+      <c r="F16" s="261"/>
+      <c r="G16" s="261"/>
+      <c r="H16" s="261"/>
+      <c r="I16" s="261"/>
+      <c r="J16" s="261"/>
+      <c r="K16" s="261"/>
+      <c r="L16" s="262"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="252" t="s">
+      <c r="A17" s="237" t="s">
         <v>227</v>
       </c>
-      <c r="B17" s="253"/>
-      <c r="C17" s="253"/>
-      <c r="D17" s="253"/>
-      <c r="E17" s="253"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="253"/>
-      <c r="I17" s="253"/>
-      <c r="J17" s="253"/>
-      <c r="K17" s="253"/>
-      <c r="L17" s="254"/>
+      <c r="B17" s="238"/>
+      <c r="C17" s="238"/>
+      <c r="D17" s="238"/>
+      <c r="E17" s="238"/>
+      <c r="F17" s="238"/>
+      <c r="G17" s="238"/>
+      <c r="H17" s="238"/>
+      <c r="I17" s="238"/>
+      <c r="J17" s="238"/>
+      <c r="K17" s="238"/>
+      <c r="L17" s="239"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="230">
         <v>1</v>
       </c>
-      <c r="B18" s="240" t="s">
+      <c r="B18" s="267" t="s">
         <v>226</v>
       </c>
-      <c r="C18" s="240"/>
-      <c r="D18" s="240"/>
-      <c r="E18" s="240"/>
-      <c r="F18" s="240"/>
-      <c r="G18" s="240"/>
-      <c r="H18" s="240"/>
-      <c r="I18" s="240"/>
-      <c r="J18" s="240"/>
-      <c r="K18" s="240"/>
-      <c r="L18" s="241"/>
+      <c r="C18" s="267"/>
+      <c r="D18" s="267"/>
+      <c r="E18" s="267"/>
+      <c r="F18" s="267"/>
+      <c r="G18" s="267"/>
+      <c r="H18" s="267"/>
+      <c r="I18" s="267"/>
+      <c r="J18" s="267"/>
+      <c r="K18" s="267"/>
+      <c r="L18" s="268"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="230">
         <v>2</v>
       </c>
-      <c r="B19" s="240" t="s">
+      <c r="B19" s="267" t="s">
         <v>344</v>
       </c>
-      <c r="C19" s="240"/>
-      <c r="D19" s="240"/>
-      <c r="E19" s="240"/>
-      <c r="F19" s="240"/>
-      <c r="G19" s="240"/>
-      <c r="H19" s="240"/>
-      <c r="I19" s="240"/>
-      <c r="J19" s="240"/>
-      <c r="K19" s="240"/>
-      <c r="L19" s="241"/>
+      <c r="C19" s="267"/>
+      <c r="D19" s="267"/>
+      <c r="E19" s="267"/>
+      <c r="F19" s="267"/>
+      <c r="G19" s="267"/>
+      <c r="H19" s="267"/>
+      <c r="I19" s="267"/>
+      <c r="J19" s="267"/>
+      <c r="K19" s="267"/>
+      <c r="L19" s="268"/>
       <c r="N19" s="106"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="230">
         <v>3</v>
       </c>
-      <c r="B20" s="240" t="s">
+      <c r="B20" s="267" t="s">
         <v>219</v>
       </c>
-      <c r="C20" s="240"/>
-      <c r="D20" s="240"/>
-      <c r="E20" s="240"/>
-      <c r="F20" s="240"/>
-      <c r="G20" s="240"/>
-      <c r="H20" s="240"/>
-      <c r="I20" s="240"/>
-      <c r="J20" s="240"/>
-      <c r="K20" s="240"/>
-      <c r="L20" s="241"/>
+      <c r="C20" s="267"/>
+      <c r="D20" s="267"/>
+      <c r="E20" s="267"/>
+      <c r="F20" s="267"/>
+      <c r="G20" s="267"/>
+      <c r="H20" s="267"/>
+      <c r="I20" s="267"/>
+      <c r="J20" s="267"/>
+      <c r="K20" s="267"/>
+      <c r="L20" s="268"/>
       <c r="N20" s="106"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="230">
         <v>4</v>
       </c>
-      <c r="B21" s="240" t="s">
+      <c r="B21" s="267" t="s">
         <v>357</v>
       </c>
-      <c r="C21" s="240"/>
-      <c r="D21" s="240"/>
-      <c r="E21" s="240"/>
-      <c r="F21" s="240"/>
-      <c r="G21" s="240"/>
-      <c r="H21" s="240"/>
-      <c r="I21" s="240"/>
-      <c r="J21" s="240"/>
-      <c r="K21" s="240"/>
-      <c r="L21" s="241"/>
+      <c r="C21" s="267"/>
+      <c r="D21" s="267"/>
+      <c r="E21" s="267"/>
+      <c r="F21" s="267"/>
+      <c r="G21" s="267"/>
+      <c r="H21" s="267"/>
+      <c r="I21" s="267"/>
+      <c r="J21" s="267"/>
+      <c r="K21" s="267"/>
+      <c r="L21" s="268"/>
       <c r="N21" s="106"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="230">
         <v>5</v>
       </c>
-      <c r="B22" s="240" t="s">
+      <c r="B22" s="267" t="s">
         <v>220</v>
       </c>
-      <c r="C22" s="240"/>
-      <c r="D22" s="240"/>
-      <c r="E22" s="240"/>
-      <c r="F22" s="240"/>
-      <c r="G22" s="240"/>
-      <c r="H22" s="240"/>
-      <c r="I22" s="240"/>
-      <c r="J22" s="240"/>
-      <c r="K22" s="240"/>
-      <c r="L22" s="241"/>
+      <c r="C22" s="267"/>
+      <c r="D22" s="267"/>
+      <c r="E22" s="267"/>
+      <c r="F22" s="267"/>
+      <c r="G22" s="267"/>
+      <c r="H22" s="267"/>
+      <c r="I22" s="267"/>
+      <c r="J22" s="267"/>
+      <c r="K22" s="267"/>
+      <c r="L22" s="268"/>
       <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="230"/>
-      <c r="B23" s="240" t="s">
+      <c r="B23" s="267" t="s">
         <v>221</v>
       </c>
-      <c r="C23" s="240"/>
-      <c r="D23" s="240"/>
-      <c r="E23" s="240"/>
-      <c r="F23" s="240"/>
-      <c r="G23" s="240"/>
-      <c r="H23" s="240"/>
-      <c r="I23" s="240"/>
-      <c r="J23" s="240"/>
-      <c r="K23" s="240"/>
-      <c r="L23" s="241"/>
+      <c r="C23" s="267"/>
+      <c r="D23" s="267"/>
+      <c r="E23" s="267"/>
+      <c r="F23" s="267"/>
+      <c r="G23" s="267"/>
+      <c r="H23" s="267"/>
+      <c r="I23" s="267"/>
+      <c r="J23" s="267"/>
+      <c r="K23" s="267"/>
+      <c r="L23" s="268"/>
       <c r="N23" s="106"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="230"/>
-      <c r="B24" s="240" t="s">
+      <c r="B24" s="267" t="s">
         <v>222</v>
       </c>
-      <c r="C24" s="240"/>
-      <c r="D24" s="240"/>
-      <c r="E24" s="240"/>
-      <c r="F24" s="240"/>
-      <c r="G24" s="240"/>
-      <c r="H24" s="240"/>
-      <c r="I24" s="240"/>
-      <c r="J24" s="240"/>
-      <c r="K24" s="240"/>
-      <c r="L24" s="241"/>
+      <c r="C24" s="267"/>
+      <c r="D24" s="267"/>
+      <c r="E24" s="267"/>
+      <c r="F24" s="267"/>
+      <c r="G24" s="267"/>
+      <c r="H24" s="267"/>
+      <c r="I24" s="267"/>
+      <c r="J24" s="267"/>
+      <c r="K24" s="267"/>
+      <c r="L24" s="268"/>
       <c r="N24" s="106"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="249" t="s">
+      <c r="A25" s="269" t="s">
         <v>228</v>
       </c>
-      <c r="B25" s="250"/>
-      <c r="C25" s="250"/>
-      <c r="D25" s="250"/>
-      <c r="E25" s="250"/>
-      <c r="F25" s="250"/>
-      <c r="G25" s="250"/>
-      <c r="H25" s="250"/>
-      <c r="I25" s="250"/>
-      <c r="J25" s="250"/>
-      <c r="K25" s="250"/>
-      <c r="L25" s="251"/>
+      <c r="B25" s="270"/>
+      <c r="C25" s="270"/>
+      <c r="D25" s="270"/>
+      <c r="E25" s="270"/>
+      <c r="F25" s="270"/>
+      <c r="G25" s="270"/>
+      <c r="H25" s="270"/>
+      <c r="I25" s="270"/>
+      <c r="J25" s="270"/>
+      <c r="K25" s="270"/>
+      <c r="L25" s="271"/>
       <c r="N25" s="106"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="230">
         <v>1</v>
       </c>
-      <c r="B26" s="240" t="s">
+      <c r="B26" s="267" t="s">
         <v>223</v>
       </c>
-      <c r="C26" s="240"/>
-      <c r="D26" s="240"/>
-      <c r="E26" s="240"/>
-      <c r="F26" s="240"/>
-      <c r="G26" s="240"/>
-      <c r="H26" s="240"/>
-      <c r="I26" s="240"/>
-      <c r="J26" s="240"/>
-      <c r="K26" s="240"/>
-      <c r="L26" s="241"/>
+      <c r="C26" s="267"/>
+      <c r="D26" s="267"/>
+      <c r="E26" s="267"/>
+      <c r="F26" s="267"/>
+      <c r="G26" s="267"/>
+      <c r="H26" s="267"/>
+      <c r="I26" s="267"/>
+      <c r="J26" s="267"/>
+      <c r="K26" s="267"/>
+      <c r="L26" s="268"/>
       <c r="N26" s="106"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="230"/>
-      <c r="B27" s="238" t="s">
+      <c r="B27" s="265" t="s">
         <v>358</v>
       </c>
-      <c r="C27" s="238"/>
-      <c r="D27" s="238"/>
-      <c r="E27" s="238"/>
-      <c r="F27" s="238"/>
-      <c r="G27" s="238"/>
-      <c r="H27" s="238"/>
-      <c r="I27" s="238"/>
-      <c r="J27" s="238"/>
-      <c r="K27" s="238"/>
-      <c r="L27" s="239"/>
+      <c r="C27" s="265"/>
+      <c r="D27" s="265"/>
+      <c r="E27" s="265"/>
+      <c r="F27" s="265"/>
+      <c r="G27" s="265"/>
+      <c r="H27" s="265"/>
+      <c r="I27" s="265"/>
+      <c r="J27" s="265"/>
+      <c r="K27" s="265"/>
+      <c r="L27" s="266"/>
       <c r="N27" s="106"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="230">
         <v>2</v>
       </c>
-      <c r="B28" s="240" t="s">
+      <c r="B28" s="267" t="s">
         <v>347</v>
       </c>
-      <c r="C28" s="240"/>
-      <c r="D28" s="240"/>
-      <c r="E28" s="240"/>
-      <c r="F28" s="240"/>
-      <c r="G28" s="240"/>
-      <c r="H28" s="240"/>
-      <c r="I28" s="240"/>
-      <c r="J28" s="240"/>
-      <c r="K28" s="240"/>
-      <c r="L28" s="241"/>
+      <c r="C28" s="267"/>
+      <c r="D28" s="267"/>
+      <c r="E28" s="267"/>
+      <c r="F28" s="267"/>
+      <c r="G28" s="267"/>
+      <c r="H28" s="267"/>
+      <c r="I28" s="267"/>
+      <c r="J28" s="267"/>
+      <c r="K28" s="267"/>
+      <c r="L28" s="268"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="230">
         <v>3</v>
       </c>
-      <c r="B29" s="240" t="s">
+      <c r="B29" s="267" t="s">
         <v>336</v>
       </c>
-      <c r="C29" s="240"/>
-      <c r="D29" s="240"/>
-      <c r="E29" s="240"/>
-      <c r="F29" s="240"/>
-      <c r="G29" s="240"/>
-      <c r="H29" s="240"/>
-      <c r="I29" s="240"/>
-      <c r="J29" s="240"/>
-      <c r="K29" s="240"/>
-      <c r="L29" s="241"/>
+      <c r="C29" s="267"/>
+      <c r="D29" s="267"/>
+      <c r="E29" s="267"/>
+      <c r="F29" s="267"/>
+      <c r="G29" s="267"/>
+      <c r="H29" s="267"/>
+      <c r="I29" s="267"/>
+      <c r="J29" s="267"/>
+      <c r="K29" s="267"/>
+      <c r="L29" s="268"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="230">
         <v>4</v>
       </c>
-      <c r="B30" s="240" t="s">
+      <c r="B30" s="267" t="s">
         <v>359</v>
       </c>
-      <c r="C30" s="240"/>
-      <c r="D30" s="240"/>
-      <c r="E30" s="240"/>
-      <c r="F30" s="240"/>
-      <c r="G30" s="240"/>
-      <c r="H30" s="240"/>
-      <c r="I30" s="240"/>
-      <c r="J30" s="240"/>
-      <c r="K30" s="240"/>
-      <c r="L30" s="241"/>
+      <c r="C30" s="267"/>
+      <c r="D30" s="267"/>
+      <c r="E30" s="267"/>
+      <c r="F30" s="267"/>
+      <c r="G30" s="267"/>
+      <c r="H30" s="267"/>
+      <c r="I30" s="267"/>
+      <c r="J30" s="267"/>
+      <c r="K30" s="267"/>
+      <c r="L30" s="268"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="230">
         <v>5</v>
       </c>
-      <c r="B31" s="238" t="s">
+      <c r="B31" s="265" t="s">
         <v>337</v>
       </c>
-      <c r="C31" s="238"/>
-      <c r="D31" s="238"/>
-      <c r="E31" s="238"/>
-      <c r="F31" s="238"/>
-      <c r="G31" s="238"/>
-      <c r="H31" s="238"/>
-      <c r="I31" s="238"/>
-      <c r="J31" s="238"/>
-      <c r="K31" s="238"/>
-      <c r="L31" s="239"/>
+      <c r="C31" s="265"/>
+      <c r="D31" s="265"/>
+      <c r="E31" s="265"/>
+      <c r="F31" s="265"/>
+      <c r="G31" s="265"/>
+      <c r="H31" s="265"/>
+      <c r="I31" s="265"/>
+      <c r="J31" s="265"/>
+      <c r="K31" s="265"/>
+      <c r="L31" s="266"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="230">
         <v>6</v>
       </c>
-      <c r="B32" s="238" t="s">
+      <c r="B32" s="265" t="s">
         <v>342</v>
       </c>
-      <c r="C32" s="238"/>
-      <c r="D32" s="238"/>
-      <c r="E32" s="238"/>
-      <c r="F32" s="238"/>
-      <c r="G32" s="238"/>
-      <c r="H32" s="238"/>
-      <c r="I32" s="238"/>
-      <c r="J32" s="238"/>
-      <c r="K32" s="238"/>
-      <c r="L32" s="239"/>
+      <c r="C32" s="265"/>
+      <c r="D32" s="265"/>
+      <c r="E32" s="265"/>
+      <c r="F32" s="265"/>
+      <c r="G32" s="265"/>
+      <c r="H32" s="265"/>
+      <c r="I32" s="265"/>
+      <c r="J32" s="265"/>
+      <c r="K32" s="265"/>
+      <c r="L32" s="266"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="230">
         <v>7</v>
       </c>
-      <c r="B33" s="240" t="s">
+      <c r="B33" s="267" t="s">
         <v>338</v>
       </c>
-      <c r="C33" s="240"/>
-      <c r="D33" s="240"/>
-      <c r="E33" s="240"/>
-      <c r="F33" s="240"/>
-      <c r="G33" s="240"/>
-      <c r="H33" s="240"/>
-      <c r="I33" s="240"/>
-      <c r="J33" s="240"/>
-      <c r="K33" s="240"/>
-      <c r="L33" s="241"/>
+      <c r="C33" s="267"/>
+      <c r="D33" s="267"/>
+      <c r="E33" s="267"/>
+      <c r="F33" s="267"/>
+      <c r="G33" s="267"/>
+      <c r="H33" s="267"/>
+      <c r="I33" s="267"/>
+      <c r="J33" s="267"/>
+      <c r="K33" s="267"/>
+      <c r="L33" s="268"/>
     </row>
     <row r="34" spans="1:12" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="230"/>
@@ -15448,56 +15460,56 @@
       <c r="L34" s="232"/>
     </row>
     <row r="35" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="249" t="s">
+      <c r="A35" s="269" t="s">
         <v>341</v>
       </c>
-      <c r="B35" s="250"/>
-      <c r="C35" s="250"/>
-      <c r="D35" s="250"/>
-      <c r="E35" s="250"/>
-      <c r="F35" s="250"/>
-      <c r="G35" s="250"/>
-      <c r="H35" s="250"/>
-      <c r="I35" s="250"/>
-      <c r="J35" s="250"/>
-      <c r="K35" s="250"/>
-      <c r="L35" s="251"/>
+      <c r="B35" s="270"/>
+      <c r="C35" s="270"/>
+      <c r="D35" s="270"/>
+      <c r="E35" s="270"/>
+      <c r="F35" s="270"/>
+      <c r="G35" s="270"/>
+      <c r="H35" s="270"/>
+      <c r="I35" s="270"/>
+      <c r="J35" s="270"/>
+      <c r="K35" s="270"/>
+      <c r="L35" s="271"/>
     </row>
     <row r="36" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="233" t="s">
         <v>339</v>
       </c>
-      <c r="B36" s="240" t="s">
+      <c r="B36" s="267" t="s">
         <v>224</v>
       </c>
-      <c r="C36" s="240"/>
-      <c r="D36" s="240"/>
-      <c r="E36" s="240"/>
-      <c r="F36" s="240"/>
-      <c r="G36" s="240"/>
-      <c r="H36" s="240"/>
-      <c r="I36" s="240"/>
-      <c r="J36" s="240"/>
-      <c r="K36" s="240"/>
-      <c r="L36" s="241"/>
+      <c r="C36" s="267"/>
+      <c r="D36" s="267"/>
+      <c r="E36" s="267"/>
+      <c r="F36" s="267"/>
+      <c r="G36" s="267"/>
+      <c r="H36" s="267"/>
+      <c r="I36" s="267"/>
+      <c r="J36" s="267"/>
+      <c r="K36" s="267"/>
+      <c r="L36" s="268"/>
     </row>
     <row r="37" spans="1:12" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="234" t="s">
         <v>340</v>
       </c>
-      <c r="B37" s="242" t="s">
+      <c r="B37" s="273" t="s">
         <v>343</v>
       </c>
-      <c r="C37" s="242"/>
-      <c r="D37" s="242"/>
-      <c r="E37" s="242"/>
-      <c r="F37" s="242"/>
-      <c r="G37" s="242"/>
-      <c r="H37" s="242"/>
-      <c r="I37" s="242"/>
-      <c r="J37" s="242"/>
-      <c r="K37" s="242"/>
-      <c r="L37" s="243"/>
+      <c r="C37" s="273"/>
+      <c r="D37" s="273"/>
+      <c r="E37" s="273"/>
+      <c r="F37" s="273"/>
+      <c r="G37" s="273"/>
+      <c r="H37" s="273"/>
+      <c r="I37" s="273"/>
+      <c r="J37" s="273"/>
+      <c r="K37" s="273"/>
+      <c r="L37" s="274"/>
     </row>
     <row r="38" spans="1:12" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="161"/>
@@ -15514,20 +15526,20 @@
       <c r="L38" s="113"/>
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="244" t="s">
+      <c r="A39" s="275" t="s">
         <v>252</v>
       </c>
-      <c r="B39" s="245"/>
-      <c r="C39" s="245"/>
-      <c r="D39" s="245"/>
-      <c r="E39" s="245"/>
-      <c r="F39" s="245"/>
-      <c r="G39" s="245"/>
-      <c r="H39" s="245"/>
-      <c r="I39" s="245"/>
-      <c r="J39" s="245"/>
-      <c r="K39" s="245"/>
-      <c r="L39" s="246"/>
+      <c r="B39" s="276"/>
+      <c r="C39" s="276"/>
+      <c r="D39" s="276"/>
+      <c r="E39" s="276"/>
+      <c r="F39" s="276"/>
+      <c r="G39" s="276"/>
+      <c r="H39" s="276"/>
+      <c r="I39" s="276"/>
+      <c r="J39" s="276"/>
+      <c r="K39" s="276"/>
+      <c r="L39" s="277"/>
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="162" t="s">
@@ -15615,72 +15627,72 @@
       <c r="B45" s="170" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="247" t="s">
+      <c r="C45" s="255" t="s">
         <v>326</v>
       </c>
-      <c r="D45" s="247"/>
-      <c r="E45" s="247"/>
-      <c r="F45" s="247"/>
-      <c r="G45" s="247"/>
-      <c r="H45" s="247"/>
-      <c r="I45" s="247"/>
-      <c r="J45" s="247"/>
-      <c r="K45" s="247"/>
-      <c r="L45" s="248"/>
+      <c r="D45" s="255"/>
+      <c r="E45" s="255"/>
+      <c r="F45" s="255"/>
+      <c r="G45" s="255"/>
+      <c r="H45" s="255"/>
+      <c r="I45" s="255"/>
+      <c r="J45" s="255"/>
+      <c r="K45" s="255"/>
+      <c r="L45" s="256"/>
     </row>
     <row r="46" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="169"/>
       <c r="B46" s="170" t="s">
         <v>146</v>
       </c>
-      <c r="C46" s="247" t="s">
+      <c r="C46" s="255" t="s">
         <v>147</v>
       </c>
-      <c r="D46" s="247"/>
-      <c r="E46" s="247"/>
-      <c r="F46" s="247"/>
-      <c r="G46" s="247"/>
-      <c r="H46" s="247"/>
-      <c r="I46" s="247"/>
-      <c r="J46" s="247"/>
-      <c r="K46" s="247"/>
-      <c r="L46" s="248"/>
+      <c r="D46" s="255"/>
+      <c r="E46" s="255"/>
+      <c r="F46" s="255"/>
+      <c r="G46" s="255"/>
+      <c r="H46" s="255"/>
+      <c r="I46" s="255"/>
+      <c r="J46" s="255"/>
+      <c r="K46" s="255"/>
+      <c r="L46" s="256"/>
     </row>
     <row r="47" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="169"/>
       <c r="B47" s="170" t="s">
         <v>250</v>
       </c>
-      <c r="C47" s="247" t="s">
+      <c r="C47" s="255" t="s">
         <v>251</v>
       </c>
-      <c r="D47" s="247"/>
-      <c r="E47" s="247"/>
-      <c r="F47" s="247"/>
-      <c r="G47" s="247"/>
-      <c r="H47" s="247"/>
-      <c r="I47" s="247"/>
-      <c r="J47" s="247"/>
-      <c r="K47" s="247"/>
-      <c r="L47" s="248"/>
+      <c r="D47" s="255"/>
+      <c r="E47" s="255"/>
+      <c r="F47" s="255"/>
+      <c r="G47" s="255"/>
+      <c r="H47" s="255"/>
+      <c r="I47" s="255"/>
+      <c r="J47" s="255"/>
+      <c r="K47" s="255"/>
+      <c r="L47" s="256"/>
     </row>
     <row r="48" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="169"/>
       <c r="B48" s="170" t="s">
         <v>327</v>
       </c>
-      <c r="C48" s="247" t="s">
+      <c r="C48" s="255" t="s">
         <v>328</v>
       </c>
-      <c r="D48" s="247"/>
-      <c r="E48" s="247"/>
-      <c r="F48" s="247"/>
-      <c r="G48" s="247"/>
-      <c r="H48" s="247"/>
-      <c r="I48" s="247"/>
-      <c r="J48" s="247"/>
-      <c r="K48" s="247"/>
-      <c r="L48" s="248"/>
+      <c r="D48" s="255"/>
+      <c r="E48" s="255"/>
+      <c r="F48" s="255"/>
+      <c r="G48" s="255"/>
+      <c r="H48" s="255"/>
+      <c r="I48" s="255"/>
+      <c r="J48" s="255"/>
+      <c r="K48" s="255"/>
+      <c r="L48" s="256"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="169"/>
@@ -15705,18 +15717,18 @@
       <c r="B50" s="170" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="247" t="s">
+      <c r="C50" s="255" t="s">
         <v>330</v>
       </c>
-      <c r="D50" s="247"/>
-      <c r="E50" s="247"/>
-      <c r="F50" s="247"/>
-      <c r="G50" s="247"/>
-      <c r="H50" s="247"/>
-      <c r="I50" s="247"/>
-      <c r="J50" s="247"/>
-      <c r="K50" s="247"/>
-      <c r="L50" s="248"/>
+      <c r="D50" s="255"/>
+      <c r="E50" s="255"/>
+      <c r="F50" s="255"/>
+      <c r="G50" s="255"/>
+      <c r="H50" s="255"/>
+      <c r="I50" s="255"/>
+      <c r="J50" s="255"/>
+      <c r="K50" s="255"/>
+      <c r="L50" s="256"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="169"/>
@@ -15798,25 +15810,51 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="237" t="s">
+      <c r="A64" s="272" t="s">
         <v>332</v>
       </c>
-      <c r="B64" s="237"/>
-      <c r="C64" s="237"/>
-      <c r="D64" s="237"/>
-      <c r="E64" s="237"/>
-      <c r="F64" s="237"/>
-      <c r="G64" s="237"/>
-      <c r="H64" s="237"/>
-      <c r="I64" s="237"/>
-      <c r="J64" s="237"/>
-      <c r="K64" s="237"/>
-      <c r="L64" s="237"/>
+      <c r="B64" s="272"/>
+      <c r="C64" s="272"/>
+      <c r="D64" s="272"/>
+      <c r="E64" s="272"/>
+      <c r="F64" s="272"/>
+      <c r="G64" s="272"/>
+      <c r="H64" s="272"/>
+      <c r="I64" s="272"/>
+      <c r="J64" s="272"/>
+      <c r="K64" s="272"/>
+      <c r="L64" s="272"/>
     </row>
     <row r="69" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="70" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A64:L64"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="C45:L45"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="C48:L48"/>
+    <mergeCell ref="C50:L50"/>
+    <mergeCell ref="A35:L35"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B18:L18"/>
+    <mergeCell ref="B19:L19"/>
+    <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="B22:L22"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="B26:L26"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B30:L30"/>
     <mergeCell ref="A17:L17"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A4:L4"/>
@@ -15831,32 +15869,6 @@
     <mergeCell ref="A16:L16"/>
     <mergeCell ref="B7:L7"/>
     <mergeCell ref="B8:L8"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B18:L18"/>
-    <mergeCell ref="B19:L19"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="B22:L22"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="B24:L24"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="B26:L26"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="A64:L64"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="C45:L45"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="C47:L47"/>
-    <mergeCell ref="C48:L48"/>
-    <mergeCell ref="C50:L50"/>
-    <mergeCell ref="A35:L35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A57" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -16514,8 +16526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BF7D8F-86F3-47E9-AB85-EE9B4CAB70E4}">
   <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16794,7 +16806,7 @@
       <c r="E21" s="28"/>
       <c r="F21" s="116"/>
       <c r="N21" s="141" t="s">
-        <v>183</v>
+        <v>361</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
@@ -16824,7 +16836,7 @@
       <c r="D23" s="111"/>
       <c r="E23" s="28"/>
       <c r="N23" s="141" t="s">
-        <v>184</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
@@ -16925,8 +16937,8 @@
       <c r="J28" s="97"/>
       <c r="K28" s="97"/>
       <c r="L28" s="97"/>
-      <c r="N28" s="139" t="s">
-        <v>186</v>
+      <c r="N28" s="141" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
@@ -17610,7 +17622,7 @@
         <v/>
       </c>
       <c r="N45" s="141" t="s">
-        <v>191</v>
+        <v>363</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.35">
@@ -21236,17 +21248,17 @@
     <hyperlink ref="N18" r:id="rId3" location="i-evaporation-rates" xr:uid="{23C61350-606E-472B-90E1-88574D6741EE}"/>
     <hyperlink ref="N19" r:id="rId4" location="ii-start-storage" xr:uid="{692C3AE6-515B-4C08-B6EC-0557E75E9511}"/>
     <hyperlink ref="N20" r:id="rId5" location="iii-protection-elevations" xr:uid="{16CC5ED4-0369-416C-AC3E-3AD6F831A454}"/>
-    <hyperlink ref="N21" r:id="rId6" location="iv-the-protection-volumes" xr:uid="{D7802E8D-5298-4564-9936-B3226B6E96DA}"/>
-    <hyperlink ref="N22" r:id="rId7" location="v-prior-9-year-lake-powell-release" display="Help 9-year prior Powell release" xr:uid="{9E773CCF-F296-48D2-ADA9-5456ABC7F062}"/>
-    <hyperlink ref="N23" r:id="rId8" location="vi-prior-9-year-paria-river-flow" xr:uid="{8CAE8559-5BD9-4D9F-8655-D1F3AE1FCD4D}"/>
+    <hyperlink ref="N21" r:id="rId6" location="iv-storage-above-protect-zone" display="Help protect volume" xr:uid="{D7802E8D-5298-4564-9936-B3226B6E96DA}"/>
+    <hyperlink ref="N22" r:id="rId7" location="v-water-conservation-program-ics-total-balance" xr:uid="{9E773CCF-F296-48D2-ADA9-5456ABC7F062}"/>
+    <hyperlink ref="N23" r:id="rId8" location="vi-remaining-storage-above-the-protect-and-ics-balances" xr:uid="{8CAE8559-5BD9-4D9F-8655-D1F3AE1FCD4D}"/>
     <hyperlink ref="N24" r:id="rId9" location="vii-delivery-to-meet-10-year-requirement" xr:uid="{B6DDA7AA-2218-4D2F-9A7A-A0EDBEFDC5B1}"/>
-    <hyperlink ref="N28" r:id="rId10" location="step-2-specify-natural-inflow-to-lake-powell" xr:uid="{78DF76B4-BE79-4AC1-9F08-EC86A0A72F91}"/>
+    <hyperlink ref="N28" r:id="rId10" location="step-2-specify-natural-inflow-to-lake-powell" display="Help Lake Mead inflow" xr:uid="{78DF76B4-BE79-4AC1-9F08-EC86A0A72F91}"/>
     <hyperlink ref="N29" r:id="rId11" location="2a-intervening-grand-canyon-flow" xr:uid="{CFD884C0-2149-42F6-AD5A-482CF40D5292}"/>
     <hyperlink ref="N30" r:id="rId12" location="2b-mead-to-imperial-dam-intervening-flow" xr:uid="{B8EF30C2-739D-4E21-B63A-F17F9947326A}"/>
     <hyperlink ref="N31" r:id="rId13" location="2c-havasuparker-evaporation-and-evapotranspiration" xr:uid="{70E7AC6A-42AC-4DE1-ADFB-FBA8230C308E}"/>
     <hyperlink ref="N35" r:id="rId14" location="step-3-split-existing-reservoir-storage-among-accounts-year-1-only" xr:uid="{B36B453C-62F8-4461-8E49-8546C848C695}"/>
-    <hyperlink ref="N42" r:id="rId15" location="3a-begin-of-year-reservoir-storage" display="Help begin year storage" xr:uid="{52EB1038-72CB-4676-AD3B-3DD4322D2D3C}"/>
-    <hyperlink ref="N45" r:id="rId16" location="3b-calculate-powell--mead-evaporation" xr:uid="{9002111C-2D36-45B1-97D8-5FCB363BD9BD}"/>
+    <hyperlink ref="N42" r:id="rId15" location="3a-begin-of-year-reservoir-storage" xr:uid="{52EB1038-72CB-4676-AD3B-3DD4322D2D3C}"/>
+    <hyperlink ref="N45" r:id="rId16" location="3b-calculate-powell--mead-evaporation" display="Help Powell + Mead evaporation" xr:uid="{9002111C-2D36-45B1-97D8-5FCB363BD9BD}"/>
     <hyperlink ref="N52" r:id="rId17" location="3c-calculate-mexico-water-allocation" xr:uid="{C14FC6B3-6E3C-48F5-B820-A74ADC9C86D6}"/>
     <hyperlink ref="N53" r:id="rId18" location="split-combined-natural-inflow-among-accounts" xr:uid="{63C31A0C-C046-4C6B-B63E-AA3031EC5E49}"/>
     <hyperlink ref="N63" r:id="rId19" location="step-5-participant-dashboards--conserve-consume-and-trade" xr:uid="{E1DA626C-61A5-4CB7-94B9-52C34A1556D5}"/>
@@ -22689,16 +22701,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="313" t="e">
+      <c r="A1" s="312" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="313"/>
-      <c r="C1" s="313"/>
-      <c r="D1" s="313"/>
-      <c r="E1" s="313"/>
-      <c r="F1" s="313"/>
-      <c r="G1" s="313"/>
+      <c r="B1" s="312"/>
+      <c r="C1" s="312"/>
+      <c r="D1" s="312"/>
+      <c r="E1" s="312"/>
+      <c r="F1" s="312"/>
+      <c r="G1" s="312"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -22807,11 +22819,11 @@
         <v>81</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="312"/>
-      <c r="D10" s="312"/>
-      <c r="E10" s="312"/>
-      <c r="F10" s="312"/>
-      <c r="G10" s="312"/>
+      <c r="C10" s="313"/>
+      <c r="D10" s="313"/>
+      <c r="E10" s="313"/>
+      <c r="F10" s="313"/>
+      <c r="G10" s="313"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -24074,12 +24086,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -24087,6 +24093,12 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>

</xml_diff>

<commit_message>
Finish Lake Mead Inflow and Split Reservoir storage in Help Guide
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADD2E151-0182-4BED-A2C0-F9BAD1D5E18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CBA8FD-B884-44C3-BA51-D98355CA9D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -3197,6 +3197,51 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3251,12 +3296,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3280,45 +3319,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3422,11 +3422,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14866,20 +14866,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="240" t="s">
+      <c r="A1" s="255" t="s">
         <v>321</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
+      <c r="B1" s="255"/>
+      <c r="C1" s="255"/>
+      <c r="D1" s="255"/>
+      <c r="E1" s="255"/>
+      <c r="F1" s="255"/>
+      <c r="G1" s="255"/>
+      <c r="H1" s="255"/>
+      <c r="I1" s="255"/>
+      <c r="J1" s="255"/>
+      <c r="K1" s="255"/>
+      <c r="L1" s="255"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -14905,41 +14905,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="241" t="s">
+      <c r="A4" s="256" t="s">
         <v>349</v>
       </c>
-      <c r="B4" s="242"/>
-      <c r="C4" s="242"/>
-      <c r="D4" s="242"/>
-      <c r="E4" s="242"/>
-      <c r="F4" s="242"/>
-      <c r="G4" s="242"/>
-      <c r="H4" s="242"/>
-      <c r="I4" s="242"/>
-      <c r="J4" s="242"/>
-      <c r="K4" s="242"/>
-      <c r="L4" s="243"/>
-      <c r="N4" s="244"/>
-      <c r="O4" s="244"/>
-      <c r="P4" s="244"/>
-      <c r="Q4" s="244"/>
-      <c r="R4" s="244"/>
+      <c r="B4" s="257"/>
+      <c r="C4" s="257"/>
+      <c r="D4" s="257"/>
+      <c r="E4" s="257"/>
+      <c r="F4" s="257"/>
+      <c r="G4" s="257"/>
+      <c r="H4" s="257"/>
+      <c r="I4" s="257"/>
+      <c r="J4" s="257"/>
+      <c r="K4" s="257"/>
+      <c r="L4" s="258"/>
+      <c r="N4" s="259"/>
+      <c r="O4" s="259"/>
+      <c r="P4" s="259"/>
+      <c r="Q4" s="259"/>
+      <c r="R4" s="259"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="245" t="s">
+      <c r="A5" s="260" t="s">
         <v>350</v>
       </c>
-      <c r="B5" s="246"/>
-      <c r="C5" s="246"/>
-      <c r="D5" s="246"/>
-      <c r="E5" s="246"/>
-      <c r="F5" s="246"/>
-      <c r="G5" s="246"/>
-      <c r="H5" s="246"/>
-      <c r="I5" s="246"/>
-      <c r="J5" s="246"/>
-      <c r="K5" s="246"/>
-      <c r="L5" s="247"/>
+      <c r="B5" s="261"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
+      <c r="G5" s="261"/>
+      <c r="H5" s="261"/>
+      <c r="I5" s="261"/>
+      <c r="J5" s="261"/>
+      <c r="K5" s="261"/>
+      <c r="L5" s="262"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -14947,20 +14947,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="245" t="s">
+      <c r="A6" s="260" t="s">
         <v>352</v>
       </c>
-      <c r="B6" s="246"/>
-      <c r="C6" s="246"/>
-      <c r="D6" s="246"/>
-      <c r="E6" s="246"/>
-      <c r="F6" s="246"/>
-      <c r="G6" s="246"/>
-      <c r="H6" s="246"/>
-      <c r="I6" s="246"/>
-      <c r="J6" s="246"/>
-      <c r="K6" s="246"/>
-      <c r="L6" s="247"/>
+      <c r="B6" s="261"/>
+      <c r="C6" s="261"/>
+      <c r="D6" s="261"/>
+      <c r="E6" s="261"/>
+      <c r="F6" s="261"/>
+      <c r="G6" s="261"/>
+      <c r="H6" s="261"/>
+      <c r="I6" s="261"/>
+      <c r="J6" s="261"/>
+      <c r="K6" s="261"/>
+      <c r="L6" s="262"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -14969,19 +14969,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="235"/>
-      <c r="B7" s="246" t="s">
+      <c r="B7" s="261" t="s">
         <v>353</v>
       </c>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246"/>
-      <c r="K7" s="246"/>
-      <c r="L7" s="247"/>
+      <c r="C7" s="261"/>
+      <c r="D7" s="261"/>
+      <c r="E7" s="261"/>
+      <c r="F7" s="261"/>
+      <c r="G7" s="261"/>
+      <c r="H7" s="261"/>
+      <c r="I7" s="261"/>
+      <c r="J7" s="261"/>
+      <c r="K7" s="261"/>
+      <c r="L7" s="262"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -14990,19 +14990,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="236"/>
-      <c r="B8" s="263" t="s">
+      <c r="B8" s="276" t="s">
         <v>354</v>
       </c>
-      <c r="C8" s="263"/>
-      <c r="D8" s="263"/>
-      <c r="E8" s="263"/>
-      <c r="F8" s="263"/>
-      <c r="G8" s="263"/>
-      <c r="H8" s="263"/>
-      <c r="I8" s="263"/>
-      <c r="J8" s="263"/>
-      <c r="K8" s="263"/>
-      <c r="L8" s="264"/>
+      <c r="C8" s="276"/>
+      <c r="D8" s="276"/>
+      <c r="E8" s="276"/>
+      <c r="F8" s="276"/>
+      <c r="G8" s="276"/>
+      <c r="H8" s="276"/>
+      <c r="I8" s="276"/>
+      <c r="J8" s="276"/>
+      <c r="K8" s="276"/>
+      <c r="L8" s="277"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15024,84 +15024,84 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="248" t="s">
+      <c r="A10" s="263" t="s">
         <v>217</v>
       </c>
-      <c r="B10" s="249"/>
-      <c r="C10" s="249"/>
-      <c r="D10" s="249"/>
-      <c r="E10" s="249"/>
-      <c r="F10" s="249"/>
-      <c r="G10" s="249"/>
-      <c r="H10" s="249"/>
-      <c r="I10" s="249"/>
-      <c r="J10" s="249"/>
-      <c r="K10" s="249"/>
-      <c r="L10" s="250"/>
+      <c r="B10" s="264"/>
+      <c r="C10" s="264"/>
+      <c r="D10" s="264"/>
+      <c r="E10" s="264"/>
+      <c r="F10" s="264"/>
+      <c r="G10" s="264"/>
+      <c r="H10" s="264"/>
+      <c r="I10" s="264"/>
+      <c r="J10" s="264"/>
+      <c r="K10" s="264"/>
+      <c r="L10" s="265"/>
     </row>
     <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="251" t="s">
+      <c r="A11" s="266" t="s">
         <v>351</v>
       </c>
-      <c r="B11" s="252"/>
-      <c r="C11" s="252"/>
-      <c r="D11" s="252"/>
-      <c r="E11" s="252"/>
-      <c r="F11" s="252"/>
-      <c r="G11" s="252"/>
-      <c r="H11" s="252"/>
-      <c r="I11" s="252"/>
-      <c r="J11" s="252"/>
-      <c r="K11" s="252"/>
-      <c r="L11" s="253"/>
+      <c r="B11" s="267"/>
+      <c r="C11" s="267"/>
+      <c r="D11" s="267"/>
+      <c r="E11" s="267"/>
+      <c r="F11" s="267"/>
+      <c r="G11" s="267"/>
+      <c r="H11" s="267"/>
+      <c r="I11" s="267"/>
+      <c r="J11" s="267"/>
+      <c r="K11" s="267"/>
+      <c r="L11" s="268"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="254" t="s">
+      <c r="A12" s="269" t="s">
         <v>355</v>
       </c>
-      <c r="B12" s="255"/>
-      <c r="C12" s="255"/>
-      <c r="D12" s="255"/>
-      <c r="E12" s="255"/>
-      <c r="F12" s="255"/>
-      <c r="G12" s="255"/>
-      <c r="H12" s="255"/>
-      <c r="I12" s="255"/>
-      <c r="J12" s="255"/>
-      <c r="K12" s="255"/>
-      <c r="L12" s="256"/>
+      <c r="B12" s="247"/>
+      <c r="C12" s="247"/>
+      <c r="D12" s="247"/>
+      <c r="E12" s="247"/>
+      <c r="F12" s="247"/>
+      <c r="G12" s="247"/>
+      <c r="H12" s="247"/>
+      <c r="I12" s="247"/>
+      <c r="J12" s="247"/>
+      <c r="K12" s="247"/>
+      <c r="L12" s="248"/>
     </row>
     <row r="13" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="254" t="s">
+      <c r="A13" s="269" t="s">
         <v>218</v>
       </c>
-      <c r="B13" s="255"/>
-      <c r="C13" s="255"/>
-      <c r="D13" s="255"/>
-      <c r="E13" s="255"/>
-      <c r="F13" s="255"/>
-      <c r="G13" s="255"/>
-      <c r="H13" s="255"/>
-      <c r="I13" s="255"/>
-      <c r="J13" s="255"/>
-      <c r="K13" s="255"/>
-      <c r="L13" s="256"/>
+      <c r="B13" s="247"/>
+      <c r="C13" s="247"/>
+      <c r="D13" s="247"/>
+      <c r="E13" s="247"/>
+      <c r="F13" s="247"/>
+      <c r="G13" s="247"/>
+      <c r="H13" s="247"/>
+      <c r="I13" s="247"/>
+      <c r="J13" s="247"/>
+      <c r="K13" s="247"/>
+      <c r="L13" s="248"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="257" t="s">
+      <c r="A14" s="270" t="s">
         <v>356</v>
       </c>
-      <c r="B14" s="258"/>
-      <c r="C14" s="258"/>
-      <c r="D14" s="258"/>
-      <c r="E14" s="258"/>
-      <c r="F14" s="258"/>
-      <c r="G14" s="258"/>
-      <c r="H14" s="258"/>
-      <c r="I14" s="258"/>
-      <c r="J14" s="258"/>
-      <c r="K14" s="258"/>
-      <c r="L14" s="259"/>
+      <c r="B14" s="271"/>
+      <c r="C14" s="271"/>
+      <c r="D14" s="271"/>
+      <c r="E14" s="271"/>
+      <c r="F14" s="271"/>
+      <c r="G14" s="271"/>
+      <c r="H14" s="271"/>
+      <c r="I14" s="271"/>
+      <c r="J14" s="271"/>
+      <c r="K14" s="271"/>
+      <c r="L14" s="272"/>
     </row>
     <row r="15" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="113"/>
@@ -15118,332 +15118,332 @@
       <c r="L15" s="113"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="260" t="s">
+      <c r="A16" s="273" t="s">
         <v>348</v>
       </c>
-      <c r="B16" s="261"/>
-      <c r="C16" s="261"/>
-      <c r="D16" s="261"/>
-      <c r="E16" s="261"/>
-      <c r="F16" s="261"/>
-      <c r="G16" s="261"/>
-      <c r="H16" s="261"/>
-      <c r="I16" s="261"/>
-      <c r="J16" s="261"/>
-      <c r="K16" s="261"/>
-      <c r="L16" s="262"/>
+      <c r="B16" s="274"/>
+      <c r="C16" s="274"/>
+      <c r="D16" s="274"/>
+      <c r="E16" s="274"/>
+      <c r="F16" s="274"/>
+      <c r="G16" s="274"/>
+      <c r="H16" s="274"/>
+      <c r="I16" s="274"/>
+      <c r="J16" s="274"/>
+      <c r="K16" s="274"/>
+      <c r="L16" s="275"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="237" t="s">
+      <c r="A17" s="252" t="s">
         <v>227</v>
       </c>
-      <c r="B17" s="238"/>
-      <c r="C17" s="238"/>
-      <c r="D17" s="238"/>
-      <c r="E17" s="238"/>
-      <c r="F17" s="238"/>
-      <c r="G17" s="238"/>
-      <c r="H17" s="238"/>
-      <c r="I17" s="238"/>
-      <c r="J17" s="238"/>
-      <c r="K17" s="238"/>
-      <c r="L17" s="239"/>
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="253"/>
+      <c r="J17" s="253"/>
+      <c r="K17" s="253"/>
+      <c r="L17" s="254"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="230">
         <v>1</v>
       </c>
-      <c r="B18" s="267" t="s">
+      <c r="B18" s="240" t="s">
         <v>226</v>
       </c>
-      <c r="C18" s="267"/>
-      <c r="D18" s="267"/>
-      <c r="E18" s="267"/>
-      <c r="F18" s="267"/>
-      <c r="G18" s="267"/>
-      <c r="H18" s="267"/>
-      <c r="I18" s="267"/>
-      <c r="J18" s="267"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="268"/>
+      <c r="C18" s="240"/>
+      <c r="D18" s="240"/>
+      <c r="E18" s="240"/>
+      <c r="F18" s="240"/>
+      <c r="G18" s="240"/>
+      <c r="H18" s="240"/>
+      <c r="I18" s="240"/>
+      <c r="J18" s="240"/>
+      <c r="K18" s="240"/>
+      <c r="L18" s="241"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="230">
         <v>2</v>
       </c>
-      <c r="B19" s="267" t="s">
+      <c r="B19" s="240" t="s">
         <v>344</v>
       </c>
-      <c r="C19" s="267"/>
-      <c r="D19" s="267"/>
-      <c r="E19" s="267"/>
-      <c r="F19" s="267"/>
-      <c r="G19" s="267"/>
-      <c r="H19" s="267"/>
-      <c r="I19" s="267"/>
-      <c r="J19" s="267"/>
-      <c r="K19" s="267"/>
-      <c r="L19" s="268"/>
+      <c r="C19" s="240"/>
+      <c r="D19" s="240"/>
+      <c r="E19" s="240"/>
+      <c r="F19" s="240"/>
+      <c r="G19" s="240"/>
+      <c r="H19" s="240"/>
+      <c r="I19" s="240"/>
+      <c r="J19" s="240"/>
+      <c r="K19" s="240"/>
+      <c r="L19" s="241"/>
       <c r="N19" s="106"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="230">
         <v>3</v>
       </c>
-      <c r="B20" s="267" t="s">
+      <c r="B20" s="240" t="s">
         <v>219</v>
       </c>
-      <c r="C20" s="267"/>
-      <c r="D20" s="267"/>
-      <c r="E20" s="267"/>
-      <c r="F20" s="267"/>
-      <c r="G20" s="267"/>
-      <c r="H20" s="267"/>
-      <c r="I20" s="267"/>
-      <c r="J20" s="267"/>
-      <c r="K20" s="267"/>
-      <c r="L20" s="268"/>
+      <c r="C20" s="240"/>
+      <c r="D20" s="240"/>
+      <c r="E20" s="240"/>
+      <c r="F20" s="240"/>
+      <c r="G20" s="240"/>
+      <c r="H20" s="240"/>
+      <c r="I20" s="240"/>
+      <c r="J20" s="240"/>
+      <c r="K20" s="240"/>
+      <c r="L20" s="241"/>
       <c r="N20" s="106"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="230">
         <v>4</v>
       </c>
-      <c r="B21" s="267" t="s">
+      <c r="B21" s="240" t="s">
         <v>357</v>
       </c>
-      <c r="C21" s="267"/>
-      <c r="D21" s="267"/>
-      <c r="E21" s="267"/>
-      <c r="F21" s="267"/>
-      <c r="G21" s="267"/>
-      <c r="H21" s="267"/>
-      <c r="I21" s="267"/>
-      <c r="J21" s="267"/>
-      <c r="K21" s="267"/>
-      <c r="L21" s="268"/>
+      <c r="C21" s="240"/>
+      <c r="D21" s="240"/>
+      <c r="E21" s="240"/>
+      <c r="F21" s="240"/>
+      <c r="G21" s="240"/>
+      <c r="H21" s="240"/>
+      <c r="I21" s="240"/>
+      <c r="J21" s="240"/>
+      <c r="K21" s="240"/>
+      <c r="L21" s="241"/>
       <c r="N21" s="106"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="230">
         <v>5</v>
       </c>
-      <c r="B22" s="267" t="s">
+      <c r="B22" s="240" t="s">
         <v>220</v>
       </c>
-      <c r="C22" s="267"/>
-      <c r="D22" s="267"/>
-      <c r="E22" s="267"/>
-      <c r="F22" s="267"/>
-      <c r="G22" s="267"/>
-      <c r="H22" s="267"/>
-      <c r="I22" s="267"/>
-      <c r="J22" s="267"/>
-      <c r="K22" s="267"/>
-      <c r="L22" s="268"/>
+      <c r="C22" s="240"/>
+      <c r="D22" s="240"/>
+      <c r="E22" s="240"/>
+      <c r="F22" s="240"/>
+      <c r="G22" s="240"/>
+      <c r="H22" s="240"/>
+      <c r="I22" s="240"/>
+      <c r="J22" s="240"/>
+      <c r="K22" s="240"/>
+      <c r="L22" s="241"/>
       <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="230"/>
-      <c r="B23" s="267" t="s">
+      <c r="B23" s="240" t="s">
         <v>221</v>
       </c>
-      <c r="C23" s="267"/>
-      <c r="D23" s="267"/>
-      <c r="E23" s="267"/>
-      <c r="F23" s="267"/>
-      <c r="G23" s="267"/>
-      <c r="H23" s="267"/>
-      <c r="I23" s="267"/>
-      <c r="J23" s="267"/>
-      <c r="K23" s="267"/>
-      <c r="L23" s="268"/>
+      <c r="C23" s="240"/>
+      <c r="D23" s="240"/>
+      <c r="E23" s="240"/>
+      <c r="F23" s="240"/>
+      <c r="G23" s="240"/>
+      <c r="H23" s="240"/>
+      <c r="I23" s="240"/>
+      <c r="J23" s="240"/>
+      <c r="K23" s="240"/>
+      <c r="L23" s="241"/>
       <c r="N23" s="106"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="230"/>
-      <c r="B24" s="267" t="s">
+      <c r="B24" s="240" t="s">
         <v>222</v>
       </c>
-      <c r="C24" s="267"/>
-      <c r="D24" s="267"/>
-      <c r="E24" s="267"/>
-      <c r="F24" s="267"/>
-      <c r="G24" s="267"/>
-      <c r="H24" s="267"/>
-      <c r="I24" s="267"/>
-      <c r="J24" s="267"/>
-      <c r="K24" s="267"/>
-      <c r="L24" s="268"/>
+      <c r="C24" s="240"/>
+      <c r="D24" s="240"/>
+      <c r="E24" s="240"/>
+      <c r="F24" s="240"/>
+      <c r="G24" s="240"/>
+      <c r="H24" s="240"/>
+      <c r="I24" s="240"/>
+      <c r="J24" s="240"/>
+      <c r="K24" s="240"/>
+      <c r="L24" s="241"/>
       <c r="N24" s="106"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="269" t="s">
+      <c r="A25" s="249" t="s">
         <v>228</v>
       </c>
-      <c r="B25" s="270"/>
-      <c r="C25" s="270"/>
-      <c r="D25" s="270"/>
-      <c r="E25" s="270"/>
-      <c r="F25" s="270"/>
-      <c r="G25" s="270"/>
-      <c r="H25" s="270"/>
-      <c r="I25" s="270"/>
-      <c r="J25" s="270"/>
-      <c r="K25" s="270"/>
-      <c r="L25" s="271"/>
+      <c r="B25" s="250"/>
+      <c r="C25" s="250"/>
+      <c r="D25" s="250"/>
+      <c r="E25" s="250"/>
+      <c r="F25" s="250"/>
+      <c r="G25" s="250"/>
+      <c r="H25" s="250"/>
+      <c r="I25" s="250"/>
+      <c r="J25" s="250"/>
+      <c r="K25" s="250"/>
+      <c r="L25" s="251"/>
       <c r="N25" s="106"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="230">
         <v>1</v>
       </c>
-      <c r="B26" s="267" t="s">
+      <c r="B26" s="240" t="s">
         <v>223</v>
       </c>
-      <c r="C26" s="267"/>
-      <c r="D26" s="267"/>
-      <c r="E26" s="267"/>
-      <c r="F26" s="267"/>
-      <c r="G26" s="267"/>
-      <c r="H26" s="267"/>
-      <c r="I26" s="267"/>
-      <c r="J26" s="267"/>
-      <c r="K26" s="267"/>
-      <c r="L26" s="268"/>
+      <c r="C26" s="240"/>
+      <c r="D26" s="240"/>
+      <c r="E26" s="240"/>
+      <c r="F26" s="240"/>
+      <c r="G26" s="240"/>
+      <c r="H26" s="240"/>
+      <c r="I26" s="240"/>
+      <c r="J26" s="240"/>
+      <c r="K26" s="240"/>
+      <c r="L26" s="241"/>
       <c r="N26" s="106"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="230"/>
-      <c r="B27" s="265" t="s">
+      <c r="B27" s="238" t="s">
         <v>358</v>
       </c>
-      <c r="C27" s="265"/>
-      <c r="D27" s="265"/>
-      <c r="E27" s="265"/>
-      <c r="F27" s="265"/>
-      <c r="G27" s="265"/>
-      <c r="H27" s="265"/>
-      <c r="I27" s="265"/>
-      <c r="J27" s="265"/>
-      <c r="K27" s="265"/>
-      <c r="L27" s="266"/>
+      <c r="C27" s="238"/>
+      <c r="D27" s="238"/>
+      <c r="E27" s="238"/>
+      <c r="F27" s="238"/>
+      <c r="G27" s="238"/>
+      <c r="H27" s="238"/>
+      <c r="I27" s="238"/>
+      <c r="J27" s="238"/>
+      <c r="K27" s="238"/>
+      <c r="L27" s="239"/>
       <c r="N27" s="106"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="230">
         <v>2</v>
       </c>
-      <c r="B28" s="267" t="s">
+      <c r="B28" s="240" t="s">
         <v>347</v>
       </c>
-      <c r="C28" s="267"/>
-      <c r="D28" s="267"/>
-      <c r="E28" s="267"/>
-      <c r="F28" s="267"/>
-      <c r="G28" s="267"/>
-      <c r="H28" s="267"/>
-      <c r="I28" s="267"/>
-      <c r="J28" s="267"/>
-      <c r="K28" s="267"/>
-      <c r="L28" s="268"/>
+      <c r="C28" s="240"/>
+      <c r="D28" s="240"/>
+      <c r="E28" s="240"/>
+      <c r="F28" s="240"/>
+      <c r="G28" s="240"/>
+      <c r="H28" s="240"/>
+      <c r="I28" s="240"/>
+      <c r="J28" s="240"/>
+      <c r="K28" s="240"/>
+      <c r="L28" s="241"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="230">
         <v>3</v>
       </c>
-      <c r="B29" s="267" t="s">
+      <c r="B29" s="240" t="s">
         <v>336</v>
       </c>
-      <c r="C29" s="267"/>
-      <c r="D29" s="267"/>
-      <c r="E29" s="267"/>
-      <c r="F29" s="267"/>
-      <c r="G29" s="267"/>
-      <c r="H29" s="267"/>
-      <c r="I29" s="267"/>
-      <c r="J29" s="267"/>
-      <c r="K29" s="267"/>
-      <c r="L29" s="268"/>
+      <c r="C29" s="240"/>
+      <c r="D29" s="240"/>
+      <c r="E29" s="240"/>
+      <c r="F29" s="240"/>
+      <c r="G29" s="240"/>
+      <c r="H29" s="240"/>
+      <c r="I29" s="240"/>
+      <c r="J29" s="240"/>
+      <c r="K29" s="240"/>
+      <c r="L29" s="241"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="230">
         <v>4</v>
       </c>
-      <c r="B30" s="267" t="s">
+      <c r="B30" s="240" t="s">
         <v>359</v>
       </c>
-      <c r="C30" s="267"/>
-      <c r="D30" s="267"/>
-      <c r="E30" s="267"/>
-      <c r="F30" s="267"/>
-      <c r="G30" s="267"/>
-      <c r="H30" s="267"/>
-      <c r="I30" s="267"/>
-      <c r="J30" s="267"/>
-      <c r="K30" s="267"/>
-      <c r="L30" s="268"/>
+      <c r="C30" s="240"/>
+      <c r="D30" s="240"/>
+      <c r="E30" s="240"/>
+      <c r="F30" s="240"/>
+      <c r="G30" s="240"/>
+      <c r="H30" s="240"/>
+      <c r="I30" s="240"/>
+      <c r="J30" s="240"/>
+      <c r="K30" s="240"/>
+      <c r="L30" s="241"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="230">
         <v>5</v>
       </c>
-      <c r="B31" s="265" t="s">
+      <c r="B31" s="238" t="s">
         <v>337</v>
       </c>
-      <c r="C31" s="265"/>
-      <c r="D31" s="265"/>
-      <c r="E31" s="265"/>
-      <c r="F31" s="265"/>
-      <c r="G31" s="265"/>
-      <c r="H31" s="265"/>
-      <c r="I31" s="265"/>
-      <c r="J31" s="265"/>
-      <c r="K31" s="265"/>
-      <c r="L31" s="266"/>
+      <c r="C31" s="238"/>
+      <c r="D31" s="238"/>
+      <c r="E31" s="238"/>
+      <c r="F31" s="238"/>
+      <c r="G31" s="238"/>
+      <c r="H31" s="238"/>
+      <c r="I31" s="238"/>
+      <c r="J31" s="238"/>
+      <c r="K31" s="238"/>
+      <c r="L31" s="239"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="230">
         <v>6</v>
       </c>
-      <c r="B32" s="265" t="s">
+      <c r="B32" s="238" t="s">
         <v>342</v>
       </c>
-      <c r="C32" s="265"/>
-      <c r="D32" s="265"/>
-      <c r="E32" s="265"/>
-      <c r="F32" s="265"/>
-      <c r="G32" s="265"/>
-      <c r="H32" s="265"/>
-      <c r="I32" s="265"/>
-      <c r="J32" s="265"/>
-      <c r="K32" s="265"/>
-      <c r="L32" s="266"/>
+      <c r="C32" s="238"/>
+      <c r="D32" s="238"/>
+      <c r="E32" s="238"/>
+      <c r="F32" s="238"/>
+      <c r="G32" s="238"/>
+      <c r="H32" s="238"/>
+      <c r="I32" s="238"/>
+      <c r="J32" s="238"/>
+      <c r="K32" s="238"/>
+      <c r="L32" s="239"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="230">
         <v>7</v>
       </c>
-      <c r="B33" s="267" t="s">
+      <c r="B33" s="240" t="s">
         <v>338</v>
       </c>
-      <c r="C33" s="267"/>
-      <c r="D33" s="267"/>
-      <c r="E33" s="267"/>
-      <c r="F33" s="267"/>
-      <c r="G33" s="267"/>
-      <c r="H33" s="267"/>
-      <c r="I33" s="267"/>
-      <c r="J33" s="267"/>
-      <c r="K33" s="267"/>
-      <c r="L33" s="268"/>
+      <c r="C33" s="240"/>
+      <c r="D33" s="240"/>
+      <c r="E33" s="240"/>
+      <c r="F33" s="240"/>
+      <c r="G33" s="240"/>
+      <c r="H33" s="240"/>
+      <c r="I33" s="240"/>
+      <c r="J33" s="240"/>
+      <c r="K33" s="240"/>
+      <c r="L33" s="241"/>
     </row>
     <row r="34" spans="1:12" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="230"/>
@@ -15460,56 +15460,56 @@
       <c r="L34" s="232"/>
     </row>
     <row r="35" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="269" t="s">
+      <c r="A35" s="249" t="s">
         <v>341</v>
       </c>
-      <c r="B35" s="270"/>
-      <c r="C35" s="270"/>
-      <c r="D35" s="270"/>
-      <c r="E35" s="270"/>
-      <c r="F35" s="270"/>
-      <c r="G35" s="270"/>
-      <c r="H35" s="270"/>
-      <c r="I35" s="270"/>
-      <c r="J35" s="270"/>
-      <c r="K35" s="270"/>
-      <c r="L35" s="271"/>
+      <c r="B35" s="250"/>
+      <c r="C35" s="250"/>
+      <c r="D35" s="250"/>
+      <c r="E35" s="250"/>
+      <c r="F35" s="250"/>
+      <c r="G35" s="250"/>
+      <c r="H35" s="250"/>
+      <c r="I35" s="250"/>
+      <c r="J35" s="250"/>
+      <c r="K35" s="250"/>
+      <c r="L35" s="251"/>
     </row>
     <row r="36" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="233" t="s">
         <v>339</v>
       </c>
-      <c r="B36" s="267" t="s">
+      <c r="B36" s="240" t="s">
         <v>224</v>
       </c>
-      <c r="C36" s="267"/>
-      <c r="D36" s="267"/>
-      <c r="E36" s="267"/>
-      <c r="F36" s="267"/>
-      <c r="G36" s="267"/>
-      <c r="H36" s="267"/>
-      <c r="I36" s="267"/>
-      <c r="J36" s="267"/>
-      <c r="K36" s="267"/>
-      <c r="L36" s="268"/>
+      <c r="C36" s="240"/>
+      <c r="D36" s="240"/>
+      <c r="E36" s="240"/>
+      <c r="F36" s="240"/>
+      <c r="G36" s="240"/>
+      <c r="H36" s="240"/>
+      <c r="I36" s="240"/>
+      <c r="J36" s="240"/>
+      <c r="K36" s="240"/>
+      <c r="L36" s="241"/>
     </row>
     <row r="37" spans="1:12" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="234" t="s">
         <v>340</v>
       </c>
-      <c r="B37" s="273" t="s">
+      <c r="B37" s="242" t="s">
         <v>343</v>
       </c>
-      <c r="C37" s="273"/>
-      <c r="D37" s="273"/>
-      <c r="E37" s="273"/>
-      <c r="F37" s="273"/>
-      <c r="G37" s="273"/>
-      <c r="H37" s="273"/>
-      <c r="I37" s="273"/>
-      <c r="J37" s="273"/>
-      <c r="K37" s="273"/>
-      <c r="L37" s="274"/>
+      <c r="C37" s="242"/>
+      <c r="D37" s="242"/>
+      <c r="E37" s="242"/>
+      <c r="F37" s="242"/>
+      <c r="G37" s="242"/>
+      <c r="H37" s="242"/>
+      <c r="I37" s="242"/>
+      <c r="J37" s="242"/>
+      <c r="K37" s="242"/>
+      <c r="L37" s="243"/>
     </row>
     <row r="38" spans="1:12" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="161"/>
@@ -15526,20 +15526,20 @@
       <c r="L38" s="113"/>
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="275" t="s">
+      <c r="A39" s="244" t="s">
         <v>252</v>
       </c>
-      <c r="B39" s="276"/>
-      <c r="C39" s="276"/>
-      <c r="D39" s="276"/>
-      <c r="E39" s="276"/>
-      <c r="F39" s="276"/>
-      <c r="G39" s="276"/>
-      <c r="H39" s="276"/>
-      <c r="I39" s="276"/>
-      <c r="J39" s="276"/>
-      <c r="K39" s="276"/>
-      <c r="L39" s="277"/>
+      <c r="B39" s="245"/>
+      <c r="C39" s="245"/>
+      <c r="D39" s="245"/>
+      <c r="E39" s="245"/>
+      <c r="F39" s="245"/>
+      <c r="G39" s="245"/>
+      <c r="H39" s="245"/>
+      <c r="I39" s="245"/>
+      <c r="J39" s="245"/>
+      <c r="K39" s="245"/>
+      <c r="L39" s="246"/>
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="162" t="s">
@@ -15627,72 +15627,72 @@
       <c r="B45" s="170" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="255" t="s">
+      <c r="C45" s="247" t="s">
         <v>326</v>
       </c>
-      <c r="D45" s="255"/>
-      <c r="E45" s="255"/>
-      <c r="F45" s="255"/>
-      <c r="G45" s="255"/>
-      <c r="H45" s="255"/>
-      <c r="I45" s="255"/>
-      <c r="J45" s="255"/>
-      <c r="K45" s="255"/>
-      <c r="L45" s="256"/>
+      <c r="D45" s="247"/>
+      <c r="E45" s="247"/>
+      <c r="F45" s="247"/>
+      <c r="G45" s="247"/>
+      <c r="H45" s="247"/>
+      <c r="I45" s="247"/>
+      <c r="J45" s="247"/>
+      <c r="K45" s="247"/>
+      <c r="L45" s="248"/>
     </row>
     <row r="46" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="169"/>
       <c r="B46" s="170" t="s">
         <v>146</v>
       </c>
-      <c r="C46" s="255" t="s">
+      <c r="C46" s="247" t="s">
         <v>147</v>
       </c>
-      <c r="D46" s="255"/>
-      <c r="E46" s="255"/>
-      <c r="F46" s="255"/>
-      <c r="G46" s="255"/>
-      <c r="H46" s="255"/>
-      <c r="I46" s="255"/>
-      <c r="J46" s="255"/>
-      <c r="K46" s="255"/>
-      <c r="L46" s="256"/>
+      <c r="D46" s="247"/>
+      <c r="E46" s="247"/>
+      <c r="F46" s="247"/>
+      <c r="G46" s="247"/>
+      <c r="H46" s="247"/>
+      <c r="I46" s="247"/>
+      <c r="J46" s="247"/>
+      <c r="K46" s="247"/>
+      <c r="L46" s="248"/>
     </row>
     <row r="47" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="169"/>
       <c r="B47" s="170" t="s">
         <v>250</v>
       </c>
-      <c r="C47" s="255" t="s">
+      <c r="C47" s="247" t="s">
         <v>251</v>
       </c>
-      <c r="D47" s="255"/>
-      <c r="E47" s="255"/>
-      <c r="F47" s="255"/>
-      <c r="G47" s="255"/>
-      <c r="H47" s="255"/>
-      <c r="I47" s="255"/>
-      <c r="J47" s="255"/>
-      <c r="K47" s="255"/>
-      <c r="L47" s="256"/>
+      <c r="D47" s="247"/>
+      <c r="E47" s="247"/>
+      <c r="F47" s="247"/>
+      <c r="G47" s="247"/>
+      <c r="H47" s="247"/>
+      <c r="I47" s="247"/>
+      <c r="J47" s="247"/>
+      <c r="K47" s="247"/>
+      <c r="L47" s="248"/>
     </row>
     <row r="48" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="169"/>
       <c r="B48" s="170" t="s">
         <v>327</v>
       </c>
-      <c r="C48" s="255" t="s">
+      <c r="C48" s="247" t="s">
         <v>328</v>
       </c>
-      <c r="D48" s="255"/>
-      <c r="E48" s="255"/>
-      <c r="F48" s="255"/>
-      <c r="G48" s="255"/>
-      <c r="H48" s="255"/>
-      <c r="I48" s="255"/>
-      <c r="J48" s="255"/>
-      <c r="K48" s="255"/>
-      <c r="L48" s="256"/>
+      <c r="D48" s="247"/>
+      <c r="E48" s="247"/>
+      <c r="F48" s="247"/>
+      <c r="G48" s="247"/>
+      <c r="H48" s="247"/>
+      <c r="I48" s="247"/>
+      <c r="J48" s="247"/>
+      <c r="K48" s="247"/>
+      <c r="L48" s="248"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="169"/>
@@ -15717,18 +15717,18 @@
       <c r="B50" s="170" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="255" t="s">
+      <c r="C50" s="247" t="s">
         <v>330</v>
       </c>
-      <c r="D50" s="255"/>
-      <c r="E50" s="255"/>
-      <c r="F50" s="255"/>
-      <c r="G50" s="255"/>
-      <c r="H50" s="255"/>
-      <c r="I50" s="255"/>
-      <c r="J50" s="255"/>
-      <c r="K50" s="255"/>
-      <c r="L50" s="256"/>
+      <c r="D50" s="247"/>
+      <c r="E50" s="247"/>
+      <c r="F50" s="247"/>
+      <c r="G50" s="247"/>
+      <c r="H50" s="247"/>
+      <c r="I50" s="247"/>
+      <c r="J50" s="247"/>
+      <c r="K50" s="247"/>
+      <c r="L50" s="248"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="169"/>
@@ -15810,37 +15810,39 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="272" t="s">
+      <c r="A64" s="237" t="s">
         <v>332</v>
       </c>
-      <c r="B64" s="272"/>
-      <c r="C64" s="272"/>
-      <c r="D64" s="272"/>
-      <c r="E64" s="272"/>
-      <c r="F64" s="272"/>
-      <c r="G64" s="272"/>
-      <c r="H64" s="272"/>
-      <c r="I64" s="272"/>
-      <c r="J64" s="272"/>
-      <c r="K64" s="272"/>
-      <c r="L64" s="272"/>
+      <c r="B64" s="237"/>
+      <c r="C64" s="237"/>
+      <c r="D64" s="237"/>
+      <c r="E64" s="237"/>
+      <c r="F64" s="237"/>
+      <c r="G64" s="237"/>
+      <c r="H64" s="237"/>
+      <c r="I64" s="237"/>
+      <c r="J64" s="237"/>
+      <c r="K64" s="237"/>
+      <c r="L64" s="237"/>
     </row>
     <row r="69" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="70" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A64:L64"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="C45:L45"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="C47:L47"/>
-    <mergeCell ref="C48:L48"/>
-    <mergeCell ref="C50:L50"/>
-    <mergeCell ref="A35:L35"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B8:L8"/>
     <mergeCell ref="B31:L31"/>
     <mergeCell ref="B18:L18"/>
     <mergeCell ref="B19:L19"/>
@@ -15855,20 +15857,18 @@
     <mergeCell ref="B29:L29"/>
     <mergeCell ref="B28:L28"/>
     <mergeCell ref="B30:L30"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="A64:L64"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="C45:L45"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="C48:L48"/>
+    <mergeCell ref="C50:L50"/>
+    <mergeCell ref="A35:L35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A57" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -16527,7 +16527,7 @@
   <dimension ref="A1:P139"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21252,7 +21252,7 @@
     <hyperlink ref="N22" r:id="rId7" location="v-water-conservation-program-ics-total-balance" xr:uid="{9E773CCF-F296-48D2-ADA9-5456ABC7F062}"/>
     <hyperlink ref="N23" r:id="rId8" location="vi-remaining-storage-above-the-protect-and-ics-balances" xr:uid="{8CAE8559-5BD9-4D9F-8655-D1F3AE1FCD4D}"/>
     <hyperlink ref="N24" r:id="rId9" location="vii-delivery-to-meet-10-year-requirement" xr:uid="{B6DDA7AA-2218-4D2F-9A7A-A0EDBEFDC5B1}"/>
-    <hyperlink ref="N28" r:id="rId10" location="step-2-specify-natural-inflow-to-lake-powell" display="Help Lake Mead inflow" xr:uid="{78DF76B4-BE79-4AC1-9F08-EC86A0A72F91}"/>
+    <hyperlink ref="N28" r:id="rId10" location="step-2-specify-lake-mead-inflow" xr:uid="{78DF76B4-BE79-4AC1-9F08-EC86A0A72F91}"/>
     <hyperlink ref="N29" r:id="rId11" location="2a-intervening-grand-canyon-flow" xr:uid="{CFD884C0-2149-42F6-AD5A-482CF40D5292}"/>
     <hyperlink ref="N30" r:id="rId12" location="2b-mead-to-imperial-dam-intervening-flow" xr:uid="{B8EF30C2-739D-4E21-B63A-F17F9947326A}"/>
     <hyperlink ref="N31" r:id="rId13" location="2c-havasuparker-evaporation-and-evapotranspiration" xr:uid="{70E7AC6A-42AC-4DE1-ADFB-FBA8230C308E}"/>
@@ -22701,16 +22701,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="312" t="e">
+      <c r="A1" s="313" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="312"/>
-      <c r="C1" s="312"/>
-      <c r="D1" s="312"/>
-      <c r="E1" s="312"/>
-      <c r="F1" s="312"/>
-      <c r="G1" s="312"/>
+      <c r="B1" s="313"/>
+      <c r="C1" s="313"/>
+      <c r="D1" s="313"/>
+      <c r="E1" s="313"/>
+      <c r="F1" s="313"/>
+      <c r="G1" s="313"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -22819,11 +22819,11 @@
         <v>81</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="313"/>
-      <c r="D10" s="313"/>
-      <c r="E10" s="313"/>
-      <c r="F10" s="313"/>
-      <c r="G10" s="313"/>
+      <c r="C10" s="312"/>
+      <c r="D10" s="312"/>
+      <c r="E10" s="312"/>
+      <c r="F10" s="312"/>
+      <c r="G10" s="312"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -24086,6 +24086,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -24093,12 +24099,6 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>

</xml_diff>

<commit_message>
Update Evaporation in the users guide
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84CBA8FD-B884-44C3-BA51-D98355CA9D41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F91525-51E4-4BEE-BF86-CEBC1288EB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="367">
   <si>
     <t>Year 1</t>
   </si>
@@ -1921,6 +1921,12 @@
   <si>
     <t>Help specify Lake Mead inflow</t>
   </si>
+  <si>
+    <t>1.3</t>
+  </si>
+  <si>
+    <t>Start documenting model with instructions and user guide.</t>
+  </si>
 </sst>
 </file>
 
@@ -3197,51 +3203,6 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3296,6 +3257,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3319,6 +3286,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3422,11 +3428,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14866,20 +14872,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="255" t="s">
+      <c r="A1" s="240" t="s">
         <v>321</v>
       </c>
-      <c r="B1" s="255"/>
-      <c r="C1" s="255"/>
-      <c r="D1" s="255"/>
-      <c r="E1" s="255"/>
-      <c r="F1" s="255"/>
-      <c r="G1" s="255"/>
-      <c r="H1" s="255"/>
-      <c r="I1" s="255"/>
-      <c r="J1" s="255"/>
-      <c r="K1" s="255"/>
-      <c r="L1" s="255"/>
+      <c r="B1" s="240"/>
+      <c r="C1" s="240"/>
+      <c r="D1" s="240"/>
+      <c r="E1" s="240"/>
+      <c r="F1" s="240"/>
+      <c r="G1" s="240"/>
+      <c r="H1" s="240"/>
+      <c r="I1" s="240"/>
+      <c r="J1" s="240"/>
+      <c r="K1" s="240"/>
+      <c r="L1" s="240"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -14905,41 +14911,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="256" t="s">
+      <c r="A4" s="241" t="s">
         <v>349</v>
       </c>
-      <c r="B4" s="257"/>
-      <c r="C4" s="257"/>
-      <c r="D4" s="257"/>
-      <c r="E4" s="257"/>
-      <c r="F4" s="257"/>
-      <c r="G4" s="257"/>
-      <c r="H4" s="257"/>
-      <c r="I4" s="257"/>
-      <c r="J4" s="257"/>
-      <c r="K4" s="257"/>
-      <c r="L4" s="258"/>
-      <c r="N4" s="259"/>
-      <c r="O4" s="259"/>
-      <c r="P4" s="259"/>
-      <c r="Q4" s="259"/>
-      <c r="R4" s="259"/>
+      <c r="B4" s="242"/>
+      <c r="C4" s="242"/>
+      <c r="D4" s="242"/>
+      <c r="E4" s="242"/>
+      <c r="F4" s="242"/>
+      <c r="G4" s="242"/>
+      <c r="H4" s="242"/>
+      <c r="I4" s="242"/>
+      <c r="J4" s="242"/>
+      <c r="K4" s="242"/>
+      <c r="L4" s="243"/>
+      <c r="N4" s="244"/>
+      <c r="O4" s="244"/>
+      <c r="P4" s="244"/>
+      <c r="Q4" s="244"/>
+      <c r="R4" s="244"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="260" t="s">
+      <c r="A5" s="245" t="s">
         <v>350</v>
       </c>
-      <c r="B5" s="261"/>
-      <c r="C5" s="261"/>
-      <c r="D5" s="261"/>
-      <c r="E5" s="261"/>
-      <c r="F5" s="261"/>
-      <c r="G5" s="261"/>
-      <c r="H5" s="261"/>
-      <c r="I5" s="261"/>
-      <c r="J5" s="261"/>
-      <c r="K5" s="261"/>
-      <c r="L5" s="262"/>
+      <c r="B5" s="246"/>
+      <c r="C5" s="246"/>
+      <c r="D5" s="246"/>
+      <c r="E5" s="246"/>
+      <c r="F5" s="246"/>
+      <c r="G5" s="246"/>
+      <c r="H5" s="246"/>
+      <c r="I5" s="246"/>
+      <c r="J5" s="246"/>
+      <c r="K5" s="246"/>
+      <c r="L5" s="247"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -14947,20 +14953,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="260" t="s">
+      <c r="A6" s="245" t="s">
         <v>352</v>
       </c>
-      <c r="B6" s="261"/>
-      <c r="C6" s="261"/>
-      <c r="D6" s="261"/>
-      <c r="E6" s="261"/>
-      <c r="F6" s="261"/>
-      <c r="G6" s="261"/>
-      <c r="H6" s="261"/>
-      <c r="I6" s="261"/>
-      <c r="J6" s="261"/>
-      <c r="K6" s="261"/>
-      <c r="L6" s="262"/>
+      <c r="B6" s="246"/>
+      <c r="C6" s="246"/>
+      <c r="D6" s="246"/>
+      <c r="E6" s="246"/>
+      <c r="F6" s="246"/>
+      <c r="G6" s="246"/>
+      <c r="H6" s="246"/>
+      <c r="I6" s="246"/>
+      <c r="J6" s="246"/>
+      <c r="K6" s="246"/>
+      <c r="L6" s="247"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -14969,19 +14975,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="235"/>
-      <c r="B7" s="261" t="s">
+      <c r="B7" s="246" t="s">
         <v>353</v>
       </c>
-      <c r="C7" s="261"/>
-      <c r="D7" s="261"/>
-      <c r="E7" s="261"/>
-      <c r="F7" s="261"/>
-      <c r="G7" s="261"/>
-      <c r="H7" s="261"/>
-      <c r="I7" s="261"/>
-      <c r="J7" s="261"/>
-      <c r="K7" s="261"/>
-      <c r="L7" s="262"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="246"/>
+      <c r="F7" s="246"/>
+      <c r="G7" s="246"/>
+      <c r="H7" s="246"/>
+      <c r="I7" s="246"/>
+      <c r="J7" s="246"/>
+      <c r="K7" s="246"/>
+      <c r="L7" s="247"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -14990,19 +14996,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="236"/>
-      <c r="B8" s="276" t="s">
+      <c r="B8" s="263" t="s">
         <v>354</v>
       </c>
-      <c r="C8" s="276"/>
-      <c r="D8" s="276"/>
-      <c r="E8" s="276"/>
-      <c r="F8" s="276"/>
-      <c r="G8" s="276"/>
-      <c r="H8" s="276"/>
-      <c r="I8" s="276"/>
-      <c r="J8" s="276"/>
-      <c r="K8" s="276"/>
-      <c r="L8" s="277"/>
+      <c r="C8" s="263"/>
+      <c r="D8" s="263"/>
+      <c r="E8" s="263"/>
+      <c r="F8" s="263"/>
+      <c r="G8" s="263"/>
+      <c r="H8" s="263"/>
+      <c r="I8" s="263"/>
+      <c r="J8" s="263"/>
+      <c r="K8" s="263"/>
+      <c r="L8" s="264"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15024,84 +15030,84 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="263" t="s">
+      <c r="A10" s="248" t="s">
         <v>217</v>
       </c>
-      <c r="B10" s="264"/>
-      <c r="C10" s="264"/>
-      <c r="D10" s="264"/>
-      <c r="E10" s="264"/>
-      <c r="F10" s="264"/>
-      <c r="G10" s="264"/>
-      <c r="H10" s="264"/>
-      <c r="I10" s="264"/>
-      <c r="J10" s="264"/>
-      <c r="K10" s="264"/>
-      <c r="L10" s="265"/>
+      <c r="B10" s="249"/>
+      <c r="C10" s="249"/>
+      <c r="D10" s="249"/>
+      <c r="E10" s="249"/>
+      <c r="F10" s="249"/>
+      <c r="G10" s="249"/>
+      <c r="H10" s="249"/>
+      <c r="I10" s="249"/>
+      <c r="J10" s="249"/>
+      <c r="K10" s="249"/>
+      <c r="L10" s="250"/>
     </row>
     <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="266" t="s">
+      <c r="A11" s="251" t="s">
         <v>351</v>
       </c>
-      <c r="B11" s="267"/>
-      <c r="C11" s="267"/>
-      <c r="D11" s="267"/>
-      <c r="E11" s="267"/>
-      <c r="F11" s="267"/>
-      <c r="G11" s="267"/>
-      <c r="H11" s="267"/>
-      <c r="I11" s="267"/>
-      <c r="J11" s="267"/>
-      <c r="K11" s="267"/>
-      <c r="L11" s="268"/>
+      <c r="B11" s="252"/>
+      <c r="C11" s="252"/>
+      <c r="D11" s="252"/>
+      <c r="E11" s="252"/>
+      <c r="F11" s="252"/>
+      <c r="G11" s="252"/>
+      <c r="H11" s="252"/>
+      <c r="I11" s="252"/>
+      <c r="J11" s="252"/>
+      <c r="K11" s="252"/>
+      <c r="L11" s="253"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="269" t="s">
+      <c r="A12" s="254" t="s">
         <v>355</v>
       </c>
-      <c r="B12" s="247"/>
-      <c r="C12" s="247"/>
-      <c r="D12" s="247"/>
-      <c r="E12" s="247"/>
-      <c r="F12" s="247"/>
-      <c r="G12" s="247"/>
-      <c r="H12" s="247"/>
-      <c r="I12" s="247"/>
-      <c r="J12" s="247"/>
-      <c r="K12" s="247"/>
-      <c r="L12" s="248"/>
+      <c r="B12" s="255"/>
+      <c r="C12" s="255"/>
+      <c r="D12" s="255"/>
+      <c r="E12" s="255"/>
+      <c r="F12" s="255"/>
+      <c r="G12" s="255"/>
+      <c r="H12" s="255"/>
+      <c r="I12" s="255"/>
+      <c r="J12" s="255"/>
+      <c r="K12" s="255"/>
+      <c r="L12" s="256"/>
     </row>
     <row r="13" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="269" t="s">
+      <c r="A13" s="254" t="s">
         <v>218</v>
       </c>
-      <c r="B13" s="247"/>
-      <c r="C13" s="247"/>
-      <c r="D13" s="247"/>
-      <c r="E13" s="247"/>
-      <c r="F13" s="247"/>
-      <c r="G13" s="247"/>
-      <c r="H13" s="247"/>
-      <c r="I13" s="247"/>
-      <c r="J13" s="247"/>
-      <c r="K13" s="247"/>
-      <c r="L13" s="248"/>
+      <c r="B13" s="255"/>
+      <c r="C13" s="255"/>
+      <c r="D13" s="255"/>
+      <c r="E13" s="255"/>
+      <c r="F13" s="255"/>
+      <c r="G13" s="255"/>
+      <c r="H13" s="255"/>
+      <c r="I13" s="255"/>
+      <c r="J13" s="255"/>
+      <c r="K13" s="255"/>
+      <c r="L13" s="256"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="270" t="s">
+      <c r="A14" s="257" t="s">
         <v>356</v>
       </c>
-      <c r="B14" s="271"/>
-      <c r="C14" s="271"/>
-      <c r="D14" s="271"/>
-      <c r="E14" s="271"/>
-      <c r="F14" s="271"/>
-      <c r="G14" s="271"/>
-      <c r="H14" s="271"/>
-      <c r="I14" s="271"/>
-      <c r="J14" s="271"/>
-      <c r="K14" s="271"/>
-      <c r="L14" s="272"/>
+      <c r="B14" s="258"/>
+      <c r="C14" s="258"/>
+      <c r="D14" s="258"/>
+      <c r="E14" s="258"/>
+      <c r="F14" s="258"/>
+      <c r="G14" s="258"/>
+      <c r="H14" s="258"/>
+      <c r="I14" s="258"/>
+      <c r="J14" s="258"/>
+      <c r="K14" s="258"/>
+      <c r="L14" s="259"/>
     </row>
     <row r="15" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="113"/>
@@ -15118,332 +15124,332 @@
       <c r="L15" s="113"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="273" t="s">
+      <c r="A16" s="260" t="s">
         <v>348</v>
       </c>
-      <c r="B16" s="274"/>
-      <c r="C16" s="274"/>
-      <c r="D16" s="274"/>
-      <c r="E16" s="274"/>
-      <c r="F16" s="274"/>
-      <c r="G16" s="274"/>
-      <c r="H16" s="274"/>
-      <c r="I16" s="274"/>
-      <c r="J16" s="274"/>
-      <c r="K16" s="274"/>
-      <c r="L16" s="275"/>
+      <c r="B16" s="261"/>
+      <c r="C16" s="261"/>
+      <c r="D16" s="261"/>
+      <c r="E16" s="261"/>
+      <c r="F16" s="261"/>
+      <c r="G16" s="261"/>
+      <c r="H16" s="261"/>
+      <c r="I16" s="261"/>
+      <c r="J16" s="261"/>
+      <c r="K16" s="261"/>
+      <c r="L16" s="262"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="252" t="s">
+      <c r="A17" s="237" t="s">
         <v>227</v>
       </c>
-      <c r="B17" s="253"/>
-      <c r="C17" s="253"/>
-      <c r="D17" s="253"/>
-      <c r="E17" s="253"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="253"/>
-      <c r="I17" s="253"/>
-      <c r="J17" s="253"/>
-      <c r="K17" s="253"/>
-      <c r="L17" s="254"/>
+      <c r="B17" s="238"/>
+      <c r="C17" s="238"/>
+      <c r="D17" s="238"/>
+      <c r="E17" s="238"/>
+      <c r="F17" s="238"/>
+      <c r="G17" s="238"/>
+      <c r="H17" s="238"/>
+      <c r="I17" s="238"/>
+      <c r="J17" s="238"/>
+      <c r="K17" s="238"/>
+      <c r="L17" s="239"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="230">
         <v>1</v>
       </c>
-      <c r="B18" s="240" t="s">
+      <c r="B18" s="267" t="s">
         <v>226</v>
       </c>
-      <c r="C18" s="240"/>
-      <c r="D18" s="240"/>
-      <c r="E18" s="240"/>
-      <c r="F18" s="240"/>
-      <c r="G18" s="240"/>
-      <c r="H18" s="240"/>
-      <c r="I18" s="240"/>
-      <c r="J18" s="240"/>
-      <c r="K18" s="240"/>
-      <c r="L18" s="241"/>
+      <c r="C18" s="267"/>
+      <c r="D18" s="267"/>
+      <c r="E18" s="267"/>
+      <c r="F18" s="267"/>
+      <c r="G18" s="267"/>
+      <c r="H18" s="267"/>
+      <c r="I18" s="267"/>
+      <c r="J18" s="267"/>
+      <c r="K18" s="267"/>
+      <c r="L18" s="268"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="230">
         <v>2</v>
       </c>
-      <c r="B19" s="240" t="s">
+      <c r="B19" s="267" t="s">
         <v>344</v>
       </c>
-      <c r="C19" s="240"/>
-      <c r="D19" s="240"/>
-      <c r="E19" s="240"/>
-      <c r="F19" s="240"/>
-      <c r="G19" s="240"/>
-      <c r="H19" s="240"/>
-      <c r="I19" s="240"/>
-      <c r="J19" s="240"/>
-      <c r="K19" s="240"/>
-      <c r="L19" s="241"/>
+      <c r="C19" s="267"/>
+      <c r="D19" s="267"/>
+      <c r="E19" s="267"/>
+      <c r="F19" s="267"/>
+      <c r="G19" s="267"/>
+      <c r="H19" s="267"/>
+      <c r="I19" s="267"/>
+      <c r="J19" s="267"/>
+      <c r="K19" s="267"/>
+      <c r="L19" s="268"/>
       <c r="N19" s="106"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="230">
         <v>3</v>
       </c>
-      <c r="B20" s="240" t="s">
+      <c r="B20" s="267" t="s">
         <v>219</v>
       </c>
-      <c r="C20" s="240"/>
-      <c r="D20" s="240"/>
-      <c r="E20" s="240"/>
-      <c r="F20" s="240"/>
-      <c r="G20" s="240"/>
-      <c r="H20" s="240"/>
-      <c r="I20" s="240"/>
-      <c r="J20" s="240"/>
-      <c r="K20" s="240"/>
-      <c r="L20" s="241"/>
+      <c r="C20" s="267"/>
+      <c r="D20" s="267"/>
+      <c r="E20" s="267"/>
+      <c r="F20" s="267"/>
+      <c r="G20" s="267"/>
+      <c r="H20" s="267"/>
+      <c r="I20" s="267"/>
+      <c r="J20" s="267"/>
+      <c r="K20" s="267"/>
+      <c r="L20" s="268"/>
       <c r="N20" s="106"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="230">
         <v>4</v>
       </c>
-      <c r="B21" s="240" t="s">
+      <c r="B21" s="267" t="s">
         <v>357</v>
       </c>
-      <c r="C21" s="240"/>
-      <c r="D21" s="240"/>
-      <c r="E21" s="240"/>
-      <c r="F21" s="240"/>
-      <c r="G21" s="240"/>
-      <c r="H21" s="240"/>
-      <c r="I21" s="240"/>
-      <c r="J21" s="240"/>
-      <c r="K21" s="240"/>
-      <c r="L21" s="241"/>
+      <c r="C21" s="267"/>
+      <c r="D21" s="267"/>
+      <c r="E21" s="267"/>
+      <c r="F21" s="267"/>
+      <c r="G21" s="267"/>
+      <c r="H21" s="267"/>
+      <c r="I21" s="267"/>
+      <c r="J21" s="267"/>
+      <c r="K21" s="267"/>
+      <c r="L21" s="268"/>
       <c r="N21" s="106"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="230">
         <v>5</v>
       </c>
-      <c r="B22" s="240" t="s">
+      <c r="B22" s="267" t="s">
         <v>220</v>
       </c>
-      <c r="C22" s="240"/>
-      <c r="D22" s="240"/>
-      <c r="E22" s="240"/>
-      <c r="F22" s="240"/>
-      <c r="G22" s="240"/>
-      <c r="H22" s="240"/>
-      <c r="I22" s="240"/>
-      <c r="J22" s="240"/>
-      <c r="K22" s="240"/>
-      <c r="L22" s="241"/>
+      <c r="C22" s="267"/>
+      <c r="D22" s="267"/>
+      <c r="E22" s="267"/>
+      <c r="F22" s="267"/>
+      <c r="G22" s="267"/>
+      <c r="H22" s="267"/>
+      <c r="I22" s="267"/>
+      <c r="J22" s="267"/>
+      <c r="K22" s="267"/>
+      <c r="L22" s="268"/>
       <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="230"/>
-      <c r="B23" s="240" t="s">
+      <c r="B23" s="267" t="s">
         <v>221</v>
       </c>
-      <c r="C23" s="240"/>
-      <c r="D23" s="240"/>
-      <c r="E23" s="240"/>
-      <c r="F23" s="240"/>
-      <c r="G23" s="240"/>
-      <c r="H23" s="240"/>
-      <c r="I23" s="240"/>
-      <c r="J23" s="240"/>
-      <c r="K23" s="240"/>
-      <c r="L23" s="241"/>
+      <c r="C23" s="267"/>
+      <c r="D23" s="267"/>
+      <c r="E23" s="267"/>
+      <c r="F23" s="267"/>
+      <c r="G23" s="267"/>
+      <c r="H23" s="267"/>
+      <c r="I23" s="267"/>
+      <c r="J23" s="267"/>
+      <c r="K23" s="267"/>
+      <c r="L23" s="268"/>
       <c r="N23" s="106"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="230"/>
-      <c r="B24" s="240" t="s">
+      <c r="B24" s="267" t="s">
         <v>222</v>
       </c>
-      <c r="C24" s="240"/>
-      <c r="D24" s="240"/>
-      <c r="E24" s="240"/>
-      <c r="F24" s="240"/>
-      <c r="G24" s="240"/>
-      <c r="H24" s="240"/>
-      <c r="I24" s="240"/>
-      <c r="J24" s="240"/>
-      <c r="K24" s="240"/>
-      <c r="L24" s="241"/>
+      <c r="C24" s="267"/>
+      <c r="D24" s="267"/>
+      <c r="E24" s="267"/>
+      <c r="F24" s="267"/>
+      <c r="G24" s="267"/>
+      <c r="H24" s="267"/>
+      <c r="I24" s="267"/>
+      <c r="J24" s="267"/>
+      <c r="K24" s="267"/>
+      <c r="L24" s="268"/>
       <c r="N24" s="106"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="249" t="s">
+      <c r="A25" s="269" t="s">
         <v>228</v>
       </c>
-      <c r="B25" s="250"/>
-      <c r="C25" s="250"/>
-      <c r="D25" s="250"/>
-      <c r="E25" s="250"/>
-      <c r="F25" s="250"/>
-      <c r="G25" s="250"/>
-      <c r="H25" s="250"/>
-      <c r="I25" s="250"/>
-      <c r="J25" s="250"/>
-      <c r="K25" s="250"/>
-      <c r="L25" s="251"/>
+      <c r="B25" s="270"/>
+      <c r="C25" s="270"/>
+      <c r="D25" s="270"/>
+      <c r="E25" s="270"/>
+      <c r="F25" s="270"/>
+      <c r="G25" s="270"/>
+      <c r="H25" s="270"/>
+      <c r="I25" s="270"/>
+      <c r="J25" s="270"/>
+      <c r="K25" s="270"/>
+      <c r="L25" s="271"/>
       <c r="N25" s="106"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="230">
         <v>1</v>
       </c>
-      <c r="B26" s="240" t="s">
+      <c r="B26" s="267" t="s">
         <v>223</v>
       </c>
-      <c r="C26" s="240"/>
-      <c r="D26" s="240"/>
-      <c r="E26" s="240"/>
-      <c r="F26" s="240"/>
-      <c r="G26" s="240"/>
-      <c r="H26" s="240"/>
-      <c r="I26" s="240"/>
-      <c r="J26" s="240"/>
-      <c r="K26" s="240"/>
-      <c r="L26" s="241"/>
+      <c r="C26" s="267"/>
+      <c r="D26" s="267"/>
+      <c r="E26" s="267"/>
+      <c r="F26" s="267"/>
+      <c r="G26" s="267"/>
+      <c r="H26" s="267"/>
+      <c r="I26" s="267"/>
+      <c r="J26" s="267"/>
+      <c r="K26" s="267"/>
+      <c r="L26" s="268"/>
       <c r="N26" s="106"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="230"/>
-      <c r="B27" s="238" t="s">
+      <c r="B27" s="265" t="s">
         <v>358</v>
       </c>
-      <c r="C27" s="238"/>
-      <c r="D27" s="238"/>
-      <c r="E27" s="238"/>
-      <c r="F27" s="238"/>
-      <c r="G27" s="238"/>
-      <c r="H27" s="238"/>
-      <c r="I27" s="238"/>
-      <c r="J27" s="238"/>
-      <c r="K27" s="238"/>
-      <c r="L27" s="239"/>
+      <c r="C27" s="265"/>
+      <c r="D27" s="265"/>
+      <c r="E27" s="265"/>
+      <c r="F27" s="265"/>
+      <c r="G27" s="265"/>
+      <c r="H27" s="265"/>
+      <c r="I27" s="265"/>
+      <c r="J27" s="265"/>
+      <c r="K27" s="265"/>
+      <c r="L27" s="266"/>
       <c r="N27" s="106"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="230">
         <v>2</v>
       </c>
-      <c r="B28" s="240" t="s">
+      <c r="B28" s="267" t="s">
         <v>347</v>
       </c>
-      <c r="C28" s="240"/>
-      <c r="D28" s="240"/>
-      <c r="E28" s="240"/>
-      <c r="F28" s="240"/>
-      <c r="G28" s="240"/>
-      <c r="H28" s="240"/>
-      <c r="I28" s="240"/>
-      <c r="J28" s="240"/>
-      <c r="K28" s="240"/>
-      <c r="L28" s="241"/>
+      <c r="C28" s="267"/>
+      <c r="D28" s="267"/>
+      <c r="E28" s="267"/>
+      <c r="F28" s="267"/>
+      <c r="G28" s="267"/>
+      <c r="H28" s="267"/>
+      <c r="I28" s="267"/>
+      <c r="J28" s="267"/>
+      <c r="K28" s="267"/>
+      <c r="L28" s="268"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="230">
         <v>3</v>
       </c>
-      <c r="B29" s="240" t="s">
+      <c r="B29" s="267" t="s">
         <v>336</v>
       </c>
-      <c r="C29" s="240"/>
-      <c r="D29" s="240"/>
-      <c r="E29" s="240"/>
-      <c r="F29" s="240"/>
-      <c r="G29" s="240"/>
-      <c r="H29" s="240"/>
-      <c r="I29" s="240"/>
-      <c r="J29" s="240"/>
-      <c r="K29" s="240"/>
-      <c r="L29" s="241"/>
+      <c r="C29" s="267"/>
+      <c r="D29" s="267"/>
+      <c r="E29" s="267"/>
+      <c r="F29" s="267"/>
+      <c r="G29" s="267"/>
+      <c r="H29" s="267"/>
+      <c r="I29" s="267"/>
+      <c r="J29" s="267"/>
+      <c r="K29" s="267"/>
+      <c r="L29" s="268"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="230">
         <v>4</v>
       </c>
-      <c r="B30" s="240" t="s">
+      <c r="B30" s="267" t="s">
         <v>359</v>
       </c>
-      <c r="C30" s="240"/>
-      <c r="D30" s="240"/>
-      <c r="E30" s="240"/>
-      <c r="F30" s="240"/>
-      <c r="G30" s="240"/>
-      <c r="H30" s="240"/>
-      <c r="I30" s="240"/>
-      <c r="J30" s="240"/>
-      <c r="K30" s="240"/>
-      <c r="L30" s="241"/>
+      <c r="C30" s="267"/>
+      <c r="D30" s="267"/>
+      <c r="E30" s="267"/>
+      <c r="F30" s="267"/>
+      <c r="G30" s="267"/>
+      <c r="H30" s="267"/>
+      <c r="I30" s="267"/>
+      <c r="J30" s="267"/>
+      <c r="K30" s="267"/>
+      <c r="L30" s="268"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="230">
         <v>5</v>
       </c>
-      <c r="B31" s="238" t="s">
+      <c r="B31" s="265" t="s">
         <v>337</v>
       </c>
-      <c r="C31" s="238"/>
-      <c r="D31" s="238"/>
-      <c r="E31" s="238"/>
-      <c r="F31" s="238"/>
-      <c r="G31" s="238"/>
-      <c r="H31" s="238"/>
-      <c r="I31" s="238"/>
-      <c r="J31" s="238"/>
-      <c r="K31" s="238"/>
-      <c r="L31" s="239"/>
+      <c r="C31" s="265"/>
+      <c r="D31" s="265"/>
+      <c r="E31" s="265"/>
+      <c r="F31" s="265"/>
+      <c r="G31" s="265"/>
+      <c r="H31" s="265"/>
+      <c r="I31" s="265"/>
+      <c r="J31" s="265"/>
+      <c r="K31" s="265"/>
+      <c r="L31" s="266"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="230">
         <v>6</v>
       </c>
-      <c r="B32" s="238" t="s">
+      <c r="B32" s="265" t="s">
         <v>342</v>
       </c>
-      <c r="C32" s="238"/>
-      <c r="D32" s="238"/>
-      <c r="E32" s="238"/>
-      <c r="F32" s="238"/>
-      <c r="G32" s="238"/>
-      <c r="H32" s="238"/>
-      <c r="I32" s="238"/>
-      <c r="J32" s="238"/>
-      <c r="K32" s="238"/>
-      <c r="L32" s="239"/>
+      <c r="C32" s="265"/>
+      <c r="D32" s="265"/>
+      <c r="E32" s="265"/>
+      <c r="F32" s="265"/>
+      <c r="G32" s="265"/>
+      <c r="H32" s="265"/>
+      <c r="I32" s="265"/>
+      <c r="J32" s="265"/>
+      <c r="K32" s="265"/>
+      <c r="L32" s="266"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="230">
         <v>7</v>
       </c>
-      <c r="B33" s="240" t="s">
+      <c r="B33" s="267" t="s">
         <v>338</v>
       </c>
-      <c r="C33" s="240"/>
-      <c r="D33" s="240"/>
-      <c r="E33" s="240"/>
-      <c r="F33" s="240"/>
-      <c r="G33" s="240"/>
-      <c r="H33" s="240"/>
-      <c r="I33" s="240"/>
-      <c r="J33" s="240"/>
-      <c r="K33" s="240"/>
-      <c r="L33" s="241"/>
+      <c r="C33" s="267"/>
+      <c r="D33" s="267"/>
+      <c r="E33" s="267"/>
+      <c r="F33" s="267"/>
+      <c r="G33" s="267"/>
+      <c r="H33" s="267"/>
+      <c r="I33" s="267"/>
+      <c r="J33" s="267"/>
+      <c r="K33" s="267"/>
+      <c r="L33" s="268"/>
     </row>
     <row r="34" spans="1:12" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="230"/>
@@ -15460,56 +15466,56 @@
       <c r="L34" s="232"/>
     </row>
     <row r="35" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="249" t="s">
+      <c r="A35" s="269" t="s">
         <v>341</v>
       </c>
-      <c r="B35" s="250"/>
-      <c r="C35" s="250"/>
-      <c r="D35" s="250"/>
-      <c r="E35" s="250"/>
-      <c r="F35" s="250"/>
-      <c r="G35" s="250"/>
-      <c r="H35" s="250"/>
-      <c r="I35" s="250"/>
-      <c r="J35" s="250"/>
-      <c r="K35" s="250"/>
-      <c r="L35" s="251"/>
+      <c r="B35" s="270"/>
+      <c r="C35" s="270"/>
+      <c r="D35" s="270"/>
+      <c r="E35" s="270"/>
+      <c r="F35" s="270"/>
+      <c r="G35" s="270"/>
+      <c r="H35" s="270"/>
+      <c r="I35" s="270"/>
+      <c r="J35" s="270"/>
+      <c r="K35" s="270"/>
+      <c r="L35" s="271"/>
     </row>
     <row r="36" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="233" t="s">
         <v>339</v>
       </c>
-      <c r="B36" s="240" t="s">
+      <c r="B36" s="267" t="s">
         <v>224</v>
       </c>
-      <c r="C36" s="240"/>
-      <c r="D36" s="240"/>
-      <c r="E36" s="240"/>
-      <c r="F36" s="240"/>
-      <c r="G36" s="240"/>
-      <c r="H36" s="240"/>
-      <c r="I36" s="240"/>
-      <c r="J36" s="240"/>
-      <c r="K36" s="240"/>
-      <c r="L36" s="241"/>
+      <c r="C36" s="267"/>
+      <c r="D36" s="267"/>
+      <c r="E36" s="267"/>
+      <c r="F36" s="267"/>
+      <c r="G36" s="267"/>
+      <c r="H36" s="267"/>
+      <c r="I36" s="267"/>
+      <c r="J36" s="267"/>
+      <c r="K36" s="267"/>
+      <c r="L36" s="268"/>
     </row>
     <row r="37" spans="1:12" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="234" t="s">
         <v>340</v>
       </c>
-      <c r="B37" s="242" t="s">
+      <c r="B37" s="273" t="s">
         <v>343</v>
       </c>
-      <c r="C37" s="242"/>
-      <c r="D37" s="242"/>
-      <c r="E37" s="242"/>
-      <c r="F37" s="242"/>
-      <c r="G37" s="242"/>
-      <c r="H37" s="242"/>
-      <c r="I37" s="242"/>
-      <c r="J37" s="242"/>
-      <c r="K37" s="242"/>
-      <c r="L37" s="243"/>
+      <c r="C37" s="273"/>
+      <c r="D37" s="273"/>
+      <c r="E37" s="273"/>
+      <c r="F37" s="273"/>
+      <c r="G37" s="273"/>
+      <c r="H37" s="273"/>
+      <c r="I37" s="273"/>
+      <c r="J37" s="273"/>
+      <c r="K37" s="273"/>
+      <c r="L37" s="274"/>
     </row>
     <row r="38" spans="1:12" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="161"/>
@@ -15526,20 +15532,20 @@
       <c r="L38" s="113"/>
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="244" t="s">
+      <c r="A39" s="275" t="s">
         <v>252</v>
       </c>
-      <c r="B39" s="245"/>
-      <c r="C39" s="245"/>
-      <c r="D39" s="245"/>
-      <c r="E39" s="245"/>
-      <c r="F39" s="245"/>
-      <c r="G39" s="245"/>
-      <c r="H39" s="245"/>
-      <c r="I39" s="245"/>
-      <c r="J39" s="245"/>
-      <c r="K39" s="245"/>
-      <c r="L39" s="246"/>
+      <c r="B39" s="276"/>
+      <c r="C39" s="276"/>
+      <c r="D39" s="276"/>
+      <c r="E39" s="276"/>
+      <c r="F39" s="276"/>
+      <c r="G39" s="276"/>
+      <c r="H39" s="276"/>
+      <c r="I39" s="276"/>
+      <c r="J39" s="276"/>
+      <c r="K39" s="276"/>
+      <c r="L39" s="277"/>
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="162" t="s">
@@ -15627,72 +15633,72 @@
       <c r="B45" s="170" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="247" t="s">
+      <c r="C45" s="255" t="s">
         <v>326</v>
       </c>
-      <c r="D45" s="247"/>
-      <c r="E45" s="247"/>
-      <c r="F45" s="247"/>
-      <c r="G45" s="247"/>
-      <c r="H45" s="247"/>
-      <c r="I45" s="247"/>
-      <c r="J45" s="247"/>
-      <c r="K45" s="247"/>
-      <c r="L45" s="248"/>
+      <c r="D45" s="255"/>
+      <c r="E45" s="255"/>
+      <c r="F45" s="255"/>
+      <c r="G45" s="255"/>
+      <c r="H45" s="255"/>
+      <c r="I45" s="255"/>
+      <c r="J45" s="255"/>
+      <c r="K45" s="255"/>
+      <c r="L45" s="256"/>
     </row>
     <row r="46" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="169"/>
       <c r="B46" s="170" t="s">
         <v>146</v>
       </c>
-      <c r="C46" s="247" t="s">
+      <c r="C46" s="255" t="s">
         <v>147</v>
       </c>
-      <c r="D46" s="247"/>
-      <c r="E46" s="247"/>
-      <c r="F46" s="247"/>
-      <c r="G46" s="247"/>
-      <c r="H46" s="247"/>
-      <c r="I46" s="247"/>
-      <c r="J46" s="247"/>
-      <c r="K46" s="247"/>
-      <c r="L46" s="248"/>
+      <c r="D46" s="255"/>
+      <c r="E46" s="255"/>
+      <c r="F46" s="255"/>
+      <c r="G46" s="255"/>
+      <c r="H46" s="255"/>
+      <c r="I46" s="255"/>
+      <c r="J46" s="255"/>
+      <c r="K46" s="255"/>
+      <c r="L46" s="256"/>
     </row>
     <row r="47" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="169"/>
       <c r="B47" s="170" t="s">
         <v>250</v>
       </c>
-      <c r="C47" s="247" t="s">
+      <c r="C47" s="255" t="s">
         <v>251</v>
       </c>
-      <c r="D47" s="247"/>
-      <c r="E47" s="247"/>
-      <c r="F47" s="247"/>
-      <c r="G47" s="247"/>
-      <c r="H47" s="247"/>
-      <c r="I47" s="247"/>
-      <c r="J47" s="247"/>
-      <c r="K47" s="247"/>
-      <c r="L47" s="248"/>
+      <c r="D47" s="255"/>
+      <c r="E47" s="255"/>
+      <c r="F47" s="255"/>
+      <c r="G47" s="255"/>
+      <c r="H47" s="255"/>
+      <c r="I47" s="255"/>
+      <c r="J47" s="255"/>
+      <c r="K47" s="255"/>
+      <c r="L47" s="256"/>
     </row>
     <row r="48" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="169"/>
       <c r="B48" s="170" t="s">
         <v>327</v>
       </c>
-      <c r="C48" s="247" t="s">
+      <c r="C48" s="255" t="s">
         <v>328</v>
       </c>
-      <c r="D48" s="247"/>
-      <c r="E48" s="247"/>
-      <c r="F48" s="247"/>
-      <c r="G48" s="247"/>
-      <c r="H48" s="247"/>
-      <c r="I48" s="247"/>
-      <c r="J48" s="247"/>
-      <c r="K48" s="247"/>
-      <c r="L48" s="248"/>
+      <c r="D48" s="255"/>
+      <c r="E48" s="255"/>
+      <c r="F48" s="255"/>
+      <c r="G48" s="255"/>
+      <c r="H48" s="255"/>
+      <c r="I48" s="255"/>
+      <c r="J48" s="255"/>
+      <c r="K48" s="255"/>
+      <c r="L48" s="256"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="169"/>
@@ -15717,18 +15723,18 @@
       <c r="B50" s="170" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="247" t="s">
+      <c r="C50" s="255" t="s">
         <v>330</v>
       </c>
-      <c r="D50" s="247"/>
-      <c r="E50" s="247"/>
-      <c r="F50" s="247"/>
-      <c r="G50" s="247"/>
-      <c r="H50" s="247"/>
-      <c r="I50" s="247"/>
-      <c r="J50" s="247"/>
-      <c r="K50" s="247"/>
-      <c r="L50" s="248"/>
+      <c r="D50" s="255"/>
+      <c r="E50" s="255"/>
+      <c r="F50" s="255"/>
+      <c r="G50" s="255"/>
+      <c r="H50" s="255"/>
+      <c r="I50" s="255"/>
+      <c r="J50" s="255"/>
+      <c r="K50" s="255"/>
+      <c r="L50" s="256"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="169"/>
@@ -15810,25 +15816,51 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="237" t="s">
+      <c r="A64" s="272" t="s">
         <v>332</v>
       </c>
-      <c r="B64" s="237"/>
-      <c r="C64" s="237"/>
-      <c r="D64" s="237"/>
-      <c r="E64" s="237"/>
-      <c r="F64" s="237"/>
-      <c r="G64" s="237"/>
-      <c r="H64" s="237"/>
-      <c r="I64" s="237"/>
-      <c r="J64" s="237"/>
-      <c r="K64" s="237"/>
-      <c r="L64" s="237"/>
+      <c r="B64" s="272"/>
+      <c r="C64" s="272"/>
+      <c r="D64" s="272"/>
+      <c r="E64" s="272"/>
+      <c r="F64" s="272"/>
+      <c r="G64" s="272"/>
+      <c r="H64" s="272"/>
+      <c r="I64" s="272"/>
+      <c r="J64" s="272"/>
+      <c r="K64" s="272"/>
+      <c r="L64" s="272"/>
     </row>
     <row r="69" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="70" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A64:L64"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="C45:L45"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="C48:L48"/>
+    <mergeCell ref="C50:L50"/>
+    <mergeCell ref="A35:L35"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B18:L18"/>
+    <mergeCell ref="B19:L19"/>
+    <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="B22:L22"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="B26:L26"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B30:L30"/>
     <mergeCell ref="A17:L17"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A4:L4"/>
@@ -15843,32 +15875,6 @@
     <mergeCell ref="A16:L16"/>
     <mergeCell ref="B7:L7"/>
     <mergeCell ref="B8:L8"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B18:L18"/>
-    <mergeCell ref="B19:L19"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="B22:L22"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="B24:L24"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="B26:L26"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="A64:L64"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="C45:L45"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="C47:L47"/>
-    <mergeCell ref="C48:L48"/>
-    <mergeCell ref="C50:L50"/>
-    <mergeCell ref="A35:L35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A57" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -16000,7 +16006,7 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16122,12 +16128,24 @@
       <c r="K4" s="40"/>
     </row>
     <row r="5" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="57"/>
-      <c r="B5" s="150"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
+      <c r="A5" s="57">
+        <v>45622</v>
+      </c>
+      <c r="B5" s="150" t="s">
+        <v>365</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>366</v>
+      </c>
+      <c r="D5" s="55">
+        <v>4</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>297</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>297</v>
+      </c>
       <c r="G5" s="57"/>
       <c r="I5" s="38"/>
       <c r="J5" s="38"/>
@@ -16526,8 +16544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BF7D8F-86F3-47E9-AB85-EE9B4CAB70E4}">
   <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N35" sqref="N35"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N45" sqref="N45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16714,8 +16732,8 @@
       <c r="C14" s="280"/>
       <c r="D14" s="281"/>
       <c r="F14">
-        <f>0.95/2</f>
-        <v>0.47499999999999998</v>
+        <f>4.5/7.2</f>
+        <v>0.625</v>
       </c>
       <c r="N14" s="142"/>
     </row>
@@ -16725,6 +16743,10 @@
       </c>
       <c r="C15" s="283"/>
       <c r="D15" s="284"/>
+      <c r="F15">
+        <f>F14*0.4</f>
+        <v>0.25</v>
+      </c>
       <c r="N15" s="142"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -17495,7 +17517,7 @@
       </c>
       <c r="N41" s="142"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>156</v>
       </c>
@@ -17550,7 +17572,7 @@
       </c>
       <c r="N43" s="142"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -21256,7 +21278,7 @@
     <hyperlink ref="N29" r:id="rId11" location="2a-intervening-grand-canyon-flow" xr:uid="{CFD884C0-2149-42F6-AD5A-482CF40D5292}"/>
     <hyperlink ref="N30" r:id="rId12" location="2b-mead-to-imperial-dam-intervening-flow" xr:uid="{B8EF30C2-739D-4E21-B63A-F17F9947326A}"/>
     <hyperlink ref="N31" r:id="rId13" location="2c-havasuparker-evaporation-and-evapotranspiration" xr:uid="{70E7AC6A-42AC-4DE1-ADFB-FBA8230C308E}"/>
-    <hyperlink ref="N35" r:id="rId14" location="step-3-split-existing-reservoir-storage-among-accounts-year-1-only" xr:uid="{B36B453C-62F8-4461-8E49-8546C848C695}"/>
+    <hyperlink ref="N35" r:id="rId14" location="step-3-split-existing-lake-mead-storage-among-accounts-year-1-only" xr:uid="{B36B453C-62F8-4461-8E49-8546C848C695}"/>
     <hyperlink ref="N42" r:id="rId15" location="3a-begin-of-year-reservoir-storage" xr:uid="{52EB1038-72CB-4676-AD3B-3DD4322D2D3C}"/>
     <hyperlink ref="N45" r:id="rId16" location="3b-calculate-powell--mead-evaporation" display="Help Powell + Mead evaporation" xr:uid="{9002111C-2D36-45B1-97D8-5FCB363BD9BD}"/>
     <hyperlink ref="N52" r:id="rId17" location="3c-calculate-mexico-water-allocation" xr:uid="{C14FC6B3-6E3C-48F5-B820-A74ADC9C86D6}"/>
@@ -22701,16 +22723,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="313" t="e">
+      <c r="A1" s="312" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="313"/>
-      <c r="C1" s="313"/>
-      <c r="D1" s="313"/>
-      <c r="E1" s="313"/>
-      <c r="F1" s="313"/>
-      <c r="G1" s="313"/>
+      <c r="B1" s="312"/>
+      <c r="C1" s="312"/>
+      <c r="D1" s="312"/>
+      <c r="E1" s="312"/>
+      <c r="F1" s="312"/>
+      <c r="G1" s="312"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -22819,11 +22841,11 @@
         <v>81</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="312"/>
-      <c r="D10" s="312"/>
-      <c r="E10" s="312"/>
-      <c r="F10" s="312"/>
-      <c r="G10" s="312"/>
+      <c r="C10" s="313"/>
+      <c r="D10" s="313"/>
+      <c r="E10" s="313"/>
+      <c r="F10" s="313"/>
+      <c r="G10" s="313"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -24086,12 +24108,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -24099,6 +24115,12 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>

</xml_diff>

<commit_message>
Update split reservoir inflow section
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F91525-51E4-4BEE-BF86-CEBC1288EB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D04564-6EA5-4C99-817F-320F10F431F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="368">
   <si>
     <t>Year 1</t>
   </si>
@@ -1927,6 +1927,9 @@
   <si>
     <t>Start documenting model with instructions and user guide.</t>
   </si>
+  <si>
+    <t>Help allocate reservoir inflow</t>
+  </si>
 </sst>
 </file>
 
@@ -3203,6 +3206,51 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3257,12 +3305,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3286,45 +3328,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="3" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="4" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3428,11 +3431,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14872,20 +14875,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="240" t="s">
+      <c r="A1" s="255" t="s">
         <v>321</v>
       </c>
-      <c r="B1" s="240"/>
-      <c r="C1" s="240"/>
-      <c r="D1" s="240"/>
-      <c r="E1" s="240"/>
-      <c r="F1" s="240"/>
-      <c r="G1" s="240"/>
-      <c r="H1" s="240"/>
-      <c r="I1" s="240"/>
-      <c r="J1" s="240"/>
-      <c r="K1" s="240"/>
-      <c r="L1" s="240"/>
+      <c r="B1" s="255"/>
+      <c r="C1" s="255"/>
+      <c r="D1" s="255"/>
+      <c r="E1" s="255"/>
+      <c r="F1" s="255"/>
+      <c r="G1" s="255"/>
+      <c r="H1" s="255"/>
+      <c r="I1" s="255"/>
+      <c r="J1" s="255"/>
+      <c r="K1" s="255"/>
+      <c r="L1" s="255"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -14911,41 +14914,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="241" t="s">
+      <c r="A4" s="256" t="s">
         <v>349</v>
       </c>
-      <c r="B4" s="242"/>
-      <c r="C4" s="242"/>
-      <c r="D4" s="242"/>
-      <c r="E4" s="242"/>
-      <c r="F4" s="242"/>
-      <c r="G4" s="242"/>
-      <c r="H4" s="242"/>
-      <c r="I4" s="242"/>
-      <c r="J4" s="242"/>
-      <c r="K4" s="242"/>
-      <c r="L4" s="243"/>
-      <c r="N4" s="244"/>
-      <c r="O4" s="244"/>
-      <c r="P4" s="244"/>
-      <c r="Q4" s="244"/>
-      <c r="R4" s="244"/>
+      <c r="B4" s="257"/>
+      <c r="C4" s="257"/>
+      <c r="D4" s="257"/>
+      <c r="E4" s="257"/>
+      <c r="F4" s="257"/>
+      <c r="G4" s="257"/>
+      <c r="H4" s="257"/>
+      <c r="I4" s="257"/>
+      <c r="J4" s="257"/>
+      <c r="K4" s="257"/>
+      <c r="L4" s="258"/>
+      <c r="N4" s="259"/>
+      <c r="O4" s="259"/>
+      <c r="P4" s="259"/>
+      <c r="Q4" s="259"/>
+      <c r="R4" s="259"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="245" t="s">
+      <c r="A5" s="260" t="s">
         <v>350</v>
       </c>
-      <c r="B5" s="246"/>
-      <c r="C5" s="246"/>
-      <c r="D5" s="246"/>
-      <c r="E5" s="246"/>
-      <c r="F5" s="246"/>
-      <c r="G5" s="246"/>
-      <c r="H5" s="246"/>
-      <c r="I5" s="246"/>
-      <c r="J5" s="246"/>
-      <c r="K5" s="246"/>
-      <c r="L5" s="247"/>
+      <c r="B5" s="261"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
+      <c r="G5" s="261"/>
+      <c r="H5" s="261"/>
+      <c r="I5" s="261"/>
+      <c r="J5" s="261"/>
+      <c r="K5" s="261"/>
+      <c r="L5" s="262"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -14953,20 +14956,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="245" t="s">
+      <c r="A6" s="260" t="s">
         <v>352</v>
       </c>
-      <c r="B6" s="246"/>
-      <c r="C6" s="246"/>
-      <c r="D6" s="246"/>
-      <c r="E6" s="246"/>
-      <c r="F6" s="246"/>
-      <c r="G6" s="246"/>
-      <c r="H6" s="246"/>
-      <c r="I6" s="246"/>
-      <c r="J6" s="246"/>
-      <c r="K6" s="246"/>
-      <c r="L6" s="247"/>
+      <c r="B6" s="261"/>
+      <c r="C6" s="261"/>
+      <c r="D6" s="261"/>
+      <c r="E6" s="261"/>
+      <c r="F6" s="261"/>
+      <c r="G6" s="261"/>
+      <c r="H6" s="261"/>
+      <c r="I6" s="261"/>
+      <c r="J6" s="261"/>
+      <c r="K6" s="261"/>
+      <c r="L6" s="262"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -14975,19 +14978,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="235"/>
-      <c r="B7" s="246" t="s">
+      <c r="B7" s="261" t="s">
         <v>353</v>
       </c>
-      <c r="C7" s="246"/>
-      <c r="D7" s="246"/>
-      <c r="E7" s="246"/>
-      <c r="F7" s="246"/>
-      <c r="G7" s="246"/>
-      <c r="H7" s="246"/>
-      <c r="I7" s="246"/>
-      <c r="J7" s="246"/>
-      <c r="K7" s="246"/>
-      <c r="L7" s="247"/>
+      <c r="C7" s="261"/>
+      <c r="D7" s="261"/>
+      <c r="E7" s="261"/>
+      <c r="F7" s="261"/>
+      <c r="G7" s="261"/>
+      <c r="H7" s="261"/>
+      <c r="I7" s="261"/>
+      <c r="J7" s="261"/>
+      <c r="K7" s="261"/>
+      <c r="L7" s="262"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -14996,19 +14999,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="236"/>
-      <c r="B8" s="263" t="s">
+      <c r="B8" s="276" t="s">
         <v>354</v>
       </c>
-      <c r="C8" s="263"/>
-      <c r="D8" s="263"/>
-      <c r="E8" s="263"/>
-      <c r="F8" s="263"/>
-      <c r="G8" s="263"/>
-      <c r="H8" s="263"/>
-      <c r="I8" s="263"/>
-      <c r="J8" s="263"/>
-      <c r="K8" s="263"/>
-      <c r="L8" s="264"/>
+      <c r="C8" s="276"/>
+      <c r="D8" s="276"/>
+      <c r="E8" s="276"/>
+      <c r="F8" s="276"/>
+      <c r="G8" s="276"/>
+      <c r="H8" s="276"/>
+      <c r="I8" s="276"/>
+      <c r="J8" s="276"/>
+      <c r="K8" s="276"/>
+      <c r="L8" s="277"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15030,84 +15033,84 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="248" t="s">
+      <c r="A10" s="263" t="s">
         <v>217</v>
       </c>
-      <c r="B10" s="249"/>
-      <c r="C10" s="249"/>
-      <c r="D10" s="249"/>
-      <c r="E10" s="249"/>
-      <c r="F10" s="249"/>
-      <c r="G10" s="249"/>
-      <c r="H10" s="249"/>
-      <c r="I10" s="249"/>
-      <c r="J10" s="249"/>
-      <c r="K10" s="249"/>
-      <c r="L10" s="250"/>
+      <c r="B10" s="264"/>
+      <c r="C10" s="264"/>
+      <c r="D10" s="264"/>
+      <c r="E10" s="264"/>
+      <c r="F10" s="264"/>
+      <c r="G10" s="264"/>
+      <c r="H10" s="264"/>
+      <c r="I10" s="264"/>
+      <c r="J10" s="264"/>
+      <c r="K10" s="264"/>
+      <c r="L10" s="265"/>
     </row>
     <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="251" t="s">
+      <c r="A11" s="266" t="s">
         <v>351</v>
       </c>
-      <c r="B11" s="252"/>
-      <c r="C11" s="252"/>
-      <c r="D11" s="252"/>
-      <c r="E11" s="252"/>
-      <c r="F11" s="252"/>
-      <c r="G11" s="252"/>
-      <c r="H11" s="252"/>
-      <c r="I11" s="252"/>
-      <c r="J11" s="252"/>
-      <c r="K11" s="252"/>
-      <c r="L11" s="253"/>
+      <c r="B11" s="267"/>
+      <c r="C11" s="267"/>
+      <c r="D11" s="267"/>
+      <c r="E11" s="267"/>
+      <c r="F11" s="267"/>
+      <c r="G11" s="267"/>
+      <c r="H11" s="267"/>
+      <c r="I11" s="267"/>
+      <c r="J11" s="267"/>
+      <c r="K11" s="267"/>
+      <c r="L11" s="268"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="254" t="s">
+      <c r="A12" s="269" t="s">
         <v>355</v>
       </c>
-      <c r="B12" s="255"/>
-      <c r="C12" s="255"/>
-      <c r="D12" s="255"/>
-      <c r="E12" s="255"/>
-      <c r="F12" s="255"/>
-      <c r="G12" s="255"/>
-      <c r="H12" s="255"/>
-      <c r="I12" s="255"/>
-      <c r="J12" s="255"/>
-      <c r="K12" s="255"/>
-      <c r="L12" s="256"/>
+      <c r="B12" s="247"/>
+      <c r="C12" s="247"/>
+      <c r="D12" s="247"/>
+      <c r="E12" s="247"/>
+      <c r="F12" s="247"/>
+      <c r="G12" s="247"/>
+      <c r="H12" s="247"/>
+      <c r="I12" s="247"/>
+      <c r="J12" s="247"/>
+      <c r="K12" s="247"/>
+      <c r="L12" s="248"/>
     </row>
     <row r="13" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="254" t="s">
+      <c r="A13" s="269" t="s">
         <v>218</v>
       </c>
-      <c r="B13" s="255"/>
-      <c r="C13" s="255"/>
-      <c r="D13" s="255"/>
-      <c r="E13" s="255"/>
-      <c r="F13" s="255"/>
-      <c r="G13" s="255"/>
-      <c r="H13" s="255"/>
-      <c r="I13" s="255"/>
-      <c r="J13" s="255"/>
-      <c r="K13" s="255"/>
-      <c r="L13" s="256"/>
+      <c r="B13" s="247"/>
+      <c r="C13" s="247"/>
+      <c r="D13" s="247"/>
+      <c r="E13" s="247"/>
+      <c r="F13" s="247"/>
+      <c r="G13" s="247"/>
+      <c r="H13" s="247"/>
+      <c r="I13" s="247"/>
+      <c r="J13" s="247"/>
+      <c r="K13" s="247"/>
+      <c r="L13" s="248"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="257" t="s">
+      <c r="A14" s="270" t="s">
         <v>356</v>
       </c>
-      <c r="B14" s="258"/>
-      <c r="C14" s="258"/>
-      <c r="D14" s="258"/>
-      <c r="E14" s="258"/>
-      <c r="F14" s="258"/>
-      <c r="G14" s="258"/>
-      <c r="H14" s="258"/>
-      <c r="I14" s="258"/>
-      <c r="J14" s="258"/>
-      <c r="K14" s="258"/>
-      <c r="L14" s="259"/>
+      <c r="B14" s="271"/>
+      <c r="C14" s="271"/>
+      <c r="D14" s="271"/>
+      <c r="E14" s="271"/>
+      <c r="F14" s="271"/>
+      <c r="G14" s="271"/>
+      <c r="H14" s="271"/>
+      <c r="I14" s="271"/>
+      <c r="J14" s="271"/>
+      <c r="K14" s="271"/>
+      <c r="L14" s="272"/>
     </row>
     <row r="15" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="113"/>
@@ -15124,332 +15127,332 @@
       <c r="L15" s="113"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="260" t="s">
+      <c r="A16" s="273" t="s">
         <v>348</v>
       </c>
-      <c r="B16" s="261"/>
-      <c r="C16" s="261"/>
-      <c r="D16" s="261"/>
-      <c r="E16" s="261"/>
-      <c r="F16" s="261"/>
-      <c r="G16" s="261"/>
-      <c r="H16" s="261"/>
-      <c r="I16" s="261"/>
-      <c r="J16" s="261"/>
-      <c r="K16" s="261"/>
-      <c r="L16" s="262"/>
+      <c r="B16" s="274"/>
+      <c r="C16" s="274"/>
+      <c r="D16" s="274"/>
+      <c r="E16" s="274"/>
+      <c r="F16" s="274"/>
+      <c r="G16" s="274"/>
+      <c r="H16" s="274"/>
+      <c r="I16" s="274"/>
+      <c r="J16" s="274"/>
+      <c r="K16" s="274"/>
+      <c r="L16" s="275"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="237" t="s">
+      <c r="A17" s="252" t="s">
         <v>227</v>
       </c>
-      <c r="B17" s="238"/>
-      <c r="C17" s="238"/>
-      <c r="D17" s="238"/>
-      <c r="E17" s="238"/>
-      <c r="F17" s="238"/>
-      <c r="G17" s="238"/>
-      <c r="H17" s="238"/>
-      <c r="I17" s="238"/>
-      <c r="J17" s="238"/>
-      <c r="K17" s="238"/>
-      <c r="L17" s="239"/>
+      <c r="B17" s="253"/>
+      <c r="C17" s="253"/>
+      <c r="D17" s="253"/>
+      <c r="E17" s="253"/>
+      <c r="F17" s="253"/>
+      <c r="G17" s="253"/>
+      <c r="H17" s="253"/>
+      <c r="I17" s="253"/>
+      <c r="J17" s="253"/>
+      <c r="K17" s="253"/>
+      <c r="L17" s="254"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="230">
         <v>1</v>
       </c>
-      <c r="B18" s="267" t="s">
+      <c r="B18" s="240" t="s">
         <v>226</v>
       </c>
-      <c r="C18" s="267"/>
-      <c r="D18" s="267"/>
-      <c r="E18" s="267"/>
-      <c r="F18" s="267"/>
-      <c r="G18" s="267"/>
-      <c r="H18" s="267"/>
-      <c r="I18" s="267"/>
-      <c r="J18" s="267"/>
-      <c r="K18" s="267"/>
-      <c r="L18" s="268"/>
+      <c r="C18" s="240"/>
+      <c r="D18" s="240"/>
+      <c r="E18" s="240"/>
+      <c r="F18" s="240"/>
+      <c r="G18" s="240"/>
+      <c r="H18" s="240"/>
+      <c r="I18" s="240"/>
+      <c r="J18" s="240"/>
+      <c r="K18" s="240"/>
+      <c r="L18" s="241"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="230">
         <v>2</v>
       </c>
-      <c r="B19" s="267" t="s">
+      <c r="B19" s="240" t="s">
         <v>344</v>
       </c>
-      <c r="C19" s="267"/>
-      <c r="D19" s="267"/>
-      <c r="E19" s="267"/>
-      <c r="F19" s="267"/>
-      <c r="G19" s="267"/>
-      <c r="H19" s="267"/>
-      <c r="I19" s="267"/>
-      <c r="J19" s="267"/>
-      <c r="K19" s="267"/>
-      <c r="L19" s="268"/>
+      <c r="C19" s="240"/>
+      <c r="D19" s="240"/>
+      <c r="E19" s="240"/>
+      <c r="F19" s="240"/>
+      <c r="G19" s="240"/>
+      <c r="H19" s="240"/>
+      <c r="I19" s="240"/>
+      <c r="J19" s="240"/>
+      <c r="K19" s="240"/>
+      <c r="L19" s="241"/>
       <c r="N19" s="106"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="230">
         <v>3</v>
       </c>
-      <c r="B20" s="267" t="s">
+      <c r="B20" s="240" t="s">
         <v>219</v>
       </c>
-      <c r="C20" s="267"/>
-      <c r="D20" s="267"/>
-      <c r="E20" s="267"/>
-      <c r="F20" s="267"/>
-      <c r="G20" s="267"/>
-      <c r="H20" s="267"/>
-      <c r="I20" s="267"/>
-      <c r="J20" s="267"/>
-      <c r="K20" s="267"/>
-      <c r="L20" s="268"/>
+      <c r="C20" s="240"/>
+      <c r="D20" s="240"/>
+      <c r="E20" s="240"/>
+      <c r="F20" s="240"/>
+      <c r="G20" s="240"/>
+      <c r="H20" s="240"/>
+      <c r="I20" s="240"/>
+      <c r="J20" s="240"/>
+      <c r="K20" s="240"/>
+      <c r="L20" s="241"/>
       <c r="N20" s="106"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="230">
         <v>4</v>
       </c>
-      <c r="B21" s="267" t="s">
+      <c r="B21" s="240" t="s">
         <v>357</v>
       </c>
-      <c r="C21" s="267"/>
-      <c r="D21" s="267"/>
-      <c r="E21" s="267"/>
-      <c r="F21" s="267"/>
-      <c r="G21" s="267"/>
-      <c r="H21" s="267"/>
-      <c r="I21" s="267"/>
-      <c r="J21" s="267"/>
-      <c r="K21" s="267"/>
-      <c r="L21" s="268"/>
+      <c r="C21" s="240"/>
+      <c r="D21" s="240"/>
+      <c r="E21" s="240"/>
+      <c r="F21" s="240"/>
+      <c r="G21" s="240"/>
+      <c r="H21" s="240"/>
+      <c r="I21" s="240"/>
+      <c r="J21" s="240"/>
+      <c r="K21" s="240"/>
+      <c r="L21" s="241"/>
       <c r="N21" s="106"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="230">
         <v>5</v>
       </c>
-      <c r="B22" s="267" t="s">
+      <c r="B22" s="240" t="s">
         <v>220</v>
       </c>
-      <c r="C22" s="267"/>
-      <c r="D22" s="267"/>
-      <c r="E22" s="267"/>
-      <c r="F22" s="267"/>
-      <c r="G22" s="267"/>
-      <c r="H22" s="267"/>
-      <c r="I22" s="267"/>
-      <c r="J22" s="267"/>
-      <c r="K22" s="267"/>
-      <c r="L22" s="268"/>
+      <c r="C22" s="240"/>
+      <c r="D22" s="240"/>
+      <c r="E22" s="240"/>
+      <c r="F22" s="240"/>
+      <c r="G22" s="240"/>
+      <c r="H22" s="240"/>
+      <c r="I22" s="240"/>
+      <c r="J22" s="240"/>
+      <c r="K22" s="240"/>
+      <c r="L22" s="241"/>
       <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="230"/>
-      <c r="B23" s="267" t="s">
+      <c r="B23" s="240" t="s">
         <v>221</v>
       </c>
-      <c r="C23" s="267"/>
-      <c r="D23" s="267"/>
-      <c r="E23" s="267"/>
-      <c r="F23" s="267"/>
-      <c r="G23" s="267"/>
-      <c r="H23" s="267"/>
-      <c r="I23" s="267"/>
-      <c r="J23" s="267"/>
-      <c r="K23" s="267"/>
-      <c r="L23" s="268"/>
+      <c r="C23" s="240"/>
+      <c r="D23" s="240"/>
+      <c r="E23" s="240"/>
+      <c r="F23" s="240"/>
+      <c r="G23" s="240"/>
+      <c r="H23" s="240"/>
+      <c r="I23" s="240"/>
+      <c r="J23" s="240"/>
+      <c r="K23" s="240"/>
+      <c r="L23" s="241"/>
       <c r="N23" s="106"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="230"/>
-      <c r="B24" s="267" t="s">
+      <c r="B24" s="240" t="s">
         <v>222</v>
       </c>
-      <c r="C24" s="267"/>
-      <c r="D24" s="267"/>
-      <c r="E24" s="267"/>
-      <c r="F24" s="267"/>
-      <c r="G24" s="267"/>
-      <c r="H24" s="267"/>
-      <c r="I24" s="267"/>
-      <c r="J24" s="267"/>
-      <c r="K24" s="267"/>
-      <c r="L24" s="268"/>
+      <c r="C24" s="240"/>
+      <c r="D24" s="240"/>
+      <c r="E24" s="240"/>
+      <c r="F24" s="240"/>
+      <c r="G24" s="240"/>
+      <c r="H24" s="240"/>
+      <c r="I24" s="240"/>
+      <c r="J24" s="240"/>
+      <c r="K24" s="240"/>
+      <c r="L24" s="241"/>
       <c r="N24" s="106"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="269" t="s">
+      <c r="A25" s="249" t="s">
         <v>228</v>
       </c>
-      <c r="B25" s="270"/>
-      <c r="C25" s="270"/>
-      <c r="D25" s="270"/>
-      <c r="E25" s="270"/>
-      <c r="F25" s="270"/>
-      <c r="G25" s="270"/>
-      <c r="H25" s="270"/>
-      <c r="I25" s="270"/>
-      <c r="J25" s="270"/>
-      <c r="K25" s="270"/>
-      <c r="L25" s="271"/>
+      <c r="B25" s="250"/>
+      <c r="C25" s="250"/>
+      <c r="D25" s="250"/>
+      <c r="E25" s="250"/>
+      <c r="F25" s="250"/>
+      <c r="G25" s="250"/>
+      <c r="H25" s="250"/>
+      <c r="I25" s="250"/>
+      <c r="J25" s="250"/>
+      <c r="K25" s="250"/>
+      <c r="L25" s="251"/>
       <c r="N25" s="106"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="230">
         <v>1</v>
       </c>
-      <c r="B26" s="267" t="s">
+      <c r="B26" s="240" t="s">
         <v>223</v>
       </c>
-      <c r="C26" s="267"/>
-      <c r="D26" s="267"/>
-      <c r="E26" s="267"/>
-      <c r="F26" s="267"/>
-      <c r="G26" s="267"/>
-      <c r="H26" s="267"/>
-      <c r="I26" s="267"/>
-      <c r="J26" s="267"/>
-      <c r="K26" s="267"/>
-      <c r="L26" s="268"/>
+      <c r="C26" s="240"/>
+      <c r="D26" s="240"/>
+      <c r="E26" s="240"/>
+      <c r="F26" s="240"/>
+      <c r="G26" s="240"/>
+      <c r="H26" s="240"/>
+      <c r="I26" s="240"/>
+      <c r="J26" s="240"/>
+      <c r="K26" s="240"/>
+      <c r="L26" s="241"/>
       <c r="N26" s="106"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="230"/>
-      <c r="B27" s="265" t="s">
+      <c r="B27" s="238" t="s">
         <v>358</v>
       </c>
-      <c r="C27" s="265"/>
-      <c r="D27" s="265"/>
-      <c r="E27" s="265"/>
-      <c r="F27" s="265"/>
-      <c r="G27" s="265"/>
-      <c r="H27" s="265"/>
-      <c r="I27" s="265"/>
-      <c r="J27" s="265"/>
-      <c r="K27" s="265"/>
-      <c r="L27" s="266"/>
+      <c r="C27" s="238"/>
+      <c r="D27" s="238"/>
+      <c r="E27" s="238"/>
+      <c r="F27" s="238"/>
+      <c r="G27" s="238"/>
+      <c r="H27" s="238"/>
+      <c r="I27" s="238"/>
+      <c r="J27" s="238"/>
+      <c r="K27" s="238"/>
+      <c r="L27" s="239"/>
       <c r="N27" s="106"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="230">
         <v>2</v>
       </c>
-      <c r="B28" s="267" t="s">
+      <c r="B28" s="240" t="s">
         <v>347</v>
       </c>
-      <c r="C28" s="267"/>
-      <c r="D28" s="267"/>
-      <c r="E28" s="267"/>
-      <c r="F28" s="267"/>
-      <c r="G28" s="267"/>
-      <c r="H28" s="267"/>
-      <c r="I28" s="267"/>
-      <c r="J28" s="267"/>
-      <c r="K28" s="267"/>
-      <c r="L28" s="268"/>
+      <c r="C28" s="240"/>
+      <c r="D28" s="240"/>
+      <c r="E28" s="240"/>
+      <c r="F28" s="240"/>
+      <c r="G28" s="240"/>
+      <c r="H28" s="240"/>
+      <c r="I28" s="240"/>
+      <c r="J28" s="240"/>
+      <c r="K28" s="240"/>
+      <c r="L28" s="241"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="230">
         <v>3</v>
       </c>
-      <c r="B29" s="267" t="s">
+      <c r="B29" s="240" t="s">
         <v>336</v>
       </c>
-      <c r="C29" s="267"/>
-      <c r="D29" s="267"/>
-      <c r="E29" s="267"/>
-      <c r="F29" s="267"/>
-      <c r="G29" s="267"/>
-      <c r="H29" s="267"/>
-      <c r="I29" s="267"/>
-      <c r="J29" s="267"/>
-      <c r="K29" s="267"/>
-      <c r="L29" s="268"/>
+      <c r="C29" s="240"/>
+      <c r="D29" s="240"/>
+      <c r="E29" s="240"/>
+      <c r="F29" s="240"/>
+      <c r="G29" s="240"/>
+      <c r="H29" s="240"/>
+      <c r="I29" s="240"/>
+      <c r="J29" s="240"/>
+      <c r="K29" s="240"/>
+      <c r="L29" s="241"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="230">
         <v>4</v>
       </c>
-      <c r="B30" s="267" t="s">
+      <c r="B30" s="240" t="s">
         <v>359</v>
       </c>
-      <c r="C30" s="267"/>
-      <c r="D30" s="267"/>
-      <c r="E30" s="267"/>
-      <c r="F30" s="267"/>
-      <c r="G30" s="267"/>
-      <c r="H30" s="267"/>
-      <c r="I30" s="267"/>
-      <c r="J30" s="267"/>
-      <c r="K30" s="267"/>
-      <c r="L30" s="268"/>
+      <c r="C30" s="240"/>
+      <c r="D30" s="240"/>
+      <c r="E30" s="240"/>
+      <c r="F30" s="240"/>
+      <c r="G30" s="240"/>
+      <c r="H30" s="240"/>
+      <c r="I30" s="240"/>
+      <c r="J30" s="240"/>
+      <c r="K30" s="240"/>
+      <c r="L30" s="241"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="230">
         <v>5</v>
       </c>
-      <c r="B31" s="265" t="s">
+      <c r="B31" s="238" t="s">
         <v>337</v>
       </c>
-      <c r="C31" s="265"/>
-      <c r="D31" s="265"/>
-      <c r="E31" s="265"/>
-      <c r="F31" s="265"/>
-      <c r="G31" s="265"/>
-      <c r="H31" s="265"/>
-      <c r="I31" s="265"/>
-      <c r="J31" s="265"/>
-      <c r="K31" s="265"/>
-      <c r="L31" s="266"/>
+      <c r="C31" s="238"/>
+      <c r="D31" s="238"/>
+      <c r="E31" s="238"/>
+      <c r="F31" s="238"/>
+      <c r="G31" s="238"/>
+      <c r="H31" s="238"/>
+      <c r="I31" s="238"/>
+      <c r="J31" s="238"/>
+      <c r="K31" s="238"/>
+      <c r="L31" s="239"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="230">
         <v>6</v>
       </c>
-      <c r="B32" s="265" t="s">
+      <c r="B32" s="238" t="s">
         <v>342</v>
       </c>
-      <c r="C32" s="265"/>
-      <c r="D32" s="265"/>
-      <c r="E32" s="265"/>
-      <c r="F32" s="265"/>
-      <c r="G32" s="265"/>
-      <c r="H32" s="265"/>
-      <c r="I32" s="265"/>
-      <c r="J32" s="265"/>
-      <c r="K32" s="265"/>
-      <c r="L32" s="266"/>
+      <c r="C32" s="238"/>
+      <c r="D32" s="238"/>
+      <c r="E32" s="238"/>
+      <c r="F32" s="238"/>
+      <c r="G32" s="238"/>
+      <c r="H32" s="238"/>
+      <c r="I32" s="238"/>
+      <c r="J32" s="238"/>
+      <c r="K32" s="238"/>
+      <c r="L32" s="239"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="230">
         <v>7</v>
       </c>
-      <c r="B33" s="267" t="s">
+      <c r="B33" s="240" t="s">
         <v>338</v>
       </c>
-      <c r="C33" s="267"/>
-      <c r="D33" s="267"/>
-      <c r="E33" s="267"/>
-      <c r="F33" s="267"/>
-      <c r="G33" s="267"/>
-      <c r="H33" s="267"/>
-      <c r="I33" s="267"/>
-      <c r="J33" s="267"/>
-      <c r="K33" s="267"/>
-      <c r="L33" s="268"/>
+      <c r="C33" s="240"/>
+      <c r="D33" s="240"/>
+      <c r="E33" s="240"/>
+      <c r="F33" s="240"/>
+      <c r="G33" s="240"/>
+      <c r="H33" s="240"/>
+      <c r="I33" s="240"/>
+      <c r="J33" s="240"/>
+      <c r="K33" s="240"/>
+      <c r="L33" s="241"/>
     </row>
     <row r="34" spans="1:12" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="230"/>
@@ -15466,56 +15469,56 @@
       <c r="L34" s="232"/>
     </row>
     <row r="35" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="269" t="s">
+      <c r="A35" s="249" t="s">
         <v>341</v>
       </c>
-      <c r="B35" s="270"/>
-      <c r="C35" s="270"/>
-      <c r="D35" s="270"/>
-      <c r="E35" s="270"/>
-      <c r="F35" s="270"/>
-      <c r="G35" s="270"/>
-      <c r="H35" s="270"/>
-      <c r="I35" s="270"/>
-      <c r="J35" s="270"/>
-      <c r="K35" s="270"/>
-      <c r="L35" s="271"/>
+      <c r="B35" s="250"/>
+      <c r="C35" s="250"/>
+      <c r="D35" s="250"/>
+      <c r="E35" s="250"/>
+      <c r="F35" s="250"/>
+      <c r="G35" s="250"/>
+      <c r="H35" s="250"/>
+      <c r="I35" s="250"/>
+      <c r="J35" s="250"/>
+      <c r="K35" s="250"/>
+      <c r="L35" s="251"/>
     </row>
     <row r="36" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="233" t="s">
         <v>339</v>
       </c>
-      <c r="B36" s="267" t="s">
+      <c r="B36" s="240" t="s">
         <v>224</v>
       </c>
-      <c r="C36" s="267"/>
-      <c r="D36" s="267"/>
-      <c r="E36" s="267"/>
-      <c r="F36" s="267"/>
-      <c r="G36" s="267"/>
-      <c r="H36" s="267"/>
-      <c r="I36" s="267"/>
-      <c r="J36" s="267"/>
-      <c r="K36" s="267"/>
-      <c r="L36" s="268"/>
+      <c r="C36" s="240"/>
+      <c r="D36" s="240"/>
+      <c r="E36" s="240"/>
+      <c r="F36" s="240"/>
+      <c r="G36" s="240"/>
+      <c r="H36" s="240"/>
+      <c r="I36" s="240"/>
+      <c r="J36" s="240"/>
+      <c r="K36" s="240"/>
+      <c r="L36" s="241"/>
     </row>
     <row r="37" spans="1:12" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="234" t="s">
         <v>340</v>
       </c>
-      <c r="B37" s="273" t="s">
+      <c r="B37" s="242" t="s">
         <v>343</v>
       </c>
-      <c r="C37" s="273"/>
-      <c r="D37" s="273"/>
-      <c r="E37" s="273"/>
-      <c r="F37" s="273"/>
-      <c r="G37" s="273"/>
-      <c r="H37" s="273"/>
-      <c r="I37" s="273"/>
-      <c r="J37" s="273"/>
-      <c r="K37" s="273"/>
-      <c r="L37" s="274"/>
+      <c r="C37" s="242"/>
+      <c r="D37" s="242"/>
+      <c r="E37" s="242"/>
+      <c r="F37" s="242"/>
+      <c r="G37" s="242"/>
+      <c r="H37" s="242"/>
+      <c r="I37" s="242"/>
+      <c r="J37" s="242"/>
+      <c r="K37" s="242"/>
+      <c r="L37" s="243"/>
     </row>
     <row r="38" spans="1:12" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="161"/>
@@ -15532,20 +15535,20 @@
       <c r="L38" s="113"/>
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="275" t="s">
+      <c r="A39" s="244" t="s">
         <v>252</v>
       </c>
-      <c r="B39" s="276"/>
-      <c r="C39" s="276"/>
-      <c r="D39" s="276"/>
-      <c r="E39" s="276"/>
-      <c r="F39" s="276"/>
-      <c r="G39" s="276"/>
-      <c r="H39" s="276"/>
-      <c r="I39" s="276"/>
-      <c r="J39" s="276"/>
-      <c r="K39" s="276"/>
-      <c r="L39" s="277"/>
+      <c r="B39" s="245"/>
+      <c r="C39" s="245"/>
+      <c r="D39" s="245"/>
+      <c r="E39" s="245"/>
+      <c r="F39" s="245"/>
+      <c r="G39" s="245"/>
+      <c r="H39" s="245"/>
+      <c r="I39" s="245"/>
+      <c r="J39" s="245"/>
+      <c r="K39" s="245"/>
+      <c r="L39" s="246"/>
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="162" t="s">
@@ -15633,72 +15636,72 @@
       <c r="B45" s="170" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="255" t="s">
+      <c r="C45" s="247" t="s">
         <v>326</v>
       </c>
-      <c r="D45" s="255"/>
-      <c r="E45" s="255"/>
-      <c r="F45" s="255"/>
-      <c r="G45" s="255"/>
-      <c r="H45" s="255"/>
-      <c r="I45" s="255"/>
-      <c r="J45" s="255"/>
-      <c r="K45" s="255"/>
-      <c r="L45" s="256"/>
+      <c r="D45" s="247"/>
+      <c r="E45" s="247"/>
+      <c r="F45" s="247"/>
+      <c r="G45" s="247"/>
+      <c r="H45" s="247"/>
+      <c r="I45" s="247"/>
+      <c r="J45" s="247"/>
+      <c r="K45" s="247"/>
+      <c r="L45" s="248"/>
     </row>
     <row r="46" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="169"/>
       <c r="B46" s="170" t="s">
         <v>146</v>
       </c>
-      <c r="C46" s="255" t="s">
+      <c r="C46" s="247" t="s">
         <v>147</v>
       </c>
-      <c r="D46" s="255"/>
-      <c r="E46" s="255"/>
-      <c r="F46" s="255"/>
-      <c r="G46" s="255"/>
-      <c r="H46" s="255"/>
-      <c r="I46" s="255"/>
-      <c r="J46" s="255"/>
-      <c r="K46" s="255"/>
-      <c r="L46" s="256"/>
+      <c r="D46" s="247"/>
+      <c r="E46" s="247"/>
+      <c r="F46" s="247"/>
+      <c r="G46" s="247"/>
+      <c r="H46" s="247"/>
+      <c r="I46" s="247"/>
+      <c r="J46" s="247"/>
+      <c r="K46" s="247"/>
+      <c r="L46" s="248"/>
     </row>
     <row r="47" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="169"/>
       <c r="B47" s="170" t="s">
         <v>250</v>
       </c>
-      <c r="C47" s="255" t="s">
+      <c r="C47" s="247" t="s">
         <v>251</v>
       </c>
-      <c r="D47" s="255"/>
-      <c r="E47" s="255"/>
-      <c r="F47" s="255"/>
-      <c r="G47" s="255"/>
-      <c r="H47" s="255"/>
-      <c r="I47" s="255"/>
-      <c r="J47" s="255"/>
-      <c r="K47" s="255"/>
-      <c r="L47" s="256"/>
+      <c r="D47" s="247"/>
+      <c r="E47" s="247"/>
+      <c r="F47" s="247"/>
+      <c r="G47" s="247"/>
+      <c r="H47" s="247"/>
+      <c r="I47" s="247"/>
+      <c r="J47" s="247"/>
+      <c r="K47" s="247"/>
+      <c r="L47" s="248"/>
     </row>
     <row r="48" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="169"/>
       <c r="B48" s="170" t="s">
         <v>327</v>
       </c>
-      <c r="C48" s="255" t="s">
+      <c r="C48" s="247" t="s">
         <v>328</v>
       </c>
-      <c r="D48" s="255"/>
-      <c r="E48" s="255"/>
-      <c r="F48" s="255"/>
-      <c r="G48" s="255"/>
-      <c r="H48" s="255"/>
-      <c r="I48" s="255"/>
-      <c r="J48" s="255"/>
-      <c r="K48" s="255"/>
-      <c r="L48" s="256"/>
+      <c r="D48" s="247"/>
+      <c r="E48" s="247"/>
+      <c r="F48" s="247"/>
+      <c r="G48" s="247"/>
+      <c r="H48" s="247"/>
+      <c r="I48" s="247"/>
+      <c r="J48" s="247"/>
+      <c r="K48" s="247"/>
+      <c r="L48" s="248"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="169"/>
@@ -15723,18 +15726,18 @@
       <c r="B50" s="170" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="255" t="s">
+      <c r="C50" s="247" t="s">
         <v>330</v>
       </c>
-      <c r="D50" s="255"/>
-      <c r="E50" s="255"/>
-      <c r="F50" s="255"/>
-      <c r="G50" s="255"/>
-      <c r="H50" s="255"/>
-      <c r="I50" s="255"/>
-      <c r="J50" s="255"/>
-      <c r="K50" s="255"/>
-      <c r="L50" s="256"/>
+      <c r="D50" s="247"/>
+      <c r="E50" s="247"/>
+      <c r="F50" s="247"/>
+      <c r="G50" s="247"/>
+      <c r="H50" s="247"/>
+      <c r="I50" s="247"/>
+      <c r="J50" s="247"/>
+      <c r="K50" s="247"/>
+      <c r="L50" s="248"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="169"/>
@@ -15816,37 +15819,39 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="272" t="s">
+      <c r="A64" s="237" t="s">
         <v>332</v>
       </c>
-      <c r="B64" s="272"/>
-      <c r="C64" s="272"/>
-      <c r="D64" s="272"/>
-      <c r="E64" s="272"/>
-      <c r="F64" s="272"/>
-      <c r="G64" s="272"/>
-      <c r="H64" s="272"/>
-      <c r="I64" s="272"/>
-      <c r="J64" s="272"/>
-      <c r="K64" s="272"/>
-      <c r="L64" s="272"/>
+      <c r="B64" s="237"/>
+      <c r="C64" s="237"/>
+      <c r="D64" s="237"/>
+      <c r="E64" s="237"/>
+      <c r="F64" s="237"/>
+      <c r="G64" s="237"/>
+      <c r="H64" s="237"/>
+      <c r="I64" s="237"/>
+      <c r="J64" s="237"/>
+      <c r="K64" s="237"/>
+      <c r="L64" s="237"/>
     </row>
     <row r="69" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="70" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A64:L64"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="C45:L45"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="C47:L47"/>
-    <mergeCell ref="C48:L48"/>
-    <mergeCell ref="C50:L50"/>
-    <mergeCell ref="A35:L35"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B8:L8"/>
     <mergeCell ref="B31:L31"/>
     <mergeCell ref="B18:L18"/>
     <mergeCell ref="B19:L19"/>
@@ -15861,20 +15866,18 @@
     <mergeCell ref="B29:L29"/>
     <mergeCell ref="B28:L28"/>
     <mergeCell ref="B30:L30"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="A64:L64"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="C45:L45"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="C48:L48"/>
+    <mergeCell ref="C50:L50"/>
+    <mergeCell ref="A35:L35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A57" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -16544,8 +16547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BF7D8F-86F3-47E9-AB85-EE9B4CAB70E4}">
   <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N52" sqref="N52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17981,7 +17984,7 @@
       </c>
       <c r="M52" s="116"/>
       <c r="N52" s="141" t="s">
-        <v>192</v>
+        <v>367</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.35">
@@ -21280,8 +21283,8 @@
     <hyperlink ref="N31" r:id="rId13" location="2c-havasuparker-evaporation-and-evapotranspiration" xr:uid="{70E7AC6A-42AC-4DE1-ADFB-FBA8230C308E}"/>
     <hyperlink ref="N35" r:id="rId14" location="step-3-split-existing-lake-mead-storage-among-accounts-year-1-only" xr:uid="{B36B453C-62F8-4461-8E49-8546C848C695}"/>
     <hyperlink ref="N42" r:id="rId15" location="3a-begin-of-year-reservoir-storage" xr:uid="{52EB1038-72CB-4676-AD3B-3DD4322D2D3C}"/>
-    <hyperlink ref="N45" r:id="rId16" location="3b-calculate-powell--mead-evaporation" display="Help Powell + Mead evaporation" xr:uid="{9002111C-2D36-45B1-97D8-5FCB363BD9BD}"/>
-    <hyperlink ref="N52" r:id="rId17" location="3c-calculate-mexico-water-allocation" xr:uid="{C14FC6B3-6E3C-48F5-B820-A74ADC9C86D6}"/>
+    <hyperlink ref="N45" r:id="rId16" location="3b-calculate-mead-evaporation" xr:uid="{9002111C-2D36-45B1-97D8-5FCB363BD9BD}"/>
+    <hyperlink ref="N52" r:id="rId17" location="3c-calculate-mexico-water-allocation" display="Help Mexico water allocation" xr:uid="{C14FC6B3-6E3C-48F5-B820-A74ADC9C86D6}"/>
     <hyperlink ref="N53" r:id="rId18" location="split-combined-natural-inflow-among-accounts" xr:uid="{63C31A0C-C046-4C6B-B63E-AA3031EC5E49}"/>
     <hyperlink ref="N63" r:id="rId19" location="step-5-participant-dashboards--conserve-consume-and-trade" xr:uid="{E1DA626C-61A5-4CB7-94B9-52C34A1556D5}"/>
     <hyperlink ref="N65" r:id="rId20" location="ii-compensation" xr:uid="{19918E71-71AD-4C9C-BB3F-A5AF3D55F1D7}"/>
@@ -22723,16 +22726,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="312" t="e">
+      <c r="A1" s="313" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="312"/>
-      <c r="C1" s="312"/>
-      <c r="D1" s="312"/>
-      <c r="E1" s="312"/>
-      <c r="F1" s="312"/>
-      <c r="G1" s="312"/>
+      <c r="B1" s="313"/>
+      <c r="C1" s="313"/>
+      <c r="D1" s="313"/>
+      <c r="E1" s="313"/>
+      <c r="F1" s="313"/>
+      <c r="G1" s="313"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -22841,11 +22844,11 @@
         <v>81</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="313"/>
-      <c r="D10" s="313"/>
-      <c r="E10" s="313"/>
-      <c r="F10" s="313"/>
-      <c r="G10" s="313"/>
+      <c r="C10" s="312"/>
+      <c r="D10" s="312"/>
+      <c r="E10" s="312"/>
+      <c r="F10" s="312"/>
+      <c r="G10" s="312"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -24108,6 +24111,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -24115,12 +24124,6 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>

</xml_diff>

<commit_message>
Finished model and users guide
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E021990-F751-4469-97C8-29520E9B57C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE2D2CF-5931-4C9F-9CEE-44F4A299B330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="62" r:id="rId1"/>
@@ -1209,9 +1209,6 @@
     <t>*** If percentage shares of total shortages for 0.3 to 1.5 maf per year specified in Lower Basin Alternative (2024) continue to total shortages for 8.0 maf per year.</t>
   </si>
   <si>
-    <t>Lake Mead Water Bank based on the Principle of Divide Reservoir Inflow</t>
-  </si>
-  <si>
     <t>User</t>
   </si>
   <si>
@@ -1926,6 +1923,9 @@
   </si>
   <si>
     <t>Help Lake Mead end of year</t>
+  </si>
+  <si>
+    <t>Immersive Model: Lake Mead Water Bank based on the Principle of Divide Reservoir Inflow</t>
   </si>
 </sst>
 </file>
@@ -14849,8 +14849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EA02F4-5F19-409C-8BC6-A0D8FEB3A90D}">
   <dimension ref="A1:R70"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14870,7 +14870,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A1" s="239" t="s">
-        <v>319</v>
+        <v>366</v>
       </c>
       <c r="B1" s="239"/>
       <c r="C1" s="239"/>
@@ -14909,7 +14909,7 @@
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="240" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B4" s="241"/>
       <c r="C4" s="241"/>
@@ -14930,7 +14930,7 @@
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="244" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B5" s="245"/>
       <c r="C5" s="245"/>
@@ -14951,7 +14951,7 @@
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="244" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B6" s="245"/>
       <c r="C6" s="245"/>
@@ -14973,7 +14973,7 @@
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="234"/>
       <c r="B7" s="245" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C7" s="245"/>
       <c r="D7" s="245"/>
@@ -14994,7 +14994,7 @@
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="235"/>
       <c r="B8" s="262" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C8" s="262"/>
       <c r="D8" s="262"/>
@@ -15044,7 +15044,7 @@
     </row>
     <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="250" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B11" s="251"/>
       <c r="C11" s="251"/>
@@ -15060,7 +15060,7 @@
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="253" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B12" s="254"/>
       <c r="C12" s="254"/>
@@ -15092,7 +15092,7 @@
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="256" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B14" s="257"/>
       <c r="C14" s="257"/>
@@ -15122,7 +15122,7 @@
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="259" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B16" s="260"/>
       <c r="C16" s="260"/>
@@ -15177,7 +15177,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="266" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C19" s="266"/>
       <c r="D19" s="266"/>
@@ -15215,7 +15215,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="266" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C21" s="266"/>
       <c r="D21" s="266"/>
@@ -15321,7 +15321,7 @@
     <row r="27" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="229"/>
       <c r="B27" s="264" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C27" s="264"/>
       <c r="D27" s="264"/>
@@ -15340,7 +15340,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="266" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C28" s="266"/>
       <c r="D28" s="266"/>
@@ -15359,7 +15359,7 @@
         <v>3</v>
       </c>
       <c r="B29" s="266" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C29" s="266"/>
       <c r="D29" s="266"/>
@@ -15378,7 +15378,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="266" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C30" s="266"/>
       <c r="D30" s="266"/>
@@ -15397,7 +15397,7 @@
         <v>5</v>
       </c>
       <c r="B31" s="264" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C31" s="264"/>
       <c r="D31" s="264"/>
@@ -15416,7 +15416,7 @@
         <v>6</v>
       </c>
       <c r="B32" s="264" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C32" s="264"/>
       <c r="D32" s="264"/>
@@ -15435,7 +15435,7 @@
         <v>7</v>
       </c>
       <c r="B33" s="266" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C33" s="266"/>
       <c r="D33" s="266"/>
@@ -15464,7 +15464,7 @@
     </row>
     <row r="35" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="268" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B35" s="269"/>
       <c r="C35" s="269"/>
@@ -15480,7 +15480,7 @@
     </row>
     <row r="36" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="232" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B36" s="266" t="s">
         <v>222</v>
@@ -15498,10 +15498,10 @@
     </row>
     <row r="37" spans="1:12" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="233" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B37" s="272" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C37" s="272"/>
       <c r="D37" s="272"/>
@@ -15631,7 +15631,7 @@
         <v>62</v>
       </c>
       <c r="C45" s="254" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D45" s="254"/>
       <c r="E45" s="254"/>
@@ -15682,10 +15682,10 @@
     <row r="48" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="168"/>
       <c r="B48" s="169" t="s">
+        <v>324</v>
+      </c>
+      <c r="C48" s="254" t="s">
         <v>325</v>
-      </c>
-      <c r="C48" s="254" t="s">
-        <v>326</v>
       </c>
       <c r="D48" s="254"/>
       <c r="E48" s="254"/>
@@ -15703,7 +15703,7 @@
         <v>213</v>
       </c>
       <c r="C49" s="170" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D49" s="170"/>
       <c r="E49" s="170"/>
@@ -15721,7 +15721,7 @@
         <v>63</v>
       </c>
       <c r="C50" s="254" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D50" s="254"/>
       <c r="E50" s="254"/>
@@ -15804,7 +15804,7 @@
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="45" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.35">
@@ -15814,7 +15814,7 @@
     </row>
     <row r="64" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="271" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B64" s="271"/>
       <c r="C64" s="271"/>
@@ -16084,7 +16084,7 @@
         <v>297</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D3" s="55">
         <v>4</v>
@@ -16105,10 +16105,10 @@
         <v>45611</v>
       </c>
       <c r="B4" s="149" t="s">
+        <v>331</v>
+      </c>
+      <c r="C4" s="56" t="s">
         <v>332</v>
-      </c>
-      <c r="C4" s="56" t="s">
-        <v>333</v>
       </c>
       <c r="D4" s="55">
         <v>0.3</v>
@@ -16129,10 +16129,10 @@
         <v>45622</v>
       </c>
       <c r="B5" s="149" t="s">
+        <v>362</v>
+      </c>
+      <c r="C5" s="56" t="s">
         <v>363</v>
-      </c>
-      <c r="C5" s="56" t="s">
-        <v>364</v>
       </c>
       <c r="D5" s="55">
         <v>4</v>
@@ -16541,8 +16541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BF7D8F-86F3-47E9-AB85-EE9B4CAB70E4}">
   <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G137" sqref="G137"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16573,7 +16573,7 @@
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="277" t="str">
         <f>'ReadMe-Directions'!A1</f>
-        <v>Lake Mead Water Bank based on the Principle of Divide Reservoir Inflow</v>
+        <v>Immersive Model: Lake Mead Water Bank based on the Principle of Divide Reservoir Inflow</v>
       </c>
       <c r="B1" s="277"/>
       <c r="C1" s="277"/>
@@ -16608,13 +16608,13 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="127" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="286" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D4" s="287"/>
       <c r="E4" s="287"/>
@@ -16686,7 +16686,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="90" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B10" s="90"/>
       <c r="C10" s="284"/>
@@ -16825,7 +16825,7 @@
       <c r="E21" s="28"/>
       <c r="F21" s="116"/>
       <c r="N21" s="141" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
@@ -16841,12 +16841,12 @@
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
       <c r="N22" s="141" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C23" s="12">
         <f>C21-C22</f>
@@ -16855,7 +16855,7 @@
       <c r="D23" s="111"/>
       <c r="E23" s="28"/>
       <c r="N23" s="141" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="24" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
@@ -16944,9 +16944,7 @@
         <v>257</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="97">
-        <v>9.5</v>
-      </c>
+      <c r="C28" s="97"/>
       <c r="D28" s="97"/>
       <c r="E28" s="97"/>
       <c r="F28" s="97"/>
@@ -16957,7 +16955,7 @@
       <c r="K28" s="97"/>
       <c r="L28" s="97"/>
       <c r="N28" s="141" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.35">
@@ -16965,9 +16963,9 @@
         <v>71</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="96">
+      <c r="C29" s="96" t="str">
         <f>IF(C$28&lt;&gt;"",0.8,"")</f>
-        <v>0.8</v>
+        <v/>
       </c>
       <c r="D29" s="96" t="str">
         <f t="shared" ref="D29:L29" si="0">IF(D$28&lt;&gt;"",0.8,"")</f>
@@ -17014,9 +17012,9 @@
         <v>144</v>
       </c>
       <c r="B30" s="1"/>
-      <c r="C30" s="96">
+      <c r="C30" s="96" t="str">
         <f>IF(C$28&lt;&gt;"",0.2,"")</f>
-        <v>0.2</v>
+        <v/>
       </c>
       <c r="D30" s="96" t="str">
         <f t="shared" ref="D30:L30" si="1">IF(D$28&lt;&gt;"",0.2,"")</f>
@@ -17063,9 +17061,9 @@
         <v>132</v>
       </c>
       <c r="B31" s="1"/>
-      <c r="C31" s="96">
+      <c r="C31" s="96" t="str">
         <f>IF(C$28&lt;&gt;"",0.6,"")</f>
-        <v>0.6</v>
+        <v/>
       </c>
       <c r="D31" s="96" t="str">
         <f t="shared" ref="D31:L31" si="2">IF(D$28&lt;&gt;"",0.6,"")</f>
@@ -17124,9 +17122,9 @@
         <v>303</v>
       </c>
       <c r="B33" s="1"/>
-      <c r="C33" s="12">
+      <c r="C33" s="12" t="str">
         <f>IF(C$28&lt;&gt;"",IF(COLUMN(C28)=COLUMN($C28),$C$19,B135),"")</f>
-        <v>8.4990979999700009</v>
+        <v/>
       </c>
       <c r="D33" s="12" t="str">
         <f>IF(D$28&lt;&gt;"",IF(COLUMN(D28)=COLUMN($C28),$C$19,C135),"")</f>
@@ -17156,9 +17154,9 @@
         <v>304</v>
       </c>
       <c r="B34" s="1"/>
-      <c r="C34" s="220">
+      <c r="C34" s="220" t="str">
         <f>IF(C$28&lt;&gt;"",IF(COLUMN(C29)=COLUMN($C29),$B$19,B136),"")</f>
-        <v>1061.22</v>
+        <v/>
       </c>
       <c r="D34" s="220" t="str">
         <f t="shared" ref="D34:G34" si="3">IF(D$28&lt;&gt;"",IF(COLUMN(D29)=COLUMN($C29),$B$19,C136),"")</f>
@@ -17221,9 +17219,9 @@
         <f>C20</f>
         <v>4.7610489999999999</v>
       </c>
-      <c r="C36" s="81">
+      <c r="C36" s="81" t="str">
         <f>IF(OR(C$28="",$A36=""),"",B36)</f>
-        <v>4.7610489999999999</v>
+        <v/>
       </c>
       <c r="D36" s="12" t="str">
         <f>IF(OR(D$28="",$A36=""),"",C128)</f>
@@ -17271,9 +17269,9 @@
       <c r="B37" s="83">
         <v>1.6619999999999999</v>
       </c>
-      <c r="C37" s="81">
+      <c r="C37" s="81" t="str">
         <f>IF(OR(C$28="",$A37=""),"",IF(C$22&lt;=C$21,B37,B37-(C$22-C$21)*B37/C$22))</f>
-        <v>1.6619999999999999</v>
+        <v/>
       </c>
       <c r="D37" s="12" t="str">
         <f t="shared" ref="D37:D41" si="7">IF(OR(D$28="",$A37=""),"",C129)</f>
@@ -17321,9 +17319,9 @@
       <c r="B38" s="83">
         <v>0.71099999999999997</v>
       </c>
-      <c r="C38" s="81">
+      <c r="C38" s="81" t="str">
         <f t="shared" ref="C38:C41" si="9">IF(OR(C$28="",$A38=""),"",IF(C$22&lt;=C$21,B38,B38-(C$22-C$21)*B38/C$22))</f>
-        <v>0.71099999999999997</v>
+        <v/>
       </c>
       <c r="D38" s="33" t="str">
         <f t="shared" si="7"/>
@@ -17371,9 +17369,9 @@
       <c r="B39" s="83">
         <v>0.9556</v>
       </c>
-      <c r="C39" s="81">
+      <c r="C39" s="81" t="str">
         <f t="shared" si="9"/>
-        <v>0.9556</v>
+        <v/>
       </c>
       <c r="D39" s="12" t="str">
         <f t="shared" si="7"/>
@@ -17421,9 +17419,9 @@
       <c r="B40" s="83">
         <v>0.21099999999999999</v>
       </c>
-      <c r="C40" s="81">
+      <c r="C40" s="81" t="str">
         <f t="shared" si="9"/>
-        <v>0.21099999999999999</v>
+        <v/>
       </c>
       <c r="D40" s="12" t="str">
         <f t="shared" si="7"/>
@@ -17472,9 +17470,9 @@
         <f>IF(C21&gt;C22,C21-C22,0)</f>
         <v>0.20404899997000125</v>
       </c>
-      <c r="C41" s="81">
+      <c r="C41" s="81" t="str">
         <f t="shared" si="9"/>
-        <v>0.20404899997000125</v>
+        <v/>
       </c>
       <c r="D41" s="12" t="str">
         <f t="shared" si="7"/>
@@ -17527,9 +17525,9 @@
       <c r="A43" t="s">
         <v>68</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C43" s="12" t="str">
         <f>IF(C$28&lt;&gt;"",IF(COLUMN(C27)=COLUMN($C27),$B$19,#REF!),"")</f>
-        <v>1061.22</v>
+        <v/>
       </c>
       <c r="D43" s="12" t="str">
         <f>IF(D$28&lt;&gt;"",IF(COLUMN(D27)=COLUMN($C27),$B$19,#REF!),"")</f>
@@ -17600,9 +17598,9 @@
         <v>259</v>
       </c>
       <c r="B45" s="188"/>
-      <c r="C45" s="12">
+      <c r="C45" s="12" t="str">
         <f>IF(C$28&lt;&gt;"",VLOOKUP(C33*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$B$18/1000000,"")</f>
-        <v>0.45716399999939999</v>
+        <v/>
       </c>
       <c r="D45" s="12" t="str">
         <f>IF(D$28&lt;&gt;"",VLOOKUP(D33*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$B$18/1000000,"")</f>
@@ -17641,7 +17639,7 @@
         <v/>
       </c>
       <c r="N45" s="141" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.35">
@@ -17649,9 +17647,9 @@
         <f t="shared" ref="A46:A51" si="10">IF(A5="","","    "&amp;A5&amp;" Share")</f>
         <v xml:space="preserve">    Reclamation - Protect Zone Share</v>
       </c>
-      <c r="C46" s="12">
+      <c r="C46" s="12" t="str">
         <f t="shared" ref="C46:G51" si="11">IF(OR(C$28="",$A46=""),"",C$45*C36/C$33)</f>
-        <v>0.25609543566162268</v>
+        <v/>
       </c>
       <c r="D46" s="12" t="str">
         <f t="shared" si="11"/>
@@ -17697,9 +17695,9 @@
         <v xml:space="preserve">    California Share</v>
       </c>
       <c r="B47" s="1"/>
-      <c r="C47" s="12">
+      <c r="C47" s="12" t="str">
         <f t="shared" si="11"/>
-        <v>8.9398494758112512E-2</v>
+        <v/>
       </c>
       <c r="D47" s="12" t="str">
         <f t="shared" si="11"/>
@@ -17745,9 +17743,9 @@
         <v xml:space="preserve">    Arizona Share</v>
       </c>
       <c r="B48" s="1"/>
-      <c r="C48" s="12">
+      <c r="C48" s="12" t="str">
         <f t="shared" si="11"/>
-        <v>3.8244482414571603E-2</v>
+        <v/>
       </c>
       <c r="D48" s="12" t="str">
         <f t="shared" si="11"/>
@@ -17793,9 +17791,9 @@
         <v xml:space="preserve">    Nevada Share</v>
       </c>
       <c r="B49" s="1"/>
-      <c r="C49" s="12">
+      <c r="C49" s="12" t="str">
         <f t="shared" si="11"/>
-        <v>5.140144500051283E-2</v>
+        <v/>
       </c>
       <c r="D49" s="12" t="str">
         <f t="shared" si="11"/>
@@ -17841,9 +17839,9 @@
         <v xml:space="preserve">    Mexico Share</v>
       </c>
       <c r="B50" s="1"/>
-      <c r="C50" s="12">
+      <c r="C50" s="12" t="str">
         <f t="shared" si="11"/>
-        <v>1.1349628395885526E-2</v>
+        <v/>
       </c>
       <c r="D50" s="12" t="str">
         <f t="shared" si="11"/>
@@ -17889,9 +17887,9 @@
         <v xml:space="preserve">    Tribal Nations of the Lower Basin Share</v>
       </c>
       <c r="B51" s="1"/>
-      <c r="C51" s="12">
+      <c r="C51" s="12" t="str">
         <f t="shared" si="11"/>
-        <v>1.0975736133704127E-2</v>
+        <v/>
       </c>
       <c r="D51" s="12" t="str">
         <f t="shared" si="11"/>
@@ -17936,9 +17934,9 @@
         <v>299</v>
       </c>
       <c r="B52" s="216"/>
-      <c r="C52" s="217">
+      <c r="C52" s="217" t="str">
         <f>IF(C28="","",SUM(C28))</f>
-        <v>9.5</v>
+        <v/>
       </c>
       <c r="D52" s="217" t="str">
         <f>IF(D28="","",SUM(D28))</f>
@@ -17978,7 +17976,7 @@
       </c>
       <c r="M52" s="116"/>
       <c r="N52" s="141" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.35">
@@ -17989,9 +17987,9 @@
       <c r="B53" s="189" t="s">
         <v>261</v>
       </c>
-      <c r="C53" s="82">
+      <c r="C53" s="82" t="str">
         <f>IF(OR(C$28="",$A55=""),"",C46)</f>
-        <v>0.25609543566162268</v>
+        <v/>
       </c>
       <c r="D53" s="82" t="str">
         <f t="shared" ref="D53:G53" si="13">IF(OR(D$28="",$A55=""),"",D46)</f>
@@ -18031,7 +18029,7 @@
       </c>
       <c r="M53" s="19">
         <f>SUM(C55:C59)</f>
-        <v>9.2439045643383793</v>
+        <v>0</v>
       </c>
       <c r="N53" s="184"/>
       <c r="P53" t="s">
@@ -18042,9 +18040,9 @@
       <c r="A54" t="s">
         <v>300</v>
       </c>
-      <c r="C54" s="82">
+      <c r="C54" s="82" t="str">
         <f>IF(OR(C$28="",$A56=""),"",C52-C53)</f>
-        <v>9.2439045643383775</v>
+        <v/>
       </c>
       <c r="D54" s="82" t="str">
         <f t="shared" ref="D54:G54" si="15">IF(OR(D$28="",$A56=""),"",D52-D53)</f>
@@ -18082,9 +18080,9 @@
         <f t="shared" ref="L54" si="20">IF(OR(L$28="",$A55=""),"",MAX(0,L53-SUM(L55:L60)))</f>
         <v/>
       </c>
-      <c r="M54" s="18">
+      <c r="M54" s="18" t="e">
         <f>SUM(M55:M59)</f>
-        <v>1</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N54" s="143"/>
       <c r="P54" s="81" t="str">
@@ -18100,9 +18098,9 @@
       <c r="B55" s="95" t="s">
         <v>315</v>
       </c>
-      <c r="C55" s="82">
+      <c r="C55" s="82" t="str">
         <f>IF(OR(C$28="",$A55=""),"",(VLOOKUP(C$54,DivideInflow!$K$19:$W$25,9)-IF($A$59&lt;&gt;"",$B$59/2))*(C$54))</f>
-        <v>3.9325624217709758</v>
+        <v/>
       </c>
       <c r="D55" s="82" t="str">
         <f>IF(OR(D$28="",$A55=""),"",(VLOOKUP(D$54,DivideInflow!$K$19:$W$25,9)-IF($A$59&lt;&gt;"",$B$59/2))*(D$54))</f>
@@ -18140,9 +18138,9 @@
         <f t="shared" ref="L55" si="25">IF(OR(L$28="",$A55=""),"",IF(L53&lt;=SUM(L56:L60),0,IF(L53&lt;=SUM(L56:L60)+2*$B$25,(L53-SUM(L56:L60))/2,IF(L53&lt;=SUM(L56:L60)+2*$B$25+$B$55-$B$25,L53-SUM(L56:L60)-$B$25,$B$55))))</f>
         <v/>
       </c>
-      <c r="M55" s="225">
+      <c r="M55" s="225" t="e">
         <f>C55/C$54</f>
-        <v>0.42542222222222226</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N55" s="143"/>
       <c r="P55" s="81" t="str">
@@ -18158,9 +18156,9 @@
       <c r="B56" s="95" t="s">
         <v>314</v>
       </c>
-      <c r="C56" s="82">
+      <c r="C56" s="82" t="str">
         <f>IF(OR(C$28="",$A56=""),"",(VLOOKUP(C$54,DivideInflow!$K$19:$W$25,7)-IF($A$59&lt;&gt;"",$B$59/2))*(C$54))</f>
-        <v>2.2892016103330417</v>
+        <v/>
       </c>
       <c r="D56" s="82" t="str">
         <f>IF(OR(D$28="",$A56=""),"",(VLOOKUP(D$54,DivideInflow!$K$19:$W$25,7)-IF($A$59&lt;&gt;"",$B$59/2))*(D$54))</f>
@@ -18198,9 +18196,9 @@
         <f t="shared" ref="L56" si="30">IF(OR(L$28="",$A56=""),"",MIN(L52,L$53-SUM(L57:L60)))</f>
         <v/>
       </c>
-      <c r="M56" s="225">
+      <c r="M56" s="225" t="e">
         <f t="shared" ref="M56:M58" si="31">C56/C$54</f>
-        <v>0.24764444444444444</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N56" s="143"/>
     </row>
@@ -18212,9 +18210,9 @@
       <c r="B57" s="213">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="C57" s="82">
+      <c r="C57" s="82" t="str">
         <f>IF(OR(C$28="",$A57=""),"",VLOOKUP(C$54,DivideInflow!$K$19:$W$25,8)*(C$54))</f>
-        <v>0.30813015214461259</v>
+        <v/>
       </c>
       <c r="D57" s="82" t="str">
         <f>IF(OR(D$28="",$A57=""),"",VLOOKUP(D$54,DivideInflow!$K$18:$W$23,8)*(D$54))</f>
@@ -18252,9 +18250,9 @@
         <f t="shared" ref="L57" si="36">IF(OR(L$28="",$A57=""),"",MIN($B57,L$53-SUM(L58:L60)))</f>
         <v/>
       </c>
-      <c r="M57" s="225">
+      <c r="M57" s="225" t="e">
         <f t="shared" si="31"/>
-        <v>3.3333333333333333E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N57" s="143"/>
     </row>
@@ -18266,9 +18264,9 @@
       <c r="B58" s="213">
         <v>0.16700000000000001</v>
       </c>
-      <c r="C58" s="82">
+      <c r="C58" s="82" t="str">
         <f>IF(OR(C$28="",$A58=""),"",VLOOKUP(C$54,DivideInflow!$K$19:$W$25,10)*(C$54))</f>
-        <v>1.5406507607230628</v>
+        <v/>
       </c>
       <c r="D58" s="82" t="str">
         <f>IF(OR(D$28="",$A58=""),"",VLOOKUP(D$54,DivideInflow!$K$18:$W$23,10)*(D$54))</f>
@@ -18306,9 +18304,9 @@
         <f t="shared" ref="L58" si="41">IF(OR(L$28="",$A58=""),"",MIN($B58,L$53-SUM(L59:L60)))</f>
         <v/>
       </c>
-      <c r="M58" s="225">
+      <c r="M58" s="225" t="e">
         <f t="shared" si="31"/>
-        <v>0.16666666666666666</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N58" s="143"/>
     </row>
@@ -18321,9 +18319,9 @@
         <f>IF(A59="","",0.952/7.5)</f>
         <v>0.12693333333333331</v>
       </c>
-      <c r="C59" s="82">
+      <c r="C59" s="82" t="str">
         <f>IF(OR(C$28="",$A59=""),"",C$54*$B59)</f>
-        <v>1.1733596193666846</v>
+        <v/>
       </c>
       <c r="D59" s="82" t="str">
         <f t="shared" ref="D59:G59" si="42">IF(OR(D$28="",$A59=""),"",D$54*$B59)</f>
@@ -18361,9 +18359,9 @@
         <f t="shared" si="43"/>
         <v/>
       </c>
-      <c r="M59" s="225">
+      <c r="M59" s="225" t="e">
         <f>IF(A59="","",C59/C$54)</f>
-        <v>0.12693333333333331</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N59" s="143"/>
     </row>
@@ -18375,9 +18373,9 @@
       <c r="B60" s="151" t="s">
         <v>209</v>
       </c>
-      <c r="C60" s="153">
+      <c r="C60" s="153" t="str">
         <f>IF(OR(C$28="",$A60=""),"",MIN(C31,C52-C59))</f>
-        <v>0.6</v>
+        <v/>
       </c>
       <c r="D60" s="153" t="str">
         <f>IF(OR(D$28="",$A60=""),"",MIN(D31,D52-D59))</f>
@@ -18525,9 +18523,9 @@
         <f>IF(A65="","","   Net trade volume all participants (should be zero)")</f>
         <v xml:space="preserve">   Net trade volume all participants (should be zero)</v>
       </c>
-      <c r="C66" s="44">
-        <f t="shared" ref="C66:M66" ca="1" si="50">IF(OR(C$28="",$A66=""),"",C$119)</f>
-        <v>0</v>
+      <c r="C66" s="44" t="str">
+        <f t="shared" ref="C66:M66" si="50">IF(OR(C$28="",$A66=""),"",C$119)</f>
+        <v/>
       </c>
       <c r="D66" s="44" t="str">
         <f t="shared" si="50"/>
@@ -18578,9 +18576,9 @@
         <f>IF(A65="","","   Available Water [maf]")</f>
         <v xml:space="preserve">   Available Water [maf]</v>
       </c>
-      <c r="C67" s="12">
+      <c r="C67" s="12" t="str">
         <f>IF(OR(C$28="",$A67=""),"",C36+C53-C46+C64)</f>
-        <v>4.7610489999999999</v>
+        <v/>
       </c>
       <c r="D67" s="12" t="str">
         <f>IF(OR(D$28="",$A67=""),"",D36+D53-D46+D64)</f>
@@ -18646,9 +18644,9 @@
         <f>IF(A68="","","   End of Year Balance [maf]")</f>
         <v xml:space="preserve">   End of Year Balance [maf]</v>
       </c>
-      <c r="C69" s="12">
+      <c r="C69" s="12" t="str">
         <f>IF(OR(C$28="",$A69=""),"",C67-C68)</f>
-        <v>4.7610489999999999</v>
+        <v/>
       </c>
       <c r="D69" s="12" t="str">
         <f t="shared" ref="D69:L69" si="52">IF(OR(D$28="",$A69=""),"",D67-D68)</f>
@@ -18768,9 +18766,9 @@
         <f>IF(A73="","",$A$66)</f>
         <v xml:space="preserve">   Net trade volume all participants (should be zero)</v>
       </c>
-      <c r="C74" s="44">
-        <f t="shared" ref="C74:M74" ca="1" si="53">IF(OR(C$28="",$A74=""),"",C$119)</f>
-        <v>0</v>
+      <c r="C74" s="44" t="str">
+        <f t="shared" ref="C74:M74" si="53">IF(OR(C$28="",$A74=""),"",C$119)</f>
+        <v/>
       </c>
       <c r="D74" s="44" t="str">
         <f t="shared" si="53"/>
@@ -18821,9 +18819,9 @@
         <f>IF(A73="","","   Available Water [maf]")</f>
         <v xml:space="preserve">   Available Water [maf]</v>
       </c>
-      <c r="C75" s="12">
+      <c r="C75" s="12" t="str">
         <f>IF(OR(C$28="",$A75=""),"",C37+C55-C47+C72)</f>
-        <v>5.5051639270128625</v>
+        <v/>
       </c>
       <c r="D75" s="12" t="str">
         <f>IF(OR(D$28="",$A75=""),"",D37+D55-D47+D72)</f>
@@ -18889,9 +18887,9 @@
         <f>IF(A76="","","   End of Year Balance [maf]")</f>
         <v xml:space="preserve">   End of Year Balance [maf]</v>
       </c>
-      <c r="C77" s="12">
+      <c r="C77" s="12" t="str">
         <f>IF(OR(C$28="",$A77=""),"",C75-C76)</f>
-        <v>5.5051639270128625</v>
+        <v/>
       </c>
       <c r="D77" s="12" t="str">
         <f t="shared" ref="D77:L77" si="55">IF(OR(D$28="",$A77=""),"",D75-D76)</f>
@@ -19011,9 +19009,9 @@
         <f>IF(A81="","",$A$66)</f>
         <v xml:space="preserve">   Net trade volume all participants (should be zero)</v>
       </c>
-      <c r="C82" s="44">
-        <f t="shared" ref="C82:M82" ca="1" si="56">IF(OR(C$28="",$A82=""),"",C$119)</f>
-        <v>0</v>
+      <c r="C82" s="44" t="str">
+        <f t="shared" ref="C82:M82" si="56">IF(OR(C$28="",$A82=""),"",C$119)</f>
+        <v/>
       </c>
       <c r="D82" s="44" t="str">
         <f t="shared" si="56"/>
@@ -19064,9 +19062,9 @@
         <f>IF(A81="","","   Available Water [maf]")</f>
         <v xml:space="preserve">   Available Water [maf]</v>
       </c>
-      <c r="C83" s="12">
+      <c r="C83" s="12" t="str">
         <f>IF(OR(C$28="",$A83=""),"",C38+C56-C48+C80)</f>
-        <v>2.96195712791847</v>
+        <v/>
       </c>
       <c r="D83" s="12" t="str">
         <f t="shared" ref="D83:L83" si="57">IF(OR(D$28="",$A83=""),"",D38+D56-D48+D80)</f>
@@ -19132,9 +19130,9 @@
         <f>IF(A84="","","   End of Year Balance [maf]")</f>
         <v xml:space="preserve">   End of Year Balance [maf]</v>
       </c>
-      <c r="C85" s="12">
+      <c r="C85" s="12" t="str">
         <f>IF(OR(C$28="",$A85=""),"",C83-C84)</f>
-        <v>2.96195712791847</v>
+        <v/>
       </c>
       <c r="D85" s="12" t="str">
         <f t="shared" ref="D85:L85" si="58">IF(OR(D$28="",$A85=""),"",D83-D84)</f>
@@ -19254,9 +19252,9 @@
         <f>IF(A89="","",$A$66)</f>
         <v xml:space="preserve">   Net trade volume all participants (should be zero)</v>
       </c>
-      <c r="C90" s="44">
-        <f t="shared" ref="C90:M90" ca="1" si="59">IF(OR(C$28="",$A90=""),"",C$119)</f>
-        <v>0</v>
+      <c r="C90" s="44" t="str">
+        <f t="shared" ref="C90:M90" si="59">IF(OR(C$28="",$A90=""),"",C$119)</f>
+        <v/>
       </c>
       <c r="D90" s="44" t="str">
         <f t="shared" si="59"/>
@@ -19307,9 +19305,9 @@
         <f>IF(A89="","","   Available Water [maf]")</f>
         <v xml:space="preserve">   Available Water [maf]</v>
       </c>
-      <c r="C91" s="12">
+      <c r="C91" s="12" t="str">
         <f>IF(OR(C$28="",$A91=""),"",C39+C57-C49+C88)</f>
-        <v>1.2123287071440998</v>
+        <v/>
       </c>
       <c r="D91" s="12" t="str">
         <f t="shared" ref="D91:L91" si="60">IF(OR(D$28="",$A91=""),"",D39+D57-D49+D88)</f>
@@ -19375,9 +19373,9 @@
         <f>IF(A92="","","   End of Year Balance [maf]")</f>
         <v xml:space="preserve">   End of Year Balance [maf]</v>
       </c>
-      <c r="C93" s="12">
+      <c r="C93" s="12" t="str">
         <f>IF(OR(C$28="",$A93=""),"",C91-C92)</f>
-        <v>1.2123287071440998</v>
+        <v/>
       </c>
       <c r="D93" s="12" t="str">
         <f t="shared" ref="D93:L93" si="61">IF(OR(D$28="",$A93=""),"",D91-D92)</f>
@@ -19497,9 +19495,9 @@
         <f>IF(A97="","",$A$66)</f>
         <v xml:space="preserve">   Net trade volume all participants (should be zero)</v>
       </c>
-      <c r="C98" s="44">
-        <f t="shared" ref="C98:M98" ca="1" si="62">IF(OR(C$28="",$A98=""),"",C$119)</f>
-        <v>0</v>
+      <c r="C98" s="44" t="str">
+        <f t="shared" ref="C98:M98" si="62">IF(OR(C$28="",$A98=""),"",C$119)</f>
+        <v/>
       </c>
       <c r="D98" s="44" t="str">
         <f t="shared" si="62"/>
@@ -19550,9 +19548,9 @@
         <f>IF(A97="","","   Available Water [maf]")</f>
         <v xml:space="preserve">   Available Water [maf]</v>
       </c>
-      <c r="C99" s="12">
+      <c r="C99" s="12" t="str">
         <f>IF(OR(C$28="",$A99=""),"",C40+C58-C50+C96)</f>
-        <v>1.7403011323271773</v>
+        <v/>
       </c>
       <c r="D99" s="12" t="str">
         <f t="shared" ref="D99:L99" si="63">IF(OR(D$28="",$A99=""),"",D40+D58-D50+D96)</f>
@@ -19618,9 +19616,9 @@
         <f>IF(A100="","","   End of Year Balance [maf]")</f>
         <v xml:space="preserve">   End of Year Balance [maf]</v>
       </c>
-      <c r="C101" s="12">
+      <c r="C101" s="12" t="str">
         <f>IF(OR(C$28="",$A101=""),"",C99-C100)</f>
-        <v>1.7403011323271773</v>
+        <v/>
       </c>
       <c r="D101" s="12" t="str">
         <f t="shared" ref="D101:L101" si="64">IF(OR(D$28="",$A101=""),"",D99-D100)</f>
@@ -19740,9 +19738,9 @@
         <f>IF(A105="","",$A$66)</f>
         <v xml:space="preserve">   Net trade volume all participants (should be zero)</v>
       </c>
-      <c r="C106" s="44">
-        <f t="shared" ref="C106:M106" ca="1" si="65">IF(OR(C$28="",$A106=""),"",C$119)</f>
-        <v>0</v>
+      <c r="C106" s="44" t="str">
+        <f t="shared" ref="C106:M106" si="65">IF(OR(C$28="",$A106=""),"",C$119)</f>
+        <v/>
       </c>
       <c r="D106" s="44" t="str">
         <f t="shared" si="65"/>
@@ -19793,9 +19791,9 @@
         <f>IF(A105="","","   Available Water [maf]")</f>
         <v xml:space="preserve">   Available Water [maf]</v>
       </c>
-      <c r="C107" s="12">
+      <c r="C107" s="12" t="str">
         <f>IF(OR(C$28="",$A107=""),"",C41+C59-C51+C104)</f>
-        <v>1.3664328832029817</v>
+        <v/>
       </c>
       <c r="D107" s="12" t="str">
         <f t="shared" ref="D107:L107" si="66">IF(OR(D$28="",$A107=""),"",D41+D59-D51+D104)</f>
@@ -19861,9 +19859,9 @@
         <f>IF(A108="","","   End of Year Balance [maf]")</f>
         <v xml:space="preserve">   End of Year Balance [maf]</v>
       </c>
-      <c r="C109" s="12">
+      <c r="C109" s="12" t="str">
         <f>IF(OR(C$28="",$A109=""),"",C107-C108)</f>
-        <v>1.3664328832029817</v>
+        <v/>
       </c>
       <c r="D109" s="12" t="str">
         <f t="shared" ref="D109:L109" si="67">IF(OR(D$28="",$A109=""),"",D107-D108)</f>
@@ -19945,9 +19943,9 @@
         <v xml:space="preserve">    Reclamation - Protect Zone</v>
       </c>
       <c r="B113" s="1"/>
-      <c r="C113" s="44">
+      <c r="C113" s="44" t="str">
         <f t="shared" ref="C113:L113" ca="1" si="69">IF(OR(C$28="",$A113=""),"",OFFSET(C$64,8*(ROW(B113)-ROW(B$113)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D113" s="44" t="str">
         <f t="shared" ca="1" si="69"/>
@@ -19997,9 +19995,9 @@
         <v xml:space="preserve">    California</v>
       </c>
       <c r="B114" s="1"/>
-      <c r="C114" s="44">
+      <c r="C114" s="44" t="str">
         <f t="shared" ref="C114:L114" ca="1" si="70">IF(OR(C$28="",$A114=""),"",OFFSET(C$64,8*(ROW(B114)-ROW(B$113)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D114" s="44" t="str">
         <f t="shared" ca="1" si="70"/>
@@ -20049,9 +20047,9 @@
         <v xml:space="preserve">    Arizona</v>
       </c>
       <c r="B115" s="1"/>
-      <c r="C115" s="44">
+      <c r="C115" s="44" t="str">
         <f t="shared" ref="C115:L115" ca="1" si="72">IF(OR(C$28="",$A115=""),"",OFFSET(C$64,8*(ROW(B115)-ROW(B$113)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D115" s="44" t="str">
         <f t="shared" ca="1" si="72"/>
@@ -20101,9 +20099,9 @@
         <v xml:space="preserve">    Nevada</v>
       </c>
       <c r="B116" s="1"/>
-      <c r="C116" s="44">
+      <c r="C116" s="44" t="str">
         <f t="shared" ref="C116:L116" ca="1" si="73">IF(OR(C$28="",$A116=""),"",OFFSET(C$64,8*(ROW(B116)-ROW(B$113)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D116" s="44" t="str">
         <f t="shared" ca="1" si="73"/>
@@ -20153,9 +20151,9 @@
         <v xml:space="preserve">    Mexico</v>
       </c>
       <c r="B117" s="1"/>
-      <c r="C117" s="44">
+      <c r="C117" s="44" t="str">
         <f t="shared" ref="C117:L117" ca="1" si="74">IF(OR(C$28="",$A117=""),"",OFFSET(C$64,8*(ROW(B117)-ROW(B$113)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D117" s="44" t="str">
         <f t="shared" ca="1" si="74"/>
@@ -20205,9 +20203,9 @@
         <v xml:space="preserve">    Tribal Nations of the Lower Basin</v>
       </c>
       <c r="B118" s="1"/>
-      <c r="C118" s="44">
+      <c r="C118" s="44" t="str">
         <f t="shared" ref="C118:L118" ca="1" si="75">IF(OR(C$28="",$A118=""),"",OFFSET(C$64,8*(ROW(B118)-ROW(B$113)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D118" s="44" t="str">
         <f t="shared" ca="1" si="75"/>
@@ -20256,9 +20254,9 @@
         <v>77</v>
       </c>
       <c r="B119" s="1"/>
-      <c r="C119" s="12">
-        <f ca="1">IF(C$28&lt;&gt;"",SUM(C113:C118),"")</f>
-        <v>0</v>
+      <c r="C119" s="12" t="str">
+        <f>IF(C$28&lt;&gt;"",SUM(C113:C118),"")</f>
+        <v/>
       </c>
       <c r="D119" s="12" t="str">
         <f t="shared" ref="D119:L119" si="76">IF(D$28&lt;&gt;"",SUM(D113:D118),"")</f>
@@ -20321,9 +20319,9 @@
         <f>IF(A5="","","    "&amp;A5&amp;" - Consumptive Use and Headwaters Losses")</f>
         <v xml:space="preserve">    Reclamation - Protect Zone - Consumptive Use and Headwaters Losses</v>
       </c>
-      <c r="C121" s="44">
+      <c r="C121" s="44" t="str">
         <f t="shared" ref="C121:L121" ca="1" si="77">IF(OR(C$28="",$A121=""),"",OFFSET(C$68,8*(ROW(B121)-ROW(B$121)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D121" s="44" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -20368,9 +20366,9 @@
         <f>IF(A6="","","    "&amp;A6&amp;" - Release from Mead")</f>
         <v xml:space="preserve">    California - Release from Mead</v>
       </c>
-      <c r="C122" s="44">
+      <c r="C122" s="44" t="str">
         <f t="shared" ref="C122:L122" ca="1" si="78">IF(OR(C$28="",$A122=""),"",OFFSET(C$68,8*(ROW(B122)-ROW(B$121)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D122" s="44" t="str">
         <f t="shared" ca="1" si="78"/>
@@ -20415,9 +20413,9 @@
         <f>IF(A7="","","    "&amp;A7&amp;" - Release from Mead")</f>
         <v xml:space="preserve">    Arizona - Release from Mead</v>
       </c>
-      <c r="C123" s="44">
+      <c r="C123" s="44" t="str">
         <f t="shared" ref="C123:L123" ca="1" si="79">IF(OR(C$28="",$A123=""),"",OFFSET(C$68,8*(ROW(B123)-ROW(B$121)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D123" s="44" t="str">
         <f t="shared" ca="1" si="79"/>
@@ -20462,9 +20460,9 @@
         <f>IF(A8="","","    "&amp;A8&amp;" - Release from Mead")</f>
         <v xml:space="preserve">    Nevada - Release from Mead</v>
       </c>
-      <c r="C124" s="44">
+      <c r="C124" s="44" t="str">
         <f t="shared" ref="C124:L124" ca="1" si="80">IF(OR(C$28="",$A124=""),"",OFFSET(C$68,8*(ROW(B124)-ROW(B$121)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D124" s="44" t="str">
         <f t="shared" ca="1" si="80"/>
@@ -20509,9 +20507,9 @@
         <f>IF(A9="","","    "&amp;A9&amp;" - Release from Mead")</f>
         <v xml:space="preserve">    Mexico - Release from Mead</v>
       </c>
-      <c r="C125" s="44">
+      <c r="C125" s="44" t="str">
         <f t="shared" ref="C125:L125" ca="1" si="81">IF(OR(C$28="",$A125=""),"",OFFSET(C$68,8*(ROW(B125)-ROW(B$121)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D125" s="44" t="str">
         <f t="shared" ca="1" si="81"/>
@@ -20556,9 +20554,9 @@
         <f>IF(A10="","","    "&amp;A10&amp;" - Release from Mead")</f>
         <v xml:space="preserve">    Tribal Nations of the Lower Basin - Release from Mead</v>
       </c>
-      <c r="C126" s="44">
+      <c r="C126" s="44" t="str">
         <f t="shared" ref="C126:L126" ca="1" si="82">IF(OR(C$28="",$A126=""),"",OFFSET(C$68,8*(ROW(B126)-ROW(B$121)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D126" s="44" t="str">
         <f t="shared" ca="1" si="82"/>
@@ -20619,9 +20617,9 @@
         <f t="shared" ref="A128:A133" si="83">IF(A5="","","    "&amp;A5)</f>
         <v xml:space="preserve">    Reclamation - Protect Zone</v>
       </c>
-      <c r="C128" s="44">
+      <c r="C128" s="44" t="str">
         <f t="shared" ref="C128:L128" ca="1" si="84">IF(OR(C$28="",$A128=""),"",OFFSET(C$69,8*(ROW(B128)-ROW(B$128)),0))</f>
-        <v>4.7610489999999999</v>
+        <v/>
       </c>
       <c r="D128" s="44" t="str">
         <f t="shared" ca="1" si="84"/>
@@ -20666,9 +20664,9 @@
         <f t="shared" si="83"/>
         <v xml:space="preserve">    California</v>
       </c>
-      <c r="C129" s="44">
+      <c r="C129" s="44" t="str">
         <f t="shared" ref="C129:L129" ca="1" si="85">IF(OR(C$28="",$A129=""),"",OFFSET(C$69,8*(ROW(B129)-ROW(B$128)),0))</f>
-        <v>5.5051639270128625</v>
+        <v/>
       </c>
       <c r="D129" s="44" t="str">
         <f t="shared" ca="1" si="85"/>
@@ -20713,9 +20711,9 @@
         <f t="shared" si="83"/>
         <v xml:space="preserve">    Arizona</v>
       </c>
-      <c r="C130" s="44">
+      <c r="C130" s="44" t="str">
         <f t="shared" ref="C130:L130" ca="1" si="86">IF(OR(C$28="",$A130=""),"",OFFSET(C$69,8*(ROW(B130)-ROW(B$128)),0))</f>
-        <v>2.96195712791847</v>
+        <v/>
       </c>
       <c r="D130" s="44" t="str">
         <f t="shared" ca="1" si="86"/>
@@ -20760,9 +20758,9 @@
         <f t="shared" si="83"/>
         <v xml:space="preserve">    Nevada</v>
       </c>
-      <c r="C131" s="44">
+      <c r="C131" s="44" t="str">
         <f t="shared" ref="C131:L131" ca="1" si="87">IF(OR(C$28="",$A131=""),"",OFFSET(C$69,8*(ROW(B131)-ROW(B$128)),0))</f>
-        <v>1.2123287071440998</v>
+        <v/>
       </c>
       <c r="D131" s="44" t="str">
         <f t="shared" ca="1" si="87"/>
@@ -20807,9 +20805,9 @@
         <f t="shared" si="83"/>
         <v xml:space="preserve">    Mexico</v>
       </c>
-      <c r="C132" s="44">
+      <c r="C132" s="44" t="str">
         <f t="shared" ref="C132:L132" ca="1" si="88">IF(OR(C$28="",$A132=""),"",OFFSET(C$69,8*(ROW(B132)-ROW(B$128)),0))</f>
-        <v>1.7403011323271773</v>
+        <v/>
       </c>
       <c r="D132" s="44" t="str">
         <f t="shared" ca="1" si="88"/>
@@ -20854,9 +20852,9 @@
         <f t="shared" si="83"/>
         <v xml:space="preserve">    Tribal Nations of the Lower Basin</v>
       </c>
-      <c r="C133" s="44">
+      <c r="C133" s="44" t="str">
         <f t="shared" ref="C133:L133" ca="1" si="89">IF(OR(C$28="",$A133=""),"",OFFSET(C$69,8*(ROW(B133)-ROW(B$128)),0))</f>
-        <v>1.3664328832029817</v>
+        <v/>
       </c>
       <c r="D133" s="44" t="str">
         <f t="shared" ca="1" si="89"/>
@@ -20921,7 +20919,7 @@
         <v/>
       </c>
       <c r="N134" s="141" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.35">
@@ -20929,9 +20927,9 @@
         <v>303</v>
       </c>
       <c r="B135" s="1"/>
-      <c r="C135" s="12">
-        <f ca="1">IF(C$28&lt;&gt;"",SUM(C128:C133),"")</f>
-        <v>17.547232777605593</v>
+      <c r="C135" s="12" t="str">
+        <f>IF(C$28&lt;&gt;"",SUM(C128:C133),"")</f>
+        <v/>
       </c>
       <c r="D135" s="12" t="str">
         <f>IF(D$28&lt;&gt;"",SUM(D128:D133),"")</f>
@@ -20961,9 +20959,9 @@
         <v>304</v>
       </c>
       <c r="B136" s="1"/>
-      <c r="C136" s="221">
-        <f ca="1">IF(C$28&lt;&gt;"",VLOOKUP(C135*1000000,'Mead-Elevation-Area'!$B$5:$H$689,7),"")</f>
-        <v>1157</v>
+      <c r="C136" s="221" t="str">
+        <f>IF(C$28&lt;&gt;"",VLOOKUP(C135*1000000,'Mead-Elevation-Area'!$B$5:$H$689,7),"")</f>
+        <v/>
       </c>
       <c r="D136" s="221" t="str">
         <f>IF(D$28&lt;&gt;"",VLOOKUP(D135*1000000,'Mead-Elevation-Area'!$B$5:$H$689,7),"")</f>
@@ -21276,7 +21274,7 @@
     <hyperlink ref="N17" r:id="rId2" location="1b-make-assumptions" xr:uid="{91CC7212-C579-4B1B-A8B8-969D4549837D}"/>
     <hyperlink ref="N18" r:id="rId3" location="i-evaporation-rates" xr:uid="{23C61350-606E-472B-90E1-88574D6741EE}"/>
     <hyperlink ref="N19" r:id="rId4" location="ii-start-storage" xr:uid="{692C3AE6-515B-4C08-B6EC-0557E75E9511}"/>
-    <hyperlink ref="N20" r:id="rId5" location="iii-protection-elevations" xr:uid="{16CC5ED4-0369-416C-AC3E-3AD6F831A454}"/>
+    <hyperlink ref="N20" r:id="rId5" location="iii-protection-elevation" xr:uid="{16CC5ED4-0369-416C-AC3E-3AD6F831A454}"/>
     <hyperlink ref="N21" r:id="rId6" location="iv-storage-above-protect-zone" display="Help protect volume" xr:uid="{D7802E8D-5298-4564-9936-B3226B6E96DA}"/>
     <hyperlink ref="N22" r:id="rId7" location="v-water-conservation-program-ics-total-balance" xr:uid="{9E773CCF-F296-48D2-ADA9-5456ABC7F062}"/>
     <hyperlink ref="N23" r:id="rId8" location="vi-remaining-storage-above-the-protect-and-ics-balances" xr:uid="{8CAE8559-5BD9-4D9F-8655-D1F3AE1FCD4D}"/>
@@ -21297,8 +21295,8 @@
     <hyperlink ref="N69" r:id="rId23" location="vi-end-of-year-balance" xr:uid="{43A45EF2-1AE7-497D-9090-A6710371091B}"/>
     <hyperlink ref="N103" r:id="rId24" location="5a-shared-reserve-dashboard" display="Help shared, reserve" xr:uid="{93564FFE-2F11-4E1B-8E30-F04D091042B0}"/>
     <hyperlink ref="N111" r:id="rId25" location="step-6-summary-of-participant-actions" xr:uid="{39E9E91B-EE9B-4603-9A19-992E43688C4C}"/>
-    <hyperlink ref="N134" r:id="rId26" location="6a-combined-storage--end-of-year" xr:uid="{18709FDC-6FB8-4FF1-82C7-3E0140C4C207}"/>
-    <hyperlink ref="N137" r:id="rId27" location="step-8-move-to-next-year" xr:uid="{0D1EBCA9-BE7F-441F-A17C-5330CFCE7596}"/>
+    <hyperlink ref="N134" r:id="rId26" location="lake-mead--end-of-year" xr:uid="{18709FDC-6FB8-4FF1-82C7-3E0140C4C207}"/>
+    <hyperlink ref="N137" r:id="rId27" location="step-7-move-to-next-year" xr:uid="{0D1EBCA9-BE7F-441F-A17C-5330CFCE7596}"/>
     <hyperlink ref="N79" r:id="rId28" location="step-5-player-dashboards--conserve-consume-and-trade" xr:uid="{115088D1-B3CF-4D72-A6D6-92770E18F116}"/>
     <hyperlink ref="N80" r:id="rId29" location="i-buy-or-sell-water-from-other-players" xr:uid="{D5A878F8-1AB0-4367-BFA6-4F25001F73AD}"/>
     <hyperlink ref="N81" r:id="rId30" location="ii-compensation" xr:uid="{74477D73-291E-4A7F-86F2-C21A0DF60CEA}"/>
@@ -21562,12 +21560,12 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.35">
@@ -23612,9 +23610,9 @@
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="M39" s="28">
+      <c r="M39" s="28" t="str">
         <f>Master!C52</f>
-        <v>9.5</v>
+        <v/>
       </c>
       <c r="N39" s="140" t="s">
         <v>193</v>
@@ -23668,9 +23666,9 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="M40" s="28">
+      <c r="M40" s="28" t="str">
         <f>Master!C53</f>
-        <v>0.25609543566162268</v>
+        <v/>
       </c>
       <c r="N40" s="143"/>
       <c r="P40" s="81"/>
@@ -23724,9 +23722,9 @@
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="M41" s="28">
+      <c r="M41" s="28" t="str">
         <f>Master!C55</f>
-        <v>3.9325624217709758</v>
+        <v/>
       </c>
       <c r="N41" s="143"/>
       <c r="P41" s="81"/>
@@ -23779,9 +23777,9 @@
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="M42" s="28">
+      <c r="M42" s="28" t="str">
         <f>Master!C56</f>
-        <v>2.2892016103330417</v>
+        <v/>
       </c>
       <c r="N42" s="143"/>
     </row>
@@ -23834,9 +23832,9 @@
         <f t="shared" si="10"/>
         <v>#REF!</v>
       </c>
-      <c r="M43" s="180">
+      <c r="M43" s="180" t="str">
         <f>Master!C57</f>
-        <v>0.30813015214461259</v>
+        <v/>
       </c>
       <c r="N43" s="143"/>
     </row>
@@ -23889,9 +23887,9 @@
         <f t="shared" si="12"/>
         <v>#REF!</v>
       </c>
-      <c r="M44" s="28">
+      <c r="M44" s="28" t="str">
         <f>Master!C58</f>
-        <v>1.5406507607230628</v>
+        <v/>
       </c>
       <c r="N44" s="143"/>
     </row>
@@ -23943,9 +23941,9 @@
         <f t="shared" si="13"/>
         <v>#REF!</v>
       </c>
-      <c r="M45" s="28">
+      <c r="M45" s="28" t="str">
         <f>Master!C59</f>
-        <v>1.1733596193666846</v>
+        <v/>
       </c>
       <c r="N45" s="143"/>
     </row>
@@ -23997,9 +23995,9 @@
         <f t="shared" si="14"/>
         <v>#REF!</v>
       </c>
-      <c r="M46" s="28">
+      <c r="M46" s="28" t="str">
         <f>Master!C60</f>
-        <v>0.6</v>
+        <v/>
       </c>
       <c r="N46" s="143"/>
     </row>

</xml_diff>

<commit_message>
Add % California of Tribal from Tribal Worksheet
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67746C17-FC2A-46FE-A8B8-122CA301DD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED68F8B-3672-43F7-B694-1312C6BE9DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="62" r:id="rId1"/>
@@ -3278,50 +3278,26 @@
     <xf numFmtId="9" fontId="3" fillId="2" borderId="10" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="21" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="166" fontId="1" fillId="21" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="172" fontId="1" fillId="21" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3377,6 +3353,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3400,6 +3382,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3503,11 +3524,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3529,27 +3550,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="1" fillId="21" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="1" fillId="21" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="1" fillId="21" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -14968,20 +14968,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="255" t="s">
+      <c r="A1" s="249" t="s">
         <v>351</v>
       </c>
-      <c r="B1" s="255"/>
-      <c r="C1" s="255"/>
-      <c r="D1" s="255"/>
-      <c r="E1" s="255"/>
-      <c r="F1" s="255"/>
-      <c r="G1" s="255"/>
-      <c r="H1" s="255"/>
-      <c r="I1" s="255"/>
-      <c r="J1" s="255"/>
-      <c r="K1" s="255"/>
-      <c r="L1" s="255"/>
+      <c r="B1" s="249"/>
+      <c r="C1" s="249"/>
+      <c r="D1" s="249"/>
+      <c r="E1" s="249"/>
+      <c r="F1" s="249"/>
+      <c r="G1" s="249"/>
+      <c r="H1" s="249"/>
+      <c r="I1" s="249"/>
+      <c r="J1" s="249"/>
+      <c r="K1" s="249"/>
+      <c r="L1" s="249"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -15007,41 +15007,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="256" t="s">
+      <c r="A4" s="250" t="s">
         <v>352</v>
       </c>
-      <c r="B4" s="257"/>
-      <c r="C4" s="257"/>
-      <c r="D4" s="257"/>
-      <c r="E4" s="257"/>
-      <c r="F4" s="257"/>
-      <c r="G4" s="257"/>
-      <c r="H4" s="257"/>
-      <c r="I4" s="257"/>
-      <c r="J4" s="257"/>
-      <c r="K4" s="257"/>
-      <c r="L4" s="258"/>
-      <c r="N4" s="259"/>
-      <c r="O4" s="259"/>
-      <c r="P4" s="259"/>
-      <c r="Q4" s="259"/>
-      <c r="R4" s="259"/>
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="252"/>
+      <c r="N4" s="253"/>
+      <c r="O4" s="253"/>
+      <c r="P4" s="253"/>
+      <c r="Q4" s="253"/>
+      <c r="R4" s="253"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="260" t="s">
+      <c r="A5" s="254" t="s">
         <v>335</v>
       </c>
-      <c r="B5" s="261"/>
-      <c r="C5" s="261"/>
-      <c r="D5" s="261"/>
-      <c r="E5" s="261"/>
-      <c r="F5" s="261"/>
-      <c r="G5" s="261"/>
-      <c r="H5" s="261"/>
-      <c r="I5" s="261"/>
-      <c r="J5" s="261"/>
-      <c r="K5" s="261"/>
-      <c r="L5" s="262"/>
+      <c r="B5" s="255"/>
+      <c r="C5" s="255"/>
+      <c r="D5" s="255"/>
+      <c r="E5" s="255"/>
+      <c r="F5" s="255"/>
+      <c r="G5" s="255"/>
+      <c r="H5" s="255"/>
+      <c r="I5" s="255"/>
+      <c r="J5" s="255"/>
+      <c r="K5" s="255"/>
+      <c r="L5" s="256"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15049,20 +15049,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="260" t="s">
+      <c r="A6" s="254" t="s">
         <v>353</v>
       </c>
-      <c r="B6" s="261"/>
-      <c r="C6" s="261"/>
-      <c r="D6" s="261"/>
-      <c r="E6" s="261"/>
-      <c r="F6" s="261"/>
-      <c r="G6" s="261"/>
-      <c r="H6" s="261"/>
-      <c r="I6" s="261"/>
-      <c r="J6" s="261"/>
-      <c r="K6" s="261"/>
-      <c r="L6" s="262"/>
+      <c r="B6" s="255"/>
+      <c r="C6" s="255"/>
+      <c r="D6" s="255"/>
+      <c r="E6" s="255"/>
+      <c r="F6" s="255"/>
+      <c r="G6" s="255"/>
+      <c r="H6" s="255"/>
+      <c r="I6" s="255"/>
+      <c r="J6" s="255"/>
+      <c r="K6" s="255"/>
+      <c r="L6" s="256"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15071,19 +15071,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="233"/>
-      <c r="B7" s="261" t="s">
+      <c r="B7" s="255" t="s">
         <v>354</v>
       </c>
-      <c r="C7" s="261"/>
-      <c r="D7" s="261"/>
-      <c r="E7" s="261"/>
-      <c r="F7" s="261"/>
-      <c r="G7" s="261"/>
-      <c r="H7" s="261"/>
-      <c r="I7" s="261"/>
-      <c r="J7" s="261"/>
-      <c r="K7" s="261"/>
-      <c r="L7" s="262"/>
+      <c r="C7" s="255"/>
+      <c r="D7" s="255"/>
+      <c r="E7" s="255"/>
+      <c r="F7" s="255"/>
+      <c r="G7" s="255"/>
+      <c r="H7" s="255"/>
+      <c r="I7" s="255"/>
+      <c r="J7" s="255"/>
+      <c r="K7" s="255"/>
+      <c r="L7" s="256"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15092,19 +15092,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="234"/>
-      <c r="B8" s="276" t="s">
+      <c r="B8" s="272" t="s">
         <v>355</v>
       </c>
-      <c r="C8" s="276"/>
-      <c r="D8" s="276"/>
-      <c r="E8" s="276"/>
-      <c r="F8" s="276"/>
-      <c r="G8" s="276"/>
-      <c r="H8" s="276"/>
-      <c r="I8" s="276"/>
-      <c r="J8" s="276"/>
-      <c r="K8" s="276"/>
-      <c r="L8" s="277"/>
+      <c r="C8" s="272"/>
+      <c r="D8" s="272"/>
+      <c r="E8" s="272"/>
+      <c r="F8" s="272"/>
+      <c r="G8" s="272"/>
+      <c r="H8" s="272"/>
+      <c r="I8" s="272"/>
+      <c r="J8" s="272"/>
+      <c r="K8" s="272"/>
+      <c r="L8" s="273"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15126,84 +15126,84 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="263" t="s">
+      <c r="A10" s="257" t="s">
         <v>205</v>
       </c>
-      <c r="B10" s="264"/>
-      <c r="C10" s="264"/>
-      <c r="D10" s="264"/>
-      <c r="E10" s="264"/>
-      <c r="F10" s="264"/>
-      <c r="G10" s="264"/>
-      <c r="H10" s="264"/>
-      <c r="I10" s="264"/>
-      <c r="J10" s="264"/>
-      <c r="K10" s="264"/>
-      <c r="L10" s="265"/>
+      <c r="B10" s="258"/>
+      <c r="C10" s="258"/>
+      <c r="D10" s="258"/>
+      <c r="E10" s="258"/>
+      <c r="F10" s="258"/>
+      <c r="G10" s="258"/>
+      <c r="H10" s="258"/>
+      <c r="I10" s="258"/>
+      <c r="J10" s="258"/>
+      <c r="K10" s="258"/>
+      <c r="L10" s="259"/>
     </row>
     <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="266" t="s">
+      <c r="A11" s="260" t="s">
         <v>336</v>
       </c>
-      <c r="B11" s="267"/>
-      <c r="C11" s="267"/>
-      <c r="D11" s="267"/>
-      <c r="E11" s="267"/>
-      <c r="F11" s="267"/>
-      <c r="G11" s="267"/>
-      <c r="H11" s="267"/>
-      <c r="I11" s="267"/>
-      <c r="J11" s="267"/>
-      <c r="K11" s="267"/>
-      <c r="L11" s="268"/>
+      <c r="B11" s="261"/>
+      <c r="C11" s="261"/>
+      <c r="D11" s="261"/>
+      <c r="E11" s="261"/>
+      <c r="F11" s="261"/>
+      <c r="G11" s="261"/>
+      <c r="H11" s="261"/>
+      <c r="I11" s="261"/>
+      <c r="J11" s="261"/>
+      <c r="K11" s="261"/>
+      <c r="L11" s="262"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="269" t="s">
+      <c r="A12" s="263" t="s">
         <v>337</v>
       </c>
-      <c r="B12" s="247"/>
-      <c r="C12" s="247"/>
-      <c r="D12" s="247"/>
-      <c r="E12" s="247"/>
-      <c r="F12" s="247"/>
-      <c r="G12" s="247"/>
-      <c r="H12" s="247"/>
-      <c r="I12" s="247"/>
-      <c r="J12" s="247"/>
-      <c r="K12" s="247"/>
-      <c r="L12" s="248"/>
+      <c r="B12" s="264"/>
+      <c r="C12" s="264"/>
+      <c r="D12" s="264"/>
+      <c r="E12" s="264"/>
+      <c r="F12" s="264"/>
+      <c r="G12" s="264"/>
+      <c r="H12" s="264"/>
+      <c r="I12" s="264"/>
+      <c r="J12" s="264"/>
+      <c r="K12" s="264"/>
+      <c r="L12" s="265"/>
     </row>
     <row r="13" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="269" t="s">
+      <c r="A13" s="263" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="247"/>
-      <c r="C13" s="247"/>
-      <c r="D13" s="247"/>
-      <c r="E13" s="247"/>
-      <c r="F13" s="247"/>
-      <c r="G13" s="247"/>
-      <c r="H13" s="247"/>
-      <c r="I13" s="247"/>
-      <c r="J13" s="247"/>
-      <c r="K13" s="247"/>
-      <c r="L13" s="248"/>
+      <c r="B13" s="264"/>
+      <c r="C13" s="264"/>
+      <c r="D13" s="264"/>
+      <c r="E13" s="264"/>
+      <c r="F13" s="264"/>
+      <c r="G13" s="264"/>
+      <c r="H13" s="264"/>
+      <c r="I13" s="264"/>
+      <c r="J13" s="264"/>
+      <c r="K13" s="264"/>
+      <c r="L13" s="265"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="270" t="s">
+      <c r="A14" s="266" t="s">
         <v>338</v>
       </c>
-      <c r="B14" s="271"/>
-      <c r="C14" s="271"/>
-      <c r="D14" s="271"/>
-      <c r="E14" s="271"/>
-      <c r="F14" s="271"/>
-      <c r="G14" s="271"/>
-      <c r="H14" s="271"/>
-      <c r="I14" s="271"/>
-      <c r="J14" s="271"/>
-      <c r="K14" s="271"/>
-      <c r="L14" s="272"/>
+      <c r="B14" s="267"/>
+      <c r="C14" s="267"/>
+      <c r="D14" s="267"/>
+      <c r="E14" s="267"/>
+      <c r="F14" s="267"/>
+      <c r="G14" s="267"/>
+      <c r="H14" s="267"/>
+      <c r="I14" s="267"/>
+      <c r="J14" s="267"/>
+      <c r="K14" s="267"/>
+      <c r="L14" s="268"/>
     </row>
     <row r="15" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="113"/>
@@ -15220,332 +15220,332 @@
       <c r="L15" s="113"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="273" t="s">
+      <c r="A16" s="269" t="s">
         <v>334</v>
       </c>
-      <c r="B16" s="274"/>
-      <c r="C16" s="274"/>
-      <c r="D16" s="274"/>
-      <c r="E16" s="274"/>
-      <c r="F16" s="274"/>
-      <c r="G16" s="274"/>
-      <c r="H16" s="274"/>
-      <c r="I16" s="274"/>
-      <c r="J16" s="274"/>
-      <c r="K16" s="274"/>
-      <c r="L16" s="275"/>
+      <c r="B16" s="270"/>
+      <c r="C16" s="270"/>
+      <c r="D16" s="270"/>
+      <c r="E16" s="270"/>
+      <c r="F16" s="270"/>
+      <c r="G16" s="270"/>
+      <c r="H16" s="270"/>
+      <c r="I16" s="270"/>
+      <c r="J16" s="270"/>
+      <c r="K16" s="270"/>
+      <c r="L16" s="271"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="252" t="s">
+      <c r="A17" s="246" t="s">
         <v>215</v>
       </c>
-      <c r="B17" s="253"/>
-      <c r="C17" s="253"/>
-      <c r="D17" s="253"/>
-      <c r="E17" s="253"/>
-      <c r="F17" s="253"/>
-      <c r="G17" s="253"/>
-      <c r="H17" s="253"/>
-      <c r="I17" s="253"/>
-      <c r="J17" s="253"/>
-      <c r="K17" s="253"/>
-      <c r="L17" s="254"/>
+      <c r="B17" s="247"/>
+      <c r="C17" s="247"/>
+      <c r="D17" s="247"/>
+      <c r="E17" s="247"/>
+      <c r="F17" s="247"/>
+      <c r="G17" s="247"/>
+      <c r="H17" s="247"/>
+      <c r="I17" s="247"/>
+      <c r="J17" s="247"/>
+      <c r="K17" s="247"/>
+      <c r="L17" s="248"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="228">
         <v>1</v>
       </c>
-      <c r="B18" s="240" t="s">
+      <c r="B18" s="276" t="s">
         <v>214</v>
       </c>
-      <c r="C18" s="240"/>
-      <c r="D18" s="240"/>
-      <c r="E18" s="240"/>
-      <c r="F18" s="240"/>
-      <c r="G18" s="240"/>
-      <c r="H18" s="240"/>
-      <c r="I18" s="240"/>
-      <c r="J18" s="240"/>
-      <c r="K18" s="240"/>
-      <c r="L18" s="241"/>
+      <c r="C18" s="276"/>
+      <c r="D18" s="276"/>
+      <c r="E18" s="276"/>
+      <c r="F18" s="276"/>
+      <c r="G18" s="276"/>
+      <c r="H18" s="276"/>
+      <c r="I18" s="276"/>
+      <c r="J18" s="276"/>
+      <c r="K18" s="276"/>
+      <c r="L18" s="277"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="228">
         <v>2</v>
       </c>
-      <c r="B19" s="240" t="s">
+      <c r="B19" s="276" t="s">
         <v>330</v>
       </c>
-      <c r="C19" s="240"/>
-      <c r="D19" s="240"/>
-      <c r="E19" s="240"/>
-      <c r="F19" s="240"/>
-      <c r="G19" s="240"/>
-      <c r="H19" s="240"/>
-      <c r="I19" s="240"/>
-      <c r="J19" s="240"/>
-      <c r="K19" s="240"/>
-      <c r="L19" s="241"/>
+      <c r="C19" s="276"/>
+      <c r="D19" s="276"/>
+      <c r="E19" s="276"/>
+      <c r="F19" s="276"/>
+      <c r="G19" s="276"/>
+      <c r="H19" s="276"/>
+      <c r="I19" s="276"/>
+      <c r="J19" s="276"/>
+      <c r="K19" s="276"/>
+      <c r="L19" s="277"/>
       <c r="N19" s="106"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="228">
         <v>3</v>
       </c>
-      <c r="B20" s="240" t="s">
+      <c r="B20" s="276" t="s">
         <v>207</v>
       </c>
-      <c r="C20" s="240"/>
-      <c r="D20" s="240"/>
-      <c r="E20" s="240"/>
-      <c r="F20" s="240"/>
-      <c r="G20" s="240"/>
-      <c r="H20" s="240"/>
-      <c r="I20" s="240"/>
-      <c r="J20" s="240"/>
-      <c r="K20" s="240"/>
-      <c r="L20" s="241"/>
+      <c r="C20" s="276"/>
+      <c r="D20" s="276"/>
+      <c r="E20" s="276"/>
+      <c r="F20" s="276"/>
+      <c r="G20" s="276"/>
+      <c r="H20" s="276"/>
+      <c r="I20" s="276"/>
+      <c r="J20" s="276"/>
+      <c r="K20" s="276"/>
+      <c r="L20" s="277"/>
       <c r="N20" s="106"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="228">
         <v>4</v>
       </c>
-      <c r="B21" s="240" t="s">
+      <c r="B21" s="276" t="s">
         <v>339</v>
       </c>
-      <c r="C21" s="240"/>
-      <c r="D21" s="240"/>
-      <c r="E21" s="240"/>
-      <c r="F21" s="240"/>
-      <c r="G21" s="240"/>
-      <c r="H21" s="240"/>
-      <c r="I21" s="240"/>
-      <c r="J21" s="240"/>
-      <c r="K21" s="240"/>
-      <c r="L21" s="241"/>
+      <c r="C21" s="276"/>
+      <c r="D21" s="276"/>
+      <c r="E21" s="276"/>
+      <c r="F21" s="276"/>
+      <c r="G21" s="276"/>
+      <c r="H21" s="276"/>
+      <c r="I21" s="276"/>
+      <c r="J21" s="276"/>
+      <c r="K21" s="276"/>
+      <c r="L21" s="277"/>
       <c r="N21" s="106"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="228">
         <v>5</v>
       </c>
-      <c r="B22" s="240" t="s">
+      <c r="B22" s="276" t="s">
         <v>208</v>
       </c>
-      <c r="C22" s="240"/>
-      <c r="D22" s="240"/>
-      <c r="E22" s="240"/>
-      <c r="F22" s="240"/>
-      <c r="G22" s="240"/>
-      <c r="H22" s="240"/>
-      <c r="I22" s="240"/>
-      <c r="J22" s="240"/>
-      <c r="K22" s="240"/>
-      <c r="L22" s="241"/>
+      <c r="C22" s="276"/>
+      <c r="D22" s="276"/>
+      <c r="E22" s="276"/>
+      <c r="F22" s="276"/>
+      <c r="G22" s="276"/>
+      <c r="H22" s="276"/>
+      <c r="I22" s="276"/>
+      <c r="J22" s="276"/>
+      <c r="K22" s="276"/>
+      <c r="L22" s="277"/>
       <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="228"/>
-      <c r="B23" s="240" t="s">
+      <c r="B23" s="276" t="s">
         <v>209</v>
       </c>
-      <c r="C23" s="240"/>
-      <c r="D23" s="240"/>
-      <c r="E23" s="240"/>
-      <c r="F23" s="240"/>
-      <c r="G23" s="240"/>
-      <c r="H23" s="240"/>
-      <c r="I23" s="240"/>
-      <c r="J23" s="240"/>
-      <c r="K23" s="240"/>
-      <c r="L23" s="241"/>
+      <c r="C23" s="276"/>
+      <c r="D23" s="276"/>
+      <c r="E23" s="276"/>
+      <c r="F23" s="276"/>
+      <c r="G23" s="276"/>
+      <c r="H23" s="276"/>
+      <c r="I23" s="276"/>
+      <c r="J23" s="276"/>
+      <c r="K23" s="276"/>
+      <c r="L23" s="277"/>
       <c r="N23" s="106"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="228"/>
-      <c r="B24" s="240" t="s">
+      <c r="B24" s="276" t="s">
         <v>210</v>
       </c>
-      <c r="C24" s="240"/>
-      <c r="D24" s="240"/>
-      <c r="E24" s="240"/>
-      <c r="F24" s="240"/>
-      <c r="G24" s="240"/>
-      <c r="H24" s="240"/>
-      <c r="I24" s="240"/>
-      <c r="J24" s="240"/>
-      <c r="K24" s="240"/>
-      <c r="L24" s="241"/>
+      <c r="C24" s="276"/>
+      <c r="D24" s="276"/>
+      <c r="E24" s="276"/>
+      <c r="F24" s="276"/>
+      <c r="G24" s="276"/>
+      <c r="H24" s="276"/>
+      <c r="I24" s="276"/>
+      <c r="J24" s="276"/>
+      <c r="K24" s="276"/>
+      <c r="L24" s="277"/>
       <c r="N24" s="106"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="249" t="s">
+      <c r="A25" s="278" t="s">
         <v>216</v>
       </c>
-      <c r="B25" s="250"/>
-      <c r="C25" s="250"/>
-      <c r="D25" s="250"/>
-      <c r="E25" s="250"/>
-      <c r="F25" s="250"/>
-      <c r="G25" s="250"/>
-      <c r="H25" s="250"/>
-      <c r="I25" s="250"/>
-      <c r="J25" s="250"/>
-      <c r="K25" s="250"/>
-      <c r="L25" s="251"/>
+      <c r="B25" s="279"/>
+      <c r="C25" s="279"/>
+      <c r="D25" s="279"/>
+      <c r="E25" s="279"/>
+      <c r="F25" s="279"/>
+      <c r="G25" s="279"/>
+      <c r="H25" s="279"/>
+      <c r="I25" s="279"/>
+      <c r="J25" s="279"/>
+      <c r="K25" s="279"/>
+      <c r="L25" s="280"/>
       <c r="N25" s="106"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="228">
         <v>1</v>
       </c>
-      <c r="B26" s="240" t="s">
+      <c r="B26" s="276" t="s">
         <v>211</v>
       </c>
-      <c r="C26" s="240"/>
-      <c r="D26" s="240"/>
-      <c r="E26" s="240"/>
-      <c r="F26" s="240"/>
-      <c r="G26" s="240"/>
-      <c r="H26" s="240"/>
-      <c r="I26" s="240"/>
-      <c r="J26" s="240"/>
-      <c r="K26" s="240"/>
-      <c r="L26" s="241"/>
+      <c r="C26" s="276"/>
+      <c r="D26" s="276"/>
+      <c r="E26" s="276"/>
+      <c r="F26" s="276"/>
+      <c r="G26" s="276"/>
+      <c r="H26" s="276"/>
+      <c r="I26" s="276"/>
+      <c r="J26" s="276"/>
+      <c r="K26" s="276"/>
+      <c r="L26" s="277"/>
       <c r="N26" s="106"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="228"/>
-      <c r="B27" s="238" t="s">
+      <c r="B27" s="274" t="s">
         <v>340</v>
       </c>
-      <c r="C27" s="238"/>
-      <c r="D27" s="238"/>
-      <c r="E27" s="238"/>
-      <c r="F27" s="238"/>
-      <c r="G27" s="238"/>
-      <c r="H27" s="238"/>
-      <c r="I27" s="238"/>
-      <c r="J27" s="238"/>
-      <c r="K27" s="238"/>
-      <c r="L27" s="239"/>
+      <c r="C27" s="274"/>
+      <c r="D27" s="274"/>
+      <c r="E27" s="274"/>
+      <c r="F27" s="274"/>
+      <c r="G27" s="274"/>
+      <c r="H27" s="274"/>
+      <c r="I27" s="274"/>
+      <c r="J27" s="274"/>
+      <c r="K27" s="274"/>
+      <c r="L27" s="275"/>
       <c r="N27" s="106"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="228">
         <v>2</v>
       </c>
-      <c r="B28" s="240" t="s">
+      <c r="B28" s="276" t="s">
         <v>333</v>
       </c>
-      <c r="C28" s="240"/>
-      <c r="D28" s="240"/>
-      <c r="E28" s="240"/>
-      <c r="F28" s="240"/>
-      <c r="G28" s="240"/>
-      <c r="H28" s="240"/>
-      <c r="I28" s="240"/>
-      <c r="J28" s="240"/>
-      <c r="K28" s="240"/>
-      <c r="L28" s="241"/>
+      <c r="C28" s="276"/>
+      <c r="D28" s="276"/>
+      <c r="E28" s="276"/>
+      <c r="F28" s="276"/>
+      <c r="G28" s="276"/>
+      <c r="H28" s="276"/>
+      <c r="I28" s="276"/>
+      <c r="J28" s="276"/>
+      <c r="K28" s="276"/>
+      <c r="L28" s="277"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="228">
         <v>3</v>
       </c>
-      <c r="B29" s="240" t="s">
+      <c r="B29" s="276" t="s">
         <v>322</v>
       </c>
-      <c r="C29" s="240"/>
-      <c r="D29" s="240"/>
-      <c r="E29" s="240"/>
-      <c r="F29" s="240"/>
-      <c r="G29" s="240"/>
-      <c r="H29" s="240"/>
-      <c r="I29" s="240"/>
-      <c r="J29" s="240"/>
-      <c r="K29" s="240"/>
-      <c r="L29" s="241"/>
+      <c r="C29" s="276"/>
+      <c r="D29" s="276"/>
+      <c r="E29" s="276"/>
+      <c r="F29" s="276"/>
+      <c r="G29" s="276"/>
+      <c r="H29" s="276"/>
+      <c r="I29" s="276"/>
+      <c r="J29" s="276"/>
+      <c r="K29" s="276"/>
+      <c r="L29" s="277"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="228">
         <v>4</v>
       </c>
-      <c r="B30" s="240" t="s">
+      <c r="B30" s="276" t="s">
         <v>341</v>
       </c>
-      <c r="C30" s="240"/>
-      <c r="D30" s="240"/>
-      <c r="E30" s="240"/>
-      <c r="F30" s="240"/>
-      <c r="G30" s="240"/>
-      <c r="H30" s="240"/>
-      <c r="I30" s="240"/>
-      <c r="J30" s="240"/>
-      <c r="K30" s="240"/>
-      <c r="L30" s="241"/>
+      <c r="C30" s="276"/>
+      <c r="D30" s="276"/>
+      <c r="E30" s="276"/>
+      <c r="F30" s="276"/>
+      <c r="G30" s="276"/>
+      <c r="H30" s="276"/>
+      <c r="I30" s="276"/>
+      <c r="J30" s="276"/>
+      <c r="K30" s="276"/>
+      <c r="L30" s="277"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="228">
         <v>5</v>
       </c>
-      <c r="B31" s="238" t="s">
+      <c r="B31" s="274" t="s">
         <v>323</v>
       </c>
-      <c r="C31" s="238"/>
-      <c r="D31" s="238"/>
-      <c r="E31" s="238"/>
-      <c r="F31" s="238"/>
-      <c r="G31" s="238"/>
-      <c r="H31" s="238"/>
-      <c r="I31" s="238"/>
-      <c r="J31" s="238"/>
-      <c r="K31" s="238"/>
-      <c r="L31" s="239"/>
+      <c r="C31" s="274"/>
+      <c r="D31" s="274"/>
+      <c r="E31" s="274"/>
+      <c r="F31" s="274"/>
+      <c r="G31" s="274"/>
+      <c r="H31" s="274"/>
+      <c r="I31" s="274"/>
+      <c r="J31" s="274"/>
+      <c r="K31" s="274"/>
+      <c r="L31" s="275"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="228">
         <v>6</v>
       </c>
-      <c r="B32" s="238" t="s">
+      <c r="B32" s="274" t="s">
         <v>328</v>
       </c>
-      <c r="C32" s="238"/>
-      <c r="D32" s="238"/>
-      <c r="E32" s="238"/>
-      <c r="F32" s="238"/>
-      <c r="G32" s="238"/>
-      <c r="H32" s="238"/>
-      <c r="I32" s="238"/>
-      <c r="J32" s="238"/>
-      <c r="K32" s="238"/>
-      <c r="L32" s="239"/>
+      <c r="C32" s="274"/>
+      <c r="D32" s="274"/>
+      <c r="E32" s="274"/>
+      <c r="F32" s="274"/>
+      <c r="G32" s="274"/>
+      <c r="H32" s="274"/>
+      <c r="I32" s="274"/>
+      <c r="J32" s="274"/>
+      <c r="K32" s="274"/>
+      <c r="L32" s="275"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="228">
         <v>7</v>
       </c>
-      <c r="B33" s="240" t="s">
+      <c r="B33" s="276" t="s">
         <v>324</v>
       </c>
-      <c r="C33" s="240"/>
-      <c r="D33" s="240"/>
-      <c r="E33" s="240"/>
-      <c r="F33" s="240"/>
-      <c r="G33" s="240"/>
-      <c r="H33" s="240"/>
-      <c r="I33" s="240"/>
-      <c r="J33" s="240"/>
-      <c r="K33" s="240"/>
-      <c r="L33" s="241"/>
+      <c r="C33" s="276"/>
+      <c r="D33" s="276"/>
+      <c r="E33" s="276"/>
+      <c r="F33" s="276"/>
+      <c r="G33" s="276"/>
+      <c r="H33" s="276"/>
+      <c r="I33" s="276"/>
+      <c r="J33" s="276"/>
+      <c r="K33" s="276"/>
+      <c r="L33" s="277"/>
     </row>
     <row r="34" spans="1:12" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="228"/>
@@ -15562,56 +15562,56 @@
       <c r="L34" s="230"/>
     </row>
     <row r="35" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="249" t="s">
+      <c r="A35" s="278" t="s">
         <v>327</v>
       </c>
-      <c r="B35" s="250"/>
-      <c r="C35" s="250"/>
-      <c r="D35" s="250"/>
-      <c r="E35" s="250"/>
-      <c r="F35" s="250"/>
-      <c r="G35" s="250"/>
-      <c r="H35" s="250"/>
-      <c r="I35" s="250"/>
-      <c r="J35" s="250"/>
-      <c r="K35" s="250"/>
-      <c r="L35" s="251"/>
+      <c r="B35" s="279"/>
+      <c r="C35" s="279"/>
+      <c r="D35" s="279"/>
+      <c r="E35" s="279"/>
+      <c r="F35" s="279"/>
+      <c r="G35" s="279"/>
+      <c r="H35" s="279"/>
+      <c r="I35" s="279"/>
+      <c r="J35" s="279"/>
+      <c r="K35" s="279"/>
+      <c r="L35" s="280"/>
     </row>
     <row r="36" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="231" t="s">
         <v>325</v>
       </c>
-      <c r="B36" s="240" t="s">
+      <c r="B36" s="276" t="s">
         <v>212</v>
       </c>
-      <c r="C36" s="240"/>
-      <c r="D36" s="240"/>
-      <c r="E36" s="240"/>
-      <c r="F36" s="240"/>
-      <c r="G36" s="240"/>
-      <c r="H36" s="240"/>
-      <c r="I36" s="240"/>
-      <c r="J36" s="240"/>
-      <c r="K36" s="240"/>
-      <c r="L36" s="241"/>
+      <c r="C36" s="276"/>
+      <c r="D36" s="276"/>
+      <c r="E36" s="276"/>
+      <c r="F36" s="276"/>
+      <c r="G36" s="276"/>
+      <c r="H36" s="276"/>
+      <c r="I36" s="276"/>
+      <c r="J36" s="276"/>
+      <c r="K36" s="276"/>
+      <c r="L36" s="277"/>
     </row>
     <row r="37" spans="1:12" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="232" t="s">
         <v>326</v>
       </c>
-      <c r="B37" s="242" t="s">
+      <c r="B37" s="282" t="s">
         <v>329</v>
       </c>
-      <c r="C37" s="242"/>
-      <c r="D37" s="242"/>
-      <c r="E37" s="242"/>
-      <c r="F37" s="242"/>
-      <c r="G37" s="242"/>
-      <c r="H37" s="242"/>
-      <c r="I37" s="242"/>
-      <c r="J37" s="242"/>
-      <c r="K37" s="242"/>
-      <c r="L37" s="243"/>
+      <c r="C37" s="282"/>
+      <c r="D37" s="282"/>
+      <c r="E37" s="282"/>
+      <c r="F37" s="282"/>
+      <c r="G37" s="282"/>
+      <c r="H37" s="282"/>
+      <c r="I37" s="282"/>
+      <c r="J37" s="282"/>
+      <c r="K37" s="282"/>
+      <c r="L37" s="283"/>
     </row>
     <row r="38" spans="1:12" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="160"/>
@@ -15628,20 +15628,20 @@
       <c r="L38" s="113"/>
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="244" t="s">
+      <c r="A39" s="284" t="s">
         <v>240</v>
       </c>
-      <c r="B39" s="245"/>
-      <c r="C39" s="245"/>
-      <c r="D39" s="245"/>
-      <c r="E39" s="245"/>
-      <c r="F39" s="245"/>
-      <c r="G39" s="245"/>
-      <c r="H39" s="245"/>
-      <c r="I39" s="245"/>
-      <c r="J39" s="245"/>
-      <c r="K39" s="245"/>
-      <c r="L39" s="246"/>
+      <c r="B39" s="285"/>
+      <c r="C39" s="285"/>
+      <c r="D39" s="285"/>
+      <c r="E39" s="285"/>
+      <c r="F39" s="285"/>
+      <c r="G39" s="285"/>
+      <c r="H39" s="285"/>
+      <c r="I39" s="285"/>
+      <c r="J39" s="285"/>
+      <c r="K39" s="285"/>
+      <c r="L39" s="286"/>
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="235" t="s">
@@ -15729,72 +15729,72 @@
       <c r="B45" s="168" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="247" t="s">
+      <c r="C45" s="264" t="s">
         <v>313</v>
       </c>
-      <c r="D45" s="247"/>
-      <c r="E45" s="247"/>
-      <c r="F45" s="247"/>
-      <c r="G45" s="247"/>
-      <c r="H45" s="247"/>
-      <c r="I45" s="247"/>
-      <c r="J45" s="247"/>
-      <c r="K45" s="247"/>
-      <c r="L45" s="248"/>
+      <c r="D45" s="264"/>
+      <c r="E45" s="264"/>
+      <c r="F45" s="264"/>
+      <c r="G45" s="264"/>
+      <c r="H45" s="264"/>
+      <c r="I45" s="264"/>
+      <c r="J45" s="264"/>
+      <c r="K45" s="264"/>
+      <c r="L45" s="265"/>
     </row>
     <row r="46" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="167"/>
       <c r="B46" s="168" t="s">
         <v>138</v>
       </c>
-      <c r="C46" s="247" t="s">
+      <c r="C46" s="264" t="s">
         <v>139</v>
       </c>
-      <c r="D46" s="247"/>
-      <c r="E46" s="247"/>
-      <c r="F46" s="247"/>
-      <c r="G46" s="247"/>
-      <c r="H46" s="247"/>
-      <c r="I46" s="247"/>
-      <c r="J46" s="247"/>
-      <c r="K46" s="247"/>
-      <c r="L46" s="248"/>
+      <c r="D46" s="264"/>
+      <c r="E46" s="264"/>
+      <c r="F46" s="264"/>
+      <c r="G46" s="264"/>
+      <c r="H46" s="264"/>
+      <c r="I46" s="264"/>
+      <c r="J46" s="264"/>
+      <c r="K46" s="264"/>
+      <c r="L46" s="265"/>
     </row>
     <row r="47" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="167"/>
       <c r="B47" s="168" t="s">
         <v>238</v>
       </c>
-      <c r="C47" s="247" t="s">
+      <c r="C47" s="264" t="s">
         <v>239</v>
       </c>
-      <c r="D47" s="247"/>
-      <c r="E47" s="247"/>
-      <c r="F47" s="247"/>
-      <c r="G47" s="247"/>
-      <c r="H47" s="247"/>
-      <c r="I47" s="247"/>
-      <c r="J47" s="247"/>
-      <c r="K47" s="247"/>
-      <c r="L47" s="248"/>
+      <c r="D47" s="264"/>
+      <c r="E47" s="264"/>
+      <c r="F47" s="264"/>
+      <c r="G47" s="264"/>
+      <c r="H47" s="264"/>
+      <c r="I47" s="264"/>
+      <c r="J47" s="264"/>
+      <c r="K47" s="264"/>
+      <c r="L47" s="265"/>
     </row>
     <row r="48" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="167"/>
       <c r="B48" s="168" t="s">
         <v>314</v>
       </c>
-      <c r="C48" s="247" t="s">
+      <c r="C48" s="264" t="s">
         <v>315</v>
       </c>
-      <c r="D48" s="247"/>
-      <c r="E48" s="247"/>
-      <c r="F48" s="247"/>
-      <c r="G48" s="247"/>
-      <c r="H48" s="247"/>
-      <c r="I48" s="247"/>
-      <c r="J48" s="247"/>
-      <c r="K48" s="247"/>
-      <c r="L48" s="248"/>
+      <c r="D48" s="264"/>
+      <c r="E48" s="264"/>
+      <c r="F48" s="264"/>
+      <c r="G48" s="264"/>
+      <c r="H48" s="264"/>
+      <c r="I48" s="264"/>
+      <c r="J48" s="264"/>
+      <c r="K48" s="264"/>
+      <c r="L48" s="265"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A49" s="167"/>
@@ -15819,18 +15819,18 @@
       <c r="B50" s="168" t="s">
         <v>63</v>
       </c>
-      <c r="C50" s="247" t="s">
+      <c r="C50" s="264" t="s">
         <v>317</v>
       </c>
-      <c r="D50" s="247"/>
-      <c r="E50" s="247"/>
-      <c r="F50" s="247"/>
-      <c r="G50" s="247"/>
-      <c r="H50" s="247"/>
-      <c r="I50" s="247"/>
-      <c r="J50" s="247"/>
-      <c r="K50" s="247"/>
-      <c r="L50" s="248"/>
+      <c r="D50" s="264"/>
+      <c r="E50" s="264"/>
+      <c r="F50" s="264"/>
+      <c r="G50" s="264"/>
+      <c r="H50" s="264"/>
+      <c r="I50" s="264"/>
+      <c r="J50" s="264"/>
+      <c r="K50" s="264"/>
+      <c r="L50" s="265"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A51" s="167"/>
@@ -15912,25 +15912,51 @@
       </c>
     </row>
     <row r="64" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="237" t="s">
+      <c r="A64" s="281" t="s">
         <v>356</v>
       </c>
-      <c r="B64" s="237"/>
-      <c r="C64" s="237"/>
-      <c r="D64" s="237"/>
-      <c r="E64" s="237"/>
-      <c r="F64" s="237"/>
-      <c r="G64" s="237"/>
-      <c r="H64" s="237"/>
-      <c r="I64" s="237"/>
-      <c r="J64" s="237"/>
-      <c r="K64" s="237"/>
-      <c r="L64" s="237"/>
+      <c r="B64" s="281"/>
+      <c r="C64" s="281"/>
+      <c r="D64" s="281"/>
+      <c r="E64" s="281"/>
+      <c r="F64" s="281"/>
+      <c r="G64" s="281"/>
+      <c r="H64" s="281"/>
+      <c r="I64" s="281"/>
+      <c r="J64" s="281"/>
+      <c r="K64" s="281"/>
+      <c r="L64" s="281"/>
     </row>
     <row r="69" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="70" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A64:L64"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="C45:L45"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="C48:L48"/>
+    <mergeCell ref="C50:L50"/>
+    <mergeCell ref="A35:L35"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B18:L18"/>
+    <mergeCell ref="B19:L19"/>
+    <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="B22:L22"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="B26:L26"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B30:L30"/>
     <mergeCell ref="A17:L17"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A4:L4"/>
@@ -15945,32 +15971,6 @@
     <mergeCell ref="A16:L16"/>
     <mergeCell ref="B7:L7"/>
     <mergeCell ref="B8:L8"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B18:L18"/>
-    <mergeCell ref="B19:L19"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="B22:L22"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="B24:L24"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="B26:L26"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="A64:L64"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="C45:L45"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="C47:L47"/>
-    <mergeCell ref="C48:L48"/>
-    <mergeCell ref="C50:L50"/>
-    <mergeCell ref="A35:L35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A57" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -30938,82 +30938,82 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="315" t="s">
+      <c r="A3" s="324" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="315"/>
-      <c r="C3" s="315"/>
+      <c r="B3" s="324"/>
+      <c r="C3" s="324"/>
       <c r="D3" s="128" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="316" t="s">
+      <c r="A4" s="325" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="316"/>
-      <c r="C4" s="316"/>
+      <c r="B4" s="325"/>
+      <c r="C4" s="325"/>
       <c r="D4" s="175" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="320" t="s">
+      <c r="A5" s="329" t="s">
         <v>223</v>
       </c>
-      <c r="B5" s="317"/>
-      <c r="C5" s="317"/>
+      <c r="B5" s="326"/>
+      <c r="C5" s="326"/>
       <c r="D5" s="176" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="318" t="s">
+      <c r="A6" s="327" t="s">
         <v>224</v>
       </c>
-      <c r="B6" s="318"/>
-      <c r="C6" s="318"/>
+      <c r="B6" s="327"/>
+      <c r="C6" s="327"/>
       <c r="D6" s="177" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="319" t="s">
+      <c r="A7" s="328" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="319"/>
-      <c r="C7" s="319"/>
+      <c r="B7" s="328"/>
+      <c r="C7" s="328"/>
       <c r="D7" s="178" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="316" t="s">
+      <c r="A11" s="325" t="s">
         <v>152</v>
       </c>
-      <c r="B11" s="316"/>
-      <c r="C11" s="316"/>
+      <c r="B11" s="325"/>
+      <c r="C11" s="325"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="317" t="s">
+      <c r="A12" s="326" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="317"/>
-      <c r="C12" s="317"/>
+      <c r="B12" s="326"/>
+      <c r="C12" s="326"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="318" t="s">
+      <c r="A13" s="327" t="s">
         <v>154</v>
       </c>
-      <c r="B13" s="318"/>
-      <c r="C13" s="318"/>
+      <c r="B13" s="327"/>
+      <c r="C13" s="327"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="319" t="s">
+      <c r="A14" s="328" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="319"/>
-      <c r="C14" s="319"/>
+      <c r="B14" s="328"/>
+      <c r="C14" s="328"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -31564,8 +31564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BF7D8F-86F3-47E9-AB85-EE9B4CAB70E4}">
   <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31594,16 +31594,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="278" t="str">
+      <c r="A1" s="287" t="str">
         <f>'ReadMe-Directions'!A1</f>
         <v>Immersive Model for Lake Mead based on the Principle of Divide Reservoir Inflow</v>
       </c>
-      <c r="B1" s="278"/>
-      <c r="C1" s="278"/>
-      <c r="D1" s="278"/>
-      <c r="E1" s="278"/>
-      <c r="F1" s="278"/>
-      <c r="G1" s="278"/>
+      <c r="B1" s="287"/>
+      <c r="C1" s="287"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -31612,15 +31612,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="286" t="s">
+      <c r="A3" s="295" t="s">
         <v>230</v>
       </c>
-      <c r="B3" s="286"/>
-      <c r="C3" s="286"/>
-      <c r="D3" s="286"/>
-      <c r="E3" s="286"/>
-      <c r="F3" s="286"/>
-      <c r="G3" s="286"/>
+      <c r="B3" s="295"/>
+      <c r="C3" s="295"/>
+      <c r="D3" s="295"/>
+      <c r="E3" s="295"/>
+      <c r="F3" s="295"/>
+      <c r="G3" s="295"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -31636,13 +31636,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="287" t="s">
+      <c r="C4" s="296" t="s">
         <v>310</v>
       </c>
-      <c r="D4" s="288"/>
-      <c r="E4" s="288"/>
-      <c r="F4" s="288"/>
-      <c r="G4" s="289"/>
+      <c r="D4" s="297"/>
+      <c r="E4" s="297"/>
+      <c r="F4" s="297"/>
+      <c r="G4" s="298"/>
       <c r="N4" s="141" t="s">
         <v>168</v>
       </c>
@@ -31652,11 +31652,11 @@
         <v>283</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="290"/>
-      <c r="D5" s="285"/>
-      <c r="E5" s="285"/>
-      <c r="F5" s="285"/>
-      <c r="G5" s="285"/>
+      <c r="C5" s="299"/>
+      <c r="D5" s="294"/>
+      <c r="E5" s="294"/>
+      <c r="F5" s="294"/>
+      <c r="G5" s="294"/>
       <c r="N5" s="141"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -31664,11 +31664,11 @@
         <v>242</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="290"/>
-      <c r="D6" s="285"/>
-      <c r="E6" s="285"/>
-      <c r="F6" s="285"/>
-      <c r="G6" s="285"/>
+      <c r="C6" s="299"/>
+      <c r="D6" s="294"/>
+      <c r="E6" s="294"/>
+      <c r="F6" s="294"/>
+      <c r="G6" s="294"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -31676,11 +31676,11 @@
         <v>243</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="290"/>
-      <c r="D7" s="285"/>
-      <c r="E7" s="285"/>
-      <c r="F7" s="285"/>
-      <c r="G7" s="285"/>
+      <c r="C7" s="299"/>
+      <c r="D7" s="294"/>
+      <c r="E7" s="294"/>
+      <c r="F7" s="294"/>
+      <c r="G7" s="294"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -31688,11 +31688,11 @@
         <v>244</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="285"/>
-      <c r="D8" s="285"/>
-      <c r="E8" s="285"/>
-      <c r="F8" s="285"/>
-      <c r="G8" s="285"/>
+      <c r="C8" s="294"/>
+      <c r="D8" s="294"/>
+      <c r="E8" s="294"/>
+      <c r="F8" s="294"/>
+      <c r="G8" s="294"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -31700,11 +31700,11 @@
         <v>18</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="291"/>
-      <c r="D9" s="291"/>
-      <c r="E9" s="291"/>
-      <c r="F9" s="291"/>
-      <c r="G9" s="291"/>
+      <c r="C9" s="300"/>
+      <c r="D9" s="300"/>
+      <c r="E9" s="300"/>
+      <c r="F9" s="300"/>
+      <c r="G9" s="300"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -31712,11 +31712,11 @@
         <v>332</v>
       </c>
       <c r="B10" s="90"/>
-      <c r="C10" s="285"/>
-      <c r="D10" s="285"/>
-      <c r="E10" s="285"/>
-      <c r="F10" s="285"/>
-      <c r="G10" s="285"/>
+      <c r="C10" s="294"/>
+      <c r="D10" s="294"/>
+      <c r="E10" s="294"/>
+      <c r="F10" s="294"/>
+      <c r="G10" s="294"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -31729,28 +31729,28 @@
       <c r="A12" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="292" t="s">
+      <c r="B12" s="301" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="293"/>
-      <c r="D12" s="294"/>
+      <c r="C12" s="302"/>
+      <c r="D12" s="303"/>
       <c r="N12" s="141" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="295" t="s">
+      <c r="B13" s="304" t="s">
         <v>229</v>
       </c>
-      <c r="C13" s="296"/>
-      <c r="D13" s="297"/>
+      <c r="C13" s="305"/>
+      <c r="D13" s="306"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="279" t="s">
+      <c r="B14" s="288" t="s">
         <v>224</v>
       </c>
-      <c r="C14" s="280"/>
-      <c r="D14" s="281"/>
+      <c r="C14" s="289"/>
+      <c r="D14" s="290"/>
       <c r="F14">
         <f>4.5/7.2</f>
         <v>0.625</v>
@@ -31758,11 +31758,11 @@
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="282" t="s">
+      <c r="B15" s="291" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="283"/>
-      <c r="D15" s="284"/>
+      <c r="C15" s="292"/>
+      <c r="D15" s="293"/>
       <c r="F15">
         <f>F14*0.4</f>
         <v>0.25</v>
@@ -31886,7 +31886,8 @@
         <v>361</v>
       </c>
       <c r="B24" s="94">
-        <v>1</v>
+        <f>TribalWater!H7</f>
+        <v>0.16438105840220965</v>
       </c>
       <c r="C24"/>
       <c r="D24" s="111"/>
@@ -31899,7 +31900,7 @@
       </c>
       <c r="B25" s="236">
         <f>1-B24</f>
-        <v>0</v>
+        <v>0.83561894159779038</v>
       </c>
       <c r="C25"/>
       <c r="D25" s="111"/>
@@ -33112,7 +33113,7 @@
       </c>
       <c r="C55" s="82">
         <f>IF(OR(C$28="",$A55=""),"",(VLOOKUP(C$54,DivideInflow!$K$19:$W$25,9)-IF($A$59&lt;&gt;"",$B$59*$B$24,0))*(C$54))</f>
-        <v>3.2590132787543</v>
+        <v>4.21403850656624</v>
       </c>
       <c r="D55" s="82" t="str">
         <f>IF(OR(D$28="",$A55=""),"",(VLOOKUP(D$54,DivideInflow!$K$19:$W$25,9)-IF($A$59&lt;&gt;"",$B$59*$B$24,0))*(D$54))</f>
@@ -33137,7 +33138,7 @@
       <c r="L55" s="81"/>
       <c r="M55" s="224">
         <f>C55/C$54</f>
-        <v>0.36195555555555559</v>
+        <v>0.4680234532090351</v>
       </c>
       <c r="N55" s="143"/>
       <c r="P55" s="81"/>
@@ -33152,7 +33153,7 @@
       </c>
       <c r="C56" s="82">
         <f>IF(OR(C$28="",$A56=""),"",(VLOOKUP(C$54,DivideInflow!$K$19:$W$25,7)-IF($A$59&lt;&gt;"",$B$59*$B$25,0))*(C$54))</f>
-        <v>2.8012147533497176</v>
+        <v>1.8461895255377774</v>
       </c>
       <c r="D56" s="82" t="str">
         <f>IF(OR(D$28="",$A56=""),"",(VLOOKUP(D$54,DivideInflow!$K$19:$W$25,7)-IF($A$59&lt;&gt;"",$B$59*$B$25,0))*(D$54))</f>
@@ -33192,7 +33193,7 @@
       </c>
       <c r="M56" s="224">
         <f t="shared" ref="M56:M58" si="26">C56/C$54</f>
-        <v>0.31111111111111112</v>
+        <v>0.2050432134576316</v>
       </c>
       <c r="N56" s="143"/>
     </row>
@@ -33815,7 +33816,7 @@
       </c>
       <c r="C75" s="12">
         <f>IF(OR(C$28="",$A75=""),"",C37+C55-C47+C72)</f>
-        <v>4.8316147839961872</v>
+        <v>5.7866400118081271</v>
       </c>
       <c r="D75" s="12" t="str">
         <f>IF(OR(D$28="",$A75=""),"",D37+D55-D47+D72)</f>
@@ -33883,7 +33884,7 @@
       </c>
       <c r="C77" s="12">
         <f>IF(OR(C$28="",$A77=""),"",C75-C76)</f>
-        <v>4.8316147839961872</v>
+        <v>5.7866400118081271</v>
       </c>
       <c r="D77" s="12" t="str">
         <f t="shared" ref="D77:L77" si="50">IF(OR(D$28="",$A77=""),"",D75-D76)</f>
@@ -34058,7 +34059,7 @@
       </c>
       <c r="C83" s="12">
         <f>IF(OR(C$28="",$A83=""),"",C38+C56-C48+C80)</f>
-        <v>3.4739702709351459</v>
+        <v>2.5189450431232059</v>
       </c>
       <c r="D83" s="12" t="str">
         <f t="shared" ref="D83:L83" si="52">IF(OR(D$28="",$A83=""),"",D38+D56-D48+D80)</f>
@@ -34126,7 +34127,7 @@
       </c>
       <c r="C85" s="12">
         <f>IF(OR(C$28="",$A85=""),"",C83-C84)</f>
-        <v>3.4739702709351459</v>
+        <v>2.5189450431232059</v>
       </c>
       <c r="D85" s="12" t="str">
         <f t="shared" ref="D85:L85" si="53">IF(OR(D$28="",$A85=""),"",D83-D84)</f>
@@ -35660,7 +35661,7 @@
       </c>
       <c r="C129" s="44">
         <f t="shared" ref="C129:L129" ca="1" si="80">IF(OR(C$28="",$A129=""),"",OFFSET(C$69,8*(ROW(B129)-ROW(B$128)),0))</f>
-        <v>4.8316147839961872</v>
+        <v>5.7866400118081271</v>
       </c>
       <c r="D129" s="44" t="str">
         <f t="shared" ca="1" si="80"/>
@@ -35707,7 +35708,7 @@
       </c>
       <c r="C130" s="44">
         <f t="shared" ref="C130:L130" ca="1" si="81">IF(OR(C$28="",$A130=""),"",OFFSET(C$69,8*(ROW(B130)-ROW(B$128)),0))</f>
-        <v>3.4739702709351459</v>
+        <v>2.5189450431232059</v>
       </c>
       <c r="D130" s="44" t="str">
         <f t="shared" ca="1" si="81"/>
@@ -36567,29 +36568,29 @@
     </row>
     <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="I5" s="310" t="s">
+      <c r="I5" s="319" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="310" t="s">
+      <c r="J5" s="319" t="s">
         <v>253</v>
       </c>
-      <c r="K5" s="310" t="s">
+      <c r="K5" s="319" t="s">
         <v>254</v>
       </c>
-      <c r="L5" s="307" t="s">
+      <c r="L5" s="316" t="s">
         <v>255</v>
       </c>
-      <c r="M5" s="308"/>
-      <c r="N5" s="308"/>
-      <c r="O5" s="308"/>
-      <c r="P5" s="309"/>
-      <c r="Q5" s="299" t="s">
+      <c r="M5" s="317"/>
+      <c r="N5" s="317"/>
+      <c r="O5" s="317"/>
+      <c r="P5" s="318"/>
+      <c r="Q5" s="308" t="s">
         <v>256</v>
       </c>
-      <c r="R5" s="300"/>
-      <c r="S5" s="300"/>
-      <c r="T5" s="300"/>
-      <c r="U5" s="301"/>
+      <c r="R5" s="309"/>
+      <c r="S5" s="309"/>
+      <c r="T5" s="309"/>
+      <c r="U5" s="310"/>
     </row>
     <row r="6" spans="1:21" s="189" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="190" t="s">
@@ -36610,9 +36611,9 @@
       <c r="G6" s="190" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="311"/>
-      <c r="J6" s="311"/>
-      <c r="K6" s="311"/>
+      <c r="I6" s="320"/>
+      <c r="J6" s="320"/>
+      <c r="K6" s="320"/>
       <c r="L6" s="191" t="s">
         <v>258</v>
       </c>
@@ -36645,14 +36646,14 @@
       </c>
     </row>
     <row r="7" spans="1:21" s="189" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="307" t="s">
+      <c r="B7" s="316" t="s">
         <v>268</v>
       </c>
-      <c r="C7" s="308"/>
-      <c r="D7" s="308"/>
-      <c r="E7" s="308"/>
-      <c r="F7" s="308"/>
-      <c r="G7" s="309"/>
+      <c r="C7" s="317"/>
+      <c r="D7" s="317"/>
+      <c r="E7" s="317"/>
+      <c r="F7" s="317"/>
+      <c r="G7" s="318"/>
       <c r="I7" s="193" t="s">
         <v>269</v>
       </c>
@@ -36920,13 +36921,13 @@
       <c r="B11" s="199" t="s">
         <v>275</v>
       </c>
-      <c r="C11" s="298" t="s">
+      <c r="C11" s="307" t="s">
         <v>276</v>
       </c>
-      <c r="D11" s="298"/>
-      <c r="E11" s="298"/>
-      <c r="F11" s="298"/>
-      <c r="G11" s="298"/>
+      <c r="D11" s="307"/>
+      <c r="E11" s="307"/>
+      <c r="F11" s="307"/>
+      <c r="G11" s="307"/>
       <c r="I11" s="193" t="s">
         <v>277</v>
       </c>
@@ -36980,14 +36981,14 @@
       </c>
     </row>
     <row r="12" spans="1:21" s="198" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B12" s="302" t="s">
+      <c r="B12" s="311" t="s">
         <v>278</v>
       </c>
-      <c r="C12" s="303"/>
-      <c r="D12" s="303"/>
-      <c r="E12" s="303"/>
-      <c r="F12" s="303"/>
-      <c r="G12" s="303"/>
+      <c r="C12" s="312"/>
+      <c r="D12" s="312"/>
+      <c r="E12" s="312"/>
+      <c r="F12" s="312"/>
+      <c r="G12" s="312"/>
       <c r="I12" s="193" t="s">
         <v>279</v>
       </c>
@@ -36997,20 +36998,20 @@
       <c r="K12" s="201" t="s">
         <v>280</v>
       </c>
-      <c r="L12" s="304" t="s">
+      <c r="L12" s="313" t="s">
         <v>276</v>
       </c>
-      <c r="M12" s="305"/>
-      <c r="N12" s="305"/>
-      <c r="O12" s="305"/>
-      <c r="P12" s="306"/>
-      <c r="Q12" s="304" t="s">
+      <c r="M12" s="314"/>
+      <c r="N12" s="314"/>
+      <c r="O12" s="314"/>
+      <c r="P12" s="315"/>
+      <c r="Q12" s="313" t="s">
         <v>276</v>
       </c>
-      <c r="R12" s="305"/>
-      <c r="S12" s="305"/>
-      <c r="T12" s="305"/>
-      <c r="U12" s="306"/>
+      <c r="R12" s="314"/>
+      <c r="S12" s="314"/>
+      <c r="T12" s="314"/>
+      <c r="U12" s="315"/>
     </row>
     <row r="13" spans="1:21" s="198" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B13" s="199">
@@ -37261,13 +37262,13 @@
       <c r="B18" s="199" t="s">
         <v>275</v>
       </c>
-      <c r="C18" s="298" t="s">
+      <c r="C18" s="307" t="s">
         <v>276</v>
       </c>
-      <c r="D18" s="298"/>
-      <c r="E18" s="298"/>
-      <c r="F18" s="298"/>
-      <c r="G18" s="298"/>
+      <c r="D18" s="307"/>
+      <c r="E18" s="307"/>
+      <c r="F18" s="307"/>
+      <c r="G18" s="307"/>
     </row>
     <row r="19" spans="2:21" s="198" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="I19" s="198" t="s">
@@ -37689,7 +37690,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876BA06C-E963-43DD-B933-307F043834EF}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -37713,25 +37714,25 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="321" t="s">
+      <c r="A4" s="237" t="s">
         <v>364</v>
       </c>
-      <c r="B4" s="321" t="s">
+      <c r="B4" s="237" t="s">
         <v>365</v>
       </c>
-      <c r="C4" s="322" t="s">
+      <c r="C4" s="238" t="s">
         <v>366</v>
       </c>
-      <c r="D4" s="322" t="s">
+      <c r="D4" s="238" t="s">
         <v>367</v>
       </c>
-      <c r="F4" s="322" t="s">
+      <c r="F4" s="238" t="s">
         <v>365</v>
       </c>
-      <c r="G4" s="322" t="s">
+      <c r="G4" s="238" t="s">
         <v>374</v>
       </c>
-      <c r="H4" s="322" t="s">
+      <c r="H4" s="238" t="s">
         <v>375</v>
       </c>
     </row>
@@ -37753,7 +37754,7 @@
         <f>SUMIFS($C$5:$C$13,$B$5:$B$13,F5)</f>
         <v>12534</v>
       </c>
-      <c r="H5" s="325">
+      <c r="H5" s="241">
         <f>G5/G$8</f>
         <v>1.3163339249519528E-2</v>
       </c>
@@ -37776,7 +37777,7 @@
         <f t="shared" ref="G6:G7" si="0">SUMIFS($C$5:$C$13,$B$5:$B$13,F6)</f>
         <v>783134</v>
       </c>
-      <c r="H6" s="325">
+      <c r="H6" s="241">
         <f t="shared" ref="H6:H8" si="1">G6/G$8</f>
         <v>0.82245560234827086</v>
       </c>
@@ -37799,7 +37800,7 @@
         <f t="shared" si="0"/>
         <v>156522</v>
       </c>
-      <c r="H7" s="325">
+      <c r="H7" s="241">
         <f t="shared" si="1"/>
         <v>0.16438105840220965</v>
       </c>
@@ -37815,14 +37816,14 @@
         <v>11340</v>
       </c>
       <c r="D8" s="24"/>
-      <c r="F8" s="328" t="s">
+      <c r="F8" s="244" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="326">
+      <c r="G8" s="242">
         <f>SUM(G5:G7)</f>
         <v>952190</v>
       </c>
-      <c r="H8" s="327">
+      <c r="H8" s="243">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -37890,15 +37891,15 @@
       </c>
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="323" t="s">
+      <c r="A14" s="239" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="323"/>
-      <c r="C14" s="324">
+      <c r="B14" s="239"/>
+      <c r="C14" s="240">
         <f>SUM(C5:C13)</f>
         <v>952190</v>
       </c>
-      <c r="D14" s="324">
+      <c r="D14" s="240">
         <f>SUM(D5:D13)</f>
         <v>22928</v>
       </c>
@@ -37909,13 +37910,13 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="321" t="s">
+      <c r="A18" s="237" t="s">
         <v>377</v>
       </c>
-      <c r="B18" s="329" t="s">
+      <c r="B18" s="245" t="s">
         <v>378</v>
       </c>
-      <c r="C18" s="329" t="s">
+      <c r="C18" s="245" t="s">
         <v>379</v>
       </c>
     </row>
@@ -37964,14 +37965,14 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="323" t="s">
+      <c r="A23" s="239" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="324">
+      <c r="B23" s="240">
         <f>SUM(B19:B22)</f>
         <v>800392</v>
       </c>
-      <c r="C23" s="324">
+      <c r="C23" s="240">
         <f>SUM(C19:C22)</f>
         <v>465096</v>
       </c>
@@ -38015,16 +38016,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="313" t="e">
+      <c r="A1" s="321" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="313"/>
-      <c r="C1" s="313"/>
-      <c r="D1" s="313"/>
-      <c r="E1" s="313"/>
-      <c r="F1" s="313"/>
-      <c r="G1" s="313"/>
+      <c r="B1" s="321"/>
+      <c r="C1" s="321"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -38033,15 +38034,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="286" t="s">
+      <c r="A3" s="295" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="286"/>
-      <c r="C3" s="286"/>
-      <c r="D3" s="286"/>
-      <c r="E3" s="286"/>
-      <c r="F3" s="286"/>
-      <c r="G3" s="286"/>
+      <c r="B3" s="295"/>
+      <c r="C3" s="295"/>
+      <c r="D3" s="295"/>
+      <c r="E3" s="295"/>
+      <c r="F3" s="295"/>
+      <c r="G3" s="295"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -38057,13 +38058,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="287" t="s">
+      <c r="C4" s="296" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="288"/>
-      <c r="E4" s="288"/>
-      <c r="F4" s="288"/>
-      <c r="G4" s="289"/>
+      <c r="D4" s="297"/>
+      <c r="E4" s="297"/>
+      <c r="F4" s="297"/>
+      <c r="G4" s="298"/>
       <c r="N4" s="139" t="s">
         <v>168</v>
       </c>
@@ -38073,11 +38074,11 @@
         <v>16</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="290"/>
-      <c r="D5" s="285"/>
-      <c r="E5" s="285"/>
-      <c r="F5" s="285"/>
-      <c r="G5" s="285"/>
+      <c r="C5" s="299"/>
+      <c r="D5" s="294"/>
+      <c r="E5" s="294"/>
+      <c r="F5" s="294"/>
+      <c r="G5" s="294"/>
       <c r="N5" s="142"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -38085,11 +38086,11 @@
         <v>17</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="290"/>
-      <c r="D6" s="285"/>
-      <c r="E6" s="285"/>
-      <c r="F6" s="285"/>
-      <c r="G6" s="285"/>
+      <c r="C6" s="299"/>
+      <c r="D6" s="294"/>
+      <c r="E6" s="294"/>
+      <c r="F6" s="294"/>
+      <c r="G6" s="294"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -38097,11 +38098,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="290"/>
-      <c r="D7" s="285"/>
-      <c r="E7" s="285"/>
-      <c r="F7" s="285"/>
-      <c r="G7" s="285"/>
+      <c r="C7" s="299"/>
+      <c r="D7" s="294"/>
+      <c r="E7" s="294"/>
+      <c r="F7" s="294"/>
+      <c r="G7" s="294"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -38109,11 +38110,11 @@
         <v>78</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="285"/>
-      <c r="D8" s="285"/>
-      <c r="E8" s="285"/>
-      <c r="F8" s="285"/>
-      <c r="G8" s="285"/>
+      <c r="C8" s="294"/>
+      <c r="D8" s="294"/>
+      <c r="E8" s="294"/>
+      <c r="F8" s="294"/>
+      <c r="G8" s="294"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -38121,11 +38122,11 @@
         <v>202</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="291"/>
-      <c r="D9" s="291"/>
-      <c r="E9" s="291"/>
-      <c r="F9" s="291"/>
-      <c r="G9" s="291"/>
+      <c r="C9" s="300"/>
+      <c r="D9" s="300"/>
+      <c r="E9" s="300"/>
+      <c r="F9" s="300"/>
+      <c r="G9" s="300"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -38133,11 +38134,11 @@
         <v>80</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="312"/>
-      <c r="D10" s="312"/>
-      <c r="E10" s="312"/>
-      <c r="F10" s="312"/>
-      <c r="G10" s="312"/>
+      <c r="C10" s="322"/>
+      <c r="D10" s="322"/>
+      <c r="E10" s="322"/>
+      <c r="F10" s="322"/>
+      <c r="G10" s="322"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -38150,37 +38151,37 @@
       <c r="A12" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="292" t="s">
+      <c r="B12" s="301" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="293"/>
-      <c r="D12" s="294"/>
+      <c r="C12" s="302"/>
+      <c r="D12" s="303"/>
       <c r="N12" s="141" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="295" t="s">
+      <c r="B13" s="304" t="s">
         <v>153</v>
       </c>
-      <c r="C13" s="296"/>
-      <c r="D13" s="297"/>
+      <c r="C13" s="305"/>
+      <c r="D13" s="306"/>
       <c r="N13" s="142"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="279" t="s">
+      <c r="B14" s="288" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="280"/>
-      <c r="D14" s="281"/>
+      <c r="C14" s="289"/>
+      <c r="D14" s="290"/>
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="282" t="s">
+      <c r="B15" s="291" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="283"/>
-      <c r="D15" s="284"/>
+      <c r="C15" s="292"/>
+      <c r="D15" s="293"/>
       <c r="N15" s="142"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -39012,7 +39013,7 @@
       </c>
       <c r="M41" s="28">
         <f>Master!C55</f>
-        <v>3.2590132787543</v>
+        <v>4.21403850656624</v>
       </c>
       <c r="N41" s="143"/>
       <c r="P41" s="81"/>
@@ -39067,7 +39068,7 @@
       </c>
       <c r="M42" s="28">
         <f>Master!C56</f>
-        <v>2.8012147533497176</v>
+        <v>1.8461895255377774</v>
       </c>
       <c r="N42" s="143"/>
     </row>
@@ -39400,12 +39401,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -39413,6 +39408,12 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>
@@ -39470,26 +39471,26 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="314" t="s">
+      <c r="D3" s="323" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="314"/>
-      <c r="F3" s="314" t="s">
+      <c r="E3" s="323"/>
+      <c r="F3" s="323" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="314"/>
-      <c r="H3" s="314"/>
-      <c r="I3" s="314" t="s">
+      <c r="G3" s="323"/>
+      <c r="H3" s="323"/>
+      <c r="I3" s="323" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="314"/>
-      <c r="K3" s="314"/>
+      <c r="J3" s="323"/>
+      <c r="K3" s="323"/>
       <c r="L3" s="134"/>
-      <c r="M3" s="314" t="s">
+      <c r="M3" s="323" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="314"/>
-      <c r="O3" s="314"/>
+      <c r="N3" s="323"/>
+      <c r="O3" s="323"/>
     </row>
     <row r="4" spans="1:16" s="47" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="46" t="s">

</xml_diff>

<commit_message>
Update Model guide with support data for Tribal Nations
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED68F8B-3672-43F7-B694-1312C6BE9DDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CEAE45-3945-4718-988A-B58FB66351D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="62" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="388">
   <si>
     <t>Year 1</t>
   </si>
@@ -2002,6 +2002,18 @@
   <si>
     <t>Transfers, Leases, Exchanges</t>
   </si>
+  <si>
+    <t>TribalWater</t>
+  </si>
+  <si>
+    <t>Shows settled water rights and current consumptive uses of Tribal Nations of the Lower Basin.</t>
+  </si>
+  <si>
+    <t>Help assign parties and specify strategies</t>
+  </si>
+  <si>
+    <t>Help percent of Tribal Nation water in CA</t>
+  </si>
 </sst>
 </file>
 
@@ -3299,6 +3311,51 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3353,12 +3410,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3382,45 +3433,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3524,11 +3536,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14946,9 +14958,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EA02F4-5F19-409C-8BC6-A0D8FEB3A90D}">
-  <dimension ref="A1:R70"/>
+  <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
@@ -14968,20 +14980,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="249" t="s">
+      <c r="A1" s="264" t="s">
         <v>351</v>
       </c>
-      <c r="B1" s="249"/>
-      <c r="C1" s="249"/>
-      <c r="D1" s="249"/>
-      <c r="E1" s="249"/>
-      <c r="F1" s="249"/>
-      <c r="G1" s="249"/>
-      <c r="H1" s="249"/>
-      <c r="I1" s="249"/>
-      <c r="J1" s="249"/>
-      <c r="K1" s="249"/>
-      <c r="L1" s="249"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="264"/>
+      <c r="J1" s="264"/>
+      <c r="K1" s="264"/>
+      <c r="L1" s="264"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -15007,41 +15019,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="250" t="s">
+      <c r="A4" s="265" t="s">
         <v>352</v>
       </c>
-      <c r="B4" s="251"/>
-      <c r="C4" s="251"/>
-      <c r="D4" s="251"/>
-      <c r="E4" s="251"/>
-      <c r="F4" s="251"/>
-      <c r="G4" s="251"/>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="252"/>
-      <c r="N4" s="253"/>
-      <c r="O4" s="253"/>
-      <c r="P4" s="253"/>
-      <c r="Q4" s="253"/>
-      <c r="R4" s="253"/>
+      <c r="B4" s="266"/>
+      <c r="C4" s="266"/>
+      <c r="D4" s="266"/>
+      <c r="E4" s="266"/>
+      <c r="F4" s="266"/>
+      <c r="G4" s="266"/>
+      <c r="H4" s="266"/>
+      <c r="I4" s="266"/>
+      <c r="J4" s="266"/>
+      <c r="K4" s="266"/>
+      <c r="L4" s="267"/>
+      <c r="N4" s="268"/>
+      <c r="O4" s="268"/>
+      <c r="P4" s="268"/>
+      <c r="Q4" s="268"/>
+      <c r="R4" s="268"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="254" t="s">
+      <c r="A5" s="269" t="s">
         <v>335</v>
       </c>
-      <c r="B5" s="255"/>
-      <c r="C5" s="255"/>
-      <c r="D5" s="255"/>
-      <c r="E5" s="255"/>
-      <c r="F5" s="255"/>
-      <c r="G5" s="255"/>
-      <c r="H5" s="255"/>
-      <c r="I5" s="255"/>
-      <c r="J5" s="255"/>
-      <c r="K5" s="255"/>
-      <c r="L5" s="256"/>
+      <c r="B5" s="270"/>
+      <c r="C5" s="270"/>
+      <c r="D5" s="270"/>
+      <c r="E5" s="270"/>
+      <c r="F5" s="270"/>
+      <c r="G5" s="270"/>
+      <c r="H5" s="270"/>
+      <c r="I5" s="270"/>
+      <c r="J5" s="270"/>
+      <c r="K5" s="270"/>
+      <c r="L5" s="271"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15049,20 +15061,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="254" t="s">
+      <c r="A6" s="269" t="s">
         <v>353</v>
       </c>
-      <c r="B6" s="255"/>
-      <c r="C6" s="255"/>
-      <c r="D6" s="255"/>
-      <c r="E6" s="255"/>
-      <c r="F6" s="255"/>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="255"/>
-      <c r="J6" s="255"/>
-      <c r="K6" s="255"/>
-      <c r="L6" s="256"/>
+      <c r="B6" s="270"/>
+      <c r="C6" s="270"/>
+      <c r="D6" s="270"/>
+      <c r="E6" s="270"/>
+      <c r="F6" s="270"/>
+      <c r="G6" s="270"/>
+      <c r="H6" s="270"/>
+      <c r="I6" s="270"/>
+      <c r="J6" s="270"/>
+      <c r="K6" s="270"/>
+      <c r="L6" s="271"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15071,19 +15083,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="233"/>
-      <c r="B7" s="255" t="s">
+      <c r="B7" s="270" t="s">
         <v>354</v>
       </c>
-      <c r="C7" s="255"/>
-      <c r="D7" s="255"/>
-      <c r="E7" s="255"/>
-      <c r="F7" s="255"/>
-      <c r="G7" s="255"/>
-      <c r="H7" s="255"/>
-      <c r="I7" s="255"/>
-      <c r="J7" s="255"/>
-      <c r="K7" s="255"/>
-      <c r="L7" s="256"/>
+      <c r="C7" s="270"/>
+      <c r="D7" s="270"/>
+      <c r="E7" s="270"/>
+      <c r="F7" s="270"/>
+      <c r="G7" s="270"/>
+      <c r="H7" s="270"/>
+      <c r="I7" s="270"/>
+      <c r="J7" s="270"/>
+      <c r="K7" s="270"/>
+      <c r="L7" s="271"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15092,19 +15104,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="234"/>
-      <c r="B8" s="272" t="s">
+      <c r="B8" s="285" t="s">
         <v>355</v>
       </c>
-      <c r="C8" s="272"/>
-      <c r="D8" s="272"/>
-      <c r="E8" s="272"/>
-      <c r="F8" s="272"/>
-      <c r="G8" s="272"/>
-      <c r="H8" s="272"/>
-      <c r="I8" s="272"/>
-      <c r="J8" s="272"/>
-      <c r="K8" s="272"/>
-      <c r="L8" s="273"/>
+      <c r="C8" s="285"/>
+      <c r="D8" s="285"/>
+      <c r="E8" s="285"/>
+      <c r="F8" s="285"/>
+      <c r="G8" s="285"/>
+      <c r="H8" s="285"/>
+      <c r="I8" s="285"/>
+      <c r="J8" s="285"/>
+      <c r="K8" s="285"/>
+      <c r="L8" s="286"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15126,84 +15138,84 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="257" t="s">
+      <c r="A10" s="272" t="s">
         <v>205</v>
       </c>
-      <c r="B10" s="258"/>
-      <c r="C10" s="258"/>
-      <c r="D10" s="258"/>
-      <c r="E10" s="258"/>
-      <c r="F10" s="258"/>
-      <c r="G10" s="258"/>
-      <c r="H10" s="258"/>
-      <c r="I10" s="258"/>
-      <c r="J10" s="258"/>
-      <c r="K10" s="258"/>
-      <c r="L10" s="259"/>
+      <c r="B10" s="273"/>
+      <c r="C10" s="273"/>
+      <c r="D10" s="273"/>
+      <c r="E10" s="273"/>
+      <c r="F10" s="273"/>
+      <c r="G10" s="273"/>
+      <c r="H10" s="273"/>
+      <c r="I10" s="273"/>
+      <c r="J10" s="273"/>
+      <c r="K10" s="273"/>
+      <c r="L10" s="274"/>
     </row>
     <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="260" t="s">
+      <c r="A11" s="275" t="s">
         <v>336</v>
       </c>
-      <c r="B11" s="261"/>
-      <c r="C11" s="261"/>
-      <c r="D11" s="261"/>
-      <c r="E11" s="261"/>
-      <c r="F11" s="261"/>
-      <c r="G11" s="261"/>
-      <c r="H11" s="261"/>
-      <c r="I11" s="261"/>
-      <c r="J11" s="261"/>
-      <c r="K11" s="261"/>
-      <c r="L11" s="262"/>
+      <c r="B11" s="276"/>
+      <c r="C11" s="276"/>
+      <c r="D11" s="276"/>
+      <c r="E11" s="276"/>
+      <c r="F11" s="276"/>
+      <c r="G11" s="276"/>
+      <c r="H11" s="276"/>
+      <c r="I11" s="276"/>
+      <c r="J11" s="276"/>
+      <c r="K11" s="276"/>
+      <c r="L11" s="277"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="263" t="s">
+      <c r="A12" s="278" t="s">
         <v>337</v>
       </c>
-      <c r="B12" s="264"/>
-      <c r="C12" s="264"/>
-      <c r="D12" s="264"/>
-      <c r="E12" s="264"/>
-      <c r="F12" s="264"/>
-      <c r="G12" s="264"/>
-      <c r="H12" s="264"/>
-      <c r="I12" s="264"/>
-      <c r="J12" s="264"/>
-      <c r="K12" s="264"/>
-      <c r="L12" s="265"/>
+      <c r="B12" s="256"/>
+      <c r="C12" s="256"/>
+      <c r="D12" s="256"/>
+      <c r="E12" s="256"/>
+      <c r="F12" s="256"/>
+      <c r="G12" s="256"/>
+      <c r="H12" s="256"/>
+      <c r="I12" s="256"/>
+      <c r="J12" s="256"/>
+      <c r="K12" s="256"/>
+      <c r="L12" s="257"/>
     </row>
     <row r="13" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="263" t="s">
+      <c r="A13" s="278" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="264"/>
-      <c r="C13" s="264"/>
-      <c r="D13" s="264"/>
-      <c r="E13" s="264"/>
-      <c r="F13" s="264"/>
-      <c r="G13" s="264"/>
-      <c r="H13" s="264"/>
-      <c r="I13" s="264"/>
-      <c r="J13" s="264"/>
-      <c r="K13" s="264"/>
-      <c r="L13" s="265"/>
+      <c r="B13" s="256"/>
+      <c r="C13" s="256"/>
+      <c r="D13" s="256"/>
+      <c r="E13" s="256"/>
+      <c r="F13" s="256"/>
+      <c r="G13" s="256"/>
+      <c r="H13" s="256"/>
+      <c r="I13" s="256"/>
+      <c r="J13" s="256"/>
+      <c r="K13" s="256"/>
+      <c r="L13" s="257"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="266" t="s">
+      <c r="A14" s="279" t="s">
         <v>338</v>
       </c>
-      <c r="B14" s="267"/>
-      <c r="C14" s="267"/>
-      <c r="D14" s="267"/>
-      <c r="E14" s="267"/>
-      <c r="F14" s="267"/>
-      <c r="G14" s="267"/>
-      <c r="H14" s="267"/>
-      <c r="I14" s="267"/>
-      <c r="J14" s="267"/>
-      <c r="K14" s="267"/>
-      <c r="L14" s="268"/>
+      <c r="B14" s="280"/>
+      <c r="C14" s="280"/>
+      <c r="D14" s="280"/>
+      <c r="E14" s="280"/>
+      <c r="F14" s="280"/>
+      <c r="G14" s="280"/>
+      <c r="H14" s="280"/>
+      <c r="I14" s="280"/>
+      <c r="J14" s="280"/>
+      <c r="K14" s="280"/>
+      <c r="L14" s="281"/>
     </row>
     <row r="15" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="113"/>
@@ -15220,332 +15232,332 @@
       <c r="L15" s="113"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="269" t="s">
+      <c r="A16" s="282" t="s">
         <v>334</v>
       </c>
-      <c r="B16" s="270"/>
-      <c r="C16" s="270"/>
-      <c r="D16" s="270"/>
-      <c r="E16" s="270"/>
-      <c r="F16" s="270"/>
-      <c r="G16" s="270"/>
-      <c r="H16" s="270"/>
-      <c r="I16" s="270"/>
-      <c r="J16" s="270"/>
-      <c r="K16" s="270"/>
-      <c r="L16" s="271"/>
+      <c r="B16" s="283"/>
+      <c r="C16" s="283"/>
+      <c r="D16" s="283"/>
+      <c r="E16" s="283"/>
+      <c r="F16" s="283"/>
+      <c r="G16" s="283"/>
+      <c r="H16" s="283"/>
+      <c r="I16" s="283"/>
+      <c r="J16" s="283"/>
+      <c r="K16" s="283"/>
+      <c r="L16" s="284"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="246" t="s">
+      <c r="A17" s="261" t="s">
         <v>215</v>
       </c>
-      <c r="B17" s="247"/>
-      <c r="C17" s="247"/>
-      <c r="D17" s="247"/>
-      <c r="E17" s="247"/>
-      <c r="F17" s="247"/>
-      <c r="G17" s="247"/>
-      <c r="H17" s="247"/>
-      <c r="I17" s="247"/>
-      <c r="J17" s="247"/>
-      <c r="K17" s="247"/>
-      <c r="L17" s="248"/>
+      <c r="B17" s="262"/>
+      <c r="C17" s="262"/>
+      <c r="D17" s="262"/>
+      <c r="E17" s="262"/>
+      <c r="F17" s="262"/>
+      <c r="G17" s="262"/>
+      <c r="H17" s="262"/>
+      <c r="I17" s="262"/>
+      <c r="J17" s="262"/>
+      <c r="K17" s="262"/>
+      <c r="L17" s="263"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="228">
         <v>1</v>
       </c>
-      <c r="B18" s="276" t="s">
+      <c r="B18" s="249" t="s">
         <v>214</v>
       </c>
-      <c r="C18" s="276"/>
-      <c r="D18" s="276"/>
-      <c r="E18" s="276"/>
-      <c r="F18" s="276"/>
-      <c r="G18" s="276"/>
-      <c r="H18" s="276"/>
-      <c r="I18" s="276"/>
-      <c r="J18" s="276"/>
-      <c r="K18" s="276"/>
-      <c r="L18" s="277"/>
+      <c r="C18" s="249"/>
+      <c r="D18" s="249"/>
+      <c r="E18" s="249"/>
+      <c r="F18" s="249"/>
+      <c r="G18" s="249"/>
+      <c r="H18" s="249"/>
+      <c r="I18" s="249"/>
+      <c r="J18" s="249"/>
+      <c r="K18" s="249"/>
+      <c r="L18" s="250"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="228">
         <v>2</v>
       </c>
-      <c r="B19" s="276" t="s">
+      <c r="B19" s="249" t="s">
         <v>330</v>
       </c>
-      <c r="C19" s="276"/>
-      <c r="D19" s="276"/>
-      <c r="E19" s="276"/>
-      <c r="F19" s="276"/>
-      <c r="G19" s="276"/>
-      <c r="H19" s="276"/>
-      <c r="I19" s="276"/>
-      <c r="J19" s="276"/>
-      <c r="K19" s="276"/>
-      <c r="L19" s="277"/>
+      <c r="C19" s="249"/>
+      <c r="D19" s="249"/>
+      <c r="E19" s="249"/>
+      <c r="F19" s="249"/>
+      <c r="G19" s="249"/>
+      <c r="H19" s="249"/>
+      <c r="I19" s="249"/>
+      <c r="J19" s="249"/>
+      <c r="K19" s="249"/>
+      <c r="L19" s="250"/>
       <c r="N19" s="106"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="228">
         <v>3</v>
       </c>
-      <c r="B20" s="276" t="s">
+      <c r="B20" s="249" t="s">
         <v>207</v>
       </c>
-      <c r="C20" s="276"/>
-      <c r="D20" s="276"/>
-      <c r="E20" s="276"/>
-      <c r="F20" s="276"/>
-      <c r="G20" s="276"/>
-      <c r="H20" s="276"/>
-      <c r="I20" s="276"/>
-      <c r="J20" s="276"/>
-      <c r="K20" s="276"/>
-      <c r="L20" s="277"/>
+      <c r="C20" s="249"/>
+      <c r="D20" s="249"/>
+      <c r="E20" s="249"/>
+      <c r="F20" s="249"/>
+      <c r="G20" s="249"/>
+      <c r="H20" s="249"/>
+      <c r="I20" s="249"/>
+      <c r="J20" s="249"/>
+      <c r="K20" s="249"/>
+      <c r="L20" s="250"/>
       <c r="N20" s="106"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="228">
         <v>4</v>
       </c>
-      <c r="B21" s="276" t="s">
+      <c r="B21" s="249" t="s">
         <v>339</v>
       </c>
-      <c r="C21" s="276"/>
-      <c r="D21" s="276"/>
-      <c r="E21" s="276"/>
-      <c r="F21" s="276"/>
-      <c r="G21" s="276"/>
-      <c r="H21" s="276"/>
-      <c r="I21" s="276"/>
-      <c r="J21" s="276"/>
-      <c r="K21" s="276"/>
-      <c r="L21" s="277"/>
+      <c r="C21" s="249"/>
+      <c r="D21" s="249"/>
+      <c r="E21" s="249"/>
+      <c r="F21" s="249"/>
+      <c r="G21" s="249"/>
+      <c r="H21" s="249"/>
+      <c r="I21" s="249"/>
+      <c r="J21" s="249"/>
+      <c r="K21" s="249"/>
+      <c r="L21" s="250"/>
       <c r="N21" s="106"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="228">
         <v>5</v>
       </c>
-      <c r="B22" s="276" t="s">
+      <c r="B22" s="249" t="s">
         <v>208</v>
       </c>
-      <c r="C22" s="276"/>
-      <c r="D22" s="276"/>
-      <c r="E22" s="276"/>
-      <c r="F22" s="276"/>
-      <c r="G22" s="276"/>
-      <c r="H22" s="276"/>
-      <c r="I22" s="276"/>
-      <c r="J22" s="276"/>
-      <c r="K22" s="276"/>
-      <c r="L22" s="277"/>
+      <c r="C22" s="249"/>
+      <c r="D22" s="249"/>
+      <c r="E22" s="249"/>
+      <c r="F22" s="249"/>
+      <c r="G22" s="249"/>
+      <c r="H22" s="249"/>
+      <c r="I22" s="249"/>
+      <c r="J22" s="249"/>
+      <c r="K22" s="249"/>
+      <c r="L22" s="250"/>
       <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="228"/>
-      <c r="B23" s="276" t="s">
+      <c r="B23" s="249" t="s">
         <v>209</v>
       </c>
-      <c r="C23" s="276"/>
-      <c r="D23" s="276"/>
-      <c r="E23" s="276"/>
-      <c r="F23" s="276"/>
-      <c r="G23" s="276"/>
-      <c r="H23" s="276"/>
-      <c r="I23" s="276"/>
-      <c r="J23" s="276"/>
-      <c r="K23" s="276"/>
-      <c r="L23" s="277"/>
+      <c r="C23" s="249"/>
+      <c r="D23" s="249"/>
+      <c r="E23" s="249"/>
+      <c r="F23" s="249"/>
+      <c r="G23" s="249"/>
+      <c r="H23" s="249"/>
+      <c r="I23" s="249"/>
+      <c r="J23" s="249"/>
+      <c r="K23" s="249"/>
+      <c r="L23" s="250"/>
       <c r="N23" s="106"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="228"/>
-      <c r="B24" s="276" t="s">
+      <c r="B24" s="249" t="s">
         <v>210</v>
       </c>
-      <c r="C24" s="276"/>
-      <c r="D24" s="276"/>
-      <c r="E24" s="276"/>
-      <c r="F24" s="276"/>
-      <c r="G24" s="276"/>
-      <c r="H24" s="276"/>
-      <c r="I24" s="276"/>
-      <c r="J24" s="276"/>
-      <c r="K24" s="276"/>
-      <c r="L24" s="277"/>
+      <c r="C24" s="249"/>
+      <c r="D24" s="249"/>
+      <c r="E24" s="249"/>
+      <c r="F24" s="249"/>
+      <c r="G24" s="249"/>
+      <c r="H24" s="249"/>
+      <c r="I24" s="249"/>
+      <c r="J24" s="249"/>
+      <c r="K24" s="249"/>
+      <c r="L24" s="250"/>
       <c r="N24" s="106"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="278" t="s">
+      <c r="A25" s="258" t="s">
         <v>216</v>
       </c>
-      <c r="B25" s="279"/>
-      <c r="C25" s="279"/>
-      <c r="D25" s="279"/>
-      <c r="E25" s="279"/>
-      <c r="F25" s="279"/>
-      <c r="G25" s="279"/>
-      <c r="H25" s="279"/>
-      <c r="I25" s="279"/>
-      <c r="J25" s="279"/>
-      <c r="K25" s="279"/>
-      <c r="L25" s="280"/>
+      <c r="B25" s="259"/>
+      <c r="C25" s="259"/>
+      <c r="D25" s="259"/>
+      <c r="E25" s="259"/>
+      <c r="F25" s="259"/>
+      <c r="G25" s="259"/>
+      <c r="H25" s="259"/>
+      <c r="I25" s="259"/>
+      <c r="J25" s="259"/>
+      <c r="K25" s="259"/>
+      <c r="L25" s="260"/>
       <c r="N25" s="106"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="228">
         <v>1</v>
       </c>
-      <c r="B26" s="276" t="s">
+      <c r="B26" s="249" t="s">
         <v>211</v>
       </c>
-      <c r="C26" s="276"/>
-      <c r="D26" s="276"/>
-      <c r="E26" s="276"/>
-      <c r="F26" s="276"/>
-      <c r="G26" s="276"/>
-      <c r="H26" s="276"/>
-      <c r="I26" s="276"/>
-      <c r="J26" s="276"/>
-      <c r="K26" s="276"/>
-      <c r="L26" s="277"/>
+      <c r="C26" s="249"/>
+      <c r="D26" s="249"/>
+      <c r="E26" s="249"/>
+      <c r="F26" s="249"/>
+      <c r="G26" s="249"/>
+      <c r="H26" s="249"/>
+      <c r="I26" s="249"/>
+      <c r="J26" s="249"/>
+      <c r="K26" s="249"/>
+      <c r="L26" s="250"/>
       <c r="N26" s="106"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="228"/>
-      <c r="B27" s="274" t="s">
+      <c r="B27" s="247" t="s">
         <v>340</v>
       </c>
-      <c r="C27" s="274"/>
-      <c r="D27" s="274"/>
-      <c r="E27" s="274"/>
-      <c r="F27" s="274"/>
-      <c r="G27" s="274"/>
-      <c r="H27" s="274"/>
-      <c r="I27" s="274"/>
-      <c r="J27" s="274"/>
-      <c r="K27" s="274"/>
-      <c r="L27" s="275"/>
+      <c r="C27" s="247"/>
+      <c r="D27" s="247"/>
+      <c r="E27" s="247"/>
+      <c r="F27" s="247"/>
+      <c r="G27" s="247"/>
+      <c r="H27" s="247"/>
+      <c r="I27" s="247"/>
+      <c r="J27" s="247"/>
+      <c r="K27" s="247"/>
+      <c r="L27" s="248"/>
       <c r="N27" s="106"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="228">
         <v>2</v>
       </c>
-      <c r="B28" s="276" t="s">
+      <c r="B28" s="249" t="s">
         <v>333</v>
       </c>
-      <c r="C28" s="276"/>
-      <c r="D28" s="276"/>
-      <c r="E28" s="276"/>
-      <c r="F28" s="276"/>
-      <c r="G28" s="276"/>
-      <c r="H28" s="276"/>
-      <c r="I28" s="276"/>
-      <c r="J28" s="276"/>
-      <c r="K28" s="276"/>
-      <c r="L28" s="277"/>
+      <c r="C28" s="249"/>
+      <c r="D28" s="249"/>
+      <c r="E28" s="249"/>
+      <c r="F28" s="249"/>
+      <c r="G28" s="249"/>
+      <c r="H28" s="249"/>
+      <c r="I28" s="249"/>
+      <c r="J28" s="249"/>
+      <c r="K28" s="249"/>
+      <c r="L28" s="250"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="228">
         <v>3</v>
       </c>
-      <c r="B29" s="276" t="s">
+      <c r="B29" s="249" t="s">
         <v>322</v>
       </c>
-      <c r="C29" s="276"/>
-      <c r="D29" s="276"/>
-      <c r="E29" s="276"/>
-      <c r="F29" s="276"/>
-      <c r="G29" s="276"/>
-      <c r="H29" s="276"/>
-      <c r="I29" s="276"/>
-      <c r="J29" s="276"/>
-      <c r="K29" s="276"/>
-      <c r="L29" s="277"/>
+      <c r="C29" s="249"/>
+      <c r="D29" s="249"/>
+      <c r="E29" s="249"/>
+      <c r="F29" s="249"/>
+      <c r="G29" s="249"/>
+      <c r="H29" s="249"/>
+      <c r="I29" s="249"/>
+      <c r="J29" s="249"/>
+      <c r="K29" s="249"/>
+      <c r="L29" s="250"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="228">
         <v>4</v>
       </c>
-      <c r="B30" s="276" t="s">
+      <c r="B30" s="249" t="s">
         <v>341</v>
       </c>
-      <c r="C30" s="276"/>
-      <c r="D30" s="276"/>
-      <c r="E30" s="276"/>
-      <c r="F30" s="276"/>
-      <c r="G30" s="276"/>
-      <c r="H30" s="276"/>
-      <c r="I30" s="276"/>
-      <c r="J30" s="276"/>
-      <c r="K30" s="276"/>
-      <c r="L30" s="277"/>
+      <c r="C30" s="249"/>
+      <c r="D30" s="249"/>
+      <c r="E30" s="249"/>
+      <c r="F30" s="249"/>
+      <c r="G30" s="249"/>
+      <c r="H30" s="249"/>
+      <c r="I30" s="249"/>
+      <c r="J30" s="249"/>
+      <c r="K30" s="249"/>
+      <c r="L30" s="250"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="228">
         <v>5</v>
       </c>
-      <c r="B31" s="274" t="s">
+      <c r="B31" s="247" t="s">
         <v>323</v>
       </c>
-      <c r="C31" s="274"/>
-      <c r="D31" s="274"/>
-      <c r="E31" s="274"/>
-      <c r="F31" s="274"/>
-      <c r="G31" s="274"/>
-      <c r="H31" s="274"/>
-      <c r="I31" s="274"/>
-      <c r="J31" s="274"/>
-      <c r="K31" s="274"/>
-      <c r="L31" s="275"/>
+      <c r="C31" s="247"/>
+      <c r="D31" s="247"/>
+      <c r="E31" s="247"/>
+      <c r="F31" s="247"/>
+      <c r="G31" s="247"/>
+      <c r="H31" s="247"/>
+      <c r="I31" s="247"/>
+      <c r="J31" s="247"/>
+      <c r="K31" s="247"/>
+      <c r="L31" s="248"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="228">
         <v>6</v>
       </c>
-      <c r="B32" s="274" t="s">
+      <c r="B32" s="247" t="s">
         <v>328</v>
       </c>
-      <c r="C32" s="274"/>
-      <c r="D32" s="274"/>
-      <c r="E32" s="274"/>
-      <c r="F32" s="274"/>
-      <c r="G32" s="274"/>
-      <c r="H32" s="274"/>
-      <c r="I32" s="274"/>
-      <c r="J32" s="274"/>
-      <c r="K32" s="274"/>
-      <c r="L32" s="275"/>
+      <c r="C32" s="247"/>
+      <c r="D32" s="247"/>
+      <c r="E32" s="247"/>
+      <c r="F32" s="247"/>
+      <c r="G32" s="247"/>
+      <c r="H32" s="247"/>
+      <c r="I32" s="247"/>
+      <c r="J32" s="247"/>
+      <c r="K32" s="247"/>
+      <c r="L32" s="248"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="228">
         <v>7</v>
       </c>
-      <c r="B33" s="276" t="s">
+      <c r="B33" s="249" t="s">
         <v>324</v>
       </c>
-      <c r="C33" s="276"/>
-      <c r="D33" s="276"/>
-      <c r="E33" s="276"/>
-      <c r="F33" s="276"/>
-      <c r="G33" s="276"/>
-      <c r="H33" s="276"/>
-      <c r="I33" s="276"/>
-      <c r="J33" s="276"/>
-      <c r="K33" s="276"/>
-      <c r="L33" s="277"/>
+      <c r="C33" s="249"/>
+      <c r="D33" s="249"/>
+      <c r="E33" s="249"/>
+      <c r="F33" s="249"/>
+      <c r="G33" s="249"/>
+      <c r="H33" s="249"/>
+      <c r="I33" s="249"/>
+      <c r="J33" s="249"/>
+      <c r="K33" s="249"/>
+      <c r="L33" s="250"/>
     </row>
     <row r="34" spans="1:12" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="228"/>
@@ -15562,56 +15574,56 @@
       <c r="L34" s="230"/>
     </row>
     <row r="35" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="278" t="s">
+      <c r="A35" s="258" t="s">
         <v>327</v>
       </c>
-      <c r="B35" s="279"/>
-      <c r="C35" s="279"/>
-      <c r="D35" s="279"/>
-      <c r="E35" s="279"/>
-      <c r="F35" s="279"/>
-      <c r="G35" s="279"/>
-      <c r="H35" s="279"/>
-      <c r="I35" s="279"/>
-      <c r="J35" s="279"/>
-      <c r="K35" s="279"/>
-      <c r="L35" s="280"/>
+      <c r="B35" s="259"/>
+      <c r="C35" s="259"/>
+      <c r="D35" s="259"/>
+      <c r="E35" s="259"/>
+      <c r="F35" s="259"/>
+      <c r="G35" s="259"/>
+      <c r="H35" s="259"/>
+      <c r="I35" s="259"/>
+      <c r="J35" s="259"/>
+      <c r="K35" s="259"/>
+      <c r="L35" s="260"/>
     </row>
     <row r="36" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="231" t="s">
         <v>325</v>
       </c>
-      <c r="B36" s="276" t="s">
+      <c r="B36" s="249" t="s">
         <v>212</v>
       </c>
-      <c r="C36" s="276"/>
-      <c r="D36" s="276"/>
-      <c r="E36" s="276"/>
-      <c r="F36" s="276"/>
-      <c r="G36" s="276"/>
-      <c r="H36" s="276"/>
-      <c r="I36" s="276"/>
-      <c r="J36" s="276"/>
-      <c r="K36" s="276"/>
-      <c r="L36" s="277"/>
+      <c r="C36" s="249"/>
+      <c r="D36" s="249"/>
+      <c r="E36" s="249"/>
+      <c r="F36" s="249"/>
+      <c r="G36" s="249"/>
+      <c r="H36" s="249"/>
+      <c r="I36" s="249"/>
+      <c r="J36" s="249"/>
+      <c r="K36" s="249"/>
+      <c r="L36" s="250"/>
     </row>
     <row r="37" spans="1:12" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="232" t="s">
         <v>326</v>
       </c>
-      <c r="B37" s="282" t="s">
+      <c r="B37" s="251" t="s">
         <v>329</v>
       </c>
-      <c r="C37" s="282"/>
-      <c r="D37" s="282"/>
-      <c r="E37" s="282"/>
-      <c r="F37" s="282"/>
-      <c r="G37" s="282"/>
-      <c r="H37" s="282"/>
-      <c r="I37" s="282"/>
-      <c r="J37" s="282"/>
-      <c r="K37" s="282"/>
-      <c r="L37" s="283"/>
+      <c r="C37" s="251"/>
+      <c r="D37" s="251"/>
+      <c r="E37" s="251"/>
+      <c r="F37" s="251"/>
+      <c r="G37" s="251"/>
+      <c r="H37" s="251"/>
+      <c r="I37" s="251"/>
+      <c r="J37" s="251"/>
+      <c r="K37" s="251"/>
+      <c r="L37" s="252"/>
     </row>
     <row r="38" spans="1:12" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="160"/>
@@ -15628,20 +15640,20 @@
       <c r="L38" s="113"/>
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="284" t="s">
+      <c r="A39" s="253" t="s">
         <v>240</v>
       </c>
-      <c r="B39" s="285"/>
-      <c r="C39" s="285"/>
-      <c r="D39" s="285"/>
-      <c r="E39" s="285"/>
-      <c r="F39" s="285"/>
-      <c r="G39" s="285"/>
-      <c r="H39" s="285"/>
-      <c r="I39" s="285"/>
-      <c r="J39" s="285"/>
-      <c r="K39" s="285"/>
-      <c r="L39" s="286"/>
+      <c r="B39" s="254"/>
+      <c r="C39" s="254"/>
+      <c r="D39" s="254"/>
+      <c r="E39" s="254"/>
+      <c r="F39" s="254"/>
+      <c r="G39" s="254"/>
+      <c r="H39" s="254"/>
+      <c r="I39" s="254"/>
+      <c r="J39" s="254"/>
+      <c r="K39" s="254"/>
+      <c r="L39" s="255"/>
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="235" t="s">
@@ -15729,220 +15741,240 @@
       <c r="B45" s="168" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="264" t="s">
+      <c r="C45" s="256" t="s">
         <v>313</v>
       </c>
-      <c r="D45" s="264"/>
-      <c r="E45" s="264"/>
-      <c r="F45" s="264"/>
-      <c r="G45" s="264"/>
-      <c r="H45" s="264"/>
-      <c r="I45" s="264"/>
-      <c r="J45" s="264"/>
-      <c r="K45" s="264"/>
-      <c r="L45" s="265"/>
-    </row>
-    <row r="46" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D45" s="256"/>
+      <c r="E45" s="256"/>
+      <c r="F45" s="256"/>
+      <c r="G45" s="256"/>
+      <c r="H45" s="256"/>
+      <c r="I45" s="256"/>
+      <c r="J45" s="256"/>
+      <c r="K45" s="256"/>
+      <c r="L45" s="257"/>
+    </row>
+    <row r="46" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="167"/>
       <c r="B46" s="168" t="s">
-        <v>138</v>
-      </c>
-      <c r="C46" s="264" t="s">
-        <v>139</v>
-      </c>
-      <c r="D46" s="264"/>
-      <c r="E46" s="264"/>
-      <c r="F46" s="264"/>
-      <c r="G46" s="264"/>
-      <c r="H46" s="264"/>
-      <c r="I46" s="264"/>
-      <c r="J46" s="264"/>
-      <c r="K46" s="264"/>
-      <c r="L46" s="265"/>
-    </row>
-    <row r="47" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="C46" s="256" t="s">
+        <v>315</v>
+      </c>
+      <c r="D46" s="256"/>
+      <c r="E46" s="256"/>
+      <c r="F46" s="256"/>
+      <c r="G46" s="256"/>
+      <c r="H46" s="256"/>
+      <c r="I46" s="256"/>
+      <c r="J46" s="256"/>
+      <c r="K46" s="256"/>
+      <c r="L46" s="257"/>
+    </row>
+    <row r="47" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="167"/>
       <c r="B47" s="168" t="s">
-        <v>238</v>
-      </c>
-      <c r="C47" s="264" t="s">
-        <v>239</v>
-      </c>
-      <c r="D47" s="264"/>
-      <c r="E47" s="264"/>
-      <c r="F47" s="264"/>
-      <c r="G47" s="264"/>
-      <c r="H47" s="264"/>
-      <c r="I47" s="264"/>
-      <c r="J47" s="264"/>
-      <c r="K47" s="264"/>
-      <c r="L47" s="265"/>
-    </row>
-    <row r="48" spans="1:12" ht="15.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>384</v>
+      </c>
+      <c r="C47" s="256" t="s">
+        <v>385</v>
+      </c>
+      <c r="D47" s="256"/>
+      <c r="E47" s="256"/>
+      <c r="F47" s="256"/>
+      <c r="G47" s="256"/>
+      <c r="H47" s="256"/>
+      <c r="I47" s="256"/>
+      <c r="J47" s="256"/>
+      <c r="K47" s="256"/>
+      <c r="L47" s="257"/>
+    </row>
+    <row r="48" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="167"/>
       <c r="B48" s="168" t="s">
-        <v>314</v>
-      </c>
-      <c r="C48" s="264" t="s">
-        <v>315</v>
-      </c>
-      <c r="D48" s="264"/>
-      <c r="E48" s="264"/>
-      <c r="F48" s="264"/>
-      <c r="G48" s="264"/>
-      <c r="H48" s="264"/>
-      <c r="I48" s="264"/>
-      <c r="J48" s="264"/>
-      <c r="K48" s="264"/>
-      <c r="L48" s="265"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+      <c r="C48" s="256" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="256"/>
+      <c r="E48" s="256"/>
+      <c r="F48" s="256"/>
+      <c r="G48" s="256"/>
+      <c r="H48" s="256"/>
+      <c r="I48" s="256"/>
+      <c r="J48" s="256"/>
+      <c r="K48" s="256"/>
+      <c r="L48" s="257"/>
+    </row>
+    <row r="49" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="167"/>
       <c r="B49" s="168" t="s">
-        <v>203</v>
-      </c>
-      <c r="C49" s="169" t="s">
-        <v>316</v>
-      </c>
-      <c r="D49" s="169"/>
-      <c r="E49" s="169"/>
-      <c r="F49" s="169"/>
-      <c r="G49" s="169"/>
-      <c r="H49" s="169"/>
-      <c r="I49" s="169"/>
-      <c r="J49" s="169"/>
-      <c r="K49" s="169"/>
-      <c r="L49" s="170"/>
-    </row>
-    <row r="50" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+      <c r="C49" s="256" t="s">
+        <v>239</v>
+      </c>
+      <c r="D49" s="256"/>
+      <c r="E49" s="256"/>
+      <c r="F49" s="256"/>
+      <c r="G49" s="256"/>
+      <c r="H49" s="256"/>
+      <c r="I49" s="256"/>
+      <c r="J49" s="256"/>
+      <c r="K49" s="256"/>
+      <c r="L49" s="257"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="167"/>
       <c r="B50" s="168" t="s">
-        <v>63</v>
-      </c>
-      <c r="C50" s="264" t="s">
-        <v>317</v>
-      </c>
-      <c r="D50" s="264"/>
-      <c r="E50" s="264"/>
-      <c r="F50" s="264"/>
-      <c r="G50" s="264"/>
-      <c r="H50" s="264"/>
-      <c r="I50" s="264"/>
-      <c r="J50" s="264"/>
-      <c r="K50" s="264"/>
-      <c r="L50" s="265"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.35">
+        <v>203</v>
+      </c>
+      <c r="C50" s="169" t="s">
+        <v>316</v>
+      </c>
+      <c r="D50" s="169"/>
+      <c r="E50" s="169"/>
+      <c r="F50" s="169"/>
+      <c r="G50" s="169"/>
+      <c r="H50" s="169"/>
+      <c r="I50" s="169"/>
+      <c r="J50" s="169"/>
+      <c r="K50" s="169"/>
+      <c r="L50" s="170"/>
+    </row>
+    <row r="51" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="167"/>
       <c r="B51" s="168" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" s="256" t="s">
+        <v>317</v>
+      </c>
+      <c r="D51" s="256"/>
+      <c r="E51" s="256"/>
+      <c r="F51" s="256"/>
+      <c r="G51" s="256"/>
+      <c r="H51" s="256"/>
+      <c r="I51" s="256"/>
+      <c r="J51" s="256"/>
+      <c r="K51" s="256"/>
+      <c r="L51" s="257"/>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A52" s="167"/>
+      <c r="B52" s="168" t="s">
         <v>75</v>
       </c>
-      <c r="C51" s="169" t="s">
+      <c r="C52" s="169" t="s">
         <v>76</v>
       </c>
-      <c r="D51" s="169"/>
-      <c r="E51" s="169"/>
-      <c r="F51" s="169"/>
-      <c r="G51" s="169"/>
-      <c r="H51" s="169"/>
-      <c r="I51" s="169"/>
-      <c r="J51" s="169"/>
-      <c r="K51" s="169"/>
-      <c r="L51" s="170"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A52" s="171"/>
-      <c r="B52" s="172" t="s">
+      <c r="D52" s="169"/>
+      <c r="E52" s="169"/>
+      <c r="F52" s="169"/>
+      <c r="G52" s="169"/>
+      <c r="H52" s="169"/>
+      <c r="I52" s="169"/>
+      <c r="J52" s="169"/>
+      <c r="K52" s="169"/>
+      <c r="L52" s="170"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A53" s="171"/>
+      <c r="B53" s="172" t="s">
         <v>159</v>
       </c>
-      <c r="C52" s="173" t="s">
+      <c r="C53" s="173" t="s">
         <v>160</v>
       </c>
-      <c r="D52" s="173"/>
-      <c r="E52" s="173"/>
-      <c r="F52" s="173"/>
-      <c r="G52" s="173"/>
-      <c r="H52" s="173"/>
-      <c r="I52" s="173"/>
-      <c r="J52" s="173"/>
-      <c r="K52" s="173"/>
-      <c r="L52" s="174"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A54" s="1" t="s">
+      <c r="D53" s="173"/>
+      <c r="E53" s="173"/>
+      <c r="F53" s="173"/>
+      <c r="G53" s="173"/>
+      <c r="H53" s="173"/>
+      <c r="I53" s="173"/>
+      <c r="J53" s="173"/>
+      <c r="K53" s="173"/>
+      <c r="L53" s="174"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A57" s="45" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A58" s="45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A59" s="45" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A59" s="45"/>
-    </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="45"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A61" s="45" t="s">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A62" s="45" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A63" s="1" t="s">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="281" t="s">
+    <row r="65" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="246" t="s">
         <v>356</v>
       </c>
-      <c r="B64" s="281"/>
-      <c r="C64" s="281"/>
-      <c r="D64" s="281"/>
-      <c r="E64" s="281"/>
-      <c r="F64" s="281"/>
-      <c r="G64" s="281"/>
-      <c r="H64" s="281"/>
-      <c r="I64" s="281"/>
-      <c r="J64" s="281"/>
-      <c r="K64" s="281"/>
-      <c r="L64" s="281"/>
-    </row>
-    <row r="69" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="70" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="B65" s="246"/>
+      <c r="C65" s="246"/>
+      <c r="D65" s="246"/>
+      <c r="E65" s="246"/>
+      <c r="F65" s="246"/>
+      <c r="G65" s="246"/>
+      <c r="H65" s="246"/>
+      <c r="I65" s="246"/>
+      <c r="J65" s="246"/>
+      <c r="K65" s="246"/>
+      <c r="L65" s="246"/>
+    </row>
+    <row r="70" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="71" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="40">
-    <mergeCell ref="A64:L64"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="C45:L45"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="C47:L47"/>
-    <mergeCell ref="C48:L48"/>
-    <mergeCell ref="C50:L50"/>
-    <mergeCell ref="A35:L35"/>
+  <mergeCells count="41">
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B8:L8"/>
     <mergeCell ref="B31:L31"/>
     <mergeCell ref="B18:L18"/>
     <mergeCell ref="B19:L19"/>
@@ -15957,25 +15989,24 @@
     <mergeCell ref="B29:L29"/>
     <mergeCell ref="B28:L28"/>
     <mergeCell ref="B30:L30"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="A65:L65"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="C45:L45"/>
+    <mergeCell ref="C48:L48"/>
+    <mergeCell ref="C49:L49"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="C51:L51"/>
+    <mergeCell ref="A35:L35"/>
+    <mergeCell ref="C47:L47"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A57" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
-    <hyperlink ref="A58" r:id="rId2" xr:uid="{66F54200-A2AB-43DA-A0E0-F2A25A075EE5}"/>
-    <hyperlink ref="A61" r:id="rId3" xr:uid="{A0F8DE06-D9FC-495F-9A01-AA199CB82365}"/>
+    <hyperlink ref="A58" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
+    <hyperlink ref="A59" r:id="rId2" xr:uid="{66F54200-A2AB-43DA-A0E0-F2A25A075EE5}"/>
+    <hyperlink ref="A62" r:id="rId3" xr:uid="{A0F8DE06-D9FC-495F-9A01-AA199CB82365}"/>
     <hyperlink ref="A39:L39" r:id="rId4" display="LETS START (visual directions as pdf)" xr:uid="{0D075873-7EBB-4309-B00A-6A62EA192A0C}"/>
     <hyperlink ref="A40" r:id="rId5" xr:uid="{25154A32-BA44-496E-9945-086DE0980DBD}"/>
   </hyperlinks>
@@ -31564,8 +31595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BF7D8F-86F3-47E9-AB85-EE9B4CAB70E4}">
   <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31644,7 +31675,7 @@
       <c r="F4" s="297"/>
       <c r="G4" s="298"/>
       <c r="N4" s="141" t="s">
-        <v>168</v>
+        <v>386</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -31892,7 +31923,9 @@
       <c r="C24"/>
       <c r="D24" s="111"/>
       <c r="E24" s="28"/>
-      <c r="N24" s="141"/>
+      <c r="N24" s="141" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
@@ -31905,7 +31938,9 @@
       <c r="C25"/>
       <c r="D25" s="111"/>
       <c r="E25" s="28"/>
-      <c r="N25" s="141"/>
+      <c r="N25" s="141" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B26" s="28"/>
@@ -36265,7 +36300,7 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="N4" r:id="rId1" location="step-1-assign-accounts-articulate-vulnerabilities-and-strategies-to-manage-vulnerability" xr:uid="{DF55C70C-AEA5-4BB4-9BD1-23B882C83781}"/>
+    <hyperlink ref="N4" r:id="rId1" location="step-1-assign-accounts-articulate-vulnerabilities-and-strategies-to-manage-vulnerability" display="Help assign parties" xr:uid="{DF55C70C-AEA5-4BB4-9BD1-23B882C83781}"/>
     <hyperlink ref="N17" r:id="rId2" location="1b-make-assumptions" xr:uid="{91CC7212-C579-4B1B-A8B8-969D4549837D}"/>
     <hyperlink ref="N18" r:id="rId3" location="i-evaporation-rates" xr:uid="{23C61350-606E-472B-90E1-88574D6741EE}"/>
     <hyperlink ref="N19" r:id="rId4" location="ii-start-storage" xr:uid="{692C3AE6-515B-4C08-B6EC-0557E75E9511}"/>
@@ -37690,8 +37725,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876BA06C-E963-43DD-B933-307F043834EF}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -38016,16 +38051,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="321" t="e">
+      <c r="A1" s="322" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="321"/>
-      <c r="C1" s="321"/>
-      <c r="D1" s="321"/>
-      <c r="E1" s="321"/>
-      <c r="F1" s="321"/>
-      <c r="G1" s="321"/>
+      <c r="B1" s="322"/>
+      <c r="C1" s="322"/>
+      <c r="D1" s="322"/>
+      <c r="E1" s="322"/>
+      <c r="F1" s="322"/>
+      <c r="G1" s="322"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -38134,11 +38169,11 @@
         <v>80</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="322"/>
-      <c r="D10" s="322"/>
-      <c r="E10" s="322"/>
-      <c r="F10" s="322"/>
-      <c r="G10" s="322"/>
+      <c r="C10" s="321"/>
+      <c r="D10" s="321"/>
+      <c r="E10" s="321"/>
+      <c r="F10" s="321"/>
+      <c r="G10" s="321"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -39401,6 +39436,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -39408,12 +39449,6 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>

</xml_diff>

<commit_message>
Update help links for Percent Tribal Waters
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CEAE45-3945-4718-988A-B58FB66351D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E718FE9-D6B9-43F2-84DD-C4936CA9C329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="62" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="389">
   <si>
     <t>Year 1</t>
   </si>
@@ -2014,6 +2014,9 @@
   <si>
     <t>Help percent of Tribal Nation water in CA</t>
   </si>
+  <si>
+    <t>Help percent of Tribal Nation water in AZ</t>
+  </si>
 </sst>
 </file>
 
@@ -3311,51 +3314,6 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3410,6 +3368,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3433,6 +3397,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3536,11 +3539,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14980,20 +14983,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="264" t="s">
+      <c r="A1" s="249" t="s">
         <v>351</v>
       </c>
-      <c r="B1" s="264"/>
-      <c r="C1" s="264"/>
-      <c r="D1" s="264"/>
-      <c r="E1" s="264"/>
-      <c r="F1" s="264"/>
-      <c r="G1" s="264"/>
-      <c r="H1" s="264"/>
-      <c r="I1" s="264"/>
-      <c r="J1" s="264"/>
-      <c r="K1" s="264"/>
-      <c r="L1" s="264"/>
+      <c r="B1" s="249"/>
+      <c r="C1" s="249"/>
+      <c r="D1" s="249"/>
+      <c r="E1" s="249"/>
+      <c r="F1" s="249"/>
+      <c r="G1" s="249"/>
+      <c r="H1" s="249"/>
+      <c r="I1" s="249"/>
+      <c r="J1" s="249"/>
+      <c r="K1" s="249"/>
+      <c r="L1" s="249"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -15019,41 +15022,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="265" t="s">
+      <c r="A4" s="250" t="s">
         <v>352</v>
       </c>
-      <c r="B4" s="266"/>
-      <c r="C4" s="266"/>
-      <c r="D4" s="266"/>
-      <c r="E4" s="266"/>
-      <c r="F4" s="266"/>
-      <c r="G4" s="266"/>
-      <c r="H4" s="266"/>
-      <c r="I4" s="266"/>
-      <c r="J4" s="266"/>
-      <c r="K4" s="266"/>
-      <c r="L4" s="267"/>
-      <c r="N4" s="268"/>
-      <c r="O4" s="268"/>
-      <c r="P4" s="268"/>
-      <c r="Q4" s="268"/>
-      <c r="R4" s="268"/>
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="252"/>
+      <c r="N4" s="253"/>
+      <c r="O4" s="253"/>
+      <c r="P4" s="253"/>
+      <c r="Q4" s="253"/>
+      <c r="R4" s="253"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="269" t="s">
+      <c r="A5" s="254" t="s">
         <v>335</v>
       </c>
-      <c r="B5" s="270"/>
-      <c r="C5" s="270"/>
-      <c r="D5" s="270"/>
-      <c r="E5" s="270"/>
-      <c r="F5" s="270"/>
-      <c r="G5" s="270"/>
-      <c r="H5" s="270"/>
-      <c r="I5" s="270"/>
-      <c r="J5" s="270"/>
-      <c r="K5" s="270"/>
-      <c r="L5" s="271"/>
+      <c r="B5" s="255"/>
+      <c r="C5" s="255"/>
+      <c r="D5" s="255"/>
+      <c r="E5" s="255"/>
+      <c r="F5" s="255"/>
+      <c r="G5" s="255"/>
+      <c r="H5" s="255"/>
+      <c r="I5" s="255"/>
+      <c r="J5" s="255"/>
+      <c r="K5" s="255"/>
+      <c r="L5" s="256"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15061,20 +15064,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="269" t="s">
+      <c r="A6" s="254" t="s">
         <v>353</v>
       </c>
-      <c r="B6" s="270"/>
-      <c r="C6" s="270"/>
-      <c r="D6" s="270"/>
-      <c r="E6" s="270"/>
-      <c r="F6" s="270"/>
-      <c r="G6" s="270"/>
-      <c r="H6" s="270"/>
-      <c r="I6" s="270"/>
-      <c r="J6" s="270"/>
-      <c r="K6" s="270"/>
-      <c r="L6" s="271"/>
+      <c r="B6" s="255"/>
+      <c r="C6" s="255"/>
+      <c r="D6" s="255"/>
+      <c r="E6" s="255"/>
+      <c r="F6" s="255"/>
+      <c r="G6" s="255"/>
+      <c r="H6" s="255"/>
+      <c r="I6" s="255"/>
+      <c r="J6" s="255"/>
+      <c r="K6" s="255"/>
+      <c r="L6" s="256"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15083,19 +15086,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="233"/>
-      <c r="B7" s="270" t="s">
+      <c r="B7" s="255" t="s">
         <v>354</v>
       </c>
-      <c r="C7" s="270"/>
-      <c r="D7" s="270"/>
-      <c r="E7" s="270"/>
-      <c r="F7" s="270"/>
-      <c r="G7" s="270"/>
-      <c r="H7" s="270"/>
-      <c r="I7" s="270"/>
-      <c r="J7" s="270"/>
-      <c r="K7" s="270"/>
-      <c r="L7" s="271"/>
+      <c r="C7" s="255"/>
+      <c r="D7" s="255"/>
+      <c r="E7" s="255"/>
+      <c r="F7" s="255"/>
+      <c r="G7" s="255"/>
+      <c r="H7" s="255"/>
+      <c r="I7" s="255"/>
+      <c r="J7" s="255"/>
+      <c r="K7" s="255"/>
+      <c r="L7" s="256"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15104,19 +15107,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="234"/>
-      <c r="B8" s="285" t="s">
+      <c r="B8" s="272" t="s">
         <v>355</v>
       </c>
-      <c r="C8" s="285"/>
-      <c r="D8" s="285"/>
-      <c r="E8" s="285"/>
-      <c r="F8" s="285"/>
-      <c r="G8" s="285"/>
-      <c r="H8" s="285"/>
-      <c r="I8" s="285"/>
-      <c r="J8" s="285"/>
-      <c r="K8" s="285"/>
-      <c r="L8" s="286"/>
+      <c r="C8" s="272"/>
+      <c r="D8" s="272"/>
+      <c r="E8" s="272"/>
+      <c r="F8" s="272"/>
+      <c r="G8" s="272"/>
+      <c r="H8" s="272"/>
+      <c r="I8" s="272"/>
+      <c r="J8" s="272"/>
+      <c r="K8" s="272"/>
+      <c r="L8" s="273"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15138,84 +15141,84 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="272" t="s">
+      <c r="A10" s="257" t="s">
         <v>205</v>
       </c>
-      <c r="B10" s="273"/>
-      <c r="C10" s="273"/>
-      <c r="D10" s="273"/>
-      <c r="E10" s="273"/>
-      <c r="F10" s="273"/>
-      <c r="G10" s="273"/>
-      <c r="H10" s="273"/>
-      <c r="I10" s="273"/>
-      <c r="J10" s="273"/>
-      <c r="K10" s="273"/>
-      <c r="L10" s="274"/>
+      <c r="B10" s="258"/>
+      <c r="C10" s="258"/>
+      <c r="D10" s="258"/>
+      <c r="E10" s="258"/>
+      <c r="F10" s="258"/>
+      <c r="G10" s="258"/>
+      <c r="H10" s="258"/>
+      <c r="I10" s="258"/>
+      <c r="J10" s="258"/>
+      <c r="K10" s="258"/>
+      <c r="L10" s="259"/>
     </row>
     <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="275" t="s">
+      <c r="A11" s="260" t="s">
         <v>336</v>
       </c>
-      <c r="B11" s="276"/>
-      <c r="C11" s="276"/>
-      <c r="D11" s="276"/>
-      <c r="E11" s="276"/>
-      <c r="F11" s="276"/>
-      <c r="G11" s="276"/>
-      <c r="H11" s="276"/>
-      <c r="I11" s="276"/>
-      <c r="J11" s="276"/>
-      <c r="K11" s="276"/>
-      <c r="L11" s="277"/>
+      <c r="B11" s="261"/>
+      <c r="C11" s="261"/>
+      <c r="D11" s="261"/>
+      <c r="E11" s="261"/>
+      <c r="F11" s="261"/>
+      <c r="G11" s="261"/>
+      <c r="H11" s="261"/>
+      <c r="I11" s="261"/>
+      <c r="J11" s="261"/>
+      <c r="K11" s="261"/>
+      <c r="L11" s="262"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="278" t="s">
+      <c r="A12" s="263" t="s">
         <v>337</v>
       </c>
-      <c r="B12" s="256"/>
-      <c r="C12" s="256"/>
-      <c r="D12" s="256"/>
-      <c r="E12" s="256"/>
-      <c r="F12" s="256"/>
-      <c r="G12" s="256"/>
-      <c r="H12" s="256"/>
-      <c r="I12" s="256"/>
-      <c r="J12" s="256"/>
-      <c r="K12" s="256"/>
-      <c r="L12" s="257"/>
+      <c r="B12" s="264"/>
+      <c r="C12" s="264"/>
+      <c r="D12" s="264"/>
+      <c r="E12" s="264"/>
+      <c r="F12" s="264"/>
+      <c r="G12" s="264"/>
+      <c r="H12" s="264"/>
+      <c r="I12" s="264"/>
+      <c r="J12" s="264"/>
+      <c r="K12" s="264"/>
+      <c r="L12" s="265"/>
     </row>
     <row r="13" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="278" t="s">
+      <c r="A13" s="263" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="256"/>
-      <c r="C13" s="256"/>
-      <c r="D13" s="256"/>
-      <c r="E13" s="256"/>
-      <c r="F13" s="256"/>
-      <c r="G13" s="256"/>
-      <c r="H13" s="256"/>
-      <c r="I13" s="256"/>
-      <c r="J13" s="256"/>
-      <c r="K13" s="256"/>
-      <c r="L13" s="257"/>
+      <c r="B13" s="264"/>
+      <c r="C13" s="264"/>
+      <c r="D13" s="264"/>
+      <c r="E13" s="264"/>
+      <c r="F13" s="264"/>
+      <c r="G13" s="264"/>
+      <c r="H13" s="264"/>
+      <c r="I13" s="264"/>
+      <c r="J13" s="264"/>
+      <c r="K13" s="264"/>
+      <c r="L13" s="265"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="279" t="s">
+      <c r="A14" s="266" t="s">
         <v>338</v>
       </c>
-      <c r="B14" s="280"/>
-      <c r="C14" s="280"/>
-      <c r="D14" s="280"/>
-      <c r="E14" s="280"/>
-      <c r="F14" s="280"/>
-      <c r="G14" s="280"/>
-      <c r="H14" s="280"/>
-      <c r="I14" s="280"/>
-      <c r="J14" s="280"/>
-      <c r="K14" s="280"/>
-      <c r="L14" s="281"/>
+      <c r="B14" s="267"/>
+      <c r="C14" s="267"/>
+      <c r="D14" s="267"/>
+      <c r="E14" s="267"/>
+      <c r="F14" s="267"/>
+      <c r="G14" s="267"/>
+      <c r="H14" s="267"/>
+      <c r="I14" s="267"/>
+      <c r="J14" s="267"/>
+      <c r="K14" s="267"/>
+      <c r="L14" s="268"/>
     </row>
     <row r="15" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="113"/>
@@ -15232,332 +15235,332 @@
       <c r="L15" s="113"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="282" t="s">
+      <c r="A16" s="269" t="s">
         <v>334</v>
       </c>
-      <c r="B16" s="283"/>
-      <c r="C16" s="283"/>
-      <c r="D16" s="283"/>
-      <c r="E16" s="283"/>
-      <c r="F16" s="283"/>
-      <c r="G16" s="283"/>
-      <c r="H16" s="283"/>
-      <c r="I16" s="283"/>
-      <c r="J16" s="283"/>
-      <c r="K16" s="283"/>
-      <c r="L16" s="284"/>
+      <c r="B16" s="270"/>
+      <c r="C16" s="270"/>
+      <c r="D16" s="270"/>
+      <c r="E16" s="270"/>
+      <c r="F16" s="270"/>
+      <c r="G16" s="270"/>
+      <c r="H16" s="270"/>
+      <c r="I16" s="270"/>
+      <c r="J16" s="270"/>
+      <c r="K16" s="270"/>
+      <c r="L16" s="271"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="261" t="s">
+      <c r="A17" s="246" t="s">
         <v>215</v>
       </c>
-      <c r="B17" s="262"/>
-      <c r="C17" s="262"/>
-      <c r="D17" s="262"/>
-      <c r="E17" s="262"/>
-      <c r="F17" s="262"/>
-      <c r="G17" s="262"/>
-      <c r="H17" s="262"/>
-      <c r="I17" s="262"/>
-      <c r="J17" s="262"/>
-      <c r="K17" s="262"/>
-      <c r="L17" s="263"/>
+      <c r="B17" s="247"/>
+      <c r="C17" s="247"/>
+      <c r="D17" s="247"/>
+      <c r="E17" s="247"/>
+      <c r="F17" s="247"/>
+      <c r="G17" s="247"/>
+      <c r="H17" s="247"/>
+      <c r="I17" s="247"/>
+      <c r="J17" s="247"/>
+      <c r="K17" s="247"/>
+      <c r="L17" s="248"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="228">
         <v>1</v>
       </c>
-      <c r="B18" s="249" t="s">
+      <c r="B18" s="276" t="s">
         <v>214</v>
       </c>
-      <c r="C18" s="249"/>
-      <c r="D18" s="249"/>
-      <c r="E18" s="249"/>
-      <c r="F18" s="249"/>
-      <c r="G18" s="249"/>
-      <c r="H18" s="249"/>
-      <c r="I18" s="249"/>
-      <c r="J18" s="249"/>
-      <c r="K18" s="249"/>
-      <c r="L18" s="250"/>
+      <c r="C18" s="276"/>
+      <c r="D18" s="276"/>
+      <c r="E18" s="276"/>
+      <c r="F18" s="276"/>
+      <c r="G18" s="276"/>
+      <c r="H18" s="276"/>
+      <c r="I18" s="276"/>
+      <c r="J18" s="276"/>
+      <c r="K18" s="276"/>
+      <c r="L18" s="277"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="228">
         <v>2</v>
       </c>
-      <c r="B19" s="249" t="s">
+      <c r="B19" s="276" t="s">
         <v>330</v>
       </c>
-      <c r="C19" s="249"/>
-      <c r="D19" s="249"/>
-      <c r="E19" s="249"/>
-      <c r="F19" s="249"/>
-      <c r="G19" s="249"/>
-      <c r="H19" s="249"/>
-      <c r="I19" s="249"/>
-      <c r="J19" s="249"/>
-      <c r="K19" s="249"/>
-      <c r="L19" s="250"/>
+      <c r="C19" s="276"/>
+      <c r="D19" s="276"/>
+      <c r="E19" s="276"/>
+      <c r="F19" s="276"/>
+      <c r="G19" s="276"/>
+      <c r="H19" s="276"/>
+      <c r="I19" s="276"/>
+      <c r="J19" s="276"/>
+      <c r="K19" s="276"/>
+      <c r="L19" s="277"/>
       <c r="N19" s="106"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="228">
         <v>3</v>
       </c>
-      <c r="B20" s="249" t="s">
+      <c r="B20" s="276" t="s">
         <v>207</v>
       </c>
-      <c r="C20" s="249"/>
-      <c r="D20" s="249"/>
-      <c r="E20" s="249"/>
-      <c r="F20" s="249"/>
-      <c r="G20" s="249"/>
-      <c r="H20" s="249"/>
-      <c r="I20" s="249"/>
-      <c r="J20" s="249"/>
-      <c r="K20" s="249"/>
-      <c r="L20" s="250"/>
+      <c r="C20" s="276"/>
+      <c r="D20" s="276"/>
+      <c r="E20" s="276"/>
+      <c r="F20" s="276"/>
+      <c r="G20" s="276"/>
+      <c r="H20" s="276"/>
+      <c r="I20" s="276"/>
+      <c r="J20" s="276"/>
+      <c r="K20" s="276"/>
+      <c r="L20" s="277"/>
       <c r="N20" s="106"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="228">
         <v>4</v>
       </c>
-      <c r="B21" s="249" t="s">
+      <c r="B21" s="276" t="s">
         <v>339</v>
       </c>
-      <c r="C21" s="249"/>
-      <c r="D21" s="249"/>
-      <c r="E21" s="249"/>
-      <c r="F21" s="249"/>
-      <c r="G21" s="249"/>
-      <c r="H21" s="249"/>
-      <c r="I21" s="249"/>
-      <c r="J21" s="249"/>
-      <c r="K21" s="249"/>
-      <c r="L21" s="250"/>
+      <c r="C21" s="276"/>
+      <c r="D21" s="276"/>
+      <c r="E21" s="276"/>
+      <c r="F21" s="276"/>
+      <c r="G21" s="276"/>
+      <c r="H21" s="276"/>
+      <c r="I21" s="276"/>
+      <c r="J21" s="276"/>
+      <c r="K21" s="276"/>
+      <c r="L21" s="277"/>
       <c r="N21" s="106"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="228">
         <v>5</v>
       </c>
-      <c r="B22" s="249" t="s">
+      <c r="B22" s="276" t="s">
         <v>208</v>
       </c>
-      <c r="C22" s="249"/>
-      <c r="D22" s="249"/>
-      <c r="E22" s="249"/>
-      <c r="F22" s="249"/>
-      <c r="G22" s="249"/>
-      <c r="H22" s="249"/>
-      <c r="I22" s="249"/>
-      <c r="J22" s="249"/>
-      <c r="K22" s="249"/>
-      <c r="L22" s="250"/>
+      <c r="C22" s="276"/>
+      <c r="D22" s="276"/>
+      <c r="E22" s="276"/>
+      <c r="F22" s="276"/>
+      <c r="G22" s="276"/>
+      <c r="H22" s="276"/>
+      <c r="I22" s="276"/>
+      <c r="J22" s="276"/>
+      <c r="K22" s="276"/>
+      <c r="L22" s="277"/>
       <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="228"/>
-      <c r="B23" s="249" t="s">
+      <c r="B23" s="276" t="s">
         <v>209</v>
       </c>
-      <c r="C23" s="249"/>
-      <c r="D23" s="249"/>
-      <c r="E23" s="249"/>
-      <c r="F23" s="249"/>
-      <c r="G23" s="249"/>
-      <c r="H23" s="249"/>
-      <c r="I23" s="249"/>
-      <c r="J23" s="249"/>
-      <c r="K23" s="249"/>
-      <c r="L23" s="250"/>
+      <c r="C23" s="276"/>
+      <c r="D23" s="276"/>
+      <c r="E23" s="276"/>
+      <c r="F23" s="276"/>
+      <c r="G23" s="276"/>
+      <c r="H23" s="276"/>
+      <c r="I23" s="276"/>
+      <c r="J23" s="276"/>
+      <c r="K23" s="276"/>
+      <c r="L23" s="277"/>
       <c r="N23" s="106"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="228"/>
-      <c r="B24" s="249" t="s">
+      <c r="B24" s="276" t="s">
         <v>210</v>
       </c>
-      <c r="C24" s="249"/>
-      <c r="D24" s="249"/>
-      <c r="E24" s="249"/>
-      <c r="F24" s="249"/>
-      <c r="G24" s="249"/>
-      <c r="H24" s="249"/>
-      <c r="I24" s="249"/>
-      <c r="J24" s="249"/>
-      <c r="K24" s="249"/>
-      <c r="L24" s="250"/>
+      <c r="C24" s="276"/>
+      <c r="D24" s="276"/>
+      <c r="E24" s="276"/>
+      <c r="F24" s="276"/>
+      <c r="G24" s="276"/>
+      <c r="H24" s="276"/>
+      <c r="I24" s="276"/>
+      <c r="J24" s="276"/>
+      <c r="K24" s="276"/>
+      <c r="L24" s="277"/>
       <c r="N24" s="106"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="258" t="s">
+      <c r="A25" s="278" t="s">
         <v>216</v>
       </c>
-      <c r="B25" s="259"/>
-      <c r="C25" s="259"/>
-      <c r="D25" s="259"/>
-      <c r="E25" s="259"/>
-      <c r="F25" s="259"/>
-      <c r="G25" s="259"/>
-      <c r="H25" s="259"/>
-      <c r="I25" s="259"/>
-      <c r="J25" s="259"/>
-      <c r="K25" s="259"/>
-      <c r="L25" s="260"/>
+      <c r="B25" s="279"/>
+      <c r="C25" s="279"/>
+      <c r="D25" s="279"/>
+      <c r="E25" s="279"/>
+      <c r="F25" s="279"/>
+      <c r="G25" s="279"/>
+      <c r="H25" s="279"/>
+      <c r="I25" s="279"/>
+      <c r="J25" s="279"/>
+      <c r="K25" s="279"/>
+      <c r="L25" s="280"/>
       <c r="N25" s="106"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="228">
         <v>1</v>
       </c>
-      <c r="B26" s="249" t="s">
+      <c r="B26" s="276" t="s">
         <v>211</v>
       </c>
-      <c r="C26" s="249"/>
-      <c r="D26" s="249"/>
-      <c r="E26" s="249"/>
-      <c r="F26" s="249"/>
-      <c r="G26" s="249"/>
-      <c r="H26" s="249"/>
-      <c r="I26" s="249"/>
-      <c r="J26" s="249"/>
-      <c r="K26" s="249"/>
-      <c r="L26" s="250"/>
+      <c r="C26" s="276"/>
+      <c r="D26" s="276"/>
+      <c r="E26" s="276"/>
+      <c r="F26" s="276"/>
+      <c r="G26" s="276"/>
+      <c r="H26" s="276"/>
+      <c r="I26" s="276"/>
+      <c r="J26" s="276"/>
+      <c r="K26" s="276"/>
+      <c r="L26" s="277"/>
       <c r="N26" s="106"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="228"/>
-      <c r="B27" s="247" t="s">
+      <c r="B27" s="274" t="s">
         <v>340</v>
       </c>
-      <c r="C27" s="247"/>
-      <c r="D27" s="247"/>
-      <c r="E27" s="247"/>
-      <c r="F27" s="247"/>
-      <c r="G27" s="247"/>
-      <c r="H27" s="247"/>
-      <c r="I27" s="247"/>
-      <c r="J27" s="247"/>
-      <c r="K27" s="247"/>
-      <c r="L27" s="248"/>
+      <c r="C27" s="274"/>
+      <c r="D27" s="274"/>
+      <c r="E27" s="274"/>
+      <c r="F27" s="274"/>
+      <c r="G27" s="274"/>
+      <c r="H27" s="274"/>
+      <c r="I27" s="274"/>
+      <c r="J27" s="274"/>
+      <c r="K27" s="274"/>
+      <c r="L27" s="275"/>
       <c r="N27" s="106"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="228">
         <v>2</v>
       </c>
-      <c r="B28" s="249" t="s">
+      <c r="B28" s="276" t="s">
         <v>333</v>
       </c>
-      <c r="C28" s="249"/>
-      <c r="D28" s="249"/>
-      <c r="E28" s="249"/>
-      <c r="F28" s="249"/>
-      <c r="G28" s="249"/>
-      <c r="H28" s="249"/>
-      <c r="I28" s="249"/>
-      <c r="J28" s="249"/>
-      <c r="K28" s="249"/>
-      <c r="L28" s="250"/>
+      <c r="C28" s="276"/>
+      <c r="D28" s="276"/>
+      <c r="E28" s="276"/>
+      <c r="F28" s="276"/>
+      <c r="G28" s="276"/>
+      <c r="H28" s="276"/>
+      <c r="I28" s="276"/>
+      <c r="J28" s="276"/>
+      <c r="K28" s="276"/>
+      <c r="L28" s="277"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="228">
         <v>3</v>
       </c>
-      <c r="B29" s="249" t="s">
+      <c r="B29" s="276" t="s">
         <v>322</v>
       </c>
-      <c r="C29" s="249"/>
-      <c r="D29" s="249"/>
-      <c r="E29" s="249"/>
-      <c r="F29" s="249"/>
-      <c r="G29" s="249"/>
-      <c r="H29" s="249"/>
-      <c r="I29" s="249"/>
-      <c r="J29" s="249"/>
-      <c r="K29" s="249"/>
-      <c r="L29" s="250"/>
+      <c r="C29" s="276"/>
+      <c r="D29" s="276"/>
+      <c r="E29" s="276"/>
+      <c r="F29" s="276"/>
+      <c r="G29" s="276"/>
+      <c r="H29" s="276"/>
+      <c r="I29" s="276"/>
+      <c r="J29" s="276"/>
+      <c r="K29" s="276"/>
+      <c r="L29" s="277"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="228">
         <v>4</v>
       </c>
-      <c r="B30" s="249" t="s">
+      <c r="B30" s="276" t="s">
         <v>341</v>
       </c>
-      <c r="C30" s="249"/>
-      <c r="D30" s="249"/>
-      <c r="E30" s="249"/>
-      <c r="F30" s="249"/>
-      <c r="G30" s="249"/>
-      <c r="H30" s="249"/>
-      <c r="I30" s="249"/>
-      <c r="J30" s="249"/>
-      <c r="K30" s="249"/>
-      <c r="L30" s="250"/>
+      <c r="C30" s="276"/>
+      <c r="D30" s="276"/>
+      <c r="E30" s="276"/>
+      <c r="F30" s="276"/>
+      <c r="G30" s="276"/>
+      <c r="H30" s="276"/>
+      <c r="I30" s="276"/>
+      <c r="J30" s="276"/>
+      <c r="K30" s="276"/>
+      <c r="L30" s="277"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="228">
         <v>5</v>
       </c>
-      <c r="B31" s="247" t="s">
+      <c r="B31" s="274" t="s">
         <v>323</v>
       </c>
-      <c r="C31" s="247"/>
-      <c r="D31" s="247"/>
-      <c r="E31" s="247"/>
-      <c r="F31" s="247"/>
-      <c r="G31" s="247"/>
-      <c r="H31" s="247"/>
-      <c r="I31" s="247"/>
-      <c r="J31" s="247"/>
-      <c r="K31" s="247"/>
-      <c r="L31" s="248"/>
+      <c r="C31" s="274"/>
+      <c r="D31" s="274"/>
+      <c r="E31" s="274"/>
+      <c r="F31" s="274"/>
+      <c r="G31" s="274"/>
+      <c r="H31" s="274"/>
+      <c r="I31" s="274"/>
+      <c r="J31" s="274"/>
+      <c r="K31" s="274"/>
+      <c r="L31" s="275"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="228">
         <v>6</v>
       </c>
-      <c r="B32" s="247" t="s">
+      <c r="B32" s="274" t="s">
         <v>328</v>
       </c>
-      <c r="C32" s="247"/>
-      <c r="D32" s="247"/>
-      <c r="E32" s="247"/>
-      <c r="F32" s="247"/>
-      <c r="G32" s="247"/>
-      <c r="H32" s="247"/>
-      <c r="I32" s="247"/>
-      <c r="J32" s="247"/>
-      <c r="K32" s="247"/>
-      <c r="L32" s="248"/>
+      <c r="C32" s="274"/>
+      <c r="D32" s="274"/>
+      <c r="E32" s="274"/>
+      <c r="F32" s="274"/>
+      <c r="G32" s="274"/>
+      <c r="H32" s="274"/>
+      <c r="I32" s="274"/>
+      <c r="J32" s="274"/>
+      <c r="K32" s="274"/>
+      <c r="L32" s="275"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="228">
         <v>7</v>
       </c>
-      <c r="B33" s="249" t="s">
+      <c r="B33" s="276" t="s">
         <v>324</v>
       </c>
-      <c r="C33" s="249"/>
-      <c r="D33" s="249"/>
-      <c r="E33" s="249"/>
-      <c r="F33" s="249"/>
-      <c r="G33" s="249"/>
-      <c r="H33" s="249"/>
-      <c r="I33" s="249"/>
-      <c r="J33" s="249"/>
-      <c r="K33" s="249"/>
-      <c r="L33" s="250"/>
+      <c r="C33" s="276"/>
+      <c r="D33" s="276"/>
+      <c r="E33" s="276"/>
+      <c r="F33" s="276"/>
+      <c r="G33" s="276"/>
+      <c r="H33" s="276"/>
+      <c r="I33" s="276"/>
+      <c r="J33" s="276"/>
+      <c r="K33" s="276"/>
+      <c r="L33" s="277"/>
     </row>
     <row r="34" spans="1:12" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="228"/>
@@ -15574,56 +15577,56 @@
       <c r="L34" s="230"/>
     </row>
     <row r="35" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="258" t="s">
+      <c r="A35" s="278" t="s">
         <v>327</v>
       </c>
-      <c r="B35" s="259"/>
-      <c r="C35" s="259"/>
-      <c r="D35" s="259"/>
-      <c r="E35" s="259"/>
-      <c r="F35" s="259"/>
-      <c r="G35" s="259"/>
-      <c r="H35" s="259"/>
-      <c r="I35" s="259"/>
-      <c r="J35" s="259"/>
-      <c r="K35" s="259"/>
-      <c r="L35" s="260"/>
+      <c r="B35" s="279"/>
+      <c r="C35" s="279"/>
+      <c r="D35" s="279"/>
+      <c r="E35" s="279"/>
+      <c r="F35" s="279"/>
+      <c r="G35" s="279"/>
+      <c r="H35" s="279"/>
+      <c r="I35" s="279"/>
+      <c r="J35" s="279"/>
+      <c r="K35" s="279"/>
+      <c r="L35" s="280"/>
     </row>
     <row r="36" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="231" t="s">
         <v>325</v>
       </c>
-      <c r="B36" s="249" t="s">
+      <c r="B36" s="276" t="s">
         <v>212</v>
       </c>
-      <c r="C36" s="249"/>
-      <c r="D36" s="249"/>
-      <c r="E36" s="249"/>
-      <c r="F36" s="249"/>
-      <c r="G36" s="249"/>
-      <c r="H36" s="249"/>
-      <c r="I36" s="249"/>
-      <c r="J36" s="249"/>
-      <c r="K36" s="249"/>
-      <c r="L36" s="250"/>
+      <c r="C36" s="276"/>
+      <c r="D36" s="276"/>
+      <c r="E36" s="276"/>
+      <c r="F36" s="276"/>
+      <c r="G36" s="276"/>
+      <c r="H36" s="276"/>
+      <c r="I36" s="276"/>
+      <c r="J36" s="276"/>
+      <c r="K36" s="276"/>
+      <c r="L36" s="277"/>
     </row>
     <row r="37" spans="1:12" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="232" t="s">
         <v>326</v>
       </c>
-      <c r="B37" s="251" t="s">
+      <c r="B37" s="282" t="s">
         <v>329</v>
       </c>
-      <c r="C37" s="251"/>
-      <c r="D37" s="251"/>
-      <c r="E37" s="251"/>
-      <c r="F37" s="251"/>
-      <c r="G37" s="251"/>
-      <c r="H37" s="251"/>
-      <c r="I37" s="251"/>
-      <c r="J37" s="251"/>
-      <c r="K37" s="251"/>
-      <c r="L37" s="252"/>
+      <c r="C37" s="282"/>
+      <c r="D37" s="282"/>
+      <c r="E37" s="282"/>
+      <c r="F37" s="282"/>
+      <c r="G37" s="282"/>
+      <c r="H37" s="282"/>
+      <c r="I37" s="282"/>
+      <c r="J37" s="282"/>
+      <c r="K37" s="282"/>
+      <c r="L37" s="283"/>
     </row>
     <row r="38" spans="1:12" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="160"/>
@@ -15640,20 +15643,20 @@
       <c r="L38" s="113"/>
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="253" t="s">
+      <c r="A39" s="284" t="s">
         <v>240</v>
       </c>
-      <c r="B39" s="254"/>
-      <c r="C39" s="254"/>
-      <c r="D39" s="254"/>
-      <c r="E39" s="254"/>
-      <c r="F39" s="254"/>
-      <c r="G39" s="254"/>
-      <c r="H39" s="254"/>
-      <c r="I39" s="254"/>
-      <c r="J39" s="254"/>
-      <c r="K39" s="254"/>
-      <c r="L39" s="255"/>
+      <c r="B39" s="285"/>
+      <c r="C39" s="285"/>
+      <c r="D39" s="285"/>
+      <c r="E39" s="285"/>
+      <c r="F39" s="285"/>
+      <c r="G39" s="285"/>
+      <c r="H39" s="285"/>
+      <c r="I39" s="285"/>
+      <c r="J39" s="285"/>
+      <c r="K39" s="285"/>
+      <c r="L39" s="286"/>
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="235" t="s">
@@ -15741,90 +15744,90 @@
       <c r="B45" s="168" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="256" t="s">
+      <c r="C45" s="264" t="s">
         <v>313</v>
       </c>
-      <c r="D45" s="256"/>
-      <c r="E45" s="256"/>
-      <c r="F45" s="256"/>
-      <c r="G45" s="256"/>
-      <c r="H45" s="256"/>
-      <c r="I45" s="256"/>
-      <c r="J45" s="256"/>
-      <c r="K45" s="256"/>
-      <c r="L45" s="257"/>
+      <c r="D45" s="264"/>
+      <c r="E45" s="264"/>
+      <c r="F45" s="264"/>
+      <c r="G45" s="264"/>
+      <c r="H45" s="264"/>
+      <c r="I45" s="264"/>
+      <c r="J45" s="264"/>
+      <c r="K45" s="264"/>
+      <c r="L45" s="265"/>
     </row>
     <row r="46" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="167"/>
       <c r="B46" s="168" t="s">
         <v>314</v>
       </c>
-      <c r="C46" s="256" t="s">
+      <c r="C46" s="264" t="s">
         <v>315</v>
       </c>
-      <c r="D46" s="256"/>
-      <c r="E46" s="256"/>
-      <c r="F46" s="256"/>
-      <c r="G46" s="256"/>
-      <c r="H46" s="256"/>
-      <c r="I46" s="256"/>
-      <c r="J46" s="256"/>
-      <c r="K46" s="256"/>
-      <c r="L46" s="257"/>
+      <c r="D46" s="264"/>
+      <c r="E46" s="264"/>
+      <c r="F46" s="264"/>
+      <c r="G46" s="264"/>
+      <c r="H46" s="264"/>
+      <c r="I46" s="264"/>
+      <c r="J46" s="264"/>
+      <c r="K46" s="264"/>
+      <c r="L46" s="265"/>
     </row>
     <row r="47" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="167"/>
       <c r="B47" s="168" t="s">
         <v>384</v>
       </c>
-      <c r="C47" s="256" t="s">
+      <c r="C47" s="264" t="s">
         <v>385</v>
       </c>
-      <c r="D47" s="256"/>
-      <c r="E47" s="256"/>
-      <c r="F47" s="256"/>
-      <c r="G47" s="256"/>
-      <c r="H47" s="256"/>
-      <c r="I47" s="256"/>
-      <c r="J47" s="256"/>
-      <c r="K47" s="256"/>
-      <c r="L47" s="257"/>
+      <c r="D47" s="264"/>
+      <c r="E47" s="264"/>
+      <c r="F47" s="264"/>
+      <c r="G47" s="264"/>
+      <c r="H47" s="264"/>
+      <c r="I47" s="264"/>
+      <c r="J47" s="264"/>
+      <c r="K47" s="264"/>
+      <c r="L47" s="265"/>
     </row>
     <row r="48" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="167"/>
       <c r="B48" s="168" t="s">
         <v>138</v>
       </c>
-      <c r="C48" s="256" t="s">
+      <c r="C48" s="264" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="256"/>
-      <c r="E48" s="256"/>
-      <c r="F48" s="256"/>
-      <c r="G48" s="256"/>
-      <c r="H48" s="256"/>
-      <c r="I48" s="256"/>
-      <c r="J48" s="256"/>
-      <c r="K48" s="256"/>
-      <c r="L48" s="257"/>
+      <c r="D48" s="264"/>
+      <c r="E48" s="264"/>
+      <c r="F48" s="264"/>
+      <c r="G48" s="264"/>
+      <c r="H48" s="264"/>
+      <c r="I48" s="264"/>
+      <c r="J48" s="264"/>
+      <c r="K48" s="264"/>
+      <c r="L48" s="265"/>
     </row>
     <row r="49" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="167"/>
       <c r="B49" s="168" t="s">
         <v>238</v>
       </c>
-      <c r="C49" s="256" t="s">
+      <c r="C49" s="264" t="s">
         <v>239</v>
       </c>
-      <c r="D49" s="256"/>
-      <c r="E49" s="256"/>
-      <c r="F49" s="256"/>
-      <c r="G49" s="256"/>
-      <c r="H49" s="256"/>
-      <c r="I49" s="256"/>
-      <c r="J49" s="256"/>
-      <c r="K49" s="256"/>
-      <c r="L49" s="257"/>
+      <c r="D49" s="264"/>
+      <c r="E49" s="264"/>
+      <c r="F49" s="264"/>
+      <c r="G49" s="264"/>
+      <c r="H49" s="264"/>
+      <c r="I49" s="264"/>
+      <c r="J49" s="264"/>
+      <c r="K49" s="264"/>
+      <c r="L49" s="265"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="167"/>
@@ -15849,18 +15852,18 @@
       <c r="B51" s="168" t="s">
         <v>63</v>
       </c>
-      <c r="C51" s="256" t="s">
+      <c r="C51" s="264" t="s">
         <v>317</v>
       </c>
-      <c r="D51" s="256"/>
-      <c r="E51" s="256"/>
-      <c r="F51" s="256"/>
-      <c r="G51" s="256"/>
-      <c r="H51" s="256"/>
-      <c r="I51" s="256"/>
-      <c r="J51" s="256"/>
-      <c r="K51" s="256"/>
-      <c r="L51" s="257"/>
+      <c r="D51" s="264"/>
+      <c r="E51" s="264"/>
+      <c r="F51" s="264"/>
+      <c r="G51" s="264"/>
+      <c r="H51" s="264"/>
+      <c r="I51" s="264"/>
+      <c r="J51" s="264"/>
+      <c r="K51" s="264"/>
+      <c r="L51" s="265"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="167"/>
@@ -15942,25 +15945,52 @@
       </c>
     </row>
     <row r="65" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="246" t="s">
+      <c r="A65" s="281" t="s">
         <v>356</v>
       </c>
-      <c r="B65" s="246"/>
-      <c r="C65" s="246"/>
-      <c r="D65" s="246"/>
-      <c r="E65" s="246"/>
-      <c r="F65" s="246"/>
-      <c r="G65" s="246"/>
-      <c r="H65" s="246"/>
-      <c r="I65" s="246"/>
-      <c r="J65" s="246"/>
-      <c r="K65" s="246"/>
-      <c r="L65" s="246"/>
+      <c r="B65" s="281"/>
+      <c r="C65" s="281"/>
+      <c r="D65" s="281"/>
+      <c r="E65" s="281"/>
+      <c r="F65" s="281"/>
+      <c r="G65" s="281"/>
+      <c r="H65" s="281"/>
+      <c r="I65" s="281"/>
+      <c r="J65" s="281"/>
+      <c r="K65" s="281"/>
+      <c r="L65" s="281"/>
     </row>
     <row r="70" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="71" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="A65:L65"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="C45:L45"/>
+    <mergeCell ref="C48:L48"/>
+    <mergeCell ref="C49:L49"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="C51:L51"/>
+    <mergeCell ref="A35:L35"/>
+    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B18:L18"/>
+    <mergeCell ref="B19:L19"/>
+    <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="B22:L22"/>
+    <mergeCell ref="B23:L23"/>
+    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="B26:L26"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B30:L30"/>
     <mergeCell ref="A17:L17"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A4:L4"/>
@@ -15975,33 +16005,6 @@
     <mergeCell ref="A16:L16"/>
     <mergeCell ref="B7:L7"/>
     <mergeCell ref="B8:L8"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B18:L18"/>
-    <mergeCell ref="B19:L19"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="B22:L22"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="B24:L24"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="B26:L26"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="A65:L65"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="C45:L45"/>
-    <mergeCell ref="C48:L48"/>
-    <mergeCell ref="C49:L49"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="C51:L51"/>
-    <mergeCell ref="A35:L35"/>
-    <mergeCell ref="C47:L47"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A58" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -31595,8 +31598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BF7D8F-86F3-47E9-AB85-EE9B4CAB70E4}">
   <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31939,7 +31942,7 @@
       <c r="D25" s="111"/>
       <c r="E25" s="28"/>
       <c r="N25" s="141" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
@@ -36356,6 +36359,8 @@
     <hyperlink ref="N101" r:id="rId54" location="vi-end-of-year-balance" xr:uid="{64582986-19BE-4DA6-A576-9ED7048A63F6}"/>
     <hyperlink ref="N98" r:id="rId55" location="iii-net-trade-volume-all-participants" xr:uid="{00DE0E22-6C57-4CFB-AC1B-701E93DC729D}"/>
     <hyperlink ref="N12" r:id="rId56" location="1a-explain-cell-types" xr:uid="{5E0F137C-003B-4215-AD3B-C722FAB0B485}"/>
+    <hyperlink ref="N24" r:id="rId57" location="vii-percent-of-tribal-nation-water-in-california" xr:uid="{01F1D035-6ABB-47DA-9902-C2811F877041}"/>
+    <hyperlink ref="N25" r:id="rId58" location="vii-percent-of-tribal-nation-water-in-arizona" xr:uid="{B1DD0B97-92EB-4086-A5FA-F5A6D9250A94}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -38051,16 +38056,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="322" t="e">
+      <c r="A1" s="321" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="322"/>
-      <c r="C1" s="322"/>
-      <c r="D1" s="322"/>
-      <c r="E1" s="322"/>
-      <c r="F1" s="322"/>
-      <c r="G1" s="322"/>
+      <c r="B1" s="321"/>
+      <c r="C1" s="321"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -38169,11 +38174,11 @@
         <v>80</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="321"/>
-      <c r="D10" s="321"/>
-      <c r="E10" s="321"/>
-      <c r="F10" s="321"/>
-      <c r="G10" s="321"/>
+      <c r="C10" s="322"/>
+      <c r="D10" s="322"/>
+      <c r="E10" s="322"/>
+      <c r="F10" s="322"/>
+      <c r="G10" s="322"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -39436,12 +39441,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -39449,6 +39448,12 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>

</xml_diff>

<commit_message>
Update hotlinks to Tribal parameter split.
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E718FE9-D6B9-43F2-84DD-C4936CA9C329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8439995-8058-40D6-A50A-C725CFA561FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="62" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="391">
   <si>
     <t>Year 1</t>
   </si>
@@ -2017,6 +2017,12 @@
   <si>
     <t>Help percent of Tribal Nation water in AZ</t>
   </si>
+  <si>
+    <t>1.4.1</t>
+  </si>
+  <si>
+    <t>Document Tribal parameter in Users Guide</t>
+  </si>
 </sst>
 </file>
 
@@ -3314,6 +3320,51 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3368,12 +3419,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3397,45 +3442,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3539,11 +3545,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -14963,7 +14969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EA02F4-5F19-409C-8BC6-A0D8FEB3A90D}">
   <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
@@ -14983,20 +14989,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="249" t="s">
+      <c r="A1" s="264" t="s">
         <v>351</v>
       </c>
-      <c r="B1" s="249"/>
-      <c r="C1" s="249"/>
-      <c r="D1" s="249"/>
-      <c r="E1" s="249"/>
-      <c r="F1" s="249"/>
-      <c r="G1" s="249"/>
-      <c r="H1" s="249"/>
-      <c r="I1" s="249"/>
-      <c r="J1" s="249"/>
-      <c r="K1" s="249"/>
-      <c r="L1" s="249"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="264"/>
+      <c r="J1" s="264"/>
+      <c r="K1" s="264"/>
+      <c r="L1" s="264"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -15022,41 +15028,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="250" t="s">
+      <c r="A4" s="265" t="s">
         <v>352</v>
       </c>
-      <c r="B4" s="251"/>
-      <c r="C4" s="251"/>
-      <c r="D4" s="251"/>
-      <c r="E4" s="251"/>
-      <c r="F4" s="251"/>
-      <c r="G4" s="251"/>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="252"/>
-      <c r="N4" s="253"/>
-      <c r="O4" s="253"/>
-      <c r="P4" s="253"/>
-      <c r="Q4" s="253"/>
-      <c r="R4" s="253"/>
+      <c r="B4" s="266"/>
+      <c r="C4" s="266"/>
+      <c r="D4" s="266"/>
+      <c r="E4" s="266"/>
+      <c r="F4" s="266"/>
+      <c r="G4" s="266"/>
+      <c r="H4" s="266"/>
+      <c r="I4" s="266"/>
+      <c r="J4" s="266"/>
+      <c r="K4" s="266"/>
+      <c r="L4" s="267"/>
+      <c r="N4" s="268"/>
+      <c r="O4" s="268"/>
+      <c r="P4" s="268"/>
+      <c r="Q4" s="268"/>
+      <c r="R4" s="268"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="254" t="s">
+      <c r="A5" s="269" t="s">
         <v>335</v>
       </c>
-      <c r="B5" s="255"/>
-      <c r="C5" s="255"/>
-      <c r="D5" s="255"/>
-      <c r="E5" s="255"/>
-      <c r="F5" s="255"/>
-      <c r="G5" s="255"/>
-      <c r="H5" s="255"/>
-      <c r="I5" s="255"/>
-      <c r="J5" s="255"/>
-      <c r="K5" s="255"/>
-      <c r="L5" s="256"/>
+      <c r="B5" s="270"/>
+      <c r="C5" s="270"/>
+      <c r="D5" s="270"/>
+      <c r="E5" s="270"/>
+      <c r="F5" s="270"/>
+      <c r="G5" s="270"/>
+      <c r="H5" s="270"/>
+      <c r="I5" s="270"/>
+      <c r="J5" s="270"/>
+      <c r="K5" s="270"/>
+      <c r="L5" s="271"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15064,20 +15070,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="254" t="s">
+      <c r="A6" s="269" t="s">
         <v>353</v>
       </c>
-      <c r="B6" s="255"/>
-      <c r="C6" s="255"/>
-      <c r="D6" s="255"/>
-      <c r="E6" s="255"/>
-      <c r="F6" s="255"/>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="255"/>
-      <c r="J6" s="255"/>
-      <c r="K6" s="255"/>
-      <c r="L6" s="256"/>
+      <c r="B6" s="270"/>
+      <c r="C6" s="270"/>
+      <c r="D6" s="270"/>
+      <c r="E6" s="270"/>
+      <c r="F6" s="270"/>
+      <c r="G6" s="270"/>
+      <c r="H6" s="270"/>
+      <c r="I6" s="270"/>
+      <c r="J6" s="270"/>
+      <c r="K6" s="270"/>
+      <c r="L6" s="271"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15086,19 +15092,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="233"/>
-      <c r="B7" s="255" t="s">
+      <c r="B7" s="270" t="s">
         <v>354</v>
       </c>
-      <c r="C7" s="255"/>
-      <c r="D7" s="255"/>
-      <c r="E7" s="255"/>
-      <c r="F7" s="255"/>
-      <c r="G7" s="255"/>
-      <c r="H7" s="255"/>
-      <c r="I7" s="255"/>
-      <c r="J7" s="255"/>
-      <c r="K7" s="255"/>
-      <c r="L7" s="256"/>
+      <c r="C7" s="270"/>
+      <c r="D7" s="270"/>
+      <c r="E7" s="270"/>
+      <c r="F7" s="270"/>
+      <c r="G7" s="270"/>
+      <c r="H7" s="270"/>
+      <c r="I7" s="270"/>
+      <c r="J7" s="270"/>
+      <c r="K7" s="270"/>
+      <c r="L7" s="271"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15107,19 +15113,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="234"/>
-      <c r="B8" s="272" t="s">
+      <c r="B8" s="285" t="s">
         <v>355</v>
       </c>
-      <c r="C8" s="272"/>
-      <c r="D8" s="272"/>
-      <c r="E8" s="272"/>
-      <c r="F8" s="272"/>
-      <c r="G8" s="272"/>
-      <c r="H8" s="272"/>
-      <c r="I8" s="272"/>
-      <c r="J8" s="272"/>
-      <c r="K8" s="272"/>
-      <c r="L8" s="273"/>
+      <c r="C8" s="285"/>
+      <c r="D8" s="285"/>
+      <c r="E8" s="285"/>
+      <c r="F8" s="285"/>
+      <c r="G8" s="285"/>
+      <c r="H8" s="285"/>
+      <c r="I8" s="285"/>
+      <c r="J8" s="285"/>
+      <c r="K8" s="285"/>
+      <c r="L8" s="286"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15141,84 +15147,84 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="257" t="s">
+      <c r="A10" s="272" t="s">
         <v>205</v>
       </c>
-      <c r="B10" s="258"/>
-      <c r="C10" s="258"/>
-      <c r="D10" s="258"/>
-      <c r="E10" s="258"/>
-      <c r="F10" s="258"/>
-      <c r="G10" s="258"/>
-      <c r="H10" s="258"/>
-      <c r="I10" s="258"/>
-      <c r="J10" s="258"/>
-      <c r="K10" s="258"/>
-      <c r="L10" s="259"/>
+      <c r="B10" s="273"/>
+      <c r="C10" s="273"/>
+      <c r="D10" s="273"/>
+      <c r="E10" s="273"/>
+      <c r="F10" s="273"/>
+      <c r="G10" s="273"/>
+      <c r="H10" s="273"/>
+      <c r="I10" s="273"/>
+      <c r="J10" s="273"/>
+      <c r="K10" s="273"/>
+      <c r="L10" s="274"/>
     </row>
     <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="260" t="s">
+      <c r="A11" s="275" t="s">
         <v>336</v>
       </c>
-      <c r="B11" s="261"/>
-      <c r="C11" s="261"/>
-      <c r="D11" s="261"/>
-      <c r="E11" s="261"/>
-      <c r="F11" s="261"/>
-      <c r="G11" s="261"/>
-      <c r="H11" s="261"/>
-      <c r="I11" s="261"/>
-      <c r="J11" s="261"/>
-      <c r="K11" s="261"/>
-      <c r="L11" s="262"/>
+      <c r="B11" s="276"/>
+      <c r="C11" s="276"/>
+      <c r="D11" s="276"/>
+      <c r="E11" s="276"/>
+      <c r="F11" s="276"/>
+      <c r="G11" s="276"/>
+      <c r="H11" s="276"/>
+      <c r="I11" s="276"/>
+      <c r="J11" s="276"/>
+      <c r="K11" s="276"/>
+      <c r="L11" s="277"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="263" t="s">
+      <c r="A12" s="278" t="s">
         <v>337</v>
       </c>
-      <c r="B12" s="264"/>
-      <c r="C12" s="264"/>
-      <c r="D12" s="264"/>
-      <c r="E12" s="264"/>
-      <c r="F12" s="264"/>
-      <c r="G12" s="264"/>
-      <c r="H12" s="264"/>
-      <c r="I12" s="264"/>
-      <c r="J12" s="264"/>
-      <c r="K12" s="264"/>
-      <c r="L12" s="265"/>
+      <c r="B12" s="256"/>
+      <c r="C12" s="256"/>
+      <c r="D12" s="256"/>
+      <c r="E12" s="256"/>
+      <c r="F12" s="256"/>
+      <c r="G12" s="256"/>
+      <c r="H12" s="256"/>
+      <c r="I12" s="256"/>
+      <c r="J12" s="256"/>
+      <c r="K12" s="256"/>
+      <c r="L12" s="257"/>
     </row>
     <row r="13" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="263" t="s">
+      <c r="A13" s="278" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="264"/>
-      <c r="C13" s="264"/>
-      <c r="D13" s="264"/>
-      <c r="E13" s="264"/>
-      <c r="F13" s="264"/>
-      <c r="G13" s="264"/>
-      <c r="H13" s="264"/>
-      <c r="I13" s="264"/>
-      <c r="J13" s="264"/>
-      <c r="K13" s="264"/>
-      <c r="L13" s="265"/>
+      <c r="B13" s="256"/>
+      <c r="C13" s="256"/>
+      <c r="D13" s="256"/>
+      <c r="E13" s="256"/>
+      <c r="F13" s="256"/>
+      <c r="G13" s="256"/>
+      <c r="H13" s="256"/>
+      <c r="I13" s="256"/>
+      <c r="J13" s="256"/>
+      <c r="K13" s="256"/>
+      <c r="L13" s="257"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="266" t="s">
+      <c r="A14" s="279" t="s">
         <v>338</v>
       </c>
-      <c r="B14" s="267"/>
-      <c r="C14" s="267"/>
-      <c r="D14" s="267"/>
-      <c r="E14" s="267"/>
-      <c r="F14" s="267"/>
-      <c r="G14" s="267"/>
-      <c r="H14" s="267"/>
-      <c r="I14" s="267"/>
-      <c r="J14" s="267"/>
-      <c r="K14" s="267"/>
-      <c r="L14" s="268"/>
+      <c r="B14" s="280"/>
+      <c r="C14" s="280"/>
+      <c r="D14" s="280"/>
+      <c r="E14" s="280"/>
+      <c r="F14" s="280"/>
+      <c r="G14" s="280"/>
+      <c r="H14" s="280"/>
+      <c r="I14" s="280"/>
+      <c r="J14" s="280"/>
+      <c r="K14" s="280"/>
+      <c r="L14" s="281"/>
     </row>
     <row r="15" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="113"/>
@@ -15235,332 +15241,332 @@
       <c r="L15" s="113"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="269" t="s">
+      <c r="A16" s="282" t="s">
         <v>334</v>
       </c>
-      <c r="B16" s="270"/>
-      <c r="C16" s="270"/>
-      <c r="D16" s="270"/>
-      <c r="E16" s="270"/>
-      <c r="F16" s="270"/>
-      <c r="G16" s="270"/>
-      <c r="H16" s="270"/>
-      <c r="I16" s="270"/>
-      <c r="J16" s="270"/>
-      <c r="K16" s="270"/>
-      <c r="L16" s="271"/>
+      <c r="B16" s="283"/>
+      <c r="C16" s="283"/>
+      <c r="D16" s="283"/>
+      <c r="E16" s="283"/>
+      <c r="F16" s="283"/>
+      <c r="G16" s="283"/>
+      <c r="H16" s="283"/>
+      <c r="I16" s="283"/>
+      <c r="J16" s="283"/>
+      <c r="K16" s="283"/>
+      <c r="L16" s="284"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="246" t="s">
+      <c r="A17" s="261" t="s">
         <v>215</v>
       </c>
-      <c r="B17" s="247"/>
-      <c r="C17" s="247"/>
-      <c r="D17" s="247"/>
-      <c r="E17" s="247"/>
-      <c r="F17" s="247"/>
-      <c r="G17" s="247"/>
-      <c r="H17" s="247"/>
-      <c r="I17" s="247"/>
-      <c r="J17" s="247"/>
-      <c r="K17" s="247"/>
-      <c r="L17" s="248"/>
+      <c r="B17" s="262"/>
+      <c r="C17" s="262"/>
+      <c r="D17" s="262"/>
+      <c r="E17" s="262"/>
+      <c r="F17" s="262"/>
+      <c r="G17" s="262"/>
+      <c r="H17" s="262"/>
+      <c r="I17" s="262"/>
+      <c r="J17" s="262"/>
+      <c r="K17" s="262"/>
+      <c r="L17" s="263"/>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="228">
         <v>1</v>
       </c>
-      <c r="B18" s="276" t="s">
+      <c r="B18" s="249" t="s">
         <v>214</v>
       </c>
-      <c r="C18" s="276"/>
-      <c r="D18" s="276"/>
-      <c r="E18" s="276"/>
-      <c r="F18" s="276"/>
-      <c r="G18" s="276"/>
-      <c r="H18" s="276"/>
-      <c r="I18" s="276"/>
-      <c r="J18" s="276"/>
-      <c r="K18" s="276"/>
-      <c r="L18" s="277"/>
+      <c r="C18" s="249"/>
+      <c r="D18" s="249"/>
+      <c r="E18" s="249"/>
+      <c r="F18" s="249"/>
+      <c r="G18" s="249"/>
+      <c r="H18" s="249"/>
+      <c r="I18" s="249"/>
+      <c r="J18" s="249"/>
+      <c r="K18" s="249"/>
+      <c r="L18" s="250"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="228">
         <v>2</v>
       </c>
-      <c r="B19" s="276" t="s">
+      <c r="B19" s="249" t="s">
         <v>330</v>
       </c>
-      <c r="C19" s="276"/>
-      <c r="D19" s="276"/>
-      <c r="E19" s="276"/>
-      <c r="F19" s="276"/>
-      <c r="G19" s="276"/>
-      <c r="H19" s="276"/>
-      <c r="I19" s="276"/>
-      <c r="J19" s="276"/>
-      <c r="K19" s="276"/>
-      <c r="L19" s="277"/>
+      <c r="C19" s="249"/>
+      <c r="D19" s="249"/>
+      <c r="E19" s="249"/>
+      <c r="F19" s="249"/>
+      <c r="G19" s="249"/>
+      <c r="H19" s="249"/>
+      <c r="I19" s="249"/>
+      <c r="J19" s="249"/>
+      <c r="K19" s="249"/>
+      <c r="L19" s="250"/>
       <c r="N19" s="106"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="228">
         <v>3</v>
       </c>
-      <c r="B20" s="276" t="s">
+      <c r="B20" s="249" t="s">
         <v>207</v>
       </c>
-      <c r="C20" s="276"/>
-      <c r="D20" s="276"/>
-      <c r="E20" s="276"/>
-      <c r="F20" s="276"/>
-      <c r="G20" s="276"/>
-      <c r="H20" s="276"/>
-      <c r="I20" s="276"/>
-      <c r="J20" s="276"/>
-      <c r="K20" s="276"/>
-      <c r="L20" s="277"/>
+      <c r="C20" s="249"/>
+      <c r="D20" s="249"/>
+      <c r="E20" s="249"/>
+      <c r="F20" s="249"/>
+      <c r="G20" s="249"/>
+      <c r="H20" s="249"/>
+      <c r="I20" s="249"/>
+      <c r="J20" s="249"/>
+      <c r="K20" s="249"/>
+      <c r="L20" s="250"/>
       <c r="N20" s="106"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="228">
         <v>4</v>
       </c>
-      <c r="B21" s="276" t="s">
+      <c r="B21" s="249" t="s">
         <v>339</v>
       </c>
-      <c r="C21" s="276"/>
-      <c r="D21" s="276"/>
-      <c r="E21" s="276"/>
-      <c r="F21" s="276"/>
-      <c r="G21" s="276"/>
-      <c r="H21" s="276"/>
-      <c r="I21" s="276"/>
-      <c r="J21" s="276"/>
-      <c r="K21" s="276"/>
-      <c r="L21" s="277"/>
+      <c r="C21" s="249"/>
+      <c r="D21" s="249"/>
+      <c r="E21" s="249"/>
+      <c r="F21" s="249"/>
+      <c r="G21" s="249"/>
+      <c r="H21" s="249"/>
+      <c r="I21" s="249"/>
+      <c r="J21" s="249"/>
+      <c r="K21" s="249"/>
+      <c r="L21" s="250"/>
       <c r="N21" s="106"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="228">
         <v>5</v>
       </c>
-      <c r="B22" s="276" t="s">
+      <c r="B22" s="249" t="s">
         <v>208</v>
       </c>
-      <c r="C22" s="276"/>
-      <c r="D22" s="276"/>
-      <c r="E22" s="276"/>
-      <c r="F22" s="276"/>
-      <c r="G22" s="276"/>
-      <c r="H22" s="276"/>
-      <c r="I22" s="276"/>
-      <c r="J22" s="276"/>
-      <c r="K22" s="276"/>
-      <c r="L22" s="277"/>
+      <c r="C22" s="249"/>
+      <c r="D22" s="249"/>
+      <c r="E22" s="249"/>
+      <c r="F22" s="249"/>
+      <c r="G22" s="249"/>
+      <c r="H22" s="249"/>
+      <c r="I22" s="249"/>
+      <c r="J22" s="249"/>
+      <c r="K22" s="249"/>
+      <c r="L22" s="250"/>
       <c r="N22" s="106"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="228"/>
-      <c r="B23" s="276" t="s">
+      <c r="B23" s="249" t="s">
         <v>209</v>
       </c>
-      <c r="C23" s="276"/>
-      <c r="D23" s="276"/>
-      <c r="E23" s="276"/>
-      <c r="F23" s="276"/>
-      <c r="G23" s="276"/>
-      <c r="H23" s="276"/>
-      <c r="I23" s="276"/>
-      <c r="J23" s="276"/>
-      <c r="K23" s="276"/>
-      <c r="L23" s="277"/>
+      <c r="C23" s="249"/>
+      <c r="D23" s="249"/>
+      <c r="E23" s="249"/>
+      <c r="F23" s="249"/>
+      <c r="G23" s="249"/>
+      <c r="H23" s="249"/>
+      <c r="I23" s="249"/>
+      <c r="J23" s="249"/>
+      <c r="K23" s="249"/>
+      <c r="L23" s="250"/>
       <c r="N23" s="106"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="228"/>
-      <c r="B24" s="276" t="s">
+      <c r="B24" s="249" t="s">
         <v>210</v>
       </c>
-      <c r="C24" s="276"/>
-      <c r="D24" s="276"/>
-      <c r="E24" s="276"/>
-      <c r="F24" s="276"/>
-      <c r="G24" s="276"/>
-      <c r="H24" s="276"/>
-      <c r="I24" s="276"/>
-      <c r="J24" s="276"/>
-      <c r="K24" s="276"/>
-      <c r="L24" s="277"/>
+      <c r="C24" s="249"/>
+      <c r="D24" s="249"/>
+      <c r="E24" s="249"/>
+      <c r="F24" s="249"/>
+      <c r="G24" s="249"/>
+      <c r="H24" s="249"/>
+      <c r="I24" s="249"/>
+      <c r="J24" s="249"/>
+      <c r="K24" s="249"/>
+      <c r="L24" s="250"/>
       <c r="N24" s="106"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="278" t="s">
+      <c r="A25" s="258" t="s">
         <v>216</v>
       </c>
-      <c r="B25" s="279"/>
-      <c r="C25" s="279"/>
-      <c r="D25" s="279"/>
-      <c r="E25" s="279"/>
-      <c r="F25" s="279"/>
-      <c r="G25" s="279"/>
-      <c r="H25" s="279"/>
-      <c r="I25" s="279"/>
-      <c r="J25" s="279"/>
-      <c r="K25" s="279"/>
-      <c r="L25" s="280"/>
+      <c r="B25" s="259"/>
+      <c r="C25" s="259"/>
+      <c r="D25" s="259"/>
+      <c r="E25" s="259"/>
+      <c r="F25" s="259"/>
+      <c r="G25" s="259"/>
+      <c r="H25" s="259"/>
+      <c r="I25" s="259"/>
+      <c r="J25" s="259"/>
+      <c r="K25" s="259"/>
+      <c r="L25" s="260"/>
       <c r="N25" s="106"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="228">
         <v>1</v>
       </c>
-      <c r="B26" s="276" t="s">
+      <c r="B26" s="249" t="s">
         <v>211</v>
       </c>
-      <c r="C26" s="276"/>
-      <c r="D26" s="276"/>
-      <c r="E26" s="276"/>
-      <c r="F26" s="276"/>
-      <c r="G26" s="276"/>
-      <c r="H26" s="276"/>
-      <c r="I26" s="276"/>
-      <c r="J26" s="276"/>
-      <c r="K26" s="276"/>
-      <c r="L26" s="277"/>
+      <c r="C26" s="249"/>
+      <c r="D26" s="249"/>
+      <c r="E26" s="249"/>
+      <c r="F26" s="249"/>
+      <c r="G26" s="249"/>
+      <c r="H26" s="249"/>
+      <c r="I26" s="249"/>
+      <c r="J26" s="249"/>
+      <c r="K26" s="249"/>
+      <c r="L26" s="250"/>
       <c r="N26" s="106"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="228"/>
-      <c r="B27" s="274" t="s">
+      <c r="B27" s="247" t="s">
         <v>340</v>
       </c>
-      <c r="C27" s="274"/>
-      <c r="D27" s="274"/>
-      <c r="E27" s="274"/>
-      <c r="F27" s="274"/>
-      <c r="G27" s="274"/>
-      <c r="H27" s="274"/>
-      <c r="I27" s="274"/>
-      <c r="J27" s="274"/>
-      <c r="K27" s="274"/>
-      <c r="L27" s="275"/>
+      <c r="C27" s="247"/>
+      <c r="D27" s="247"/>
+      <c r="E27" s="247"/>
+      <c r="F27" s="247"/>
+      <c r="G27" s="247"/>
+      <c r="H27" s="247"/>
+      <c r="I27" s="247"/>
+      <c r="J27" s="247"/>
+      <c r="K27" s="247"/>
+      <c r="L27" s="248"/>
       <c r="N27" s="106"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="228">
         <v>2</v>
       </c>
-      <c r="B28" s="276" t="s">
+      <c r="B28" s="249" t="s">
         <v>333</v>
       </c>
-      <c r="C28" s="276"/>
-      <c r="D28" s="276"/>
-      <c r="E28" s="276"/>
-      <c r="F28" s="276"/>
-      <c r="G28" s="276"/>
-      <c r="H28" s="276"/>
-      <c r="I28" s="276"/>
-      <c r="J28" s="276"/>
-      <c r="K28" s="276"/>
-      <c r="L28" s="277"/>
+      <c r="C28" s="249"/>
+      <c r="D28" s="249"/>
+      <c r="E28" s="249"/>
+      <c r="F28" s="249"/>
+      <c r="G28" s="249"/>
+      <c r="H28" s="249"/>
+      <c r="I28" s="249"/>
+      <c r="J28" s="249"/>
+      <c r="K28" s="249"/>
+      <c r="L28" s="250"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="228">
         <v>3</v>
       </c>
-      <c r="B29" s="276" t="s">
+      <c r="B29" s="249" t="s">
         <v>322</v>
       </c>
-      <c r="C29" s="276"/>
-      <c r="D29" s="276"/>
-      <c r="E29" s="276"/>
-      <c r="F29" s="276"/>
-      <c r="G29" s="276"/>
-      <c r="H29" s="276"/>
-      <c r="I29" s="276"/>
-      <c r="J29" s="276"/>
-      <c r="K29" s="276"/>
-      <c r="L29" s="277"/>
+      <c r="C29" s="249"/>
+      <c r="D29" s="249"/>
+      <c r="E29" s="249"/>
+      <c r="F29" s="249"/>
+      <c r="G29" s="249"/>
+      <c r="H29" s="249"/>
+      <c r="I29" s="249"/>
+      <c r="J29" s="249"/>
+      <c r="K29" s="249"/>
+      <c r="L29" s="250"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="228">
         <v>4</v>
       </c>
-      <c r="B30" s="276" t="s">
+      <c r="B30" s="249" t="s">
         <v>341</v>
       </c>
-      <c r="C30" s="276"/>
-      <c r="D30" s="276"/>
-      <c r="E30" s="276"/>
-      <c r="F30" s="276"/>
-      <c r="G30" s="276"/>
-      <c r="H30" s="276"/>
-      <c r="I30" s="276"/>
-      <c r="J30" s="276"/>
-      <c r="K30" s="276"/>
-      <c r="L30" s="277"/>
+      <c r="C30" s="249"/>
+      <c r="D30" s="249"/>
+      <c r="E30" s="249"/>
+      <c r="F30" s="249"/>
+      <c r="G30" s="249"/>
+      <c r="H30" s="249"/>
+      <c r="I30" s="249"/>
+      <c r="J30" s="249"/>
+      <c r="K30" s="249"/>
+      <c r="L30" s="250"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="228">
         <v>5</v>
       </c>
-      <c r="B31" s="274" t="s">
+      <c r="B31" s="247" t="s">
         <v>323</v>
       </c>
-      <c r="C31" s="274"/>
-      <c r="D31" s="274"/>
-      <c r="E31" s="274"/>
-      <c r="F31" s="274"/>
-      <c r="G31" s="274"/>
-      <c r="H31" s="274"/>
-      <c r="I31" s="274"/>
-      <c r="J31" s="274"/>
-      <c r="K31" s="274"/>
-      <c r="L31" s="275"/>
+      <c r="C31" s="247"/>
+      <c r="D31" s="247"/>
+      <c r="E31" s="247"/>
+      <c r="F31" s="247"/>
+      <c r="G31" s="247"/>
+      <c r="H31" s="247"/>
+      <c r="I31" s="247"/>
+      <c r="J31" s="247"/>
+      <c r="K31" s="247"/>
+      <c r="L31" s="248"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="228">
         <v>6</v>
       </c>
-      <c r="B32" s="274" t="s">
+      <c r="B32" s="247" t="s">
         <v>328</v>
       </c>
-      <c r="C32" s="274"/>
-      <c r="D32" s="274"/>
-      <c r="E32" s="274"/>
-      <c r="F32" s="274"/>
-      <c r="G32" s="274"/>
-      <c r="H32" s="274"/>
-      <c r="I32" s="274"/>
-      <c r="J32" s="274"/>
-      <c r="K32" s="274"/>
-      <c r="L32" s="275"/>
+      <c r="C32" s="247"/>
+      <c r="D32" s="247"/>
+      <c r="E32" s="247"/>
+      <c r="F32" s="247"/>
+      <c r="G32" s="247"/>
+      <c r="H32" s="247"/>
+      <c r="I32" s="247"/>
+      <c r="J32" s="247"/>
+      <c r="K32" s="247"/>
+      <c r="L32" s="248"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="228">
         <v>7</v>
       </c>
-      <c r="B33" s="276" t="s">
+      <c r="B33" s="249" t="s">
         <v>324</v>
       </c>
-      <c r="C33" s="276"/>
-      <c r="D33" s="276"/>
-      <c r="E33" s="276"/>
-      <c r="F33" s="276"/>
-      <c r="G33" s="276"/>
-      <c r="H33" s="276"/>
-      <c r="I33" s="276"/>
-      <c r="J33" s="276"/>
-      <c r="K33" s="276"/>
-      <c r="L33" s="277"/>
+      <c r="C33" s="249"/>
+      <c r="D33" s="249"/>
+      <c r="E33" s="249"/>
+      <c r="F33" s="249"/>
+      <c r="G33" s="249"/>
+      <c r="H33" s="249"/>
+      <c r="I33" s="249"/>
+      <c r="J33" s="249"/>
+      <c r="K33" s="249"/>
+      <c r="L33" s="250"/>
     </row>
     <row r="34" spans="1:12" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="228"/>
@@ -15577,56 +15583,56 @@
       <c r="L34" s="230"/>
     </row>
     <row r="35" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="278" t="s">
+      <c r="A35" s="258" t="s">
         <v>327</v>
       </c>
-      <c r="B35" s="279"/>
-      <c r="C35" s="279"/>
-      <c r="D35" s="279"/>
-      <c r="E35" s="279"/>
-      <c r="F35" s="279"/>
-      <c r="G35" s="279"/>
-      <c r="H35" s="279"/>
-      <c r="I35" s="279"/>
-      <c r="J35" s="279"/>
-      <c r="K35" s="279"/>
-      <c r="L35" s="280"/>
+      <c r="B35" s="259"/>
+      <c r="C35" s="259"/>
+      <c r="D35" s="259"/>
+      <c r="E35" s="259"/>
+      <c r="F35" s="259"/>
+      <c r="G35" s="259"/>
+      <c r="H35" s="259"/>
+      <c r="I35" s="259"/>
+      <c r="J35" s="259"/>
+      <c r="K35" s="259"/>
+      <c r="L35" s="260"/>
     </row>
     <row r="36" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="231" t="s">
         <v>325</v>
       </c>
-      <c r="B36" s="276" t="s">
+      <c r="B36" s="249" t="s">
         <v>212</v>
       </c>
-      <c r="C36" s="276"/>
-      <c r="D36" s="276"/>
-      <c r="E36" s="276"/>
-      <c r="F36" s="276"/>
-      <c r="G36" s="276"/>
-      <c r="H36" s="276"/>
-      <c r="I36" s="276"/>
-      <c r="J36" s="276"/>
-      <c r="K36" s="276"/>
-      <c r="L36" s="277"/>
+      <c r="C36" s="249"/>
+      <c r="D36" s="249"/>
+      <c r="E36" s="249"/>
+      <c r="F36" s="249"/>
+      <c r="G36" s="249"/>
+      <c r="H36" s="249"/>
+      <c r="I36" s="249"/>
+      <c r="J36" s="249"/>
+      <c r="K36" s="249"/>
+      <c r="L36" s="250"/>
     </row>
     <row r="37" spans="1:12" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="232" t="s">
         <v>326</v>
       </c>
-      <c r="B37" s="282" t="s">
+      <c r="B37" s="251" t="s">
         <v>329</v>
       </c>
-      <c r="C37" s="282"/>
-      <c r="D37" s="282"/>
-      <c r="E37" s="282"/>
-      <c r="F37" s="282"/>
-      <c r="G37" s="282"/>
-      <c r="H37" s="282"/>
-      <c r="I37" s="282"/>
-      <c r="J37" s="282"/>
-      <c r="K37" s="282"/>
-      <c r="L37" s="283"/>
+      <c r="C37" s="251"/>
+      <c r="D37" s="251"/>
+      <c r="E37" s="251"/>
+      <c r="F37" s="251"/>
+      <c r="G37" s="251"/>
+      <c r="H37" s="251"/>
+      <c r="I37" s="251"/>
+      <c r="J37" s="251"/>
+      <c r="K37" s="251"/>
+      <c r="L37" s="252"/>
     </row>
     <row r="38" spans="1:12" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="160"/>
@@ -15643,20 +15649,20 @@
       <c r="L38" s="113"/>
     </row>
     <row r="39" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="284" t="s">
+      <c r="A39" s="253" t="s">
         <v>240</v>
       </c>
-      <c r="B39" s="285"/>
-      <c r="C39" s="285"/>
-      <c r="D39" s="285"/>
-      <c r="E39" s="285"/>
-      <c r="F39" s="285"/>
-      <c r="G39" s="285"/>
-      <c r="H39" s="285"/>
-      <c r="I39" s="285"/>
-      <c r="J39" s="285"/>
-      <c r="K39" s="285"/>
-      <c r="L39" s="286"/>
+      <c r="B39" s="254"/>
+      <c r="C39" s="254"/>
+      <c r="D39" s="254"/>
+      <c r="E39" s="254"/>
+      <c r="F39" s="254"/>
+      <c r="G39" s="254"/>
+      <c r="H39" s="254"/>
+      <c r="I39" s="254"/>
+      <c r="J39" s="254"/>
+      <c r="K39" s="254"/>
+      <c r="L39" s="255"/>
     </row>
     <row r="40" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="235" t="s">
@@ -15744,90 +15750,90 @@
       <c r="B45" s="168" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="264" t="s">
+      <c r="C45" s="256" t="s">
         <v>313</v>
       </c>
-      <c r="D45" s="264"/>
-      <c r="E45" s="264"/>
-      <c r="F45" s="264"/>
-      <c r="G45" s="264"/>
-      <c r="H45" s="264"/>
-      <c r="I45" s="264"/>
-      <c r="J45" s="264"/>
-      <c r="K45" s="264"/>
-      <c r="L45" s="265"/>
+      <c r="D45" s="256"/>
+      <c r="E45" s="256"/>
+      <c r="F45" s="256"/>
+      <c r="G45" s="256"/>
+      <c r="H45" s="256"/>
+      <c r="I45" s="256"/>
+      <c r="J45" s="256"/>
+      <c r="K45" s="256"/>
+      <c r="L45" s="257"/>
     </row>
     <row r="46" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="167"/>
       <c r="B46" s="168" t="s">
         <v>314</v>
       </c>
-      <c r="C46" s="264" t="s">
+      <c r="C46" s="256" t="s">
         <v>315</v>
       </c>
-      <c r="D46" s="264"/>
-      <c r="E46" s="264"/>
-      <c r="F46" s="264"/>
-      <c r="G46" s="264"/>
-      <c r="H46" s="264"/>
-      <c r="I46" s="264"/>
-      <c r="J46" s="264"/>
-      <c r="K46" s="264"/>
-      <c r="L46" s="265"/>
+      <c r="D46" s="256"/>
+      <c r="E46" s="256"/>
+      <c r="F46" s="256"/>
+      <c r="G46" s="256"/>
+      <c r="H46" s="256"/>
+      <c r="I46" s="256"/>
+      <c r="J46" s="256"/>
+      <c r="K46" s="256"/>
+      <c r="L46" s="257"/>
     </row>
     <row r="47" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="167"/>
       <c r="B47" s="168" t="s">
         <v>384</v>
       </c>
-      <c r="C47" s="264" t="s">
+      <c r="C47" s="256" t="s">
         <v>385</v>
       </c>
-      <c r="D47" s="264"/>
-      <c r="E47" s="264"/>
-      <c r="F47" s="264"/>
-      <c r="G47" s="264"/>
-      <c r="H47" s="264"/>
-      <c r="I47" s="264"/>
-      <c r="J47" s="264"/>
-      <c r="K47" s="264"/>
-      <c r="L47" s="265"/>
+      <c r="D47" s="256"/>
+      <c r="E47" s="256"/>
+      <c r="F47" s="256"/>
+      <c r="G47" s="256"/>
+      <c r="H47" s="256"/>
+      <c r="I47" s="256"/>
+      <c r="J47" s="256"/>
+      <c r="K47" s="256"/>
+      <c r="L47" s="257"/>
     </row>
     <row r="48" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="167"/>
       <c r="B48" s="168" t="s">
         <v>138</v>
       </c>
-      <c r="C48" s="264" t="s">
+      <c r="C48" s="256" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="264"/>
-      <c r="E48" s="264"/>
-      <c r="F48" s="264"/>
-      <c r="G48" s="264"/>
-      <c r="H48" s="264"/>
-      <c r="I48" s="264"/>
-      <c r="J48" s="264"/>
-      <c r="K48" s="264"/>
-      <c r="L48" s="265"/>
+      <c r="D48" s="256"/>
+      <c r="E48" s="256"/>
+      <c r="F48" s="256"/>
+      <c r="G48" s="256"/>
+      <c r="H48" s="256"/>
+      <c r="I48" s="256"/>
+      <c r="J48" s="256"/>
+      <c r="K48" s="256"/>
+      <c r="L48" s="257"/>
     </row>
     <row r="49" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="167"/>
       <c r="B49" s="168" t="s">
         <v>238</v>
       </c>
-      <c r="C49" s="264" t="s">
+      <c r="C49" s="256" t="s">
         <v>239</v>
       </c>
-      <c r="D49" s="264"/>
-      <c r="E49" s="264"/>
-      <c r="F49" s="264"/>
-      <c r="G49" s="264"/>
-      <c r="H49" s="264"/>
-      <c r="I49" s="264"/>
-      <c r="J49" s="264"/>
-      <c r="K49" s="264"/>
-      <c r="L49" s="265"/>
+      <c r="D49" s="256"/>
+      <c r="E49" s="256"/>
+      <c r="F49" s="256"/>
+      <c r="G49" s="256"/>
+      <c r="H49" s="256"/>
+      <c r="I49" s="256"/>
+      <c r="J49" s="256"/>
+      <c r="K49" s="256"/>
+      <c r="L49" s="257"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A50" s="167"/>
@@ -15852,18 +15858,18 @@
       <c r="B51" s="168" t="s">
         <v>63</v>
       </c>
-      <c r="C51" s="264" t="s">
+      <c r="C51" s="256" t="s">
         <v>317</v>
       </c>
-      <c r="D51" s="264"/>
-      <c r="E51" s="264"/>
-      <c r="F51" s="264"/>
-      <c r="G51" s="264"/>
-      <c r="H51" s="264"/>
-      <c r="I51" s="264"/>
-      <c r="J51" s="264"/>
-      <c r="K51" s="264"/>
-      <c r="L51" s="265"/>
+      <c r="D51" s="256"/>
+      <c r="E51" s="256"/>
+      <c r="F51" s="256"/>
+      <c r="G51" s="256"/>
+      <c r="H51" s="256"/>
+      <c r="I51" s="256"/>
+      <c r="J51" s="256"/>
+      <c r="K51" s="256"/>
+      <c r="L51" s="257"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A52" s="167"/>
@@ -15945,38 +15951,39 @@
       </c>
     </row>
     <row r="65" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="281" t="s">
+      <c r="A65" s="246" t="s">
         <v>356</v>
       </c>
-      <c r="B65" s="281"/>
-      <c r="C65" s="281"/>
-      <c r="D65" s="281"/>
-      <c r="E65" s="281"/>
-      <c r="F65" s="281"/>
-      <c r="G65" s="281"/>
-      <c r="H65" s="281"/>
-      <c r="I65" s="281"/>
-      <c r="J65" s="281"/>
-      <c r="K65" s="281"/>
-      <c r="L65" s="281"/>
+      <c r="B65" s="246"/>
+      <c r="C65" s="246"/>
+      <c r="D65" s="246"/>
+      <c r="E65" s="246"/>
+      <c r="F65" s="246"/>
+      <c r="G65" s="246"/>
+      <c r="H65" s="246"/>
+      <c r="I65" s="246"/>
+      <c r="J65" s="246"/>
+      <c r="K65" s="246"/>
+      <c r="L65" s="246"/>
     </row>
     <row r="70" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="71" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A65:L65"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="C45:L45"/>
-    <mergeCell ref="C48:L48"/>
-    <mergeCell ref="C49:L49"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="C51:L51"/>
-    <mergeCell ref="A35:L35"/>
-    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B8:L8"/>
     <mergeCell ref="B31:L31"/>
     <mergeCell ref="B18:L18"/>
     <mergeCell ref="B19:L19"/>
@@ -15991,20 +15998,19 @@
     <mergeCell ref="B29:L29"/>
     <mergeCell ref="B28:L28"/>
     <mergeCell ref="B30:L30"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="A65:L65"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="C45:L45"/>
+    <mergeCell ref="C48:L48"/>
+    <mergeCell ref="C49:L49"/>
+    <mergeCell ref="C46:L46"/>
+    <mergeCell ref="C51:L51"/>
+    <mergeCell ref="A35:L35"/>
+    <mergeCell ref="C47:L47"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A58" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -31069,8 +31075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BF02C3-B992-44C7-A79C-D1E41573911A}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31263,13 +31269,25 @@
       <c r="J7" s="41"/>
       <c r="K7" s="40"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="57"/>
-      <c r="B8" s="149"/>
-      <c r="C8" s="56"/>
-      <c r="D8" s="55"/>
-      <c r="E8" s="55"/>
-      <c r="F8" s="55"/>
+    <row r="8" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="57">
+        <v>45671</v>
+      </c>
+      <c r="B8" s="149" t="s">
+        <v>389</v>
+      </c>
+      <c r="C8" s="56" t="s">
+        <v>390</v>
+      </c>
+      <c r="D8" s="55">
+        <v>0.5</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>285</v>
+      </c>
+      <c r="F8" s="55" t="s">
+        <v>285</v>
+      </c>
       <c r="G8" s="57"/>
       <c r="I8" s="38"/>
       <c r="J8" s="41"/>
@@ -31598,8 +31616,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BF7D8F-86F3-47E9-AB85-EE9B4CAB70E4}">
   <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N25" sqref="N25"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -38056,16 +38074,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="321" t="e">
+      <c r="A1" s="322" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="321"/>
-      <c r="C1" s="321"/>
-      <c r="D1" s="321"/>
-      <c r="E1" s="321"/>
-      <c r="F1" s="321"/>
-      <c r="G1" s="321"/>
+      <c r="B1" s="322"/>
+      <c r="C1" s="322"/>
+      <c r="D1" s="322"/>
+      <c r="E1" s="322"/>
+      <c r="F1" s="322"/>
+      <c r="G1" s="322"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -38174,11 +38192,11 @@
         <v>80</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="322"/>
-      <c r="D10" s="322"/>
-      <c r="E10" s="322"/>
-      <c r="F10" s="322"/>
-      <c r="G10" s="322"/>
+      <c r="C10" s="321"/>
+      <c r="D10" s="321"/>
+      <c r="E10" s="321"/>
+      <c r="F10" s="321"/>
+      <c r="G10" s="321"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -39441,6 +39459,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -39448,12 +39472,6 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>

</xml_diff>

<commit_message>
Update Lets Start with Tribal Nations Split.
Also add Erik Porse / UCANR; Add key ideas to ReadMe-Directions worksheet in Excel File
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8439995-8058-40D6-A50A-C725CFA561FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464EC48D-2716-4A20-B930-F71F02B4D1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="57480" yWindow="-1260" windowWidth="29040" windowHeight="15720" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="62" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="401">
   <si>
     <t>Year 1</t>
   </si>
@@ -1919,9 +1919,6 @@
     <t>b) Give users more autonomy to manage their conflicting vulnerabilities to water shortages.</t>
   </si>
   <si>
-    <t>David E. Rosenberg, Erik Porse (2024). "Immersive Model for Lake Mead Based on the Principle of Division of Reservoir Inflow." Utah State University, Logan, UT. https://github.com/dzeke/ColoradoRiverCollaborate/tree/main/LakeMeadWaterBankDivideInflow.</t>
-  </si>
-  <si>
     <t>1.3.1</t>
   </si>
   <si>
@@ -2023,6 +2020,39 @@
   <si>
     <t>Document Tribal parameter in Users Guide</t>
   </si>
+  <si>
+    <t>KEY IDEAS</t>
+  </si>
+  <si>
+    <t>1)</t>
+  </si>
+  <si>
+    <t>2)</t>
+  </si>
+  <si>
+    <t>3)</t>
+  </si>
+  <si>
+    <t>Lake Mead water level is the sum of the protection elevation and each user’s available water.</t>
+  </si>
+  <si>
+    <t>Each user manages all their available water not just prior conserved water.</t>
+  </si>
+  <si>
+    <t>Tribal Nations of the Lower Basin manage their own settled water rights (16.4% is from California, 82.4% is from Arizona). Ignore Nevada.</t>
+  </si>
+  <si>
+    <t>Eric Porse</t>
+  </si>
+  <si>
+    <t>University of California Agricultural and Natural Resources</t>
+  </si>
+  <si>
+    <t>David E. Rosenberg, Erik Porse (2025). "Immersive Model for Lake Mead Based on the Principle of Division of Reservoir Inflow." Utah State University, Logan, UT. https://github.com/dzeke/ColoradoRiverCollaborate/tree/main/LakeMeadWaterBankDivideInflow.</t>
+  </si>
+  <si>
+    <t>eporse@ucanr.edu</t>
+  </si>
 </sst>
 </file>
 
@@ -2043,7 +2073,7 @@
     <numFmt numFmtId="173" formatCode="#,##0.0_);\(#,##0.0\)"/>
     <numFmt numFmtId="174" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2234,6 +2264,13 @@
       <b/>
       <sz val="16"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2665,7 +2702,7 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="330">
+  <cellXfs count="341">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3320,51 +3357,6 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3419,6 +3411,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3442,6 +3440,45 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3545,11 +3582,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3572,6 +3609,35 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="20% - Accent1" xfId="12" builtinId="30"/>
@@ -14400,6 +14466,55 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>144135</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1098246</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B81C37B0-5399-07E0-623D-92904A69DFAC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="276225" y="3173085"/>
+          <a:ext cx="4968875" cy="954111"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
     <xdr:ext cx="13008022" cy="9439701"/>
@@ -14431,7 +14546,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
@@ -14487,7 +14602,7 @@
 </c:userShapes>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -14589,7 +14704,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -14967,9 +15082,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EA02F4-5F19-409C-8BC6-A0D8FEB3A90D}">
-  <dimension ref="A1:R71"/>
+  <dimension ref="A1:R81"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
@@ -14989,20 +15104,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="264" t="s">
+      <c r="A1" s="249" t="s">
         <v>351</v>
       </c>
-      <c r="B1" s="264"/>
-      <c r="C1" s="264"/>
-      <c r="D1" s="264"/>
-      <c r="E1" s="264"/>
-      <c r="F1" s="264"/>
-      <c r="G1" s="264"/>
-      <c r="H1" s="264"/>
-      <c r="I1" s="264"/>
-      <c r="J1" s="264"/>
-      <c r="K1" s="264"/>
-      <c r="L1" s="264"/>
+      <c r="B1" s="249"/>
+      <c r="C1" s="249"/>
+      <c r="D1" s="249"/>
+      <c r="E1" s="249"/>
+      <c r="F1" s="249"/>
+      <c r="G1" s="249"/>
+      <c r="H1" s="249"/>
+      <c r="I1" s="249"/>
+      <c r="J1" s="249"/>
+      <c r="K1" s="249"/>
+      <c r="L1" s="249"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -15028,41 +15143,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="265" t="s">
+      <c r="A4" s="250" t="s">
         <v>352</v>
       </c>
-      <c r="B4" s="266"/>
-      <c r="C4" s="266"/>
-      <c r="D4" s="266"/>
-      <c r="E4" s="266"/>
-      <c r="F4" s="266"/>
-      <c r="G4" s="266"/>
-      <c r="H4" s="266"/>
-      <c r="I4" s="266"/>
-      <c r="J4" s="266"/>
-      <c r="K4" s="266"/>
-      <c r="L4" s="267"/>
-      <c r="N4" s="268"/>
-      <c r="O4" s="268"/>
-      <c r="P4" s="268"/>
-      <c r="Q4" s="268"/>
-      <c r="R4" s="268"/>
+      <c r="B4" s="251"/>
+      <c r="C4" s="251"/>
+      <c r="D4" s="251"/>
+      <c r="E4" s="251"/>
+      <c r="F4" s="251"/>
+      <c r="G4" s="251"/>
+      <c r="H4" s="251"/>
+      <c r="I4" s="251"/>
+      <c r="J4" s="251"/>
+      <c r="K4" s="251"/>
+      <c r="L4" s="252"/>
+      <c r="N4" s="253"/>
+      <c r="O4" s="253"/>
+      <c r="P4" s="253"/>
+      <c r="Q4" s="253"/>
+      <c r="R4" s="253"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="269" t="s">
+      <c r="A5" s="254" t="s">
         <v>335</v>
       </c>
-      <c r="B5" s="270"/>
-      <c r="C5" s="270"/>
-      <c r="D5" s="270"/>
-      <c r="E5" s="270"/>
-      <c r="F5" s="270"/>
-      <c r="G5" s="270"/>
-      <c r="H5" s="270"/>
-      <c r="I5" s="270"/>
-      <c r="J5" s="270"/>
-      <c r="K5" s="270"/>
-      <c r="L5" s="271"/>
+      <c r="B5" s="255"/>
+      <c r="C5" s="255"/>
+      <c r="D5" s="255"/>
+      <c r="E5" s="255"/>
+      <c r="F5" s="255"/>
+      <c r="G5" s="255"/>
+      <c r="H5" s="255"/>
+      <c r="I5" s="255"/>
+      <c r="J5" s="255"/>
+      <c r="K5" s="255"/>
+      <c r="L5" s="256"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15070,20 +15185,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="269" t="s">
+      <c r="A6" s="254" t="s">
         <v>353</v>
       </c>
-      <c r="B6" s="270"/>
-      <c r="C6" s="270"/>
-      <c r="D6" s="270"/>
-      <c r="E6" s="270"/>
-      <c r="F6" s="270"/>
-      <c r="G6" s="270"/>
-      <c r="H6" s="270"/>
-      <c r="I6" s="270"/>
-      <c r="J6" s="270"/>
-      <c r="K6" s="270"/>
-      <c r="L6" s="271"/>
+      <c r="B6" s="255"/>
+      <c r="C6" s="255"/>
+      <c r="D6" s="255"/>
+      <c r="E6" s="255"/>
+      <c r="F6" s="255"/>
+      <c r="G6" s="255"/>
+      <c r="H6" s="255"/>
+      <c r="I6" s="255"/>
+      <c r="J6" s="255"/>
+      <c r="K6" s="255"/>
+      <c r="L6" s="256"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15092,19 +15207,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="233"/>
-      <c r="B7" s="270" t="s">
+      <c r="B7" s="255" t="s">
         <v>354</v>
       </c>
-      <c r="C7" s="270"/>
-      <c r="D7" s="270"/>
-      <c r="E7" s="270"/>
-      <c r="F7" s="270"/>
-      <c r="G7" s="270"/>
-      <c r="H7" s="270"/>
-      <c r="I7" s="270"/>
-      <c r="J7" s="270"/>
-      <c r="K7" s="270"/>
-      <c r="L7" s="271"/>
+      <c r="C7" s="255"/>
+      <c r="D7" s="255"/>
+      <c r="E7" s="255"/>
+      <c r="F7" s="255"/>
+      <c r="G7" s="255"/>
+      <c r="H7" s="255"/>
+      <c r="I7" s="255"/>
+      <c r="J7" s="255"/>
+      <c r="K7" s="255"/>
+      <c r="L7" s="256"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15113,19 +15228,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="234"/>
-      <c r="B8" s="285" t="s">
+      <c r="B8" s="272" t="s">
         <v>355</v>
       </c>
-      <c r="C8" s="285"/>
-      <c r="D8" s="285"/>
-      <c r="E8" s="285"/>
-      <c r="F8" s="285"/>
-      <c r="G8" s="285"/>
-      <c r="H8" s="285"/>
-      <c r="I8" s="285"/>
-      <c r="J8" s="285"/>
-      <c r="K8" s="285"/>
-      <c r="L8" s="286"/>
+      <c r="C8" s="272"/>
+      <c r="D8" s="272"/>
+      <c r="E8" s="272"/>
+      <c r="F8" s="272"/>
+      <c r="G8" s="272"/>
+      <c r="H8" s="272"/>
+      <c r="I8" s="272"/>
+      <c r="J8" s="272"/>
+      <c r="K8" s="272"/>
+      <c r="L8" s="273"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15147,84 +15262,88 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="272" t="s">
-        <v>205</v>
-      </c>
-      <c r="B10" s="273"/>
-      <c r="C10" s="273"/>
-      <c r="D10" s="273"/>
-      <c r="E10" s="273"/>
-      <c r="F10" s="273"/>
-      <c r="G10" s="273"/>
-      <c r="H10" s="273"/>
-      <c r="I10" s="273"/>
-      <c r="J10" s="273"/>
-      <c r="K10" s="273"/>
-      <c r="L10" s="274"/>
+      <c r="A10" s="330" t="s">
+        <v>390</v>
+      </c>
+      <c r="B10" s="331"/>
+      <c r="C10" s="331"/>
+      <c r="D10" s="331"/>
+      <c r="E10" s="331"/>
+      <c r="F10" s="331"/>
+      <c r="G10" s="331"/>
+      <c r="H10" s="331"/>
+      <c r="I10" s="331"/>
+      <c r="J10" s="331"/>
+      <c r="K10" s="331"/>
+      <c r="L10" s="332"/>
     </row>
     <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="275" t="s">
-        <v>336</v>
-      </c>
-      <c r="B11" s="276"/>
-      <c r="C11" s="276"/>
-      <c r="D11" s="276"/>
-      <c r="E11" s="276"/>
-      <c r="F11" s="276"/>
-      <c r="G11" s="276"/>
-      <c r="H11" s="276"/>
-      <c r="I11" s="276"/>
-      <c r="J11" s="276"/>
-      <c r="K11" s="276"/>
-      <c r="L11" s="277"/>
+      <c r="A11" s="333" t="s">
+        <v>391</v>
+      </c>
+      <c r="B11" s="334" t="s">
+        <v>394</v>
+      </c>
+      <c r="C11" s="334"/>
+      <c r="D11" s="334"/>
+      <c r="E11" s="334"/>
+      <c r="F11" s="334"/>
+      <c r="G11" s="334"/>
+      <c r="H11" s="334"/>
+      <c r="I11" s="334"/>
+      <c r="J11" s="334"/>
+      <c r="K11" s="334"/>
+      <c r="L11" s="335"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="278" t="s">
-        <v>337</v>
-      </c>
-      <c r="B12" s="256"/>
-      <c r="C12" s="256"/>
-      <c r="D12" s="256"/>
-      <c r="E12" s="256"/>
-      <c r="F12" s="256"/>
-      <c r="G12" s="256"/>
-      <c r="H12" s="256"/>
-      <c r="I12" s="256"/>
-      <c r="J12" s="256"/>
-      <c r="K12" s="256"/>
-      <c r="L12" s="257"/>
-    </row>
-    <row r="13" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="278" t="s">
-        <v>206</v>
-      </c>
-      <c r="B13" s="256"/>
-      <c r="C13" s="256"/>
-      <c r="D13" s="256"/>
-      <c r="E13" s="256"/>
-      <c r="F13" s="256"/>
-      <c r="G13" s="256"/>
-      <c r="H13" s="256"/>
-      <c r="I13" s="256"/>
-      <c r="J13" s="256"/>
-      <c r="K13" s="256"/>
-      <c r="L13" s="257"/>
-    </row>
-    <row r="14" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="279" t="s">
-        <v>338</v>
-      </c>
-      <c r="B14" s="280"/>
-      <c r="C14" s="280"/>
-      <c r="D14" s="280"/>
-      <c r="E14" s="280"/>
-      <c r="F14" s="280"/>
-      <c r="G14" s="280"/>
-      <c r="H14" s="280"/>
-      <c r="I14" s="280"/>
-      <c r="J14" s="280"/>
-      <c r="K14" s="280"/>
-      <c r="L14" s="281"/>
+      <c r="A12" s="333" t="s">
+        <v>392</v>
+      </c>
+      <c r="B12" s="334" t="s">
+        <v>395</v>
+      </c>
+      <c r="C12" s="334"/>
+      <c r="D12" s="334"/>
+      <c r="E12" s="334"/>
+      <c r="F12" s="334"/>
+      <c r="G12" s="334"/>
+      <c r="H12" s="334"/>
+      <c r="I12" s="334"/>
+      <c r="J12" s="334"/>
+      <c r="K12" s="334"/>
+      <c r="L12" s="335"/>
+    </row>
+    <row r="13" spans="1:18" s="59" customFormat="1" ht="90.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="333"/>
+      <c r="B13" s="334"/>
+      <c r="C13" s="334"/>
+      <c r="D13" s="334"/>
+      <c r="E13" s="334"/>
+      <c r="F13" s="334"/>
+      <c r="G13" s="334"/>
+      <c r="H13" s="334"/>
+      <c r="I13" s="334"/>
+      <c r="J13" s="334"/>
+      <c r="K13" s="334"/>
+      <c r="L13" s="335"/>
+    </row>
+    <row r="14" spans="1:18" s="59" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="336" t="s">
+        <v>393</v>
+      </c>
+      <c r="B14" s="337" t="s">
+        <v>396</v>
+      </c>
+      <c r="C14" s="337"/>
+      <c r="D14" s="337"/>
+      <c r="E14" s="337"/>
+      <c r="F14" s="337"/>
+      <c r="G14" s="337"/>
+      <c r="H14" s="337"/>
+      <c r="I14" s="337"/>
+      <c r="J14" s="337"/>
+      <c r="K14" s="337"/>
+      <c r="L14" s="338"/>
     </row>
     <row r="15" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="113"/>
@@ -15240,608 +15359,594 @@
       <c r="K15" s="113"/>
       <c r="L15" s="113"/>
     </row>
-    <row r="16" spans="1:18" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="282" t="s">
+    <row r="16" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="257" t="s">
+        <v>205</v>
+      </c>
+      <c r="B16" s="258"/>
+      <c r="C16" s="258"/>
+      <c r="D16" s="258"/>
+      <c r="E16" s="258"/>
+      <c r="F16" s="258"/>
+      <c r="G16" s="258"/>
+      <c r="H16" s="258"/>
+      <c r="I16" s="258"/>
+      <c r="J16" s="258"/>
+      <c r="K16" s="258"/>
+      <c r="L16" s="259"/>
+    </row>
+    <row r="17" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="260" t="s">
+        <v>336</v>
+      </c>
+      <c r="B17" s="261"/>
+      <c r="C17" s="261"/>
+      <c r="D17" s="261"/>
+      <c r="E17" s="261"/>
+      <c r="F17" s="261"/>
+      <c r="G17" s="261"/>
+      <c r="H17" s="261"/>
+      <c r="I17" s="261"/>
+      <c r="J17" s="261"/>
+      <c r="K17" s="261"/>
+      <c r="L17" s="262"/>
+    </row>
+    <row r="18" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="263" t="s">
+        <v>337</v>
+      </c>
+      <c r="B18" s="264"/>
+      <c r="C18" s="264"/>
+      <c r="D18" s="264"/>
+      <c r="E18" s="264"/>
+      <c r="F18" s="264"/>
+      <c r="G18" s="264"/>
+      <c r="H18" s="264"/>
+      <c r="I18" s="264"/>
+      <c r="J18" s="264"/>
+      <c r="K18" s="264"/>
+      <c r="L18" s="265"/>
+    </row>
+    <row r="19" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="263" t="s">
+        <v>206</v>
+      </c>
+      <c r="B19" s="264"/>
+      <c r="C19" s="264"/>
+      <c r="D19" s="264"/>
+      <c r="E19" s="264"/>
+      <c r="F19" s="264"/>
+      <c r="G19" s="264"/>
+      <c r="H19" s="264"/>
+      <c r="I19" s="264"/>
+      <c r="J19" s="264"/>
+      <c r="K19" s="264"/>
+      <c r="L19" s="265"/>
+    </row>
+    <row r="20" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="266" t="s">
+        <v>338</v>
+      </c>
+      <c r="B20" s="267"/>
+      <c r="C20" s="267"/>
+      <c r="D20" s="267"/>
+      <c r="E20" s="267"/>
+      <c r="F20" s="267"/>
+      <c r="G20" s="267"/>
+      <c r="H20" s="267"/>
+      <c r="I20" s="267"/>
+      <c r="J20" s="267"/>
+      <c r="K20" s="267"/>
+      <c r="L20" s="268"/>
+    </row>
+    <row r="21" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
+      <c r="C21" s="113"/>
+      <c r="D21" s="113"/>
+      <c r="E21" s="113"/>
+      <c r="F21" s="113"/>
+      <c r="G21" s="113"/>
+      <c r="H21" s="113"/>
+      <c r="I21" s="113"/>
+      <c r="J21" s="113"/>
+      <c r="K21" s="113"/>
+      <c r="L21" s="113"/>
+    </row>
+    <row r="22" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="269" t="s">
         <v>334</v>
       </c>
-      <c r="B16" s="283"/>
-      <c r="C16" s="283"/>
-      <c r="D16" s="283"/>
-      <c r="E16" s="283"/>
-      <c r="F16" s="283"/>
-      <c r="G16" s="283"/>
-      <c r="H16" s="283"/>
-      <c r="I16" s="283"/>
-      <c r="J16" s="283"/>
-      <c r="K16" s="283"/>
-      <c r="L16" s="284"/>
-      <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="261" t="s">
+      <c r="B22" s="270"/>
+      <c r="C22" s="270"/>
+      <c r="D22" s="270"/>
+      <c r="E22" s="270"/>
+      <c r="F22" s="270"/>
+      <c r="G22" s="270"/>
+      <c r="H22" s="270"/>
+      <c r="I22" s="270"/>
+      <c r="J22" s="270"/>
+      <c r="K22" s="270"/>
+      <c r="L22" s="271"/>
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="246" t="s">
         <v>215</v>
       </c>
-      <c r="B17" s="262"/>
-      <c r="C17" s="262"/>
-      <c r="D17" s="262"/>
-      <c r="E17" s="262"/>
-      <c r="F17" s="262"/>
-      <c r="G17" s="262"/>
-      <c r="H17" s="262"/>
-      <c r="I17" s="262"/>
-      <c r="J17" s="262"/>
-      <c r="K17" s="262"/>
-      <c r="L17" s="263"/>
-      <c r="N17" s="1"/>
-    </row>
-    <row r="18" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="228">
+      <c r="B23" s="247"/>
+      <c r="C23" s="247"/>
+      <c r="D23" s="247"/>
+      <c r="E23" s="247"/>
+      <c r="F23" s="247"/>
+      <c r="G23" s="247"/>
+      <c r="H23" s="247"/>
+      <c r="I23" s="247"/>
+      <c r="J23" s="247"/>
+      <c r="K23" s="247"/>
+      <c r="L23" s="248"/>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="228">
         <v>1</v>
       </c>
-      <c r="B18" s="249" t="s">
+      <c r="B24" s="276" t="s">
         <v>214</v>
       </c>
-      <c r="C18" s="249"/>
-      <c r="D18" s="249"/>
-      <c r="E18" s="249"/>
-      <c r="F18" s="249"/>
-      <c r="G18" s="249"/>
-      <c r="H18" s="249"/>
-      <c r="I18" s="249"/>
-      <c r="J18" s="249"/>
-      <c r="K18" s="249"/>
-      <c r="L18" s="250"/>
-    </row>
-    <row r="19" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="228">
+      <c r="C24" s="276"/>
+      <c r="D24" s="276"/>
+      <c r="E24" s="276"/>
+      <c r="F24" s="276"/>
+      <c r="G24" s="276"/>
+      <c r="H24" s="276"/>
+      <c r="I24" s="276"/>
+      <c r="J24" s="276"/>
+      <c r="K24" s="276"/>
+      <c r="L24" s="277"/>
+    </row>
+    <row r="25" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="228">
         <v>2</v>
       </c>
-      <c r="B19" s="249" t="s">
+      <c r="B25" s="276" t="s">
         <v>330</v>
       </c>
-      <c r="C19" s="249"/>
-      <c r="D19" s="249"/>
-      <c r="E19" s="249"/>
-      <c r="F19" s="249"/>
-      <c r="G19" s="249"/>
-      <c r="H19" s="249"/>
-      <c r="I19" s="249"/>
-      <c r="J19" s="249"/>
-      <c r="K19" s="249"/>
-      <c r="L19" s="250"/>
-      <c r="N19" s="106"/>
-    </row>
-    <row r="20" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="228">
-        <v>3</v>
-      </c>
-      <c r="B20" s="249" t="s">
-        <v>207</v>
-      </c>
-      <c r="C20" s="249"/>
-      <c r="D20" s="249"/>
-      <c r="E20" s="249"/>
-      <c r="F20" s="249"/>
-      <c r="G20" s="249"/>
-      <c r="H20" s="249"/>
-      <c r="I20" s="249"/>
-      <c r="J20" s="249"/>
-      <c r="K20" s="249"/>
-      <c r="L20" s="250"/>
-      <c r="N20" s="106"/>
-    </row>
-    <row r="21" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="228">
-        <v>4</v>
-      </c>
-      <c r="B21" s="249" t="s">
-        <v>339</v>
-      </c>
-      <c r="C21" s="249"/>
-      <c r="D21" s="249"/>
-      <c r="E21" s="249"/>
-      <c r="F21" s="249"/>
-      <c r="G21" s="249"/>
-      <c r="H21" s="249"/>
-      <c r="I21" s="249"/>
-      <c r="J21" s="249"/>
-      <c r="K21" s="249"/>
-      <c r="L21" s="250"/>
-      <c r="N21" s="106"/>
-    </row>
-    <row r="22" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="228">
-        <v>5</v>
-      </c>
-      <c r="B22" s="249" t="s">
-        <v>208</v>
-      </c>
-      <c r="C22" s="249"/>
-      <c r="D22" s="249"/>
-      <c r="E22" s="249"/>
-      <c r="F22" s="249"/>
-      <c r="G22" s="249"/>
-      <c r="H22" s="249"/>
-      <c r="I22" s="249"/>
-      <c r="J22" s="249"/>
-      <c r="K22" s="249"/>
-      <c r="L22" s="250"/>
-      <c r="N22" s="106"/>
-    </row>
-    <row r="23" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="228"/>
-      <c r="B23" s="249" t="s">
-        <v>209</v>
-      </c>
-      <c r="C23" s="249"/>
-      <c r="D23" s="249"/>
-      <c r="E23" s="249"/>
-      <c r="F23" s="249"/>
-      <c r="G23" s="249"/>
-      <c r="H23" s="249"/>
-      <c r="I23" s="249"/>
-      <c r="J23" s="249"/>
-      <c r="K23" s="249"/>
-      <c r="L23" s="250"/>
-      <c r="N23" s="106"/>
-    </row>
-    <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="228"/>
-      <c r="B24" s="249" t="s">
-        <v>210</v>
-      </c>
-      <c r="C24" s="249"/>
-      <c r="D24" s="249"/>
-      <c r="E24" s="249"/>
-      <c r="F24" s="249"/>
-      <c r="G24" s="249"/>
-      <c r="H24" s="249"/>
-      <c r="I24" s="249"/>
-      <c r="J24" s="249"/>
-      <c r="K24" s="249"/>
-      <c r="L24" s="250"/>
-      <c r="N24" s="106"/>
-    </row>
-    <row r="25" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="258" t="s">
-        <v>216</v>
-      </c>
-      <c r="B25" s="259"/>
-      <c r="C25" s="259"/>
-      <c r="D25" s="259"/>
-      <c r="E25" s="259"/>
-      <c r="F25" s="259"/>
-      <c r="G25" s="259"/>
-      <c r="H25" s="259"/>
-      <c r="I25" s="259"/>
-      <c r="J25" s="259"/>
-      <c r="K25" s="259"/>
-      <c r="L25" s="260"/>
+      <c r="C25" s="276"/>
+      <c r="D25" s="276"/>
+      <c r="E25" s="276"/>
+      <c r="F25" s="276"/>
+      <c r="G25" s="276"/>
+      <c r="H25" s="276"/>
+      <c r="I25" s="276"/>
+      <c r="J25" s="276"/>
+      <c r="K25" s="276"/>
+      <c r="L25" s="277"/>
       <c r="N25" s="106"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="228">
+        <v>3</v>
+      </c>
+      <c r="B26" s="276" t="s">
+        <v>207</v>
+      </c>
+      <c r="C26" s="276"/>
+      <c r="D26" s="276"/>
+      <c r="E26" s="276"/>
+      <c r="F26" s="276"/>
+      <c r="G26" s="276"/>
+      <c r="H26" s="276"/>
+      <c r="I26" s="276"/>
+      <c r="J26" s="276"/>
+      <c r="K26" s="276"/>
+      <c r="L26" s="277"/>
+      <c r="N26" s="106"/>
+    </row>
+    <row r="27" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="228">
+        <v>4</v>
+      </c>
+      <c r="B27" s="276" t="s">
+        <v>339</v>
+      </c>
+      <c r="C27" s="276"/>
+      <c r="D27" s="276"/>
+      <c r="E27" s="276"/>
+      <c r="F27" s="276"/>
+      <c r="G27" s="276"/>
+      <c r="H27" s="276"/>
+      <c r="I27" s="276"/>
+      <c r="J27" s="276"/>
+      <c r="K27" s="276"/>
+      <c r="L27" s="277"/>
+      <c r="N27" s="106"/>
+    </row>
+    <row r="28" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="228">
+        <v>5</v>
+      </c>
+      <c r="B28" s="276" t="s">
+        <v>208</v>
+      </c>
+      <c r="C28" s="276"/>
+      <c r="D28" s="276"/>
+      <c r="E28" s="276"/>
+      <c r="F28" s="276"/>
+      <c r="G28" s="276"/>
+      <c r="H28" s="276"/>
+      <c r="I28" s="276"/>
+      <c r="J28" s="276"/>
+      <c r="K28" s="276"/>
+      <c r="L28" s="277"/>
+      <c r="N28" s="106"/>
+    </row>
+    <row r="29" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="228"/>
+      <c r="B29" s="276" t="s">
+        <v>209</v>
+      </c>
+      <c r="C29" s="276"/>
+      <c r="D29" s="276"/>
+      <c r="E29" s="276"/>
+      <c r="F29" s="276"/>
+      <c r="G29" s="276"/>
+      <c r="H29" s="276"/>
+      <c r="I29" s="276"/>
+      <c r="J29" s="276"/>
+      <c r="K29" s="276"/>
+      <c r="L29" s="277"/>
+      <c r="N29" s="106"/>
+    </row>
+    <row r="30" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="228"/>
+      <c r="B30" s="276" t="s">
+        <v>210</v>
+      </c>
+      <c r="C30" s="276"/>
+      <c r="D30" s="276"/>
+      <c r="E30" s="276"/>
+      <c r="F30" s="276"/>
+      <c r="G30" s="276"/>
+      <c r="H30" s="276"/>
+      <c r="I30" s="276"/>
+      <c r="J30" s="276"/>
+      <c r="K30" s="276"/>
+      <c r="L30" s="277"/>
+      <c r="N30" s="106"/>
+    </row>
+    <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="278" t="s">
+        <v>216</v>
+      </c>
+      <c r="B31" s="279"/>
+      <c r="C31" s="279"/>
+      <c r="D31" s="279"/>
+      <c r="E31" s="279"/>
+      <c r="F31" s="279"/>
+      <c r="G31" s="279"/>
+      <c r="H31" s="279"/>
+      <c r="I31" s="279"/>
+      <c r="J31" s="279"/>
+      <c r="K31" s="279"/>
+      <c r="L31" s="280"/>
+      <c r="N31" s="106"/>
+    </row>
+    <row r="32" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="228">
         <v>1</v>
       </c>
-      <c r="B26" s="249" t="s">
+      <c r="B32" s="276" t="s">
         <v>211</v>
       </c>
-      <c r="C26" s="249"/>
-      <c r="D26" s="249"/>
-      <c r="E26" s="249"/>
-      <c r="F26" s="249"/>
-      <c r="G26" s="249"/>
-      <c r="H26" s="249"/>
-      <c r="I26" s="249"/>
-      <c r="J26" s="249"/>
-      <c r="K26" s="249"/>
-      <c r="L26" s="250"/>
-      <c r="N26" s="106"/>
-    </row>
-    <row r="27" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="228"/>
-      <c r="B27" s="247" t="s">
+      <c r="C32" s="276"/>
+      <c r="D32" s="276"/>
+      <c r="E32" s="276"/>
+      <c r="F32" s="276"/>
+      <c r="G32" s="276"/>
+      <c r="H32" s="276"/>
+      <c r="I32" s="276"/>
+      <c r="J32" s="276"/>
+      <c r="K32" s="276"/>
+      <c r="L32" s="277"/>
+      <c r="N32" s="106"/>
+    </row>
+    <row r="33" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="228"/>
+      <c r="B33" s="274" t="s">
         <v>340</v>
       </c>
-      <c r="C27" s="247"/>
-      <c r="D27" s="247"/>
-      <c r="E27" s="247"/>
-      <c r="F27" s="247"/>
-      <c r="G27" s="247"/>
-      <c r="H27" s="247"/>
-      <c r="I27" s="247"/>
-      <c r="J27" s="247"/>
-      <c r="K27" s="247"/>
-      <c r="L27" s="248"/>
-      <c r="N27" s="106"/>
-    </row>
-    <row r="28" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="228">
+      <c r="C33" s="274"/>
+      <c r="D33" s="274"/>
+      <c r="E33" s="274"/>
+      <c r="F33" s="274"/>
+      <c r="G33" s="274"/>
+      <c r="H33" s="274"/>
+      <c r="I33" s="274"/>
+      <c r="J33" s="274"/>
+      <c r="K33" s="274"/>
+      <c r="L33" s="275"/>
+      <c r="N33" s="106"/>
+    </row>
+    <row r="34" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="228">
         <v>2</v>
       </c>
-      <c r="B28" s="249" t="s">
+      <c r="B34" s="276" t="s">
         <v>333</v>
       </c>
-      <c r="C28" s="249"/>
-      <c r="D28" s="249"/>
-      <c r="E28" s="249"/>
-      <c r="F28" s="249"/>
-      <c r="G28" s="249"/>
-      <c r="H28" s="249"/>
-      <c r="I28" s="249"/>
-      <c r="J28" s="249"/>
-      <c r="K28" s="249"/>
-      <c r="L28" s="250"/>
-      <c r="N28" s="106"/>
-    </row>
-    <row r="29" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="228">
+      <c r="C34" s="276"/>
+      <c r="D34" s="276"/>
+      <c r="E34" s="276"/>
+      <c r="F34" s="276"/>
+      <c r="G34" s="276"/>
+      <c r="H34" s="276"/>
+      <c r="I34" s="276"/>
+      <c r="J34" s="276"/>
+      <c r="K34" s="276"/>
+      <c r="L34" s="277"/>
+      <c r="N34" s="106"/>
+    </row>
+    <row r="35" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="228">
         <v>3</v>
       </c>
-      <c r="B29" s="249" t="s">
+      <c r="B35" s="276" t="s">
         <v>322</v>
       </c>
-      <c r="C29" s="249"/>
-      <c r="D29" s="249"/>
-      <c r="E29" s="249"/>
-      <c r="F29" s="249"/>
-      <c r="G29" s="249"/>
-      <c r="H29" s="249"/>
-      <c r="I29" s="249"/>
-      <c r="J29" s="249"/>
-      <c r="K29" s="249"/>
-      <c r="L29" s="250"/>
-      <c r="N29" s="106"/>
-    </row>
-    <row r="30" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="228">
+      <c r="C35" s="276"/>
+      <c r="D35" s="276"/>
+      <c r="E35" s="276"/>
+      <c r="F35" s="276"/>
+      <c r="G35" s="276"/>
+      <c r="H35" s="276"/>
+      <c r="I35" s="276"/>
+      <c r="J35" s="276"/>
+      <c r="K35" s="276"/>
+      <c r="L35" s="277"/>
+      <c r="N35" s="106"/>
+    </row>
+    <row r="36" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="228">
         <v>4</v>
       </c>
-      <c r="B30" s="249" t="s">
+      <c r="B36" s="276" t="s">
         <v>341</v>
       </c>
-      <c r="C30" s="249"/>
-      <c r="D30" s="249"/>
-      <c r="E30" s="249"/>
-      <c r="F30" s="249"/>
-      <c r="G30" s="249"/>
-      <c r="H30" s="249"/>
-      <c r="I30" s="249"/>
-      <c r="J30" s="249"/>
-      <c r="K30" s="249"/>
-      <c r="L30" s="250"/>
-      <c r="N30" s="106"/>
-    </row>
-    <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="228">
+      <c r="C36" s="276"/>
+      <c r="D36" s="276"/>
+      <c r="E36" s="276"/>
+      <c r="F36" s="276"/>
+      <c r="G36" s="276"/>
+      <c r="H36" s="276"/>
+      <c r="I36" s="276"/>
+      <c r="J36" s="276"/>
+      <c r="K36" s="276"/>
+      <c r="L36" s="277"/>
+      <c r="N36" s="106"/>
+    </row>
+    <row r="37" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="228">
         <v>5</v>
       </c>
-      <c r="B31" s="247" t="s">
+      <c r="B37" s="274" t="s">
         <v>323</v>
       </c>
-      <c r="C31" s="247"/>
-      <c r="D31" s="247"/>
-      <c r="E31" s="247"/>
-      <c r="F31" s="247"/>
-      <c r="G31" s="247"/>
-      <c r="H31" s="247"/>
-      <c r="I31" s="247"/>
-      <c r="J31" s="247"/>
-      <c r="K31" s="247"/>
-      <c r="L31" s="248"/>
-      <c r="N31" s="106"/>
-    </row>
-    <row r="32" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="228">
+      <c r="C37" s="274"/>
+      <c r="D37" s="274"/>
+      <c r="E37" s="274"/>
+      <c r="F37" s="274"/>
+      <c r="G37" s="274"/>
+      <c r="H37" s="274"/>
+      <c r="I37" s="274"/>
+      <c r="J37" s="274"/>
+      <c r="K37" s="274"/>
+      <c r="L37" s="275"/>
+      <c r="N37" s="106"/>
+    </row>
+    <row r="38" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="228">
         <v>6</v>
       </c>
-      <c r="B32" s="247" t="s">
+      <c r="B38" s="274" t="s">
         <v>328</v>
       </c>
-      <c r="C32" s="247"/>
-      <c r="D32" s="247"/>
-      <c r="E32" s="247"/>
-      <c r="F32" s="247"/>
-      <c r="G32" s="247"/>
-      <c r="H32" s="247"/>
-      <c r="I32" s="247"/>
-      <c r="J32" s="247"/>
-      <c r="K32" s="247"/>
-      <c r="L32" s="248"/>
-      <c r="N32" s="106"/>
-    </row>
-    <row r="33" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="228">
+      <c r="C38" s="274"/>
+      <c r="D38" s="274"/>
+      <c r="E38" s="274"/>
+      <c r="F38" s="274"/>
+      <c r="G38" s="274"/>
+      <c r="H38" s="274"/>
+      <c r="I38" s="274"/>
+      <c r="J38" s="274"/>
+      <c r="K38" s="274"/>
+      <c r="L38" s="275"/>
+      <c r="N38" s="106"/>
+    </row>
+    <row r="39" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="228">
         <v>7</v>
       </c>
-      <c r="B33" s="249" t="s">
+      <c r="B39" s="276" t="s">
         <v>324</v>
       </c>
-      <c r="C33" s="249"/>
-      <c r="D33" s="249"/>
-      <c r="E33" s="249"/>
-      <c r="F33" s="249"/>
-      <c r="G33" s="249"/>
-      <c r="H33" s="249"/>
-      <c r="I33" s="249"/>
-      <c r="J33" s="249"/>
-      <c r="K33" s="249"/>
-      <c r="L33" s="250"/>
-    </row>
-    <row r="34" spans="1:12" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="228"/>
-      <c r="B34" s="229"/>
-      <c r="C34" s="229"/>
-      <c r="D34" s="229"/>
-      <c r="E34" s="229"/>
-      <c r="F34" s="229"/>
-      <c r="G34" s="229"/>
-      <c r="H34" s="229"/>
-      <c r="I34" s="229"/>
-      <c r="J34" s="229"/>
-      <c r="K34" s="229"/>
-      <c r="L34" s="230"/>
-    </row>
-    <row r="35" spans="1:12" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="258" t="s">
+      <c r="C39" s="276"/>
+      <c r="D39" s="276"/>
+      <c r="E39" s="276"/>
+      <c r="F39" s="276"/>
+      <c r="G39" s="276"/>
+      <c r="H39" s="276"/>
+      <c r="I39" s="276"/>
+      <c r="J39" s="276"/>
+      <c r="K39" s="276"/>
+      <c r="L39" s="277"/>
+    </row>
+    <row r="40" spans="1:14" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="228"/>
+      <c r="B40" s="229"/>
+      <c r="C40" s="229"/>
+      <c r="D40" s="229"/>
+      <c r="E40" s="229"/>
+      <c r="F40" s="229"/>
+      <c r="G40" s="229"/>
+      <c r="H40" s="229"/>
+      <c r="I40" s="229"/>
+      <c r="J40" s="229"/>
+      <c r="K40" s="229"/>
+      <c r="L40" s="230"/>
+    </row>
+    <row r="41" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="278" t="s">
         <v>327</v>
       </c>
-      <c r="B35" s="259"/>
-      <c r="C35" s="259"/>
-      <c r="D35" s="259"/>
-      <c r="E35" s="259"/>
-      <c r="F35" s="259"/>
-      <c r="G35" s="259"/>
-      <c r="H35" s="259"/>
-      <c r="I35" s="259"/>
-      <c r="J35" s="259"/>
-      <c r="K35" s="259"/>
-      <c r="L35" s="260"/>
-    </row>
-    <row r="36" spans="1:12" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="231" t="s">
+      <c r="B41" s="279"/>
+      <c r="C41" s="279"/>
+      <c r="D41" s="279"/>
+      <c r="E41" s="279"/>
+      <c r="F41" s="279"/>
+      <c r="G41" s="279"/>
+      <c r="H41" s="279"/>
+      <c r="I41" s="279"/>
+      <c r="J41" s="279"/>
+      <c r="K41" s="279"/>
+      <c r="L41" s="280"/>
+    </row>
+    <row r="42" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="231" t="s">
         <v>325</v>
       </c>
-      <c r="B36" s="249" t="s">
+      <c r="B42" s="276" t="s">
         <v>212</v>
       </c>
-      <c r="C36" s="249"/>
-      <c r="D36" s="249"/>
-      <c r="E36" s="249"/>
-      <c r="F36" s="249"/>
-      <c r="G36" s="249"/>
-      <c r="H36" s="249"/>
-      <c r="I36" s="249"/>
-      <c r="J36" s="249"/>
-      <c r="K36" s="249"/>
-      <c r="L36" s="250"/>
-    </row>
-    <row r="37" spans="1:12" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="232" t="s">
+      <c r="C42" s="276"/>
+      <c r="D42" s="276"/>
+      <c r="E42" s="276"/>
+      <c r="F42" s="276"/>
+      <c r="G42" s="276"/>
+      <c r="H42" s="276"/>
+      <c r="I42" s="276"/>
+      <c r="J42" s="276"/>
+      <c r="K42" s="276"/>
+      <c r="L42" s="277"/>
+    </row>
+    <row r="43" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="232" t="s">
         <v>326</v>
       </c>
-      <c r="B37" s="251" t="s">
+      <c r="B43" s="282" t="s">
         <v>329</v>
       </c>
-      <c r="C37" s="251"/>
-      <c r="D37" s="251"/>
-      <c r="E37" s="251"/>
-      <c r="F37" s="251"/>
-      <c r="G37" s="251"/>
-      <c r="H37" s="251"/>
-      <c r="I37" s="251"/>
-      <c r="J37" s="251"/>
-      <c r="K37" s="251"/>
-      <c r="L37" s="252"/>
-    </row>
-    <row r="38" spans="1:12" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="160"/>
-      <c r="B38" s="113"/>
-      <c r="C38" s="113"/>
-      <c r="D38" s="113"/>
-      <c r="E38" s="113"/>
-      <c r="F38" s="113"/>
-      <c r="G38" s="113"/>
-      <c r="H38" s="113"/>
-      <c r="I38" s="113"/>
-      <c r="J38" s="113"/>
-      <c r="K38" s="113"/>
-      <c r="L38" s="113"/>
-    </row>
-    <row r="39" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="253" t="s">
+      <c r="C43" s="282"/>
+      <c r="D43" s="282"/>
+      <c r="E43" s="282"/>
+      <c r="F43" s="282"/>
+      <c r="G43" s="282"/>
+      <c r="H43" s="282"/>
+      <c r="I43" s="282"/>
+      <c r="J43" s="282"/>
+      <c r="K43" s="282"/>
+      <c r="L43" s="283"/>
+    </row>
+    <row r="44" spans="1:14" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="160"/>
+      <c r="B44" s="113"/>
+      <c r="C44" s="113"/>
+      <c r="D44" s="113"/>
+      <c r="E44" s="113"/>
+      <c r="F44" s="113"/>
+      <c r="G44" s="113"/>
+      <c r="H44" s="113"/>
+      <c r="I44" s="113"/>
+      <c r="J44" s="113"/>
+      <c r="K44" s="113"/>
+      <c r="L44" s="113"/>
+    </row>
+    <row r="45" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="284" t="s">
         <v>240</v>
       </c>
-      <c r="B39" s="254"/>
-      <c r="C39" s="254"/>
-      <c r="D39" s="254"/>
-      <c r="E39" s="254"/>
-      <c r="F39" s="254"/>
-      <c r="G39" s="254"/>
-      <c r="H39" s="254"/>
-      <c r="I39" s="254"/>
-      <c r="J39" s="254"/>
-      <c r="K39" s="254"/>
-      <c r="L39" s="255"/>
-    </row>
-    <row r="40" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="235" t="s">
+      <c r="B45" s="285"/>
+      <c r="C45" s="285"/>
+      <c r="D45" s="285"/>
+      <c r="E45" s="285"/>
+      <c r="F45" s="285"/>
+      <c r="G45" s="285"/>
+      <c r="H45" s="285"/>
+      <c r="I45" s="285"/>
+      <c r="J45" s="285"/>
+      <c r="K45" s="285"/>
+      <c r="L45" s="286"/>
+    </row>
+    <row r="46" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="235" t="s">
         <v>213</v>
       </c>
-      <c r="B40" s="161"/>
-      <c r="C40" s="161"/>
-      <c r="D40" s="161"/>
-      <c r="E40" s="161"/>
-      <c r="F40" s="161"/>
-      <c r="G40" s="161"/>
-      <c r="H40" s="161"/>
-      <c r="I40" s="161"/>
-      <c r="J40" s="161"/>
-      <c r="K40" s="161"/>
-      <c r="L40" s="162"/>
-    </row>
-    <row r="41" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="84"/>
-      <c r="C41" s="84"/>
-      <c r="D41" s="84"/>
-      <c r="E41" s="84"/>
-      <c r="F41" s="84"/>
-      <c r="G41" s="84"/>
-      <c r="H41" s="84"/>
-      <c r="I41" s="84"/>
-      <c r="J41" s="84"/>
-      <c r="K41" s="84"/>
-      <c r="L41" s="84"/>
-    </row>
-    <row r="42" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="163" t="s">
+      <c r="B46" s="161"/>
+      <c r="C46" s="161"/>
+      <c r="D46" s="161"/>
+      <c r="E46" s="161"/>
+      <c r="F46" s="161"/>
+      <c r="G46" s="161"/>
+      <c r="H46" s="161"/>
+      <c r="I46" s="161"/>
+      <c r="J46" s="161"/>
+      <c r="K46" s="161"/>
+      <c r="L46" s="162"/>
+    </row>
+    <row r="47" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="84"/>
+      <c r="C47" s="84"/>
+      <c r="D47" s="84"/>
+      <c r="E47" s="84"/>
+      <c r="F47" s="84"/>
+      <c r="G47" s="84"/>
+      <c r="H47" s="84"/>
+      <c r="I47" s="84"/>
+      <c r="J47" s="84"/>
+      <c r="K47" s="84"/>
+      <c r="L47" s="84"/>
+    </row>
+    <row r="48" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="163" t="s">
         <v>166</v>
       </c>
-      <c r="B42" s="164"/>
-      <c r="C42" s="164"/>
-      <c r="D42" s="165"/>
-      <c r="E42" s="164"/>
-      <c r="F42" s="164"/>
-      <c r="G42" s="164"/>
-      <c r="H42" s="164"/>
-      <c r="I42" s="164"/>
-      <c r="J42" s="164"/>
-      <c r="K42" s="164"/>
-      <c r="L42" s="166"/>
-    </row>
-    <row r="43" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="167"/>
-      <c r="B43" s="168" t="s">
-        <v>62</v>
-      </c>
-      <c r="C43" s="169" t="s">
-        <v>79</v>
-      </c>
-      <c r="D43" s="169"/>
-      <c r="E43" s="169"/>
-      <c r="F43" s="169"/>
-      <c r="G43" s="169"/>
-      <c r="H43" s="169"/>
-      <c r="I43" s="169"/>
-      <c r="J43" s="169"/>
-      <c r="K43" s="169"/>
-      <c r="L43" s="170"/>
-    </row>
-    <row r="44" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="167"/>
-      <c r="B44" s="168" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" s="169" t="s">
-        <v>91</v>
-      </c>
-      <c r="D44" s="169"/>
-      <c r="E44" s="169"/>
-      <c r="F44" s="169"/>
-      <c r="G44" s="169"/>
-      <c r="H44" s="169"/>
-      <c r="I44" s="169"/>
-      <c r="J44" s="169"/>
-      <c r="K44" s="169"/>
-      <c r="L44" s="170"/>
-    </row>
-    <row r="45" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="167"/>
-      <c r="B45" s="168" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="256" t="s">
-        <v>313</v>
-      </c>
-      <c r="D45" s="256"/>
-      <c r="E45" s="256"/>
-      <c r="F45" s="256"/>
-      <c r="G45" s="256"/>
-      <c r="H45" s="256"/>
-      <c r="I45" s="256"/>
-      <c r="J45" s="256"/>
-      <c r="K45" s="256"/>
-      <c r="L45" s="257"/>
-    </row>
-    <row r="46" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="167"/>
-      <c r="B46" s="168" t="s">
-        <v>314</v>
-      </c>
-      <c r="C46" s="256" t="s">
-        <v>315</v>
-      </c>
-      <c r="D46" s="256"/>
-      <c r="E46" s="256"/>
-      <c r="F46" s="256"/>
-      <c r="G46" s="256"/>
-      <c r="H46" s="256"/>
-      <c r="I46" s="256"/>
-      <c r="J46" s="256"/>
-      <c r="K46" s="256"/>
-      <c r="L46" s="257"/>
-    </row>
-    <row r="47" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="167"/>
-      <c r="B47" s="168" t="s">
-        <v>384</v>
-      </c>
-      <c r="C47" s="256" t="s">
-        <v>385</v>
-      </c>
-      <c r="D47" s="256"/>
-      <c r="E47" s="256"/>
-      <c r="F47" s="256"/>
-      <c r="G47" s="256"/>
-      <c r="H47" s="256"/>
-      <c r="I47" s="256"/>
-      <c r="J47" s="256"/>
-      <c r="K47" s="256"/>
-      <c r="L47" s="257"/>
-    </row>
-    <row r="48" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="167"/>
-      <c r="B48" s="168" t="s">
-        <v>138</v>
-      </c>
-      <c r="C48" s="256" t="s">
-        <v>139</v>
-      </c>
-      <c r="D48" s="256"/>
-      <c r="E48" s="256"/>
-      <c r="F48" s="256"/>
-      <c r="G48" s="256"/>
-      <c r="H48" s="256"/>
-      <c r="I48" s="256"/>
-      <c r="J48" s="256"/>
-      <c r="K48" s="256"/>
-      <c r="L48" s="257"/>
-    </row>
-    <row r="49" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="164"/>
+      <c r="C48" s="164"/>
+      <c r="D48" s="165"/>
+      <c r="E48" s="164"/>
+      <c r="F48" s="164"/>
+      <c r="G48" s="164"/>
+      <c r="H48" s="164"/>
+      <c r="I48" s="164"/>
+      <c r="J48" s="164"/>
+      <c r="K48" s="164"/>
+      <c r="L48" s="166"/>
+    </row>
+    <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="167"/>
       <c r="B49" s="168" t="s">
-        <v>238</v>
-      </c>
-      <c r="C49" s="256" t="s">
-        <v>239</v>
-      </c>
-      <c r="D49" s="256"/>
-      <c r="E49" s="256"/>
-      <c r="F49" s="256"/>
-      <c r="G49" s="256"/>
-      <c r="H49" s="256"/>
-      <c r="I49" s="256"/>
-      <c r="J49" s="256"/>
-      <c r="K49" s="256"/>
-      <c r="L49" s="257"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="C49" s="169" t="s">
+        <v>79</v>
+      </c>
+      <c r="D49" s="169"/>
+      <c r="E49" s="169"/>
+      <c r="F49" s="169"/>
+      <c r="G49" s="169"/>
+      <c r="H49" s="169"/>
+      <c r="I49" s="169"/>
+      <c r="J49" s="169"/>
+      <c r="K49" s="169"/>
+      <c r="L49" s="170"/>
+    </row>
+    <row r="50" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="167"/>
       <c r="B50" s="168" t="s">
-        <v>203</v>
+        <v>81</v>
       </c>
       <c r="C50" s="169" t="s">
-        <v>316</v>
+        <v>91</v>
       </c>
       <c r="D50" s="169"/>
       <c r="E50" s="169"/>
@@ -15853,173 +15958,306 @@
       <c r="K50" s="169"/>
       <c r="L50" s="170"/>
     </row>
-    <row r="51" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="167"/>
       <c r="B51" s="168" t="s">
-        <v>63</v>
-      </c>
-      <c r="C51" s="256" t="s">
-        <v>317</v>
-      </c>
-      <c r="D51" s="256"/>
-      <c r="E51" s="256"/>
-      <c r="F51" s="256"/>
-      <c r="G51" s="256"/>
-      <c r="H51" s="256"/>
-      <c r="I51" s="256"/>
-      <c r="J51" s="256"/>
-      <c r="K51" s="256"/>
-      <c r="L51" s="257"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="C51" s="264" t="s">
+        <v>313</v>
+      </c>
+      <c r="D51" s="264"/>
+      <c r="E51" s="264"/>
+      <c r="F51" s="264"/>
+      <c r="G51" s="264"/>
+      <c r="H51" s="264"/>
+      <c r="I51" s="264"/>
+      <c r="J51" s="264"/>
+      <c r="K51" s="264"/>
+      <c r="L51" s="265"/>
+    </row>
+    <row r="52" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="167"/>
       <c r="B52" s="168" t="s">
+        <v>314</v>
+      </c>
+      <c r="C52" s="264" t="s">
+        <v>315</v>
+      </c>
+      <c r="D52" s="264"/>
+      <c r="E52" s="264"/>
+      <c r="F52" s="264"/>
+      <c r="G52" s="264"/>
+      <c r="H52" s="264"/>
+      <c r="I52" s="264"/>
+      <c r="J52" s="264"/>
+      <c r="K52" s="264"/>
+      <c r="L52" s="265"/>
+    </row>
+    <row r="53" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="167"/>
+      <c r="B53" s="168" t="s">
+        <v>383</v>
+      </c>
+      <c r="C53" s="264" t="s">
+        <v>384</v>
+      </c>
+      <c r="D53" s="264"/>
+      <c r="E53" s="264"/>
+      <c r="F53" s="264"/>
+      <c r="G53" s="264"/>
+      <c r="H53" s="264"/>
+      <c r="I53" s="264"/>
+      <c r="J53" s="264"/>
+      <c r="K53" s="264"/>
+      <c r="L53" s="265"/>
+    </row>
+    <row r="54" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="167"/>
+      <c r="B54" s="168" t="s">
+        <v>138</v>
+      </c>
+      <c r="C54" s="264" t="s">
+        <v>139</v>
+      </c>
+      <c r="D54" s="264"/>
+      <c r="E54" s="264"/>
+      <c r="F54" s="264"/>
+      <c r="G54" s="264"/>
+      <c r="H54" s="264"/>
+      <c r="I54" s="264"/>
+      <c r="J54" s="264"/>
+      <c r="K54" s="264"/>
+      <c r="L54" s="265"/>
+    </row>
+    <row r="55" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="167"/>
+      <c r="B55" s="168" t="s">
+        <v>238</v>
+      </c>
+      <c r="C55" s="264" t="s">
+        <v>239</v>
+      </c>
+      <c r="D55" s="264"/>
+      <c r="E55" s="264"/>
+      <c r="F55" s="264"/>
+      <c r="G55" s="264"/>
+      <c r="H55" s="264"/>
+      <c r="I55" s="264"/>
+      <c r="J55" s="264"/>
+      <c r="K55" s="264"/>
+      <c r="L55" s="265"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A56" s="167"/>
+      <c r="B56" s="168" t="s">
+        <v>203</v>
+      </c>
+      <c r="C56" s="169" t="s">
+        <v>316</v>
+      </c>
+      <c r="D56" s="169"/>
+      <c r="E56" s="169"/>
+      <c r="F56" s="169"/>
+      <c r="G56" s="169"/>
+      <c r="H56" s="169"/>
+      <c r="I56" s="169"/>
+      <c r="J56" s="169"/>
+      <c r="K56" s="169"/>
+      <c r="L56" s="170"/>
+    </row>
+    <row r="57" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="167"/>
+      <c r="B57" s="168" t="s">
+        <v>63</v>
+      </c>
+      <c r="C57" s="264" t="s">
+        <v>317</v>
+      </c>
+      <c r="D57" s="264"/>
+      <c r="E57" s="264"/>
+      <c r="F57" s="264"/>
+      <c r="G57" s="264"/>
+      <c r="H57" s="264"/>
+      <c r="I57" s="264"/>
+      <c r="J57" s="264"/>
+      <c r="K57" s="264"/>
+      <c r="L57" s="265"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A58" s="167"/>
+      <c r="B58" s="168" t="s">
         <v>75</v>
       </c>
-      <c r="C52" s="169" t="s">
+      <c r="C58" s="169" t="s">
         <v>76</v>
       </c>
-      <c r="D52" s="169"/>
-      <c r="E52" s="169"/>
-      <c r="F52" s="169"/>
-      <c r="G52" s="169"/>
-      <c r="H52" s="169"/>
-      <c r="I52" s="169"/>
-      <c r="J52" s="169"/>
-      <c r="K52" s="169"/>
-      <c r="L52" s="170"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A53" s="171"/>
-      <c r="B53" s="172" t="s">
+      <c r="D58" s="169"/>
+      <c r="E58" s="169"/>
+      <c r="F58" s="169"/>
+      <c r="G58" s="169"/>
+      <c r="H58" s="169"/>
+      <c r="I58" s="169"/>
+      <c r="J58" s="169"/>
+      <c r="K58" s="169"/>
+      <c r="L58" s="170"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A59" s="171"/>
+      <c r="B59" s="172" t="s">
         <v>159</v>
       </c>
-      <c r="C53" s="173" t="s">
+      <c r="C59" s="173" t="s">
         <v>160</v>
       </c>
-      <c r="D53" s="173"/>
-      <c r="E53" s="173"/>
-      <c r="F53" s="173"/>
-      <c r="G53" s="173"/>
-      <c r="H53" s="173"/>
-      <c r="I53" s="173"/>
-      <c r="J53" s="173"/>
-      <c r="K53" s="173"/>
-      <c r="L53" s="174"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A55" s="1" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A58" s="45" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A59" s="45" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A60" s="45"/>
+      <c r="D59" s="173"/>
+      <c r="E59" s="173"/>
+      <c r="F59" s="173"/>
+      <c r="G59" s="173"/>
+      <c r="H59" s="173"/>
+      <c r="I59" s="173"/>
+      <c r="J59" s="173"/>
+      <c r="K59" s="173"/>
+      <c r="L59" s="174"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A64" s="45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A65" s="45" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A66" s="45"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A67" s="340" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A68" s="339" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A69" s="45" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A70" s="45"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A62" s="45" t="s">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A72" s="45" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A64" s="1" t="s">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="246" t="s">
-        <v>356</v>
-      </c>
-      <c r="B65" s="246"/>
-      <c r="C65" s="246"/>
-      <c r="D65" s="246"/>
-      <c r="E65" s="246"/>
-      <c r="F65" s="246"/>
-      <c r="G65" s="246"/>
-      <c r="H65" s="246"/>
-      <c r="I65" s="246"/>
-      <c r="J65" s="246"/>
-      <c r="K65" s="246"/>
-      <c r="L65" s="246"/>
-    </row>
-    <row r="70" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="71" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="75" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="281" t="s">
+        <v>399</v>
+      </c>
+      <c r="B75" s="281"/>
+      <c r="C75" s="281"/>
+      <c r="D75" s="281"/>
+      <c r="E75" s="281"/>
+      <c r="F75" s="281"/>
+      <c r="G75" s="281"/>
+      <c r="H75" s="281"/>
+      <c r="I75" s="281"/>
+      <c r="J75" s="281"/>
+      <c r="K75" s="281"/>
+      <c r="L75" s="281"/>
+    </row>
+    <row r="80" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="81" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="41">
-    <mergeCell ref="A17:L17"/>
+  <mergeCells count="46">
+    <mergeCell ref="B12:L12"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="A75:L75"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="B39:L39"/>
+    <mergeCell ref="B42:L42"/>
+    <mergeCell ref="B43:L43"/>
+    <mergeCell ref="A45:L45"/>
+    <mergeCell ref="C51:L51"/>
+    <mergeCell ref="C54:L54"/>
+    <mergeCell ref="C55:L55"/>
+    <mergeCell ref="C52:L52"/>
+    <mergeCell ref="C57:L57"/>
+    <mergeCell ref="A41:L41"/>
+    <mergeCell ref="C53:L53"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="B25:L25"/>
+    <mergeCell ref="B26:L26"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B30:L30"/>
+    <mergeCell ref="A31:L31"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="B34:L34"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="A23:L23"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A4:L4"/>
     <mergeCell ref="N4:R4"/>
     <mergeCell ref="A5:L5"/>
     <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A14:L14"/>
     <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A22:L22"/>
     <mergeCell ref="B7:L7"/>
     <mergeCell ref="B8:L8"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B18:L18"/>
-    <mergeCell ref="B19:L19"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="B22:L22"/>
-    <mergeCell ref="B23:L23"/>
-    <mergeCell ref="B24:L24"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="B26:L26"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="A65:L65"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="C45:L45"/>
-    <mergeCell ref="C48:L48"/>
-    <mergeCell ref="C49:L49"/>
-    <mergeCell ref="C46:L46"/>
-    <mergeCell ref="C51:L51"/>
-    <mergeCell ref="A35:L35"/>
-    <mergeCell ref="C47:L47"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="B11:L11"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A58" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
-    <hyperlink ref="A59" r:id="rId2" xr:uid="{66F54200-A2AB-43DA-A0E0-F2A25A075EE5}"/>
-    <hyperlink ref="A62" r:id="rId3" xr:uid="{A0F8DE06-D9FC-495F-9A01-AA199CB82365}"/>
-    <hyperlink ref="A39:L39" r:id="rId4" display="LETS START (visual directions as pdf)" xr:uid="{0D075873-7EBB-4309-B00A-6A62EA192A0C}"/>
-    <hyperlink ref="A40" r:id="rId5" xr:uid="{25154A32-BA44-496E-9945-086DE0980DBD}"/>
+    <hyperlink ref="A64" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
+    <hyperlink ref="A65" r:id="rId2" xr:uid="{66F54200-A2AB-43DA-A0E0-F2A25A075EE5}"/>
+    <hyperlink ref="A72" r:id="rId3" xr:uid="{A0F8DE06-D9FC-495F-9A01-AA199CB82365}"/>
+    <hyperlink ref="A45:L45" r:id="rId4" display="LETS START (visual directions as pdf)" xr:uid="{0D075873-7EBB-4309-B00A-6A62EA192A0C}"/>
+    <hyperlink ref="A46" r:id="rId5" xr:uid="{25154A32-BA44-496E-9945-086DE0980DBD}"/>
+    <hyperlink ref="A69" r:id="rId6" xr:uid="{AA792CE4-4071-4CE8-87C6-993A0BA6C6A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -31226,10 +31464,10 @@
         <v>45666</v>
       </c>
       <c r="B6" s="149" t="s">
+        <v>356</v>
+      </c>
+      <c r="C6" s="56" t="s">
         <v>357</v>
-      </c>
-      <c r="C6" s="56" t="s">
-        <v>358</v>
       </c>
       <c r="D6" s="55">
         <v>3</v>
@@ -31250,10 +31488,10 @@
         <v>45670</v>
       </c>
       <c r="B7" s="149" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D7" s="55">
         <v>0.5</v>
@@ -31274,10 +31512,10 @@
         <v>45671</v>
       </c>
       <c r="B8" s="149" t="s">
+        <v>388</v>
+      </c>
+      <c r="C8" s="56" t="s">
         <v>389</v>
-      </c>
-      <c r="C8" s="56" t="s">
-        <v>390</v>
       </c>
       <c r="D8" s="55">
         <v>0.5</v>
@@ -31696,7 +31934,7 @@
       <c r="F4" s="297"/>
       <c r="G4" s="298"/>
       <c r="N4" s="141" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
@@ -31935,7 +32173,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B24" s="94">
         <f>TribalWater!H7</f>
@@ -31945,12 +32183,12 @@
       <c r="D24" s="111"/>
       <c r="E24" s="28"/>
       <c r="N24" s="141" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B25" s="236">
         <f>1-B24</f>
@@ -31960,7 +32198,7 @@
       <c r="D25" s="111"/>
       <c r="E25" s="28"/>
       <c r="N25" s="141" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
@@ -37748,7 +37986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876BA06C-E963-43DD-B933-307F043834EF}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:D14"/>
     </sheetView>
   </sheetViews>
@@ -37763,40 +38001,40 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="237" t="s">
+        <v>363</v>
+      </c>
+      <c r="B4" s="237" t="s">
         <v>364</v>
       </c>
-      <c r="B4" s="237" t="s">
+      <c r="C4" s="238" t="s">
         <v>365</v>
       </c>
-      <c r="C4" s="238" t="s">
+      <c r="D4" s="238" t="s">
         <v>366</v>
       </c>
-      <c r="D4" s="238" t="s">
-        <v>367</v>
-      </c>
       <c r="F4" s="238" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="G4" s="238" t="s">
+        <v>373</v>
+      </c>
+      <c r="H4" s="238" t="s">
         <v>374</v>
-      </c>
-      <c r="H4" s="238" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="23" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B5" s="23" t="s">
         <v>244</v>
@@ -37819,7 +38057,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="23" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B6" s="23" t="s">
         <v>243</v>
@@ -37842,7 +38080,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="23" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>242</v>
@@ -37865,7 +38103,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="23" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B8" s="23" t="s">
         <v>242</v>
@@ -37888,7 +38126,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B9" s="23" t="s">
         <v>243</v>
@@ -37900,7 +38138,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="23" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B10" s="23" t="s">
         <v>242</v>
@@ -37912,7 +38150,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="23" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B11" s="23" t="s">
         <v>243</v>
@@ -37924,7 +38162,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="23" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B12" s="23" t="s">
         <v>242</v>
@@ -37936,7 +38174,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="23" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B13" s="23" t="s">
         <v>243</v>
@@ -37964,23 +38202,23 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="237" t="s">
+        <v>376</v>
+      </c>
+      <c r="B18" s="245" t="s">
         <v>377</v>
       </c>
-      <c r="B18" s="245" t="s">
+      <c r="C18" s="245" t="s">
         <v>378</v>
-      </c>
-      <c r="C18" s="245" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="23" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B19" s="24">
         <v>769208</v>
@@ -37991,7 +38229,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="23" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B20" s="24">
         <v>15340</v>
@@ -38002,7 +38240,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="23" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B21" s="24">
         <v>2844</v>
@@ -38013,7 +38251,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="23" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B22" s="24">
         <v>13000</v>
@@ -38074,16 +38312,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="322" t="e">
+      <c r="A1" s="321" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="322"/>
-      <c r="C1" s="322"/>
-      <c r="D1" s="322"/>
-      <c r="E1" s="322"/>
-      <c r="F1" s="322"/>
-      <c r="G1" s="322"/>
+      <c r="B1" s="321"/>
+      <c r="C1" s="321"/>
+      <c r="D1" s="321"/>
+      <c r="E1" s="321"/>
+      <c r="F1" s="321"/>
+      <c r="G1" s="321"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -38192,11 +38430,11 @@
         <v>80</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="321"/>
-      <c r="D10" s="321"/>
-      <c r="E10" s="321"/>
-      <c r="F10" s="321"/>
-      <c r="G10" s="321"/>
+      <c r="C10" s="322"/>
+      <c r="D10" s="322"/>
+      <c r="E10" s="322"/>
+      <c r="F10" s="322"/>
+      <c r="G10" s="322"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -39459,12 +39697,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -39472,6 +39704,12 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>

</xml_diff>

<commit_message>
Add line See visuals of key ideas to ReadMe-Directions worksheet in Excel file
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464EC48D-2716-4A20-B930-F71F02B4D1DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C8C66A-1F32-41AF-AE1B-35BE64C14302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-1260" windowWidth="29040" windowHeight="15720" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="403">
   <si>
     <t>Year 1</t>
   </si>
@@ -2053,6 +2053,12 @@
   <si>
     <t>eporse@ucanr.edu</t>
   </si>
+  <si>
+    <t>See Let's Start Guide for visualizations of Key Ideas ---</t>
+  </si>
+  <si>
+    <t>Here</t>
+  </si>
 </sst>
 </file>
 
@@ -2702,7 +2708,7 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="341">
+  <cellXfs count="343">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3357,6 +3363,59 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3411,12 +3470,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3441,44 +3494,14 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3582,11 +3605,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3609,35 +3632,24 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="7" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="20% - Accent1" xfId="12" builtinId="30"/>
@@ -15082,7 +15094,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EA02F4-5F19-409C-8BC6-A0D8FEB3A90D}">
-  <dimension ref="A1:R81"/>
+  <dimension ref="A1:R82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection sqref="A1:L1"/>
@@ -15104,20 +15116,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="249" t="s">
+      <c r="A1" s="268" t="s">
         <v>351</v>
       </c>
-      <c r="B1" s="249"/>
-      <c r="C1" s="249"/>
-      <c r="D1" s="249"/>
-      <c r="E1" s="249"/>
-      <c r="F1" s="249"/>
-      <c r="G1" s="249"/>
-      <c r="H1" s="249"/>
-      <c r="I1" s="249"/>
-      <c r="J1" s="249"/>
-      <c r="K1" s="249"/>
-      <c r="L1" s="249"/>
+      <c r="B1" s="268"/>
+      <c r="C1" s="268"/>
+      <c r="D1" s="268"/>
+      <c r="E1" s="268"/>
+      <c r="F1" s="268"/>
+      <c r="G1" s="268"/>
+      <c r="H1" s="268"/>
+      <c r="I1" s="268"/>
+      <c r="J1" s="268"/>
+      <c r="K1" s="268"/>
+      <c r="L1" s="268"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -15143,41 +15155,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="250" t="s">
+      <c r="A4" s="269" t="s">
         <v>352</v>
       </c>
-      <c r="B4" s="251"/>
-      <c r="C4" s="251"/>
-      <c r="D4" s="251"/>
-      <c r="E4" s="251"/>
-      <c r="F4" s="251"/>
-      <c r="G4" s="251"/>
-      <c r="H4" s="251"/>
-      <c r="I4" s="251"/>
-      <c r="J4" s="251"/>
-      <c r="K4" s="251"/>
-      <c r="L4" s="252"/>
-      <c r="N4" s="253"/>
-      <c r="O4" s="253"/>
-      <c r="P4" s="253"/>
-      <c r="Q4" s="253"/>
-      <c r="R4" s="253"/>
+      <c r="B4" s="270"/>
+      <c r="C4" s="270"/>
+      <c r="D4" s="270"/>
+      <c r="E4" s="270"/>
+      <c r="F4" s="270"/>
+      <c r="G4" s="270"/>
+      <c r="H4" s="270"/>
+      <c r="I4" s="270"/>
+      <c r="J4" s="270"/>
+      <c r="K4" s="270"/>
+      <c r="L4" s="271"/>
+      <c r="N4" s="272"/>
+      <c r="O4" s="272"/>
+      <c r="P4" s="272"/>
+      <c r="Q4" s="272"/>
+      <c r="R4" s="272"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="254" t="s">
+      <c r="A5" s="273" t="s">
         <v>335</v>
       </c>
-      <c r="B5" s="255"/>
-      <c r="C5" s="255"/>
-      <c r="D5" s="255"/>
-      <c r="E5" s="255"/>
-      <c r="F5" s="255"/>
-      <c r="G5" s="255"/>
-      <c r="H5" s="255"/>
-      <c r="I5" s="255"/>
-      <c r="J5" s="255"/>
-      <c r="K5" s="255"/>
-      <c r="L5" s="256"/>
+      <c r="B5" s="274"/>
+      <c r="C5" s="274"/>
+      <c r="D5" s="274"/>
+      <c r="E5" s="274"/>
+      <c r="F5" s="274"/>
+      <c r="G5" s="274"/>
+      <c r="H5" s="274"/>
+      <c r="I5" s="274"/>
+      <c r="J5" s="274"/>
+      <c r="K5" s="274"/>
+      <c r="L5" s="275"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15185,20 +15197,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="254" t="s">
+      <c r="A6" s="273" t="s">
         <v>353</v>
       </c>
-      <c r="B6" s="255"/>
-      <c r="C6" s="255"/>
-      <c r="D6" s="255"/>
-      <c r="E6" s="255"/>
-      <c r="F6" s="255"/>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="255"/>
-      <c r="J6" s="255"/>
-      <c r="K6" s="255"/>
-      <c r="L6" s="256"/>
+      <c r="B6" s="274"/>
+      <c r="C6" s="274"/>
+      <c r="D6" s="274"/>
+      <c r="E6" s="274"/>
+      <c r="F6" s="274"/>
+      <c r="G6" s="274"/>
+      <c r="H6" s="274"/>
+      <c r="I6" s="274"/>
+      <c r="J6" s="274"/>
+      <c r="K6" s="274"/>
+      <c r="L6" s="275"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15207,19 +15219,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="233"/>
-      <c r="B7" s="255" t="s">
+      <c r="B7" s="274" t="s">
         <v>354</v>
       </c>
-      <c r="C7" s="255"/>
-      <c r="D7" s="255"/>
-      <c r="E7" s="255"/>
-      <c r="F7" s="255"/>
-      <c r="G7" s="255"/>
-      <c r="H7" s="255"/>
-      <c r="I7" s="255"/>
-      <c r="J7" s="255"/>
-      <c r="K7" s="255"/>
-      <c r="L7" s="256"/>
+      <c r="C7" s="274"/>
+      <c r="D7" s="274"/>
+      <c r="E7" s="274"/>
+      <c r="F7" s="274"/>
+      <c r="G7" s="274"/>
+      <c r="H7" s="274"/>
+      <c r="I7" s="274"/>
+      <c r="J7" s="274"/>
+      <c r="K7" s="274"/>
+      <c r="L7" s="275"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15228,19 +15240,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="234"/>
-      <c r="B8" s="272" t="s">
+      <c r="B8" s="289" t="s">
         <v>355</v>
       </c>
-      <c r="C8" s="272"/>
-      <c r="D8" s="272"/>
-      <c r="E8" s="272"/>
-      <c r="F8" s="272"/>
-      <c r="G8" s="272"/>
-      <c r="H8" s="272"/>
-      <c r="I8" s="272"/>
-      <c r="J8" s="272"/>
-      <c r="K8" s="272"/>
-      <c r="L8" s="273"/>
+      <c r="C8" s="289"/>
+      <c r="D8" s="289"/>
+      <c r="E8" s="289"/>
+      <c r="F8" s="289"/>
+      <c r="G8" s="289"/>
+      <c r="H8" s="289"/>
+      <c r="I8" s="289"/>
+      <c r="J8" s="289"/>
+      <c r="K8" s="289"/>
+      <c r="L8" s="290"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15262,73 +15274,73 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="330" t="s">
+      <c r="A10" s="291" t="s">
         <v>390</v>
       </c>
-      <c r="B10" s="331"/>
-      <c r="C10" s="331"/>
-      <c r="D10" s="331"/>
-      <c r="E10" s="331"/>
-      <c r="F10" s="331"/>
-      <c r="G10" s="331"/>
-      <c r="H10" s="331"/>
-      <c r="I10" s="331"/>
-      <c r="J10" s="331"/>
-      <c r="K10" s="331"/>
-      <c r="L10" s="332"/>
+      <c r="B10" s="292"/>
+      <c r="C10" s="292"/>
+      <c r="D10" s="292"/>
+      <c r="E10" s="292"/>
+      <c r="F10" s="292"/>
+      <c r="G10" s="292"/>
+      <c r="H10" s="292"/>
+      <c r="I10" s="292"/>
+      <c r="J10" s="292"/>
+      <c r="K10" s="292"/>
+      <c r="L10" s="293"/>
     </row>
     <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="333" t="s">
+      <c r="A11" s="246" t="s">
         <v>391</v>
       </c>
-      <c r="B11" s="334" t="s">
+      <c r="B11" s="337" t="s">
         <v>394</v>
       </c>
-      <c r="C11" s="334"/>
-      <c r="D11" s="334"/>
-      <c r="E11" s="334"/>
-      <c r="F11" s="334"/>
-      <c r="G11" s="334"/>
-      <c r="H11" s="334"/>
-      <c r="I11" s="334"/>
-      <c r="J11" s="334"/>
-      <c r="K11" s="334"/>
-      <c r="L11" s="335"/>
+      <c r="C11" s="337"/>
+      <c r="D11" s="337"/>
+      <c r="E11" s="337"/>
+      <c r="F11" s="337"/>
+      <c r="G11" s="337"/>
+      <c r="H11" s="337"/>
+      <c r="I11" s="337"/>
+      <c r="J11" s="337"/>
+      <c r="K11" s="337"/>
+      <c r="L11" s="249"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="333" t="s">
+      <c r="A12" s="246" t="s">
         <v>392</v>
       </c>
-      <c r="B12" s="334" t="s">
+      <c r="B12" s="337" t="s">
         <v>395</v>
       </c>
-      <c r="C12" s="334"/>
-      <c r="D12" s="334"/>
-      <c r="E12" s="334"/>
-      <c r="F12" s="334"/>
-      <c r="G12" s="334"/>
-      <c r="H12" s="334"/>
-      <c r="I12" s="334"/>
-      <c r="J12" s="334"/>
-      <c r="K12" s="334"/>
-      <c r="L12" s="335"/>
+      <c r="C12" s="337"/>
+      <c r="D12" s="337"/>
+      <c r="E12" s="337"/>
+      <c r="F12" s="337"/>
+      <c r="G12" s="337"/>
+      <c r="H12" s="337"/>
+      <c r="I12" s="337"/>
+      <c r="J12" s="337"/>
+      <c r="K12" s="337"/>
+      <c r="L12" s="249"/>
     </row>
     <row r="13" spans="1:18" s="59" customFormat="1" ht="90.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="333"/>
-      <c r="B13" s="334"/>
-      <c r="C13" s="334"/>
-      <c r="D13" s="334"/>
-      <c r="E13" s="334"/>
-      <c r="F13" s="334"/>
-      <c r="G13" s="334"/>
-      <c r="H13" s="334"/>
-      <c r="I13" s="334"/>
-      <c r="J13" s="334"/>
-      <c r="K13" s="334"/>
-      <c r="L13" s="335"/>
+      <c r="A13" s="246"/>
+      <c r="B13" s="337"/>
+      <c r="C13" s="337"/>
+      <c r="D13" s="337"/>
+      <c r="E13" s="337"/>
+      <c r="F13" s="337"/>
+      <c r="G13" s="337"/>
+      <c r="H13" s="337"/>
+      <c r="I13" s="337"/>
+      <c r="J13" s="337"/>
+      <c r="K13" s="337"/>
+      <c r="L13" s="249"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="336" t="s">
+      <c r="A14" s="246" t="s">
         <v>393</v>
       </c>
       <c r="B14" s="337" t="s">
@@ -15343,610 +15355,610 @@
       <c r="I14" s="337"/>
       <c r="J14" s="337"/>
       <c r="K14" s="337"/>
-      <c r="L14" s="338"/>
+      <c r="L14" s="249"/>
     </row>
     <row r="15" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="113"/>
-      <c r="B15" s="113"/>
-      <c r="C15" s="113"/>
-      <c r="D15" s="113"/>
-      <c r="E15" s="113"/>
-      <c r="F15" s="113"/>
-      <c r="G15" s="113"/>
-      <c r="H15" s="113"/>
-      <c r="I15" s="113"/>
-      <c r="J15" s="113"/>
-      <c r="K15" s="113"/>
-      <c r="L15" s="113"/>
+      <c r="A15" s="338" t="s">
+        <v>401</v>
+      </c>
+      <c r="B15" s="339"/>
+      <c r="C15" s="339"/>
+      <c r="D15" s="339"/>
+      <c r="E15" s="342" t="s">
+        <v>402</v>
+      </c>
+      <c r="F15" s="340"/>
+      <c r="G15" s="340"/>
+      <c r="H15" s="340"/>
+      <c r="I15" s="340"/>
+      <c r="J15" s="340"/>
+      <c r="K15" s="340"/>
+      <c r="L15" s="341"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="257" t="s">
+      <c r="A16" s="113"/>
+      <c r="B16" s="113"/>
+      <c r="C16" s="113"/>
+      <c r="D16" s="113"/>
+      <c r="E16" s="113"/>
+      <c r="F16" s="113"/>
+      <c r="G16" s="113"/>
+      <c r="H16" s="113"/>
+      <c r="I16" s="113"/>
+      <c r="J16" s="113"/>
+      <c r="K16" s="113"/>
+      <c r="L16" s="113"/>
+    </row>
+    <row r="17" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="276" t="s">
         <v>205</v>
       </c>
-      <c r="B16" s="258"/>
-      <c r="C16" s="258"/>
-      <c r="D16" s="258"/>
-      <c r="E16" s="258"/>
-      <c r="F16" s="258"/>
-      <c r="G16" s="258"/>
-      <c r="H16" s="258"/>
-      <c r="I16" s="258"/>
-      <c r="J16" s="258"/>
-      <c r="K16" s="258"/>
-      <c r="L16" s="259"/>
-    </row>
-    <row r="17" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="260" t="s">
+      <c r="B17" s="277"/>
+      <c r="C17" s="277"/>
+      <c r="D17" s="277"/>
+      <c r="E17" s="277"/>
+      <c r="F17" s="277"/>
+      <c r="G17" s="277"/>
+      <c r="H17" s="277"/>
+      <c r="I17" s="277"/>
+      <c r="J17" s="277"/>
+      <c r="K17" s="277"/>
+      <c r="L17" s="278"/>
+    </row>
+    <row r="18" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="279" t="s">
         <v>336</v>
       </c>
-      <c r="B17" s="261"/>
-      <c r="C17" s="261"/>
-      <c r="D17" s="261"/>
-      <c r="E17" s="261"/>
-      <c r="F17" s="261"/>
-      <c r="G17" s="261"/>
-      <c r="H17" s="261"/>
-      <c r="I17" s="261"/>
-      <c r="J17" s="261"/>
-      <c r="K17" s="261"/>
-      <c r="L17" s="262"/>
-    </row>
-    <row r="18" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="263" t="s">
+      <c r="B18" s="280"/>
+      <c r="C18" s="280"/>
+      <c r="D18" s="280"/>
+      <c r="E18" s="280"/>
+      <c r="F18" s="280"/>
+      <c r="G18" s="280"/>
+      <c r="H18" s="280"/>
+      <c r="I18" s="280"/>
+      <c r="J18" s="280"/>
+      <c r="K18" s="280"/>
+      <c r="L18" s="281"/>
+    </row>
+    <row r="19" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="282" t="s">
         <v>337</v>
       </c>
-      <c r="B18" s="264"/>
-      <c r="C18" s="264"/>
-      <c r="D18" s="264"/>
-      <c r="E18" s="264"/>
-      <c r="F18" s="264"/>
-      <c r="G18" s="264"/>
-      <c r="H18" s="264"/>
-      <c r="I18" s="264"/>
-      <c r="J18" s="264"/>
-      <c r="K18" s="264"/>
-      <c r="L18" s="265"/>
-    </row>
-    <row r="19" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="263" t="s">
+      <c r="B19" s="260"/>
+      <c r="C19" s="260"/>
+      <c r="D19" s="260"/>
+      <c r="E19" s="260"/>
+      <c r="F19" s="260"/>
+      <c r="G19" s="260"/>
+      <c r="H19" s="260"/>
+      <c r="I19" s="260"/>
+      <c r="J19" s="260"/>
+      <c r="K19" s="260"/>
+      <c r="L19" s="261"/>
+    </row>
+    <row r="20" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="282" t="s">
         <v>206</v>
       </c>
-      <c r="B19" s="264"/>
-      <c r="C19" s="264"/>
-      <c r="D19" s="264"/>
-      <c r="E19" s="264"/>
-      <c r="F19" s="264"/>
-      <c r="G19" s="264"/>
-      <c r="H19" s="264"/>
-      <c r="I19" s="264"/>
-      <c r="J19" s="264"/>
-      <c r="K19" s="264"/>
-      <c r="L19" s="265"/>
-    </row>
-    <row r="20" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="266" t="s">
+      <c r="B20" s="260"/>
+      <c r="C20" s="260"/>
+      <c r="D20" s="260"/>
+      <c r="E20" s="260"/>
+      <c r="F20" s="260"/>
+      <c r="G20" s="260"/>
+      <c r="H20" s="260"/>
+      <c r="I20" s="260"/>
+      <c r="J20" s="260"/>
+      <c r="K20" s="260"/>
+      <c r="L20" s="261"/>
+    </row>
+    <row r="21" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="283" t="s">
         <v>338</v>
       </c>
-      <c r="B20" s="267"/>
-      <c r="C20" s="267"/>
-      <c r="D20" s="267"/>
-      <c r="E20" s="267"/>
-      <c r="F20" s="267"/>
-      <c r="G20" s="267"/>
-      <c r="H20" s="267"/>
-      <c r="I20" s="267"/>
-      <c r="J20" s="267"/>
-      <c r="K20" s="267"/>
-      <c r="L20" s="268"/>
-    </row>
-    <row r="21" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="113"/>
-      <c r="B21" s="113"/>
-      <c r="C21" s="113"/>
-      <c r="D21" s="113"/>
-      <c r="E21" s="113"/>
-      <c r="F21" s="113"/>
-      <c r="G21" s="113"/>
-      <c r="H21" s="113"/>
-      <c r="I21" s="113"/>
-      <c r="J21" s="113"/>
-      <c r="K21" s="113"/>
-      <c r="L21" s="113"/>
-    </row>
-    <row r="22" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="269" t="s">
+      <c r="B21" s="284"/>
+      <c r="C21" s="284"/>
+      <c r="D21" s="284"/>
+      <c r="E21" s="284"/>
+      <c r="F21" s="284"/>
+      <c r="G21" s="284"/>
+      <c r="H21" s="284"/>
+      <c r="I21" s="284"/>
+      <c r="J21" s="284"/>
+      <c r="K21" s="284"/>
+      <c r="L21" s="285"/>
+    </row>
+    <row r="22" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="113"/>
+      <c r="B22" s="113"/>
+      <c r="C22" s="113"/>
+      <c r="D22" s="113"/>
+      <c r="E22" s="113"/>
+      <c r="F22" s="113"/>
+      <c r="G22" s="113"/>
+      <c r="H22" s="113"/>
+      <c r="I22" s="113"/>
+      <c r="J22" s="113"/>
+      <c r="K22" s="113"/>
+      <c r="L22" s="113"/>
+    </row>
+    <row r="23" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="286" t="s">
         <v>334</v>
       </c>
-      <c r="B22" s="270"/>
-      <c r="C22" s="270"/>
-      <c r="D22" s="270"/>
-      <c r="E22" s="270"/>
-      <c r="F22" s="270"/>
-      <c r="G22" s="270"/>
-      <c r="H22" s="270"/>
-      <c r="I22" s="270"/>
-      <c r="J22" s="270"/>
-      <c r="K22" s="270"/>
-      <c r="L22" s="271"/>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="246" t="s">
+      <c r="B23" s="287"/>
+      <c r="C23" s="287"/>
+      <c r="D23" s="287"/>
+      <c r="E23" s="287"/>
+      <c r="F23" s="287"/>
+      <c r="G23" s="287"/>
+      <c r="H23" s="287"/>
+      <c r="I23" s="287"/>
+      <c r="J23" s="287"/>
+      <c r="K23" s="287"/>
+      <c r="L23" s="288"/>
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="265" t="s">
         <v>215</v>
       </c>
-      <c r="B23" s="247"/>
-      <c r="C23" s="247"/>
-      <c r="D23" s="247"/>
-      <c r="E23" s="247"/>
-      <c r="F23" s="247"/>
-      <c r="G23" s="247"/>
-      <c r="H23" s="247"/>
-      <c r="I23" s="247"/>
-      <c r="J23" s="247"/>
-      <c r="K23" s="247"/>
-      <c r="L23" s="248"/>
-      <c r="N23" s="1"/>
-    </row>
-    <row r="24" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="228">
+      <c r="B24" s="266"/>
+      <c r="C24" s="266"/>
+      <c r="D24" s="266"/>
+      <c r="E24" s="266"/>
+      <c r="F24" s="266"/>
+      <c r="G24" s="266"/>
+      <c r="H24" s="266"/>
+      <c r="I24" s="266"/>
+      <c r="J24" s="266"/>
+      <c r="K24" s="266"/>
+      <c r="L24" s="267"/>
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="228">
         <v>1</v>
       </c>
-      <c r="B24" s="276" t="s">
+      <c r="B25" s="253" t="s">
         <v>214</v>
       </c>
-      <c r="C24" s="276"/>
-      <c r="D24" s="276"/>
-      <c r="E24" s="276"/>
-      <c r="F24" s="276"/>
-      <c r="G24" s="276"/>
-      <c r="H24" s="276"/>
-      <c r="I24" s="276"/>
-      <c r="J24" s="276"/>
-      <c r="K24" s="276"/>
-      <c r="L24" s="277"/>
-    </row>
-    <row r="25" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="228">
+      <c r="C25" s="253"/>
+      <c r="D25" s="253"/>
+      <c r="E25" s="253"/>
+      <c r="F25" s="253"/>
+      <c r="G25" s="253"/>
+      <c r="H25" s="253"/>
+      <c r="I25" s="253"/>
+      <c r="J25" s="253"/>
+      <c r="K25" s="253"/>
+      <c r="L25" s="254"/>
+    </row>
+    <row r="26" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="228">
         <v>2</v>
       </c>
-      <c r="B25" s="276" t="s">
+      <c r="B26" s="253" t="s">
         <v>330</v>
       </c>
-      <c r="C25" s="276"/>
-      <c r="D25" s="276"/>
-      <c r="E25" s="276"/>
-      <c r="F25" s="276"/>
-      <c r="G25" s="276"/>
-      <c r="H25" s="276"/>
-      <c r="I25" s="276"/>
-      <c r="J25" s="276"/>
-      <c r="K25" s="276"/>
-      <c r="L25" s="277"/>
-      <c r="N25" s="106"/>
-    </row>
-    <row r="26" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="228">
-        <v>3</v>
-      </c>
-      <c r="B26" s="276" t="s">
-        <v>207</v>
-      </c>
-      <c r="C26" s="276"/>
-      <c r="D26" s="276"/>
-      <c r="E26" s="276"/>
-      <c r="F26" s="276"/>
-      <c r="G26" s="276"/>
-      <c r="H26" s="276"/>
-      <c r="I26" s="276"/>
-      <c r="J26" s="276"/>
-      <c r="K26" s="276"/>
-      <c r="L26" s="277"/>
+      <c r="C26" s="253"/>
+      <c r="D26" s="253"/>
+      <c r="E26" s="253"/>
+      <c r="F26" s="253"/>
+      <c r="G26" s="253"/>
+      <c r="H26" s="253"/>
+      <c r="I26" s="253"/>
+      <c r="J26" s="253"/>
+      <c r="K26" s="253"/>
+      <c r="L26" s="254"/>
       <c r="N26" s="106"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="228">
-        <v>4</v>
-      </c>
-      <c r="B27" s="276" t="s">
-        <v>339</v>
-      </c>
-      <c r="C27" s="276"/>
-      <c r="D27" s="276"/>
-      <c r="E27" s="276"/>
-      <c r="F27" s="276"/>
-      <c r="G27" s="276"/>
-      <c r="H27" s="276"/>
-      <c r="I27" s="276"/>
-      <c r="J27" s="276"/>
-      <c r="K27" s="276"/>
-      <c r="L27" s="277"/>
+        <v>3</v>
+      </c>
+      <c r="B27" s="253" t="s">
+        <v>207</v>
+      </c>
+      <c r="C27" s="253"/>
+      <c r="D27" s="253"/>
+      <c r="E27" s="253"/>
+      <c r="F27" s="253"/>
+      <c r="G27" s="253"/>
+      <c r="H27" s="253"/>
+      <c r="I27" s="253"/>
+      <c r="J27" s="253"/>
+      <c r="K27" s="253"/>
+      <c r="L27" s="254"/>
       <c r="N27" s="106"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="228">
+        <v>4</v>
+      </c>
+      <c r="B28" s="253" t="s">
+        <v>339</v>
+      </c>
+      <c r="C28" s="253"/>
+      <c r="D28" s="253"/>
+      <c r="E28" s="253"/>
+      <c r="F28" s="253"/>
+      <c r="G28" s="253"/>
+      <c r="H28" s="253"/>
+      <c r="I28" s="253"/>
+      <c r="J28" s="253"/>
+      <c r="K28" s="253"/>
+      <c r="L28" s="254"/>
+      <c r="N28" s="106"/>
+    </row>
+    <row r="29" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="228">
         <v>5</v>
       </c>
-      <c r="B28" s="276" t="s">
+      <c r="B29" s="253" t="s">
         <v>208</v>
       </c>
-      <c r="C28" s="276"/>
-      <c r="D28" s="276"/>
-      <c r="E28" s="276"/>
-      <c r="F28" s="276"/>
-      <c r="G28" s="276"/>
-      <c r="H28" s="276"/>
-      <c r="I28" s="276"/>
-      <c r="J28" s="276"/>
-      <c r="K28" s="276"/>
-      <c r="L28" s="277"/>
-      <c r="N28" s="106"/>
-    </row>
-    <row r="29" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="228"/>
-      <c r="B29" s="276" t="s">
-        <v>209</v>
-      </c>
-      <c r="C29" s="276"/>
-      <c r="D29" s="276"/>
-      <c r="E29" s="276"/>
-      <c r="F29" s="276"/>
-      <c r="G29" s="276"/>
-      <c r="H29" s="276"/>
-      <c r="I29" s="276"/>
-      <c r="J29" s="276"/>
-      <c r="K29" s="276"/>
-      <c r="L29" s="277"/>
+      <c r="C29" s="253"/>
+      <c r="D29" s="253"/>
+      <c r="E29" s="253"/>
+      <c r="F29" s="253"/>
+      <c r="G29" s="253"/>
+      <c r="H29" s="253"/>
+      <c r="I29" s="253"/>
+      <c r="J29" s="253"/>
+      <c r="K29" s="253"/>
+      <c r="L29" s="254"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="228"/>
-      <c r="B30" s="276" t="s">
+      <c r="B30" s="253" t="s">
+        <v>209</v>
+      </c>
+      <c r="C30" s="253"/>
+      <c r="D30" s="253"/>
+      <c r="E30" s="253"/>
+      <c r="F30" s="253"/>
+      <c r="G30" s="253"/>
+      <c r="H30" s="253"/>
+      <c r="I30" s="253"/>
+      <c r="J30" s="253"/>
+      <c r="K30" s="253"/>
+      <c r="L30" s="254"/>
+      <c r="N30" s="106"/>
+    </row>
+    <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="228"/>
+      <c r="B31" s="253" t="s">
         <v>210</v>
       </c>
-      <c r="C30" s="276"/>
-      <c r="D30" s="276"/>
-      <c r="E30" s="276"/>
-      <c r="F30" s="276"/>
-      <c r="G30" s="276"/>
-      <c r="H30" s="276"/>
-      <c r="I30" s="276"/>
-      <c r="J30" s="276"/>
-      <c r="K30" s="276"/>
-      <c r="L30" s="277"/>
-      <c r="N30" s="106"/>
-    </row>
-    <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="278" t="s">
+      <c r="C31" s="253"/>
+      <c r="D31" s="253"/>
+      <c r="E31" s="253"/>
+      <c r="F31" s="253"/>
+      <c r="G31" s="253"/>
+      <c r="H31" s="253"/>
+      <c r="I31" s="253"/>
+      <c r="J31" s="253"/>
+      <c r="K31" s="253"/>
+      <c r="L31" s="254"/>
+      <c r="N31" s="106"/>
+    </row>
+    <row r="32" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="262" t="s">
         <v>216</v>
       </c>
-      <c r="B31" s="279"/>
-      <c r="C31" s="279"/>
-      <c r="D31" s="279"/>
-      <c r="E31" s="279"/>
-      <c r="F31" s="279"/>
-      <c r="G31" s="279"/>
-      <c r="H31" s="279"/>
-      <c r="I31" s="279"/>
-      <c r="J31" s="279"/>
-      <c r="K31" s="279"/>
-      <c r="L31" s="280"/>
-      <c r="N31" s="106"/>
-    </row>
-    <row r="32" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="228">
+      <c r="B32" s="263"/>
+      <c r="C32" s="263"/>
+      <c r="D32" s="263"/>
+      <c r="E32" s="263"/>
+      <c r="F32" s="263"/>
+      <c r="G32" s="263"/>
+      <c r="H32" s="263"/>
+      <c r="I32" s="263"/>
+      <c r="J32" s="263"/>
+      <c r="K32" s="263"/>
+      <c r="L32" s="264"/>
+      <c r="N32" s="106"/>
+    </row>
+    <row r="33" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="228">
         <v>1</v>
       </c>
-      <c r="B32" s="276" t="s">
+      <c r="B33" s="253" t="s">
         <v>211</v>
       </c>
-      <c r="C32" s="276"/>
-      <c r="D32" s="276"/>
-      <c r="E32" s="276"/>
-      <c r="F32" s="276"/>
-      <c r="G32" s="276"/>
-      <c r="H32" s="276"/>
-      <c r="I32" s="276"/>
-      <c r="J32" s="276"/>
-      <c r="K32" s="276"/>
-      <c r="L32" s="277"/>
-      <c r="N32" s="106"/>
-    </row>
-    <row r="33" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="228"/>
-      <c r="B33" s="274" t="s">
+      <c r="C33" s="253"/>
+      <c r="D33" s="253"/>
+      <c r="E33" s="253"/>
+      <c r="F33" s="253"/>
+      <c r="G33" s="253"/>
+      <c r="H33" s="253"/>
+      <c r="I33" s="253"/>
+      <c r="J33" s="253"/>
+      <c r="K33" s="253"/>
+      <c r="L33" s="254"/>
+      <c r="N33" s="106"/>
+    </row>
+    <row r="34" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="228"/>
+      <c r="B34" s="251" t="s">
         <v>340</v>
       </c>
-      <c r="C33" s="274"/>
-      <c r="D33" s="274"/>
-      <c r="E33" s="274"/>
-      <c r="F33" s="274"/>
-      <c r="G33" s="274"/>
-      <c r="H33" s="274"/>
-      <c r="I33" s="274"/>
-      <c r="J33" s="274"/>
-      <c r="K33" s="274"/>
-      <c r="L33" s="275"/>
-      <c r="N33" s="106"/>
-    </row>
-    <row r="34" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="228">
+      <c r="C34" s="251"/>
+      <c r="D34" s="251"/>
+      <c r="E34" s="251"/>
+      <c r="F34" s="251"/>
+      <c r="G34" s="251"/>
+      <c r="H34" s="251"/>
+      <c r="I34" s="251"/>
+      <c r="J34" s="251"/>
+      <c r="K34" s="251"/>
+      <c r="L34" s="252"/>
+      <c r="N34" s="106"/>
+    </row>
+    <row r="35" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="228">
         <v>2</v>
       </c>
-      <c r="B34" s="276" t="s">
+      <c r="B35" s="253" t="s">
         <v>333</v>
       </c>
-      <c r="C34" s="276"/>
-      <c r="D34" s="276"/>
-      <c r="E34" s="276"/>
-      <c r="F34" s="276"/>
-      <c r="G34" s="276"/>
-      <c r="H34" s="276"/>
-      <c r="I34" s="276"/>
-      <c r="J34" s="276"/>
-      <c r="K34" s="276"/>
-      <c r="L34" s="277"/>
-      <c r="N34" s="106"/>
-    </row>
-    <row r="35" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="228">
-        <v>3</v>
-      </c>
-      <c r="B35" s="276" t="s">
-        <v>322</v>
-      </c>
-      <c r="C35" s="276"/>
-      <c r="D35" s="276"/>
-      <c r="E35" s="276"/>
-      <c r="F35" s="276"/>
-      <c r="G35" s="276"/>
-      <c r="H35" s="276"/>
-      <c r="I35" s="276"/>
-      <c r="J35" s="276"/>
-      <c r="K35" s="276"/>
-      <c r="L35" s="277"/>
+      <c r="C35" s="253"/>
+      <c r="D35" s="253"/>
+      <c r="E35" s="253"/>
+      <c r="F35" s="253"/>
+      <c r="G35" s="253"/>
+      <c r="H35" s="253"/>
+      <c r="I35" s="253"/>
+      <c r="J35" s="253"/>
+      <c r="K35" s="253"/>
+      <c r="L35" s="254"/>
       <c r="N35" s="106"/>
     </row>
     <row r="36" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="228">
+        <v>3</v>
+      </c>
+      <c r="B36" s="253" t="s">
+        <v>322</v>
+      </c>
+      <c r="C36" s="253"/>
+      <c r="D36" s="253"/>
+      <c r="E36" s="253"/>
+      <c r="F36" s="253"/>
+      <c r="G36" s="253"/>
+      <c r="H36" s="253"/>
+      <c r="I36" s="253"/>
+      <c r="J36" s="253"/>
+      <c r="K36" s="253"/>
+      <c r="L36" s="254"/>
+      <c r="N36" s="106"/>
+    </row>
+    <row r="37" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="228">
         <v>4</v>
       </c>
-      <c r="B36" s="276" t="s">
+      <c r="B37" s="253" t="s">
         <v>341</v>
       </c>
-      <c r="C36" s="276"/>
-      <c r="D36" s="276"/>
-      <c r="E36" s="276"/>
-      <c r="F36" s="276"/>
-      <c r="G36" s="276"/>
-      <c r="H36" s="276"/>
-      <c r="I36" s="276"/>
-      <c r="J36" s="276"/>
-      <c r="K36" s="276"/>
-      <c r="L36" s="277"/>
-      <c r="N36" s="106"/>
-    </row>
-    <row r="37" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="228">
+      <c r="C37" s="253"/>
+      <c r="D37" s="253"/>
+      <c r="E37" s="253"/>
+      <c r="F37" s="253"/>
+      <c r="G37" s="253"/>
+      <c r="H37" s="253"/>
+      <c r="I37" s="253"/>
+      <c r="J37" s="253"/>
+      <c r="K37" s="253"/>
+      <c r="L37" s="254"/>
+      <c r="N37" s="106"/>
+    </row>
+    <row r="38" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="228">
         <v>5</v>
       </c>
-      <c r="B37" s="274" t="s">
+      <c r="B38" s="251" t="s">
         <v>323</v>
       </c>
-      <c r="C37" s="274"/>
-      <c r="D37" s="274"/>
-      <c r="E37" s="274"/>
-      <c r="F37" s="274"/>
-      <c r="G37" s="274"/>
-      <c r="H37" s="274"/>
-      <c r="I37" s="274"/>
-      <c r="J37" s="274"/>
-      <c r="K37" s="274"/>
-      <c r="L37" s="275"/>
-      <c r="N37" s="106"/>
-    </row>
-    <row r="38" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="228">
+      <c r="C38" s="251"/>
+      <c r="D38" s="251"/>
+      <c r="E38" s="251"/>
+      <c r="F38" s="251"/>
+      <c r="G38" s="251"/>
+      <c r="H38" s="251"/>
+      <c r="I38" s="251"/>
+      <c r="J38" s="251"/>
+      <c r="K38" s="251"/>
+      <c r="L38" s="252"/>
+      <c r="N38" s="106"/>
+    </row>
+    <row r="39" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="228">
         <v>6</v>
       </c>
-      <c r="B38" s="274" t="s">
+      <c r="B39" s="251" t="s">
         <v>328</v>
       </c>
-      <c r="C38" s="274"/>
-      <c r="D38" s="274"/>
-      <c r="E38" s="274"/>
-      <c r="F38" s="274"/>
-      <c r="G38" s="274"/>
-      <c r="H38" s="274"/>
-      <c r="I38" s="274"/>
-      <c r="J38" s="274"/>
-      <c r="K38" s="274"/>
-      <c r="L38" s="275"/>
-      <c r="N38" s="106"/>
-    </row>
-    <row r="39" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="228">
+      <c r="C39" s="251"/>
+      <c r="D39" s="251"/>
+      <c r="E39" s="251"/>
+      <c r="F39" s="251"/>
+      <c r="G39" s="251"/>
+      <c r="H39" s="251"/>
+      <c r="I39" s="251"/>
+      <c r="J39" s="251"/>
+      <c r="K39" s="251"/>
+      <c r="L39" s="252"/>
+      <c r="N39" s="106"/>
+    </row>
+    <row r="40" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="228">
         <v>7</v>
       </c>
-      <c r="B39" s="276" t="s">
+      <c r="B40" s="253" t="s">
         <v>324</v>
       </c>
-      <c r="C39" s="276"/>
-      <c r="D39" s="276"/>
-      <c r="E39" s="276"/>
-      <c r="F39" s="276"/>
-      <c r="G39" s="276"/>
-      <c r="H39" s="276"/>
-      <c r="I39" s="276"/>
-      <c r="J39" s="276"/>
-      <c r="K39" s="276"/>
-      <c r="L39" s="277"/>
-    </row>
-    <row r="40" spans="1:14" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="228"/>
-      <c r="B40" s="229"/>
-      <c r="C40" s="229"/>
-      <c r="D40" s="229"/>
-      <c r="E40" s="229"/>
-      <c r="F40" s="229"/>
-      <c r="G40" s="229"/>
-      <c r="H40" s="229"/>
-      <c r="I40" s="229"/>
-      <c r="J40" s="229"/>
-      <c r="K40" s="229"/>
-      <c r="L40" s="230"/>
-    </row>
-    <row r="41" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="278" t="s">
+      <c r="C40" s="253"/>
+      <c r="D40" s="253"/>
+      <c r="E40" s="253"/>
+      <c r="F40" s="253"/>
+      <c r="G40" s="253"/>
+      <c r="H40" s="253"/>
+      <c r="I40" s="253"/>
+      <c r="J40" s="253"/>
+      <c r="K40" s="253"/>
+      <c r="L40" s="254"/>
+    </row>
+    <row r="41" spans="1:14" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="228"/>
+      <c r="B41" s="229"/>
+      <c r="C41" s="229"/>
+      <c r="D41" s="229"/>
+      <c r="E41" s="229"/>
+      <c r="F41" s="229"/>
+      <c r="G41" s="229"/>
+      <c r="H41" s="229"/>
+      <c r="I41" s="229"/>
+      <c r="J41" s="229"/>
+      <c r="K41" s="229"/>
+      <c r="L41" s="230"/>
+    </row>
+    <row r="42" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="262" t="s">
         <v>327</v>
       </c>
-      <c r="B41" s="279"/>
-      <c r="C41" s="279"/>
-      <c r="D41" s="279"/>
-      <c r="E41" s="279"/>
-      <c r="F41" s="279"/>
-      <c r="G41" s="279"/>
-      <c r="H41" s="279"/>
-      <c r="I41" s="279"/>
-      <c r="J41" s="279"/>
-      <c r="K41" s="279"/>
-      <c r="L41" s="280"/>
-    </row>
-    <row r="42" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="231" t="s">
+      <c r="B42" s="263"/>
+      <c r="C42" s="263"/>
+      <c r="D42" s="263"/>
+      <c r="E42" s="263"/>
+      <c r="F42" s="263"/>
+      <c r="G42" s="263"/>
+      <c r="H42" s="263"/>
+      <c r="I42" s="263"/>
+      <c r="J42" s="263"/>
+      <c r="K42" s="263"/>
+      <c r="L42" s="264"/>
+    </row>
+    <row r="43" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="231" t="s">
         <v>325</v>
       </c>
-      <c r="B42" s="276" t="s">
+      <c r="B43" s="253" t="s">
         <v>212</v>
       </c>
-      <c r="C42" s="276"/>
-      <c r="D42" s="276"/>
-      <c r="E42" s="276"/>
-      <c r="F42" s="276"/>
-      <c r="G42" s="276"/>
-      <c r="H42" s="276"/>
-      <c r="I42" s="276"/>
-      <c r="J42" s="276"/>
-      <c r="K42" s="276"/>
-      <c r="L42" s="277"/>
-    </row>
-    <row r="43" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="232" t="s">
+      <c r="C43" s="253"/>
+      <c r="D43" s="253"/>
+      <c r="E43" s="253"/>
+      <c r="F43" s="253"/>
+      <c r="G43" s="253"/>
+      <c r="H43" s="253"/>
+      <c r="I43" s="253"/>
+      <c r="J43" s="253"/>
+      <c r="K43" s="253"/>
+      <c r="L43" s="254"/>
+    </row>
+    <row r="44" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="232" t="s">
         <v>326</v>
       </c>
-      <c r="B43" s="282" t="s">
+      <c r="B44" s="255" t="s">
         <v>329</v>
       </c>
-      <c r="C43" s="282"/>
-      <c r="D43" s="282"/>
-      <c r="E43" s="282"/>
-      <c r="F43" s="282"/>
-      <c r="G43" s="282"/>
-      <c r="H43" s="282"/>
-      <c r="I43" s="282"/>
-      <c r="J43" s="282"/>
-      <c r="K43" s="282"/>
-      <c r="L43" s="283"/>
-    </row>
-    <row r="44" spans="1:14" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="160"/>
-      <c r="B44" s="113"/>
-      <c r="C44" s="113"/>
-      <c r="D44" s="113"/>
-      <c r="E44" s="113"/>
-      <c r="F44" s="113"/>
-      <c r="G44" s="113"/>
-      <c r="H44" s="113"/>
-      <c r="I44" s="113"/>
-      <c r="J44" s="113"/>
-      <c r="K44" s="113"/>
-      <c r="L44" s="113"/>
-    </row>
-    <row r="45" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="284" t="s">
+      <c r="C44" s="255"/>
+      <c r="D44" s="255"/>
+      <c r="E44" s="255"/>
+      <c r="F44" s="255"/>
+      <c r="G44" s="255"/>
+      <c r="H44" s="255"/>
+      <c r="I44" s="255"/>
+      <c r="J44" s="255"/>
+      <c r="K44" s="255"/>
+      <c r="L44" s="256"/>
+    </row>
+    <row r="45" spans="1:14" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="160"/>
+      <c r="B45" s="113"/>
+      <c r="C45" s="113"/>
+      <c r="D45" s="113"/>
+      <c r="E45" s="113"/>
+      <c r="F45" s="113"/>
+      <c r="G45" s="113"/>
+      <c r="H45" s="113"/>
+      <c r="I45" s="113"/>
+      <c r="J45" s="113"/>
+      <c r="K45" s="113"/>
+      <c r="L45" s="113"/>
+    </row>
+    <row r="46" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="257" t="s">
         <v>240</v>
       </c>
-      <c r="B45" s="285"/>
-      <c r="C45" s="285"/>
-      <c r="D45" s="285"/>
-      <c r="E45" s="285"/>
-      <c r="F45" s="285"/>
-      <c r="G45" s="285"/>
-      <c r="H45" s="285"/>
-      <c r="I45" s="285"/>
-      <c r="J45" s="285"/>
-      <c r="K45" s="285"/>
-      <c r="L45" s="286"/>
-    </row>
-    <row r="46" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="235" t="s">
+      <c r="B46" s="258"/>
+      <c r="C46" s="258"/>
+      <c r="D46" s="258"/>
+      <c r="E46" s="258"/>
+      <c r="F46" s="258"/>
+      <c r="G46" s="258"/>
+      <c r="H46" s="258"/>
+      <c r="I46" s="258"/>
+      <c r="J46" s="258"/>
+      <c r="K46" s="258"/>
+      <c r="L46" s="259"/>
+    </row>
+    <row r="47" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="235" t="s">
         <v>213</v>
       </c>
-      <c r="B46" s="161"/>
-      <c r="C46" s="161"/>
-      <c r="D46" s="161"/>
-      <c r="E46" s="161"/>
-      <c r="F46" s="161"/>
-      <c r="G46" s="161"/>
-      <c r="H46" s="161"/>
-      <c r="I46" s="161"/>
-      <c r="J46" s="161"/>
-      <c r="K46" s="161"/>
-      <c r="L46" s="162"/>
-    </row>
-    <row r="47" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B47" s="84"/>
-      <c r="C47" s="84"/>
-      <c r="D47" s="84"/>
-      <c r="E47" s="84"/>
-      <c r="F47" s="84"/>
-      <c r="G47" s="84"/>
-      <c r="H47" s="84"/>
-      <c r="I47" s="84"/>
-      <c r="J47" s="84"/>
-      <c r="K47" s="84"/>
-      <c r="L47" s="84"/>
-    </row>
-    <row r="48" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="163" t="s">
+      <c r="B47" s="161"/>
+      <c r="C47" s="161"/>
+      <c r="D47" s="161"/>
+      <c r="E47" s="161"/>
+      <c r="F47" s="161"/>
+      <c r="G47" s="161"/>
+      <c r="H47" s="161"/>
+      <c r="I47" s="161"/>
+      <c r="J47" s="161"/>
+      <c r="K47" s="161"/>
+      <c r="L47" s="162"/>
+    </row>
+    <row r="48" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="84"/>
+      <c r="C48" s="84"/>
+      <c r="D48" s="84"/>
+      <c r="E48" s="84"/>
+      <c r="F48" s="84"/>
+      <c r="G48" s="84"/>
+      <c r="H48" s="84"/>
+      <c r="I48" s="84"/>
+      <c r="J48" s="84"/>
+      <c r="K48" s="84"/>
+      <c r="L48" s="84"/>
+    </row>
+    <row r="49" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="163" t="s">
         <v>166</v>
       </c>
-      <c r="B48" s="164"/>
-      <c r="C48" s="164"/>
-      <c r="D48" s="165"/>
-      <c r="E48" s="164"/>
-      <c r="F48" s="164"/>
-      <c r="G48" s="164"/>
-      <c r="H48" s="164"/>
-      <c r="I48" s="164"/>
-      <c r="J48" s="164"/>
-      <c r="K48" s="164"/>
-      <c r="L48" s="166"/>
-    </row>
-    <row r="49" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="167"/>
-      <c r="B49" s="168" t="s">
-        <v>62</v>
-      </c>
-      <c r="C49" s="169" t="s">
-        <v>79</v>
-      </c>
-      <c r="D49" s="169"/>
-      <c r="E49" s="169"/>
-      <c r="F49" s="169"/>
-      <c r="G49" s="169"/>
-      <c r="H49" s="169"/>
-      <c r="I49" s="169"/>
-      <c r="J49" s="169"/>
-      <c r="K49" s="169"/>
-      <c r="L49" s="170"/>
-    </row>
-    <row r="50" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="164"/>
+      <c r="C49" s="164"/>
+      <c r="D49" s="165"/>
+      <c r="E49" s="164"/>
+      <c r="F49" s="164"/>
+      <c r="G49" s="164"/>
+      <c r="H49" s="164"/>
+      <c r="I49" s="164"/>
+      <c r="J49" s="164"/>
+      <c r="K49" s="164"/>
+      <c r="L49" s="166"/>
+    </row>
+    <row r="50" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="167"/>
       <c r="B50" s="168" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="C50" s="169" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="D50" s="169"/>
       <c r="E50" s="169"/>
@@ -15958,306 +15970,326 @@
       <c r="K50" s="169"/>
       <c r="L50" s="170"/>
     </row>
-    <row r="51" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="167"/>
       <c r="B51" s="168" t="s">
-        <v>62</v>
-      </c>
-      <c r="C51" s="264" t="s">
-        <v>313</v>
-      </c>
-      <c r="D51" s="264"/>
-      <c r="E51" s="264"/>
-      <c r="F51" s="264"/>
-      <c r="G51" s="264"/>
-      <c r="H51" s="264"/>
-      <c r="I51" s="264"/>
-      <c r="J51" s="264"/>
-      <c r="K51" s="264"/>
-      <c r="L51" s="265"/>
+        <v>81</v>
+      </c>
+      <c r="C51" s="169" t="s">
+        <v>91</v>
+      </c>
+      <c r="D51" s="169"/>
+      <c r="E51" s="169"/>
+      <c r="F51" s="169"/>
+      <c r="G51" s="169"/>
+      <c r="H51" s="169"/>
+      <c r="I51" s="169"/>
+      <c r="J51" s="169"/>
+      <c r="K51" s="169"/>
+      <c r="L51" s="170"/>
     </row>
     <row r="52" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="167"/>
       <c r="B52" s="168" t="s">
-        <v>314</v>
-      </c>
-      <c r="C52" s="264" t="s">
-        <v>315</v>
-      </c>
-      <c r="D52" s="264"/>
-      <c r="E52" s="264"/>
-      <c r="F52" s="264"/>
-      <c r="G52" s="264"/>
-      <c r="H52" s="264"/>
-      <c r="I52" s="264"/>
-      <c r="J52" s="264"/>
-      <c r="K52" s="264"/>
-      <c r="L52" s="265"/>
+        <v>62</v>
+      </c>
+      <c r="C52" s="260" t="s">
+        <v>313</v>
+      </c>
+      <c r="D52" s="260"/>
+      <c r="E52" s="260"/>
+      <c r="F52" s="260"/>
+      <c r="G52" s="260"/>
+      <c r="H52" s="260"/>
+      <c r="I52" s="260"/>
+      <c r="J52" s="260"/>
+      <c r="K52" s="260"/>
+      <c r="L52" s="261"/>
     </row>
     <row r="53" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="167"/>
       <c r="B53" s="168" t="s">
-        <v>383</v>
-      </c>
-      <c r="C53" s="264" t="s">
-        <v>384</v>
-      </c>
-      <c r="D53" s="264"/>
-      <c r="E53" s="264"/>
-      <c r="F53" s="264"/>
-      <c r="G53" s="264"/>
-      <c r="H53" s="264"/>
-      <c r="I53" s="264"/>
-      <c r="J53" s="264"/>
-      <c r="K53" s="264"/>
-      <c r="L53" s="265"/>
-    </row>
-    <row r="54" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>314</v>
+      </c>
+      <c r="C53" s="260" t="s">
+        <v>315</v>
+      </c>
+      <c r="D53" s="260"/>
+      <c r="E53" s="260"/>
+      <c r="F53" s="260"/>
+      <c r="G53" s="260"/>
+      <c r="H53" s="260"/>
+      <c r="I53" s="260"/>
+      <c r="J53" s="260"/>
+      <c r="K53" s="260"/>
+      <c r="L53" s="261"/>
+    </row>
+    <row r="54" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="167"/>
       <c r="B54" s="168" t="s">
-        <v>138</v>
-      </c>
-      <c r="C54" s="264" t="s">
-        <v>139</v>
-      </c>
-      <c r="D54" s="264"/>
-      <c r="E54" s="264"/>
-      <c r="F54" s="264"/>
-      <c r="G54" s="264"/>
-      <c r="H54" s="264"/>
-      <c r="I54" s="264"/>
-      <c r="J54" s="264"/>
-      <c r="K54" s="264"/>
-      <c r="L54" s="265"/>
+        <v>383</v>
+      </c>
+      <c r="C54" s="260" t="s">
+        <v>384</v>
+      </c>
+      <c r="D54" s="260"/>
+      <c r="E54" s="260"/>
+      <c r="F54" s="260"/>
+      <c r="G54" s="260"/>
+      <c r="H54" s="260"/>
+      <c r="I54" s="260"/>
+      <c r="J54" s="260"/>
+      <c r="K54" s="260"/>
+      <c r="L54" s="261"/>
     </row>
     <row r="55" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="167"/>
       <c r="B55" s="168" t="s">
-        <v>238</v>
-      </c>
-      <c r="C55" s="264" t="s">
-        <v>239</v>
-      </c>
-      <c r="D55" s="264"/>
-      <c r="E55" s="264"/>
-      <c r="F55" s="264"/>
-      <c r="G55" s="264"/>
-      <c r="H55" s="264"/>
-      <c r="I55" s="264"/>
-      <c r="J55" s="264"/>
-      <c r="K55" s="264"/>
-      <c r="L55" s="265"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+      <c r="C55" s="260" t="s">
+        <v>139</v>
+      </c>
+      <c r="D55" s="260"/>
+      <c r="E55" s="260"/>
+      <c r="F55" s="260"/>
+      <c r="G55" s="260"/>
+      <c r="H55" s="260"/>
+      <c r="I55" s="260"/>
+      <c r="J55" s="260"/>
+      <c r="K55" s="260"/>
+      <c r="L55" s="261"/>
+    </row>
+    <row r="56" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="167"/>
       <c r="B56" s="168" t="s">
-        <v>203</v>
-      </c>
-      <c r="C56" s="169" t="s">
-        <v>316</v>
-      </c>
-      <c r="D56" s="169"/>
-      <c r="E56" s="169"/>
-      <c r="F56" s="169"/>
-      <c r="G56" s="169"/>
-      <c r="H56" s="169"/>
-      <c r="I56" s="169"/>
-      <c r="J56" s="169"/>
-      <c r="K56" s="169"/>
-      <c r="L56" s="170"/>
-    </row>
-    <row r="57" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+      <c r="C56" s="260" t="s">
+        <v>239</v>
+      </c>
+      <c r="D56" s="260"/>
+      <c r="E56" s="260"/>
+      <c r="F56" s="260"/>
+      <c r="G56" s="260"/>
+      <c r="H56" s="260"/>
+      <c r="I56" s="260"/>
+      <c r="J56" s="260"/>
+      <c r="K56" s="260"/>
+      <c r="L56" s="261"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="167"/>
       <c r="B57" s="168" t="s">
-        <v>63</v>
-      </c>
-      <c r="C57" s="264" t="s">
-        <v>317</v>
-      </c>
-      <c r="D57" s="264"/>
-      <c r="E57" s="264"/>
-      <c r="F57" s="264"/>
-      <c r="G57" s="264"/>
-      <c r="H57" s="264"/>
-      <c r="I57" s="264"/>
-      <c r="J57" s="264"/>
-      <c r="K57" s="264"/>
-      <c r="L57" s="265"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.35">
+        <v>203</v>
+      </c>
+      <c r="C57" s="169" t="s">
+        <v>316</v>
+      </c>
+      <c r="D57" s="169"/>
+      <c r="E57" s="169"/>
+      <c r="F57" s="169"/>
+      <c r="G57" s="169"/>
+      <c r="H57" s="169"/>
+      <c r="I57" s="169"/>
+      <c r="J57" s="169"/>
+      <c r="K57" s="169"/>
+      <c r="L57" s="170"/>
+    </row>
+    <row r="58" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="167"/>
       <c r="B58" s="168" t="s">
+        <v>63</v>
+      </c>
+      <c r="C58" s="260" t="s">
+        <v>317</v>
+      </c>
+      <c r="D58" s="260"/>
+      <c r="E58" s="260"/>
+      <c r="F58" s="260"/>
+      <c r="G58" s="260"/>
+      <c r="H58" s="260"/>
+      <c r="I58" s="260"/>
+      <c r="J58" s="260"/>
+      <c r="K58" s="260"/>
+      <c r="L58" s="261"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A59" s="167"/>
+      <c r="B59" s="168" t="s">
         <v>75</v>
       </c>
-      <c r="C58" s="169" t="s">
+      <c r="C59" s="169" t="s">
         <v>76</v>
       </c>
-      <c r="D58" s="169"/>
-      <c r="E58" s="169"/>
-      <c r="F58" s="169"/>
-      <c r="G58" s="169"/>
-      <c r="H58" s="169"/>
-      <c r="I58" s="169"/>
-      <c r="J58" s="169"/>
-      <c r="K58" s="169"/>
-      <c r="L58" s="170"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A59" s="171"/>
-      <c r="B59" s="172" t="s">
+      <c r="D59" s="169"/>
+      <c r="E59" s="169"/>
+      <c r="F59" s="169"/>
+      <c r="G59" s="169"/>
+      <c r="H59" s="169"/>
+      <c r="I59" s="169"/>
+      <c r="J59" s="169"/>
+      <c r="K59" s="169"/>
+      <c r="L59" s="170"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A60" s="171"/>
+      <c r="B60" s="172" t="s">
         <v>159</v>
       </c>
-      <c r="C59" s="173" t="s">
+      <c r="C60" s="173" t="s">
         <v>160</v>
       </c>
-      <c r="D59" s="173"/>
-      <c r="E59" s="173"/>
-      <c r="F59" s="173"/>
-      <c r="G59" s="173"/>
-      <c r="H59" s="173"/>
-      <c r="I59" s="173"/>
-      <c r="J59" s="173"/>
-      <c r="K59" s="173"/>
-      <c r="L59" s="174"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A61" s="1" t="s">
-        <v>92</v>
-      </c>
+      <c r="D60" s="173"/>
+      <c r="E60" s="173"/>
+      <c r="F60" s="173"/>
+      <c r="G60" s="173"/>
+      <c r="H60" s="173"/>
+      <c r="I60" s="173"/>
+      <c r="J60" s="173"/>
+      <c r="K60" s="173"/>
+      <c r="L60" s="174"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A64" s="45" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A65" s="45" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A66" s="45" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A66" s="45"/>
-    </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A67" s="340" t="s">
+      <c r="A67" s="45"/>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A68" s="248" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A68" s="339" t="s">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A69" s="247" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A69" s="45" t="s">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A70" s="45" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A70" s="45"/>
-    </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="45"/>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A72" s="45" t="s">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A73" s="45" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="75" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A75" s="281" t="s">
+    <row r="76" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="250" t="s">
         <v>399</v>
       </c>
-      <c r="B75" s="281"/>
-      <c r="C75" s="281"/>
-      <c r="D75" s="281"/>
-      <c r="E75" s="281"/>
-      <c r="F75" s="281"/>
-      <c r="G75" s="281"/>
-      <c r="H75" s="281"/>
-      <c r="I75" s="281"/>
-      <c r="J75" s="281"/>
-      <c r="K75" s="281"/>
-      <c r="L75" s="281"/>
-    </row>
-    <row r="80" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="81" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="B76" s="250"/>
+      <c r="C76" s="250"/>
+      <c r="D76" s="250"/>
+      <c r="E76" s="250"/>
+      <c r="F76" s="250"/>
+      <c r="G76" s="250"/>
+      <c r="H76" s="250"/>
+      <c r="I76" s="250"/>
+      <c r="J76" s="250"/>
+      <c r="K76" s="250"/>
+      <c r="L76" s="250"/>
+    </row>
+    <row r="81" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="82" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="B12:L12"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="B14:L14"/>
-    <mergeCell ref="A75:L75"/>
+  <mergeCells count="47">
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="B11:L11"/>
     <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="B42:L42"/>
-    <mergeCell ref="B43:L43"/>
-    <mergeCell ref="A45:L45"/>
-    <mergeCell ref="C51:L51"/>
-    <mergeCell ref="C54:L54"/>
-    <mergeCell ref="C55:L55"/>
-    <mergeCell ref="C52:L52"/>
-    <mergeCell ref="C57:L57"/>
-    <mergeCell ref="A41:L41"/>
-    <mergeCell ref="C53:L53"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="B24:L24"/>
     <mergeCell ref="B25:L25"/>
     <mergeCell ref="B26:L26"/>
     <mergeCell ref="B27:L27"/>
     <mergeCell ref="B28:L28"/>
     <mergeCell ref="B29:L29"/>
     <mergeCell ref="B30:L30"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="A32:L32"/>
     <mergeCell ref="B33:L33"/>
-    <mergeCell ref="B35:L35"/>
     <mergeCell ref="B34:L34"/>
     <mergeCell ref="B36:L36"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B8:L8"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B12:L12"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="A76:L76"/>
+    <mergeCell ref="B39:L39"/>
+    <mergeCell ref="B40:L40"/>
+    <mergeCell ref="B43:L43"/>
+    <mergeCell ref="B44:L44"/>
+    <mergeCell ref="A46:L46"/>
+    <mergeCell ref="C52:L52"/>
+    <mergeCell ref="C55:L55"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="C53:L53"/>
+    <mergeCell ref="C58:L58"/>
+    <mergeCell ref="A42:L42"/>
+    <mergeCell ref="C54:L54"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A64" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
-    <hyperlink ref="A65" r:id="rId2" xr:uid="{66F54200-A2AB-43DA-A0E0-F2A25A075EE5}"/>
-    <hyperlink ref="A72" r:id="rId3" xr:uid="{A0F8DE06-D9FC-495F-9A01-AA199CB82365}"/>
-    <hyperlink ref="A45:L45" r:id="rId4" display="LETS START (visual directions as pdf)" xr:uid="{0D075873-7EBB-4309-B00A-6A62EA192A0C}"/>
-    <hyperlink ref="A46" r:id="rId5" xr:uid="{25154A32-BA44-496E-9945-086DE0980DBD}"/>
-    <hyperlink ref="A69" r:id="rId6" xr:uid="{AA792CE4-4071-4CE8-87C6-993A0BA6C6A5}"/>
+    <hyperlink ref="A65" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
+    <hyperlink ref="A66" r:id="rId2" xr:uid="{66F54200-A2AB-43DA-A0E0-F2A25A075EE5}"/>
+    <hyperlink ref="A73" r:id="rId3" xr:uid="{A0F8DE06-D9FC-495F-9A01-AA199CB82365}"/>
+    <hyperlink ref="A46:L46" r:id="rId4" display="LETS START (visual directions as pdf)" xr:uid="{0D075873-7EBB-4309-B00A-6A62EA192A0C}"/>
+    <hyperlink ref="A47" r:id="rId5" xr:uid="{25154A32-BA44-496E-9945-086DE0980DBD}"/>
+    <hyperlink ref="A70" r:id="rId6" xr:uid="{AA792CE4-4071-4CE8-87C6-993A0BA6C6A5}"/>
+    <hyperlink ref="E15" r:id="rId7" xr:uid="{218FEB9D-6782-4420-9DCE-4D6F20EDE6D5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId7"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -31216,82 +31248,82 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="324" t="s">
+      <c r="A3" s="331" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="324"/>
-      <c r="C3" s="324"/>
+      <c r="B3" s="331"/>
+      <c r="C3" s="331"/>
       <c r="D3" s="128" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="325" t="s">
+      <c r="A4" s="332" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="325"/>
-      <c r="C4" s="325"/>
+      <c r="B4" s="332"/>
+      <c r="C4" s="332"/>
       <c r="D4" s="175" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="329" t="s">
+      <c r="A5" s="336" t="s">
         <v>223</v>
       </c>
-      <c r="B5" s="326"/>
-      <c r="C5" s="326"/>
+      <c r="B5" s="333"/>
+      <c r="C5" s="333"/>
       <c r="D5" s="176" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="327" t="s">
+      <c r="A6" s="334" t="s">
         <v>224</v>
       </c>
-      <c r="B6" s="327"/>
-      <c r="C6" s="327"/>
+      <c r="B6" s="334"/>
+      <c r="C6" s="334"/>
       <c r="D6" s="177" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="328" t="s">
+      <c r="A7" s="335" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="328"/>
-      <c r="C7" s="328"/>
+      <c r="B7" s="335"/>
+      <c r="C7" s="335"/>
       <c r="D7" s="178" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="325" t="s">
+      <c r="A11" s="332" t="s">
         <v>152</v>
       </c>
-      <c r="B11" s="325"/>
-      <c r="C11" s="325"/>
+      <c r="B11" s="332"/>
+      <c r="C11" s="332"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="326" t="s">
+      <c r="A12" s="333" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="326"/>
-      <c r="C12" s="326"/>
+      <c r="B12" s="333"/>
+      <c r="C12" s="333"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="327" t="s">
+      <c r="A13" s="334" t="s">
         <v>154</v>
       </c>
-      <c r="B13" s="327"/>
-      <c r="C13" s="327"/>
+      <c r="B13" s="334"/>
+      <c r="C13" s="334"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="328" t="s">
+      <c r="A14" s="335" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="328"/>
-      <c r="C14" s="328"/>
+      <c r="B14" s="335"/>
+      <c r="C14" s="335"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -31884,16 +31916,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="287" t="str">
+      <c r="A1" s="294" t="str">
         <f>'ReadMe-Directions'!A1</f>
         <v>Immersive Model for Lake Mead based on the Principle of Divide Reservoir Inflow</v>
       </c>
-      <c r="B1" s="287"/>
-      <c r="C1" s="287"/>
-      <c r="D1" s="287"/>
-      <c r="E1" s="287"/>
-      <c r="F1" s="287"/>
-      <c r="G1" s="287"/>
+      <c r="B1" s="294"/>
+      <c r="C1" s="294"/>
+      <c r="D1" s="294"/>
+      <c r="E1" s="294"/>
+      <c r="F1" s="294"/>
+      <c r="G1" s="294"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -31902,15 +31934,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="295" t="s">
+      <c r="A3" s="302" t="s">
         <v>230</v>
       </c>
-      <c r="B3" s="295"/>
-      <c r="C3" s="295"/>
-      <c r="D3" s="295"/>
-      <c r="E3" s="295"/>
-      <c r="F3" s="295"/>
-      <c r="G3" s="295"/>
+      <c r="B3" s="302"/>
+      <c r="C3" s="302"/>
+      <c r="D3" s="302"/>
+      <c r="E3" s="302"/>
+      <c r="F3" s="302"/>
+      <c r="G3" s="302"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -31926,13 +31958,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="296" t="s">
+      <c r="C4" s="303" t="s">
         <v>310</v>
       </c>
-      <c r="D4" s="297"/>
-      <c r="E4" s="297"/>
-      <c r="F4" s="297"/>
-      <c r="G4" s="298"/>
+      <c r="D4" s="304"/>
+      <c r="E4" s="304"/>
+      <c r="F4" s="304"/>
+      <c r="G4" s="305"/>
       <c r="N4" s="141" t="s">
         <v>385</v>
       </c>
@@ -31942,11 +31974,11 @@
         <v>283</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="299"/>
-      <c r="D5" s="294"/>
-      <c r="E5" s="294"/>
-      <c r="F5" s="294"/>
-      <c r="G5" s="294"/>
+      <c r="C5" s="306"/>
+      <c r="D5" s="301"/>
+      <c r="E5" s="301"/>
+      <c r="F5" s="301"/>
+      <c r="G5" s="301"/>
       <c r="N5" s="141"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -31954,11 +31986,11 @@
         <v>242</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="299"/>
-      <c r="D6" s="294"/>
-      <c r="E6" s="294"/>
-      <c r="F6" s="294"/>
-      <c r="G6" s="294"/>
+      <c r="C6" s="306"/>
+      <c r="D6" s="301"/>
+      <c r="E6" s="301"/>
+      <c r="F6" s="301"/>
+      <c r="G6" s="301"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -31966,11 +31998,11 @@
         <v>243</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="299"/>
-      <c r="D7" s="294"/>
-      <c r="E7" s="294"/>
-      <c r="F7" s="294"/>
-      <c r="G7" s="294"/>
+      <c r="C7" s="306"/>
+      <c r="D7" s="301"/>
+      <c r="E7" s="301"/>
+      <c r="F7" s="301"/>
+      <c r="G7" s="301"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -31978,11 +32010,11 @@
         <v>244</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="294"/>
-      <c r="D8" s="294"/>
-      <c r="E8" s="294"/>
-      <c r="F8" s="294"/>
-      <c r="G8" s="294"/>
+      <c r="C8" s="301"/>
+      <c r="D8" s="301"/>
+      <c r="E8" s="301"/>
+      <c r="F8" s="301"/>
+      <c r="G8" s="301"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -31990,11 +32022,11 @@
         <v>18</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="300"/>
-      <c r="D9" s="300"/>
-      <c r="E9" s="300"/>
-      <c r="F9" s="300"/>
-      <c r="G9" s="300"/>
+      <c r="C9" s="307"/>
+      <c r="D9" s="307"/>
+      <c r="E9" s="307"/>
+      <c r="F9" s="307"/>
+      <c r="G9" s="307"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -32002,11 +32034,11 @@
         <v>332</v>
       </c>
       <c r="B10" s="90"/>
-      <c r="C10" s="294"/>
-      <c r="D10" s="294"/>
-      <c r="E10" s="294"/>
-      <c r="F10" s="294"/>
-      <c r="G10" s="294"/>
+      <c r="C10" s="301"/>
+      <c r="D10" s="301"/>
+      <c r="E10" s="301"/>
+      <c r="F10" s="301"/>
+      <c r="G10" s="301"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -32019,28 +32051,28 @@
       <c r="A12" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="301" t="s">
+      <c r="B12" s="308" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="302"/>
-      <c r="D12" s="303"/>
+      <c r="C12" s="309"/>
+      <c r="D12" s="310"/>
       <c r="N12" s="141" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="304" t="s">
+      <c r="B13" s="311" t="s">
         <v>229</v>
       </c>
-      <c r="C13" s="305"/>
-      <c r="D13" s="306"/>
+      <c r="C13" s="312"/>
+      <c r="D13" s="313"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="288" t="s">
+      <c r="B14" s="295" t="s">
         <v>224</v>
       </c>
-      <c r="C14" s="289"/>
-      <c r="D14" s="290"/>
+      <c r="C14" s="296"/>
+      <c r="D14" s="297"/>
       <c r="F14">
         <f>4.5/7.2</f>
         <v>0.625</v>
@@ -32048,11 +32080,11 @@
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="291" t="s">
+      <c r="B15" s="298" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="292"/>
-      <c r="D15" s="293"/>
+      <c r="C15" s="299"/>
+      <c r="D15" s="300"/>
       <c r="F15">
         <f>F14*0.4</f>
         <v>0.25</v>
@@ -36864,29 +36896,29 @@
     </row>
     <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="I5" s="319" t="s">
+      <c r="I5" s="326" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="319" t="s">
+      <c r="J5" s="326" t="s">
         <v>253</v>
       </c>
-      <c r="K5" s="319" t="s">
+      <c r="K5" s="326" t="s">
         <v>254</v>
       </c>
-      <c r="L5" s="316" t="s">
+      <c r="L5" s="323" t="s">
         <v>255</v>
       </c>
-      <c r="M5" s="317"/>
-      <c r="N5" s="317"/>
-      <c r="O5" s="317"/>
-      <c r="P5" s="318"/>
-      <c r="Q5" s="308" t="s">
+      <c r="M5" s="324"/>
+      <c r="N5" s="324"/>
+      <c r="O5" s="324"/>
+      <c r="P5" s="325"/>
+      <c r="Q5" s="315" t="s">
         <v>256</v>
       </c>
-      <c r="R5" s="309"/>
-      <c r="S5" s="309"/>
-      <c r="T5" s="309"/>
-      <c r="U5" s="310"/>
+      <c r="R5" s="316"/>
+      <c r="S5" s="316"/>
+      <c r="T5" s="316"/>
+      <c r="U5" s="317"/>
     </row>
     <row r="6" spans="1:21" s="189" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="190" t="s">
@@ -36907,9 +36939,9 @@
       <c r="G6" s="190" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="320"/>
-      <c r="J6" s="320"/>
-      <c r="K6" s="320"/>
+      <c r="I6" s="327"/>
+      <c r="J6" s="327"/>
+      <c r="K6" s="327"/>
       <c r="L6" s="191" t="s">
         <v>258</v>
       </c>
@@ -36942,14 +36974,14 @@
       </c>
     </row>
     <row r="7" spans="1:21" s="189" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="316" t="s">
+      <c r="B7" s="323" t="s">
         <v>268</v>
       </c>
-      <c r="C7" s="317"/>
-      <c r="D7" s="317"/>
-      <c r="E7" s="317"/>
-      <c r="F7" s="317"/>
-      <c r="G7" s="318"/>
+      <c r="C7" s="324"/>
+      <c r="D7" s="324"/>
+      <c r="E7" s="324"/>
+      <c r="F7" s="324"/>
+      <c r="G7" s="325"/>
       <c r="I7" s="193" t="s">
         <v>269</v>
       </c>
@@ -37217,13 +37249,13 @@
       <c r="B11" s="199" t="s">
         <v>275</v>
       </c>
-      <c r="C11" s="307" t="s">
+      <c r="C11" s="314" t="s">
         <v>276</v>
       </c>
-      <c r="D11" s="307"/>
-      <c r="E11" s="307"/>
-      <c r="F11" s="307"/>
-      <c r="G11" s="307"/>
+      <c r="D11" s="314"/>
+      <c r="E11" s="314"/>
+      <c r="F11" s="314"/>
+      <c r="G11" s="314"/>
       <c r="I11" s="193" t="s">
         <v>277</v>
       </c>
@@ -37277,14 +37309,14 @@
       </c>
     </row>
     <row r="12" spans="1:21" s="198" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B12" s="311" t="s">
+      <c r="B12" s="318" t="s">
         <v>278</v>
       </c>
-      <c r="C12" s="312"/>
-      <c r="D12" s="312"/>
-      <c r="E12" s="312"/>
-      <c r="F12" s="312"/>
-      <c r="G12" s="312"/>
+      <c r="C12" s="319"/>
+      <c r="D12" s="319"/>
+      <c r="E12" s="319"/>
+      <c r="F12" s="319"/>
+      <c r="G12" s="319"/>
       <c r="I12" s="193" t="s">
         <v>279</v>
       </c>
@@ -37294,20 +37326,20 @@
       <c r="K12" s="201" t="s">
         <v>280</v>
       </c>
-      <c r="L12" s="313" t="s">
+      <c r="L12" s="320" t="s">
         <v>276</v>
       </c>
-      <c r="M12" s="314"/>
-      <c r="N12" s="314"/>
-      <c r="O12" s="314"/>
-      <c r="P12" s="315"/>
-      <c r="Q12" s="313" t="s">
+      <c r="M12" s="321"/>
+      <c r="N12" s="321"/>
+      <c r="O12" s="321"/>
+      <c r="P12" s="322"/>
+      <c r="Q12" s="320" t="s">
         <v>276</v>
       </c>
-      <c r="R12" s="314"/>
-      <c r="S12" s="314"/>
-      <c r="T12" s="314"/>
-      <c r="U12" s="315"/>
+      <c r="R12" s="321"/>
+      <c r="S12" s="321"/>
+      <c r="T12" s="321"/>
+      <c r="U12" s="322"/>
     </row>
     <row r="13" spans="1:21" s="198" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B13" s="199">
@@ -37558,13 +37590,13 @@
       <c r="B18" s="199" t="s">
         <v>275</v>
       </c>
-      <c r="C18" s="307" t="s">
+      <c r="C18" s="314" t="s">
         <v>276</v>
       </c>
-      <c r="D18" s="307"/>
-      <c r="E18" s="307"/>
-      <c r="F18" s="307"/>
-      <c r="G18" s="307"/>
+      <c r="D18" s="314"/>
+      <c r="E18" s="314"/>
+      <c r="F18" s="314"/>
+      <c r="G18" s="314"/>
     </row>
     <row r="19" spans="2:21" s="198" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="I19" s="198" t="s">
@@ -38312,16 +38344,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="321" t="e">
+      <c r="A1" s="329" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="321"/>
-      <c r="C1" s="321"/>
-      <c r="D1" s="321"/>
-      <c r="E1" s="321"/>
-      <c r="F1" s="321"/>
-      <c r="G1" s="321"/>
+      <c r="B1" s="329"/>
+      <c r="C1" s="329"/>
+      <c r="D1" s="329"/>
+      <c r="E1" s="329"/>
+      <c r="F1" s="329"/>
+      <c r="G1" s="329"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -38330,15 +38362,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="295" t="s">
+      <c r="A3" s="302" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="295"/>
-      <c r="C3" s="295"/>
-      <c r="D3" s="295"/>
-      <c r="E3" s="295"/>
-      <c r="F3" s="295"/>
-      <c r="G3" s="295"/>
+      <c r="B3" s="302"/>
+      <c r="C3" s="302"/>
+      <c r="D3" s="302"/>
+      <c r="E3" s="302"/>
+      <c r="F3" s="302"/>
+      <c r="G3" s="302"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -38354,13 +38386,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="296" t="s">
+      <c r="C4" s="303" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="297"/>
-      <c r="E4" s="297"/>
-      <c r="F4" s="297"/>
-      <c r="G4" s="298"/>
+      <c r="D4" s="304"/>
+      <c r="E4" s="304"/>
+      <c r="F4" s="304"/>
+      <c r="G4" s="305"/>
       <c r="N4" s="139" t="s">
         <v>168</v>
       </c>
@@ -38370,11 +38402,11 @@
         <v>16</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="299"/>
-      <c r="D5" s="294"/>
-      <c r="E5" s="294"/>
-      <c r="F5" s="294"/>
-      <c r="G5" s="294"/>
+      <c r="C5" s="306"/>
+      <c r="D5" s="301"/>
+      <c r="E5" s="301"/>
+      <c r="F5" s="301"/>
+      <c r="G5" s="301"/>
       <c r="N5" s="142"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -38382,11 +38414,11 @@
         <v>17</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="299"/>
-      <c r="D6" s="294"/>
-      <c r="E6" s="294"/>
-      <c r="F6" s="294"/>
-      <c r="G6" s="294"/>
+      <c r="C6" s="306"/>
+      <c r="D6" s="301"/>
+      <c r="E6" s="301"/>
+      <c r="F6" s="301"/>
+      <c r="G6" s="301"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -38394,11 +38426,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="299"/>
-      <c r="D7" s="294"/>
-      <c r="E7" s="294"/>
-      <c r="F7" s="294"/>
-      <c r="G7" s="294"/>
+      <c r="C7" s="306"/>
+      <c r="D7" s="301"/>
+      <c r="E7" s="301"/>
+      <c r="F7" s="301"/>
+      <c r="G7" s="301"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -38406,11 +38438,11 @@
         <v>78</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="294"/>
-      <c r="D8" s="294"/>
-      <c r="E8" s="294"/>
-      <c r="F8" s="294"/>
-      <c r="G8" s="294"/>
+      <c r="C8" s="301"/>
+      <c r="D8" s="301"/>
+      <c r="E8" s="301"/>
+      <c r="F8" s="301"/>
+      <c r="G8" s="301"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -38418,11 +38450,11 @@
         <v>202</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="300"/>
-      <c r="D9" s="300"/>
-      <c r="E9" s="300"/>
-      <c r="F9" s="300"/>
-      <c r="G9" s="300"/>
+      <c r="C9" s="307"/>
+      <c r="D9" s="307"/>
+      <c r="E9" s="307"/>
+      <c r="F9" s="307"/>
+      <c r="G9" s="307"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -38430,11 +38462,11 @@
         <v>80</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="322"/>
-      <c r="D10" s="322"/>
-      <c r="E10" s="322"/>
-      <c r="F10" s="322"/>
-      <c r="G10" s="322"/>
+      <c r="C10" s="328"/>
+      <c r="D10" s="328"/>
+      <c r="E10" s="328"/>
+      <c r="F10" s="328"/>
+      <c r="G10" s="328"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -38447,37 +38479,37 @@
       <c r="A12" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="301" t="s">
+      <c r="B12" s="308" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="302"/>
-      <c r="D12" s="303"/>
+      <c r="C12" s="309"/>
+      <c r="D12" s="310"/>
       <c r="N12" s="141" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="304" t="s">
+      <c r="B13" s="311" t="s">
         <v>153</v>
       </c>
-      <c r="C13" s="305"/>
-      <c r="D13" s="306"/>
+      <c r="C13" s="312"/>
+      <c r="D13" s="313"/>
       <c r="N13" s="142"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="288" t="s">
+      <c r="B14" s="295" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="289"/>
-      <c r="D14" s="290"/>
+      <c r="C14" s="296"/>
+      <c r="D14" s="297"/>
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="291" t="s">
+      <c r="B15" s="298" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="292"/>
-      <c r="D15" s="293"/>
+      <c r="C15" s="299"/>
+      <c r="D15" s="300"/>
       <c r="N15" s="142"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -39697,6 +39729,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -39704,12 +39742,6 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>
@@ -39767,26 +39799,26 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="323" t="s">
+      <c r="D3" s="330" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="323"/>
-      <c r="F3" s="323" t="s">
+      <c r="E3" s="330"/>
+      <c r="F3" s="330" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="323"/>
-      <c r="H3" s="323"/>
-      <c r="I3" s="323" t="s">
+      <c r="G3" s="330"/>
+      <c r="H3" s="330"/>
+      <c r="I3" s="330" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="323"/>
-      <c r="K3" s="323"/>
+      <c r="J3" s="330"/>
+      <c r="K3" s="330"/>
       <c r="L3" s="134"/>
-      <c r="M3" s="323" t="s">
+      <c r="M3" s="330" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="323"/>
-      <c r="O3" s="323"/>
+      <c r="N3" s="330"/>
+      <c r="O3" s="330"/>
     </row>
     <row r="4" spans="1:16" s="47" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="46" t="s">

</xml_diff>

<commit_message>
Update purpose in user guide and let's start. Change account balance to prior available water.
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C8C66A-1F32-41AF-AE1B-35BE64C14302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA5BF9D2-572B-48D4-AB62-418420D3C624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-1260" windowWidth="29040" windowHeight="15720" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="62" r:id="rId1"/>
@@ -3368,52 +3368,19 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="6" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="7" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3470,6 +3437,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3502,6 +3475,51 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3605,11 +3623,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3631,24 +3649,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="7" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -14481,22 +14481,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:colOff>321469</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>144135</xdr:rowOff>
+      <xdr:rowOff>11906</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1098246</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>403469</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>22141</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16">
+        <xdr:cNvPr id="16" name="Picture 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B81C37B0-5399-07E0-623D-92904A69DFAC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4E4771B-F3CD-1D28-8876-667B9E51458D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14512,8 +14512,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="276225" y="3173085"/>
-          <a:ext cx="4968875" cy="954111"/>
+          <a:off x="571500" y="2988469"/>
+          <a:ext cx="5791047" cy="1165141"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -15116,20 +15116,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="268" t="s">
+      <c r="A1" s="257" t="s">
         <v>351</v>
       </c>
-      <c r="B1" s="268"/>
-      <c r="C1" s="268"/>
-      <c r="D1" s="268"/>
-      <c r="E1" s="268"/>
-      <c r="F1" s="268"/>
-      <c r="G1" s="268"/>
-      <c r="H1" s="268"/>
-      <c r="I1" s="268"/>
-      <c r="J1" s="268"/>
-      <c r="K1" s="268"/>
-      <c r="L1" s="268"/>
+      <c r="B1" s="257"/>
+      <c r="C1" s="257"/>
+      <c r="D1" s="257"/>
+      <c r="E1" s="257"/>
+      <c r="F1" s="257"/>
+      <c r="G1" s="257"/>
+      <c r="H1" s="257"/>
+      <c r="I1" s="257"/>
+      <c r="J1" s="257"/>
+      <c r="K1" s="257"/>
+      <c r="L1" s="257"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -15155,41 +15155,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="61" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="269" t="s">
+      <c r="A4" s="258" t="s">
         <v>352</v>
       </c>
-      <c r="B4" s="270"/>
-      <c r="C4" s="270"/>
-      <c r="D4" s="270"/>
-      <c r="E4" s="270"/>
-      <c r="F4" s="270"/>
-      <c r="G4" s="270"/>
-      <c r="H4" s="270"/>
-      <c r="I4" s="270"/>
-      <c r="J4" s="270"/>
-      <c r="K4" s="270"/>
-      <c r="L4" s="271"/>
-      <c r="N4" s="272"/>
-      <c r="O4" s="272"/>
-      <c r="P4" s="272"/>
-      <c r="Q4" s="272"/>
-      <c r="R4" s="272"/>
+      <c r="B4" s="259"/>
+      <c r="C4" s="259"/>
+      <c r="D4" s="259"/>
+      <c r="E4" s="259"/>
+      <c r="F4" s="259"/>
+      <c r="G4" s="259"/>
+      <c r="H4" s="259"/>
+      <c r="I4" s="259"/>
+      <c r="J4" s="259"/>
+      <c r="K4" s="259"/>
+      <c r="L4" s="260"/>
+      <c r="N4" s="261"/>
+      <c r="O4" s="261"/>
+      <c r="P4" s="261"/>
+      <c r="Q4" s="261"/>
+      <c r="R4" s="261"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="273" t="s">
+      <c r="A5" s="262" t="s">
         <v>335</v>
       </c>
-      <c r="B5" s="274"/>
-      <c r="C5" s="274"/>
-      <c r="D5" s="274"/>
-      <c r="E5" s="274"/>
-      <c r="F5" s="274"/>
-      <c r="G5" s="274"/>
-      <c r="H5" s="274"/>
-      <c r="I5" s="274"/>
-      <c r="J5" s="274"/>
-      <c r="K5" s="274"/>
-      <c r="L5" s="275"/>
+      <c r="B5" s="263"/>
+      <c r="C5" s="263"/>
+      <c r="D5" s="263"/>
+      <c r="E5" s="263"/>
+      <c r="F5" s="263"/>
+      <c r="G5" s="263"/>
+      <c r="H5" s="263"/>
+      <c r="I5" s="263"/>
+      <c r="J5" s="263"/>
+      <c r="K5" s="263"/>
+      <c r="L5" s="264"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15197,20 +15197,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="273" t="s">
+      <c r="A6" s="262" t="s">
         <v>353</v>
       </c>
-      <c r="B6" s="274"/>
-      <c r="C6" s="274"/>
-      <c r="D6" s="274"/>
-      <c r="E6" s="274"/>
-      <c r="F6" s="274"/>
-      <c r="G6" s="274"/>
-      <c r="H6" s="274"/>
-      <c r="I6" s="274"/>
-      <c r="J6" s="274"/>
-      <c r="K6" s="274"/>
-      <c r="L6" s="275"/>
+      <c r="B6" s="263"/>
+      <c r="C6" s="263"/>
+      <c r="D6" s="263"/>
+      <c r="E6" s="263"/>
+      <c r="F6" s="263"/>
+      <c r="G6" s="263"/>
+      <c r="H6" s="263"/>
+      <c r="I6" s="263"/>
+      <c r="J6" s="263"/>
+      <c r="K6" s="263"/>
+      <c r="L6" s="264"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15219,19 +15219,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="233"/>
-      <c r="B7" s="274" t="s">
+      <c r="B7" s="263" t="s">
         <v>354</v>
       </c>
-      <c r="C7" s="274"/>
-      <c r="D7" s="274"/>
-      <c r="E7" s="274"/>
-      <c r="F7" s="274"/>
-      <c r="G7" s="274"/>
-      <c r="H7" s="274"/>
-      <c r="I7" s="274"/>
-      <c r="J7" s="274"/>
-      <c r="K7" s="274"/>
-      <c r="L7" s="275"/>
+      <c r="C7" s="263"/>
+      <c r="D7" s="263"/>
+      <c r="E7" s="263"/>
+      <c r="F7" s="263"/>
+      <c r="G7" s="263"/>
+      <c r="H7" s="263"/>
+      <c r="I7" s="263"/>
+      <c r="J7" s="263"/>
+      <c r="K7" s="263"/>
+      <c r="L7" s="264"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15240,19 +15240,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="234"/>
-      <c r="B8" s="289" t="s">
+      <c r="B8" s="280" t="s">
         <v>355</v>
       </c>
-      <c r="C8" s="289"/>
-      <c r="D8" s="289"/>
-      <c r="E8" s="289"/>
-      <c r="F8" s="289"/>
-      <c r="G8" s="289"/>
-      <c r="H8" s="289"/>
-      <c r="I8" s="289"/>
-      <c r="J8" s="289"/>
-      <c r="K8" s="289"/>
-      <c r="L8" s="290"/>
+      <c r="C8" s="280"/>
+      <c r="D8" s="280"/>
+      <c r="E8" s="280"/>
+      <c r="F8" s="280"/>
+      <c r="G8" s="280"/>
+      <c r="H8" s="280"/>
+      <c r="I8" s="280"/>
+      <c r="J8" s="280"/>
+      <c r="K8" s="280"/>
+      <c r="L8" s="281"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15274,106 +15274,106 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="291" t="s">
+      <c r="A10" s="282" t="s">
         <v>390</v>
       </c>
-      <c r="B10" s="292"/>
-      <c r="C10" s="292"/>
-      <c r="D10" s="292"/>
-      <c r="E10" s="292"/>
-      <c r="F10" s="292"/>
-      <c r="G10" s="292"/>
-      <c r="H10" s="292"/>
-      <c r="I10" s="292"/>
-      <c r="J10" s="292"/>
-      <c r="K10" s="292"/>
-      <c r="L10" s="293"/>
+      <c r="B10" s="283"/>
+      <c r="C10" s="283"/>
+      <c r="D10" s="283"/>
+      <c r="E10" s="283"/>
+      <c r="F10" s="283"/>
+      <c r="G10" s="283"/>
+      <c r="H10" s="283"/>
+      <c r="I10" s="283"/>
+      <c r="J10" s="283"/>
+      <c r="K10" s="283"/>
+      <c r="L10" s="284"/>
     </row>
     <row r="11" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="246" t="s">
         <v>391</v>
       </c>
-      <c r="B11" s="337" t="s">
+      <c r="B11" s="285" t="s">
         <v>394</v>
       </c>
-      <c r="C11" s="337"/>
-      <c r="D11" s="337"/>
-      <c r="E11" s="337"/>
-      <c r="F11" s="337"/>
-      <c r="G11" s="337"/>
-      <c r="H11" s="337"/>
-      <c r="I11" s="337"/>
-      <c r="J11" s="337"/>
-      <c r="K11" s="337"/>
-      <c r="L11" s="249"/>
+      <c r="C11" s="285"/>
+      <c r="D11" s="285"/>
+      <c r="E11" s="285"/>
+      <c r="F11" s="285"/>
+      <c r="G11" s="285"/>
+      <c r="H11" s="285"/>
+      <c r="I11" s="285"/>
+      <c r="J11" s="285"/>
+      <c r="K11" s="285"/>
+      <c r="L11" s="286"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="246" t="s">
         <v>392</v>
       </c>
-      <c r="B12" s="337" t="s">
+      <c r="B12" s="285" t="s">
         <v>395</v>
       </c>
-      <c r="C12" s="337"/>
-      <c r="D12" s="337"/>
-      <c r="E12" s="337"/>
-      <c r="F12" s="337"/>
-      <c r="G12" s="337"/>
-      <c r="H12" s="337"/>
-      <c r="I12" s="337"/>
-      <c r="J12" s="337"/>
-      <c r="K12" s="337"/>
-      <c r="L12" s="249"/>
+      <c r="C12" s="285"/>
+      <c r="D12" s="285"/>
+      <c r="E12" s="285"/>
+      <c r="F12" s="285"/>
+      <c r="G12" s="285"/>
+      <c r="H12" s="285"/>
+      <c r="I12" s="285"/>
+      <c r="J12" s="285"/>
+      <c r="K12" s="285"/>
+      <c r="L12" s="286"/>
     </row>
     <row r="13" spans="1:18" s="59" customFormat="1" ht="90.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="246"/>
-      <c r="B13" s="337"/>
-      <c r="C13" s="337"/>
-      <c r="D13" s="337"/>
-      <c r="E13" s="337"/>
-      <c r="F13" s="337"/>
-      <c r="G13" s="337"/>
-      <c r="H13" s="337"/>
-      <c r="I13" s="337"/>
-      <c r="J13" s="337"/>
-      <c r="K13" s="337"/>
-      <c r="L13" s="249"/>
+      <c r="B13" s="285"/>
+      <c r="C13" s="285"/>
+      <c r="D13" s="285"/>
+      <c r="E13" s="285"/>
+      <c r="F13" s="285"/>
+      <c r="G13" s="285"/>
+      <c r="H13" s="285"/>
+      <c r="I13" s="285"/>
+      <c r="J13" s="285"/>
+      <c r="K13" s="285"/>
+      <c r="L13" s="286"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="246" t="s">
         <v>393</v>
       </c>
-      <c r="B14" s="337" t="s">
+      <c r="B14" s="285" t="s">
         <v>396</v>
       </c>
-      <c r="C14" s="337"/>
-      <c r="D14" s="337"/>
-      <c r="E14" s="337"/>
-      <c r="F14" s="337"/>
-      <c r="G14" s="337"/>
-      <c r="H14" s="337"/>
-      <c r="I14" s="337"/>
-      <c r="J14" s="337"/>
-      <c r="K14" s="337"/>
-      <c r="L14" s="249"/>
+      <c r="C14" s="285"/>
+      <c r="D14" s="285"/>
+      <c r="E14" s="285"/>
+      <c r="F14" s="285"/>
+      <c r="G14" s="285"/>
+      <c r="H14" s="285"/>
+      <c r="I14" s="285"/>
+      <c r="J14" s="285"/>
+      <c r="K14" s="285"/>
+      <c r="L14" s="286"/>
     </row>
     <row r="15" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="338" t="s">
+      <c r="A15" s="252" t="s">
         <v>401</v>
       </c>
-      <c r="B15" s="339"/>
-      <c r="C15" s="339"/>
-      <c r="D15" s="339"/>
-      <c r="E15" s="342" t="s">
+      <c r="B15" s="253"/>
+      <c r="C15" s="253"/>
+      <c r="D15" s="253"/>
+      <c r="E15" s="251" t="s">
         <v>402</v>
       </c>
-      <c r="F15" s="340"/>
-      <c r="G15" s="340"/>
-      <c r="H15" s="340"/>
-      <c r="I15" s="340"/>
-      <c r="J15" s="340"/>
-      <c r="K15" s="340"/>
-      <c r="L15" s="341"/>
+      <c r="F15" s="249"/>
+      <c r="G15" s="249"/>
+      <c r="H15" s="249"/>
+      <c r="I15" s="249"/>
+      <c r="J15" s="249"/>
+      <c r="K15" s="249"/>
+      <c r="L15" s="250"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="113"/>
@@ -15390,84 +15390,84 @@
       <c r="L16" s="113"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="276" t="s">
+      <c r="A17" s="265" t="s">
         <v>205</v>
       </c>
-      <c r="B17" s="277"/>
-      <c r="C17" s="277"/>
-      <c r="D17" s="277"/>
-      <c r="E17" s="277"/>
-      <c r="F17" s="277"/>
-      <c r="G17" s="277"/>
-      <c r="H17" s="277"/>
-      <c r="I17" s="277"/>
-      <c r="J17" s="277"/>
-      <c r="K17" s="277"/>
-      <c r="L17" s="278"/>
+      <c r="B17" s="266"/>
+      <c r="C17" s="266"/>
+      <c r="D17" s="266"/>
+      <c r="E17" s="266"/>
+      <c r="F17" s="266"/>
+      <c r="G17" s="266"/>
+      <c r="H17" s="266"/>
+      <c r="I17" s="266"/>
+      <c r="J17" s="266"/>
+      <c r="K17" s="266"/>
+      <c r="L17" s="267"/>
     </row>
     <row r="18" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="279" t="s">
+      <c r="A18" s="268" t="s">
         <v>336</v>
       </c>
-      <c r="B18" s="280"/>
-      <c r="C18" s="280"/>
-      <c r="D18" s="280"/>
-      <c r="E18" s="280"/>
-      <c r="F18" s="280"/>
-      <c r="G18" s="280"/>
-      <c r="H18" s="280"/>
-      <c r="I18" s="280"/>
-      <c r="J18" s="280"/>
-      <c r="K18" s="280"/>
-      <c r="L18" s="281"/>
+      <c r="B18" s="269"/>
+      <c r="C18" s="269"/>
+      <c r="D18" s="269"/>
+      <c r="E18" s="269"/>
+      <c r="F18" s="269"/>
+      <c r="G18" s="269"/>
+      <c r="H18" s="269"/>
+      <c r="I18" s="269"/>
+      <c r="J18" s="269"/>
+      <c r="K18" s="269"/>
+      <c r="L18" s="270"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="282" t="s">
+      <c r="A19" s="271" t="s">
         <v>337</v>
       </c>
-      <c r="B19" s="260"/>
-      <c r="C19" s="260"/>
-      <c r="D19" s="260"/>
-      <c r="E19" s="260"/>
-      <c r="F19" s="260"/>
-      <c r="G19" s="260"/>
-      <c r="H19" s="260"/>
-      <c r="I19" s="260"/>
-      <c r="J19" s="260"/>
-      <c r="K19" s="260"/>
-      <c r="L19" s="261"/>
+      <c r="B19" s="272"/>
+      <c r="C19" s="272"/>
+      <c r="D19" s="272"/>
+      <c r="E19" s="272"/>
+      <c r="F19" s="272"/>
+      <c r="G19" s="272"/>
+      <c r="H19" s="272"/>
+      <c r="I19" s="272"/>
+      <c r="J19" s="272"/>
+      <c r="K19" s="272"/>
+      <c r="L19" s="273"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="282" t="s">
+      <c r="A20" s="271" t="s">
         <v>206</v>
       </c>
-      <c r="B20" s="260"/>
-      <c r="C20" s="260"/>
-      <c r="D20" s="260"/>
-      <c r="E20" s="260"/>
-      <c r="F20" s="260"/>
-      <c r="G20" s="260"/>
-      <c r="H20" s="260"/>
-      <c r="I20" s="260"/>
-      <c r="J20" s="260"/>
-      <c r="K20" s="260"/>
-      <c r="L20" s="261"/>
+      <c r="B20" s="272"/>
+      <c r="C20" s="272"/>
+      <c r="D20" s="272"/>
+      <c r="E20" s="272"/>
+      <c r="F20" s="272"/>
+      <c r="G20" s="272"/>
+      <c r="H20" s="272"/>
+      <c r="I20" s="272"/>
+      <c r="J20" s="272"/>
+      <c r="K20" s="272"/>
+      <c r="L20" s="273"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="283" t="s">
+      <c r="A21" s="274" t="s">
         <v>338</v>
       </c>
-      <c r="B21" s="284"/>
-      <c r="C21" s="284"/>
-      <c r="D21" s="284"/>
-      <c r="E21" s="284"/>
-      <c r="F21" s="284"/>
-      <c r="G21" s="284"/>
-      <c r="H21" s="284"/>
-      <c r="I21" s="284"/>
-      <c r="J21" s="284"/>
-      <c r="K21" s="284"/>
-      <c r="L21" s="285"/>
+      <c r="B21" s="275"/>
+      <c r="C21" s="275"/>
+      <c r="D21" s="275"/>
+      <c r="E21" s="275"/>
+      <c r="F21" s="275"/>
+      <c r="G21" s="275"/>
+      <c r="H21" s="275"/>
+      <c r="I21" s="275"/>
+      <c r="J21" s="275"/>
+      <c r="K21" s="275"/>
+      <c r="L21" s="276"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="113"/>
@@ -15484,332 +15484,332 @@
       <c r="L22" s="113"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="286" t="s">
+      <c r="A23" s="277" t="s">
         <v>334</v>
       </c>
-      <c r="B23" s="287"/>
-      <c r="C23" s="287"/>
-      <c r="D23" s="287"/>
-      <c r="E23" s="287"/>
-      <c r="F23" s="287"/>
-      <c r="G23" s="287"/>
-      <c r="H23" s="287"/>
-      <c r="I23" s="287"/>
-      <c r="J23" s="287"/>
-      <c r="K23" s="287"/>
-      <c r="L23" s="288"/>
+      <c r="B23" s="278"/>
+      <c r="C23" s="278"/>
+      <c r="D23" s="278"/>
+      <c r="E23" s="278"/>
+      <c r="F23" s="278"/>
+      <c r="G23" s="278"/>
+      <c r="H23" s="278"/>
+      <c r="I23" s="278"/>
+      <c r="J23" s="278"/>
+      <c r="K23" s="278"/>
+      <c r="L23" s="279"/>
       <c r="N23" s="1"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="265" t="s">
+      <c r="A24" s="254" t="s">
         <v>215</v>
       </c>
-      <c r="B24" s="266"/>
-      <c r="C24" s="266"/>
-      <c r="D24" s="266"/>
-      <c r="E24" s="266"/>
-      <c r="F24" s="266"/>
-      <c r="G24" s="266"/>
-      <c r="H24" s="266"/>
-      <c r="I24" s="266"/>
-      <c r="J24" s="266"/>
-      <c r="K24" s="266"/>
-      <c r="L24" s="267"/>
+      <c r="B24" s="255"/>
+      <c r="C24" s="255"/>
+      <c r="D24" s="255"/>
+      <c r="E24" s="255"/>
+      <c r="F24" s="255"/>
+      <c r="G24" s="255"/>
+      <c r="H24" s="255"/>
+      <c r="I24" s="255"/>
+      <c r="J24" s="255"/>
+      <c r="K24" s="255"/>
+      <c r="L24" s="256"/>
       <c r="N24" s="1"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="228">
         <v>1</v>
       </c>
-      <c r="B25" s="253" t="s">
+      <c r="B25" s="289" t="s">
         <v>214</v>
       </c>
-      <c r="C25" s="253"/>
-      <c r="D25" s="253"/>
-      <c r="E25" s="253"/>
-      <c r="F25" s="253"/>
-      <c r="G25" s="253"/>
-      <c r="H25" s="253"/>
-      <c r="I25" s="253"/>
-      <c r="J25" s="253"/>
-      <c r="K25" s="253"/>
-      <c r="L25" s="254"/>
+      <c r="C25" s="289"/>
+      <c r="D25" s="289"/>
+      <c r="E25" s="289"/>
+      <c r="F25" s="289"/>
+      <c r="G25" s="289"/>
+      <c r="H25" s="289"/>
+      <c r="I25" s="289"/>
+      <c r="J25" s="289"/>
+      <c r="K25" s="289"/>
+      <c r="L25" s="290"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="228">
         <v>2</v>
       </c>
-      <c r="B26" s="253" t="s">
+      <c r="B26" s="289" t="s">
         <v>330</v>
       </c>
-      <c r="C26" s="253"/>
-      <c r="D26" s="253"/>
-      <c r="E26" s="253"/>
-      <c r="F26" s="253"/>
-      <c r="G26" s="253"/>
-      <c r="H26" s="253"/>
-      <c r="I26" s="253"/>
-      <c r="J26" s="253"/>
-      <c r="K26" s="253"/>
-      <c r="L26" s="254"/>
+      <c r="C26" s="289"/>
+      <c r="D26" s="289"/>
+      <c r="E26" s="289"/>
+      <c r="F26" s="289"/>
+      <c r="G26" s="289"/>
+      <c r="H26" s="289"/>
+      <c r="I26" s="289"/>
+      <c r="J26" s="289"/>
+      <c r="K26" s="289"/>
+      <c r="L26" s="290"/>
       <c r="N26" s="106"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="228">
         <v>3</v>
       </c>
-      <c r="B27" s="253" t="s">
+      <c r="B27" s="289" t="s">
         <v>207</v>
       </c>
-      <c r="C27" s="253"/>
-      <c r="D27" s="253"/>
-      <c r="E27" s="253"/>
-      <c r="F27" s="253"/>
-      <c r="G27" s="253"/>
-      <c r="H27" s="253"/>
-      <c r="I27" s="253"/>
-      <c r="J27" s="253"/>
-      <c r="K27" s="253"/>
-      <c r="L27" s="254"/>
+      <c r="C27" s="289"/>
+      <c r="D27" s="289"/>
+      <c r="E27" s="289"/>
+      <c r="F27" s="289"/>
+      <c r="G27" s="289"/>
+      <c r="H27" s="289"/>
+      <c r="I27" s="289"/>
+      <c r="J27" s="289"/>
+      <c r="K27" s="289"/>
+      <c r="L27" s="290"/>
       <c r="N27" s="106"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="228">
         <v>4</v>
       </c>
-      <c r="B28" s="253" t="s">
+      <c r="B28" s="289" t="s">
         <v>339</v>
       </c>
-      <c r="C28" s="253"/>
-      <c r="D28" s="253"/>
-      <c r="E28" s="253"/>
-      <c r="F28" s="253"/>
-      <c r="G28" s="253"/>
-      <c r="H28" s="253"/>
-      <c r="I28" s="253"/>
-      <c r="J28" s="253"/>
-      <c r="K28" s="253"/>
-      <c r="L28" s="254"/>
+      <c r="C28" s="289"/>
+      <c r="D28" s="289"/>
+      <c r="E28" s="289"/>
+      <c r="F28" s="289"/>
+      <c r="G28" s="289"/>
+      <c r="H28" s="289"/>
+      <c r="I28" s="289"/>
+      <c r="J28" s="289"/>
+      <c r="K28" s="289"/>
+      <c r="L28" s="290"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="228">
         <v>5</v>
       </c>
-      <c r="B29" s="253" t="s">
+      <c r="B29" s="289" t="s">
         <v>208</v>
       </c>
-      <c r="C29" s="253"/>
-      <c r="D29" s="253"/>
-      <c r="E29" s="253"/>
-      <c r="F29" s="253"/>
-      <c r="G29" s="253"/>
-      <c r="H29" s="253"/>
-      <c r="I29" s="253"/>
-      <c r="J29" s="253"/>
-      <c r="K29" s="253"/>
-      <c r="L29" s="254"/>
+      <c r="C29" s="289"/>
+      <c r="D29" s="289"/>
+      <c r="E29" s="289"/>
+      <c r="F29" s="289"/>
+      <c r="G29" s="289"/>
+      <c r="H29" s="289"/>
+      <c r="I29" s="289"/>
+      <c r="J29" s="289"/>
+      <c r="K29" s="289"/>
+      <c r="L29" s="290"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="228"/>
-      <c r="B30" s="253" t="s">
+      <c r="B30" s="289" t="s">
         <v>209</v>
       </c>
-      <c r="C30" s="253"/>
-      <c r="D30" s="253"/>
-      <c r="E30" s="253"/>
-      <c r="F30" s="253"/>
-      <c r="G30" s="253"/>
-      <c r="H30" s="253"/>
-      <c r="I30" s="253"/>
-      <c r="J30" s="253"/>
-      <c r="K30" s="253"/>
-      <c r="L30" s="254"/>
+      <c r="C30" s="289"/>
+      <c r="D30" s="289"/>
+      <c r="E30" s="289"/>
+      <c r="F30" s="289"/>
+      <c r="G30" s="289"/>
+      <c r="H30" s="289"/>
+      <c r="I30" s="289"/>
+      <c r="J30" s="289"/>
+      <c r="K30" s="289"/>
+      <c r="L30" s="290"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="228"/>
-      <c r="B31" s="253" t="s">
+      <c r="B31" s="289" t="s">
         <v>210</v>
       </c>
-      <c r="C31" s="253"/>
-      <c r="D31" s="253"/>
-      <c r="E31" s="253"/>
-      <c r="F31" s="253"/>
-      <c r="G31" s="253"/>
-      <c r="H31" s="253"/>
-      <c r="I31" s="253"/>
-      <c r="J31" s="253"/>
-      <c r="K31" s="253"/>
-      <c r="L31" s="254"/>
+      <c r="C31" s="289"/>
+      <c r="D31" s="289"/>
+      <c r="E31" s="289"/>
+      <c r="F31" s="289"/>
+      <c r="G31" s="289"/>
+      <c r="H31" s="289"/>
+      <c r="I31" s="289"/>
+      <c r="J31" s="289"/>
+      <c r="K31" s="289"/>
+      <c r="L31" s="290"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="262" t="s">
+      <c r="A32" s="291" t="s">
         <v>216</v>
       </c>
-      <c r="B32" s="263"/>
-      <c r="C32" s="263"/>
-      <c r="D32" s="263"/>
-      <c r="E32" s="263"/>
-      <c r="F32" s="263"/>
-      <c r="G32" s="263"/>
-      <c r="H32" s="263"/>
-      <c r="I32" s="263"/>
-      <c r="J32" s="263"/>
-      <c r="K32" s="263"/>
-      <c r="L32" s="264"/>
+      <c r="B32" s="292"/>
+      <c r="C32" s="292"/>
+      <c r="D32" s="292"/>
+      <c r="E32" s="292"/>
+      <c r="F32" s="292"/>
+      <c r="G32" s="292"/>
+      <c r="H32" s="292"/>
+      <c r="I32" s="292"/>
+      <c r="J32" s="292"/>
+      <c r="K32" s="292"/>
+      <c r="L32" s="293"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="228">
         <v>1</v>
       </c>
-      <c r="B33" s="253" t="s">
+      <c r="B33" s="289" t="s">
         <v>211</v>
       </c>
-      <c r="C33" s="253"/>
-      <c r="D33" s="253"/>
-      <c r="E33" s="253"/>
-      <c r="F33" s="253"/>
-      <c r="G33" s="253"/>
-      <c r="H33" s="253"/>
-      <c r="I33" s="253"/>
-      <c r="J33" s="253"/>
-      <c r="K33" s="253"/>
-      <c r="L33" s="254"/>
+      <c r="C33" s="289"/>
+      <c r="D33" s="289"/>
+      <c r="E33" s="289"/>
+      <c r="F33" s="289"/>
+      <c r="G33" s="289"/>
+      <c r="H33" s="289"/>
+      <c r="I33" s="289"/>
+      <c r="J33" s="289"/>
+      <c r="K33" s="289"/>
+      <c r="L33" s="290"/>
       <c r="N33" s="106"/>
     </row>
     <row r="34" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="228"/>
-      <c r="B34" s="251" t="s">
+      <c r="B34" s="287" t="s">
         <v>340</v>
       </c>
-      <c r="C34" s="251"/>
-      <c r="D34" s="251"/>
-      <c r="E34" s="251"/>
-      <c r="F34" s="251"/>
-      <c r="G34" s="251"/>
-      <c r="H34" s="251"/>
-      <c r="I34" s="251"/>
-      <c r="J34" s="251"/>
-      <c r="K34" s="251"/>
-      <c r="L34" s="252"/>
+      <c r="C34" s="287"/>
+      <c r="D34" s="287"/>
+      <c r="E34" s="287"/>
+      <c r="F34" s="287"/>
+      <c r="G34" s="287"/>
+      <c r="H34" s="287"/>
+      <c r="I34" s="287"/>
+      <c r="J34" s="287"/>
+      <c r="K34" s="287"/>
+      <c r="L34" s="288"/>
       <c r="N34" s="106"/>
     </row>
     <row r="35" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="228">
         <v>2</v>
       </c>
-      <c r="B35" s="253" t="s">
+      <c r="B35" s="289" t="s">
         <v>333</v>
       </c>
-      <c r="C35" s="253"/>
-      <c r="D35" s="253"/>
-      <c r="E35" s="253"/>
-      <c r="F35" s="253"/>
-      <c r="G35" s="253"/>
-      <c r="H35" s="253"/>
-      <c r="I35" s="253"/>
-      <c r="J35" s="253"/>
-      <c r="K35" s="253"/>
-      <c r="L35" s="254"/>
+      <c r="C35" s="289"/>
+      <c r="D35" s="289"/>
+      <c r="E35" s="289"/>
+      <c r="F35" s="289"/>
+      <c r="G35" s="289"/>
+      <c r="H35" s="289"/>
+      <c r="I35" s="289"/>
+      <c r="J35" s="289"/>
+      <c r="K35" s="289"/>
+      <c r="L35" s="290"/>
       <c r="N35" s="106"/>
     </row>
     <row r="36" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="228">
         <v>3</v>
       </c>
-      <c r="B36" s="253" t="s">
+      <c r="B36" s="289" t="s">
         <v>322</v>
       </c>
-      <c r="C36" s="253"/>
-      <c r="D36" s="253"/>
-      <c r="E36" s="253"/>
-      <c r="F36" s="253"/>
-      <c r="G36" s="253"/>
-      <c r="H36" s="253"/>
-      <c r="I36" s="253"/>
-      <c r="J36" s="253"/>
-      <c r="K36" s="253"/>
-      <c r="L36" s="254"/>
+      <c r="C36" s="289"/>
+      <c r="D36" s="289"/>
+      <c r="E36" s="289"/>
+      <c r="F36" s="289"/>
+      <c r="G36" s="289"/>
+      <c r="H36" s="289"/>
+      <c r="I36" s="289"/>
+      <c r="J36" s="289"/>
+      <c r="K36" s="289"/>
+      <c r="L36" s="290"/>
       <c r="N36" s="106"/>
     </row>
     <row r="37" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="228">
         <v>4</v>
       </c>
-      <c r="B37" s="253" t="s">
+      <c r="B37" s="289" t="s">
         <v>341</v>
       </c>
-      <c r="C37" s="253"/>
-      <c r="D37" s="253"/>
-      <c r="E37" s="253"/>
-      <c r="F37" s="253"/>
-      <c r="G37" s="253"/>
-      <c r="H37" s="253"/>
-      <c r="I37" s="253"/>
-      <c r="J37" s="253"/>
-      <c r="K37" s="253"/>
-      <c r="L37" s="254"/>
+      <c r="C37" s="289"/>
+      <c r="D37" s="289"/>
+      <c r="E37" s="289"/>
+      <c r="F37" s="289"/>
+      <c r="G37" s="289"/>
+      <c r="H37" s="289"/>
+      <c r="I37" s="289"/>
+      <c r="J37" s="289"/>
+      <c r="K37" s="289"/>
+      <c r="L37" s="290"/>
       <c r="N37" s="106"/>
     </row>
     <row r="38" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="228">
         <v>5</v>
       </c>
-      <c r="B38" s="251" t="s">
+      <c r="B38" s="287" t="s">
         <v>323</v>
       </c>
-      <c r="C38" s="251"/>
-      <c r="D38" s="251"/>
-      <c r="E38" s="251"/>
-      <c r="F38" s="251"/>
-      <c r="G38" s="251"/>
-      <c r="H38" s="251"/>
-      <c r="I38" s="251"/>
-      <c r="J38" s="251"/>
-      <c r="K38" s="251"/>
-      <c r="L38" s="252"/>
+      <c r="C38" s="287"/>
+      <c r="D38" s="287"/>
+      <c r="E38" s="287"/>
+      <c r="F38" s="287"/>
+      <c r="G38" s="287"/>
+      <c r="H38" s="287"/>
+      <c r="I38" s="287"/>
+      <c r="J38" s="287"/>
+      <c r="K38" s="287"/>
+      <c r="L38" s="288"/>
       <c r="N38" s="106"/>
     </row>
     <row r="39" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="228">
         <v>6</v>
       </c>
-      <c r="B39" s="251" t="s">
+      <c r="B39" s="287" t="s">
         <v>328</v>
       </c>
-      <c r="C39" s="251"/>
-      <c r="D39" s="251"/>
-      <c r="E39" s="251"/>
-      <c r="F39" s="251"/>
-      <c r="G39" s="251"/>
-      <c r="H39" s="251"/>
-      <c r="I39" s="251"/>
-      <c r="J39" s="251"/>
-      <c r="K39" s="251"/>
-      <c r="L39" s="252"/>
+      <c r="C39" s="287"/>
+      <c r="D39" s="287"/>
+      <c r="E39" s="287"/>
+      <c r="F39" s="287"/>
+      <c r="G39" s="287"/>
+      <c r="H39" s="287"/>
+      <c r="I39" s="287"/>
+      <c r="J39" s="287"/>
+      <c r="K39" s="287"/>
+      <c r="L39" s="288"/>
       <c r="N39" s="106"/>
     </row>
     <row r="40" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="228">
         <v>7</v>
       </c>
-      <c r="B40" s="253" t="s">
+      <c r="B40" s="289" t="s">
         <v>324</v>
       </c>
-      <c r="C40" s="253"/>
-      <c r="D40" s="253"/>
-      <c r="E40" s="253"/>
-      <c r="F40" s="253"/>
-      <c r="G40" s="253"/>
-      <c r="H40" s="253"/>
-      <c r="I40" s="253"/>
-      <c r="J40" s="253"/>
-      <c r="K40" s="253"/>
-      <c r="L40" s="254"/>
+      <c r="C40" s="289"/>
+      <c r="D40" s="289"/>
+      <c r="E40" s="289"/>
+      <c r="F40" s="289"/>
+      <c r="G40" s="289"/>
+      <c r="H40" s="289"/>
+      <c r="I40" s="289"/>
+      <c r="J40" s="289"/>
+      <c r="K40" s="289"/>
+      <c r="L40" s="290"/>
     </row>
     <row r="41" spans="1:14" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="228"/>
@@ -15826,56 +15826,56 @@
       <c r="L41" s="230"/>
     </row>
     <row r="42" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="262" t="s">
+      <c r="A42" s="291" t="s">
         <v>327</v>
       </c>
-      <c r="B42" s="263"/>
-      <c r="C42" s="263"/>
-      <c r="D42" s="263"/>
-      <c r="E42" s="263"/>
-      <c r="F42" s="263"/>
-      <c r="G42" s="263"/>
-      <c r="H42" s="263"/>
-      <c r="I42" s="263"/>
-      <c r="J42" s="263"/>
-      <c r="K42" s="263"/>
-      <c r="L42" s="264"/>
+      <c r="B42" s="292"/>
+      <c r="C42" s="292"/>
+      <c r="D42" s="292"/>
+      <c r="E42" s="292"/>
+      <c r="F42" s="292"/>
+      <c r="G42" s="292"/>
+      <c r="H42" s="292"/>
+      <c r="I42" s="292"/>
+      <c r="J42" s="292"/>
+      <c r="K42" s="292"/>
+      <c r="L42" s="293"/>
     </row>
     <row r="43" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="231" t="s">
         <v>325</v>
       </c>
-      <c r="B43" s="253" t="s">
+      <c r="B43" s="289" t="s">
         <v>212</v>
       </c>
-      <c r="C43" s="253"/>
-      <c r="D43" s="253"/>
-      <c r="E43" s="253"/>
-      <c r="F43" s="253"/>
-      <c r="G43" s="253"/>
-      <c r="H43" s="253"/>
-      <c r="I43" s="253"/>
-      <c r="J43" s="253"/>
-      <c r="K43" s="253"/>
-      <c r="L43" s="254"/>
+      <c r="C43" s="289"/>
+      <c r="D43" s="289"/>
+      <c r="E43" s="289"/>
+      <c r="F43" s="289"/>
+      <c r="G43" s="289"/>
+      <c r="H43" s="289"/>
+      <c r="I43" s="289"/>
+      <c r="J43" s="289"/>
+      <c r="K43" s="289"/>
+      <c r="L43" s="290"/>
     </row>
     <row r="44" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="232" t="s">
         <v>326</v>
       </c>
-      <c r="B44" s="255" t="s">
+      <c r="B44" s="295" t="s">
         <v>329</v>
       </c>
-      <c r="C44" s="255"/>
-      <c r="D44" s="255"/>
-      <c r="E44" s="255"/>
-      <c r="F44" s="255"/>
-      <c r="G44" s="255"/>
-      <c r="H44" s="255"/>
-      <c r="I44" s="255"/>
-      <c r="J44" s="255"/>
-      <c r="K44" s="255"/>
-      <c r="L44" s="256"/>
+      <c r="C44" s="295"/>
+      <c r="D44" s="295"/>
+      <c r="E44" s="295"/>
+      <c r="F44" s="295"/>
+      <c r="G44" s="295"/>
+      <c r="H44" s="295"/>
+      <c r="I44" s="295"/>
+      <c r="J44" s="295"/>
+      <c r="K44" s="295"/>
+      <c r="L44" s="296"/>
     </row>
     <row r="45" spans="1:14" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="160"/>
@@ -15892,20 +15892,20 @@
       <c r="L45" s="113"/>
     </row>
     <row r="46" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="257" t="s">
+      <c r="A46" s="297" t="s">
         <v>240</v>
       </c>
-      <c r="B46" s="258"/>
-      <c r="C46" s="258"/>
-      <c r="D46" s="258"/>
-      <c r="E46" s="258"/>
-      <c r="F46" s="258"/>
-      <c r="G46" s="258"/>
-      <c r="H46" s="258"/>
-      <c r="I46" s="258"/>
-      <c r="J46" s="258"/>
-      <c r="K46" s="258"/>
-      <c r="L46" s="259"/>
+      <c r="B46" s="298"/>
+      <c r="C46" s="298"/>
+      <c r="D46" s="298"/>
+      <c r="E46" s="298"/>
+      <c r="F46" s="298"/>
+      <c r="G46" s="298"/>
+      <c r="H46" s="298"/>
+      <c r="I46" s="298"/>
+      <c r="J46" s="298"/>
+      <c r="K46" s="298"/>
+      <c r="L46" s="299"/>
     </row>
     <row r="47" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="235" t="s">
@@ -15993,90 +15993,90 @@
       <c r="B52" s="168" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="260" t="s">
+      <c r="C52" s="272" t="s">
         <v>313</v>
       </c>
-      <c r="D52" s="260"/>
-      <c r="E52" s="260"/>
-      <c r="F52" s="260"/>
-      <c r="G52" s="260"/>
-      <c r="H52" s="260"/>
-      <c r="I52" s="260"/>
-      <c r="J52" s="260"/>
-      <c r="K52" s="260"/>
-      <c r="L52" s="261"/>
+      <c r="D52" s="272"/>
+      <c r="E52" s="272"/>
+      <c r="F52" s="272"/>
+      <c r="G52" s="272"/>
+      <c r="H52" s="272"/>
+      <c r="I52" s="272"/>
+      <c r="J52" s="272"/>
+      <c r="K52" s="272"/>
+      <c r="L52" s="273"/>
     </row>
     <row r="53" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="167"/>
       <c r="B53" s="168" t="s">
         <v>314</v>
       </c>
-      <c r="C53" s="260" t="s">
+      <c r="C53" s="272" t="s">
         <v>315</v>
       </c>
-      <c r="D53" s="260"/>
-      <c r="E53" s="260"/>
-      <c r="F53" s="260"/>
-      <c r="G53" s="260"/>
-      <c r="H53" s="260"/>
-      <c r="I53" s="260"/>
-      <c r="J53" s="260"/>
-      <c r="K53" s="260"/>
-      <c r="L53" s="261"/>
+      <c r="D53" s="272"/>
+      <c r="E53" s="272"/>
+      <c r="F53" s="272"/>
+      <c r="G53" s="272"/>
+      <c r="H53" s="272"/>
+      <c r="I53" s="272"/>
+      <c r="J53" s="272"/>
+      <c r="K53" s="272"/>
+      <c r="L53" s="273"/>
     </row>
     <row r="54" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="167"/>
       <c r="B54" s="168" t="s">
         <v>383</v>
       </c>
-      <c r="C54" s="260" t="s">
+      <c r="C54" s="272" t="s">
         <v>384</v>
       </c>
-      <c r="D54" s="260"/>
-      <c r="E54" s="260"/>
-      <c r="F54" s="260"/>
-      <c r="G54" s="260"/>
-      <c r="H54" s="260"/>
-      <c r="I54" s="260"/>
-      <c r="J54" s="260"/>
-      <c r="K54" s="260"/>
-      <c r="L54" s="261"/>
+      <c r="D54" s="272"/>
+      <c r="E54" s="272"/>
+      <c r="F54" s="272"/>
+      <c r="G54" s="272"/>
+      <c r="H54" s="272"/>
+      <c r="I54" s="272"/>
+      <c r="J54" s="272"/>
+      <c r="K54" s="272"/>
+      <c r="L54" s="273"/>
     </row>
     <row r="55" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="167"/>
       <c r="B55" s="168" t="s">
         <v>138</v>
       </c>
-      <c r="C55" s="260" t="s">
+      <c r="C55" s="272" t="s">
         <v>139</v>
       </c>
-      <c r="D55" s="260"/>
-      <c r="E55" s="260"/>
-      <c r="F55" s="260"/>
-      <c r="G55" s="260"/>
-      <c r="H55" s="260"/>
-      <c r="I55" s="260"/>
-      <c r="J55" s="260"/>
-      <c r="K55" s="260"/>
-      <c r="L55" s="261"/>
+      <c r="D55" s="272"/>
+      <c r="E55" s="272"/>
+      <c r="F55" s="272"/>
+      <c r="G55" s="272"/>
+      <c r="H55" s="272"/>
+      <c r="I55" s="272"/>
+      <c r="J55" s="272"/>
+      <c r="K55" s="272"/>
+      <c r="L55" s="273"/>
     </row>
     <row r="56" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="167"/>
       <c r="B56" s="168" t="s">
         <v>238</v>
       </c>
-      <c r="C56" s="260" t="s">
+      <c r="C56" s="272" t="s">
         <v>239</v>
       </c>
-      <c r="D56" s="260"/>
-      <c r="E56" s="260"/>
-      <c r="F56" s="260"/>
-      <c r="G56" s="260"/>
-      <c r="H56" s="260"/>
-      <c r="I56" s="260"/>
-      <c r="J56" s="260"/>
-      <c r="K56" s="260"/>
-      <c r="L56" s="261"/>
+      <c r="D56" s="272"/>
+      <c r="E56" s="272"/>
+      <c r="F56" s="272"/>
+      <c r="G56" s="272"/>
+      <c r="H56" s="272"/>
+      <c r="I56" s="272"/>
+      <c r="J56" s="272"/>
+      <c r="K56" s="272"/>
+      <c r="L56" s="273"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A57" s="167"/>
@@ -16101,18 +16101,18 @@
       <c r="B58" s="168" t="s">
         <v>63</v>
       </c>
-      <c r="C58" s="260" t="s">
+      <c r="C58" s="272" t="s">
         <v>317</v>
       </c>
-      <c r="D58" s="260"/>
-      <c r="E58" s="260"/>
-      <c r="F58" s="260"/>
-      <c r="G58" s="260"/>
-      <c r="H58" s="260"/>
-      <c r="I58" s="260"/>
-      <c r="J58" s="260"/>
-      <c r="K58" s="260"/>
-      <c r="L58" s="261"/>
+      <c r="D58" s="272"/>
+      <c r="E58" s="272"/>
+      <c r="F58" s="272"/>
+      <c r="G58" s="272"/>
+      <c r="H58" s="272"/>
+      <c r="I58" s="272"/>
+      <c r="J58" s="272"/>
+      <c r="K58" s="272"/>
+      <c r="L58" s="273"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="167"/>
@@ -16212,25 +16212,56 @@
       </c>
     </row>
     <row r="76" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A76" s="250" t="s">
+      <c r="A76" s="294" t="s">
         <v>399</v>
       </c>
-      <c r="B76" s="250"/>
-      <c r="C76" s="250"/>
-      <c r="D76" s="250"/>
-      <c r="E76" s="250"/>
-      <c r="F76" s="250"/>
-      <c r="G76" s="250"/>
-      <c r="H76" s="250"/>
-      <c r="I76" s="250"/>
-      <c r="J76" s="250"/>
-      <c r="K76" s="250"/>
-      <c r="L76" s="250"/>
+      <c r="B76" s="294"/>
+      <c r="C76" s="294"/>
+      <c r="D76" s="294"/>
+      <c r="E76" s="294"/>
+      <c r="F76" s="294"/>
+      <c r="G76" s="294"/>
+      <c r="H76" s="294"/>
+      <c r="I76" s="294"/>
+      <c r="J76" s="294"/>
+      <c r="K76" s="294"/>
+      <c r="L76" s="294"/>
     </row>
     <row r="81" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="82" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="A76:L76"/>
+    <mergeCell ref="B39:L39"/>
+    <mergeCell ref="B40:L40"/>
+    <mergeCell ref="B43:L43"/>
+    <mergeCell ref="B44:L44"/>
+    <mergeCell ref="A46:L46"/>
+    <mergeCell ref="C52:L52"/>
+    <mergeCell ref="C55:L55"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="C53:L53"/>
+    <mergeCell ref="C58:L58"/>
+    <mergeCell ref="A42:L42"/>
+    <mergeCell ref="C54:L54"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="B25:L25"/>
+    <mergeCell ref="B26:L26"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B30:L30"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="A32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="B34:L34"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B12:L12"/>
     <mergeCell ref="A15:D15"/>
     <mergeCell ref="A24:L24"/>
     <mergeCell ref="A1:L1"/>
@@ -16247,37 +16278,6 @@
     <mergeCell ref="B7:L7"/>
     <mergeCell ref="B8:L8"/>
     <mergeCell ref="A10:L10"/>
-    <mergeCell ref="B11:L11"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B25:L25"/>
-    <mergeCell ref="B26:L26"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="A32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="B34:L34"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="B12:L12"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="B14:L14"/>
-    <mergeCell ref="A76:L76"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="B40:L40"/>
-    <mergeCell ref="B43:L43"/>
-    <mergeCell ref="B44:L44"/>
-    <mergeCell ref="A46:L46"/>
-    <mergeCell ref="C52:L52"/>
-    <mergeCell ref="C55:L55"/>
-    <mergeCell ref="C56:L56"/>
-    <mergeCell ref="C53:L53"/>
-    <mergeCell ref="C58:L58"/>
-    <mergeCell ref="A42:L42"/>
-    <mergeCell ref="C54:L54"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A65" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -31248,82 +31248,82 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="331" t="s">
+      <c r="A3" s="337" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="331"/>
-      <c r="C3" s="331"/>
+      <c r="B3" s="337"/>
+      <c r="C3" s="337"/>
       <c r="D3" s="128" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="332" t="s">
+      <c r="A4" s="338" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="332"/>
-      <c r="C4" s="332"/>
+      <c r="B4" s="338"/>
+      <c r="C4" s="338"/>
       <c r="D4" s="175" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="336" t="s">
+      <c r="A5" s="342" t="s">
         <v>223</v>
       </c>
-      <c r="B5" s="333"/>
-      <c r="C5" s="333"/>
+      <c r="B5" s="339"/>
+      <c r="C5" s="339"/>
       <c r="D5" s="176" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="334" t="s">
+      <c r="A6" s="340" t="s">
         <v>224</v>
       </c>
-      <c r="B6" s="334"/>
-      <c r="C6" s="334"/>
+      <c r="B6" s="340"/>
+      <c r="C6" s="340"/>
       <c r="D6" s="177" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="335" t="s">
+      <c r="A7" s="341" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="335"/>
-      <c r="C7" s="335"/>
+      <c r="B7" s="341"/>
+      <c r="C7" s="341"/>
       <c r="D7" s="178" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="332" t="s">
+      <c r="A11" s="338" t="s">
         <v>152</v>
       </c>
-      <c r="B11" s="332"/>
-      <c r="C11" s="332"/>
+      <c r="B11" s="338"/>
+      <c r="C11" s="338"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="333" t="s">
+      <c r="A12" s="339" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="333"/>
-      <c r="C12" s="333"/>
+      <c r="B12" s="339"/>
+      <c r="C12" s="339"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="334" t="s">
+      <c r="A13" s="340" t="s">
         <v>154</v>
       </c>
-      <c r="B13" s="334"/>
-      <c r="C13" s="334"/>
+      <c r="B13" s="340"/>
+      <c r="C13" s="340"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="335" t="s">
+      <c r="A14" s="341" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="335"/>
-      <c r="C14" s="335"/>
+      <c r="B14" s="341"/>
+      <c r="C14" s="341"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -31916,16 +31916,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="294" t="str">
+      <c r="A1" s="300" t="str">
         <f>'ReadMe-Directions'!A1</f>
         <v>Immersive Model for Lake Mead based on the Principle of Divide Reservoir Inflow</v>
       </c>
-      <c r="B1" s="294"/>
-      <c r="C1" s="294"/>
-      <c r="D1" s="294"/>
-      <c r="E1" s="294"/>
-      <c r="F1" s="294"/>
-      <c r="G1" s="294"/>
+      <c r="B1" s="300"/>
+      <c r="C1" s="300"/>
+      <c r="D1" s="300"/>
+      <c r="E1" s="300"/>
+      <c r="F1" s="300"/>
+      <c r="G1" s="300"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -31934,15 +31934,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="302" t="s">
+      <c r="A3" s="308" t="s">
         <v>230</v>
       </c>
-      <c r="B3" s="302"/>
-      <c r="C3" s="302"/>
-      <c r="D3" s="302"/>
-      <c r="E3" s="302"/>
-      <c r="F3" s="302"/>
-      <c r="G3" s="302"/>
+      <c r="B3" s="308"/>
+      <c r="C3" s="308"/>
+      <c r="D3" s="308"/>
+      <c r="E3" s="308"/>
+      <c r="F3" s="308"/>
+      <c r="G3" s="308"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -31958,13 +31958,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="303" t="s">
+      <c r="C4" s="309" t="s">
         <v>310</v>
       </c>
-      <c r="D4" s="304"/>
-      <c r="E4" s="304"/>
-      <c r="F4" s="304"/>
-      <c r="G4" s="305"/>
+      <c r="D4" s="310"/>
+      <c r="E4" s="310"/>
+      <c r="F4" s="310"/>
+      <c r="G4" s="311"/>
       <c r="N4" s="141" t="s">
         <v>385</v>
       </c>
@@ -31974,11 +31974,11 @@
         <v>283</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="306"/>
-      <c r="D5" s="301"/>
-      <c r="E5" s="301"/>
-      <c r="F5" s="301"/>
-      <c r="G5" s="301"/>
+      <c r="C5" s="312"/>
+      <c r="D5" s="307"/>
+      <c r="E5" s="307"/>
+      <c r="F5" s="307"/>
+      <c r="G5" s="307"/>
       <c r="N5" s="141"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -31986,11 +31986,11 @@
         <v>242</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="306"/>
-      <c r="D6" s="301"/>
-      <c r="E6" s="301"/>
-      <c r="F6" s="301"/>
-      <c r="G6" s="301"/>
+      <c r="C6" s="312"/>
+      <c r="D6" s="307"/>
+      <c r="E6" s="307"/>
+      <c r="F6" s="307"/>
+      <c r="G6" s="307"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -31998,11 +31998,11 @@
         <v>243</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="306"/>
-      <c r="D7" s="301"/>
-      <c r="E7" s="301"/>
-      <c r="F7" s="301"/>
-      <c r="G7" s="301"/>
+      <c r="C7" s="312"/>
+      <c r="D7" s="307"/>
+      <c r="E7" s="307"/>
+      <c r="F7" s="307"/>
+      <c r="G7" s="307"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -32010,11 +32010,11 @@
         <v>244</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="301"/>
-      <c r="D8" s="301"/>
-      <c r="E8" s="301"/>
-      <c r="F8" s="301"/>
-      <c r="G8" s="301"/>
+      <c r="C8" s="307"/>
+      <c r="D8" s="307"/>
+      <c r="E8" s="307"/>
+      <c r="F8" s="307"/>
+      <c r="G8" s="307"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -32022,11 +32022,11 @@
         <v>18</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="307"/>
-      <c r="D9" s="307"/>
-      <c r="E9" s="307"/>
-      <c r="F9" s="307"/>
-      <c r="G9" s="307"/>
+      <c r="C9" s="313"/>
+      <c r="D9" s="313"/>
+      <c r="E9" s="313"/>
+      <c r="F9" s="313"/>
+      <c r="G9" s="313"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -32034,11 +32034,11 @@
         <v>332</v>
       </c>
       <c r="B10" s="90"/>
-      <c r="C10" s="301"/>
-      <c r="D10" s="301"/>
-      <c r="E10" s="301"/>
-      <c r="F10" s="301"/>
-      <c r="G10" s="301"/>
+      <c r="C10" s="307"/>
+      <c r="D10" s="307"/>
+      <c r="E10" s="307"/>
+      <c r="F10" s="307"/>
+      <c r="G10" s="307"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -32051,28 +32051,28 @@
       <c r="A12" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="308" t="s">
+      <c r="B12" s="314" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="309"/>
-      <c r="D12" s="310"/>
+      <c r="C12" s="315"/>
+      <c r="D12" s="316"/>
       <c r="N12" s="141" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="311" t="s">
+      <c r="B13" s="317" t="s">
         <v>229</v>
       </c>
-      <c r="C13" s="312"/>
-      <c r="D13" s="313"/>
+      <c r="C13" s="318"/>
+      <c r="D13" s="319"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="295" t="s">
+      <c r="B14" s="301" t="s">
         <v>224</v>
       </c>
-      <c r="C14" s="296"/>
-      <c r="D14" s="297"/>
+      <c r="C14" s="302"/>
+      <c r="D14" s="303"/>
       <c r="F14">
         <f>4.5/7.2</f>
         <v>0.625</v>
@@ -32080,11 +32080,11 @@
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="298" t="s">
+      <c r="B15" s="304" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="299"/>
-      <c r="D15" s="300"/>
+      <c r="C15" s="305"/>
+      <c r="D15" s="306"/>
       <c r="F15">
         <f>F14*0.4</f>
         <v>0.25</v>
@@ -36896,29 +36896,29 @@
     </row>
     <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="I5" s="326" t="s">
+      <c r="I5" s="332" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="326" t="s">
+      <c r="J5" s="332" t="s">
         <v>253</v>
       </c>
-      <c r="K5" s="326" t="s">
+      <c r="K5" s="332" t="s">
         <v>254</v>
       </c>
-      <c r="L5" s="323" t="s">
+      <c r="L5" s="329" t="s">
         <v>255</v>
       </c>
-      <c r="M5" s="324"/>
-      <c r="N5" s="324"/>
-      <c r="O5" s="324"/>
-      <c r="P5" s="325"/>
-      <c r="Q5" s="315" t="s">
+      <c r="M5" s="330"/>
+      <c r="N5" s="330"/>
+      <c r="O5" s="330"/>
+      <c r="P5" s="331"/>
+      <c r="Q5" s="321" t="s">
         <v>256</v>
       </c>
-      <c r="R5" s="316"/>
-      <c r="S5" s="316"/>
-      <c r="T5" s="316"/>
-      <c r="U5" s="317"/>
+      <c r="R5" s="322"/>
+      <c r="S5" s="322"/>
+      <c r="T5" s="322"/>
+      <c r="U5" s="323"/>
     </row>
     <row r="6" spans="1:21" s="189" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="190" t="s">
@@ -36939,9 +36939,9 @@
       <c r="G6" s="190" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="327"/>
-      <c r="J6" s="327"/>
-      <c r="K6" s="327"/>
+      <c r="I6" s="333"/>
+      <c r="J6" s="333"/>
+      <c r="K6" s="333"/>
       <c r="L6" s="191" t="s">
         <v>258</v>
       </c>
@@ -36974,14 +36974,14 @@
       </c>
     </row>
     <row r="7" spans="1:21" s="189" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="323" t="s">
+      <c r="B7" s="329" t="s">
         <v>268</v>
       </c>
-      <c r="C7" s="324"/>
-      <c r="D7" s="324"/>
-      <c r="E7" s="324"/>
-      <c r="F7" s="324"/>
-      <c r="G7" s="325"/>
+      <c r="C7" s="330"/>
+      <c r="D7" s="330"/>
+      <c r="E7" s="330"/>
+      <c r="F7" s="330"/>
+      <c r="G7" s="331"/>
       <c r="I7" s="193" t="s">
         <v>269</v>
       </c>
@@ -37249,13 +37249,13 @@
       <c r="B11" s="199" t="s">
         <v>275</v>
       </c>
-      <c r="C11" s="314" t="s">
+      <c r="C11" s="320" t="s">
         <v>276</v>
       </c>
-      <c r="D11" s="314"/>
-      <c r="E11" s="314"/>
-      <c r="F11" s="314"/>
-      <c r="G11" s="314"/>
+      <c r="D11" s="320"/>
+      <c r="E11" s="320"/>
+      <c r="F11" s="320"/>
+      <c r="G11" s="320"/>
       <c r="I11" s="193" t="s">
         <v>277</v>
       </c>
@@ -37309,14 +37309,14 @@
       </c>
     </row>
     <row r="12" spans="1:21" s="198" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B12" s="318" t="s">
+      <c r="B12" s="324" t="s">
         <v>278</v>
       </c>
-      <c r="C12" s="319"/>
-      <c r="D12" s="319"/>
-      <c r="E12" s="319"/>
-      <c r="F12" s="319"/>
-      <c r="G12" s="319"/>
+      <c r="C12" s="325"/>
+      <c r="D12" s="325"/>
+      <c r="E12" s="325"/>
+      <c r="F12" s="325"/>
+      <c r="G12" s="325"/>
       <c r="I12" s="193" t="s">
         <v>279</v>
       </c>
@@ -37326,20 +37326,20 @@
       <c r="K12" s="201" t="s">
         <v>280</v>
       </c>
-      <c r="L12" s="320" t="s">
+      <c r="L12" s="326" t="s">
         <v>276</v>
       </c>
-      <c r="M12" s="321"/>
-      <c r="N12" s="321"/>
-      <c r="O12" s="321"/>
-      <c r="P12" s="322"/>
-      <c r="Q12" s="320" t="s">
+      <c r="M12" s="327"/>
+      <c r="N12" s="327"/>
+      <c r="O12" s="327"/>
+      <c r="P12" s="328"/>
+      <c r="Q12" s="326" t="s">
         <v>276</v>
       </c>
-      <c r="R12" s="321"/>
-      <c r="S12" s="321"/>
-      <c r="T12" s="321"/>
-      <c r="U12" s="322"/>
+      <c r="R12" s="327"/>
+      <c r="S12" s="327"/>
+      <c r="T12" s="327"/>
+      <c r="U12" s="328"/>
     </row>
     <row r="13" spans="1:21" s="198" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B13" s="199">
@@ -37590,13 +37590,13 @@
       <c r="B18" s="199" t="s">
         <v>275</v>
       </c>
-      <c r="C18" s="314" t="s">
+      <c r="C18" s="320" t="s">
         <v>276</v>
       </c>
-      <c r="D18" s="314"/>
-      <c r="E18" s="314"/>
-      <c r="F18" s="314"/>
-      <c r="G18" s="314"/>
+      <c r="D18" s="320"/>
+      <c r="E18" s="320"/>
+      <c r="F18" s="320"/>
+      <c r="G18" s="320"/>
     </row>
     <row r="19" spans="2:21" s="198" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="I19" s="198" t="s">
@@ -38344,16 +38344,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="329" t="e">
+      <c r="A1" s="334" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="329"/>
-      <c r="C1" s="329"/>
-      <c r="D1" s="329"/>
-      <c r="E1" s="329"/>
-      <c r="F1" s="329"/>
-      <c r="G1" s="329"/>
+      <c r="B1" s="334"/>
+      <c r="C1" s="334"/>
+      <c r="D1" s="334"/>
+      <c r="E1" s="334"/>
+      <c r="F1" s="334"/>
+      <c r="G1" s="334"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -38362,15 +38362,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="302" t="s">
+      <c r="A3" s="308" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="302"/>
-      <c r="C3" s="302"/>
-      <c r="D3" s="302"/>
-      <c r="E3" s="302"/>
-      <c r="F3" s="302"/>
-      <c r="G3" s="302"/>
+      <c r="B3" s="308"/>
+      <c r="C3" s="308"/>
+      <c r="D3" s="308"/>
+      <c r="E3" s="308"/>
+      <c r="F3" s="308"/>
+      <c r="G3" s="308"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -38386,13 +38386,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="303" t="s">
+      <c r="C4" s="309" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="304"/>
-      <c r="E4" s="304"/>
-      <c r="F4" s="304"/>
-      <c r="G4" s="305"/>
+      <c r="D4" s="310"/>
+      <c r="E4" s="310"/>
+      <c r="F4" s="310"/>
+      <c r="G4" s="311"/>
       <c r="N4" s="139" t="s">
         <v>168</v>
       </c>
@@ -38402,11 +38402,11 @@
         <v>16</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="306"/>
-      <c r="D5" s="301"/>
-      <c r="E5" s="301"/>
-      <c r="F5" s="301"/>
-      <c r="G5" s="301"/>
+      <c r="C5" s="312"/>
+      <c r="D5" s="307"/>
+      <c r="E5" s="307"/>
+      <c r="F5" s="307"/>
+      <c r="G5" s="307"/>
       <c r="N5" s="142"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -38414,11 +38414,11 @@
         <v>17</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="306"/>
-      <c r="D6" s="301"/>
-      <c r="E6" s="301"/>
-      <c r="F6" s="301"/>
-      <c r="G6" s="301"/>
+      <c r="C6" s="312"/>
+      <c r="D6" s="307"/>
+      <c r="E6" s="307"/>
+      <c r="F6" s="307"/>
+      <c r="G6" s="307"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -38426,11 +38426,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="306"/>
-      <c r="D7" s="301"/>
-      <c r="E7" s="301"/>
-      <c r="F7" s="301"/>
-      <c r="G7" s="301"/>
+      <c r="C7" s="312"/>
+      <c r="D7" s="307"/>
+      <c r="E7" s="307"/>
+      <c r="F7" s="307"/>
+      <c r="G7" s="307"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -38438,11 +38438,11 @@
         <v>78</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="301"/>
-      <c r="D8" s="301"/>
-      <c r="E8" s="301"/>
-      <c r="F8" s="301"/>
-      <c r="G8" s="301"/>
+      <c r="C8" s="307"/>
+      <c r="D8" s="307"/>
+      <c r="E8" s="307"/>
+      <c r="F8" s="307"/>
+      <c r="G8" s="307"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -38450,11 +38450,11 @@
         <v>202</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="307"/>
-      <c r="D9" s="307"/>
-      <c r="E9" s="307"/>
-      <c r="F9" s="307"/>
-      <c r="G9" s="307"/>
+      <c r="C9" s="313"/>
+      <c r="D9" s="313"/>
+      <c r="E9" s="313"/>
+      <c r="F9" s="313"/>
+      <c r="G9" s="313"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -38462,11 +38462,11 @@
         <v>80</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="328"/>
-      <c r="D10" s="328"/>
-      <c r="E10" s="328"/>
-      <c r="F10" s="328"/>
-      <c r="G10" s="328"/>
+      <c r="C10" s="335"/>
+      <c r="D10" s="335"/>
+      <c r="E10" s="335"/>
+      <c r="F10" s="335"/>
+      <c r="G10" s="335"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -38479,37 +38479,37 @@
       <c r="A12" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="308" t="s">
+      <c r="B12" s="314" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="309"/>
-      <c r="D12" s="310"/>
+      <c r="C12" s="315"/>
+      <c r="D12" s="316"/>
       <c r="N12" s="141" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="311" t="s">
+      <c r="B13" s="317" t="s">
         <v>153</v>
       </c>
-      <c r="C13" s="312"/>
-      <c r="D13" s="313"/>
+      <c r="C13" s="318"/>
+      <c r="D13" s="319"/>
       <c r="N13" s="142"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="295" t="s">
+      <c r="B14" s="301" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="296"/>
-      <c r="D14" s="297"/>
+      <c r="C14" s="302"/>
+      <c r="D14" s="303"/>
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="298" t="s">
+      <c r="B15" s="304" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="299"/>
-      <c r="D15" s="300"/>
+      <c r="C15" s="305"/>
+      <c r="D15" s="306"/>
       <c r="N15" s="142"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -39729,12 +39729,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -39742,6 +39736,12 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>
@@ -39799,26 +39799,26 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="330" t="s">
+      <c r="D3" s="336" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="330"/>
-      <c r="F3" s="330" t="s">
+      <c r="E3" s="336"/>
+      <c r="F3" s="336" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="330"/>
-      <c r="H3" s="330"/>
-      <c r="I3" s="330" t="s">
+      <c r="G3" s="336"/>
+      <c r="H3" s="336"/>
+      <c r="I3" s="336" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="330"/>
-      <c r="K3" s="330"/>
+      <c r="J3" s="336"/>
+      <c r="K3" s="336"/>
       <c r="L3" s="134"/>
-      <c r="M3" s="330" t="s">
+      <c r="M3" s="336" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="330"/>
-      <c r="O3" s="330"/>
+      <c r="N3" s="336"/>
+      <c r="O3" s="336"/>
     </row>
     <row r="4" spans="1:16" s="47" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="46" t="s">

</xml_diff>

<commit_message>
Update hotlinks in dashboard to User Guide in LakeMeadDiviveInflow folder
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D739891B-C360-476F-94FD-0EC5C93B80C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF70758-8E02-4BF3-B1EF-03B296A6A459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -3394,63 +3394,10 @@
     <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3505,6 +3452,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3536,6 +3489,63 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3640,11 +3650,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3667,16 +3677,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="20% - Accent1" xfId="12" builtinId="30"/>
@@ -15236,20 +15236,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="275" t="s">
+      <c r="A1" s="258" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="275"/>
-      <c r="C1" s="275"/>
-      <c r="D1" s="275"/>
-      <c r="E1" s="275"/>
-      <c r="F1" s="275"/>
-      <c r="G1" s="275"/>
-      <c r="H1" s="275"/>
-      <c r="I1" s="275"/>
-      <c r="J1" s="275"/>
-      <c r="K1" s="275"/>
-      <c r="L1" s="275"/>
+      <c r="B1" s="258"/>
+      <c r="C1" s="258"/>
+      <c r="D1" s="258"/>
+      <c r="E1" s="258"/>
+      <c r="F1" s="258"/>
+      <c r="G1" s="258"/>
+      <c r="H1" s="258"/>
+      <c r="I1" s="258"/>
+      <c r="J1" s="258"/>
+      <c r="K1" s="258"/>
+      <c r="L1" s="258"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -15275,41 +15275,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="276" t="s">
+      <c r="A4" s="259" t="s">
         <v>351</v>
       </c>
-      <c r="B4" s="277"/>
-      <c r="C4" s="277"/>
-      <c r="D4" s="277"/>
-      <c r="E4" s="277"/>
-      <c r="F4" s="277"/>
-      <c r="G4" s="277"/>
-      <c r="H4" s="277"/>
-      <c r="I4" s="277"/>
-      <c r="J4" s="277"/>
-      <c r="K4" s="277"/>
-      <c r="L4" s="278"/>
-      <c r="N4" s="279"/>
-      <c r="O4" s="279"/>
-      <c r="P4" s="279"/>
-      <c r="Q4" s="279"/>
-      <c r="R4" s="279"/>
+      <c r="B4" s="260"/>
+      <c r="C4" s="260"/>
+      <c r="D4" s="260"/>
+      <c r="E4" s="260"/>
+      <c r="F4" s="260"/>
+      <c r="G4" s="260"/>
+      <c r="H4" s="260"/>
+      <c r="I4" s="260"/>
+      <c r="J4" s="260"/>
+      <c r="K4" s="260"/>
+      <c r="L4" s="261"/>
+      <c r="N4" s="262"/>
+      <c r="O4" s="262"/>
+      <c r="P4" s="262"/>
+      <c r="Q4" s="262"/>
+      <c r="R4" s="262"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="280" t="s">
+      <c r="A5" s="263" t="s">
         <v>334</v>
       </c>
-      <c r="B5" s="281"/>
-      <c r="C5" s="281"/>
-      <c r="D5" s="281"/>
-      <c r="E5" s="281"/>
-      <c r="F5" s="281"/>
-      <c r="G5" s="281"/>
-      <c r="H5" s="281"/>
-      <c r="I5" s="281"/>
-      <c r="J5" s="281"/>
-      <c r="K5" s="281"/>
-      <c r="L5" s="282"/>
+      <c r="B5" s="264"/>
+      <c r="C5" s="264"/>
+      <c r="D5" s="264"/>
+      <c r="E5" s="264"/>
+      <c r="F5" s="264"/>
+      <c r="G5" s="264"/>
+      <c r="H5" s="264"/>
+      <c r="I5" s="264"/>
+      <c r="J5" s="264"/>
+      <c r="K5" s="264"/>
+      <c r="L5" s="265"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15317,20 +15317,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="280" t="s">
+      <c r="A6" s="263" t="s">
         <v>352</v>
       </c>
-      <c r="B6" s="281"/>
-      <c r="C6" s="281"/>
-      <c r="D6" s="281"/>
-      <c r="E6" s="281"/>
-      <c r="F6" s="281"/>
-      <c r="G6" s="281"/>
-      <c r="H6" s="281"/>
-      <c r="I6" s="281"/>
-      <c r="J6" s="281"/>
-      <c r="K6" s="281"/>
-      <c r="L6" s="282"/>
+      <c r="B6" s="264"/>
+      <c r="C6" s="264"/>
+      <c r="D6" s="264"/>
+      <c r="E6" s="264"/>
+      <c r="F6" s="264"/>
+      <c r="G6" s="264"/>
+      <c r="H6" s="264"/>
+      <c r="I6" s="264"/>
+      <c r="J6" s="264"/>
+      <c r="K6" s="264"/>
+      <c r="L6" s="265"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15339,19 +15339,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="232"/>
-      <c r="B7" s="281" t="s">
+      <c r="B7" s="264" t="s">
         <v>353</v>
       </c>
-      <c r="C7" s="281"/>
-      <c r="D7" s="281"/>
-      <c r="E7" s="281"/>
-      <c r="F7" s="281"/>
-      <c r="G7" s="281"/>
-      <c r="H7" s="281"/>
-      <c r="I7" s="281"/>
-      <c r="J7" s="281"/>
-      <c r="K7" s="281"/>
-      <c r="L7" s="282"/>
+      <c r="C7" s="264"/>
+      <c r="D7" s="264"/>
+      <c r="E7" s="264"/>
+      <c r="F7" s="264"/>
+      <c r="G7" s="264"/>
+      <c r="H7" s="264"/>
+      <c r="I7" s="264"/>
+      <c r="J7" s="264"/>
+      <c r="K7" s="264"/>
+      <c r="L7" s="265"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15360,19 +15360,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="233"/>
-      <c r="B8" s="296" t="s">
+      <c r="B8" s="281" t="s">
         <v>354</v>
       </c>
-      <c r="C8" s="296"/>
-      <c r="D8" s="296"/>
-      <c r="E8" s="296"/>
-      <c r="F8" s="296"/>
-      <c r="G8" s="296"/>
-      <c r="H8" s="296"/>
-      <c r="I8" s="296"/>
-      <c r="J8" s="296"/>
-      <c r="K8" s="296"/>
-      <c r="L8" s="297"/>
+      <c r="C8" s="281"/>
+      <c r="D8" s="281"/>
+      <c r="E8" s="281"/>
+      <c r="F8" s="281"/>
+      <c r="G8" s="281"/>
+      <c r="H8" s="281"/>
+      <c r="I8" s="281"/>
+      <c r="J8" s="281"/>
+      <c r="K8" s="281"/>
+      <c r="L8" s="282"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15394,38 +15394,38 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="298" t="s">
+      <c r="A10" s="283" t="s">
         <v>389</v>
       </c>
-      <c r="B10" s="299"/>
-      <c r="C10" s="299"/>
-      <c r="D10" s="299"/>
-      <c r="E10" s="299"/>
-      <c r="F10" s="299"/>
-      <c r="G10" s="299"/>
-      <c r="H10" s="299"/>
-      <c r="I10" s="299"/>
-      <c r="J10" s="299"/>
-      <c r="K10" s="299"/>
-      <c r="L10" s="300"/>
+      <c r="B10" s="284"/>
+      <c r="C10" s="284"/>
+      <c r="D10" s="284"/>
+      <c r="E10" s="284"/>
+      <c r="F10" s="284"/>
+      <c r="G10" s="284"/>
+      <c r="H10" s="284"/>
+      <c r="I10" s="284"/>
+      <c r="J10" s="284"/>
+      <c r="K10" s="284"/>
+      <c r="L10" s="285"/>
     </row>
     <row r="11" spans="1:18" s="58" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="344" t="s">
+      <c r="A11" s="253" t="s">
         <v>390</v>
       </c>
-      <c r="B11" s="345" t="s">
+      <c r="B11" s="286" t="s">
         <v>393</v>
       </c>
-      <c r="C11" s="345"/>
-      <c r="D11" s="345"/>
-      <c r="E11" s="345"/>
-      <c r="F11" s="345"/>
-      <c r="G11" s="345"/>
-      <c r="H11" s="345"/>
-      <c r="I11" s="345"/>
-      <c r="J11" s="345"/>
-      <c r="K11" s="345"/>
-      <c r="L11" s="346"/>
+      <c r="C11" s="286"/>
+      <c r="D11" s="286"/>
+      <c r="E11" s="286"/>
+      <c r="F11" s="286"/>
+      <c r="G11" s="286"/>
+      <c r="H11" s="286"/>
+      <c r="I11" s="286"/>
+      <c r="J11" s="286"/>
+      <c r="K11" s="286"/>
+      <c r="L11" s="287"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="161.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="245"/>
@@ -15442,54 +15442,54 @@
       <c r="L12" s="252"/>
     </row>
     <row r="13" spans="1:18" s="58" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="344" t="s">
+      <c r="A13" s="253" t="s">
         <v>391</v>
       </c>
-      <c r="B13" s="345" t="s">
+      <c r="B13" s="286" t="s">
         <v>394</v>
       </c>
-      <c r="C13" s="345"/>
-      <c r="D13" s="345"/>
-      <c r="E13" s="345"/>
-      <c r="F13" s="345"/>
-      <c r="G13" s="345"/>
-      <c r="H13" s="345"/>
-      <c r="I13" s="345"/>
-      <c r="J13" s="345"/>
-      <c r="K13" s="345"/>
-      <c r="L13" s="346"/>
+      <c r="C13" s="286"/>
+      <c r="D13" s="286"/>
+      <c r="E13" s="286"/>
+      <c r="F13" s="286"/>
+      <c r="G13" s="286"/>
+      <c r="H13" s="286"/>
+      <c r="I13" s="286"/>
+      <c r="J13" s="286"/>
+      <c r="K13" s="286"/>
+      <c r="L13" s="287"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="90.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="245"/>
-      <c r="B14" s="253"/>
-      <c r="C14" s="253"/>
-      <c r="D14" s="253"/>
-      <c r="E14" s="253"/>
-      <c r="F14" s="253"/>
-      <c r="G14" s="253"/>
-      <c r="H14" s="253"/>
-      <c r="I14" s="253"/>
-      <c r="J14" s="253"/>
-      <c r="K14" s="253"/>
-      <c r="L14" s="254"/>
+      <c r="B14" s="295"/>
+      <c r="C14" s="295"/>
+      <c r="D14" s="295"/>
+      <c r="E14" s="295"/>
+      <c r="F14" s="295"/>
+      <c r="G14" s="295"/>
+      <c r="H14" s="295"/>
+      <c r="I14" s="295"/>
+      <c r="J14" s="295"/>
+      <c r="K14" s="295"/>
+      <c r="L14" s="296"/>
     </row>
     <row r="15" spans="1:18" s="58" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="344" t="s">
+      <c r="A15" s="253" t="s">
         <v>392</v>
       </c>
-      <c r="B15" s="345" t="s">
+      <c r="B15" s="286" t="s">
         <v>395</v>
       </c>
-      <c r="C15" s="345"/>
-      <c r="D15" s="345"/>
-      <c r="E15" s="345"/>
-      <c r="F15" s="345"/>
-      <c r="G15" s="345"/>
-      <c r="H15" s="345"/>
-      <c r="I15" s="345"/>
-      <c r="J15" s="345"/>
-      <c r="K15" s="345"/>
-      <c r="L15" s="346"/>
+      <c r="C15" s="286"/>
+      <c r="D15" s="286"/>
+      <c r="E15" s="286"/>
+      <c r="F15" s="286"/>
+      <c r="G15" s="286"/>
+      <c r="H15" s="286"/>
+      <c r="I15" s="286"/>
+      <c r="J15" s="286"/>
+      <c r="K15" s="286"/>
+      <c r="L15" s="287"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="245"/>
@@ -15506,12 +15506,12 @@
       <c r="L16" s="252"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="270" t="s">
+      <c r="A17" s="303" t="s">
         <v>400</v>
       </c>
-      <c r="B17" s="271"/>
-      <c r="C17" s="271"/>
-      <c r="D17" s="271"/>
+      <c r="B17" s="304"/>
+      <c r="C17" s="304"/>
+      <c r="D17" s="304"/>
       <c r="E17" s="250" t="s">
         <v>401</v>
       </c>
@@ -15538,84 +15538,84 @@
       <c r="L18" s="113"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="283" t="s">
+      <c r="A19" s="266" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="284"/>
-      <c r="C19" s="284"/>
-      <c r="D19" s="284"/>
-      <c r="E19" s="284"/>
-      <c r="F19" s="284"/>
-      <c r="G19" s="284"/>
-      <c r="H19" s="284"/>
-      <c r="I19" s="284"/>
-      <c r="J19" s="284"/>
-      <c r="K19" s="284"/>
-      <c r="L19" s="285"/>
+      <c r="B19" s="267"/>
+      <c r="C19" s="267"/>
+      <c r="D19" s="267"/>
+      <c r="E19" s="267"/>
+      <c r="F19" s="267"/>
+      <c r="G19" s="267"/>
+      <c r="H19" s="267"/>
+      <c r="I19" s="267"/>
+      <c r="J19" s="267"/>
+      <c r="K19" s="267"/>
+      <c r="L19" s="268"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="286" t="s">
+      <c r="A20" s="269" t="s">
         <v>335</v>
       </c>
-      <c r="B20" s="287"/>
-      <c r="C20" s="287"/>
-      <c r="D20" s="287"/>
-      <c r="E20" s="287"/>
-      <c r="F20" s="287"/>
-      <c r="G20" s="287"/>
-      <c r="H20" s="287"/>
-      <c r="I20" s="287"/>
-      <c r="J20" s="287"/>
-      <c r="K20" s="287"/>
-      <c r="L20" s="288"/>
+      <c r="B20" s="270"/>
+      <c r="C20" s="270"/>
+      <c r="D20" s="270"/>
+      <c r="E20" s="270"/>
+      <c r="F20" s="270"/>
+      <c r="G20" s="270"/>
+      <c r="H20" s="270"/>
+      <c r="I20" s="270"/>
+      <c r="J20" s="270"/>
+      <c r="K20" s="270"/>
+      <c r="L20" s="271"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="289" t="s">
+      <c r="A21" s="272" t="s">
         <v>336</v>
       </c>
-      <c r="B21" s="265"/>
-      <c r="C21" s="265"/>
-      <c r="D21" s="265"/>
-      <c r="E21" s="265"/>
-      <c r="F21" s="265"/>
-      <c r="G21" s="265"/>
-      <c r="H21" s="265"/>
-      <c r="I21" s="265"/>
-      <c r="J21" s="265"/>
-      <c r="K21" s="265"/>
-      <c r="L21" s="266"/>
+      <c r="B21" s="273"/>
+      <c r="C21" s="273"/>
+      <c r="D21" s="273"/>
+      <c r="E21" s="273"/>
+      <c r="F21" s="273"/>
+      <c r="G21" s="273"/>
+      <c r="H21" s="273"/>
+      <c r="I21" s="273"/>
+      <c r="J21" s="273"/>
+      <c r="K21" s="273"/>
+      <c r="L21" s="274"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="289" t="s">
+      <c r="A22" s="272" t="s">
         <v>206</v>
       </c>
-      <c r="B22" s="265"/>
-      <c r="C22" s="265"/>
-      <c r="D22" s="265"/>
-      <c r="E22" s="265"/>
-      <c r="F22" s="265"/>
-      <c r="G22" s="265"/>
-      <c r="H22" s="265"/>
-      <c r="I22" s="265"/>
-      <c r="J22" s="265"/>
-      <c r="K22" s="265"/>
-      <c r="L22" s="266"/>
+      <c r="B22" s="273"/>
+      <c r="C22" s="273"/>
+      <c r="D22" s="273"/>
+      <c r="E22" s="273"/>
+      <c r="F22" s="273"/>
+      <c r="G22" s="273"/>
+      <c r="H22" s="273"/>
+      <c r="I22" s="273"/>
+      <c r="J22" s="273"/>
+      <c r="K22" s="273"/>
+      <c r="L22" s="274"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="290" t="s">
+      <c r="A23" s="275" t="s">
         <v>337</v>
       </c>
-      <c r="B23" s="291"/>
-      <c r="C23" s="291"/>
-      <c r="D23" s="291"/>
-      <c r="E23" s="291"/>
-      <c r="F23" s="291"/>
-      <c r="G23" s="291"/>
-      <c r="H23" s="291"/>
-      <c r="I23" s="291"/>
-      <c r="J23" s="291"/>
-      <c r="K23" s="291"/>
-      <c r="L23" s="292"/>
+      <c r="B23" s="276"/>
+      <c r="C23" s="276"/>
+      <c r="D23" s="276"/>
+      <c r="E23" s="276"/>
+      <c r="F23" s="276"/>
+      <c r="G23" s="276"/>
+      <c r="H23" s="276"/>
+      <c r="I23" s="276"/>
+      <c r="J23" s="276"/>
+      <c r="K23" s="276"/>
+      <c r="L23" s="277"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="113"/>
@@ -15632,332 +15632,332 @@
       <c r="L24" s="113"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="293" t="s">
+      <c r="A25" s="278" t="s">
         <v>333</v>
       </c>
-      <c r="B25" s="294"/>
-      <c r="C25" s="294"/>
-      <c r="D25" s="294"/>
-      <c r="E25" s="294"/>
-      <c r="F25" s="294"/>
-      <c r="G25" s="294"/>
-      <c r="H25" s="294"/>
-      <c r="I25" s="294"/>
-      <c r="J25" s="294"/>
-      <c r="K25" s="294"/>
-      <c r="L25" s="295"/>
+      <c r="B25" s="279"/>
+      <c r="C25" s="279"/>
+      <c r="D25" s="279"/>
+      <c r="E25" s="279"/>
+      <c r="F25" s="279"/>
+      <c r="G25" s="279"/>
+      <c r="H25" s="279"/>
+      <c r="I25" s="279"/>
+      <c r="J25" s="279"/>
+      <c r="K25" s="279"/>
+      <c r="L25" s="280"/>
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="272" t="s">
+      <c r="A26" s="255" t="s">
         <v>215</v>
       </c>
-      <c r="B26" s="273"/>
-      <c r="C26" s="273"/>
-      <c r="D26" s="273"/>
-      <c r="E26" s="273"/>
-      <c r="F26" s="273"/>
-      <c r="G26" s="273"/>
-      <c r="H26" s="273"/>
-      <c r="I26" s="273"/>
-      <c r="J26" s="273"/>
-      <c r="K26" s="273"/>
-      <c r="L26" s="274"/>
+      <c r="B26" s="256"/>
+      <c r="C26" s="256"/>
+      <c r="D26" s="256"/>
+      <c r="E26" s="256"/>
+      <c r="F26" s="256"/>
+      <c r="G26" s="256"/>
+      <c r="H26" s="256"/>
+      <c r="I26" s="256"/>
+      <c r="J26" s="256"/>
+      <c r="K26" s="256"/>
+      <c r="L26" s="257"/>
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="227">
         <v>1</v>
       </c>
-      <c r="B27" s="258" t="s">
+      <c r="B27" s="290" t="s">
         <v>214</v>
       </c>
-      <c r="C27" s="258"/>
-      <c r="D27" s="258"/>
-      <c r="E27" s="258"/>
-      <c r="F27" s="258"/>
-      <c r="G27" s="258"/>
-      <c r="H27" s="258"/>
-      <c r="I27" s="258"/>
-      <c r="J27" s="258"/>
-      <c r="K27" s="258"/>
-      <c r="L27" s="259"/>
+      <c r="C27" s="290"/>
+      <c r="D27" s="290"/>
+      <c r="E27" s="290"/>
+      <c r="F27" s="290"/>
+      <c r="G27" s="290"/>
+      <c r="H27" s="290"/>
+      <c r="I27" s="290"/>
+      <c r="J27" s="290"/>
+      <c r="K27" s="290"/>
+      <c r="L27" s="291"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="227">
         <v>2</v>
       </c>
-      <c r="B28" s="258" t="s">
+      <c r="B28" s="290" t="s">
         <v>329</v>
       </c>
-      <c r="C28" s="258"/>
-      <c r="D28" s="258"/>
-      <c r="E28" s="258"/>
-      <c r="F28" s="258"/>
-      <c r="G28" s="258"/>
-      <c r="H28" s="258"/>
-      <c r="I28" s="258"/>
-      <c r="J28" s="258"/>
-      <c r="K28" s="258"/>
-      <c r="L28" s="259"/>
+      <c r="C28" s="290"/>
+      <c r="D28" s="290"/>
+      <c r="E28" s="290"/>
+      <c r="F28" s="290"/>
+      <c r="G28" s="290"/>
+      <c r="H28" s="290"/>
+      <c r="I28" s="290"/>
+      <c r="J28" s="290"/>
+      <c r="K28" s="290"/>
+      <c r="L28" s="291"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="227">
         <v>3</v>
       </c>
-      <c r="B29" s="258" t="s">
+      <c r="B29" s="290" t="s">
         <v>207</v>
       </c>
-      <c r="C29" s="258"/>
-      <c r="D29" s="258"/>
-      <c r="E29" s="258"/>
-      <c r="F29" s="258"/>
-      <c r="G29" s="258"/>
-      <c r="H29" s="258"/>
-      <c r="I29" s="258"/>
-      <c r="J29" s="258"/>
-      <c r="K29" s="258"/>
-      <c r="L29" s="259"/>
+      <c r="C29" s="290"/>
+      <c r="D29" s="290"/>
+      <c r="E29" s="290"/>
+      <c r="F29" s="290"/>
+      <c r="G29" s="290"/>
+      <c r="H29" s="290"/>
+      <c r="I29" s="290"/>
+      <c r="J29" s="290"/>
+      <c r="K29" s="290"/>
+      <c r="L29" s="291"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="227">
         <v>4</v>
       </c>
-      <c r="B30" s="258" t="s">
+      <c r="B30" s="290" t="s">
         <v>338</v>
       </c>
-      <c r="C30" s="258"/>
-      <c r="D30" s="258"/>
-      <c r="E30" s="258"/>
-      <c r="F30" s="258"/>
-      <c r="G30" s="258"/>
-      <c r="H30" s="258"/>
-      <c r="I30" s="258"/>
-      <c r="J30" s="258"/>
-      <c r="K30" s="258"/>
-      <c r="L30" s="259"/>
+      <c r="C30" s="290"/>
+      <c r="D30" s="290"/>
+      <c r="E30" s="290"/>
+      <c r="F30" s="290"/>
+      <c r="G30" s="290"/>
+      <c r="H30" s="290"/>
+      <c r="I30" s="290"/>
+      <c r="J30" s="290"/>
+      <c r="K30" s="290"/>
+      <c r="L30" s="291"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="227">
         <v>5</v>
       </c>
-      <c r="B31" s="258" t="s">
+      <c r="B31" s="290" t="s">
         <v>208</v>
       </c>
-      <c r="C31" s="258"/>
-      <c r="D31" s="258"/>
-      <c r="E31" s="258"/>
-      <c r="F31" s="258"/>
-      <c r="G31" s="258"/>
-      <c r="H31" s="258"/>
-      <c r="I31" s="258"/>
-      <c r="J31" s="258"/>
-      <c r="K31" s="258"/>
-      <c r="L31" s="259"/>
+      <c r="C31" s="290"/>
+      <c r="D31" s="290"/>
+      <c r="E31" s="290"/>
+      <c r="F31" s="290"/>
+      <c r="G31" s="290"/>
+      <c r="H31" s="290"/>
+      <c r="I31" s="290"/>
+      <c r="J31" s="290"/>
+      <c r="K31" s="290"/>
+      <c r="L31" s="291"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="227"/>
-      <c r="B32" s="258" t="s">
+      <c r="B32" s="290" t="s">
         <v>209</v>
       </c>
-      <c r="C32" s="258"/>
-      <c r="D32" s="258"/>
-      <c r="E32" s="258"/>
-      <c r="F32" s="258"/>
-      <c r="G32" s="258"/>
-      <c r="H32" s="258"/>
-      <c r="I32" s="258"/>
-      <c r="J32" s="258"/>
-      <c r="K32" s="258"/>
-      <c r="L32" s="259"/>
+      <c r="C32" s="290"/>
+      <c r="D32" s="290"/>
+      <c r="E32" s="290"/>
+      <c r="F32" s="290"/>
+      <c r="G32" s="290"/>
+      <c r="H32" s="290"/>
+      <c r="I32" s="290"/>
+      <c r="J32" s="290"/>
+      <c r="K32" s="290"/>
+      <c r="L32" s="291"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="227"/>
-      <c r="B33" s="258" t="s">
+      <c r="B33" s="290" t="s">
         <v>210</v>
       </c>
-      <c r="C33" s="258"/>
-      <c r="D33" s="258"/>
-      <c r="E33" s="258"/>
-      <c r="F33" s="258"/>
-      <c r="G33" s="258"/>
-      <c r="H33" s="258"/>
-      <c r="I33" s="258"/>
-      <c r="J33" s="258"/>
-      <c r="K33" s="258"/>
-      <c r="L33" s="259"/>
+      <c r="C33" s="290"/>
+      <c r="D33" s="290"/>
+      <c r="E33" s="290"/>
+      <c r="F33" s="290"/>
+      <c r="G33" s="290"/>
+      <c r="H33" s="290"/>
+      <c r="I33" s="290"/>
+      <c r="J33" s="290"/>
+      <c r="K33" s="290"/>
+      <c r="L33" s="291"/>
       <c r="N33" s="106"/>
     </row>
     <row r="34" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="267" t="s">
+      <c r="A34" s="292" t="s">
         <v>216</v>
       </c>
-      <c r="B34" s="268"/>
-      <c r="C34" s="268"/>
-      <c r="D34" s="268"/>
-      <c r="E34" s="268"/>
-      <c r="F34" s="268"/>
-      <c r="G34" s="268"/>
-      <c r="H34" s="268"/>
-      <c r="I34" s="268"/>
-      <c r="J34" s="268"/>
-      <c r="K34" s="268"/>
-      <c r="L34" s="269"/>
+      <c r="B34" s="293"/>
+      <c r="C34" s="293"/>
+      <c r="D34" s="293"/>
+      <c r="E34" s="293"/>
+      <c r="F34" s="293"/>
+      <c r="G34" s="293"/>
+      <c r="H34" s="293"/>
+      <c r="I34" s="293"/>
+      <c r="J34" s="293"/>
+      <c r="K34" s="293"/>
+      <c r="L34" s="294"/>
       <c r="N34" s="106"/>
     </row>
     <row r="35" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="227">
         <v>1</v>
       </c>
-      <c r="B35" s="258" t="s">
+      <c r="B35" s="290" t="s">
         <v>211</v>
       </c>
-      <c r="C35" s="258"/>
-      <c r="D35" s="258"/>
-      <c r="E35" s="258"/>
-      <c r="F35" s="258"/>
-      <c r="G35" s="258"/>
-      <c r="H35" s="258"/>
-      <c r="I35" s="258"/>
-      <c r="J35" s="258"/>
-      <c r="K35" s="258"/>
-      <c r="L35" s="259"/>
+      <c r="C35" s="290"/>
+      <c r="D35" s="290"/>
+      <c r="E35" s="290"/>
+      <c r="F35" s="290"/>
+      <c r="G35" s="290"/>
+      <c r="H35" s="290"/>
+      <c r="I35" s="290"/>
+      <c r="J35" s="290"/>
+      <c r="K35" s="290"/>
+      <c r="L35" s="291"/>
       <c r="N35" s="106"/>
     </row>
     <row r="36" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="227"/>
-      <c r="B36" s="256" t="s">
+      <c r="B36" s="288" t="s">
         <v>339</v>
       </c>
-      <c r="C36" s="256"/>
-      <c r="D36" s="256"/>
-      <c r="E36" s="256"/>
-      <c r="F36" s="256"/>
-      <c r="G36" s="256"/>
-      <c r="H36" s="256"/>
-      <c r="I36" s="256"/>
-      <c r="J36" s="256"/>
-      <c r="K36" s="256"/>
-      <c r="L36" s="257"/>
+      <c r="C36" s="288"/>
+      <c r="D36" s="288"/>
+      <c r="E36" s="288"/>
+      <c r="F36" s="288"/>
+      <c r="G36" s="288"/>
+      <c r="H36" s="288"/>
+      <c r="I36" s="288"/>
+      <c r="J36" s="288"/>
+      <c r="K36" s="288"/>
+      <c r="L36" s="289"/>
       <c r="N36" s="106"/>
     </row>
     <row r="37" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="227">
         <v>2</v>
       </c>
-      <c r="B37" s="258" t="s">
+      <c r="B37" s="290" t="s">
         <v>332</v>
       </c>
-      <c r="C37" s="258"/>
-      <c r="D37" s="258"/>
-      <c r="E37" s="258"/>
-      <c r="F37" s="258"/>
-      <c r="G37" s="258"/>
-      <c r="H37" s="258"/>
-      <c r="I37" s="258"/>
-      <c r="J37" s="258"/>
-      <c r="K37" s="258"/>
-      <c r="L37" s="259"/>
+      <c r="C37" s="290"/>
+      <c r="D37" s="290"/>
+      <c r="E37" s="290"/>
+      <c r="F37" s="290"/>
+      <c r="G37" s="290"/>
+      <c r="H37" s="290"/>
+      <c r="I37" s="290"/>
+      <c r="J37" s="290"/>
+      <c r="K37" s="290"/>
+      <c r="L37" s="291"/>
       <c r="N37" s="106"/>
     </row>
     <row r="38" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="227">
         <v>3</v>
       </c>
-      <c r="B38" s="258" t="s">
+      <c r="B38" s="290" t="s">
         <v>321</v>
       </c>
-      <c r="C38" s="258"/>
-      <c r="D38" s="258"/>
-      <c r="E38" s="258"/>
-      <c r="F38" s="258"/>
-      <c r="G38" s="258"/>
-      <c r="H38" s="258"/>
-      <c r="I38" s="258"/>
-      <c r="J38" s="258"/>
-      <c r="K38" s="258"/>
-      <c r="L38" s="259"/>
+      <c r="C38" s="290"/>
+      <c r="D38" s="290"/>
+      <c r="E38" s="290"/>
+      <c r="F38" s="290"/>
+      <c r="G38" s="290"/>
+      <c r="H38" s="290"/>
+      <c r="I38" s="290"/>
+      <c r="J38" s="290"/>
+      <c r="K38" s="290"/>
+      <c r="L38" s="291"/>
       <c r="N38" s="106"/>
     </row>
     <row r="39" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="227">
         <v>4</v>
       </c>
-      <c r="B39" s="258" t="s">
+      <c r="B39" s="290" t="s">
         <v>340</v>
       </c>
-      <c r="C39" s="258"/>
-      <c r="D39" s="258"/>
-      <c r="E39" s="258"/>
-      <c r="F39" s="258"/>
-      <c r="G39" s="258"/>
-      <c r="H39" s="258"/>
-      <c r="I39" s="258"/>
-      <c r="J39" s="258"/>
-      <c r="K39" s="258"/>
-      <c r="L39" s="259"/>
+      <c r="C39" s="290"/>
+      <c r="D39" s="290"/>
+      <c r="E39" s="290"/>
+      <c r="F39" s="290"/>
+      <c r="G39" s="290"/>
+      <c r="H39" s="290"/>
+      <c r="I39" s="290"/>
+      <c r="J39" s="290"/>
+      <c r="K39" s="290"/>
+      <c r="L39" s="291"/>
       <c r="N39" s="106"/>
     </row>
     <row r="40" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="227">
         <v>5</v>
       </c>
-      <c r="B40" s="256" t="s">
+      <c r="B40" s="288" t="s">
         <v>322</v>
       </c>
-      <c r="C40" s="256"/>
-      <c r="D40" s="256"/>
-      <c r="E40" s="256"/>
-      <c r="F40" s="256"/>
-      <c r="G40" s="256"/>
-      <c r="H40" s="256"/>
-      <c r="I40" s="256"/>
-      <c r="J40" s="256"/>
-      <c r="K40" s="256"/>
-      <c r="L40" s="257"/>
+      <c r="C40" s="288"/>
+      <c r="D40" s="288"/>
+      <c r="E40" s="288"/>
+      <c r="F40" s="288"/>
+      <c r="G40" s="288"/>
+      <c r="H40" s="288"/>
+      <c r="I40" s="288"/>
+      <c r="J40" s="288"/>
+      <c r="K40" s="288"/>
+      <c r="L40" s="289"/>
       <c r="N40" s="106"/>
     </row>
     <row r="41" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="227">
         <v>6</v>
       </c>
-      <c r="B41" s="256" t="s">
+      <c r="B41" s="288" t="s">
         <v>327</v>
       </c>
-      <c r="C41" s="256"/>
-      <c r="D41" s="256"/>
-      <c r="E41" s="256"/>
-      <c r="F41" s="256"/>
-      <c r="G41" s="256"/>
-      <c r="H41" s="256"/>
-      <c r="I41" s="256"/>
-      <c r="J41" s="256"/>
-      <c r="K41" s="256"/>
-      <c r="L41" s="257"/>
+      <c r="C41" s="288"/>
+      <c r="D41" s="288"/>
+      <c r="E41" s="288"/>
+      <c r="F41" s="288"/>
+      <c r="G41" s="288"/>
+      <c r="H41" s="288"/>
+      <c r="I41" s="288"/>
+      <c r="J41" s="288"/>
+      <c r="K41" s="288"/>
+      <c r="L41" s="289"/>
       <c r="N41" s="106"/>
     </row>
     <row r="42" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="227">
         <v>7</v>
       </c>
-      <c r="B42" s="258" t="s">
+      <c r="B42" s="290" t="s">
         <v>323</v>
       </c>
-      <c r="C42" s="258"/>
-      <c r="D42" s="258"/>
-      <c r="E42" s="258"/>
-      <c r="F42" s="258"/>
-      <c r="G42" s="258"/>
-      <c r="H42" s="258"/>
-      <c r="I42" s="258"/>
-      <c r="J42" s="258"/>
-      <c r="K42" s="258"/>
-      <c r="L42" s="259"/>
+      <c r="C42" s="290"/>
+      <c r="D42" s="290"/>
+      <c r="E42" s="290"/>
+      <c r="F42" s="290"/>
+      <c r="G42" s="290"/>
+      <c r="H42" s="290"/>
+      <c r="I42" s="290"/>
+      <c r="J42" s="290"/>
+      <c r="K42" s="290"/>
+      <c r="L42" s="291"/>
     </row>
     <row r="43" spans="1:14" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="227"/>
@@ -15974,56 +15974,56 @@
       <c r="L43" s="229"/>
     </row>
     <row r="44" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="267" t="s">
+      <c r="A44" s="292" t="s">
         <v>326</v>
       </c>
-      <c r="B44" s="268"/>
-      <c r="C44" s="268"/>
-      <c r="D44" s="268"/>
-      <c r="E44" s="268"/>
-      <c r="F44" s="268"/>
-      <c r="G44" s="268"/>
-      <c r="H44" s="268"/>
-      <c r="I44" s="268"/>
-      <c r="J44" s="268"/>
-      <c r="K44" s="268"/>
-      <c r="L44" s="269"/>
+      <c r="B44" s="293"/>
+      <c r="C44" s="293"/>
+      <c r="D44" s="293"/>
+      <c r="E44" s="293"/>
+      <c r="F44" s="293"/>
+      <c r="G44" s="293"/>
+      <c r="H44" s="293"/>
+      <c r="I44" s="293"/>
+      <c r="J44" s="293"/>
+      <c r="K44" s="293"/>
+      <c r="L44" s="294"/>
     </row>
     <row r="45" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="230" t="s">
         <v>324</v>
       </c>
-      <c r="B45" s="258" t="s">
+      <c r="B45" s="290" t="s">
         <v>212</v>
       </c>
-      <c r="C45" s="258"/>
-      <c r="D45" s="258"/>
-      <c r="E45" s="258"/>
-      <c r="F45" s="258"/>
-      <c r="G45" s="258"/>
-      <c r="H45" s="258"/>
-      <c r="I45" s="258"/>
-      <c r="J45" s="258"/>
-      <c r="K45" s="258"/>
-      <c r="L45" s="259"/>
+      <c r="C45" s="290"/>
+      <c r="D45" s="290"/>
+      <c r="E45" s="290"/>
+      <c r="F45" s="290"/>
+      <c r="G45" s="290"/>
+      <c r="H45" s="290"/>
+      <c r="I45" s="290"/>
+      <c r="J45" s="290"/>
+      <c r="K45" s="290"/>
+      <c r="L45" s="291"/>
     </row>
     <row r="46" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="231" t="s">
         <v>325</v>
       </c>
-      <c r="B46" s="260" t="s">
+      <c r="B46" s="298" t="s">
         <v>328</v>
       </c>
-      <c r="C46" s="260"/>
-      <c r="D46" s="260"/>
-      <c r="E46" s="260"/>
-      <c r="F46" s="260"/>
-      <c r="G46" s="260"/>
-      <c r="H46" s="260"/>
-      <c r="I46" s="260"/>
-      <c r="J46" s="260"/>
-      <c r="K46" s="260"/>
-      <c r="L46" s="261"/>
+      <c r="C46" s="298"/>
+      <c r="D46" s="298"/>
+      <c r="E46" s="298"/>
+      <c r="F46" s="298"/>
+      <c r="G46" s="298"/>
+      <c r="H46" s="298"/>
+      <c r="I46" s="298"/>
+      <c r="J46" s="298"/>
+      <c r="K46" s="298"/>
+      <c r="L46" s="299"/>
     </row>
     <row r="47" spans="1:14" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="160"/>
@@ -16040,20 +16040,20 @@
       <c r="L47" s="113"/>
     </row>
     <row r="48" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="262" t="s">
+      <c r="A48" s="300" t="s">
         <v>240</v>
       </c>
-      <c r="B48" s="263"/>
-      <c r="C48" s="263"/>
-      <c r="D48" s="263"/>
-      <c r="E48" s="263"/>
-      <c r="F48" s="263"/>
-      <c r="G48" s="263"/>
-      <c r="H48" s="263"/>
-      <c r="I48" s="263"/>
-      <c r="J48" s="263"/>
-      <c r="K48" s="263"/>
-      <c r="L48" s="264"/>
+      <c r="B48" s="301"/>
+      <c r="C48" s="301"/>
+      <c r="D48" s="301"/>
+      <c r="E48" s="301"/>
+      <c r="F48" s="301"/>
+      <c r="G48" s="301"/>
+      <c r="H48" s="301"/>
+      <c r="I48" s="301"/>
+      <c r="J48" s="301"/>
+      <c r="K48" s="301"/>
+      <c r="L48" s="302"/>
     </row>
     <row r="49" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="234" t="s">
@@ -16141,90 +16141,90 @@
       <c r="B54" s="168" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="265" t="s">
+      <c r="C54" s="273" t="s">
         <v>312</v>
       </c>
-      <c r="D54" s="265"/>
-      <c r="E54" s="265"/>
-      <c r="F54" s="265"/>
-      <c r="G54" s="265"/>
-      <c r="H54" s="265"/>
-      <c r="I54" s="265"/>
-      <c r="J54" s="265"/>
-      <c r="K54" s="265"/>
-      <c r="L54" s="266"/>
+      <c r="D54" s="273"/>
+      <c r="E54" s="273"/>
+      <c r="F54" s="273"/>
+      <c r="G54" s="273"/>
+      <c r="H54" s="273"/>
+      <c r="I54" s="273"/>
+      <c r="J54" s="273"/>
+      <c r="K54" s="273"/>
+      <c r="L54" s="274"/>
     </row>
     <row r="55" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="167"/>
       <c r="B55" s="168" t="s">
         <v>313</v>
       </c>
-      <c r="C55" s="265" t="s">
+      <c r="C55" s="273" t="s">
         <v>314</v>
       </c>
-      <c r="D55" s="265"/>
-      <c r="E55" s="265"/>
-      <c r="F55" s="265"/>
-      <c r="G55" s="265"/>
-      <c r="H55" s="265"/>
-      <c r="I55" s="265"/>
-      <c r="J55" s="265"/>
-      <c r="K55" s="265"/>
-      <c r="L55" s="266"/>
+      <c r="D55" s="273"/>
+      <c r="E55" s="273"/>
+      <c r="F55" s="273"/>
+      <c r="G55" s="273"/>
+      <c r="H55" s="273"/>
+      <c r="I55" s="273"/>
+      <c r="J55" s="273"/>
+      <c r="K55" s="273"/>
+      <c r="L55" s="274"/>
     </row>
     <row r="56" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="167"/>
       <c r="B56" s="168" t="s">
         <v>382</v>
       </c>
-      <c r="C56" s="265" t="s">
+      <c r="C56" s="273" t="s">
         <v>383</v>
       </c>
-      <c r="D56" s="265"/>
-      <c r="E56" s="265"/>
-      <c r="F56" s="265"/>
-      <c r="G56" s="265"/>
-      <c r="H56" s="265"/>
-      <c r="I56" s="265"/>
-      <c r="J56" s="265"/>
-      <c r="K56" s="265"/>
-      <c r="L56" s="266"/>
+      <c r="D56" s="273"/>
+      <c r="E56" s="273"/>
+      <c r="F56" s="273"/>
+      <c r="G56" s="273"/>
+      <c r="H56" s="273"/>
+      <c r="I56" s="273"/>
+      <c r="J56" s="273"/>
+      <c r="K56" s="273"/>
+      <c r="L56" s="274"/>
     </row>
     <row r="57" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="167"/>
       <c r="B57" s="168" t="s">
         <v>138</v>
       </c>
-      <c r="C57" s="265" t="s">
+      <c r="C57" s="273" t="s">
         <v>139</v>
       </c>
-      <c r="D57" s="265"/>
-      <c r="E57" s="265"/>
-      <c r="F57" s="265"/>
-      <c r="G57" s="265"/>
-      <c r="H57" s="265"/>
-      <c r="I57" s="265"/>
-      <c r="J57" s="265"/>
-      <c r="K57" s="265"/>
-      <c r="L57" s="266"/>
+      <c r="D57" s="273"/>
+      <c r="E57" s="273"/>
+      <c r="F57" s="273"/>
+      <c r="G57" s="273"/>
+      <c r="H57" s="273"/>
+      <c r="I57" s="273"/>
+      <c r="J57" s="273"/>
+      <c r="K57" s="273"/>
+      <c r="L57" s="274"/>
     </row>
     <row r="58" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="167"/>
       <c r="B58" s="168" t="s">
         <v>238</v>
       </c>
-      <c r="C58" s="265" t="s">
+      <c r="C58" s="273" t="s">
         <v>239</v>
       </c>
-      <c r="D58" s="265"/>
-      <c r="E58" s="265"/>
-      <c r="F58" s="265"/>
-      <c r="G58" s="265"/>
-      <c r="H58" s="265"/>
-      <c r="I58" s="265"/>
-      <c r="J58" s="265"/>
-      <c r="K58" s="265"/>
-      <c r="L58" s="266"/>
+      <c r="D58" s="273"/>
+      <c r="E58" s="273"/>
+      <c r="F58" s="273"/>
+      <c r="G58" s="273"/>
+      <c r="H58" s="273"/>
+      <c r="I58" s="273"/>
+      <c r="J58" s="273"/>
+      <c r="K58" s="273"/>
+      <c r="L58" s="274"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="167"/>
@@ -16249,18 +16249,18 @@
       <c r="B60" s="168" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="265" t="s">
+      <c r="C60" s="273" t="s">
         <v>316</v>
       </c>
-      <c r="D60" s="265"/>
-      <c r="E60" s="265"/>
-      <c r="F60" s="265"/>
-      <c r="G60" s="265"/>
-      <c r="H60" s="265"/>
-      <c r="I60" s="265"/>
-      <c r="J60" s="265"/>
-      <c r="K60" s="265"/>
-      <c r="L60" s="266"/>
+      <c r="D60" s="273"/>
+      <c r="E60" s="273"/>
+      <c r="F60" s="273"/>
+      <c r="G60" s="273"/>
+      <c r="H60" s="273"/>
+      <c r="I60" s="273"/>
+      <c r="J60" s="273"/>
+      <c r="K60" s="273"/>
+      <c r="L60" s="274"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="167"/>
@@ -16360,25 +16360,56 @@
       </c>
     </row>
     <row r="78" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="255" t="s">
+      <c r="A78" s="297" t="s">
         <v>398</v>
       </c>
-      <c r="B78" s="255"/>
-      <c r="C78" s="255"/>
-      <c r="D78" s="255"/>
-      <c r="E78" s="255"/>
-      <c r="F78" s="255"/>
-      <c r="G78" s="255"/>
-      <c r="H78" s="255"/>
-      <c r="I78" s="255"/>
-      <c r="J78" s="255"/>
-      <c r="K78" s="255"/>
-      <c r="L78" s="255"/>
+      <c r="B78" s="297"/>
+      <c r="C78" s="297"/>
+      <c r="D78" s="297"/>
+      <c r="E78" s="297"/>
+      <c r="F78" s="297"/>
+      <c r="G78" s="297"/>
+      <c r="H78" s="297"/>
+      <c r="I78" s="297"/>
+      <c r="J78" s="297"/>
+      <c r="K78" s="297"/>
+      <c r="L78" s="297"/>
     </row>
     <row r="83" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="84" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="A78:L78"/>
+    <mergeCell ref="B41:L41"/>
+    <mergeCell ref="B42:L42"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="A48:L48"/>
+    <mergeCell ref="C54:L54"/>
+    <mergeCell ref="C57:L57"/>
+    <mergeCell ref="C58:L58"/>
+    <mergeCell ref="C55:L55"/>
+    <mergeCell ref="C60:L60"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="B40:L40"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B30:L30"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B39:L39"/>
     <mergeCell ref="A26:L26"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A4:L4"/>
@@ -16395,37 +16426,6 @@
     <mergeCell ref="B8:L8"/>
     <mergeCell ref="A10:L10"/>
     <mergeCell ref="B11:L11"/>
-    <mergeCell ref="B40:L40"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="B14:L14"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="A78:L78"/>
-    <mergeCell ref="B41:L41"/>
-    <mergeCell ref="B42:L42"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="A48:L48"/>
-    <mergeCell ref="C54:L54"/>
-    <mergeCell ref="C57:L57"/>
-    <mergeCell ref="C58:L58"/>
-    <mergeCell ref="C55:L55"/>
-    <mergeCell ref="C60:L60"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="C56:L56"/>
-    <mergeCell ref="A17:D17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A67" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -31396,82 +31396,82 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="338" t="s">
+      <c r="A3" s="342" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="338"/>
-      <c r="C3" s="338"/>
+      <c r="B3" s="342"/>
+      <c r="C3" s="342"/>
       <c r="D3" s="128" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="339" t="s">
+      <c r="A4" s="343" t="s">
         <v>152</v>
       </c>
-      <c r="B4" s="339"/>
-      <c r="C4" s="339"/>
+      <c r="B4" s="343"/>
+      <c r="C4" s="343"/>
       <c r="D4" s="175" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="343" t="s">
+      <c r="A5" s="347" t="s">
         <v>223</v>
       </c>
-      <c r="B5" s="340"/>
-      <c r="C5" s="340"/>
+      <c r="B5" s="344"/>
+      <c r="C5" s="344"/>
       <c r="D5" s="176" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="341" t="s">
+      <c r="A6" s="345" t="s">
         <v>224</v>
       </c>
-      <c r="B6" s="341"/>
-      <c r="C6" s="341"/>
+      <c r="B6" s="345"/>
+      <c r="C6" s="345"/>
       <c r="D6" s="177" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="342" t="s">
+      <c r="A7" s="346" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="342"/>
-      <c r="C7" s="342"/>
+      <c r="B7" s="346"/>
+      <c r="C7" s="346"/>
       <c r="D7" s="178" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="339" t="s">
+      <c r="A11" s="343" t="s">
         <v>152</v>
       </c>
-      <c r="B11" s="339"/>
-      <c r="C11" s="339"/>
+      <c r="B11" s="343"/>
+      <c r="C11" s="343"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="340" t="s">
+      <c r="A12" s="344" t="s">
         <v>153</v>
       </c>
-      <c r="B12" s="340"/>
-      <c r="C12" s="340"/>
+      <c r="B12" s="344"/>
+      <c r="C12" s="344"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="341" t="s">
+      <c r="A13" s="345" t="s">
         <v>154</v>
       </c>
-      <c r="B13" s="341"/>
-      <c r="C13" s="341"/>
+      <c r="B13" s="345"/>
+      <c r="C13" s="345"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="342" t="s">
+      <c r="A14" s="346" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="342"/>
-      <c r="C14" s="342"/>
+      <c r="B14" s="346"/>
+      <c r="C14" s="346"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -32053,7 +32053,7 @@
   <dimension ref="A1:P139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="N109" sqref="N109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32082,16 +32082,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.5">
-      <c r="A1" s="301" t="str">
+      <c r="A1" s="305" t="str">
         <f>'ReadMe-Directions'!A1</f>
         <v>Immersive Model for Lake Mead based on the Principle of Divide Reservoir Inflow</v>
       </c>
-      <c r="B1" s="301"/>
-      <c r="C1" s="301"/>
-      <c r="D1" s="301"/>
-      <c r="E1" s="301"/>
-      <c r="F1" s="301"/>
-      <c r="G1" s="301"/>
+      <c r="B1" s="305"/>
+      <c r="C1" s="305"/>
+      <c r="D1" s="305"/>
+      <c r="E1" s="305"/>
+      <c r="F1" s="305"/>
+      <c r="G1" s="305"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -32100,15 +32100,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="309" t="s">
+      <c r="A3" s="313" t="s">
         <v>230</v>
       </c>
-      <c r="B3" s="309"/>
-      <c r="C3" s="309"/>
-      <c r="D3" s="309"/>
-      <c r="E3" s="309"/>
-      <c r="F3" s="309"/>
-      <c r="G3" s="309"/>
+      <c r="B3" s="313"/>
+      <c r="C3" s="313"/>
+      <c r="D3" s="313"/>
+      <c r="E3" s="313"/>
+      <c r="F3" s="313"/>
+      <c r="G3" s="313"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -32124,13 +32124,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="310" t="s">
+      <c r="C4" s="314" t="s">
         <v>309</v>
       </c>
-      <c r="D4" s="311"/>
-      <c r="E4" s="311"/>
-      <c r="F4" s="311"/>
-      <c r="G4" s="312"/>
+      <c r="D4" s="315"/>
+      <c r="E4" s="315"/>
+      <c r="F4" s="315"/>
+      <c r="G4" s="316"/>
       <c r="N4" s="141" t="s">
         <v>384</v>
       </c>
@@ -32140,11 +32140,11 @@
         <v>283</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="313"/>
-      <c r="D5" s="308"/>
-      <c r="E5" s="308"/>
-      <c r="F5" s="308"/>
-      <c r="G5" s="308"/>
+      <c r="C5" s="317"/>
+      <c r="D5" s="312"/>
+      <c r="E5" s="312"/>
+      <c r="F5" s="312"/>
+      <c r="G5" s="312"/>
       <c r="N5" s="141"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -32152,11 +32152,11 @@
         <v>242</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="313"/>
-      <c r="D6" s="308"/>
-      <c r="E6" s="308"/>
-      <c r="F6" s="308"/>
-      <c r="G6" s="308"/>
+      <c r="C6" s="317"/>
+      <c r="D6" s="312"/>
+      <c r="E6" s="312"/>
+      <c r="F6" s="312"/>
+      <c r="G6" s="312"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -32164,11 +32164,11 @@
         <v>243</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="313"/>
-      <c r="D7" s="308"/>
-      <c r="E7" s="308"/>
-      <c r="F7" s="308"/>
-      <c r="G7" s="308"/>
+      <c r="C7" s="317"/>
+      <c r="D7" s="312"/>
+      <c r="E7" s="312"/>
+      <c r="F7" s="312"/>
+      <c r="G7" s="312"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -32176,11 +32176,11 @@
         <v>244</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="308"/>
-      <c r="D8" s="308"/>
-      <c r="E8" s="308"/>
-      <c r="F8" s="308"/>
-      <c r="G8" s="308"/>
+      <c r="C8" s="312"/>
+      <c r="D8" s="312"/>
+      <c r="E8" s="312"/>
+      <c r="F8" s="312"/>
+      <c r="G8" s="312"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -32188,11 +32188,11 @@
         <v>18</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="314"/>
-      <c r="D9" s="314"/>
-      <c r="E9" s="314"/>
-      <c r="F9" s="314"/>
-      <c r="G9" s="314"/>
+      <c r="C9" s="318"/>
+      <c r="D9" s="318"/>
+      <c r="E9" s="318"/>
+      <c r="F9" s="318"/>
+      <c r="G9" s="318"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -32200,11 +32200,11 @@
         <v>331</v>
       </c>
       <c r="B10" s="90"/>
-      <c r="C10" s="308"/>
-      <c r="D10" s="308"/>
-      <c r="E10" s="308"/>
-      <c r="F10" s="308"/>
-      <c r="G10" s="308"/>
+      <c r="C10" s="312"/>
+      <c r="D10" s="312"/>
+      <c r="E10" s="312"/>
+      <c r="F10" s="312"/>
+      <c r="G10" s="312"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -32217,28 +32217,28 @@
       <c r="A12" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="315" t="s">
+      <c r="B12" s="319" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="316"/>
-      <c r="D12" s="317"/>
+      <c r="C12" s="320"/>
+      <c r="D12" s="321"/>
       <c r="N12" s="141" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="318" t="s">
+      <c r="B13" s="322" t="s">
         <v>229</v>
       </c>
-      <c r="C13" s="319"/>
-      <c r="D13" s="320"/>
+      <c r="C13" s="323"/>
+      <c r="D13" s="324"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="302" t="s">
+      <c r="B14" s="306" t="s">
         <v>224</v>
       </c>
-      <c r="C14" s="303"/>
-      <c r="D14" s="304"/>
+      <c r="C14" s="307"/>
+      <c r="D14" s="308"/>
       <c r="F14">
         <f>4.5/7.2</f>
         <v>0.625</v>
@@ -32246,11 +32246,11 @@
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="305" t="s">
+      <c r="B15" s="309" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="306"/>
-      <c r="D15" s="307"/>
+      <c r="C15" s="310"/>
+      <c r="D15" s="311"/>
       <c r="F15">
         <f>F14*0.4</f>
         <v>0.25</v>
@@ -32300,7 +32300,7 @@
       <c r="D19" s="129" t="s">
         <v>406</v>
       </c>
-      <c r="F19" s="347" t="s">
+      <c r="F19" s="254" t="s">
         <v>248</v>
       </c>
       <c r="N19" s="141" t="s">
@@ -36777,43 +36777,49 @@
     <hyperlink ref="N67" r:id="rId20" location="iv-available-water" xr:uid="{4566CC8F-1D0F-43BA-BAD8-C66179151606}"/>
     <hyperlink ref="N68" r:id="rId21" location="v-enter-withdraw-within-available-water" xr:uid="{FA435611-F017-4A4C-84C0-3BC240C90BC3}"/>
     <hyperlink ref="N69" r:id="rId22" location="vi-end-of-year-balance" xr:uid="{43A45EF2-1AE7-497D-9090-A6710371091B}"/>
-    <hyperlink ref="N103" r:id="rId23" location="5a-shared-reserve-dashboard" display="Help shared, reserve" xr:uid="{93564FFE-2F11-4E1B-8E30-F04D091042B0}"/>
-    <hyperlink ref="N111" r:id="rId24" location="step-6-summary-of-participant-actions" xr:uid="{39E9E91B-EE9B-4603-9A19-992E43688C4C}"/>
-    <hyperlink ref="N134" r:id="rId25" location="lake-mead--end-of-year" xr:uid="{18709FDC-6FB8-4FF1-82C7-3E0140C4C207}"/>
-    <hyperlink ref="N137" r:id="rId26" location="step-7-move-to-next-year" xr:uid="{0D1EBCA9-BE7F-441F-A17C-5330CFCE7596}"/>
-    <hyperlink ref="N79" r:id="rId27" location="step-5-player-dashboards--conserve-consume-and-trade" xr:uid="{115088D1-B3CF-4D72-A6D6-92770E18F116}"/>
-    <hyperlink ref="N80" r:id="rId28" location="i-buy-or-sell-water-from-other-players" xr:uid="{D5A878F8-1AB0-4367-BFA6-4F25001F73AD}"/>
-    <hyperlink ref="N81" r:id="rId29" location="ii-compensation" xr:uid="{74477D73-291E-4A7F-86F2-C21A0DF60CEA}"/>
-    <hyperlink ref="N83" r:id="rId30" location="iv-available-water" xr:uid="{096A8B03-D32B-4628-BC3E-B3E64954FA42}"/>
-    <hyperlink ref="N84" r:id="rId31" location="v-enter-withdraw-within-available-water" display="Help withdraw" xr:uid="{4ED17C45-EBF9-4C45-9229-5218A5ECD61F}"/>
-    <hyperlink ref="N85" r:id="rId32" location="vi-end-of-year-balance" xr:uid="{C6E40832-042B-43D8-90B9-CD82703389C7}"/>
-    <hyperlink ref="N64" r:id="rId33" location="i-buy-or-sell-water-from-other-participantss" xr:uid="{D2AC05B4-FD61-425B-9046-D87C8AAAAEA0}"/>
-    <hyperlink ref="N71" r:id="rId34" location="step-5-participant-dashboards--conserve-consume-and-trade" xr:uid="{D67E6EF8-391E-4D21-9E33-260AECB2DB20}"/>
-    <hyperlink ref="N73" r:id="rId35" location="ii-compensation" xr:uid="{5D3E22F6-98D1-4F8D-AC9B-79BC60BD9D4C}"/>
-    <hyperlink ref="N74" r:id="rId36" location="iii-net-trade-volume-all-participants" xr:uid="{E4C097D5-D12A-4D05-9CB5-F12180A8841F}"/>
-    <hyperlink ref="N75" r:id="rId37" location="iv-available-water" xr:uid="{92A2BD5E-9234-4CDA-B631-2F26F1EDA2F6}"/>
-    <hyperlink ref="N76" r:id="rId38" location="v-enter-withdraw-within-available-water" display="Help withdraw" xr:uid="{D566555A-5FE4-4D77-A91F-AB8CA37C5882}"/>
-    <hyperlink ref="N77" r:id="rId39" location="vi-end-of-year-balance" xr:uid="{43994CDC-2740-40CF-8975-5A1D654DE92E}"/>
-    <hyperlink ref="N72" r:id="rId40" location="i-buy-or-sell-water-from-other-participantss" xr:uid="{99CA01B4-F83D-4392-BFD6-E3696F3B060F}"/>
-    <hyperlink ref="N82" r:id="rId41" location="iii-net-trade-volume-all-participants" xr:uid="{35106ED0-ED39-4B94-A4D9-B79EFE11A2E6}"/>
-    <hyperlink ref="N87" r:id="rId42" location="step-5-player-dashboards--conserve-consume-and-trade" xr:uid="{AEF1AABF-406E-492C-A9C6-6D4F230E19E9}"/>
-    <hyperlink ref="N88" r:id="rId43" location="i-buy-or-sell-water-from-other-players" xr:uid="{A414CAB3-AC71-40F2-BCEE-3B4BD79CCEC2}"/>
-    <hyperlink ref="N89" r:id="rId44" location="ii-compensation" xr:uid="{8233903D-3600-4882-9905-8BB60669B1D3}"/>
-    <hyperlink ref="N91" r:id="rId45" location="iv-available-water" xr:uid="{BD162207-CEDD-4927-ACFE-B798DB92B590}"/>
-    <hyperlink ref="N92" r:id="rId46" location="v-enter-withdraw-within-available-water" display="Help withdraw" xr:uid="{80D88F54-62DF-498A-A03F-9FC4097F6B84}"/>
-    <hyperlink ref="N93" r:id="rId47" location="vi-end-of-year-balance" xr:uid="{3C22C7BF-428B-4FE8-9C2E-F555E1D2FB9F}"/>
-    <hyperlink ref="N90" r:id="rId48" location="iii-net-trade-volume-all-participants" xr:uid="{4F49F47E-D9E6-4681-A7EF-3B21819F5A2A}"/>
-    <hyperlink ref="N95" r:id="rId49" location="step-5-player-dashboards--conserve-consume-and-trade" xr:uid="{0EF1BC22-639A-4CAC-8C5C-1003B2A67B6B}"/>
-    <hyperlink ref="N96" r:id="rId50" location="i-buy-or-sell-water-from-other-players" xr:uid="{7B556B5C-2F11-4498-8C4A-C03479306858}"/>
-    <hyperlink ref="N97" r:id="rId51" location="ii-compensation" xr:uid="{9ABDDEAE-D66A-426B-9D45-11CC8D3256D9}"/>
-    <hyperlink ref="N99" r:id="rId52" location="iv-available-water" xr:uid="{7C9A8246-47D9-49E9-B1F6-3C1231D8F415}"/>
-    <hyperlink ref="N100" r:id="rId53" location="v-enter-withdraw-within-available-water" display="Help withdraw" xr:uid="{3ACF8917-D3A9-467E-B1B3-4EFD5F90425B}"/>
-    <hyperlink ref="N101" r:id="rId54" location="vi-end-of-year-balance" xr:uid="{64582986-19BE-4DA6-A576-9ED7048A63F6}"/>
-    <hyperlink ref="N98" r:id="rId55" location="iii-net-trade-volume-all-participants" xr:uid="{00DE0E22-6C57-4CFB-AC1B-701E93DC729D}"/>
-    <hyperlink ref="N12" r:id="rId56" location="1a-explain-cell-types" xr:uid="{5E0F137C-003B-4215-AD3B-C722FAB0B485}"/>
-    <hyperlink ref="N24" r:id="rId57" location="vii-percent-of-tribal-nation-water-in-california" xr:uid="{01F1D035-6ABB-47DA-9902-C2811F877041}"/>
-    <hyperlink ref="N25" r:id="rId58" location="vii-percent-of-tribal-nation-water-in-arizona" xr:uid="{B1DD0B97-92EB-4086-A5FA-F5A6D9250A94}"/>
-    <hyperlink ref="F19" r:id="rId59" xr:uid="{CD397428-8500-47BF-8A64-FE41EFAB9B3F}"/>
+    <hyperlink ref="N111" r:id="rId23" location="step-6-summary-of-participant-actions" xr:uid="{39E9E91B-EE9B-4603-9A19-992E43688C4C}"/>
+    <hyperlink ref="N134" r:id="rId24" location="lake-mead--end-of-year" xr:uid="{18709FDC-6FB8-4FF1-82C7-3E0140C4C207}"/>
+    <hyperlink ref="N137" r:id="rId25" location="step-7-move-to-next-year" xr:uid="{0D1EBCA9-BE7F-441F-A17C-5330CFCE7596}"/>
+    <hyperlink ref="N64" r:id="rId26" location="i-buy-or-sell-water-from-other-participantss" xr:uid="{D2AC05B4-FD61-425B-9046-D87C8AAAAEA0}"/>
+    <hyperlink ref="N12" r:id="rId27" location="1a-explain-cell-types" xr:uid="{5E0F137C-003B-4215-AD3B-C722FAB0B485}"/>
+    <hyperlink ref="N24" r:id="rId28" location="vii-percent-of-tribal-nation-water-in-california" xr:uid="{01F1D035-6ABB-47DA-9902-C2811F877041}"/>
+    <hyperlink ref="N25" r:id="rId29" location="vii-percent-of-tribal-nation-water-in-arizona" xr:uid="{B1DD0B97-92EB-4086-A5FA-F5A6D9250A94}"/>
+    <hyperlink ref="F19" r:id="rId30" xr:uid="{CD397428-8500-47BF-8A64-FE41EFAB9B3F}"/>
+    <hyperlink ref="N71" r:id="rId31" location="step-5-participant-dashboards--conserve-consume-and-trade" xr:uid="{397FD8F0-2E30-496A-BE44-5B257A0157EE}"/>
+    <hyperlink ref="N73" r:id="rId32" location="ii-compensation" xr:uid="{F57B98BC-FD8A-4B97-9BA7-72787CDB74DE}"/>
+    <hyperlink ref="N74" r:id="rId33" location="iii-net-trade-volume-all-participants" xr:uid="{1B926EB5-4EDA-4705-B3ED-7A6C02210193}"/>
+    <hyperlink ref="N75" r:id="rId34" location="iv-available-water" xr:uid="{4AA187F2-EAF6-461B-9CFE-0AE554B5221C}"/>
+    <hyperlink ref="N76" r:id="rId35" location="v-enter-withdraw-within-available-water" xr:uid="{34772F54-52B5-496C-94CA-EC810414913E}"/>
+    <hyperlink ref="N77" r:id="rId36" location="vi-end-of-year-balance" xr:uid="{7E6C6019-B9DB-4F73-8888-9D49C202C8D4}"/>
+    <hyperlink ref="N72" r:id="rId37" location="i-buy-or-sell-water-from-other-participantss" xr:uid="{E7375CF2-EC0F-401A-8AFE-0454313662AF}"/>
+    <hyperlink ref="N79" r:id="rId38" location="step-5-participant-dashboards--conserve-consume-and-trade" xr:uid="{A70DB134-907F-477F-AB0B-5659C9C11813}"/>
+    <hyperlink ref="N81" r:id="rId39" location="ii-compensation" xr:uid="{684D57EC-6721-4F25-AF68-0018C1E34745}"/>
+    <hyperlink ref="N82" r:id="rId40" location="iii-net-trade-volume-all-participants" xr:uid="{37DA7529-DE0A-4A6F-8E12-612AF82A188A}"/>
+    <hyperlink ref="N83" r:id="rId41" location="iv-available-water" xr:uid="{96EA80FC-ACDC-444F-82AF-0E44E2936515}"/>
+    <hyperlink ref="N84" r:id="rId42" location="v-enter-withdraw-within-available-water" xr:uid="{089A3863-E8AF-452C-8335-69D9F1C56707}"/>
+    <hyperlink ref="N85" r:id="rId43" location="vi-end-of-year-balance" xr:uid="{475FD103-8EBA-4CD9-ACE9-66204501082E}"/>
+    <hyperlink ref="N80" r:id="rId44" location="i-buy-or-sell-water-from-other-participantss" xr:uid="{BA50878C-D141-4CB0-B547-DD4E0AB28999}"/>
+    <hyperlink ref="N87" r:id="rId45" location="step-5-participant-dashboards--conserve-consume-and-trade" xr:uid="{39EC330A-C201-45C3-99B6-B424E8A32D15}"/>
+    <hyperlink ref="N89" r:id="rId46" location="ii-compensation" xr:uid="{83B18F55-633C-453C-814E-1C950087B924}"/>
+    <hyperlink ref="N90" r:id="rId47" location="iii-net-trade-volume-all-participants" xr:uid="{428C6409-0DD6-4EB4-9EB1-0D06FB68C519}"/>
+    <hyperlink ref="N91" r:id="rId48" location="iv-available-water" xr:uid="{D2F44442-7A66-450B-97C3-DB62319C8041}"/>
+    <hyperlink ref="N92" r:id="rId49" location="v-enter-withdraw-within-available-water" xr:uid="{8511206C-7A63-4135-A4AC-03ED1A7FF5BA}"/>
+    <hyperlink ref="N93" r:id="rId50" location="vi-end-of-year-balance" xr:uid="{B922D973-A534-4E90-B9F3-EF812FD44F7A}"/>
+    <hyperlink ref="N88" r:id="rId51" location="i-buy-or-sell-water-from-other-participantss" xr:uid="{A5C5B388-17B6-437D-A672-71973A49D5E7}"/>
+    <hyperlink ref="N95" r:id="rId52" location="step-5-participant-dashboards--conserve-consume-and-trade" xr:uid="{9D4E2F1A-09BE-48C9-9068-C731FDB7E63B}"/>
+    <hyperlink ref="N97" r:id="rId53" location="ii-compensation" xr:uid="{7A619A05-DF2E-44B2-B251-8B6219653520}"/>
+    <hyperlink ref="N98" r:id="rId54" location="iii-net-trade-volume-all-participants" xr:uid="{32C1A2E5-D297-4111-B6D0-5CF58DD1D352}"/>
+    <hyperlink ref="N99" r:id="rId55" location="iv-available-water" xr:uid="{CB765DE1-3875-46F1-8FBF-E0A429B0AF7C}"/>
+    <hyperlink ref="N100" r:id="rId56" location="v-enter-withdraw-within-available-water" xr:uid="{4A2CF82E-D869-4A43-8DDC-871D0CC63292}"/>
+    <hyperlink ref="N101" r:id="rId57" location="vi-end-of-year-balance" xr:uid="{25EBA77D-5DF6-49B3-AA19-FB1D17E5F9F4}"/>
+    <hyperlink ref="N96" r:id="rId58" location="i-buy-or-sell-water-from-other-participantss" xr:uid="{FAB9FF44-F4B9-4203-BBC6-8852F3D9A20B}"/>
+    <hyperlink ref="N103" r:id="rId59" location="step-5-participant-dashboards--conserve-consume-and-trade" xr:uid="{E770BD7B-95C0-4128-95DC-F80C83C66E2B}"/>
+    <hyperlink ref="N105" r:id="rId60" location="ii-compensation" xr:uid="{33C35802-FAB0-4790-B941-1A3E7257395B}"/>
+    <hyperlink ref="N106" r:id="rId61" location="iii-net-trade-volume-all-participants" xr:uid="{836F4C5D-BBF9-4976-9ADE-859356E14210}"/>
+    <hyperlink ref="N107" r:id="rId62" location="iv-available-water" xr:uid="{06AED8BC-115A-4B9E-8553-F960DEF913FF}"/>
+    <hyperlink ref="N108" r:id="rId63" location="v-enter-withdraw-within-available-water" xr:uid="{28B406B7-C3AF-4DAD-90AB-E74B9A16207B}"/>
+    <hyperlink ref="N109" r:id="rId64" location="vi-end-of-year-balance" xr:uid="{9FD845D0-38C3-41FD-ABEC-D3B2368EEF38}"/>
+    <hyperlink ref="N104" r:id="rId65" location="i-buy-or-sell-water-from-other-participantss" xr:uid="{0294E6B9-5E30-4F0F-A0BF-7C0B7042CF51}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -37061,29 +37067,29 @@
     </row>
     <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="I5" s="333" t="s">
+      <c r="I5" s="337" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="333" t="s">
+      <c r="J5" s="337" t="s">
         <v>253</v>
       </c>
-      <c r="K5" s="333" t="s">
+      <c r="K5" s="337" t="s">
         <v>254</v>
       </c>
-      <c r="L5" s="330" t="s">
+      <c r="L5" s="334" t="s">
         <v>255</v>
       </c>
-      <c r="M5" s="331"/>
-      <c r="N5" s="331"/>
-      <c r="O5" s="331"/>
-      <c r="P5" s="332"/>
-      <c r="Q5" s="322" t="s">
+      <c r="M5" s="335"/>
+      <c r="N5" s="335"/>
+      <c r="O5" s="335"/>
+      <c r="P5" s="336"/>
+      <c r="Q5" s="326" t="s">
         <v>256</v>
       </c>
-      <c r="R5" s="323"/>
-      <c r="S5" s="323"/>
-      <c r="T5" s="323"/>
-      <c r="U5" s="324"/>
+      <c r="R5" s="327"/>
+      <c r="S5" s="327"/>
+      <c r="T5" s="327"/>
+      <c r="U5" s="328"/>
     </row>
     <row r="6" spans="1:21" s="188" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="189" t="s">
@@ -37104,9 +37110,9 @@
       <c r="G6" s="189" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="334"/>
-      <c r="J6" s="334"/>
-      <c r="K6" s="334"/>
+      <c r="I6" s="338"/>
+      <c r="J6" s="338"/>
+      <c r="K6" s="338"/>
       <c r="L6" s="190" t="s">
         <v>258</v>
       </c>
@@ -37139,14 +37145,14 @@
       </c>
     </row>
     <row r="7" spans="1:21" s="188" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="330" t="s">
+      <c r="B7" s="334" t="s">
         <v>268</v>
       </c>
-      <c r="C7" s="331"/>
-      <c r="D7" s="331"/>
-      <c r="E7" s="331"/>
-      <c r="F7" s="331"/>
-      <c r="G7" s="332"/>
+      <c r="C7" s="335"/>
+      <c r="D7" s="335"/>
+      <c r="E7" s="335"/>
+      <c r="F7" s="335"/>
+      <c r="G7" s="336"/>
       <c r="I7" s="192" t="s">
         <v>269</v>
       </c>
@@ -37414,13 +37420,13 @@
       <c r="B11" s="198" t="s">
         <v>275</v>
       </c>
-      <c r="C11" s="321" t="s">
+      <c r="C11" s="325" t="s">
         <v>276</v>
       </c>
-      <c r="D11" s="321"/>
-      <c r="E11" s="321"/>
-      <c r="F11" s="321"/>
-      <c r="G11" s="321"/>
+      <c r="D11" s="325"/>
+      <c r="E11" s="325"/>
+      <c r="F11" s="325"/>
+      <c r="G11" s="325"/>
       <c r="I11" s="192" t="s">
         <v>277</v>
       </c>
@@ -37474,14 +37480,14 @@
       </c>
     </row>
     <row r="12" spans="1:21" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.3">
-      <c r="B12" s="325" t="s">
+      <c r="B12" s="329" t="s">
         <v>278</v>
       </c>
-      <c r="C12" s="326"/>
-      <c r="D12" s="326"/>
-      <c r="E12" s="326"/>
-      <c r="F12" s="326"/>
-      <c r="G12" s="326"/>
+      <c r="C12" s="330"/>
+      <c r="D12" s="330"/>
+      <c r="E12" s="330"/>
+      <c r="F12" s="330"/>
+      <c r="G12" s="330"/>
       <c r="I12" s="192" t="s">
         <v>279</v>
       </c>
@@ -37491,20 +37497,20 @@
       <c r="K12" s="200" t="s">
         <v>280</v>
       </c>
-      <c r="L12" s="327" t="s">
+      <c r="L12" s="331" t="s">
         <v>276</v>
       </c>
-      <c r="M12" s="328"/>
-      <c r="N12" s="328"/>
-      <c r="O12" s="328"/>
-      <c r="P12" s="329"/>
-      <c r="Q12" s="327" t="s">
+      <c r="M12" s="332"/>
+      <c r="N12" s="332"/>
+      <c r="O12" s="332"/>
+      <c r="P12" s="333"/>
+      <c r="Q12" s="331" t="s">
         <v>276</v>
       </c>
-      <c r="R12" s="328"/>
-      <c r="S12" s="328"/>
-      <c r="T12" s="328"/>
-      <c r="U12" s="329"/>
+      <c r="R12" s="332"/>
+      <c r="S12" s="332"/>
+      <c r="T12" s="332"/>
+      <c r="U12" s="333"/>
     </row>
     <row r="13" spans="1:21" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="B13" s="198">
@@ -37755,13 +37761,13 @@
       <c r="B18" s="198" t="s">
         <v>275</v>
       </c>
-      <c r="C18" s="321" t="s">
+      <c r="C18" s="325" t="s">
         <v>276</v>
       </c>
-      <c r="D18" s="321"/>
-      <c r="E18" s="321"/>
-      <c r="F18" s="321"/>
-      <c r="G18" s="321"/>
+      <c r="D18" s="325"/>
+      <c r="E18" s="325"/>
+      <c r="F18" s="325"/>
+      <c r="G18" s="325"/>
     </row>
     <row r="19" spans="2:21" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.3">
       <c r="I19" s="197" t="s">
@@ -38509,16 +38515,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="336" t="e">
+      <c r="A1" s="339" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="336"/>
-      <c r="C1" s="336"/>
-      <c r="D1" s="336"/>
-      <c r="E1" s="336"/>
-      <c r="F1" s="336"/>
-      <c r="G1" s="336"/>
+      <c r="B1" s="339"/>
+      <c r="C1" s="339"/>
+      <c r="D1" s="339"/>
+      <c r="E1" s="339"/>
+      <c r="F1" s="339"/>
+      <c r="G1" s="339"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -38527,15 +38533,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="309" t="s">
+      <c r="A3" s="313" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="309"/>
-      <c r="C3" s="309"/>
-      <c r="D3" s="309"/>
-      <c r="E3" s="309"/>
-      <c r="F3" s="309"/>
-      <c r="G3" s="309"/>
+      <c r="B3" s="313"/>
+      <c r="C3" s="313"/>
+      <c r="D3" s="313"/>
+      <c r="E3" s="313"/>
+      <c r="F3" s="313"/>
+      <c r="G3" s="313"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -38551,13 +38557,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="310" t="s">
+      <c r="C4" s="314" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="311"/>
-      <c r="E4" s="311"/>
-      <c r="F4" s="311"/>
-      <c r="G4" s="312"/>
+      <c r="D4" s="315"/>
+      <c r="E4" s="315"/>
+      <c r="F4" s="315"/>
+      <c r="G4" s="316"/>
       <c r="N4" s="139" t="s">
         <v>168</v>
       </c>
@@ -38567,11 +38573,11 @@
         <v>16</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="313"/>
-      <c r="D5" s="308"/>
-      <c r="E5" s="308"/>
-      <c r="F5" s="308"/>
-      <c r="G5" s="308"/>
+      <c r="C5" s="317"/>
+      <c r="D5" s="312"/>
+      <c r="E5" s="312"/>
+      <c r="F5" s="312"/>
+      <c r="G5" s="312"/>
       <c r="N5" s="142"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
@@ -38579,11 +38585,11 @@
         <v>17</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="313"/>
-      <c r="D6" s="308"/>
-      <c r="E6" s="308"/>
-      <c r="F6" s="308"/>
-      <c r="G6" s="308"/>
+      <c r="C6" s="317"/>
+      <c r="D6" s="312"/>
+      <c r="E6" s="312"/>
+      <c r="F6" s="312"/>
+      <c r="G6" s="312"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
@@ -38591,11 +38597,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="313"/>
-      <c r="D7" s="308"/>
-      <c r="E7" s="308"/>
-      <c r="F7" s="308"/>
-      <c r="G7" s="308"/>
+      <c r="C7" s="317"/>
+      <c r="D7" s="312"/>
+      <c r="E7" s="312"/>
+      <c r="F7" s="312"/>
+      <c r="G7" s="312"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
@@ -38603,11 +38609,11 @@
         <v>78</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="308"/>
-      <c r="D8" s="308"/>
-      <c r="E8" s="308"/>
-      <c r="F8" s="308"/>
-      <c r="G8" s="308"/>
+      <c r="C8" s="312"/>
+      <c r="D8" s="312"/>
+      <c r="E8" s="312"/>
+      <c r="F8" s="312"/>
+      <c r="G8" s="312"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
@@ -38615,11 +38621,11 @@
         <v>202</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="314"/>
-      <c r="D9" s="314"/>
-      <c r="E9" s="314"/>
-      <c r="F9" s="314"/>
-      <c r="G9" s="314"/>
+      <c r="C9" s="318"/>
+      <c r="D9" s="318"/>
+      <c r="E9" s="318"/>
+      <c r="F9" s="318"/>
+      <c r="G9" s="318"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
@@ -38627,11 +38633,11 @@
         <v>80</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="335"/>
-      <c r="D10" s="335"/>
-      <c r="E10" s="335"/>
-      <c r="F10" s="335"/>
-      <c r="G10" s="335"/>
+      <c r="C10" s="340"/>
+      <c r="D10" s="340"/>
+      <c r="E10" s="340"/>
+      <c r="F10" s="340"/>
+      <c r="G10" s="340"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -38644,37 +38650,37 @@
       <c r="A12" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="315" t="s">
+      <c r="B12" s="319" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="316"/>
-      <c r="D12" s="317"/>
+      <c r="C12" s="320"/>
+      <c r="D12" s="321"/>
       <c r="N12" s="141" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B13" s="318" t="s">
+      <c r="B13" s="322" t="s">
         <v>153</v>
       </c>
-      <c r="C13" s="319"/>
-      <c r="D13" s="320"/>
+      <c r="C13" s="323"/>
+      <c r="D13" s="324"/>
       <c r="N13" s="142"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B14" s="302" t="s">
+      <c r="B14" s="306" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="303"/>
-      <c r="D14" s="304"/>
+      <c r="C14" s="307"/>
+      <c r="D14" s="308"/>
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B15" s="305" t="s">
+      <c r="B15" s="309" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="306"/>
-      <c r="D15" s="307"/>
+      <c r="C15" s="310"/>
+      <c r="D15" s="311"/>
       <c r="N15" s="142"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -39894,12 +39900,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -39907,6 +39907,12 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>
@@ -39964,26 +39970,26 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D3" s="337" t="s">
+      <c r="D3" s="341" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="337"/>
-      <c r="F3" s="337" t="s">
+      <c r="E3" s="341"/>
+      <c r="F3" s="341" t="s">
         <v>100</v>
       </c>
-      <c r="G3" s="337"/>
-      <c r="H3" s="337"/>
-      <c r="I3" s="337" t="s">
+      <c r="G3" s="341"/>
+      <c r="H3" s="341"/>
+      <c r="I3" s="341" t="s">
         <v>101</v>
       </c>
-      <c r="J3" s="337"/>
-      <c r="K3" s="337"/>
+      <c r="J3" s="341"/>
+      <c r="K3" s="341"/>
       <c r="L3" s="134"/>
-      <c r="M3" s="337" t="s">
+      <c r="M3" s="341" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="337"/>
-      <c r="O3" s="337"/>
+      <c r="N3" s="341"/>
+      <c r="O3" s="341"/>
     </row>
     <row r="4" spans="1:16" s="47" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="46" t="s">

</xml_diff>

<commit_message>
Add recent historical use to model guide
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF70758-8E02-4BF3-B1EF-03B296A6A459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7D8118-AA92-43ED-A44D-5411C0203CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -3398,6 +3398,69 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3452,12 +3515,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3489,63 +3546,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3650,11 +3650,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -15236,20 +15236,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="258" t="s">
+      <c r="A1" s="279" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="258"/>
-      <c r="C1" s="258"/>
-      <c r="D1" s="258"/>
-      <c r="E1" s="258"/>
-      <c r="F1" s="258"/>
-      <c r="G1" s="258"/>
-      <c r="H1" s="258"/>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="258"/>
-      <c r="L1" s="258"/>
+      <c r="B1" s="279"/>
+      <c r="C1" s="279"/>
+      <c r="D1" s="279"/>
+      <c r="E1" s="279"/>
+      <c r="F1" s="279"/>
+      <c r="G1" s="279"/>
+      <c r="H1" s="279"/>
+      <c r="I1" s="279"/>
+      <c r="J1" s="279"/>
+      <c r="K1" s="279"/>
+      <c r="L1" s="279"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -15275,41 +15275,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="259" t="s">
+      <c r="A4" s="280" t="s">
         <v>351</v>
       </c>
-      <c r="B4" s="260"/>
-      <c r="C4" s="260"/>
-      <c r="D4" s="260"/>
-      <c r="E4" s="260"/>
-      <c r="F4" s="260"/>
-      <c r="G4" s="260"/>
-      <c r="H4" s="260"/>
-      <c r="I4" s="260"/>
-      <c r="J4" s="260"/>
-      <c r="K4" s="260"/>
-      <c r="L4" s="261"/>
-      <c r="N4" s="262"/>
-      <c r="O4" s="262"/>
-      <c r="P4" s="262"/>
-      <c r="Q4" s="262"/>
-      <c r="R4" s="262"/>
+      <c r="B4" s="281"/>
+      <c r="C4" s="281"/>
+      <c r="D4" s="281"/>
+      <c r="E4" s="281"/>
+      <c r="F4" s="281"/>
+      <c r="G4" s="281"/>
+      <c r="H4" s="281"/>
+      <c r="I4" s="281"/>
+      <c r="J4" s="281"/>
+      <c r="K4" s="281"/>
+      <c r="L4" s="282"/>
+      <c r="N4" s="283"/>
+      <c r="O4" s="283"/>
+      <c r="P4" s="283"/>
+      <c r="Q4" s="283"/>
+      <c r="R4" s="283"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="263" t="s">
+      <c r="A5" s="284" t="s">
         <v>334</v>
       </c>
-      <c r="B5" s="264"/>
-      <c r="C5" s="264"/>
-      <c r="D5" s="264"/>
-      <c r="E5" s="264"/>
-      <c r="F5" s="264"/>
-      <c r="G5" s="264"/>
-      <c r="H5" s="264"/>
-      <c r="I5" s="264"/>
-      <c r="J5" s="264"/>
-      <c r="K5" s="264"/>
-      <c r="L5" s="265"/>
+      <c r="B5" s="285"/>
+      <c r="C5" s="285"/>
+      <c r="D5" s="285"/>
+      <c r="E5" s="285"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="285"/>
+      <c r="H5" s="285"/>
+      <c r="I5" s="285"/>
+      <c r="J5" s="285"/>
+      <c r="K5" s="285"/>
+      <c r="L5" s="286"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15317,20 +15317,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="263" t="s">
+      <c r="A6" s="284" t="s">
         <v>352</v>
       </c>
-      <c r="B6" s="264"/>
-      <c r="C6" s="264"/>
-      <c r="D6" s="264"/>
-      <c r="E6" s="264"/>
-      <c r="F6" s="264"/>
-      <c r="G6" s="264"/>
-      <c r="H6" s="264"/>
-      <c r="I6" s="264"/>
-      <c r="J6" s="264"/>
-      <c r="K6" s="264"/>
-      <c r="L6" s="265"/>
+      <c r="B6" s="285"/>
+      <c r="C6" s="285"/>
+      <c r="D6" s="285"/>
+      <c r="E6" s="285"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="285"/>
+      <c r="H6" s="285"/>
+      <c r="I6" s="285"/>
+      <c r="J6" s="285"/>
+      <c r="K6" s="285"/>
+      <c r="L6" s="286"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15339,19 +15339,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="232"/>
-      <c r="B7" s="264" t="s">
+      <c r="B7" s="285" t="s">
         <v>353</v>
       </c>
-      <c r="C7" s="264"/>
-      <c r="D7" s="264"/>
-      <c r="E7" s="264"/>
-      <c r="F7" s="264"/>
-      <c r="G7" s="264"/>
-      <c r="H7" s="264"/>
-      <c r="I7" s="264"/>
-      <c r="J7" s="264"/>
-      <c r="K7" s="264"/>
-      <c r="L7" s="265"/>
+      <c r="C7" s="285"/>
+      <c r="D7" s="285"/>
+      <c r="E7" s="285"/>
+      <c r="F7" s="285"/>
+      <c r="G7" s="285"/>
+      <c r="H7" s="285"/>
+      <c r="I7" s="285"/>
+      <c r="J7" s="285"/>
+      <c r="K7" s="285"/>
+      <c r="L7" s="286"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15360,19 +15360,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="233"/>
-      <c r="B8" s="281" t="s">
+      <c r="B8" s="300" t="s">
         <v>354</v>
       </c>
-      <c r="C8" s="281"/>
-      <c r="D8" s="281"/>
-      <c r="E8" s="281"/>
-      <c r="F8" s="281"/>
-      <c r="G8" s="281"/>
-      <c r="H8" s="281"/>
-      <c r="I8" s="281"/>
-      <c r="J8" s="281"/>
-      <c r="K8" s="281"/>
-      <c r="L8" s="282"/>
+      <c r="C8" s="300"/>
+      <c r="D8" s="300"/>
+      <c r="E8" s="300"/>
+      <c r="F8" s="300"/>
+      <c r="G8" s="300"/>
+      <c r="H8" s="300"/>
+      <c r="I8" s="300"/>
+      <c r="J8" s="300"/>
+      <c r="K8" s="300"/>
+      <c r="L8" s="301"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15394,38 +15394,38 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="283" t="s">
+      <c r="A10" s="302" t="s">
         <v>389</v>
       </c>
-      <c r="B10" s="284"/>
-      <c r="C10" s="284"/>
-      <c r="D10" s="284"/>
-      <c r="E10" s="284"/>
-      <c r="F10" s="284"/>
-      <c r="G10" s="284"/>
-      <c r="H10" s="284"/>
-      <c r="I10" s="284"/>
-      <c r="J10" s="284"/>
-      <c r="K10" s="284"/>
-      <c r="L10" s="285"/>
+      <c r="B10" s="303"/>
+      <c r="C10" s="303"/>
+      <c r="D10" s="303"/>
+      <c r="E10" s="303"/>
+      <c r="F10" s="303"/>
+      <c r="G10" s="303"/>
+      <c r="H10" s="303"/>
+      <c r="I10" s="303"/>
+      <c r="J10" s="303"/>
+      <c r="K10" s="303"/>
+      <c r="L10" s="304"/>
     </row>
     <row r="11" spans="1:18" s="58" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="253" t="s">
         <v>390</v>
       </c>
-      <c r="B11" s="286" t="s">
+      <c r="B11" s="257" t="s">
         <v>393</v>
       </c>
-      <c r="C11" s="286"/>
-      <c r="D11" s="286"/>
-      <c r="E11" s="286"/>
-      <c r="F11" s="286"/>
-      <c r="G11" s="286"/>
-      <c r="H11" s="286"/>
-      <c r="I11" s="286"/>
-      <c r="J11" s="286"/>
-      <c r="K11" s="286"/>
-      <c r="L11" s="287"/>
+      <c r="C11" s="257"/>
+      <c r="D11" s="257"/>
+      <c r="E11" s="257"/>
+      <c r="F11" s="257"/>
+      <c r="G11" s="257"/>
+      <c r="H11" s="257"/>
+      <c r="I11" s="257"/>
+      <c r="J11" s="257"/>
+      <c r="K11" s="257"/>
+      <c r="L11" s="258"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="161.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="245"/>
@@ -15445,51 +15445,51 @@
       <c r="A13" s="253" t="s">
         <v>391</v>
       </c>
-      <c r="B13" s="286" t="s">
+      <c r="B13" s="257" t="s">
         <v>394</v>
       </c>
-      <c r="C13" s="286"/>
-      <c r="D13" s="286"/>
-      <c r="E13" s="286"/>
-      <c r="F13" s="286"/>
-      <c r="G13" s="286"/>
-      <c r="H13" s="286"/>
-      <c r="I13" s="286"/>
-      <c r="J13" s="286"/>
-      <c r="K13" s="286"/>
-      <c r="L13" s="287"/>
+      <c r="C13" s="257"/>
+      <c r="D13" s="257"/>
+      <c r="E13" s="257"/>
+      <c r="F13" s="257"/>
+      <c r="G13" s="257"/>
+      <c r="H13" s="257"/>
+      <c r="I13" s="257"/>
+      <c r="J13" s="257"/>
+      <c r="K13" s="257"/>
+      <c r="L13" s="258"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="90.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="245"/>
-      <c r="B14" s="295"/>
-      <c r="C14" s="295"/>
-      <c r="D14" s="295"/>
-      <c r="E14" s="295"/>
-      <c r="F14" s="295"/>
-      <c r="G14" s="295"/>
-      <c r="H14" s="295"/>
-      <c r="I14" s="295"/>
-      <c r="J14" s="295"/>
-      <c r="K14" s="295"/>
-      <c r="L14" s="296"/>
+      <c r="B14" s="259"/>
+      <c r="C14" s="259"/>
+      <c r="D14" s="259"/>
+      <c r="E14" s="259"/>
+      <c r="F14" s="259"/>
+      <c r="G14" s="259"/>
+      <c r="H14" s="259"/>
+      <c r="I14" s="259"/>
+      <c r="J14" s="259"/>
+      <c r="K14" s="259"/>
+      <c r="L14" s="260"/>
     </row>
     <row r="15" spans="1:18" s="58" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="253" t="s">
         <v>392</v>
       </c>
-      <c r="B15" s="286" t="s">
+      <c r="B15" s="257" t="s">
         <v>395</v>
       </c>
-      <c r="C15" s="286"/>
-      <c r="D15" s="286"/>
-      <c r="E15" s="286"/>
-      <c r="F15" s="286"/>
-      <c r="G15" s="286"/>
-      <c r="H15" s="286"/>
-      <c r="I15" s="286"/>
-      <c r="J15" s="286"/>
-      <c r="K15" s="286"/>
-      <c r="L15" s="287"/>
+      <c r="C15" s="257"/>
+      <c r="D15" s="257"/>
+      <c r="E15" s="257"/>
+      <c r="F15" s="257"/>
+      <c r="G15" s="257"/>
+      <c r="H15" s="257"/>
+      <c r="I15" s="257"/>
+      <c r="J15" s="257"/>
+      <c r="K15" s="257"/>
+      <c r="L15" s="258"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="245"/>
@@ -15506,12 +15506,12 @@
       <c r="L16" s="252"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="303" t="s">
+      <c r="A17" s="255" t="s">
         <v>400</v>
       </c>
-      <c r="B17" s="304"/>
-      <c r="C17" s="304"/>
-      <c r="D17" s="304"/>
+      <c r="B17" s="256"/>
+      <c r="C17" s="256"/>
+      <c r="D17" s="256"/>
       <c r="E17" s="250" t="s">
         <v>401</v>
       </c>
@@ -15538,84 +15538,84 @@
       <c r="L18" s="113"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="266" t="s">
+      <c r="A19" s="287" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="267"/>
-      <c r="C19" s="267"/>
-      <c r="D19" s="267"/>
-      <c r="E19" s="267"/>
-      <c r="F19" s="267"/>
-      <c r="G19" s="267"/>
-      <c r="H19" s="267"/>
-      <c r="I19" s="267"/>
-      <c r="J19" s="267"/>
-      <c r="K19" s="267"/>
-      <c r="L19" s="268"/>
+      <c r="B19" s="288"/>
+      <c r="C19" s="288"/>
+      <c r="D19" s="288"/>
+      <c r="E19" s="288"/>
+      <c r="F19" s="288"/>
+      <c r="G19" s="288"/>
+      <c r="H19" s="288"/>
+      <c r="I19" s="288"/>
+      <c r="J19" s="288"/>
+      <c r="K19" s="288"/>
+      <c r="L19" s="289"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="269" t="s">
+      <c r="A20" s="290" t="s">
         <v>335</v>
       </c>
-      <c r="B20" s="270"/>
-      <c r="C20" s="270"/>
-      <c r="D20" s="270"/>
-      <c r="E20" s="270"/>
-      <c r="F20" s="270"/>
-      <c r="G20" s="270"/>
-      <c r="H20" s="270"/>
-      <c r="I20" s="270"/>
-      <c r="J20" s="270"/>
-      <c r="K20" s="270"/>
-      <c r="L20" s="271"/>
+      <c r="B20" s="291"/>
+      <c r="C20" s="291"/>
+      <c r="D20" s="291"/>
+      <c r="E20" s="291"/>
+      <c r="F20" s="291"/>
+      <c r="G20" s="291"/>
+      <c r="H20" s="291"/>
+      <c r="I20" s="291"/>
+      <c r="J20" s="291"/>
+      <c r="K20" s="291"/>
+      <c r="L20" s="292"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="272" t="s">
+      <c r="A21" s="293" t="s">
         <v>336</v>
       </c>
-      <c r="B21" s="273"/>
-      <c r="C21" s="273"/>
-      <c r="D21" s="273"/>
-      <c r="E21" s="273"/>
-      <c r="F21" s="273"/>
-      <c r="G21" s="273"/>
-      <c r="H21" s="273"/>
-      <c r="I21" s="273"/>
-      <c r="J21" s="273"/>
-      <c r="K21" s="273"/>
-      <c r="L21" s="274"/>
+      <c r="B21" s="271"/>
+      <c r="C21" s="271"/>
+      <c r="D21" s="271"/>
+      <c r="E21" s="271"/>
+      <c r="F21" s="271"/>
+      <c r="G21" s="271"/>
+      <c r="H21" s="271"/>
+      <c r="I21" s="271"/>
+      <c r="J21" s="271"/>
+      <c r="K21" s="271"/>
+      <c r="L21" s="272"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="272" t="s">
+      <c r="A22" s="293" t="s">
         <v>206</v>
       </c>
-      <c r="B22" s="273"/>
-      <c r="C22" s="273"/>
-      <c r="D22" s="273"/>
-      <c r="E22" s="273"/>
-      <c r="F22" s="273"/>
-      <c r="G22" s="273"/>
-      <c r="H22" s="273"/>
-      <c r="I22" s="273"/>
-      <c r="J22" s="273"/>
-      <c r="K22" s="273"/>
-      <c r="L22" s="274"/>
+      <c r="B22" s="271"/>
+      <c r="C22" s="271"/>
+      <c r="D22" s="271"/>
+      <c r="E22" s="271"/>
+      <c r="F22" s="271"/>
+      <c r="G22" s="271"/>
+      <c r="H22" s="271"/>
+      <c r="I22" s="271"/>
+      <c r="J22" s="271"/>
+      <c r="K22" s="271"/>
+      <c r="L22" s="272"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="275" t="s">
+      <c r="A23" s="294" t="s">
         <v>337</v>
       </c>
-      <c r="B23" s="276"/>
-      <c r="C23" s="276"/>
-      <c r="D23" s="276"/>
-      <c r="E23" s="276"/>
-      <c r="F23" s="276"/>
-      <c r="G23" s="276"/>
-      <c r="H23" s="276"/>
-      <c r="I23" s="276"/>
-      <c r="J23" s="276"/>
-      <c r="K23" s="276"/>
-      <c r="L23" s="277"/>
+      <c r="B23" s="295"/>
+      <c r="C23" s="295"/>
+      <c r="D23" s="295"/>
+      <c r="E23" s="295"/>
+      <c r="F23" s="295"/>
+      <c r="G23" s="295"/>
+      <c r="H23" s="295"/>
+      <c r="I23" s="295"/>
+      <c r="J23" s="295"/>
+      <c r="K23" s="295"/>
+      <c r="L23" s="296"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="113"/>
@@ -15632,332 +15632,332 @@
       <c r="L24" s="113"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="278" t="s">
+      <c r="A25" s="297" t="s">
         <v>333</v>
       </c>
-      <c r="B25" s="279"/>
-      <c r="C25" s="279"/>
-      <c r="D25" s="279"/>
-      <c r="E25" s="279"/>
-      <c r="F25" s="279"/>
-      <c r="G25" s="279"/>
-      <c r="H25" s="279"/>
-      <c r="I25" s="279"/>
-      <c r="J25" s="279"/>
-      <c r="K25" s="279"/>
-      <c r="L25" s="280"/>
+      <c r="B25" s="298"/>
+      <c r="C25" s="298"/>
+      <c r="D25" s="298"/>
+      <c r="E25" s="298"/>
+      <c r="F25" s="298"/>
+      <c r="G25" s="298"/>
+      <c r="H25" s="298"/>
+      <c r="I25" s="298"/>
+      <c r="J25" s="298"/>
+      <c r="K25" s="298"/>
+      <c r="L25" s="299"/>
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="255" t="s">
+      <c r="A26" s="276" t="s">
         <v>215</v>
       </c>
-      <c r="B26" s="256"/>
-      <c r="C26" s="256"/>
-      <c r="D26" s="256"/>
-      <c r="E26" s="256"/>
-      <c r="F26" s="256"/>
-      <c r="G26" s="256"/>
-      <c r="H26" s="256"/>
-      <c r="I26" s="256"/>
-      <c r="J26" s="256"/>
-      <c r="K26" s="256"/>
-      <c r="L26" s="257"/>
+      <c r="B26" s="277"/>
+      <c r="C26" s="277"/>
+      <c r="D26" s="277"/>
+      <c r="E26" s="277"/>
+      <c r="F26" s="277"/>
+      <c r="G26" s="277"/>
+      <c r="H26" s="277"/>
+      <c r="I26" s="277"/>
+      <c r="J26" s="277"/>
+      <c r="K26" s="277"/>
+      <c r="L26" s="278"/>
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="227">
         <v>1</v>
       </c>
-      <c r="B27" s="290" t="s">
+      <c r="B27" s="264" t="s">
         <v>214</v>
       </c>
-      <c r="C27" s="290"/>
-      <c r="D27" s="290"/>
-      <c r="E27" s="290"/>
-      <c r="F27" s="290"/>
-      <c r="G27" s="290"/>
-      <c r="H27" s="290"/>
-      <c r="I27" s="290"/>
-      <c r="J27" s="290"/>
-      <c r="K27" s="290"/>
-      <c r="L27" s="291"/>
+      <c r="C27" s="264"/>
+      <c r="D27" s="264"/>
+      <c r="E27" s="264"/>
+      <c r="F27" s="264"/>
+      <c r="G27" s="264"/>
+      <c r="H27" s="264"/>
+      <c r="I27" s="264"/>
+      <c r="J27" s="264"/>
+      <c r="K27" s="264"/>
+      <c r="L27" s="265"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="227">
         <v>2</v>
       </c>
-      <c r="B28" s="290" t="s">
+      <c r="B28" s="264" t="s">
         <v>329</v>
       </c>
-      <c r="C28" s="290"/>
-      <c r="D28" s="290"/>
-      <c r="E28" s="290"/>
-      <c r="F28" s="290"/>
-      <c r="G28" s="290"/>
-      <c r="H28" s="290"/>
-      <c r="I28" s="290"/>
-      <c r="J28" s="290"/>
-      <c r="K28" s="290"/>
-      <c r="L28" s="291"/>
+      <c r="C28" s="264"/>
+      <c r="D28" s="264"/>
+      <c r="E28" s="264"/>
+      <c r="F28" s="264"/>
+      <c r="G28" s="264"/>
+      <c r="H28" s="264"/>
+      <c r="I28" s="264"/>
+      <c r="J28" s="264"/>
+      <c r="K28" s="264"/>
+      <c r="L28" s="265"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="227">
         <v>3</v>
       </c>
-      <c r="B29" s="290" t="s">
+      <c r="B29" s="264" t="s">
         <v>207</v>
       </c>
-      <c r="C29" s="290"/>
-      <c r="D29" s="290"/>
-      <c r="E29" s="290"/>
-      <c r="F29" s="290"/>
-      <c r="G29" s="290"/>
-      <c r="H29" s="290"/>
-      <c r="I29" s="290"/>
-      <c r="J29" s="290"/>
-      <c r="K29" s="290"/>
-      <c r="L29" s="291"/>
+      <c r="C29" s="264"/>
+      <c r="D29" s="264"/>
+      <c r="E29" s="264"/>
+      <c r="F29" s="264"/>
+      <c r="G29" s="264"/>
+      <c r="H29" s="264"/>
+      <c r="I29" s="264"/>
+      <c r="J29" s="264"/>
+      <c r="K29" s="264"/>
+      <c r="L29" s="265"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="227">
         <v>4</v>
       </c>
-      <c r="B30" s="290" t="s">
+      <c r="B30" s="264" t="s">
         <v>338</v>
       </c>
-      <c r="C30" s="290"/>
-      <c r="D30" s="290"/>
-      <c r="E30" s="290"/>
-      <c r="F30" s="290"/>
-      <c r="G30" s="290"/>
-      <c r="H30" s="290"/>
-      <c r="I30" s="290"/>
-      <c r="J30" s="290"/>
-      <c r="K30" s="290"/>
-      <c r="L30" s="291"/>
+      <c r="C30" s="264"/>
+      <c r="D30" s="264"/>
+      <c r="E30" s="264"/>
+      <c r="F30" s="264"/>
+      <c r="G30" s="264"/>
+      <c r="H30" s="264"/>
+      <c r="I30" s="264"/>
+      <c r="J30" s="264"/>
+      <c r="K30" s="264"/>
+      <c r="L30" s="265"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="227">
         <v>5</v>
       </c>
-      <c r="B31" s="290" t="s">
+      <c r="B31" s="264" t="s">
         <v>208</v>
       </c>
-      <c r="C31" s="290"/>
-      <c r="D31" s="290"/>
-      <c r="E31" s="290"/>
-      <c r="F31" s="290"/>
-      <c r="G31" s="290"/>
-      <c r="H31" s="290"/>
-      <c r="I31" s="290"/>
-      <c r="J31" s="290"/>
-      <c r="K31" s="290"/>
-      <c r="L31" s="291"/>
+      <c r="C31" s="264"/>
+      <c r="D31" s="264"/>
+      <c r="E31" s="264"/>
+      <c r="F31" s="264"/>
+      <c r="G31" s="264"/>
+      <c r="H31" s="264"/>
+      <c r="I31" s="264"/>
+      <c r="J31" s="264"/>
+      <c r="K31" s="264"/>
+      <c r="L31" s="265"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="227"/>
-      <c r="B32" s="290" t="s">
+      <c r="B32" s="264" t="s">
         <v>209</v>
       </c>
-      <c r="C32" s="290"/>
-      <c r="D32" s="290"/>
-      <c r="E32" s="290"/>
-      <c r="F32" s="290"/>
-      <c r="G32" s="290"/>
-      <c r="H32" s="290"/>
-      <c r="I32" s="290"/>
-      <c r="J32" s="290"/>
-      <c r="K32" s="290"/>
-      <c r="L32" s="291"/>
+      <c r="C32" s="264"/>
+      <c r="D32" s="264"/>
+      <c r="E32" s="264"/>
+      <c r="F32" s="264"/>
+      <c r="G32" s="264"/>
+      <c r="H32" s="264"/>
+      <c r="I32" s="264"/>
+      <c r="J32" s="264"/>
+      <c r="K32" s="264"/>
+      <c r="L32" s="265"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="227"/>
-      <c r="B33" s="290" t="s">
+      <c r="B33" s="264" t="s">
         <v>210</v>
       </c>
-      <c r="C33" s="290"/>
-      <c r="D33" s="290"/>
-      <c r="E33" s="290"/>
-      <c r="F33" s="290"/>
-      <c r="G33" s="290"/>
-      <c r="H33" s="290"/>
-      <c r="I33" s="290"/>
-      <c r="J33" s="290"/>
-      <c r="K33" s="290"/>
-      <c r="L33" s="291"/>
+      <c r="C33" s="264"/>
+      <c r="D33" s="264"/>
+      <c r="E33" s="264"/>
+      <c r="F33" s="264"/>
+      <c r="G33" s="264"/>
+      <c r="H33" s="264"/>
+      <c r="I33" s="264"/>
+      <c r="J33" s="264"/>
+      <c r="K33" s="264"/>
+      <c r="L33" s="265"/>
       <c r="N33" s="106"/>
     </row>
     <row r="34" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="292" t="s">
+      <c r="A34" s="273" t="s">
         <v>216</v>
       </c>
-      <c r="B34" s="293"/>
-      <c r="C34" s="293"/>
-      <c r="D34" s="293"/>
-      <c r="E34" s="293"/>
-      <c r="F34" s="293"/>
-      <c r="G34" s="293"/>
-      <c r="H34" s="293"/>
-      <c r="I34" s="293"/>
-      <c r="J34" s="293"/>
-      <c r="K34" s="293"/>
-      <c r="L34" s="294"/>
+      <c r="B34" s="274"/>
+      <c r="C34" s="274"/>
+      <c r="D34" s="274"/>
+      <c r="E34" s="274"/>
+      <c r="F34" s="274"/>
+      <c r="G34" s="274"/>
+      <c r="H34" s="274"/>
+      <c r="I34" s="274"/>
+      <c r="J34" s="274"/>
+      <c r="K34" s="274"/>
+      <c r="L34" s="275"/>
       <c r="N34" s="106"/>
     </row>
     <row r="35" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="227">
         <v>1</v>
       </c>
-      <c r="B35" s="290" t="s">
+      <c r="B35" s="264" t="s">
         <v>211</v>
       </c>
-      <c r="C35" s="290"/>
-      <c r="D35" s="290"/>
-      <c r="E35" s="290"/>
-      <c r="F35" s="290"/>
-      <c r="G35" s="290"/>
-      <c r="H35" s="290"/>
-      <c r="I35" s="290"/>
-      <c r="J35" s="290"/>
-      <c r="K35" s="290"/>
-      <c r="L35" s="291"/>
+      <c r="C35" s="264"/>
+      <c r="D35" s="264"/>
+      <c r="E35" s="264"/>
+      <c r="F35" s="264"/>
+      <c r="G35" s="264"/>
+      <c r="H35" s="264"/>
+      <c r="I35" s="264"/>
+      <c r="J35" s="264"/>
+      <c r="K35" s="264"/>
+      <c r="L35" s="265"/>
       <c r="N35" s="106"/>
     </row>
     <row r="36" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="227"/>
-      <c r="B36" s="288" t="s">
+      <c r="B36" s="262" t="s">
         <v>339</v>
       </c>
-      <c r="C36" s="288"/>
-      <c r="D36" s="288"/>
-      <c r="E36" s="288"/>
-      <c r="F36" s="288"/>
-      <c r="G36" s="288"/>
-      <c r="H36" s="288"/>
-      <c r="I36" s="288"/>
-      <c r="J36" s="288"/>
-      <c r="K36" s="288"/>
-      <c r="L36" s="289"/>
+      <c r="C36" s="262"/>
+      <c r="D36" s="262"/>
+      <c r="E36" s="262"/>
+      <c r="F36" s="262"/>
+      <c r="G36" s="262"/>
+      <c r="H36" s="262"/>
+      <c r="I36" s="262"/>
+      <c r="J36" s="262"/>
+      <c r="K36" s="262"/>
+      <c r="L36" s="263"/>
       <c r="N36" s="106"/>
     </row>
     <row r="37" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="227">
         <v>2</v>
       </c>
-      <c r="B37" s="290" t="s">
+      <c r="B37" s="264" t="s">
         <v>332</v>
       </c>
-      <c r="C37" s="290"/>
-      <c r="D37" s="290"/>
-      <c r="E37" s="290"/>
-      <c r="F37" s="290"/>
-      <c r="G37" s="290"/>
-      <c r="H37" s="290"/>
-      <c r="I37" s="290"/>
-      <c r="J37" s="290"/>
-      <c r="K37" s="290"/>
-      <c r="L37" s="291"/>
+      <c r="C37" s="264"/>
+      <c r="D37" s="264"/>
+      <c r="E37" s="264"/>
+      <c r="F37" s="264"/>
+      <c r="G37" s="264"/>
+      <c r="H37" s="264"/>
+      <c r="I37" s="264"/>
+      <c r="J37" s="264"/>
+      <c r="K37" s="264"/>
+      <c r="L37" s="265"/>
       <c r="N37" s="106"/>
     </row>
     <row r="38" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="227">
         <v>3</v>
       </c>
-      <c r="B38" s="290" t="s">
+      <c r="B38" s="264" t="s">
         <v>321</v>
       </c>
-      <c r="C38" s="290"/>
-      <c r="D38" s="290"/>
-      <c r="E38" s="290"/>
-      <c r="F38" s="290"/>
-      <c r="G38" s="290"/>
-      <c r="H38" s="290"/>
-      <c r="I38" s="290"/>
-      <c r="J38" s="290"/>
-      <c r="K38" s="290"/>
-      <c r="L38" s="291"/>
+      <c r="C38" s="264"/>
+      <c r="D38" s="264"/>
+      <c r="E38" s="264"/>
+      <c r="F38" s="264"/>
+      <c r="G38" s="264"/>
+      <c r="H38" s="264"/>
+      <c r="I38" s="264"/>
+      <c r="J38" s="264"/>
+      <c r="K38" s="264"/>
+      <c r="L38" s="265"/>
       <c r="N38" s="106"/>
     </row>
     <row r="39" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="227">
         <v>4</v>
       </c>
-      <c r="B39" s="290" t="s">
+      <c r="B39" s="264" t="s">
         <v>340</v>
       </c>
-      <c r="C39" s="290"/>
-      <c r="D39" s="290"/>
-      <c r="E39" s="290"/>
-      <c r="F39" s="290"/>
-      <c r="G39" s="290"/>
-      <c r="H39" s="290"/>
-      <c r="I39" s="290"/>
-      <c r="J39" s="290"/>
-      <c r="K39" s="290"/>
-      <c r="L39" s="291"/>
+      <c r="C39" s="264"/>
+      <c r="D39" s="264"/>
+      <c r="E39" s="264"/>
+      <c r="F39" s="264"/>
+      <c r="G39" s="264"/>
+      <c r="H39" s="264"/>
+      <c r="I39" s="264"/>
+      <c r="J39" s="264"/>
+      <c r="K39" s="264"/>
+      <c r="L39" s="265"/>
       <c r="N39" s="106"/>
     </row>
     <row r="40" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="227">
         <v>5</v>
       </c>
-      <c r="B40" s="288" t="s">
+      <c r="B40" s="262" t="s">
         <v>322</v>
       </c>
-      <c r="C40" s="288"/>
-      <c r="D40" s="288"/>
-      <c r="E40" s="288"/>
-      <c r="F40" s="288"/>
-      <c r="G40" s="288"/>
-      <c r="H40" s="288"/>
-      <c r="I40" s="288"/>
-      <c r="J40" s="288"/>
-      <c r="K40" s="288"/>
-      <c r="L40" s="289"/>
+      <c r="C40" s="262"/>
+      <c r="D40" s="262"/>
+      <c r="E40" s="262"/>
+      <c r="F40" s="262"/>
+      <c r="G40" s="262"/>
+      <c r="H40" s="262"/>
+      <c r="I40" s="262"/>
+      <c r="J40" s="262"/>
+      <c r="K40" s="262"/>
+      <c r="L40" s="263"/>
       <c r="N40" s="106"/>
     </row>
     <row r="41" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="227">
         <v>6</v>
       </c>
-      <c r="B41" s="288" t="s">
+      <c r="B41" s="262" t="s">
         <v>327</v>
       </c>
-      <c r="C41" s="288"/>
-      <c r="D41" s="288"/>
-      <c r="E41" s="288"/>
-      <c r="F41" s="288"/>
-      <c r="G41" s="288"/>
-      <c r="H41" s="288"/>
-      <c r="I41" s="288"/>
-      <c r="J41" s="288"/>
-      <c r="K41" s="288"/>
-      <c r="L41" s="289"/>
+      <c r="C41" s="262"/>
+      <c r="D41" s="262"/>
+      <c r="E41" s="262"/>
+      <c r="F41" s="262"/>
+      <c r="G41" s="262"/>
+      <c r="H41" s="262"/>
+      <c r="I41" s="262"/>
+      <c r="J41" s="262"/>
+      <c r="K41" s="262"/>
+      <c r="L41" s="263"/>
       <c r="N41" s="106"/>
     </row>
     <row r="42" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="227">
         <v>7</v>
       </c>
-      <c r="B42" s="290" t="s">
+      <c r="B42" s="264" t="s">
         <v>323</v>
       </c>
-      <c r="C42" s="290"/>
-      <c r="D42" s="290"/>
-      <c r="E42" s="290"/>
-      <c r="F42" s="290"/>
-      <c r="G42" s="290"/>
-      <c r="H42" s="290"/>
-      <c r="I42" s="290"/>
-      <c r="J42" s="290"/>
-      <c r="K42" s="290"/>
-      <c r="L42" s="291"/>
+      <c r="C42" s="264"/>
+      <c r="D42" s="264"/>
+      <c r="E42" s="264"/>
+      <c r="F42" s="264"/>
+      <c r="G42" s="264"/>
+      <c r="H42" s="264"/>
+      <c r="I42" s="264"/>
+      <c r="J42" s="264"/>
+      <c r="K42" s="264"/>
+      <c r="L42" s="265"/>
     </row>
     <row r="43" spans="1:14" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="227"/>
@@ -15974,56 +15974,56 @@
       <c r="L43" s="229"/>
     </row>
     <row r="44" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="292" t="s">
+      <c r="A44" s="273" t="s">
         <v>326</v>
       </c>
-      <c r="B44" s="293"/>
-      <c r="C44" s="293"/>
-      <c r="D44" s="293"/>
-      <c r="E44" s="293"/>
-      <c r="F44" s="293"/>
-      <c r="G44" s="293"/>
-      <c r="H44" s="293"/>
-      <c r="I44" s="293"/>
-      <c r="J44" s="293"/>
-      <c r="K44" s="293"/>
-      <c r="L44" s="294"/>
+      <c r="B44" s="274"/>
+      <c r="C44" s="274"/>
+      <c r="D44" s="274"/>
+      <c r="E44" s="274"/>
+      <c r="F44" s="274"/>
+      <c r="G44" s="274"/>
+      <c r="H44" s="274"/>
+      <c r="I44" s="274"/>
+      <c r="J44" s="274"/>
+      <c r="K44" s="274"/>
+      <c r="L44" s="275"/>
     </row>
     <row r="45" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="230" t="s">
         <v>324</v>
       </c>
-      <c r="B45" s="290" t="s">
+      <c r="B45" s="264" t="s">
         <v>212</v>
       </c>
-      <c r="C45" s="290"/>
-      <c r="D45" s="290"/>
-      <c r="E45" s="290"/>
-      <c r="F45" s="290"/>
-      <c r="G45" s="290"/>
-      <c r="H45" s="290"/>
-      <c r="I45" s="290"/>
-      <c r="J45" s="290"/>
-      <c r="K45" s="290"/>
-      <c r="L45" s="291"/>
+      <c r="C45" s="264"/>
+      <c r="D45" s="264"/>
+      <c r="E45" s="264"/>
+      <c r="F45" s="264"/>
+      <c r="G45" s="264"/>
+      <c r="H45" s="264"/>
+      <c r="I45" s="264"/>
+      <c r="J45" s="264"/>
+      <c r="K45" s="264"/>
+      <c r="L45" s="265"/>
     </row>
     <row r="46" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="231" t="s">
         <v>325</v>
       </c>
-      <c r="B46" s="298" t="s">
+      <c r="B46" s="266" t="s">
         <v>328</v>
       </c>
-      <c r="C46" s="298"/>
-      <c r="D46" s="298"/>
-      <c r="E46" s="298"/>
-      <c r="F46" s="298"/>
-      <c r="G46" s="298"/>
-      <c r="H46" s="298"/>
-      <c r="I46" s="298"/>
-      <c r="J46" s="298"/>
-      <c r="K46" s="298"/>
-      <c r="L46" s="299"/>
+      <c r="C46" s="266"/>
+      <c r="D46" s="266"/>
+      <c r="E46" s="266"/>
+      <c r="F46" s="266"/>
+      <c r="G46" s="266"/>
+      <c r="H46" s="266"/>
+      <c r="I46" s="266"/>
+      <c r="J46" s="266"/>
+      <c r="K46" s="266"/>
+      <c r="L46" s="267"/>
     </row>
     <row r="47" spans="1:14" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="160"/>
@@ -16040,20 +16040,20 @@
       <c r="L47" s="113"/>
     </row>
     <row r="48" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="300" t="s">
+      <c r="A48" s="268" t="s">
         <v>240</v>
       </c>
-      <c r="B48" s="301"/>
-      <c r="C48" s="301"/>
-      <c r="D48" s="301"/>
-      <c r="E48" s="301"/>
-      <c r="F48" s="301"/>
-      <c r="G48" s="301"/>
-      <c r="H48" s="301"/>
-      <c r="I48" s="301"/>
-      <c r="J48" s="301"/>
-      <c r="K48" s="301"/>
-      <c r="L48" s="302"/>
+      <c r="B48" s="269"/>
+      <c r="C48" s="269"/>
+      <c r="D48" s="269"/>
+      <c r="E48" s="269"/>
+      <c r="F48" s="269"/>
+      <c r="G48" s="269"/>
+      <c r="H48" s="269"/>
+      <c r="I48" s="269"/>
+      <c r="J48" s="269"/>
+      <c r="K48" s="269"/>
+      <c r="L48" s="270"/>
     </row>
     <row r="49" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="234" t="s">
@@ -16141,90 +16141,90 @@
       <c r="B54" s="168" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="273" t="s">
+      <c r="C54" s="271" t="s">
         <v>312</v>
       </c>
-      <c r="D54" s="273"/>
-      <c r="E54" s="273"/>
-      <c r="F54" s="273"/>
-      <c r="G54" s="273"/>
-      <c r="H54" s="273"/>
-      <c r="I54" s="273"/>
-      <c r="J54" s="273"/>
-      <c r="K54" s="273"/>
-      <c r="L54" s="274"/>
+      <c r="D54" s="271"/>
+      <c r="E54" s="271"/>
+      <c r="F54" s="271"/>
+      <c r="G54" s="271"/>
+      <c r="H54" s="271"/>
+      <c r="I54" s="271"/>
+      <c r="J54" s="271"/>
+      <c r="K54" s="271"/>
+      <c r="L54" s="272"/>
     </row>
     <row r="55" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="167"/>
       <c r="B55" s="168" t="s">
         <v>313</v>
       </c>
-      <c r="C55" s="273" t="s">
+      <c r="C55" s="271" t="s">
         <v>314</v>
       </c>
-      <c r="D55" s="273"/>
-      <c r="E55" s="273"/>
-      <c r="F55" s="273"/>
-      <c r="G55" s="273"/>
-      <c r="H55" s="273"/>
-      <c r="I55" s="273"/>
-      <c r="J55" s="273"/>
-      <c r="K55" s="273"/>
-      <c r="L55" s="274"/>
+      <c r="D55" s="271"/>
+      <c r="E55" s="271"/>
+      <c r="F55" s="271"/>
+      <c r="G55" s="271"/>
+      <c r="H55" s="271"/>
+      <c r="I55" s="271"/>
+      <c r="J55" s="271"/>
+      <c r="K55" s="271"/>
+      <c r="L55" s="272"/>
     </row>
     <row r="56" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="167"/>
       <c r="B56" s="168" t="s">
         <v>382</v>
       </c>
-      <c r="C56" s="273" t="s">
+      <c r="C56" s="271" t="s">
         <v>383</v>
       </c>
-      <c r="D56" s="273"/>
-      <c r="E56" s="273"/>
-      <c r="F56" s="273"/>
-      <c r="G56" s="273"/>
-      <c r="H56" s="273"/>
-      <c r="I56" s="273"/>
-      <c r="J56" s="273"/>
-      <c r="K56" s="273"/>
-      <c r="L56" s="274"/>
+      <c r="D56" s="271"/>
+      <c r="E56" s="271"/>
+      <c r="F56" s="271"/>
+      <c r="G56" s="271"/>
+      <c r="H56" s="271"/>
+      <c r="I56" s="271"/>
+      <c r="J56" s="271"/>
+      <c r="K56" s="271"/>
+      <c r="L56" s="272"/>
     </row>
     <row r="57" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="167"/>
       <c r="B57" s="168" t="s">
         <v>138</v>
       </c>
-      <c r="C57" s="273" t="s">
+      <c r="C57" s="271" t="s">
         <v>139</v>
       </c>
-      <c r="D57" s="273"/>
-      <c r="E57" s="273"/>
-      <c r="F57" s="273"/>
-      <c r="G57" s="273"/>
-      <c r="H57" s="273"/>
-      <c r="I57" s="273"/>
-      <c r="J57" s="273"/>
-      <c r="K57" s="273"/>
-      <c r="L57" s="274"/>
+      <c r="D57" s="271"/>
+      <c r="E57" s="271"/>
+      <c r="F57" s="271"/>
+      <c r="G57" s="271"/>
+      <c r="H57" s="271"/>
+      <c r="I57" s="271"/>
+      <c r="J57" s="271"/>
+      <c r="K57" s="271"/>
+      <c r="L57" s="272"/>
     </row>
     <row r="58" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="167"/>
       <c r="B58" s="168" t="s">
         <v>238</v>
       </c>
-      <c r="C58" s="273" t="s">
+      <c r="C58" s="271" t="s">
         <v>239</v>
       </c>
-      <c r="D58" s="273"/>
-      <c r="E58" s="273"/>
-      <c r="F58" s="273"/>
-      <c r="G58" s="273"/>
-      <c r="H58" s="273"/>
-      <c r="I58" s="273"/>
-      <c r="J58" s="273"/>
-      <c r="K58" s="273"/>
-      <c r="L58" s="274"/>
+      <c r="D58" s="271"/>
+      <c r="E58" s="271"/>
+      <c r="F58" s="271"/>
+      <c r="G58" s="271"/>
+      <c r="H58" s="271"/>
+      <c r="I58" s="271"/>
+      <c r="J58" s="271"/>
+      <c r="K58" s="271"/>
+      <c r="L58" s="272"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="167"/>
@@ -16249,18 +16249,18 @@
       <c r="B60" s="168" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="273" t="s">
+      <c r="C60" s="271" t="s">
         <v>316</v>
       </c>
-      <c r="D60" s="273"/>
-      <c r="E60" s="273"/>
-      <c r="F60" s="273"/>
-      <c r="G60" s="273"/>
-      <c r="H60" s="273"/>
-      <c r="I60" s="273"/>
-      <c r="J60" s="273"/>
-      <c r="K60" s="273"/>
-      <c r="L60" s="274"/>
+      <c r="D60" s="271"/>
+      <c r="E60" s="271"/>
+      <c r="F60" s="271"/>
+      <c r="G60" s="271"/>
+      <c r="H60" s="271"/>
+      <c r="I60" s="271"/>
+      <c r="J60" s="271"/>
+      <c r="K60" s="271"/>
+      <c r="L60" s="272"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="167"/>
@@ -16360,25 +16360,56 @@
       </c>
     </row>
     <row r="78" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="297" t="s">
+      <c r="A78" s="261" t="s">
         <v>398</v>
       </c>
-      <c r="B78" s="297"/>
-      <c r="C78" s="297"/>
-      <c r="D78" s="297"/>
-      <c r="E78" s="297"/>
-      <c r="F78" s="297"/>
-      <c r="G78" s="297"/>
-      <c r="H78" s="297"/>
-      <c r="I78" s="297"/>
-      <c r="J78" s="297"/>
-      <c r="K78" s="297"/>
-      <c r="L78" s="297"/>
+      <c r="B78" s="261"/>
+      <c r="C78" s="261"/>
+      <c r="D78" s="261"/>
+      <c r="E78" s="261"/>
+      <c r="F78" s="261"/>
+      <c r="G78" s="261"/>
+      <c r="H78" s="261"/>
+      <c r="I78" s="261"/>
+      <c r="J78" s="261"/>
+      <c r="K78" s="261"/>
+      <c r="L78" s="261"/>
     </row>
     <row r="83" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="84" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="B40:L40"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B30:L30"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B39:L39"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="B13:L13"/>
     <mergeCell ref="B14:L14"/>
@@ -16395,37 +16426,6 @@
     <mergeCell ref="C55:L55"/>
     <mergeCell ref="C60:L60"/>
     <mergeCell ref="A44:L44"/>
-    <mergeCell ref="C56:L56"/>
-    <mergeCell ref="B40:L40"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B8:L8"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="B11:L11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A67" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -38190,12 +38190,12 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:D14"/>
+      <selection activeCell="A18" sqref="A18:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.08984375" customWidth="1"/>
+    <col min="1" max="1" width="28.6328125" customWidth="1"/>
     <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="20.1796875" customWidth="1"/>
@@ -38515,16 +38515,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="339" t="e">
+      <c r="A1" s="340" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="339"/>
-      <c r="C1" s="339"/>
-      <c r="D1" s="339"/>
-      <c r="E1" s="339"/>
-      <c r="F1" s="339"/>
-      <c r="G1" s="339"/>
+      <c r="B1" s="340"/>
+      <c r="C1" s="340"/>
+      <c r="D1" s="340"/>
+      <c r="E1" s="340"/>
+      <c r="F1" s="340"/>
+      <c r="G1" s="340"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -38633,11 +38633,11 @@
         <v>80</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="340"/>
-      <c r="D10" s="340"/>
-      <c r="E10" s="340"/>
-      <c r="F10" s="340"/>
-      <c r="G10" s="340"/>
+      <c r="C10" s="339"/>
+      <c r="D10" s="339"/>
+      <c r="E10" s="339"/>
+      <c r="F10" s="339"/>
+      <c r="G10" s="339"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -39900,6 +39900,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -39907,12 +39913,6 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>

</xml_diff>

<commit_message>
Update version in Excel model file
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7D8118-AA92-43ED-A44D-5411C0203CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2867F2C-3146-420C-8131-53A63EFA3A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="408">
   <si>
     <t>Year 1</t>
   </si>
@@ -2063,13 +2063,16 @@
     <t>Add images of key ideas to ReadMe</t>
   </si>
   <si>
-    <t>Add context of recent user water use</t>
-  </si>
-  <si>
     <t>CEE 6490 students; Akbar</t>
   </si>
   <si>
     <t>Dec, 2024</t>
+  </si>
+  <si>
+    <t>1.4.3</t>
+  </si>
+  <si>
+    <t>Add recent water use in Model Guide</t>
   </si>
 </sst>
 </file>
@@ -3398,69 +3401,6 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3515,6 +3455,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3547,6 +3493,63 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3650,11 +3653,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -15236,20 +15239,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="279" t="s">
+      <c r="A1" s="258" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="279"/>
-      <c r="C1" s="279"/>
-      <c r="D1" s="279"/>
-      <c r="E1" s="279"/>
-      <c r="F1" s="279"/>
-      <c r="G1" s="279"/>
-      <c r="H1" s="279"/>
-      <c r="I1" s="279"/>
-      <c r="J1" s="279"/>
-      <c r="K1" s="279"/>
-      <c r="L1" s="279"/>
+      <c r="B1" s="258"/>
+      <c r="C1" s="258"/>
+      <c r="D1" s="258"/>
+      <c r="E1" s="258"/>
+      <c r="F1" s="258"/>
+      <c r="G1" s="258"/>
+      <c r="H1" s="258"/>
+      <c r="I1" s="258"/>
+      <c r="J1" s="258"/>
+      <c r="K1" s="258"/>
+      <c r="L1" s="258"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -15275,41 +15278,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="280" t="s">
+      <c r="A4" s="259" t="s">
         <v>351</v>
       </c>
-      <c r="B4" s="281"/>
-      <c r="C4" s="281"/>
-      <c r="D4" s="281"/>
-      <c r="E4" s="281"/>
-      <c r="F4" s="281"/>
-      <c r="G4" s="281"/>
-      <c r="H4" s="281"/>
-      <c r="I4" s="281"/>
-      <c r="J4" s="281"/>
-      <c r="K4" s="281"/>
-      <c r="L4" s="282"/>
-      <c r="N4" s="283"/>
-      <c r="O4" s="283"/>
-      <c r="P4" s="283"/>
-      <c r="Q4" s="283"/>
-      <c r="R4" s="283"/>
+      <c r="B4" s="260"/>
+      <c r="C4" s="260"/>
+      <c r="D4" s="260"/>
+      <c r="E4" s="260"/>
+      <c r="F4" s="260"/>
+      <c r="G4" s="260"/>
+      <c r="H4" s="260"/>
+      <c r="I4" s="260"/>
+      <c r="J4" s="260"/>
+      <c r="K4" s="260"/>
+      <c r="L4" s="261"/>
+      <c r="N4" s="262"/>
+      <c r="O4" s="262"/>
+      <c r="P4" s="262"/>
+      <c r="Q4" s="262"/>
+      <c r="R4" s="262"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="284" t="s">
+      <c r="A5" s="263" t="s">
         <v>334</v>
       </c>
-      <c r="B5" s="285"/>
-      <c r="C5" s="285"/>
-      <c r="D5" s="285"/>
-      <c r="E5" s="285"/>
-      <c r="F5" s="285"/>
-      <c r="G5" s="285"/>
-      <c r="H5" s="285"/>
-      <c r="I5" s="285"/>
-      <c r="J5" s="285"/>
-      <c r="K5" s="285"/>
-      <c r="L5" s="286"/>
+      <c r="B5" s="264"/>
+      <c r="C5" s="264"/>
+      <c r="D5" s="264"/>
+      <c r="E5" s="264"/>
+      <c r="F5" s="264"/>
+      <c r="G5" s="264"/>
+      <c r="H5" s="264"/>
+      <c r="I5" s="264"/>
+      <c r="J5" s="264"/>
+      <c r="K5" s="264"/>
+      <c r="L5" s="265"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15317,20 +15320,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="284" t="s">
+      <c r="A6" s="263" t="s">
         <v>352</v>
       </c>
-      <c r="B6" s="285"/>
-      <c r="C6" s="285"/>
-      <c r="D6" s="285"/>
-      <c r="E6" s="285"/>
-      <c r="F6" s="285"/>
-      <c r="G6" s="285"/>
-      <c r="H6" s="285"/>
-      <c r="I6" s="285"/>
-      <c r="J6" s="285"/>
-      <c r="K6" s="285"/>
-      <c r="L6" s="286"/>
+      <c r="B6" s="264"/>
+      <c r="C6" s="264"/>
+      <c r="D6" s="264"/>
+      <c r="E6" s="264"/>
+      <c r="F6" s="264"/>
+      <c r="G6" s="264"/>
+      <c r="H6" s="264"/>
+      <c r="I6" s="264"/>
+      <c r="J6" s="264"/>
+      <c r="K6" s="264"/>
+      <c r="L6" s="265"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15339,19 +15342,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="232"/>
-      <c r="B7" s="285" t="s">
+      <c r="B7" s="264" t="s">
         <v>353</v>
       </c>
-      <c r="C7" s="285"/>
-      <c r="D7" s="285"/>
-      <c r="E7" s="285"/>
-      <c r="F7" s="285"/>
-      <c r="G7" s="285"/>
-      <c r="H7" s="285"/>
-      <c r="I7" s="285"/>
-      <c r="J7" s="285"/>
-      <c r="K7" s="285"/>
-      <c r="L7" s="286"/>
+      <c r="C7" s="264"/>
+      <c r="D7" s="264"/>
+      <c r="E7" s="264"/>
+      <c r="F7" s="264"/>
+      <c r="G7" s="264"/>
+      <c r="H7" s="264"/>
+      <c r="I7" s="264"/>
+      <c r="J7" s="264"/>
+      <c r="K7" s="264"/>
+      <c r="L7" s="265"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15360,19 +15363,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="233"/>
-      <c r="B8" s="300" t="s">
+      <c r="B8" s="281" t="s">
         <v>354</v>
       </c>
-      <c r="C8" s="300"/>
-      <c r="D8" s="300"/>
-      <c r="E8" s="300"/>
-      <c r="F8" s="300"/>
-      <c r="G8" s="300"/>
-      <c r="H8" s="300"/>
-      <c r="I8" s="300"/>
-      <c r="J8" s="300"/>
-      <c r="K8" s="300"/>
-      <c r="L8" s="301"/>
+      <c r="C8" s="281"/>
+      <c r="D8" s="281"/>
+      <c r="E8" s="281"/>
+      <c r="F8" s="281"/>
+      <c r="G8" s="281"/>
+      <c r="H8" s="281"/>
+      <c r="I8" s="281"/>
+      <c r="J8" s="281"/>
+      <c r="K8" s="281"/>
+      <c r="L8" s="282"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15394,38 +15397,38 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="302" t="s">
+      <c r="A10" s="283" t="s">
         <v>389</v>
       </c>
-      <c r="B10" s="303"/>
-      <c r="C10" s="303"/>
-      <c r="D10" s="303"/>
-      <c r="E10" s="303"/>
-      <c r="F10" s="303"/>
-      <c r="G10" s="303"/>
-      <c r="H10" s="303"/>
-      <c r="I10" s="303"/>
-      <c r="J10" s="303"/>
-      <c r="K10" s="303"/>
-      <c r="L10" s="304"/>
+      <c r="B10" s="284"/>
+      <c r="C10" s="284"/>
+      <c r="D10" s="284"/>
+      <c r="E10" s="284"/>
+      <c r="F10" s="284"/>
+      <c r="G10" s="284"/>
+      <c r="H10" s="284"/>
+      <c r="I10" s="284"/>
+      <c r="J10" s="284"/>
+      <c r="K10" s="284"/>
+      <c r="L10" s="285"/>
     </row>
     <row r="11" spans="1:18" s="58" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="253" t="s">
         <v>390</v>
       </c>
-      <c r="B11" s="257" t="s">
+      <c r="B11" s="286" t="s">
         <v>393</v>
       </c>
-      <c r="C11" s="257"/>
-      <c r="D11" s="257"/>
-      <c r="E11" s="257"/>
-      <c r="F11" s="257"/>
-      <c r="G11" s="257"/>
-      <c r="H11" s="257"/>
-      <c r="I11" s="257"/>
-      <c r="J11" s="257"/>
-      <c r="K11" s="257"/>
-      <c r="L11" s="258"/>
+      <c r="C11" s="286"/>
+      <c r="D11" s="286"/>
+      <c r="E11" s="286"/>
+      <c r="F11" s="286"/>
+      <c r="G11" s="286"/>
+      <c r="H11" s="286"/>
+      <c r="I11" s="286"/>
+      <c r="J11" s="286"/>
+      <c r="K11" s="286"/>
+      <c r="L11" s="287"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="161.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="245"/>
@@ -15445,51 +15448,51 @@
       <c r="A13" s="253" t="s">
         <v>391</v>
       </c>
-      <c r="B13" s="257" t="s">
+      <c r="B13" s="286" t="s">
         <v>394</v>
       </c>
-      <c r="C13" s="257"/>
-      <c r="D13" s="257"/>
-      <c r="E13" s="257"/>
-      <c r="F13" s="257"/>
-      <c r="G13" s="257"/>
-      <c r="H13" s="257"/>
-      <c r="I13" s="257"/>
-      <c r="J13" s="257"/>
-      <c r="K13" s="257"/>
-      <c r="L13" s="258"/>
+      <c r="C13" s="286"/>
+      <c r="D13" s="286"/>
+      <c r="E13" s="286"/>
+      <c r="F13" s="286"/>
+      <c r="G13" s="286"/>
+      <c r="H13" s="286"/>
+      <c r="I13" s="286"/>
+      <c r="J13" s="286"/>
+      <c r="K13" s="286"/>
+      <c r="L13" s="287"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="90.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="245"/>
-      <c r="B14" s="259"/>
-      <c r="C14" s="259"/>
-      <c r="D14" s="259"/>
-      <c r="E14" s="259"/>
-      <c r="F14" s="259"/>
-      <c r="G14" s="259"/>
-      <c r="H14" s="259"/>
-      <c r="I14" s="259"/>
-      <c r="J14" s="259"/>
-      <c r="K14" s="259"/>
-      <c r="L14" s="260"/>
+      <c r="B14" s="297"/>
+      <c r="C14" s="297"/>
+      <c r="D14" s="297"/>
+      <c r="E14" s="297"/>
+      <c r="F14" s="297"/>
+      <c r="G14" s="297"/>
+      <c r="H14" s="297"/>
+      <c r="I14" s="297"/>
+      <c r="J14" s="297"/>
+      <c r="K14" s="297"/>
+      <c r="L14" s="298"/>
     </row>
     <row r="15" spans="1:18" s="58" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="253" t="s">
         <v>392</v>
       </c>
-      <c r="B15" s="257" t="s">
+      <c r="B15" s="286" t="s">
         <v>395</v>
       </c>
-      <c r="C15" s="257"/>
-      <c r="D15" s="257"/>
-      <c r="E15" s="257"/>
-      <c r="F15" s="257"/>
-      <c r="G15" s="257"/>
-      <c r="H15" s="257"/>
-      <c r="I15" s="257"/>
-      <c r="J15" s="257"/>
-      <c r="K15" s="257"/>
-      <c r="L15" s="258"/>
+      <c r="C15" s="286"/>
+      <c r="D15" s="286"/>
+      <c r="E15" s="286"/>
+      <c r="F15" s="286"/>
+      <c r="G15" s="286"/>
+      <c r="H15" s="286"/>
+      <c r="I15" s="286"/>
+      <c r="J15" s="286"/>
+      <c r="K15" s="286"/>
+      <c r="L15" s="287"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="245"/>
@@ -15506,12 +15509,12 @@
       <c r="L16" s="252"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="255" t="s">
+      <c r="A17" s="295" t="s">
         <v>400</v>
       </c>
-      <c r="B17" s="256"/>
-      <c r="C17" s="256"/>
-      <c r="D17" s="256"/>
+      <c r="B17" s="296"/>
+      <c r="C17" s="296"/>
+      <c r="D17" s="296"/>
       <c r="E17" s="250" t="s">
         <v>401</v>
       </c>
@@ -15538,84 +15541,84 @@
       <c r="L18" s="113"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="287" t="s">
+      <c r="A19" s="266" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="288"/>
-      <c r="C19" s="288"/>
-      <c r="D19" s="288"/>
-      <c r="E19" s="288"/>
-      <c r="F19" s="288"/>
-      <c r="G19" s="288"/>
-      <c r="H19" s="288"/>
-      <c r="I19" s="288"/>
-      <c r="J19" s="288"/>
-      <c r="K19" s="288"/>
-      <c r="L19" s="289"/>
+      <c r="B19" s="267"/>
+      <c r="C19" s="267"/>
+      <c r="D19" s="267"/>
+      <c r="E19" s="267"/>
+      <c r="F19" s="267"/>
+      <c r="G19" s="267"/>
+      <c r="H19" s="267"/>
+      <c r="I19" s="267"/>
+      <c r="J19" s="267"/>
+      <c r="K19" s="267"/>
+      <c r="L19" s="268"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="290" t="s">
+      <c r="A20" s="269" t="s">
         <v>335</v>
       </c>
-      <c r="B20" s="291"/>
-      <c r="C20" s="291"/>
-      <c r="D20" s="291"/>
-      <c r="E20" s="291"/>
-      <c r="F20" s="291"/>
-      <c r="G20" s="291"/>
-      <c r="H20" s="291"/>
-      <c r="I20" s="291"/>
-      <c r="J20" s="291"/>
-      <c r="K20" s="291"/>
-      <c r="L20" s="292"/>
+      <c r="B20" s="270"/>
+      <c r="C20" s="270"/>
+      <c r="D20" s="270"/>
+      <c r="E20" s="270"/>
+      <c r="F20" s="270"/>
+      <c r="G20" s="270"/>
+      <c r="H20" s="270"/>
+      <c r="I20" s="270"/>
+      <c r="J20" s="270"/>
+      <c r="K20" s="270"/>
+      <c r="L20" s="271"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="293" t="s">
+      <c r="A21" s="272" t="s">
         <v>336</v>
       </c>
-      <c r="B21" s="271"/>
-      <c r="C21" s="271"/>
-      <c r="D21" s="271"/>
-      <c r="E21" s="271"/>
-      <c r="F21" s="271"/>
-      <c r="G21" s="271"/>
-      <c r="H21" s="271"/>
-      <c r="I21" s="271"/>
-      <c r="J21" s="271"/>
-      <c r="K21" s="271"/>
-      <c r="L21" s="272"/>
+      <c r="B21" s="273"/>
+      <c r="C21" s="273"/>
+      <c r="D21" s="273"/>
+      <c r="E21" s="273"/>
+      <c r="F21" s="273"/>
+      <c r="G21" s="273"/>
+      <c r="H21" s="273"/>
+      <c r="I21" s="273"/>
+      <c r="J21" s="273"/>
+      <c r="K21" s="273"/>
+      <c r="L21" s="274"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="293" t="s">
+      <c r="A22" s="272" t="s">
         <v>206</v>
       </c>
-      <c r="B22" s="271"/>
-      <c r="C22" s="271"/>
-      <c r="D22" s="271"/>
-      <c r="E22" s="271"/>
-      <c r="F22" s="271"/>
-      <c r="G22" s="271"/>
-      <c r="H22" s="271"/>
-      <c r="I22" s="271"/>
-      <c r="J22" s="271"/>
-      <c r="K22" s="271"/>
-      <c r="L22" s="272"/>
+      <c r="B22" s="273"/>
+      <c r="C22" s="273"/>
+      <c r="D22" s="273"/>
+      <c r="E22" s="273"/>
+      <c r="F22" s="273"/>
+      <c r="G22" s="273"/>
+      <c r="H22" s="273"/>
+      <c r="I22" s="273"/>
+      <c r="J22" s="273"/>
+      <c r="K22" s="273"/>
+      <c r="L22" s="274"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="294" t="s">
+      <c r="A23" s="275" t="s">
         <v>337</v>
       </c>
-      <c r="B23" s="295"/>
-      <c r="C23" s="295"/>
-      <c r="D23" s="295"/>
-      <c r="E23" s="295"/>
-      <c r="F23" s="295"/>
-      <c r="G23" s="295"/>
-      <c r="H23" s="295"/>
-      <c r="I23" s="295"/>
-      <c r="J23" s="295"/>
-      <c r="K23" s="295"/>
-      <c r="L23" s="296"/>
+      <c r="B23" s="276"/>
+      <c r="C23" s="276"/>
+      <c r="D23" s="276"/>
+      <c r="E23" s="276"/>
+      <c r="F23" s="276"/>
+      <c r="G23" s="276"/>
+      <c r="H23" s="276"/>
+      <c r="I23" s="276"/>
+      <c r="J23" s="276"/>
+      <c r="K23" s="276"/>
+      <c r="L23" s="277"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="113"/>
@@ -15632,332 +15635,332 @@
       <c r="L24" s="113"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="297" t="s">
+      <c r="A25" s="278" t="s">
         <v>333</v>
       </c>
-      <c r="B25" s="298"/>
-      <c r="C25" s="298"/>
-      <c r="D25" s="298"/>
-      <c r="E25" s="298"/>
-      <c r="F25" s="298"/>
-      <c r="G25" s="298"/>
-      <c r="H25" s="298"/>
-      <c r="I25" s="298"/>
-      <c r="J25" s="298"/>
-      <c r="K25" s="298"/>
-      <c r="L25" s="299"/>
+      <c r="B25" s="279"/>
+      <c r="C25" s="279"/>
+      <c r="D25" s="279"/>
+      <c r="E25" s="279"/>
+      <c r="F25" s="279"/>
+      <c r="G25" s="279"/>
+      <c r="H25" s="279"/>
+      <c r="I25" s="279"/>
+      <c r="J25" s="279"/>
+      <c r="K25" s="279"/>
+      <c r="L25" s="280"/>
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="276" t="s">
+      <c r="A26" s="255" t="s">
         <v>215</v>
       </c>
-      <c r="B26" s="277"/>
-      <c r="C26" s="277"/>
-      <c r="D26" s="277"/>
-      <c r="E26" s="277"/>
-      <c r="F26" s="277"/>
-      <c r="G26" s="277"/>
-      <c r="H26" s="277"/>
-      <c r="I26" s="277"/>
-      <c r="J26" s="277"/>
-      <c r="K26" s="277"/>
-      <c r="L26" s="278"/>
+      <c r="B26" s="256"/>
+      <c r="C26" s="256"/>
+      <c r="D26" s="256"/>
+      <c r="E26" s="256"/>
+      <c r="F26" s="256"/>
+      <c r="G26" s="256"/>
+      <c r="H26" s="256"/>
+      <c r="I26" s="256"/>
+      <c r="J26" s="256"/>
+      <c r="K26" s="256"/>
+      <c r="L26" s="257"/>
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="227">
         <v>1</v>
       </c>
-      <c r="B27" s="264" t="s">
+      <c r="B27" s="290" t="s">
         <v>214</v>
       </c>
-      <c r="C27" s="264"/>
-      <c r="D27" s="264"/>
-      <c r="E27" s="264"/>
-      <c r="F27" s="264"/>
-      <c r="G27" s="264"/>
-      <c r="H27" s="264"/>
-      <c r="I27" s="264"/>
-      <c r="J27" s="264"/>
-      <c r="K27" s="264"/>
-      <c r="L27" s="265"/>
+      <c r="C27" s="290"/>
+      <c r="D27" s="290"/>
+      <c r="E27" s="290"/>
+      <c r="F27" s="290"/>
+      <c r="G27" s="290"/>
+      <c r="H27" s="290"/>
+      <c r="I27" s="290"/>
+      <c r="J27" s="290"/>
+      <c r="K27" s="290"/>
+      <c r="L27" s="291"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="227">
         <v>2</v>
       </c>
-      <c r="B28" s="264" t="s">
+      <c r="B28" s="290" t="s">
         <v>329</v>
       </c>
-      <c r="C28" s="264"/>
-      <c r="D28" s="264"/>
-      <c r="E28" s="264"/>
-      <c r="F28" s="264"/>
-      <c r="G28" s="264"/>
-      <c r="H28" s="264"/>
-      <c r="I28" s="264"/>
-      <c r="J28" s="264"/>
-      <c r="K28" s="264"/>
-      <c r="L28" s="265"/>
+      <c r="C28" s="290"/>
+      <c r="D28" s="290"/>
+      <c r="E28" s="290"/>
+      <c r="F28" s="290"/>
+      <c r="G28" s="290"/>
+      <c r="H28" s="290"/>
+      <c r="I28" s="290"/>
+      <c r="J28" s="290"/>
+      <c r="K28" s="290"/>
+      <c r="L28" s="291"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="227">
         <v>3</v>
       </c>
-      <c r="B29" s="264" t="s">
+      <c r="B29" s="290" t="s">
         <v>207</v>
       </c>
-      <c r="C29" s="264"/>
-      <c r="D29" s="264"/>
-      <c r="E29" s="264"/>
-      <c r="F29" s="264"/>
-      <c r="G29" s="264"/>
-      <c r="H29" s="264"/>
-      <c r="I29" s="264"/>
-      <c r="J29" s="264"/>
-      <c r="K29" s="264"/>
-      <c r="L29" s="265"/>
+      <c r="C29" s="290"/>
+      <c r="D29" s="290"/>
+      <c r="E29" s="290"/>
+      <c r="F29" s="290"/>
+      <c r="G29" s="290"/>
+      <c r="H29" s="290"/>
+      <c r="I29" s="290"/>
+      <c r="J29" s="290"/>
+      <c r="K29" s="290"/>
+      <c r="L29" s="291"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="227">
         <v>4</v>
       </c>
-      <c r="B30" s="264" t="s">
+      <c r="B30" s="290" t="s">
         <v>338</v>
       </c>
-      <c r="C30" s="264"/>
-      <c r="D30" s="264"/>
-      <c r="E30" s="264"/>
-      <c r="F30" s="264"/>
-      <c r="G30" s="264"/>
-      <c r="H30" s="264"/>
-      <c r="I30" s="264"/>
-      <c r="J30" s="264"/>
-      <c r="K30" s="264"/>
-      <c r="L30" s="265"/>
+      <c r="C30" s="290"/>
+      <c r="D30" s="290"/>
+      <c r="E30" s="290"/>
+      <c r="F30" s="290"/>
+      <c r="G30" s="290"/>
+      <c r="H30" s="290"/>
+      <c r="I30" s="290"/>
+      <c r="J30" s="290"/>
+      <c r="K30" s="290"/>
+      <c r="L30" s="291"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="227">
         <v>5</v>
       </c>
-      <c r="B31" s="264" t="s">
+      <c r="B31" s="290" t="s">
         <v>208</v>
       </c>
-      <c r="C31" s="264"/>
-      <c r="D31" s="264"/>
-      <c r="E31" s="264"/>
-      <c r="F31" s="264"/>
-      <c r="G31" s="264"/>
-      <c r="H31" s="264"/>
-      <c r="I31" s="264"/>
-      <c r="J31" s="264"/>
-      <c r="K31" s="264"/>
-      <c r="L31" s="265"/>
+      <c r="C31" s="290"/>
+      <c r="D31" s="290"/>
+      <c r="E31" s="290"/>
+      <c r="F31" s="290"/>
+      <c r="G31" s="290"/>
+      <c r="H31" s="290"/>
+      <c r="I31" s="290"/>
+      <c r="J31" s="290"/>
+      <c r="K31" s="290"/>
+      <c r="L31" s="291"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="227"/>
-      <c r="B32" s="264" t="s">
+      <c r="B32" s="290" t="s">
         <v>209</v>
       </c>
-      <c r="C32" s="264"/>
-      <c r="D32" s="264"/>
-      <c r="E32" s="264"/>
-      <c r="F32" s="264"/>
-      <c r="G32" s="264"/>
-      <c r="H32" s="264"/>
-      <c r="I32" s="264"/>
-      <c r="J32" s="264"/>
-      <c r="K32" s="264"/>
-      <c r="L32" s="265"/>
+      <c r="C32" s="290"/>
+      <c r="D32" s="290"/>
+      <c r="E32" s="290"/>
+      <c r="F32" s="290"/>
+      <c r="G32" s="290"/>
+      <c r="H32" s="290"/>
+      <c r="I32" s="290"/>
+      <c r="J32" s="290"/>
+      <c r="K32" s="290"/>
+      <c r="L32" s="291"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="227"/>
-      <c r="B33" s="264" t="s">
+      <c r="B33" s="290" t="s">
         <v>210</v>
       </c>
-      <c r="C33" s="264"/>
-      <c r="D33" s="264"/>
-      <c r="E33" s="264"/>
-      <c r="F33" s="264"/>
-      <c r="G33" s="264"/>
-      <c r="H33" s="264"/>
-      <c r="I33" s="264"/>
-      <c r="J33" s="264"/>
-      <c r="K33" s="264"/>
-      <c r="L33" s="265"/>
+      <c r="C33" s="290"/>
+      <c r="D33" s="290"/>
+      <c r="E33" s="290"/>
+      <c r="F33" s="290"/>
+      <c r="G33" s="290"/>
+      <c r="H33" s="290"/>
+      <c r="I33" s="290"/>
+      <c r="J33" s="290"/>
+      <c r="K33" s="290"/>
+      <c r="L33" s="291"/>
       <c r="N33" s="106"/>
     </row>
     <row r="34" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="273" t="s">
+      <c r="A34" s="292" t="s">
         <v>216</v>
       </c>
-      <c r="B34" s="274"/>
-      <c r="C34" s="274"/>
-      <c r="D34" s="274"/>
-      <c r="E34" s="274"/>
-      <c r="F34" s="274"/>
-      <c r="G34" s="274"/>
-      <c r="H34" s="274"/>
-      <c r="I34" s="274"/>
-      <c r="J34" s="274"/>
-      <c r="K34" s="274"/>
-      <c r="L34" s="275"/>
+      <c r="B34" s="293"/>
+      <c r="C34" s="293"/>
+      <c r="D34" s="293"/>
+      <c r="E34" s="293"/>
+      <c r="F34" s="293"/>
+      <c r="G34" s="293"/>
+      <c r="H34" s="293"/>
+      <c r="I34" s="293"/>
+      <c r="J34" s="293"/>
+      <c r="K34" s="293"/>
+      <c r="L34" s="294"/>
       <c r="N34" s="106"/>
     </row>
     <row r="35" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="227">
         <v>1</v>
       </c>
-      <c r="B35" s="264" t="s">
+      <c r="B35" s="290" t="s">
         <v>211</v>
       </c>
-      <c r="C35" s="264"/>
-      <c r="D35" s="264"/>
-      <c r="E35" s="264"/>
-      <c r="F35" s="264"/>
-      <c r="G35" s="264"/>
-      <c r="H35" s="264"/>
-      <c r="I35" s="264"/>
-      <c r="J35" s="264"/>
-      <c r="K35" s="264"/>
-      <c r="L35" s="265"/>
+      <c r="C35" s="290"/>
+      <c r="D35" s="290"/>
+      <c r="E35" s="290"/>
+      <c r="F35" s="290"/>
+      <c r="G35" s="290"/>
+      <c r="H35" s="290"/>
+      <c r="I35" s="290"/>
+      <c r="J35" s="290"/>
+      <c r="K35" s="290"/>
+      <c r="L35" s="291"/>
       <c r="N35" s="106"/>
     </row>
     <row r="36" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="227"/>
-      <c r="B36" s="262" t="s">
+      <c r="B36" s="288" t="s">
         <v>339</v>
       </c>
-      <c r="C36" s="262"/>
-      <c r="D36" s="262"/>
-      <c r="E36" s="262"/>
-      <c r="F36" s="262"/>
-      <c r="G36" s="262"/>
-      <c r="H36" s="262"/>
-      <c r="I36" s="262"/>
-      <c r="J36" s="262"/>
-      <c r="K36" s="262"/>
-      <c r="L36" s="263"/>
+      <c r="C36" s="288"/>
+      <c r="D36" s="288"/>
+      <c r="E36" s="288"/>
+      <c r="F36" s="288"/>
+      <c r="G36" s="288"/>
+      <c r="H36" s="288"/>
+      <c r="I36" s="288"/>
+      <c r="J36" s="288"/>
+      <c r="K36" s="288"/>
+      <c r="L36" s="289"/>
       <c r="N36" s="106"/>
     </row>
     <row r="37" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="227">
         <v>2</v>
       </c>
-      <c r="B37" s="264" t="s">
+      <c r="B37" s="290" t="s">
         <v>332</v>
       </c>
-      <c r="C37" s="264"/>
-      <c r="D37" s="264"/>
-      <c r="E37" s="264"/>
-      <c r="F37" s="264"/>
-      <c r="G37" s="264"/>
-      <c r="H37" s="264"/>
-      <c r="I37" s="264"/>
-      <c r="J37" s="264"/>
-      <c r="K37" s="264"/>
-      <c r="L37" s="265"/>
+      <c r="C37" s="290"/>
+      <c r="D37" s="290"/>
+      <c r="E37" s="290"/>
+      <c r="F37" s="290"/>
+      <c r="G37" s="290"/>
+      <c r="H37" s="290"/>
+      <c r="I37" s="290"/>
+      <c r="J37" s="290"/>
+      <c r="K37" s="290"/>
+      <c r="L37" s="291"/>
       <c r="N37" s="106"/>
     </row>
     <row r="38" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="227">
         <v>3</v>
       </c>
-      <c r="B38" s="264" t="s">
+      <c r="B38" s="290" t="s">
         <v>321</v>
       </c>
-      <c r="C38" s="264"/>
-      <c r="D38" s="264"/>
-      <c r="E38" s="264"/>
-      <c r="F38" s="264"/>
-      <c r="G38" s="264"/>
-      <c r="H38" s="264"/>
-      <c r="I38" s="264"/>
-      <c r="J38" s="264"/>
-      <c r="K38" s="264"/>
-      <c r="L38" s="265"/>
+      <c r="C38" s="290"/>
+      <c r="D38" s="290"/>
+      <c r="E38" s="290"/>
+      <c r="F38" s="290"/>
+      <c r="G38" s="290"/>
+      <c r="H38" s="290"/>
+      <c r="I38" s="290"/>
+      <c r="J38" s="290"/>
+      <c r="K38" s="290"/>
+      <c r="L38" s="291"/>
       <c r="N38" s="106"/>
     </row>
     <row r="39" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="227">
         <v>4</v>
       </c>
-      <c r="B39" s="264" t="s">
+      <c r="B39" s="290" t="s">
         <v>340</v>
       </c>
-      <c r="C39" s="264"/>
-      <c r="D39" s="264"/>
-      <c r="E39" s="264"/>
-      <c r="F39" s="264"/>
-      <c r="G39" s="264"/>
-      <c r="H39" s="264"/>
-      <c r="I39" s="264"/>
-      <c r="J39" s="264"/>
-      <c r="K39" s="264"/>
-      <c r="L39" s="265"/>
+      <c r="C39" s="290"/>
+      <c r="D39" s="290"/>
+      <c r="E39" s="290"/>
+      <c r="F39" s="290"/>
+      <c r="G39" s="290"/>
+      <c r="H39" s="290"/>
+      <c r="I39" s="290"/>
+      <c r="J39" s="290"/>
+      <c r="K39" s="290"/>
+      <c r="L39" s="291"/>
       <c r="N39" s="106"/>
     </row>
     <row r="40" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="227">
         <v>5</v>
       </c>
-      <c r="B40" s="262" t="s">
+      <c r="B40" s="288" t="s">
         <v>322</v>
       </c>
-      <c r="C40" s="262"/>
-      <c r="D40" s="262"/>
-      <c r="E40" s="262"/>
-      <c r="F40" s="262"/>
-      <c r="G40" s="262"/>
-      <c r="H40" s="262"/>
-      <c r="I40" s="262"/>
-      <c r="J40" s="262"/>
-      <c r="K40" s="262"/>
-      <c r="L40" s="263"/>
+      <c r="C40" s="288"/>
+      <c r="D40" s="288"/>
+      <c r="E40" s="288"/>
+      <c r="F40" s="288"/>
+      <c r="G40" s="288"/>
+      <c r="H40" s="288"/>
+      <c r="I40" s="288"/>
+      <c r="J40" s="288"/>
+      <c r="K40" s="288"/>
+      <c r="L40" s="289"/>
       <c r="N40" s="106"/>
     </row>
     <row r="41" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="227">
         <v>6</v>
       </c>
-      <c r="B41" s="262" t="s">
+      <c r="B41" s="288" t="s">
         <v>327</v>
       </c>
-      <c r="C41" s="262"/>
-      <c r="D41" s="262"/>
-      <c r="E41" s="262"/>
-      <c r="F41" s="262"/>
-      <c r="G41" s="262"/>
-      <c r="H41" s="262"/>
-      <c r="I41" s="262"/>
-      <c r="J41" s="262"/>
-      <c r="K41" s="262"/>
-      <c r="L41" s="263"/>
+      <c r="C41" s="288"/>
+      <c r="D41" s="288"/>
+      <c r="E41" s="288"/>
+      <c r="F41" s="288"/>
+      <c r="G41" s="288"/>
+      <c r="H41" s="288"/>
+      <c r="I41" s="288"/>
+      <c r="J41" s="288"/>
+      <c r="K41" s="288"/>
+      <c r="L41" s="289"/>
       <c r="N41" s="106"/>
     </row>
     <row r="42" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="227">
         <v>7</v>
       </c>
-      <c r="B42" s="264" t="s">
+      <c r="B42" s="290" t="s">
         <v>323</v>
       </c>
-      <c r="C42" s="264"/>
-      <c r="D42" s="264"/>
-      <c r="E42" s="264"/>
-      <c r="F42" s="264"/>
-      <c r="G42" s="264"/>
-      <c r="H42" s="264"/>
-      <c r="I42" s="264"/>
-      <c r="J42" s="264"/>
-      <c r="K42" s="264"/>
-      <c r="L42" s="265"/>
+      <c r="C42" s="290"/>
+      <c r="D42" s="290"/>
+      <c r="E42" s="290"/>
+      <c r="F42" s="290"/>
+      <c r="G42" s="290"/>
+      <c r="H42" s="290"/>
+      <c r="I42" s="290"/>
+      <c r="J42" s="290"/>
+      <c r="K42" s="290"/>
+      <c r="L42" s="291"/>
     </row>
     <row r="43" spans="1:14" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="227"/>
@@ -15974,56 +15977,56 @@
       <c r="L43" s="229"/>
     </row>
     <row r="44" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="273" t="s">
+      <c r="A44" s="292" t="s">
         <v>326</v>
       </c>
-      <c r="B44" s="274"/>
-      <c r="C44" s="274"/>
-      <c r="D44" s="274"/>
-      <c r="E44" s="274"/>
-      <c r="F44" s="274"/>
-      <c r="G44" s="274"/>
-      <c r="H44" s="274"/>
-      <c r="I44" s="274"/>
-      <c r="J44" s="274"/>
-      <c r="K44" s="274"/>
-      <c r="L44" s="275"/>
+      <c r="B44" s="293"/>
+      <c r="C44" s="293"/>
+      <c r="D44" s="293"/>
+      <c r="E44" s="293"/>
+      <c r="F44" s="293"/>
+      <c r="G44" s="293"/>
+      <c r="H44" s="293"/>
+      <c r="I44" s="293"/>
+      <c r="J44" s="293"/>
+      <c r="K44" s="293"/>
+      <c r="L44" s="294"/>
     </row>
     <row r="45" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="230" t="s">
         <v>324</v>
       </c>
-      <c r="B45" s="264" t="s">
+      <c r="B45" s="290" t="s">
         <v>212</v>
       </c>
-      <c r="C45" s="264"/>
-      <c r="D45" s="264"/>
-      <c r="E45" s="264"/>
-      <c r="F45" s="264"/>
-      <c r="G45" s="264"/>
-      <c r="H45" s="264"/>
-      <c r="I45" s="264"/>
-      <c r="J45" s="264"/>
-      <c r="K45" s="264"/>
-      <c r="L45" s="265"/>
+      <c r="C45" s="290"/>
+      <c r="D45" s="290"/>
+      <c r="E45" s="290"/>
+      <c r="F45" s="290"/>
+      <c r="G45" s="290"/>
+      <c r="H45" s="290"/>
+      <c r="I45" s="290"/>
+      <c r="J45" s="290"/>
+      <c r="K45" s="290"/>
+      <c r="L45" s="291"/>
     </row>
     <row r="46" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="231" t="s">
         <v>325</v>
       </c>
-      <c r="B46" s="266" t="s">
+      <c r="B46" s="300" t="s">
         <v>328</v>
       </c>
-      <c r="C46" s="266"/>
-      <c r="D46" s="266"/>
-      <c r="E46" s="266"/>
-      <c r="F46" s="266"/>
-      <c r="G46" s="266"/>
-      <c r="H46" s="266"/>
-      <c r="I46" s="266"/>
-      <c r="J46" s="266"/>
-      <c r="K46" s="266"/>
-      <c r="L46" s="267"/>
+      <c r="C46" s="300"/>
+      <c r="D46" s="300"/>
+      <c r="E46" s="300"/>
+      <c r="F46" s="300"/>
+      <c r="G46" s="300"/>
+      <c r="H46" s="300"/>
+      <c r="I46" s="300"/>
+      <c r="J46" s="300"/>
+      <c r="K46" s="300"/>
+      <c r="L46" s="301"/>
     </row>
     <row r="47" spans="1:14" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="160"/>
@@ -16040,20 +16043,20 @@
       <c r="L47" s="113"/>
     </row>
     <row r="48" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="268" t="s">
+      <c r="A48" s="302" t="s">
         <v>240</v>
       </c>
-      <c r="B48" s="269"/>
-      <c r="C48" s="269"/>
-      <c r="D48" s="269"/>
-      <c r="E48" s="269"/>
-      <c r="F48" s="269"/>
-      <c r="G48" s="269"/>
-      <c r="H48" s="269"/>
-      <c r="I48" s="269"/>
-      <c r="J48" s="269"/>
-      <c r="K48" s="269"/>
-      <c r="L48" s="270"/>
+      <c r="B48" s="303"/>
+      <c r="C48" s="303"/>
+      <c r="D48" s="303"/>
+      <c r="E48" s="303"/>
+      <c r="F48" s="303"/>
+      <c r="G48" s="303"/>
+      <c r="H48" s="303"/>
+      <c r="I48" s="303"/>
+      <c r="J48" s="303"/>
+      <c r="K48" s="303"/>
+      <c r="L48" s="304"/>
     </row>
     <row r="49" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="234" t="s">
@@ -16141,90 +16144,90 @@
       <c r="B54" s="168" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="271" t="s">
+      <c r="C54" s="273" t="s">
         <v>312</v>
       </c>
-      <c r="D54" s="271"/>
-      <c r="E54" s="271"/>
-      <c r="F54" s="271"/>
-      <c r="G54" s="271"/>
-      <c r="H54" s="271"/>
-      <c r="I54" s="271"/>
-      <c r="J54" s="271"/>
-      <c r="K54" s="271"/>
-      <c r="L54" s="272"/>
+      <c r="D54" s="273"/>
+      <c r="E54" s="273"/>
+      <c r="F54" s="273"/>
+      <c r="G54" s="273"/>
+      <c r="H54" s="273"/>
+      <c r="I54" s="273"/>
+      <c r="J54" s="273"/>
+      <c r="K54" s="273"/>
+      <c r="L54" s="274"/>
     </row>
     <row r="55" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="167"/>
       <c r="B55" s="168" t="s">
         <v>313</v>
       </c>
-      <c r="C55" s="271" t="s">
+      <c r="C55" s="273" t="s">
         <v>314</v>
       </c>
-      <c r="D55" s="271"/>
-      <c r="E55" s="271"/>
-      <c r="F55" s="271"/>
-      <c r="G55" s="271"/>
-      <c r="H55" s="271"/>
-      <c r="I55" s="271"/>
-      <c r="J55" s="271"/>
-      <c r="K55" s="271"/>
-      <c r="L55" s="272"/>
+      <c r="D55" s="273"/>
+      <c r="E55" s="273"/>
+      <c r="F55" s="273"/>
+      <c r="G55" s="273"/>
+      <c r="H55" s="273"/>
+      <c r="I55" s="273"/>
+      <c r="J55" s="273"/>
+      <c r="K55" s="273"/>
+      <c r="L55" s="274"/>
     </row>
     <row r="56" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="167"/>
       <c r="B56" s="168" t="s">
         <v>382</v>
       </c>
-      <c r="C56" s="271" t="s">
+      <c r="C56" s="273" t="s">
         <v>383</v>
       </c>
-      <c r="D56" s="271"/>
-      <c r="E56" s="271"/>
-      <c r="F56" s="271"/>
-      <c r="G56" s="271"/>
-      <c r="H56" s="271"/>
-      <c r="I56" s="271"/>
-      <c r="J56" s="271"/>
-      <c r="K56" s="271"/>
-      <c r="L56" s="272"/>
+      <c r="D56" s="273"/>
+      <c r="E56" s="273"/>
+      <c r="F56" s="273"/>
+      <c r="G56" s="273"/>
+      <c r="H56" s="273"/>
+      <c r="I56" s="273"/>
+      <c r="J56" s="273"/>
+      <c r="K56" s="273"/>
+      <c r="L56" s="274"/>
     </row>
     <row r="57" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="167"/>
       <c r="B57" s="168" t="s">
         <v>138</v>
       </c>
-      <c r="C57" s="271" t="s">
+      <c r="C57" s="273" t="s">
         <v>139</v>
       </c>
-      <c r="D57" s="271"/>
-      <c r="E57" s="271"/>
-      <c r="F57" s="271"/>
-      <c r="G57" s="271"/>
-      <c r="H57" s="271"/>
-      <c r="I57" s="271"/>
-      <c r="J57" s="271"/>
-      <c r="K57" s="271"/>
-      <c r="L57" s="272"/>
+      <c r="D57" s="273"/>
+      <c r="E57" s="273"/>
+      <c r="F57" s="273"/>
+      <c r="G57" s="273"/>
+      <c r="H57" s="273"/>
+      <c r="I57" s="273"/>
+      <c r="J57" s="273"/>
+      <c r="K57" s="273"/>
+      <c r="L57" s="274"/>
     </row>
     <row r="58" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="167"/>
       <c r="B58" s="168" t="s">
         <v>238</v>
       </c>
-      <c r="C58" s="271" t="s">
+      <c r="C58" s="273" t="s">
         <v>239</v>
       </c>
-      <c r="D58" s="271"/>
-      <c r="E58" s="271"/>
-      <c r="F58" s="271"/>
-      <c r="G58" s="271"/>
-      <c r="H58" s="271"/>
-      <c r="I58" s="271"/>
-      <c r="J58" s="271"/>
-      <c r="K58" s="271"/>
-      <c r="L58" s="272"/>
+      <c r="D58" s="273"/>
+      <c r="E58" s="273"/>
+      <c r="F58" s="273"/>
+      <c r="G58" s="273"/>
+      <c r="H58" s="273"/>
+      <c r="I58" s="273"/>
+      <c r="J58" s="273"/>
+      <c r="K58" s="273"/>
+      <c r="L58" s="274"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="167"/>
@@ -16249,18 +16252,18 @@
       <c r="B60" s="168" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="271" t="s">
+      <c r="C60" s="273" t="s">
         <v>316</v>
       </c>
-      <c r="D60" s="271"/>
-      <c r="E60" s="271"/>
-      <c r="F60" s="271"/>
-      <c r="G60" s="271"/>
-      <c r="H60" s="271"/>
-      <c r="I60" s="271"/>
-      <c r="J60" s="271"/>
-      <c r="K60" s="271"/>
-      <c r="L60" s="272"/>
+      <c r="D60" s="273"/>
+      <c r="E60" s="273"/>
+      <c r="F60" s="273"/>
+      <c r="G60" s="273"/>
+      <c r="H60" s="273"/>
+      <c r="I60" s="273"/>
+      <c r="J60" s="273"/>
+      <c r="K60" s="273"/>
+      <c r="L60" s="274"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="167"/>
@@ -16360,25 +16363,56 @@
       </c>
     </row>
     <row r="78" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="261" t="s">
+      <c r="A78" s="299" t="s">
         <v>398</v>
       </c>
-      <c r="B78" s="261"/>
-      <c r="C78" s="261"/>
-      <c r="D78" s="261"/>
-      <c r="E78" s="261"/>
-      <c r="F78" s="261"/>
-      <c r="G78" s="261"/>
-      <c r="H78" s="261"/>
-      <c r="I78" s="261"/>
-      <c r="J78" s="261"/>
-      <c r="K78" s="261"/>
-      <c r="L78" s="261"/>
+      <c r="B78" s="299"/>
+      <c r="C78" s="299"/>
+      <c r="D78" s="299"/>
+      <c r="E78" s="299"/>
+      <c r="F78" s="299"/>
+      <c r="G78" s="299"/>
+      <c r="H78" s="299"/>
+      <c r="I78" s="299"/>
+      <c r="J78" s="299"/>
+      <c r="K78" s="299"/>
+      <c r="L78" s="299"/>
     </row>
     <row r="83" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="84" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="A78:L78"/>
+    <mergeCell ref="B41:L41"/>
+    <mergeCell ref="B42:L42"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="A48:L48"/>
+    <mergeCell ref="C54:L54"/>
+    <mergeCell ref="C57:L57"/>
+    <mergeCell ref="C58:L58"/>
+    <mergeCell ref="C55:L55"/>
+    <mergeCell ref="C60:L60"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="B40:L40"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B30:L30"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B39:L39"/>
     <mergeCell ref="A26:L26"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A4:L4"/>
@@ -16395,37 +16429,6 @@
     <mergeCell ref="B8:L8"/>
     <mergeCell ref="A10:L10"/>
     <mergeCell ref="B11:L11"/>
-    <mergeCell ref="C56:L56"/>
-    <mergeCell ref="B40:L40"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="B14:L14"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="A78:L78"/>
-    <mergeCell ref="B41:L41"/>
-    <mergeCell ref="B42:L42"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="A48:L48"/>
-    <mergeCell ref="C54:L54"/>
-    <mergeCell ref="C57:L57"/>
-    <mergeCell ref="C58:L58"/>
-    <mergeCell ref="C55:L55"/>
-    <mergeCell ref="C60:L60"/>
-    <mergeCell ref="A44:L44"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A67" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -31494,7 +31497,7 @@
   <dimension ref="A1:K48"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31563,15 +31566,9 @@
         <v>285</v>
       </c>
       <c r="G2" s="57"/>
-      <c r="I2" s="38" t="s">
-        <v>404</v>
-      </c>
-      <c r="J2" s="38" t="s">
-        <v>405</v>
-      </c>
-      <c r="K2" s="40">
-        <v>45678</v>
-      </c>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="40"/>
     </row>
     <row r="3" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="57">
@@ -31741,14 +31738,28 @@
       <c r="J9" s="38"/>
       <c r="K9" s="40"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="57"/>
-      <c r="B10" s="149"/>
-      <c r="C10" s="56"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="55"/>
-      <c r="F10" s="55"/>
-      <c r="G10" s="57"/>
+    <row r="10" spans="1:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="57">
+        <v>45681</v>
+      </c>
+      <c r="B10" s="149" t="s">
+        <v>406</v>
+      </c>
+      <c r="C10" s="56" t="s">
+        <v>407</v>
+      </c>
+      <c r="D10" s="55">
+        <v>1</v>
+      </c>
+      <c r="E10" s="55" t="s">
+        <v>285</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>404</v>
+      </c>
+      <c r="G10" s="57">
+        <v>45678</v>
+      </c>
       <c r="I10" s="38"/>
       <c r="J10" s="41"/>
       <c r="K10" s="40"/>
@@ -32053,7 +32064,7 @@
   <dimension ref="A1:P139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N109" sqref="N109"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32298,7 +32309,7 @@
         <v>8.6522179999999995</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F19" s="254" t="s">
         <v>248</v>
@@ -38515,16 +38526,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="340" t="e">
+      <c r="A1" s="339" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="340"/>
-      <c r="C1" s="340"/>
-      <c r="D1" s="340"/>
-      <c r="E1" s="340"/>
-      <c r="F1" s="340"/>
-      <c r="G1" s="340"/>
+      <c r="B1" s="339"/>
+      <c r="C1" s="339"/>
+      <c r="D1" s="339"/>
+      <c r="E1" s="339"/>
+      <c r="F1" s="339"/>
+      <c r="G1" s="339"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -38633,11 +38644,11 @@
         <v>80</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="339"/>
-      <c r="D10" s="339"/>
-      <c r="E10" s="339"/>
-      <c r="F10" s="339"/>
-      <c r="G10" s="339"/>
+      <c r="C10" s="340"/>
+      <c r="D10" s="340"/>
+      <c r="E10" s="340"/>
+      <c r="F10" s="340"/>
+      <c r="G10" s="340"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -39900,12 +39911,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -39913,6 +39918,12 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>

</xml_diff>

<commit_message>
Add desal cost in model guide. Turn Protect elevation default value to 1020.
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2867F2C-3146-420C-8131-53A63EFA3A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148B973D-35CE-44C7-9162-87E3DE8F8600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="62" r:id="rId1"/>
@@ -15219,8 +15219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EA02F4-5F19-409C-8BC6-A0D8FEB3A90D}">
   <dimension ref="A1:R84"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32063,8 +32063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BF7D8F-86F3-47E9-AB85-EE9B4CAB70E4}">
   <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N65" sqref="N65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32250,10 +32250,6 @@
       </c>
       <c r="C14" s="307"/>
       <c r="D14" s="308"/>
-      <c r="F14">
-        <f>4.5/7.2</f>
-        <v>0.625</v>
-      </c>
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
@@ -32262,10 +32258,6 @@
       </c>
       <c r="C15" s="310"/>
       <c r="D15" s="311"/>
-      <c r="F15">
-        <f>F14*0.4</f>
-        <v>0.25</v>
-      </c>
       <c r="N15" s="142"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
@@ -32323,10 +32315,12 @@
         <f>"     Set "&amp;A5</f>
         <v xml:space="preserve">     Set Reclamation - Protect Zone</v>
       </c>
-      <c r="B20" s="184"/>
+      <c r="B20" s="184">
+        <v>1020</v>
+      </c>
       <c r="C20" s="12">
         <f>VLOOKUP(IF(B20="",895,B20),'Mead-Elevation-Area'!$A$5:$B$689,2)/1000000</f>
-        <v>0</v>
+        <v>5.664593</v>
       </c>
       <c r="D20" s="10"/>
       <c r="N20" s="141" t="s">
@@ -32339,7 +32333,7 @@
       </c>
       <c r="C21" s="12">
         <f>C19-C20</f>
-        <v>8.6522179999999995</v>
+        <v>2.9876249999999995</v>
       </c>
       <c r="D21" s="116"/>
       <c r="E21" s="28"/>
@@ -32370,7 +32364,7 @@
       </c>
       <c r="C23" s="12">
         <f>C21-C22</f>
-        <v>5.1182179999999997</v>
+        <v>-0.54637500000000028</v>
       </c>
       <c r="D23" s="111"/>
       <c r="E23" s="28"/>
@@ -32463,7 +32457,7 @@
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="97">
-        <v>9.26</v>
+        <v>8</v>
       </c>
       <c r="D28" s="97"/>
       <c r="E28" s="97"/>
@@ -32737,11 +32731,11 @@
       </c>
       <c r="B36" s="83">
         <f>C20</f>
-        <v>0</v>
+        <v>5.664593</v>
       </c>
       <c r="C36" s="81">
         <f>IF(OR(C$28="",$A36=""),"",B36)</f>
-        <v>0</v>
+        <v>5.664593</v>
       </c>
       <c r="D36" s="12" t="str">
         <f>IF(OR(D$28="",$A36=""),"",C128)</f>
@@ -32779,6 +32773,7 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
+      <c r="M36" s="28"/>
       <c r="N36" s="142"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.35">
@@ -32791,7 +32786,7 @@
       </c>
       <c r="C37" s="81">
         <f>IF(OR(C$28="",$A37=""),"",IF(C$22&lt;=C$21,B37,B37-(C$22-C$21)*B37/C$22))</f>
-        <v>1.6619999999999999</v>
+        <v>1.4050460526315787</v>
       </c>
       <c r="D37" s="12" t="str">
         <f t="shared" ref="D37:D41" si="7">IF(OR(D$28="",$A37=""),"",C129)</f>
@@ -32829,6 +32824,7 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="M37" s="28"/>
       <c r="N37" s="142"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.35">
@@ -32841,7 +32837,7 @@
       </c>
       <c r="C38" s="81">
         <f t="shared" ref="C38:C41" si="9">IF(OR(C$28="",$A38=""),"",IF(C$22&lt;=C$21,B38,B38-(C$22-C$21)*B38/C$22))</f>
-        <v>0.71099999999999997</v>
+        <v>0.60107565789473671</v>
       </c>
       <c r="D38" s="33" t="str">
         <f t="shared" si="7"/>
@@ -32879,6 +32875,7 @@
         <f t="shared" si="8"/>
         <v/>
       </c>
+      <c r="M38" s="28"/>
       <c r="N38" s="142"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
@@ -32891,7 +32888,7 @@
       </c>
       <c r="C39" s="81">
         <f t="shared" si="9"/>
-        <v>0.9556</v>
+        <v>0.80785921052631571</v>
       </c>
       <c r="D39" s="12" t="str">
         <f t="shared" si="7"/>
@@ -32941,7 +32938,7 @@
       </c>
       <c r="C40" s="81">
         <f t="shared" si="9"/>
-        <v>0.21099999999999999</v>
+        <v>0.17837828947368417</v>
       </c>
       <c r="D40" s="12" t="str">
         <f t="shared" si="7"/>
@@ -32988,11 +32985,11 @@
       </c>
       <c r="B41" s="83">
         <f>IF(C21&gt;C22,C21-C22,0)</f>
-        <v>5.1182179999999997</v>
+        <v>0</v>
       </c>
       <c r="C41" s="81">
         <f t="shared" si="9"/>
-        <v>5.1182179999999997</v>
+        <v>0</v>
       </c>
       <c r="D41" s="12" t="str">
         <f t="shared" si="7"/>
@@ -33169,7 +33166,7 @@
       </c>
       <c r="C46" s="12">
         <f t="shared" ref="C46:G51" si="11">IF(OR(C$28="",$A46=""),"",C$45*C36/C$33)</f>
-        <v>0</v>
+        <v>0.30214853419597149</v>
       </c>
       <c r="D46" s="12" t="str">
         <f t="shared" si="11"/>
@@ -33217,7 +33214,7 @@
       <c r="B47" s="1"/>
       <c r="C47" s="12">
         <f t="shared" si="11"/>
-        <v>8.8650828723917954E-2</v>
+        <v>7.4944944019891158E-2</v>
       </c>
       <c r="D47" s="12" t="str">
         <f t="shared" si="11"/>
@@ -33265,7 +33262,7 @@
       <c r="B48" s="1"/>
       <c r="C48" s="12">
         <f t="shared" si="11"/>
-        <v>3.7924632504636381E-2</v>
+        <v>3.206128471609062E-2</v>
       </c>
       <c r="D48" s="12" t="str">
         <f t="shared" si="11"/>
@@ -33313,7 +33310,7 @@
       <c r="B49" s="1"/>
       <c r="C49" s="12">
         <f t="shared" si="11"/>
-        <v>5.0971559523812278E-2</v>
+        <v>4.3091088150064981E-2</v>
       </c>
       <c r="D49" s="12" t="str">
         <f t="shared" si="11"/>
@@ -33361,7 +33358,7 @@
       <c r="B50" s="1"/>
       <c r="C50" s="12">
         <f t="shared" si="11"/>
-        <v>1.1254708099125564E-2</v>
+        <v>9.5146709916949651E-3</v>
       </c>
       <c r="D50" s="12" t="str">
         <f t="shared" si="11"/>
@@ -33409,7 +33406,7 @@
       <c r="B51" s="1"/>
       <c r="C51" s="12">
         <f t="shared" si="11"/>
-        <v>0.27300497430184956</v>
+        <v>0</v>
       </c>
       <c r="D51" s="12" t="str">
         <f t="shared" si="11"/>
@@ -33456,7 +33453,7 @@
       <c r="B52" s="214"/>
       <c r="C52" s="215">
         <f>IF(C28="","",SUM(C28))</f>
-        <v>9.26</v>
+        <v>8</v>
       </c>
       <c r="D52" s="215" t="str">
         <f>IF(D28="","",SUM(D28))</f>
@@ -33509,7 +33506,7 @@
       </c>
       <c r="C53" s="82">
         <f>IF(OR(C$28="",$A55=""),"",C46)</f>
-        <v>0</v>
+        <v>0.30214853419597149</v>
       </c>
       <c r="D53" s="82" t="str">
         <f t="shared" ref="D53:G53" si="13">IF(OR(D$28="",$A55=""),"",D46)</f>
@@ -33549,7 +33546,7 @@
       </c>
       <c r="M53" s="19">
         <f>SUM(C55:C59)</f>
-        <v>9.26</v>
+        <v>7.6978514658040282</v>
       </c>
       <c r="N53" s="183"/>
     </row>
@@ -33559,7 +33556,7 @@
       </c>
       <c r="C54" s="82">
         <f>IF(OR(C$28="",$A56=""),"",C52-C53)</f>
-        <v>9.26</v>
+        <v>7.6978514658040282</v>
       </c>
       <c r="D54" s="82" t="str">
         <f t="shared" ref="D54:G54" si="15">IF(OR(D$28="",$A56=""),"",D52-D53)</f>
@@ -33614,7 +33611,7 @@
       </c>
       <c r="C55" s="82">
         <f>IF(OR(C$28="",$A55=""),"",(VLOOKUP(C$54,DivideInflow!$K$19:$W$25,9)-IF($A$59&lt;&gt;"",$B$59*$B$24,0))*(C$54))</f>
-        <v>4.3338971767156647</v>
+        <v>3.9038054941039078</v>
       </c>
       <c r="D55" s="82" t="str">
         <f>IF(OR(D$28="",$A55=""),"",(VLOOKUP(D$54,DivideInflow!$K$19:$W$25,9)-IF($A$59&lt;&gt;"",$B$59*$B$24,0))*(D$54))</f>
@@ -33639,7 +33636,7 @@
       <c r="L55" s="81"/>
       <c r="M55" s="223">
         <f>C55/C$54</f>
-        <v>0.46802345320903505</v>
+        <v>0.50712923098681295</v>
       </c>
       <c r="N55" s="143"/>
       <c r="P55" s="81"/>
@@ -33654,7 +33651,7 @@
       </c>
       <c r="C56" s="82">
         <f>IF(OR(C$28="",$A56=""),"",(VLOOKUP(C$54,DivideInflow!$K$19:$W$25,7)-IF($A$59&lt;&gt;"",$B$59*$B$25,0))*(C$54))</f>
-        <v>1.8987001566176687</v>
+        <v>1.2773617324799242</v>
       </c>
       <c r="D56" s="82" t="str">
         <f>IF(OR(D$28="",$A56=""),"",(VLOOKUP(D$54,DivideInflow!$K$19:$W$25,7)-IF($A$59&lt;&gt;"",$B$59*$B$25,0))*(D$54))</f>
@@ -33694,7 +33691,7 @@
       </c>
       <c r="M56" s="223">
         <f t="shared" ref="M56:M58" si="26">C56/C$54</f>
-        <v>0.2050432134576316</v>
+        <v>0.16593743567985381</v>
       </c>
       <c r="N56" s="143"/>
     </row>
@@ -33708,7 +33705,7 @@
       </c>
       <c r="C57" s="82">
         <f>IF(OR(C$28="",$A57=""),"",VLOOKUP(C$54,DivideInflow!$K$19:$W$25,8)*(C$54))</f>
-        <v>0.30866666666666664</v>
+        <v>0.2566463678699063</v>
       </c>
       <c r="D57" s="82" t="str">
         <f>IF(OR(D$28="",$A57=""),"",VLOOKUP(D$54,DivideInflow!$K$18:$W$23,8)*(D$54))</f>
@@ -33748,7 +33745,7 @@
       </c>
       <c r="M57" s="223">
         <f t="shared" si="26"/>
-        <v>3.3333333333333333E-2</v>
+        <v>3.3340000000000002E-2</v>
       </c>
       <c r="N57" s="143"/>
     </row>
@@ -33762,7 +33759,7 @@
       </c>
       <c r="C58" s="82">
         <f>IF(OR(C$28="",$A58=""),"",VLOOKUP(C$54,DivideInflow!$K$19:$W$25,10)*(C$54))</f>
-        <v>1.5433333333333332</v>
+        <v>1.2829239252908993</v>
       </c>
       <c r="D58" s="82" t="str">
         <f>IF(OR(D$28="",$A58=""),"",VLOOKUP(D$54,DivideInflow!$K$18:$W$23,10)*(D$54))</f>
@@ -33802,7 +33799,7 @@
       </c>
       <c r="M58" s="223">
         <f t="shared" si="26"/>
-        <v>0.16666666666666666</v>
+        <v>0.16666</v>
       </c>
       <c r="N58" s="143"/>
     </row>
@@ -33817,7 +33814,7 @@
       </c>
       <c r="C59" s="82">
         <f>IF(OR(C$28="",$A59=""),"",C$54*$B59)</f>
-        <v>1.1754026666666664</v>
+        <v>0.97711394605939117</v>
       </c>
       <c r="D59" s="82" t="str">
         <f t="shared" ref="D59:G59" si="37">IF(OR(D$28="",$A59=""),"",D$54*$B59)</f>
@@ -34074,7 +34071,7 @@
       </c>
       <c r="C67" s="12">
         <f>IF(OR(C$28="",$A67=""),"",C36+C53-C46+C64)</f>
-        <v>0</v>
+        <v>5.664593</v>
       </c>
       <c r="D67" s="12" t="str">
         <f>IF(OR(D$28="",$A67=""),"",D36+D53-D46+D64)</f>
@@ -34142,7 +34139,7 @@
       </c>
       <c r="C69" s="12">
         <f>IF(OR(C$28="",$A69=""),"",C67-C68)</f>
-        <v>0</v>
+        <v>5.664593</v>
       </c>
       <c r="D69" s="12" t="str">
         <f t="shared" ref="D69:L69" si="47">IF(OR(D$28="",$A69=""),"",D67-D68)</f>
@@ -34317,7 +34314,7 @@
       </c>
       <c r="C75" s="12">
         <f>IF(OR(C$28="",$A75=""),"",C37+C55-C47+C72)</f>
-        <v>5.9072463479917463</v>
+        <v>5.2339066027155949</v>
       </c>
       <c r="D75" s="12" t="str">
         <f>IF(OR(D$28="",$A75=""),"",D37+D55-D47+D72)</f>
@@ -34385,7 +34382,7 @@
       </c>
       <c r="C77" s="12">
         <f>IF(OR(C$28="",$A77=""),"",C75-C76)</f>
-        <v>5.9072463479917463</v>
+        <v>5.2339066027155949</v>
       </c>
       <c r="D77" s="12" t="str">
         <f t="shared" ref="D77:L77" si="50">IF(OR(D$28="",$A77=""),"",D75-D76)</f>
@@ -34560,7 +34557,7 @@
       </c>
       <c r="C83" s="12">
         <f>IF(OR(C$28="",$A83=""),"",C38+C56-C48+C80)</f>
-        <v>2.5717755241130322</v>
+        <v>1.8463761056585704</v>
       </c>
       <c r="D83" s="12" t="str">
         <f t="shared" ref="D83:L83" si="52">IF(OR(D$28="",$A83=""),"",D38+D56-D48+D80)</f>
@@ -34628,7 +34625,7 @@
       </c>
       <c r="C85" s="12">
         <f>IF(OR(C$28="",$A85=""),"",C83-C84)</f>
-        <v>2.5717755241130322</v>
+        <v>1.8463761056585704</v>
       </c>
       <c r="D85" s="12" t="str">
         <f t="shared" ref="D85:L85" si="53">IF(OR(D$28="",$A85=""),"",D83-D84)</f>
@@ -34803,7 +34800,7 @@
       </c>
       <c r="C91" s="12">
         <f>IF(OR(C$28="",$A91=""),"",C39+C57-C49+C88)</f>
-        <v>1.2132951071428544</v>
+        <v>1.021414490246157</v>
       </c>
       <c r="D91" s="12" t="str">
         <f t="shared" ref="D91:L91" si="55">IF(OR(D$28="",$A91=""),"",D39+D57-D49+D88)</f>
@@ -34871,7 +34868,7 @@
       </c>
       <c r="C93" s="12">
         <f>IF(OR(C$28="",$A93=""),"",C91-C92)</f>
-        <v>1.2132951071428544</v>
+        <v>1.021414490246157</v>
       </c>
       <c r="D93" s="12" t="str">
         <f t="shared" ref="D93:L93" si="56">IF(OR(D$28="",$A93=""),"",D91-D92)</f>
@@ -35046,7 +35043,7 @@
       </c>
       <c r="C99" s="12">
         <f>IF(OR(C$28="",$A99=""),"",C40+C58-C50+C96)</f>
-        <v>1.7430786252342076</v>
+        <v>1.4517875437728884</v>
       </c>
       <c r="D99" s="12" t="str">
         <f t="shared" ref="D99:L99" si="58">IF(OR(D$28="",$A99=""),"",D40+D58-D50+D96)</f>
@@ -35114,7 +35111,7 @@
       </c>
       <c r="C101" s="12">
         <f>IF(OR(C$28="",$A101=""),"",C99-C100)</f>
-        <v>1.7430786252342076</v>
+        <v>1.4517875437728884</v>
       </c>
       <c r="D101" s="12" t="str">
         <f t="shared" ref="D101:L101" si="59">IF(OR(D$28="",$A101=""),"",D99-D100)</f>
@@ -35289,7 +35286,7 @@
       </c>
       <c r="C107" s="12">
         <f>IF(OR(C$28="",$A107=""),"",C41+C59-C51+C104)</f>
-        <v>6.0206156923648164</v>
+        <v>0.97711394605939117</v>
       </c>
       <c r="D107" s="12" t="str">
         <f t="shared" ref="D107:L107" si="61">IF(OR(D$28="",$A107=""),"",D41+D59-D51+D104)</f>
@@ -35357,7 +35354,7 @@
       </c>
       <c r="C109" s="12">
         <f>IF(OR(C$28="",$A109=""),"",C107-C108)</f>
-        <v>6.0206156923648164</v>
+        <v>0.97711394605939117</v>
       </c>
       <c r="D109" s="12" t="str">
         <f t="shared" ref="D109:L109" si="62">IF(OR(D$28="",$A109=""),"",D107-D108)</f>
@@ -36115,7 +36112,7 @@
       </c>
       <c r="C128" s="44">
         <f t="shared" ref="C128:L128" ca="1" si="79">IF(OR(C$28="",$A128=""),"",OFFSET(C$69,8*(ROW(B128)-ROW(B$128)),0))</f>
-        <v>0</v>
+        <v>5.664593</v>
       </c>
       <c r="D128" s="44" t="str">
         <f t="shared" ca="1" si="79"/>
@@ -36162,7 +36159,7 @@
       </c>
       <c r="C129" s="44">
         <f t="shared" ref="C129:L129" ca="1" si="80">IF(OR(C$28="",$A129=""),"",OFFSET(C$69,8*(ROW(B129)-ROW(B$128)),0))</f>
-        <v>5.9072463479917463</v>
+        <v>5.2339066027155949</v>
       </c>
       <c r="D129" s="44" t="str">
         <f t="shared" ca="1" si="80"/>
@@ -36209,7 +36206,7 @@
       </c>
       <c r="C130" s="44">
         <f t="shared" ref="C130:L130" ca="1" si="81">IF(OR(C$28="",$A130=""),"",OFFSET(C$69,8*(ROW(B130)-ROW(B$128)),0))</f>
-        <v>2.5717755241130322</v>
+        <v>1.8463761056585704</v>
       </c>
       <c r="D130" s="44" t="str">
         <f t="shared" ca="1" si="81"/>
@@ -36256,7 +36253,7 @@
       </c>
       <c r="C131" s="44">
         <f t="shared" ref="C131:L131" ca="1" si="82">IF(OR(C$28="",$A131=""),"",OFFSET(C$69,8*(ROW(B131)-ROW(B$128)),0))</f>
-        <v>1.2132951071428544</v>
+        <v>1.021414490246157</v>
       </c>
       <c r="D131" s="44" t="str">
         <f t="shared" ca="1" si="82"/>
@@ -36303,7 +36300,7 @@
       </c>
       <c r="C132" s="44">
         <f t="shared" ref="C132:L132" ca="1" si="83">IF(OR(C$28="",$A132=""),"",OFFSET(C$69,8*(ROW(B132)-ROW(B$128)),0))</f>
-        <v>1.7430786252342076</v>
+        <v>1.4517875437728884</v>
       </c>
       <c r="D132" s="44" t="str">
         <f t="shared" ca="1" si="83"/>
@@ -36350,7 +36347,7 @@
       </c>
       <c r="C133" s="44">
         <f t="shared" ref="C133:L133" ca="1" si="84">IF(OR(C$28="",$A133=""),"",OFFSET(C$69,8*(ROW(B133)-ROW(B$128)),0))</f>
-        <v>6.0206156923648164</v>
+        <v>0.97711394605939117</v>
       </c>
       <c r="D133" s="44" t="str">
         <f t="shared" ca="1" si="84"/>
@@ -36425,7 +36422,7 @@
       <c r="B135" s="1"/>
       <c r="C135" s="12">
         <f ca="1">IF(C$28&lt;&gt;"",SUM(C128:C133),"")</f>
-        <v>17.456011296846658</v>
+        <v>16.195191688452603</v>
       </c>
       <c r="D135" s="12" t="str">
         <f>IF(D$28&lt;&gt;"",SUM(D128:D133),"")</f>
@@ -36457,7 +36454,7 @@
       <c r="B136" s="1"/>
       <c r="C136" s="219">
         <f ca="1">IF(C$28&lt;&gt;"",VLOOKUP(C135*1000000,'Mead-Elevation-Area'!$B$5:$H$689,7),"")</f>
-        <v>1156</v>
+        <v>1145</v>
       </c>
       <c r="D136" s="219" t="str">
         <f>IF(D$28&lt;&gt;"",VLOOKUP(D135*1000000,'Mead-Elevation-Area'!$B$5:$H$689,7),"")</f>
@@ -39411,7 +39408,7 @@
       </c>
       <c r="M39" s="28">
         <f>Master!C52</f>
-        <v>9.26</v>
+        <v>8</v>
       </c>
       <c r="N39" s="140" t="s">
         <v>185</v>
@@ -39467,7 +39464,7 @@
       </c>
       <c r="M40" s="28">
         <f>Master!C53</f>
-        <v>0</v>
+        <v>0.30214853419597149</v>
       </c>
       <c r="N40" s="143"/>
       <c r="P40" s="81"/>
@@ -39523,7 +39520,7 @@
       </c>
       <c r="M41" s="28">
         <f>Master!C55</f>
-        <v>4.3338971767156647</v>
+        <v>3.9038054941039078</v>
       </c>
       <c r="N41" s="143"/>
       <c r="P41" s="81"/>
@@ -39578,7 +39575,7 @@
       </c>
       <c r="M42" s="28">
         <f>Master!C56</f>
-        <v>1.8987001566176687</v>
+        <v>1.2773617324799242</v>
       </c>
       <c r="N42" s="143"/>
     </row>
@@ -39633,7 +39630,7 @@
       </c>
       <c r="M43" s="179">
         <f>Master!C57</f>
-        <v>0.30866666666666664</v>
+        <v>0.2566463678699063</v>
       </c>
       <c r="N43" s="143"/>
     </row>
@@ -39688,7 +39685,7 @@
       </c>
       <c r="M44" s="28">
         <f>Master!C58</f>
-        <v>1.5433333333333332</v>
+        <v>1.2829239252908993</v>
       </c>
       <c r="N44" s="143"/>
     </row>
@@ -39742,7 +39739,7 @@
       </c>
       <c r="M45" s="28">
         <f>Master!C59</f>
-        <v>1.1754026666666664</v>
+        <v>0.97711394605939117</v>
       </c>
       <c r="N45" s="143"/>
     </row>

</xml_diff>

<commit_message>
Add Hadia as co-author
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148B973D-35CE-44C7-9162-87E3DE8F8600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE4A06A-523F-436C-B8BE-892C085EBEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -2045,9 +2045,6 @@
     <t>University of California Agricultural and Natural Resources</t>
   </si>
   <si>
-    <t>David E. Rosenberg, Erik Porse (2025). "Immersive Model for Lake Mead Based on the Principle of Division of Reservoir Inflow." Utah State University, Logan, UT. https://github.com/dzeke/ColoradoRiverCollaborate/tree/main/LakeMeadWaterBankDivideInflow.</t>
-  </si>
-  <si>
     <t>eporse@ucanr.edu</t>
   </si>
   <si>
@@ -2073,6 +2070,9 @@
   </si>
   <si>
     <t>Add recent water use in Model Guide</t>
+  </si>
+  <si>
+    <t>David E. Rosenberg, Hadia Akbar, Erik Porse (2025). "Immersive Model for Lake Mead Based on the Principle of Division of Reservoir Inflow." Utah State University, Logan, UT. https://github.com/dzeke/ColoradoRiverCollaborate/tree/main/LakeMeadWaterBankDivideInflow.</t>
   </si>
 </sst>
 </file>
@@ -3401,6 +3401,69 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3455,12 +3518,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3493,63 +3550,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3653,11 +3653,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -15239,20 +15239,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="258" t="s">
+      <c r="A1" s="279" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="258"/>
-      <c r="C1" s="258"/>
-      <c r="D1" s="258"/>
-      <c r="E1" s="258"/>
-      <c r="F1" s="258"/>
-      <c r="G1" s="258"/>
-      <c r="H1" s="258"/>
-      <c r="I1" s="258"/>
-      <c r="J1" s="258"/>
-      <c r="K1" s="258"/>
-      <c r="L1" s="258"/>
+      <c r="B1" s="279"/>
+      <c r="C1" s="279"/>
+      <c r="D1" s="279"/>
+      <c r="E1" s="279"/>
+      <c r="F1" s="279"/>
+      <c r="G1" s="279"/>
+      <c r="H1" s="279"/>
+      <c r="I1" s="279"/>
+      <c r="J1" s="279"/>
+      <c r="K1" s="279"/>
+      <c r="L1" s="279"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -15278,41 +15278,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="259" t="s">
+      <c r="A4" s="280" t="s">
         <v>351</v>
       </c>
-      <c r="B4" s="260"/>
-      <c r="C4" s="260"/>
-      <c r="D4" s="260"/>
-      <c r="E4" s="260"/>
-      <c r="F4" s="260"/>
-      <c r="G4" s="260"/>
-      <c r="H4" s="260"/>
-      <c r="I4" s="260"/>
-      <c r="J4" s="260"/>
-      <c r="K4" s="260"/>
-      <c r="L4" s="261"/>
-      <c r="N4" s="262"/>
-      <c r="O4" s="262"/>
-      <c r="P4" s="262"/>
-      <c r="Q4" s="262"/>
-      <c r="R4" s="262"/>
+      <c r="B4" s="281"/>
+      <c r="C4" s="281"/>
+      <c r="D4" s="281"/>
+      <c r="E4" s="281"/>
+      <c r="F4" s="281"/>
+      <c r="G4" s="281"/>
+      <c r="H4" s="281"/>
+      <c r="I4" s="281"/>
+      <c r="J4" s="281"/>
+      <c r="K4" s="281"/>
+      <c r="L4" s="282"/>
+      <c r="N4" s="283"/>
+      <c r="O4" s="283"/>
+      <c r="P4" s="283"/>
+      <c r="Q4" s="283"/>
+      <c r="R4" s="283"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="263" t="s">
+      <c r="A5" s="284" t="s">
         <v>334</v>
       </c>
-      <c r="B5" s="264"/>
-      <c r="C5" s="264"/>
-      <c r="D5" s="264"/>
-      <c r="E5" s="264"/>
-      <c r="F5" s="264"/>
-      <c r="G5" s="264"/>
-      <c r="H5" s="264"/>
-      <c r="I5" s="264"/>
-      <c r="J5" s="264"/>
-      <c r="K5" s="264"/>
-      <c r="L5" s="265"/>
+      <c r="B5" s="285"/>
+      <c r="C5" s="285"/>
+      <c r="D5" s="285"/>
+      <c r="E5" s="285"/>
+      <c r="F5" s="285"/>
+      <c r="G5" s="285"/>
+      <c r="H5" s="285"/>
+      <c r="I5" s="285"/>
+      <c r="J5" s="285"/>
+      <c r="K5" s="285"/>
+      <c r="L5" s="286"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15320,20 +15320,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="263" t="s">
+      <c r="A6" s="284" t="s">
         <v>352</v>
       </c>
-      <c r="B6" s="264"/>
-      <c r="C6" s="264"/>
-      <c r="D6" s="264"/>
-      <c r="E6" s="264"/>
-      <c r="F6" s="264"/>
-      <c r="G6" s="264"/>
-      <c r="H6" s="264"/>
-      <c r="I6" s="264"/>
-      <c r="J6" s="264"/>
-      <c r="K6" s="264"/>
-      <c r="L6" s="265"/>
+      <c r="B6" s="285"/>
+      <c r="C6" s="285"/>
+      <c r="D6" s="285"/>
+      <c r="E6" s="285"/>
+      <c r="F6" s="285"/>
+      <c r="G6" s="285"/>
+      <c r="H6" s="285"/>
+      <c r="I6" s="285"/>
+      <c r="J6" s="285"/>
+      <c r="K6" s="285"/>
+      <c r="L6" s="286"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15342,19 +15342,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="232"/>
-      <c r="B7" s="264" t="s">
+      <c r="B7" s="285" t="s">
         <v>353</v>
       </c>
-      <c r="C7" s="264"/>
-      <c r="D7" s="264"/>
-      <c r="E7" s="264"/>
-      <c r="F7" s="264"/>
-      <c r="G7" s="264"/>
-      <c r="H7" s="264"/>
-      <c r="I7" s="264"/>
-      <c r="J7" s="264"/>
-      <c r="K7" s="264"/>
-      <c r="L7" s="265"/>
+      <c r="C7" s="285"/>
+      <c r="D7" s="285"/>
+      <c r="E7" s="285"/>
+      <c r="F7" s="285"/>
+      <c r="G7" s="285"/>
+      <c r="H7" s="285"/>
+      <c r="I7" s="285"/>
+      <c r="J7" s="285"/>
+      <c r="K7" s="285"/>
+      <c r="L7" s="286"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15363,19 +15363,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="233"/>
-      <c r="B8" s="281" t="s">
+      <c r="B8" s="300" t="s">
         <v>354</v>
       </c>
-      <c r="C8" s="281"/>
-      <c r="D8" s="281"/>
-      <c r="E8" s="281"/>
-      <c r="F8" s="281"/>
-      <c r="G8" s="281"/>
-      <c r="H8" s="281"/>
-      <c r="I8" s="281"/>
-      <c r="J8" s="281"/>
-      <c r="K8" s="281"/>
-      <c r="L8" s="282"/>
+      <c r="C8" s="300"/>
+      <c r="D8" s="300"/>
+      <c r="E8" s="300"/>
+      <c r="F8" s="300"/>
+      <c r="G8" s="300"/>
+      <c r="H8" s="300"/>
+      <c r="I8" s="300"/>
+      <c r="J8" s="300"/>
+      <c r="K8" s="300"/>
+      <c r="L8" s="301"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15397,38 +15397,38 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="283" t="s">
+      <c r="A10" s="302" t="s">
         <v>389</v>
       </c>
-      <c r="B10" s="284"/>
-      <c r="C10" s="284"/>
-      <c r="D10" s="284"/>
-      <c r="E10" s="284"/>
-      <c r="F10" s="284"/>
-      <c r="G10" s="284"/>
-      <c r="H10" s="284"/>
-      <c r="I10" s="284"/>
-      <c r="J10" s="284"/>
-      <c r="K10" s="284"/>
-      <c r="L10" s="285"/>
+      <c r="B10" s="303"/>
+      <c r="C10" s="303"/>
+      <c r="D10" s="303"/>
+      <c r="E10" s="303"/>
+      <c r="F10" s="303"/>
+      <c r="G10" s="303"/>
+      <c r="H10" s="303"/>
+      <c r="I10" s="303"/>
+      <c r="J10" s="303"/>
+      <c r="K10" s="303"/>
+      <c r="L10" s="304"/>
     </row>
     <row r="11" spans="1:18" s="58" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="253" t="s">
         <v>390</v>
       </c>
-      <c r="B11" s="286" t="s">
+      <c r="B11" s="257" t="s">
         <v>393</v>
       </c>
-      <c r="C11" s="286"/>
-      <c r="D11" s="286"/>
-      <c r="E11" s="286"/>
-      <c r="F11" s="286"/>
-      <c r="G11" s="286"/>
-      <c r="H11" s="286"/>
-      <c r="I11" s="286"/>
-      <c r="J11" s="286"/>
-      <c r="K11" s="286"/>
-      <c r="L11" s="287"/>
+      <c r="C11" s="257"/>
+      <c r="D11" s="257"/>
+      <c r="E11" s="257"/>
+      <c r="F11" s="257"/>
+      <c r="G11" s="257"/>
+      <c r="H11" s="257"/>
+      <c r="I11" s="257"/>
+      <c r="J11" s="257"/>
+      <c r="K11" s="257"/>
+      <c r="L11" s="258"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="161.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="245"/>
@@ -15448,51 +15448,51 @@
       <c r="A13" s="253" t="s">
         <v>391</v>
       </c>
-      <c r="B13" s="286" t="s">
+      <c r="B13" s="257" t="s">
         <v>394</v>
       </c>
-      <c r="C13" s="286"/>
-      <c r="D13" s="286"/>
-      <c r="E13" s="286"/>
-      <c r="F13" s="286"/>
-      <c r="G13" s="286"/>
-      <c r="H13" s="286"/>
-      <c r="I13" s="286"/>
-      <c r="J13" s="286"/>
-      <c r="K13" s="286"/>
-      <c r="L13" s="287"/>
+      <c r="C13" s="257"/>
+      <c r="D13" s="257"/>
+      <c r="E13" s="257"/>
+      <c r="F13" s="257"/>
+      <c r="G13" s="257"/>
+      <c r="H13" s="257"/>
+      <c r="I13" s="257"/>
+      <c r="J13" s="257"/>
+      <c r="K13" s="257"/>
+      <c r="L13" s="258"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="90.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="245"/>
-      <c r="B14" s="297"/>
-      <c r="C14" s="297"/>
-      <c r="D14" s="297"/>
-      <c r="E14" s="297"/>
-      <c r="F14" s="297"/>
-      <c r="G14" s="297"/>
-      <c r="H14" s="297"/>
-      <c r="I14" s="297"/>
-      <c r="J14" s="297"/>
-      <c r="K14" s="297"/>
-      <c r="L14" s="298"/>
+      <c r="B14" s="259"/>
+      <c r="C14" s="259"/>
+      <c r="D14" s="259"/>
+      <c r="E14" s="259"/>
+      <c r="F14" s="259"/>
+      <c r="G14" s="259"/>
+      <c r="H14" s="259"/>
+      <c r="I14" s="259"/>
+      <c r="J14" s="259"/>
+      <c r="K14" s="259"/>
+      <c r="L14" s="260"/>
     </row>
     <row r="15" spans="1:18" s="58" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="253" t="s">
         <v>392</v>
       </c>
-      <c r="B15" s="286" t="s">
+      <c r="B15" s="257" t="s">
         <v>395</v>
       </c>
-      <c r="C15" s="286"/>
-      <c r="D15" s="286"/>
-      <c r="E15" s="286"/>
-      <c r="F15" s="286"/>
-      <c r="G15" s="286"/>
-      <c r="H15" s="286"/>
-      <c r="I15" s="286"/>
-      <c r="J15" s="286"/>
-      <c r="K15" s="286"/>
-      <c r="L15" s="287"/>
+      <c r="C15" s="257"/>
+      <c r="D15" s="257"/>
+      <c r="E15" s="257"/>
+      <c r="F15" s="257"/>
+      <c r="G15" s="257"/>
+      <c r="H15" s="257"/>
+      <c r="I15" s="257"/>
+      <c r="J15" s="257"/>
+      <c r="K15" s="257"/>
+      <c r="L15" s="258"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="245"/>
@@ -15509,14 +15509,14 @@
       <c r="L16" s="252"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="295" t="s">
+      <c r="A17" s="255" t="s">
+        <v>399</v>
+      </c>
+      <c r="B17" s="256"/>
+      <c r="C17" s="256"/>
+      <c r="D17" s="256"/>
+      <c r="E17" s="250" t="s">
         <v>400</v>
-      </c>
-      <c r="B17" s="296"/>
-      <c r="C17" s="296"/>
-      <c r="D17" s="296"/>
-      <c r="E17" s="250" t="s">
-        <v>401</v>
       </c>
       <c r="F17" s="248"/>
       <c r="G17" s="248"/>
@@ -15541,84 +15541,84 @@
       <c r="L18" s="113"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="266" t="s">
+      <c r="A19" s="287" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="267"/>
-      <c r="C19" s="267"/>
-      <c r="D19" s="267"/>
-      <c r="E19" s="267"/>
-      <c r="F19" s="267"/>
-      <c r="G19" s="267"/>
-      <c r="H19" s="267"/>
-      <c r="I19" s="267"/>
-      <c r="J19" s="267"/>
-      <c r="K19" s="267"/>
-      <c r="L19" s="268"/>
+      <c r="B19" s="288"/>
+      <c r="C19" s="288"/>
+      <c r="D19" s="288"/>
+      <c r="E19" s="288"/>
+      <c r="F19" s="288"/>
+      <c r="G19" s="288"/>
+      <c r="H19" s="288"/>
+      <c r="I19" s="288"/>
+      <c r="J19" s="288"/>
+      <c r="K19" s="288"/>
+      <c r="L19" s="289"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="269" t="s">
+      <c r="A20" s="290" t="s">
         <v>335</v>
       </c>
-      <c r="B20" s="270"/>
-      <c r="C20" s="270"/>
-      <c r="D20" s="270"/>
-      <c r="E20" s="270"/>
-      <c r="F20" s="270"/>
-      <c r="G20" s="270"/>
-      <c r="H20" s="270"/>
-      <c r="I20" s="270"/>
-      <c r="J20" s="270"/>
-      <c r="K20" s="270"/>
-      <c r="L20" s="271"/>
+      <c r="B20" s="291"/>
+      <c r="C20" s="291"/>
+      <c r="D20" s="291"/>
+      <c r="E20" s="291"/>
+      <c r="F20" s="291"/>
+      <c r="G20" s="291"/>
+      <c r="H20" s="291"/>
+      <c r="I20" s="291"/>
+      <c r="J20" s="291"/>
+      <c r="K20" s="291"/>
+      <c r="L20" s="292"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="272" t="s">
+      <c r="A21" s="293" t="s">
         <v>336</v>
       </c>
-      <c r="B21" s="273"/>
-      <c r="C21" s="273"/>
-      <c r="D21" s="273"/>
-      <c r="E21" s="273"/>
-      <c r="F21" s="273"/>
-      <c r="G21" s="273"/>
-      <c r="H21" s="273"/>
-      <c r="I21" s="273"/>
-      <c r="J21" s="273"/>
-      <c r="K21" s="273"/>
-      <c r="L21" s="274"/>
+      <c r="B21" s="271"/>
+      <c r="C21" s="271"/>
+      <c r="D21" s="271"/>
+      <c r="E21" s="271"/>
+      <c r="F21" s="271"/>
+      <c r="G21" s="271"/>
+      <c r="H21" s="271"/>
+      <c r="I21" s="271"/>
+      <c r="J21" s="271"/>
+      <c r="K21" s="271"/>
+      <c r="L21" s="272"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="272" t="s">
+      <c r="A22" s="293" t="s">
         <v>206</v>
       </c>
-      <c r="B22" s="273"/>
-      <c r="C22" s="273"/>
-      <c r="D22" s="273"/>
-      <c r="E22" s="273"/>
-      <c r="F22" s="273"/>
-      <c r="G22" s="273"/>
-      <c r="H22" s="273"/>
-      <c r="I22" s="273"/>
-      <c r="J22" s="273"/>
-      <c r="K22" s="273"/>
-      <c r="L22" s="274"/>
+      <c r="B22" s="271"/>
+      <c r="C22" s="271"/>
+      <c r="D22" s="271"/>
+      <c r="E22" s="271"/>
+      <c r="F22" s="271"/>
+      <c r="G22" s="271"/>
+      <c r="H22" s="271"/>
+      <c r="I22" s="271"/>
+      <c r="J22" s="271"/>
+      <c r="K22" s="271"/>
+      <c r="L22" s="272"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="275" t="s">
+      <c r="A23" s="294" t="s">
         <v>337</v>
       </c>
-      <c r="B23" s="276"/>
-      <c r="C23" s="276"/>
-      <c r="D23" s="276"/>
-      <c r="E23" s="276"/>
-      <c r="F23" s="276"/>
-      <c r="G23" s="276"/>
-      <c r="H23" s="276"/>
-      <c r="I23" s="276"/>
-      <c r="J23" s="276"/>
-      <c r="K23" s="276"/>
-      <c r="L23" s="277"/>
+      <c r="B23" s="295"/>
+      <c r="C23" s="295"/>
+      <c r="D23" s="295"/>
+      <c r="E23" s="295"/>
+      <c r="F23" s="295"/>
+      <c r="G23" s="295"/>
+      <c r="H23" s="295"/>
+      <c r="I23" s="295"/>
+      <c r="J23" s="295"/>
+      <c r="K23" s="295"/>
+      <c r="L23" s="296"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="113"/>
@@ -15635,332 +15635,332 @@
       <c r="L24" s="113"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="278" t="s">
+      <c r="A25" s="297" t="s">
         <v>333</v>
       </c>
-      <c r="B25" s="279"/>
-      <c r="C25" s="279"/>
-      <c r="D25" s="279"/>
-      <c r="E25" s="279"/>
-      <c r="F25" s="279"/>
-      <c r="G25" s="279"/>
-      <c r="H25" s="279"/>
-      <c r="I25" s="279"/>
-      <c r="J25" s="279"/>
-      <c r="K25" s="279"/>
-      <c r="L25" s="280"/>
+      <c r="B25" s="298"/>
+      <c r="C25" s="298"/>
+      <c r="D25" s="298"/>
+      <c r="E25" s="298"/>
+      <c r="F25" s="298"/>
+      <c r="G25" s="298"/>
+      <c r="H25" s="298"/>
+      <c r="I25" s="298"/>
+      <c r="J25" s="298"/>
+      <c r="K25" s="298"/>
+      <c r="L25" s="299"/>
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="255" t="s">
+      <c r="A26" s="276" t="s">
         <v>215</v>
       </c>
-      <c r="B26" s="256"/>
-      <c r="C26" s="256"/>
-      <c r="D26" s="256"/>
-      <c r="E26" s="256"/>
-      <c r="F26" s="256"/>
-      <c r="G26" s="256"/>
-      <c r="H26" s="256"/>
-      <c r="I26" s="256"/>
-      <c r="J26" s="256"/>
-      <c r="K26" s="256"/>
-      <c r="L26" s="257"/>
+      <c r="B26" s="277"/>
+      <c r="C26" s="277"/>
+      <c r="D26" s="277"/>
+      <c r="E26" s="277"/>
+      <c r="F26" s="277"/>
+      <c r="G26" s="277"/>
+      <c r="H26" s="277"/>
+      <c r="I26" s="277"/>
+      <c r="J26" s="277"/>
+      <c r="K26" s="277"/>
+      <c r="L26" s="278"/>
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="227">
         <v>1</v>
       </c>
-      <c r="B27" s="290" t="s">
+      <c r="B27" s="264" t="s">
         <v>214</v>
       </c>
-      <c r="C27" s="290"/>
-      <c r="D27" s="290"/>
-      <c r="E27" s="290"/>
-      <c r="F27" s="290"/>
-      <c r="G27" s="290"/>
-      <c r="H27" s="290"/>
-      <c r="I27" s="290"/>
-      <c r="J27" s="290"/>
-      <c r="K27" s="290"/>
-      <c r="L27" s="291"/>
+      <c r="C27" s="264"/>
+      <c r="D27" s="264"/>
+      <c r="E27" s="264"/>
+      <c r="F27" s="264"/>
+      <c r="G27" s="264"/>
+      <c r="H27" s="264"/>
+      <c r="I27" s="264"/>
+      <c r="J27" s="264"/>
+      <c r="K27" s="264"/>
+      <c r="L27" s="265"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="227">
         <v>2</v>
       </c>
-      <c r="B28" s="290" t="s">
+      <c r="B28" s="264" t="s">
         <v>329</v>
       </c>
-      <c r="C28" s="290"/>
-      <c r="D28" s="290"/>
-      <c r="E28" s="290"/>
-      <c r="F28" s="290"/>
-      <c r="G28" s="290"/>
-      <c r="H28" s="290"/>
-      <c r="I28" s="290"/>
-      <c r="J28" s="290"/>
-      <c r="K28" s="290"/>
-      <c r="L28" s="291"/>
+      <c r="C28" s="264"/>
+      <c r="D28" s="264"/>
+      <c r="E28" s="264"/>
+      <c r="F28" s="264"/>
+      <c r="G28" s="264"/>
+      <c r="H28" s="264"/>
+      <c r="I28" s="264"/>
+      <c r="J28" s="264"/>
+      <c r="K28" s="264"/>
+      <c r="L28" s="265"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="227">
         <v>3</v>
       </c>
-      <c r="B29" s="290" t="s">
+      <c r="B29" s="264" t="s">
         <v>207</v>
       </c>
-      <c r="C29" s="290"/>
-      <c r="D29" s="290"/>
-      <c r="E29" s="290"/>
-      <c r="F29" s="290"/>
-      <c r="G29" s="290"/>
-      <c r="H29" s="290"/>
-      <c r="I29" s="290"/>
-      <c r="J29" s="290"/>
-      <c r="K29" s="290"/>
-      <c r="L29" s="291"/>
+      <c r="C29" s="264"/>
+      <c r="D29" s="264"/>
+      <c r="E29" s="264"/>
+      <c r="F29" s="264"/>
+      <c r="G29" s="264"/>
+      <c r="H29" s="264"/>
+      <c r="I29" s="264"/>
+      <c r="J29" s="264"/>
+      <c r="K29" s="264"/>
+      <c r="L29" s="265"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="227">
         <v>4</v>
       </c>
-      <c r="B30" s="290" t="s">
+      <c r="B30" s="264" t="s">
         <v>338</v>
       </c>
-      <c r="C30" s="290"/>
-      <c r="D30" s="290"/>
-      <c r="E30" s="290"/>
-      <c r="F30" s="290"/>
-      <c r="G30" s="290"/>
-      <c r="H30" s="290"/>
-      <c r="I30" s="290"/>
-      <c r="J30" s="290"/>
-      <c r="K30" s="290"/>
-      <c r="L30" s="291"/>
+      <c r="C30" s="264"/>
+      <c r="D30" s="264"/>
+      <c r="E30" s="264"/>
+      <c r="F30" s="264"/>
+      <c r="G30" s="264"/>
+      <c r="H30" s="264"/>
+      <c r="I30" s="264"/>
+      <c r="J30" s="264"/>
+      <c r="K30" s="264"/>
+      <c r="L30" s="265"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="227">
         <v>5</v>
       </c>
-      <c r="B31" s="290" t="s">
+      <c r="B31" s="264" t="s">
         <v>208</v>
       </c>
-      <c r="C31" s="290"/>
-      <c r="D31" s="290"/>
-      <c r="E31" s="290"/>
-      <c r="F31" s="290"/>
-      <c r="G31" s="290"/>
-      <c r="H31" s="290"/>
-      <c r="I31" s="290"/>
-      <c r="J31" s="290"/>
-      <c r="K31" s="290"/>
-      <c r="L31" s="291"/>
+      <c r="C31" s="264"/>
+      <c r="D31" s="264"/>
+      <c r="E31" s="264"/>
+      <c r="F31" s="264"/>
+      <c r="G31" s="264"/>
+      <c r="H31" s="264"/>
+      <c r="I31" s="264"/>
+      <c r="J31" s="264"/>
+      <c r="K31" s="264"/>
+      <c r="L31" s="265"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="227"/>
-      <c r="B32" s="290" t="s">
+      <c r="B32" s="264" t="s">
         <v>209</v>
       </c>
-      <c r="C32" s="290"/>
-      <c r="D32" s="290"/>
-      <c r="E32" s="290"/>
-      <c r="F32" s="290"/>
-      <c r="G32" s="290"/>
-      <c r="H32" s="290"/>
-      <c r="I32" s="290"/>
-      <c r="J32" s="290"/>
-      <c r="K32" s="290"/>
-      <c r="L32" s="291"/>
+      <c r="C32" s="264"/>
+      <c r="D32" s="264"/>
+      <c r="E32" s="264"/>
+      <c r="F32" s="264"/>
+      <c r="G32" s="264"/>
+      <c r="H32" s="264"/>
+      <c r="I32" s="264"/>
+      <c r="J32" s="264"/>
+      <c r="K32" s="264"/>
+      <c r="L32" s="265"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="227"/>
-      <c r="B33" s="290" t="s">
+      <c r="B33" s="264" t="s">
         <v>210</v>
       </c>
-      <c r="C33" s="290"/>
-      <c r="D33" s="290"/>
-      <c r="E33" s="290"/>
-      <c r="F33" s="290"/>
-      <c r="G33" s="290"/>
-      <c r="H33" s="290"/>
-      <c r="I33" s="290"/>
-      <c r="J33" s="290"/>
-      <c r="K33" s="290"/>
-      <c r="L33" s="291"/>
+      <c r="C33" s="264"/>
+      <c r="D33" s="264"/>
+      <c r="E33" s="264"/>
+      <c r="F33" s="264"/>
+      <c r="G33" s="264"/>
+      <c r="H33" s="264"/>
+      <c r="I33" s="264"/>
+      <c r="J33" s="264"/>
+      <c r="K33" s="264"/>
+      <c r="L33" s="265"/>
       <c r="N33" s="106"/>
     </row>
     <row r="34" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="292" t="s">
+      <c r="A34" s="273" t="s">
         <v>216</v>
       </c>
-      <c r="B34" s="293"/>
-      <c r="C34" s="293"/>
-      <c r="D34" s="293"/>
-      <c r="E34" s="293"/>
-      <c r="F34" s="293"/>
-      <c r="G34" s="293"/>
-      <c r="H34" s="293"/>
-      <c r="I34" s="293"/>
-      <c r="J34" s="293"/>
-      <c r="K34" s="293"/>
-      <c r="L34" s="294"/>
+      <c r="B34" s="274"/>
+      <c r="C34" s="274"/>
+      <c r="D34" s="274"/>
+      <c r="E34" s="274"/>
+      <c r="F34" s="274"/>
+      <c r="G34" s="274"/>
+      <c r="H34" s="274"/>
+      <c r="I34" s="274"/>
+      <c r="J34" s="274"/>
+      <c r="K34" s="274"/>
+      <c r="L34" s="275"/>
       <c r="N34" s="106"/>
     </row>
     <row r="35" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="227">
         <v>1</v>
       </c>
-      <c r="B35" s="290" t="s">
+      <c r="B35" s="264" t="s">
         <v>211</v>
       </c>
-      <c r="C35" s="290"/>
-      <c r="D35" s="290"/>
-      <c r="E35" s="290"/>
-      <c r="F35" s="290"/>
-      <c r="G35" s="290"/>
-      <c r="H35" s="290"/>
-      <c r="I35" s="290"/>
-      <c r="J35" s="290"/>
-      <c r="K35" s="290"/>
-      <c r="L35" s="291"/>
+      <c r="C35" s="264"/>
+      <c r="D35" s="264"/>
+      <c r="E35" s="264"/>
+      <c r="F35" s="264"/>
+      <c r="G35" s="264"/>
+      <c r="H35" s="264"/>
+      <c r="I35" s="264"/>
+      <c r="J35" s="264"/>
+      <c r="K35" s="264"/>
+      <c r="L35" s="265"/>
       <c r="N35" s="106"/>
     </row>
     <row r="36" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="227"/>
-      <c r="B36" s="288" t="s">
+      <c r="B36" s="262" t="s">
         <v>339</v>
       </c>
-      <c r="C36" s="288"/>
-      <c r="D36" s="288"/>
-      <c r="E36" s="288"/>
-      <c r="F36" s="288"/>
-      <c r="G36" s="288"/>
-      <c r="H36" s="288"/>
-      <c r="I36" s="288"/>
-      <c r="J36" s="288"/>
-      <c r="K36" s="288"/>
-      <c r="L36" s="289"/>
+      <c r="C36" s="262"/>
+      <c r="D36" s="262"/>
+      <c r="E36" s="262"/>
+      <c r="F36" s="262"/>
+      <c r="G36" s="262"/>
+      <c r="H36" s="262"/>
+      <c r="I36" s="262"/>
+      <c r="J36" s="262"/>
+      <c r="K36" s="262"/>
+      <c r="L36" s="263"/>
       <c r="N36" s="106"/>
     </row>
     <row r="37" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="227">
         <v>2</v>
       </c>
-      <c r="B37" s="290" t="s">
+      <c r="B37" s="264" t="s">
         <v>332</v>
       </c>
-      <c r="C37" s="290"/>
-      <c r="D37" s="290"/>
-      <c r="E37" s="290"/>
-      <c r="F37" s="290"/>
-      <c r="G37" s="290"/>
-      <c r="H37" s="290"/>
-      <c r="I37" s="290"/>
-      <c r="J37" s="290"/>
-      <c r="K37" s="290"/>
-      <c r="L37" s="291"/>
+      <c r="C37" s="264"/>
+      <c r="D37" s="264"/>
+      <c r="E37" s="264"/>
+      <c r="F37" s="264"/>
+      <c r="G37" s="264"/>
+      <c r="H37" s="264"/>
+      <c r="I37" s="264"/>
+      <c r="J37" s="264"/>
+      <c r="K37" s="264"/>
+      <c r="L37" s="265"/>
       <c r="N37" s="106"/>
     </row>
     <row r="38" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="227">
         <v>3</v>
       </c>
-      <c r="B38" s="290" t="s">
+      <c r="B38" s="264" t="s">
         <v>321</v>
       </c>
-      <c r="C38" s="290"/>
-      <c r="D38" s="290"/>
-      <c r="E38" s="290"/>
-      <c r="F38" s="290"/>
-      <c r="G38" s="290"/>
-      <c r="H38" s="290"/>
-      <c r="I38" s="290"/>
-      <c r="J38" s="290"/>
-      <c r="K38" s="290"/>
-      <c r="L38" s="291"/>
+      <c r="C38" s="264"/>
+      <c r="D38" s="264"/>
+      <c r="E38" s="264"/>
+      <c r="F38" s="264"/>
+      <c r="G38" s="264"/>
+      <c r="H38" s="264"/>
+      <c r="I38" s="264"/>
+      <c r="J38" s="264"/>
+      <c r="K38" s="264"/>
+      <c r="L38" s="265"/>
       <c r="N38" s="106"/>
     </row>
     <row r="39" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="227">
         <v>4</v>
       </c>
-      <c r="B39" s="290" t="s">
+      <c r="B39" s="264" t="s">
         <v>340</v>
       </c>
-      <c r="C39" s="290"/>
-      <c r="D39" s="290"/>
-      <c r="E39" s="290"/>
-      <c r="F39" s="290"/>
-      <c r="G39" s="290"/>
-      <c r="H39" s="290"/>
-      <c r="I39" s="290"/>
-      <c r="J39" s="290"/>
-      <c r="K39" s="290"/>
-      <c r="L39" s="291"/>
+      <c r="C39" s="264"/>
+      <c r="D39" s="264"/>
+      <c r="E39" s="264"/>
+      <c r="F39" s="264"/>
+      <c r="G39" s="264"/>
+      <c r="H39" s="264"/>
+      <c r="I39" s="264"/>
+      <c r="J39" s="264"/>
+      <c r="K39" s="264"/>
+      <c r="L39" s="265"/>
       <c r="N39" s="106"/>
     </row>
     <row r="40" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="227">
         <v>5</v>
       </c>
-      <c r="B40" s="288" t="s">
+      <c r="B40" s="262" t="s">
         <v>322</v>
       </c>
-      <c r="C40" s="288"/>
-      <c r="D40" s="288"/>
-      <c r="E40" s="288"/>
-      <c r="F40" s="288"/>
-      <c r="G40" s="288"/>
-      <c r="H40" s="288"/>
-      <c r="I40" s="288"/>
-      <c r="J40" s="288"/>
-      <c r="K40" s="288"/>
-      <c r="L40" s="289"/>
+      <c r="C40" s="262"/>
+      <c r="D40" s="262"/>
+      <c r="E40" s="262"/>
+      <c r="F40" s="262"/>
+      <c r="G40" s="262"/>
+      <c r="H40" s="262"/>
+      <c r="I40" s="262"/>
+      <c r="J40" s="262"/>
+      <c r="K40" s="262"/>
+      <c r="L40" s="263"/>
       <c r="N40" s="106"/>
     </row>
     <row r="41" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="227">
         <v>6</v>
       </c>
-      <c r="B41" s="288" t="s">
+      <c r="B41" s="262" t="s">
         <v>327</v>
       </c>
-      <c r="C41" s="288"/>
-      <c r="D41" s="288"/>
-      <c r="E41" s="288"/>
-      <c r="F41" s="288"/>
-      <c r="G41" s="288"/>
-      <c r="H41" s="288"/>
-      <c r="I41" s="288"/>
-      <c r="J41" s="288"/>
-      <c r="K41" s="288"/>
-      <c r="L41" s="289"/>
+      <c r="C41" s="262"/>
+      <c r="D41" s="262"/>
+      <c r="E41" s="262"/>
+      <c r="F41" s="262"/>
+      <c r="G41" s="262"/>
+      <c r="H41" s="262"/>
+      <c r="I41" s="262"/>
+      <c r="J41" s="262"/>
+      <c r="K41" s="262"/>
+      <c r="L41" s="263"/>
       <c r="N41" s="106"/>
     </row>
     <row r="42" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="227">
         <v>7</v>
       </c>
-      <c r="B42" s="290" t="s">
+      <c r="B42" s="264" t="s">
         <v>323</v>
       </c>
-      <c r="C42" s="290"/>
-      <c r="D42" s="290"/>
-      <c r="E42" s="290"/>
-      <c r="F42" s="290"/>
-      <c r="G42" s="290"/>
-      <c r="H42" s="290"/>
-      <c r="I42" s="290"/>
-      <c r="J42" s="290"/>
-      <c r="K42" s="290"/>
-      <c r="L42" s="291"/>
+      <c r="C42" s="264"/>
+      <c r="D42" s="264"/>
+      <c r="E42" s="264"/>
+      <c r="F42" s="264"/>
+      <c r="G42" s="264"/>
+      <c r="H42" s="264"/>
+      <c r="I42" s="264"/>
+      <c r="J42" s="264"/>
+      <c r="K42" s="264"/>
+      <c r="L42" s="265"/>
     </row>
     <row r="43" spans="1:14" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="227"/>
@@ -15977,56 +15977,56 @@
       <c r="L43" s="229"/>
     </row>
     <row r="44" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="292" t="s">
+      <c r="A44" s="273" t="s">
         <v>326</v>
       </c>
-      <c r="B44" s="293"/>
-      <c r="C44" s="293"/>
-      <c r="D44" s="293"/>
-      <c r="E44" s="293"/>
-      <c r="F44" s="293"/>
-      <c r="G44" s="293"/>
-      <c r="H44" s="293"/>
-      <c r="I44" s="293"/>
-      <c r="J44" s="293"/>
-      <c r="K44" s="293"/>
-      <c r="L44" s="294"/>
+      <c r="B44" s="274"/>
+      <c r="C44" s="274"/>
+      <c r="D44" s="274"/>
+      <c r="E44" s="274"/>
+      <c r="F44" s="274"/>
+      <c r="G44" s="274"/>
+      <c r="H44" s="274"/>
+      <c r="I44" s="274"/>
+      <c r="J44" s="274"/>
+      <c r="K44" s="274"/>
+      <c r="L44" s="275"/>
     </row>
     <row r="45" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="230" t="s">
         <v>324</v>
       </c>
-      <c r="B45" s="290" t="s">
+      <c r="B45" s="264" t="s">
         <v>212</v>
       </c>
-      <c r="C45" s="290"/>
-      <c r="D45" s="290"/>
-      <c r="E45" s="290"/>
-      <c r="F45" s="290"/>
-      <c r="G45" s="290"/>
-      <c r="H45" s="290"/>
-      <c r="I45" s="290"/>
-      <c r="J45" s="290"/>
-      <c r="K45" s="290"/>
-      <c r="L45" s="291"/>
+      <c r="C45" s="264"/>
+      <c r="D45" s="264"/>
+      <c r="E45" s="264"/>
+      <c r="F45" s="264"/>
+      <c r="G45" s="264"/>
+      <c r="H45" s="264"/>
+      <c r="I45" s="264"/>
+      <c r="J45" s="264"/>
+      <c r="K45" s="264"/>
+      <c r="L45" s="265"/>
     </row>
     <row r="46" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="231" t="s">
         <v>325</v>
       </c>
-      <c r="B46" s="300" t="s">
+      <c r="B46" s="266" t="s">
         <v>328</v>
       </c>
-      <c r="C46" s="300"/>
-      <c r="D46" s="300"/>
-      <c r="E46" s="300"/>
-      <c r="F46" s="300"/>
-      <c r="G46" s="300"/>
-      <c r="H46" s="300"/>
-      <c r="I46" s="300"/>
-      <c r="J46" s="300"/>
-      <c r="K46" s="300"/>
-      <c r="L46" s="301"/>
+      <c r="C46" s="266"/>
+      <c r="D46" s="266"/>
+      <c r="E46" s="266"/>
+      <c r="F46" s="266"/>
+      <c r="G46" s="266"/>
+      <c r="H46" s="266"/>
+      <c r="I46" s="266"/>
+      <c r="J46" s="266"/>
+      <c r="K46" s="266"/>
+      <c r="L46" s="267"/>
     </row>
     <row r="47" spans="1:14" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="160"/>
@@ -16043,20 +16043,20 @@
       <c r="L47" s="113"/>
     </row>
     <row r="48" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="302" t="s">
+      <c r="A48" s="268" t="s">
         <v>240</v>
       </c>
-      <c r="B48" s="303"/>
-      <c r="C48" s="303"/>
-      <c r="D48" s="303"/>
-      <c r="E48" s="303"/>
-      <c r="F48" s="303"/>
-      <c r="G48" s="303"/>
-      <c r="H48" s="303"/>
-      <c r="I48" s="303"/>
-      <c r="J48" s="303"/>
-      <c r="K48" s="303"/>
-      <c r="L48" s="304"/>
+      <c r="B48" s="269"/>
+      <c r="C48" s="269"/>
+      <c r="D48" s="269"/>
+      <c r="E48" s="269"/>
+      <c r="F48" s="269"/>
+      <c r="G48" s="269"/>
+      <c r="H48" s="269"/>
+      <c r="I48" s="269"/>
+      <c r="J48" s="269"/>
+      <c r="K48" s="269"/>
+      <c r="L48" s="270"/>
     </row>
     <row r="49" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="234" t="s">
@@ -16144,90 +16144,90 @@
       <c r="B54" s="168" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="273" t="s">
+      <c r="C54" s="271" t="s">
         <v>312</v>
       </c>
-      <c r="D54" s="273"/>
-      <c r="E54" s="273"/>
-      <c r="F54" s="273"/>
-      <c r="G54" s="273"/>
-      <c r="H54" s="273"/>
-      <c r="I54" s="273"/>
-      <c r="J54" s="273"/>
-      <c r="K54" s="273"/>
-      <c r="L54" s="274"/>
+      <c r="D54" s="271"/>
+      <c r="E54" s="271"/>
+      <c r="F54" s="271"/>
+      <c r="G54" s="271"/>
+      <c r="H54" s="271"/>
+      <c r="I54" s="271"/>
+      <c r="J54" s="271"/>
+      <c r="K54" s="271"/>
+      <c r="L54" s="272"/>
     </row>
     <row r="55" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="167"/>
       <c r="B55" s="168" t="s">
         <v>313</v>
       </c>
-      <c r="C55" s="273" t="s">
+      <c r="C55" s="271" t="s">
         <v>314</v>
       </c>
-      <c r="D55" s="273"/>
-      <c r="E55" s="273"/>
-      <c r="F55" s="273"/>
-      <c r="G55" s="273"/>
-      <c r="H55" s="273"/>
-      <c r="I55" s="273"/>
-      <c r="J55" s="273"/>
-      <c r="K55" s="273"/>
-      <c r="L55" s="274"/>
+      <c r="D55" s="271"/>
+      <c r="E55" s="271"/>
+      <c r="F55" s="271"/>
+      <c r="G55" s="271"/>
+      <c r="H55" s="271"/>
+      <c r="I55" s="271"/>
+      <c r="J55" s="271"/>
+      <c r="K55" s="271"/>
+      <c r="L55" s="272"/>
     </row>
     <row r="56" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="167"/>
       <c r="B56" s="168" t="s">
         <v>382</v>
       </c>
-      <c r="C56" s="273" t="s">
+      <c r="C56" s="271" t="s">
         <v>383</v>
       </c>
-      <c r="D56" s="273"/>
-      <c r="E56" s="273"/>
-      <c r="F56" s="273"/>
-      <c r="G56" s="273"/>
-      <c r="H56" s="273"/>
-      <c r="I56" s="273"/>
-      <c r="J56" s="273"/>
-      <c r="K56" s="273"/>
-      <c r="L56" s="274"/>
+      <c r="D56" s="271"/>
+      <c r="E56" s="271"/>
+      <c r="F56" s="271"/>
+      <c r="G56" s="271"/>
+      <c r="H56" s="271"/>
+      <c r="I56" s="271"/>
+      <c r="J56" s="271"/>
+      <c r="K56" s="271"/>
+      <c r="L56" s="272"/>
     </row>
     <row r="57" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="167"/>
       <c r="B57" s="168" t="s">
         <v>138</v>
       </c>
-      <c r="C57" s="273" t="s">
+      <c r="C57" s="271" t="s">
         <v>139</v>
       </c>
-      <c r="D57" s="273"/>
-      <c r="E57" s="273"/>
-      <c r="F57" s="273"/>
-      <c r="G57" s="273"/>
-      <c r="H57" s="273"/>
-      <c r="I57" s="273"/>
-      <c r="J57" s="273"/>
-      <c r="K57" s="273"/>
-      <c r="L57" s="274"/>
+      <c r="D57" s="271"/>
+      <c r="E57" s="271"/>
+      <c r="F57" s="271"/>
+      <c r="G57" s="271"/>
+      <c r="H57" s="271"/>
+      <c r="I57" s="271"/>
+      <c r="J57" s="271"/>
+      <c r="K57" s="271"/>
+      <c r="L57" s="272"/>
     </row>
     <row r="58" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="167"/>
       <c r="B58" s="168" t="s">
         <v>238</v>
       </c>
-      <c r="C58" s="273" t="s">
+      <c r="C58" s="271" t="s">
         <v>239</v>
       </c>
-      <c r="D58" s="273"/>
-      <c r="E58" s="273"/>
-      <c r="F58" s="273"/>
-      <c r="G58" s="273"/>
-      <c r="H58" s="273"/>
-      <c r="I58" s="273"/>
-      <c r="J58" s="273"/>
-      <c r="K58" s="273"/>
-      <c r="L58" s="274"/>
+      <c r="D58" s="271"/>
+      <c r="E58" s="271"/>
+      <c r="F58" s="271"/>
+      <c r="G58" s="271"/>
+      <c r="H58" s="271"/>
+      <c r="I58" s="271"/>
+      <c r="J58" s="271"/>
+      <c r="K58" s="271"/>
+      <c r="L58" s="272"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="167"/>
@@ -16252,18 +16252,18 @@
       <c r="B60" s="168" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="273" t="s">
+      <c r="C60" s="271" t="s">
         <v>316</v>
       </c>
-      <c r="D60" s="273"/>
-      <c r="E60" s="273"/>
-      <c r="F60" s="273"/>
-      <c r="G60" s="273"/>
-      <c r="H60" s="273"/>
-      <c r="I60" s="273"/>
-      <c r="J60" s="273"/>
-      <c r="K60" s="273"/>
-      <c r="L60" s="274"/>
+      <c r="D60" s="271"/>
+      <c r="E60" s="271"/>
+      <c r="F60" s="271"/>
+      <c r="G60" s="271"/>
+      <c r="H60" s="271"/>
+      <c r="I60" s="271"/>
+      <c r="J60" s="271"/>
+      <c r="K60" s="271"/>
+      <c r="L60" s="272"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="167"/>
@@ -16341,7 +16341,7 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A72" s="45" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.35">
@@ -16363,25 +16363,56 @@
       </c>
     </row>
     <row r="78" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="299" t="s">
-        <v>398</v>
-      </c>
-      <c r="B78" s="299"/>
-      <c r="C78" s="299"/>
-      <c r="D78" s="299"/>
-      <c r="E78" s="299"/>
-      <c r="F78" s="299"/>
-      <c r="G78" s="299"/>
-      <c r="H78" s="299"/>
-      <c r="I78" s="299"/>
-      <c r="J78" s="299"/>
-      <c r="K78" s="299"/>
-      <c r="L78" s="299"/>
+      <c r="A78" s="261" t="s">
+        <v>407</v>
+      </c>
+      <c r="B78" s="261"/>
+      <c r="C78" s="261"/>
+      <c r="D78" s="261"/>
+      <c r="E78" s="261"/>
+      <c r="F78" s="261"/>
+      <c r="G78" s="261"/>
+      <c r="H78" s="261"/>
+      <c r="I78" s="261"/>
+      <c r="J78" s="261"/>
+      <c r="K78" s="261"/>
+      <c r="L78" s="261"/>
     </row>
     <row r="83" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="84" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="B40:L40"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B30:L30"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B39:L39"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="B13:L13"/>
     <mergeCell ref="B14:L14"/>
@@ -16398,37 +16429,6 @@
     <mergeCell ref="C55:L55"/>
     <mergeCell ref="C60:L60"/>
     <mergeCell ref="A44:L44"/>
-    <mergeCell ref="C56:L56"/>
-    <mergeCell ref="B40:L40"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B8:L8"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="B11:L11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A67" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -31719,10 +31719,10 @@
         <v>45681</v>
       </c>
       <c r="B9" s="149" t="s">
+        <v>401</v>
+      </c>
+      <c r="C9" s="56" t="s">
         <v>402</v>
-      </c>
-      <c r="C9" s="56" t="s">
-        <v>403</v>
       </c>
       <c r="D9" s="55">
         <v>0.25</v>
@@ -31743,10 +31743,10 @@
         <v>45681</v>
       </c>
       <c r="B10" s="149" t="s">
+        <v>405</v>
+      </c>
+      <c r="C10" s="56" t="s">
         <v>406</v>
-      </c>
-      <c r="C10" s="56" t="s">
-        <v>407</v>
       </c>
       <c r="D10" s="55">
         <v>1</v>
@@ -31755,7 +31755,7 @@
         <v>285</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G10" s="57">
         <v>45678</v>
@@ -32301,7 +32301,7 @@
         <v>8.6522179999999995</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="F19" s="254" t="s">
         <v>248</v>
@@ -38523,16 +38523,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="339" t="e">
+      <c r="A1" s="340" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="339"/>
-      <c r="C1" s="339"/>
-      <c r="D1" s="339"/>
-      <c r="E1" s="339"/>
-      <c r="F1" s="339"/>
-      <c r="G1" s="339"/>
+      <c r="B1" s="340"/>
+      <c r="C1" s="340"/>
+      <c r="D1" s="340"/>
+      <c r="E1" s="340"/>
+      <c r="F1" s="340"/>
+      <c r="G1" s="340"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -38641,11 +38641,11 @@
         <v>80</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="340"/>
-      <c r="D10" s="340"/>
-      <c r="E10" s="340"/>
-      <c r="F10" s="340"/>
-      <c r="G10" s="340"/>
+      <c r="C10" s="339"/>
+      <c r="D10" s="339"/>
+      <c r="E10" s="339"/>
+      <c r="F10" s="339"/>
+      <c r="G10" s="339"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -39908,6 +39908,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -39915,12 +39921,6 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>

</xml_diff>

<commit_message>
Clear all entries in excel file
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE4A06A-523F-436C-B8BE-892C085EBEE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA7DA3E-1374-41BB-B7F8-C79DB2B9721C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="62" r:id="rId1"/>
@@ -3401,69 +3401,6 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="6" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3518,6 +3455,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3550,6 +3493,63 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3653,11 +3653,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -15239,20 +15239,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="279" t="s">
+      <c r="A1" s="258" t="s">
         <v>350</v>
       </c>
-      <c r="B1" s="279"/>
-      <c r="C1" s="279"/>
-      <c r="D1" s="279"/>
-      <c r="E1" s="279"/>
-      <c r="F1" s="279"/>
-      <c r="G1" s="279"/>
-      <c r="H1" s="279"/>
-      <c r="I1" s="279"/>
-      <c r="J1" s="279"/>
-      <c r="K1" s="279"/>
-      <c r="L1" s="279"/>
+      <c r="B1" s="258"/>
+      <c r="C1" s="258"/>
+      <c r="D1" s="258"/>
+      <c r="E1" s="258"/>
+      <c r="F1" s="258"/>
+      <c r="G1" s="258"/>
+      <c r="H1" s="258"/>
+      <c r="I1" s="258"/>
+      <c r="J1" s="258"/>
+      <c r="K1" s="258"/>
+      <c r="L1" s="258"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -15278,41 +15278,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="280" t="s">
+      <c r="A4" s="259" t="s">
         <v>351</v>
       </c>
-      <c r="B4" s="281"/>
-      <c r="C4" s="281"/>
-      <c r="D4" s="281"/>
-      <c r="E4" s="281"/>
-      <c r="F4" s="281"/>
-      <c r="G4" s="281"/>
-      <c r="H4" s="281"/>
-      <c r="I4" s="281"/>
-      <c r="J4" s="281"/>
-      <c r="K4" s="281"/>
-      <c r="L4" s="282"/>
-      <c r="N4" s="283"/>
-      <c r="O4" s="283"/>
-      <c r="P4" s="283"/>
-      <c r="Q4" s="283"/>
-      <c r="R4" s="283"/>
+      <c r="B4" s="260"/>
+      <c r="C4" s="260"/>
+      <c r="D4" s="260"/>
+      <c r="E4" s="260"/>
+      <c r="F4" s="260"/>
+      <c r="G4" s="260"/>
+      <c r="H4" s="260"/>
+      <c r="I4" s="260"/>
+      <c r="J4" s="260"/>
+      <c r="K4" s="260"/>
+      <c r="L4" s="261"/>
+      <c r="N4" s="262"/>
+      <c r="O4" s="262"/>
+      <c r="P4" s="262"/>
+      <c r="Q4" s="262"/>
+      <c r="R4" s="262"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="284" t="s">
+      <c r="A5" s="263" t="s">
         <v>334</v>
       </c>
-      <c r="B5" s="285"/>
-      <c r="C5" s="285"/>
-      <c r="D5" s="285"/>
-      <c r="E5" s="285"/>
-      <c r="F5" s="285"/>
-      <c r="G5" s="285"/>
-      <c r="H5" s="285"/>
-      <c r="I5" s="285"/>
-      <c r="J5" s="285"/>
-      <c r="K5" s="285"/>
-      <c r="L5" s="286"/>
+      <c r="B5" s="264"/>
+      <c r="C5" s="264"/>
+      <c r="D5" s="264"/>
+      <c r="E5" s="264"/>
+      <c r="F5" s="264"/>
+      <c r="G5" s="264"/>
+      <c r="H5" s="264"/>
+      <c r="I5" s="264"/>
+      <c r="J5" s="264"/>
+      <c r="K5" s="264"/>
+      <c r="L5" s="265"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15320,20 +15320,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="284" t="s">
+      <c r="A6" s="263" t="s">
         <v>352</v>
       </c>
-      <c r="B6" s="285"/>
-      <c r="C6" s="285"/>
-      <c r="D6" s="285"/>
-      <c r="E6" s="285"/>
-      <c r="F6" s="285"/>
-      <c r="G6" s="285"/>
-      <c r="H6" s="285"/>
-      <c r="I6" s="285"/>
-      <c r="J6" s="285"/>
-      <c r="K6" s="285"/>
-      <c r="L6" s="286"/>
+      <c r="B6" s="264"/>
+      <c r="C6" s="264"/>
+      <c r="D6" s="264"/>
+      <c r="E6" s="264"/>
+      <c r="F6" s="264"/>
+      <c r="G6" s="264"/>
+      <c r="H6" s="264"/>
+      <c r="I6" s="264"/>
+      <c r="J6" s="264"/>
+      <c r="K6" s="264"/>
+      <c r="L6" s="265"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15342,19 +15342,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="232"/>
-      <c r="B7" s="285" t="s">
+      <c r="B7" s="264" t="s">
         <v>353</v>
       </c>
-      <c r="C7" s="285"/>
-      <c r="D7" s="285"/>
-      <c r="E7" s="285"/>
-      <c r="F7" s="285"/>
-      <c r="G7" s="285"/>
-      <c r="H7" s="285"/>
-      <c r="I7" s="285"/>
-      <c r="J7" s="285"/>
-      <c r="K7" s="285"/>
-      <c r="L7" s="286"/>
+      <c r="C7" s="264"/>
+      <c r="D7" s="264"/>
+      <c r="E7" s="264"/>
+      <c r="F7" s="264"/>
+      <c r="G7" s="264"/>
+      <c r="H7" s="264"/>
+      <c r="I7" s="264"/>
+      <c r="J7" s="264"/>
+      <c r="K7" s="264"/>
+      <c r="L7" s="265"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15363,19 +15363,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="233"/>
-      <c r="B8" s="300" t="s">
+      <c r="B8" s="281" t="s">
         <v>354</v>
       </c>
-      <c r="C8" s="300"/>
-      <c r="D8" s="300"/>
-      <c r="E8" s="300"/>
-      <c r="F8" s="300"/>
-      <c r="G8" s="300"/>
-      <c r="H8" s="300"/>
-      <c r="I8" s="300"/>
-      <c r="J8" s="300"/>
-      <c r="K8" s="300"/>
-      <c r="L8" s="301"/>
+      <c r="C8" s="281"/>
+      <c r="D8" s="281"/>
+      <c r="E8" s="281"/>
+      <c r="F8" s="281"/>
+      <c r="G8" s="281"/>
+      <c r="H8" s="281"/>
+      <c r="I8" s="281"/>
+      <c r="J8" s="281"/>
+      <c r="K8" s="281"/>
+      <c r="L8" s="282"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15397,38 +15397,38 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="302" t="s">
+      <c r="A10" s="283" t="s">
         <v>389</v>
       </c>
-      <c r="B10" s="303"/>
-      <c r="C10" s="303"/>
-      <c r="D10" s="303"/>
-      <c r="E10" s="303"/>
-      <c r="F10" s="303"/>
-      <c r="G10" s="303"/>
-      <c r="H10" s="303"/>
-      <c r="I10" s="303"/>
-      <c r="J10" s="303"/>
-      <c r="K10" s="303"/>
-      <c r="L10" s="304"/>
+      <c r="B10" s="284"/>
+      <c r="C10" s="284"/>
+      <c r="D10" s="284"/>
+      <c r="E10" s="284"/>
+      <c r="F10" s="284"/>
+      <c r="G10" s="284"/>
+      <c r="H10" s="284"/>
+      <c r="I10" s="284"/>
+      <c r="J10" s="284"/>
+      <c r="K10" s="284"/>
+      <c r="L10" s="285"/>
     </row>
     <row r="11" spans="1:18" s="58" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="253" t="s">
         <v>390</v>
       </c>
-      <c r="B11" s="257" t="s">
+      <c r="B11" s="286" t="s">
         <v>393</v>
       </c>
-      <c r="C11" s="257"/>
-      <c r="D11" s="257"/>
-      <c r="E11" s="257"/>
-      <c r="F11" s="257"/>
-      <c r="G11" s="257"/>
-      <c r="H11" s="257"/>
-      <c r="I11" s="257"/>
-      <c r="J11" s="257"/>
-      <c r="K11" s="257"/>
-      <c r="L11" s="258"/>
+      <c r="C11" s="286"/>
+      <c r="D11" s="286"/>
+      <c r="E11" s="286"/>
+      <c r="F11" s="286"/>
+      <c r="G11" s="286"/>
+      <c r="H11" s="286"/>
+      <c r="I11" s="286"/>
+      <c r="J11" s="286"/>
+      <c r="K11" s="286"/>
+      <c r="L11" s="287"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="161.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="245"/>
@@ -15448,51 +15448,51 @@
       <c r="A13" s="253" t="s">
         <v>391</v>
       </c>
-      <c r="B13" s="257" t="s">
+      <c r="B13" s="286" t="s">
         <v>394</v>
       </c>
-      <c r="C13" s="257"/>
-      <c r="D13" s="257"/>
-      <c r="E13" s="257"/>
-      <c r="F13" s="257"/>
-      <c r="G13" s="257"/>
-      <c r="H13" s="257"/>
-      <c r="I13" s="257"/>
-      <c r="J13" s="257"/>
-      <c r="K13" s="257"/>
-      <c r="L13" s="258"/>
+      <c r="C13" s="286"/>
+      <c r="D13" s="286"/>
+      <c r="E13" s="286"/>
+      <c r="F13" s="286"/>
+      <c r="G13" s="286"/>
+      <c r="H13" s="286"/>
+      <c r="I13" s="286"/>
+      <c r="J13" s="286"/>
+      <c r="K13" s="286"/>
+      <c r="L13" s="287"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="90.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="245"/>
-      <c r="B14" s="259"/>
-      <c r="C14" s="259"/>
-      <c r="D14" s="259"/>
-      <c r="E14" s="259"/>
-      <c r="F14" s="259"/>
-      <c r="G14" s="259"/>
-      <c r="H14" s="259"/>
-      <c r="I14" s="259"/>
-      <c r="J14" s="259"/>
-      <c r="K14" s="259"/>
-      <c r="L14" s="260"/>
+      <c r="B14" s="297"/>
+      <c r="C14" s="297"/>
+      <c r="D14" s="297"/>
+      <c r="E14" s="297"/>
+      <c r="F14" s="297"/>
+      <c r="G14" s="297"/>
+      <c r="H14" s="297"/>
+      <c r="I14" s="297"/>
+      <c r="J14" s="297"/>
+      <c r="K14" s="297"/>
+      <c r="L14" s="298"/>
     </row>
     <row r="15" spans="1:18" s="58" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="253" t="s">
         <v>392</v>
       </c>
-      <c r="B15" s="257" t="s">
+      <c r="B15" s="286" t="s">
         <v>395</v>
       </c>
-      <c r="C15" s="257"/>
-      <c r="D15" s="257"/>
-      <c r="E15" s="257"/>
-      <c r="F15" s="257"/>
-      <c r="G15" s="257"/>
-      <c r="H15" s="257"/>
-      <c r="I15" s="257"/>
-      <c r="J15" s="257"/>
-      <c r="K15" s="257"/>
-      <c r="L15" s="258"/>
+      <c r="C15" s="286"/>
+      <c r="D15" s="286"/>
+      <c r="E15" s="286"/>
+      <c r="F15" s="286"/>
+      <c r="G15" s="286"/>
+      <c r="H15" s="286"/>
+      <c r="I15" s="286"/>
+      <c r="J15" s="286"/>
+      <c r="K15" s="286"/>
+      <c r="L15" s="287"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="245"/>
@@ -15509,12 +15509,12 @@
       <c r="L16" s="252"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="255" t="s">
+      <c r="A17" s="295" t="s">
         <v>399</v>
       </c>
-      <c r="B17" s="256"/>
-      <c r="C17" s="256"/>
-      <c r="D17" s="256"/>
+      <c r="B17" s="296"/>
+      <c r="C17" s="296"/>
+      <c r="D17" s="296"/>
       <c r="E17" s="250" t="s">
         <v>400</v>
       </c>
@@ -15541,84 +15541,84 @@
       <c r="L18" s="113"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="287" t="s">
+      <c r="A19" s="266" t="s">
         <v>205</v>
       </c>
-      <c r="B19" s="288"/>
-      <c r="C19" s="288"/>
-      <c r="D19" s="288"/>
-      <c r="E19" s="288"/>
-      <c r="F19" s="288"/>
-      <c r="G19" s="288"/>
-      <c r="H19" s="288"/>
-      <c r="I19" s="288"/>
-      <c r="J19" s="288"/>
-      <c r="K19" s="288"/>
-      <c r="L19" s="289"/>
+      <c r="B19" s="267"/>
+      <c r="C19" s="267"/>
+      <c r="D19" s="267"/>
+      <c r="E19" s="267"/>
+      <c r="F19" s="267"/>
+      <c r="G19" s="267"/>
+      <c r="H19" s="267"/>
+      <c r="I19" s="267"/>
+      <c r="J19" s="267"/>
+      <c r="K19" s="267"/>
+      <c r="L19" s="268"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="290" t="s">
+      <c r="A20" s="269" t="s">
         <v>335</v>
       </c>
-      <c r="B20" s="291"/>
-      <c r="C20" s="291"/>
-      <c r="D20" s="291"/>
-      <c r="E20" s="291"/>
-      <c r="F20" s="291"/>
-      <c r="G20" s="291"/>
-      <c r="H20" s="291"/>
-      <c r="I20" s="291"/>
-      <c r="J20" s="291"/>
-      <c r="K20" s="291"/>
-      <c r="L20" s="292"/>
+      <c r="B20" s="270"/>
+      <c r="C20" s="270"/>
+      <c r="D20" s="270"/>
+      <c r="E20" s="270"/>
+      <c r="F20" s="270"/>
+      <c r="G20" s="270"/>
+      <c r="H20" s="270"/>
+      <c r="I20" s="270"/>
+      <c r="J20" s="270"/>
+      <c r="K20" s="270"/>
+      <c r="L20" s="271"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="293" t="s">
+      <c r="A21" s="272" t="s">
         <v>336</v>
       </c>
-      <c r="B21" s="271"/>
-      <c r="C21" s="271"/>
-      <c r="D21" s="271"/>
-      <c r="E21" s="271"/>
-      <c r="F21" s="271"/>
-      <c r="G21" s="271"/>
-      <c r="H21" s="271"/>
-      <c r="I21" s="271"/>
-      <c r="J21" s="271"/>
-      <c r="K21" s="271"/>
-      <c r="L21" s="272"/>
+      <c r="B21" s="273"/>
+      <c r="C21" s="273"/>
+      <c r="D21" s="273"/>
+      <c r="E21" s="273"/>
+      <c r="F21" s="273"/>
+      <c r="G21" s="273"/>
+      <c r="H21" s="273"/>
+      <c r="I21" s="273"/>
+      <c r="J21" s="273"/>
+      <c r="K21" s="273"/>
+      <c r="L21" s="274"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="293" t="s">
+      <c r="A22" s="272" t="s">
         <v>206</v>
       </c>
-      <c r="B22" s="271"/>
-      <c r="C22" s="271"/>
-      <c r="D22" s="271"/>
-      <c r="E22" s="271"/>
-      <c r="F22" s="271"/>
-      <c r="G22" s="271"/>
-      <c r="H22" s="271"/>
-      <c r="I22" s="271"/>
-      <c r="J22" s="271"/>
-      <c r="K22" s="271"/>
-      <c r="L22" s="272"/>
+      <c r="B22" s="273"/>
+      <c r="C22" s="273"/>
+      <c r="D22" s="273"/>
+      <c r="E22" s="273"/>
+      <c r="F22" s="273"/>
+      <c r="G22" s="273"/>
+      <c r="H22" s="273"/>
+      <c r="I22" s="273"/>
+      <c r="J22" s="273"/>
+      <c r="K22" s="273"/>
+      <c r="L22" s="274"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="294" t="s">
+      <c r="A23" s="275" t="s">
         <v>337</v>
       </c>
-      <c r="B23" s="295"/>
-      <c r="C23" s="295"/>
-      <c r="D23" s="295"/>
-      <c r="E23" s="295"/>
-      <c r="F23" s="295"/>
-      <c r="G23" s="295"/>
-      <c r="H23" s="295"/>
-      <c r="I23" s="295"/>
-      <c r="J23" s="295"/>
-      <c r="K23" s="295"/>
-      <c r="L23" s="296"/>
+      <c r="B23" s="276"/>
+      <c r="C23" s="276"/>
+      <c r="D23" s="276"/>
+      <c r="E23" s="276"/>
+      <c r="F23" s="276"/>
+      <c r="G23" s="276"/>
+      <c r="H23" s="276"/>
+      <c r="I23" s="276"/>
+      <c r="J23" s="276"/>
+      <c r="K23" s="276"/>
+      <c r="L23" s="277"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="113"/>
@@ -15635,332 +15635,332 @@
       <c r="L24" s="113"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="297" t="s">
+      <c r="A25" s="278" t="s">
         <v>333</v>
       </c>
-      <c r="B25" s="298"/>
-      <c r="C25" s="298"/>
-      <c r="D25" s="298"/>
-      <c r="E25" s="298"/>
-      <c r="F25" s="298"/>
-      <c r="G25" s="298"/>
-      <c r="H25" s="298"/>
-      <c r="I25" s="298"/>
-      <c r="J25" s="298"/>
-      <c r="K25" s="298"/>
-      <c r="L25" s="299"/>
+      <c r="B25" s="279"/>
+      <c r="C25" s="279"/>
+      <c r="D25" s="279"/>
+      <c r="E25" s="279"/>
+      <c r="F25" s="279"/>
+      <c r="G25" s="279"/>
+      <c r="H25" s="279"/>
+      <c r="I25" s="279"/>
+      <c r="J25" s="279"/>
+      <c r="K25" s="279"/>
+      <c r="L25" s="280"/>
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="276" t="s">
+      <c r="A26" s="255" t="s">
         <v>215</v>
       </c>
-      <c r="B26" s="277"/>
-      <c r="C26" s="277"/>
-      <c r="D26" s="277"/>
-      <c r="E26" s="277"/>
-      <c r="F26" s="277"/>
-      <c r="G26" s="277"/>
-      <c r="H26" s="277"/>
-      <c r="I26" s="277"/>
-      <c r="J26" s="277"/>
-      <c r="K26" s="277"/>
-      <c r="L26" s="278"/>
+      <c r="B26" s="256"/>
+      <c r="C26" s="256"/>
+      <c r="D26" s="256"/>
+      <c r="E26" s="256"/>
+      <c r="F26" s="256"/>
+      <c r="G26" s="256"/>
+      <c r="H26" s="256"/>
+      <c r="I26" s="256"/>
+      <c r="J26" s="256"/>
+      <c r="K26" s="256"/>
+      <c r="L26" s="257"/>
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="227">
         <v>1</v>
       </c>
-      <c r="B27" s="264" t="s">
+      <c r="B27" s="290" t="s">
         <v>214</v>
       </c>
-      <c r="C27" s="264"/>
-      <c r="D27" s="264"/>
-      <c r="E27" s="264"/>
-      <c r="F27" s="264"/>
-      <c r="G27" s="264"/>
-      <c r="H27" s="264"/>
-      <c r="I27" s="264"/>
-      <c r="J27" s="264"/>
-      <c r="K27" s="264"/>
-      <c r="L27" s="265"/>
+      <c r="C27" s="290"/>
+      <c r="D27" s="290"/>
+      <c r="E27" s="290"/>
+      <c r="F27" s="290"/>
+      <c r="G27" s="290"/>
+      <c r="H27" s="290"/>
+      <c r="I27" s="290"/>
+      <c r="J27" s="290"/>
+      <c r="K27" s="290"/>
+      <c r="L27" s="291"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="227">
         <v>2</v>
       </c>
-      <c r="B28" s="264" t="s">
+      <c r="B28" s="290" t="s">
         <v>329</v>
       </c>
-      <c r="C28" s="264"/>
-      <c r="D28" s="264"/>
-      <c r="E28" s="264"/>
-      <c r="F28" s="264"/>
-      <c r="G28" s="264"/>
-      <c r="H28" s="264"/>
-      <c r="I28" s="264"/>
-      <c r="J28" s="264"/>
-      <c r="K28" s="264"/>
-      <c r="L28" s="265"/>
+      <c r="C28" s="290"/>
+      <c r="D28" s="290"/>
+      <c r="E28" s="290"/>
+      <c r="F28" s="290"/>
+      <c r="G28" s="290"/>
+      <c r="H28" s="290"/>
+      <c r="I28" s="290"/>
+      <c r="J28" s="290"/>
+      <c r="K28" s="290"/>
+      <c r="L28" s="291"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="227">
         <v>3</v>
       </c>
-      <c r="B29" s="264" t="s">
+      <c r="B29" s="290" t="s">
         <v>207</v>
       </c>
-      <c r="C29" s="264"/>
-      <c r="D29" s="264"/>
-      <c r="E29" s="264"/>
-      <c r="F29" s="264"/>
-      <c r="G29" s="264"/>
-      <c r="H29" s="264"/>
-      <c r="I29" s="264"/>
-      <c r="J29" s="264"/>
-      <c r="K29" s="264"/>
-      <c r="L29" s="265"/>
+      <c r="C29" s="290"/>
+      <c r="D29" s="290"/>
+      <c r="E29" s="290"/>
+      <c r="F29" s="290"/>
+      <c r="G29" s="290"/>
+      <c r="H29" s="290"/>
+      <c r="I29" s="290"/>
+      <c r="J29" s="290"/>
+      <c r="K29" s="290"/>
+      <c r="L29" s="291"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="227">
         <v>4</v>
       </c>
-      <c r="B30" s="264" t="s">
+      <c r="B30" s="290" t="s">
         <v>338</v>
       </c>
-      <c r="C30" s="264"/>
-      <c r="D30" s="264"/>
-      <c r="E30" s="264"/>
-      <c r="F30" s="264"/>
-      <c r="G30" s="264"/>
-      <c r="H30" s="264"/>
-      <c r="I30" s="264"/>
-      <c r="J30" s="264"/>
-      <c r="K30" s="264"/>
-      <c r="L30" s="265"/>
+      <c r="C30" s="290"/>
+      <c r="D30" s="290"/>
+      <c r="E30" s="290"/>
+      <c r="F30" s="290"/>
+      <c r="G30" s="290"/>
+      <c r="H30" s="290"/>
+      <c r="I30" s="290"/>
+      <c r="J30" s="290"/>
+      <c r="K30" s="290"/>
+      <c r="L30" s="291"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="227">
         <v>5</v>
       </c>
-      <c r="B31" s="264" t="s">
+      <c r="B31" s="290" t="s">
         <v>208</v>
       </c>
-      <c r="C31" s="264"/>
-      <c r="D31" s="264"/>
-      <c r="E31" s="264"/>
-      <c r="F31" s="264"/>
-      <c r="G31" s="264"/>
-      <c r="H31" s="264"/>
-      <c r="I31" s="264"/>
-      <c r="J31" s="264"/>
-      <c r="K31" s="264"/>
-      <c r="L31" s="265"/>
+      <c r="C31" s="290"/>
+      <c r="D31" s="290"/>
+      <c r="E31" s="290"/>
+      <c r="F31" s="290"/>
+      <c r="G31" s="290"/>
+      <c r="H31" s="290"/>
+      <c r="I31" s="290"/>
+      <c r="J31" s="290"/>
+      <c r="K31" s="290"/>
+      <c r="L31" s="291"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="227"/>
-      <c r="B32" s="264" t="s">
+      <c r="B32" s="290" t="s">
         <v>209</v>
       </c>
-      <c r="C32" s="264"/>
-      <c r="D32" s="264"/>
-      <c r="E32" s="264"/>
-      <c r="F32" s="264"/>
-      <c r="G32" s="264"/>
-      <c r="H32" s="264"/>
-      <c r="I32" s="264"/>
-      <c r="J32" s="264"/>
-      <c r="K32" s="264"/>
-      <c r="L32" s="265"/>
+      <c r="C32" s="290"/>
+      <c r="D32" s="290"/>
+      <c r="E32" s="290"/>
+      <c r="F32" s="290"/>
+      <c r="G32" s="290"/>
+      <c r="H32" s="290"/>
+      <c r="I32" s="290"/>
+      <c r="J32" s="290"/>
+      <c r="K32" s="290"/>
+      <c r="L32" s="291"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="227"/>
-      <c r="B33" s="264" t="s">
+      <c r="B33" s="290" t="s">
         <v>210</v>
       </c>
-      <c r="C33" s="264"/>
-      <c r="D33" s="264"/>
-      <c r="E33" s="264"/>
-      <c r="F33" s="264"/>
-      <c r="G33" s="264"/>
-      <c r="H33" s="264"/>
-      <c r="I33" s="264"/>
-      <c r="J33" s="264"/>
-      <c r="K33" s="264"/>
-      <c r="L33" s="265"/>
+      <c r="C33" s="290"/>
+      <c r="D33" s="290"/>
+      <c r="E33" s="290"/>
+      <c r="F33" s="290"/>
+      <c r="G33" s="290"/>
+      <c r="H33" s="290"/>
+      <c r="I33" s="290"/>
+      <c r="J33" s="290"/>
+      <c r="K33" s="290"/>
+      <c r="L33" s="291"/>
       <c r="N33" s="106"/>
     </row>
     <row r="34" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="273" t="s">
+      <c r="A34" s="292" t="s">
         <v>216</v>
       </c>
-      <c r="B34" s="274"/>
-      <c r="C34" s="274"/>
-      <c r="D34" s="274"/>
-      <c r="E34" s="274"/>
-      <c r="F34" s="274"/>
-      <c r="G34" s="274"/>
-      <c r="H34" s="274"/>
-      <c r="I34" s="274"/>
-      <c r="J34" s="274"/>
-      <c r="K34" s="274"/>
-      <c r="L34" s="275"/>
+      <c r="B34" s="293"/>
+      <c r="C34" s="293"/>
+      <c r="D34" s="293"/>
+      <c r="E34" s="293"/>
+      <c r="F34" s="293"/>
+      <c r="G34" s="293"/>
+      <c r="H34" s="293"/>
+      <c r="I34" s="293"/>
+      <c r="J34" s="293"/>
+      <c r="K34" s="293"/>
+      <c r="L34" s="294"/>
       <c r="N34" s="106"/>
     </row>
     <row r="35" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="227">
         <v>1</v>
       </c>
-      <c r="B35" s="264" t="s">
+      <c r="B35" s="290" t="s">
         <v>211</v>
       </c>
-      <c r="C35" s="264"/>
-      <c r="D35" s="264"/>
-      <c r="E35" s="264"/>
-      <c r="F35" s="264"/>
-      <c r="G35" s="264"/>
-      <c r="H35" s="264"/>
-      <c r="I35" s="264"/>
-      <c r="J35" s="264"/>
-      <c r="K35" s="264"/>
-      <c r="L35" s="265"/>
+      <c r="C35" s="290"/>
+      <c r="D35" s="290"/>
+      <c r="E35" s="290"/>
+      <c r="F35" s="290"/>
+      <c r="G35" s="290"/>
+      <c r="H35" s="290"/>
+      <c r="I35" s="290"/>
+      <c r="J35" s="290"/>
+      <c r="K35" s="290"/>
+      <c r="L35" s="291"/>
       <c r="N35" s="106"/>
     </row>
     <row r="36" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="227"/>
-      <c r="B36" s="262" t="s">
+      <c r="B36" s="288" t="s">
         <v>339</v>
       </c>
-      <c r="C36" s="262"/>
-      <c r="D36" s="262"/>
-      <c r="E36" s="262"/>
-      <c r="F36" s="262"/>
-      <c r="G36" s="262"/>
-      <c r="H36" s="262"/>
-      <c r="I36" s="262"/>
-      <c r="J36" s="262"/>
-      <c r="K36" s="262"/>
-      <c r="L36" s="263"/>
+      <c r="C36" s="288"/>
+      <c r="D36" s="288"/>
+      <c r="E36" s="288"/>
+      <c r="F36" s="288"/>
+      <c r="G36" s="288"/>
+      <c r="H36" s="288"/>
+      <c r="I36" s="288"/>
+      <c r="J36" s="288"/>
+      <c r="K36" s="288"/>
+      <c r="L36" s="289"/>
       <c r="N36" s="106"/>
     </row>
     <row r="37" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="227">
         <v>2</v>
       </c>
-      <c r="B37" s="264" t="s">
+      <c r="B37" s="290" t="s">
         <v>332</v>
       </c>
-      <c r="C37" s="264"/>
-      <c r="D37" s="264"/>
-      <c r="E37" s="264"/>
-      <c r="F37" s="264"/>
-      <c r="G37" s="264"/>
-      <c r="H37" s="264"/>
-      <c r="I37" s="264"/>
-      <c r="J37" s="264"/>
-      <c r="K37" s="264"/>
-      <c r="L37" s="265"/>
+      <c r="C37" s="290"/>
+      <c r="D37" s="290"/>
+      <c r="E37" s="290"/>
+      <c r="F37" s="290"/>
+      <c r="G37" s="290"/>
+      <c r="H37" s="290"/>
+      <c r="I37" s="290"/>
+      <c r="J37" s="290"/>
+      <c r="K37" s="290"/>
+      <c r="L37" s="291"/>
       <c r="N37" s="106"/>
     </row>
     <row r="38" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="227">
         <v>3</v>
       </c>
-      <c r="B38" s="264" t="s">
+      <c r="B38" s="290" t="s">
         <v>321</v>
       </c>
-      <c r="C38" s="264"/>
-      <c r="D38" s="264"/>
-      <c r="E38" s="264"/>
-      <c r="F38" s="264"/>
-      <c r="G38" s="264"/>
-      <c r="H38" s="264"/>
-      <c r="I38" s="264"/>
-      <c r="J38" s="264"/>
-      <c r="K38" s="264"/>
-      <c r="L38" s="265"/>
+      <c r="C38" s="290"/>
+      <c r="D38" s="290"/>
+      <c r="E38" s="290"/>
+      <c r="F38" s="290"/>
+      <c r="G38" s="290"/>
+      <c r="H38" s="290"/>
+      <c r="I38" s="290"/>
+      <c r="J38" s="290"/>
+      <c r="K38" s="290"/>
+      <c r="L38" s="291"/>
       <c r="N38" s="106"/>
     </row>
     <row r="39" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="227">
         <v>4</v>
       </c>
-      <c r="B39" s="264" t="s">
+      <c r="B39" s="290" t="s">
         <v>340</v>
       </c>
-      <c r="C39" s="264"/>
-      <c r="D39" s="264"/>
-      <c r="E39" s="264"/>
-      <c r="F39" s="264"/>
-      <c r="G39" s="264"/>
-      <c r="H39" s="264"/>
-      <c r="I39" s="264"/>
-      <c r="J39" s="264"/>
-      <c r="K39" s="264"/>
-      <c r="L39" s="265"/>
+      <c r="C39" s="290"/>
+      <c r="D39" s="290"/>
+      <c r="E39" s="290"/>
+      <c r="F39" s="290"/>
+      <c r="G39" s="290"/>
+      <c r="H39" s="290"/>
+      <c r="I39" s="290"/>
+      <c r="J39" s="290"/>
+      <c r="K39" s="290"/>
+      <c r="L39" s="291"/>
       <c r="N39" s="106"/>
     </row>
     <row r="40" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="227">
         <v>5</v>
       </c>
-      <c r="B40" s="262" t="s">
+      <c r="B40" s="288" t="s">
         <v>322</v>
       </c>
-      <c r="C40" s="262"/>
-      <c r="D40" s="262"/>
-      <c r="E40" s="262"/>
-      <c r="F40" s="262"/>
-      <c r="G40" s="262"/>
-      <c r="H40" s="262"/>
-      <c r="I40" s="262"/>
-      <c r="J40" s="262"/>
-      <c r="K40" s="262"/>
-      <c r="L40" s="263"/>
+      <c r="C40" s="288"/>
+      <c r="D40" s="288"/>
+      <c r="E40" s="288"/>
+      <c r="F40" s="288"/>
+      <c r="G40" s="288"/>
+      <c r="H40" s="288"/>
+      <c r="I40" s="288"/>
+      <c r="J40" s="288"/>
+      <c r="K40" s="288"/>
+      <c r="L40" s="289"/>
       <c r="N40" s="106"/>
     </row>
     <row r="41" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="227">
         <v>6</v>
       </c>
-      <c r="B41" s="262" t="s">
+      <c r="B41" s="288" t="s">
         <v>327</v>
       </c>
-      <c r="C41" s="262"/>
-      <c r="D41" s="262"/>
-      <c r="E41" s="262"/>
-      <c r="F41" s="262"/>
-      <c r="G41" s="262"/>
-      <c r="H41" s="262"/>
-      <c r="I41" s="262"/>
-      <c r="J41" s="262"/>
-      <c r="K41" s="262"/>
-      <c r="L41" s="263"/>
+      <c r="C41" s="288"/>
+      <c r="D41" s="288"/>
+      <c r="E41" s="288"/>
+      <c r="F41" s="288"/>
+      <c r="G41" s="288"/>
+      <c r="H41" s="288"/>
+      <c r="I41" s="288"/>
+      <c r="J41" s="288"/>
+      <c r="K41" s="288"/>
+      <c r="L41" s="289"/>
       <c r="N41" s="106"/>
     </row>
     <row r="42" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="227">
         <v>7</v>
       </c>
-      <c r="B42" s="264" t="s">
+      <c r="B42" s="290" t="s">
         <v>323</v>
       </c>
-      <c r="C42" s="264"/>
-      <c r="D42" s="264"/>
-      <c r="E42" s="264"/>
-      <c r="F42" s="264"/>
-      <c r="G42" s="264"/>
-      <c r="H42" s="264"/>
-      <c r="I42" s="264"/>
-      <c r="J42" s="264"/>
-      <c r="K42" s="264"/>
-      <c r="L42" s="265"/>
+      <c r="C42" s="290"/>
+      <c r="D42" s="290"/>
+      <c r="E42" s="290"/>
+      <c r="F42" s="290"/>
+      <c r="G42" s="290"/>
+      <c r="H42" s="290"/>
+      <c r="I42" s="290"/>
+      <c r="J42" s="290"/>
+      <c r="K42" s="290"/>
+      <c r="L42" s="291"/>
     </row>
     <row r="43" spans="1:14" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="227"/>
@@ -15977,56 +15977,56 @@
       <c r="L43" s="229"/>
     </row>
     <row r="44" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="273" t="s">
+      <c r="A44" s="292" t="s">
         <v>326</v>
       </c>
-      <c r="B44" s="274"/>
-      <c r="C44" s="274"/>
-      <c r="D44" s="274"/>
-      <c r="E44" s="274"/>
-      <c r="F44" s="274"/>
-      <c r="G44" s="274"/>
-      <c r="H44" s="274"/>
-      <c r="I44" s="274"/>
-      <c r="J44" s="274"/>
-      <c r="K44" s="274"/>
-      <c r="L44" s="275"/>
+      <c r="B44" s="293"/>
+      <c r="C44" s="293"/>
+      <c r="D44" s="293"/>
+      <c r="E44" s="293"/>
+      <c r="F44" s="293"/>
+      <c r="G44" s="293"/>
+      <c r="H44" s="293"/>
+      <c r="I44" s="293"/>
+      <c r="J44" s="293"/>
+      <c r="K44" s="293"/>
+      <c r="L44" s="294"/>
     </row>
     <row r="45" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="230" t="s">
         <v>324</v>
       </c>
-      <c r="B45" s="264" t="s">
+      <c r="B45" s="290" t="s">
         <v>212</v>
       </c>
-      <c r="C45" s="264"/>
-      <c r="D45" s="264"/>
-      <c r="E45" s="264"/>
-      <c r="F45" s="264"/>
-      <c r="G45" s="264"/>
-      <c r="H45" s="264"/>
-      <c r="I45" s="264"/>
-      <c r="J45" s="264"/>
-      <c r="K45" s="264"/>
-      <c r="L45" s="265"/>
+      <c r="C45" s="290"/>
+      <c r="D45" s="290"/>
+      <c r="E45" s="290"/>
+      <c r="F45" s="290"/>
+      <c r="G45" s="290"/>
+      <c r="H45" s="290"/>
+      <c r="I45" s="290"/>
+      <c r="J45" s="290"/>
+      <c r="K45" s="290"/>
+      <c r="L45" s="291"/>
     </row>
     <row r="46" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="231" t="s">
         <v>325</v>
       </c>
-      <c r="B46" s="266" t="s">
+      <c r="B46" s="300" t="s">
         <v>328</v>
       </c>
-      <c r="C46" s="266"/>
-      <c r="D46" s="266"/>
-      <c r="E46" s="266"/>
-      <c r="F46" s="266"/>
-      <c r="G46" s="266"/>
-      <c r="H46" s="266"/>
-      <c r="I46" s="266"/>
-      <c r="J46" s="266"/>
-      <c r="K46" s="266"/>
-      <c r="L46" s="267"/>
+      <c r="C46" s="300"/>
+      <c r="D46" s="300"/>
+      <c r="E46" s="300"/>
+      <c r="F46" s="300"/>
+      <c r="G46" s="300"/>
+      <c r="H46" s="300"/>
+      <c r="I46" s="300"/>
+      <c r="J46" s="300"/>
+      <c r="K46" s="300"/>
+      <c r="L46" s="301"/>
     </row>
     <row r="47" spans="1:14" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="160"/>
@@ -16043,20 +16043,20 @@
       <c r="L47" s="113"/>
     </row>
     <row r="48" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="268" t="s">
+      <c r="A48" s="302" t="s">
         <v>240</v>
       </c>
-      <c r="B48" s="269"/>
-      <c r="C48" s="269"/>
-      <c r="D48" s="269"/>
-      <c r="E48" s="269"/>
-      <c r="F48" s="269"/>
-      <c r="G48" s="269"/>
-      <c r="H48" s="269"/>
-      <c r="I48" s="269"/>
-      <c r="J48" s="269"/>
-      <c r="K48" s="269"/>
-      <c r="L48" s="270"/>
+      <c r="B48" s="303"/>
+      <c r="C48" s="303"/>
+      <c r="D48" s="303"/>
+      <c r="E48" s="303"/>
+      <c r="F48" s="303"/>
+      <c r="G48" s="303"/>
+      <c r="H48" s="303"/>
+      <c r="I48" s="303"/>
+      <c r="J48" s="303"/>
+      <c r="K48" s="303"/>
+      <c r="L48" s="304"/>
     </row>
     <row r="49" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="234" t="s">
@@ -16144,90 +16144,90 @@
       <c r="B54" s="168" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="271" t="s">
+      <c r="C54" s="273" t="s">
         <v>312</v>
       </c>
-      <c r="D54" s="271"/>
-      <c r="E54" s="271"/>
-      <c r="F54" s="271"/>
-      <c r="G54" s="271"/>
-      <c r="H54" s="271"/>
-      <c r="I54" s="271"/>
-      <c r="J54" s="271"/>
-      <c r="K54" s="271"/>
-      <c r="L54" s="272"/>
+      <c r="D54" s="273"/>
+      <c r="E54" s="273"/>
+      <c r="F54" s="273"/>
+      <c r="G54" s="273"/>
+      <c r="H54" s="273"/>
+      <c r="I54" s="273"/>
+      <c r="J54" s="273"/>
+      <c r="K54" s="273"/>
+      <c r="L54" s="274"/>
     </row>
     <row r="55" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="167"/>
       <c r="B55" s="168" t="s">
         <v>313</v>
       </c>
-      <c r="C55" s="271" t="s">
+      <c r="C55" s="273" t="s">
         <v>314</v>
       </c>
-      <c r="D55" s="271"/>
-      <c r="E55" s="271"/>
-      <c r="F55" s="271"/>
-      <c r="G55" s="271"/>
-      <c r="H55" s="271"/>
-      <c r="I55" s="271"/>
-      <c r="J55" s="271"/>
-      <c r="K55" s="271"/>
-      <c r="L55" s="272"/>
+      <c r="D55" s="273"/>
+      <c r="E55" s="273"/>
+      <c r="F55" s="273"/>
+      <c r="G55" s="273"/>
+      <c r="H55" s="273"/>
+      <c r="I55" s="273"/>
+      <c r="J55" s="273"/>
+      <c r="K55" s="273"/>
+      <c r="L55" s="274"/>
     </row>
     <row r="56" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="167"/>
       <c r="B56" s="168" t="s">
         <v>382</v>
       </c>
-      <c r="C56" s="271" t="s">
+      <c r="C56" s="273" t="s">
         <v>383</v>
       </c>
-      <c r="D56" s="271"/>
-      <c r="E56" s="271"/>
-      <c r="F56" s="271"/>
-      <c r="G56" s="271"/>
-      <c r="H56" s="271"/>
-      <c r="I56" s="271"/>
-      <c r="J56" s="271"/>
-      <c r="K56" s="271"/>
-      <c r="L56" s="272"/>
+      <c r="D56" s="273"/>
+      <c r="E56" s="273"/>
+      <c r="F56" s="273"/>
+      <c r="G56" s="273"/>
+      <c r="H56" s="273"/>
+      <c r="I56" s="273"/>
+      <c r="J56" s="273"/>
+      <c r="K56" s="273"/>
+      <c r="L56" s="274"/>
     </row>
     <row r="57" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="167"/>
       <c r="B57" s="168" t="s">
         <v>138</v>
       </c>
-      <c r="C57" s="271" t="s">
+      <c r="C57" s="273" t="s">
         <v>139</v>
       </c>
-      <c r="D57" s="271"/>
-      <c r="E57" s="271"/>
-      <c r="F57" s="271"/>
-      <c r="G57" s="271"/>
-      <c r="H57" s="271"/>
-      <c r="I57" s="271"/>
-      <c r="J57" s="271"/>
-      <c r="K57" s="271"/>
-      <c r="L57" s="272"/>
+      <c r="D57" s="273"/>
+      <c r="E57" s="273"/>
+      <c r="F57" s="273"/>
+      <c r="G57" s="273"/>
+      <c r="H57" s="273"/>
+      <c r="I57" s="273"/>
+      <c r="J57" s="273"/>
+      <c r="K57" s="273"/>
+      <c r="L57" s="274"/>
     </row>
     <row r="58" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="167"/>
       <c r="B58" s="168" t="s">
         <v>238</v>
       </c>
-      <c r="C58" s="271" t="s">
+      <c r="C58" s="273" t="s">
         <v>239</v>
       </c>
-      <c r="D58" s="271"/>
-      <c r="E58" s="271"/>
-      <c r="F58" s="271"/>
-      <c r="G58" s="271"/>
-      <c r="H58" s="271"/>
-      <c r="I58" s="271"/>
-      <c r="J58" s="271"/>
-      <c r="K58" s="271"/>
-      <c r="L58" s="272"/>
+      <c r="D58" s="273"/>
+      <c r="E58" s="273"/>
+      <c r="F58" s="273"/>
+      <c r="G58" s="273"/>
+      <c r="H58" s="273"/>
+      <c r="I58" s="273"/>
+      <c r="J58" s="273"/>
+      <c r="K58" s="273"/>
+      <c r="L58" s="274"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A59" s="167"/>
@@ -16252,18 +16252,18 @@
       <c r="B60" s="168" t="s">
         <v>63</v>
       </c>
-      <c r="C60" s="271" t="s">
+      <c r="C60" s="273" t="s">
         <v>316</v>
       </c>
-      <c r="D60" s="271"/>
-      <c r="E60" s="271"/>
-      <c r="F60" s="271"/>
-      <c r="G60" s="271"/>
-      <c r="H60" s="271"/>
-      <c r="I60" s="271"/>
-      <c r="J60" s="271"/>
-      <c r="K60" s="271"/>
-      <c r="L60" s="272"/>
+      <c r="D60" s="273"/>
+      <c r="E60" s="273"/>
+      <c r="F60" s="273"/>
+      <c r="G60" s="273"/>
+      <c r="H60" s="273"/>
+      <c r="I60" s="273"/>
+      <c r="J60" s="273"/>
+      <c r="K60" s="273"/>
+      <c r="L60" s="274"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="167"/>
@@ -16363,25 +16363,56 @@
       </c>
     </row>
     <row r="78" spans="1:12" ht="29.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="261" t="s">
+      <c r="A78" s="299" t="s">
         <v>407</v>
       </c>
-      <c r="B78" s="261"/>
-      <c r="C78" s="261"/>
-      <c r="D78" s="261"/>
-      <c r="E78" s="261"/>
-      <c r="F78" s="261"/>
-      <c r="G78" s="261"/>
-      <c r="H78" s="261"/>
-      <c r="I78" s="261"/>
-      <c r="J78" s="261"/>
-      <c r="K78" s="261"/>
-      <c r="L78" s="261"/>
+      <c r="B78" s="299"/>
+      <c r="C78" s="299"/>
+      <c r="D78" s="299"/>
+      <c r="E78" s="299"/>
+      <c r="F78" s="299"/>
+      <c r="G78" s="299"/>
+      <c r="H78" s="299"/>
+      <c r="I78" s="299"/>
+      <c r="J78" s="299"/>
+      <c r="K78" s="299"/>
+      <c r="L78" s="299"/>
     </row>
     <row r="83" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="84" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="A78:L78"/>
+    <mergeCell ref="B41:L41"/>
+    <mergeCell ref="B42:L42"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="A48:L48"/>
+    <mergeCell ref="C54:L54"/>
+    <mergeCell ref="C57:L57"/>
+    <mergeCell ref="C58:L58"/>
+    <mergeCell ref="C55:L55"/>
+    <mergeCell ref="C60:L60"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="B40:L40"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B30:L30"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B39:L39"/>
     <mergeCell ref="A26:L26"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A4:L4"/>
@@ -16398,37 +16429,6 @@
     <mergeCell ref="B8:L8"/>
     <mergeCell ref="A10:L10"/>
     <mergeCell ref="B11:L11"/>
-    <mergeCell ref="C56:L56"/>
-    <mergeCell ref="B40:L40"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="B14:L14"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="A78:L78"/>
-    <mergeCell ref="B41:L41"/>
-    <mergeCell ref="B42:L42"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="A48:L48"/>
-    <mergeCell ref="C54:L54"/>
-    <mergeCell ref="C57:L57"/>
-    <mergeCell ref="C58:L58"/>
-    <mergeCell ref="C55:L55"/>
-    <mergeCell ref="C60:L60"/>
-    <mergeCell ref="A44:L44"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A67" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -32064,7 +32064,7 @@
   <dimension ref="A1:P139"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="N65" sqref="N65"/>
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32315,12 +32315,10 @@
         <f>"     Set "&amp;A5</f>
         <v xml:space="preserve">     Set Reclamation - Protect Zone</v>
       </c>
-      <c r="B20" s="184">
-        <v>1020</v>
-      </c>
+      <c r="B20" s="184"/>
       <c r="C20" s="12">
         <f>VLOOKUP(IF(B20="",895,B20),'Mead-Elevation-Area'!$A$5:$B$689,2)/1000000</f>
-        <v>5.664593</v>
+        <v>0</v>
       </c>
       <c r="D20" s="10"/>
       <c r="N20" s="141" t="s">
@@ -32333,7 +32331,7 @@
       </c>
       <c r="C21" s="12">
         <f>C19-C20</f>
-        <v>2.9876249999999995</v>
+        <v>8.6522179999999995</v>
       </c>
       <c r="D21" s="116"/>
       <c r="E21" s="28"/>
@@ -32364,7 +32362,7 @@
       </c>
       <c r="C23" s="12">
         <f>C21-C22</f>
-        <v>-0.54637500000000028</v>
+        <v>5.1182179999999997</v>
       </c>
       <c r="D23" s="111"/>
       <c r="E23" s="28"/>
@@ -32456,9 +32454,7 @@
         <v>247</v>
       </c>
       <c r="B28" s="1"/>
-      <c r="C28" s="97">
-        <v>8</v>
-      </c>
+      <c r="C28" s="97"/>
       <c r="D28" s="97"/>
       <c r="E28" s="97"/>
       <c r="F28" s="97"/>
@@ -32477,9 +32473,9 @@
         <v>71</v>
       </c>
       <c r="B29" s="1"/>
-      <c r="C29" s="96">
+      <c r="C29" s="96" t="str">
         <f>IF(C$28&lt;&gt;"",0.8,"")</f>
-        <v>0.8</v>
+        <v/>
       </c>
       <c r="D29" s="96" t="str">
         <f t="shared" ref="D29:L29" si="0">IF(D$28&lt;&gt;"",0.8,"")</f>
@@ -32526,9 +32522,9 @@
         <v>137</v>
       </c>
       <c r="B30" s="1"/>
-      <c r="C30" s="96">
+      <c r="C30" s="96" t="str">
         <f>IF(C$28&lt;&gt;"",0.2,"")</f>
-        <v>0.2</v>
+        <v/>
       </c>
       <c r="D30" s="96" t="str">
         <f t="shared" ref="D30:L30" si="1">IF(D$28&lt;&gt;"",0.2,"")</f>
@@ -32575,9 +32571,9 @@
         <v>126</v>
       </c>
       <c r="B31" s="1"/>
-      <c r="C31" s="96">
+      <c r="C31" s="96" t="str">
         <f>IF(C$28&lt;&gt;"",0.6,"")</f>
-        <v>0.6</v>
+        <v/>
       </c>
       <c r="D31" s="96" t="str">
         <f t="shared" ref="D31:L31" si="2">IF(D$28&lt;&gt;"",0.6,"")</f>
@@ -32636,9 +32632,9 @@
         <v>293</v>
       </c>
       <c r="B33" s="1"/>
-      <c r="C33" s="12">
+      <c r="C33" s="12" t="str">
         <f>IF(C$28&lt;&gt;"",IF(COLUMN(C28)=COLUMN($C28),$C$19,B135),"")</f>
-        <v>8.6522179999999995</v>
+        <v/>
       </c>
       <c r="D33" s="12" t="str">
         <f>IF(D$28&lt;&gt;"",IF(COLUMN(D28)=COLUMN($C28),$C$19,C135),"")</f>
@@ -32668,9 +32664,9 @@
         <v>294</v>
       </c>
       <c r="B34" s="1"/>
-      <c r="C34" s="218">
+      <c r="C34" s="218" t="str">
         <f>IF(C$28&lt;&gt;"",IF(COLUMN(C29)=COLUMN($C29),$B$19,B136),"")</f>
-        <v>1063.29</v>
+        <v/>
       </c>
       <c r="D34" s="218" t="str">
         <f t="shared" ref="D34:G34" si="3">IF(D$28&lt;&gt;"",IF(COLUMN(D29)=COLUMN($C29),$B$19,C136),"")</f>
@@ -32731,11 +32727,11 @@
       </c>
       <c r="B36" s="83">
         <f>C20</f>
-        <v>5.664593</v>
-      </c>
-      <c r="C36" s="81">
+        <v>0</v>
+      </c>
+      <c r="C36" s="81" t="str">
         <f>IF(OR(C$28="",$A36=""),"",B36)</f>
-        <v>5.664593</v>
+        <v/>
       </c>
       <c r="D36" s="12" t="str">
         <f>IF(OR(D$28="",$A36=""),"",C128)</f>
@@ -32784,9 +32780,9 @@
       <c r="B37" s="83">
         <v>1.6619999999999999</v>
       </c>
-      <c r="C37" s="81">
+      <c r="C37" s="81" t="str">
         <f>IF(OR(C$28="",$A37=""),"",IF(C$22&lt;=C$21,B37,B37-(C$22-C$21)*B37/C$22))</f>
-        <v>1.4050460526315787</v>
+        <v/>
       </c>
       <c r="D37" s="12" t="str">
         <f t="shared" ref="D37:D41" si="7">IF(OR(D$28="",$A37=""),"",C129)</f>
@@ -32835,9 +32831,9 @@
       <c r="B38" s="83">
         <v>0.71099999999999997</v>
       </c>
-      <c r="C38" s="81">
+      <c r="C38" s="81" t="str">
         <f t="shared" ref="C38:C41" si="9">IF(OR(C$28="",$A38=""),"",IF(C$22&lt;=C$21,B38,B38-(C$22-C$21)*B38/C$22))</f>
-        <v>0.60107565789473671</v>
+        <v/>
       </c>
       <c r="D38" s="33" t="str">
         <f t="shared" si="7"/>
@@ -32886,9 +32882,9 @@
       <c r="B39" s="83">
         <v>0.9556</v>
       </c>
-      <c r="C39" s="81">
+      <c r="C39" s="81" t="str">
         <f t="shared" si="9"/>
-        <v>0.80785921052631571</v>
+        <v/>
       </c>
       <c r="D39" s="12" t="str">
         <f t="shared" si="7"/>
@@ -32936,9 +32932,9 @@
       <c r="B40" s="83">
         <v>0.21099999999999999</v>
       </c>
-      <c r="C40" s="81">
+      <c r="C40" s="81" t="str">
         <f t="shared" si="9"/>
-        <v>0.17837828947368417</v>
+        <v/>
       </c>
       <c r="D40" s="12" t="str">
         <f t="shared" si="7"/>
@@ -32985,11 +32981,11 @@
       </c>
       <c r="B41" s="83">
         <f>IF(C21&gt;C22,C21-C22,0)</f>
-        <v>0</v>
-      </c>
-      <c r="C41" s="81">
+        <v>5.1182179999999997</v>
+      </c>
+      <c r="C41" s="81" t="str">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D41" s="12" t="str">
         <f t="shared" si="7"/>
@@ -33042,9 +33038,9 @@
       <c r="A43" t="s">
         <v>68</v>
       </c>
-      <c r="C43" s="12">
+      <c r="C43" s="12" t="str">
         <f>IF(C$28&lt;&gt;"",IF(COLUMN(C27)=COLUMN($C27),$B$19,#REF!),"")</f>
-        <v>1063.29</v>
+        <v/>
       </c>
       <c r="D43" s="12" t="str">
         <f>IF(D$28&lt;&gt;"",IF(COLUMN(D27)=COLUMN($C27),$B$19,#REF!),"")</f>
@@ -33115,9 +33111,9 @@
         <v>249</v>
       </c>
       <c r="B45" s="186"/>
-      <c r="C45" s="12">
+      <c r="C45" s="12" t="str">
         <f>IF(C$28&lt;&gt;"",VLOOKUP(C33*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$B$18/1000000,"")</f>
-        <v>0.46150799999999997</v>
+        <v/>
       </c>
       <c r="D45" s="12" t="str">
         <f>IF(D$28&lt;&gt;"",VLOOKUP(D33*1000000,'Mead-Elevation-Area'!$B$5:$D$676,3)*$B$18/1000000,"")</f>
@@ -33164,9 +33160,9 @@
         <f t="shared" ref="A46:A51" si="10">IF(A5="","","    "&amp;A5&amp;" Share")</f>
         <v xml:space="preserve">    Reclamation - Protect Zone Share</v>
       </c>
-      <c r="C46" s="12">
+      <c r="C46" s="12" t="str">
         <f t="shared" ref="C46:G51" si="11">IF(OR(C$28="",$A46=""),"",C$45*C36/C$33)</f>
-        <v>0.30214853419597149</v>
+        <v/>
       </c>
       <c r="D46" s="12" t="str">
         <f t="shared" si="11"/>
@@ -33212,9 +33208,9 @@
         <v xml:space="preserve">    California Share</v>
       </c>
       <c r="B47" s="1"/>
-      <c r="C47" s="12">
+      <c r="C47" s="12" t="str">
         <f t="shared" si="11"/>
-        <v>7.4944944019891158E-2</v>
+        <v/>
       </c>
       <c r="D47" s="12" t="str">
         <f t="shared" si="11"/>
@@ -33260,9 +33256,9 @@
         <v xml:space="preserve">    Arizona Share</v>
       </c>
       <c r="B48" s="1"/>
-      <c r="C48" s="12">
+      <c r="C48" s="12" t="str">
         <f t="shared" si="11"/>
-        <v>3.206128471609062E-2</v>
+        <v/>
       </c>
       <c r="D48" s="12" t="str">
         <f t="shared" si="11"/>
@@ -33308,9 +33304,9 @@
         <v xml:space="preserve">    Nevada Share</v>
       </c>
       <c r="B49" s="1"/>
-      <c r="C49" s="12">
+      <c r="C49" s="12" t="str">
         <f t="shared" si="11"/>
-        <v>4.3091088150064981E-2</v>
+        <v/>
       </c>
       <c r="D49" s="12" t="str">
         <f t="shared" si="11"/>
@@ -33356,9 +33352,9 @@
         <v xml:space="preserve">    Mexico Share</v>
       </c>
       <c r="B50" s="1"/>
-      <c r="C50" s="12">
+      <c r="C50" s="12" t="str">
         <f t="shared" si="11"/>
-        <v>9.5146709916949651E-3</v>
+        <v/>
       </c>
       <c r="D50" s="12" t="str">
         <f t="shared" si="11"/>
@@ -33404,9 +33400,9 @@
         <v xml:space="preserve">    Tribal Nations of the Lower Basin Share</v>
       </c>
       <c r="B51" s="1"/>
-      <c r="C51" s="12">
+      <c r="C51" s="12" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D51" s="12" t="str">
         <f t="shared" si="11"/>
@@ -33451,9 +33447,9 @@
         <v>289</v>
       </c>
       <c r="B52" s="214"/>
-      <c r="C52" s="215">
+      <c r="C52" s="215" t="str">
         <f>IF(C28="","",SUM(C28))</f>
-        <v>8</v>
+        <v/>
       </c>
       <c r="D52" s="215" t="str">
         <f>IF(D28="","",SUM(D28))</f>
@@ -33504,9 +33500,9 @@
       <c r="B53" s="187" t="s">
         <v>251</v>
       </c>
-      <c r="C53" s="82">
+      <c r="C53" s="82" t="str">
         <f>IF(OR(C$28="",$A55=""),"",C46)</f>
-        <v>0.30214853419597149</v>
+        <v/>
       </c>
       <c r="D53" s="82" t="str">
         <f t="shared" ref="D53:G53" si="13">IF(OR(D$28="",$A55=""),"",D46)</f>
@@ -33546,7 +33542,7 @@
       </c>
       <c r="M53" s="19">
         <f>SUM(C55:C59)</f>
-        <v>7.6978514658040282</v>
+        <v>0</v>
       </c>
       <c r="N53" s="183"/>
     </row>
@@ -33554,9 +33550,9 @@
       <c r="A54" t="s">
         <v>290</v>
       </c>
-      <c r="C54" s="82">
+      <c r="C54" s="82" t="str">
         <f>IF(OR(C$28="",$A56=""),"",C52-C53)</f>
-        <v>7.6978514658040282</v>
+        <v/>
       </c>
       <c r="D54" s="82" t="str">
         <f t="shared" ref="D54:G54" si="15">IF(OR(D$28="",$A56=""),"",D52-D53)</f>
@@ -33594,9 +33590,9 @@
         <f t="shared" ref="L54" si="20">IF(OR(L$28="",$A55=""),"",MAX(0,L53-SUM(L55:L60)))</f>
         <v/>
       </c>
-      <c r="M54" s="18">
+      <c r="M54" s="18" t="e">
         <f>SUM(M55:M59)</f>
-        <v>1</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N54" s="143"/>
       <c r="P54" s="81"/>
@@ -33609,9 +33605,9 @@
       <c r="B55" s="95" t="s">
         <v>304</v>
       </c>
-      <c r="C55" s="82">
+      <c r="C55" s="82" t="str">
         <f>IF(OR(C$28="",$A55=""),"",(VLOOKUP(C$54,DivideInflow!$K$19:$W$25,9)-IF($A$59&lt;&gt;"",$B$59*$B$24,0))*(C$54))</f>
-        <v>3.9038054941039078</v>
+        <v/>
       </c>
       <c r="D55" s="82" t="str">
         <f>IF(OR(D$28="",$A55=""),"",(VLOOKUP(D$54,DivideInflow!$K$19:$W$25,9)-IF($A$59&lt;&gt;"",$B$59*$B$24,0))*(D$54))</f>
@@ -33634,9 +33630,9 @@
       <c r="J55" s="81"/>
       <c r="K55" s="81"/>
       <c r="L55" s="81"/>
-      <c r="M55" s="223">
+      <c r="M55" s="223" t="e">
         <f>C55/C$54</f>
-        <v>0.50712923098681295</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N55" s="143"/>
       <c r="P55" s="81"/>
@@ -33649,9 +33645,9 @@
       <c r="B56" s="95" t="s">
         <v>303</v>
       </c>
-      <c r="C56" s="82">
+      <c r="C56" s="82" t="str">
         <f>IF(OR(C$28="",$A56=""),"",(VLOOKUP(C$54,DivideInflow!$K$19:$W$25,7)-IF($A$59&lt;&gt;"",$B$59*$B$25,0))*(C$54))</f>
-        <v>1.2773617324799242</v>
+        <v/>
       </c>
       <c r="D56" s="82" t="str">
         <f>IF(OR(D$28="",$A56=""),"",(VLOOKUP(D$54,DivideInflow!$K$19:$W$25,7)-IF($A$59&lt;&gt;"",$B$59*$B$25,0))*(D$54))</f>
@@ -33689,9 +33685,9 @@
         <f t="shared" ref="L56" si="25">IF(OR(L$28="",$A56=""),"",MIN(L52,L$53-SUM(L57:L60)))</f>
         <v/>
       </c>
-      <c r="M56" s="223">
+      <c r="M56" s="223" t="e">
         <f t="shared" ref="M56:M58" si="26">C56/C$54</f>
-        <v>0.16593743567985381</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N56" s="143"/>
     </row>
@@ -33703,9 +33699,9 @@
       <c r="B57" s="211">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="C57" s="82">
+      <c r="C57" s="82" t="str">
         <f>IF(OR(C$28="",$A57=""),"",VLOOKUP(C$54,DivideInflow!$K$19:$W$25,8)*(C$54))</f>
-        <v>0.2566463678699063</v>
+        <v/>
       </c>
       <c r="D57" s="82" t="str">
         <f>IF(OR(D$28="",$A57=""),"",VLOOKUP(D$54,DivideInflow!$K$18:$W$23,8)*(D$54))</f>
@@ -33743,9 +33739,9 @@
         <f t="shared" ref="L57" si="31">IF(OR(L$28="",$A57=""),"",MIN($B57,L$53-SUM(L58:L60)))</f>
         <v/>
       </c>
-      <c r="M57" s="223">
+      <c r="M57" s="223" t="e">
         <f t="shared" si="26"/>
-        <v>3.3340000000000002E-2</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N57" s="143"/>
     </row>
@@ -33757,9 +33753,9 @@
       <c r="B58" s="211">
         <v>0.16700000000000001</v>
       </c>
-      <c r="C58" s="82">
+      <c r="C58" s="82" t="str">
         <f>IF(OR(C$28="",$A58=""),"",VLOOKUP(C$54,DivideInflow!$K$19:$W$25,10)*(C$54))</f>
-        <v>1.2829239252908993</v>
+        <v/>
       </c>
       <c r="D58" s="82" t="str">
         <f>IF(OR(D$28="",$A58=""),"",VLOOKUP(D$54,DivideInflow!$K$18:$W$23,10)*(D$54))</f>
@@ -33797,9 +33793,9 @@
         <f t="shared" ref="L58" si="36">IF(OR(L$28="",$A58=""),"",MIN($B58,L$53-SUM(L59:L60)))</f>
         <v/>
       </c>
-      <c r="M58" s="223">
+      <c r="M58" s="223" t="e">
         <f t="shared" si="26"/>
-        <v>0.16666</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N58" s="143"/>
     </row>
@@ -33812,9 +33808,9 @@
         <f>IF(A59="","",0.952/7.5)</f>
         <v>0.12693333333333331</v>
       </c>
-      <c r="C59" s="82">
+      <c r="C59" s="82" t="str">
         <f>IF(OR(C$28="",$A59=""),"",C$54*$B59)</f>
-        <v>0.97711394605939117</v>
+        <v/>
       </c>
       <c r="D59" s="82" t="str">
         <f t="shared" ref="D59:G59" si="37">IF(OR(D$28="",$A59=""),"",D$54*$B59)</f>
@@ -33852,9 +33848,9 @@
         <f t="shared" si="38"/>
         <v/>
       </c>
-      <c r="M59" s="223">
+      <c r="M59" s="223" t="e">
         <f>IF(A59="","",C59/C$54)</f>
-        <v>0.12693333333333331</v>
+        <v>#VALUE!</v>
       </c>
       <c r="N59" s="143"/>
     </row>
@@ -33866,9 +33862,9 @@
       <c r="B60" s="151" t="s">
         <v>199</v>
       </c>
-      <c r="C60" s="153">
+      <c r="C60" s="153" t="str">
         <f>IF(OR(C$28="",$A60=""),"",MIN(C31,C52-C59))</f>
-        <v>0.6</v>
+        <v/>
       </c>
       <c r="D60" s="153" t="str">
         <f>IF(OR(D$28="",$A60=""),"",MIN(D31,D52-D59))</f>
@@ -34016,9 +34012,9 @@
         <f>IF(A65="","","   Net trade volume all participants (should be zero)")</f>
         <v xml:space="preserve">   Net trade volume all participants (should be zero)</v>
       </c>
-      <c r="C66" s="44">
-        <f t="shared" ref="C66:M66" ca="1" si="45">IF(OR(C$28="",$A66=""),"",C$119)</f>
-        <v>0</v>
+      <c r="C66" s="44" t="str">
+        <f t="shared" ref="C66:M66" si="45">IF(OR(C$28="",$A66=""),"",C$119)</f>
+        <v/>
       </c>
       <c r="D66" s="44" t="str">
         <f t="shared" si="45"/>
@@ -34069,9 +34065,9 @@
         <f>IF(A65="","","   Available Water [maf]")</f>
         <v xml:space="preserve">   Available Water [maf]</v>
       </c>
-      <c r="C67" s="12">
+      <c r="C67" s="12" t="str">
         <f>IF(OR(C$28="",$A67=""),"",C36+C53-C46+C64)</f>
-        <v>5.664593</v>
+        <v/>
       </c>
       <c r="D67" s="12" t="str">
         <f>IF(OR(D$28="",$A67=""),"",D36+D53-D46+D64)</f>
@@ -34137,9 +34133,9 @@
         <f>IF(A68="","","   End of Year Balance [maf]")</f>
         <v xml:space="preserve">   End of Year Balance [maf]</v>
       </c>
-      <c r="C69" s="12">
+      <c r="C69" s="12" t="str">
         <f>IF(OR(C$28="",$A69=""),"",C67-C68)</f>
-        <v>5.664593</v>
+        <v/>
       </c>
       <c r="D69" s="12" t="str">
         <f t="shared" ref="D69:L69" si="47">IF(OR(D$28="",$A69=""),"",D67-D68)</f>
@@ -34259,9 +34255,9 @@
         <f>IF(A73="","",$A$66)</f>
         <v xml:space="preserve">   Net trade volume all participants (should be zero)</v>
       </c>
-      <c r="C74" s="44">
-        <f t="shared" ref="C74:M74" ca="1" si="48">IF(OR(C$28="",$A74=""),"",C$119)</f>
-        <v>0</v>
+      <c r="C74" s="44" t="str">
+        <f t="shared" ref="C74:M74" si="48">IF(OR(C$28="",$A74=""),"",C$119)</f>
+        <v/>
       </c>
       <c r="D74" s="44" t="str">
         <f t="shared" si="48"/>
@@ -34312,9 +34308,9 @@
         <f>IF(A73="","","   Available Water [maf]")</f>
         <v xml:space="preserve">   Available Water [maf]</v>
       </c>
-      <c r="C75" s="12">
+      <c r="C75" s="12" t="str">
         <f>IF(OR(C$28="",$A75=""),"",C37+C55-C47+C72)</f>
-        <v>5.2339066027155949</v>
+        <v/>
       </c>
       <c r="D75" s="12" t="str">
         <f>IF(OR(D$28="",$A75=""),"",D37+D55-D47+D72)</f>
@@ -34380,9 +34376,9 @@
         <f>IF(A76="","","   End of Year Balance [maf]")</f>
         <v xml:space="preserve">   End of Year Balance [maf]</v>
       </c>
-      <c r="C77" s="12">
+      <c r="C77" s="12" t="str">
         <f>IF(OR(C$28="",$A77=""),"",C75-C76)</f>
-        <v>5.2339066027155949</v>
+        <v/>
       </c>
       <c r="D77" s="12" t="str">
         <f t="shared" ref="D77:L77" si="50">IF(OR(D$28="",$A77=""),"",D75-D76)</f>
@@ -34502,9 +34498,9 @@
         <f>IF(A81="","",$A$66)</f>
         <v xml:space="preserve">   Net trade volume all participants (should be zero)</v>
       </c>
-      <c r="C82" s="44">
-        <f t="shared" ref="C82:M82" ca="1" si="51">IF(OR(C$28="",$A82=""),"",C$119)</f>
-        <v>0</v>
+      <c r="C82" s="44" t="str">
+        <f t="shared" ref="C82:M82" si="51">IF(OR(C$28="",$A82=""),"",C$119)</f>
+        <v/>
       </c>
       <c r="D82" s="44" t="str">
         <f t="shared" si="51"/>
@@ -34555,9 +34551,9 @@
         <f>IF(A81="","","   Available Water [maf]")</f>
         <v xml:space="preserve">   Available Water [maf]</v>
       </c>
-      <c r="C83" s="12">
+      <c r="C83" s="12" t="str">
         <f>IF(OR(C$28="",$A83=""),"",C38+C56-C48+C80)</f>
-        <v>1.8463761056585704</v>
+        <v/>
       </c>
       <c r="D83" s="12" t="str">
         <f t="shared" ref="D83:L83" si="52">IF(OR(D$28="",$A83=""),"",D38+D56-D48+D80)</f>
@@ -34623,9 +34619,9 @@
         <f>IF(A84="","","   End of Year Balance [maf]")</f>
         <v xml:space="preserve">   End of Year Balance [maf]</v>
       </c>
-      <c r="C85" s="12">
+      <c r="C85" s="12" t="str">
         <f>IF(OR(C$28="",$A85=""),"",C83-C84)</f>
-        <v>1.8463761056585704</v>
+        <v/>
       </c>
       <c r="D85" s="12" t="str">
         <f t="shared" ref="D85:L85" si="53">IF(OR(D$28="",$A85=""),"",D83-D84)</f>
@@ -34745,9 +34741,9 @@
         <f>IF(A89="","",$A$66)</f>
         <v xml:space="preserve">   Net trade volume all participants (should be zero)</v>
       </c>
-      <c r="C90" s="44">
-        <f t="shared" ref="C90:M90" ca="1" si="54">IF(OR(C$28="",$A90=""),"",C$119)</f>
-        <v>0</v>
+      <c r="C90" s="44" t="str">
+        <f t="shared" ref="C90:M90" si="54">IF(OR(C$28="",$A90=""),"",C$119)</f>
+        <v/>
       </c>
       <c r="D90" s="44" t="str">
         <f t="shared" si="54"/>
@@ -34798,9 +34794,9 @@
         <f>IF(A89="","","   Available Water [maf]")</f>
         <v xml:space="preserve">   Available Water [maf]</v>
       </c>
-      <c r="C91" s="12">
+      <c r="C91" s="12" t="str">
         <f>IF(OR(C$28="",$A91=""),"",C39+C57-C49+C88)</f>
-        <v>1.021414490246157</v>
+        <v/>
       </c>
       <c r="D91" s="12" t="str">
         <f t="shared" ref="D91:L91" si="55">IF(OR(D$28="",$A91=""),"",D39+D57-D49+D88)</f>
@@ -34866,9 +34862,9 @@
         <f>IF(A92="","","   End of Year Balance [maf]")</f>
         <v xml:space="preserve">   End of Year Balance [maf]</v>
       </c>
-      <c r="C93" s="12">
+      <c r="C93" s="12" t="str">
         <f>IF(OR(C$28="",$A93=""),"",C91-C92)</f>
-        <v>1.021414490246157</v>
+        <v/>
       </c>
       <c r="D93" s="12" t="str">
         <f t="shared" ref="D93:L93" si="56">IF(OR(D$28="",$A93=""),"",D91-D92)</f>
@@ -34988,9 +34984,9 @@
         <f>IF(A97="","",$A$66)</f>
         <v xml:space="preserve">   Net trade volume all participants (should be zero)</v>
       </c>
-      <c r="C98" s="44">
-        <f t="shared" ref="C98:M98" ca="1" si="57">IF(OR(C$28="",$A98=""),"",C$119)</f>
-        <v>0</v>
+      <c r="C98" s="44" t="str">
+        <f t="shared" ref="C98:M98" si="57">IF(OR(C$28="",$A98=""),"",C$119)</f>
+        <v/>
       </c>
       <c r="D98" s="44" t="str">
         <f t="shared" si="57"/>
@@ -35041,9 +35037,9 @@
         <f>IF(A97="","","   Available Water [maf]")</f>
         <v xml:space="preserve">   Available Water [maf]</v>
       </c>
-      <c r="C99" s="12">
+      <c r="C99" s="12" t="str">
         <f>IF(OR(C$28="",$A99=""),"",C40+C58-C50+C96)</f>
-        <v>1.4517875437728884</v>
+        <v/>
       </c>
       <c r="D99" s="12" t="str">
         <f t="shared" ref="D99:L99" si="58">IF(OR(D$28="",$A99=""),"",D40+D58-D50+D96)</f>
@@ -35109,9 +35105,9 @@
         <f>IF(A100="","","   End of Year Balance [maf]")</f>
         <v xml:space="preserve">   End of Year Balance [maf]</v>
       </c>
-      <c r="C101" s="12">
+      <c r="C101" s="12" t="str">
         <f>IF(OR(C$28="",$A101=""),"",C99-C100)</f>
-        <v>1.4517875437728884</v>
+        <v/>
       </c>
       <c r="D101" s="12" t="str">
         <f t="shared" ref="D101:L101" si="59">IF(OR(D$28="",$A101=""),"",D99-D100)</f>
@@ -35231,9 +35227,9 @@
         <f>IF(A105="","",$A$66)</f>
         <v xml:space="preserve">   Net trade volume all participants (should be zero)</v>
       </c>
-      <c r="C106" s="44">
-        <f t="shared" ref="C106:M106" ca="1" si="60">IF(OR(C$28="",$A106=""),"",C$119)</f>
-        <v>0</v>
+      <c r="C106" s="44" t="str">
+        <f t="shared" ref="C106:M106" si="60">IF(OR(C$28="",$A106=""),"",C$119)</f>
+        <v/>
       </c>
       <c r="D106" s="44" t="str">
         <f t="shared" si="60"/>
@@ -35284,9 +35280,9 @@
         <f>IF(A105="","","   Available Water [maf]")</f>
         <v xml:space="preserve">   Available Water [maf]</v>
       </c>
-      <c r="C107" s="12">
+      <c r="C107" s="12" t="str">
         <f>IF(OR(C$28="",$A107=""),"",C41+C59-C51+C104)</f>
-        <v>0.97711394605939117</v>
+        <v/>
       </c>
       <c r="D107" s="12" t="str">
         <f t="shared" ref="D107:L107" si="61">IF(OR(D$28="",$A107=""),"",D41+D59-D51+D104)</f>
@@ -35352,9 +35348,9 @@
         <f>IF(A108="","","   End of Year Balance [maf]")</f>
         <v xml:space="preserve">   End of Year Balance [maf]</v>
       </c>
-      <c r="C109" s="12">
+      <c r="C109" s="12" t="str">
         <f>IF(OR(C$28="",$A109=""),"",C107-C108)</f>
-        <v>0.97711394605939117</v>
+        <v/>
       </c>
       <c r="D109" s="12" t="str">
         <f t="shared" ref="D109:L109" si="62">IF(OR(D$28="",$A109=""),"",D107-D108)</f>
@@ -35436,9 +35432,9 @@
         <v xml:space="preserve">    Reclamation - Protect Zone</v>
       </c>
       <c r="B113" s="1"/>
-      <c r="C113" s="44">
+      <c r="C113" s="44" t="str">
         <f t="shared" ref="C113:L113" ca="1" si="64">IF(OR(C$28="",$A113=""),"",OFFSET(C$64,8*(ROW(B113)-ROW(B$113)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D113" s="44" t="str">
         <f t="shared" ca="1" si="64"/>
@@ -35488,9 +35484,9 @@
         <v xml:space="preserve">    California</v>
       </c>
       <c r="B114" s="1"/>
-      <c r="C114" s="44">
+      <c r="C114" s="44" t="str">
         <f t="shared" ref="C114:L114" ca="1" si="65">IF(OR(C$28="",$A114=""),"",OFFSET(C$64,8*(ROW(B114)-ROW(B$113)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D114" s="44" t="str">
         <f t="shared" ca="1" si="65"/>
@@ -35540,9 +35536,9 @@
         <v xml:space="preserve">    Arizona</v>
       </c>
       <c r="B115" s="1"/>
-      <c r="C115" s="44">
+      <c r="C115" s="44" t="str">
         <f t="shared" ref="C115:L115" ca="1" si="67">IF(OR(C$28="",$A115=""),"",OFFSET(C$64,8*(ROW(B115)-ROW(B$113)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D115" s="44" t="str">
         <f t="shared" ca="1" si="67"/>
@@ -35592,9 +35588,9 @@
         <v xml:space="preserve">    Nevada</v>
       </c>
       <c r="B116" s="1"/>
-      <c r="C116" s="44">
+      <c r="C116" s="44" t="str">
         <f t="shared" ref="C116:L116" ca="1" si="68">IF(OR(C$28="",$A116=""),"",OFFSET(C$64,8*(ROW(B116)-ROW(B$113)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D116" s="44" t="str">
         <f t="shared" ca="1" si="68"/>
@@ -35644,9 +35640,9 @@
         <v xml:space="preserve">    Mexico</v>
       </c>
       <c r="B117" s="1"/>
-      <c r="C117" s="44">
+      <c r="C117" s="44" t="str">
         <f t="shared" ref="C117:L117" ca="1" si="69">IF(OR(C$28="",$A117=""),"",OFFSET(C$64,8*(ROW(B117)-ROW(B$113)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D117" s="44" t="str">
         <f t="shared" ca="1" si="69"/>
@@ -35696,9 +35692,9 @@
         <v xml:space="preserve">    Tribal Nations of the Lower Basin</v>
       </c>
       <c r="B118" s="1"/>
-      <c r="C118" s="44">
+      <c r="C118" s="44" t="str">
         <f t="shared" ref="C118:L118" ca="1" si="70">IF(OR(C$28="",$A118=""),"",OFFSET(C$64,8*(ROW(B118)-ROW(B$113)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D118" s="44" t="str">
         <f t="shared" ca="1" si="70"/>
@@ -35747,9 +35743,9 @@
         <v>77</v>
       </c>
       <c r="B119" s="1"/>
-      <c r="C119" s="12">
-        <f ca="1">IF(C$28&lt;&gt;"",SUM(C113:C118),"")</f>
-        <v>0</v>
+      <c r="C119" s="12" t="str">
+        <f>IF(C$28&lt;&gt;"",SUM(C113:C118),"")</f>
+        <v/>
       </c>
       <c r="D119" s="12" t="str">
         <f t="shared" ref="D119:L119" si="71">IF(D$28&lt;&gt;"",SUM(D113:D118),"")</f>
@@ -35812,9 +35808,9 @@
         <f>IF(A5="","","    "&amp;A5&amp;" - Consumptive Use and Headwaters Losses")</f>
         <v xml:space="preserve">    Reclamation - Protect Zone - Consumptive Use and Headwaters Losses</v>
       </c>
-      <c r="C121" s="44">
+      <c r="C121" s="44" t="str">
         <f t="shared" ref="C121:L121" ca="1" si="72">IF(OR(C$28="",$A121=""),"",OFFSET(C$68,8*(ROW(B121)-ROW(B$121)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D121" s="44" t="str">
         <f t="shared" ca="1" si="72"/>
@@ -35859,9 +35855,9 @@
         <f>IF(A6="","","    "&amp;A6&amp;" - Release from Mead")</f>
         <v xml:space="preserve">    California - Release from Mead</v>
       </c>
-      <c r="C122" s="44">
+      <c r="C122" s="44" t="str">
         <f t="shared" ref="C122:L122" ca="1" si="73">IF(OR(C$28="",$A122=""),"",OFFSET(C$68,8*(ROW(B122)-ROW(B$121)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D122" s="44" t="str">
         <f t="shared" ca="1" si="73"/>
@@ -35906,9 +35902,9 @@
         <f>IF(A7="","","    "&amp;A7&amp;" - Release from Mead")</f>
         <v xml:space="preserve">    Arizona - Release from Mead</v>
       </c>
-      <c r="C123" s="44">
+      <c r="C123" s="44" t="str">
         <f t="shared" ref="C123:L123" ca="1" si="74">IF(OR(C$28="",$A123=""),"",OFFSET(C$68,8*(ROW(B123)-ROW(B$121)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D123" s="44" t="str">
         <f t="shared" ca="1" si="74"/>
@@ -35953,9 +35949,9 @@
         <f>IF(A8="","","    "&amp;A8&amp;" - Release from Mead")</f>
         <v xml:space="preserve">    Nevada - Release from Mead</v>
       </c>
-      <c r="C124" s="44">
+      <c r="C124" s="44" t="str">
         <f t="shared" ref="C124:L124" ca="1" si="75">IF(OR(C$28="",$A124=""),"",OFFSET(C$68,8*(ROW(B124)-ROW(B$121)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D124" s="44" t="str">
         <f t="shared" ca="1" si="75"/>
@@ -36000,9 +35996,9 @@
         <f>IF(A9="","","    "&amp;A9&amp;" - Release from Mead")</f>
         <v xml:space="preserve">    Mexico - Release from Mead</v>
       </c>
-      <c r="C125" s="44">
+      <c r="C125" s="44" t="str">
         <f t="shared" ref="C125:L125" ca="1" si="76">IF(OR(C$28="",$A125=""),"",OFFSET(C$68,8*(ROW(B125)-ROW(B$121)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D125" s="44" t="str">
         <f t="shared" ca="1" si="76"/>
@@ -36047,9 +36043,9 @@
         <f>IF(A10="","","    "&amp;A10&amp;" - Release from Mead")</f>
         <v xml:space="preserve">    Tribal Nations of the Lower Basin - Release from Mead</v>
       </c>
-      <c r="C126" s="44">
+      <c r="C126" s="44" t="str">
         <f t="shared" ref="C126:L126" ca="1" si="77">IF(OR(C$28="",$A126=""),"",OFFSET(C$68,8*(ROW(B126)-ROW(B$121)),0))</f>
-        <v>0</v>
+        <v/>
       </c>
       <c r="D126" s="44" t="str">
         <f t="shared" ca="1" si="77"/>
@@ -36110,9 +36106,9 @@
         <f t="shared" ref="A128:A133" si="78">IF(A5="","","    "&amp;A5)</f>
         <v xml:space="preserve">    Reclamation - Protect Zone</v>
       </c>
-      <c r="C128" s="44">
+      <c r="C128" s="44" t="str">
         <f t="shared" ref="C128:L128" ca="1" si="79">IF(OR(C$28="",$A128=""),"",OFFSET(C$69,8*(ROW(B128)-ROW(B$128)),0))</f>
-        <v>5.664593</v>
+        <v/>
       </c>
       <c r="D128" s="44" t="str">
         <f t="shared" ca="1" si="79"/>
@@ -36157,9 +36153,9 @@
         <f t="shared" si="78"/>
         <v xml:space="preserve">    California</v>
       </c>
-      <c r="C129" s="44">
+      <c r="C129" s="44" t="str">
         <f t="shared" ref="C129:L129" ca="1" si="80">IF(OR(C$28="",$A129=""),"",OFFSET(C$69,8*(ROW(B129)-ROW(B$128)),0))</f>
-        <v>5.2339066027155949</v>
+        <v/>
       </c>
       <c r="D129" s="44" t="str">
         <f t="shared" ca="1" si="80"/>
@@ -36204,9 +36200,9 @@
         <f t="shared" si="78"/>
         <v xml:space="preserve">    Arizona</v>
       </c>
-      <c r="C130" s="44">
+      <c r="C130" s="44" t="str">
         <f t="shared" ref="C130:L130" ca="1" si="81">IF(OR(C$28="",$A130=""),"",OFFSET(C$69,8*(ROW(B130)-ROW(B$128)),0))</f>
-        <v>1.8463761056585704</v>
+        <v/>
       </c>
       <c r="D130" s="44" t="str">
         <f t="shared" ca="1" si="81"/>
@@ -36251,9 +36247,9 @@
         <f t="shared" si="78"/>
         <v xml:space="preserve">    Nevada</v>
       </c>
-      <c r="C131" s="44">
+      <c r="C131" s="44" t="str">
         <f t="shared" ref="C131:L131" ca="1" si="82">IF(OR(C$28="",$A131=""),"",OFFSET(C$69,8*(ROW(B131)-ROW(B$128)),0))</f>
-        <v>1.021414490246157</v>
+        <v/>
       </c>
       <c r="D131" s="44" t="str">
         <f t="shared" ca="1" si="82"/>
@@ -36298,9 +36294,9 @@
         <f t="shared" si="78"/>
         <v xml:space="preserve">    Mexico</v>
       </c>
-      <c r="C132" s="44">
+      <c r="C132" s="44" t="str">
         <f t="shared" ref="C132:L132" ca="1" si="83">IF(OR(C$28="",$A132=""),"",OFFSET(C$69,8*(ROW(B132)-ROW(B$128)),0))</f>
-        <v>1.4517875437728884</v>
+        <v/>
       </c>
       <c r="D132" s="44" t="str">
         <f t="shared" ca="1" si="83"/>
@@ -36345,9 +36341,9 @@
         <f t="shared" si="78"/>
         <v xml:space="preserve">    Tribal Nations of the Lower Basin</v>
       </c>
-      <c r="C133" s="44">
+      <c r="C133" s="44" t="str">
         <f t="shared" ref="C133:L133" ca="1" si="84">IF(OR(C$28="",$A133=""),"",OFFSET(C$69,8*(ROW(B133)-ROW(B$128)),0))</f>
-        <v>0.97711394605939117</v>
+        <v/>
       </c>
       <c r="D133" s="44" t="str">
         <f t="shared" ca="1" si="84"/>
@@ -36420,9 +36416,9 @@
         <v>293</v>
       </c>
       <c r="B135" s="1"/>
-      <c r="C135" s="12">
-        <f ca="1">IF(C$28&lt;&gt;"",SUM(C128:C133),"")</f>
-        <v>16.195191688452603</v>
+      <c r="C135" s="12" t="str">
+        <f>IF(C$28&lt;&gt;"",SUM(C128:C133),"")</f>
+        <v/>
       </c>
       <c r="D135" s="12" t="str">
         <f>IF(D$28&lt;&gt;"",SUM(D128:D133),"")</f>
@@ -36452,9 +36448,9 @@
         <v>294</v>
       </c>
       <c r="B136" s="1"/>
-      <c r="C136" s="219">
-        <f ca="1">IF(C$28&lt;&gt;"",VLOOKUP(C135*1000000,'Mead-Elevation-Area'!$B$5:$H$689,7),"")</f>
-        <v>1145</v>
+      <c r="C136" s="219" t="str">
+        <f>IF(C$28&lt;&gt;"",VLOOKUP(C135*1000000,'Mead-Elevation-Area'!$B$5:$H$689,7),"")</f>
+        <v/>
       </c>
       <c r="D136" s="219" t="str">
         <f>IF(D$28&lt;&gt;"",VLOOKUP(D135*1000000,'Mead-Elevation-Area'!$B$5:$H$689,7),"")</f>
@@ -38523,16 +38519,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="340" t="e">
+      <c r="A1" s="339" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="340"/>
-      <c r="C1" s="340"/>
-      <c r="D1" s="340"/>
-      <c r="E1" s="340"/>
-      <c r="F1" s="340"/>
-      <c r="G1" s="340"/>
+      <c r="B1" s="339"/>
+      <c r="C1" s="339"/>
+      <c r="D1" s="339"/>
+      <c r="E1" s="339"/>
+      <c r="F1" s="339"/>
+      <c r="G1" s="339"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -38641,11 +38637,11 @@
         <v>80</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="339"/>
-      <c r="D10" s="339"/>
-      <c r="E10" s="339"/>
-      <c r="F10" s="339"/>
-      <c r="G10" s="339"/>
+      <c r="C10" s="340"/>
+      <c r="D10" s="340"/>
+      <c r="E10" s="340"/>
+      <c r="F10" s="340"/>
+      <c r="G10" s="340"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
@@ -39406,9 +39402,9 @@
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
-      <c r="M39" s="28">
+      <c r="M39" s="28" t="str">
         <f>Master!C52</f>
-        <v>8</v>
+        <v/>
       </c>
       <c r="N39" s="140" t="s">
         <v>185</v>
@@ -39462,9 +39458,9 @@
         <f t="shared" si="7"/>
         <v>#REF!</v>
       </c>
-      <c r="M40" s="28">
+      <c r="M40" s="28" t="str">
         <f>Master!C53</f>
-        <v>0.30214853419597149</v>
+        <v/>
       </c>
       <c r="N40" s="143"/>
       <c r="P40" s="81"/>
@@ -39518,9 +39514,9 @@
         <f t="shared" si="8"/>
         <v>#REF!</v>
       </c>
-      <c r="M41" s="28">
+      <c r="M41" s="28" t="str">
         <f>Master!C55</f>
-        <v>3.9038054941039078</v>
+        <v/>
       </c>
       <c r="N41" s="143"/>
       <c r="P41" s="81"/>
@@ -39573,9 +39569,9 @@
         <f t="shared" si="9"/>
         <v>#REF!</v>
       </c>
-      <c r="M42" s="28">
+      <c r="M42" s="28" t="str">
         <f>Master!C56</f>
-        <v>1.2773617324799242</v>
+        <v/>
       </c>
       <c r="N42" s="143"/>
     </row>
@@ -39628,9 +39624,9 @@
         <f t="shared" si="10"/>
         <v>#REF!</v>
       </c>
-      <c r="M43" s="179">
+      <c r="M43" s="179" t="str">
         <f>Master!C57</f>
-        <v>0.2566463678699063</v>
+        <v/>
       </c>
       <c r="N43" s="143"/>
     </row>
@@ -39683,9 +39679,9 @@
         <f t="shared" si="12"/>
         <v>#REF!</v>
       </c>
-      <c r="M44" s="28">
+      <c r="M44" s="28" t="str">
         <f>Master!C58</f>
-        <v>1.2829239252908993</v>
+        <v/>
       </c>
       <c r="N44" s="143"/>
     </row>
@@ -39737,9 +39733,9 @@
         <f t="shared" si="13"/>
         <v>#REF!</v>
       </c>
-      <c r="M45" s="28">
+      <c r="M45" s="28" t="str">
         <f>Master!C59</f>
-        <v>0.97711394605939117</v>
+        <v/>
       </c>
       <c r="N45" s="143"/>
     </row>
@@ -39791,9 +39787,9 @@
         <f t="shared" si="14"/>
         <v>#REF!</v>
       </c>
-      <c r="M46" s="28">
+      <c r="M46" s="28" t="str">
         <f>Master!C60</f>
-        <v>0.6</v>
+        <v/>
       </c>
       <c r="N46" s="143"/>
     </row>
@@ -39908,12 +39904,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -39921,6 +39911,12 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>

</xml_diff>

<commit_message>
Anabelle added new worksheet of inflow scenarios
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anabelle/Documents/HydrologicScenarios/ColoradoRiverCollaborate/LakeMeadWaterBankDivideInflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1502254-8023-2A4B-9BFE-C7244DFEF2A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCBDB13-F4FC-B045-9744-F4175AEA06AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="3" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="62" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="PowellReleaseTemperature" sheetId="43" r:id="rId9"/>
     <sheet name="Mead-Elevation-Area" sheetId="10" r:id="rId10"/>
     <sheet name="CellType" sheetId="54" r:id="rId11"/>
+    <sheet name="LakeMeadInflowScenarios" sheetId="64" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="420">
   <si>
     <t>Year 1</t>
   </si>
@@ -121,9 +122,6 @@
   </si>
   <si>
     <t>Master</t>
-  </si>
-  <si>
-    <t>HydrologicScenarios</t>
   </si>
   <si>
     <t>Total</t>
@@ -1086,9 +1084,6 @@
     <t>Lookup table of Lower Basin and Mexico mandatory cuts versus Lake Mead elevation (for reference; not used in the Lake Mead Water Bank)</t>
   </si>
   <si>
-    <t>Shares scenarios of Lake Mead Inflow based on historical data.</t>
-  </si>
-  <si>
     <t>https://github.com/dzeke/ColoradoRiverCollaborate/tree/main/LakeMeadWaterBankDivideInflow</t>
   </si>
   <si>
@@ -1957,7 +1952,182 @@
     <t>Add recent water use in Model Guide</t>
   </si>
   <si>
-    <t>David E. Rosenberg, Hadia Akbar, Erik Porse (2025). "Immersive Model for Lake Mead Based on the Principle of Division of Reservoir Inflow." Utah State University, Logan, UT. https://github.com/dzeke/ColoradoRiverCollaborate/tree/main/LakeMeadWaterBankDivideInflow.</t>
+    <t>Ensemble</t>
+  </si>
+  <si>
+    <t># of Traces</t>
+  </si>
+  <si>
+    <t>Minimum Summation of Ensemble</t>
+  </si>
+  <si>
+    <t>Trace</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First </t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>Third</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>CMIP5_LOCA</t>
+  </si>
+  <si>
+    <t>RCP_85_100</t>
+  </si>
+  <si>
+    <t>trace17</t>
+  </si>
+  <si>
+    <t>AR1</t>
+  </si>
+  <si>
+    <t>CMIP5_BCSD</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>CMIP3</t>
+  </si>
+  <si>
+    <t>Trace55</t>
+  </si>
+  <si>
+    <t>Drought_Mid20th</t>
+  </si>
+  <si>
+    <t>Trace33</t>
+  </si>
+  <si>
+    <t>RCP85_065</t>
+  </si>
+  <si>
+    <t>NPC_1988_2020</t>
+  </si>
+  <si>
+    <t>Trace1</t>
+  </si>
+  <si>
+    <t>Drought_Paleo</t>
+  </si>
+  <si>
+    <t>Trace42</t>
+  </si>
+  <si>
+    <t>RCP45_100</t>
+  </si>
+  <si>
+    <t>Drought_Millennium</t>
+  </si>
+  <si>
+    <t>Trace46</t>
+  </si>
+  <si>
+    <t>NPC_1906_2020</t>
+  </si>
+  <si>
+    <t>Trace18</t>
+  </si>
+  <si>
+    <t>NPC_2000_2020</t>
+  </si>
+  <si>
+    <t>Trace94</t>
+  </si>
+  <si>
+    <t>ISM_TRM17SK</t>
+  </si>
+  <si>
+    <t>TreeRingFlows</t>
+  </si>
+  <si>
+    <t>RCP45_065</t>
+  </si>
+  <si>
+    <t>RCP85_030</t>
+  </si>
+  <si>
+    <t>RCP45_030</t>
+  </si>
+  <si>
+    <t>trace18</t>
+  </si>
+  <si>
+    <t>Mill_5YrBlockRes</t>
+  </si>
+  <si>
+    <t>Trace27</t>
+  </si>
+  <si>
+    <t>ISM_Full</t>
+  </si>
+  <si>
+    <t>ISM_PluvialRemoved</t>
+  </si>
+  <si>
+    <t>ISM_StressTest</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The annual Lake Mead inflow magnitude has been determined by using data from the data sheet, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+      </rPr>
+      <t xml:space="preserve">HydrologicScenarios </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos"/>
+      </rPr>
+      <t>(Salehabadi DATE). All Ensembles and traces were used in determining Lake Mead’s inflow. Using code written in Python, three consecutive smallest values in each trace were found.</t>
+    </r>
+  </si>
+  <si>
+    <t>Scenarios of Extreme Lake Mead Inflow</t>
+  </si>
+  <si>
+    <t>Lake Mead Inflow Scenarios</t>
+  </si>
+  <si>
+    <t>Extreme low inflow Lake Mead Scenarios. Lowest three year sequences from HydrologicScenarios (Salehabadi)</t>
+  </si>
+  <si>
+    <t>Anabelle Myers</t>
+  </si>
+  <si>
+    <t>A02369941@aggies.usu.edu</t>
+  </si>
+  <si>
+    <t>David E. Rosenberg, Anabelle Myers, Hadia Akbar, Erik Porse (2025). "Immersive Model for Lake Mead Based on the Principle of Division of Reservoir Inflow." Utah State University, Logan, UT. https://github.com/dzeke/ColoradoRiverCollaborate/tree/main/LakeMeadWaterBankDivideInflow.</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>Add extreme low Lake Mead inflow hydrologic scenarios</t>
+  </si>
+  <si>
+    <t>Myers</t>
+  </si>
+  <si>
+    <t>Collaborators in model session</t>
   </si>
 </sst>
 </file>
@@ -1979,7 +2149,7 @@
     <numFmt numFmtId="173" formatCode="#,##0.0_);\(#,##0.0\)"/>
     <numFmt numFmtId="174" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="27" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2181,8 +2351,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+    </font>
   </fonts>
-  <fills count="29">
+  <fills count="31">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2347,8 +2549,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -2590,6 +2804,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2608,7 +2915,7 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="348">
+  <cellXfs count="363">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3565,6 +3872,33 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="20% - Accent1" xfId="12" builtinId="30"/>
@@ -15102,9 +15436,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EA02F4-5F19-409C-8BC6-A0D8FEB3A90D}">
-  <dimension ref="A1:R84"/>
+  <dimension ref="A1:R88"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
@@ -15125,7 +15459,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="279" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="B1" s="279"/>
       <c r="C1" s="279"/>
@@ -15147,7 +15481,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="154" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" s="155"/>
       <c r="C3" s="156"/>
@@ -15164,7 +15498,7 @@
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="280" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B4" s="281"/>
       <c r="C4" s="281"/>
@@ -15185,7 +15519,7 @@
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="284" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B5" s="285"/>
       <c r="C5" s="285"/>
@@ -15206,7 +15540,7 @@
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="284" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B6" s="285"/>
       <c r="C6" s="285"/>
@@ -15228,7 +15562,7 @@
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="232"/>
       <c r="B7" s="285" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C7" s="285"/>
       <c r="D7" s="285"/>
@@ -15249,7 +15583,7 @@
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="233"/>
       <c r="B8" s="300" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C8" s="300"/>
       <c r="D8" s="300"/>
@@ -15283,7 +15617,7 @@
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="302" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B10" s="303"/>
       <c r="C10" s="303"/>
@@ -15299,10 +15633,10 @@
     </row>
     <row r="11" spans="1:18" s="58" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="253" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B11" s="257" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="C11" s="257"/>
       <c r="D11" s="257"/>
@@ -15331,10 +15665,10 @@
     </row>
     <row r="13" spans="1:18" s="58" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="253" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B13" s="257" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C13" s="257"/>
       <c r="D13" s="257"/>
@@ -15363,10 +15697,10 @@
     </row>
     <row r="15" spans="1:18" s="58" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="253" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B15" s="257" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C15" s="257"/>
       <c r="D15" s="257"/>
@@ -15395,13 +15729,13 @@
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="255" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B17" s="256"/>
       <c r="C17" s="256"/>
       <c r="D17" s="256"/>
       <c r="E17" s="250" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F17" s="248"/>
       <c r="G17" s="248"/>
@@ -15427,7 +15761,7 @@
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="287" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B19" s="288"/>
       <c r="C19" s="288"/>
@@ -15443,7 +15777,7 @@
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="290" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B20" s="291"/>
       <c r="C20" s="291"/>
@@ -15459,7 +15793,7 @@
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="293" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B21" s="271"/>
       <c r="C21" s="271"/>
@@ -15475,7 +15809,7 @@
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="293" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B22" s="271"/>
       <c r="C22" s="271"/>
@@ -15491,7 +15825,7 @@
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="294" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B23" s="295"/>
       <c r="C23" s="295"/>
@@ -15521,7 +15855,7 @@
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="297" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B25" s="298"/>
       <c r="C25" s="298"/>
@@ -15538,7 +15872,7 @@
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="276" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B26" s="277"/>
       <c r="C26" s="277"/>
@@ -15558,7 +15892,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="264" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C27" s="264"/>
       <c r="D27" s="264"/>
@@ -15576,7 +15910,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="264" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C28" s="264"/>
       <c r="D28" s="264"/>
@@ -15595,7 +15929,7 @@
         <v>3</v>
       </c>
       <c r="B29" s="264" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C29" s="264"/>
       <c r="D29" s="264"/>
@@ -15614,7 +15948,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="264" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C30" s="264"/>
       <c r="D30" s="264"/>
@@ -15633,7 +15967,7 @@
         <v>5</v>
       </c>
       <c r="B31" s="264" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C31" s="264"/>
       <c r="D31" s="264"/>
@@ -15650,7 +15984,7 @@
     <row r="32" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="227"/>
       <c r="B32" s="264" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C32" s="264"/>
       <c r="D32" s="264"/>
@@ -15667,7 +16001,7 @@
     <row r="33" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="227"/>
       <c r="B33" s="264" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C33" s="264"/>
       <c r="D33" s="264"/>
@@ -15683,7 +16017,7 @@
     </row>
     <row r="34" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="273" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B34" s="274"/>
       <c r="C34" s="274"/>
@@ -15703,7 +16037,7 @@
         <v>1</v>
       </c>
       <c r="B35" s="264" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C35" s="264"/>
       <c r="D35" s="264"/>
@@ -15720,7 +16054,7 @@
     <row r="36" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="227"/>
       <c r="B36" s="262" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C36" s="262"/>
       <c r="D36" s="262"/>
@@ -15739,7 +16073,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="264" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C37" s="264"/>
       <c r="D37" s="264"/>
@@ -15758,7 +16092,7 @@
         <v>3</v>
       </c>
       <c r="B38" s="264" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C38" s="264"/>
       <c r="D38" s="264"/>
@@ -15777,7 +16111,7 @@
         <v>4</v>
       </c>
       <c r="B39" s="264" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C39" s="264"/>
       <c r="D39" s="264"/>
@@ -15796,7 +16130,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="262" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="C40" s="262"/>
       <c r="D40" s="262"/>
@@ -15815,7 +16149,7 @@
         <v>6</v>
       </c>
       <c r="B41" s="262" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C41" s="262"/>
       <c r="D41" s="262"/>
@@ -15834,7 +16168,7 @@
         <v>7</v>
       </c>
       <c r="B42" s="264" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C42" s="264"/>
       <c r="D42" s="264"/>
@@ -15863,7 +16197,7 @@
     </row>
     <row r="44" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="273" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B44" s="274"/>
       <c r="C44" s="274"/>
@@ -15879,10 +16213,10 @@
     </row>
     <row r="45" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="230" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B45" s="264" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C45" s="264"/>
       <c r="D45" s="264"/>
@@ -15897,10 +16231,10 @@
     </row>
     <row r="46" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="231" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B46" s="266" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C46" s="266"/>
       <c r="D46" s="266"/>
@@ -15929,7 +16263,7 @@
     </row>
     <row r="48" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="268" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B48" s="269"/>
       <c r="C48" s="269"/>
@@ -15945,7 +16279,7 @@
     </row>
     <row r="49" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="234" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B49" s="161"/>
       <c r="C49" s="161"/>
@@ -15974,7 +16308,7 @@
     </row>
     <row r="51" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="163" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B51" s="164"/>
       <c r="C51" s="164"/>
@@ -15994,7 +16328,7 @@
         <v>24</v>
       </c>
       <c r="C52" s="169" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D52" s="169"/>
       <c r="E52" s="169"/>
@@ -16009,10 +16343,10 @@
     <row r="53" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="167"/>
       <c r="B53" s="168" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C53" s="169" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D53" s="169"/>
       <c r="E53" s="169"/>
@@ -16030,7 +16364,7 @@
         <v>24</v>
       </c>
       <c r="C54" s="271" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D54" s="271"/>
       <c r="E54" s="271"/>
@@ -16045,10 +16379,10 @@
     <row r="55" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="167"/>
       <c r="B55" s="168" t="s">
+        <v>274</v>
+      </c>
+      <c r="C55" s="271" t="s">
         <v>275</v>
-      </c>
-      <c r="C55" s="271" t="s">
-        <v>276</v>
       </c>
       <c r="D55" s="271"/>
       <c r="E55" s="271"/>
@@ -16063,10 +16397,10 @@
     <row r="56" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="167"/>
       <c r="B56" s="168" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C56" s="271" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D56" s="271"/>
       <c r="E56" s="271"/>
@@ -16081,10 +16415,10 @@
     <row r="57" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="167"/>
       <c r="B57" s="168" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" s="271" t="s">
         <v>100</v>
-      </c>
-      <c r="C57" s="271" t="s">
-        <v>101</v>
       </c>
       <c r="D57" s="271"/>
       <c r="E57" s="271"/>
@@ -16099,10 +16433,10 @@
     <row r="58" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="167"/>
       <c r="B58" s="168" t="s">
+        <v>199</v>
+      </c>
+      <c r="C58" s="271" t="s">
         <v>200</v>
-      </c>
-      <c r="C58" s="271" t="s">
-        <v>201</v>
       </c>
       <c r="D58" s="271"/>
       <c r="E58" s="271"/>
@@ -16117,10 +16451,10 @@
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="167"/>
       <c r="B59" s="168" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C59" s="169" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D59" s="169"/>
       <c r="E59" s="169"/>
@@ -16135,10 +16469,10 @@
     <row r="60" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="167"/>
       <c r="B60" s="168" t="s">
-        <v>25</v>
+        <v>411</v>
       </c>
       <c r="C60" s="271" t="s">
-        <v>278</v>
+        <v>412</v>
       </c>
       <c r="D60" s="271"/>
       <c r="E60" s="271"/>
@@ -16153,10 +16487,10 @@
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="167"/>
       <c r="B61" s="168" t="s">
+        <v>36</v>
+      </c>
+      <c r="C61" s="169" t="s">
         <v>37</v>
-      </c>
-      <c r="C61" s="169" t="s">
-        <v>38</v>
       </c>
       <c r="D61" s="169"/>
       <c r="E61" s="169"/>
@@ -16171,10 +16505,10 @@
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="171"/>
       <c r="B62" s="172" t="s">
+        <v>120</v>
+      </c>
+      <c r="C62" s="173" t="s">
         <v>121</v>
-      </c>
-      <c r="C62" s="173" t="s">
-        <v>122</v>
       </c>
       <c r="D62" s="173"/>
       <c r="E62" s="173"/>
@@ -16188,83 +16522,104 @@
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A65" s="1" t="s">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="45" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A67" s="45" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="45" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A68" s="45" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="45"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A70" s="247" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="45"/>
+      <c r="B70" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="45"/>
+      <c r="B71" s="362" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="45"/>
+      <c r="B72" s="45" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="45"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="247" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="246" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="45" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A71" s="246" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A72" s="45" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A73" s="45"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A74" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A75" s="45" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A77" s="1" t="s">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="45"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="45" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="261" t="s">
-        <v>369</v>
-      </c>
-      <c r="B78" s="261"/>
-      <c r="C78" s="261"/>
-      <c r="D78" s="261"/>
-      <c r="E78" s="261"/>
-      <c r="F78" s="261"/>
-      <c r="G78" s="261"/>
-      <c r="H78" s="261"/>
-      <c r="I78" s="261"/>
-      <c r="J78" s="261"/>
-      <c r="K78" s="261"/>
-      <c r="L78" s="261"/>
-    </row>
-    <row r="83" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="261" t="s">
+        <v>415</v>
+      </c>
+      <c r="B82" s="261"/>
+      <c r="C82" s="261"/>
+      <c r="D82" s="261"/>
+      <c r="E82" s="261"/>
+      <c r="F82" s="261"/>
+      <c r="G82" s="261"/>
+      <c r="H82" s="261"/>
+      <c r="I82" s="261"/>
+      <c r="J82" s="261"/>
+      <c r="K82" s="261"/>
+      <c r="L82" s="261"/>
+    </row>
+    <row r="87" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="47">
     <mergeCell ref="A26:L26"/>
@@ -16302,7 +16657,7 @@
     <mergeCell ref="B13:L13"/>
     <mergeCell ref="B14:L14"/>
     <mergeCell ref="B15:L15"/>
-    <mergeCell ref="A78:L78"/>
+    <mergeCell ref="A82:L82"/>
     <mergeCell ref="B41:L41"/>
     <mergeCell ref="B42:L42"/>
     <mergeCell ref="B45:L45"/>
@@ -16318,14 +16673,15 @@
   <hyperlinks>
     <hyperlink ref="A67" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
     <hyperlink ref="A68" r:id="rId2" xr:uid="{66F54200-A2AB-43DA-A0E0-F2A25A075EE5}"/>
-    <hyperlink ref="A75" r:id="rId3" xr:uid="{A0F8DE06-D9FC-495F-9A01-AA199CB82365}"/>
+    <hyperlink ref="A79" r:id="rId3" xr:uid="{A0F8DE06-D9FC-495F-9A01-AA199CB82365}"/>
     <hyperlink ref="A48:L48" r:id="rId4" display="LETS START (visual directions as pdf)" xr:uid="{0D075873-7EBB-4309-B00A-6A62EA192A0C}"/>
     <hyperlink ref="A49" r:id="rId5" xr:uid="{25154A32-BA44-496E-9945-086DE0980DBD}"/>
-    <hyperlink ref="A72" r:id="rId6" xr:uid="{AA792CE4-4071-4CE8-87C6-993A0BA6C6A5}"/>
+    <hyperlink ref="A76" r:id="rId6" xr:uid="{AA792CE4-4071-4CE8-87C6-993A0BA6C6A5}"/>
     <hyperlink ref="E17" r:id="rId7" xr:uid="{218FEB9D-6782-4420-9DCE-4D6F20EDE6D5}"/>
+    <hyperlink ref="B72" r:id="rId8" xr:uid="{E4DF21D7-58D7-F94D-825D-01575427A9FE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId8"/>
+  <drawing r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -16346,47 +16702,47 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="59" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="342" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B3" s="342"/>
       <c r="C3" s="342"/>
       <c r="D3" s="128" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="343" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="343"/>
       <c r="C4" s="343"/>
       <c r="D4" s="175" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="347" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B5" s="344"/>
       <c r="C5" s="344"/>
       <c r="D5" s="176" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="345" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B6" s="345"/>
       <c r="C6" s="345"/>
       <c r="D6" s="177" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
@@ -16396,26 +16752,26 @@
       <c r="B7" s="346"/>
       <c r="C7" s="346"/>
       <c r="D7" s="178" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="343" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B11" s="343"/>
       <c r="C11" s="343"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="344" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B12" s="344"/>
       <c r="C12" s="344"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="345" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B13" s="345"/>
       <c r="C13" s="345"/>
@@ -16443,12 +16799,727 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD0CEE0E-0924-954A-8EB1-099546BF662D}">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="361" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="348" t="s">
+        <v>367</v>
+      </c>
+      <c r="B5" s="349" t="s">
+        <v>368</v>
+      </c>
+      <c r="C5" s="350" t="s">
+        <v>369</v>
+      </c>
+      <c r="D5" s="350" t="s">
+        <v>370</v>
+      </c>
+      <c r="E5" s="350" t="s">
+        <v>371</v>
+      </c>
+      <c r="F5" s="350" t="s">
+        <v>372</v>
+      </c>
+      <c r="G5" s="350" t="s">
+        <v>373</v>
+      </c>
+      <c r="H5" s="350" t="s">
+        <v>374</v>
+      </c>
+      <c r="I5" s="351" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="352" t="s">
+        <v>376</v>
+      </c>
+      <c r="B6" s="353">
+        <v>64</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>122</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="354">
+        <f>AVERAGE(F6:H6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="352" t="s">
+        <v>377</v>
+      </c>
+      <c r="B7" s="353">
+        <v>112</v>
+      </c>
+      <c r="C7" s="353">
+        <v>11.6</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E7">
+        <v>81</v>
+      </c>
+      <c r="F7">
+        <v>2.8</v>
+      </c>
+      <c r="G7">
+        <v>4.7</v>
+      </c>
+      <c r="H7">
+        <v>4.2</v>
+      </c>
+      <c r="I7" s="354">
+        <f>AVERAGE(F7:H7)</f>
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="352" t="s">
+        <v>379</v>
+      </c>
+      <c r="B8" s="353">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>14.1</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E8">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>-1.3</v>
+      </c>
+      <c r="H8">
+        <v>5.4</v>
+      </c>
+      <c r="I8" s="354">
+        <f>AVERAGE(F8:H8)</f>
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="352" t="s">
+        <v>380</v>
+      </c>
+      <c r="B9" s="353">
+        <v>97</v>
+      </c>
+      <c r="C9">
+        <v>14.1</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="E9">
+        <v>147</v>
+      </c>
+      <c r="F9">
+        <v>3.8</v>
+      </c>
+      <c r="G9">
+        <v>6.3</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9" s="354">
+        <f>AVERAGE(F9:H9)</f>
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="352" t="s">
+        <v>382</v>
+      </c>
+      <c r="B10" s="353">
+        <v>112</v>
+      </c>
+      <c r="C10">
+        <v>16.5</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="E10">
+        <v>103</v>
+      </c>
+      <c r="F10">
+        <v>5.9</v>
+      </c>
+      <c r="G10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="H10">
+        <v>5.5</v>
+      </c>
+      <c r="I10" s="354">
+        <f>AVERAGE(F10:H10)</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="352" t="s">
+        <v>384</v>
+      </c>
+      <c r="B11" s="353">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="E11">
+        <v>26</v>
+      </c>
+      <c r="F11">
+        <v>5.5</v>
+      </c>
+      <c r="G11">
+        <v>5.5</v>
+      </c>
+      <c r="H11">
+        <v>5.5</v>
+      </c>
+      <c r="I11" s="354">
+        <f>AVERAGE(F11:H11)</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="352" t="s">
+        <v>386</v>
+      </c>
+      <c r="B12" s="353">
+        <v>112</v>
+      </c>
+      <c r="C12" s="353">
+        <v>16.600000000000001</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E12">
+        <v>81</v>
+      </c>
+      <c r="F12">
+        <v>3.8</v>
+      </c>
+      <c r="G12">
+        <v>6.6</v>
+      </c>
+      <c r="H12">
+        <v>6.1</v>
+      </c>
+      <c r="I12" s="354">
+        <f>AVERAGE(F12:H12)</f>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="352" t="s">
+        <v>387</v>
+      </c>
+      <c r="B13" s="353">
+        <v>100</v>
+      </c>
+      <c r="C13" s="353">
+        <v>17.8</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E13">
+        <v>31</v>
+      </c>
+      <c r="F13">
+        <v>5.9</v>
+      </c>
+      <c r="G13">
+        <v>5.9</v>
+      </c>
+      <c r="H13">
+        <v>5.9</v>
+      </c>
+      <c r="I13" s="354">
+        <f>AVERAGE(F13:H13)</f>
+        <v>5.9000000000000012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="352" t="s">
+        <v>389</v>
+      </c>
+      <c r="B14" s="353">
+        <v>100</v>
+      </c>
+      <c r="C14">
+        <v>18</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="E14">
+        <v>18</v>
+      </c>
+      <c r="F14">
+        <v>11</v>
+      </c>
+      <c r="G14">
+        <v>5.6</v>
+      </c>
+      <c r="H14">
+        <v>8.1</v>
+      </c>
+      <c r="I14" s="354">
+        <f>AVERAGE(F14:H14)</f>
+        <v>8.2333333333333343</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="352" t="s">
+        <v>391</v>
+      </c>
+      <c r="B15" s="353">
+        <v>112</v>
+      </c>
+      <c r="C15" s="353">
+        <v>19.3</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E15">
+        <v>81</v>
+      </c>
+      <c r="F15">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G15">
+        <v>7.8</v>
+      </c>
+      <c r="H15">
+        <v>7.2</v>
+      </c>
+      <c r="I15" s="354">
+        <f>AVERAGE(F15:H15)</f>
+        <v>6.4666666666666659</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="352" t="s">
+        <v>392</v>
+      </c>
+      <c r="B16" s="353">
+        <v>100</v>
+      </c>
+      <c r="C16">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="E16">
+        <v>48</v>
+      </c>
+      <c r="F16">
+        <v>5.9</v>
+      </c>
+      <c r="G16">
+        <v>5.9</v>
+      </c>
+      <c r="H16">
+        <v>8.5</v>
+      </c>
+      <c r="I16" s="354">
+        <f>AVERAGE(F16:H16)</f>
+        <v>6.7666666666666666</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="352" t="s">
+        <v>394</v>
+      </c>
+      <c r="B17" s="353">
+        <v>100</v>
+      </c>
+      <c r="C17" s="353">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E17">
+        <v>45</v>
+      </c>
+      <c r="F17">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="G17">
+        <v>6.6</v>
+      </c>
+      <c r="H17">
+        <v>5.5</v>
+      </c>
+      <c r="I17" s="354">
+        <f>AVERAGE(F17:H17)</f>
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="352" t="s">
+        <v>396</v>
+      </c>
+      <c r="B18" s="353">
+        <v>100</v>
+      </c>
+      <c r="C18" s="353">
+        <v>20.5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>8.6</v>
+      </c>
+      <c r="G18">
+        <v>5.9</v>
+      </c>
+      <c r="H18">
+        <v>5.9</v>
+      </c>
+      <c r="I18" s="354">
+        <f>AVERAGE(F18:H18)</f>
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="352" t="s">
+        <v>398</v>
+      </c>
+      <c r="B19" s="353">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>20.9</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E19">
+        <v>430</v>
+      </c>
+      <c r="F19">
+        <v>6.4</v>
+      </c>
+      <c r="G19">
+        <v>8.4</v>
+      </c>
+      <c r="H19">
+        <v>6.1</v>
+      </c>
+      <c r="I19" s="354">
+        <f>AVERAGE(F19:H19)</f>
+        <v>6.9666666666666659</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="352" t="s">
+        <v>399</v>
+      </c>
+      <c r="B20" s="353">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>20.9</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E20">
+        <v>430</v>
+      </c>
+      <c r="F20">
+        <v>6.4</v>
+      </c>
+      <c r="G20">
+        <v>8.4</v>
+      </c>
+      <c r="H20">
+        <v>6.1</v>
+      </c>
+      <c r="I20" s="354">
+        <f>AVERAGE(F20:H20)</f>
+        <v>6.9666666666666659</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="352" t="s">
+        <v>400</v>
+      </c>
+      <c r="B21" s="353">
+        <v>112</v>
+      </c>
+      <c r="C21" s="353">
+        <v>21.7</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E21">
+        <v>81</v>
+      </c>
+      <c r="F21">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G21">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="H21">
+        <v>8.1</v>
+      </c>
+      <c r="I21" s="354">
+        <f>AVERAGE(F21:H21)</f>
+        <v>7.2333333333333334</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="352" t="s">
+        <v>401</v>
+      </c>
+      <c r="B22" s="353">
+        <v>112</v>
+      </c>
+      <c r="C22" s="353">
+        <v>21.8</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="E22">
+        <v>81</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="H22">
+        <v>8.1</v>
+      </c>
+      <c r="I22" s="354">
+        <f>AVERAGE(F22:H22)</f>
+        <v>7.2666666666666657</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="352" t="s">
+        <v>402</v>
+      </c>
+      <c r="B23" s="353">
+        <v>112</v>
+      </c>
+      <c r="C23" s="353">
+        <v>24.2</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="E23">
+        <v>80</v>
+      </c>
+      <c r="F23">
+        <v>5.5</v>
+      </c>
+      <c r="G23">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="H23">
+        <v>9</v>
+      </c>
+      <c r="I23" s="354">
+        <f>AVERAGE(F23:H23)</f>
+        <v>8.0666666666666664</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="352" t="s">
+        <v>404</v>
+      </c>
+      <c r="B24" s="353">
+        <v>100</v>
+      </c>
+      <c r="C24" s="353">
+        <v>24.8</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E24">
+        <v>5</v>
+      </c>
+      <c r="F24">
+        <v>8.4</v>
+      </c>
+      <c r="G24">
+        <v>5.9</v>
+      </c>
+      <c r="H24">
+        <v>10.5</v>
+      </c>
+      <c r="I24" s="354">
+        <f>AVERAGE(F24:H24)</f>
+        <v>8.2666666666666675</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="352" t="s">
+        <v>406</v>
+      </c>
+      <c r="B25" s="353">
+        <v>1</v>
+      </c>
+      <c r="C25" s="353">
+        <v>26.1</v>
+      </c>
+      <c r="D25" s="355" t="s">
+        <v>388</v>
+      </c>
+      <c r="E25" s="353">
+        <v>97</v>
+      </c>
+      <c r="F25" s="353">
+        <v>5.9</v>
+      </c>
+      <c r="G25" s="353">
+        <v>10.5</v>
+      </c>
+      <c r="H25" s="353">
+        <v>9.6</v>
+      </c>
+      <c r="I25" s="354">
+        <f>AVERAGE(F25:H25)</f>
+        <v>8.6666666666666661</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="352" t="s">
+        <v>407</v>
+      </c>
+      <c r="B26" s="353">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>26.1</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="E26">
+        <v>72</v>
+      </c>
+      <c r="F26">
+        <v>5.9</v>
+      </c>
+      <c r="G26">
+        <v>10.5</v>
+      </c>
+      <c r="H26">
+        <v>9.6</v>
+      </c>
+      <c r="I26" s="354">
+        <f>AVERAGE(F26:H26)</f>
+        <v>8.6666666666666661</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="356" t="s">
+        <v>408</v>
+      </c>
+      <c r="B27" s="357">
+        <v>1</v>
+      </c>
+      <c r="C27" s="358">
+        <v>26.1</v>
+      </c>
+      <c r="D27" s="359" t="s">
+        <v>388</v>
+      </c>
+      <c r="E27" s="358">
+        <v>15</v>
+      </c>
+      <c r="F27" s="358">
+        <v>5.9</v>
+      </c>
+      <c r="G27" s="358">
+        <v>10.5</v>
+      </c>
+      <c r="H27" s="358">
+        <v>9.6</v>
+      </c>
+      <c r="I27" s="360">
+        <f>AVERAGE(F27:H27)</f>
+        <v>8.6666666666666661</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BF02C3-B992-44C7-A79C-D1E41573911A}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16467,34 +17538,34 @@
   <sheetData>
     <row r="1" spans="1:11" s="35" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="148" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="148" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="36" t="s">
+        <v>247</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="36" t="s">
-        <v>248</v>
-      </c>
-      <c r="E1" s="36" t="s">
+      <c r="G1" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>48</v>
-      </c>
       <c r="I1" s="107" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J1" s="107" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K1" s="108" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="32" x14ac:dyDescent="0.2">
@@ -16502,19 +17573,19 @@
         <v>45413</v>
       </c>
       <c r="B2" s="149" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C2" s="56" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D2" s="55">
         <v>0.3</v>
       </c>
       <c r="E2" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F2" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G2" s="57"/>
       <c r="I2" s="38"/>
@@ -16526,19 +17597,19 @@
         <v>45604</v>
       </c>
       <c r="B3" s="149" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C3" s="56" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D3" s="55">
         <v>4</v>
       </c>
       <c r="E3" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F3" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G3" s="57"/>
       <c r="I3" s="38"/>
@@ -16550,19 +17621,19 @@
         <v>45611</v>
       </c>
       <c r="B4" s="149" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D4" s="55">
         <v>0.3</v>
       </c>
       <c r="E4" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F4" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G4" s="57"/>
       <c r="I4" s="38"/>
@@ -16574,19 +17645,19 @@
         <v>45622</v>
       </c>
       <c r="B5" s="149" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D5" s="55">
         <v>4</v>
       </c>
       <c r="E5" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F5" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G5" s="57"/>
       <c r="I5" s="38"/>
@@ -16598,19 +17669,19 @@
         <v>45666</v>
       </c>
       <c r="B6" s="149" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C6" s="56" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D6" s="55">
         <v>3</v>
       </c>
       <c r="E6" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F6" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G6" s="57"/>
       <c r="I6" s="38"/>
@@ -16622,19 +17693,19 @@
         <v>45670</v>
       </c>
       <c r="B7" s="149" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C7" s="38" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D7" s="55">
         <v>0.5</v>
       </c>
       <c r="E7" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F7" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G7" s="57"/>
       <c r="I7" s="38"/>
@@ -16646,19 +17717,19 @@
         <v>45671</v>
       </c>
       <c r="B8" s="149" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C8" s="56" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D8" s="55">
         <v>0.5</v>
       </c>
       <c r="E8" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F8" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G8" s="57"/>
       <c r="I8" s="38"/>
@@ -16670,19 +17741,19 @@
         <v>45681</v>
       </c>
       <c r="B9" s="149" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C9" s="56" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D9" s="55">
         <v>0.25</v>
       </c>
       <c r="E9" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F9" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G9" s="57"/>
       <c r="I9" s="38"/>
@@ -16694,19 +17765,19 @@
         <v>45681</v>
       </c>
       <c r="B10" s="149" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D10" s="55">
         <v>1</v>
       </c>
       <c r="E10" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F10" s="38" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G10" s="57">
         <v>45678</v>
@@ -16715,14 +17786,28 @@
       <c r="J10" s="41"/>
       <c r="K10" s="40"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="57"/>
-      <c r="B11" s="149"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="57"/>
+    <row r="11" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="57">
+        <v>45762</v>
+      </c>
+      <c r="B11" s="149" t="s">
+        <v>416</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>417</v>
+      </c>
+      <c r="D11" s="55">
+        <v>12</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>418</v>
+      </c>
+      <c r="F11" s="55" t="s">
+        <v>419</v>
+      </c>
+      <c r="G11" s="57">
+        <v>45702</v>
+      </c>
       <c r="I11" s="38"/>
       <c r="J11" s="41"/>
       <c r="K11" s="40"/>
@@ -17057,13 +18142,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="313" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B3" s="313"/>
       <c r="C3" s="313"/>
@@ -17076,30 +18161,30 @@
       <c r="J3" s="84"/>
       <c r="K3" s="84"/>
       <c r="N3" s="137" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="127" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="314" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D4" s="315"/>
       <c r="E4" s="315"/>
       <c r="F4" s="315"/>
       <c r="G4" s="316"/>
       <c r="N4" s="141" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="90" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B5" s="114"/>
       <c r="C5" s="317"/>
@@ -17111,7 +18196,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="90" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B6" s="114"/>
       <c r="C6" s="317"/>
@@ -17123,7 +18208,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="90" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B7" s="114"/>
       <c r="C7" s="317"/>
@@ -17135,7 +18220,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="114" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B8" s="90"/>
       <c r="C8" s="312"/>
@@ -17159,7 +18244,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="90" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B10" s="90"/>
       <c r="C10" s="312"/>
@@ -17177,27 +18262,27 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" s="319" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C12" s="320"/>
       <c r="D12" s="321"/>
       <c r="N12" s="141" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B13" s="322" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C13" s="323"/>
       <c r="D13" s="324"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B14" s="306" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C14" s="307"/>
       <c r="D14" s="308"/>
@@ -17216,33 +18301,33 @@
     </row>
     <row r="17" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B17" s="226" t="s">
+        <v>206</v>
+      </c>
+      <c r="C17" s="226" t="s">
         <v>207</v>
       </c>
-      <c r="C17" s="226" t="s">
-        <v>208</v>
-      </c>
       <c r="N17" s="141" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B18" s="225">
         <v>6</v>
       </c>
       <c r="D18" s="16"/>
       <c r="N18" s="141" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B19" s="217">
         <v>1063.29</v>
@@ -17252,13 +18337,13 @@
         <v>8.6522179999999995</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="F19" s="254" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N19" s="141" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
@@ -17273,12 +18358,12 @@
       </c>
       <c r="D20" s="10"/>
       <c r="N20" s="141" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C21" s="12">
         <f>C19-C20</f>
@@ -17288,28 +18373,28 @@
       <c r="E21" s="28"/>
       <c r="F21" s="116"/>
       <c r="N21" s="141" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C22" s="185">
         <v>3.5339999999999998</v>
       </c>
       <c r="D22" s="111" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
       <c r="N22" s="141" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C23" s="12">
         <f>C21-C22</f>
@@ -17318,12 +18403,12 @@
       <c r="D23" s="111"/>
       <c r="E23" s="28"/>
       <c r="N23" s="141" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B24" s="94">
         <f>TribalWater!H7</f>
@@ -17333,12 +18418,12 @@
       <c r="D24" s="111"/>
       <c r="E24" s="28"/>
       <c r="N24" s="141" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B25" s="235">
         <f>1-B24</f>
@@ -17348,7 +18433,7 @@
       <c r="D25" s="111"/>
       <c r="E25" s="28"/>
       <c r="N25" s="141" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -17357,7 +18442,7 @@
     </row>
     <row r="27" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="102" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B27" s="103" t="s">
         <v>22</v>
@@ -17393,7 +18478,7 @@
         <v>15</v>
       </c>
       <c r="M27" s="103" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N27" s="138" t="str">
         <f>N3</f>
@@ -17402,7 +18487,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="125" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="97"/>
@@ -17416,12 +18501,12 @@
       <c r="K28" s="97"/>
       <c r="L28" s="97"/>
       <c r="N28" s="141" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="29" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="96" t="str">
@@ -17465,12 +18550,12 @@
         <v/>
       </c>
       <c r="N29" s="141" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="96" t="str">
@@ -17514,12 +18599,12 @@
         <v/>
       </c>
       <c r="N30" s="141" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="96" t="str">
@@ -17563,12 +18648,12 @@
         <v/>
       </c>
       <c r="N31" s="141" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B32" s="1"/>
       <c r="H32" s="96"/>
@@ -17580,7 +18665,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="12" t="str">
@@ -17612,7 +18697,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="218" t="str">
@@ -17644,7 +18729,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="125" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C35"/>
       <c r="H35" s="12" t="str">
@@ -17668,7 +18753,7 @@
         <v/>
       </c>
       <c r="N35" s="141" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
@@ -17978,16 +19063,16 @@
     </row>
     <row r="42" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C42"/>
       <c r="N42" s="141" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="43" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C43" s="12" t="str">
         <f>IF(C$28&lt;&gt;"",IF(COLUMN(C27)=COLUMN($C27),$B$19,#REF!),"")</f>
@@ -18033,7 +19118,7 @@
     </row>
     <row r="44" spans="1:14" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H44" s="12" t="str">
         <f>IF(H$28&lt;&gt;"",IF(COLUMN(H28)=COLUMN($C28),$C$19,#REF!),"")</f>
@@ -18059,7 +19144,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B45" s="186"/>
       <c r="C45" s="12" t="str">
@@ -18103,7 +19188,7 @@
         <v/>
       </c>
       <c r="N45" s="141" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
@@ -18395,7 +19480,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A52" s="125" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B52" s="214"/>
       <c r="C52" s="215" t="str">
@@ -18440,7 +19525,7 @@
       </c>
       <c r="M52" s="116"/>
       <c r="N52" s="141" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
@@ -18449,7 +19534,7 @@
         <v xml:space="preserve">    To Reclamation - Protect Zone</v>
       </c>
       <c r="B53" s="187" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C53" s="82" t="str">
         <f>IF(OR(C$28="",$A55=""),"",C46)</f>
@@ -18499,7 +19584,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C54" s="82" t="str">
         <f>IF(OR(C$28="",$A56=""),"",C52-C53)</f>
@@ -18554,7 +19639,7 @@
         <v xml:space="preserve">       To California</v>
       </c>
       <c r="B55" s="95" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C55" s="82" t="str">
         <f>IF(OR(C$28="",$A55=""),"",(VLOOKUP(C$54,DivideInflow!$K$19:$W$25,9)-IF($A$59&lt;&gt;"",$B$59*$B$24,0))*(C$54))</f>
@@ -18594,7 +19679,7 @@
         <v xml:space="preserve">       To Arizona</v>
       </c>
       <c r="B56" s="95" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C56" s="82" t="str">
         <f>IF(OR(C$28="",$A56=""),"",(VLOOKUP(C$54,DivideInflow!$K$19:$W$25,7)-IF($A$59&lt;&gt;"",$B$59*$B$25,0))*(C$54))</f>
@@ -18811,7 +19896,7 @@
         <v xml:space="preserve">    To Havasu / Parker evaporation and ET</v>
       </c>
       <c r="B60" s="151" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C60" s="153" t="str">
         <f>IF(OR(C$28="",$A60=""),"",MIN(C31,C52-C59))</f>
@@ -18870,7 +19955,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="101" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B62" s="98"/>
       <c r="C62" s="98"/>
@@ -18906,10 +19991,10 @@
       <c r="K63" s="99"/>
       <c r="L63" s="99"/>
       <c r="M63" s="100" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N63" s="139" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
@@ -18932,7 +20017,7 @@
         <v>0</v>
       </c>
       <c r="N64" s="144" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.2">
@@ -18955,7 +20040,7 @@
         <v>0</v>
       </c>
       <c r="N65" s="145" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.2">
@@ -19008,7 +20093,7 @@
         <v/>
       </c>
       <c r="N66" s="141" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.2">
@@ -19057,7 +20142,7 @@
         <v/>
       </c>
       <c r="N67" s="141" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.2">
@@ -19076,7 +20161,7 @@
       <c r="K68" s="93"/>
       <c r="L68" s="93"/>
       <c r="N68" s="141" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.2">
@@ -19125,7 +20210,7 @@
         <v/>
       </c>
       <c r="N69" s="141" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.2">
@@ -19149,10 +20234,10 @@
       <c r="K71" s="99"/>
       <c r="L71" s="99"/>
       <c r="M71" s="100" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N71" s="139" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.2">
@@ -19175,7 +20260,7 @@
         <v>0</v>
       </c>
       <c r="N72" s="144" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.2">
@@ -19198,7 +20283,7 @@
         <v>0</v>
       </c>
       <c r="N73" s="145" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.2">
@@ -19251,7 +20336,7 @@
         <v/>
       </c>
       <c r="N74" s="141" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.2">
@@ -19300,7 +20385,7 @@
         <v/>
       </c>
       <c r="N75" s="141" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.2">
@@ -19319,7 +20404,7 @@
       <c r="K76" s="93"/>
       <c r="L76" s="93"/>
       <c r="N76" s="141" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.2">
@@ -19368,7 +20453,7 @@
         <v/>
       </c>
       <c r="N77" s="141" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.2">
@@ -19392,10 +20477,10 @@
       <c r="K79" s="99"/>
       <c r="L79" s="99"/>
       <c r="M79" s="100" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N79" s="139" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.2">
@@ -19418,7 +20503,7 @@
         <v>0</v>
       </c>
       <c r="N80" s="144" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.2">
@@ -19441,7 +20526,7 @@
         <v>0</v>
       </c>
       <c r="N81" s="145" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.2">
@@ -19494,7 +20579,7 @@
         <v/>
       </c>
       <c r="N82" s="141" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.2">
@@ -19543,7 +20628,7 @@
         <v/>
       </c>
       <c r="N83" s="141" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.2">
@@ -19562,7 +20647,7 @@
       <c r="K84" s="93"/>
       <c r="L84" s="93"/>
       <c r="N84" s="141" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.2">
@@ -19611,7 +20696,7 @@
         <v/>
       </c>
       <c r="N85" s="141" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
@@ -19635,10 +20720,10 @@
       <c r="K87" s="99"/>
       <c r="L87" s="99"/>
       <c r="M87" s="100" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N87" s="139" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.2">
@@ -19661,7 +20746,7 @@
         <v>0</v>
       </c>
       <c r="N88" s="144" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.2">
@@ -19684,7 +20769,7 @@
         <v>0</v>
       </c>
       <c r="N89" s="145" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.2">
@@ -19737,7 +20822,7 @@
         <v/>
       </c>
       <c r="N90" s="141" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.2">
@@ -19786,7 +20871,7 @@
         <v/>
       </c>
       <c r="N91" s="141" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
@@ -19805,7 +20890,7 @@
       <c r="K92" s="118"/>
       <c r="L92" s="118"/>
       <c r="N92" s="141" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
@@ -19854,7 +20939,7 @@
         <v/>
       </c>
       <c r="N93" s="141" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.2">
@@ -19878,10 +20963,10 @@
       <c r="K95" s="99"/>
       <c r="L95" s="99"/>
       <c r="M95" s="100" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N95" s="139" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.2">
@@ -19904,7 +20989,7 @@
         <v>0</v>
       </c>
       <c r="N96" s="144" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
@@ -19927,7 +21012,7 @@
         <v>0</v>
       </c>
       <c r="N97" s="145" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
@@ -19980,7 +21065,7 @@
         <v/>
       </c>
       <c r="N98" s="141" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
@@ -20029,7 +21114,7 @@
         <v/>
       </c>
       <c r="N99" s="141" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
@@ -20048,7 +21133,7 @@
       <c r="K100" s="93"/>
       <c r="L100" s="93"/>
       <c r="N100" s="141" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
@@ -20097,7 +21182,7 @@
         <v/>
       </c>
       <c r="N101" s="141" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
@@ -20121,10 +21206,10 @@
       <c r="K103" s="99"/>
       <c r="L103" s="99"/>
       <c r="M103" s="100" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N103" s="139" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
@@ -20147,7 +21232,7 @@
         <v>0</v>
       </c>
       <c r="N104" s="144" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
@@ -20170,7 +21255,7 @@
         <v>0</v>
       </c>
       <c r="N105" s="145" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
@@ -20223,7 +21308,7 @@
         <v/>
       </c>
       <c r="N106" s="141" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
@@ -20272,7 +21357,7 @@
         <v/>
       </c>
       <c r="N107" s="141" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
@@ -20291,7 +21376,7 @@
       <c r="K108" s="27"/>
       <c r="L108" s="27"/>
       <c r="N108" s="141" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
@@ -20340,7 +21425,7 @@
         <v/>
       </c>
       <c r="N109" s="141" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
@@ -20349,7 +21434,7 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" s="101" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B111" s="101"/>
       <c r="C111" s="101"/>
@@ -20364,16 +21449,16 @@
       <c r="L111" s="101"/>
       <c r="M111" s="101"/>
       <c r="N111" s="141" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C112"/>
       <c r="M112" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N112" s="142"/>
     </row>
@@ -20691,7 +21776,7 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B119" s="1"/>
       <c r="C119" s="12" t="str">
@@ -20739,7 +21824,7 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B120" s="1"/>
       <c r="C120" s="34"/>
@@ -21038,7 +22123,7 @@
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B127" s="1"/>
       <c r="D127" s="2"/>
@@ -21336,7 +22421,7 @@
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H134" s="12" t="str">
         <f t="shared" ref="H134:L134" si="85">IF(H$28&lt;&gt;"",SUM(H128:H133),"")</f>
@@ -21359,12 +22444,12 @@
         <v/>
       </c>
       <c r="N134" s="141" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="135" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B135" s="1"/>
       <c r="C135" s="12" t="str">
@@ -21396,7 +22481,7 @@
     </row>
     <row r="136" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B136" s="1"/>
       <c r="C136" s="219" t="str">
@@ -21428,11 +22513,11 @@
     </row>
     <row r="137" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A137" s="125" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C137" s="18"/>
       <c r="N137" s="141" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="139" spans="1:14" x14ac:dyDescent="0.2">
@@ -21980,7 +23065,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA15763-059F-401A-BB99-8A737E404CC4}">
   <dimension ref="A1:U32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -22007,17 +23092,17 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -22026,20 +23111,20 @@
         <v>13</v>
       </c>
       <c r="J5" s="337" t="s">
+        <v>214</v>
+      </c>
+      <c r="K5" s="337" t="s">
         <v>215</v>
       </c>
-      <c r="K5" s="337" t="s">
+      <c r="L5" s="334" t="s">
         <v>216</v>
-      </c>
-      <c r="L5" s="334" t="s">
-        <v>217</v>
       </c>
       <c r="M5" s="335"/>
       <c r="N5" s="335"/>
       <c r="O5" s="335"/>
       <c r="P5" s="336"/>
       <c r="Q5" s="326" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="R5" s="327"/>
       <c r="S5" s="327"/>
@@ -22048,60 +23133,60 @@
     </row>
     <row r="6" spans="1:21" s="188" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="189" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C6" s="189" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" s="189" t="s">
         <v>205</v>
       </c>
-      <c r="D6" s="189" t="s">
-        <v>206</v>
-      </c>
       <c r="E6" s="189" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F6" s="189" t="s">
         <v>18</v>
       </c>
       <c r="G6" s="189" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I6" s="338"/>
       <c r="J6" s="338"/>
       <c r="K6" s="338"/>
       <c r="L6" s="190" t="s">
+        <v>219</v>
+      </c>
+      <c r="M6" s="190" t="s">
         <v>220</v>
       </c>
-      <c r="M6" s="190" t="s">
+      <c r="N6" s="190" t="s">
         <v>221</v>
       </c>
-      <c r="N6" s="190" t="s">
+      <c r="O6" s="190" t="s">
         <v>222</v>
       </c>
-      <c r="O6" s="190" t="s">
+      <c r="P6" s="190" t="s">
         <v>223</v>
       </c>
-      <c r="P6" s="190" t="s">
+      <c r="Q6" s="191" t="s">
         <v>224</v>
       </c>
-      <c r="Q6" s="191" t="s">
+      <c r="R6" s="191" t="s">
         <v>225</v>
       </c>
-      <c r="R6" s="191" t="s">
+      <c r="S6" s="191" t="s">
         <v>226</v>
       </c>
-      <c r="S6" s="191" t="s">
+      <c r="T6" s="191" t="s">
         <v>227</v>
       </c>
-      <c r="T6" s="191" t="s">
+      <c r="U6" s="191" t="s">
         <v>228</v>
-      </c>
-      <c r="U6" s="191" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:21" s="188" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="334" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C7" s="335"/>
       <c r="D7" s="335"/>
@@ -22109,7 +23194,7 @@
       <c r="F7" s="335"/>
       <c r="G7" s="336"/>
       <c r="I7" s="192" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J7" s="192">
         <f>B13</f>
@@ -22176,7 +23261,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="192" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J8" s="192">
         <f>B14</f>
@@ -22229,7 +23314,7 @@
     </row>
     <row r="9" spans="1:21" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B9" s="198" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C9" s="202">
         <v>0.8</v>
@@ -22248,7 +23333,7 @@
         <v>1</v>
       </c>
       <c r="I9" s="192" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J9" s="192">
         <f>B15</f>
@@ -22301,7 +23386,7 @@
     </row>
     <row r="10" spans="1:21" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B10" s="198" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C10" s="202">
         <v>0.43330000000000002</v>
@@ -22320,7 +23405,7 @@
         <v>1</v>
       </c>
       <c r="I10" s="192" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J10" s="192">
         <f>B16</f>
@@ -22373,17 +23458,17 @@
     </row>
     <row r="11" spans="1:21" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B11" s="198" t="s">
+        <v>236</v>
+      </c>
+      <c r="C11" s="325" t="s">
         <v>237</v>
-      </c>
-      <c r="C11" s="325" t="s">
-        <v>238</v>
       </c>
       <c r="D11" s="325"/>
       <c r="E11" s="325"/>
       <c r="F11" s="325"/>
       <c r="G11" s="325"/>
       <c r="I11" s="192" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J11" s="192">
         <f>B17</f>
@@ -22436,7 +23521,7 @@
     </row>
     <row r="12" spans="1:21" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B12" s="329" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C12" s="330"/>
       <c r="D12" s="330"/>
@@ -22444,23 +23529,23 @@
       <c r="F12" s="330"/>
       <c r="G12" s="330"/>
       <c r="I12" s="192" t="s">
+        <v>240</v>
+      </c>
+      <c r="J12" s="192" t="s">
+        <v>236</v>
+      </c>
+      <c r="K12" s="200" t="s">
         <v>241</v>
       </c>
-      <c r="J12" s="192" t="s">
+      <c r="L12" s="331" t="s">
         <v>237</v>
-      </c>
-      <c r="K12" s="200" t="s">
-        <v>242</v>
-      </c>
-      <c r="L12" s="331" t="s">
-        <v>238</v>
       </c>
       <c r="M12" s="332"/>
       <c r="N12" s="332"/>
       <c r="O12" s="332"/>
       <c r="P12" s="333"/>
       <c r="Q12" s="331" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="R12" s="332"/>
       <c r="S12" s="332"/>
@@ -22488,7 +23573,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="192" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J13" s="192">
         <v>2.7</v>
@@ -22563,7 +23648,7 @@
         <v>0.3</v>
       </c>
       <c r="I14" s="192" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J14" s="192">
         <v>8</v>
@@ -22638,7 +23723,7 @@
         <v>0.4</v>
       </c>
       <c r="I15" s="204" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J15" s="205"/>
       <c r="K15" s="206"/>
@@ -22678,7 +23763,7 @@
         <v>0.99999999999999989</v>
       </c>
       <c r="I16" s="205" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J16" s="205"/>
       <c r="U16" s="210"/>
@@ -22708,16 +23793,16 @@
         <v>1.5</v>
       </c>
       <c r="I17" s="205" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U17" s="210"/>
     </row>
     <row r="18" spans="2:21" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="198" t="s">
+        <v>236</v>
+      </c>
+      <c r="C18" s="325" t="s">
         <v>237</v>
-      </c>
-      <c r="C18" s="325" t="s">
-        <v>238</v>
       </c>
       <c r="D18" s="325"/>
       <c r="E18" s="325"/>
@@ -22726,7 +23811,7 @@
     </row>
     <row r="19" spans="2:21" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="I19" s="197" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J19" s="206">
         <f t="shared" ref="J19:U19" si="9">J14</f>
@@ -23144,7 +24229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876BA06C-E963-43DD-B933-307F043834EF}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A18" sqref="A18:C23"/>
     </sheetView>
   </sheetViews>
@@ -23159,50 +24244,50 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="236" t="s">
+        <v>322</v>
+      </c>
+      <c r="B4" s="236" t="s">
+        <v>323</v>
+      </c>
+      <c r="C4" s="237" t="s">
         <v>324</v>
       </c>
-      <c r="B4" s="236" t="s">
+      <c r="D4" s="237" t="s">
         <v>325</v>
       </c>
-      <c r="C4" s="237" t="s">
-        <v>326</v>
-      </c>
-      <c r="D4" s="237" t="s">
-        <v>327</v>
-      </c>
       <c r="F4" s="237" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G4" s="237" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="H4" s="237" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C5" s="24">
         <v>12534</v>
       </c>
       <c r="D5" s="24"/>
       <c r="F5" s="22" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G5" s="31">
         <f>SUMIFS($C$5:$C$13,$B$5:$B$13,F5)</f>
@@ -23215,17 +24300,17 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C6" s="24">
         <v>103535</v>
       </c>
       <c r="D6" s="24"/>
       <c r="F6" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G6" s="31">
         <f t="shared" ref="G6:G7" si="0">SUMIFS($C$5:$C$13,$B$5:$B$13,F6)</f>
@@ -23238,17 +24323,17 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C7" s="24">
         <v>16720</v>
       </c>
       <c r="D7" s="24"/>
       <c r="F7" s="22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G7" s="31">
         <f t="shared" si="0"/>
@@ -23261,17 +24346,17 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C8" s="24">
         <v>11340</v>
       </c>
       <c r="D8" s="24"/>
       <c r="F8" s="243" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G8" s="241">
         <f>SUM(G5:G7)</f>
@@ -23284,10 +24369,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C9" s="24">
         <v>662402</v>
@@ -23296,10 +24381,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C10" s="24">
         <v>56846</v>
@@ -23308,10 +24393,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C11" s="24">
         <v>6350</v>
@@ -23320,10 +24405,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C12" s="24">
         <v>71616</v>
@@ -23332,10 +24417,10 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C13" s="24">
         <v>10847</v>
@@ -23346,7 +24431,7 @@
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="238" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="238"/>
       <c r="C14" s="239">
@@ -23360,23 +24445,23 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="236" t="s">
+        <v>335</v>
+      </c>
+      <c r="B18" s="244" t="s">
+        <v>336</v>
+      </c>
+      <c r="C18" s="244" t="s">
         <v>337</v>
-      </c>
-      <c r="B18" s="244" t="s">
-        <v>338</v>
-      </c>
-      <c r="C18" s="244" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B19" s="24">
         <v>769208</v>
@@ -23387,7 +24472,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B20" s="24">
         <v>15340</v>
@@ -23398,7 +24483,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="23" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B21" s="24">
         <v>2844</v>
@@ -23409,7 +24494,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B22" s="24">
         <v>13000</v>
@@ -23420,7 +24505,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="238" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="239">
         <f>SUM(B19:B22)</f>
@@ -23483,13 +24568,13 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="313" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" s="313"/>
       <c r="C3" s="313"/>
@@ -23502,12 +24587,12 @@
       <c r="J3" s="84"/>
       <c r="K3" s="84"/>
       <c r="N3" s="137" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="127" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="127" t="s">
         <v>19</v>
@@ -23520,7 +24605,7 @@
       <c r="F4" s="315"/>
       <c r="G4" s="316"/>
       <c r="N4" s="139" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -23561,7 +24646,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="114" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" s="90"/>
       <c r="C8" s="312"/>
@@ -23573,7 +24658,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="114" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B9" s="90"/>
       <c r="C9" s="318"/>
@@ -23585,7 +24670,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="115" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="115"/>
       <c r="C10" s="339"/>
@@ -23603,20 +24688,20 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" s="319" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C12" s="320"/>
       <c r="D12" s="321"/>
       <c r="N12" s="141" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B13" s="322" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C13" s="323"/>
       <c r="D13" s="324"/>
@@ -23624,7 +24709,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B14" s="306" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C14" s="307"/>
       <c r="D14" s="308"/>
@@ -23643,21 +24728,21 @@
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>29</v>
-      </c>
       <c r="N17" s="141" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="110">
         <v>5.73</v>
@@ -23667,12 +24752,12 @@
       </c>
       <c r="D18" s="16"/>
       <c r="N18" s="141" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B19" s="110">
         <v>7.2</v>
@@ -23681,16 +24766,16 @@
         <v>9</v>
       </c>
       <c r="D19" s="129" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F19" s="129"/>
       <c r="N19" s="141" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="159">
         <v>3525</v>
@@ -23700,12 +24785,12 @@
       </c>
       <c r="D20" s="10"/>
       <c r="N20" s="141" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="110" t="e">
         <f>VLOOKUP(B20,#REF!,2)/1000000</f>
@@ -23718,12 +24803,12 @@
       <c r="D21" s="10"/>
       <c r="E21" s="28"/>
       <c r="N21" s="141" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B22" s="110">
         <f>78.1</f>
@@ -23733,12 +24818,12 @@
       <c r="D22" s="111"/>
       <c r="E22" s="28"/>
       <c r="N22" s="141" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B23" s="130">
         <v>0.17</v>
@@ -23747,12 +24832,12 @@
       <c r="D23" s="111"/>
       <c r="E23" s="28"/>
       <c r="N23" s="141" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B24" s="110">
         <f>10*(7.5+1.5/2)-B22-B23</f>
@@ -23762,12 +24847,12 @@
       <c r="D24" s="111"/>
       <c r="E24" s="28"/>
       <c r="N24" s="141" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B25" s="110">
         <f>2.3 - IF(A9&lt;&gt;"",1.06,0)</f>
@@ -23777,7 +24862,7 @@
       <c r="D25" s="111"/>
       <c r="E25" s="28"/>
       <c r="N25" s="141" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.2">
@@ -23786,7 +24871,7 @@
     </row>
     <row r="27" spans="1:14" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="102" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B27" s="103" t="s">
         <v>22</v>
@@ -23822,7 +24907,7 @@
         <v>15</v>
       </c>
       <c r="M27" s="103" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N27" s="138" t="str">
         <f>N3</f>
@@ -23831,7 +24916,7 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="125" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="97">
@@ -23865,12 +24950,12 @@
         <v>16</v>
       </c>
       <c r="N28" s="139" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="96">
@@ -23912,12 +24997,12 @@
         <v>0.8</v>
       </c>
       <c r="N29" s="141" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="96">
@@ -23959,12 +25044,12 @@
         <v>0.2</v>
       </c>
       <c r="N30" s="141" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="96">
@@ -24008,21 +25093,21 @@
         <v>0.6</v>
       </c>
       <c r="N31" s="141" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C32"/>
       <c r="N32" s="141" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33" s="12">
         <f>IF(C$28&lt;&gt;"",IF(COLUMN(C27)=COLUMN($C27),$B$19,#REF!),"")</f>
@@ -24068,7 +25153,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" s="12">
         <f>IF(C$28&lt;&gt;"",IF(COLUMN(C28)=COLUMN($C28),$C$19,#REF!),"")</f>
@@ -24114,7 +25199,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B35" s="49"/>
       <c r="C35" s="12" t="e">
@@ -24161,7 +25246,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="12" t="e">
@@ -24205,7 +25290,7 @@
         <v>#REF!</v>
       </c>
       <c r="N36" s="141" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
@@ -24258,7 +25343,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B38" s="50"/>
       <c r="C38" s="30">
@@ -24305,12 +25390,12 @@
         <v>16</v>
       </c>
       <c r="N38" s="141" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" s="125" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="12">
@@ -24358,7 +25443,7 @@
         <v/>
       </c>
       <c r="N39" s="140" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
@@ -24367,7 +25452,7 @@
         <v xml:space="preserve">    To Upper Basin</v>
       </c>
       <c r="B40" s="94" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C40" s="81" t="e">
         <f>IF(OR(C$28="",$A41=""),"",MAX(0,C39-SUM(C41:C46)))</f>
@@ -24478,7 +25563,7 @@
         <v xml:space="preserve">    To Mexico</v>
       </c>
       <c r="B42" s="95" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C42" s="82" t="e">
         <f>IF(OR(C$28="",$A42=""),"",MIN(C38,C$39-SUM(C43:C46)))</f>
@@ -24642,7 +25727,7 @@
         <v xml:space="preserve">    To Shared, Reserve</v>
       </c>
       <c r="B45" s="95" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C45" s="180" t="e">
         <f>IF(OR(C$28="",$A45=""),"",IF(C$39&gt;C37,C37,C39))</f>
@@ -24696,7 +25781,7 @@
         <v xml:space="preserve">    To Havasu / Parker evaporation and ET</v>
       </c>
       <c r="B46" s="151" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C46" s="181" t="e">
         <f>IF(OR(C$28="",$A46=""),"",MIN(C31,C39-C45))</f>
@@ -24755,7 +25840,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C48" s="179" t="e">
         <f>SUM(C40:C46)</f>
@@ -24810,7 +25895,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B53">
         <v>8.1999999999999993</v>
@@ -24818,7 +25903,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B54">
         <v>1.2</v>
@@ -24826,7 +25911,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B55">
         <v>0.95</v>
@@ -24834,7 +25919,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B56">
         <f>1.5/2</f>
@@ -24843,7 +25928,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B57">
         <f>B53-SUM(B54:B56)</f>
@@ -24921,21 +26006,21 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D3" s="341" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="341"/>
       <c r="F3" s="341" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" s="341"/>
       <c r="H3" s="341"/>
       <c r="I3" s="341" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J3" s="341"/>
       <c r="K3" s="341"/>
@@ -24948,52 +26033,52 @@
     </row>
     <row r="4" spans="1:16" s="47" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="C4" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="46" t="s">
+        <v>63</v>
+      </c>
+      <c r="J4" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="46" t="s">
+        <v>65</v>
+      </c>
+      <c r="L4" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="M4" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="N4" s="46" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="P4" s="46" t="s">
         <v>35</v>
-      </c>
-      <c r="C4" s="46" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="G4" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="H4" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="I4" s="46" t="s">
-        <v>64</v>
-      </c>
-      <c r="J4" s="46" t="s">
-        <v>65</v>
-      </c>
-      <c r="K4" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="L4" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="M4" s="46" t="s">
-        <v>68</v>
-      </c>
-      <c r="N4" s="46" t="s">
-        <v>69</v>
-      </c>
-      <c r="O4" s="46" t="s">
-        <v>67</v>
-      </c>
-      <c r="P4" s="46" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
@@ -25517,7 +26602,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
@@ -26021,40 +27106,40 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="I3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="53" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D4" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="B4" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>81</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>76</v>
-      </c>
       <c r="E4" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="F4" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="F4" s="36" t="s">
-        <v>92</v>
-      </c>
       <c r="G4" s="120" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:9" s="53" customFormat="1" ht="48" x14ac:dyDescent="0.2">
@@ -26063,20 +27148,20 @@
         <v>#REF!</v>
       </c>
       <c r="B5" s="80" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" s="65" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="66" t="str">
         <f>D7</f>
         <v>Highest uncertainty for native fish. Also represent a substantial risk to the tailwater trout fishery, as sustained temperatures of 19oC or higher are unsuitable for trout.</v>
       </c>
       <c r="E5" s="86" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" s="86" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G5" s="121" t="e">
         <f>VLOOKUP(A5,#REF!,2)/1000000</f>
@@ -26092,7 +27177,7 @@
         <v>&gt; 18</v>
       </c>
       <c r="C6" s="62" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D6" s="63" t="str">
         <f>D7</f>
@@ -26103,7 +27188,7 @@
         <v>Highly uncertain</v>
       </c>
       <c r="F6" s="86" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G6" s="121" t="e">
         <f>VLOOKUP(A6,#REF!,2)/1000000</f>
@@ -26115,20 +27200,20 @@
         <v>3490</v>
       </c>
       <c r="B7" s="68" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C7" s="68" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" s="69" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="62" t="str">
         <f>E6</f>
         <v>Highly uncertain</v>
       </c>
       <c r="F7" s="86" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G7" s="121" t="e">
         <f>VLOOKUP(A7,#REF!,2)/1000000</f>
@@ -26140,19 +27225,19 @@
         <v>3525</v>
       </c>
       <c r="B8" s="71" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C8" s="71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D8" s="72" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E8" s="87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F8" s="87" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G8" s="122" t="e">
         <f>VLOOKUP(A8,#REF!,2)/1000000</f>
@@ -26164,16 +27249,16 @@
         <v>3600</v>
       </c>
       <c r="B9" s="74" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="74" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D9" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="88" t="s">
         <v>89</v>
-      </c>
-      <c r="E9" s="88" t="s">
-        <v>90</v>
       </c>
       <c r="F9" s="88" t="str">
         <f>F8</f>
@@ -26189,19 +27274,19 @@
         <v>3675</v>
       </c>
       <c r="B10" s="77" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="77" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D10" s="78" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E10" s="89" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F10" s="89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G10" s="124" t="e">
         <f>VLOOKUP(A10,#REF!,2)/1000000</f>
@@ -26217,7 +27302,7 @@
         <v>&lt; 12</v>
       </c>
       <c r="C11" s="77" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11" s="79" t="str">
         <f>D10</f>
@@ -26228,7 +27313,7 @@
         <v>Help grow, reproduce, and survive</v>
       </c>
       <c r="F11" s="89" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G11" s="124" t="e">
         <f>VLOOKUP(A11,#REF!,2)/1000000</f>
@@ -26291,7 +27376,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Anabelle added a table
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anabelle/Documents/ColoradoRiverCollaborate/LakeMeadWaterBankDivideInflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDAF20C-8C14-154C-A42A-3BF949D8442D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077DA555-3B6F-7D45-9308-FE11F390E736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="616" uniqueCount="426">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="428">
   <si>
     <t>Year 1</t>
   </si>
@@ -2148,6 +2148,12 @@
   <si>
     <t>Tribal Nations Included in Lake Mead Inflow Allocation</t>
   </si>
+  <si>
+    <t>Percentage of Inflow</t>
+  </si>
+  <si>
+    <t>Share of Lake Mead Inflow as a Volume</t>
+  </si>
 </sst>
 </file>
 
@@ -2934,7 +2940,7 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="378">
+  <cellXfs count="373">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3626,6 +3632,93 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="19" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="19" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3680,12 +3773,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3718,63 +3805,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3836,6 +3866,21 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3847,6 +3892,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3872,11 +3920,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3899,68 +3947,9 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="19" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="19" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="19" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="15">
     <cellStyle name="20% - Accent1" xfId="12" builtinId="30"/>
@@ -15520,20 +15509,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="268" t="s">
+      <c r="A1" s="297" t="s">
         <v>304</v>
       </c>
-      <c r="B1" s="268"/>
-      <c r="C1" s="268"/>
-      <c r="D1" s="268"/>
-      <c r="E1" s="268"/>
-      <c r="F1" s="268"/>
-      <c r="G1" s="268"/>
-      <c r="H1" s="268"/>
-      <c r="I1" s="268"/>
-      <c r="J1" s="268"/>
-      <c r="K1" s="268"/>
-      <c r="L1" s="268"/>
+      <c r="B1" s="297"/>
+      <c r="C1" s="297"/>
+      <c r="D1" s="297"/>
+      <c r="E1" s="297"/>
+      <c r="F1" s="297"/>
+      <c r="G1" s="297"/>
+      <c r="H1" s="297"/>
+      <c r="I1" s="297"/>
+      <c r="J1" s="297"/>
+      <c r="K1" s="297"/>
+      <c r="L1" s="297"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -15559,41 +15548,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="269" t="s">
+      <c r="A4" s="298" t="s">
         <v>305</v>
       </c>
-      <c r="B4" s="270"/>
-      <c r="C4" s="270"/>
-      <c r="D4" s="270"/>
-      <c r="E4" s="270"/>
-      <c r="F4" s="270"/>
-      <c r="G4" s="270"/>
-      <c r="H4" s="270"/>
-      <c r="I4" s="270"/>
-      <c r="J4" s="270"/>
-      <c r="K4" s="270"/>
-      <c r="L4" s="271"/>
-      <c r="N4" s="272"/>
-      <c r="O4" s="272"/>
-      <c r="P4" s="272"/>
-      <c r="Q4" s="272"/>
-      <c r="R4" s="272"/>
+      <c r="B4" s="299"/>
+      <c r="C4" s="299"/>
+      <c r="D4" s="299"/>
+      <c r="E4" s="299"/>
+      <c r="F4" s="299"/>
+      <c r="G4" s="299"/>
+      <c r="H4" s="299"/>
+      <c r="I4" s="299"/>
+      <c r="J4" s="299"/>
+      <c r="K4" s="299"/>
+      <c r="L4" s="300"/>
+      <c r="N4" s="301"/>
+      <c r="O4" s="301"/>
+      <c r="P4" s="301"/>
+      <c r="Q4" s="301"/>
+      <c r="R4" s="301"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="273" t="s">
+      <c r="A5" s="302" t="s">
         <v>288</v>
       </c>
-      <c r="B5" s="274"/>
-      <c r="C5" s="274"/>
-      <c r="D5" s="274"/>
-      <c r="E5" s="274"/>
-      <c r="F5" s="274"/>
-      <c r="G5" s="274"/>
-      <c r="H5" s="274"/>
-      <c r="I5" s="274"/>
-      <c r="J5" s="274"/>
-      <c r="K5" s="274"/>
-      <c r="L5" s="275"/>
+      <c r="B5" s="303"/>
+      <c r="C5" s="303"/>
+      <c r="D5" s="303"/>
+      <c r="E5" s="303"/>
+      <c r="F5" s="303"/>
+      <c r="G5" s="303"/>
+      <c r="H5" s="303"/>
+      <c r="I5" s="303"/>
+      <c r="J5" s="303"/>
+      <c r="K5" s="303"/>
+      <c r="L5" s="304"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15601,20 +15590,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="273" t="s">
+      <c r="A6" s="302" t="s">
         <v>306</v>
       </c>
-      <c r="B6" s="274"/>
-      <c r="C6" s="274"/>
-      <c r="D6" s="274"/>
-      <c r="E6" s="274"/>
-      <c r="F6" s="274"/>
-      <c r="G6" s="274"/>
-      <c r="H6" s="274"/>
-      <c r="I6" s="274"/>
-      <c r="J6" s="274"/>
-      <c r="K6" s="274"/>
-      <c r="L6" s="275"/>
+      <c r="B6" s="303"/>
+      <c r="C6" s="303"/>
+      <c r="D6" s="303"/>
+      <c r="E6" s="303"/>
+      <c r="F6" s="303"/>
+      <c r="G6" s="303"/>
+      <c r="H6" s="303"/>
+      <c r="I6" s="303"/>
+      <c r="J6" s="303"/>
+      <c r="K6" s="303"/>
+      <c r="L6" s="304"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15623,19 +15612,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="228"/>
-      <c r="B7" s="274" t="s">
+      <c r="B7" s="303" t="s">
         <v>307</v>
       </c>
-      <c r="C7" s="274"/>
-      <c r="D7" s="274"/>
-      <c r="E7" s="274"/>
-      <c r="F7" s="274"/>
-      <c r="G7" s="274"/>
-      <c r="H7" s="274"/>
-      <c r="I7" s="274"/>
-      <c r="J7" s="274"/>
-      <c r="K7" s="274"/>
-      <c r="L7" s="275"/>
+      <c r="C7" s="303"/>
+      <c r="D7" s="303"/>
+      <c r="E7" s="303"/>
+      <c r="F7" s="303"/>
+      <c r="G7" s="303"/>
+      <c r="H7" s="303"/>
+      <c r="I7" s="303"/>
+      <c r="J7" s="303"/>
+      <c r="K7" s="303"/>
+      <c r="L7" s="304"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15644,19 +15633,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="229"/>
-      <c r="B8" s="291" t="s">
+      <c r="B8" s="318" t="s">
         <v>308</v>
       </c>
-      <c r="C8" s="291"/>
-      <c r="D8" s="291"/>
-      <c r="E8" s="291"/>
-      <c r="F8" s="291"/>
-      <c r="G8" s="291"/>
-      <c r="H8" s="291"/>
-      <c r="I8" s="291"/>
-      <c r="J8" s="291"/>
-      <c r="K8" s="291"/>
-      <c r="L8" s="292"/>
+      <c r="C8" s="318"/>
+      <c r="D8" s="318"/>
+      <c r="E8" s="318"/>
+      <c r="F8" s="318"/>
+      <c r="G8" s="318"/>
+      <c r="H8" s="318"/>
+      <c r="I8" s="318"/>
+      <c r="J8" s="318"/>
+      <c r="K8" s="318"/>
+      <c r="L8" s="319"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15678,38 +15667,38 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="293" t="s">
+      <c r="A10" s="320" t="s">
         <v>343</v>
       </c>
-      <c r="B10" s="294"/>
-      <c r="C10" s="294"/>
-      <c r="D10" s="294"/>
-      <c r="E10" s="294"/>
-      <c r="F10" s="294"/>
-      <c r="G10" s="294"/>
-      <c r="H10" s="294"/>
-      <c r="I10" s="294"/>
-      <c r="J10" s="294"/>
-      <c r="K10" s="294"/>
-      <c r="L10" s="295"/>
+      <c r="B10" s="321"/>
+      <c r="C10" s="321"/>
+      <c r="D10" s="321"/>
+      <c r="E10" s="321"/>
+      <c r="F10" s="321"/>
+      <c r="G10" s="321"/>
+      <c r="H10" s="321"/>
+      <c r="I10" s="321"/>
+      <c r="J10" s="321"/>
+      <c r="K10" s="321"/>
+      <c r="L10" s="322"/>
     </row>
     <row r="11" spans="1:18" s="58" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="249" t="s">
         <v>344</v>
       </c>
-      <c r="B11" s="296" t="s">
+      <c r="B11" s="275" t="s">
         <v>347</v>
       </c>
-      <c r="C11" s="296"/>
-      <c r="D11" s="296"/>
-      <c r="E11" s="296"/>
-      <c r="F11" s="296"/>
-      <c r="G11" s="296"/>
-      <c r="H11" s="296"/>
-      <c r="I11" s="296"/>
-      <c r="J11" s="296"/>
-      <c r="K11" s="296"/>
-      <c r="L11" s="297"/>
+      <c r="C11" s="275"/>
+      <c r="D11" s="275"/>
+      <c r="E11" s="275"/>
+      <c r="F11" s="275"/>
+      <c r="G11" s="275"/>
+      <c r="H11" s="275"/>
+      <c r="I11" s="275"/>
+      <c r="J11" s="275"/>
+      <c r="K11" s="275"/>
+      <c r="L11" s="276"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="161.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="241"/>
@@ -15729,51 +15718,51 @@
       <c r="A13" s="249" t="s">
         <v>345</v>
       </c>
-      <c r="B13" s="296" t="s">
+      <c r="B13" s="275" t="s">
         <v>348</v>
       </c>
-      <c r="C13" s="296"/>
-      <c r="D13" s="296"/>
-      <c r="E13" s="296"/>
-      <c r="F13" s="296"/>
-      <c r="G13" s="296"/>
-      <c r="H13" s="296"/>
-      <c r="I13" s="296"/>
-      <c r="J13" s="296"/>
-      <c r="K13" s="296"/>
-      <c r="L13" s="297"/>
+      <c r="C13" s="275"/>
+      <c r="D13" s="275"/>
+      <c r="E13" s="275"/>
+      <c r="F13" s="275"/>
+      <c r="G13" s="275"/>
+      <c r="H13" s="275"/>
+      <c r="I13" s="275"/>
+      <c r="J13" s="275"/>
+      <c r="K13" s="275"/>
+      <c r="L13" s="276"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="90.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="241"/>
-      <c r="B14" s="307"/>
-      <c r="C14" s="307"/>
-      <c r="D14" s="307"/>
-      <c r="E14" s="307"/>
-      <c r="F14" s="307"/>
-      <c r="G14" s="307"/>
-      <c r="H14" s="307"/>
-      <c r="I14" s="307"/>
-      <c r="J14" s="307"/>
-      <c r="K14" s="307"/>
-      <c r="L14" s="308"/>
+      <c r="B14" s="277"/>
+      <c r="C14" s="277"/>
+      <c r="D14" s="277"/>
+      <c r="E14" s="277"/>
+      <c r="F14" s="277"/>
+      <c r="G14" s="277"/>
+      <c r="H14" s="277"/>
+      <c r="I14" s="277"/>
+      <c r="J14" s="277"/>
+      <c r="K14" s="277"/>
+      <c r="L14" s="278"/>
     </row>
     <row r="15" spans="1:18" s="58" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="249" t="s">
         <v>346</v>
       </c>
-      <c r="B15" s="296" t="s">
+      <c r="B15" s="275" t="s">
         <v>349</v>
       </c>
-      <c r="C15" s="296"/>
-      <c r="D15" s="296"/>
-      <c r="E15" s="296"/>
-      <c r="F15" s="296"/>
-      <c r="G15" s="296"/>
-      <c r="H15" s="296"/>
-      <c r="I15" s="296"/>
-      <c r="J15" s="296"/>
-      <c r="K15" s="296"/>
-      <c r="L15" s="297"/>
+      <c r="C15" s="275"/>
+      <c r="D15" s="275"/>
+      <c r="E15" s="275"/>
+      <c r="F15" s="275"/>
+      <c r="G15" s="275"/>
+      <c r="H15" s="275"/>
+      <c r="I15" s="275"/>
+      <c r="J15" s="275"/>
+      <c r="K15" s="275"/>
+      <c r="L15" s="276"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="241"/>
@@ -15790,12 +15779,12 @@
       <c r="L16" s="248"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="305" t="s">
+      <c r="A17" s="273" t="s">
         <v>353</v>
       </c>
-      <c r="B17" s="306"/>
-      <c r="C17" s="306"/>
-      <c r="D17" s="306"/>
+      <c r="B17" s="274"/>
+      <c r="C17" s="274"/>
+      <c r="D17" s="274"/>
       <c r="E17" s="246" t="s">
         <v>354</v>
       </c>
@@ -15822,84 +15811,84 @@
       <c r="L18" s="113"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="276" t="s">
+      <c r="A19" s="305" t="s">
         <v>166</v>
       </c>
-      <c r="B19" s="277"/>
-      <c r="C19" s="277"/>
-      <c r="D19" s="277"/>
-      <c r="E19" s="277"/>
-      <c r="F19" s="277"/>
-      <c r="G19" s="277"/>
-      <c r="H19" s="277"/>
-      <c r="I19" s="277"/>
-      <c r="J19" s="277"/>
-      <c r="K19" s="277"/>
-      <c r="L19" s="278"/>
+      <c r="B19" s="306"/>
+      <c r="C19" s="306"/>
+      <c r="D19" s="306"/>
+      <c r="E19" s="306"/>
+      <c r="F19" s="306"/>
+      <c r="G19" s="306"/>
+      <c r="H19" s="306"/>
+      <c r="I19" s="306"/>
+      <c r="J19" s="306"/>
+      <c r="K19" s="306"/>
+      <c r="L19" s="307"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="279" t="s">
+      <c r="A20" s="308" t="s">
         <v>289</v>
       </c>
-      <c r="B20" s="280"/>
-      <c r="C20" s="280"/>
-      <c r="D20" s="280"/>
-      <c r="E20" s="280"/>
-      <c r="F20" s="280"/>
-      <c r="G20" s="280"/>
-      <c r="H20" s="280"/>
-      <c r="I20" s="280"/>
-      <c r="J20" s="280"/>
-      <c r="K20" s="280"/>
-      <c r="L20" s="281"/>
+      <c r="B20" s="309"/>
+      <c r="C20" s="309"/>
+      <c r="D20" s="309"/>
+      <c r="E20" s="309"/>
+      <c r="F20" s="309"/>
+      <c r="G20" s="309"/>
+      <c r="H20" s="309"/>
+      <c r="I20" s="309"/>
+      <c r="J20" s="309"/>
+      <c r="K20" s="309"/>
+      <c r="L20" s="310"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="282" t="s">
+      <c r="A21" s="311" t="s">
         <v>290</v>
       </c>
-      <c r="B21" s="283"/>
-      <c r="C21" s="283"/>
-      <c r="D21" s="283"/>
-      <c r="E21" s="283"/>
-      <c r="F21" s="283"/>
-      <c r="G21" s="283"/>
-      <c r="H21" s="283"/>
-      <c r="I21" s="283"/>
-      <c r="J21" s="283"/>
-      <c r="K21" s="283"/>
-      <c r="L21" s="284"/>
+      <c r="B21" s="289"/>
+      <c r="C21" s="289"/>
+      <c r="D21" s="289"/>
+      <c r="E21" s="289"/>
+      <c r="F21" s="289"/>
+      <c r="G21" s="289"/>
+      <c r="H21" s="289"/>
+      <c r="I21" s="289"/>
+      <c r="J21" s="289"/>
+      <c r="K21" s="289"/>
+      <c r="L21" s="290"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="282" t="s">
+      <c r="A22" s="311" t="s">
         <v>167</v>
       </c>
-      <c r="B22" s="283"/>
-      <c r="C22" s="283"/>
-      <c r="D22" s="283"/>
-      <c r="E22" s="283"/>
-      <c r="F22" s="283"/>
-      <c r="G22" s="283"/>
-      <c r="H22" s="283"/>
-      <c r="I22" s="283"/>
-      <c r="J22" s="283"/>
-      <c r="K22" s="283"/>
-      <c r="L22" s="284"/>
+      <c r="B22" s="289"/>
+      <c r="C22" s="289"/>
+      <c r="D22" s="289"/>
+      <c r="E22" s="289"/>
+      <c r="F22" s="289"/>
+      <c r="G22" s="289"/>
+      <c r="H22" s="289"/>
+      <c r="I22" s="289"/>
+      <c r="J22" s="289"/>
+      <c r="K22" s="289"/>
+      <c r="L22" s="290"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="285" t="s">
+      <c r="A23" s="312" t="s">
         <v>291</v>
       </c>
-      <c r="B23" s="286"/>
-      <c r="C23" s="286"/>
-      <c r="D23" s="286"/>
-      <c r="E23" s="286"/>
-      <c r="F23" s="286"/>
-      <c r="G23" s="286"/>
-      <c r="H23" s="286"/>
-      <c r="I23" s="286"/>
-      <c r="J23" s="286"/>
-      <c r="K23" s="286"/>
-      <c r="L23" s="287"/>
+      <c r="B23" s="313"/>
+      <c r="C23" s="313"/>
+      <c r="D23" s="313"/>
+      <c r="E23" s="313"/>
+      <c r="F23" s="313"/>
+      <c r="G23" s="313"/>
+      <c r="H23" s="313"/>
+      <c r="I23" s="313"/>
+      <c r="J23" s="313"/>
+      <c r="K23" s="313"/>
+      <c r="L23" s="314"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="113"/>
@@ -15916,332 +15905,332 @@
       <c r="L24" s="113"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="288" t="s">
+      <c r="A25" s="315" t="s">
         <v>287</v>
       </c>
-      <c r="B25" s="289"/>
-      <c r="C25" s="289"/>
-      <c r="D25" s="289"/>
-      <c r="E25" s="289"/>
-      <c r="F25" s="289"/>
-      <c r="G25" s="289"/>
-      <c r="H25" s="289"/>
-      <c r="I25" s="289"/>
-      <c r="J25" s="289"/>
-      <c r="K25" s="289"/>
-      <c r="L25" s="290"/>
+      <c r="B25" s="316"/>
+      <c r="C25" s="316"/>
+      <c r="D25" s="316"/>
+      <c r="E25" s="316"/>
+      <c r="F25" s="316"/>
+      <c r="G25" s="316"/>
+      <c r="H25" s="316"/>
+      <c r="I25" s="316"/>
+      <c r="J25" s="316"/>
+      <c r="K25" s="316"/>
+      <c r="L25" s="317"/>
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="265" t="s">
+      <c r="A26" s="294" t="s">
         <v>176</v>
       </c>
-      <c r="B26" s="266"/>
-      <c r="C26" s="266"/>
-      <c r="D26" s="266"/>
-      <c r="E26" s="266"/>
-      <c r="F26" s="266"/>
-      <c r="G26" s="266"/>
-      <c r="H26" s="266"/>
-      <c r="I26" s="266"/>
-      <c r="J26" s="266"/>
-      <c r="K26" s="266"/>
-      <c r="L26" s="267"/>
+      <c r="B26" s="295"/>
+      <c r="C26" s="295"/>
+      <c r="D26" s="295"/>
+      <c r="E26" s="295"/>
+      <c r="F26" s="295"/>
+      <c r="G26" s="295"/>
+      <c r="H26" s="295"/>
+      <c r="I26" s="295"/>
+      <c r="J26" s="295"/>
+      <c r="K26" s="295"/>
+      <c r="L26" s="296"/>
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="223">
         <v>1</v>
       </c>
-      <c r="B27" s="300" t="s">
+      <c r="B27" s="282" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="300"/>
-      <c r="D27" s="300"/>
-      <c r="E27" s="300"/>
-      <c r="F27" s="300"/>
-      <c r="G27" s="300"/>
-      <c r="H27" s="300"/>
-      <c r="I27" s="300"/>
-      <c r="J27" s="300"/>
-      <c r="K27" s="300"/>
-      <c r="L27" s="301"/>
+      <c r="C27" s="282"/>
+      <c r="D27" s="282"/>
+      <c r="E27" s="282"/>
+      <c r="F27" s="282"/>
+      <c r="G27" s="282"/>
+      <c r="H27" s="282"/>
+      <c r="I27" s="282"/>
+      <c r="J27" s="282"/>
+      <c r="K27" s="282"/>
+      <c r="L27" s="283"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="223">
         <v>2</v>
       </c>
-      <c r="B28" s="300" t="s">
+      <c r="B28" s="282" t="s">
         <v>283</v>
       </c>
-      <c r="C28" s="300"/>
-      <c r="D28" s="300"/>
-      <c r="E28" s="300"/>
-      <c r="F28" s="300"/>
-      <c r="G28" s="300"/>
-      <c r="H28" s="300"/>
-      <c r="I28" s="300"/>
-      <c r="J28" s="300"/>
-      <c r="K28" s="300"/>
-      <c r="L28" s="301"/>
+      <c r="C28" s="282"/>
+      <c r="D28" s="282"/>
+      <c r="E28" s="282"/>
+      <c r="F28" s="282"/>
+      <c r="G28" s="282"/>
+      <c r="H28" s="282"/>
+      <c r="I28" s="282"/>
+      <c r="J28" s="282"/>
+      <c r="K28" s="282"/>
+      <c r="L28" s="283"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="223">
         <v>3</v>
       </c>
-      <c r="B29" s="300" t="s">
+      <c r="B29" s="282" t="s">
         <v>168</v>
       </c>
-      <c r="C29" s="300"/>
-      <c r="D29" s="300"/>
-      <c r="E29" s="300"/>
-      <c r="F29" s="300"/>
-      <c r="G29" s="300"/>
-      <c r="H29" s="300"/>
-      <c r="I29" s="300"/>
-      <c r="J29" s="300"/>
-      <c r="K29" s="300"/>
-      <c r="L29" s="301"/>
+      <c r="C29" s="282"/>
+      <c r="D29" s="282"/>
+      <c r="E29" s="282"/>
+      <c r="F29" s="282"/>
+      <c r="G29" s="282"/>
+      <c r="H29" s="282"/>
+      <c r="I29" s="282"/>
+      <c r="J29" s="282"/>
+      <c r="K29" s="282"/>
+      <c r="L29" s="283"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="223">
         <v>4</v>
       </c>
-      <c r="B30" s="300" t="s">
+      <c r="B30" s="282" t="s">
         <v>292</v>
       </c>
-      <c r="C30" s="300"/>
-      <c r="D30" s="300"/>
-      <c r="E30" s="300"/>
-      <c r="F30" s="300"/>
-      <c r="G30" s="300"/>
-      <c r="H30" s="300"/>
-      <c r="I30" s="300"/>
-      <c r="J30" s="300"/>
-      <c r="K30" s="300"/>
-      <c r="L30" s="301"/>
+      <c r="C30" s="282"/>
+      <c r="D30" s="282"/>
+      <c r="E30" s="282"/>
+      <c r="F30" s="282"/>
+      <c r="G30" s="282"/>
+      <c r="H30" s="282"/>
+      <c r="I30" s="282"/>
+      <c r="J30" s="282"/>
+      <c r="K30" s="282"/>
+      <c r="L30" s="283"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="223">
         <v>5</v>
       </c>
-      <c r="B31" s="300" t="s">
+      <c r="B31" s="282" t="s">
         <v>169</v>
       </c>
-      <c r="C31" s="300"/>
-      <c r="D31" s="300"/>
-      <c r="E31" s="300"/>
-      <c r="F31" s="300"/>
-      <c r="G31" s="300"/>
-      <c r="H31" s="300"/>
-      <c r="I31" s="300"/>
-      <c r="J31" s="300"/>
-      <c r="K31" s="300"/>
-      <c r="L31" s="301"/>
+      <c r="C31" s="282"/>
+      <c r="D31" s="282"/>
+      <c r="E31" s="282"/>
+      <c r="F31" s="282"/>
+      <c r="G31" s="282"/>
+      <c r="H31" s="282"/>
+      <c r="I31" s="282"/>
+      <c r="J31" s="282"/>
+      <c r="K31" s="282"/>
+      <c r="L31" s="283"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="223"/>
-      <c r="B32" s="300" t="s">
+      <c r="B32" s="282" t="s">
         <v>170</v>
       </c>
-      <c r="C32" s="300"/>
-      <c r="D32" s="300"/>
-      <c r="E32" s="300"/>
-      <c r="F32" s="300"/>
-      <c r="G32" s="300"/>
-      <c r="H32" s="300"/>
-      <c r="I32" s="300"/>
-      <c r="J32" s="300"/>
-      <c r="K32" s="300"/>
-      <c r="L32" s="301"/>
+      <c r="C32" s="282"/>
+      <c r="D32" s="282"/>
+      <c r="E32" s="282"/>
+      <c r="F32" s="282"/>
+      <c r="G32" s="282"/>
+      <c r="H32" s="282"/>
+      <c r="I32" s="282"/>
+      <c r="J32" s="282"/>
+      <c r="K32" s="282"/>
+      <c r="L32" s="283"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="223"/>
-      <c r="B33" s="300" t="s">
+      <c r="B33" s="282" t="s">
         <v>171</v>
       </c>
-      <c r="C33" s="300"/>
-      <c r="D33" s="300"/>
-      <c r="E33" s="300"/>
-      <c r="F33" s="300"/>
-      <c r="G33" s="300"/>
-      <c r="H33" s="300"/>
-      <c r="I33" s="300"/>
-      <c r="J33" s="300"/>
-      <c r="K33" s="300"/>
-      <c r="L33" s="301"/>
+      <c r="C33" s="282"/>
+      <c r="D33" s="282"/>
+      <c r="E33" s="282"/>
+      <c r="F33" s="282"/>
+      <c r="G33" s="282"/>
+      <c r="H33" s="282"/>
+      <c r="I33" s="282"/>
+      <c r="J33" s="282"/>
+      <c r="K33" s="282"/>
+      <c r="L33" s="283"/>
       <c r="N33" s="106"/>
     </row>
     <row r="34" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="302" t="s">
+      <c r="A34" s="291" t="s">
         <v>177</v>
       </c>
-      <c r="B34" s="303"/>
-      <c r="C34" s="303"/>
-      <c r="D34" s="303"/>
-      <c r="E34" s="303"/>
-      <c r="F34" s="303"/>
-      <c r="G34" s="303"/>
-      <c r="H34" s="303"/>
-      <c r="I34" s="303"/>
-      <c r="J34" s="303"/>
-      <c r="K34" s="303"/>
-      <c r="L34" s="304"/>
+      <c r="B34" s="292"/>
+      <c r="C34" s="292"/>
+      <c r="D34" s="292"/>
+      <c r="E34" s="292"/>
+      <c r="F34" s="292"/>
+      <c r="G34" s="292"/>
+      <c r="H34" s="292"/>
+      <c r="I34" s="292"/>
+      <c r="J34" s="292"/>
+      <c r="K34" s="292"/>
+      <c r="L34" s="293"/>
       <c r="N34" s="106"/>
     </row>
     <row r="35" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="223">
         <v>1</v>
       </c>
-      <c r="B35" s="300" t="s">
+      <c r="B35" s="282" t="s">
         <v>172</v>
       </c>
-      <c r="C35" s="300"/>
-      <c r="D35" s="300"/>
-      <c r="E35" s="300"/>
-      <c r="F35" s="300"/>
-      <c r="G35" s="300"/>
-      <c r="H35" s="300"/>
-      <c r="I35" s="300"/>
-      <c r="J35" s="300"/>
-      <c r="K35" s="300"/>
-      <c r="L35" s="301"/>
+      <c r="C35" s="282"/>
+      <c r="D35" s="282"/>
+      <c r="E35" s="282"/>
+      <c r="F35" s="282"/>
+      <c r="G35" s="282"/>
+      <c r="H35" s="282"/>
+      <c r="I35" s="282"/>
+      <c r="J35" s="282"/>
+      <c r="K35" s="282"/>
+      <c r="L35" s="283"/>
       <c r="N35" s="106"/>
     </row>
     <row r="36" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="223"/>
-      <c r="B36" s="298" t="s">
+      <c r="B36" s="280" t="s">
         <v>293</v>
       </c>
-      <c r="C36" s="298"/>
-      <c r="D36" s="298"/>
-      <c r="E36" s="298"/>
-      <c r="F36" s="298"/>
-      <c r="G36" s="298"/>
-      <c r="H36" s="298"/>
-      <c r="I36" s="298"/>
-      <c r="J36" s="298"/>
-      <c r="K36" s="298"/>
-      <c r="L36" s="299"/>
+      <c r="C36" s="280"/>
+      <c r="D36" s="280"/>
+      <c r="E36" s="280"/>
+      <c r="F36" s="280"/>
+      <c r="G36" s="280"/>
+      <c r="H36" s="280"/>
+      <c r="I36" s="280"/>
+      <c r="J36" s="280"/>
+      <c r="K36" s="280"/>
+      <c r="L36" s="281"/>
       <c r="N36" s="106"/>
     </row>
     <row r="37" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="223">
         <v>2</v>
       </c>
-      <c r="B37" s="300" t="s">
+      <c r="B37" s="282" t="s">
         <v>286</v>
       </c>
-      <c r="C37" s="300"/>
-      <c r="D37" s="300"/>
-      <c r="E37" s="300"/>
-      <c r="F37" s="300"/>
-      <c r="G37" s="300"/>
-      <c r="H37" s="300"/>
-      <c r="I37" s="300"/>
-      <c r="J37" s="300"/>
-      <c r="K37" s="300"/>
-      <c r="L37" s="301"/>
+      <c r="C37" s="282"/>
+      <c r="D37" s="282"/>
+      <c r="E37" s="282"/>
+      <c r="F37" s="282"/>
+      <c r="G37" s="282"/>
+      <c r="H37" s="282"/>
+      <c r="I37" s="282"/>
+      <c r="J37" s="282"/>
+      <c r="K37" s="282"/>
+      <c r="L37" s="283"/>
       <c r="N37" s="106"/>
     </row>
     <row r="38" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="223">
         <v>3</v>
       </c>
-      <c r="B38" s="300" t="s">
+      <c r="B38" s="282" t="s">
         <v>275</v>
       </c>
-      <c r="C38" s="300"/>
-      <c r="D38" s="300"/>
-      <c r="E38" s="300"/>
-      <c r="F38" s="300"/>
-      <c r="G38" s="300"/>
-      <c r="H38" s="300"/>
-      <c r="I38" s="300"/>
-      <c r="J38" s="300"/>
-      <c r="K38" s="300"/>
-      <c r="L38" s="301"/>
+      <c r="C38" s="282"/>
+      <c r="D38" s="282"/>
+      <c r="E38" s="282"/>
+      <c r="F38" s="282"/>
+      <c r="G38" s="282"/>
+      <c r="H38" s="282"/>
+      <c r="I38" s="282"/>
+      <c r="J38" s="282"/>
+      <c r="K38" s="282"/>
+      <c r="L38" s="283"/>
       <c r="N38" s="106"/>
     </row>
     <row r="39" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="223">
         <v>4</v>
       </c>
-      <c r="B39" s="300" t="s">
+      <c r="B39" s="282" t="s">
         <v>294</v>
       </c>
-      <c r="C39" s="300"/>
-      <c r="D39" s="300"/>
-      <c r="E39" s="300"/>
-      <c r="F39" s="300"/>
-      <c r="G39" s="300"/>
-      <c r="H39" s="300"/>
-      <c r="I39" s="300"/>
-      <c r="J39" s="300"/>
-      <c r="K39" s="300"/>
-      <c r="L39" s="301"/>
+      <c r="C39" s="282"/>
+      <c r="D39" s="282"/>
+      <c r="E39" s="282"/>
+      <c r="F39" s="282"/>
+      <c r="G39" s="282"/>
+      <c r="H39" s="282"/>
+      <c r="I39" s="282"/>
+      <c r="J39" s="282"/>
+      <c r="K39" s="282"/>
+      <c r="L39" s="283"/>
       <c r="N39" s="106"/>
     </row>
     <row r="40" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="223">
         <v>5</v>
       </c>
-      <c r="B40" s="298" t="s">
+      <c r="B40" s="280" t="s">
         <v>276</v>
       </c>
-      <c r="C40" s="298"/>
-      <c r="D40" s="298"/>
-      <c r="E40" s="298"/>
-      <c r="F40" s="298"/>
-      <c r="G40" s="298"/>
-      <c r="H40" s="298"/>
-      <c r="I40" s="298"/>
-      <c r="J40" s="298"/>
-      <c r="K40" s="298"/>
-      <c r="L40" s="299"/>
+      <c r="C40" s="280"/>
+      <c r="D40" s="280"/>
+      <c r="E40" s="280"/>
+      <c r="F40" s="280"/>
+      <c r="G40" s="280"/>
+      <c r="H40" s="280"/>
+      <c r="I40" s="280"/>
+      <c r="J40" s="280"/>
+      <c r="K40" s="280"/>
+      <c r="L40" s="281"/>
       <c r="N40" s="106"/>
     </row>
     <row r="41" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="223">
         <v>6</v>
       </c>
-      <c r="B41" s="298" t="s">
+      <c r="B41" s="280" t="s">
         <v>281</v>
       </c>
-      <c r="C41" s="298"/>
-      <c r="D41" s="298"/>
-      <c r="E41" s="298"/>
-      <c r="F41" s="298"/>
-      <c r="G41" s="298"/>
-      <c r="H41" s="298"/>
-      <c r="I41" s="298"/>
-      <c r="J41" s="298"/>
-      <c r="K41" s="298"/>
-      <c r="L41" s="299"/>
+      <c r="C41" s="280"/>
+      <c r="D41" s="280"/>
+      <c r="E41" s="280"/>
+      <c r="F41" s="280"/>
+      <c r="G41" s="280"/>
+      <c r="H41" s="280"/>
+      <c r="I41" s="280"/>
+      <c r="J41" s="280"/>
+      <c r="K41" s="280"/>
+      <c r="L41" s="281"/>
       <c r="N41" s="106"/>
     </row>
     <row r="42" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="223">
         <v>7</v>
       </c>
-      <c r="B42" s="300" t="s">
+      <c r="B42" s="282" t="s">
         <v>277</v>
       </c>
-      <c r="C42" s="300"/>
-      <c r="D42" s="300"/>
-      <c r="E42" s="300"/>
-      <c r="F42" s="300"/>
-      <c r="G42" s="300"/>
-      <c r="H42" s="300"/>
-      <c r="I42" s="300"/>
-      <c r="J42" s="300"/>
-      <c r="K42" s="300"/>
-      <c r="L42" s="301"/>
+      <c r="C42" s="282"/>
+      <c r="D42" s="282"/>
+      <c r="E42" s="282"/>
+      <c r="F42" s="282"/>
+      <c r="G42" s="282"/>
+      <c r="H42" s="282"/>
+      <c r="I42" s="282"/>
+      <c r="J42" s="282"/>
+      <c r="K42" s="282"/>
+      <c r="L42" s="283"/>
     </row>
     <row r="43" spans="1:14" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="223"/>
@@ -16258,56 +16247,56 @@
       <c r="L43" s="225"/>
     </row>
     <row r="44" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="302" t="s">
+      <c r="A44" s="291" t="s">
         <v>280</v>
       </c>
-      <c r="B44" s="303"/>
-      <c r="C44" s="303"/>
-      <c r="D44" s="303"/>
-      <c r="E44" s="303"/>
-      <c r="F44" s="303"/>
-      <c r="G44" s="303"/>
-      <c r="H44" s="303"/>
-      <c r="I44" s="303"/>
-      <c r="J44" s="303"/>
-      <c r="K44" s="303"/>
-      <c r="L44" s="304"/>
+      <c r="B44" s="292"/>
+      <c r="C44" s="292"/>
+      <c r="D44" s="292"/>
+      <c r="E44" s="292"/>
+      <c r="F44" s="292"/>
+      <c r="G44" s="292"/>
+      <c r="H44" s="292"/>
+      <c r="I44" s="292"/>
+      <c r="J44" s="292"/>
+      <c r="K44" s="292"/>
+      <c r="L44" s="293"/>
     </row>
     <row r="45" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="226" t="s">
         <v>278</v>
       </c>
-      <c r="B45" s="300" t="s">
+      <c r="B45" s="282" t="s">
         <v>173</v>
       </c>
-      <c r="C45" s="300"/>
-      <c r="D45" s="300"/>
-      <c r="E45" s="300"/>
-      <c r="F45" s="300"/>
-      <c r="G45" s="300"/>
-      <c r="H45" s="300"/>
-      <c r="I45" s="300"/>
-      <c r="J45" s="300"/>
-      <c r="K45" s="300"/>
-      <c r="L45" s="301"/>
+      <c r="C45" s="282"/>
+      <c r="D45" s="282"/>
+      <c r="E45" s="282"/>
+      <c r="F45" s="282"/>
+      <c r="G45" s="282"/>
+      <c r="H45" s="282"/>
+      <c r="I45" s="282"/>
+      <c r="J45" s="282"/>
+      <c r="K45" s="282"/>
+      <c r="L45" s="283"/>
     </row>
     <row r="46" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="227" t="s">
         <v>279</v>
       </c>
-      <c r="B46" s="310" t="s">
+      <c r="B46" s="284" t="s">
         <v>282</v>
       </c>
-      <c r="C46" s="310"/>
-      <c r="D46" s="310"/>
-      <c r="E46" s="310"/>
-      <c r="F46" s="310"/>
-      <c r="G46" s="310"/>
-      <c r="H46" s="310"/>
-      <c r="I46" s="310"/>
-      <c r="J46" s="310"/>
-      <c r="K46" s="310"/>
-      <c r="L46" s="311"/>
+      <c r="C46" s="284"/>
+      <c r="D46" s="284"/>
+      <c r="E46" s="284"/>
+      <c r="F46" s="284"/>
+      <c r="G46" s="284"/>
+      <c r="H46" s="284"/>
+      <c r="I46" s="284"/>
+      <c r="J46" s="284"/>
+      <c r="K46" s="284"/>
+      <c r="L46" s="285"/>
     </row>
     <row r="47" spans="1:14" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="160"/>
@@ -16324,20 +16313,20 @@
       <c r="L47" s="113"/>
     </row>
     <row r="48" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="312" t="s">
+      <c r="A48" s="286" t="s">
         <v>201</v>
       </c>
-      <c r="B48" s="313"/>
-      <c r="C48" s="313"/>
-      <c r="D48" s="313"/>
-      <c r="E48" s="313"/>
-      <c r="F48" s="313"/>
-      <c r="G48" s="313"/>
-      <c r="H48" s="313"/>
-      <c r="I48" s="313"/>
-      <c r="J48" s="313"/>
-      <c r="K48" s="313"/>
-      <c r="L48" s="314"/>
+      <c r="B48" s="287"/>
+      <c r="C48" s="287"/>
+      <c r="D48" s="287"/>
+      <c r="E48" s="287"/>
+      <c r="F48" s="287"/>
+      <c r="G48" s="287"/>
+      <c r="H48" s="287"/>
+      <c r="I48" s="287"/>
+      <c r="J48" s="287"/>
+      <c r="K48" s="287"/>
+      <c r="L48" s="288"/>
     </row>
     <row r="49" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="230" t="s">
@@ -16425,90 +16414,90 @@
       <c r="B54" s="168" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="283" t="s">
+      <c r="C54" s="289" t="s">
         <v>267</v>
       </c>
-      <c r="D54" s="283"/>
-      <c r="E54" s="283"/>
-      <c r="F54" s="283"/>
-      <c r="G54" s="283"/>
-      <c r="H54" s="283"/>
-      <c r="I54" s="283"/>
-      <c r="J54" s="283"/>
-      <c r="K54" s="283"/>
-      <c r="L54" s="284"/>
+      <c r="D54" s="289"/>
+      <c r="E54" s="289"/>
+      <c r="F54" s="289"/>
+      <c r="G54" s="289"/>
+      <c r="H54" s="289"/>
+      <c r="I54" s="289"/>
+      <c r="J54" s="289"/>
+      <c r="K54" s="289"/>
+      <c r="L54" s="290"/>
     </row>
     <row r="55" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="167"/>
       <c r="B55" s="168" t="s">
         <v>268</v>
       </c>
-      <c r="C55" s="283" t="s">
+      <c r="C55" s="289" t="s">
         <v>269</v>
       </c>
-      <c r="D55" s="283"/>
-      <c r="E55" s="283"/>
-      <c r="F55" s="283"/>
-      <c r="G55" s="283"/>
-      <c r="H55" s="283"/>
-      <c r="I55" s="283"/>
-      <c r="J55" s="283"/>
-      <c r="K55" s="283"/>
-      <c r="L55" s="284"/>
+      <c r="D55" s="289"/>
+      <c r="E55" s="289"/>
+      <c r="F55" s="289"/>
+      <c r="G55" s="289"/>
+      <c r="H55" s="289"/>
+      <c r="I55" s="289"/>
+      <c r="J55" s="289"/>
+      <c r="K55" s="289"/>
+      <c r="L55" s="290"/>
     </row>
     <row r="56" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="167"/>
       <c r="B56" s="168" t="s">
         <v>336</v>
       </c>
-      <c r="C56" s="283" t="s">
+      <c r="C56" s="289" t="s">
         <v>337</v>
       </c>
-      <c r="D56" s="283"/>
-      <c r="E56" s="283"/>
-      <c r="F56" s="283"/>
-      <c r="G56" s="283"/>
-      <c r="H56" s="283"/>
-      <c r="I56" s="283"/>
-      <c r="J56" s="283"/>
-      <c r="K56" s="283"/>
-      <c r="L56" s="284"/>
+      <c r="D56" s="289"/>
+      <c r="E56" s="289"/>
+      <c r="F56" s="289"/>
+      <c r="G56" s="289"/>
+      <c r="H56" s="289"/>
+      <c r="I56" s="289"/>
+      <c r="J56" s="289"/>
+      <c r="K56" s="289"/>
+      <c r="L56" s="290"/>
     </row>
     <row r="57" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="167"/>
       <c r="B57" s="168" t="s">
         <v>99</v>
       </c>
-      <c r="C57" s="283" t="s">
+      <c r="C57" s="289" t="s">
         <v>100</v>
       </c>
-      <c r="D57" s="283"/>
-      <c r="E57" s="283"/>
-      <c r="F57" s="283"/>
-      <c r="G57" s="283"/>
-      <c r="H57" s="283"/>
-      <c r="I57" s="283"/>
-      <c r="J57" s="283"/>
-      <c r="K57" s="283"/>
-      <c r="L57" s="284"/>
+      <c r="D57" s="289"/>
+      <c r="E57" s="289"/>
+      <c r="F57" s="289"/>
+      <c r="G57" s="289"/>
+      <c r="H57" s="289"/>
+      <c r="I57" s="289"/>
+      <c r="J57" s="289"/>
+      <c r="K57" s="289"/>
+      <c r="L57" s="290"/>
     </row>
     <row r="58" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="167"/>
       <c r="B58" s="168" t="s">
         <v>199</v>
       </c>
-      <c r="C58" s="283" t="s">
+      <c r="C58" s="289" t="s">
         <v>200</v>
       </c>
-      <c r="D58" s="283"/>
-      <c r="E58" s="283"/>
-      <c r="F58" s="283"/>
-      <c r="G58" s="283"/>
-      <c r="H58" s="283"/>
-      <c r="I58" s="283"/>
-      <c r="J58" s="283"/>
-      <c r="K58" s="283"/>
-      <c r="L58" s="284"/>
+      <c r="D58" s="289"/>
+      <c r="E58" s="289"/>
+      <c r="F58" s="289"/>
+      <c r="G58" s="289"/>
+      <c r="H58" s="289"/>
+      <c r="I58" s="289"/>
+      <c r="J58" s="289"/>
+      <c r="K58" s="289"/>
+      <c r="L58" s="290"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="167"/>
@@ -16533,18 +16522,18 @@
       <c r="B60" s="168" t="s">
         <v>405</v>
       </c>
-      <c r="C60" s="283" t="s">
+      <c r="C60" s="289" t="s">
         <v>406</v>
       </c>
-      <c r="D60" s="283"/>
-      <c r="E60" s="283"/>
-      <c r="F60" s="283"/>
-      <c r="G60" s="283"/>
-      <c r="H60" s="283"/>
-      <c r="I60" s="283"/>
-      <c r="J60" s="283"/>
-      <c r="K60" s="283"/>
-      <c r="L60" s="284"/>
+      <c r="D60" s="289"/>
+      <c r="E60" s="289"/>
+      <c r="F60" s="289"/>
+      <c r="G60" s="289"/>
+      <c r="H60" s="289"/>
+      <c r="I60" s="289"/>
+      <c r="J60" s="289"/>
+      <c r="K60" s="289"/>
+      <c r="L60" s="290"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="167"/>
@@ -16665,25 +16654,56 @@
       </c>
     </row>
     <row r="82" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="309" t="s">
+      <c r="A82" s="279" t="s">
         <v>409</v>
       </c>
-      <c r="B82" s="309"/>
-      <c r="C82" s="309"/>
-      <c r="D82" s="309"/>
-      <c r="E82" s="309"/>
-      <c r="F82" s="309"/>
-      <c r="G82" s="309"/>
-      <c r="H82" s="309"/>
-      <c r="I82" s="309"/>
-      <c r="J82" s="309"/>
-      <c r="K82" s="309"/>
-      <c r="L82" s="309"/>
+      <c r="B82" s="279"/>
+      <c r="C82" s="279"/>
+      <c r="D82" s="279"/>
+      <c r="E82" s="279"/>
+      <c r="F82" s="279"/>
+      <c r="G82" s="279"/>
+      <c r="H82" s="279"/>
+      <c r="I82" s="279"/>
+      <c r="J82" s="279"/>
+      <c r="K82" s="279"/>
+      <c r="L82" s="279"/>
     </row>
     <row r="87" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="88" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="B40:L40"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B30:L30"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B39:L39"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="B13:L13"/>
     <mergeCell ref="B14:L14"/>
@@ -16700,37 +16720,6 @@
     <mergeCell ref="C55:L55"/>
     <mergeCell ref="C60:L60"/>
     <mergeCell ref="A44:L44"/>
-    <mergeCell ref="C56:L56"/>
-    <mergeCell ref="B40:L40"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B8:L8"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="B11:L11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A67" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -16768,82 +16757,82 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="350" t="s">
+      <c r="A3" s="364" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="350"/>
-      <c r="C3" s="350"/>
+      <c r="B3" s="364"/>
+      <c r="C3" s="364"/>
       <c r="D3" s="128" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="351" t="s">
+      <c r="A4" s="365" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="351"/>
-      <c r="C4" s="351"/>
+      <c r="B4" s="365"/>
+      <c r="C4" s="365"/>
       <c r="D4" s="175" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="355" t="s">
+      <c r="A5" s="369" t="s">
         <v>184</v>
       </c>
-      <c r="B5" s="352"/>
-      <c r="C5" s="352"/>
+      <c r="B5" s="366"/>
+      <c r="C5" s="366"/>
       <c r="D5" s="176" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="353" t="s">
+      <c r="A6" s="367" t="s">
         <v>185</v>
       </c>
-      <c r="B6" s="353"/>
-      <c r="C6" s="353"/>
+      <c r="B6" s="367"/>
+      <c r="C6" s="367"/>
       <c r="D6" s="177" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="354" t="s">
+      <c r="A7" s="368" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="354"/>
-      <c r="C7" s="354"/>
+      <c r="B7" s="368"/>
+      <c r="C7" s="368"/>
       <c r="D7" s="178" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="351" t="s">
+      <c r="A11" s="365" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="351"/>
-      <c r="C11" s="351"/>
+      <c r="B11" s="365"/>
+      <c r="C11" s="365"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="352" t="s">
+      <c r="A12" s="366" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="352"/>
-      <c r="C12" s="352"/>
+      <c r="B12" s="366"/>
+      <c r="C12" s="366"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="353" t="s">
+      <c r="A13" s="367" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="353"/>
-      <c r="C13" s="353"/>
+      <c r="B13" s="367"/>
+      <c r="C13" s="367"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="354" t="s">
+      <c r="A14" s="368" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="354"/>
-      <c r="C14" s="354"/>
+      <c r="B14" s="368"/>
+      <c r="C14" s="368"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -18161,7 +18150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BF7D8F-86F3-47E9-AB85-EE9B4CAB70E4}">
   <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView topLeftCell="A122" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A21" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
@@ -18191,16 +18180,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="315" t="str">
+      <c r="A1" s="323" t="str">
         <f>'ReadMe-Directions'!A1</f>
         <v>Immersive Model for Lake Mead based on the Principle of Divide Reservoir Inflow</v>
       </c>
-      <c r="B1" s="315"/>
-      <c r="C1" s="315"/>
-      <c r="D1" s="315"/>
-      <c r="E1" s="315"/>
-      <c r="F1" s="315"/>
-      <c r="G1" s="315"/>
+      <c r="B1" s="323"/>
+      <c r="C1" s="323"/>
+      <c r="D1" s="323"/>
+      <c r="E1" s="323"/>
+      <c r="F1" s="323"/>
+      <c r="G1" s="323"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -18209,15 +18198,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="323" t="s">
+      <c r="A3" s="331" t="s">
         <v>191</v>
       </c>
-      <c r="B3" s="323"/>
-      <c r="C3" s="323"/>
-      <c r="D3" s="323"/>
-      <c r="E3" s="323"/>
-      <c r="F3" s="323"/>
-      <c r="G3" s="323"/>
+      <c r="B3" s="331"/>
+      <c r="C3" s="331"/>
+      <c r="D3" s="331"/>
+      <c r="E3" s="331"/>
+      <c r="F3" s="331"/>
+      <c r="G3" s="331"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -18233,13 +18222,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="324" t="s">
+      <c r="C4" s="332" t="s">
         <v>264</v>
       </c>
-      <c r="D4" s="325"/>
-      <c r="E4" s="325"/>
-      <c r="F4" s="325"/>
-      <c r="G4" s="326"/>
+      <c r="D4" s="333"/>
+      <c r="E4" s="333"/>
+      <c r="F4" s="333"/>
+      <c r="G4" s="334"/>
       <c r="N4" s="141" t="s">
         <v>338</v>
       </c>
@@ -18249,11 +18238,11 @@
         <v>241</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="327"/>
-      <c r="D5" s="322"/>
-      <c r="E5" s="322"/>
-      <c r="F5" s="322"/>
-      <c r="G5" s="322"/>
+      <c r="C5" s="335"/>
+      <c r="D5" s="330"/>
+      <c r="E5" s="330"/>
+      <c r="F5" s="330"/>
+      <c r="G5" s="330"/>
       <c r="N5" s="141"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -18261,11 +18250,11 @@
         <v>203</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="327"/>
-      <c r="D6" s="322"/>
-      <c r="E6" s="322"/>
-      <c r="F6" s="322"/>
-      <c r="G6" s="322"/>
+      <c r="C6" s="335"/>
+      <c r="D6" s="330"/>
+      <c r="E6" s="330"/>
+      <c r="F6" s="330"/>
+      <c r="G6" s="330"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -18273,11 +18262,11 @@
         <v>204</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="327"/>
-      <c r="D7" s="322"/>
-      <c r="E7" s="322"/>
-      <c r="F7" s="322"/>
-      <c r="G7" s="322"/>
+      <c r="C7" s="335"/>
+      <c r="D7" s="330"/>
+      <c r="E7" s="330"/>
+      <c r="F7" s="330"/>
+      <c r="G7" s="330"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -18285,11 +18274,11 @@
         <v>205</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="322"/>
-      <c r="D8" s="322"/>
-      <c r="E8" s="322"/>
-      <c r="F8" s="322"/>
-      <c r="G8" s="322"/>
+      <c r="C8" s="330"/>
+      <c r="D8" s="330"/>
+      <c r="E8" s="330"/>
+      <c r="F8" s="330"/>
+      <c r="G8" s="330"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -18297,11 +18286,11 @@
         <v>18</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="328"/>
-      <c r="D9" s="328"/>
-      <c r="E9" s="328"/>
-      <c r="F9" s="328"/>
-      <c r="G9" s="328"/>
+      <c r="C9" s="336"/>
+      <c r="D9" s="336"/>
+      <c r="E9" s="336"/>
+      <c r="F9" s="336"/>
+      <c r="G9" s="336"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -18309,11 +18298,11 @@
         <v>285</v>
       </c>
       <c r="B10" s="90"/>
-      <c r="C10" s="322"/>
-      <c r="D10" s="322"/>
-      <c r="E10" s="322"/>
-      <c r="F10" s="322"/>
-      <c r="G10" s="322"/>
+      <c r="C10" s="330"/>
+      <c r="D10" s="330"/>
+      <c r="E10" s="330"/>
+      <c r="F10" s="330"/>
+      <c r="G10" s="330"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -18326,36 +18315,36 @@
       <c r="A12" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="329" t="s">
+      <c r="B12" s="337" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="330"/>
-      <c r="D12" s="331"/>
+      <c r="C12" s="338"/>
+      <c r="D12" s="339"/>
       <c r="N12" s="141" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="332" t="s">
+      <c r="B13" s="340" t="s">
         <v>190</v>
       </c>
-      <c r="C13" s="333"/>
-      <c r="D13" s="334"/>
+      <c r="C13" s="341"/>
+      <c r="D13" s="342"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="316" t="s">
+      <c r="B14" s="324" t="s">
         <v>185</v>
       </c>
-      <c r="C14" s="317"/>
-      <c r="D14" s="318"/>
+      <c r="C14" s="325"/>
+      <c r="D14" s="326"/>
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="319" t="s">
+      <c r="B15" s="327" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="320"/>
-      <c r="D15" s="321"/>
+      <c r="C15" s="328"/>
+      <c r="D15" s="329"/>
       <c r="N15" s="142"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -23125,10 +23114,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA15763-059F-401A-BB99-8A737E404CC4}">
-  <dimension ref="A1:W37"/>
+  <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23169,29 +23158,29 @@
     </row>
     <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I5" s="345" t="s">
+      <c r="I5" s="359" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="345" t="s">
+      <c r="J5" s="359" t="s">
         <v>214</v>
       </c>
-      <c r="K5" s="345" t="s">
+      <c r="K5" s="359" t="s">
         <v>215</v>
       </c>
-      <c r="L5" s="342" t="s">
+      <c r="L5" s="356" t="s">
         <v>216</v>
       </c>
-      <c r="M5" s="343"/>
-      <c r="N5" s="343"/>
-      <c r="O5" s="343"/>
-      <c r="P5" s="344"/>
-      <c r="Q5" s="336" t="s">
+      <c r="M5" s="357"/>
+      <c r="N5" s="357"/>
+      <c r="O5" s="357"/>
+      <c r="P5" s="358"/>
+      <c r="Q5" s="349" t="s">
         <v>217</v>
       </c>
-      <c r="R5" s="337"/>
-      <c r="S5" s="337"/>
-      <c r="T5" s="337"/>
-      <c r="U5" s="338"/>
+      <c r="R5" s="350"/>
+      <c r="S5" s="350"/>
+      <c r="T5" s="350"/>
+      <c r="U5" s="351"/>
     </row>
     <row r="6" spans="1:21" s="188" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="189" t="s">
@@ -23212,9 +23201,9 @@
       <c r="G6" s="189" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="346"/>
-      <c r="J6" s="346"/>
-      <c r="K6" s="346"/>
+      <c r="I6" s="360"/>
+      <c r="J6" s="360"/>
+      <c r="K6" s="360"/>
       <c r="L6" s="190" t="s">
         <v>219</v>
       </c>
@@ -23247,14 +23236,14 @@
       </c>
     </row>
     <row r="7" spans="1:21" s="188" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="342" t="s">
+      <c r="B7" s="356" t="s">
         <v>229</v>
       </c>
-      <c r="C7" s="343"/>
-      <c r="D7" s="343"/>
-      <c r="E7" s="343"/>
-      <c r="F7" s="343"/>
-      <c r="G7" s="344"/>
+      <c r="C7" s="357"/>
+      <c r="D7" s="357"/>
+      <c r="E7" s="357"/>
+      <c r="F7" s="357"/>
+      <c r="G7" s="358"/>
       <c r="I7" s="192" t="s">
         <v>414</v>
       </c>
@@ -23335,7 +23324,7 @@
       </c>
       <c r="L8" s="201">
         <f t="shared" ref="L8:O11" si="1">L$7-C14</f>
-        <v>2.5599999999999996</v>
+        <v>2.67001</v>
       </c>
       <c r="M8" s="201">
         <f t="shared" si="1"/>
@@ -23343,7 +23332,7 @@
       </c>
       <c r="N8" s="201">
         <f t="shared" si="1"/>
-        <v>4.4000000000000004</v>
+        <v>4.2899900000000004</v>
       </c>
       <c r="O8" s="201">
         <f t="shared" si="1"/>
@@ -23351,11 +23340,11 @@
       </c>
       <c r="P8" s="194">
         <f t="shared" ref="P8:P11" si="2">SUM(L8:O8)</f>
-        <v>8.6999999999999993</v>
+        <v>8.7000000000000011</v>
       </c>
       <c r="Q8" s="195">
         <f t="shared" si="0"/>
-        <v>0.29425287356321839</v>
+        <v>0.30689770114942533</v>
       </c>
       <c r="R8" s="195">
         <f t="shared" si="0"/>
@@ -23363,7 +23352,7 @@
       </c>
       <c r="S8" s="195">
         <f t="shared" si="0"/>
-        <v>0.50574712643678166</v>
+        <v>0.49310229885057483</v>
       </c>
       <c r="T8" s="195">
         <f t="shared" si="0"/>
@@ -23371,7 +23360,7 @@
       </c>
       <c r="U8" s="196">
         <f t="shared" ref="U8:U16" si="3">SUM(Q8:T8)</f>
-        <v>1</v>
+        <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
@@ -23407,7 +23396,7 @@
       </c>
       <c r="L9" s="201">
         <f t="shared" si="1"/>
-        <v>2.51667</v>
+        <v>2.6266799999999999</v>
       </c>
       <c r="M9" s="201">
         <f t="shared" si="1"/>
@@ -23415,7 +23404,7 @@
       </c>
       <c r="N9" s="201">
         <f t="shared" si="1"/>
-        <v>4.3633300000000004</v>
+        <v>4.2533200000000004</v>
       </c>
       <c r="O9" s="201">
         <f t="shared" si="1"/>
@@ -23427,7 +23416,7 @@
       </c>
       <c r="Q9" s="195">
         <f t="shared" si="0"/>
-        <v>0.29263604651162789</v>
+        <v>0.30542790697674421</v>
       </c>
       <c r="R9" s="195">
         <f t="shared" si="0"/>
@@ -23435,7 +23424,7 @@
       </c>
       <c r="S9" s="195">
         <f t="shared" si="0"/>
-        <v>0.50736395348837215</v>
+        <v>0.49457209302325589</v>
       </c>
       <c r="T9" s="195">
         <f t="shared" si="0"/>
@@ -23479,7 +23468,7 @@
       </c>
       <c r="L10" s="201">
         <f t="shared" si="1"/>
-        <v>2.2566899999999999</v>
+        <v>2.3666999999999998</v>
       </c>
       <c r="M10" s="201">
         <f t="shared" si="1"/>
@@ -23487,7 +23476,7 @@
       </c>
       <c r="N10" s="201">
         <f t="shared" si="1"/>
-        <v>4.1433100000000005</v>
+        <v>4.0333000000000006</v>
       </c>
       <c r="O10" s="201">
         <f t="shared" si="1"/>
@@ -23499,7 +23488,7 @@
       </c>
       <c r="Q10" s="195">
         <f t="shared" si="0"/>
-        <v>0.28208624999999998</v>
+        <v>0.29583749999999998</v>
       </c>
       <c r="R10" s="195">
         <f t="shared" si="0"/>
@@ -23507,7 +23496,7 @@
       </c>
       <c r="S10" s="195">
         <f t="shared" si="0"/>
-        <v>0.51791375000000006</v>
+        <v>0.50416250000000007</v>
       </c>
       <c r="T10" s="195">
         <f t="shared" si="0"/>
@@ -23522,13 +23511,13 @@
       <c r="B11" s="198" t="s">
         <v>235</v>
       </c>
-      <c r="C11" s="335" t="s">
+      <c r="C11" s="348" t="s">
         <v>236</v>
       </c>
-      <c r="D11" s="335"/>
-      <c r="E11" s="335"/>
-      <c r="F11" s="335"/>
-      <c r="G11" s="335"/>
+      <c r="D11" s="348"/>
+      <c r="E11" s="348"/>
+      <c r="F11" s="348"/>
+      <c r="G11" s="348"/>
       <c r="I11" s="192" t="s">
         <v>237</v>
       </c>
@@ -23542,7 +23531,7 @@
       </c>
       <c r="L11" s="201">
         <f t="shared" si="1"/>
-        <v>2.0400399999999999</v>
+        <v>2.1500499999999998</v>
       </c>
       <c r="M11" s="201">
         <f t="shared" si="1"/>
@@ -23550,7 +23539,7 @@
       </c>
       <c r="N11" s="201">
         <f t="shared" si="1"/>
-        <v>3.9599600000000001</v>
+        <v>3.8499500000000002</v>
       </c>
       <c r="O11" s="201">
         <f t="shared" si="1"/>
@@ -23562,7 +23551,7 @@
       </c>
       <c r="Q11" s="195">
         <f t="shared" si="0"/>
-        <v>0.27200533333333332</v>
+        <v>0.28667333333333328</v>
       </c>
       <c r="R11" s="195">
         <f t="shared" si="0"/>
@@ -23570,7 +23559,7 @@
       </c>
       <c r="S11" s="195">
         <f t="shared" si="0"/>
-        <v>0.52799466666666672</v>
+        <v>0.51332666666666671</v>
       </c>
       <c r="T11" s="195">
         <f t="shared" si="0"/>
@@ -23582,14 +23571,14 @@
       </c>
     </row>
     <row r="12" spans="1:21" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B12" s="376" t="s">
+      <c r="B12" s="352" t="s">
         <v>238</v>
       </c>
-      <c r="C12" s="376"/>
-      <c r="D12" s="376"/>
-      <c r="E12" s="376"/>
-      <c r="F12" s="376"/>
-      <c r="G12" s="376"/>
+      <c r="C12" s="352"/>
+      <c r="D12" s="352"/>
+      <c r="E12" s="352"/>
+      <c r="F12" s="352"/>
+      <c r="G12" s="352"/>
       <c r="I12" s="192" t="s">
         <v>239</v>
       </c>
@@ -23599,20 +23588,20 @@
       <c r="K12" s="200" t="s">
         <v>240</v>
       </c>
-      <c r="L12" s="339" t="s">
+      <c r="L12" s="353" t="s">
         <v>236</v>
       </c>
-      <c r="M12" s="340"/>
-      <c r="N12" s="340"/>
-      <c r="O12" s="340"/>
-      <c r="P12" s="341"/>
-      <c r="Q12" s="339" t="s">
+      <c r="M12" s="354"/>
+      <c r="N12" s="354"/>
+      <c r="O12" s="354"/>
+      <c r="P12" s="355"/>
+      <c r="Q12" s="353" t="s">
         <v>236</v>
       </c>
-      <c r="R12" s="340"/>
-      <c r="S12" s="340"/>
-      <c r="T12" s="340"/>
-      <c r="U12" s="341"/>
+      <c r="R12" s="354"/>
+      <c r="S12" s="354"/>
+      <c r="T12" s="354"/>
+      <c r="U12" s="355"/>
     </row>
     <row r="13" spans="1:21" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B13" s="198">
@@ -23646,7 +23635,7 @@
       </c>
       <c r="L13" s="201">
         <f>L11-C10*($K11-$K13)</f>
-        <v>1.5200799999999997</v>
+        <v>1.6300899999999996</v>
       </c>
       <c r="M13" s="201">
         <f>M11-D10*($K11-$K13)</f>
@@ -23654,7 +23643,7 @@
       </c>
       <c r="N13" s="201">
         <f>N11-E10*($K11-$K13)</f>
-        <v>3.5199199999999999</v>
+        <v>3.40991</v>
       </c>
       <c r="O13" s="201">
         <f>O11-F10*($K11-$K13)</f>
@@ -23666,7 +23655,7 @@
       </c>
       <c r="Q13" s="195">
         <f>L13/$K13</f>
-        <v>0.24128253968253963</v>
+        <v>0.25874444444444439</v>
       </c>
       <c r="R13" s="195">
         <f>M13/$K13</f>
@@ -23674,7 +23663,7 @@
       </c>
       <c r="S13" s="195">
         <f>N13/$K13</f>
-        <v>0.55871746031746028</v>
+        <v>0.5412555555555556</v>
       </c>
       <c r="T13" s="195">
         <f>O13/$K13</f>
@@ -23690,19 +23679,19 @@
         <v>0.3</v>
       </c>
       <c r="C14" s="201">
-        <f>$B14*C9</f>
-        <v>0.24</v>
+        <f>$B14*C$10</f>
+        <v>0.12998999999999999</v>
       </c>
       <c r="D14" s="201">
-        <f>$B14*D9</f>
+        <f t="shared" ref="D14:F17" si="5">$B14*D$10</f>
         <v>9.9900000000000006E-3</v>
       </c>
       <c r="E14" s="201">
-        <f>$B14*E9</f>
-        <v>0</v>
+        <f t="shared" si="5"/>
+        <v>0.11001000000000001</v>
       </c>
       <c r="F14" s="201">
-        <f>$B14*F9</f>
+        <f t="shared" si="5"/>
         <v>5.0009999999999992E-2</v>
       </c>
       <c r="G14" s="201">
@@ -23712,47 +23701,47 @@
       <c r="I14" s="192" t="s">
         <v>416</v>
       </c>
-      <c r="J14" s="356">
+      <c r="J14" s="265">
         <f>9-K14</f>
         <v>4</v>
       </c>
-      <c r="K14" s="369">
+      <c r="K14" s="269">
         <v>5</v>
       </c>
-      <c r="L14" s="357">
+      <c r="L14" s="266">
         <f>L11-C10*($K11-$K14)</f>
-        <v>0.95678999999999981</v>
-      </c>
-      <c r="M14" s="357">
+        <v>1.0667999999999997</v>
+      </c>
+      <c r="M14" s="266">
         <f>M11-D10*($K11-$K14)</f>
         <v>0.1668</v>
       </c>
-      <c r="N14" s="357">
-        <f t="shared" ref="N14:P14" si="5">N11-E10*($K11-$K14)</f>
-        <v>3.0432100000000002</v>
-      </c>
-      <c r="O14" s="357">
-        <f t="shared" si="5"/>
+      <c r="N14" s="266">
+        <f t="shared" ref="N14:P14" si="6">N11-E10*($K11-$K14)</f>
+        <v>2.9332000000000003</v>
+      </c>
+      <c r="O14" s="266">
+        <f t="shared" si="6"/>
         <v>0.83320000000000016</v>
       </c>
-      <c r="P14" s="357">
-        <f t="shared" si="5"/>
+      <c r="P14" s="266">
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="Q14" s="195">
         <f>L14/$K14</f>
-        <v>0.19135799999999997</v>
+        <v>0.21335999999999994</v>
       </c>
       <c r="R14" s="195">
-        <f t="shared" ref="R14:R16" si="6">M14/$K14</f>
+        <f t="shared" ref="R14:R16" si="7">M14/$K14</f>
         <v>3.3360000000000001E-2</v>
       </c>
       <c r="S14" s="195">
-        <f t="shared" ref="S14:S16" si="7">N14/$K14</f>
-        <v>0.60864200000000002</v>
+        <f t="shared" ref="S14:S16" si="8">N14/$K14</f>
+        <v>0.58664000000000005</v>
       </c>
       <c r="T14" s="195">
-        <f t="shared" ref="T14:T16" si="8">O14/$K14</f>
+        <f t="shared" ref="T14:T16" si="9">O14/$K14</f>
         <v>0.16664000000000004</v>
       </c>
       <c r="U14" s="196">
@@ -23765,69 +23754,69 @@
         <v>0.4</v>
       </c>
       <c r="C15" s="201">
-        <f t="shared" ref="C15:F17" si="9">C$14+C$10*($B15-$B$14)</f>
-        <v>0.28333000000000003</v>
+        <f t="shared" ref="C15:C17" si="10">$B15*C$10</f>
+        <v>0.17332000000000003</v>
       </c>
       <c r="D15" s="201">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>1.3320000000000002E-2</v>
       </c>
       <c r="E15" s="201">
-        <f t="shared" si="9"/>
-        <v>3.6670000000000015E-2</v>
+        <f t="shared" si="5"/>
+        <v>0.14668</v>
       </c>
       <c r="F15" s="201">
-        <f t="shared" si="9"/>
-        <v>6.6679999999999989E-2</v>
+        <f t="shared" si="5"/>
+        <v>6.6680000000000003E-2</v>
       </c>
       <c r="G15" s="201">
         <f>SUM(C15:F15)</f>
-        <v>0.4</v>
+        <v>0.40000000000000008</v>
       </c>
       <c r="I15" s="192" t="s">
         <v>417</v>
       </c>
-      <c r="J15" s="356">
-        <f t="shared" ref="J15:J16" si="10">9-K15</f>
+      <c r="J15" s="265">
+        <f t="shared" ref="J15:J16" si="11">9-K15</f>
         <v>4.4000000000000004</v>
       </c>
-      <c r="K15" s="356">
+      <c r="K15" s="265">
         <v>4.5999999999999996</v>
       </c>
-      <c r="L15" s="357">
+      <c r="L15" s="266">
         <f>L11-C10*($K11-$K15)</f>
-        <v>0.78346999999999967</v>
-      </c>
-      <c r="M15" s="357">
-        <f t="shared" ref="M15:P15" si="11">M11-D10*($K11-$K15)</f>
+        <v>0.89347999999999961</v>
+      </c>
+      <c r="M15" s="266">
+        <f t="shared" ref="M15:P15" si="12">M11-D10*($K11-$K15)</f>
         <v>0.15347999999999998</v>
       </c>
-      <c r="N15" s="357">
-        <f t="shared" si="11"/>
-        <v>2.8965300000000003</v>
-      </c>
-      <c r="O15" s="357">
-        <f t="shared" si="11"/>
+      <c r="N15" s="266">
+        <f t="shared" si="12"/>
+        <v>2.7865200000000003</v>
+      </c>
+      <c r="O15" s="266">
+        <f t="shared" si="12"/>
         <v>0.76652000000000009</v>
       </c>
-      <c r="P15" s="357">
-        <f t="shared" si="11"/>
+      <c r="P15" s="266">
+        <f t="shared" si="12"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="Q15" s="195">
-        <f t="shared" ref="Q14:Q16" si="12">L15/$K15</f>
-        <v>0.17031956521739125</v>
+        <f t="shared" ref="Q15:Q16" si="13">L15/$K15</f>
+        <v>0.19423478260869559</v>
       </c>
       <c r="R15" s="195">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.3365217391304346E-2</v>
       </c>
       <c r="S15" s="195">
-        <f t="shared" si="7"/>
-        <v>0.62968043478260882</v>
+        <f t="shared" si="8"/>
+        <v>0.60576521739130451</v>
       </c>
       <c r="T15" s="195">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.16663478260869569</v>
       </c>
       <c r="U15" s="196">
@@ -23840,69 +23829,69 @@
         <v>1</v>
       </c>
       <c r="C16" s="201">
-        <f t="shared" si="9"/>
-        <v>0.54330999999999996</v>
+        <f t="shared" si="10"/>
+        <v>0.43330000000000002</v>
       </c>
       <c r="D16" s="201">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>3.3300000000000003E-2</v>
       </c>
       <c r="E16" s="201">
-        <f t="shared" si="9"/>
-        <v>0.25669000000000003</v>
+        <f t="shared" si="5"/>
+        <v>0.36670000000000003</v>
       </c>
       <c r="F16" s="201">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>0.16669999999999999</v>
       </c>
       <c r="G16" s="201">
-        <f t="shared" ref="G16:G17" si="13">SUM(C16:F16)</f>
-        <v>0.99999999999999989</v>
+        <f t="shared" ref="G16:G17" si="14">SUM(C16:F16)</f>
+        <v>1</v>
       </c>
       <c r="I16" s="192" t="s">
         <v>418</v>
       </c>
-      <c r="J16" s="356">
-        <f t="shared" si="10"/>
+      <c r="J16" s="265">
+        <f t="shared" si="11"/>
         <v>5.2</v>
       </c>
-      <c r="K16" s="356">
+      <c r="K16" s="265">
         <v>3.8</v>
       </c>
-      <c r="L16" s="357">
+      <c r="L16" s="266">
         <f>L11-C10*($K11-$K16)</f>
-        <v>0.43682999999999961</v>
-      </c>
-      <c r="M16" s="357">
-        <f t="shared" ref="M16:P16" si="14">M11-D10*($K11-$K16)</f>
+        <v>0.54683999999999955</v>
+      </c>
+      <c r="M16" s="266">
+        <f t="shared" ref="M16:P16" si="15">M11-D10*($K11-$K16)</f>
         <v>0.12683999999999998</v>
       </c>
-      <c r="N16" s="357">
-        <f t="shared" si="14"/>
-        <v>2.60317</v>
-      </c>
-      <c r="O16" s="357">
-        <f t="shared" si="14"/>
+      <c r="N16" s="266">
+        <f t="shared" si="15"/>
+        <v>2.49316</v>
+      </c>
+      <c r="O16" s="266">
+        <f t="shared" si="15"/>
         <v>0.63316000000000017</v>
       </c>
-      <c r="P16" s="357">
-        <f t="shared" si="14"/>
+      <c r="P16" s="266">
+        <f t="shared" si="15"/>
         <v>3.8</v>
       </c>
       <c r="Q16" s="195">
-        <f t="shared" si="12"/>
-        <v>0.11495526315789464</v>
+        <f t="shared" si="13"/>
+        <v>0.14390526315789462</v>
       </c>
       <c r="R16" s="195">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.337894736842105E-2</v>
       </c>
       <c r="S16" s="195">
-        <f t="shared" si="7"/>
-        <v>0.68504473684210532</v>
+        <f t="shared" si="8"/>
+        <v>0.65609473684210529</v>
       </c>
       <c r="T16" s="195">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0.166621052631579</v>
       </c>
       <c r="U16" s="196">
@@ -23915,23 +23904,23 @@
         <v>1.5</v>
       </c>
       <c r="C17" s="201">
-        <f t="shared" si="9"/>
-        <v>0.75995999999999997</v>
+        <f t="shared" si="10"/>
+        <v>0.64995000000000003</v>
       </c>
       <c r="D17" s="201">
-        <f t="shared" si="9"/>
-        <v>4.9950000000000001E-2</v>
+        <f t="shared" si="5"/>
+        <v>4.9950000000000008E-2</v>
       </c>
       <c r="E17" s="201">
-        <f t="shared" si="9"/>
-        <v>0.44004000000000004</v>
+        <f t="shared" si="5"/>
+        <v>0.55005000000000004</v>
       </c>
       <c r="F17" s="201">
-        <f t="shared" si="9"/>
-        <v>0.25004999999999994</v>
+        <f t="shared" si="5"/>
+        <v>0.25004999999999999</v>
       </c>
       <c r="G17" s="201">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>1.5</v>
       </c>
       <c r="I17" s="192" t="s">
@@ -23946,7 +23935,7 @@
       </c>
       <c r="L17" s="201">
         <f>$K17*Q17</f>
-        <v>0.24128253968253963</v>
+        <v>0.25874444444444439</v>
       </c>
       <c r="M17" s="201">
         <f>$K17*R17</f>
@@ -23954,7 +23943,7 @@
       </c>
       <c r="N17" s="201">
         <f>$K17*S17</f>
-        <v>0.55871746031746028</v>
+        <v>0.5412555555555556</v>
       </c>
       <c r="O17" s="201">
         <f>$K17*T17</f>
@@ -23966,7 +23955,7 @@
       </c>
       <c r="Q17" s="195">
         <f>Q13</f>
-        <v>0.24128253968253963</v>
+        <v>0.25874444444444439</v>
       </c>
       <c r="R17" s="195">
         <f>R13</f>
@@ -23974,7 +23963,7 @@
       </c>
       <c r="S17" s="195">
         <f>S13</f>
-        <v>0.55871746031746028</v>
+        <v>0.5412555555555556</v>
       </c>
       <c r="T17" s="195">
         <f>T13</f>
@@ -23989,13 +23978,13 @@
       <c r="B18" s="198" t="s">
         <v>235</v>
       </c>
-      <c r="C18" s="335" t="s">
+      <c r="C18" s="348" t="s">
         <v>236</v>
       </c>
-      <c r="D18" s="335"/>
-      <c r="E18" s="335"/>
-      <c r="F18" s="335"/>
-      <c r="G18" s="335"/>
+      <c r="D18" s="348"/>
+      <c r="E18" s="348"/>
+      <c r="F18" s="348"/>
+      <c r="G18" s="348"/>
       <c r="I18" s="204" t="s">
         <v>420</v>
       </c>
@@ -24018,6 +24007,12 @@
       <c r="U19" s="209"/>
     </row>
     <row r="20" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="B20" s="197" t="s">
+        <v>427</v>
+      </c>
+      <c r="C20" s="197" t="s">
+        <v>426</v>
+      </c>
       <c r="I20" s="205" t="s">
         <v>422</v>
       </c>
@@ -24035,76 +24030,161 @@
       <c r="U20" s="209"/>
     </row>
     <row r="21" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="H21" s="362"/>
-      <c r="I21" s="362"/>
-      <c r="J21" s="363"/>
-      <c r="K21" s="363"/>
-      <c r="L21" s="364"/>
-      <c r="M21" s="364"/>
-      <c r="N21" s="364"/>
-      <c r="O21" s="364"/>
-      <c r="P21" s="364"/>
-      <c r="Q21" s="365"/>
-      <c r="R21" s="365"/>
-      <c r="S21" s="365"/>
-      <c r="T21" s="365"/>
-      <c r="U21" s="366"/>
-      <c r="V21" s="362"/>
-      <c r="W21" s="362"/>
+      <c r="B21" s="370">
+        <f>G21-B13</f>
+        <v>9</v>
+      </c>
+      <c r="C21" s="194">
+        <v>2.8</v>
+      </c>
+      <c r="D21" s="194">
+        <v>0.3</v>
+      </c>
+      <c r="E21" s="194">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="F21" s="194">
+        <v>1.5</v>
+      </c>
+      <c r="G21" s="194">
+        <f>SUM(C21:F21)</f>
+        <v>9</v>
+      </c>
+      <c r="J21" s="206"/>
+      <c r="K21" s="206"/>
+      <c r="L21" s="207"/>
+      <c r="M21" s="207"/>
+      <c r="N21" s="207"/>
+      <c r="O21" s="207"/>
+      <c r="P21" s="207"/>
+      <c r="Q21" s="267"/>
+      <c r="R21" s="267"/>
+      <c r="S21" s="267"/>
+      <c r="T21" s="267"/>
+      <c r="U21" s="268"/>
     </row>
     <row r="22" spans="2:23" s="197" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H22" s="362"/>
-      <c r="I22" s="358" t="s">
+      <c r="B22" s="370">
+        <f>B21-B15</f>
+        <v>8.6</v>
+      </c>
+      <c r="C22" s="371">
+        <f>C$21-C15</f>
+        <v>2.6266799999999999</v>
+      </c>
+      <c r="D22" s="371">
+        <f t="shared" ref="D22:G22" si="16">D$21-D15</f>
+        <v>0.28667999999999999</v>
+      </c>
+      <c r="E22" s="371">
+        <f t="shared" si="16"/>
+        <v>4.2533200000000004</v>
+      </c>
+      <c r="F22" s="371">
+        <f t="shared" si="16"/>
+        <v>1.4333199999999999</v>
+      </c>
+      <c r="G22" s="371">
+        <f t="shared" si="16"/>
+        <v>8.6</v>
+      </c>
+      <c r="I22" s="345" t="s">
         <v>425</v>
       </c>
-      <c r="J22" s="358"/>
-      <c r="K22" s="358"/>
-      <c r="L22" s="358"/>
-      <c r="M22" s="358"/>
-      <c r="N22" s="358"/>
-      <c r="O22" s="358"/>
-      <c r="P22" s="358"/>
-      <c r="Q22" s="358"/>
-      <c r="R22" s="358"/>
-      <c r="S22" s="358"/>
-      <c r="T22" s="358"/>
-      <c r="U22" s="358"/>
-      <c r="V22" s="358"/>
-      <c r="W22" s="358"/>
+      <c r="J22" s="345"/>
+      <c r="K22" s="345"/>
+      <c r="L22" s="345"/>
+      <c r="M22" s="345"/>
+      <c r="N22" s="345"/>
+      <c r="O22" s="345"/>
+      <c r="P22" s="345"/>
+      <c r="Q22" s="345"/>
+      <c r="R22" s="345"/>
+      <c r="S22" s="345"/>
+      <c r="T22" s="345"/>
+      <c r="U22" s="345"/>
+      <c r="V22" s="345"/>
+      <c r="W22" s="345"/>
     </row>
     <row r="23" spans="2:23" s="197" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H23" s="362"/>
-      <c r="I23" s="373" t="s">
+      <c r="B23" s="370">
+        <f>B21-B16</f>
+        <v>8</v>
+      </c>
+      <c r="C23" s="371">
+        <f t="shared" ref="C23:G24" si="17">C$21-C16</f>
+        <v>2.3666999999999998</v>
+      </c>
+      <c r="D23" s="371">
+        <f t="shared" si="17"/>
+        <v>0.26669999999999999</v>
+      </c>
+      <c r="E23" s="371">
+        <f t="shared" si="17"/>
+        <v>4.0333000000000006</v>
+      </c>
+      <c r="F23" s="371">
+        <f t="shared" si="17"/>
+        <v>1.3332999999999999</v>
+      </c>
+      <c r="G23" s="371">
+        <f t="shared" si="17"/>
+        <v>8</v>
+      </c>
+      <c r="I23" s="347" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="373" t="s">
+      <c r="J23" s="347" t="s">
         <v>214</v>
       </c>
-      <c r="K23" s="373" t="s">
+      <c r="K23" s="347" t="s">
         <v>215</v>
       </c>
-      <c r="L23" s="374" t="s">
+      <c r="L23" s="346" t="s">
         <v>216</v>
       </c>
-      <c r="M23" s="374"/>
-      <c r="N23" s="374"/>
-      <c r="O23" s="374"/>
-      <c r="P23" s="374"/>
-      <c r="Q23" s="374"/>
-      <c r="R23" s="359" t="s">
+      <c r="M23" s="346"/>
+      <c r="N23" s="346"/>
+      <c r="O23" s="346"/>
+      <c r="P23" s="346"/>
+      <c r="Q23" s="346"/>
+      <c r="R23" s="343" t="s">
         <v>217</v>
       </c>
-      <c r="S23" s="359"/>
-      <c r="T23" s="359"/>
-      <c r="U23" s="359"/>
-      <c r="V23" s="359"/>
-      <c r="W23" s="359"/>
+      <c r="S23" s="343"/>
+      <c r="T23" s="343"/>
+      <c r="U23" s="343"/>
+      <c r="V23" s="343"/>
+      <c r="W23" s="343"/>
     </row>
     <row r="24" spans="2:23" s="197" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="H24" s="362"/>
-      <c r="I24" s="373"/>
-      <c r="J24" s="373"/>
-      <c r="K24" s="373"/>
+      <c r="B24" s="370">
+        <f>B21-B17</f>
+        <v>7.5</v>
+      </c>
+      <c r="C24" s="371">
+        <f t="shared" si="17"/>
+        <v>2.1500499999999998</v>
+      </c>
+      <c r="D24" s="371">
+        <f t="shared" si="17"/>
+        <v>0.25004999999999999</v>
+      </c>
+      <c r="E24" s="371">
+        <f t="shared" si="17"/>
+        <v>3.8499500000000002</v>
+      </c>
+      <c r="F24" s="371">
+        <f t="shared" si="17"/>
+        <v>1.2499500000000001</v>
+      </c>
+      <c r="G24" s="371">
+        <f t="shared" si="17"/>
+        <v>7.5</v>
+      </c>
+      <c r="I24" s="347"/>
+      <c r="J24" s="347"/>
+      <c r="K24" s="347"/>
       <c r="L24" s="190" t="s">
         <v>219</v>
       </c>
@@ -24143,634 +24223,681 @@
       </c>
     </row>
     <row r="25" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="H25" s="362"/>
-      <c r="I25" s="360" t="s">
+      <c r="I25" s="265" t="s">
         <v>414</v>
       </c>
-      <c r="J25" s="360">
+      <c r="J25" s="265">
         <v>0</v>
       </c>
-      <c r="K25" s="370">
+      <c r="K25" s="269">
         <v>9</v>
       </c>
-      <c r="L25" s="361">
+      <c r="L25" s="266">
         <f>L7-(0.824*L7)</f>
         <v>0.4927999999999999</v>
       </c>
-      <c r="M25" s="361">
+      <c r="M25" s="266">
         <v>0.3</v>
       </c>
-      <c r="N25" s="361">
+      <c r="N25" s="266">
         <f>N7-(N7*0.164)</f>
         <v>3.6784000000000003</v>
       </c>
-      <c r="O25" s="361">
+      <c r="O25" s="266">
         <v>1.5</v>
       </c>
       <c r="P25" s="201">
         <f>(0.164*N7)+(0.824*L7)</f>
         <v>3.0287999999999999</v>
       </c>
-      <c r="Q25" s="361">
+      <c r="Q25" s="266">
         <f>SUM(L25:P25)</f>
         <v>9</v>
       </c>
-      <c r="R25" s="371">
+      <c r="R25" s="270">
         <f>L25/K25</f>
         <v>5.4755555555555543E-2</v>
       </c>
-      <c r="S25" s="371">
+      <c r="S25" s="270">
         <v>3.3333333333333333E-2</v>
       </c>
-      <c r="T25" s="371">
+      <c r="T25" s="270">
         <f>N25/K25</f>
         <v>0.40871111111111114</v>
       </c>
-      <c r="U25" s="371">
+      <c r="U25" s="270">
         <v>0.16666666666666666</v>
       </c>
-      <c r="V25" s="375">
+      <c r="V25" s="271">
         <f>P25/K25</f>
         <v>0.33653333333333335</v>
       </c>
-      <c r="W25" s="377">
+      <c r="W25" s="272">
         <f>SUM(R25:V25)</f>
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="H26" s="362"/>
-      <c r="I26" s="360" t="s">
+      <c r="C26" s="372"/>
+      <c r="D26" s="372"/>
+      <c r="E26" s="372"/>
+      <c r="F26" s="372"/>
+      <c r="G26" s="372"/>
+      <c r="I26" s="265" t="s">
         <v>230</v>
       </c>
-      <c r="J26" s="360">
+      <c r="J26" s="265">
         <v>0.3</v>
       </c>
-      <c r="K26" s="370">
+      <c r="K26" s="269">
         <v>8.6999999999999993</v>
       </c>
-      <c r="L26" s="361">
-        <f t="shared" ref="L26:L29" si="15">L8-(0.824*L8)</f>
-        <v>0.45055999999999985</v>
-      </c>
-      <c r="M26" s="361">
+      <c r="L26" s="266">
+        <f t="shared" ref="L26:L29" si="18">L8-(0.824*L8)</f>
+        <v>0.46992176000000008</v>
+      </c>
+      <c r="M26" s="266">
         <v>0.29000999999999999</v>
       </c>
-      <c r="N26" s="361">
+      <c r="N26" s="266">
         <f>N8-(N8*0.164)</f>
-        <v>3.6784000000000003</v>
-      </c>
-      <c r="O26" s="361">
+        <v>3.5864316400000003</v>
+      </c>
+      <c r="O26" s="266">
         <v>1.4499900000000001</v>
       </c>
       <c r="P26" s="201">
         <f>(0.164*N8)+(0.824*L8)</f>
-        <v>2.8310399999999998</v>
-      </c>
-      <c r="Q26" s="361">
-        <f t="shared" ref="Q26:Q28" si="16">SUM(L26:P26)</f>
-        <v>8.6999999999999993</v>
-      </c>
-      <c r="R26" s="371">
-        <f t="shared" ref="R26:R29" si="17">L26/K26</f>
-        <v>5.1788505747126422E-2</v>
-      </c>
-      <c r="S26" s="371">
+        <v>2.9036466000000001</v>
+      </c>
+      <c r="Q26" s="266">
+        <f t="shared" ref="Q26:Q28" si="19">SUM(L26:P26)</f>
+        <v>8.7000000000000011</v>
+      </c>
+      <c r="R26" s="270">
+        <f t="shared" ref="R26:R29" si="20">L26/K26</f>
+        <v>5.4013995402298863E-2</v>
+      </c>
+      <c r="S26" s="270">
         <v>3.3334482758620693E-2</v>
       </c>
-      <c r="T26" s="371">
-        <f t="shared" ref="T26:T29" si="18">N26/K26</f>
-        <v>0.42280459770114948</v>
-      </c>
-      <c r="U26" s="371">
+      <c r="T26" s="270">
+        <f t="shared" ref="T26:T29" si="21">N26/K26</f>
+        <v>0.41223352183908052</v>
+      </c>
+      <c r="U26" s="270">
         <v>0.16666551724137935</v>
       </c>
-      <c r="V26" s="375">
-        <f t="shared" ref="V26:V29" si="19">P26/K26</f>
-        <v>0.32540689655172411</v>
-      </c>
-      <c r="W26" s="377">
-        <f t="shared" ref="W26:W29" si="20">SUM(R26:V26)</f>
+      <c r="V26" s="271">
+        <f t="shared" ref="V26:V29" si="22">P26/K26</f>
+        <v>0.33375248275862074</v>
+      </c>
+      <c r="W26" s="272">
+        <f t="shared" ref="W26:W29" si="23">SUM(R26:V26)</f>
+        <v>1.0000000000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="C27" s="372"/>
+      <c r="D27" s="372"/>
+      <c r="E27" s="372"/>
+      <c r="F27" s="372"/>
+      <c r="G27" s="372"/>
+      <c r="I27" s="265" t="s">
+        <v>232</v>
+      </c>
+      <c r="J27" s="265">
+        <v>0.4</v>
+      </c>
+      <c r="K27" s="269">
+        <v>8.6</v>
+      </c>
+      <c r="L27" s="266">
+        <f t="shared" si="18"/>
+        <v>0.46229567999999999</v>
+      </c>
+      <c r="M27" s="266">
+        <v>0.28667999999999999</v>
+      </c>
+      <c r="N27" s="266">
+        <f t="shared" ref="N27:N29" si="24">N9-(N9*0.164)</f>
+        <v>3.5557755200000001</v>
+      </c>
+      <c r="O27" s="266">
+        <v>1.4333199999999999</v>
+      </c>
+      <c r="P27" s="201">
+        <f t="shared" ref="P27:P29" si="25">(0.164*N9)+(0.824*L9)</f>
+        <v>2.8619288000000003</v>
+      </c>
+      <c r="Q27" s="266">
+        <f t="shared" si="19"/>
+        <v>8.6000000000000014</v>
+      </c>
+      <c r="R27" s="270">
+        <f t="shared" si="20"/>
+        <v>5.3755311627906976E-2</v>
+      </c>
+      <c r="S27" s="270">
+        <v>3.3334883720930235E-2</v>
+      </c>
+      <c r="T27" s="270">
+        <f t="shared" si="21"/>
+        <v>0.41346226976744188</v>
+      </c>
+      <c r="U27" s="270">
+        <v>0.16666511627906977</v>
+      </c>
+      <c r="V27" s="271">
+        <f t="shared" si="22"/>
+        <v>0.33278241860465119</v>
+      </c>
+      <c r="W27" s="272">
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="H27" s="362"/>
-      <c r="I27" s="360" t="s">
-        <v>232</v>
-      </c>
-      <c r="J27" s="360">
-        <v>0.4</v>
-      </c>
-      <c r="K27" s="370">
+    <row r="28" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="I28" s="265" t="s">
+        <v>234</v>
+      </c>
+      <c r="J28" s="265">
+        <v>1</v>
+      </c>
+      <c r="K28" s="269">
+        <v>8</v>
+      </c>
+      <c r="L28" s="266">
+        <f t="shared" si="18"/>
+        <v>0.41653920000000011</v>
+      </c>
+      <c r="M28" s="266">
+        <v>0.26669999999999999</v>
+      </c>
+      <c r="N28" s="266">
+        <f t="shared" si="24"/>
+        <v>3.3718388000000004</v>
+      </c>
+      <c r="O28" s="266">
+        <v>1.3332999999999999</v>
+      </c>
+      <c r="P28" s="201">
+        <f t="shared" si="25"/>
+        <v>2.6116219999999997</v>
+      </c>
+      <c r="Q28" s="266">
+        <f t="shared" si="19"/>
+        <v>7.9999999999999991</v>
+      </c>
+      <c r="R28" s="270">
+        <f t="shared" si="20"/>
+        <v>5.2067400000000014E-2</v>
+      </c>
+      <c r="S28" s="270">
+        <v>3.3337499999999999E-2</v>
+      </c>
+      <c r="T28" s="270">
+        <f t="shared" si="21"/>
+        <v>0.42147985000000004</v>
+      </c>
+      <c r="U28" s="270">
+        <v>0.16666249999999999</v>
+      </c>
+      <c r="V28" s="271">
+        <f t="shared" si="22"/>
+        <v>0.32645274999999996</v>
+      </c>
+      <c r="W28" s="272">
+        <f t="shared" si="23"/>
+        <v>0.99999999999999989</v>
+      </c>
+    </row>
+    <row r="29" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="B29" s="197">
+        <v>9</v>
+      </c>
+      <c r="C29" s="372">
+        <f>C21/$B$21</f>
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="D29" s="372">
+        <f t="shared" ref="D29:G29" si="26">D21/$B$21</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="E29" s="372">
+        <f t="shared" si="26"/>
+        <v>0.48888888888888893</v>
+      </c>
+      <c r="F29" s="372">
+        <f t="shared" si="26"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="G29" s="372">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+      <c r="I29" s="265" t="s">
+        <v>237</v>
+      </c>
+      <c r="J29" s="265">
+        <v>1.5</v>
+      </c>
+      <c r="K29" s="269">
+        <v>7.5</v>
+      </c>
+      <c r="L29" s="266">
+        <f t="shared" si="18"/>
+        <v>0.3784088000000001</v>
+      </c>
+      <c r="M29" s="266">
+        <v>0.25004999999999999</v>
+      </c>
+      <c r="N29" s="266">
+        <f t="shared" si="24"/>
+        <v>3.2185582000000004</v>
+      </c>
+      <c r="O29" s="266">
+        <v>1.2499500000000001</v>
+      </c>
+      <c r="P29" s="201">
+        <f t="shared" si="25"/>
+        <v>2.4030329999999998</v>
+      </c>
+      <c r="Q29" s="266">
+        <f>SUM(L29:P29)</f>
+        <v>7.5000000000000009</v>
+      </c>
+      <c r="R29" s="270">
+        <f t="shared" si="20"/>
+        <v>5.0454506666666683E-2</v>
+      </c>
+      <c r="S29" s="270">
+        <v>3.3340000000000002E-2</v>
+      </c>
+      <c r="T29" s="270">
+        <f t="shared" si="21"/>
+        <v>0.42914109333333339</v>
+      </c>
+      <c r="U29" s="270">
+        <v>0.16666</v>
+      </c>
+      <c r="V29" s="271">
+        <f t="shared" si="22"/>
+        <v>0.32040439999999998</v>
+      </c>
+      <c r="W29" s="272">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="B30" s="197">
         <v>8.6</v>
       </c>
-      <c r="L27" s="361">
-        <f t="shared" si="15"/>
-        <v>0.4429339200000002</v>
-      </c>
-      <c r="M27" s="361">
-        <v>0.28667999999999999</v>
-      </c>
-      <c r="N27" s="361">
-        <f t="shared" ref="N26:N29" si="21">N9-(N9*0.164)</f>
-        <v>3.6477438800000002</v>
-      </c>
-      <c r="O27" s="361">
-        <v>1.4333199999999999</v>
-      </c>
-      <c r="P27" s="201">
-        <f t="shared" ref="P26:P29" si="22">(0.164*N9)+(0.824*L9)</f>
-        <v>2.7893222</v>
-      </c>
-      <c r="Q27" s="361">
-        <f t="shared" si="16"/>
-        <v>8.6000000000000014</v>
-      </c>
-      <c r="R27" s="371">
-        <f t="shared" si="17"/>
-        <v>5.1503944186046535E-2</v>
-      </c>
-      <c r="S27" s="371">
+      <c r="C30" s="372">
+        <f>C22/$B$22</f>
+        <v>0.30542790697674421</v>
+      </c>
+      <c r="D30" s="372">
+        <f t="shared" ref="D30:G30" si="27">D22/$B$22</f>
         <v>3.3334883720930235E-2</v>
       </c>
-      <c r="T27" s="371">
-        <f t="shared" si="18"/>
-        <v>0.42415626511627913</v>
-      </c>
-      <c r="U27" s="371">
+      <c r="E30" s="372">
+        <f t="shared" si="27"/>
+        <v>0.49457209302325589</v>
+      </c>
+      <c r="F30" s="372">
+        <f t="shared" si="27"/>
         <v>0.16666511627906977</v>
       </c>
-      <c r="V27" s="375">
-        <f t="shared" si="19"/>
-        <v>0.32433979069767443</v>
-      </c>
-      <c r="W27" s="377">
-        <f t="shared" si="20"/>
+      <c r="G30" s="372">
+        <f t="shared" si="27"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="H28" s="362"/>
-      <c r="I28" s="360" t="s">
-        <v>234</v>
-      </c>
-      <c r="J28" s="360">
+      <c r="I30" s="265" t="s">
+        <v>239</v>
+      </c>
+      <c r="J30" s="265" t="s">
+        <v>235</v>
+      </c>
+      <c r="K30" s="265" t="s">
+        <v>240</v>
+      </c>
+      <c r="L30" s="344" t="s">
+        <v>236</v>
+      </c>
+      <c r="M30" s="344"/>
+      <c r="N30" s="344"/>
+      <c r="O30" s="344"/>
+      <c r="P30" s="344"/>
+      <c r="Q30" s="344"/>
+      <c r="R30" s="344" t="s">
+        <v>236</v>
+      </c>
+      <c r="S30" s="344"/>
+      <c r="T30" s="344"/>
+      <c r="U30" s="344"/>
+      <c r="V30" s="344"/>
+      <c r="W30" s="344"/>
+    </row>
+    <row r="31" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+      <c r="B31" s="197">
+        <v>8</v>
+      </c>
+      <c r="C31" s="372">
+        <f>C23/$B$23</f>
+        <v>0.29583749999999998</v>
+      </c>
+      <c r="D31" s="372">
+        <f>D23/$B$23</f>
+        <v>3.3337499999999999E-2</v>
+      </c>
+      <c r="E31" s="372">
+        <f t="shared" ref="E31:G31" si="28">E23/$B$23</f>
+        <v>0.50416250000000007</v>
+      </c>
+      <c r="F31" s="372">
+        <f t="shared" si="28"/>
+        <v>0.16666249999999999</v>
+      </c>
+      <c r="G31" s="372">
+        <f t="shared" si="28"/>
         <v>1</v>
       </c>
-      <c r="K28" s="370">
-        <v>8</v>
-      </c>
-      <c r="L28" s="361">
-        <f t="shared" si="15"/>
-        <v>0.3971774400000001</v>
-      </c>
-      <c r="M28" s="361">
-        <v>0.26669999999999999</v>
-      </c>
-      <c r="N28" s="361">
-        <f t="shared" si="21"/>
-        <v>3.4638071600000004</v>
-      </c>
-      <c r="O28" s="361">
-        <v>1.3332999999999999</v>
-      </c>
-      <c r="P28" s="201">
-        <f t="shared" si="22"/>
-        <v>2.5390153999999998</v>
-      </c>
-      <c r="Q28" s="361">
-        <f t="shared" si="16"/>
-        <v>8</v>
-      </c>
-      <c r="R28" s="371">
-        <f t="shared" si="17"/>
-        <v>4.9647180000000013E-2</v>
-      </c>
-      <c r="S28" s="371">
-        <v>3.3337499999999999E-2</v>
-      </c>
-      <c r="T28" s="371">
-        <f t="shared" si="18"/>
-        <v>0.43297589500000006</v>
-      </c>
-      <c r="U28" s="371">
-        <v>0.16666249999999999</v>
-      </c>
-      <c r="V28" s="375">
-        <f t="shared" si="19"/>
-        <v>0.31737692499999998</v>
-      </c>
-      <c r="W28" s="377">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="H29" s="362"/>
-      <c r="I29" s="360" t="s">
-        <v>237</v>
-      </c>
-      <c r="J29" s="360">
-        <v>1.5</v>
-      </c>
-      <c r="K29" s="370">
-        <v>7.5</v>
-      </c>
-      <c r="L29" s="361">
-        <f t="shared" si="15"/>
-        <v>0.3590470400000001</v>
-      </c>
-      <c r="M29" s="361">
-        <v>0.25004999999999999</v>
-      </c>
-      <c r="N29" s="361">
-        <f t="shared" si="21"/>
-        <v>3.31052656</v>
-      </c>
-      <c r="O29" s="361">
-        <v>1.2499500000000001</v>
-      </c>
-      <c r="P29" s="201">
-        <f t="shared" si="22"/>
-        <v>2.3304263999999999</v>
-      </c>
-      <c r="Q29" s="361">
-        <f>SUM(L29:P29)</f>
-        <v>7.5</v>
-      </c>
-      <c r="R29" s="371">
-        <f t="shared" si="17"/>
-        <v>4.7872938666666677E-2</v>
-      </c>
-      <c r="S29" s="371">
-        <v>3.3340000000000002E-2</v>
-      </c>
-      <c r="T29" s="371">
-        <f t="shared" si="18"/>
-        <v>0.44140354133333332</v>
-      </c>
-      <c r="U29" s="371">
-        <v>0.16666</v>
-      </c>
-      <c r="V29" s="375">
-        <f t="shared" si="19"/>
-        <v>0.31072351999999998</v>
-      </c>
-      <c r="W29" s="377">
-        <f t="shared" si="20"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="H30" s="362"/>
-      <c r="I30" s="360" t="s">
-        <v>239</v>
-      </c>
-      <c r="J30" s="360" t="s">
-        <v>235</v>
-      </c>
-      <c r="K30" s="360" t="s">
-        <v>240</v>
-      </c>
-      <c r="L30" s="372" t="s">
-        <v>236</v>
-      </c>
-      <c r="M30" s="372"/>
-      <c r="N30" s="372"/>
-      <c r="O30" s="372"/>
-      <c r="P30" s="372"/>
-      <c r="Q30" s="372"/>
-      <c r="R30" s="372" t="s">
-        <v>236</v>
-      </c>
-      <c r="S30" s="372"/>
-      <c r="T30" s="372"/>
-      <c r="U30" s="372"/>
-      <c r="V30" s="372"/>
-      <c r="W30" s="372"/>
-    </row>
-    <row r="31" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="H31" s="362"/>
-      <c r="I31" s="360" t="s">
+      <c r="I31" s="265" t="s">
         <v>415</v>
       </c>
-      <c r="J31" s="360">
+      <c r="J31" s="265">
         <v>2.7</v>
       </c>
-      <c r="K31" s="370">
+      <c r="K31" s="269">
         <v>6.3</v>
       </c>
-      <c r="L31" s="361">
+      <c r="L31" s="266">
         <f>L13-(L13*0.824)</f>
-        <v>0.26753408000000012</v>
-      </c>
-      <c r="M31" s="361">
+        <v>0.2868958399999999</v>
+      </c>
+      <c r="M31" s="266">
         <v>0.21009</v>
       </c>
-      <c r="N31" s="361">
+      <c r="N31" s="266">
         <f>N13-(N13*0.164)</f>
-        <v>2.9426531200000001</v>
-      </c>
-      <c r="O31" s="361">
+        <v>2.85068476</v>
+      </c>
+      <c r="O31" s="266">
         <v>1.0499100000000001</v>
       </c>
       <c r="P31" s="201">
         <f>(N13*0.164)+(L13*0.824)</f>
-        <v>1.8298127999999996</v>
-      </c>
-      <c r="Q31" s="361">
+        <v>1.9024193999999999</v>
+      </c>
+      <c r="Q31" s="266">
         <v>6.3</v>
       </c>
-      <c r="R31" s="371">
+      <c r="R31" s="270">
         <f>L31/K31</f>
-        <v>4.2465726984127004E-2</v>
-      </c>
-      <c r="S31" s="371">
+        <v>4.5539022222222211E-2</v>
+      </c>
+      <c r="S31" s="270">
         <v>3.334761904761905E-2</v>
       </c>
-      <c r="T31" s="371">
+      <c r="T31" s="270">
         <f>N31/K31</f>
-        <v>0.46708779682539686</v>
-      </c>
-      <c r="U31" s="371">
+        <v>0.45248964444444445</v>
+      </c>
+      <c r="U31" s="270">
         <v>0.16665238095238097</v>
       </c>
-      <c r="V31" s="375">
+      <c r="V31" s="271">
         <f>P31/K31</f>
-        <v>0.29044647619047614</v>
-      </c>
-      <c r="W31" s="377">
+        <v>0.30197133333333331</v>
+      </c>
+      <c r="W31" s="272">
         <f>SUM(R31:V31)</f>
         <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="H32" s="362"/>
-      <c r="I32" s="360" t="s">
-        <v>416</v>
-      </c>
-      <c r="J32" s="360">
-        <v>4</v>
-      </c>
-      <c r="K32" s="370">
-        <v>5</v>
-      </c>
-      <c r="L32" s="361">
-        <f t="shared" ref="L32:L35" si="23">L14-(L14*0.824)</f>
-        <v>0.16839504000000005</v>
-      </c>
-      <c r="M32" s="361">
-        <v>0.1668</v>
-      </c>
-      <c r="N32" s="361">
-        <f t="shared" ref="N32:N35" si="24">N14-(N14*0.164)</f>
-        <v>2.5441235600000001</v>
-      </c>
-      <c r="O32" s="361">
-        <v>0.83320000000000016</v>
-      </c>
-      <c r="P32" s="201">
-        <f t="shared" ref="P32:P35" si="25">(N14*0.164)+(L14*0.824)</f>
-        <v>1.2874813999999999</v>
-      </c>
-      <c r="Q32" s="361">
-        <v>5</v>
-      </c>
-      <c r="R32" s="371">
-        <f t="shared" ref="R32:R35" si="26">L32/K32</f>
-        <v>3.367900800000001E-2</v>
-      </c>
-      <c r="S32" s="371">
-        <v>3.3360000000000001E-2</v>
-      </c>
-      <c r="T32" s="371">
-        <f t="shared" ref="T32:T35" si="27">N32/K32</f>
-        <v>0.50882471200000001</v>
-      </c>
-      <c r="U32" s="371">
-        <v>0.16664000000000004</v>
-      </c>
-      <c r="V32" s="375">
-        <f t="shared" ref="V32:V35" si="28">P32/K32</f>
-        <v>0.25749627999999997</v>
-      </c>
-      <c r="W32" s="377">
-        <f t="shared" ref="W32:W35" si="29">SUM(R32:V32)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="H33" s="367"/>
-      <c r="I33" s="360" t="s">
-        <v>417</v>
-      </c>
-      <c r="J33" s="360">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="K33" s="370">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="L33" s="361">
-        <f t="shared" si="23"/>
-        <v>0.13789072000000002</v>
-      </c>
-      <c r="M33" s="361">
-        <v>0.15347999999999998</v>
-      </c>
-      <c r="N33" s="361">
-        <f t="shared" si="24"/>
-        <v>2.4214990800000002</v>
-      </c>
-      <c r="O33" s="361">
-        <v>0.76652000000000009</v>
-      </c>
-      <c r="P33" s="201">
-        <f t="shared" si="25"/>
-        <v>1.1206101999999998</v>
-      </c>
-      <c r="Q33" s="361">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="R33" s="371">
-        <f t="shared" si="26"/>
-        <v>2.9976243478260875E-2</v>
-      </c>
-      <c r="S33" s="371">
-        <v>3.3365217391304346E-2</v>
-      </c>
-      <c r="T33" s="371">
-        <f t="shared" si="27"/>
-        <v>0.52641284347826101</v>
-      </c>
-      <c r="U33" s="371">
-        <v>0.16663478260869569</v>
-      </c>
-      <c r="V33" s="375">
-        <f t="shared" si="28"/>
-        <v>0.24361091304347823</v>
-      </c>
-      <c r="W33" s="377">
+      <c r="B32" s="197">
+        <v>7.5</v>
+      </c>
+      <c r="C32" s="372">
+        <f>C24/$B$24</f>
+        <v>0.28667333333333328</v>
+      </c>
+      <c r="D32" s="372">
+        <f t="shared" ref="D32:G32" si="29">D24/$B$24</f>
+        <v>3.3340000000000002E-2</v>
+      </c>
+      <c r="E32" s="372">
+        <f t="shared" si="29"/>
+        <v>0.51332666666666671</v>
+      </c>
+      <c r="F32" s="372">
+        <f t="shared" si="29"/>
+        <v>0.16666</v>
+      </c>
+      <c r="G32" s="372">
         <f t="shared" si="29"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="H34" s="367"/>
-      <c r="I34" s="360" t="s">
+      <c r="I32" s="265" t="s">
+        <v>416</v>
+      </c>
+      <c r="J32" s="265">
+        <v>4</v>
+      </c>
+      <c r="K32" s="269">
+        <v>5</v>
+      </c>
+      <c r="L32" s="266">
+        <f t="shared" ref="L32:L35" si="30">L14-(L14*0.824)</f>
+        <v>0.18775680000000006</v>
+      </c>
+      <c r="M32" s="266">
+        <v>0.1668</v>
+      </c>
+      <c r="N32" s="266">
+        <f t="shared" ref="N32:N35" si="31">N14-(N14*0.164)</f>
+        <v>2.4521552</v>
+      </c>
+      <c r="O32" s="266">
+        <v>0.83320000000000016</v>
+      </c>
+      <c r="P32" s="201">
+        <f t="shared" ref="P32:P35" si="32">(N14*0.164)+(L14*0.824)</f>
+        <v>1.3600879999999997</v>
+      </c>
+      <c r="Q32" s="266">
+        <v>5</v>
+      </c>
+      <c r="R32" s="270">
+        <f t="shared" ref="R32:R35" si="33">L32/K32</f>
+        <v>3.7551360000000013E-2</v>
+      </c>
+      <c r="S32" s="270">
+        <v>3.3360000000000001E-2</v>
+      </c>
+      <c r="T32" s="270">
+        <f t="shared" ref="T32:T35" si="34">N32/K32</f>
+        <v>0.49043103999999998</v>
+      </c>
+      <c r="U32" s="270">
+        <v>0.16664000000000004</v>
+      </c>
+      <c r="V32" s="271">
+        <f t="shared" ref="V32:V35" si="35">P32/K32</f>
+        <v>0.27201759999999997</v>
+      </c>
+      <c r="W32" s="272">
+        <f t="shared" ref="W32:W35" si="36">SUM(R32:V32)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="9:23" x14ac:dyDescent="0.2">
+      <c r="I33" s="265" t="s">
+        <v>417</v>
+      </c>
+      <c r="J33" s="265">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K33" s="269">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L33" s="266">
+        <f t="shared" si="30"/>
+        <v>0.15725247999999992</v>
+      </c>
+      <c r="M33" s="266">
+        <v>0.15347999999999998</v>
+      </c>
+      <c r="N33" s="266">
+        <f t="shared" si="31"/>
+        <v>2.3295307200000002</v>
+      </c>
+      <c r="O33" s="266">
+        <v>0.76652000000000009</v>
+      </c>
+      <c r="P33" s="201">
+        <f t="shared" si="32"/>
+        <v>1.1932167999999996</v>
+      </c>
+      <c r="Q33" s="266">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R33" s="270">
+        <f t="shared" si="33"/>
+        <v>3.4185321739130421E-2</v>
+      </c>
+      <c r="S33" s="270">
+        <v>3.3365217391304346E-2</v>
+      </c>
+      <c r="T33" s="270">
+        <f t="shared" si="34"/>
+        <v>0.50641972173913052</v>
+      </c>
+      <c r="U33" s="270">
+        <v>0.16663478260869569</v>
+      </c>
+      <c r="V33" s="271">
+        <f t="shared" si="35"/>
+        <v>0.25939495652173905</v>
+      </c>
+      <c r="W33" s="272">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="9:23" x14ac:dyDescent="0.2">
+      <c r="I34" s="265" t="s">
         <v>418</v>
       </c>
-      <c r="J34" s="360">
+      <c r="J34" s="265">
         <v>5.2</v>
       </c>
-      <c r="K34" s="370">
+      <c r="K34" s="269">
         <v>3.8</v>
       </c>
-      <c r="L34" s="361">
-        <f t="shared" si="23"/>
-        <v>7.6882079999999964E-2</v>
-      </c>
-      <c r="M34" s="361">
+      <c r="L34" s="266">
+        <f t="shared" si="30"/>
+        <v>9.6243839999999969E-2</v>
+      </c>
+      <c r="M34" s="266">
         <v>0.12683999999999998</v>
       </c>
-      <c r="N34" s="361">
-        <f t="shared" si="24"/>
-        <v>2.1762501199999997</v>
-      </c>
-      <c r="O34" s="361">
+      <c r="N34" s="266">
+        <f t="shared" si="31"/>
+        <v>2.0842817600000001</v>
+      </c>
+      <c r="O34" s="266">
         <v>0.63316000000000017</v>
       </c>
       <c r="P34" s="201">
-        <f t="shared" si="25"/>
-        <v>0.78686779999999967</v>
-      </c>
-      <c r="Q34" s="361">
+        <f t="shared" si="32"/>
+        <v>0.85947439999999964</v>
+      </c>
+      <c r="Q34" s="266">
         <v>3.8</v>
       </c>
-      <c r="R34" s="371">
-        <f t="shared" si="26"/>
-        <v>2.0232126315789464E-2</v>
-      </c>
-      <c r="S34" s="371">
+      <c r="R34" s="270">
+        <f t="shared" si="33"/>
+        <v>2.5327326315789468E-2</v>
+      </c>
+      <c r="S34" s="270">
         <v>3.337894736842105E-2</v>
       </c>
-      <c r="T34" s="371">
-        <f t="shared" si="27"/>
-        <v>0.57269739999999991</v>
-      </c>
-      <c r="U34" s="371">
+      <c r="T34" s="270">
+        <f t="shared" si="34"/>
+        <v>0.54849520000000007</v>
+      </c>
+      <c r="U34" s="270">
         <v>0.166621052631579</v>
       </c>
-      <c r="V34" s="375">
-        <f t="shared" si="28"/>
-        <v>0.20707047368421044</v>
-      </c>
-      <c r="W34" s="377">
-        <f t="shared" si="29"/>
-        <v>0.99999999999999978</v>
-      </c>
-    </row>
-    <row r="35" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="H35" s="367"/>
-      <c r="I35" s="360" t="s">
+      <c r="V34" s="271">
+        <f t="shared" si="35"/>
+        <v>0.22617747368421043</v>
+      </c>
+      <c r="W34" s="272">
+        <f t="shared" si="36"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="9:23" x14ac:dyDescent="0.2">
+      <c r="I35" s="265" t="s">
         <v>419</v>
       </c>
-      <c r="J35" s="360">
+      <c r="J35" s="265">
         <v>8</v>
       </c>
-      <c r="K35" s="370">
+      <c r="K35" s="269">
         <v>1</v>
       </c>
-      <c r="L35" s="361">
-        <f t="shared" si="23"/>
-        <v>4.2465726984126984E-2</v>
-      </c>
-      <c r="M35" s="361">
+      <c r="L35" s="266">
+        <f t="shared" si="30"/>
+        <v>4.5539022222222225E-2</v>
+      </c>
+      <c r="M35" s="266">
         <v>3.334761904761905E-2</v>
       </c>
-      <c r="N35" s="361">
-        <f t="shared" si="24"/>
-        <v>0.46708779682539681</v>
-      </c>
-      <c r="O35" s="361">
+      <c r="N35" s="266">
+        <f t="shared" si="31"/>
+        <v>0.45248964444444451</v>
+      </c>
+      <c r="O35" s="266">
         <v>0.16665238095238097</v>
       </c>
       <c r="P35" s="201">
-        <f t="shared" si="25"/>
-        <v>0.29044647619047614</v>
-      </c>
-      <c r="Q35" s="361">
+        <f t="shared" si="32"/>
+        <v>0.30197133333333326</v>
+      </c>
+      <c r="Q35" s="266">
         <v>1</v>
       </c>
-      <c r="R35" s="371">
-        <f t="shared" si="26"/>
-        <v>4.2465726984126984E-2</v>
-      </c>
-      <c r="S35" s="371">
+      <c r="R35" s="270">
+        <f t="shared" si="33"/>
+        <v>4.5539022222222225E-2</v>
+      </c>
+      <c r="S35" s="270">
         <v>3.334761904761905E-2</v>
       </c>
-      <c r="T35" s="371">
-        <f t="shared" si="27"/>
-        <v>0.46708779682539681</v>
-      </c>
-      <c r="U35" s="371">
+      <c r="T35" s="270">
+        <f t="shared" si="34"/>
+        <v>0.45248964444444451</v>
+      </c>
+      <c r="U35" s="270">
         <v>0.16665238095238097</v>
       </c>
-      <c r="V35" s="375">
-        <f t="shared" si="28"/>
-        <v>0.29044647619047614</v>
-      </c>
-      <c r="W35" s="377">
-        <f t="shared" si="29"/>
+      <c r="V35" s="271">
+        <f t="shared" si="35"/>
+        <v>0.30197133333333326</v>
+      </c>
+      <c r="W35" s="272">
+        <f t="shared" si="36"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="H36" s="367"/>
-      <c r="I36" s="367"/>
-      <c r="J36" s="367"/>
-      <c r="K36" s="367"/>
-      <c r="L36" s="367"/>
-      <c r="M36" s="367"/>
-      <c r="N36" s="367"/>
-      <c r="O36" s="367"/>
-      <c r="P36" s="367"/>
-      <c r="Q36" s="367"/>
-      <c r="R36" s="367"/>
-      <c r="S36" s="367"/>
-      <c r="T36" s="367"/>
-      <c r="U36" s="368"/>
-      <c r="V36" s="367"/>
-      <c r="W36" s="367"/>
-    </row>
-    <row r="37" spans="8:23" x14ac:dyDescent="0.2">
-      <c r="H37" s="367"/>
-      <c r="I37" s="367"/>
-      <c r="J37" s="367"/>
-      <c r="K37" s="367"/>
-      <c r="L37" s="367"/>
-      <c r="M37" s="367"/>
-      <c r="N37" s="367"/>
-      <c r="O37" s="367"/>
-      <c r="P37" s="367"/>
-      <c r="Q37" s="367"/>
-      <c r="R37" s="367"/>
-      <c r="S37" s="367"/>
-      <c r="T37" s="367"/>
-      <c r="U37" s="368"/>
-      <c r="V37" s="367"/>
-      <c r="W37" s="367"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="R23:W23"/>
-    <mergeCell ref="L30:Q30"/>
-    <mergeCell ref="R30:W30"/>
-    <mergeCell ref="I22:W22"/>
-    <mergeCell ref="L23:Q23"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="K23:K24"/>
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="Q5:U5"/>
     <mergeCell ref="C11:G11"/>
@@ -24782,6 +24909,14 @@
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:P5"/>
+    <mergeCell ref="R23:W23"/>
+    <mergeCell ref="L30:Q30"/>
+    <mergeCell ref="R30:W30"/>
+    <mergeCell ref="I22:W22"/>
+    <mergeCell ref="L23:Q23"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="K23:K24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -25117,16 +25252,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="347" t="e">
+      <c r="A1" s="362" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="347"/>
-      <c r="C1" s="347"/>
-      <c r="D1" s="347"/>
-      <c r="E1" s="347"/>
-      <c r="F1" s="347"/>
-      <c r="G1" s="347"/>
+      <c r="B1" s="362"/>
+      <c r="C1" s="362"/>
+      <c r="D1" s="362"/>
+      <c r="E1" s="362"/>
+      <c r="F1" s="362"/>
+      <c r="G1" s="362"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -25135,15 +25270,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="323" t="s">
+      <c r="A3" s="331" t="s">
         <v>178</v>
       </c>
-      <c r="B3" s="323"/>
-      <c r="C3" s="323"/>
-      <c r="D3" s="323"/>
-      <c r="E3" s="323"/>
-      <c r="F3" s="323"/>
-      <c r="G3" s="323"/>
+      <c r="B3" s="331"/>
+      <c r="C3" s="331"/>
+      <c r="D3" s="331"/>
+      <c r="E3" s="331"/>
+      <c r="F3" s="331"/>
+      <c r="G3" s="331"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -25159,13 +25294,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="324" t="s">
+      <c r="C4" s="332" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="325"/>
-      <c r="E4" s="325"/>
-      <c r="F4" s="325"/>
-      <c r="G4" s="326"/>
+      <c r="D4" s="333"/>
+      <c r="E4" s="333"/>
+      <c r="F4" s="333"/>
+      <c r="G4" s="334"/>
       <c r="N4" s="139" t="s">
         <v>129</v>
       </c>
@@ -25175,11 +25310,11 @@
         <v>16</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="327"/>
-      <c r="D5" s="322"/>
-      <c r="E5" s="322"/>
-      <c r="F5" s="322"/>
-      <c r="G5" s="322"/>
+      <c r="C5" s="335"/>
+      <c r="D5" s="330"/>
+      <c r="E5" s="330"/>
+      <c r="F5" s="330"/>
+      <c r="G5" s="330"/>
       <c r="N5" s="142"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -25187,11 +25322,11 @@
         <v>17</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="327"/>
-      <c r="D6" s="322"/>
-      <c r="E6" s="322"/>
-      <c r="F6" s="322"/>
-      <c r="G6" s="322"/>
+      <c r="C6" s="335"/>
+      <c r="D6" s="330"/>
+      <c r="E6" s="330"/>
+      <c r="F6" s="330"/>
+      <c r="G6" s="330"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -25199,11 +25334,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="327"/>
-      <c r="D7" s="322"/>
-      <c r="E7" s="322"/>
-      <c r="F7" s="322"/>
-      <c r="G7" s="322"/>
+      <c r="C7" s="335"/>
+      <c r="D7" s="330"/>
+      <c r="E7" s="330"/>
+      <c r="F7" s="330"/>
+      <c r="G7" s="330"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -25211,11 +25346,11 @@
         <v>39</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="322"/>
-      <c r="D8" s="322"/>
-      <c r="E8" s="322"/>
-      <c r="F8" s="322"/>
-      <c r="G8" s="322"/>
+      <c r="C8" s="330"/>
+      <c r="D8" s="330"/>
+      <c r="E8" s="330"/>
+      <c r="F8" s="330"/>
+      <c r="G8" s="330"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -25223,11 +25358,11 @@
         <v>163</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="328"/>
-      <c r="D9" s="328"/>
-      <c r="E9" s="328"/>
-      <c r="F9" s="328"/>
-      <c r="G9" s="328"/>
+      <c r="C9" s="336"/>
+      <c r="D9" s="336"/>
+      <c r="E9" s="336"/>
+      <c r="F9" s="336"/>
+      <c r="G9" s="336"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -25235,11 +25370,11 @@
         <v>41</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="348"/>
-      <c r="D10" s="348"/>
-      <c r="E10" s="348"/>
-      <c r="F10" s="348"/>
-      <c r="G10" s="348"/>
+      <c r="C10" s="361"/>
+      <c r="D10" s="361"/>
+      <c r="E10" s="361"/>
+      <c r="F10" s="361"/>
+      <c r="G10" s="361"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -25252,37 +25387,37 @@
       <c r="A12" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="329" t="s">
+      <c r="B12" s="337" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="330"/>
-      <c r="D12" s="331"/>
+      <c r="C12" s="338"/>
+      <c r="D12" s="339"/>
       <c r="N12" s="141" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="332" t="s">
+      <c r="B13" s="340" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="333"/>
-      <c r="D13" s="334"/>
+      <c r="C13" s="341"/>
+      <c r="D13" s="342"/>
       <c r="N13" s="142"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="316" t="s">
+      <c r="B14" s="324" t="s">
         <v>115</v>
       </c>
-      <c r="C14" s="317"/>
-      <c r="D14" s="318"/>
+      <c r="C14" s="325"/>
+      <c r="D14" s="326"/>
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="319" t="s">
+      <c r="B15" s="327" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="320"/>
-      <c r="D15" s="321"/>
+      <c r="C15" s="328"/>
+      <c r="D15" s="329"/>
       <c r="N15" s="142"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -26502,6 +26637,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -26509,12 +26650,6 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>
@@ -26572,26 +26707,26 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="349" t="s">
+      <c r="D3" s="363" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="349"/>
-      <c r="F3" s="349" t="s">
+      <c r="E3" s="363"/>
+      <c r="F3" s="363" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="349"/>
-      <c r="H3" s="349"/>
-      <c r="I3" s="349" t="s">
+      <c r="G3" s="363"/>
+      <c r="H3" s="363"/>
+      <c r="I3" s="363" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="349"/>
-      <c r="K3" s="349"/>
+      <c r="J3" s="363"/>
+      <c r="K3" s="363"/>
       <c r="L3" s="134"/>
-      <c r="M3" s="349" t="s">
+      <c r="M3" s="363" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="349"/>
-      <c r="O3" s="349"/>
+      <c r="N3" s="363"/>
+      <c r="O3" s="363"/>
     </row>
     <row r="4" spans="1:16" s="47" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">

</xml_diff>

<commit_message>
Updated tribal nations error again
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anabelle/Documents/ColoradoRiverCollaborate/LakeMeadWaterBankDivideInflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE655D3-23F6-7046-86F6-7C988F259722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69EB8F9-DF1A-5047-9638-B857DE3D0408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="3" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="62" r:id="rId1"/>
@@ -2928,7 +2928,7 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="26" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="371">
+  <cellXfs count="369">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3641,6 +3641,75 @@
     <xf numFmtId="9" fontId="19" fillId="0" borderId="9" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="172" fontId="19" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3695,12 +3764,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3733,63 +3796,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3851,6 +3857,18 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3881,23 +3899,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3919,16 +3925,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="172" fontId="19" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -15489,20 +15485,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="275" t="s">
+      <c r="A1" s="300" t="s">
         <v>302</v>
       </c>
-      <c r="B1" s="275"/>
-      <c r="C1" s="275"/>
-      <c r="D1" s="275"/>
-      <c r="E1" s="275"/>
-      <c r="F1" s="275"/>
-      <c r="G1" s="275"/>
-      <c r="H1" s="275"/>
-      <c r="I1" s="275"/>
-      <c r="J1" s="275"/>
-      <c r="K1" s="275"/>
-      <c r="L1" s="275"/>
+      <c r="B1" s="300"/>
+      <c r="C1" s="300"/>
+      <c r="D1" s="300"/>
+      <c r="E1" s="300"/>
+      <c r="F1" s="300"/>
+      <c r="G1" s="300"/>
+      <c r="H1" s="300"/>
+      <c r="I1" s="300"/>
+      <c r="J1" s="300"/>
+      <c r="K1" s="300"/>
+      <c r="L1" s="300"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -15528,41 +15524,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="276" t="s">
+      <c r="A4" s="301" t="s">
         <v>303</v>
       </c>
-      <c r="B4" s="277"/>
-      <c r="C4" s="277"/>
-      <c r="D4" s="277"/>
-      <c r="E4" s="277"/>
-      <c r="F4" s="277"/>
-      <c r="G4" s="277"/>
-      <c r="H4" s="277"/>
-      <c r="I4" s="277"/>
-      <c r="J4" s="277"/>
-      <c r="K4" s="277"/>
-      <c r="L4" s="278"/>
-      <c r="N4" s="279"/>
-      <c r="O4" s="279"/>
-      <c r="P4" s="279"/>
-      <c r="Q4" s="279"/>
-      <c r="R4" s="279"/>
+      <c r="B4" s="302"/>
+      <c r="C4" s="302"/>
+      <c r="D4" s="302"/>
+      <c r="E4" s="302"/>
+      <c r="F4" s="302"/>
+      <c r="G4" s="302"/>
+      <c r="H4" s="302"/>
+      <c r="I4" s="302"/>
+      <c r="J4" s="302"/>
+      <c r="K4" s="302"/>
+      <c r="L4" s="303"/>
+      <c r="N4" s="304"/>
+      <c r="O4" s="304"/>
+      <c r="P4" s="304"/>
+      <c r="Q4" s="304"/>
+      <c r="R4" s="304"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="280" t="s">
+      <c r="A5" s="305" t="s">
         <v>286</v>
       </c>
-      <c r="B5" s="281"/>
-      <c r="C5" s="281"/>
-      <c r="D5" s="281"/>
-      <c r="E5" s="281"/>
-      <c r="F5" s="281"/>
-      <c r="G5" s="281"/>
-      <c r="H5" s="281"/>
-      <c r="I5" s="281"/>
-      <c r="J5" s="281"/>
-      <c r="K5" s="281"/>
-      <c r="L5" s="282"/>
+      <c r="B5" s="306"/>
+      <c r="C5" s="306"/>
+      <c r="D5" s="306"/>
+      <c r="E5" s="306"/>
+      <c r="F5" s="306"/>
+      <c r="G5" s="306"/>
+      <c r="H5" s="306"/>
+      <c r="I5" s="306"/>
+      <c r="J5" s="306"/>
+      <c r="K5" s="306"/>
+      <c r="L5" s="307"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15570,20 +15566,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="280" t="s">
+      <c r="A6" s="305" t="s">
         <v>304</v>
       </c>
-      <c r="B6" s="281"/>
-      <c r="C6" s="281"/>
-      <c r="D6" s="281"/>
-      <c r="E6" s="281"/>
-      <c r="F6" s="281"/>
-      <c r="G6" s="281"/>
-      <c r="H6" s="281"/>
-      <c r="I6" s="281"/>
-      <c r="J6" s="281"/>
-      <c r="K6" s="281"/>
-      <c r="L6" s="282"/>
+      <c r="B6" s="306"/>
+      <c r="C6" s="306"/>
+      <c r="D6" s="306"/>
+      <c r="E6" s="306"/>
+      <c r="F6" s="306"/>
+      <c r="G6" s="306"/>
+      <c r="H6" s="306"/>
+      <c r="I6" s="306"/>
+      <c r="J6" s="306"/>
+      <c r="K6" s="306"/>
+      <c r="L6" s="307"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15592,19 +15588,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="227"/>
-      <c r="B7" s="281" t="s">
+      <c r="B7" s="306" t="s">
         <v>305</v>
       </c>
-      <c r="C7" s="281"/>
-      <c r="D7" s="281"/>
-      <c r="E7" s="281"/>
-      <c r="F7" s="281"/>
-      <c r="G7" s="281"/>
-      <c r="H7" s="281"/>
-      <c r="I7" s="281"/>
-      <c r="J7" s="281"/>
-      <c r="K7" s="281"/>
-      <c r="L7" s="282"/>
+      <c r="C7" s="306"/>
+      <c r="D7" s="306"/>
+      <c r="E7" s="306"/>
+      <c r="F7" s="306"/>
+      <c r="G7" s="306"/>
+      <c r="H7" s="306"/>
+      <c r="I7" s="306"/>
+      <c r="J7" s="306"/>
+      <c r="K7" s="306"/>
+      <c r="L7" s="307"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15613,19 +15609,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="228"/>
-      <c r="B8" s="298" t="s">
+      <c r="B8" s="321" t="s">
         <v>306</v>
       </c>
-      <c r="C8" s="298"/>
-      <c r="D8" s="298"/>
-      <c r="E8" s="298"/>
-      <c r="F8" s="298"/>
-      <c r="G8" s="298"/>
-      <c r="H8" s="298"/>
-      <c r="I8" s="298"/>
-      <c r="J8" s="298"/>
-      <c r="K8" s="298"/>
-      <c r="L8" s="299"/>
+      <c r="C8" s="321"/>
+      <c r="D8" s="321"/>
+      <c r="E8" s="321"/>
+      <c r="F8" s="321"/>
+      <c r="G8" s="321"/>
+      <c r="H8" s="321"/>
+      <c r="I8" s="321"/>
+      <c r="J8" s="321"/>
+      <c r="K8" s="321"/>
+      <c r="L8" s="322"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15647,38 +15643,38 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="300" t="s">
+      <c r="A10" s="323" t="s">
         <v>341</v>
       </c>
-      <c r="B10" s="301"/>
-      <c r="C10" s="301"/>
-      <c r="D10" s="301"/>
-      <c r="E10" s="301"/>
-      <c r="F10" s="301"/>
-      <c r="G10" s="301"/>
-      <c r="H10" s="301"/>
-      <c r="I10" s="301"/>
-      <c r="J10" s="301"/>
-      <c r="K10" s="301"/>
-      <c r="L10" s="302"/>
+      <c r="B10" s="324"/>
+      <c r="C10" s="324"/>
+      <c r="D10" s="324"/>
+      <c r="E10" s="324"/>
+      <c r="F10" s="324"/>
+      <c r="G10" s="324"/>
+      <c r="H10" s="324"/>
+      <c r="I10" s="324"/>
+      <c r="J10" s="324"/>
+      <c r="K10" s="324"/>
+      <c r="L10" s="325"/>
     </row>
     <row r="11" spans="1:18" s="58" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="248" t="s">
         <v>342</v>
       </c>
-      <c r="B11" s="303" t="s">
+      <c r="B11" s="278" t="s">
         <v>345</v>
       </c>
-      <c r="C11" s="303"/>
-      <c r="D11" s="303"/>
-      <c r="E11" s="303"/>
-      <c r="F11" s="303"/>
-      <c r="G11" s="303"/>
-      <c r="H11" s="303"/>
-      <c r="I11" s="303"/>
-      <c r="J11" s="303"/>
-      <c r="K11" s="303"/>
-      <c r="L11" s="304"/>
+      <c r="C11" s="278"/>
+      <c r="D11" s="278"/>
+      <c r="E11" s="278"/>
+      <c r="F11" s="278"/>
+      <c r="G11" s="278"/>
+      <c r="H11" s="278"/>
+      <c r="I11" s="278"/>
+      <c r="J11" s="278"/>
+      <c r="K11" s="278"/>
+      <c r="L11" s="279"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="161.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="240"/>
@@ -15698,51 +15694,51 @@
       <c r="A13" s="248" t="s">
         <v>343</v>
       </c>
-      <c r="B13" s="303" t="s">
+      <c r="B13" s="278" t="s">
         <v>346</v>
       </c>
-      <c r="C13" s="303"/>
-      <c r="D13" s="303"/>
-      <c r="E13" s="303"/>
-      <c r="F13" s="303"/>
-      <c r="G13" s="303"/>
-      <c r="H13" s="303"/>
-      <c r="I13" s="303"/>
-      <c r="J13" s="303"/>
-      <c r="K13" s="303"/>
-      <c r="L13" s="304"/>
+      <c r="C13" s="278"/>
+      <c r="D13" s="278"/>
+      <c r="E13" s="278"/>
+      <c r="F13" s="278"/>
+      <c r="G13" s="278"/>
+      <c r="H13" s="278"/>
+      <c r="I13" s="278"/>
+      <c r="J13" s="278"/>
+      <c r="K13" s="278"/>
+      <c r="L13" s="279"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="90.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="240"/>
-      <c r="B14" s="314"/>
-      <c r="C14" s="314"/>
-      <c r="D14" s="314"/>
-      <c r="E14" s="314"/>
-      <c r="F14" s="314"/>
-      <c r="G14" s="314"/>
-      <c r="H14" s="314"/>
-      <c r="I14" s="314"/>
-      <c r="J14" s="314"/>
-      <c r="K14" s="314"/>
-      <c r="L14" s="315"/>
+      <c r="B14" s="280"/>
+      <c r="C14" s="280"/>
+      <c r="D14" s="280"/>
+      <c r="E14" s="280"/>
+      <c r="F14" s="280"/>
+      <c r="G14" s="280"/>
+      <c r="H14" s="280"/>
+      <c r="I14" s="280"/>
+      <c r="J14" s="280"/>
+      <c r="K14" s="280"/>
+      <c r="L14" s="281"/>
     </row>
     <row r="15" spans="1:18" s="58" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="248" t="s">
         <v>344</v>
       </c>
-      <c r="B15" s="303" t="s">
+      <c r="B15" s="278" t="s">
         <v>347</v>
       </c>
-      <c r="C15" s="303"/>
-      <c r="D15" s="303"/>
-      <c r="E15" s="303"/>
-      <c r="F15" s="303"/>
-      <c r="G15" s="303"/>
-      <c r="H15" s="303"/>
-      <c r="I15" s="303"/>
-      <c r="J15" s="303"/>
-      <c r="K15" s="303"/>
-      <c r="L15" s="304"/>
+      <c r="C15" s="278"/>
+      <c r="D15" s="278"/>
+      <c r="E15" s="278"/>
+      <c r="F15" s="278"/>
+      <c r="G15" s="278"/>
+      <c r="H15" s="278"/>
+      <c r="I15" s="278"/>
+      <c r="J15" s="278"/>
+      <c r="K15" s="278"/>
+      <c r="L15" s="279"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="240"/>
@@ -15759,12 +15755,12 @@
       <c r="L16" s="247"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="312" t="s">
+      <c r="A17" s="276" t="s">
         <v>351</v>
       </c>
-      <c r="B17" s="313"/>
-      <c r="C17" s="313"/>
-      <c r="D17" s="313"/>
+      <c r="B17" s="277"/>
+      <c r="C17" s="277"/>
+      <c r="D17" s="277"/>
       <c r="E17" s="245" t="s">
         <v>352</v>
       </c>
@@ -15791,84 +15787,84 @@
       <c r="L18" s="113"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="283" t="s">
+      <c r="A19" s="308" t="s">
         <v>166</v>
       </c>
-      <c r="B19" s="284"/>
-      <c r="C19" s="284"/>
-      <c r="D19" s="284"/>
-      <c r="E19" s="284"/>
-      <c r="F19" s="284"/>
-      <c r="G19" s="284"/>
-      <c r="H19" s="284"/>
-      <c r="I19" s="284"/>
-      <c r="J19" s="284"/>
-      <c r="K19" s="284"/>
-      <c r="L19" s="285"/>
+      <c r="B19" s="309"/>
+      <c r="C19" s="309"/>
+      <c r="D19" s="309"/>
+      <c r="E19" s="309"/>
+      <c r="F19" s="309"/>
+      <c r="G19" s="309"/>
+      <c r="H19" s="309"/>
+      <c r="I19" s="309"/>
+      <c r="J19" s="309"/>
+      <c r="K19" s="309"/>
+      <c r="L19" s="310"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="286" t="s">
+      <c r="A20" s="311" t="s">
         <v>287</v>
       </c>
-      <c r="B20" s="287"/>
-      <c r="C20" s="287"/>
-      <c r="D20" s="287"/>
-      <c r="E20" s="287"/>
-      <c r="F20" s="287"/>
-      <c r="G20" s="287"/>
-      <c r="H20" s="287"/>
-      <c r="I20" s="287"/>
-      <c r="J20" s="287"/>
-      <c r="K20" s="287"/>
-      <c r="L20" s="288"/>
+      <c r="B20" s="312"/>
+      <c r="C20" s="312"/>
+      <c r="D20" s="312"/>
+      <c r="E20" s="312"/>
+      <c r="F20" s="312"/>
+      <c r="G20" s="312"/>
+      <c r="H20" s="312"/>
+      <c r="I20" s="312"/>
+      <c r="J20" s="312"/>
+      <c r="K20" s="312"/>
+      <c r="L20" s="313"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="289" t="s">
+      <c r="A21" s="314" t="s">
         <v>288</v>
       </c>
-      <c r="B21" s="290"/>
-      <c r="C21" s="290"/>
-      <c r="D21" s="290"/>
-      <c r="E21" s="290"/>
-      <c r="F21" s="290"/>
-      <c r="G21" s="290"/>
-      <c r="H21" s="290"/>
-      <c r="I21" s="290"/>
-      <c r="J21" s="290"/>
-      <c r="K21" s="290"/>
-      <c r="L21" s="291"/>
+      <c r="B21" s="292"/>
+      <c r="C21" s="292"/>
+      <c r="D21" s="292"/>
+      <c r="E21" s="292"/>
+      <c r="F21" s="292"/>
+      <c r="G21" s="292"/>
+      <c r="H21" s="292"/>
+      <c r="I21" s="292"/>
+      <c r="J21" s="292"/>
+      <c r="K21" s="292"/>
+      <c r="L21" s="293"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="289" t="s">
+      <c r="A22" s="314" t="s">
         <v>167</v>
       </c>
-      <c r="B22" s="290"/>
-      <c r="C22" s="290"/>
-      <c r="D22" s="290"/>
-      <c r="E22" s="290"/>
-      <c r="F22" s="290"/>
-      <c r="G22" s="290"/>
-      <c r="H22" s="290"/>
-      <c r="I22" s="290"/>
-      <c r="J22" s="290"/>
-      <c r="K22" s="290"/>
-      <c r="L22" s="291"/>
+      <c r="B22" s="292"/>
+      <c r="C22" s="292"/>
+      <c r="D22" s="292"/>
+      <c r="E22" s="292"/>
+      <c r="F22" s="292"/>
+      <c r="G22" s="292"/>
+      <c r="H22" s="292"/>
+      <c r="I22" s="292"/>
+      <c r="J22" s="292"/>
+      <c r="K22" s="292"/>
+      <c r="L22" s="293"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="292" t="s">
+      <c r="A23" s="315" t="s">
         <v>289</v>
       </c>
-      <c r="B23" s="293"/>
-      <c r="C23" s="293"/>
-      <c r="D23" s="293"/>
-      <c r="E23" s="293"/>
-      <c r="F23" s="293"/>
-      <c r="G23" s="293"/>
-      <c r="H23" s="293"/>
-      <c r="I23" s="293"/>
-      <c r="J23" s="293"/>
-      <c r="K23" s="293"/>
-      <c r="L23" s="294"/>
+      <c r="B23" s="316"/>
+      <c r="C23" s="316"/>
+      <c r="D23" s="316"/>
+      <c r="E23" s="316"/>
+      <c r="F23" s="316"/>
+      <c r="G23" s="316"/>
+      <c r="H23" s="316"/>
+      <c r="I23" s="316"/>
+      <c r="J23" s="316"/>
+      <c r="K23" s="316"/>
+      <c r="L23" s="317"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="113"/>
@@ -15885,332 +15881,332 @@
       <c r="L24" s="113"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="295" t="s">
+      <c r="A25" s="318" t="s">
         <v>285</v>
       </c>
-      <c r="B25" s="296"/>
-      <c r="C25" s="296"/>
-      <c r="D25" s="296"/>
-      <c r="E25" s="296"/>
-      <c r="F25" s="296"/>
-      <c r="G25" s="296"/>
-      <c r="H25" s="296"/>
-      <c r="I25" s="296"/>
-      <c r="J25" s="296"/>
-      <c r="K25" s="296"/>
-      <c r="L25" s="297"/>
+      <c r="B25" s="319"/>
+      <c r="C25" s="319"/>
+      <c r="D25" s="319"/>
+      <c r="E25" s="319"/>
+      <c r="F25" s="319"/>
+      <c r="G25" s="319"/>
+      <c r="H25" s="319"/>
+      <c r="I25" s="319"/>
+      <c r="J25" s="319"/>
+      <c r="K25" s="319"/>
+      <c r="L25" s="320"/>
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="272" t="s">
+      <c r="A26" s="297" t="s">
         <v>176</v>
       </c>
-      <c r="B26" s="273"/>
-      <c r="C26" s="273"/>
-      <c r="D26" s="273"/>
-      <c r="E26" s="273"/>
-      <c r="F26" s="273"/>
-      <c r="G26" s="273"/>
-      <c r="H26" s="273"/>
-      <c r="I26" s="273"/>
-      <c r="J26" s="273"/>
-      <c r="K26" s="273"/>
-      <c r="L26" s="274"/>
+      <c r="B26" s="298"/>
+      <c r="C26" s="298"/>
+      <c r="D26" s="298"/>
+      <c r="E26" s="298"/>
+      <c r="F26" s="298"/>
+      <c r="G26" s="298"/>
+      <c r="H26" s="298"/>
+      <c r="I26" s="298"/>
+      <c r="J26" s="298"/>
+      <c r="K26" s="298"/>
+      <c r="L26" s="299"/>
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="222">
         <v>1</v>
       </c>
-      <c r="B27" s="307" t="s">
+      <c r="B27" s="285" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="307"/>
-      <c r="D27" s="307"/>
-      <c r="E27" s="307"/>
-      <c r="F27" s="307"/>
-      <c r="G27" s="307"/>
-      <c r="H27" s="307"/>
-      <c r="I27" s="307"/>
-      <c r="J27" s="307"/>
-      <c r="K27" s="307"/>
-      <c r="L27" s="308"/>
+      <c r="C27" s="285"/>
+      <c r="D27" s="285"/>
+      <c r="E27" s="285"/>
+      <c r="F27" s="285"/>
+      <c r="G27" s="285"/>
+      <c r="H27" s="285"/>
+      <c r="I27" s="285"/>
+      <c r="J27" s="285"/>
+      <c r="K27" s="285"/>
+      <c r="L27" s="286"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="222">
         <v>2</v>
       </c>
-      <c r="B28" s="307" t="s">
+      <c r="B28" s="285" t="s">
         <v>281</v>
       </c>
-      <c r="C28" s="307"/>
-      <c r="D28" s="307"/>
-      <c r="E28" s="307"/>
-      <c r="F28" s="307"/>
-      <c r="G28" s="307"/>
-      <c r="H28" s="307"/>
-      <c r="I28" s="307"/>
-      <c r="J28" s="307"/>
-      <c r="K28" s="307"/>
-      <c r="L28" s="308"/>
+      <c r="C28" s="285"/>
+      <c r="D28" s="285"/>
+      <c r="E28" s="285"/>
+      <c r="F28" s="285"/>
+      <c r="G28" s="285"/>
+      <c r="H28" s="285"/>
+      <c r="I28" s="285"/>
+      <c r="J28" s="285"/>
+      <c r="K28" s="285"/>
+      <c r="L28" s="286"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="222">
         <v>3</v>
       </c>
-      <c r="B29" s="307" t="s">
+      <c r="B29" s="285" t="s">
         <v>168</v>
       </c>
-      <c r="C29" s="307"/>
-      <c r="D29" s="307"/>
-      <c r="E29" s="307"/>
-      <c r="F29" s="307"/>
-      <c r="G29" s="307"/>
-      <c r="H29" s="307"/>
-      <c r="I29" s="307"/>
-      <c r="J29" s="307"/>
-      <c r="K29" s="307"/>
-      <c r="L29" s="308"/>
+      <c r="C29" s="285"/>
+      <c r="D29" s="285"/>
+      <c r="E29" s="285"/>
+      <c r="F29" s="285"/>
+      <c r="G29" s="285"/>
+      <c r="H29" s="285"/>
+      <c r="I29" s="285"/>
+      <c r="J29" s="285"/>
+      <c r="K29" s="285"/>
+      <c r="L29" s="286"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="222">
         <v>4</v>
       </c>
-      <c r="B30" s="307" t="s">
+      <c r="B30" s="285" t="s">
         <v>290</v>
       </c>
-      <c r="C30" s="307"/>
-      <c r="D30" s="307"/>
-      <c r="E30" s="307"/>
-      <c r="F30" s="307"/>
-      <c r="G30" s="307"/>
-      <c r="H30" s="307"/>
-      <c r="I30" s="307"/>
-      <c r="J30" s="307"/>
-      <c r="K30" s="307"/>
-      <c r="L30" s="308"/>
+      <c r="C30" s="285"/>
+      <c r="D30" s="285"/>
+      <c r="E30" s="285"/>
+      <c r="F30" s="285"/>
+      <c r="G30" s="285"/>
+      <c r="H30" s="285"/>
+      <c r="I30" s="285"/>
+      <c r="J30" s="285"/>
+      <c r="K30" s="285"/>
+      <c r="L30" s="286"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="222">
         <v>5</v>
       </c>
-      <c r="B31" s="307" t="s">
+      <c r="B31" s="285" t="s">
         <v>169</v>
       </c>
-      <c r="C31" s="307"/>
-      <c r="D31" s="307"/>
-      <c r="E31" s="307"/>
-      <c r="F31" s="307"/>
-      <c r="G31" s="307"/>
-      <c r="H31" s="307"/>
-      <c r="I31" s="307"/>
-      <c r="J31" s="307"/>
-      <c r="K31" s="307"/>
-      <c r="L31" s="308"/>
+      <c r="C31" s="285"/>
+      <c r="D31" s="285"/>
+      <c r="E31" s="285"/>
+      <c r="F31" s="285"/>
+      <c r="G31" s="285"/>
+      <c r="H31" s="285"/>
+      <c r="I31" s="285"/>
+      <c r="J31" s="285"/>
+      <c r="K31" s="285"/>
+      <c r="L31" s="286"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="222"/>
-      <c r="B32" s="307" t="s">
+      <c r="B32" s="285" t="s">
         <v>170</v>
       </c>
-      <c r="C32" s="307"/>
-      <c r="D32" s="307"/>
-      <c r="E32" s="307"/>
-      <c r="F32" s="307"/>
-      <c r="G32" s="307"/>
-      <c r="H32" s="307"/>
-      <c r="I32" s="307"/>
-      <c r="J32" s="307"/>
-      <c r="K32" s="307"/>
-      <c r="L32" s="308"/>
+      <c r="C32" s="285"/>
+      <c r="D32" s="285"/>
+      <c r="E32" s="285"/>
+      <c r="F32" s="285"/>
+      <c r="G32" s="285"/>
+      <c r="H32" s="285"/>
+      <c r="I32" s="285"/>
+      <c r="J32" s="285"/>
+      <c r="K32" s="285"/>
+      <c r="L32" s="286"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="222"/>
-      <c r="B33" s="307" t="s">
+      <c r="B33" s="285" t="s">
         <v>171</v>
       </c>
-      <c r="C33" s="307"/>
-      <c r="D33" s="307"/>
-      <c r="E33" s="307"/>
-      <c r="F33" s="307"/>
-      <c r="G33" s="307"/>
-      <c r="H33" s="307"/>
-      <c r="I33" s="307"/>
-      <c r="J33" s="307"/>
-      <c r="K33" s="307"/>
-      <c r="L33" s="308"/>
+      <c r="C33" s="285"/>
+      <c r="D33" s="285"/>
+      <c r="E33" s="285"/>
+      <c r="F33" s="285"/>
+      <c r="G33" s="285"/>
+      <c r="H33" s="285"/>
+      <c r="I33" s="285"/>
+      <c r="J33" s="285"/>
+      <c r="K33" s="285"/>
+      <c r="L33" s="286"/>
       <c r="N33" s="106"/>
     </row>
     <row r="34" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="309" t="s">
+      <c r="A34" s="294" t="s">
         <v>177</v>
       </c>
-      <c r="B34" s="310"/>
-      <c r="C34" s="310"/>
-      <c r="D34" s="310"/>
-      <c r="E34" s="310"/>
-      <c r="F34" s="310"/>
-      <c r="G34" s="310"/>
-      <c r="H34" s="310"/>
-      <c r="I34" s="310"/>
-      <c r="J34" s="310"/>
-      <c r="K34" s="310"/>
-      <c r="L34" s="311"/>
+      <c r="B34" s="295"/>
+      <c r="C34" s="295"/>
+      <c r="D34" s="295"/>
+      <c r="E34" s="295"/>
+      <c r="F34" s="295"/>
+      <c r="G34" s="295"/>
+      <c r="H34" s="295"/>
+      <c r="I34" s="295"/>
+      <c r="J34" s="295"/>
+      <c r="K34" s="295"/>
+      <c r="L34" s="296"/>
       <c r="N34" s="106"/>
     </row>
     <row r="35" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="222">
         <v>1</v>
       </c>
-      <c r="B35" s="307" t="s">
+      <c r="B35" s="285" t="s">
         <v>172</v>
       </c>
-      <c r="C35" s="307"/>
-      <c r="D35" s="307"/>
-      <c r="E35" s="307"/>
-      <c r="F35" s="307"/>
-      <c r="G35" s="307"/>
-      <c r="H35" s="307"/>
-      <c r="I35" s="307"/>
-      <c r="J35" s="307"/>
-      <c r="K35" s="307"/>
-      <c r="L35" s="308"/>
+      <c r="C35" s="285"/>
+      <c r="D35" s="285"/>
+      <c r="E35" s="285"/>
+      <c r="F35" s="285"/>
+      <c r="G35" s="285"/>
+      <c r="H35" s="285"/>
+      <c r="I35" s="285"/>
+      <c r="J35" s="285"/>
+      <c r="K35" s="285"/>
+      <c r="L35" s="286"/>
       <c r="N35" s="106"/>
     </row>
     <row r="36" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="222"/>
-      <c r="B36" s="305" t="s">
+      <c r="B36" s="283" t="s">
         <v>291</v>
       </c>
-      <c r="C36" s="305"/>
-      <c r="D36" s="305"/>
-      <c r="E36" s="305"/>
-      <c r="F36" s="305"/>
-      <c r="G36" s="305"/>
-      <c r="H36" s="305"/>
-      <c r="I36" s="305"/>
-      <c r="J36" s="305"/>
-      <c r="K36" s="305"/>
-      <c r="L36" s="306"/>
+      <c r="C36" s="283"/>
+      <c r="D36" s="283"/>
+      <c r="E36" s="283"/>
+      <c r="F36" s="283"/>
+      <c r="G36" s="283"/>
+      <c r="H36" s="283"/>
+      <c r="I36" s="283"/>
+      <c r="J36" s="283"/>
+      <c r="K36" s="283"/>
+      <c r="L36" s="284"/>
       <c r="N36" s="106"/>
     </row>
     <row r="37" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="222">
         <v>2</v>
       </c>
-      <c r="B37" s="307" t="s">
+      <c r="B37" s="285" t="s">
         <v>284</v>
       </c>
-      <c r="C37" s="307"/>
-      <c r="D37" s="307"/>
-      <c r="E37" s="307"/>
-      <c r="F37" s="307"/>
-      <c r="G37" s="307"/>
-      <c r="H37" s="307"/>
-      <c r="I37" s="307"/>
-      <c r="J37" s="307"/>
-      <c r="K37" s="307"/>
-      <c r="L37" s="308"/>
+      <c r="C37" s="285"/>
+      <c r="D37" s="285"/>
+      <c r="E37" s="285"/>
+      <c r="F37" s="285"/>
+      <c r="G37" s="285"/>
+      <c r="H37" s="285"/>
+      <c r="I37" s="285"/>
+      <c r="J37" s="285"/>
+      <c r="K37" s="285"/>
+      <c r="L37" s="286"/>
       <c r="N37" s="106"/>
     </row>
     <row r="38" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="222">
         <v>3</v>
       </c>
-      <c r="B38" s="307" t="s">
+      <c r="B38" s="285" t="s">
         <v>273</v>
       </c>
-      <c r="C38" s="307"/>
-      <c r="D38" s="307"/>
-      <c r="E38" s="307"/>
-      <c r="F38" s="307"/>
-      <c r="G38" s="307"/>
-      <c r="H38" s="307"/>
-      <c r="I38" s="307"/>
-      <c r="J38" s="307"/>
-      <c r="K38" s="307"/>
-      <c r="L38" s="308"/>
+      <c r="C38" s="285"/>
+      <c r="D38" s="285"/>
+      <c r="E38" s="285"/>
+      <c r="F38" s="285"/>
+      <c r="G38" s="285"/>
+      <c r="H38" s="285"/>
+      <c r="I38" s="285"/>
+      <c r="J38" s="285"/>
+      <c r="K38" s="285"/>
+      <c r="L38" s="286"/>
       <c r="N38" s="106"/>
     </row>
     <row r="39" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="222">
         <v>4</v>
       </c>
-      <c r="B39" s="307" t="s">
+      <c r="B39" s="285" t="s">
         <v>292</v>
       </c>
-      <c r="C39" s="307"/>
-      <c r="D39" s="307"/>
-      <c r="E39" s="307"/>
-      <c r="F39" s="307"/>
-      <c r="G39" s="307"/>
-      <c r="H39" s="307"/>
-      <c r="I39" s="307"/>
-      <c r="J39" s="307"/>
-      <c r="K39" s="307"/>
-      <c r="L39" s="308"/>
+      <c r="C39" s="285"/>
+      <c r="D39" s="285"/>
+      <c r="E39" s="285"/>
+      <c r="F39" s="285"/>
+      <c r="G39" s="285"/>
+      <c r="H39" s="285"/>
+      <c r="I39" s="285"/>
+      <c r="J39" s="285"/>
+      <c r="K39" s="285"/>
+      <c r="L39" s="286"/>
       <c r="N39" s="106"/>
     </row>
     <row r="40" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="222">
         <v>5</v>
       </c>
-      <c r="B40" s="305" t="s">
+      <c r="B40" s="283" t="s">
         <v>274</v>
       </c>
-      <c r="C40" s="305"/>
-      <c r="D40" s="305"/>
-      <c r="E40" s="305"/>
-      <c r="F40" s="305"/>
-      <c r="G40" s="305"/>
-      <c r="H40" s="305"/>
-      <c r="I40" s="305"/>
-      <c r="J40" s="305"/>
-      <c r="K40" s="305"/>
-      <c r="L40" s="306"/>
+      <c r="C40" s="283"/>
+      <c r="D40" s="283"/>
+      <c r="E40" s="283"/>
+      <c r="F40" s="283"/>
+      <c r="G40" s="283"/>
+      <c r="H40" s="283"/>
+      <c r="I40" s="283"/>
+      <c r="J40" s="283"/>
+      <c r="K40" s="283"/>
+      <c r="L40" s="284"/>
       <c r="N40" s="106"/>
     </row>
     <row r="41" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="222">
         <v>6</v>
       </c>
-      <c r="B41" s="305" t="s">
+      <c r="B41" s="283" t="s">
         <v>279</v>
       </c>
-      <c r="C41" s="305"/>
-      <c r="D41" s="305"/>
-      <c r="E41" s="305"/>
-      <c r="F41" s="305"/>
-      <c r="G41" s="305"/>
-      <c r="H41" s="305"/>
-      <c r="I41" s="305"/>
-      <c r="J41" s="305"/>
-      <c r="K41" s="305"/>
-      <c r="L41" s="306"/>
+      <c r="C41" s="283"/>
+      <c r="D41" s="283"/>
+      <c r="E41" s="283"/>
+      <c r="F41" s="283"/>
+      <c r="G41" s="283"/>
+      <c r="H41" s="283"/>
+      <c r="I41" s="283"/>
+      <c r="J41" s="283"/>
+      <c r="K41" s="283"/>
+      <c r="L41" s="284"/>
       <c r="N41" s="106"/>
     </row>
     <row r="42" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="222">
         <v>7</v>
       </c>
-      <c r="B42" s="307" t="s">
+      <c r="B42" s="285" t="s">
         <v>275</v>
       </c>
-      <c r="C42" s="307"/>
-      <c r="D42" s="307"/>
-      <c r="E42" s="307"/>
-      <c r="F42" s="307"/>
-      <c r="G42" s="307"/>
-      <c r="H42" s="307"/>
-      <c r="I42" s="307"/>
-      <c r="J42" s="307"/>
-      <c r="K42" s="307"/>
-      <c r="L42" s="308"/>
+      <c r="C42" s="285"/>
+      <c r="D42" s="285"/>
+      <c r="E42" s="285"/>
+      <c r="F42" s="285"/>
+      <c r="G42" s="285"/>
+      <c r="H42" s="285"/>
+      <c r="I42" s="285"/>
+      <c r="J42" s="285"/>
+      <c r="K42" s="285"/>
+      <c r="L42" s="286"/>
     </row>
     <row r="43" spans="1:14" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="222"/>
@@ -16227,56 +16223,56 @@
       <c r="L43" s="224"/>
     </row>
     <row r="44" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="309" t="s">
+      <c r="A44" s="294" t="s">
         <v>278</v>
       </c>
-      <c r="B44" s="310"/>
-      <c r="C44" s="310"/>
-      <c r="D44" s="310"/>
-      <c r="E44" s="310"/>
-      <c r="F44" s="310"/>
-      <c r="G44" s="310"/>
-      <c r="H44" s="310"/>
-      <c r="I44" s="310"/>
-      <c r="J44" s="310"/>
-      <c r="K44" s="310"/>
-      <c r="L44" s="311"/>
+      <c r="B44" s="295"/>
+      <c r="C44" s="295"/>
+      <c r="D44" s="295"/>
+      <c r="E44" s="295"/>
+      <c r="F44" s="295"/>
+      <c r="G44" s="295"/>
+      <c r="H44" s="295"/>
+      <c r="I44" s="295"/>
+      <c r="J44" s="295"/>
+      <c r="K44" s="295"/>
+      <c r="L44" s="296"/>
     </row>
     <row r="45" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="225" t="s">
         <v>276</v>
       </c>
-      <c r="B45" s="307" t="s">
+      <c r="B45" s="285" t="s">
         <v>173</v>
       </c>
-      <c r="C45" s="307"/>
-      <c r="D45" s="307"/>
-      <c r="E45" s="307"/>
-      <c r="F45" s="307"/>
-      <c r="G45" s="307"/>
-      <c r="H45" s="307"/>
-      <c r="I45" s="307"/>
-      <c r="J45" s="307"/>
-      <c r="K45" s="307"/>
-      <c r="L45" s="308"/>
+      <c r="C45" s="285"/>
+      <c r="D45" s="285"/>
+      <c r="E45" s="285"/>
+      <c r="F45" s="285"/>
+      <c r="G45" s="285"/>
+      <c r="H45" s="285"/>
+      <c r="I45" s="285"/>
+      <c r="J45" s="285"/>
+      <c r="K45" s="285"/>
+      <c r="L45" s="286"/>
     </row>
     <row r="46" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="226" t="s">
         <v>277</v>
       </c>
-      <c r="B46" s="317" t="s">
+      <c r="B46" s="287" t="s">
         <v>280</v>
       </c>
-      <c r="C46" s="317"/>
-      <c r="D46" s="317"/>
-      <c r="E46" s="317"/>
-      <c r="F46" s="317"/>
-      <c r="G46" s="317"/>
-      <c r="H46" s="317"/>
-      <c r="I46" s="317"/>
-      <c r="J46" s="317"/>
-      <c r="K46" s="317"/>
-      <c r="L46" s="318"/>
+      <c r="C46" s="287"/>
+      <c r="D46" s="287"/>
+      <c r="E46" s="287"/>
+      <c r="F46" s="287"/>
+      <c r="G46" s="287"/>
+      <c r="H46" s="287"/>
+      <c r="I46" s="287"/>
+      <c r="J46" s="287"/>
+      <c r="K46" s="287"/>
+      <c r="L46" s="288"/>
     </row>
     <row r="47" spans="1:14" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="160"/>
@@ -16293,20 +16289,20 @@
       <c r="L47" s="113"/>
     </row>
     <row r="48" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="319" t="s">
+      <c r="A48" s="289" t="s">
         <v>201</v>
       </c>
-      <c r="B48" s="320"/>
-      <c r="C48" s="320"/>
-      <c r="D48" s="320"/>
-      <c r="E48" s="320"/>
-      <c r="F48" s="320"/>
-      <c r="G48" s="320"/>
-      <c r="H48" s="320"/>
-      <c r="I48" s="320"/>
-      <c r="J48" s="320"/>
-      <c r="K48" s="320"/>
-      <c r="L48" s="321"/>
+      <c r="B48" s="290"/>
+      <c r="C48" s="290"/>
+      <c r="D48" s="290"/>
+      <c r="E48" s="290"/>
+      <c r="F48" s="290"/>
+      <c r="G48" s="290"/>
+      <c r="H48" s="290"/>
+      <c r="I48" s="290"/>
+      <c r="J48" s="290"/>
+      <c r="K48" s="290"/>
+      <c r="L48" s="291"/>
     </row>
     <row r="49" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="229" t="s">
@@ -16394,90 +16390,90 @@
       <c r="B54" s="168" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="290" t="s">
+      <c r="C54" s="292" t="s">
         <v>265</v>
       </c>
-      <c r="D54" s="290"/>
-      <c r="E54" s="290"/>
-      <c r="F54" s="290"/>
-      <c r="G54" s="290"/>
-      <c r="H54" s="290"/>
-      <c r="I54" s="290"/>
-      <c r="J54" s="290"/>
-      <c r="K54" s="290"/>
-      <c r="L54" s="291"/>
+      <c r="D54" s="292"/>
+      <c r="E54" s="292"/>
+      <c r="F54" s="292"/>
+      <c r="G54" s="292"/>
+      <c r="H54" s="292"/>
+      <c r="I54" s="292"/>
+      <c r="J54" s="292"/>
+      <c r="K54" s="292"/>
+      <c r="L54" s="293"/>
     </row>
     <row r="55" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="167"/>
       <c r="B55" s="168" t="s">
         <v>266</v>
       </c>
-      <c r="C55" s="290" t="s">
+      <c r="C55" s="292" t="s">
         <v>267</v>
       </c>
-      <c r="D55" s="290"/>
-      <c r="E55" s="290"/>
-      <c r="F55" s="290"/>
-      <c r="G55" s="290"/>
-      <c r="H55" s="290"/>
-      <c r="I55" s="290"/>
-      <c r="J55" s="290"/>
-      <c r="K55" s="290"/>
-      <c r="L55" s="291"/>
+      <c r="D55" s="292"/>
+      <c r="E55" s="292"/>
+      <c r="F55" s="292"/>
+      <c r="G55" s="292"/>
+      <c r="H55" s="292"/>
+      <c r="I55" s="292"/>
+      <c r="J55" s="292"/>
+      <c r="K55" s="292"/>
+      <c r="L55" s="293"/>
     </row>
     <row r="56" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="167"/>
       <c r="B56" s="168" t="s">
         <v>334</v>
       </c>
-      <c r="C56" s="290" t="s">
+      <c r="C56" s="292" t="s">
         <v>335</v>
       </c>
-      <c r="D56" s="290"/>
-      <c r="E56" s="290"/>
-      <c r="F56" s="290"/>
-      <c r="G56" s="290"/>
-      <c r="H56" s="290"/>
-      <c r="I56" s="290"/>
-      <c r="J56" s="290"/>
-      <c r="K56" s="290"/>
-      <c r="L56" s="291"/>
+      <c r="D56" s="292"/>
+      <c r="E56" s="292"/>
+      <c r="F56" s="292"/>
+      <c r="G56" s="292"/>
+      <c r="H56" s="292"/>
+      <c r="I56" s="292"/>
+      <c r="J56" s="292"/>
+      <c r="K56" s="292"/>
+      <c r="L56" s="293"/>
     </row>
     <row r="57" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="167"/>
       <c r="B57" s="168" t="s">
         <v>99</v>
       </c>
-      <c r="C57" s="290" t="s">
+      <c r="C57" s="292" t="s">
         <v>100</v>
       </c>
-      <c r="D57" s="290"/>
-      <c r="E57" s="290"/>
-      <c r="F57" s="290"/>
-      <c r="G57" s="290"/>
-      <c r="H57" s="290"/>
-      <c r="I57" s="290"/>
-      <c r="J57" s="290"/>
-      <c r="K57" s="290"/>
-      <c r="L57" s="291"/>
+      <c r="D57" s="292"/>
+      <c r="E57" s="292"/>
+      <c r="F57" s="292"/>
+      <c r="G57" s="292"/>
+      <c r="H57" s="292"/>
+      <c r="I57" s="292"/>
+      <c r="J57" s="292"/>
+      <c r="K57" s="292"/>
+      <c r="L57" s="293"/>
     </row>
     <row r="58" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="167"/>
       <c r="B58" s="168" t="s">
         <v>199</v>
       </c>
-      <c r="C58" s="290" t="s">
+      <c r="C58" s="292" t="s">
         <v>200</v>
       </c>
-      <c r="D58" s="290"/>
-      <c r="E58" s="290"/>
-      <c r="F58" s="290"/>
-      <c r="G58" s="290"/>
-      <c r="H58" s="290"/>
-      <c r="I58" s="290"/>
-      <c r="J58" s="290"/>
-      <c r="K58" s="290"/>
-      <c r="L58" s="291"/>
+      <c r="D58" s="292"/>
+      <c r="E58" s="292"/>
+      <c r="F58" s="292"/>
+      <c r="G58" s="292"/>
+      <c r="H58" s="292"/>
+      <c r="I58" s="292"/>
+      <c r="J58" s="292"/>
+      <c r="K58" s="292"/>
+      <c r="L58" s="293"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="167"/>
@@ -16502,18 +16498,18 @@
       <c r="B60" s="168" t="s">
         <v>403</v>
       </c>
-      <c r="C60" s="290" t="s">
+      <c r="C60" s="292" t="s">
         <v>404</v>
       </c>
-      <c r="D60" s="290"/>
-      <c r="E60" s="290"/>
-      <c r="F60" s="290"/>
-      <c r="G60" s="290"/>
-      <c r="H60" s="290"/>
-      <c r="I60" s="290"/>
-      <c r="J60" s="290"/>
-      <c r="K60" s="290"/>
-      <c r="L60" s="291"/>
+      <c r="D60" s="292"/>
+      <c r="E60" s="292"/>
+      <c r="F60" s="292"/>
+      <c r="G60" s="292"/>
+      <c r="H60" s="292"/>
+      <c r="I60" s="292"/>
+      <c r="J60" s="292"/>
+      <c r="K60" s="292"/>
+      <c r="L60" s="293"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="167"/>
@@ -16634,25 +16630,56 @@
       </c>
     </row>
     <row r="82" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="316" t="s">
+      <c r="A82" s="282" t="s">
         <v>407</v>
       </c>
-      <c r="B82" s="316"/>
-      <c r="C82" s="316"/>
-      <c r="D82" s="316"/>
-      <c r="E82" s="316"/>
-      <c r="F82" s="316"/>
-      <c r="G82" s="316"/>
-      <c r="H82" s="316"/>
-      <c r="I82" s="316"/>
-      <c r="J82" s="316"/>
-      <c r="K82" s="316"/>
-      <c r="L82" s="316"/>
+      <c r="B82" s="282"/>
+      <c r="C82" s="282"/>
+      <c r="D82" s="282"/>
+      <c r="E82" s="282"/>
+      <c r="F82" s="282"/>
+      <c r="G82" s="282"/>
+      <c r="H82" s="282"/>
+      <c r="I82" s="282"/>
+      <c r="J82" s="282"/>
+      <c r="K82" s="282"/>
+      <c r="L82" s="282"/>
     </row>
     <row r="87" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="88" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="B7:L7"/>
+    <mergeCell ref="B8:L8"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="B40:L40"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B30:L30"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B39:L39"/>
     <mergeCell ref="A17:D17"/>
     <mergeCell ref="B13:L13"/>
     <mergeCell ref="B14:L14"/>
@@ -16669,37 +16696,6 @@
     <mergeCell ref="C55:L55"/>
     <mergeCell ref="C60:L60"/>
     <mergeCell ref="A44:L44"/>
-    <mergeCell ref="C56:L56"/>
-    <mergeCell ref="B40:L40"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="B7:L7"/>
-    <mergeCell ref="B8:L8"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="B11:L11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A67" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -16737,82 +16733,82 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="359" t="s">
+      <c r="A3" s="363" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="359"/>
-      <c r="C3" s="359"/>
+      <c r="B3" s="363"/>
+      <c r="C3" s="363"/>
       <c r="D3" s="128" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="360" t="s">
+      <c r="A4" s="364" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="360"/>
-      <c r="C4" s="360"/>
+      <c r="B4" s="364"/>
+      <c r="C4" s="364"/>
       <c r="D4" s="175" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="364" t="s">
+      <c r="A5" s="368" t="s">
         <v>184</v>
       </c>
-      <c r="B5" s="361"/>
-      <c r="C5" s="361"/>
+      <c r="B5" s="365"/>
+      <c r="C5" s="365"/>
       <c r="D5" s="176" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="362" t="s">
+      <c r="A6" s="366" t="s">
         <v>185</v>
       </c>
-      <c r="B6" s="362"/>
-      <c r="C6" s="362"/>
+      <c r="B6" s="366"/>
+      <c r="C6" s="366"/>
       <c r="D6" s="177" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="363" t="s">
+      <c r="A7" s="367" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="363"/>
-      <c r="C7" s="363"/>
+      <c r="B7" s="367"/>
+      <c r="C7" s="367"/>
       <c r="D7" s="178" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="360" t="s">
+      <c r="A11" s="364" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="360"/>
-      <c r="C11" s="360"/>
+      <c r="B11" s="364"/>
+      <c r="C11" s="364"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="361" t="s">
+      <c r="A12" s="365" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="361"/>
-      <c r="C12" s="361"/>
+      <c r="B12" s="365"/>
+      <c r="C12" s="365"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="362" t="s">
+      <c r="A13" s="366" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="362"/>
-      <c r="C13" s="362"/>
+      <c r="B13" s="366"/>
+      <c r="C13" s="366"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="363" t="s">
+      <c r="A14" s="367" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="363"/>
-      <c r="C14" s="363"/>
+      <c r="B14" s="367"/>
+      <c r="C14" s="367"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -18160,16 +18156,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="322" t="str">
+      <c r="A1" s="326" t="str">
         <f>'ReadMe-Directions'!A1</f>
         <v>Immersive Model for Lake Mead based on the Principle of Divide Reservoir Inflow</v>
       </c>
-      <c r="B1" s="322"/>
-      <c r="C1" s="322"/>
-      <c r="D1" s="322"/>
-      <c r="E1" s="322"/>
-      <c r="F1" s="322"/>
-      <c r="G1" s="322"/>
+      <c r="B1" s="326"/>
+      <c r="C1" s="326"/>
+      <c r="D1" s="326"/>
+      <c r="E1" s="326"/>
+      <c r="F1" s="326"/>
+      <c r="G1" s="326"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -18178,15 +18174,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="330" t="s">
+      <c r="A3" s="334" t="s">
         <v>191</v>
       </c>
-      <c r="B3" s="330"/>
-      <c r="C3" s="330"/>
-      <c r="D3" s="330"/>
-      <c r="E3" s="330"/>
-      <c r="F3" s="330"/>
-      <c r="G3" s="330"/>
+      <c r="B3" s="334"/>
+      <c r="C3" s="334"/>
+      <c r="D3" s="334"/>
+      <c r="E3" s="334"/>
+      <c r="F3" s="334"/>
+      <c r="G3" s="334"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -18202,13 +18198,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="331" t="s">
+      <c r="C4" s="335" t="s">
         <v>262</v>
       </c>
-      <c r="D4" s="332"/>
-      <c r="E4" s="332"/>
-      <c r="F4" s="332"/>
-      <c r="G4" s="333"/>
+      <c r="D4" s="336"/>
+      <c r="E4" s="336"/>
+      <c r="F4" s="336"/>
+      <c r="G4" s="337"/>
       <c r="N4" s="141" t="s">
         <v>336</v>
       </c>
@@ -18218,11 +18214,11 @@
         <v>239</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="334"/>
-      <c r="D5" s="329"/>
-      <c r="E5" s="329"/>
-      <c r="F5" s="329"/>
-      <c r="G5" s="329"/>
+      <c r="C5" s="338"/>
+      <c r="D5" s="333"/>
+      <c r="E5" s="333"/>
+      <c r="F5" s="333"/>
+      <c r="G5" s="333"/>
       <c r="N5" s="141"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -18230,11 +18226,11 @@
         <v>203</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="334"/>
-      <c r="D6" s="329"/>
-      <c r="E6" s="329"/>
-      <c r="F6" s="329"/>
-      <c r="G6" s="329"/>
+      <c r="C6" s="338"/>
+      <c r="D6" s="333"/>
+      <c r="E6" s="333"/>
+      <c r="F6" s="333"/>
+      <c r="G6" s="333"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -18242,11 +18238,11 @@
         <v>204</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="334"/>
-      <c r="D7" s="329"/>
-      <c r="E7" s="329"/>
-      <c r="F7" s="329"/>
-      <c r="G7" s="329"/>
+      <c r="C7" s="338"/>
+      <c r="D7" s="333"/>
+      <c r="E7" s="333"/>
+      <c r="F7" s="333"/>
+      <c r="G7" s="333"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -18254,11 +18250,11 @@
         <v>205</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="329"/>
-      <c r="D8" s="329"/>
-      <c r="E8" s="329"/>
-      <c r="F8" s="329"/>
-      <c r="G8" s="329"/>
+      <c r="C8" s="333"/>
+      <c r="D8" s="333"/>
+      <c r="E8" s="333"/>
+      <c r="F8" s="333"/>
+      <c r="G8" s="333"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -18266,11 +18262,11 @@
         <v>18</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="335"/>
-      <c r="D9" s="335"/>
-      <c r="E9" s="335"/>
-      <c r="F9" s="335"/>
-      <c r="G9" s="335"/>
+      <c r="C9" s="339"/>
+      <c r="D9" s="339"/>
+      <c r="E9" s="339"/>
+      <c r="F9" s="339"/>
+      <c r="G9" s="339"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -18278,11 +18274,11 @@
         <v>283</v>
       </c>
       <c r="B10" s="90"/>
-      <c r="C10" s="329"/>
-      <c r="D10" s="329"/>
-      <c r="E10" s="329"/>
-      <c r="F10" s="329"/>
-      <c r="G10" s="329"/>
+      <c r="C10" s="333"/>
+      <c r="D10" s="333"/>
+      <c r="E10" s="333"/>
+      <c r="F10" s="333"/>
+      <c r="G10" s="333"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -18295,36 +18291,36 @@
       <c r="A12" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="336" t="s">
+      <c r="B12" s="340" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="337"/>
-      <c r="D12" s="338"/>
+      <c r="C12" s="341"/>
+      <c r="D12" s="342"/>
       <c r="N12" s="141" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="339" t="s">
+      <c r="B13" s="343" t="s">
         <v>190</v>
       </c>
-      <c r="C13" s="340"/>
-      <c r="D13" s="341"/>
+      <c r="C13" s="344"/>
+      <c r="D13" s="345"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="323" t="s">
+      <c r="B14" s="327" t="s">
         <v>185</v>
       </c>
-      <c r="C14" s="324"/>
-      <c r="D14" s="325"/>
+      <c r="C14" s="328"/>
+      <c r="D14" s="329"/>
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="326" t="s">
+      <c r="B15" s="330" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="327"/>
-      <c r="D15" s="328"/>
+      <c r="C15" s="331"/>
+      <c r="D15" s="332"/>
       <c r="N15" s="142"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -23096,8 +23092,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA15763-059F-401A-BB99-8A737E404CC4}">
   <dimension ref="A1:W34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E6" zoomScale="125" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="125" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23138,29 +23134,29 @@
     </row>
     <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:21" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I5" s="350" t="s">
+      <c r="I5" s="358" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="350" t="s">
+      <c r="J5" s="358" t="s">
         <v>214</v>
       </c>
-      <c r="K5" s="350" t="s">
+      <c r="K5" s="358" t="s">
         <v>215</v>
       </c>
-      <c r="L5" s="347" t="s">
+      <c r="L5" s="355" t="s">
         <v>216</v>
       </c>
-      <c r="M5" s="348"/>
-      <c r="N5" s="348"/>
-      <c r="O5" s="348"/>
-      <c r="P5" s="349"/>
-      <c r="Q5" s="343" t="s">
+      <c r="M5" s="356"/>
+      <c r="N5" s="356"/>
+      <c r="O5" s="356"/>
+      <c r="P5" s="357"/>
+      <c r="Q5" s="351" t="s">
         <v>217</v>
       </c>
-      <c r="R5" s="344"/>
-      <c r="S5" s="344"/>
-      <c r="T5" s="344"/>
-      <c r="U5" s="345"/>
+      <c r="R5" s="352"/>
+      <c r="S5" s="352"/>
+      <c r="T5" s="352"/>
+      <c r="U5" s="353"/>
     </row>
     <row r="6" spans="1:21" s="188" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="189" t="s">
@@ -23181,9 +23177,9 @@
       <c r="G6" s="189" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="351"/>
-      <c r="J6" s="351"/>
-      <c r="K6" s="351"/>
+      <c r="I6" s="359"/>
+      <c r="J6" s="359"/>
+      <c r="K6" s="359"/>
       <c r="L6" s="190" t="s">
         <v>219</v>
       </c>
@@ -23216,14 +23212,14 @@
       </c>
     </row>
     <row r="7" spans="1:21" s="188" customFormat="1" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="347" t="s">
+      <c r="B7" s="355" t="s">
         <v>229</v>
       </c>
-      <c r="C7" s="348"/>
-      <c r="D7" s="348"/>
-      <c r="E7" s="348"/>
-      <c r="F7" s="348"/>
-      <c r="G7" s="349"/>
+      <c r="C7" s="356"/>
+      <c r="D7" s="356"/>
+      <c r="E7" s="356"/>
+      <c r="F7" s="356"/>
+      <c r="G7" s="357"/>
       <c r="I7" s="192" t="s">
         <v>412</v>
       </c>
@@ -23491,13 +23487,13 @@
       <c r="B11" s="198" t="s">
         <v>235</v>
       </c>
-      <c r="C11" s="342" t="s">
+      <c r="C11" s="350" t="s">
         <v>236</v>
       </c>
-      <c r="D11" s="342"/>
-      <c r="E11" s="342"/>
-      <c r="F11" s="342"/>
-      <c r="G11" s="342"/>
+      <c r="D11" s="350"/>
+      <c r="E11" s="350"/>
+      <c r="F11" s="350"/>
+      <c r="G11" s="350"/>
       <c r="I11" s="192" t="s">
         <v>237</v>
       </c>
@@ -23551,14 +23547,14 @@
       </c>
     </row>
     <row r="12" spans="1:21" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B12" s="346" t="s">
+      <c r="B12" s="354" t="s">
         <v>238</v>
       </c>
-      <c r="C12" s="346"/>
-      <c r="D12" s="346"/>
-      <c r="E12" s="346"/>
-      <c r="F12" s="346"/>
-      <c r="G12" s="346"/>
+      <c r="C12" s="354"/>
+      <c r="D12" s="354"/>
+      <c r="E12" s="354"/>
+      <c r="F12" s="354"/>
+      <c r="G12" s="354"/>
       <c r="I12" s="192" t="s">
         <v>413</v>
       </c>
@@ -23590,19 +23586,19 @@
         <v>6.3</v>
       </c>
       <c r="Q12" s="195">
-        <f>L12/$K12</f>
+        <f t="shared" ref="Q12:T15" si="5">L12/$K12</f>
         <v>0.25874444444444439</v>
       </c>
       <c r="R12" s="195">
-        <f>M12/$K12</f>
+        <f t="shared" si="5"/>
         <v>3.334761904761905E-2</v>
       </c>
       <c r="S12" s="195">
-        <f>N12/$K12</f>
+        <f t="shared" si="5"/>
         <v>0.5412555555555556</v>
       </c>
       <c r="T12" s="195">
-        <f>O12/$K12</f>
+        <f t="shared" si="5"/>
         <v>0.16665238095238097</v>
       </c>
       <c r="U12" s="196">
@@ -23661,19 +23657,19 @@
         <v>5</v>
       </c>
       <c r="Q13" s="195">
-        <f>L13/$K13</f>
+        <f t="shared" si="5"/>
         <v>0.21335999999999994</v>
       </c>
       <c r="R13" s="195">
-        <f>M13/$K13</f>
+        <f t="shared" si="5"/>
         <v>3.3360000000000001E-2</v>
       </c>
       <c r="S13" s="195">
-        <f>N13/$K13</f>
+        <f t="shared" si="5"/>
         <v>0.58664000000000005</v>
       </c>
       <c r="T13" s="195">
-        <f>O13/$K13</f>
+        <f t="shared" si="5"/>
         <v>0.16664000000000004</v>
       </c>
       <c r="U13" s="196">
@@ -23690,15 +23686,15 @@
         <v>0.12998999999999999</v>
       </c>
       <c r="D14" s="201">
-        <f t="shared" ref="D14:F17" si="5">$B14*D$10</f>
+        <f t="shared" ref="D14:F17" si="6">$B14*D$10</f>
         <v>9.9900000000000006E-3</v>
       </c>
       <c r="E14" s="201">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.11001000000000001</v>
       </c>
       <c r="F14" s="201">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.0009999999999992E-2</v>
       </c>
       <c r="G14" s="201">
@@ -23736,19 +23732,19 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="Q14" s="195">
-        <f>L14/$K14</f>
+        <f t="shared" si="5"/>
         <v>0.19423478260869559</v>
       </c>
       <c r="R14" s="195">
-        <f>M14/$K14</f>
+        <f t="shared" si="5"/>
         <v>3.3365217391304346E-2</v>
       </c>
       <c r="S14" s="195">
-        <f>N14/$K14</f>
+        <f t="shared" si="5"/>
         <v>0.60576521739130451</v>
       </c>
       <c r="T14" s="195">
-        <f>O14/$K14</f>
+        <f t="shared" si="5"/>
         <v>0.16663478260869569</v>
       </c>
       <c r="U14" s="196">
@@ -23761,19 +23757,19 @@
         <v>0.4</v>
       </c>
       <c r="C15" s="201">
-        <f t="shared" ref="C15:C17" si="6">$B15*C$10</f>
+        <f t="shared" ref="C15:C17" si="7">$B15*C$10</f>
         <v>0.17332000000000003</v>
       </c>
       <c r="D15" s="201">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.3320000000000002E-2</v>
       </c>
       <c r="E15" s="201">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.14668</v>
       </c>
       <c r="F15" s="201">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.6680000000000003E-2</v>
       </c>
       <c r="G15" s="201">
@@ -23811,19 +23807,19 @@
         <v>3.8</v>
       </c>
       <c r="Q15" s="195">
-        <f>L15/$K15</f>
+        <f t="shared" si="5"/>
         <v>0.14390526315789462</v>
       </c>
       <c r="R15" s="195">
-        <f>M15/$K15</f>
+        <f t="shared" si="5"/>
         <v>3.337894736842105E-2</v>
       </c>
       <c r="S15" s="195">
-        <f>N15/$K15</f>
+        <f t="shared" si="5"/>
         <v>0.65609473684210529</v>
       </c>
       <c r="T15" s="195">
-        <f>O15/$K15</f>
+        <f t="shared" si="5"/>
         <v>0.166621052631579</v>
       </c>
       <c r="U15" s="196">
@@ -23836,23 +23832,23 @@
         <v>1</v>
       </c>
       <c r="C16" s="201">
+        <f t="shared" si="7"/>
+        <v>0.43330000000000002</v>
+      </c>
+      <c r="D16" s="201">
         <f t="shared" si="6"/>
-        <v>0.43330000000000002</v>
-      </c>
-      <c r="D16" s="201">
-        <f t="shared" si="5"/>
         <v>3.3300000000000003E-2</v>
       </c>
       <c r="E16" s="201">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.36670000000000003</v>
       </c>
       <c r="F16" s="201">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.16669999999999999</v>
       </c>
       <c r="G16" s="201">
-        <f t="shared" ref="G16:G17" si="7">SUM(C16:F16)</f>
+        <f t="shared" ref="G16:G17" si="8">SUM(C16:F16)</f>
         <v>1</v>
       </c>
       <c r="I16" s="192" t="s">
@@ -23911,39 +23907,38 @@
         <v>1.5</v>
       </c>
       <c r="C17" s="201">
+        <f t="shared" si="7"/>
+        <v>0.64995000000000003</v>
+      </c>
+      <c r="D17" s="201">
         <f t="shared" si="6"/>
-        <v>0.64995000000000003</v>
-      </c>
-      <c r="D17" s="201">
-        <f t="shared" si="5"/>
         <v>4.9950000000000008E-2</v>
       </c>
       <c r="E17" s="201">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.55005000000000004</v>
       </c>
       <c r="F17" s="201">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.25004999999999999</v>
       </c>
       <c r="G17" s="201">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1.5</v>
       </c>
-      <c r="I17" s="365"/>
     </row>
     <row r="18" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="B18" s="198" t="s">
         <v>235</v>
       </c>
-      <c r="C18" s="342" t="s">
+      <c r="C18" s="350" t="s">
         <v>236</v>
       </c>
-      <c r="D18" s="342"/>
-      <c r="E18" s="342"/>
-      <c r="F18" s="342"/>
-      <c r="G18" s="342"/>
-      <c r="I18" s="370" t="s">
+      <c r="D18" s="350"/>
+      <c r="E18" s="350"/>
+      <c r="F18" s="350"/>
+      <c r="G18" s="350"/>
+      <c r="I18" s="204" t="s">
         <v>418</v>
       </c>
     </row>
@@ -23965,12 +23960,6 @@
       <c r="U19" s="208"/>
     </row>
     <row r="20" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B20" s="365"/>
-      <c r="C20" s="365"/>
-      <c r="D20" s="365"/>
-      <c r="E20" s="365"/>
-      <c r="F20" s="365"/>
-      <c r="G20" s="365"/>
       <c r="I20" s="204" t="s">
         <v>420</v>
       </c>
@@ -23988,12 +23977,12 @@
       <c r="U20" s="208"/>
     </row>
     <row r="21" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B21" s="366"/>
-      <c r="C21" s="367"/>
-      <c r="D21" s="367"/>
-      <c r="E21" s="367"/>
-      <c r="F21" s="367"/>
-      <c r="G21" s="367"/>
+      <c r="B21" s="272"/>
+      <c r="C21" s="273"/>
+      <c r="D21" s="273"/>
+      <c r="E21" s="273"/>
+      <c r="F21" s="273"/>
+      <c r="G21" s="273"/>
       <c r="J21" s="205"/>
       <c r="K21" s="205"/>
       <c r="L21" s="206"/>
@@ -24008,73 +23997,73 @@
       <c r="U21" s="267"/>
     </row>
     <row r="22" spans="2:23" s="197" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B22" s="366"/>
-      <c r="C22" s="368"/>
-      <c r="D22" s="368"/>
-      <c r="E22" s="368"/>
-      <c r="F22" s="368"/>
-      <c r="G22" s="368"/>
-      <c r="I22" s="353" t="s">
+      <c r="B22" s="272"/>
+      <c r="C22" s="274"/>
+      <c r="D22" s="274"/>
+      <c r="E22" s="274"/>
+      <c r="F22" s="274"/>
+      <c r="G22" s="274"/>
+      <c r="I22" s="347" t="s">
         <v>423</v>
       </c>
-      <c r="J22" s="353"/>
-      <c r="K22" s="353"/>
-      <c r="L22" s="353"/>
-      <c r="M22" s="353"/>
-      <c r="N22" s="353"/>
-      <c r="O22" s="353"/>
-      <c r="P22" s="353"/>
-      <c r="Q22" s="353"/>
-      <c r="R22" s="353"/>
-      <c r="S22" s="353"/>
-      <c r="T22" s="353"/>
-      <c r="U22" s="353"/>
-      <c r="V22" s="353"/>
-      <c r="W22" s="353"/>
+      <c r="J22" s="347"/>
+      <c r="K22" s="347"/>
+      <c r="L22" s="347"/>
+      <c r="M22" s="347"/>
+      <c r="N22" s="347"/>
+      <c r="O22" s="347"/>
+      <c r="P22" s="347"/>
+      <c r="Q22" s="347"/>
+      <c r="R22" s="347"/>
+      <c r="S22" s="347"/>
+      <c r="T22" s="347"/>
+      <c r="U22" s="347"/>
+      <c r="V22" s="347"/>
+      <c r="W22" s="347"/>
     </row>
     <row r="23" spans="2:23" s="197" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B23" s="366"/>
-      <c r="C23" s="368"/>
-      <c r="D23" s="368"/>
-      <c r="E23" s="368"/>
-      <c r="F23" s="368"/>
-      <c r="G23" s="368"/>
-      <c r="I23" s="355" t="s">
+      <c r="B23" s="272"/>
+      <c r="C23" s="274"/>
+      <c r="D23" s="274"/>
+      <c r="E23" s="274"/>
+      <c r="F23" s="274"/>
+      <c r="G23" s="274"/>
+      <c r="I23" s="349" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="355" t="s">
+      <c r="J23" s="349" t="s">
         <v>214</v>
       </c>
-      <c r="K23" s="355" t="s">
+      <c r="K23" s="349" t="s">
         <v>215</v>
       </c>
-      <c r="L23" s="354" t="s">
+      <c r="L23" s="348" t="s">
         <v>216</v>
       </c>
-      <c r="M23" s="354"/>
-      <c r="N23" s="354"/>
-      <c r="O23" s="354"/>
-      <c r="P23" s="354"/>
-      <c r="Q23" s="354"/>
-      <c r="R23" s="352" t="s">
+      <c r="M23" s="348"/>
+      <c r="N23" s="348"/>
+      <c r="O23" s="348"/>
+      <c r="P23" s="348"/>
+      <c r="Q23" s="348"/>
+      <c r="R23" s="346" t="s">
         <v>217</v>
       </c>
-      <c r="S23" s="352"/>
-      <c r="T23" s="352"/>
-      <c r="U23" s="352"/>
-      <c r="V23" s="352"/>
-      <c r="W23" s="352"/>
+      <c r="S23" s="346"/>
+      <c r="T23" s="346"/>
+      <c r="U23" s="346"/>
+      <c r="V23" s="346"/>
+      <c r="W23" s="346"/>
     </row>
     <row r="24" spans="2:23" s="197" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B24" s="366"/>
-      <c r="C24" s="368"/>
-      <c r="D24" s="368"/>
-      <c r="E24" s="368"/>
-      <c r="F24" s="368"/>
-      <c r="G24" s="368"/>
-      <c r="I24" s="355"/>
-      <c r="J24" s="355"/>
-      <c r="K24" s="355"/>
+      <c r="B24" s="272"/>
+      <c r="C24" s="274"/>
+      <c r="D24" s="274"/>
+      <c r="E24" s="274"/>
+      <c r="F24" s="274"/>
+      <c r="G24" s="274"/>
+      <c r="I24" s="349"/>
+      <c r="J24" s="349"/>
+      <c r="K24" s="349"/>
       <c r="L24" s="190" t="s">
         <v>219</v>
       </c>
@@ -24113,12 +24102,6 @@
       </c>
     </row>
     <row r="25" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B25" s="365"/>
-      <c r="C25" s="365"/>
-      <c r="D25" s="365"/>
-      <c r="E25" s="365"/>
-      <c r="F25" s="365"/>
-      <c r="G25" s="365"/>
       <c r="I25" s="264" t="s">
         <v>412</v>
       </c>
@@ -24129,14 +24112,14 @@
         <v>9</v>
       </c>
       <c r="L25" s="265">
-        <f>L7-(0.824*P25)</f>
+        <f>L7-(0.824*P$25)</f>
         <v>2.0171999999999999</v>
       </c>
       <c r="M25" s="265">
         <v>0.3</v>
       </c>
       <c r="N25" s="265">
-        <f>N7-(P25*0.164)</f>
+        <f>N7-(P$25*0.164)</f>
         <v>4.2442000000000002</v>
       </c>
       <c r="O25" s="265">
@@ -24173,12 +24156,11 @@
       </c>
     </row>
     <row r="26" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B26" s="365"/>
-      <c r="C26" s="369"/>
-      <c r="D26" s="369"/>
-      <c r="E26" s="369"/>
-      <c r="F26" s="369"/>
-      <c r="G26" s="369"/>
+      <c r="C26" s="275"/>
+      <c r="D26" s="275"/>
+      <c r="E26" s="275"/>
+      <c r="F26" s="275"/>
+      <c r="G26" s="275"/>
       <c r="I26" s="264" t="s">
         <v>230</v>
       </c>
@@ -24189,57 +24171,56 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="L26" s="265">
-        <f t="shared" ref="L26:L34" si="8">L8-(0.824*P26)</f>
-        <v>0.27740520160000015</v>
+        <f t="shared" ref="L26:L34" si="9">L8-(0.824*P$25)</f>
+        <v>1.8872100000000001</v>
       </c>
       <c r="M26" s="265">
         <v>0.29000999999999999</v>
       </c>
       <c r="N26" s="265">
-        <f t="shared" ref="N26:N34" si="9">N8-(P26*0.164)</f>
-        <v>3.8137919576000003</v>
+        <f t="shared" ref="N26:N34" si="10">N8-(P$25*0.164)</f>
+        <v>4.1341900000000003</v>
       </c>
       <c r="O26" s="265">
         <v>1.4499900000000001</v>
       </c>
       <c r="P26" s="201">
-        <f>(0.164*N8)+(0.824*L8)</f>
-        <v>2.9036466000000001</v>
+        <f>L26+N26</f>
+        <v>6.0213999999999999</v>
       </c>
       <c r="Q26" s="265">
-        <f t="shared" ref="Q26:Q28" si="10">SUM(L26:P26)</f>
-        <v>8.7348437592000003</v>
+        <f t="shared" ref="Q26:Q28" si="11">SUM(L26:P26)</f>
+        <v>13.7828</v>
       </c>
       <c r="R26" s="269">
-        <f t="shared" ref="R26:R29" si="11">L26/K26</f>
-        <v>3.188565535632186E-2</v>
+        <f t="shared" ref="R26:R29" si="12">L26/K26</f>
+        <v>0.21692068965517244</v>
       </c>
       <c r="S26" s="269">
         <v>3.3334482758620693E-2</v>
       </c>
       <c r="T26" s="269">
-        <f t="shared" ref="T26:T29" si="12">N26/K26</f>
-        <v>0.43836689167816101</v>
+        <f t="shared" ref="T26:T29" si="13">N26/K26</f>
+        <v>0.47519425287356326</v>
       </c>
       <c r="U26" s="269">
         <v>0.16666551724137935</v>
       </c>
       <c r="V26" s="270">
-        <f t="shared" ref="V26:V29" si="13">P26/K26</f>
-        <v>0.33375248275862074</v>
+        <f t="shared" ref="V26:V29" si="14">P26/K26</f>
+        <v>0.69211494252873562</v>
       </c>
       <c r="W26" s="271">
-        <f t="shared" ref="W26:W29" si="14">SUM(R26:V26)</f>
-        <v>1.0040050297931036</v>
+        <f t="shared" ref="W26:W29" si="15">SUM(R26:V26)</f>
+        <v>1.5842298850574714</v>
       </c>
     </row>
     <row r="27" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B27" s="365"/>
-      <c r="C27" s="369"/>
-      <c r="D27" s="369"/>
-      <c r="E27" s="369"/>
-      <c r="F27" s="369"/>
-      <c r="G27" s="369"/>
+      <c r="C27" s="275"/>
+      <c r="D27" s="275"/>
+      <c r="E27" s="275"/>
+      <c r="F27" s="275"/>
+      <c r="G27" s="275"/>
       <c r="I27" s="264" t="s">
         <v>232</v>
       </c>
@@ -24250,57 +24231,51 @@
         <v>8.6</v>
       </c>
       <c r="L27" s="265">
-        <f t="shared" si="8"/>
-        <v>0.2684506687999999</v>
+        <f t="shared" si="9"/>
+        <v>1.84388</v>
       </c>
       <c r="M27" s="265">
         <v>0.28667999999999999</v>
       </c>
       <c r="N27" s="265">
-        <f t="shared" si="9"/>
-        <v>3.7839636768000005</v>
+        <f t="shared" si="10"/>
+        <v>4.0975200000000003</v>
       </c>
       <c r="O27" s="265">
         <v>1.4333199999999999</v>
       </c>
       <c r="P27" s="201">
-        <f t="shared" ref="P27:P29" si="15">(0.164*N9)+(0.824*L9)</f>
-        <v>2.8619288000000003</v>
+        <f t="shared" ref="P27:P34" si="16">L27+N27</f>
+        <v>5.9413999999999998</v>
       </c>
       <c r="Q27" s="265">
-        <f t="shared" si="10"/>
-        <v>8.6343431456000008</v>
+        <f t="shared" si="11"/>
+        <v>13.6028</v>
       </c>
       <c r="R27" s="269">
-        <f t="shared" si="11"/>
-        <v>3.1215194046511619E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.2144046511627907</v>
       </c>
       <c r="S27" s="269">
         <v>3.3334883720930235E-2</v>
       </c>
       <c r="T27" s="269">
-        <f t="shared" si="12"/>
-        <v>0.43999577637209308</v>
+        <f t="shared" si="13"/>
+        <v>0.47645581395348841</v>
       </c>
       <c r="U27" s="269">
         <v>0.16666511627906977</v>
       </c>
       <c r="V27" s="270">
-        <f t="shared" si="13"/>
-        <v>0.33278241860465119</v>
+        <f t="shared" si="14"/>
+        <v>0.69086046511627908</v>
       </c>
       <c r="W27" s="271">
-        <f t="shared" si="14"/>
-        <v>1.0039933890232557</v>
+        <f t="shared" si="15"/>
+        <v>1.5817209302325583</v>
       </c>
     </row>
     <row r="28" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B28" s="365"/>
-      <c r="C28" s="365"/>
-      <c r="D28" s="365"/>
-      <c r="E28" s="365"/>
-      <c r="F28" s="365"/>
-      <c r="G28" s="365"/>
       <c r="I28" s="264" t="s">
         <v>234</v>
       </c>
@@ -24311,57 +24286,56 @@
         <v>8</v>
       </c>
       <c r="L28" s="265">
-        <f t="shared" si="8"/>
-        <v>0.21472347200000019</v>
+        <f t="shared" si="9"/>
+        <v>1.5838999999999999</v>
       </c>
       <c r="M28" s="265">
         <v>0.26669999999999999</v>
       </c>
       <c r="N28" s="265">
-        <f t="shared" si="9"/>
-        <v>3.6049939920000007</v>
+        <f t="shared" si="10"/>
+        <v>3.8775000000000004</v>
       </c>
       <c r="O28" s="265">
         <v>1.3332999999999999</v>
       </c>
       <c r="P28" s="201">
-        <f t="shared" si="15"/>
-        <v>2.6116219999999997</v>
+        <f t="shared" si="16"/>
+        <v>5.4614000000000003</v>
       </c>
       <c r="Q28" s="265">
-        <f t="shared" si="10"/>
-        <v>8.031339464000002</v>
+        <f t="shared" si="11"/>
+        <v>12.5228</v>
       </c>
       <c r="R28" s="269">
-        <f t="shared" si="11"/>
-        <v>2.6840434000000024E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.19798749999999998</v>
       </c>
       <c r="S28" s="269">
         <v>3.3337499999999999E-2</v>
       </c>
       <c r="T28" s="269">
-        <f t="shared" si="12"/>
-        <v>0.45062424900000009</v>
+        <f t="shared" si="13"/>
+        <v>0.48468750000000005</v>
       </c>
       <c r="U28" s="269">
         <v>0.16666249999999999</v>
       </c>
       <c r="V28" s="270">
-        <f t="shared" si="13"/>
-        <v>0.32645274999999996</v>
+        <f t="shared" si="14"/>
+        <v>0.68267500000000003</v>
       </c>
       <c r="W28" s="271">
-        <f t="shared" si="14"/>
-        <v>1.0039174330000002</v>
+        <f t="shared" si="15"/>
+        <v>1.56535</v>
       </c>
     </row>
     <row r="29" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B29" s="365"/>
-      <c r="C29" s="369"/>
-      <c r="D29" s="369"/>
-      <c r="E29" s="369"/>
-      <c r="F29" s="369"/>
-      <c r="G29" s="369"/>
+      <c r="C29" s="275"/>
+      <c r="D29" s="275"/>
+      <c r="E29" s="275"/>
+      <c r="F29" s="275"/>
+      <c r="G29" s="275"/>
       <c r="I29" s="264" t="s">
         <v>237</v>
       </c>
@@ -24372,57 +24346,56 @@
         <v>7.5</v>
       </c>
       <c r="L29" s="265">
-        <f t="shared" si="8"/>
-        <v>0.16995080800000006</v>
+        <f t="shared" si="9"/>
+        <v>1.3672499999999999</v>
       </c>
       <c r="M29" s="265">
         <v>0.25004999999999999</v>
       </c>
       <c r="N29" s="265">
-        <f t="shared" si="9"/>
-        <v>3.4558525880000004</v>
+        <f t="shared" si="10"/>
+        <v>3.69415</v>
       </c>
       <c r="O29" s="265">
         <v>1.2499500000000001</v>
       </c>
       <c r="P29" s="201">
-        <f t="shared" si="15"/>
-        <v>2.4030329999999998</v>
+        <f t="shared" si="16"/>
+        <v>5.0613999999999999</v>
       </c>
       <c r="Q29" s="265">
         <f>SUM(L29:P29)</f>
-        <v>7.528836396</v>
+        <v>11.6228</v>
       </c>
       <c r="R29" s="269">
-        <f t="shared" si="11"/>
-        <v>2.2660107733333341E-2</v>
+        <f t="shared" si="12"/>
+        <v>0.18229999999999999</v>
       </c>
       <c r="S29" s="269">
         <v>3.3340000000000002E-2</v>
       </c>
       <c r="T29" s="269">
-        <f t="shared" si="12"/>
-        <v>0.46078034506666671</v>
+        <f t="shared" si="13"/>
+        <v>0.49255333333333334</v>
       </c>
       <c r="U29" s="269">
         <v>0.16666</v>
       </c>
       <c r="V29" s="270">
-        <f t="shared" si="13"/>
-        <v>0.32040439999999998</v>
+        <f t="shared" si="14"/>
+        <v>0.67485333333333331</v>
       </c>
       <c r="W29" s="271">
-        <f t="shared" si="14"/>
-        <v>1.0038448528000001</v>
+        <f t="shared" si="15"/>
+        <v>1.5497066666666668</v>
       </c>
     </row>
     <row r="30" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B30" s="365"/>
-      <c r="C30" s="369"/>
-      <c r="D30" s="369"/>
-      <c r="E30" s="369"/>
-      <c r="F30" s="369"/>
-      <c r="G30" s="369"/>
+      <c r="C30" s="275"/>
+      <c r="D30" s="275"/>
+      <c r="E30" s="275"/>
+      <c r="F30" s="275"/>
+      <c r="G30" s="275"/>
       <c r="I30" s="264" t="s">
         <v>413</v>
       </c>
@@ -24433,56 +24406,55 @@
         <v>6.3</v>
       </c>
       <c r="L30" s="265">
-        <f t="shared" si="8"/>
-        <v>6.2496414399999756E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.84728999999999965</v>
       </c>
       <c r="M30" s="265">
         <v>0.21009</v>
       </c>
       <c r="N30" s="265">
-        <f t="shared" si="9"/>
-        <v>3.0979132184</v>
+        <f t="shared" si="10"/>
+        <v>3.2541099999999998</v>
       </c>
       <c r="O30" s="265">
         <v>1.0499100000000001</v>
       </c>
       <c r="P30" s="201">
-        <f>(N12*0.164)+(L12*0.824)</f>
-        <v>1.9024193999999999</v>
+        <f t="shared" si="16"/>
+        <v>4.1013999999999999</v>
       </c>
       <c r="Q30" s="265">
         <v>6.3</v>
       </c>
       <c r="R30" s="269">
         <f>L30/K30</f>
-        <v>9.9200657777777385E-3</v>
+        <v>0.13449047619047613</v>
       </c>
       <c r="S30" s="269">
         <v>3.334761904761905E-2</v>
       </c>
       <c r="T30" s="269">
         <f>N30/K30</f>
-        <v>0.49173225688888889</v>
+        <v>0.51652539682539678</v>
       </c>
       <c r="U30" s="269">
         <v>0.16665238095238097</v>
       </c>
       <c r="V30" s="270">
         <f>P30/K30</f>
-        <v>0.30197133333333331</v>
+        <v>0.65101587301587305</v>
       </c>
       <c r="W30" s="271">
         <f>SUM(R30:V30)</f>
-        <v>1.003623656</v>
+        <v>1.5020317460317461</v>
       </c>
     </row>
     <row r="31" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B31" s="365"/>
-      <c r="C31" s="369"/>
-      <c r="D31" s="369"/>
-      <c r="E31" s="369"/>
-      <c r="F31" s="369"/>
-      <c r="G31" s="369"/>
+      <c r="C31" s="275"/>
+      <c r="D31" s="275"/>
+      <c r="E31" s="275"/>
+      <c r="F31" s="275"/>
+      <c r="G31" s="275"/>
       <c r="I31" s="264" t="s">
         <v>414</v>
       </c>
@@ -24493,56 +24465,55 @@
         <v>5</v>
       </c>
       <c r="L31" s="265">
-        <f t="shared" si="8"/>
-        <v>-5.3912511999999913E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.28399999999999981</v>
       </c>
       <c r="M31" s="265">
         <v>0.1668</v>
       </c>
       <c r="N31" s="265">
-        <f t="shared" si="9"/>
-        <v>2.7101455680000002</v>
+        <f t="shared" si="10"/>
+        <v>2.7774000000000001</v>
       </c>
       <c r="O31" s="265">
         <v>0.83320000000000016</v>
       </c>
       <c r="P31" s="201">
-        <f>(N13*0.164)+(L13*0.824)</f>
-        <v>1.3600879999999997</v>
+        <f t="shared" si="16"/>
+        <v>3.0613999999999999</v>
       </c>
       <c r="Q31" s="265">
         <v>5</v>
       </c>
       <c r="R31" s="269">
-        <f t="shared" ref="R31:R34" si="16">L31/K31</f>
-        <v>-1.0782502399999982E-2</v>
+        <f t="shared" ref="R31:R34" si="17">L31/K31</f>
+        <v>5.6799999999999962E-2</v>
       </c>
       <c r="S31" s="269">
         <v>3.3360000000000001E-2</v>
       </c>
       <c r="T31" s="269">
-        <f t="shared" ref="T31:T34" si="17">N31/K31</f>
-        <v>0.54202911360000006</v>
+        <f t="shared" ref="T31:T34" si="18">N31/K31</f>
+        <v>0.55547999999999997</v>
       </c>
       <c r="U31" s="269">
         <v>0.16664000000000004</v>
       </c>
       <c r="V31" s="270">
-        <f t="shared" ref="V31:V34" si="18">P31/K31</f>
-        <v>0.27201759999999997</v>
+        <f t="shared" ref="V31:V34" si="19">P31/K31</f>
+        <v>0.61227999999999994</v>
       </c>
       <c r="W31" s="271">
-        <f t="shared" ref="W31:W34" si="19">SUM(R31:V31)</f>
-        <v>1.0032642112000001</v>
+        <f t="shared" ref="W31:W34" si="20">SUM(R31:V31)</f>
+        <v>1.42456</v>
       </c>
     </row>
     <row r="32" spans="2:23" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B32" s="365"/>
-      <c r="C32" s="369"/>
-      <c r="D32" s="369"/>
-      <c r="E32" s="369"/>
-      <c r="F32" s="369"/>
-      <c r="G32" s="369"/>
+      <c r="C32" s="275"/>
+      <c r="D32" s="275"/>
+      <c r="E32" s="275"/>
+      <c r="F32" s="275"/>
+      <c r="G32" s="275"/>
       <c r="I32" s="264" t="s">
         <v>415</v>
       </c>
@@ -24553,47 +24524,47 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="L32" s="265">
-        <f t="shared" si="8"/>
-        <v>-8.9730643200000015E-2</v>
+        <f t="shared" si="9"/>
+        <v>0.11067999999999967</v>
       </c>
       <c r="M32" s="265">
         <v>0.15347999999999998</v>
       </c>
       <c r="N32" s="265">
-        <f t="shared" si="9"/>
-        <v>2.5908324448000002</v>
+        <f t="shared" si="10"/>
+        <v>2.6307200000000002</v>
       </c>
       <c r="O32" s="265">
         <v>0.76652000000000009</v>
       </c>
       <c r="P32" s="201">
-        <f>(N14*0.164)+(L14*0.824)</f>
-        <v>1.1932167999999996</v>
+        <f t="shared" si="16"/>
+        <v>2.7413999999999996</v>
       </c>
       <c r="Q32" s="265">
         <v>4.5999999999999996</v>
       </c>
       <c r="R32" s="269">
-        <f t="shared" si="16"/>
-        <v>-1.9506661565217395E-2</v>
+        <f t="shared" si="17"/>
+        <v>2.4060869565217319E-2</v>
       </c>
       <c r="S32" s="269">
         <v>3.3365217391304346E-2</v>
       </c>
       <c r="T32" s="269">
-        <f t="shared" si="17"/>
-        <v>0.56322444452173925</v>
+        <f t="shared" si="18"/>
+        <v>0.57189565217391314</v>
       </c>
       <c r="U32" s="269">
         <v>0.16663478260869569</v>
       </c>
       <c r="V32" s="270">
-        <f t="shared" si="18"/>
-        <v>0.25939495652173905</v>
+        <f t="shared" si="19"/>
+        <v>0.59595652173913038</v>
       </c>
       <c r="W32" s="271">
-        <f t="shared" si="19"/>
-        <v>1.0031127394782611</v>
+        <f t="shared" si="20"/>
+        <v>1.3919130434782607</v>
       </c>
     </row>
     <row r="33" spans="9:23" x14ac:dyDescent="0.2">
@@ -24607,47 +24578,47 @@
         <v>3.8</v>
       </c>
       <c r="L33" s="265">
-        <f t="shared" si="8"/>
-        <v>-0.16136690560000011</v>
+        <f t="shared" si="9"/>
+        <v>-0.23596000000000039</v>
       </c>
       <c r="M33" s="265">
         <v>0.12683999999999998</v>
       </c>
       <c r="N33" s="265">
-        <f t="shared" si="9"/>
-        <v>2.3522061984000002</v>
+        <f t="shared" si="10"/>
+        <v>2.3373599999999999</v>
       </c>
       <c r="O33" s="265">
         <v>0.63316000000000017</v>
       </c>
       <c r="P33" s="201">
-        <f>(N15*0.164)+(L15*0.824)</f>
-        <v>0.85947439999999964</v>
+        <f t="shared" si="16"/>
+        <v>2.1013999999999995</v>
       </c>
       <c r="Q33" s="265">
         <v>3.8</v>
       </c>
       <c r="R33" s="269">
-        <f t="shared" si="16"/>
-        <v>-4.2464975157894769E-2</v>
+        <f t="shared" si="17"/>
+        <v>-6.2094736842105369E-2</v>
       </c>
       <c r="S33" s="269">
         <v>3.337894736842105E-2</v>
       </c>
       <c r="T33" s="269">
-        <f t="shared" si="17"/>
-        <v>0.61900163115789486</v>
+        <f t="shared" si="18"/>
+        <v>0.61509473684210525</v>
       </c>
       <c r="U33" s="269">
         <v>0.166621052631579</v>
       </c>
       <c r="V33" s="270">
-        <f t="shared" si="18"/>
-        <v>0.22617747368421043</v>
+        <f t="shared" si="19"/>
+        <v>0.55299999999999994</v>
       </c>
       <c r="W33" s="271">
-        <f t="shared" si="19"/>
-        <v>1.0027141296842106</v>
+        <f t="shared" si="20"/>
+        <v>1.3059999999999998</v>
       </c>
     </row>
     <row r="34" spans="9:23" x14ac:dyDescent="0.2">
@@ -24661,57 +24632,51 @@
         <v>1</v>
       </c>
       <c r="L34" s="265">
-        <f t="shared" si="8"/>
-        <v>9.9200657777777923E-3</v>
+        <f t="shared" si="9"/>
+        <v>-0.5240555555555555</v>
       </c>
       <c r="M34" s="265">
         <v>3.334761904761905E-2</v>
       </c>
       <c r="N34" s="265">
-        <f t="shared" si="9"/>
-        <v>0.49173225688888894</v>
+        <f t="shared" si="10"/>
+        <v>0.38545555555555561</v>
       </c>
       <c r="O34" s="265">
         <v>0.16665238095238097</v>
       </c>
       <c r="P34" s="201">
-        <f>(N16*0.164)+(L16*0.824)</f>
-        <v>0.30197133333333326</v>
+        <f t="shared" si="16"/>
+        <v>-0.13859999999999989</v>
       </c>
       <c r="Q34" s="265">
         <v>1</v>
       </c>
       <c r="R34" s="269">
-        <f t="shared" si="16"/>
-        <v>9.9200657777777923E-3</v>
+        <f t="shared" si="17"/>
+        <v>-0.5240555555555555</v>
       </c>
       <c r="S34" s="269">
         <v>3.334761904761905E-2</v>
       </c>
       <c r="T34" s="269">
-        <f t="shared" si="17"/>
-        <v>0.49173225688888894</v>
+        <f t="shared" si="18"/>
+        <v>0.38545555555555561</v>
       </c>
       <c r="U34" s="269">
         <v>0.16665238095238097</v>
       </c>
       <c r="V34" s="270">
-        <f t="shared" si="18"/>
-        <v>0.30197133333333326</v>
+        <f t="shared" si="19"/>
+        <v>-0.13859999999999989</v>
       </c>
       <c r="W34" s="271">
-        <f t="shared" si="19"/>
-        <v>1.003623656</v>
+        <f t="shared" si="20"/>
+        <v>-7.7199999999999741E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="R23:W23"/>
-    <mergeCell ref="I22:W22"/>
-    <mergeCell ref="L23:Q23"/>
-    <mergeCell ref="I23:I24"/>
-    <mergeCell ref="J23:J24"/>
-    <mergeCell ref="K23:K24"/>
     <mergeCell ref="C18:G18"/>
     <mergeCell ref="Q5:U5"/>
     <mergeCell ref="C11:G11"/>
@@ -24721,6 +24686,12 @@
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:P5"/>
+    <mergeCell ref="R23:W23"/>
+    <mergeCell ref="I22:W22"/>
+    <mergeCell ref="L23:Q23"/>
+    <mergeCell ref="I23:I24"/>
+    <mergeCell ref="J23:J24"/>
+    <mergeCell ref="K23:K24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -25056,16 +25027,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="356" t="e">
+      <c r="A1" s="361" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="356"/>
-      <c r="C1" s="356"/>
-      <c r="D1" s="356"/>
-      <c r="E1" s="356"/>
-      <c r="F1" s="356"/>
-      <c r="G1" s="356"/>
+      <c r="B1" s="361"/>
+      <c r="C1" s="361"/>
+      <c r="D1" s="361"/>
+      <c r="E1" s="361"/>
+      <c r="F1" s="361"/>
+      <c r="G1" s="361"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -25074,15 +25045,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="330" t="s">
+      <c r="A3" s="334" t="s">
         <v>178</v>
       </c>
-      <c r="B3" s="330"/>
-      <c r="C3" s="330"/>
-      <c r="D3" s="330"/>
-      <c r="E3" s="330"/>
-      <c r="F3" s="330"/>
-      <c r="G3" s="330"/>
+      <c r="B3" s="334"/>
+      <c r="C3" s="334"/>
+      <c r="D3" s="334"/>
+      <c r="E3" s="334"/>
+      <c r="F3" s="334"/>
+      <c r="G3" s="334"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -25098,13 +25069,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="331" t="s">
+      <c r="C4" s="335" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="332"/>
-      <c r="E4" s="332"/>
-      <c r="F4" s="332"/>
-      <c r="G4" s="333"/>
+      <c r="D4" s="336"/>
+      <c r="E4" s="336"/>
+      <c r="F4" s="336"/>
+      <c r="G4" s="337"/>
       <c r="N4" s="139" t="s">
         <v>129</v>
       </c>
@@ -25114,11 +25085,11 @@
         <v>16</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="334"/>
-      <c r="D5" s="329"/>
-      <c r="E5" s="329"/>
-      <c r="F5" s="329"/>
-      <c r="G5" s="329"/>
+      <c r="C5" s="338"/>
+      <c r="D5" s="333"/>
+      <c r="E5" s="333"/>
+      <c r="F5" s="333"/>
+      <c r="G5" s="333"/>
       <c r="N5" s="142"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -25126,11 +25097,11 @@
         <v>17</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="334"/>
-      <c r="D6" s="329"/>
-      <c r="E6" s="329"/>
-      <c r="F6" s="329"/>
-      <c r="G6" s="329"/>
+      <c r="C6" s="338"/>
+      <c r="D6" s="333"/>
+      <c r="E6" s="333"/>
+      <c r="F6" s="333"/>
+      <c r="G6" s="333"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -25138,11 +25109,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="334"/>
-      <c r="D7" s="329"/>
-      <c r="E7" s="329"/>
-      <c r="F7" s="329"/>
-      <c r="G7" s="329"/>
+      <c r="C7" s="338"/>
+      <c r="D7" s="333"/>
+      <c r="E7" s="333"/>
+      <c r="F7" s="333"/>
+      <c r="G7" s="333"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -25150,11 +25121,11 @@
         <v>39</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="329"/>
-      <c r="D8" s="329"/>
-      <c r="E8" s="329"/>
-      <c r="F8" s="329"/>
-      <c r="G8" s="329"/>
+      <c r="C8" s="333"/>
+      <c r="D8" s="333"/>
+      <c r="E8" s="333"/>
+      <c r="F8" s="333"/>
+      <c r="G8" s="333"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -25162,11 +25133,11 @@
         <v>163</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="335"/>
-      <c r="D9" s="335"/>
-      <c r="E9" s="335"/>
-      <c r="F9" s="335"/>
-      <c r="G9" s="335"/>
+      <c r="C9" s="339"/>
+      <c r="D9" s="339"/>
+      <c r="E9" s="339"/>
+      <c r="F9" s="339"/>
+      <c r="G9" s="339"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -25174,11 +25145,11 @@
         <v>41</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="357"/>
-      <c r="D10" s="357"/>
-      <c r="E10" s="357"/>
-      <c r="F10" s="357"/>
-      <c r="G10" s="357"/>
+      <c r="C10" s="360"/>
+      <c r="D10" s="360"/>
+      <c r="E10" s="360"/>
+      <c r="F10" s="360"/>
+      <c r="G10" s="360"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -25191,37 +25162,37 @@
       <c r="A12" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="336" t="s">
+      <c r="B12" s="340" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="337"/>
-      <c r="D12" s="338"/>
+      <c r="C12" s="341"/>
+      <c r="D12" s="342"/>
       <c r="N12" s="141" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="339" t="s">
+      <c r="B13" s="343" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="340"/>
-      <c r="D13" s="341"/>
+      <c r="C13" s="344"/>
+      <c r="D13" s="345"/>
       <c r="N13" s="142"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="323" t="s">
+      <c r="B14" s="327" t="s">
         <v>115</v>
       </c>
-      <c r="C14" s="324"/>
-      <c r="D14" s="325"/>
+      <c r="C14" s="328"/>
+      <c r="D14" s="329"/>
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="326" t="s">
+      <c r="B15" s="330" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="327"/>
-      <c r="D15" s="328"/>
+      <c r="C15" s="331"/>
+      <c r="D15" s="332"/>
       <c r="N15" s="142"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -26441,6 +26412,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -26448,12 +26425,6 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>
@@ -26511,26 +26482,26 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="358" t="s">
+      <c r="D3" s="362" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="358"/>
-      <c r="F3" s="358" t="s">
+      <c r="E3" s="362"/>
+      <c r="F3" s="362" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="358"/>
-      <c r="H3" s="358"/>
-      <c r="I3" s="358" t="s">
+      <c r="G3" s="362"/>
+      <c r="H3" s="362"/>
+      <c r="I3" s="362" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="358"/>
-      <c r="K3" s="358"/>
+      <c r="J3" s="362"/>
+      <c r="K3" s="362"/>
       <c r="L3" s="134"/>
-      <c r="M3" s="358" t="s">
+      <c r="M3" s="362" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="358"/>
-      <c r="O3" s="358"/>
+      <c r="N3" s="362"/>
+      <c r="O3" s="362"/>
     </row>
     <row r="4" spans="1:16" s="47" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">

</xml_diff>

<commit_message>
Anabelle updated version sheet
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anabelle/Documents/ColoradoRiverCollaborate/LakeMeadWaterBankDivideInflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80961537-936D-DA44-8A26-593CE805736F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74491010-B274-6E44-8D4B-0A4A007124C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="443">
   <si>
     <t>Year 1</t>
   </si>
@@ -2210,6 +2210,9 @@
   <si>
     <t>[6]</t>
   </si>
+  <si>
+    <t>1.5.1</t>
+  </si>
 </sst>
 </file>
 
@@ -3800,68 +3803,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="18" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="31" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="28" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3917,6 +3866,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -3949,6 +3904,63 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="28" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4025,8 +4037,47 @@
     <xf numFmtId="0" fontId="18" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4049,50 +4100,11 @@
     <xf numFmtId="0" fontId="18" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4120,15 +4132,6 @@
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="18" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="31" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="9" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="15">
@@ -15689,20 +15692,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="319" t="s">
+      <c r="A1" s="301" t="s">
         <v>300</v>
       </c>
-      <c r="B1" s="319"/>
-      <c r="C1" s="319"/>
-      <c r="D1" s="319"/>
-      <c r="E1" s="319"/>
-      <c r="F1" s="319"/>
-      <c r="G1" s="319"/>
-      <c r="H1" s="319"/>
-      <c r="I1" s="319"/>
-      <c r="J1" s="319"/>
-      <c r="K1" s="319"/>
-      <c r="L1" s="319"/>
+      <c r="B1" s="301"/>
+      <c r="C1" s="301"/>
+      <c r="D1" s="301"/>
+      <c r="E1" s="301"/>
+      <c r="F1" s="301"/>
+      <c r="G1" s="301"/>
+      <c r="H1" s="301"/>
+      <c r="I1" s="301"/>
+      <c r="J1" s="301"/>
+      <c r="K1" s="301"/>
+      <c r="L1" s="301"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -15728,41 +15731,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="54" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="320" t="s">
+      <c r="A4" s="302" t="s">
         <v>301</v>
       </c>
-      <c r="B4" s="321"/>
-      <c r="C4" s="321"/>
-      <c r="D4" s="321"/>
-      <c r="E4" s="321"/>
-      <c r="F4" s="321"/>
-      <c r="G4" s="321"/>
-      <c r="H4" s="321"/>
-      <c r="I4" s="321"/>
-      <c r="J4" s="321"/>
-      <c r="K4" s="321"/>
-      <c r="L4" s="322"/>
-      <c r="N4" s="323"/>
-      <c r="O4" s="323"/>
-      <c r="P4" s="323"/>
-      <c r="Q4" s="323"/>
-      <c r="R4" s="323"/>
+      <c r="B4" s="303"/>
+      <c r="C4" s="303"/>
+      <c r="D4" s="303"/>
+      <c r="E4" s="303"/>
+      <c r="F4" s="303"/>
+      <c r="G4" s="303"/>
+      <c r="H4" s="303"/>
+      <c r="I4" s="303"/>
+      <c r="J4" s="303"/>
+      <c r="K4" s="303"/>
+      <c r="L4" s="304"/>
+      <c r="N4" s="305"/>
+      <c r="O4" s="305"/>
+      <c r="P4" s="305"/>
+      <c r="Q4" s="305"/>
+      <c r="R4" s="305"/>
     </row>
     <row r="5" spans="1:18" s="54" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="324" t="s">
+      <c r="A5" s="306" t="s">
         <v>284</v>
       </c>
-      <c r="B5" s="325"/>
-      <c r="C5" s="325"/>
-      <c r="D5" s="325"/>
-      <c r="E5" s="325"/>
-      <c r="F5" s="325"/>
-      <c r="G5" s="325"/>
-      <c r="H5" s="325"/>
-      <c r="I5" s="325"/>
-      <c r="J5" s="325"/>
-      <c r="K5" s="325"/>
-      <c r="L5" s="326"/>
+      <c r="B5" s="307"/>
+      <c r="C5" s="307"/>
+      <c r="D5" s="307"/>
+      <c r="E5" s="307"/>
+      <c r="F5" s="307"/>
+      <c r="G5" s="307"/>
+      <c r="H5" s="307"/>
+      <c r="I5" s="307"/>
+      <c r="J5" s="307"/>
+      <c r="K5" s="307"/>
+      <c r="L5" s="308"/>
       <c r="N5" s="113"/>
       <c r="O5" s="113"/>
       <c r="P5" s="113"/>
@@ -15770,20 +15773,20 @@
       <c r="R5" s="113"/>
     </row>
     <row r="6" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="324" t="s">
+      <c r="A6" s="306" t="s">
         <v>302</v>
       </c>
-      <c r="B6" s="325"/>
-      <c r="C6" s="325"/>
-      <c r="D6" s="325"/>
-      <c r="E6" s="325"/>
-      <c r="F6" s="325"/>
-      <c r="G6" s="325"/>
-      <c r="H6" s="325"/>
-      <c r="I6" s="325"/>
-      <c r="J6" s="325"/>
-      <c r="K6" s="325"/>
-      <c r="L6" s="326"/>
+      <c r="B6" s="307"/>
+      <c r="C6" s="307"/>
+      <c r="D6" s="307"/>
+      <c r="E6" s="307"/>
+      <c r="F6" s="307"/>
+      <c r="G6" s="307"/>
+      <c r="H6" s="307"/>
+      <c r="I6" s="307"/>
+      <c r="J6" s="307"/>
+      <c r="K6" s="307"/>
+      <c r="L6" s="308"/>
       <c r="N6" s="113"/>
       <c r="O6" s="113"/>
       <c r="P6" s="113"/>
@@ -15792,19 +15795,19 @@
     </row>
     <row r="7" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="227"/>
-      <c r="B7" s="325" t="s">
+      <c r="B7" s="307" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="325"/>
-      <c r="D7" s="325"/>
-      <c r="E7" s="325"/>
-      <c r="F7" s="325"/>
-      <c r="G7" s="325"/>
-      <c r="H7" s="325"/>
-      <c r="I7" s="325"/>
-      <c r="J7" s="325"/>
-      <c r="K7" s="325"/>
-      <c r="L7" s="326"/>
+      <c r="C7" s="307"/>
+      <c r="D7" s="307"/>
+      <c r="E7" s="307"/>
+      <c r="F7" s="307"/>
+      <c r="G7" s="307"/>
+      <c r="H7" s="307"/>
+      <c r="I7" s="307"/>
+      <c r="J7" s="307"/>
+      <c r="K7" s="307"/>
+      <c r="L7" s="308"/>
       <c r="N7" s="113"/>
       <c r="O7" s="113"/>
       <c r="P7" s="113"/>
@@ -15813,19 +15816,19 @@
     </row>
     <row r="8" spans="1:18" s="54" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="228"/>
-      <c r="B8" s="340" t="s">
+      <c r="B8" s="324" t="s">
         <v>304</v>
       </c>
-      <c r="C8" s="340"/>
-      <c r="D8" s="340"/>
-      <c r="E8" s="340"/>
-      <c r="F8" s="340"/>
-      <c r="G8" s="340"/>
-      <c r="H8" s="340"/>
-      <c r="I8" s="340"/>
-      <c r="J8" s="340"/>
-      <c r="K8" s="340"/>
-      <c r="L8" s="341"/>
+      <c r="C8" s="324"/>
+      <c r="D8" s="324"/>
+      <c r="E8" s="324"/>
+      <c r="F8" s="324"/>
+      <c r="G8" s="324"/>
+      <c r="H8" s="324"/>
+      <c r="I8" s="324"/>
+      <c r="J8" s="324"/>
+      <c r="K8" s="324"/>
+      <c r="L8" s="325"/>
       <c r="N8" s="113"/>
       <c r="O8" s="113"/>
       <c r="P8" s="113"/>
@@ -15847,38 +15850,38 @@
       <c r="L9" s="113"/>
     </row>
     <row r="10" spans="1:18" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="342" t="s">
+      <c r="A10" s="326" t="s">
         <v>339</v>
       </c>
-      <c r="B10" s="343"/>
-      <c r="C10" s="343"/>
-      <c r="D10" s="343"/>
-      <c r="E10" s="343"/>
-      <c r="F10" s="343"/>
-      <c r="G10" s="343"/>
-      <c r="H10" s="343"/>
-      <c r="I10" s="343"/>
-      <c r="J10" s="343"/>
-      <c r="K10" s="343"/>
-      <c r="L10" s="344"/>
+      <c r="B10" s="327"/>
+      <c r="C10" s="327"/>
+      <c r="D10" s="327"/>
+      <c r="E10" s="327"/>
+      <c r="F10" s="327"/>
+      <c r="G10" s="327"/>
+      <c r="H10" s="327"/>
+      <c r="I10" s="327"/>
+      <c r="J10" s="327"/>
+      <c r="K10" s="327"/>
+      <c r="L10" s="328"/>
     </row>
     <row r="11" spans="1:18" s="58" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="248" t="s">
         <v>340</v>
       </c>
-      <c r="B11" s="297" t="s">
+      <c r="B11" s="329" t="s">
         <v>343</v>
       </c>
-      <c r="C11" s="297"/>
-      <c r="D11" s="297"/>
-      <c r="E11" s="297"/>
-      <c r="F11" s="297"/>
-      <c r="G11" s="297"/>
-      <c r="H11" s="297"/>
-      <c r="I11" s="297"/>
-      <c r="J11" s="297"/>
-      <c r="K11" s="297"/>
-      <c r="L11" s="298"/>
+      <c r="C11" s="329"/>
+      <c r="D11" s="329"/>
+      <c r="E11" s="329"/>
+      <c r="F11" s="329"/>
+      <c r="G11" s="329"/>
+      <c r="H11" s="329"/>
+      <c r="I11" s="329"/>
+      <c r="J11" s="329"/>
+      <c r="K11" s="329"/>
+      <c r="L11" s="330"/>
     </row>
     <row r="12" spans="1:18" s="59" customFormat="1" ht="161.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="240"/>
@@ -15898,51 +15901,51 @@
       <c r="A13" s="248" t="s">
         <v>341</v>
       </c>
-      <c r="B13" s="297" t="s">
+      <c r="B13" s="329" t="s">
         <v>344</v>
       </c>
-      <c r="C13" s="297"/>
-      <c r="D13" s="297"/>
-      <c r="E13" s="297"/>
-      <c r="F13" s="297"/>
-      <c r="G13" s="297"/>
-      <c r="H13" s="297"/>
-      <c r="I13" s="297"/>
-      <c r="J13" s="297"/>
-      <c r="K13" s="297"/>
-      <c r="L13" s="298"/>
+      <c r="C13" s="329"/>
+      <c r="D13" s="329"/>
+      <c r="E13" s="329"/>
+      <c r="F13" s="329"/>
+      <c r="G13" s="329"/>
+      <c r="H13" s="329"/>
+      <c r="I13" s="329"/>
+      <c r="J13" s="329"/>
+      <c r="K13" s="329"/>
+      <c r="L13" s="330"/>
     </row>
     <row r="14" spans="1:18" s="59" customFormat="1" ht="90.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="240"/>
-      <c r="B14" s="299"/>
-      <c r="C14" s="299"/>
-      <c r="D14" s="299"/>
-      <c r="E14" s="299"/>
-      <c r="F14" s="299"/>
-      <c r="G14" s="299"/>
-      <c r="H14" s="299"/>
-      <c r="I14" s="299"/>
-      <c r="J14" s="299"/>
-      <c r="K14" s="299"/>
-      <c r="L14" s="300"/>
+      <c r="B14" s="340"/>
+      <c r="C14" s="340"/>
+      <c r="D14" s="340"/>
+      <c r="E14" s="340"/>
+      <c r="F14" s="340"/>
+      <c r="G14" s="340"/>
+      <c r="H14" s="340"/>
+      <c r="I14" s="340"/>
+      <c r="J14" s="340"/>
+      <c r="K14" s="340"/>
+      <c r="L14" s="341"/>
     </row>
     <row r="15" spans="1:18" s="58" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="248" t="s">
         <v>342</v>
       </c>
-      <c r="B15" s="297" t="s">
+      <c r="B15" s="329" t="s">
         <v>345</v>
       </c>
-      <c r="C15" s="297"/>
-      <c r="D15" s="297"/>
-      <c r="E15" s="297"/>
-      <c r="F15" s="297"/>
-      <c r="G15" s="297"/>
-      <c r="H15" s="297"/>
-      <c r="I15" s="297"/>
-      <c r="J15" s="297"/>
-      <c r="K15" s="297"/>
-      <c r="L15" s="298"/>
+      <c r="C15" s="329"/>
+      <c r="D15" s="329"/>
+      <c r="E15" s="329"/>
+      <c r="F15" s="329"/>
+      <c r="G15" s="329"/>
+      <c r="H15" s="329"/>
+      <c r="I15" s="329"/>
+      <c r="J15" s="329"/>
+      <c r="K15" s="329"/>
+      <c r="L15" s="330"/>
     </row>
     <row r="16" spans="1:18" s="59" customFormat="1" ht="94.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="240"/>
@@ -15959,12 +15962,12 @@
       <c r="L16" s="247"/>
     </row>
     <row r="17" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="295" t="s">
+      <c r="A17" s="338" t="s">
         <v>349</v>
       </c>
-      <c r="B17" s="296"/>
-      <c r="C17" s="296"/>
-      <c r="D17" s="296"/>
+      <c r="B17" s="339"/>
+      <c r="C17" s="339"/>
+      <c r="D17" s="339"/>
       <c r="E17" s="245" t="s">
         <v>350</v>
       </c>
@@ -15991,84 +15994,84 @@
       <c r="L18" s="113"/>
     </row>
     <row r="19" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="327" t="s">
+      <c r="A19" s="309" t="s">
         <v>166</v>
       </c>
-      <c r="B19" s="328"/>
-      <c r="C19" s="328"/>
-      <c r="D19" s="328"/>
-      <c r="E19" s="328"/>
-      <c r="F19" s="328"/>
-      <c r="G19" s="328"/>
-      <c r="H19" s="328"/>
-      <c r="I19" s="328"/>
-      <c r="J19" s="328"/>
-      <c r="K19" s="328"/>
-      <c r="L19" s="329"/>
+      <c r="B19" s="310"/>
+      <c r="C19" s="310"/>
+      <c r="D19" s="310"/>
+      <c r="E19" s="310"/>
+      <c r="F19" s="310"/>
+      <c r="G19" s="310"/>
+      <c r="H19" s="310"/>
+      <c r="I19" s="310"/>
+      <c r="J19" s="310"/>
+      <c r="K19" s="310"/>
+      <c r="L19" s="311"/>
     </row>
     <row r="20" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="330" t="s">
+      <c r="A20" s="312" t="s">
         <v>285</v>
       </c>
-      <c r="B20" s="331"/>
-      <c r="C20" s="331"/>
-      <c r="D20" s="331"/>
-      <c r="E20" s="331"/>
-      <c r="F20" s="331"/>
-      <c r="G20" s="331"/>
-      <c r="H20" s="331"/>
-      <c r="I20" s="331"/>
-      <c r="J20" s="331"/>
-      <c r="K20" s="331"/>
-      <c r="L20" s="332"/>
+      <c r="B20" s="313"/>
+      <c r="C20" s="313"/>
+      <c r="D20" s="313"/>
+      <c r="E20" s="313"/>
+      <c r="F20" s="313"/>
+      <c r="G20" s="313"/>
+      <c r="H20" s="313"/>
+      <c r="I20" s="313"/>
+      <c r="J20" s="313"/>
+      <c r="K20" s="313"/>
+      <c r="L20" s="314"/>
     </row>
     <row r="21" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="333" t="s">
+      <c r="A21" s="315" t="s">
         <v>286</v>
       </c>
-      <c r="B21" s="311"/>
-      <c r="C21" s="311"/>
-      <c r="D21" s="311"/>
-      <c r="E21" s="311"/>
-      <c r="F21" s="311"/>
-      <c r="G21" s="311"/>
-      <c r="H21" s="311"/>
-      <c r="I21" s="311"/>
-      <c r="J21" s="311"/>
-      <c r="K21" s="311"/>
-      <c r="L21" s="312"/>
+      <c r="B21" s="316"/>
+      <c r="C21" s="316"/>
+      <c r="D21" s="316"/>
+      <c r="E21" s="316"/>
+      <c r="F21" s="316"/>
+      <c r="G21" s="316"/>
+      <c r="H21" s="316"/>
+      <c r="I21" s="316"/>
+      <c r="J21" s="316"/>
+      <c r="K21" s="316"/>
+      <c r="L21" s="317"/>
     </row>
     <row r="22" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="333" t="s">
+      <c r="A22" s="315" t="s">
         <v>167</v>
       </c>
-      <c r="B22" s="311"/>
-      <c r="C22" s="311"/>
-      <c r="D22" s="311"/>
-      <c r="E22" s="311"/>
-      <c r="F22" s="311"/>
-      <c r="G22" s="311"/>
-      <c r="H22" s="311"/>
-      <c r="I22" s="311"/>
-      <c r="J22" s="311"/>
-      <c r="K22" s="311"/>
-      <c r="L22" s="312"/>
+      <c r="B22" s="316"/>
+      <c r="C22" s="316"/>
+      <c r="D22" s="316"/>
+      <c r="E22" s="316"/>
+      <c r="F22" s="316"/>
+      <c r="G22" s="316"/>
+      <c r="H22" s="316"/>
+      <c r="I22" s="316"/>
+      <c r="J22" s="316"/>
+      <c r="K22" s="316"/>
+      <c r="L22" s="317"/>
     </row>
     <row r="23" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="334" t="s">
+      <c r="A23" s="318" t="s">
         <v>287</v>
       </c>
-      <c r="B23" s="335"/>
-      <c r="C23" s="335"/>
-      <c r="D23" s="335"/>
-      <c r="E23" s="335"/>
-      <c r="F23" s="335"/>
-      <c r="G23" s="335"/>
-      <c r="H23" s="335"/>
-      <c r="I23" s="335"/>
-      <c r="J23" s="335"/>
-      <c r="K23" s="335"/>
-      <c r="L23" s="336"/>
+      <c r="B23" s="319"/>
+      <c r="C23" s="319"/>
+      <c r="D23" s="319"/>
+      <c r="E23" s="319"/>
+      <c r="F23" s="319"/>
+      <c r="G23" s="319"/>
+      <c r="H23" s="319"/>
+      <c r="I23" s="319"/>
+      <c r="J23" s="319"/>
+      <c r="K23" s="319"/>
+      <c r="L23" s="320"/>
     </row>
     <row r="24" spans="1:14" s="59" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="113"/>
@@ -16085,332 +16088,332 @@
       <c r="L24" s="113"/>
     </row>
     <row r="25" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="337" t="s">
+      <c r="A25" s="321" t="s">
         <v>283</v>
       </c>
-      <c r="B25" s="338"/>
-      <c r="C25" s="338"/>
-      <c r="D25" s="338"/>
-      <c r="E25" s="338"/>
-      <c r="F25" s="338"/>
-      <c r="G25" s="338"/>
-      <c r="H25" s="338"/>
-      <c r="I25" s="338"/>
-      <c r="J25" s="338"/>
-      <c r="K25" s="338"/>
-      <c r="L25" s="339"/>
+      <c r="B25" s="322"/>
+      <c r="C25" s="322"/>
+      <c r="D25" s="322"/>
+      <c r="E25" s="322"/>
+      <c r="F25" s="322"/>
+      <c r="G25" s="322"/>
+      <c r="H25" s="322"/>
+      <c r="I25" s="322"/>
+      <c r="J25" s="322"/>
+      <c r="K25" s="322"/>
+      <c r="L25" s="323"/>
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="316" t="s">
+      <c r="A26" s="298" t="s">
         <v>176</v>
       </c>
-      <c r="B26" s="317"/>
-      <c r="C26" s="317"/>
-      <c r="D26" s="317"/>
-      <c r="E26" s="317"/>
-      <c r="F26" s="317"/>
-      <c r="G26" s="317"/>
-      <c r="H26" s="317"/>
-      <c r="I26" s="317"/>
-      <c r="J26" s="317"/>
-      <c r="K26" s="317"/>
-      <c r="L26" s="318"/>
+      <c r="B26" s="299"/>
+      <c r="C26" s="299"/>
+      <c r="D26" s="299"/>
+      <c r="E26" s="299"/>
+      <c r="F26" s="299"/>
+      <c r="G26" s="299"/>
+      <c r="H26" s="299"/>
+      <c r="I26" s="299"/>
+      <c r="J26" s="299"/>
+      <c r="K26" s="299"/>
+      <c r="L26" s="300"/>
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="222">
         <v>1</v>
       </c>
-      <c r="B27" s="304" t="s">
+      <c r="B27" s="333" t="s">
         <v>175</v>
       </c>
-      <c r="C27" s="304"/>
-      <c r="D27" s="304"/>
-      <c r="E27" s="304"/>
-      <c r="F27" s="304"/>
-      <c r="G27" s="304"/>
-      <c r="H27" s="304"/>
-      <c r="I27" s="304"/>
-      <c r="J27" s="304"/>
-      <c r="K27" s="304"/>
-      <c r="L27" s="305"/>
+      <c r="C27" s="333"/>
+      <c r="D27" s="333"/>
+      <c r="E27" s="333"/>
+      <c r="F27" s="333"/>
+      <c r="G27" s="333"/>
+      <c r="H27" s="333"/>
+      <c r="I27" s="333"/>
+      <c r="J27" s="333"/>
+      <c r="K27" s="333"/>
+      <c r="L27" s="334"/>
     </row>
     <row r="28" spans="1:14" s="59" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="222">
         <v>2</v>
       </c>
-      <c r="B28" s="304" t="s">
+      <c r="B28" s="333" t="s">
         <v>279</v>
       </c>
-      <c r="C28" s="304"/>
-      <c r="D28" s="304"/>
-      <c r="E28" s="304"/>
-      <c r="F28" s="304"/>
-      <c r="G28" s="304"/>
-      <c r="H28" s="304"/>
-      <c r="I28" s="304"/>
-      <c r="J28" s="304"/>
-      <c r="K28" s="304"/>
-      <c r="L28" s="305"/>
+      <c r="C28" s="333"/>
+      <c r="D28" s="333"/>
+      <c r="E28" s="333"/>
+      <c r="F28" s="333"/>
+      <c r="G28" s="333"/>
+      <c r="H28" s="333"/>
+      <c r="I28" s="333"/>
+      <c r="J28" s="333"/>
+      <c r="K28" s="333"/>
+      <c r="L28" s="334"/>
       <c r="N28" s="106"/>
     </row>
     <row r="29" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="222">
         <v>3</v>
       </c>
-      <c r="B29" s="304" t="s">
+      <c r="B29" s="333" t="s">
         <v>168</v>
       </c>
-      <c r="C29" s="304"/>
-      <c r="D29" s="304"/>
-      <c r="E29" s="304"/>
-      <c r="F29" s="304"/>
-      <c r="G29" s="304"/>
-      <c r="H29" s="304"/>
-      <c r="I29" s="304"/>
-      <c r="J29" s="304"/>
-      <c r="K29" s="304"/>
-      <c r="L29" s="305"/>
+      <c r="C29" s="333"/>
+      <c r="D29" s="333"/>
+      <c r="E29" s="333"/>
+      <c r="F29" s="333"/>
+      <c r="G29" s="333"/>
+      <c r="H29" s="333"/>
+      <c r="I29" s="333"/>
+      <c r="J29" s="333"/>
+      <c r="K29" s="333"/>
+      <c r="L29" s="334"/>
       <c r="N29" s="106"/>
     </row>
     <row r="30" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="222">
         <v>4</v>
       </c>
-      <c r="B30" s="304" t="s">
+      <c r="B30" s="333" t="s">
         <v>288</v>
       </c>
-      <c r="C30" s="304"/>
-      <c r="D30" s="304"/>
-      <c r="E30" s="304"/>
-      <c r="F30" s="304"/>
-      <c r="G30" s="304"/>
-      <c r="H30" s="304"/>
-      <c r="I30" s="304"/>
-      <c r="J30" s="304"/>
-      <c r="K30" s="304"/>
-      <c r="L30" s="305"/>
+      <c r="C30" s="333"/>
+      <c r="D30" s="333"/>
+      <c r="E30" s="333"/>
+      <c r="F30" s="333"/>
+      <c r="G30" s="333"/>
+      <c r="H30" s="333"/>
+      <c r="I30" s="333"/>
+      <c r="J30" s="333"/>
+      <c r="K30" s="333"/>
+      <c r="L30" s="334"/>
       <c r="N30" s="106"/>
     </row>
     <row r="31" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="222">
         <v>5</v>
       </c>
-      <c r="B31" s="304" t="s">
+      <c r="B31" s="333" t="s">
         <v>169</v>
       </c>
-      <c r="C31" s="304"/>
-      <c r="D31" s="304"/>
-      <c r="E31" s="304"/>
-      <c r="F31" s="304"/>
-      <c r="G31" s="304"/>
-      <c r="H31" s="304"/>
-      <c r="I31" s="304"/>
-      <c r="J31" s="304"/>
-      <c r="K31" s="304"/>
-      <c r="L31" s="305"/>
+      <c r="C31" s="333"/>
+      <c r="D31" s="333"/>
+      <c r="E31" s="333"/>
+      <c r="F31" s="333"/>
+      <c r="G31" s="333"/>
+      <c r="H31" s="333"/>
+      <c r="I31" s="333"/>
+      <c r="J31" s="333"/>
+      <c r="K31" s="333"/>
+      <c r="L31" s="334"/>
       <c r="N31" s="106"/>
     </row>
     <row r="32" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="222"/>
-      <c r="B32" s="304" t="s">
+      <c r="B32" s="333" t="s">
         <v>170</v>
       </c>
-      <c r="C32" s="304"/>
-      <c r="D32" s="304"/>
-      <c r="E32" s="304"/>
-      <c r="F32" s="304"/>
-      <c r="G32" s="304"/>
-      <c r="H32" s="304"/>
-      <c r="I32" s="304"/>
-      <c r="J32" s="304"/>
-      <c r="K32" s="304"/>
-      <c r="L32" s="305"/>
+      <c r="C32" s="333"/>
+      <c r="D32" s="333"/>
+      <c r="E32" s="333"/>
+      <c r="F32" s="333"/>
+      <c r="G32" s="333"/>
+      <c r="H32" s="333"/>
+      <c r="I32" s="333"/>
+      <c r="J32" s="333"/>
+      <c r="K32" s="333"/>
+      <c r="L32" s="334"/>
       <c r="N32" s="106"/>
     </row>
     <row r="33" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="222"/>
-      <c r="B33" s="304" t="s">
+      <c r="B33" s="333" t="s">
         <v>171</v>
       </c>
-      <c r="C33" s="304"/>
-      <c r="D33" s="304"/>
-      <c r="E33" s="304"/>
-      <c r="F33" s="304"/>
-      <c r="G33" s="304"/>
-      <c r="H33" s="304"/>
-      <c r="I33" s="304"/>
-      <c r="J33" s="304"/>
-      <c r="K33" s="304"/>
-      <c r="L33" s="305"/>
+      <c r="C33" s="333"/>
+      <c r="D33" s="333"/>
+      <c r="E33" s="333"/>
+      <c r="F33" s="333"/>
+      <c r="G33" s="333"/>
+      <c r="H33" s="333"/>
+      <c r="I33" s="333"/>
+      <c r="J33" s="333"/>
+      <c r="K33" s="333"/>
+      <c r="L33" s="334"/>
       <c r="N33" s="106"/>
     </row>
     <row r="34" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="313" t="s">
+      <c r="A34" s="335" t="s">
         <v>177</v>
       </c>
-      <c r="B34" s="314"/>
-      <c r="C34" s="314"/>
-      <c r="D34" s="314"/>
-      <c r="E34" s="314"/>
-      <c r="F34" s="314"/>
-      <c r="G34" s="314"/>
-      <c r="H34" s="314"/>
-      <c r="I34" s="314"/>
-      <c r="J34" s="314"/>
-      <c r="K34" s="314"/>
-      <c r="L34" s="315"/>
+      <c r="B34" s="336"/>
+      <c r="C34" s="336"/>
+      <c r="D34" s="336"/>
+      <c r="E34" s="336"/>
+      <c r="F34" s="336"/>
+      <c r="G34" s="336"/>
+      <c r="H34" s="336"/>
+      <c r="I34" s="336"/>
+      <c r="J34" s="336"/>
+      <c r="K34" s="336"/>
+      <c r="L34" s="337"/>
       <c r="N34" s="106"/>
     </row>
     <row r="35" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="222">
         <v>1</v>
       </c>
-      <c r="B35" s="304" t="s">
+      <c r="B35" s="333" t="s">
         <v>172</v>
       </c>
-      <c r="C35" s="304"/>
-      <c r="D35" s="304"/>
-      <c r="E35" s="304"/>
-      <c r="F35" s="304"/>
-      <c r="G35" s="304"/>
-      <c r="H35" s="304"/>
-      <c r="I35" s="304"/>
-      <c r="J35" s="304"/>
-      <c r="K35" s="304"/>
-      <c r="L35" s="305"/>
+      <c r="C35" s="333"/>
+      <c r="D35" s="333"/>
+      <c r="E35" s="333"/>
+      <c r="F35" s="333"/>
+      <c r="G35" s="333"/>
+      <c r="H35" s="333"/>
+      <c r="I35" s="333"/>
+      <c r="J35" s="333"/>
+      <c r="K35" s="333"/>
+      <c r="L35" s="334"/>
       <c r="N35" s="106"/>
     </row>
     <row r="36" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="222"/>
-      <c r="B36" s="302" t="s">
+      <c r="B36" s="331" t="s">
         <v>289</v>
       </c>
-      <c r="C36" s="302"/>
-      <c r="D36" s="302"/>
-      <c r="E36" s="302"/>
-      <c r="F36" s="302"/>
-      <c r="G36" s="302"/>
-      <c r="H36" s="302"/>
-      <c r="I36" s="302"/>
-      <c r="J36" s="302"/>
-      <c r="K36" s="302"/>
-      <c r="L36" s="303"/>
+      <c r="C36" s="331"/>
+      <c r="D36" s="331"/>
+      <c r="E36" s="331"/>
+      <c r="F36" s="331"/>
+      <c r="G36" s="331"/>
+      <c r="H36" s="331"/>
+      <c r="I36" s="331"/>
+      <c r="J36" s="331"/>
+      <c r="K36" s="331"/>
+      <c r="L36" s="332"/>
       <c r="N36" s="106"/>
     </row>
     <row r="37" spans="1:14" s="59" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="222">
         <v>2</v>
       </c>
-      <c r="B37" s="304" t="s">
+      <c r="B37" s="333" t="s">
         <v>282</v>
       </c>
-      <c r="C37" s="304"/>
-      <c r="D37" s="304"/>
-      <c r="E37" s="304"/>
-      <c r="F37" s="304"/>
-      <c r="G37" s="304"/>
-      <c r="H37" s="304"/>
-      <c r="I37" s="304"/>
-      <c r="J37" s="304"/>
-      <c r="K37" s="304"/>
-      <c r="L37" s="305"/>
+      <c r="C37" s="333"/>
+      <c r="D37" s="333"/>
+      <c r="E37" s="333"/>
+      <c r="F37" s="333"/>
+      <c r="G37" s="333"/>
+      <c r="H37" s="333"/>
+      <c r="I37" s="333"/>
+      <c r="J37" s="333"/>
+      <c r="K37" s="333"/>
+      <c r="L37" s="334"/>
       <c r="N37" s="106"/>
     </row>
     <row r="38" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="222">
         <v>3</v>
       </c>
-      <c r="B38" s="304" t="s">
+      <c r="B38" s="333" t="s">
         <v>271</v>
       </c>
-      <c r="C38" s="304"/>
-      <c r="D38" s="304"/>
-      <c r="E38" s="304"/>
-      <c r="F38" s="304"/>
-      <c r="G38" s="304"/>
-      <c r="H38" s="304"/>
-      <c r="I38" s="304"/>
-      <c r="J38" s="304"/>
-      <c r="K38" s="304"/>
-      <c r="L38" s="305"/>
+      <c r="C38" s="333"/>
+      <c r="D38" s="333"/>
+      <c r="E38" s="333"/>
+      <c r="F38" s="333"/>
+      <c r="G38" s="333"/>
+      <c r="H38" s="333"/>
+      <c r="I38" s="333"/>
+      <c r="J38" s="333"/>
+      <c r="K38" s="333"/>
+      <c r="L38" s="334"/>
       <c r="N38" s="106"/>
     </row>
     <row r="39" spans="1:14" s="59" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="222">
         <v>4</v>
       </c>
-      <c r="B39" s="304" t="s">
+      <c r="B39" s="333" t="s">
         <v>290</v>
       </c>
-      <c r="C39" s="304"/>
-      <c r="D39" s="304"/>
-      <c r="E39" s="304"/>
-      <c r="F39" s="304"/>
-      <c r="G39" s="304"/>
-      <c r="H39" s="304"/>
-      <c r="I39" s="304"/>
-      <c r="J39" s="304"/>
-      <c r="K39" s="304"/>
-      <c r="L39" s="305"/>
+      <c r="C39" s="333"/>
+      <c r="D39" s="333"/>
+      <c r="E39" s="333"/>
+      <c r="F39" s="333"/>
+      <c r="G39" s="333"/>
+      <c r="H39" s="333"/>
+      <c r="I39" s="333"/>
+      <c r="J39" s="333"/>
+      <c r="K39" s="333"/>
+      <c r="L39" s="334"/>
       <c r="N39" s="106"/>
     </row>
     <row r="40" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="222">
         <v>5</v>
       </c>
-      <c r="B40" s="302" t="s">
+      <c r="B40" s="331" t="s">
         <v>272</v>
       </c>
-      <c r="C40" s="302"/>
-      <c r="D40" s="302"/>
-      <c r="E40" s="302"/>
-      <c r="F40" s="302"/>
-      <c r="G40" s="302"/>
-      <c r="H40" s="302"/>
-      <c r="I40" s="302"/>
-      <c r="J40" s="302"/>
-      <c r="K40" s="302"/>
-      <c r="L40" s="303"/>
+      <c r="C40" s="331"/>
+      <c r="D40" s="331"/>
+      <c r="E40" s="331"/>
+      <c r="F40" s="331"/>
+      <c r="G40" s="331"/>
+      <c r="H40" s="331"/>
+      <c r="I40" s="331"/>
+      <c r="J40" s="331"/>
+      <c r="K40" s="331"/>
+      <c r="L40" s="332"/>
       <c r="N40" s="106"/>
     </row>
     <row r="41" spans="1:14" s="59" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="222">
         <v>6</v>
       </c>
-      <c r="B41" s="302" t="s">
+      <c r="B41" s="331" t="s">
         <v>277</v>
       </c>
-      <c r="C41" s="302"/>
-      <c r="D41" s="302"/>
-      <c r="E41" s="302"/>
-      <c r="F41" s="302"/>
-      <c r="G41" s="302"/>
-      <c r="H41" s="302"/>
-      <c r="I41" s="302"/>
-      <c r="J41" s="302"/>
-      <c r="K41" s="302"/>
-      <c r="L41" s="303"/>
+      <c r="C41" s="331"/>
+      <c r="D41" s="331"/>
+      <c r="E41" s="331"/>
+      <c r="F41" s="331"/>
+      <c r="G41" s="331"/>
+      <c r="H41" s="331"/>
+      <c r="I41" s="331"/>
+      <c r="J41" s="331"/>
+      <c r="K41" s="331"/>
+      <c r="L41" s="332"/>
       <c r="N41" s="106"/>
     </row>
     <row r="42" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="222">
         <v>7</v>
       </c>
-      <c r="B42" s="304" t="s">
+      <c r="B42" s="333" t="s">
         <v>273</v>
       </c>
-      <c r="C42" s="304"/>
-      <c r="D42" s="304"/>
-      <c r="E42" s="304"/>
-      <c r="F42" s="304"/>
-      <c r="G42" s="304"/>
-      <c r="H42" s="304"/>
-      <c r="I42" s="304"/>
-      <c r="J42" s="304"/>
-      <c r="K42" s="304"/>
-      <c r="L42" s="305"/>
+      <c r="C42" s="333"/>
+      <c r="D42" s="333"/>
+      <c r="E42" s="333"/>
+      <c r="F42" s="333"/>
+      <c r="G42" s="333"/>
+      <c r="H42" s="333"/>
+      <c r="I42" s="333"/>
+      <c r="J42" s="333"/>
+      <c r="K42" s="333"/>
+      <c r="L42" s="334"/>
     </row>
     <row r="43" spans="1:14" s="59" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="222"/>
@@ -16427,56 +16430,56 @@
       <c r="L43" s="224"/>
     </row>
     <row r="44" spans="1:14" s="59" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="313" t="s">
+      <c r="A44" s="335" t="s">
         <v>276</v>
       </c>
-      <c r="B44" s="314"/>
-      <c r="C44" s="314"/>
-      <c r="D44" s="314"/>
-      <c r="E44" s="314"/>
-      <c r="F44" s="314"/>
-      <c r="G44" s="314"/>
-      <c r="H44" s="314"/>
-      <c r="I44" s="314"/>
-      <c r="J44" s="314"/>
-      <c r="K44" s="314"/>
-      <c r="L44" s="315"/>
+      <c r="B44" s="336"/>
+      <c r="C44" s="336"/>
+      <c r="D44" s="336"/>
+      <c r="E44" s="336"/>
+      <c r="F44" s="336"/>
+      <c r="G44" s="336"/>
+      <c r="H44" s="336"/>
+      <c r="I44" s="336"/>
+      <c r="J44" s="336"/>
+      <c r="K44" s="336"/>
+      <c r="L44" s="337"/>
     </row>
     <row r="45" spans="1:14" s="59" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="225" t="s">
         <v>274</v>
       </c>
-      <c r="B45" s="304" t="s">
+      <c r="B45" s="333" t="s">
         <v>173</v>
       </c>
-      <c r="C45" s="304"/>
-      <c r="D45" s="304"/>
-      <c r="E45" s="304"/>
-      <c r="F45" s="304"/>
-      <c r="G45" s="304"/>
-      <c r="H45" s="304"/>
-      <c r="I45" s="304"/>
-      <c r="J45" s="304"/>
-      <c r="K45" s="304"/>
-      <c r="L45" s="305"/>
+      <c r="C45" s="333"/>
+      <c r="D45" s="333"/>
+      <c r="E45" s="333"/>
+      <c r="F45" s="333"/>
+      <c r="G45" s="333"/>
+      <c r="H45" s="333"/>
+      <c r="I45" s="333"/>
+      <c r="J45" s="333"/>
+      <c r="K45" s="333"/>
+      <c r="L45" s="334"/>
     </row>
     <row r="46" spans="1:14" s="59" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="226" t="s">
         <v>275</v>
       </c>
-      <c r="B46" s="306" t="s">
+      <c r="B46" s="343" t="s">
         <v>278</v>
       </c>
-      <c r="C46" s="306"/>
-      <c r="D46" s="306"/>
-      <c r="E46" s="306"/>
-      <c r="F46" s="306"/>
-      <c r="G46" s="306"/>
-      <c r="H46" s="306"/>
-      <c r="I46" s="306"/>
-      <c r="J46" s="306"/>
-      <c r="K46" s="306"/>
-      <c r="L46" s="307"/>
+      <c r="C46" s="343"/>
+      <c r="D46" s="343"/>
+      <c r="E46" s="343"/>
+      <c r="F46" s="343"/>
+      <c r="G46" s="343"/>
+      <c r="H46" s="343"/>
+      <c r="I46" s="343"/>
+      <c r="J46" s="343"/>
+      <c r="K46" s="343"/>
+      <c r="L46" s="344"/>
     </row>
     <row r="47" spans="1:14" s="59" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="160"/>
@@ -16493,20 +16496,20 @@
       <c r="L47" s="113"/>
     </row>
     <row r="48" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="308" t="s">
+      <c r="A48" s="345" t="s">
         <v>201</v>
       </c>
-      <c r="B48" s="309"/>
-      <c r="C48" s="309"/>
-      <c r="D48" s="309"/>
-      <c r="E48" s="309"/>
-      <c r="F48" s="309"/>
-      <c r="G48" s="309"/>
-      <c r="H48" s="309"/>
-      <c r="I48" s="309"/>
-      <c r="J48" s="309"/>
-      <c r="K48" s="309"/>
-      <c r="L48" s="310"/>
+      <c r="B48" s="346"/>
+      <c r="C48" s="346"/>
+      <c r="D48" s="346"/>
+      <c r="E48" s="346"/>
+      <c r="F48" s="346"/>
+      <c r="G48" s="346"/>
+      <c r="H48" s="346"/>
+      <c r="I48" s="346"/>
+      <c r="J48" s="346"/>
+      <c r="K48" s="346"/>
+      <c r="L48" s="347"/>
     </row>
     <row r="49" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="229" t="s">
@@ -16594,90 +16597,90 @@
       <c r="B54" s="168" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="311" t="s">
+      <c r="C54" s="316" t="s">
         <v>263</v>
       </c>
-      <c r="D54" s="311"/>
-      <c r="E54" s="311"/>
-      <c r="F54" s="311"/>
-      <c r="G54" s="311"/>
-      <c r="H54" s="311"/>
-      <c r="I54" s="311"/>
-      <c r="J54" s="311"/>
-      <c r="K54" s="311"/>
-      <c r="L54" s="312"/>
+      <c r="D54" s="316"/>
+      <c r="E54" s="316"/>
+      <c r="F54" s="316"/>
+      <c r="G54" s="316"/>
+      <c r="H54" s="316"/>
+      <c r="I54" s="316"/>
+      <c r="J54" s="316"/>
+      <c r="K54" s="316"/>
+      <c r="L54" s="317"/>
     </row>
     <row r="55" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="167"/>
       <c r="B55" s="168" t="s">
         <v>264</v>
       </c>
-      <c r="C55" s="311" t="s">
+      <c r="C55" s="316" t="s">
         <v>265</v>
       </c>
-      <c r="D55" s="311"/>
-      <c r="E55" s="311"/>
-      <c r="F55" s="311"/>
-      <c r="G55" s="311"/>
-      <c r="H55" s="311"/>
-      <c r="I55" s="311"/>
-      <c r="J55" s="311"/>
-      <c r="K55" s="311"/>
-      <c r="L55" s="312"/>
+      <c r="D55" s="316"/>
+      <c r="E55" s="316"/>
+      <c r="F55" s="316"/>
+      <c r="G55" s="316"/>
+      <c r="H55" s="316"/>
+      <c r="I55" s="316"/>
+      <c r="J55" s="316"/>
+      <c r="K55" s="316"/>
+      <c r="L55" s="317"/>
     </row>
     <row r="56" spans="1:12" s="58" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="167"/>
       <c r="B56" s="168" t="s">
         <v>332</v>
       </c>
-      <c r="C56" s="311" t="s">
+      <c r="C56" s="316" t="s">
         <v>333</v>
       </c>
-      <c r="D56" s="311"/>
-      <c r="E56" s="311"/>
-      <c r="F56" s="311"/>
-      <c r="G56" s="311"/>
-      <c r="H56" s="311"/>
-      <c r="I56" s="311"/>
-      <c r="J56" s="311"/>
-      <c r="K56" s="311"/>
-      <c r="L56" s="312"/>
+      <c r="D56" s="316"/>
+      <c r="E56" s="316"/>
+      <c r="F56" s="316"/>
+      <c r="G56" s="316"/>
+      <c r="H56" s="316"/>
+      <c r="I56" s="316"/>
+      <c r="J56" s="316"/>
+      <c r="K56" s="316"/>
+      <c r="L56" s="317"/>
     </row>
     <row r="57" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="167"/>
       <c r="B57" s="168" t="s">
         <v>99</v>
       </c>
-      <c r="C57" s="311" t="s">
+      <c r="C57" s="316" t="s">
         <v>100</v>
       </c>
-      <c r="D57" s="311"/>
-      <c r="E57" s="311"/>
-      <c r="F57" s="311"/>
-      <c r="G57" s="311"/>
-      <c r="H57" s="311"/>
-      <c r="I57" s="311"/>
-      <c r="J57" s="311"/>
-      <c r="K57" s="311"/>
-      <c r="L57" s="312"/>
+      <c r="D57" s="316"/>
+      <c r="E57" s="316"/>
+      <c r="F57" s="316"/>
+      <c r="G57" s="316"/>
+      <c r="H57" s="316"/>
+      <c r="I57" s="316"/>
+      <c r="J57" s="316"/>
+      <c r="K57" s="316"/>
+      <c r="L57" s="317"/>
     </row>
     <row r="58" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="167"/>
       <c r="B58" s="168" t="s">
         <v>199</v>
       </c>
-      <c r="C58" s="311" t="s">
+      <c r="C58" s="316" t="s">
         <v>200</v>
       </c>
-      <c r="D58" s="311"/>
-      <c r="E58" s="311"/>
-      <c r="F58" s="311"/>
-      <c r="G58" s="311"/>
-      <c r="H58" s="311"/>
-      <c r="I58" s="311"/>
-      <c r="J58" s="311"/>
-      <c r="K58" s="311"/>
-      <c r="L58" s="312"/>
+      <c r="D58" s="316"/>
+      <c r="E58" s="316"/>
+      <c r="F58" s="316"/>
+      <c r="G58" s="316"/>
+      <c r="H58" s="316"/>
+      <c r="I58" s="316"/>
+      <c r="J58" s="316"/>
+      <c r="K58" s="316"/>
+      <c r="L58" s="317"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="167"/>
@@ -16702,18 +16705,18 @@
       <c r="B60" s="168" t="s">
         <v>399</v>
       </c>
-      <c r="C60" s="311" t="s">
+      <c r="C60" s="316" t="s">
         <v>400</v>
       </c>
-      <c r="D60" s="311"/>
-      <c r="E60" s="311"/>
-      <c r="F60" s="311"/>
-      <c r="G60" s="311"/>
-      <c r="H60" s="311"/>
-      <c r="I60" s="311"/>
-      <c r="J60" s="311"/>
-      <c r="K60" s="311"/>
-      <c r="L60" s="312"/>
+      <c r="D60" s="316"/>
+      <c r="E60" s="316"/>
+      <c r="F60" s="316"/>
+      <c r="G60" s="316"/>
+      <c r="H60" s="316"/>
+      <c r="I60" s="316"/>
+      <c r="J60" s="316"/>
+      <c r="K60" s="316"/>
+      <c r="L60" s="317"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="167"/>
@@ -16834,25 +16837,56 @@
       </c>
     </row>
     <row r="82" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="301" t="s">
+      <c r="A82" s="342" t="s">
         <v>403</v>
       </c>
-      <c r="B82" s="301"/>
-      <c r="C82" s="301"/>
-      <c r="D82" s="301"/>
-      <c r="E82" s="301"/>
-      <c r="F82" s="301"/>
-      <c r="G82" s="301"/>
-      <c r="H82" s="301"/>
-      <c r="I82" s="301"/>
-      <c r="J82" s="301"/>
-      <c r="K82" s="301"/>
-      <c r="L82" s="301"/>
+      <c r="B82" s="342"/>
+      <c r="C82" s="342"/>
+      <c r="D82" s="342"/>
+      <c r="E82" s="342"/>
+      <c r="F82" s="342"/>
+      <c r="G82" s="342"/>
+      <c r="H82" s="342"/>
+      <c r="I82" s="342"/>
+      <c r="J82" s="342"/>
+      <c r="K82" s="342"/>
+      <c r="L82" s="342"/>
     </row>
     <row r="87" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="88" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="A82:L82"/>
+    <mergeCell ref="B41:L41"/>
+    <mergeCell ref="B42:L42"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="A48:L48"/>
+    <mergeCell ref="C54:L54"/>
+    <mergeCell ref="C57:L57"/>
+    <mergeCell ref="C58:L58"/>
+    <mergeCell ref="C55:L55"/>
+    <mergeCell ref="C60:L60"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="B40:L40"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B30:L30"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B39:L39"/>
     <mergeCell ref="A26:L26"/>
     <mergeCell ref="A1:L1"/>
     <mergeCell ref="A4:L4"/>
@@ -16869,37 +16903,6 @@
     <mergeCell ref="B8:L8"/>
     <mergeCell ref="A10:L10"/>
     <mergeCell ref="B11:L11"/>
-    <mergeCell ref="C56:L56"/>
-    <mergeCell ref="B40:L40"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="B14:L14"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="A82:L82"/>
-    <mergeCell ref="B41:L41"/>
-    <mergeCell ref="B42:L42"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="A48:L48"/>
-    <mergeCell ref="C54:L54"/>
-    <mergeCell ref="C57:L57"/>
-    <mergeCell ref="C58:L58"/>
-    <mergeCell ref="C55:L55"/>
-    <mergeCell ref="C60:L60"/>
-    <mergeCell ref="A44:L44"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A67" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -16937,82 +16940,82 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="394" t="s">
+      <c r="A3" s="397" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="394"/>
-      <c r="C3" s="394"/>
+      <c r="B3" s="397"/>
+      <c r="C3" s="397"/>
       <c r="D3" s="128" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="395" t="s">
+      <c r="A4" s="398" t="s">
         <v>113</v>
       </c>
-      <c r="B4" s="395"/>
-      <c r="C4" s="395"/>
+      <c r="B4" s="398"/>
+      <c r="C4" s="398"/>
       <c r="D4" s="175" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="399" t="s">
+      <c r="A5" s="402" t="s">
         <v>184</v>
       </c>
-      <c r="B5" s="396"/>
-      <c r="C5" s="396"/>
+      <c r="B5" s="399"/>
+      <c r="C5" s="399"/>
       <c r="D5" s="176" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="397" t="s">
+      <c r="A6" s="400" t="s">
         <v>185</v>
       </c>
-      <c r="B6" s="397"/>
-      <c r="C6" s="397"/>
+      <c r="B6" s="400"/>
+      <c r="C6" s="400"/>
       <c r="D6" s="177" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="398" t="s">
+      <c r="A7" s="401" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="398"/>
-      <c r="C7" s="398"/>
+      <c r="B7" s="401"/>
+      <c r="C7" s="401"/>
       <c r="D7" s="178" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="395" t="s">
+      <c r="A11" s="398" t="s">
         <v>113</v>
       </c>
-      <c r="B11" s="395"/>
-      <c r="C11" s="395"/>
+      <c r="B11" s="398"/>
+      <c r="C11" s="398"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="396" t="s">
+      <c r="A12" s="399" t="s">
         <v>114</v>
       </c>
-      <c r="B12" s="396"/>
-      <c r="C12" s="396"/>
+      <c r="B12" s="399"/>
+      <c r="C12" s="399"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="397" t="s">
+      <c r="A13" s="400" t="s">
         <v>115</v>
       </c>
-      <c r="B13" s="397"/>
-      <c r="C13" s="397"/>
+      <c r="B13" s="400"/>
+      <c r="C13" s="400"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="398" t="s">
+      <c r="A14" s="401" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="398"/>
-      <c r="C14" s="398"/>
+      <c r="B14" s="401"/>
+      <c r="C14" s="401"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -17050,28 +17053,28 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="400" t="s">
+      <c r="A2" s="403" t="s">
         <v>434</v>
       </c>
-      <c r="B2" s="401"/>
-      <c r="C2" s="401"/>
-      <c r="D2" s="401"/>
-      <c r="E2" s="401"/>
-      <c r="F2" s="401"/>
-      <c r="G2" s="401"/>
-      <c r="H2" s="401"/>
-      <c r="I2" s="401"/>
-      <c r="J2" s="401"/>
-      <c r="K2" s="401"/>
-      <c r="L2" s="401"/>
-      <c r="M2" s="401"/>
-      <c r="N2" s="401"/>
-      <c r="O2" s="401"/>
-      <c r="P2" s="401"/>
-      <c r="Q2" s="401"/>
-      <c r="R2" s="401"/>
-      <c r="S2" s="401"/>
-      <c r="T2" s="401"/>
+      <c r="B2" s="404"/>
+      <c r="C2" s="404"/>
+      <c r="D2" s="404"/>
+      <c r="E2" s="404"/>
+      <c r="F2" s="404"/>
+      <c r="G2" s="404"/>
+      <c r="H2" s="404"/>
+      <c r="I2" s="404"/>
+      <c r="J2" s="404"/>
+      <c r="K2" s="404"/>
+      <c r="L2" s="404"/>
+      <c r="M2" s="404"/>
+      <c r="N2" s="404"/>
+      <c r="O2" s="404"/>
+      <c r="P2" s="404"/>
+      <c r="Q2" s="404"/>
+      <c r="R2" s="404"/>
+      <c r="S2" s="404"/>
+      <c r="T2" s="404"/>
     </row>
     <row r="3" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:20" ht="32" x14ac:dyDescent="0.2">
@@ -17784,8 +17787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BF02C3-B992-44C7-A79C-D1E41573911A}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18079,8 +18082,12 @@
       <c r="K11" s="40"/>
     </row>
     <row r="12" spans="1:11" ht="48" x14ac:dyDescent="0.2">
-      <c r="A12" s="57"/>
-      <c r="B12" s="149"/>
+      <c r="A12" s="57">
+        <v>45798</v>
+      </c>
+      <c r="B12" s="149" t="s">
+        <v>442</v>
+      </c>
       <c r="C12" s="56" t="s">
         <v>432</v>
       </c>
@@ -18375,8 +18382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BF7D8F-86F3-47E9-AB85-EE9B4CAB70E4}">
   <dimension ref="A1:P139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="141" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="141" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18405,16 +18412,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="345" t="str">
+      <c r="A1" s="348" t="str">
         <f>'ReadMe-Directions'!A1</f>
         <v>Immersive Model for Lake Mead based on the Principle of Divide Reservoir Inflow</v>
       </c>
-      <c r="B1" s="345"/>
-      <c r="C1" s="345"/>
-      <c r="D1" s="345"/>
-      <c r="E1" s="345"/>
-      <c r="F1" s="345"/>
-      <c r="G1" s="345"/>
+      <c r="B1" s="348"/>
+      <c r="C1" s="348"/>
+      <c r="D1" s="348"/>
+      <c r="E1" s="348"/>
+      <c r="F1" s="348"/>
+      <c r="G1" s="348"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -18423,15 +18430,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="353" t="s">
+      <c r="A3" s="356" t="s">
         <v>191</v>
       </c>
-      <c r="B3" s="353"/>
-      <c r="C3" s="353"/>
-      <c r="D3" s="353"/>
-      <c r="E3" s="353"/>
-      <c r="F3" s="353"/>
-      <c r="G3" s="353"/>
+      <c r="B3" s="356"/>
+      <c r="C3" s="356"/>
+      <c r="D3" s="356"/>
+      <c r="E3" s="356"/>
+      <c r="F3" s="356"/>
+      <c r="G3" s="356"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -18447,13 +18454,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="354" t="s">
+      <c r="C4" s="357" t="s">
         <v>260</v>
       </c>
-      <c r="D4" s="355"/>
-      <c r="E4" s="355"/>
-      <c r="F4" s="355"/>
-      <c r="G4" s="356"/>
+      <c r="D4" s="358"/>
+      <c r="E4" s="358"/>
+      <c r="F4" s="358"/>
+      <c r="G4" s="359"/>
       <c r="N4" s="141" t="s">
         <v>334</v>
       </c>
@@ -18463,11 +18470,11 @@
         <v>239</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="357"/>
-      <c r="D5" s="352"/>
-      <c r="E5" s="352"/>
-      <c r="F5" s="352"/>
-      <c r="G5" s="352"/>
+      <c r="C5" s="360"/>
+      <c r="D5" s="355"/>
+      <c r="E5" s="355"/>
+      <c r="F5" s="355"/>
+      <c r="G5" s="355"/>
       <c r="N5" s="141"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -18475,11 +18482,11 @@
         <v>203</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="357"/>
-      <c r="D6" s="352"/>
-      <c r="E6" s="352"/>
-      <c r="F6" s="352"/>
-      <c r="G6" s="352"/>
+      <c r="C6" s="360"/>
+      <c r="D6" s="355"/>
+      <c r="E6" s="355"/>
+      <c r="F6" s="355"/>
+      <c r="G6" s="355"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -18487,11 +18494,11 @@
         <v>204</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="357"/>
-      <c r="D7" s="352"/>
-      <c r="E7" s="352"/>
-      <c r="F7" s="352"/>
-      <c r="G7" s="352"/>
+      <c r="C7" s="360"/>
+      <c r="D7" s="355"/>
+      <c r="E7" s="355"/>
+      <c r="F7" s="355"/>
+      <c r="G7" s="355"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -18499,11 +18506,11 @@
         <v>205</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="352"/>
-      <c r="D8" s="352"/>
-      <c r="E8" s="352"/>
-      <c r="F8" s="352"/>
-      <c r="G8" s="352"/>
+      <c r="C8" s="355"/>
+      <c r="D8" s="355"/>
+      <c r="E8" s="355"/>
+      <c r="F8" s="355"/>
+      <c r="G8" s="355"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -18511,11 +18518,11 @@
         <v>18</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="358"/>
-      <c r="D9" s="358"/>
-      <c r="E9" s="358"/>
-      <c r="F9" s="358"/>
-      <c r="G9" s="358"/>
+      <c r="C9" s="361"/>
+      <c r="D9" s="361"/>
+      <c r="E9" s="361"/>
+      <c r="F9" s="361"/>
+      <c r="G9" s="361"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -18523,11 +18530,11 @@
         <v>281</v>
       </c>
       <c r="B10" s="90"/>
-      <c r="C10" s="352"/>
-      <c r="D10" s="352"/>
-      <c r="E10" s="352"/>
-      <c r="F10" s="352"/>
-      <c r="G10" s="352"/>
+      <c r="C10" s="355"/>
+      <c r="D10" s="355"/>
+      <c r="E10" s="355"/>
+      <c r="F10" s="355"/>
+      <c r="G10" s="355"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -18540,36 +18547,36 @@
       <c r="A12" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="359" t="s">
+      <c r="B12" s="362" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="360"/>
-      <c r="D12" s="361"/>
+      <c r="C12" s="363"/>
+      <c r="D12" s="364"/>
       <c r="N12" s="141" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="362" t="s">
+      <c r="B13" s="365" t="s">
         <v>190</v>
       </c>
-      <c r="C13" s="363"/>
-      <c r="D13" s="364"/>
+      <c r="C13" s="366"/>
+      <c r="D13" s="367"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="346" t="s">
+      <c r="B14" s="349" t="s">
         <v>185</v>
       </c>
-      <c r="C14" s="347"/>
-      <c r="D14" s="348"/>
+      <c r="C14" s="350"/>
+      <c r="D14" s="351"/>
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="349" t="s">
+      <c r="B15" s="352" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="350"/>
-      <c r="D15" s="351"/>
+      <c r="C15" s="353"/>
+      <c r="D15" s="354"/>
       <c r="N15" s="142"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -19812,7 +19819,7 @@
       <c r="B53" s="187" t="s">
         <v>212</v>
       </c>
-      <c r="C53" s="402" t="str">
+      <c r="C53" s="295" t="str">
         <f>IF(OR(C$28="",$A55=""),"",C46)</f>
         <v/>
       </c>
@@ -19862,7 +19869,7 @@
       <c r="A54" t="s">
         <v>246</v>
       </c>
-      <c r="C54" s="404" t="str">
+      <c r="C54" s="297" t="str">
         <f>IF(OR(C$28="",$A56=""),"",C52-C53)</f>
         <v/>
       </c>
@@ -19918,23 +19925,23 @@
         <f>DivideInflow!AJ29</f>
         <v>0.49593533333333339</v>
       </c>
-      <c r="C55" s="403" t="str">
+      <c r="C55" s="296" t="str">
         <f>IF(OR(C$28="",$A55=""),"",($B55*C$54))</f>
         <v/>
       </c>
-      <c r="D55" s="403" t="str">
+      <c r="D55" s="296" t="str">
         <f t="shared" ref="D55:G55" si="21">IF(OR(D$28="",$A55=""),"",($B55*D$54))</f>
         <v/>
       </c>
-      <c r="E55" s="403" t="str">
+      <c r="E55" s="296" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="F55" s="403" t="str">
+      <c r="F55" s="296" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
-      <c r="G55" s="403" t="str">
+      <c r="G55" s="296" t="str">
         <f t="shared" si="21"/>
         <v/>
       </c>
@@ -19959,23 +19966,23 @@
         <f>DivideInflow!AH29</f>
         <v>0.19965844444444442</v>
       </c>
-      <c r="C56" s="403" t="str">
+      <c r="C56" s="296" t="str">
         <f t="shared" ref="C56:G59" si="22">IF(OR(C$28="",$A56=""),"",($B56*C$54))</f>
         <v/>
       </c>
-      <c r="D56" s="403" t="str">
+      <c r="D56" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="E56" s="403" t="str">
+      <c r="E56" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="F56" s="403" t="str">
+      <c r="F56" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="G56" s="403" t="str">
+      <c r="G56" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
@@ -20014,23 +20021,23 @@
         <f>DivideInflow!AI25</f>
         <v>3.1940666666666666E-2</v>
       </c>
-      <c r="C57" s="403" t="str">
+      <c r="C57" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="D57" s="403" t="str">
+      <c r="D57" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="E57" s="403" t="str">
+      <c r="E57" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="F57" s="403" t="str">
+      <c r="F57" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="G57" s="403" t="str">
+      <c r="G57" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
@@ -20069,23 +20076,23 @@
         <f>DivideInflow!AK25</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C58" s="403" t="str">
+      <c r="C58" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="D58" s="403" t="str">
+      <c r="D58" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="E58" s="403" t="str">
+      <c r="E58" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="F58" s="403" t="str">
+      <c r="F58" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="G58" s="403" t="str">
+      <c r="G58" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
@@ -20124,23 +20131,23 @@
         <f>IF(A59="","",DivideInflow!AL25)</f>
         <v>0.10579888888888889</v>
       </c>
-      <c r="C59" s="403" t="str">
+      <c r="C59" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="D59" s="403" t="str">
+      <c r="D59" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="E59" s="403" t="str">
+      <c r="E59" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="F59" s="403" t="str">
+      <c r="F59" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
-      <c r="G59" s="403" t="str">
+      <c r="G59" s="296" t="str">
         <f t="shared" si="22"/>
         <v/>
       </c>
@@ -23394,36 +23401,36 @@
       </c>
     </row>
     <row r="4" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I4" s="384" t="s">
+      <c r="I4" s="381" t="s">
         <v>440</v>
       </c>
-      <c r="J4" s="384"/>
-      <c r="K4" s="384"/>
-      <c r="L4" s="384"/>
-      <c r="M4" s="384"/>
-      <c r="N4" s="384"/>
-      <c r="O4" s="384"/>
-      <c r="P4" s="384"/>
-      <c r="Q4" s="384"/>
-      <c r="R4" s="384"/>
-      <c r="S4" s="384"/>
-      <c r="T4" s="384"/>
-      <c r="U4" s="384"/>
-      <c r="Y4" s="384" t="s">
+      <c r="J4" s="381"/>
+      <c r="K4" s="381"/>
+      <c r="L4" s="381"/>
+      <c r="M4" s="381"/>
+      <c r="N4" s="381"/>
+      <c r="O4" s="381"/>
+      <c r="P4" s="381"/>
+      <c r="Q4" s="381"/>
+      <c r="R4" s="381"/>
+      <c r="S4" s="381"/>
+      <c r="T4" s="381"/>
+      <c r="U4" s="381"/>
+      <c r="Y4" s="381" t="s">
         <v>438</v>
       </c>
-      <c r="Z4" s="384"/>
-      <c r="AA4" s="384"/>
-      <c r="AB4" s="384"/>
-      <c r="AC4" s="384"/>
-      <c r="AD4" s="384"/>
-      <c r="AE4" s="384"/>
-      <c r="AF4" s="384"/>
-      <c r="AG4" s="384"/>
-      <c r="AH4" s="384"/>
-      <c r="AI4" s="384"/>
-      <c r="AJ4" s="384"/>
-      <c r="AK4" s="384"/>
+      <c r="Z4" s="381"/>
+      <c r="AA4" s="381"/>
+      <c r="AB4" s="381"/>
+      <c r="AC4" s="381"/>
+      <c r="AD4" s="381"/>
+      <c r="AE4" s="381"/>
+      <c r="AF4" s="381"/>
+      <c r="AG4" s="381"/>
+      <c r="AH4" s="381"/>
+      <c r="AI4" s="381"/>
+      <c r="AJ4" s="381"/>
+      <c r="AK4" s="381"/>
     </row>
     <row r="5" spans="1:37" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="189" t="s">
@@ -23444,22 +23451,22 @@
       <c r="G5" s="189" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="365" t="s">
+      <c r="I5" s="368" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="365" t="s">
+      <c r="J5" s="368" t="s">
         <v>214</v>
       </c>
-      <c r="K5" s="365" t="s">
+      <c r="K5" s="368" t="s">
         <v>215</v>
       </c>
-      <c r="L5" s="367" t="s">
+      <c r="L5" s="370" t="s">
         <v>216</v>
       </c>
-      <c r="M5" s="368"/>
-      <c r="N5" s="368"/>
-      <c r="O5" s="368"/>
-      <c r="P5" s="369"/>
+      <c r="M5" s="371"/>
+      <c r="N5" s="371"/>
+      <c r="O5" s="371"/>
+      <c r="P5" s="372"/>
       <c r="Q5" s="378" t="s">
         <v>217</v>
       </c>
@@ -23467,22 +23474,22 @@
       <c r="S5" s="379"/>
       <c r="T5" s="379"/>
       <c r="U5" s="380"/>
-      <c r="Y5" s="385" t="s">
+      <c r="Y5" s="382" t="s">
         <v>13</v>
       </c>
-      <c r="Z5" s="365" t="s">
+      <c r="Z5" s="368" t="s">
         <v>418</v>
       </c>
-      <c r="AA5" s="365" t="s">
+      <c r="AA5" s="368" t="s">
         <v>419</v>
       </c>
-      <c r="AB5" s="387" t="s">
+      <c r="AB5" s="384" t="s">
         <v>216</v>
       </c>
-      <c r="AC5" s="388"/>
-      <c r="AD5" s="388"/>
-      <c r="AE5" s="388"/>
-      <c r="AF5" s="389"/>
+      <c r="AC5" s="385"/>
+      <c r="AD5" s="385"/>
+      <c r="AE5" s="385"/>
+      <c r="AF5" s="386"/>
       <c r="AG5" s="378" t="s">
         <v>217</v>
       </c>
@@ -23492,17 +23499,17 @@
       <c r="AK5" s="380"/>
     </row>
     <row r="6" spans="1:37" s="188" customFormat="1" ht="27.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="367" t="s">
+      <c r="B6" s="370" t="s">
         <v>229</v>
       </c>
-      <c r="C6" s="368"/>
-      <c r="D6" s="368"/>
-      <c r="E6" s="368"/>
-      <c r="F6" s="368"/>
-      <c r="G6" s="369"/>
-      <c r="I6" s="366"/>
-      <c r="J6" s="366"/>
-      <c r="K6" s="366"/>
+      <c r="C6" s="371"/>
+      <c r="D6" s="371"/>
+      <c r="E6" s="371"/>
+      <c r="F6" s="371"/>
+      <c r="G6" s="372"/>
+      <c r="I6" s="369"/>
+      <c r="J6" s="369"/>
+      <c r="K6" s="369"/>
       <c r="L6" s="190" t="s">
         <v>219</v>
       </c>
@@ -23533,9 +23540,9 @@
       <c r="U6" s="191" t="s">
         <v>228</v>
       </c>
-      <c r="Y6" s="386"/>
-      <c r="Z6" s="386"/>
-      <c r="AA6" s="386"/>
+      <c r="Y6" s="383"/>
+      <c r="Z6" s="383"/>
+      <c r="AA6" s="383"/>
       <c r="AB6" s="190" t="s">
         <v>219</v>
       </c>
@@ -23775,7 +23782,7 @@
         <v>1.4499900000000001</v>
       </c>
       <c r="AF8" s="281">
-        <f t="shared" ref="AF7:AF16" si="10">SUM(AB8:AE8)</f>
+        <f t="shared" ref="AF8:AF16" si="10">SUM(AB8:AE8)</f>
         <v>8.6999999999999993</v>
       </c>
       <c r="AG8" s="283">
@@ -23911,14 +23918,14 @@
       </c>
     </row>
     <row r="10" spans="1:37" s="197" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B10" s="370" t="s">
+      <c r="B10" s="374" t="s">
         <v>238</v>
       </c>
-      <c r="C10" s="370"/>
-      <c r="D10" s="370"/>
-      <c r="E10" s="370"/>
-      <c r="F10" s="370"/>
-      <c r="G10" s="370"/>
+      <c r="C10" s="374"/>
+      <c r="D10" s="374"/>
+      <c r="E10" s="374"/>
+      <c r="F10" s="374"/>
+      <c r="G10" s="374"/>
       <c r="I10" s="257" t="s">
         <v>234</v>
       </c>
@@ -24611,13 +24618,13 @@
       <c r="B16" s="198" t="s">
         <v>235</v>
       </c>
-      <c r="C16" s="371" t="s">
+      <c r="C16" s="387" t="s">
         <v>236</v>
       </c>
-      <c r="D16" s="372"/>
-      <c r="E16" s="372"/>
-      <c r="F16" s="372"/>
-      <c r="G16" s="373"/>
+      <c r="D16" s="388"/>
+      <c r="E16" s="388"/>
+      <c r="F16" s="388"/>
+      <c r="G16" s="389"/>
       <c r="I16" s="257" t="s">
         <v>412</v>
       </c>
@@ -24768,40 +24775,40 @@
       <c r="U21" s="260"/>
     </row>
     <row r="22" spans="2:40" s="197" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I22" s="381" t="s">
+      <c r="I22" s="375" t="s">
         <v>437</v>
       </c>
-      <c r="J22" s="382"/>
-      <c r="K22" s="382"/>
-      <c r="L22" s="382"/>
-      <c r="M22" s="382"/>
-      <c r="N22" s="382"/>
-      <c r="O22" s="382"/>
-      <c r="P22" s="382"/>
-      <c r="Q22" s="382"/>
-      <c r="R22" s="382"/>
-      <c r="S22" s="382"/>
-      <c r="T22" s="382"/>
-      <c r="U22" s="382"/>
-      <c r="V22" s="382"/>
-      <c r="W22" s="383"/>
-      <c r="Y22" s="381" t="s">
+      <c r="J22" s="376"/>
+      <c r="K22" s="376"/>
+      <c r="L22" s="376"/>
+      <c r="M22" s="376"/>
+      <c r="N22" s="376"/>
+      <c r="O22" s="376"/>
+      <c r="P22" s="376"/>
+      <c r="Q22" s="376"/>
+      <c r="R22" s="376"/>
+      <c r="S22" s="376"/>
+      <c r="T22" s="376"/>
+      <c r="U22" s="376"/>
+      <c r="V22" s="376"/>
+      <c r="W22" s="377"/>
+      <c r="Y22" s="375" t="s">
         <v>439</v>
       </c>
-      <c r="Z22" s="382"/>
-      <c r="AA22" s="382"/>
-      <c r="AB22" s="382"/>
-      <c r="AC22" s="382"/>
-      <c r="AD22" s="382"/>
-      <c r="AE22" s="382"/>
-      <c r="AF22" s="382"/>
-      <c r="AG22" s="382"/>
-      <c r="AH22" s="382"/>
-      <c r="AI22" s="382"/>
-      <c r="AJ22" s="382"/>
-      <c r="AK22" s="382"/>
-      <c r="AL22" s="382"/>
-      <c r="AM22" s="383"/>
+      <c r="Z22" s="376"/>
+      <c r="AA22" s="376"/>
+      <c r="AB22" s="376"/>
+      <c r="AC22" s="376"/>
+      <c r="AD22" s="376"/>
+      <c r="AE22" s="376"/>
+      <c r="AF22" s="376"/>
+      <c r="AG22" s="376"/>
+      <c r="AH22" s="376"/>
+      <c r="AI22" s="376"/>
+      <c r="AJ22" s="376"/>
+      <c r="AK22" s="376"/>
+      <c r="AL22" s="376"/>
+      <c r="AM22" s="377"/>
     </row>
     <row r="23" spans="2:40" s="197" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="285"/>
@@ -24810,23 +24817,23 @@
       <c r="E23" s="266"/>
       <c r="F23" s="266"/>
       <c r="G23" s="266"/>
-      <c r="I23" s="365" t="s">
+      <c r="I23" s="368" t="s">
         <v>13</v>
       </c>
-      <c r="J23" s="365" t="s">
+      <c r="J23" s="368" t="s">
         <v>214</v>
       </c>
-      <c r="K23" s="365" t="s">
+      <c r="K23" s="368" t="s">
         <v>215</v>
       </c>
-      <c r="L23" s="367" t="s">
+      <c r="L23" s="370" t="s">
         <v>216</v>
       </c>
-      <c r="M23" s="368"/>
-      <c r="N23" s="368"/>
-      <c r="O23" s="368"/>
-      <c r="P23" s="368"/>
-      <c r="Q23" s="369"/>
+      <c r="M23" s="371"/>
+      <c r="N23" s="371"/>
+      <c r="O23" s="371"/>
+      <c r="P23" s="371"/>
+      <c r="Q23" s="372"/>
       <c r="R23" s="378" t="s">
         <v>217</v>
       </c>
@@ -24835,23 +24842,23 @@
       <c r="U23" s="379"/>
       <c r="V23" s="379"/>
       <c r="W23" s="380"/>
-      <c r="Y23" s="385" t="s">
+      <c r="Y23" s="382" t="s">
         <v>13</v>
       </c>
-      <c r="Z23" s="365" t="s">
+      <c r="Z23" s="368" t="s">
         <v>420</v>
       </c>
-      <c r="AA23" s="365" t="s">
+      <c r="AA23" s="368" t="s">
         <v>419</v>
       </c>
-      <c r="AB23" s="387" t="s">
+      <c r="AB23" s="384" t="s">
         <v>216</v>
       </c>
-      <c r="AC23" s="388"/>
-      <c r="AD23" s="388"/>
-      <c r="AE23" s="388"/>
-      <c r="AF23" s="388"/>
-      <c r="AG23" s="389"/>
+      <c r="AC23" s="385"/>
+      <c r="AD23" s="385"/>
+      <c r="AE23" s="385"/>
+      <c r="AF23" s="385"/>
+      <c r="AG23" s="386"/>
       <c r="AH23" s="378" t="s">
         <v>217</v>
       </c>
@@ -24868,9 +24875,9 @@
       <c r="E24" s="266"/>
       <c r="F24" s="266"/>
       <c r="G24" s="266"/>
-      <c r="I24" s="366"/>
-      <c r="J24" s="366"/>
-      <c r="K24" s="366"/>
+      <c r="I24" s="369"/>
+      <c r="J24" s="369"/>
+      <c r="K24" s="369"/>
       <c r="L24" s="190" t="s">
         <v>219</v>
       </c>
@@ -24907,9 +24914,9 @@
       <c r="W24" s="191" t="s">
         <v>228</v>
       </c>
-      <c r="Y24" s="386"/>
-      <c r="Z24" s="386"/>
-      <c r="AA24" s="386"/>
+      <c r="Y24" s="383"/>
+      <c r="Z24" s="383"/>
+      <c r="AA24" s="383"/>
       <c r="AB24" s="190" t="s">
         <v>421</v>
       </c>
@@ -25049,7 +25056,7 @@
         <v>0.47149755555555561</v>
       </c>
       <c r="AK25" s="283">
-        <f t="shared" ref="AK25:AK34" si="18">AE25/$AA25</f>
+        <f t="shared" ref="AK25" si="18">AE25/$AA25</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="AL25" s="283">
@@ -26103,32 +26110,32 @@
       </c>
     </row>
     <row r="37" spans="1:39" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="375" t="s">
+      <c r="A37" s="391" t="s">
         <v>430</v>
       </c>
-      <c r="B37" s="376"/>
-      <c r="C37" s="376"/>
-      <c r="D37" s="376"/>
-      <c r="E37" s="376"/>
-      <c r="F37" s="376"/>
-      <c r="G37" s="377"/>
-      <c r="I37" s="381" t="s">
+      <c r="B37" s="392"/>
+      <c r="C37" s="392"/>
+      <c r="D37" s="392"/>
+      <c r="E37" s="392"/>
+      <c r="F37" s="392"/>
+      <c r="G37" s="393"/>
+      <c r="I37" s="375" t="s">
         <v>428</v>
       </c>
-      <c r="J37" s="382"/>
-      <c r="K37" s="382"/>
-      <c r="L37" s="382"/>
-      <c r="M37" s="382"/>
-      <c r="N37" s="382"/>
-      <c r="O37" s="382"/>
-      <c r="P37" s="382"/>
-      <c r="Q37" s="382"/>
-      <c r="R37" s="382"/>
-      <c r="S37" s="382"/>
-      <c r="T37" s="382"/>
-      <c r="U37" s="382"/>
-      <c r="V37" s="382"/>
-      <c r="W37" s="383"/>
+      <c r="J37" s="376"/>
+      <c r="K37" s="376"/>
+      <c r="L37" s="376"/>
+      <c r="M37" s="376"/>
+      <c r="N37" s="376"/>
+      <c r="O37" s="376"/>
+      <c r="P37" s="376"/>
+      <c r="Q37" s="376"/>
+      <c r="R37" s="376"/>
+      <c r="S37" s="376"/>
+      <c r="T37" s="376"/>
+      <c r="U37" s="376"/>
+      <c r="V37" s="376"/>
+      <c r="W37" s="377"/>
       <c r="Y37" s="279"/>
       <c r="Z37" s="279"/>
       <c r="AA37" s="279"/>
@@ -26167,23 +26174,23 @@
       <c r="G38" s="189" t="s">
         <v>25</v>
       </c>
-      <c r="I38" s="365" t="s">
+      <c r="I38" s="368" t="s">
         <v>13</v>
       </c>
-      <c r="J38" s="365" t="s">
+      <c r="J38" s="368" t="s">
         <v>214</v>
       </c>
-      <c r="K38" s="365" t="s">
+      <c r="K38" s="368" t="s">
         <v>215</v>
       </c>
-      <c r="L38" s="367" t="s">
+      <c r="L38" s="370" t="s">
         <v>216</v>
       </c>
-      <c r="M38" s="368"/>
-      <c r="N38" s="368"/>
-      <c r="O38" s="368"/>
-      <c r="P38" s="368"/>
-      <c r="Q38" s="369"/>
+      <c r="M38" s="371"/>
+      <c r="N38" s="371"/>
+      <c r="O38" s="371"/>
+      <c r="P38" s="371"/>
+      <c r="Q38" s="372"/>
       <c r="R38" s="378" t="s">
         <v>217</v>
       </c>
@@ -26209,18 +26216,18 @@
       <c r="AM38" s="279"/>
     </row>
     <row r="39" spans="1:39" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="374" t="s">
+      <c r="A39" s="390" t="s">
         <v>229</v>
       </c>
-      <c r="B39" s="374"/>
-      <c r="C39" s="374"/>
-      <c r="D39" s="374"/>
-      <c r="E39" s="374"/>
-      <c r="F39" s="374"/>
-      <c r="G39" s="374"/>
-      <c r="I39" s="366"/>
-      <c r="J39" s="366"/>
-      <c r="K39" s="366"/>
+      <c r="B39" s="390"/>
+      <c r="C39" s="390"/>
+      <c r="D39" s="390"/>
+      <c r="E39" s="390"/>
+      <c r="F39" s="390"/>
+      <c r="G39" s="390"/>
+      <c r="I39" s="369"/>
+      <c r="J39" s="369"/>
+      <c r="K39" s="369"/>
       <c r="L39" s="190" t="s">
         <v>219</v>
       </c>
@@ -26556,14 +26563,14 @@
       <c r="A43" s="198" t="s">
         <v>235</v>
       </c>
-      <c r="B43" s="390" t="s">
+      <c r="B43" s="373" t="s">
         <v>236</v>
       </c>
-      <c r="C43" s="390"/>
-      <c r="D43" s="390"/>
-      <c r="E43" s="390"/>
-      <c r="F43" s="390"/>
-      <c r="G43" s="390"/>
+      <c r="C43" s="373"/>
+      <c r="D43" s="373"/>
+      <c r="E43" s="373"/>
+      <c r="F43" s="373"/>
+      <c r="G43" s="373"/>
       <c r="I43" s="257" t="s">
         <v>234</v>
       </c>
@@ -26636,15 +26643,15 @@
       <c r="AM43" s="277"/>
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A44" s="370" t="s">
+      <c r="A44" s="374" t="s">
         <v>238</v>
       </c>
-      <c r="B44" s="370"/>
-      <c r="C44" s="370"/>
-      <c r="D44" s="370"/>
-      <c r="E44" s="370"/>
-      <c r="F44" s="370"/>
-      <c r="G44" s="370"/>
+      <c r="B44" s="374"/>
+      <c r="C44" s="374"/>
+      <c r="D44" s="374"/>
+      <c r="E44" s="374"/>
+      <c r="F44" s="374"/>
+      <c r="G44" s="374"/>
       <c r="I44" s="257" t="s">
         <v>237</v>
       </c>
@@ -27210,14 +27217,14 @@
       <c r="A50" s="198" t="s">
         <v>235</v>
       </c>
-      <c r="B50" s="390" t="s">
+      <c r="B50" s="373" t="s">
         <v>236</v>
       </c>
-      <c r="C50" s="390"/>
-      <c r="D50" s="390"/>
-      <c r="E50" s="390"/>
-      <c r="F50" s="390"/>
-      <c r="G50" s="390"/>
+      <c r="C50" s="373"/>
+      <c r="D50" s="373"/>
+      <c r="E50" s="373"/>
+      <c r="F50" s="373"/>
+      <c r="G50" s="373"/>
     </row>
     <row r="51" spans="1:39" x14ac:dyDescent="0.2">
       <c r="B51" s="271"/>
@@ -27229,6 +27236,28 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="C16:G16"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="R38:W38"/>
+    <mergeCell ref="I37:W37"/>
+    <mergeCell ref="I4:U4"/>
+    <mergeCell ref="Y4:AK4"/>
+    <mergeCell ref="Y22:AM22"/>
+    <mergeCell ref="Y23:Y24"/>
+    <mergeCell ref="Z23:Z24"/>
+    <mergeCell ref="AA23:AA24"/>
+    <mergeCell ref="AB23:AG23"/>
+    <mergeCell ref="AH23:AM23"/>
+    <mergeCell ref="Z5:Z6"/>
+    <mergeCell ref="AA5:AA6"/>
+    <mergeCell ref="AB5:AF5"/>
+    <mergeCell ref="AG5:AK5"/>
+    <mergeCell ref="Y5:Y6"/>
+    <mergeCell ref="Q5:U5"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="L5:P5"/>
@@ -27245,28 +27274,6 @@
     <mergeCell ref="J38:J39"/>
     <mergeCell ref="K38:K39"/>
     <mergeCell ref="L38:Q38"/>
-    <mergeCell ref="R38:W38"/>
-    <mergeCell ref="I37:W37"/>
-    <mergeCell ref="I4:U4"/>
-    <mergeCell ref="Y4:AK4"/>
-    <mergeCell ref="Y22:AM22"/>
-    <mergeCell ref="Y23:Y24"/>
-    <mergeCell ref="Z23:Z24"/>
-    <mergeCell ref="AA23:AA24"/>
-    <mergeCell ref="AB23:AG23"/>
-    <mergeCell ref="AH23:AM23"/>
-    <mergeCell ref="Z5:Z6"/>
-    <mergeCell ref="AA5:AA6"/>
-    <mergeCell ref="AB5:AF5"/>
-    <mergeCell ref="AG5:AK5"/>
-    <mergeCell ref="Y5:Y6"/>
-    <mergeCell ref="Q5:U5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="C16:G16"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="A37:G37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -27606,16 +27613,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="392" t="e">
+      <c r="A1" s="394" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="392"/>
-      <c r="C1" s="392"/>
-      <c r="D1" s="392"/>
-      <c r="E1" s="392"/>
-      <c r="F1" s="392"/>
-      <c r="G1" s="392"/>
+      <c r="B1" s="394"/>
+      <c r="C1" s="394"/>
+      <c r="D1" s="394"/>
+      <c r="E1" s="394"/>
+      <c r="F1" s="394"/>
+      <c r="G1" s="394"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -27624,15 +27631,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="353" t="s">
+      <c r="A3" s="356" t="s">
         <v>178</v>
       </c>
-      <c r="B3" s="353"/>
-      <c r="C3" s="353"/>
-      <c r="D3" s="353"/>
-      <c r="E3" s="353"/>
-      <c r="F3" s="353"/>
-      <c r="G3" s="353"/>
+      <c r="B3" s="356"/>
+      <c r="C3" s="356"/>
+      <c r="D3" s="356"/>
+      <c r="E3" s="356"/>
+      <c r="F3" s="356"/>
+      <c r="G3" s="356"/>
       <c r="H3" s="84"/>
       <c r="I3" s="84"/>
       <c r="J3" s="84"/>
@@ -27648,13 +27655,13 @@
       <c r="B4" s="127" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="354" t="s">
+      <c r="C4" s="357" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="355"/>
-      <c r="E4" s="355"/>
-      <c r="F4" s="355"/>
-      <c r="G4" s="356"/>
+      <c r="D4" s="358"/>
+      <c r="E4" s="358"/>
+      <c r="F4" s="358"/>
+      <c r="G4" s="359"/>
       <c r="N4" s="139" t="s">
         <v>129</v>
       </c>
@@ -27664,11 +27671,11 @@
         <v>16</v>
       </c>
       <c r="B5" s="114"/>
-      <c r="C5" s="357"/>
-      <c r="D5" s="352"/>
-      <c r="E5" s="352"/>
-      <c r="F5" s="352"/>
-      <c r="G5" s="352"/>
+      <c r="C5" s="360"/>
+      <c r="D5" s="355"/>
+      <c r="E5" s="355"/>
+      <c r="F5" s="355"/>
+      <c r="G5" s="355"/>
       <c r="N5" s="142"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -27676,11 +27683,11 @@
         <v>17</v>
       </c>
       <c r="B6" s="114"/>
-      <c r="C6" s="357"/>
-      <c r="D6" s="352"/>
-      <c r="E6" s="352"/>
-      <c r="F6" s="352"/>
-      <c r="G6" s="352"/>
+      <c r="C6" s="360"/>
+      <c r="D6" s="355"/>
+      <c r="E6" s="355"/>
+      <c r="F6" s="355"/>
+      <c r="G6" s="355"/>
       <c r="N6" s="142"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -27688,11 +27695,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="114"/>
-      <c r="C7" s="357"/>
-      <c r="D7" s="352"/>
-      <c r="E7" s="352"/>
-      <c r="F7" s="352"/>
-      <c r="G7" s="352"/>
+      <c r="C7" s="360"/>
+      <c r="D7" s="355"/>
+      <c r="E7" s="355"/>
+      <c r="F7" s="355"/>
+      <c r="G7" s="355"/>
       <c r="N7" s="142"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -27700,11 +27707,11 @@
         <v>39</v>
       </c>
       <c r="B8" s="90"/>
-      <c r="C8" s="352"/>
-      <c r="D8" s="352"/>
-      <c r="E8" s="352"/>
-      <c r="F8" s="352"/>
-      <c r="G8" s="352"/>
+      <c r="C8" s="355"/>
+      <c r="D8" s="355"/>
+      <c r="E8" s="355"/>
+      <c r="F8" s="355"/>
+      <c r="G8" s="355"/>
       <c r="N8" s="142"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -27712,11 +27719,11 @@
         <v>163</v>
       </c>
       <c r="B9" s="90"/>
-      <c r="C9" s="358"/>
-      <c r="D9" s="358"/>
-      <c r="E9" s="358"/>
-      <c r="F9" s="358"/>
-      <c r="G9" s="358"/>
+      <c r="C9" s="361"/>
+      <c r="D9" s="361"/>
+      <c r="E9" s="361"/>
+      <c r="F9" s="361"/>
+      <c r="G9" s="361"/>
       <c r="N9" s="142"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -27724,11 +27731,11 @@
         <v>41</v>
       </c>
       <c r="B10" s="115"/>
-      <c r="C10" s="391"/>
-      <c r="D10" s="391"/>
-      <c r="E10" s="391"/>
-      <c r="F10" s="391"/>
-      <c r="G10" s="391"/>
+      <c r="C10" s="395"/>
+      <c r="D10" s="395"/>
+      <c r="E10" s="395"/>
+      <c r="F10" s="395"/>
+      <c r="G10" s="395"/>
       <c r="N10" s="142"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -27741,37 +27748,37 @@
       <c r="A12" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="359" t="s">
+      <c r="B12" s="362" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="360"/>
-      <c r="D12" s="361"/>
+      <c r="C12" s="363"/>
+      <c r="D12" s="364"/>
       <c r="N12" s="141" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="362" t="s">
+      <c r="B13" s="365" t="s">
         <v>114</v>
       </c>
-      <c r="C13" s="363"/>
-      <c r="D13" s="364"/>
+      <c r="C13" s="366"/>
+      <c r="D13" s="367"/>
       <c r="N13" s="142"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="346" t="s">
+      <c r="B14" s="349" t="s">
         <v>115</v>
       </c>
-      <c r="C14" s="347"/>
-      <c r="D14" s="348"/>
+      <c r="C14" s="350"/>
+      <c r="D14" s="351"/>
       <c r="N14" s="142"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="349" t="s">
+      <c r="B15" s="352" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="350"/>
-      <c r="D15" s="351"/>
+      <c r="C15" s="353"/>
+      <c r="D15" s="354"/>
       <c r="N15" s="142"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -28991,12 +28998,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -29004,6 +29005,12 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>
@@ -29061,26 +29068,26 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="393" t="s">
+      <c r="D3" s="396" t="s">
         <v>60</v>
       </c>
-      <c r="E3" s="393"/>
-      <c r="F3" s="393" t="s">
+      <c r="E3" s="396"/>
+      <c r="F3" s="396" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="393"/>
-      <c r="H3" s="393"/>
-      <c r="I3" s="393" t="s">
+      <c r="G3" s="396"/>
+      <c r="H3" s="396"/>
+      <c r="I3" s="396" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="393"/>
-      <c r="K3" s="393"/>
+      <c r="J3" s="396"/>
+      <c r="K3" s="396"/>
       <c r="L3" s="134"/>
-      <c r="M3" s="393" t="s">
+      <c r="M3" s="396" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="393"/>
-      <c r="O3" s="393"/>
+      <c r="N3" s="396"/>
+      <c r="O3" s="396"/>
     </row>
     <row r="4" spans="1:16" s="47" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">

</xml_diff>

<commit_message>
Anabelle explained the new figure in the model guide and moved the key in the model for historical allocations.
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anabelle/Documents/ColoradoRiverCollaborate/LakeMeadWaterBankDivideInflow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6294FE5E-BDC9-E14E-B4A6-61405E23C740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531AEBE7-C771-874C-A5C7-1442C2D49AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="1" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="3" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe-Directions" sheetId="62" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="469">
   <si>
     <t>Year 1</t>
   </si>
@@ -4080,68 +4080,14 @@
     <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="27" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="27" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="27" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4197,6 +4143,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4229,6 +4178,63 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="27" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="27" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4290,12 +4296,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4304,15 +4304,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4344,6 +4335,9 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4353,11 +4347,23 @@
     <xf numFmtId="0" fontId="18" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4385,12 +4391,6 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -16014,20 +16014,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="364" t="s">
+      <c r="A1" s="346" t="s">
         <v>296</v>
       </c>
-      <c r="B1" s="364"/>
-      <c r="C1" s="364"/>
-      <c r="D1" s="364"/>
-      <c r="E1" s="364"/>
-      <c r="F1" s="364"/>
-      <c r="G1" s="364"/>
-      <c r="H1" s="364"/>
-      <c r="I1" s="364"/>
-      <c r="J1" s="364"/>
-      <c r="K1" s="364"/>
-      <c r="L1" s="364"/>
+      <c r="B1" s="346"/>
+      <c r="C1" s="346"/>
+      <c r="D1" s="346"/>
+      <c r="E1" s="346"/>
+      <c r="F1" s="346"/>
+      <c r="G1" s="346"/>
+      <c r="H1" s="346"/>
+      <c r="I1" s="346"/>
+      <c r="J1" s="346"/>
+      <c r="K1" s="346"/>
+      <c r="L1" s="346"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -16053,41 +16053,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="52" customFormat="1" ht="53.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="365" t="s">
+      <c r="A4" s="347" t="s">
         <v>297</v>
       </c>
-      <c r="B4" s="366"/>
-      <c r="C4" s="366"/>
-      <c r="D4" s="366"/>
-      <c r="E4" s="366"/>
-      <c r="F4" s="366"/>
-      <c r="G4" s="366"/>
-      <c r="H4" s="366"/>
-      <c r="I4" s="366"/>
-      <c r="J4" s="366"/>
-      <c r="K4" s="366"/>
-      <c r="L4" s="367"/>
-      <c r="N4" s="368"/>
-      <c r="O4" s="368"/>
-      <c r="P4" s="368"/>
-      <c r="Q4" s="368"/>
-      <c r="R4" s="368"/>
+      <c r="B4" s="348"/>
+      <c r="C4" s="348"/>
+      <c r="D4" s="348"/>
+      <c r="E4" s="348"/>
+      <c r="F4" s="348"/>
+      <c r="G4" s="348"/>
+      <c r="H4" s="348"/>
+      <c r="I4" s="348"/>
+      <c r="J4" s="348"/>
+      <c r="K4" s="348"/>
+      <c r="L4" s="349"/>
+      <c r="N4" s="350"/>
+      <c r="O4" s="350"/>
+      <c r="P4" s="350"/>
+      <c r="Q4" s="350"/>
+      <c r="R4" s="350"/>
     </row>
     <row r="5" spans="1:18" s="52" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="369" t="s">
+      <c r="A5" s="351" t="s">
         <v>281</v>
       </c>
-      <c r="B5" s="370"/>
-      <c r="C5" s="370"/>
-      <c r="D5" s="370"/>
-      <c r="E5" s="370"/>
-      <c r="F5" s="370"/>
-      <c r="G5" s="370"/>
-      <c r="H5" s="370"/>
-      <c r="I5" s="370"/>
-      <c r="J5" s="370"/>
-      <c r="K5" s="370"/>
-      <c r="L5" s="371"/>
+      <c r="B5" s="352"/>
+      <c r="C5" s="352"/>
+      <c r="D5" s="352"/>
+      <c r="E5" s="352"/>
+      <c r="F5" s="352"/>
+      <c r="G5" s="352"/>
+      <c r="H5" s="352"/>
+      <c r="I5" s="352"/>
+      <c r="J5" s="352"/>
+      <c r="K5" s="352"/>
+      <c r="L5" s="353"/>
       <c r="N5" s="110"/>
       <c r="O5" s="110"/>
       <c r="P5" s="110"/>
@@ -16095,20 +16095,20 @@
       <c r="R5" s="110"/>
     </row>
     <row r="6" spans="1:18" s="52" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="369" t="s">
+      <c r="A6" s="351" t="s">
         <v>298</v>
       </c>
-      <c r="B6" s="370"/>
-      <c r="C6" s="370"/>
-      <c r="D6" s="370"/>
-      <c r="E6" s="370"/>
-      <c r="F6" s="370"/>
-      <c r="G6" s="370"/>
-      <c r="H6" s="370"/>
-      <c r="I6" s="370"/>
-      <c r="J6" s="370"/>
-      <c r="K6" s="370"/>
-      <c r="L6" s="371"/>
+      <c r="B6" s="352"/>
+      <c r="C6" s="352"/>
+      <c r="D6" s="352"/>
+      <c r="E6" s="352"/>
+      <c r="F6" s="352"/>
+      <c r="G6" s="352"/>
+      <c r="H6" s="352"/>
+      <c r="I6" s="352"/>
+      <c r="J6" s="352"/>
+      <c r="K6" s="352"/>
+      <c r="L6" s="353"/>
       <c r="N6" s="110"/>
       <c r="O6" s="110"/>
       <c r="P6" s="110"/>
@@ -16117,19 +16117,19 @@
     </row>
     <row r="7" spans="1:18" s="52" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="216"/>
-      <c r="B7" s="370" t="s">
+      <c r="B7" s="352" t="s">
         <v>299</v>
       </c>
-      <c r="C7" s="370"/>
-      <c r="D7" s="370"/>
-      <c r="E7" s="370"/>
-      <c r="F7" s="370"/>
-      <c r="G7" s="370"/>
-      <c r="H7" s="370"/>
-      <c r="I7" s="370"/>
-      <c r="J7" s="370"/>
-      <c r="K7" s="370"/>
-      <c r="L7" s="371"/>
+      <c r="C7" s="352"/>
+      <c r="D7" s="352"/>
+      <c r="E7" s="352"/>
+      <c r="F7" s="352"/>
+      <c r="G7" s="352"/>
+      <c r="H7" s="352"/>
+      <c r="I7" s="352"/>
+      <c r="J7" s="352"/>
+      <c r="K7" s="352"/>
+      <c r="L7" s="353"/>
       <c r="N7" s="110"/>
       <c r="O7" s="110"/>
       <c r="P7" s="110"/>
@@ -16138,19 +16138,19 @@
     </row>
     <row r="8" spans="1:18" s="52" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="217"/>
-      <c r="B8" s="385" t="s">
+      <c r="B8" s="368" t="s">
         <v>300</v>
       </c>
-      <c r="C8" s="385"/>
-      <c r="D8" s="385"/>
-      <c r="E8" s="385"/>
-      <c r="F8" s="385"/>
-      <c r="G8" s="385"/>
-      <c r="H8" s="385"/>
-      <c r="I8" s="385"/>
-      <c r="J8" s="385"/>
-      <c r="K8" s="385"/>
-      <c r="L8" s="386"/>
+      <c r="C8" s="368"/>
+      <c r="D8" s="368"/>
+      <c r="E8" s="368"/>
+      <c r="F8" s="368"/>
+      <c r="G8" s="368"/>
+      <c r="H8" s="368"/>
+      <c r="I8" s="368"/>
+      <c r="J8" s="368"/>
+      <c r="K8" s="368"/>
+      <c r="L8" s="369"/>
       <c r="N8" s="110"/>
       <c r="O8" s="110"/>
       <c r="P8" s="110"/>
@@ -16172,38 +16172,38 @@
       <c r="L9" s="110"/>
     </row>
     <row r="10" spans="1:18" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="387" t="s">
+      <c r="A10" s="370" t="s">
         <v>335</v>
       </c>
-      <c r="B10" s="388"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
-      <c r="G10" s="388"/>
-      <c r="H10" s="388"/>
-      <c r="I10" s="388"/>
-      <c r="J10" s="388"/>
-      <c r="K10" s="388"/>
-      <c r="L10" s="389"/>
+      <c r="B10" s="371"/>
+      <c r="C10" s="371"/>
+      <c r="D10" s="371"/>
+      <c r="E10" s="371"/>
+      <c r="F10" s="371"/>
+      <c r="G10" s="371"/>
+      <c r="H10" s="371"/>
+      <c r="I10" s="371"/>
+      <c r="J10" s="371"/>
+      <c r="K10" s="371"/>
+      <c r="L10" s="372"/>
     </row>
     <row r="11" spans="1:18" s="56" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="237" t="s">
         <v>336</v>
       </c>
-      <c r="B11" s="342" t="s">
+      <c r="B11" s="373" t="s">
         <v>339</v>
       </c>
-      <c r="C11" s="342"/>
-      <c r="D11" s="342"/>
-      <c r="E11" s="342"/>
-      <c r="F11" s="342"/>
-      <c r="G11" s="342"/>
-      <c r="H11" s="342"/>
-      <c r="I11" s="342"/>
-      <c r="J11" s="342"/>
-      <c r="K11" s="342"/>
-      <c r="L11" s="343"/>
+      <c r="C11" s="373"/>
+      <c r="D11" s="373"/>
+      <c r="E11" s="373"/>
+      <c r="F11" s="373"/>
+      <c r="G11" s="373"/>
+      <c r="H11" s="373"/>
+      <c r="I11" s="373"/>
+      <c r="J11" s="373"/>
+      <c r="K11" s="373"/>
+      <c r="L11" s="374"/>
     </row>
     <row r="12" spans="1:18" s="57" customFormat="1" ht="161.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="229"/>
@@ -16223,51 +16223,51 @@
       <c r="A13" s="237" t="s">
         <v>337</v>
       </c>
-      <c r="B13" s="342" t="s">
+      <c r="B13" s="373" t="s">
         <v>340</v>
       </c>
-      <c r="C13" s="342"/>
-      <c r="D13" s="342"/>
-      <c r="E13" s="342"/>
-      <c r="F13" s="342"/>
-      <c r="G13" s="342"/>
-      <c r="H13" s="342"/>
-      <c r="I13" s="342"/>
-      <c r="J13" s="342"/>
-      <c r="K13" s="342"/>
-      <c r="L13" s="343"/>
+      <c r="C13" s="373"/>
+      <c r="D13" s="373"/>
+      <c r="E13" s="373"/>
+      <c r="F13" s="373"/>
+      <c r="G13" s="373"/>
+      <c r="H13" s="373"/>
+      <c r="I13" s="373"/>
+      <c r="J13" s="373"/>
+      <c r="K13" s="373"/>
+      <c r="L13" s="374"/>
     </row>
     <row r="14" spans="1:18" s="57" customFormat="1" ht="90.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="229"/>
-      <c r="B14" s="344"/>
-      <c r="C14" s="344"/>
-      <c r="D14" s="344"/>
-      <c r="E14" s="344"/>
-      <c r="F14" s="344"/>
-      <c r="G14" s="344"/>
-      <c r="H14" s="344"/>
-      <c r="I14" s="344"/>
-      <c r="J14" s="344"/>
-      <c r="K14" s="344"/>
-      <c r="L14" s="345"/>
+      <c r="B14" s="384"/>
+      <c r="C14" s="384"/>
+      <c r="D14" s="384"/>
+      <c r="E14" s="384"/>
+      <c r="F14" s="384"/>
+      <c r="G14" s="384"/>
+      <c r="H14" s="384"/>
+      <c r="I14" s="384"/>
+      <c r="J14" s="384"/>
+      <c r="K14" s="384"/>
+      <c r="L14" s="385"/>
     </row>
     <row r="15" spans="1:18" s="56" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="237" t="s">
         <v>338</v>
       </c>
-      <c r="B15" s="342" t="s">
+      <c r="B15" s="373" t="s">
         <v>467</v>
       </c>
-      <c r="C15" s="342"/>
-      <c r="D15" s="342"/>
-      <c r="E15" s="342"/>
-      <c r="F15" s="342"/>
-      <c r="G15" s="342"/>
-      <c r="H15" s="342"/>
-      <c r="I15" s="342"/>
-      <c r="J15" s="342"/>
-      <c r="K15" s="342"/>
-      <c r="L15" s="343"/>
+      <c r="C15" s="373"/>
+      <c r="D15" s="373"/>
+      <c r="E15" s="373"/>
+      <c r="F15" s="373"/>
+      <c r="G15" s="373"/>
+      <c r="H15" s="373"/>
+      <c r="I15" s="373"/>
+      <c r="J15" s="373"/>
+      <c r="K15" s="373"/>
+      <c r="L15" s="374"/>
     </row>
     <row r="16" spans="1:18" s="57" customFormat="1" ht="269" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="229"/>
@@ -16284,12 +16284,12 @@
       <c r="L16" s="236"/>
     </row>
     <row r="17" spans="1:14" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="340" t="s">
+      <c r="A17" s="382" t="s">
         <v>344</v>
       </c>
-      <c r="B17" s="341"/>
-      <c r="C17" s="341"/>
-      <c r="D17" s="341"/>
+      <c r="B17" s="383"/>
+      <c r="C17" s="383"/>
+      <c r="D17" s="383"/>
       <c r="E17" s="234" t="s">
         <v>345</v>
       </c>
@@ -16316,84 +16316,84 @@
       <c r="L18" s="110"/>
     </row>
     <row r="19" spans="1:14" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="372" t="s">
+      <c r="A19" s="354" t="s">
         <v>165</v>
       </c>
-      <c r="B19" s="373"/>
-      <c r="C19" s="373"/>
-      <c r="D19" s="373"/>
-      <c r="E19" s="373"/>
-      <c r="F19" s="373"/>
-      <c r="G19" s="373"/>
-      <c r="H19" s="373"/>
-      <c r="I19" s="373"/>
-      <c r="J19" s="373"/>
-      <c r="K19" s="373"/>
-      <c r="L19" s="374"/>
+      <c r="B19" s="355"/>
+      <c r="C19" s="355"/>
+      <c r="D19" s="355"/>
+      <c r="E19" s="355"/>
+      <c r="F19" s="355"/>
+      <c r="G19" s="355"/>
+      <c r="H19" s="355"/>
+      <c r="I19" s="355"/>
+      <c r="J19" s="355"/>
+      <c r="K19" s="355"/>
+      <c r="L19" s="356"/>
     </row>
     <row r="20" spans="1:14" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="375" t="s">
+      <c r="A20" s="357" t="s">
         <v>282</v>
       </c>
-      <c r="B20" s="376"/>
-      <c r="C20" s="376"/>
-      <c r="D20" s="376"/>
-      <c r="E20" s="376"/>
-      <c r="F20" s="376"/>
-      <c r="G20" s="376"/>
-      <c r="H20" s="376"/>
-      <c r="I20" s="376"/>
-      <c r="J20" s="376"/>
-      <c r="K20" s="376"/>
-      <c r="L20" s="377"/>
+      <c r="B20" s="358"/>
+      <c r="C20" s="358"/>
+      <c r="D20" s="358"/>
+      <c r="E20" s="358"/>
+      <c r="F20" s="358"/>
+      <c r="G20" s="358"/>
+      <c r="H20" s="358"/>
+      <c r="I20" s="358"/>
+      <c r="J20" s="358"/>
+      <c r="K20" s="358"/>
+      <c r="L20" s="359"/>
     </row>
     <row r="21" spans="1:14" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="378" t="s">
+      <c r="A21" s="360" t="s">
         <v>283</v>
       </c>
-      <c r="B21" s="356"/>
-      <c r="C21" s="356"/>
-      <c r="D21" s="356"/>
-      <c r="E21" s="356"/>
-      <c r="F21" s="356"/>
-      <c r="G21" s="356"/>
-      <c r="H21" s="356"/>
-      <c r="I21" s="356"/>
-      <c r="J21" s="356"/>
-      <c r="K21" s="356"/>
-      <c r="L21" s="357"/>
+      <c r="B21" s="340"/>
+      <c r="C21" s="340"/>
+      <c r="D21" s="340"/>
+      <c r="E21" s="340"/>
+      <c r="F21" s="340"/>
+      <c r="G21" s="340"/>
+      <c r="H21" s="340"/>
+      <c r="I21" s="340"/>
+      <c r="J21" s="340"/>
+      <c r="K21" s="340"/>
+      <c r="L21" s="361"/>
     </row>
     <row r="22" spans="1:14" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="378" t="s">
+      <c r="A22" s="360" t="s">
         <v>166</v>
       </c>
-      <c r="B22" s="356"/>
-      <c r="C22" s="356"/>
-      <c r="D22" s="356"/>
-      <c r="E22" s="356"/>
-      <c r="F22" s="356"/>
-      <c r="G22" s="356"/>
-      <c r="H22" s="356"/>
-      <c r="I22" s="356"/>
-      <c r="J22" s="356"/>
-      <c r="K22" s="356"/>
-      <c r="L22" s="357"/>
+      <c r="B22" s="340"/>
+      <c r="C22" s="340"/>
+      <c r="D22" s="340"/>
+      <c r="E22" s="340"/>
+      <c r="F22" s="340"/>
+      <c r="G22" s="340"/>
+      <c r="H22" s="340"/>
+      <c r="I22" s="340"/>
+      <c r="J22" s="340"/>
+      <c r="K22" s="340"/>
+      <c r="L22" s="361"/>
     </row>
     <row r="23" spans="1:14" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="379" t="s">
+      <c r="A23" s="362" t="s">
         <v>284</v>
       </c>
-      <c r="B23" s="380"/>
-      <c r="C23" s="380"/>
-      <c r="D23" s="380"/>
-      <c r="E23" s="380"/>
-      <c r="F23" s="380"/>
-      <c r="G23" s="380"/>
-      <c r="H23" s="380"/>
-      <c r="I23" s="380"/>
-      <c r="J23" s="380"/>
-      <c r="K23" s="380"/>
-      <c r="L23" s="381"/>
+      <c r="B23" s="363"/>
+      <c r="C23" s="363"/>
+      <c r="D23" s="363"/>
+      <c r="E23" s="363"/>
+      <c r="F23" s="363"/>
+      <c r="G23" s="363"/>
+      <c r="H23" s="363"/>
+      <c r="I23" s="363"/>
+      <c r="J23" s="363"/>
+      <c r="K23" s="363"/>
+      <c r="L23" s="364"/>
     </row>
     <row r="24" spans="1:14" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="110"/>
@@ -16410,332 +16410,332 @@
       <c r="L24" s="110"/>
     </row>
     <row r="25" spans="1:14" s="57" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="382" t="s">
+      <c r="A25" s="365" t="s">
         <v>280</v>
       </c>
-      <c r="B25" s="383"/>
-      <c r="C25" s="383"/>
-      <c r="D25" s="383"/>
-      <c r="E25" s="383"/>
-      <c r="F25" s="383"/>
-      <c r="G25" s="383"/>
-      <c r="H25" s="383"/>
-      <c r="I25" s="383"/>
-      <c r="J25" s="383"/>
-      <c r="K25" s="383"/>
-      <c r="L25" s="384"/>
+      <c r="B25" s="366"/>
+      <c r="C25" s="366"/>
+      <c r="D25" s="366"/>
+      <c r="E25" s="366"/>
+      <c r="F25" s="366"/>
+      <c r="G25" s="366"/>
+      <c r="H25" s="366"/>
+      <c r="I25" s="366"/>
+      <c r="J25" s="366"/>
+      <c r="K25" s="366"/>
+      <c r="L25" s="367"/>
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14" s="57" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="361" t="s">
+      <c r="A26" s="343" t="s">
         <v>175</v>
       </c>
-      <c r="B26" s="362"/>
-      <c r="C26" s="362"/>
-      <c r="D26" s="362"/>
-      <c r="E26" s="362"/>
-      <c r="F26" s="362"/>
-      <c r="G26" s="362"/>
-      <c r="H26" s="362"/>
-      <c r="I26" s="362"/>
-      <c r="J26" s="362"/>
-      <c r="K26" s="362"/>
-      <c r="L26" s="363"/>
+      <c r="B26" s="344"/>
+      <c r="C26" s="344"/>
+      <c r="D26" s="344"/>
+      <c r="E26" s="344"/>
+      <c r="F26" s="344"/>
+      <c r="G26" s="344"/>
+      <c r="H26" s="344"/>
+      <c r="I26" s="344"/>
+      <c r="J26" s="344"/>
+      <c r="K26" s="344"/>
+      <c r="L26" s="345"/>
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="211">
         <v>1</v>
       </c>
-      <c r="B27" s="349" t="s">
+      <c r="B27" s="377" t="s">
         <v>174</v>
       </c>
-      <c r="C27" s="349"/>
-      <c r="D27" s="349"/>
-      <c r="E27" s="349"/>
-      <c r="F27" s="349"/>
-      <c r="G27" s="349"/>
-      <c r="H27" s="349"/>
-      <c r="I27" s="349"/>
-      <c r="J27" s="349"/>
-      <c r="K27" s="349"/>
-      <c r="L27" s="350"/>
+      <c r="C27" s="377"/>
+      <c r="D27" s="377"/>
+      <c r="E27" s="377"/>
+      <c r="F27" s="377"/>
+      <c r="G27" s="377"/>
+      <c r="H27" s="377"/>
+      <c r="I27" s="377"/>
+      <c r="J27" s="377"/>
+      <c r="K27" s="377"/>
+      <c r="L27" s="378"/>
     </row>
     <row r="28" spans="1:14" s="57" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="211">
         <v>2</v>
       </c>
-      <c r="B28" s="349" t="s">
+      <c r="B28" s="377" t="s">
         <v>276</v>
       </c>
-      <c r="C28" s="349"/>
-      <c r="D28" s="349"/>
-      <c r="E28" s="349"/>
-      <c r="F28" s="349"/>
-      <c r="G28" s="349"/>
-      <c r="H28" s="349"/>
-      <c r="I28" s="349"/>
-      <c r="J28" s="349"/>
-      <c r="K28" s="349"/>
-      <c r="L28" s="350"/>
+      <c r="C28" s="377"/>
+      <c r="D28" s="377"/>
+      <c r="E28" s="377"/>
+      <c r="F28" s="377"/>
+      <c r="G28" s="377"/>
+      <c r="H28" s="377"/>
+      <c r="I28" s="377"/>
+      <c r="J28" s="377"/>
+      <c r="K28" s="377"/>
+      <c r="L28" s="378"/>
       <c r="N28" s="104"/>
     </row>
     <row r="29" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="211">
         <v>3</v>
       </c>
-      <c r="B29" s="349" t="s">
+      <c r="B29" s="377" t="s">
         <v>167</v>
       </c>
-      <c r="C29" s="349"/>
-      <c r="D29" s="349"/>
-      <c r="E29" s="349"/>
-      <c r="F29" s="349"/>
-      <c r="G29" s="349"/>
-      <c r="H29" s="349"/>
-      <c r="I29" s="349"/>
-      <c r="J29" s="349"/>
-      <c r="K29" s="349"/>
-      <c r="L29" s="350"/>
+      <c r="C29" s="377"/>
+      <c r="D29" s="377"/>
+      <c r="E29" s="377"/>
+      <c r="F29" s="377"/>
+      <c r="G29" s="377"/>
+      <c r="H29" s="377"/>
+      <c r="I29" s="377"/>
+      <c r="J29" s="377"/>
+      <c r="K29" s="377"/>
+      <c r="L29" s="378"/>
       <c r="N29" s="104"/>
     </row>
     <row r="30" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="211">
         <v>4</v>
       </c>
-      <c r="B30" s="349" t="s">
+      <c r="B30" s="377" t="s">
         <v>285</v>
       </c>
-      <c r="C30" s="349"/>
-      <c r="D30" s="349"/>
-      <c r="E30" s="349"/>
-      <c r="F30" s="349"/>
-      <c r="G30" s="349"/>
-      <c r="H30" s="349"/>
-      <c r="I30" s="349"/>
-      <c r="J30" s="349"/>
-      <c r="K30" s="349"/>
-      <c r="L30" s="350"/>
+      <c r="C30" s="377"/>
+      <c r="D30" s="377"/>
+      <c r="E30" s="377"/>
+      <c r="F30" s="377"/>
+      <c r="G30" s="377"/>
+      <c r="H30" s="377"/>
+      <c r="I30" s="377"/>
+      <c r="J30" s="377"/>
+      <c r="K30" s="377"/>
+      <c r="L30" s="378"/>
       <c r="N30" s="104"/>
     </row>
     <row r="31" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="211">
         <v>5</v>
       </c>
-      <c r="B31" s="349" t="s">
+      <c r="B31" s="377" t="s">
         <v>168</v>
       </c>
-      <c r="C31" s="349"/>
-      <c r="D31" s="349"/>
-      <c r="E31" s="349"/>
-      <c r="F31" s="349"/>
-      <c r="G31" s="349"/>
-      <c r="H31" s="349"/>
-      <c r="I31" s="349"/>
-      <c r="J31" s="349"/>
-      <c r="K31" s="349"/>
-      <c r="L31" s="350"/>
+      <c r="C31" s="377"/>
+      <c r="D31" s="377"/>
+      <c r="E31" s="377"/>
+      <c r="F31" s="377"/>
+      <c r="G31" s="377"/>
+      <c r="H31" s="377"/>
+      <c r="I31" s="377"/>
+      <c r="J31" s="377"/>
+      <c r="K31" s="377"/>
+      <c r="L31" s="378"/>
       <c r="N31" s="104"/>
     </row>
     <row r="32" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="211"/>
-      <c r="B32" s="349" t="s">
+      <c r="B32" s="377" t="s">
         <v>169</v>
       </c>
-      <c r="C32" s="349"/>
-      <c r="D32" s="349"/>
-      <c r="E32" s="349"/>
-      <c r="F32" s="349"/>
-      <c r="G32" s="349"/>
-      <c r="H32" s="349"/>
-      <c r="I32" s="349"/>
-      <c r="J32" s="349"/>
-      <c r="K32" s="349"/>
-      <c r="L32" s="350"/>
+      <c r="C32" s="377"/>
+      <c r="D32" s="377"/>
+      <c r="E32" s="377"/>
+      <c r="F32" s="377"/>
+      <c r="G32" s="377"/>
+      <c r="H32" s="377"/>
+      <c r="I32" s="377"/>
+      <c r="J32" s="377"/>
+      <c r="K32" s="377"/>
+      <c r="L32" s="378"/>
       <c r="N32" s="104"/>
     </row>
     <row r="33" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="211"/>
-      <c r="B33" s="349" t="s">
+      <c r="B33" s="377" t="s">
         <v>170</v>
       </c>
-      <c r="C33" s="349"/>
-      <c r="D33" s="349"/>
-      <c r="E33" s="349"/>
-      <c r="F33" s="349"/>
-      <c r="G33" s="349"/>
-      <c r="H33" s="349"/>
-      <c r="I33" s="349"/>
-      <c r="J33" s="349"/>
-      <c r="K33" s="349"/>
-      <c r="L33" s="350"/>
+      <c r="C33" s="377"/>
+      <c r="D33" s="377"/>
+      <c r="E33" s="377"/>
+      <c r="F33" s="377"/>
+      <c r="G33" s="377"/>
+      <c r="H33" s="377"/>
+      <c r="I33" s="377"/>
+      <c r="J33" s="377"/>
+      <c r="K33" s="377"/>
+      <c r="L33" s="378"/>
       <c r="N33" s="104"/>
     </row>
     <row r="34" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="358" t="s">
+      <c r="A34" s="379" t="s">
         <v>176</v>
       </c>
-      <c r="B34" s="359"/>
-      <c r="C34" s="359"/>
-      <c r="D34" s="359"/>
-      <c r="E34" s="359"/>
-      <c r="F34" s="359"/>
-      <c r="G34" s="359"/>
-      <c r="H34" s="359"/>
-      <c r="I34" s="359"/>
-      <c r="J34" s="359"/>
-      <c r="K34" s="359"/>
-      <c r="L34" s="360"/>
+      <c r="B34" s="380"/>
+      <c r="C34" s="380"/>
+      <c r="D34" s="380"/>
+      <c r="E34" s="380"/>
+      <c r="F34" s="380"/>
+      <c r="G34" s="380"/>
+      <c r="H34" s="380"/>
+      <c r="I34" s="380"/>
+      <c r="J34" s="380"/>
+      <c r="K34" s="380"/>
+      <c r="L34" s="381"/>
       <c r="N34" s="104"/>
     </row>
     <row r="35" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="211">
         <v>1</v>
       </c>
-      <c r="B35" s="349" t="s">
+      <c r="B35" s="377" t="s">
         <v>171</v>
       </c>
-      <c r="C35" s="349"/>
-      <c r="D35" s="349"/>
-      <c r="E35" s="349"/>
-      <c r="F35" s="349"/>
-      <c r="G35" s="349"/>
-      <c r="H35" s="349"/>
-      <c r="I35" s="349"/>
-      <c r="J35" s="349"/>
-      <c r="K35" s="349"/>
-      <c r="L35" s="350"/>
+      <c r="C35" s="377"/>
+      <c r="D35" s="377"/>
+      <c r="E35" s="377"/>
+      <c r="F35" s="377"/>
+      <c r="G35" s="377"/>
+      <c r="H35" s="377"/>
+      <c r="I35" s="377"/>
+      <c r="J35" s="377"/>
+      <c r="K35" s="377"/>
+      <c r="L35" s="378"/>
       <c r="N35" s="104"/>
     </row>
     <row r="36" spans="1:14" s="57" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="211"/>
-      <c r="B36" s="347" t="s">
+      <c r="B36" s="375" t="s">
         <v>427</v>
       </c>
-      <c r="C36" s="347"/>
-      <c r="D36" s="347"/>
-      <c r="E36" s="347"/>
-      <c r="F36" s="347"/>
-      <c r="G36" s="347"/>
-      <c r="H36" s="347"/>
-      <c r="I36" s="347"/>
-      <c r="J36" s="347"/>
-      <c r="K36" s="347"/>
-      <c r="L36" s="348"/>
+      <c r="C36" s="375"/>
+      <c r="D36" s="375"/>
+      <c r="E36" s="375"/>
+      <c r="F36" s="375"/>
+      <c r="G36" s="375"/>
+      <c r="H36" s="375"/>
+      <c r="I36" s="375"/>
+      <c r="J36" s="375"/>
+      <c r="K36" s="375"/>
+      <c r="L36" s="376"/>
       <c r="N36" s="104"/>
     </row>
     <row r="37" spans="1:14" s="57" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="211">
         <v>2</v>
       </c>
-      <c r="B37" s="349" t="s">
+      <c r="B37" s="377" t="s">
         <v>279</v>
       </c>
-      <c r="C37" s="349"/>
-      <c r="D37" s="349"/>
-      <c r="E37" s="349"/>
-      <c r="F37" s="349"/>
-      <c r="G37" s="349"/>
-      <c r="H37" s="349"/>
-      <c r="I37" s="349"/>
-      <c r="J37" s="349"/>
-      <c r="K37" s="349"/>
-      <c r="L37" s="350"/>
+      <c r="C37" s="377"/>
+      <c r="D37" s="377"/>
+      <c r="E37" s="377"/>
+      <c r="F37" s="377"/>
+      <c r="G37" s="377"/>
+      <c r="H37" s="377"/>
+      <c r="I37" s="377"/>
+      <c r="J37" s="377"/>
+      <c r="K37" s="377"/>
+      <c r="L37" s="378"/>
       <c r="N37" s="104"/>
     </row>
     <row r="38" spans="1:14" s="57" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="211">
         <v>3</v>
       </c>
-      <c r="B38" s="349" t="s">
+      <c r="B38" s="377" t="s">
         <v>269</v>
       </c>
-      <c r="C38" s="349"/>
-      <c r="D38" s="349"/>
-      <c r="E38" s="349"/>
-      <c r="F38" s="349"/>
-      <c r="G38" s="349"/>
-      <c r="H38" s="349"/>
-      <c r="I38" s="349"/>
-      <c r="J38" s="349"/>
-      <c r="K38" s="349"/>
-      <c r="L38" s="350"/>
+      <c r="C38" s="377"/>
+      <c r="D38" s="377"/>
+      <c r="E38" s="377"/>
+      <c r="F38" s="377"/>
+      <c r="G38" s="377"/>
+      <c r="H38" s="377"/>
+      <c r="I38" s="377"/>
+      <c r="J38" s="377"/>
+      <c r="K38" s="377"/>
+      <c r="L38" s="378"/>
       <c r="N38" s="104"/>
     </row>
     <row r="39" spans="1:14" s="57" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="211">
         <v>4</v>
       </c>
-      <c r="B39" s="349" t="s">
+      <c r="B39" s="377" t="s">
         <v>286</v>
       </c>
-      <c r="C39" s="349"/>
-      <c r="D39" s="349"/>
-      <c r="E39" s="349"/>
-      <c r="F39" s="349"/>
-      <c r="G39" s="349"/>
-      <c r="H39" s="349"/>
-      <c r="I39" s="349"/>
-      <c r="J39" s="349"/>
-      <c r="K39" s="349"/>
-      <c r="L39" s="350"/>
+      <c r="C39" s="377"/>
+      <c r="D39" s="377"/>
+      <c r="E39" s="377"/>
+      <c r="F39" s="377"/>
+      <c r="G39" s="377"/>
+      <c r="H39" s="377"/>
+      <c r="I39" s="377"/>
+      <c r="J39" s="377"/>
+      <c r="K39" s="377"/>
+      <c r="L39" s="378"/>
       <c r="N39" s="104"/>
     </row>
     <row r="40" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="211">
         <v>5</v>
       </c>
-      <c r="B40" s="347" t="s">
+      <c r="B40" s="375" t="s">
         <v>270</v>
       </c>
-      <c r="C40" s="347"/>
-      <c r="D40" s="347"/>
-      <c r="E40" s="347"/>
-      <c r="F40" s="347"/>
-      <c r="G40" s="347"/>
-      <c r="H40" s="347"/>
-      <c r="I40" s="347"/>
-      <c r="J40" s="347"/>
-      <c r="K40" s="347"/>
-      <c r="L40" s="348"/>
+      <c r="C40" s="375"/>
+      <c r="D40" s="375"/>
+      <c r="E40" s="375"/>
+      <c r="F40" s="375"/>
+      <c r="G40" s="375"/>
+      <c r="H40" s="375"/>
+      <c r="I40" s="375"/>
+      <c r="J40" s="375"/>
+      <c r="K40" s="375"/>
+      <c r="L40" s="376"/>
       <c r="N40" s="104"/>
     </row>
     <row r="41" spans="1:14" s="57" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="211">
         <v>6</v>
       </c>
-      <c r="B41" s="347" t="s">
+      <c r="B41" s="375" t="s">
         <v>466</v>
       </c>
-      <c r="C41" s="347"/>
-      <c r="D41" s="347"/>
-      <c r="E41" s="347"/>
-      <c r="F41" s="347"/>
-      <c r="G41" s="347"/>
-      <c r="H41" s="347"/>
-      <c r="I41" s="347"/>
-      <c r="J41" s="347"/>
-      <c r="K41" s="347"/>
-      <c r="L41" s="348"/>
+      <c r="C41" s="375"/>
+      <c r="D41" s="375"/>
+      <c r="E41" s="375"/>
+      <c r="F41" s="375"/>
+      <c r="G41" s="375"/>
+      <c r="H41" s="375"/>
+      <c r="I41" s="375"/>
+      <c r="J41" s="375"/>
+      <c r="K41" s="375"/>
+      <c r="L41" s="376"/>
       <c r="N41" s="104"/>
     </row>
     <row r="42" spans="1:14" s="57" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="211">
         <v>7</v>
       </c>
-      <c r="B42" s="349" t="s">
+      <c r="B42" s="377" t="s">
         <v>271</v>
       </c>
-      <c r="C42" s="349"/>
-      <c r="D42" s="349"/>
-      <c r="E42" s="349"/>
-      <c r="F42" s="349"/>
-      <c r="G42" s="349"/>
-      <c r="H42" s="349"/>
-      <c r="I42" s="349"/>
-      <c r="J42" s="349"/>
-      <c r="K42" s="349"/>
-      <c r="L42" s="350"/>
+      <c r="C42" s="377"/>
+      <c r="D42" s="377"/>
+      <c r="E42" s="377"/>
+      <c r="F42" s="377"/>
+      <c r="G42" s="377"/>
+      <c r="H42" s="377"/>
+      <c r="I42" s="377"/>
+      <c r="J42" s="377"/>
+      <c r="K42" s="377"/>
+      <c r="L42" s="378"/>
     </row>
     <row r="43" spans="1:14" s="57" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="211"/>
@@ -16752,56 +16752,56 @@
       <c r="L43" s="213"/>
     </row>
     <row r="44" spans="1:14" s="57" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="358" t="s">
+      <c r="A44" s="379" t="s">
         <v>274</v>
       </c>
-      <c r="B44" s="359"/>
-      <c r="C44" s="359"/>
-      <c r="D44" s="359"/>
-      <c r="E44" s="359"/>
-      <c r="F44" s="359"/>
-      <c r="G44" s="359"/>
-      <c r="H44" s="359"/>
-      <c r="I44" s="359"/>
-      <c r="J44" s="359"/>
-      <c r="K44" s="359"/>
-      <c r="L44" s="360"/>
+      <c r="B44" s="380"/>
+      <c r="C44" s="380"/>
+      <c r="D44" s="380"/>
+      <c r="E44" s="380"/>
+      <c r="F44" s="380"/>
+      <c r="G44" s="380"/>
+      <c r="H44" s="380"/>
+      <c r="I44" s="380"/>
+      <c r="J44" s="380"/>
+      <c r="K44" s="380"/>
+      <c r="L44" s="381"/>
     </row>
     <row r="45" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="214" t="s">
         <v>272</v>
       </c>
-      <c r="B45" s="349" t="s">
+      <c r="B45" s="377" t="s">
         <v>172</v>
       </c>
-      <c r="C45" s="349"/>
-      <c r="D45" s="349"/>
-      <c r="E45" s="349"/>
-      <c r="F45" s="349"/>
-      <c r="G45" s="349"/>
-      <c r="H45" s="349"/>
-      <c r="I45" s="349"/>
-      <c r="J45" s="349"/>
-      <c r="K45" s="349"/>
-      <c r="L45" s="350"/>
+      <c r="C45" s="377"/>
+      <c r="D45" s="377"/>
+      <c r="E45" s="377"/>
+      <c r="F45" s="377"/>
+      <c r="G45" s="377"/>
+      <c r="H45" s="377"/>
+      <c r="I45" s="377"/>
+      <c r="J45" s="377"/>
+      <c r="K45" s="377"/>
+      <c r="L45" s="378"/>
     </row>
     <row r="46" spans="1:14" s="57" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="215" t="s">
         <v>273</v>
       </c>
-      <c r="B46" s="351" t="s">
+      <c r="B46" s="387" t="s">
         <v>275</v>
       </c>
-      <c r="C46" s="351"/>
-      <c r="D46" s="351"/>
-      <c r="E46" s="351"/>
-      <c r="F46" s="351"/>
-      <c r="G46" s="351"/>
-      <c r="H46" s="351"/>
-      <c r="I46" s="351"/>
-      <c r="J46" s="351"/>
-      <c r="K46" s="351"/>
-      <c r="L46" s="352"/>
+      <c r="C46" s="387"/>
+      <c r="D46" s="387"/>
+      <c r="E46" s="387"/>
+      <c r="F46" s="387"/>
+      <c r="G46" s="387"/>
+      <c r="H46" s="387"/>
+      <c r="I46" s="387"/>
+      <c r="J46" s="387"/>
+      <c r="K46" s="387"/>
+      <c r="L46" s="388"/>
     </row>
     <row r="47" spans="1:14" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="157"/>
@@ -16818,20 +16818,20 @@
       <c r="L47" s="110"/>
     </row>
     <row r="48" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="353" t="s">
+      <c r="A48" s="389" t="s">
         <v>200</v>
       </c>
-      <c r="B48" s="354"/>
-      <c r="C48" s="354"/>
-      <c r="D48" s="354"/>
-      <c r="E48" s="354"/>
-      <c r="F48" s="354"/>
-      <c r="G48" s="354"/>
-      <c r="H48" s="354"/>
-      <c r="I48" s="354"/>
-      <c r="J48" s="354"/>
-      <c r="K48" s="354"/>
-      <c r="L48" s="355"/>
+      <c r="B48" s="390"/>
+      <c r="C48" s="390"/>
+      <c r="D48" s="390"/>
+      <c r="E48" s="390"/>
+      <c r="F48" s="390"/>
+      <c r="G48" s="390"/>
+      <c r="H48" s="390"/>
+      <c r="I48" s="390"/>
+      <c r="J48" s="390"/>
+      <c r="K48" s="390"/>
+      <c r="L48" s="391"/>
     </row>
     <row r="49" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="218" t="s">
@@ -16919,126 +16919,126 @@
       <c r="B54" s="165" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="356" t="s">
+      <c r="C54" s="340" t="s">
         <v>262</v>
       </c>
-      <c r="D54" s="356"/>
-      <c r="E54" s="356"/>
-      <c r="F54" s="356"/>
-      <c r="G54" s="356"/>
-      <c r="H54" s="356"/>
-      <c r="I54" s="356"/>
-      <c r="J54" s="356"/>
-      <c r="K54" s="356"/>
-      <c r="L54" s="357"/>
+      <c r="D54" s="340"/>
+      <c r="E54" s="340"/>
+      <c r="F54" s="340"/>
+      <c r="G54" s="340"/>
+      <c r="H54" s="340"/>
+      <c r="I54" s="340"/>
+      <c r="J54" s="340"/>
+      <c r="K54" s="340"/>
+      <c r="L54" s="361"/>
     </row>
     <row r="55" spans="1:12" s="56" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="164"/>
       <c r="B55" s="165" t="s">
         <v>263</v>
       </c>
-      <c r="C55" s="356" t="s">
+      <c r="C55" s="340" t="s">
         <v>264</v>
       </c>
-      <c r="D55" s="356"/>
-      <c r="E55" s="356"/>
-      <c r="F55" s="356"/>
-      <c r="G55" s="356"/>
-      <c r="H55" s="356"/>
-      <c r="I55" s="356"/>
-      <c r="J55" s="356"/>
-      <c r="K55" s="356"/>
-      <c r="L55" s="357"/>
+      <c r="D55" s="340"/>
+      <c r="E55" s="340"/>
+      <c r="F55" s="340"/>
+      <c r="G55" s="340"/>
+      <c r="H55" s="340"/>
+      <c r="I55" s="340"/>
+      <c r="J55" s="340"/>
+      <c r="K55" s="340"/>
+      <c r="L55" s="361"/>
     </row>
     <row r="56" spans="1:12" s="56" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="164"/>
       <c r="B56" s="165" t="s">
         <v>328</v>
       </c>
-      <c r="C56" s="356" t="s">
+      <c r="C56" s="340" t="s">
         <v>329</v>
       </c>
-      <c r="D56" s="356"/>
-      <c r="E56" s="356"/>
-      <c r="F56" s="356"/>
-      <c r="G56" s="356"/>
-      <c r="H56" s="356"/>
-      <c r="I56" s="356"/>
-      <c r="J56" s="356"/>
-      <c r="K56" s="356"/>
-      <c r="L56" s="357"/>
+      <c r="D56" s="340"/>
+      <c r="E56" s="340"/>
+      <c r="F56" s="340"/>
+      <c r="G56" s="340"/>
+      <c r="H56" s="340"/>
+      <c r="I56" s="340"/>
+      <c r="J56" s="340"/>
+      <c r="K56" s="340"/>
+      <c r="L56" s="361"/>
     </row>
     <row r="57" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="164"/>
       <c r="B57" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="C57" s="356" t="s">
+      <c r="C57" s="340" t="s">
         <v>99</v>
       </c>
-      <c r="D57" s="356"/>
-      <c r="E57" s="356"/>
-      <c r="F57" s="356"/>
-      <c r="G57" s="356"/>
-      <c r="H57" s="356"/>
-      <c r="I57" s="356"/>
-      <c r="J57" s="356"/>
-      <c r="K57" s="356"/>
-      <c r="L57" s="357"/>
+      <c r="D57" s="340"/>
+      <c r="E57" s="340"/>
+      <c r="F57" s="340"/>
+      <c r="G57" s="340"/>
+      <c r="H57" s="340"/>
+      <c r="I57" s="340"/>
+      <c r="J57" s="340"/>
+      <c r="K57" s="340"/>
+      <c r="L57" s="361"/>
     </row>
     <row r="58" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="164"/>
       <c r="B58" s="165" t="s">
         <v>198</v>
       </c>
-      <c r="C58" s="356" t="s">
+      <c r="C58" s="340" t="s">
         <v>199</v>
       </c>
-      <c r="D58" s="356"/>
-      <c r="E58" s="356"/>
-      <c r="F58" s="356"/>
-      <c r="G58" s="356"/>
-      <c r="H58" s="356"/>
-      <c r="I58" s="356"/>
-      <c r="J58" s="356"/>
-      <c r="K58" s="356"/>
-      <c r="L58" s="357"/>
+      <c r="D58" s="340"/>
+      <c r="E58" s="340"/>
+      <c r="F58" s="340"/>
+      <c r="G58" s="340"/>
+      <c r="H58" s="340"/>
+      <c r="I58" s="340"/>
+      <c r="J58" s="340"/>
+      <c r="K58" s="340"/>
+      <c r="L58" s="361"/>
     </row>
     <row r="59" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="164"/>
       <c r="B59" s="165" t="s">
         <v>163</v>
       </c>
-      <c r="C59" s="356" t="s">
+      <c r="C59" s="340" t="s">
         <v>468</v>
       </c>
-      <c r="D59" s="442"/>
-      <c r="E59" s="442"/>
-      <c r="F59" s="442"/>
-      <c r="G59" s="442"/>
-      <c r="H59" s="442"/>
-      <c r="I59" s="442"/>
-      <c r="J59" s="442"/>
-      <c r="K59" s="442"/>
-      <c r="L59" s="443"/>
+      <c r="D59" s="341"/>
+      <c r="E59" s="341"/>
+      <c r="F59" s="341"/>
+      <c r="G59" s="341"/>
+      <c r="H59" s="341"/>
+      <c r="I59" s="341"/>
+      <c r="J59" s="341"/>
+      <c r="K59" s="341"/>
+      <c r="L59" s="342"/>
     </row>
     <row r="60" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="164"/>
       <c r="B60" s="165" t="s">
         <v>394</v>
       </c>
-      <c r="C60" s="356" t="s">
+      <c r="C60" s="340" t="s">
         <v>395</v>
       </c>
-      <c r="D60" s="356"/>
-      <c r="E60" s="356"/>
-      <c r="F60" s="356"/>
-      <c r="G60" s="356"/>
-      <c r="H60" s="356"/>
-      <c r="I60" s="356"/>
-      <c r="J60" s="356"/>
-      <c r="K60" s="356"/>
-      <c r="L60" s="357"/>
+      <c r="D60" s="340"/>
+      <c r="E60" s="340"/>
+      <c r="F60" s="340"/>
+      <c r="G60" s="340"/>
+      <c r="H60" s="340"/>
+      <c r="I60" s="340"/>
+      <c r="J60" s="340"/>
+      <c r="K60" s="340"/>
+      <c r="L60" s="361"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="164"/>
@@ -17156,25 +17156,57 @@
       </c>
     </row>
     <row r="82" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="346" t="s">
+      <c r="A82" s="386" t="s">
         <v>398</v>
       </c>
-      <c r="B82" s="346"/>
-      <c r="C82" s="346"/>
-      <c r="D82" s="346"/>
-      <c r="E82" s="346"/>
-      <c r="F82" s="346"/>
-      <c r="G82" s="346"/>
-      <c r="H82" s="346"/>
-      <c r="I82" s="346"/>
-      <c r="J82" s="346"/>
-      <c r="K82" s="346"/>
-      <c r="L82" s="346"/>
+      <c r="B82" s="386"/>
+      <c r="C82" s="386"/>
+      <c r="D82" s="386"/>
+      <c r="E82" s="386"/>
+      <c r="F82" s="386"/>
+      <c r="G82" s="386"/>
+      <c r="H82" s="386"/>
+      <c r="I82" s="386"/>
+      <c r="J82" s="386"/>
+      <c r="K82" s="386"/>
+      <c r="L82" s="386"/>
     </row>
     <row r="87" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="88" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="A82:L82"/>
+    <mergeCell ref="B41:L41"/>
+    <mergeCell ref="B42:L42"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="A48:L48"/>
+    <mergeCell ref="C54:L54"/>
+    <mergeCell ref="C57:L57"/>
+    <mergeCell ref="C58:L58"/>
+    <mergeCell ref="C55:L55"/>
+    <mergeCell ref="C60:L60"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="B40:L40"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B30:L30"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B39:L39"/>
     <mergeCell ref="C59:L59"/>
     <mergeCell ref="A26:L26"/>
     <mergeCell ref="A1:L1"/>
@@ -17191,38 +17223,6 @@
     <mergeCell ref="B7:L7"/>
     <mergeCell ref="B8:L8"/>
     <mergeCell ref="A10:L10"/>
-    <mergeCell ref="B11:L11"/>
-    <mergeCell ref="C56:L56"/>
-    <mergeCell ref="B40:L40"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="B14:L14"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="A82:L82"/>
-    <mergeCell ref="B41:L41"/>
-    <mergeCell ref="B42:L42"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="A48:L48"/>
-    <mergeCell ref="C54:L54"/>
-    <mergeCell ref="C57:L57"/>
-    <mergeCell ref="C58:L58"/>
-    <mergeCell ref="C55:L55"/>
-    <mergeCell ref="C60:L60"/>
-    <mergeCell ref="A44:L44"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A67" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -17260,82 +17260,82 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="434" t="s">
+      <c r="A3" s="436" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="434"/>
-      <c r="C3" s="434"/>
+      <c r="B3" s="436"/>
+      <c r="C3" s="436"/>
       <c r="D3" s="125" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="435" t="s">
+      <c r="A4" s="437" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="435"/>
-      <c r="C4" s="435"/>
+      <c r="B4" s="437"/>
+      <c r="C4" s="437"/>
       <c r="D4" s="172" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="439" t="s">
+      <c r="A5" s="441" t="s">
         <v>183</v>
       </c>
-      <c r="B5" s="436"/>
-      <c r="C5" s="436"/>
+      <c r="B5" s="438"/>
+      <c r="C5" s="438"/>
       <c r="D5" s="173" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="437" t="s">
+      <c r="A6" s="439" t="s">
         <v>184</v>
       </c>
-      <c r="B6" s="437"/>
-      <c r="C6" s="437"/>
+      <c r="B6" s="439"/>
+      <c r="C6" s="439"/>
       <c r="D6" s="174" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="438" t="s">
+      <c r="A7" s="440" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="438"/>
-      <c r="C7" s="438"/>
+      <c r="B7" s="440"/>
+      <c r="C7" s="440"/>
       <c r="D7" s="175" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="435" t="s">
+      <c r="A11" s="437" t="s">
         <v>112</v>
       </c>
-      <c r="B11" s="435"/>
-      <c r="C11" s="435"/>
+      <c r="B11" s="437"/>
+      <c r="C11" s="437"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="436" t="s">
+      <c r="A12" s="438" t="s">
         <v>113</v>
       </c>
-      <c r="B12" s="436"/>
-      <c r="C12" s="436"/>
+      <c r="B12" s="438"/>
+      <c r="C12" s="438"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="437" t="s">
+      <c r="A13" s="439" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="437"/>
-      <c r="C13" s="437"/>
+      <c r="B13" s="439"/>
+      <c r="C13" s="439"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="438" t="s">
+      <c r="A14" s="440" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="438"/>
-      <c r="C14" s="438"/>
+      <c r="B14" s="440"/>
+      <c r="C14" s="440"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -17606,28 +17606,28 @@
       </c>
     </row>
     <row r="2" spans="1:20" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="440" t="s">
+      <c r="A2" s="442" t="s">
         <v>421</v>
       </c>
-      <c r="B2" s="441"/>
-      <c r="C2" s="441"/>
-      <c r="D2" s="441"/>
-      <c r="E2" s="441"/>
-      <c r="F2" s="441"/>
-      <c r="G2" s="441"/>
-      <c r="H2" s="441"/>
-      <c r="I2" s="441"/>
-      <c r="J2" s="441"/>
-      <c r="K2" s="441"/>
-      <c r="L2" s="441"/>
-      <c r="M2" s="441"/>
-      <c r="N2" s="441"/>
-      <c r="O2" s="441"/>
-      <c r="P2" s="441"/>
-      <c r="Q2" s="441"/>
-      <c r="R2" s="441"/>
-      <c r="S2" s="441"/>
-      <c r="T2" s="441"/>
+      <c r="B2" s="443"/>
+      <c r="C2" s="443"/>
+      <c r="D2" s="443"/>
+      <c r="E2" s="443"/>
+      <c r="F2" s="443"/>
+      <c r="G2" s="443"/>
+      <c r="H2" s="443"/>
+      <c r="I2" s="443"/>
+      <c r="J2" s="443"/>
+      <c r="K2" s="443"/>
+      <c r="L2" s="443"/>
+      <c r="M2" s="443"/>
+      <c r="N2" s="443"/>
+      <c r="O2" s="443"/>
+      <c r="P2" s="443"/>
+      <c r="Q2" s="443"/>
+      <c r="R2" s="443"/>
+      <c r="S2" s="443"/>
+      <c r="T2" s="443"/>
     </row>
     <row r="3" spans="1:20" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:20" ht="32" x14ac:dyDescent="0.2">
@@ -18340,7 +18340,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9BF02C3-B992-44C7-A79C-D1E41573911A}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -18963,7 +18963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5BF7D8F-86F3-47E9-AB85-EE9B4CAB70E4}">
   <dimension ref="A1:P145"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A93" zoomScale="125" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C112" sqref="C112"/>
     </sheetView>
   </sheetViews>
@@ -18993,16 +18993,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="390" t="str">
+      <c r="A1" s="392" t="str">
         <f>'ReadMe-Directions'!A1</f>
         <v>Immersive Model for Lake Mead based on the Principle of Divide Reservoir Inflow</v>
       </c>
-      <c r="B1" s="390"/>
-      <c r="C1" s="390"/>
-      <c r="D1" s="390"/>
-      <c r="E1" s="390"/>
-      <c r="F1" s="390"/>
-      <c r="G1" s="390"/>
+      <c r="B1" s="392"/>
+      <c r="C1" s="392"/>
+      <c r="D1" s="392"/>
+      <c r="E1" s="392"/>
+      <c r="F1" s="392"/>
+      <c r="G1" s="392"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -19011,15 +19011,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="398" t="s">
+      <c r="A3" s="400" t="s">
         <v>190</v>
       </c>
-      <c r="B3" s="398"/>
-      <c r="C3" s="398"/>
-      <c r="D3" s="398"/>
-      <c r="E3" s="398"/>
-      <c r="F3" s="398"/>
-      <c r="G3" s="398"/>
+      <c r="B3" s="400"/>
+      <c r="C3" s="400"/>
+      <c r="D3" s="400"/>
+      <c r="E3" s="400"/>
+      <c r="F3" s="400"/>
+      <c r="G3" s="400"/>
       <c r="H3" s="82"/>
       <c r="I3" s="82"/>
       <c r="J3" s="82"/>
@@ -19035,13 +19035,13 @@
       <c r="B4" s="124" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="399" t="s">
+      <c r="C4" s="401" t="s">
         <v>259</v>
       </c>
-      <c r="D4" s="400"/>
-      <c r="E4" s="400"/>
-      <c r="F4" s="400"/>
-      <c r="G4" s="401"/>
+      <c r="D4" s="402"/>
+      <c r="E4" s="402"/>
+      <c r="F4" s="402"/>
+      <c r="G4" s="403"/>
       <c r="N4" s="138" t="s">
         <v>330</v>
       </c>
@@ -19051,11 +19051,11 @@
         <v>238</v>
       </c>
       <c r="B5" s="111"/>
-      <c r="C5" s="402"/>
-      <c r="D5" s="397"/>
-      <c r="E5" s="397"/>
-      <c r="F5" s="397"/>
-      <c r="G5" s="397"/>
+      <c r="C5" s="404"/>
+      <c r="D5" s="399"/>
+      <c r="E5" s="399"/>
+      <c r="F5" s="399"/>
+      <c r="G5" s="399"/>
       <c r="N5" s="138"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -19063,11 +19063,11 @@
         <v>202</v>
       </c>
       <c r="B6" s="111"/>
-      <c r="C6" s="402"/>
-      <c r="D6" s="397"/>
-      <c r="E6" s="397"/>
-      <c r="F6" s="397"/>
-      <c r="G6" s="397"/>
+      <c r="C6" s="404"/>
+      <c r="D6" s="399"/>
+      <c r="E6" s="399"/>
+      <c r="F6" s="399"/>
+      <c r="G6" s="399"/>
       <c r="N6" s="139"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -19075,11 +19075,11 @@
         <v>203</v>
       </c>
       <c r="B7" s="111"/>
-      <c r="C7" s="402"/>
-      <c r="D7" s="397"/>
-      <c r="E7" s="397"/>
-      <c r="F7" s="397"/>
-      <c r="G7" s="397"/>
+      <c r="C7" s="404"/>
+      <c r="D7" s="399"/>
+      <c r="E7" s="399"/>
+      <c r="F7" s="399"/>
+      <c r="G7" s="399"/>
       <c r="N7" s="139"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -19087,11 +19087,11 @@
         <v>204</v>
       </c>
       <c r="B8" s="88"/>
-      <c r="C8" s="397"/>
-      <c r="D8" s="397"/>
-      <c r="E8" s="397"/>
-      <c r="F8" s="397"/>
-      <c r="G8" s="397"/>
+      <c r="C8" s="399"/>
+      <c r="D8" s="399"/>
+      <c r="E8" s="399"/>
+      <c r="F8" s="399"/>
+      <c r="G8" s="399"/>
       <c r="N8" s="139"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -19099,11 +19099,11 @@
         <v>18</v>
       </c>
       <c r="B9" s="88"/>
-      <c r="C9" s="403"/>
-      <c r="D9" s="403"/>
-      <c r="E9" s="403"/>
-      <c r="F9" s="403"/>
-      <c r="G9" s="403"/>
+      <c r="C9" s="405"/>
+      <c r="D9" s="405"/>
+      <c r="E9" s="405"/>
+      <c r="F9" s="405"/>
+      <c r="G9" s="405"/>
       <c r="N9" s="139"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -19111,11 +19111,11 @@
         <v>278</v>
       </c>
       <c r="B10" s="88"/>
-      <c r="C10" s="397"/>
-      <c r="D10" s="397"/>
-      <c r="E10" s="397"/>
-      <c r="F10" s="397"/>
-      <c r="G10" s="397"/>
+      <c r="C10" s="399"/>
+      <c r="D10" s="399"/>
+      <c r="E10" s="399"/>
+      <c r="F10" s="399"/>
+      <c r="G10" s="399"/>
       <c r="N10" s="139"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -19128,36 +19128,36 @@
       <c r="A12" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="B12" s="404" t="s">
+      <c r="B12" s="406" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="405"/>
-      <c r="D12" s="406"/>
+      <c r="C12" s="407"/>
+      <c r="D12" s="408"/>
       <c r="N12" s="138" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="407" t="s">
+      <c r="B13" s="409" t="s">
         <v>189</v>
       </c>
-      <c r="C13" s="408"/>
-      <c r="D13" s="409"/>
+      <c r="C13" s="410"/>
+      <c r="D13" s="411"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="391" t="s">
+      <c r="B14" s="393" t="s">
         <v>184</v>
       </c>
-      <c r="C14" s="392"/>
-      <c r="D14" s="393"/>
+      <c r="C14" s="394"/>
+      <c r="D14" s="395"/>
       <c r="N14" s="139"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="394" t="s">
+      <c r="B15" s="396" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="395"/>
-      <c r="D15" s="396"/>
+      <c r="C15" s="397"/>
+      <c r="D15" s="398"/>
       <c r="N15" s="139"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -24640,8 +24640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA15763-059F-401A-BB99-8A737E404CC4}">
   <dimension ref="A1:BF51"/>
   <sheetViews>
-    <sheetView zoomScale="50" zoomScaleNormal="279" workbookViewId="0">
-      <selection activeCell="AD8" sqref="AD8"/>
+    <sheetView tabSelected="1" topLeftCell="J17" zoomScale="132" zoomScaleNormal="279" workbookViewId="0">
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -24713,23 +24713,23 @@
       <c r="G5" s="186" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="423" t="s">
+      <c r="I5" s="420" t="s">
         <v>424</v>
       </c>
-      <c r="J5" s="424"/>
-      <c r="K5" s="424"/>
-      <c r="L5" s="424"/>
-      <c r="M5" s="424"/>
-      <c r="N5" s="424"/>
-      <c r="O5" s="424"/>
-      <c r="P5" s="424"/>
-      <c r="Q5" s="424"/>
-      <c r="R5" s="424"/>
-      <c r="S5" s="424"/>
-      <c r="T5" s="424"/>
-      <c r="U5" s="424"/>
-      <c r="V5" s="424"/>
-      <c r="W5" s="425"/>
+      <c r="J5" s="421"/>
+      <c r="K5" s="421"/>
+      <c r="L5" s="421"/>
+      <c r="M5" s="421"/>
+      <c r="N5" s="421"/>
+      <c r="O5" s="421"/>
+      <c r="P5" s="421"/>
+      <c r="Q5" s="421"/>
+      <c r="R5" s="421"/>
+      <c r="S5" s="421"/>
+      <c r="T5" s="421"/>
+      <c r="U5" s="421"/>
+      <c r="V5" s="421"/>
+      <c r="W5" s="422"/>
       <c r="Y5" s="193"/>
       <c r="Z5" s="193"/>
       <c r="AA5" s="193"/>
@@ -24744,31 +24744,31 @@
       <c r="E6" s="413"/>
       <c r="F6" s="413"/>
       <c r="G6" s="414"/>
-      <c r="I6" s="426" t="s">
+      <c r="I6" s="423" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="410" t="s">
+      <c r="J6" s="425" t="s">
         <v>410</v>
       </c>
-      <c r="K6" s="410" t="s">
+      <c r="K6" s="425" t="s">
         <v>409</v>
       </c>
-      <c r="L6" s="428" t="s">
+      <c r="L6" s="426" t="s">
         <v>215</v>
       </c>
-      <c r="M6" s="429"/>
-      <c r="N6" s="429"/>
-      <c r="O6" s="429"/>
-      <c r="P6" s="429"/>
-      <c r="Q6" s="430"/>
-      <c r="R6" s="415" t="s">
+      <c r="M6" s="427"/>
+      <c r="N6" s="427"/>
+      <c r="O6" s="427"/>
+      <c r="P6" s="427"/>
+      <c r="Q6" s="428"/>
+      <c r="R6" s="429" t="s">
         <v>216</v>
       </c>
-      <c r="S6" s="416"/>
-      <c r="T6" s="416"/>
-      <c r="U6" s="416"/>
-      <c r="V6" s="416"/>
-      <c r="W6" s="417"/>
+      <c r="S6" s="430"/>
+      <c r="T6" s="430"/>
+      <c r="U6" s="430"/>
+      <c r="V6" s="430"/>
+      <c r="W6" s="431"/>
       <c r="Y6" s="309"/>
       <c r="Z6" s="309"/>
       <c r="AA6" s="309"/>
@@ -24794,9 +24794,9 @@
         <f>SUM(C7:F7)</f>
         <v>0</v>
       </c>
-      <c r="I7" s="427"/>
-      <c r="J7" s="427"/>
-      <c r="K7" s="427"/>
+      <c r="I7" s="424"/>
+      <c r="J7" s="424"/>
+      <c r="K7" s="424"/>
       <c r="L7" s="187" t="s">
         <v>411</v>
       </c>
@@ -25000,14 +25000,14 @@
       <c r="AZ9" s="287"/>
     </row>
     <row r="10" spans="1:53" s="193" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B10" s="418" t="s">
+      <c r="B10" s="415" t="s">
         <v>237</v>
       </c>
-      <c r="C10" s="418"/>
-      <c r="D10" s="418"/>
-      <c r="E10" s="418"/>
-      <c r="F10" s="418"/>
-      <c r="G10" s="418"/>
+      <c r="C10" s="415"/>
+      <c r="D10" s="415"/>
+      <c r="E10" s="415"/>
+      <c r="F10" s="415"/>
+      <c r="G10" s="415"/>
       <c r="I10" s="246" t="s">
         <v>231</v>
       </c>
@@ -25491,13 +25491,13 @@
       <c r="B16" s="194" t="s">
         <v>234</v>
       </c>
-      <c r="C16" s="419" t="s">
+      <c r="C16" s="416" t="s">
         <v>235</v>
       </c>
-      <c r="D16" s="420"/>
-      <c r="E16" s="420"/>
-      <c r="F16" s="420"/>
-      <c r="G16" s="421"/>
+      <c r="D16" s="417"/>
+      <c r="E16" s="417"/>
+      <c r="F16" s="417"/>
+      <c r="G16" s="418"/>
       <c r="I16" s="246" t="s">
         <v>405</v>
       </c>
@@ -25613,34 +25613,34 @@
     </row>
     <row r="18" spans="2:58" s="193" customFormat="1" ht="14" x14ac:dyDescent="0.15"/>
     <row r="19" spans="2:58" s="193" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I19" s="422" t="s">
+      <c r="I19" s="419" t="s">
         <v>425</v>
       </c>
-      <c r="J19" s="422"/>
-      <c r="K19" s="422"/>
-      <c r="L19" s="422"/>
-      <c r="M19" s="422"/>
-      <c r="N19" s="422"/>
-      <c r="O19" s="422"/>
-      <c r="P19" s="422"/>
-      <c r="Q19" s="422"/>
-      <c r="R19" s="422"/>
-      <c r="S19" s="422"/>
-      <c r="T19" s="422"/>
-      <c r="U19" s="422"/>
+      <c r="J19" s="419"/>
+      <c r="K19" s="419"/>
+      <c r="L19" s="419"/>
+      <c r="M19" s="419"/>
+      <c r="N19" s="419"/>
+      <c r="O19" s="419"/>
+      <c r="P19" s="419"/>
+      <c r="Q19" s="419"/>
+      <c r="R19" s="419"/>
+      <c r="S19" s="419"/>
+      <c r="T19" s="419"/>
+      <c r="U19" s="419"/>
       <c r="Z19" s="252"/>
       <c r="AA19" s="252"/>
       <c r="AB19" s="252"/>
       <c r="AC19" s="252"/>
     </row>
     <row r="20" spans="2:58" s="193" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I20" s="410" t="s">
+      <c r="I20" s="425" t="s">
         <v>13</v>
       </c>
-      <c r="J20" s="410" t="s">
+      <c r="J20" s="425" t="s">
         <v>213</v>
       </c>
-      <c r="K20" s="410" t="s">
+      <c r="K20" s="425" t="s">
         <v>214</v>
       </c>
       <c r="L20" s="412" t="s">
@@ -25650,22 +25650,22 @@
       <c r="N20" s="413"/>
       <c r="O20" s="413"/>
       <c r="P20" s="414"/>
-      <c r="Q20" s="415" t="s">
+      <c r="Q20" s="429" t="s">
         <v>216</v>
       </c>
-      <c r="R20" s="416"/>
-      <c r="S20" s="416"/>
-      <c r="T20" s="416"/>
-      <c r="U20" s="417"/>
+      <c r="R20" s="430"/>
+      <c r="S20" s="430"/>
+      <c r="T20" s="430"/>
+      <c r="U20" s="431"/>
       <c r="Z20" s="256"/>
       <c r="AA20" s="256"/>
       <c r="AB20" s="256"/>
       <c r="AC20" s="256"/>
     </row>
     <row r="21" spans="2:58" s="193" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I21" s="411"/>
-      <c r="J21" s="411"/>
-      <c r="K21" s="411"/>
+      <c r="I21" s="432"/>
+      <c r="J21" s="432"/>
+      <c r="K21" s="432"/>
       <c r="L21" s="187" t="s">
         <v>218</v>
       </c>
@@ -25747,7 +25747,9 @@
         <f>SUM(Q22:T22)</f>
         <v>1</v>
       </c>
-      <c r="V22" s="260"/>
+      <c r="V22" s="193" t="s">
+        <v>432</v>
+      </c>
       <c r="W22" s="260"/>
       <c r="AF22" s="338"/>
     </row>
@@ -26685,6 +26687,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:P20"/>
+    <mergeCell ref="Q20:U20"/>
     <mergeCell ref="B6:G6"/>
     <mergeCell ref="B10:G10"/>
     <mergeCell ref="C16:G16"/>
@@ -26695,11 +26702,6 @@
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="L6:Q6"/>
     <mergeCell ref="R6:W6"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:P20"/>
-    <mergeCell ref="Q20:U20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -27042,16 +27044,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="432" t="e">
+      <c r="A1" s="433" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B1" s="432"/>
-      <c r="C1" s="432"/>
-      <c r="D1" s="432"/>
-      <c r="E1" s="432"/>
-      <c r="F1" s="432"/>
-      <c r="G1" s="432"/>
+      <c r="B1" s="433"/>
+      <c r="C1" s="433"/>
+      <c r="D1" s="433"/>
+      <c r="E1" s="433"/>
+      <c r="F1" s="433"/>
+      <c r="G1" s="433"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -27060,15 +27062,15 @@
       <c r="B2" s="1"/>
     </row>
     <row r="3" spans="1:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="398" t="s">
+      <c r="A3" s="400" t="s">
         <v>177</v>
       </c>
-      <c r="B3" s="398"/>
-      <c r="C3" s="398"/>
-      <c r="D3" s="398"/>
-      <c r="E3" s="398"/>
-      <c r="F3" s="398"/>
-      <c r="G3" s="398"/>
+      <c r="B3" s="400"/>
+      <c r="C3" s="400"/>
+      <c r="D3" s="400"/>
+      <c r="E3" s="400"/>
+      <c r="F3" s="400"/>
+      <c r="G3" s="400"/>
       <c r="H3" s="82"/>
       <c r="I3" s="82"/>
       <c r="J3" s="82"/>
@@ -27084,13 +27086,13 @@
       <c r="B4" s="124" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="399" t="s">
+      <c r="C4" s="401" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="400"/>
-      <c r="E4" s="400"/>
-      <c r="F4" s="400"/>
-      <c r="G4" s="401"/>
+      <c r="D4" s="402"/>
+      <c r="E4" s="402"/>
+      <c r="F4" s="402"/>
+      <c r="G4" s="403"/>
       <c r="N4" s="136" t="s">
         <v>128</v>
       </c>
@@ -27100,11 +27102,11 @@
         <v>16</v>
       </c>
       <c r="B5" s="111"/>
-      <c r="C5" s="402"/>
-      <c r="D5" s="397"/>
-      <c r="E5" s="397"/>
-      <c r="F5" s="397"/>
-      <c r="G5" s="397"/>
+      <c r="C5" s="404"/>
+      <c r="D5" s="399"/>
+      <c r="E5" s="399"/>
+      <c r="F5" s="399"/>
+      <c r="G5" s="399"/>
       <c r="N5" s="139"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -27112,11 +27114,11 @@
         <v>17</v>
       </c>
       <c r="B6" s="111"/>
-      <c r="C6" s="402"/>
-      <c r="D6" s="397"/>
-      <c r="E6" s="397"/>
-      <c r="F6" s="397"/>
-      <c r="G6" s="397"/>
+      <c r="C6" s="404"/>
+      <c r="D6" s="399"/>
+      <c r="E6" s="399"/>
+      <c r="F6" s="399"/>
+      <c r="G6" s="399"/>
       <c r="N6" s="139"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -27124,11 +27126,11 @@
         <v>18</v>
       </c>
       <c r="B7" s="111"/>
-      <c r="C7" s="402"/>
-      <c r="D7" s="397"/>
-      <c r="E7" s="397"/>
-      <c r="F7" s="397"/>
-      <c r="G7" s="397"/>
+      <c r="C7" s="404"/>
+      <c r="D7" s="399"/>
+      <c r="E7" s="399"/>
+      <c r="F7" s="399"/>
+      <c r="G7" s="399"/>
       <c r="N7" s="139"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -27136,11 +27138,11 @@
         <v>39</v>
       </c>
       <c r="B8" s="88"/>
-      <c r="C8" s="397"/>
-      <c r="D8" s="397"/>
-      <c r="E8" s="397"/>
-      <c r="F8" s="397"/>
-      <c r="G8" s="397"/>
+      <c r="C8" s="399"/>
+      <c r="D8" s="399"/>
+      <c r="E8" s="399"/>
+      <c r="F8" s="399"/>
+      <c r="G8" s="399"/>
       <c r="N8" s="139"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -27148,11 +27150,11 @@
         <v>162</v>
       </c>
       <c r="B9" s="88"/>
-      <c r="C9" s="403"/>
-      <c r="D9" s="403"/>
-      <c r="E9" s="403"/>
-      <c r="F9" s="403"/>
-      <c r="G9" s="403"/>
+      <c r="C9" s="405"/>
+      <c r="D9" s="405"/>
+      <c r="E9" s="405"/>
+      <c r="F9" s="405"/>
+      <c r="G9" s="405"/>
       <c r="N9" s="139"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -27160,11 +27162,11 @@
         <v>40</v>
       </c>
       <c r="B10" s="112"/>
-      <c r="C10" s="431"/>
-      <c r="D10" s="431"/>
-      <c r="E10" s="431"/>
-      <c r="F10" s="431"/>
-      <c r="G10" s="431"/>
+      <c r="C10" s="434"/>
+      <c r="D10" s="434"/>
+      <c r="E10" s="434"/>
+      <c r="F10" s="434"/>
+      <c r="G10" s="434"/>
       <c r="N10" s="139"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -27177,37 +27179,37 @@
       <c r="A12" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="B12" s="404" t="s">
+      <c r="B12" s="406" t="s">
         <v>112</v>
       </c>
-      <c r="C12" s="405"/>
-      <c r="D12" s="406"/>
+      <c r="C12" s="407"/>
+      <c r="D12" s="408"/>
       <c r="N12" s="138" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="407" t="s">
+      <c r="B13" s="409" t="s">
         <v>113</v>
       </c>
-      <c r="C13" s="408"/>
-      <c r="D13" s="409"/>
+      <c r="C13" s="410"/>
+      <c r="D13" s="411"/>
       <c r="N13" s="139"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="391" t="s">
+      <c r="B14" s="393" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="392"/>
-      <c r="D14" s="393"/>
+      <c r="C14" s="394"/>
+      <c r="D14" s="395"/>
       <c r="N14" s="139"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="394" t="s">
+      <c r="B15" s="396" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="395"/>
-      <c r="D15" s="396"/>
+      <c r="C15" s="397"/>
+      <c r="D15" s="398"/>
       <c r="N15" s="139"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
@@ -28427,12 +28429,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C7:G7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="C5:G5"/>
-    <mergeCell ref="C6:G6"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
@@ -28440,6 +28436,12 @@
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="C4:G4"/>
+    <mergeCell ref="C5:G5"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N4" r:id="rId1" location="step-1-assign-parties-person-playing-and-strategies" xr:uid="{726B234F-7B54-4D33-A192-8F1604C6B04C}"/>
@@ -28497,26 +28499,26 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="D3" s="433" t="s">
+      <c r="D3" s="435" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="433"/>
-      <c r="F3" s="433" t="s">
+      <c r="E3" s="435"/>
+      <c r="F3" s="435" t="s">
         <v>60</v>
       </c>
-      <c r="G3" s="433"/>
-      <c r="H3" s="433"/>
-      <c r="I3" s="433" t="s">
+      <c r="G3" s="435"/>
+      <c r="H3" s="435"/>
+      <c r="I3" s="435" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="433"/>
-      <c r="K3" s="433"/>
+      <c r="J3" s="435"/>
+      <c r="K3" s="435"/>
       <c r="L3" s="131"/>
-      <c r="M3" s="433" t="s">
+      <c r="M3" s="435" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="433"/>
-      <c r="O3" s="433"/>
+      <c r="N3" s="435"/>
+      <c r="O3" s="435"/>
     </row>
     <row r="4" spans="1:16" s="45" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="44" t="s">

</xml_diff>

<commit_message>
Changes in Model Guide to inflow calculations
</commit_message>
<xml_diff>
--- a/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
+++ b/LakeMeadWaterBankDivideInflow/LakeMeadWaterBankDivideInflow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCollaborate\LakeMeadWaterBankDivideInflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BD1880-9C35-4982-A4AC-2D0235F4488B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7DA72A-9BA8-4C2A-92F8-B5011E4A92BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1965" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{5373AB19-D84C-490D-97DC-C516D358024A}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="470">
   <si>
     <t>Year 1</t>
   </si>
@@ -1956,10 +1956,6 @@
 [F]</t>
   </si>
   <si>
-    <t>Tribal
-Nations [T]</t>
-  </si>
-  <si>
     <t>Lake Mead Inflow
 (maf per year) [B]</t>
   </si>
@@ -2289,6 +2285,17 @@
   </si>
   <si>
     <t>Chosen for percentage split if no Tribal User</t>
+  </si>
+  <si>
+    <t>Tribal
+Nations [G]</t>
+  </si>
+  <si>
+    <t>Tribal
+Nations [L]</t>
+  </si>
+  <si>
+    <t>Total [M]</t>
   </si>
 </sst>
 </file>
@@ -4088,67 +4095,44 @@
     <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="32" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="19" fillId="32" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="32" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="172" fontId="19" fillId="32" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="32" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="27" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="1" fillId="27" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4211,6 +4195,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4243,6 +4230,63 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="21" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="27" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="27" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="27" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="2" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="3" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="4" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4304,12 +4348,6 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4318,15 +4356,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4358,6 +4387,9 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="19" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4367,11 +4399,23 @@
     <xf numFmtId="0" fontId="18" fillId="19" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4399,43 +4443,6 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="32" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="19" fillId="32" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="32" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="172" fontId="19" fillId="32" borderId="9" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="32" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="14">
@@ -16059,20 +16066,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="364" t="s">
+      <c r="A1" s="357" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="364"/>
-      <c r="C1" s="364"/>
-      <c r="D1" s="364"/>
-      <c r="E1" s="364"/>
-      <c r="F1" s="364"/>
-      <c r="G1" s="364"/>
-      <c r="H1" s="364"/>
-      <c r="I1" s="364"/>
-      <c r="J1" s="364"/>
-      <c r="K1" s="364"/>
-      <c r="L1" s="364"/>
+      <c r="B1" s="357"/>
+      <c r="C1" s="357"/>
+      <c r="D1" s="357"/>
+      <c r="E1" s="357"/>
+      <c r="F1" s="357"/>
+      <c r="G1" s="357"/>
+      <c r="H1" s="357"/>
+      <c r="I1" s="357"/>
+      <c r="J1" s="357"/>
+      <c r="K1" s="357"/>
+      <c r="L1" s="357"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
@@ -16098,41 +16105,41 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:18" s="52" customFormat="1" ht="56.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="365" t="s">
+      <c r="A4" s="358" t="s">
         <v>296</v>
       </c>
-      <c r="B4" s="366"/>
-      <c r="C4" s="366"/>
-      <c r="D4" s="366"/>
-      <c r="E4" s="366"/>
-      <c r="F4" s="366"/>
-      <c r="G4" s="366"/>
-      <c r="H4" s="366"/>
-      <c r="I4" s="366"/>
-      <c r="J4" s="366"/>
-      <c r="K4" s="366"/>
-      <c r="L4" s="367"/>
-      <c r="N4" s="368"/>
-      <c r="O4" s="368"/>
-      <c r="P4" s="368"/>
-      <c r="Q4" s="368"/>
-      <c r="R4" s="368"/>
+      <c r="B4" s="359"/>
+      <c r="C4" s="359"/>
+      <c r="D4" s="359"/>
+      <c r="E4" s="359"/>
+      <c r="F4" s="359"/>
+      <c r="G4" s="359"/>
+      <c r="H4" s="359"/>
+      <c r="I4" s="359"/>
+      <c r="J4" s="359"/>
+      <c r="K4" s="359"/>
+      <c r="L4" s="360"/>
+      <c r="N4" s="361"/>
+      <c r="O4" s="361"/>
+      <c r="P4" s="361"/>
+      <c r="Q4" s="361"/>
+      <c r="R4" s="361"/>
     </row>
     <row r="5" spans="1:18" s="52" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="369" t="s">
+      <c r="A5" s="362" t="s">
         <v>280</v>
       </c>
-      <c r="B5" s="370"/>
-      <c r="C5" s="370"/>
-      <c r="D5" s="370"/>
-      <c r="E5" s="370"/>
-      <c r="F5" s="370"/>
-      <c r="G5" s="370"/>
-      <c r="H5" s="370"/>
-      <c r="I5" s="370"/>
-      <c r="J5" s="370"/>
-      <c r="K5" s="370"/>
-      <c r="L5" s="371"/>
+      <c r="B5" s="363"/>
+      <c r="C5" s="363"/>
+      <c r="D5" s="363"/>
+      <c r="E5" s="363"/>
+      <c r="F5" s="363"/>
+      <c r="G5" s="363"/>
+      <c r="H5" s="363"/>
+      <c r="I5" s="363"/>
+      <c r="J5" s="363"/>
+      <c r="K5" s="363"/>
+      <c r="L5" s="364"/>
       <c r="N5" s="110"/>
       <c r="O5" s="110"/>
       <c r="P5" s="110"/>
@@ -16140,20 +16147,20 @@
       <c r="R5" s="110"/>
     </row>
     <row r="6" spans="1:18" s="52" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="369" t="s">
+      <c r="A6" s="362" t="s">
         <v>297</v>
       </c>
-      <c r="B6" s="370"/>
-      <c r="C6" s="370"/>
-      <c r="D6" s="370"/>
-      <c r="E6" s="370"/>
-      <c r="F6" s="370"/>
-      <c r="G6" s="370"/>
-      <c r="H6" s="370"/>
-      <c r="I6" s="370"/>
-      <c r="J6" s="370"/>
-      <c r="K6" s="370"/>
-      <c r="L6" s="371"/>
+      <c r="B6" s="363"/>
+      <c r="C6" s="363"/>
+      <c r="D6" s="363"/>
+      <c r="E6" s="363"/>
+      <c r="F6" s="363"/>
+      <c r="G6" s="363"/>
+      <c r="H6" s="363"/>
+      <c r="I6" s="363"/>
+      <c r="J6" s="363"/>
+      <c r="K6" s="363"/>
+      <c r="L6" s="364"/>
       <c r="N6" s="110"/>
       <c r="O6" s="110"/>
       <c r="P6" s="110"/>
@@ -16162,19 +16169,19 @@
     </row>
     <row r="7" spans="1:18" s="52" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="216"/>
-      <c r="B7" s="370" t="s">
+      <c r="B7" s="363" t="s">
         <v>298</v>
       </c>
-      <c r="C7" s="370"/>
-      <c r="D7" s="370"/>
-      <c r="E7" s="370"/>
-      <c r="F7" s="370"/>
-      <c r="G7" s="370"/>
-      <c r="H7" s="370"/>
-      <c r="I7" s="370"/>
-      <c r="J7" s="370"/>
-      <c r="K7" s="370"/>
-      <c r="L7" s="371"/>
+      <c r="C7" s="363"/>
+      <c r="D7" s="363"/>
+      <c r="E7" s="363"/>
+      <c r="F7" s="363"/>
+      <c r="G7" s="363"/>
+      <c r="H7" s="363"/>
+      <c r="I7" s="363"/>
+      <c r="J7" s="363"/>
+      <c r="K7" s="363"/>
+      <c r="L7" s="364"/>
       <c r="N7" s="110"/>
       <c r="O7" s="110"/>
       <c r="P7" s="110"/>
@@ -16183,19 +16190,19 @@
     </row>
     <row r="8" spans="1:18" s="52" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="217"/>
-      <c r="B8" s="385" t="s">
+      <c r="B8" s="379" t="s">
         <v>299</v>
       </c>
-      <c r="C8" s="385"/>
-      <c r="D8" s="385"/>
-      <c r="E8" s="385"/>
-      <c r="F8" s="385"/>
-      <c r="G8" s="385"/>
-      <c r="H8" s="385"/>
-      <c r="I8" s="385"/>
-      <c r="J8" s="385"/>
-      <c r="K8" s="385"/>
-      <c r="L8" s="386"/>
+      <c r="C8" s="379"/>
+      <c r="D8" s="379"/>
+      <c r="E8" s="379"/>
+      <c r="F8" s="379"/>
+      <c r="G8" s="379"/>
+      <c r="H8" s="379"/>
+      <c r="I8" s="379"/>
+      <c r="J8" s="379"/>
+      <c r="K8" s="379"/>
+      <c r="L8" s="380"/>
       <c r="N8" s="110"/>
       <c r="O8" s="110"/>
       <c r="P8" s="110"/>
@@ -16217,38 +16224,38 @@
       <c r="L9" s="110"/>
     </row>
     <row r="10" spans="1:18" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="387" t="s">
+      <c r="A10" s="381" t="s">
         <v>334</v>
       </c>
-      <c r="B10" s="388"/>
-      <c r="C10" s="388"/>
-      <c r="D10" s="388"/>
-      <c r="E10" s="388"/>
-      <c r="F10" s="388"/>
-      <c r="G10" s="388"/>
-      <c r="H10" s="388"/>
-      <c r="I10" s="388"/>
-      <c r="J10" s="388"/>
-      <c r="K10" s="388"/>
-      <c r="L10" s="389"/>
+      <c r="B10" s="382"/>
+      <c r="C10" s="382"/>
+      <c r="D10" s="382"/>
+      <c r="E10" s="382"/>
+      <c r="F10" s="382"/>
+      <c r="G10" s="382"/>
+      <c r="H10" s="382"/>
+      <c r="I10" s="382"/>
+      <c r="J10" s="382"/>
+      <c r="K10" s="382"/>
+      <c r="L10" s="383"/>
     </row>
     <row r="11" spans="1:18" s="56" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="237" t="s">
         <v>335</v>
       </c>
-      <c r="B11" s="340" t="s">
+      <c r="B11" s="384" t="s">
         <v>338</v>
       </c>
-      <c r="C11" s="340"/>
-      <c r="D11" s="340"/>
-      <c r="E11" s="340"/>
-      <c r="F11" s="340"/>
-      <c r="G11" s="340"/>
-      <c r="H11" s="340"/>
-      <c r="I11" s="340"/>
-      <c r="J11" s="340"/>
-      <c r="K11" s="340"/>
-      <c r="L11" s="341"/>
+      <c r="C11" s="384"/>
+      <c r="D11" s="384"/>
+      <c r="E11" s="384"/>
+      <c r="F11" s="384"/>
+      <c r="G11" s="384"/>
+      <c r="H11" s="384"/>
+      <c r="I11" s="384"/>
+      <c r="J11" s="384"/>
+      <c r="K11" s="384"/>
+      <c r="L11" s="385"/>
     </row>
     <row r="12" spans="1:18" s="57" customFormat="1" ht="161.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="229"/>
@@ -16268,51 +16275,51 @@
       <c r="A13" s="237" t="s">
         <v>336</v>
       </c>
-      <c r="B13" s="340" t="s">
+      <c r="B13" s="384" t="s">
         <v>339</v>
       </c>
-      <c r="C13" s="340"/>
-      <c r="D13" s="340"/>
-      <c r="E13" s="340"/>
-      <c r="F13" s="340"/>
-      <c r="G13" s="340"/>
-      <c r="H13" s="340"/>
-      <c r="I13" s="340"/>
-      <c r="J13" s="340"/>
-      <c r="K13" s="340"/>
-      <c r="L13" s="341"/>
+      <c r="C13" s="384"/>
+      <c r="D13" s="384"/>
+      <c r="E13" s="384"/>
+      <c r="F13" s="384"/>
+      <c r="G13" s="384"/>
+      <c r="H13" s="384"/>
+      <c r="I13" s="384"/>
+      <c r="J13" s="384"/>
+      <c r="K13" s="384"/>
+      <c r="L13" s="385"/>
     </row>
     <row r="14" spans="1:18" s="57" customFormat="1" ht="90.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="229"/>
-      <c r="B14" s="342"/>
-      <c r="C14" s="342"/>
-      <c r="D14" s="342"/>
-      <c r="E14" s="342"/>
-      <c r="F14" s="342"/>
-      <c r="G14" s="342"/>
-      <c r="H14" s="342"/>
-      <c r="I14" s="342"/>
-      <c r="J14" s="342"/>
-      <c r="K14" s="342"/>
-      <c r="L14" s="343"/>
+      <c r="B14" s="395"/>
+      <c r="C14" s="395"/>
+      <c r="D14" s="395"/>
+      <c r="E14" s="395"/>
+      <c r="F14" s="395"/>
+      <c r="G14" s="395"/>
+      <c r="H14" s="395"/>
+      <c r="I14" s="395"/>
+      <c r="J14" s="395"/>
+      <c r="K14" s="395"/>
+      <c r="L14" s="396"/>
     </row>
     <row r="15" spans="1:18" s="56" customFormat="1" ht="29" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="237" t="s">
         <v>337</v>
       </c>
-      <c r="B15" s="340" t="s">
-        <v>462</v>
-      </c>
-      <c r="C15" s="340"/>
-      <c r="D15" s="340"/>
-      <c r="E15" s="340"/>
-      <c r="F15" s="340"/>
-      <c r="G15" s="340"/>
-      <c r="H15" s="340"/>
-      <c r="I15" s="340"/>
-      <c r="J15" s="340"/>
-      <c r="K15" s="340"/>
-      <c r="L15" s="341"/>
+      <c r="B15" s="384" t="s">
+        <v>461</v>
+      </c>
+      <c r="C15" s="384"/>
+      <c r="D15" s="384"/>
+      <c r="E15" s="384"/>
+      <c r="F15" s="384"/>
+      <c r="G15" s="384"/>
+      <c r="H15" s="384"/>
+      <c r="I15" s="384"/>
+      <c r="J15" s="384"/>
+      <c r="K15" s="384"/>
+      <c r="L15" s="385"/>
     </row>
     <row r="16" spans="1:18" s="57" customFormat="1" ht="269" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="229"/>
@@ -16329,12 +16336,12 @@
       <c r="L16" s="236"/>
     </row>
     <row r="17" spans="1:14" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="338" t="s">
+      <c r="A17" s="393" t="s">
         <v>343</v>
       </c>
-      <c r="B17" s="339"/>
-      <c r="C17" s="339"/>
-      <c r="D17" s="339"/>
+      <c r="B17" s="394"/>
+      <c r="C17" s="394"/>
+      <c r="D17" s="394"/>
       <c r="E17" s="234" t="s">
         <v>344</v>
       </c>
@@ -16361,84 +16368,84 @@
       <c r="L18" s="110"/>
     </row>
     <row r="19" spans="1:14" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="372" t="s">
+      <c r="A19" s="365" t="s">
         <v>165</v>
       </c>
-      <c r="B19" s="373"/>
-      <c r="C19" s="373"/>
-      <c r="D19" s="373"/>
-      <c r="E19" s="373"/>
-      <c r="F19" s="373"/>
-      <c r="G19" s="373"/>
-      <c r="H19" s="373"/>
-      <c r="I19" s="373"/>
-      <c r="J19" s="373"/>
-      <c r="K19" s="373"/>
-      <c r="L19" s="374"/>
+      <c r="B19" s="366"/>
+      <c r="C19" s="366"/>
+      <c r="D19" s="366"/>
+      <c r="E19" s="366"/>
+      <c r="F19" s="366"/>
+      <c r="G19" s="366"/>
+      <c r="H19" s="366"/>
+      <c r="I19" s="366"/>
+      <c r="J19" s="366"/>
+      <c r="K19" s="366"/>
+      <c r="L19" s="367"/>
     </row>
     <row r="20" spans="1:14" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="375" t="s">
+      <c r="A20" s="368" t="s">
         <v>281</v>
       </c>
-      <c r="B20" s="376"/>
-      <c r="C20" s="376"/>
-      <c r="D20" s="376"/>
-      <c r="E20" s="376"/>
-      <c r="F20" s="376"/>
-      <c r="G20" s="376"/>
-      <c r="H20" s="376"/>
-      <c r="I20" s="376"/>
-      <c r="J20" s="376"/>
-      <c r="K20" s="376"/>
-      <c r="L20" s="377"/>
+      <c r="B20" s="369"/>
+      <c r="C20" s="369"/>
+      <c r="D20" s="369"/>
+      <c r="E20" s="369"/>
+      <c r="F20" s="369"/>
+      <c r="G20" s="369"/>
+      <c r="H20" s="369"/>
+      <c r="I20" s="369"/>
+      <c r="J20" s="369"/>
+      <c r="K20" s="369"/>
+      <c r="L20" s="370"/>
     </row>
     <row r="21" spans="1:14" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="378" t="s">
+      <c r="A21" s="371" t="s">
         <v>282</v>
       </c>
-      <c r="B21" s="354"/>
-      <c r="C21" s="354"/>
-      <c r="D21" s="354"/>
-      <c r="E21" s="354"/>
-      <c r="F21" s="354"/>
-      <c r="G21" s="354"/>
-      <c r="H21" s="354"/>
-      <c r="I21" s="354"/>
-      <c r="J21" s="354"/>
-      <c r="K21" s="354"/>
-      <c r="L21" s="355"/>
+      <c r="B21" s="351"/>
+      <c r="C21" s="351"/>
+      <c r="D21" s="351"/>
+      <c r="E21" s="351"/>
+      <c r="F21" s="351"/>
+      <c r="G21" s="351"/>
+      <c r="H21" s="351"/>
+      <c r="I21" s="351"/>
+      <c r="J21" s="351"/>
+      <c r="K21" s="351"/>
+      <c r="L21" s="372"/>
     </row>
     <row r="22" spans="1:14" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="378" t="s">
+      <c r="A22" s="371" t="s">
         <v>166</v>
       </c>
-      <c r="B22" s="354"/>
-      <c r="C22" s="354"/>
-      <c r="D22" s="354"/>
-      <c r="E22" s="354"/>
-      <c r="F22" s="354"/>
-      <c r="G22" s="354"/>
-      <c r="H22" s="354"/>
-      <c r="I22" s="354"/>
-      <c r="J22" s="354"/>
-      <c r="K22" s="354"/>
-      <c r="L22" s="355"/>
+      <c r="B22" s="351"/>
+      <c r="C22" s="351"/>
+      <c r="D22" s="351"/>
+      <c r="E22" s="351"/>
+      <c r="F22" s="351"/>
+      <c r="G22" s="351"/>
+      <c r="H22" s="351"/>
+      <c r="I22" s="351"/>
+      <c r="J22" s="351"/>
+      <c r="K22" s="351"/>
+      <c r="L22" s="372"/>
     </row>
     <row r="23" spans="1:14" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="379" t="s">
+      <c r="A23" s="373" t="s">
         <v>283</v>
       </c>
-      <c r="B23" s="380"/>
-      <c r="C23" s="380"/>
-      <c r="D23" s="380"/>
-      <c r="E23" s="380"/>
-      <c r="F23" s="380"/>
-      <c r="G23" s="380"/>
-      <c r="H23" s="380"/>
-      <c r="I23" s="380"/>
-      <c r="J23" s="380"/>
-      <c r="K23" s="380"/>
-      <c r="L23" s="381"/>
+      <c r="B23" s="374"/>
+      <c r="C23" s="374"/>
+      <c r="D23" s="374"/>
+      <c r="E23" s="374"/>
+      <c r="F23" s="374"/>
+      <c r="G23" s="374"/>
+      <c r="H23" s="374"/>
+      <c r="I23" s="374"/>
+      <c r="J23" s="374"/>
+      <c r="K23" s="374"/>
+      <c r="L23" s="375"/>
     </row>
     <row r="24" spans="1:14" s="57" customFormat="1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="110"/>
@@ -16455,332 +16462,332 @@
       <c r="L24" s="110"/>
     </row>
     <row r="25" spans="1:14" s="57" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="382" t="s">
+      <c r="A25" s="376" t="s">
         <v>279</v>
       </c>
-      <c r="B25" s="383"/>
-      <c r="C25" s="383"/>
-      <c r="D25" s="383"/>
-      <c r="E25" s="383"/>
-      <c r="F25" s="383"/>
-      <c r="G25" s="383"/>
-      <c r="H25" s="383"/>
-      <c r="I25" s="383"/>
-      <c r="J25" s="383"/>
-      <c r="K25" s="383"/>
-      <c r="L25" s="384"/>
+      <c r="B25" s="377"/>
+      <c r="C25" s="377"/>
+      <c r="D25" s="377"/>
+      <c r="E25" s="377"/>
+      <c r="F25" s="377"/>
+      <c r="G25" s="377"/>
+      <c r="H25" s="377"/>
+      <c r="I25" s="377"/>
+      <c r="J25" s="377"/>
+      <c r="K25" s="377"/>
+      <c r="L25" s="378"/>
       <c r="N25" s="1"/>
     </row>
     <row r="26" spans="1:14" s="57" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="361" t="s">
+      <c r="A26" s="354" t="s">
         <v>175</v>
       </c>
-      <c r="B26" s="362"/>
-      <c r="C26" s="362"/>
-      <c r="D26" s="362"/>
-      <c r="E26" s="362"/>
-      <c r="F26" s="362"/>
-      <c r="G26" s="362"/>
-      <c r="H26" s="362"/>
-      <c r="I26" s="362"/>
-      <c r="J26" s="362"/>
-      <c r="K26" s="362"/>
-      <c r="L26" s="363"/>
+      <c r="B26" s="355"/>
+      <c r="C26" s="355"/>
+      <c r="D26" s="355"/>
+      <c r="E26" s="355"/>
+      <c r="F26" s="355"/>
+      <c r="G26" s="355"/>
+      <c r="H26" s="355"/>
+      <c r="I26" s="355"/>
+      <c r="J26" s="355"/>
+      <c r="K26" s="355"/>
+      <c r="L26" s="356"/>
       <c r="N26" s="1"/>
     </row>
     <row r="27" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="211">
         <v>1</v>
       </c>
-      <c r="B27" s="347" t="s">
+      <c r="B27" s="388" t="s">
         <v>174</v>
       </c>
-      <c r="C27" s="347"/>
-      <c r="D27" s="347"/>
-      <c r="E27" s="347"/>
-      <c r="F27" s="347"/>
-      <c r="G27" s="347"/>
-      <c r="H27" s="347"/>
-      <c r="I27" s="347"/>
-      <c r="J27" s="347"/>
-      <c r="K27" s="347"/>
-      <c r="L27" s="348"/>
+      <c r="C27" s="388"/>
+      <c r="D27" s="388"/>
+      <c r="E27" s="388"/>
+      <c r="F27" s="388"/>
+      <c r="G27" s="388"/>
+      <c r="H27" s="388"/>
+      <c r="I27" s="388"/>
+      <c r="J27" s="388"/>
+      <c r="K27" s="388"/>
+      <c r="L27" s="389"/>
     </row>
     <row r="28" spans="1:14" s="57" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="211">
         <v>2</v>
       </c>
-      <c r="B28" s="347" t="s">
+      <c r="B28" s="388" t="s">
         <v>275</v>
       </c>
-      <c r="C28" s="347"/>
-      <c r="D28" s="347"/>
-      <c r="E28" s="347"/>
-      <c r="F28" s="347"/>
-      <c r="G28" s="347"/>
-      <c r="H28" s="347"/>
-      <c r="I28" s="347"/>
-      <c r="J28" s="347"/>
-      <c r="K28" s="347"/>
-      <c r="L28" s="348"/>
+      <c r="C28" s="388"/>
+      <c r="D28" s="388"/>
+      <c r="E28" s="388"/>
+      <c r="F28" s="388"/>
+      <c r="G28" s="388"/>
+      <c r="H28" s="388"/>
+      <c r="I28" s="388"/>
+      <c r="J28" s="388"/>
+      <c r="K28" s="388"/>
+      <c r="L28" s="389"/>
       <c r="N28" s="104"/>
     </row>
     <row r="29" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="211">
         <v>3</v>
       </c>
-      <c r="B29" s="347" t="s">
+      <c r="B29" s="388" t="s">
         <v>167</v>
       </c>
-      <c r="C29" s="347"/>
-      <c r="D29" s="347"/>
-      <c r="E29" s="347"/>
-      <c r="F29" s="347"/>
-      <c r="G29" s="347"/>
-      <c r="H29" s="347"/>
-      <c r="I29" s="347"/>
-      <c r="J29" s="347"/>
-      <c r="K29" s="347"/>
-      <c r="L29" s="348"/>
+      <c r="C29" s="388"/>
+      <c r="D29" s="388"/>
+      <c r="E29" s="388"/>
+      <c r="F29" s="388"/>
+      <c r="G29" s="388"/>
+      <c r="H29" s="388"/>
+      <c r="I29" s="388"/>
+      <c r="J29" s="388"/>
+      <c r="K29" s="388"/>
+      <c r="L29" s="389"/>
       <c r="N29" s="104"/>
     </row>
     <row r="30" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="211">
         <v>4</v>
       </c>
-      <c r="B30" s="347" t="s">
+      <c r="B30" s="388" t="s">
         <v>284</v>
       </c>
-      <c r="C30" s="347"/>
-      <c r="D30" s="347"/>
-      <c r="E30" s="347"/>
-      <c r="F30" s="347"/>
-      <c r="G30" s="347"/>
-      <c r="H30" s="347"/>
-      <c r="I30" s="347"/>
-      <c r="J30" s="347"/>
-      <c r="K30" s="347"/>
-      <c r="L30" s="348"/>
+      <c r="C30" s="388"/>
+      <c r="D30" s="388"/>
+      <c r="E30" s="388"/>
+      <c r="F30" s="388"/>
+      <c r="G30" s="388"/>
+      <c r="H30" s="388"/>
+      <c r="I30" s="388"/>
+      <c r="J30" s="388"/>
+      <c r="K30" s="388"/>
+      <c r="L30" s="389"/>
       <c r="N30" s="104"/>
     </row>
     <row r="31" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="211">
         <v>5</v>
       </c>
-      <c r="B31" s="347" t="s">
+      <c r="B31" s="388" t="s">
         <v>168</v>
       </c>
-      <c r="C31" s="347"/>
-      <c r="D31" s="347"/>
-      <c r="E31" s="347"/>
-      <c r="F31" s="347"/>
-      <c r="G31" s="347"/>
-      <c r="H31" s="347"/>
-      <c r="I31" s="347"/>
-      <c r="J31" s="347"/>
-      <c r="K31" s="347"/>
-      <c r="L31" s="348"/>
+      <c r="C31" s="388"/>
+      <c r="D31" s="388"/>
+      <c r="E31" s="388"/>
+      <c r="F31" s="388"/>
+      <c r="G31" s="388"/>
+      <c r="H31" s="388"/>
+      <c r="I31" s="388"/>
+      <c r="J31" s="388"/>
+      <c r="K31" s="388"/>
+      <c r="L31" s="389"/>
       <c r="N31" s="104"/>
     </row>
     <row r="32" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="211"/>
-      <c r="B32" s="347" t="s">
+      <c r="B32" s="388" t="s">
         <v>169</v>
       </c>
-      <c r="C32" s="347"/>
-      <c r="D32" s="347"/>
-      <c r="E32" s="347"/>
-      <c r="F32" s="347"/>
-      <c r="G32" s="347"/>
-      <c r="H32" s="347"/>
-      <c r="I32" s="347"/>
-      <c r="J32" s="347"/>
-      <c r="K32" s="347"/>
-      <c r="L32" s="348"/>
+      <c r="C32" s="388"/>
+      <c r="D32" s="388"/>
+      <c r="E32" s="388"/>
+      <c r="F32" s="388"/>
+      <c r="G32" s="388"/>
+      <c r="H32" s="388"/>
+      <c r="I32" s="388"/>
+      <c r="J32" s="388"/>
+      <c r="K32" s="388"/>
+      <c r="L32" s="389"/>
       <c r="N32" s="104"/>
     </row>
     <row r="33" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="211"/>
-      <c r="B33" s="347" t="s">
+      <c r="B33" s="388" t="s">
         <v>170</v>
       </c>
-      <c r="C33" s="347"/>
-      <c r="D33" s="347"/>
-      <c r="E33" s="347"/>
-      <c r="F33" s="347"/>
-      <c r="G33" s="347"/>
-      <c r="H33" s="347"/>
-      <c r="I33" s="347"/>
-      <c r="J33" s="347"/>
-      <c r="K33" s="347"/>
-      <c r="L33" s="348"/>
+      <c r="C33" s="388"/>
+      <c r="D33" s="388"/>
+      <c r="E33" s="388"/>
+      <c r="F33" s="388"/>
+      <c r="G33" s="388"/>
+      <c r="H33" s="388"/>
+      <c r="I33" s="388"/>
+      <c r="J33" s="388"/>
+      <c r="K33" s="388"/>
+      <c r="L33" s="389"/>
       <c r="N33" s="104"/>
     </row>
     <row r="34" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="356" t="s">
+      <c r="A34" s="390" t="s">
         <v>176</v>
       </c>
-      <c r="B34" s="357"/>
-      <c r="C34" s="357"/>
-      <c r="D34" s="357"/>
-      <c r="E34" s="357"/>
-      <c r="F34" s="357"/>
-      <c r="G34" s="357"/>
-      <c r="H34" s="357"/>
-      <c r="I34" s="357"/>
-      <c r="J34" s="357"/>
-      <c r="K34" s="357"/>
-      <c r="L34" s="358"/>
+      <c r="B34" s="391"/>
+      <c r="C34" s="391"/>
+      <c r="D34" s="391"/>
+      <c r="E34" s="391"/>
+      <c r="F34" s="391"/>
+      <c r="G34" s="391"/>
+      <c r="H34" s="391"/>
+      <c r="I34" s="391"/>
+      <c r="J34" s="391"/>
+      <c r="K34" s="391"/>
+      <c r="L34" s="392"/>
       <c r="N34" s="104"/>
     </row>
     <row r="35" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="211">
         <v>1</v>
       </c>
-      <c r="B35" s="347" t="s">
+      <c r="B35" s="388" t="s">
         <v>171</v>
       </c>
-      <c r="C35" s="347"/>
-      <c r="D35" s="347"/>
-      <c r="E35" s="347"/>
-      <c r="F35" s="347"/>
-      <c r="G35" s="347"/>
-      <c r="H35" s="347"/>
-      <c r="I35" s="347"/>
-      <c r="J35" s="347"/>
-      <c r="K35" s="347"/>
-      <c r="L35" s="348"/>
+      <c r="C35" s="388"/>
+      <c r="D35" s="388"/>
+      <c r="E35" s="388"/>
+      <c r="F35" s="388"/>
+      <c r="G35" s="388"/>
+      <c r="H35" s="388"/>
+      <c r="I35" s="388"/>
+      <c r="J35" s="388"/>
+      <c r="K35" s="388"/>
+      <c r="L35" s="389"/>
       <c r="N35" s="104"/>
     </row>
     <row r="36" spans="1:14" s="57" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="211"/>
-      <c r="B36" s="345" t="s">
-        <v>425</v>
-      </c>
-      <c r="C36" s="345"/>
-      <c r="D36" s="345"/>
-      <c r="E36" s="345"/>
-      <c r="F36" s="345"/>
-      <c r="G36" s="345"/>
-      <c r="H36" s="345"/>
-      <c r="I36" s="345"/>
-      <c r="J36" s="345"/>
-      <c r="K36" s="345"/>
-      <c r="L36" s="346"/>
+      <c r="B36" s="386" t="s">
+        <v>424</v>
+      </c>
+      <c r="C36" s="386"/>
+      <c r="D36" s="386"/>
+      <c r="E36" s="386"/>
+      <c r="F36" s="386"/>
+      <c r="G36" s="386"/>
+      <c r="H36" s="386"/>
+      <c r="I36" s="386"/>
+      <c r="J36" s="386"/>
+      <c r="K36" s="386"/>
+      <c r="L36" s="387"/>
       <c r="N36" s="104"/>
     </row>
     <row r="37" spans="1:14" s="57" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="211">
         <v>2</v>
       </c>
-      <c r="B37" s="347" t="s">
+      <c r="B37" s="388" t="s">
         <v>278</v>
       </c>
-      <c r="C37" s="347"/>
-      <c r="D37" s="347"/>
-      <c r="E37" s="347"/>
-      <c r="F37" s="347"/>
-      <c r="G37" s="347"/>
-      <c r="H37" s="347"/>
-      <c r="I37" s="347"/>
-      <c r="J37" s="347"/>
-      <c r="K37" s="347"/>
-      <c r="L37" s="348"/>
+      <c r="C37" s="388"/>
+      <c r="D37" s="388"/>
+      <c r="E37" s="388"/>
+      <c r="F37" s="388"/>
+      <c r="G37" s="388"/>
+      <c r="H37" s="388"/>
+      <c r="I37" s="388"/>
+      <c r="J37" s="388"/>
+      <c r="K37" s="388"/>
+      <c r="L37" s="389"/>
       <c r="N37" s="104"/>
     </row>
     <row r="38" spans="1:14" s="57" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="211">
         <v>3</v>
       </c>
-      <c r="B38" s="347" t="s">
+      <c r="B38" s="388" t="s">
         <v>268</v>
       </c>
-      <c r="C38" s="347"/>
-      <c r="D38" s="347"/>
-      <c r="E38" s="347"/>
-      <c r="F38" s="347"/>
-      <c r="G38" s="347"/>
-      <c r="H38" s="347"/>
-      <c r="I38" s="347"/>
-      <c r="J38" s="347"/>
-      <c r="K38" s="347"/>
-      <c r="L38" s="348"/>
+      <c r="C38" s="388"/>
+      <c r="D38" s="388"/>
+      <c r="E38" s="388"/>
+      <c r="F38" s="388"/>
+      <c r="G38" s="388"/>
+      <c r="H38" s="388"/>
+      <c r="I38" s="388"/>
+      <c r="J38" s="388"/>
+      <c r="K38" s="388"/>
+      <c r="L38" s="389"/>
       <c r="N38" s="104"/>
     </row>
     <row r="39" spans="1:14" s="57" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="211">
         <v>4</v>
       </c>
-      <c r="B39" s="347" t="s">
+      <c r="B39" s="388" t="s">
         <v>285</v>
       </c>
-      <c r="C39" s="347"/>
-      <c r="D39" s="347"/>
-      <c r="E39" s="347"/>
-      <c r="F39" s="347"/>
-      <c r="G39" s="347"/>
-      <c r="H39" s="347"/>
-      <c r="I39" s="347"/>
-      <c r="J39" s="347"/>
-      <c r="K39" s="347"/>
-      <c r="L39" s="348"/>
+      <c r="C39" s="388"/>
+      <c r="D39" s="388"/>
+      <c r="E39" s="388"/>
+      <c r="F39" s="388"/>
+      <c r="G39" s="388"/>
+      <c r="H39" s="388"/>
+      <c r="I39" s="388"/>
+      <c r="J39" s="388"/>
+      <c r="K39" s="388"/>
+      <c r="L39" s="389"/>
       <c r="N39" s="104"/>
     </row>
     <row r="40" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="211">
         <v>5</v>
       </c>
-      <c r="B40" s="345" t="s">
+      <c r="B40" s="386" t="s">
         <v>269</v>
       </c>
-      <c r="C40" s="345"/>
-      <c r="D40" s="345"/>
-      <c r="E40" s="345"/>
-      <c r="F40" s="345"/>
-      <c r="G40" s="345"/>
-      <c r="H40" s="345"/>
-      <c r="I40" s="345"/>
-      <c r="J40" s="345"/>
-      <c r="K40" s="345"/>
-      <c r="L40" s="346"/>
+      <c r="C40" s="386"/>
+      <c r="D40" s="386"/>
+      <c r="E40" s="386"/>
+      <c r="F40" s="386"/>
+      <c r="G40" s="386"/>
+      <c r="H40" s="386"/>
+      <c r="I40" s="386"/>
+      <c r="J40" s="386"/>
+      <c r="K40" s="386"/>
+      <c r="L40" s="387"/>
       <c r="N40" s="104"/>
     </row>
     <row r="41" spans="1:14" s="57" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="211">
         <v>6</v>
       </c>
-      <c r="B41" s="345" t="s">
-        <v>461</v>
-      </c>
-      <c r="C41" s="345"/>
-      <c r="D41" s="345"/>
-      <c r="E41" s="345"/>
-      <c r="F41" s="345"/>
-      <c r="G41" s="345"/>
-      <c r="H41" s="345"/>
-      <c r="I41" s="345"/>
-      <c r="J41" s="345"/>
-      <c r="K41" s="345"/>
-      <c r="L41" s="346"/>
+      <c r="B41" s="386" t="s">
+        <v>460</v>
+      </c>
+      <c r="C41" s="386"/>
+      <c r="D41" s="386"/>
+      <c r="E41" s="386"/>
+      <c r="F41" s="386"/>
+      <c r="G41" s="386"/>
+      <c r="H41" s="386"/>
+      <c r="I41" s="386"/>
+      <c r="J41" s="386"/>
+      <c r="K41" s="386"/>
+      <c r="L41" s="387"/>
       <c r="N41" s="104"/>
     </row>
     <row r="42" spans="1:14" s="57" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="211">
         <v>7</v>
       </c>
-      <c r="B42" s="347" t="s">
+      <c r="B42" s="388" t="s">
         <v>270</v>
       </c>
-      <c r="C42" s="347"/>
-      <c r="D42" s="347"/>
-      <c r="E42" s="347"/>
-      <c r="F42" s="347"/>
-      <c r="G42" s="347"/>
-      <c r="H42" s="347"/>
-      <c r="I42" s="347"/>
-      <c r="J42" s="347"/>
-      <c r="K42" s="347"/>
-      <c r="L42" s="348"/>
+      <c r="C42" s="388"/>
+      <c r="D42" s="388"/>
+      <c r="E42" s="388"/>
+      <c r="F42" s="388"/>
+      <c r="G42" s="388"/>
+      <c r="H42" s="388"/>
+      <c r="I42" s="388"/>
+      <c r="J42" s="388"/>
+      <c r="K42" s="388"/>
+      <c r="L42" s="389"/>
     </row>
     <row r="43" spans="1:14" s="57" customFormat="1" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="211"/>
@@ -16797,56 +16804,56 @@
       <c r="L43" s="213"/>
     </row>
     <row r="44" spans="1:14" s="57" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="356" t="s">
+      <c r="A44" s="390" t="s">
         <v>273</v>
       </c>
-      <c r="B44" s="357"/>
-      <c r="C44" s="357"/>
-      <c r="D44" s="357"/>
-      <c r="E44" s="357"/>
-      <c r="F44" s="357"/>
-      <c r="G44" s="357"/>
-      <c r="H44" s="357"/>
-      <c r="I44" s="357"/>
-      <c r="J44" s="357"/>
-      <c r="K44" s="357"/>
-      <c r="L44" s="358"/>
+      <c r="B44" s="391"/>
+      <c r="C44" s="391"/>
+      <c r="D44" s="391"/>
+      <c r="E44" s="391"/>
+      <c r="F44" s="391"/>
+      <c r="G44" s="391"/>
+      <c r="H44" s="391"/>
+      <c r="I44" s="391"/>
+      <c r="J44" s="391"/>
+      <c r="K44" s="391"/>
+      <c r="L44" s="392"/>
     </row>
     <row r="45" spans="1:14" s="57" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="214" t="s">
         <v>271</v>
       </c>
-      <c r="B45" s="347" t="s">
+      <c r="B45" s="388" t="s">
         <v>172</v>
       </c>
-      <c r="C45" s="347"/>
-      <c r="D45" s="347"/>
-      <c r="E45" s="347"/>
-      <c r="F45" s="347"/>
-      <c r="G45" s="347"/>
-      <c r="H45" s="347"/>
-      <c r="I45" s="347"/>
-      <c r="J45" s="347"/>
-      <c r="K45" s="347"/>
-      <c r="L45" s="348"/>
+      <c r="C45" s="388"/>
+      <c r="D45" s="388"/>
+      <c r="E45" s="388"/>
+      <c r="F45" s="388"/>
+      <c r="G45" s="388"/>
+      <c r="H45" s="388"/>
+      <c r="I45" s="388"/>
+      <c r="J45" s="388"/>
+      <c r="K45" s="388"/>
+      <c r="L45" s="389"/>
     </row>
     <row r="46" spans="1:14" s="57" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="215" t="s">
         <v>272</v>
       </c>
-      <c r="B46" s="349" t="s">
+      <c r="B46" s="398" t="s">
         <v>274</v>
       </c>
-      <c r="C46" s="349"/>
-      <c r="D46" s="349"/>
-      <c r="E46" s="349"/>
-      <c r="F46" s="349"/>
-      <c r="G46" s="349"/>
-      <c r="H46" s="349"/>
-      <c r="I46" s="349"/>
-      <c r="J46" s="349"/>
-      <c r="K46" s="349"/>
-      <c r="L46" s="350"/>
+      <c r="C46" s="398"/>
+      <c r="D46" s="398"/>
+      <c r="E46" s="398"/>
+      <c r="F46" s="398"/>
+      <c r="G46" s="398"/>
+      <c r="H46" s="398"/>
+      <c r="I46" s="398"/>
+      <c r="J46" s="398"/>
+      <c r="K46" s="398"/>
+      <c r="L46" s="399"/>
     </row>
     <row r="47" spans="1:14" s="57" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="157"/>
@@ -16863,20 +16870,20 @@
       <c r="L47" s="110"/>
     </row>
     <row r="48" spans="1:14" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="351" t="s">
+      <c r="A48" s="400" t="s">
         <v>200</v>
       </c>
-      <c r="B48" s="352"/>
-      <c r="C48" s="352"/>
-      <c r="D48" s="352"/>
-      <c r="E48" s="352"/>
-      <c r="F48" s="352"/>
-      <c r="G48" s="352"/>
-      <c r="H48" s="352"/>
-      <c r="I48" s="352"/>
-      <c r="J48" s="352"/>
-      <c r="K48" s="352"/>
-      <c r="L48" s="353"/>
+      <c r="B48" s="401"/>
+      <c r="C48" s="401"/>
+      <c r="D48" s="401"/>
+      <c r="E48" s="401"/>
+      <c r="F48" s="401"/>
+      <c r="G48" s="401"/>
+      <c r="H48" s="401"/>
+      <c r="I48" s="401"/>
+      <c r="J48" s="401"/>
+      <c r="K48" s="401"/>
+      <c r="L48" s="402"/>
     </row>
     <row r="49" spans="1:12" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="218" t="s">
@@ -16929,7 +16936,7 @@
         <v>24</v>
       </c>
       <c r="C52" s="166" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D52" s="166"/>
       <c r="E52" s="166"/>
@@ -16964,126 +16971,126 @@
       <c r="B54" s="165" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="354" t="s">
+      <c r="C54" s="351" t="s">
         <v>261</v>
       </c>
-      <c r="D54" s="354"/>
-      <c r="E54" s="354"/>
-      <c r="F54" s="354"/>
-      <c r="G54" s="354"/>
-      <c r="H54" s="354"/>
-      <c r="I54" s="354"/>
-      <c r="J54" s="354"/>
-      <c r="K54" s="354"/>
-      <c r="L54" s="355"/>
+      <c r="D54" s="351"/>
+      <c r="E54" s="351"/>
+      <c r="F54" s="351"/>
+      <c r="G54" s="351"/>
+      <c r="H54" s="351"/>
+      <c r="I54" s="351"/>
+      <c r="J54" s="351"/>
+      <c r="K54" s="351"/>
+      <c r="L54" s="372"/>
     </row>
     <row r="55" spans="1:12" s="56" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="164"/>
       <c r="B55" s="165" t="s">
         <v>262</v>
       </c>
-      <c r="C55" s="354" t="s">
+      <c r="C55" s="351" t="s">
         <v>263</v>
       </c>
-      <c r="D55" s="354"/>
-      <c r="E55" s="354"/>
-      <c r="F55" s="354"/>
-      <c r="G55" s="354"/>
-      <c r="H55" s="354"/>
-      <c r="I55" s="354"/>
-      <c r="J55" s="354"/>
-      <c r="K55" s="354"/>
-      <c r="L55" s="355"/>
+      <c r="D55" s="351"/>
+      <c r="E55" s="351"/>
+      <c r="F55" s="351"/>
+      <c r="G55" s="351"/>
+      <c r="H55" s="351"/>
+      <c r="I55" s="351"/>
+      <c r="J55" s="351"/>
+      <c r="K55" s="351"/>
+      <c r="L55" s="372"/>
     </row>
     <row r="56" spans="1:12" s="56" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="164"/>
       <c r="B56" s="165" t="s">
         <v>327</v>
       </c>
-      <c r="C56" s="354" t="s">
+      <c r="C56" s="351" t="s">
         <v>328</v>
       </c>
-      <c r="D56" s="354"/>
-      <c r="E56" s="354"/>
-      <c r="F56" s="354"/>
-      <c r="G56" s="354"/>
-      <c r="H56" s="354"/>
-      <c r="I56" s="354"/>
-      <c r="J56" s="354"/>
-      <c r="K56" s="354"/>
-      <c r="L56" s="355"/>
+      <c r="D56" s="351"/>
+      <c r="E56" s="351"/>
+      <c r="F56" s="351"/>
+      <c r="G56" s="351"/>
+      <c r="H56" s="351"/>
+      <c r="I56" s="351"/>
+      <c r="J56" s="351"/>
+      <c r="K56" s="351"/>
+      <c r="L56" s="372"/>
     </row>
     <row r="57" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="164"/>
       <c r="B57" s="165" t="s">
         <v>98</v>
       </c>
-      <c r="C57" s="354" t="s">
+      <c r="C57" s="351" t="s">
         <v>99</v>
       </c>
-      <c r="D57" s="354"/>
-      <c r="E57" s="354"/>
-      <c r="F57" s="354"/>
-      <c r="G57" s="354"/>
-      <c r="H57" s="354"/>
-      <c r="I57" s="354"/>
-      <c r="J57" s="354"/>
-      <c r="K57" s="354"/>
-      <c r="L57" s="355"/>
+      <c r="D57" s="351"/>
+      <c r="E57" s="351"/>
+      <c r="F57" s="351"/>
+      <c r="G57" s="351"/>
+      <c r="H57" s="351"/>
+      <c r="I57" s="351"/>
+      <c r="J57" s="351"/>
+      <c r="K57" s="351"/>
+      <c r="L57" s="372"/>
     </row>
     <row r="58" spans="1:12" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="164"/>
       <c r="B58" s="165" t="s">
         <v>198</v>
       </c>
-      <c r="C58" s="354" t="s">
+      <c r="C58" s="351" t="s">
         <v>199</v>
       </c>
-      <c r="D58" s="354"/>
-      <c r="E58" s="354"/>
-      <c r="F58" s="354"/>
-      <c r="G58" s="354"/>
-      <c r="H58" s="354"/>
-      <c r="I58" s="354"/>
-      <c r="J58" s="354"/>
-      <c r="K58" s="354"/>
-      <c r="L58" s="355"/>
+      <c r="D58" s="351"/>
+      <c r="E58" s="351"/>
+      <c r="F58" s="351"/>
+      <c r="G58" s="351"/>
+      <c r="H58" s="351"/>
+      <c r="I58" s="351"/>
+      <c r="J58" s="351"/>
+      <c r="K58" s="351"/>
+      <c r="L58" s="372"/>
     </row>
     <row r="59" spans="1:12" ht="31" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="164"/>
       <c r="B59" s="165" t="s">
         <v>163</v>
       </c>
-      <c r="C59" s="354" t="s">
-        <v>463</v>
-      </c>
-      <c r="D59" s="359"/>
-      <c r="E59" s="359"/>
-      <c r="F59" s="359"/>
-      <c r="G59" s="359"/>
-      <c r="H59" s="359"/>
-      <c r="I59" s="359"/>
-      <c r="J59" s="359"/>
-      <c r="K59" s="359"/>
-      <c r="L59" s="360"/>
+      <c r="C59" s="351" t="s">
+        <v>462</v>
+      </c>
+      <c r="D59" s="352"/>
+      <c r="E59" s="352"/>
+      <c r="F59" s="352"/>
+      <c r="G59" s="352"/>
+      <c r="H59" s="352"/>
+      <c r="I59" s="352"/>
+      <c r="J59" s="352"/>
+      <c r="K59" s="352"/>
+      <c r="L59" s="353"/>
     </row>
     <row r="60" spans="1:12" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="164"/>
       <c r="B60" s="165" t="s">
         <v>392</v>
       </c>
-      <c r="C60" s="354" t="s">
+      <c r="C60" s="351" t="s">
         <v>393</v>
       </c>
-      <c r="D60" s="354"/>
-      <c r="E60" s="354"/>
-      <c r="F60" s="354"/>
-      <c r="G60" s="354"/>
-      <c r="H60" s="354"/>
-      <c r="I60" s="354"/>
-      <c r="J60" s="354"/>
-      <c r="K60" s="354"/>
-      <c r="L60" s="355"/>
+      <c r="D60" s="351"/>
+      <c r="E60" s="351"/>
+      <c r="F60" s="351"/>
+      <c r="G60" s="351"/>
+      <c r="H60" s="351"/>
+      <c r="I60" s="351"/>
+      <c r="J60" s="351"/>
+      <c r="K60" s="351"/>
+      <c r="L60" s="372"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A61" s="164"/>
@@ -17201,25 +17208,57 @@
       </c>
     </row>
     <row r="82" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="344" t="s">
+      <c r="A82" s="397" t="s">
         <v>396</v>
       </c>
-      <c r="B82" s="344"/>
-      <c r="C82" s="344"/>
-      <c r="D82" s="344"/>
-      <c r="E82" s="344"/>
-      <c r="F82" s="344"/>
-      <c r="G82" s="344"/>
-      <c r="H82" s="344"/>
-      <c r="I82" s="344"/>
-      <c r="J82" s="344"/>
-      <c r="K82" s="344"/>
-      <c r="L82" s="344"/>
+      <c r="B82" s="397"/>
+      <c r="C82" s="397"/>
+      <c r="D82" s="397"/>
+      <c r="E82" s="397"/>
+      <c r="F82" s="397"/>
+      <c r="G82" s="397"/>
+      <c r="H82" s="397"/>
+      <c r="I82" s="397"/>
+      <c r="J82" s="397"/>
+      <c r="K82" s="397"/>
+      <c r="L82" s="397"/>
     </row>
     <row r="87" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="88" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="B13:L13"/>
+    <mergeCell ref="B14:L14"/>
+    <mergeCell ref="B15:L15"/>
+    <mergeCell ref="A82:L82"/>
+    <mergeCell ref="B41:L41"/>
+    <mergeCell ref="B42:L42"/>
+    <mergeCell ref="B45:L45"/>
+    <mergeCell ref="B46:L46"/>
+    <mergeCell ref="A48:L48"/>
+    <mergeCell ref="C54:L54"/>
+    <mergeCell ref="C57:L57"/>
+    <mergeCell ref="C58:L58"/>
+    <mergeCell ref="C55:L55"/>
+    <mergeCell ref="C60:L60"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="C56:L56"/>
+    <mergeCell ref="B40:L40"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B28:L28"/>
+    <mergeCell ref="B29:L29"/>
+    <mergeCell ref="B30:L30"/>
+    <mergeCell ref="B31:L31"/>
+    <mergeCell ref="B32:L32"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="B36:L36"/>
+    <mergeCell ref="B38:L38"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B39:L39"/>
     <mergeCell ref="C59:L59"/>
     <mergeCell ref="A26:L26"/>
     <mergeCell ref="A1:L1"/>
@@ -17236,38 +17275,6 @@
     <mergeCell ref="B7:L7"/>
     <mergeCell ref="B8:L8"/>
     <mergeCell ref="A10:L10"/>
-    <mergeCell ref="B11:L11"/>
-    <mergeCell ref="C56:L56"/>
-    <mergeCell ref="B40:L40"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B28:L28"/>
-    <mergeCell ref="B29:L29"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="B32:L32"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="B36:L36"/>
-    <mergeCell ref="B38:L38"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="B39:L39"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="B13:L13"/>
-    <mergeCell ref="B14:L14"/>
-    <mergeCell ref="B15:L15"/>
-    <mergeCell ref="A82:L82"/>
-    <mergeCell ref="B41:L41"/>
-    <mergeCell ref="B42:L42"/>
-    <mergeCell ref="B45:L45"/>
-    <mergeCell ref="B46:L46"/>
-    <mergeCell ref="A48:L48"/>
-    <mergeCell ref="C54:L54"/>
-    <mergeCell ref="C57:L57"/>
-    <mergeCell ref="C58:L58"/>
-    <mergeCell ref="C55:L55"/>
-    <mergeCell ref="C60:L60"/>
-    <mergeCell ref="A44:L44"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A67" r:id="rId1" xr:uid="{C9866D44-2827-49D7-B9C3-89CF23FACDC1}"/>
@@ -17305,82 +17312,82 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="434" t="s">
+      <c r="A3" s="447" t="s">
         <v>116</v>
       </c>
-      <c r="B3" s="434"/>
-      <c r="C3" s="434"/>
+      <c r="B3" s="447"/>
+      <c r="C3" s="447"/>
       <c r="D3" s="125" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="435" t="s">
+      <c r="A4" s="448" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="435"/>
-      <c r="C4" s="435"/>
+      <c r="B4" s="448"/>
+      <c r="C4" s="448"/>
       <c r="D4" s="172" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="439" t="s">
+      <c r="A5" s="452" t="s">
         <v>183</v>
       </c>
-      <c r="B5" s="436"/>
-      <c r="C5" s="436"/>
+      <c r="B5" s="449"/>
+      <c r="C5" s="449"/>
       <c r="D5" s="173" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="57.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="437" t="s">
+      <c r="A6" s="450" t="s">
         <v>184</v>
       </c>
-      <c r="B6" s="437"/>
-      <c r="C6" s="437"/>
+      <c r="B6" s="450"/>
+      <c r="C6" s="450"/>
       <c r="D6" s="174" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A7" s="438" t="s">
+      <c r="A7" s="451" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="438"/>
-      <c r="C7" s="438"/>
+      <c r="B7" s="451"/>
+      <c r="C7" s="451"/>
       <c r="D7" s="175" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="435" t="s">
+      <c r="A11" s="448" t="s">
         <v>112</v>
       </c>
-      <c r="B11" s="435"/>
-      <c r="C11" s="435"/>
+      <c r="B11" s="448"/>
+      <c r="C11" s="448"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="436" t="s">
+      <c r="A12" s="449" t="s">
         <v>113</v>
       </c>
-      <c r="B12" s="436"/>
-      <c r="C12" s="436"/>
+      <c r="B12" s="449"/>
+      <c r="C12" s="449"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="437" t="s">
+      <c r="A13" s="450" t="s">
         <v>114</v>
       </c>
-      <c r="B13" s="437"/>
-      <c r="C13" s="437"/>
+      <c r="B13" s="450"/>
+      <c r="C13" s="450"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="438" t="s">
+      <c r="A14" s="451" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="438"/>
-      <c r="C14" s="438"/>
+      <c r="B14" s="451"/>
+      <c r="C14" s="451"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -17418,35 +17425,35 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="36" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C3" s="35" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="F3" s="321"/>
     </row>
     <row r="4" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="323" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B4" s="322"/>
       <c r="C4" s="322"/>
@@ -17456,7 +17463,7 @@
     </row>
     <row r="5" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="319" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B5" s="320"/>
       <c r="C5" s="320"/>
@@ -17466,16 +17473,16 @@
     </row>
     <row r="6" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="37" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B6" s="38" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C6" s="311">
         <v>0.17499999999999999</v>
       </c>
       <c r="D6" s="38" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E6" s="309">
         <v>29.8</v>
@@ -17484,7 +17491,7 @@
     </row>
     <row r="7" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="37" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B7" s="38">
         <v>2023</v>
@@ -17494,7 +17501,7 @@
         <v>3.7811999999999998E-2</v>
       </c>
       <c r="D7" s="38" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E7" s="309">
         <f>0.992+1.205+5.344+8.335</f>
@@ -17504,16 +17511,16 @@
     </row>
     <row r="8" spans="1:6" ht="17.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="37" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B8" s="38" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C8" s="311">
         <v>2.2116E-2</v>
       </c>
       <c r="D8" s="38" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E8" s="309">
         <v>4.5599999999999996</v>
@@ -17522,7 +17529,7 @@
     </row>
     <row r="9" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="319" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B9" s="320"/>
       <c r="C9" s="320"/>
@@ -17531,43 +17538,43 @@
     </row>
     <row r="10" spans="1:6" s="57" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="37" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C10" s="311">
         <v>4.0999999999999996</v>
       </c>
       <c r="D10" s="38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E10" s="309" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F10" s="318"/>
     </row>
     <row r="11" spans="1:6" s="57" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="37" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C11" s="311">
         <v>0.63121000000000005</v>
       </c>
       <c r="D11" s="38" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E11" s="309" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="F11" s="318"/>
     </row>
     <row r="12" spans="1:6" s="56" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="317" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B12" s="315"/>
       <c r="C12" s="316"/>
@@ -17577,44 +17584,44 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="37" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B13" s="21">
         <v>2021</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>436</v>
+        <v>435</v>
